<commit_message>
Updated games of 2019-04-14
</commit_message>
<xml_diff>
--- a/laval.xlsx
+++ b/laval.xlsx
@@ -1954,7 +1954,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="304">
+  <cellXfs count="305">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2363,9 +2363,6 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2404,9 +2401,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="103" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2453,27 +2447,6 @@
     <xf numFmtId="0" fontId="19" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2486,12 +2459,117 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="113" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="114" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="95" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2501,18 +2579,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="86" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="87" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="88" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="87" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="95" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2525,130 +2618,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="86" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="88" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="113" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="114" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="95" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3872,161 +3875,161 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="C1" s="268"/>
-      <c r="D1" s="268"/>
-      <c r="E1" s="268"/>
-      <c r="F1" s="268"/>
-      <c r="G1" s="268"/>
-      <c r="H1" s="268"/>
-      <c r="I1" s="268"/>
-      <c r="J1" s="268"/>
-      <c r="K1" s="268"/>
-      <c r="L1" s="268"/>
-      <c r="M1" s="268"/>
-      <c r="N1" s="268"/>
-      <c r="O1" s="268"/>
-      <c r="P1" s="269"/>
-      <c r="Q1" s="269"/>
-      <c r="R1" s="269"/>
-      <c r="S1" s="269"/>
-      <c r="T1" s="269"/>
-      <c r="U1" s="269"/>
-      <c r="V1" s="269"/>
-      <c r="W1" s="269"/>
-      <c r="X1" s="269"/>
-      <c r="Y1" s="269"/>
-      <c r="Z1" s="269"/>
-      <c r="AA1" s="269"/>
-      <c r="AB1" s="269"/>
-      <c r="AC1" s="269"/>
-      <c r="AD1" s="269"/>
-      <c r="AE1" s="269"/>
-      <c r="AF1" s="269"/>
-      <c r="AG1" s="269"/>
-      <c r="AH1" s="269"/>
-      <c r="AI1" s="269"/>
-      <c r="AJ1" s="269"/>
+      <c r="C1" s="266"/>
+      <c r="D1" s="266"/>
+      <c r="E1" s="266"/>
+      <c r="F1" s="266"/>
+      <c r="G1" s="266"/>
+      <c r="H1" s="266"/>
+      <c r="I1" s="266"/>
+      <c r="J1" s="266"/>
+      <c r="K1" s="266"/>
+      <c r="L1" s="266"/>
+      <c r="M1" s="266"/>
+      <c r="N1" s="266"/>
+      <c r="O1" s="266"/>
+      <c r="P1" s="267"/>
+      <c r="Q1" s="267"/>
+      <c r="R1" s="267"/>
+      <c r="S1" s="267"/>
+      <c r="T1" s="267"/>
+      <c r="U1" s="267"/>
+      <c r="V1" s="267"/>
+      <c r="W1" s="267"/>
+      <c r="X1" s="267"/>
+      <c r="Y1" s="267"/>
+      <c r="Z1" s="267"/>
+      <c r="AA1" s="267"/>
+      <c r="AB1" s="267"/>
+      <c r="AC1" s="267"/>
+      <c r="AD1" s="267"/>
+      <c r="AE1" s="267"/>
+      <c r="AF1" s="267"/>
+      <c r="AG1" s="267"/>
+      <c r="AH1" s="267"/>
+      <c r="AI1" s="267"/>
+      <c r="AJ1" s="267"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="41"/>
-      <c r="C2" s="270" t="s">
+      <c r="C2" s="268" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="270"/>
-      <c r="E2" s="270"/>
-      <c r="F2" s="270"/>
-      <c r="G2" s="270"/>
-      <c r="H2" s="270"/>
-      <c r="I2" s="270"/>
-      <c r="J2" s="270"/>
-      <c r="K2" s="270"/>
-      <c r="L2" s="270"/>
-      <c r="M2" s="270"/>
-      <c r="N2" s="270"/>
-      <c r="O2" s="270"/>
-      <c r="P2" s="270"/>
-      <c r="Q2" s="271" t="s">
+      <c r="D2" s="268"/>
+      <c r="E2" s="268"/>
+      <c r="F2" s="268"/>
+      <c r="G2" s="268"/>
+      <c r="H2" s="268"/>
+      <c r="I2" s="268"/>
+      <c r="J2" s="268"/>
+      <c r="K2" s="268"/>
+      <c r="L2" s="268"/>
+      <c r="M2" s="268"/>
+      <c r="N2" s="268"/>
+      <c r="O2" s="268"/>
+      <c r="P2" s="268"/>
+      <c r="Q2" s="269" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="269"/>
-      <c r="S2" s="269"/>
-      <c r="T2" s="269"/>
-      <c r="U2" s="269"/>
-      <c r="V2" s="269"/>
-      <c r="W2" s="269"/>
-      <c r="X2" s="269"/>
-      <c r="Y2" s="269"/>
-      <c r="Z2" s="269"/>
-      <c r="AA2" s="269"/>
-      <c r="AB2" s="269"/>
-      <c r="AC2" s="269"/>
-      <c r="AD2" s="269"/>
-      <c r="AE2" s="269"/>
-      <c r="AF2" s="269"/>
-      <c r="AG2" s="269"/>
-      <c r="AH2" s="269"/>
-      <c r="AI2" s="269"/>
-      <c r="AJ2" s="269"/>
+      <c r="R2" s="267"/>
+      <c r="S2" s="267"/>
+      <c r="T2" s="267"/>
+      <c r="U2" s="267"/>
+      <c r="V2" s="267"/>
+      <c r="W2" s="267"/>
+      <c r="X2" s="267"/>
+      <c r="Y2" s="267"/>
+      <c r="Z2" s="267"/>
+      <c r="AA2" s="267"/>
+      <c r="AB2" s="267"/>
+      <c r="AC2" s="267"/>
+      <c r="AD2" s="267"/>
+      <c r="AE2" s="267"/>
+      <c r="AF2" s="267"/>
+      <c r="AG2" s="267"/>
+      <c r="AH2" s="267"/>
+      <c r="AI2" s="267"/>
+      <c r="AJ2" s="267"/>
     </row>
     <row r="3" spans="1:38" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="268"/>
-      <c r="D3" s="268"/>
-      <c r="E3" s="268"/>
-      <c r="F3" s="268"/>
-      <c r="G3" s="268"/>
-      <c r="H3" s="268"/>
-      <c r="I3" s="268"/>
-      <c r="J3" s="268"/>
-      <c r="K3" s="268"/>
-      <c r="L3" s="268"/>
-      <c r="M3" s="268"/>
-      <c r="N3" s="268"/>
-      <c r="O3" s="268"/>
-      <c r="P3" s="269"/>
-      <c r="Q3" s="269"/>
-      <c r="R3" s="269"/>
-      <c r="S3" s="269"/>
-      <c r="T3" s="269"/>
-      <c r="U3" s="269"/>
-      <c r="V3" s="269"/>
-      <c r="W3" s="269"/>
-      <c r="X3" s="269"/>
-      <c r="Y3" s="269"/>
-      <c r="Z3" s="269"/>
-      <c r="AA3" s="269"/>
-      <c r="AB3" s="269"/>
-      <c r="AC3" s="269"/>
-      <c r="AD3" s="269"/>
-      <c r="AE3" s="269"/>
-      <c r="AF3" s="269"/>
-      <c r="AG3" s="269"/>
-      <c r="AH3" s="269"/>
-      <c r="AI3" s="269"/>
-      <c r="AJ3" s="269"/>
+      <c r="C3" s="266"/>
+      <c r="D3" s="266"/>
+      <c r="E3" s="266"/>
+      <c r="F3" s="266"/>
+      <c r="G3" s="266"/>
+      <c r="H3" s="266"/>
+      <c r="I3" s="266"/>
+      <c r="J3" s="266"/>
+      <c r="K3" s="266"/>
+      <c r="L3" s="266"/>
+      <c r="M3" s="266"/>
+      <c r="N3" s="266"/>
+      <c r="O3" s="266"/>
+      <c r="P3" s="267"/>
+      <c r="Q3" s="267"/>
+      <c r="R3" s="267"/>
+      <c r="S3" s="267"/>
+      <c r="T3" s="267"/>
+      <c r="U3" s="267"/>
+      <c r="V3" s="267"/>
+      <c r="W3" s="267"/>
+      <c r="X3" s="267"/>
+      <c r="Y3" s="267"/>
+      <c r="Z3" s="267"/>
+      <c r="AA3" s="267"/>
+      <c r="AB3" s="267"/>
+      <c r="AC3" s="267"/>
+      <c r="AD3" s="267"/>
+      <c r="AE3" s="267"/>
+      <c r="AF3" s="267"/>
+      <c r="AG3" s="267"/>
+      <c r="AH3" s="267"/>
+      <c r="AI3" s="267"/>
+      <c r="AJ3" s="267"/>
     </row>
     <row r="4" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="293" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="294"/>
-      <c r="E4" s="294"/>
-      <c r="F4" s="294"/>
-      <c r="G4" s="294"/>
-      <c r="H4" s="294"/>
-      <c r="I4" s="294"/>
-      <c r="J4" s="294"/>
-      <c r="K4" s="294"/>
-      <c r="L4" s="294"/>
-      <c r="M4" s="294"/>
-      <c r="N4" s="294"/>
-      <c r="O4" s="294"/>
-      <c r="P4" s="294"/>
-      <c r="Q4" s="294"/>
-      <c r="R4" s="294"/>
-      <c r="S4" s="295"/>
-      <c r="T4" s="293" t="s">
+      <c r="C4" s="250" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="251"/>
+      <c r="E4" s="251"/>
+      <c r="F4" s="251"/>
+      <c r="G4" s="251"/>
+      <c r="H4" s="251"/>
+      <c r="I4" s="251"/>
+      <c r="J4" s="251"/>
+      <c r="K4" s="251"/>
+      <c r="L4" s="251"/>
+      <c r="M4" s="251"/>
+      <c r="N4" s="251"/>
+      <c r="O4" s="251"/>
+      <c r="P4" s="251"/>
+      <c r="Q4" s="251"/>
+      <c r="R4" s="251"/>
+      <c r="S4" s="252"/>
+      <c r="T4" s="250" t="s">
         <v>1</v>
       </c>
-      <c r="U4" s="294"/>
-      <c r="V4" s="294"/>
-      <c r="W4" s="294"/>
-      <c r="X4" s="294"/>
-      <c r="Y4" s="294"/>
-      <c r="Z4" s="294"/>
-      <c r="AA4" s="294"/>
-      <c r="AB4" s="295"/>
-      <c r="AC4" s="293" t="s">
+      <c r="U4" s="251"/>
+      <c r="V4" s="251"/>
+      <c r="W4" s="251"/>
+      <c r="X4" s="251"/>
+      <c r="Y4" s="251"/>
+      <c r="Z4" s="251"/>
+      <c r="AA4" s="251"/>
+      <c r="AB4" s="252"/>
+      <c r="AC4" s="250" t="s">
         <v>2</v>
       </c>
-      <c r="AD4" s="294"/>
-      <c r="AE4" s="294"/>
-      <c r="AF4" s="294"/>
-      <c r="AG4" s="302"/>
-      <c r="AH4" s="293" t="s">
+      <c r="AD4" s="251"/>
+      <c r="AE4" s="251"/>
+      <c r="AF4" s="251"/>
+      <c r="AG4" s="261"/>
+      <c r="AH4" s="250" t="s">
         <v>10</v>
       </c>
-      <c r="AI4" s="294"/>
-      <c r="AJ4" s="295"/>
+      <c r="AI4" s="251"/>
+      <c r="AJ4" s="252"/>
     </row>
     <row r="5" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32"/>
@@ -4034,55 +4037,55 @@
       <c r="C5" s="262" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="263"/>
-      <c r="E5" s="263"/>
-      <c r="F5" s="263"/>
-      <c r="G5" s="263"/>
-      <c r="H5" s="263"/>
-      <c r="I5" s="263"/>
-      <c r="J5" s="264"/>
-      <c r="K5" s="300" t="s">
+      <c r="D5" s="258"/>
+      <c r="E5" s="258"/>
+      <c r="F5" s="258"/>
+      <c r="G5" s="258"/>
+      <c r="H5" s="258"/>
+      <c r="I5" s="258"/>
+      <c r="J5" s="259"/>
+      <c r="K5" s="257" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="263"/>
-      <c r="M5" s="263"/>
-      <c r="N5" s="263"/>
-      <c r="O5" s="263"/>
-      <c r="P5" s="263"/>
-      <c r="Q5" s="263"/>
-      <c r="R5" s="264"/>
-      <c r="S5" s="296" t="s">
+      <c r="L5" s="258"/>
+      <c r="M5" s="258"/>
+      <c r="N5" s="258"/>
+      <c r="O5" s="258"/>
+      <c r="P5" s="258"/>
+      <c r="Q5" s="258"/>
+      <c r="R5" s="259"/>
+      <c r="S5" s="253" t="s">
         <v>12</v>
       </c>
       <c r="T5" s="262" t="s">
         <v>9</v>
       </c>
-      <c r="U5" s="263"/>
-      <c r="V5" s="263"/>
-      <c r="W5" s="264"/>
-      <c r="X5" s="300" t="s">
+      <c r="U5" s="258"/>
+      <c r="V5" s="258"/>
+      <c r="W5" s="259"/>
+      <c r="X5" s="257" t="s">
         <v>8</v>
       </c>
-      <c r="Y5" s="263"/>
-      <c r="Z5" s="263"/>
-      <c r="AA5" s="264"/>
-      <c r="AB5" s="296" t="s">
+      <c r="Y5" s="258"/>
+      <c r="Z5" s="258"/>
+      <c r="AA5" s="259"/>
+      <c r="AB5" s="253" t="s">
         <v>13</v>
       </c>
-      <c r="AC5" s="301" t="s">
+      <c r="AC5" s="260" t="s">
         <v>9</v>
       </c>
-      <c r="AD5" s="264"/>
-      <c r="AE5" s="300" t="s">
+      <c r="AD5" s="259"/>
+      <c r="AE5" s="257" t="s">
         <v>8</v>
       </c>
-      <c r="AF5" s="264"/>
-      <c r="AG5" s="296" t="s">
+      <c r="AF5" s="259"/>
+      <c r="AG5" s="253" t="s">
         <v>14</v>
       </c>
       <c r="AH5" s="56"/>
       <c r="AI5" s="25"/>
-      <c r="AJ5" s="296" t="s">
+      <c r="AJ5" s="253" t="s">
         <v>15</v>
       </c>
       <c r="AK5" s="4"/>
@@ -4096,7 +4099,7 @@
       </c>
       <c r="D6" s="108">
         <f>Résultats!$J$4</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" s="173">
         <f>Résultats!$J$6</f>
@@ -4116,7 +4119,7 @@
       </c>
       <c r="I6" s="173">
         <f>Résultats!$J$13</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J6" s="108">
         <f>Résultats!$J$14</f>
@@ -4132,7 +4135,7 @@
       </c>
       <c r="M6" s="173">
         <f>Résultats!$J$20</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6" s="109">
         <f>Résultats!$J$21</f>
@@ -4152,9 +4155,9 @@
       </c>
       <c r="R6" s="108">
         <f>Résultats!$J$28</f>
-        <v>1</v>
-      </c>
-      <c r="S6" s="297"/>
+        <v>2</v>
+      </c>
+      <c r="S6" s="254"/>
       <c r="T6" s="170">
         <f>Résultats!$V$6</f>
         <v>0</v>
@@ -4187,7 +4190,7 @@
         <f>Résultats!$V$25</f>
         <v>0</v>
       </c>
-      <c r="AB6" s="297"/>
+      <c r="AB6" s="254"/>
       <c r="AC6" s="111">
         <f>Résultats!$AH$8</f>
         <v>0</v>
@@ -4204,8 +4207,8 @@
         <f>Résultats!$AH$23</f>
         <v>0</v>
       </c>
-      <c r="AG6" s="297"/>
-      <c r="AH6" s="214">
+      <c r="AG6" s="254"/>
+      <c r="AH6" s="213">
         <f>Résultats!$AH$15</f>
         <v>0</v>
       </c>
@@ -4213,7 +4216,7 @@
         <f>Résultats!$AH$16</f>
         <v>0</v>
       </c>
-      <c r="AJ6" s="297"/>
+      <c r="AJ6" s="254"/>
       <c r="AK6" s="37"/>
     </row>
     <row r="7" spans="1:38" s="39" customFormat="1" ht="58.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -4239,7 +4242,7 @@
       <c r="P7" s="118"/>
       <c r="Q7" s="119"/>
       <c r="R7" s="117"/>
-      <c r="S7" s="297"/>
+      <c r="S7" s="254"/>
       <c r="T7" s="171"/>
       <c r="U7" s="117"/>
       <c r="V7" s="174"/>
@@ -4248,15 +4251,15 @@
       <c r="Y7" s="118"/>
       <c r="Z7" s="119"/>
       <c r="AA7" s="117"/>
-      <c r="AB7" s="297"/>
+      <c r="AB7" s="254"/>
       <c r="AC7" s="119"/>
       <c r="AD7" s="117"/>
       <c r="AE7" s="120"/>
       <c r="AF7" s="117"/>
-      <c r="AG7" s="297"/>
-      <c r="AH7" s="214"/>
+      <c r="AG7" s="254"/>
+      <c r="AH7" s="213"/>
       <c r="AI7" s="112"/>
-      <c r="AJ7" s="297"/>
+      <c r="AJ7" s="254"/>
       <c r="AK7" s="37"/>
     </row>
     <row r="8" spans="1:38" s="39" customFormat="1" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4326,7 +4329,7 @@
         <f>Résultats!$B$28</f>
         <v>VEGAS</v>
       </c>
-      <c r="S8" s="297"/>
+      <c r="S8" s="254"/>
       <c r="T8" s="172" t="str">
         <f>Résultats!$N$6</f>
         <v xml:space="preserve"> </v>
@@ -4359,7 +4362,7 @@
         <f>Résultats!$N$25</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AB8" s="297"/>
+      <c r="AB8" s="254"/>
       <c r="AC8" s="178" t="str">
         <f>Résultats!$Z$8</f>
         <v xml:space="preserve"> </v>
@@ -4376,16 +4379,16 @@
         <f>Résultats!$Z$23</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AG8" s="297"/>
-      <c r="AH8" s="215" t="str">
+      <c r="AG8" s="254"/>
+      <c r="AH8" s="214" t="str">
         <f>Résultats!$Z$15</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AI8" s="216" t="str">
+      <c r="AI8" s="215" t="str">
         <f>Résultats!$Z$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ8" s="297"/>
+      <c r="AJ8" s="254"/>
       <c r="AK8" s="37"/>
     </row>
     <row r="9" spans="1:38" s="39" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4459,7 +4462,7 @@
         <f>Résultats!$A$28</f>
         <v>P3</v>
       </c>
-      <c r="S9" s="299"/>
+      <c r="S9" s="256"/>
       <c r="T9" s="180" t="str">
         <f>Résultats!$M$6</f>
         <v xml:space="preserve"> </v>
@@ -4492,7 +4495,7 @@
         <f>Résultats!$M$25</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AB9" s="298"/>
+      <c r="AB9" s="255"/>
       <c r="AC9" s="184" t="str">
         <f>Résultats!$Y$8</f>
         <v xml:space="preserve"> </v>
@@ -4509,16 +4512,16 @@
         <f>Résultats!$Y$23</f>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="AG9" s="298"/>
-      <c r="AH9" s="217" t="str">
+      <c r="AG9" s="255"/>
+      <c r="AH9" s="216" t="str">
         <f>Résultats!$Y$15</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AI9" s="218" t="str">
+      <c r="AI9" s="217" t="str">
         <f>Résultats!$Y$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ9" s="299"/>
+      <c r="AJ9" s="256"/>
       <c r="AK9" s="114" t="s">
         <v>51</v>
       </c>
@@ -4531,15 +4534,15 @@
         <f>RANK(AL10,$AL$10:$AL$97,)</f>
         <v>1</v>
       </c>
-      <c r="B10" s="213" t="s">
-        <v>72</v>
+      <c r="B10" s="212" t="s">
+        <v>65</v>
       </c>
       <c r="C10" s="188">
         <v>4</v>
       </c>
       <c r="D10" s="189"/>
       <c r="E10" s="192">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" s="189"/>
       <c r="G10" s="193">
@@ -4547,35 +4550,35 @@
       </c>
       <c r="H10" s="190"/>
       <c r="I10" s="192">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J10" s="190"/>
       <c r="K10" s="191">
+        <v>7</v>
+      </c>
+      <c r="L10" s="190"/>
+      <c r="M10" s="192">
         <v>5</v>
       </c>
-      <c r="L10" s="190"/>
-      <c r="M10" s="192"/>
-      <c r="N10" s="189">
-        <v>7</v>
-      </c>
+      <c r="N10" s="189"/>
       <c r="O10" s="192">
+        <v>4</v>
+      </c>
+      <c r="P10" s="189"/>
+      <c r="Q10" s="193"/>
+      <c r="R10" s="194">
         <v>6</v>
       </c>
-      <c r="P10" s="189"/>
-      <c r="Q10" s="193">
-        <v>7</v>
-      </c>
-      <c r="R10" s="194"/>
-      <c r="S10" s="198">
+      <c r="S10" s="195">
         <f>SUM(C11:R11)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T10" s="188"/>
       <c r="U10" s="190"/>
       <c r="V10" s="192"/>
       <c r="W10" s="190"/>
       <c r="X10" s="191"/>
-      <c r="Y10" s="189"/>
+      <c r="Y10" s="297"/>
       <c r="Z10" s="193"/>
       <c r="AA10" s="194"/>
       <c r="AB10" s="195">
@@ -4602,7 +4605,7 @@
       </c>
       <c r="AL10" s="195">
         <f>$S10+$AB10+$AG10+$AJ10</f>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -4628,7 +4631,7 @@
       <c r="H11" s="135"/>
       <c r="I11" s="136">
         <f>(IF($I10&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I10=$I$6+$J$6,$O$103,0),0),0)+IF($J10&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J10=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J11" s="137"/>
       <c r="K11" s="138">
@@ -4638,7 +4641,7 @@
       <c r="L11" s="135"/>
       <c r="M11" s="133">
         <f>(IF($M10&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M10=$M$6+$N$6,$O$103,0),0),0)+IF($N10&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N10=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N11" s="135"/>
       <c r="O11" s="136">
@@ -4648,7 +4651,7 @@
       <c r="P11" s="135"/>
       <c r="Q11" s="136">
         <f>(IF($Q10&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q10=$Q$6+$R$6,$O$103,0),0),0)+IF($R10&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R10=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R11" s="139"/>
       <c r="S11" s="129"/>
@@ -4925,17 +4928,17 @@
     <row r="14" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="122">
         <f>RANK(AL14,$AL$10:$AL$97,)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" s="88" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C14" s="46">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D14" s="45"/>
       <c r="E14" s="44">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F14" s="45"/>
       <c r="G14" s="48">
@@ -4947,24 +4950,24 @@
       </c>
       <c r="J14" s="47"/>
       <c r="K14" s="49">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="L14" s="47"/>
       <c r="M14" s="44">
         <v>5</v>
       </c>
       <c r="N14" s="45"/>
-      <c r="O14" s="44">
-        <v>4</v>
-      </c>
-      <c r="P14" s="45"/>
+      <c r="O14" s="44"/>
+      <c r="P14" s="45">
+        <v>7</v>
+      </c>
       <c r="Q14" s="48"/>
       <c r="R14" s="50">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S14" s="130">
         <f>SUM(C15:R15)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="T14" s="46"/>
       <c r="U14" s="47"/>
@@ -4979,7 +4982,7 @@
         <v>0</v>
       </c>
       <c r="AC14" s="48"/>
-      <c r="AD14" s="47"/>
+      <c r="AD14" s="234"/>
       <c r="AE14" s="49"/>
       <c r="AF14" s="47"/>
       <c r="AG14" s="130">
@@ -4994,11 +4997,11 @@
       </c>
       <c r="AK14" s="116">
         <f>MAX($AL$10:$AL$97) - AL14</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AL14" s="130">
         <f>$S14+$AB14+$AG14+$AJ14</f>
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5024,7 +5027,7 @@
       <c r="H15" s="151"/>
       <c r="I15" s="127">
         <f>(IF($I14&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I14=$I$6+$J$6,$O$103,0),0),0)+IF($J14&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J14=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J15" s="152"/>
       <c r="K15" s="153">
@@ -5034,7 +5037,7 @@
       <c r="L15" s="151"/>
       <c r="M15" s="133">
         <f>(IF($M14&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M14=$M$6+$N$6,$O$103,0),0),0)+IF($N14&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N14=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N15" s="151"/>
       <c r="O15" s="127">
@@ -5044,7 +5047,7 @@
       <c r="P15" s="151"/>
       <c r="Q15" s="127">
         <f>(IF($Q14&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q14=$Q$6+$R$6,$O$103,0),0),0)+IF($R14&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R14=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R15" s="154"/>
       <c r="S15" s="155"/>
@@ -5067,7 +5070,7 @@
       <c r="AJ15" s="129"/>
       <c r="AK15" s="96">
         <f>MAX($AL$10:$AL$97) - AL15</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AL15" s="129"/>
     </row>
@@ -5324,46 +5327,46 @@
     <row r="18" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="187">
         <f>RANK(AL18,$AL$10:$AL$97,)</f>
-        <v>2</v>
-      </c>
-      <c r="B18" s="213" t="s">
-        <v>69</v>
+        <v>1</v>
+      </c>
+      <c r="B18" s="212" t="s">
+        <v>72</v>
       </c>
       <c r="C18" s="199">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18" s="200"/>
       <c r="E18" s="201">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F18" s="200"/>
       <c r="G18" s="202">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H18" s="203"/>
       <c r="I18" s="201">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J18" s="203"/>
       <c r="K18" s="204">
         <v>5</v>
       </c>
       <c r="L18" s="203"/>
-      <c r="M18" s="201">
+      <c r="M18" s="201"/>
+      <c r="N18" s="200">
+        <v>7</v>
+      </c>
+      <c r="O18" s="201">
         <v>6</v>
-      </c>
-      <c r="N18" s="200"/>
-      <c r="O18" s="201">
-        <v>5</v>
       </c>
       <c r="P18" s="200"/>
       <c r="Q18" s="202">
         <v>7</v>
       </c>
       <c r="R18" s="205"/>
-      <c r="S18" s="206">
+      <c r="S18" s="293">
         <f>SUM(C19:R19)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="T18" s="199"/>
       <c r="U18" s="203"/>
@@ -5371,9 +5374,9 @@
       <c r="W18" s="203"/>
       <c r="X18" s="204"/>
       <c r="Y18" s="200"/>
-      <c r="Z18" s="210"/>
+      <c r="Z18" s="202"/>
       <c r="AA18" s="205"/>
-      <c r="AB18" s="207">
+      <c r="AB18" s="206">
         <f>SUM(T19:AA19)</f>
         <v>0</v>
       </c>
@@ -5381,23 +5384,23 @@
       <c r="AD18" s="203"/>
       <c r="AE18" s="204"/>
       <c r="AF18" s="203"/>
-      <c r="AG18" s="207">
+      <c r="AG18" s="206">
         <f>SUM(AC19:AF19)</f>
         <v>0</v>
       </c>
-      <c r="AH18" s="248"/>
-      <c r="AI18" s="208"/>
-      <c r="AJ18" s="207">
+      <c r="AH18" s="239"/>
+      <c r="AI18" s="207"/>
+      <c r="AJ18" s="206">
         <f>AH19</f>
         <v>0</v>
       </c>
-      <c r="AK18" s="209">
+      <c r="AK18" s="208">
         <f>MAX($AL$10:$AL$97) - AL18</f>
-        <v>2</v>
-      </c>
-      <c r="AL18" s="207">
+        <v>0</v>
+      </c>
+      <c r="AL18" s="206">
         <f>$S18+$AB18+$AG18+$AJ18</f>
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5423,7 +5426,7 @@
       <c r="H19" s="151"/>
       <c r="I19" s="127">
         <f>(IF($I18&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I18=$I$6+$J$6,$O$103,0),0),0)+IF($J18&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J18=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J19" s="152"/>
       <c r="K19" s="153">
@@ -5433,7 +5436,7 @@
       <c r="L19" s="151"/>
       <c r="M19" s="127">
         <f>(IF($M18&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M18=$M$6+$N$6,$O$103,0),0),0)+IF($N18&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N18=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N19" s="151"/>
       <c r="O19" s="127">
@@ -5466,7 +5469,7 @@
       <c r="AJ19" s="155"/>
       <c r="AK19" s="163">
         <f>MAX($AL$10:$AL$97) - AL19</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AL19" s="129"/>
     </row>
@@ -5723,46 +5726,46 @@
     <row r="22" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="122">
         <f>RANK(AL22,$AL$10:$AL$97,)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B22" s="88" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="C22" s="46">
         <v>5</v>
       </c>
       <c r="D22" s="45"/>
       <c r="E22" s="44">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F22" s="45"/>
       <c r="G22" s="48">
         <v>5</v>
       </c>
       <c r="H22" s="47"/>
-      <c r="I22" s="44"/>
-      <c r="J22" s="47">
+      <c r="I22" s="44">
         <v>6</v>
       </c>
+      <c r="J22" s="47"/>
       <c r="K22" s="49">
         <v>5</v>
       </c>
       <c r="L22" s="47"/>
-      <c r="M22" s="44"/>
-      <c r="N22" s="45">
+      <c r="M22" s="44">
         <v>6</v>
       </c>
+      <c r="N22" s="45"/>
       <c r="O22" s="44">
         <v>5</v>
       </c>
       <c r="P22" s="45"/>
-      <c r="Q22" s="48"/>
-      <c r="R22" s="50">
-        <v>6</v>
-      </c>
+      <c r="Q22" s="48">
+        <v>7</v>
+      </c>
+      <c r="R22" s="50"/>
       <c r="S22" s="130">
         <f>SUM(C23:R23)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="T22" s="46"/>
       <c r="U22" s="47"/>
@@ -5770,7 +5773,7 @@
       <c r="W22" s="47"/>
       <c r="X22" s="49"/>
       <c r="Y22" s="45"/>
-      <c r="Z22" s="48"/>
+      <c r="Z22" s="123"/>
       <c r="AA22" s="50"/>
       <c r="AB22" s="130">
         <f>SUM(T23:AA23)</f>
@@ -5784,7 +5787,7 @@
         <f>SUM(AC23:AF23)</f>
         <v>0</v>
       </c>
-      <c r="AH22" s="303"/>
+      <c r="AH22" s="294"/>
       <c r="AI22" s="57"/>
       <c r="AJ22" s="130">
         <f>AH23</f>
@@ -5792,11 +5795,11 @@
       </c>
       <c r="AK22" s="116">
         <f>MAX($AL$10:$AL$97) - AL22</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AL22" s="130">
         <f>$S22+$AB22+$AG22+$AJ22</f>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5822,7 +5825,7 @@
       <c r="H23" s="164"/>
       <c r="I23" s="133">
         <f>(IF($I22&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I22=$I$6+$J$6,$O$103,0),0),0)+IF($J22&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J22=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J23" s="165"/>
       <c r="K23" s="166">
@@ -5832,7 +5835,7 @@
       <c r="L23" s="164"/>
       <c r="M23" s="133">
         <f>(IF($M22&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M22=$M$6+$N$6,$O$103,0),0),0)+IF($N22&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N22=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N23" s="164"/>
       <c r="O23" s="133">
@@ -5865,7 +5868,7 @@
       <c r="AJ23" s="155"/>
       <c r="AK23" s="163">
         <f>MAX($AL$10:$AL$97) - AL23</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AL23" s="129"/>
     </row>
@@ -6122,21 +6125,21 @@
     <row r="26" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="187">
         <f>RANK(AL26,$AL$10:$AL$97,)</f>
-        <v>2</v>
-      </c>
-      <c r="B26" s="213" t="s">
-        <v>70</v>
+        <v>5</v>
+      </c>
+      <c r="B26" s="212" t="s">
+        <v>85</v>
       </c>
       <c r="C26" s="199">
         <v>5</v>
       </c>
       <c r="D26" s="200"/>
       <c r="E26" s="201">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F26" s="200"/>
       <c r="G26" s="202">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H26" s="203"/>
       <c r="I26" s="201"/>
@@ -6152,16 +6155,16 @@
         <v>6</v>
       </c>
       <c r="O26" s="201">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P26" s="200"/>
-      <c r="Q26" s="202">
+      <c r="Q26" s="202"/>
+      <c r="R26" s="205">
         <v>6</v>
       </c>
-      <c r="R26" s="205"/>
-      <c r="S26" s="207">
+      <c r="S26" s="206">
         <f>SUM(C27:R27)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="T26" s="199"/>
       <c r="U26" s="203"/>
@@ -6171,7 +6174,7 @@
       <c r="Y26" s="200"/>
       <c r="Z26" s="202"/>
       <c r="AA26" s="205"/>
-      <c r="AB26" s="207">
+      <c r="AB26" s="206">
         <f>SUM(T27:AA27)</f>
         <v>0</v>
       </c>
@@ -6179,23 +6182,23 @@
       <c r="AD26" s="203"/>
       <c r="AE26" s="204"/>
       <c r="AF26" s="203"/>
-      <c r="AG26" s="207">
+      <c r="AG26" s="206">
         <f>SUM(AC27:AF27)</f>
         <v>0</v>
       </c>
-      <c r="AH26" s="237"/>
+      <c r="AH26" s="235"/>
       <c r="AI26" s="197"/>
-      <c r="AJ26" s="207">
+      <c r="AJ26" s="206">
         <f>AH27</f>
         <v>0</v>
       </c>
-      <c r="AK26" s="209">
+      <c r="AK26" s="208">
         <f>MAX($AL$10:$AL$97) - AL26</f>
         <v>2</v>
       </c>
-      <c r="AL26" s="207">
+      <c r="AL26" s="206">
         <f>$S26+$AB26+$AG26+$AJ26</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6241,7 +6244,7 @@
       <c r="P27" s="151"/>
       <c r="Q27" s="127">
         <f>(IF($Q26&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q26=$Q$6+$R$6,$O$103,0),0),0)+IF($R26&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R26=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R27" s="154"/>
       <c r="S27" s="155"/>
@@ -6264,7 +6267,7 @@
       <c r="AJ27" s="155"/>
       <c r="AK27" s="163">
         <f>MAX($AL$10:$AL$97) - AL27</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AL27" s="129"/>
     </row>
@@ -6521,7 +6524,7 @@
     <row r="30" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="122">
         <f>RANK(AL30,$AL$10:$AL$97,)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B30" s="88" t="s">
         <v>79</v>
@@ -6560,7 +6563,7 @@
       </c>
       <c r="S30" s="130">
         <f>SUM(C31:R31)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="T30" s="46"/>
       <c r="U30" s="47"/>
@@ -6594,7 +6597,7 @@
       </c>
       <c r="AL30" s="130">
         <f>$S30+$AB30+$AG30+$AJ30</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6640,7 +6643,7 @@
       <c r="P31" s="80"/>
       <c r="Q31" s="81">
         <f>(IF($Q30&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q30=$Q$6+$R$6,$O$103,0),0),0)+IF($R30&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R30=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R31" s="84"/>
       <c r="S31" s="129"/>
@@ -6663,7 +6666,7 @@
       <c r="AJ31" s="129"/>
       <c r="AK31" s="96">
         <f>MAX($AL$10:$AL$97) - AL31</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AL31" s="129"/>
     </row>
@@ -6920,80 +6923,80 @@
     <row r="34" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="187">
         <f>RANK(AL34,$AL$10:$AL$97,)</f>
-        <v>2</v>
-      </c>
-      <c r="B34" s="213" t="s">
-        <v>71</v>
+        <v>5</v>
+      </c>
+      <c r="B34" s="212" t="s">
+        <v>74</v>
       </c>
       <c r="C34" s="199">
         <v>5</v>
       </c>
       <c r="D34" s="200"/>
       <c r="E34" s="201">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F34" s="200"/>
       <c r="G34" s="202">
         <v>6</v>
       </c>
       <c r="H34" s="203"/>
-      <c r="I34" s="201">
+      <c r="I34" s="201"/>
+      <c r="J34" s="203">
+        <v>7</v>
+      </c>
+      <c r="K34" s="204">
+        <v>5</v>
+      </c>
+      <c r="L34" s="203"/>
+      <c r="M34" s="201"/>
+      <c r="N34" s="200">
         <v>6</v>
       </c>
-      <c r="J34" s="203"/>
-      <c r="K34" s="204">
-        <v>4</v>
-      </c>
-      <c r="L34" s="203"/>
-      <c r="M34" s="201">
-        <v>5</v>
-      </c>
-      <c r="N34" s="200"/>
-      <c r="O34" s="201"/>
-      <c r="P34" s="200">
+      <c r="O34" s="201">
         <v>7</v>
       </c>
+      <c r="P34" s="200"/>
       <c r="Q34" s="202"/>
       <c r="R34" s="205">
-        <v>7</v>
-      </c>
-      <c r="S34" s="207">
+        <v>6</v>
+      </c>
+      <c r="S34" s="206">
         <f>SUM(C35:R35)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="T34" s="199"/>
       <c r="U34" s="203"/>
       <c r="V34" s="201"/>
       <c r="W34" s="203"/>
       <c r="X34" s="204"/>
-      <c r="Y34" s="220"/>
+      <c r="Y34" s="200"/>
       <c r="Z34" s="202"/>
       <c r="AA34" s="203"/>
-      <c r="AB34" s="207">
+      <c r="AB34" s="206">
         <f>SUM(T35:AA35)</f>
         <v>0</v>
       </c>
       <c r="AC34" s="202"/>
-      <c r="AD34" s="250"/>
+      <c r="AD34" s="203"/>
       <c r="AE34" s="204"/>
       <c r="AF34" s="203"/>
-      <c r="AG34" s="207">
+      <c r="AG34" s="206">
         <f>SUM(AC35:AF35)</f>
         <v>0</v>
       </c>
-      <c r="AH34" s="211"/>
+      <c r="AH34" s="210"/>
       <c r="AI34" s="197"/>
-      <c r="AJ34" s="207">
+      <c r="AJ34" s="206">
         <f>AH35</f>
         <v>0</v>
       </c>
-      <c r="AK34" s="209">
+      <c r="AK34" s="208">
         <f>MAX($AL$10:$AL$97) - AL34</f>
         <v>2</v>
       </c>
-      <c r="AL34" s="207">
+      <c r="AL34" s="206">
         <f>$S34+$AB34+$AG34+$AJ34</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7019,7 +7022,7 @@
       <c r="H35" s="80"/>
       <c r="I35" s="81">
         <f>(IF($I34&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I34=$I$6+$J$6,$O$103,0),0),0)+IF($J34&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J34=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J35" s="82"/>
       <c r="K35" s="83">
@@ -7029,7 +7032,7 @@
       <c r="L35" s="80"/>
       <c r="M35" s="81">
         <f>(IF($M34&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M34=$M$6+$N$6,$O$103,0),0),0)+IF($N34&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N34=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N35" s="80"/>
       <c r="O35" s="81">
@@ -7039,7 +7042,7 @@
       <c r="P35" s="80"/>
       <c r="Q35" s="81">
         <f>(IF($Q34&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q34=$Q$6+$R$6,$O$103,0),0),0)+IF($R34&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R34=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R35" s="84"/>
       <c r="S35" s="129"/>
@@ -7062,7 +7065,7 @@
       <c r="AJ35" s="129"/>
       <c r="AK35" s="96">
         <f>MAX($AL$10:$AL$97) - AL35</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AL35" s="129"/>
     </row>
@@ -7319,43 +7322,43 @@
     <row r="38" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="122">
         <f>RANK(AL38,$AL$10:$AL$97,)</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B38" s="88" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="C38" s="46">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D38" s="45"/>
-      <c r="E38" s="44">
-        <v>5</v>
-      </c>
-      <c r="F38" s="45"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="45">
+        <v>7</v>
+      </c>
       <c r="G38" s="48">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H38" s="47"/>
       <c r="I38" s="44"/>
       <c r="J38" s="47">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K38" s="49">
         <v>6</v>
       </c>
       <c r="L38" s="47"/>
-      <c r="M38" s="44"/>
-      <c r="N38" s="45">
+      <c r="M38" s="44">
+        <v>6</v>
+      </c>
+      <c r="N38" s="45"/>
+      <c r="O38" s="44">
         <v>7</v>
       </c>
-      <c r="O38" s="44">
+      <c r="P38" s="45"/>
+      <c r="Q38" s="48"/>
+      <c r="R38" s="50">
         <v>6</v>
       </c>
-      <c r="P38" s="45"/>
-      <c r="Q38" s="48">
-        <v>7</v>
-      </c>
-      <c r="R38" s="50"/>
       <c r="S38" s="130">
         <f>SUM(C39:R39)</f>
         <v>8</v>
@@ -7365,8 +7368,8 @@
       <c r="V38" s="44"/>
       <c r="W38" s="47"/>
       <c r="X38" s="49"/>
-      <c r="Y38" s="45"/>
-      <c r="Z38" s="123"/>
+      <c r="Y38" s="128"/>
+      <c r="Z38" s="48"/>
       <c r="AA38" s="47"/>
       <c r="AB38" s="130">
         <f>SUM(T39:AA39)</f>
@@ -7388,7 +7391,7 @@
       </c>
       <c r="AK38" s="116">
         <f>MAX($AL$10:$AL$97) - AL38</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL38" s="130">
         <f>$S38+$AB38+$AG38+$AJ38</f>
@@ -7428,7 +7431,7 @@
       <c r="L39" s="80"/>
       <c r="M39" s="81">
         <f>(IF($M38&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M38=$M$6+$N$6,$O$103,0),0),0)+IF($N38&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N38=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N39" s="80"/>
       <c r="O39" s="81">
@@ -7438,7 +7441,7 @@
       <c r="P39" s="80"/>
       <c r="Q39" s="81">
         <f>(IF($Q38&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q38=$Q$6+$R$6,$O$103,0),0),0)+IF($R38&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R38=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R39" s="84"/>
       <c r="S39" s="129"/>
@@ -7461,7 +7464,7 @@
       <c r="AJ39" s="129"/>
       <c r="AK39" s="96">
         <f>MAX($AL$10:$AL$97) - AL39</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AL39" s="129"/>
     </row>
@@ -7718,17 +7721,17 @@
     <row r="42" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="187">
         <f>RANK(AL42,$AL$10:$AL$97,)</f>
-        <v>2</v>
-      </c>
-      <c r="B42" s="213" t="s">
-        <v>74</v>
+        <v>8</v>
+      </c>
+      <c r="B42" s="212" t="s">
+        <v>67</v>
       </c>
       <c r="C42" s="199">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D42" s="200"/>
       <c r="E42" s="201">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F42" s="200"/>
       <c r="G42" s="202">
@@ -7737,25 +7740,25 @@
       <c r="H42" s="203"/>
       <c r="I42" s="201"/>
       <c r="J42" s="203">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K42" s="204">
+        <v>6</v>
+      </c>
+      <c r="L42" s="203"/>
+      <c r="M42" s="201">
         <v>5</v>
       </c>
-      <c r="L42" s="203"/>
-      <c r="M42" s="201"/>
-      <c r="N42" s="200">
+      <c r="N42" s="200"/>
+      <c r="O42" s="201">
         <v>6</v>
-      </c>
-      <c r="O42" s="201">
-        <v>7</v>
       </c>
       <c r="P42" s="200"/>
       <c r="Q42" s="202"/>
       <c r="R42" s="205">
         <v>6</v>
       </c>
-      <c r="S42" s="207">
+      <c r="S42" s="206">
         <f>SUM(C43:R43)</f>
         <v>8</v>
       </c>
@@ -7765,31 +7768,31 @@
       <c r="W42" s="203"/>
       <c r="X42" s="204"/>
       <c r="Y42" s="200"/>
-      <c r="Z42" s="202"/>
+      <c r="Z42" s="209"/>
       <c r="AA42" s="203"/>
-      <c r="AB42" s="207">
+      <c r="AB42" s="206">
         <f>SUM(T43:AA43)</f>
         <v>0</v>
       </c>
       <c r="AC42" s="202"/>
-      <c r="AD42" s="203"/>
+      <c r="AD42" s="240"/>
       <c r="AE42" s="204"/>
       <c r="AF42" s="203"/>
-      <c r="AG42" s="207">
+      <c r="AG42" s="206">
         <f>SUM(AC43:AF43)</f>
         <v>0</v>
       </c>
-      <c r="AH42" s="211"/>
+      <c r="AH42" s="210"/>
       <c r="AI42" s="197"/>
-      <c r="AJ42" s="207">
+      <c r="AJ42" s="206">
         <f>AH43</f>
         <v>0</v>
       </c>
-      <c r="AK42" s="209">
+      <c r="AK42" s="208">
         <f>MAX($AL$10:$AL$97) - AL42</f>
-        <v>2</v>
-      </c>
-      <c r="AL42" s="207">
+        <v>3</v>
+      </c>
+      <c r="AL42" s="206">
         <f>$S42+$AB42+$AG42+$AJ42</f>
         <v>8</v>
       </c>
@@ -7827,7 +7830,7 @@
       <c r="L43" s="80"/>
       <c r="M43" s="81">
         <f>(IF($M42&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M42=$M$6+$N$6,$O$103,0),0),0)+IF($N42&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N42=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N43" s="80"/>
       <c r="O43" s="81">
@@ -7837,7 +7840,7 @@
       <c r="P43" s="80"/>
       <c r="Q43" s="81">
         <f>(IF($Q42&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q42=$Q$6+$R$6,$O$103,0),0),0)+IF($R42&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R42=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R43" s="84"/>
       <c r="S43" s="129"/>
@@ -7860,7 +7863,7 @@
       <c r="AJ43" s="129"/>
       <c r="AK43" s="116">
         <f>MAX($AL$10:$AL$97) - AL43</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AL43" s="129"/>
     </row>
@@ -8117,46 +8120,46 @@
     <row r="46" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="122">
         <f>RANK(AL46,$AL$10:$AL$97,)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B46" s="88" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C46" s="46">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D46" s="45"/>
-      <c r="E46" s="44">
-        <v>6</v>
-      </c>
-      <c r="F46" s="45"/>
-      <c r="G46" s="48"/>
-      <c r="H46" s="47">
+      <c r="E46" s="44"/>
+      <c r="F46" s="45">
         <v>7</v>
       </c>
+      <c r="G46" s="48">
+        <v>7</v>
+      </c>
+      <c r="H46" s="47"/>
       <c r="I46" s="44"/>
       <c r="J46" s="47">
         <v>6</v>
       </c>
       <c r="K46" s="49">
+        <v>6</v>
+      </c>
+      <c r="L46" s="47"/>
+      <c r="M46" s="44">
+        <v>7</v>
+      </c>
+      <c r="N46" s="45"/>
+      <c r="O46" s="44">
         <v>5</v>
       </c>
-      <c r="L46" s="47"/>
-      <c r="M46" s="44"/>
-      <c r="N46" s="45">
+      <c r="P46" s="45"/>
+      <c r="Q46" s="48"/>
+      <c r="R46" s="50">
         <v>6</v>
       </c>
-      <c r="O46" s="44">
-        <v>6</v>
-      </c>
-      <c r="P46" s="45"/>
-      <c r="Q46" s="48">
-        <v>6</v>
-      </c>
-      <c r="R46" s="50"/>
       <c r="S46" s="130">
         <f>SUM(C47:R47)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="T46" s="46"/>
       <c r="U46" s="47"/>
@@ -8186,11 +8189,11 @@
       </c>
       <c r="AK46" s="116">
         <f>MAX($AL$10:$AL$97) - AL46</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AL46" s="130">
         <f>$S46+$AB46+$AG46+$AJ46</f>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -8211,7 +8214,7 @@
       <c r="F47" s="80"/>
       <c r="G47" s="81">
         <f>(IF($G46&lt;&gt;"",($G$6*$O$104)+IF($G$6=4,($O$102)+IF($G46=$G$6+$H$6,$O$103,0),0),0)+IF($H46&lt;&gt;"",($H$6*$O$104)+IF($H$6=4,($O$102)+IF($H46=$G$6+$H$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H47" s="80"/>
       <c r="I47" s="81">
@@ -8226,7 +8229,7 @@
       <c r="L47" s="80"/>
       <c r="M47" s="81">
         <f>(IF($M46&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M46=$M$6+$N$6,$O$103,0),0),0)+IF($N46&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N46=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N47" s="80"/>
       <c r="O47" s="81">
@@ -8236,7 +8239,7 @@
       <c r="P47" s="80"/>
       <c r="Q47" s="81">
         <f>(IF($Q46&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q46=$Q$6+$R$6,$O$103,0),0),0)+IF($R46&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R46=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R47" s="84"/>
       <c r="S47" s="129"/>
@@ -8259,7 +8262,7 @@
       <c r="AJ47" s="129"/>
       <c r="AK47" s="116">
         <f>MAX($AL$10:$AL$97) - AL47</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AL47" s="129"/>
     </row>
@@ -8516,56 +8519,56 @@
     <row r="50" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="187">
         <f>RANK(AL50,$AL$10:$AL$97,)</f>
-        <v>10</v>
-      </c>
-      <c r="B50" s="213" t="s">
-        <v>66</v>
-      </c>
-      <c r="C50" s="199">
+        <v>8</v>
+      </c>
+      <c r="B50" s="212" t="s">
+        <v>68</v>
+      </c>
+      <c r="C50" s="298">
         <v>5</v>
       </c>
-      <c r="D50" s="200"/>
-      <c r="E50" s="201"/>
-      <c r="F50" s="200">
+      <c r="D50" s="299"/>
+      <c r="E50" s="300">
+        <v>6</v>
+      </c>
+      <c r="F50" s="299"/>
+      <c r="G50" s="301">
+        <v>5</v>
+      </c>
+      <c r="H50" s="302"/>
+      <c r="I50" s="300"/>
+      <c r="J50" s="302">
+        <v>6</v>
+      </c>
+      <c r="K50" s="303">
+        <v>6</v>
+      </c>
+      <c r="L50" s="302"/>
+      <c r="M50" s="300">
         <v>7</v>
       </c>
-      <c r="G50" s="202">
-        <v>4</v>
-      </c>
-      <c r="H50" s="203"/>
-      <c r="I50" s="201"/>
-      <c r="J50" s="203">
-        <v>7</v>
-      </c>
-      <c r="K50" s="204">
+      <c r="N50" s="299"/>
+      <c r="O50" s="300">
         <v>6</v>
       </c>
-      <c r="L50" s="203"/>
-      <c r="M50" s="201">
+      <c r="P50" s="299"/>
+      <c r="Q50" s="301"/>
+      <c r="R50" s="304">
         <v>6</v>
       </c>
-      <c r="N50" s="200"/>
-      <c r="O50" s="201">
-        <v>7</v>
-      </c>
-      <c r="P50" s="200"/>
-      <c r="Q50" s="202"/>
-      <c r="R50" s="205">
-        <v>6</v>
-      </c>
-      <c r="S50" s="207">
+      <c r="S50" s="206">
         <f>SUM(C51:R51)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="T50" s="199"/>
       <c r="U50" s="203"/>
       <c r="V50" s="201"/>
       <c r="W50" s="203"/>
       <c r="X50" s="204"/>
-      <c r="Y50" s="220"/>
+      <c r="Y50" s="200"/>
       <c r="Z50" s="202"/>
       <c r="AA50" s="203"/>
-      <c r="AB50" s="207">
+      <c r="AB50" s="206">
         <f>SUM(T51:AA51)</f>
         <v>0</v>
       </c>
@@ -8573,23 +8576,23 @@
       <c r="AD50" s="203"/>
       <c r="AE50" s="204"/>
       <c r="AF50" s="203"/>
-      <c r="AG50" s="207">
+      <c r="AG50" s="206">
         <f>SUM(AC51:AF51)</f>
         <v>0</v>
       </c>
-      <c r="AH50" s="211"/>
+      <c r="AH50" s="210"/>
       <c r="AI50" s="197"/>
-      <c r="AJ50" s="207">
+      <c r="AJ50" s="206">
         <f>AH51</f>
         <v>0</v>
       </c>
-      <c r="AK50" s="209">
+      <c r="AK50" s="208">
         <f>MAX($AL$10:$AL$97) - AL50</f>
-        <v>4</v>
-      </c>
-      <c r="AL50" s="207">
+        <v>3</v>
+      </c>
+      <c r="AL50" s="206">
         <f>$S50+$AB50+$AG50+$AJ50</f>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -8625,7 +8628,7 @@
       <c r="L51" s="135"/>
       <c r="M51" s="133">
         <f>(IF($M50&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M50=$M$6+$N$6,$O$103,0),0),0)+IF($N50&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N50=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N51" s="135"/>
       <c r="O51" s="136">
@@ -8635,7 +8638,7 @@
       <c r="P51" s="135"/>
       <c r="Q51" s="136">
         <f>(IF($Q50&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q50=$Q$6+$R$6,$O$103,0),0),0)+IF($R50&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R50=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R51" s="139"/>
       <c r="S51" s="129"/>
@@ -8912,61 +8915,61 @@
     <row r="54" spans="1:38" s="27" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="122">
         <f>RANK(AL54,$AL$10:$AL$97,)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B54" s="88" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C54" s="46">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D54" s="45"/>
-      <c r="E54" s="44">
-        <v>4</v>
-      </c>
-      <c r="F54" s="45"/>
+      <c r="E54" s="44"/>
+      <c r="F54" s="45">
+        <v>7</v>
+      </c>
       <c r="G54" s="48">
         <v>6</v>
       </c>
       <c r="H54" s="47"/>
       <c r="I54" s="44"/>
       <c r="J54" s="47">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K54" s="49">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L54" s="47"/>
       <c r="M54" s="44">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N54" s="45"/>
       <c r="O54" s="44">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P54" s="45"/>
       <c r="Q54" s="48"/>
       <c r="R54" s="50">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S54" s="130">
         <f>SUM(C55:R55)</f>
-        <v>6</v>
-      </c>
-      <c r="T54" s="46"/>
+        <v>8</v>
+      </c>
+      <c r="T54" s="296"/>
       <c r="U54" s="47"/>
       <c r="V54" s="44"/>
       <c r="W54" s="47"/>
       <c r="X54" s="49"/>
       <c r="Y54" s="45"/>
-      <c r="Z54" s="123"/>
+      <c r="Z54" s="48"/>
       <c r="AA54" s="47"/>
       <c r="AB54" s="130">
         <f>SUM(T55:AA55)</f>
         <v>0</v>
       </c>
       <c r="AC54" s="48"/>
-      <c r="AD54" s="236"/>
+      <c r="AD54" s="47"/>
       <c r="AE54" s="49"/>
       <c r="AF54" s="47"/>
       <c r="AG54" s="130">
@@ -8981,11 +8984,11 @@
       </c>
       <c r="AK54" s="116">
         <f>MAX($AL$10:$AL$97) - AL54</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AL54" s="130">
         <f>$S54+$AB54+$AG54+$AJ54</f>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -9021,7 +9024,7 @@
       <c r="L55" s="135"/>
       <c r="M55" s="133">
         <f>(IF($M54&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M54=$M$6+$N$6,$O$103,0),0),0)+IF($N54&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N54=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N55" s="135"/>
       <c r="O55" s="136">
@@ -9031,7 +9034,7 @@
       <c r="P55" s="135"/>
       <c r="Q55" s="136">
         <f>(IF($Q54&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q54=$Q$6+$R$6,$O$103,0),0),0)+IF($R54&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R54=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R55" s="139"/>
       <c r="S55" s="129"/>
@@ -9308,21 +9311,21 @@
     <row r="58" spans="1:38" s="27" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="187">
         <f>RANK(AL58,$AL$10:$AL$97,)</f>
-        <v>10</v>
-      </c>
-      <c r="B58" s="213" t="s">
-        <v>84</v>
+        <v>8</v>
+      </c>
+      <c r="B58" s="212" t="s">
+        <v>70</v>
       </c>
       <c r="C58" s="199">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D58" s="200"/>
-      <c r="E58" s="201"/>
-      <c r="F58" s="200">
+      <c r="E58" s="201">
         <v>7</v>
       </c>
+      <c r="F58" s="200"/>
       <c r="G58" s="202">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H58" s="203"/>
       <c r="I58" s="201"/>
@@ -9330,24 +9333,24 @@
         <v>6</v>
       </c>
       <c r="K58" s="204">
+        <v>5</v>
+      </c>
+      <c r="L58" s="203"/>
+      <c r="M58" s="201"/>
+      <c r="N58" s="200">
         <v>6</v>
       </c>
-      <c r="L58" s="203"/>
-      <c r="M58" s="201">
+      <c r="O58" s="201">
         <v>7</v>
       </c>
-      <c r="N58" s="200"/>
-      <c r="O58" s="201">
-        <v>5</v>
-      </c>
       <c r="P58" s="200"/>
-      <c r="Q58" s="202"/>
-      <c r="R58" s="205">
+      <c r="Q58" s="202">
         <v>6</v>
       </c>
-      <c r="S58" s="207">
+      <c r="R58" s="205"/>
+      <c r="S58" s="206">
         <f>SUM(C59:R59)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="T58" s="199"/>
       <c r="U58" s="203"/>
@@ -9357,7 +9360,7 @@
       <c r="Y58" s="200"/>
       <c r="Z58" s="202"/>
       <c r="AA58" s="203"/>
-      <c r="AB58" s="207">
+      <c r="AB58" s="206">
         <f>SUM(T59:AA59)</f>
         <v>0</v>
       </c>
@@ -9365,23 +9368,23 @@
       <c r="AD58" s="203"/>
       <c r="AE58" s="204"/>
       <c r="AF58" s="203"/>
-      <c r="AG58" s="207">
+      <c r="AG58" s="206">
         <f>SUM(AC59:AF59)</f>
         <v>0</v>
       </c>
-      <c r="AH58" s="211"/>
+      <c r="AH58" s="295"/>
       <c r="AI58" s="197"/>
-      <c r="AJ58" s="207">
+      <c r="AJ58" s="206">
         <f>AH59</f>
         <v>0</v>
       </c>
-      <c r="AK58" s="209">
+      <c r="AK58" s="208">
         <f>MAX($AL$10:$AL$97) - AL58</f>
-        <v>4</v>
-      </c>
-      <c r="AL58" s="207">
+        <v>3</v>
+      </c>
+      <c r="AL58" s="206">
         <f>$S58+$AB58+$AG58+$AJ58</f>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -9417,7 +9420,7 @@
       <c r="L59" s="135"/>
       <c r="M59" s="133">
         <f>(IF($M58&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M58=$M$6+$N$6,$O$103,0),0),0)+IF($N58&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N58=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N59" s="135"/>
       <c r="O59" s="136">
@@ -9704,46 +9707,46 @@
     <row r="62" spans="1:38" s="27" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="122">
         <f>RANK(AL62,$AL$10:$AL$97,)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B62" s="88" t="s">
-        <v>68</v>
-      </c>
-      <c r="C62" s="238">
+        <v>82</v>
+      </c>
+      <c r="C62" s="46">
+        <v>6</v>
+      </c>
+      <c r="D62" s="45"/>
+      <c r="E62" s="44">
+        <v>6</v>
+      </c>
+      <c r="F62" s="45"/>
+      <c r="G62" s="48">
+        <v>6</v>
+      </c>
+      <c r="H62" s="47"/>
+      <c r="I62" s="44"/>
+      <c r="J62" s="47">
+        <v>7</v>
+      </c>
+      <c r="K62" s="49">
         <v>5</v>
       </c>
-      <c r="D62" s="239"/>
-      <c r="E62" s="240">
+      <c r="L62" s="47"/>
+      <c r="M62" s="44">
+        <v>7</v>
+      </c>
+      <c r="N62" s="45"/>
+      <c r="O62" s="44">
         <v>6</v>
       </c>
-      <c r="F62" s="239"/>
-      <c r="G62" s="241">
-        <v>5</v>
-      </c>
-      <c r="H62" s="242"/>
-      <c r="I62" s="240"/>
-      <c r="J62" s="242">
-        <v>6</v>
-      </c>
-      <c r="K62" s="243">
-        <v>6</v>
-      </c>
-      <c r="L62" s="242"/>
-      <c r="M62" s="240">
-        <v>7</v>
-      </c>
-      <c r="N62" s="239"/>
-      <c r="O62" s="240">
-        <v>6</v>
-      </c>
-      <c r="P62" s="239"/>
-      <c r="Q62" s="241"/>
-      <c r="R62" s="244">
+      <c r="P62" s="45"/>
+      <c r="Q62" s="48"/>
+      <c r="R62" s="50">
         <v>6</v>
       </c>
       <c r="S62" s="130">
         <f>SUM(C63:R63)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="T62" s="46"/>
       <c r="U62" s="47"/>
@@ -9773,11 +9776,11 @@
       </c>
       <c r="AK62" s="116">
         <f>MAX($AL$10:$AL$97) - AL62</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AL62" s="130">
         <f>$S62+$AB62+$AG62+$AJ62</f>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -9813,7 +9816,7 @@
       <c r="L63" s="135"/>
       <c r="M63" s="133">
         <f>(IF($M62&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M62=$M$6+$N$6,$O$103,0),0),0)+IF($N62&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N62=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N63" s="135"/>
       <c r="O63" s="136">
@@ -9823,7 +9826,7 @@
       <c r="P63" s="135"/>
       <c r="Q63" s="136">
         <f>(IF($Q62&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q62=$Q$6+$R$6,$O$103,0),0),0)+IF($R62&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R62=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R63" s="139"/>
       <c r="S63" s="129"/>
@@ -10100,29 +10103,29 @@
     <row r="66" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="187">
         <f>RANK(AL66,$AL$10:$AL$97,)</f>
-        <v>10</v>
-      </c>
-      <c r="B66" s="213" t="s">
-        <v>78</v>
+        <v>8</v>
+      </c>
+      <c r="B66" s="212" t="s">
+        <v>80</v>
       </c>
       <c r="C66" s="199">
         <v>5</v>
       </c>
       <c r="D66" s="200"/>
-      <c r="E66" s="201"/>
-      <c r="F66" s="200">
-        <v>7</v>
-      </c>
+      <c r="E66" s="201">
+        <v>6</v>
+      </c>
+      <c r="F66" s="200"/>
       <c r="G66" s="202">
         <v>6</v>
       </c>
       <c r="H66" s="203"/>
       <c r="I66" s="201"/>
       <c r="J66" s="203">
+        <v>6</v>
+      </c>
+      <c r="K66" s="204">
         <v>7</v>
-      </c>
-      <c r="K66" s="204">
-        <v>5</v>
       </c>
       <c r="L66" s="203"/>
       <c r="M66" s="201">
@@ -10130,18 +10133,18 @@
       </c>
       <c r="N66" s="200"/>
       <c r="O66" s="201">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P66" s="200"/>
       <c r="Q66" s="202"/>
       <c r="R66" s="205">
-        <v>7</v>
-      </c>
-      <c r="S66" s="207">
+        <v>6</v>
+      </c>
+      <c r="S66" s="206">
         <f>SUM(C67:R67)</f>
-        <v>6</v>
-      </c>
-      <c r="T66" s="249"/>
+        <v>8</v>
+      </c>
+      <c r="T66" s="199"/>
       <c r="U66" s="203"/>
       <c r="V66" s="201"/>
       <c r="W66" s="203"/>
@@ -10149,7 +10152,7 @@
       <c r="Y66" s="200"/>
       <c r="Z66" s="202"/>
       <c r="AA66" s="203"/>
-      <c r="AB66" s="207">
+      <c r="AB66" s="206">
         <f>SUM(T67:AA67)</f>
         <v>0</v>
       </c>
@@ -10157,23 +10160,23 @@
       <c r="AD66" s="203"/>
       <c r="AE66" s="204"/>
       <c r="AF66" s="203"/>
-      <c r="AG66" s="207">
+      <c r="AG66" s="206">
         <f>SUM(AC67:AF67)</f>
         <v>0</v>
       </c>
-      <c r="AH66" s="212"/>
-      <c r="AI66" s="208"/>
-      <c r="AJ66" s="207">
+      <c r="AH66" s="211"/>
+      <c r="AI66" s="207"/>
+      <c r="AJ66" s="206">
         <f>AH67</f>
         <v>0</v>
       </c>
-      <c r="AK66" s="209">
+      <c r="AK66" s="208">
         <f>MAX($AL$10:$AL$97) - AL66</f>
-        <v>4</v>
-      </c>
-      <c r="AL66" s="207">
+        <v>3</v>
+      </c>
+      <c r="AL66" s="206">
         <f>$S66+$AB66+$AG66+$AJ66</f>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="67" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -10209,7 +10212,7 @@
       <c r="L67" s="135"/>
       <c r="M67" s="133">
         <f>(IF($M66&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M66=$M$6+$N$6,$O$103,0),0),0)+IF($N66&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N66=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N67" s="135"/>
       <c r="O67" s="136">
@@ -10219,7 +10222,7 @@
       <c r="P67" s="135"/>
       <c r="Q67" s="136">
         <f>(IF($Q66&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q66=$Q$6+$R$6,$O$103,0),0),0)+IF($R66&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R66=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R67" s="139"/>
       <c r="S67" s="129"/>
@@ -10496,46 +10499,46 @@
     <row r="70" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="122">
         <f>RANK(AL70,$AL$10:$AL$97,)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B70" s="88" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C70" s="46">
         <v>6</v>
       </c>
       <c r="D70" s="45"/>
       <c r="E70" s="44">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F70" s="45"/>
       <c r="G70" s="48">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H70" s="47"/>
       <c r="I70" s="44"/>
       <c r="J70" s="47">
+        <v>6</v>
+      </c>
+      <c r="K70" s="49">
+        <v>6</v>
+      </c>
+      <c r="L70" s="47"/>
+      <c r="M70" s="44"/>
+      <c r="N70" s="45">
         <v>7</v>
       </c>
-      <c r="K70" s="49">
-        <v>5</v>
-      </c>
-      <c r="L70" s="47"/>
-      <c r="M70" s="44">
-        <v>7</v>
-      </c>
-      <c r="N70" s="45"/>
       <c r="O70" s="44">
         <v>6</v>
       </c>
       <c r="P70" s="45"/>
-      <c r="Q70" s="48"/>
-      <c r="R70" s="50">
-        <v>6</v>
-      </c>
+      <c r="Q70" s="48">
+        <v>7</v>
+      </c>
+      <c r="R70" s="50"/>
       <c r="S70" s="130">
         <f>SUM(C71:R71)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="T70" s="46"/>
       <c r="U70" s="47"/>
@@ -10543,7 +10546,7 @@
       <c r="W70" s="47"/>
       <c r="X70" s="49"/>
       <c r="Y70" s="45"/>
-      <c r="Z70" s="48"/>
+      <c r="Z70" s="123"/>
       <c r="AA70" s="47"/>
       <c r="AB70" s="130">
         <f>SUM(T71:AA71)</f>
@@ -10565,11 +10568,11 @@
       </c>
       <c r="AK70" s="116">
         <f>MAX($AL$10:$AL$97) - AL70</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AL70" s="130">
         <f>$S70+$AB70+$AG70+$AJ70</f>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="71" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -10605,7 +10608,7 @@
       <c r="L71" s="135"/>
       <c r="M71" s="133">
         <f>(IF($M70&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M70=$M$6+$N$6,$O$103,0),0),0)+IF($N70&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N70=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N71" s="135"/>
       <c r="O71" s="136">
@@ -10892,10 +10895,10 @@
     <row r="74" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="187">
         <f>RANK(AL74,$AL$10:$AL$97,)</f>
-        <v>10</v>
-      </c>
-      <c r="B74" s="213" t="s">
-        <v>80</v>
+        <v>8</v>
+      </c>
+      <c r="B74" s="212" t="s">
+        <v>75</v>
       </c>
       <c r="C74" s="199">
         <v>5</v>
@@ -10914,24 +10917,24 @@
         <v>6</v>
       </c>
       <c r="K74" s="204">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L74" s="203"/>
       <c r="M74" s="201">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N74" s="200"/>
       <c r="O74" s="201">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P74" s="200"/>
       <c r="Q74" s="202"/>
       <c r="R74" s="205">
-        <v>6</v>
-      </c>
-      <c r="S74" s="207">
+        <v>7</v>
+      </c>
+      <c r="S74" s="206">
         <f>SUM(C75:R75)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="T74" s="199"/>
       <c r="U74" s="203"/>
@@ -10939,9 +10942,9 @@
       <c r="W74" s="203"/>
       <c r="X74" s="204"/>
       <c r="Y74" s="200"/>
-      <c r="Z74" s="202"/>
+      <c r="Z74" s="209"/>
       <c r="AA74" s="203"/>
-      <c r="AB74" s="207">
+      <c r="AB74" s="206">
         <f>SUM(T75:AA75)</f>
         <v>0</v>
       </c>
@@ -10949,23 +10952,23 @@
       <c r="AD74" s="203"/>
       <c r="AE74" s="204"/>
       <c r="AF74" s="203"/>
-      <c r="AG74" s="207">
+      <c r="AG74" s="206">
         <f>SUM(AC75:AF75)</f>
         <v>0</v>
       </c>
-      <c r="AH74" s="212"/>
-      <c r="AI74" s="208"/>
-      <c r="AJ74" s="207">
+      <c r="AH74" s="211"/>
+      <c r="AI74" s="207"/>
+      <c r="AJ74" s="206">
         <f>AH75</f>
         <v>0</v>
       </c>
-      <c r="AK74" s="209">
+      <c r="AK74" s="208">
         <f>MAX($AL$10:$AL$97) - AL74</f>
-        <v>4</v>
-      </c>
-      <c r="AL74" s="207">
+        <v>3</v>
+      </c>
+      <c r="AL74" s="206">
         <f>$S74+$AB74+$AG74+$AJ74</f>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="75" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11001,7 +11004,7 @@
       <c r="L75" s="135"/>
       <c r="M75" s="133">
         <f>(IF($M74&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M74=$M$6+$N$6,$O$103,0),0),0)+IF($N74&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N74=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N75" s="135"/>
       <c r="O75" s="136">
@@ -11011,7 +11014,7 @@
       <c r="P75" s="135"/>
       <c r="Q75" s="136">
         <f>(IF($Q74&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q74=$Q$6+$R$6,$O$103,0),0),0)+IF($R74&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R74=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R75" s="139"/>
       <c r="S75" s="129"/>
@@ -11288,46 +11291,46 @@
     <row r="78" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="122">
         <f>RANK(AL78,$AL$10:$AL$97,)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B78" s="88" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C78" s="46">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D78" s="45"/>
       <c r="E78" s="44">
+        <v>7</v>
+      </c>
+      <c r="F78" s="45"/>
+      <c r="G78" s="48">
         <v>6</v>
       </c>
-      <c r="F78" s="45"/>
-      <c r="G78" s="48"/>
-      <c r="H78" s="47">
-        <v>7</v>
-      </c>
+      <c r="H78" s="47"/>
       <c r="I78" s="44"/>
       <c r="J78" s="47">
+        <v>7</v>
+      </c>
+      <c r="K78" s="49">
+        <v>7</v>
+      </c>
+      <c r="L78" s="47"/>
+      <c r="M78" s="44">
         <v>6</v>
       </c>
-      <c r="K78" s="49">
-        <v>5</v>
-      </c>
-      <c r="L78" s="47"/>
-      <c r="M78" s="44"/>
-      <c r="N78" s="45">
-        <v>7</v>
-      </c>
+      <c r="N78" s="45"/>
       <c r="O78" s="44">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P78" s="45"/>
       <c r="Q78" s="48"/>
       <c r="R78" s="50">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S78" s="130">
         <f>SUM(C79:R79)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="T78" s="46"/>
       <c r="U78" s="47"/>
@@ -11335,7 +11338,7 @@
       <c r="W78" s="47"/>
       <c r="X78" s="49"/>
       <c r="Y78" s="45"/>
-      <c r="Z78" s="123"/>
+      <c r="Z78" s="48"/>
       <c r="AA78" s="47"/>
       <c r="AB78" s="130">
         <f>SUM(T79:AA79)</f>
@@ -11357,11 +11360,11 @@
       </c>
       <c r="AK78" s="116">
         <f>MAX($AL$10:$AL$97) - AL78</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AL78" s="130">
         <f>$S78+$AB78+$AG78+$AJ78</f>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="79" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11382,7 +11385,7 @@
       <c r="F79" s="135"/>
       <c r="G79" s="133">
         <f>(IF($G78&lt;&gt;"",($G$6*$O$104)+IF($G$6=4,($O$102)+IF($G78=$G$6+$H$6,$O$103,0),0),0)+IF($H78&lt;&gt;"",($H$6*$O$104)+IF($H$6=4,($O$102)+IF($H78=$G$6+$H$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H79" s="135"/>
       <c r="I79" s="136">
@@ -11397,7 +11400,7 @@
       <c r="L79" s="135"/>
       <c r="M79" s="133">
         <f>(IF($M78&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M78=$M$6+$N$6,$O$103,0),0),0)+IF($N78&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N78=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N79" s="135"/>
       <c r="O79" s="136">
@@ -11407,7 +11410,7 @@
       <c r="P79" s="135"/>
       <c r="Q79" s="136">
         <f>(IF($Q78&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q78=$Q$6+$R$6,$O$103,0),0),0)+IF($R78&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R78=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R79" s="139"/>
       <c r="S79" s="129"/>
@@ -11684,10 +11687,10 @@
     <row r="82" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="187">
         <f>RANK(AL82,$AL$10:$AL$97,)</f>
-        <v>10</v>
-      </c>
-      <c r="B82" s="213" t="s">
-        <v>75</v>
+        <v>19</v>
+      </c>
+      <c r="B82" s="212" t="s">
+        <v>73</v>
       </c>
       <c r="C82" s="199">
         <v>5</v>
@@ -11697,33 +11700,33 @@
         <v>6</v>
       </c>
       <c r="F82" s="200"/>
-      <c r="G82" s="202">
-        <v>6</v>
-      </c>
-      <c r="H82" s="203"/>
+      <c r="G82" s="202"/>
+      <c r="H82" s="203">
+        <v>7</v>
+      </c>
       <c r="I82" s="201"/>
       <c r="J82" s="203">
         <v>6</v>
       </c>
       <c r="K82" s="204">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L82" s="203"/>
-      <c r="M82" s="201">
+      <c r="M82" s="201"/>
+      <c r="N82" s="200">
         <v>7</v>
       </c>
-      <c r="N82" s="200"/>
       <c r="O82" s="201">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P82" s="200"/>
       <c r="Q82" s="202"/>
       <c r="R82" s="205">
+        <v>6</v>
+      </c>
+      <c r="S82" s="206">
+        <f>SUM(C83:R83)</f>
         <v>7</v>
-      </c>
-      <c r="S82" s="207">
-        <f>SUM(C83:R83)</f>
-        <v>6</v>
       </c>
       <c r="T82" s="199"/>
       <c r="U82" s="203"/>
@@ -11731,9 +11734,9 @@
       <c r="W82" s="203"/>
       <c r="X82" s="204"/>
       <c r="Y82" s="200"/>
-      <c r="Z82" s="210"/>
+      <c r="Z82" s="209"/>
       <c r="AA82" s="203"/>
-      <c r="AB82" s="207">
+      <c r="AB82" s="206">
         <f>SUM(T83:AA83)</f>
         <v>0</v>
       </c>
@@ -11741,23 +11744,23 @@
       <c r="AD82" s="203"/>
       <c r="AE82" s="204"/>
       <c r="AF82" s="203"/>
-      <c r="AG82" s="207">
+      <c r="AG82" s="206">
         <f>SUM(AC83:AF83)</f>
         <v>0</v>
       </c>
-      <c r="AH82" s="212"/>
-      <c r="AI82" s="208"/>
-      <c r="AJ82" s="207">
+      <c r="AH82" s="211"/>
+      <c r="AI82" s="207"/>
+      <c r="AJ82" s="206">
         <f>AH83</f>
         <v>0</v>
       </c>
-      <c r="AK82" s="209">
+      <c r="AK82" s="208">
         <f>MAX($AL$10:$AL$97) - AL82</f>
         <v>4</v>
       </c>
-      <c r="AL82" s="207">
+      <c r="AL82" s="206">
         <f>$S82+$AB82+$AG82+$AJ82</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="83" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11778,7 +11781,7 @@
       <c r="F83" s="135"/>
       <c r="G83" s="133">
         <f>(IF($G82&lt;&gt;"",($G$6*$O$104)+IF($G$6=4,($O$102)+IF($G82=$G$6+$H$6,$O$103,0),0),0)+IF($H82&lt;&gt;"",($H$6*$O$104)+IF($H$6=4,($O$102)+IF($H82=$G$6+$H$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H83" s="135"/>
       <c r="I83" s="136">
@@ -11793,7 +11796,7 @@
       <c r="L83" s="135"/>
       <c r="M83" s="133">
         <f>(IF($M82&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M82=$M$6+$N$6,$O$103,0),0),0)+IF($N82&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N82=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N83" s="135"/>
       <c r="O83" s="136">
@@ -11803,7 +11806,7 @@
       <c r="P83" s="135"/>
       <c r="Q83" s="136">
         <f>(IF($Q82&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q82=$Q$6+$R$6,$O$103,0),0),0)+IF($R82&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R82=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R83" s="139"/>
       <c r="S83" s="129"/>
@@ -12080,7 +12083,7 @@
     <row r="86" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="122">
         <f>RANK(AL86,$AL$10:$AL$97,)</f>
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B86" s="88" t="s">
         <v>83</v>
@@ -12119,7 +12122,7 @@
       <c r="R86" s="50"/>
       <c r="S86" s="130">
         <f>SUM(C87:R87)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="T86" s="46"/>
       <c r="U86" s="47"/>
@@ -12153,7 +12156,7 @@
       </c>
       <c r="AL86" s="130">
         <f>$S86+$AB86+$AG86+$AJ86</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="87" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -12189,7 +12192,7 @@
       <c r="L87" s="135"/>
       <c r="M87" s="133">
         <f>(IF($M86&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M86=$M$6+$N$6,$O$103,0),0),0)+IF($N86&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N86=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N87" s="135"/>
       <c r="O87" s="136">
@@ -12476,44 +12479,44 @@
     <row r="90" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="187">
         <f>RANK(AL90,$AL$10:$AL$97,)</f>
-        <v>10</v>
-      </c>
-      <c r="B90" s="213" t="s">
-        <v>76</v>
+        <v>21</v>
+      </c>
+      <c r="B90" s="212" t="s">
+        <v>77</v>
       </c>
       <c r="C90" s="199">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D90" s="200"/>
       <c r="E90" s="201">
+        <v>6</v>
+      </c>
+      <c r="F90" s="200"/>
+      <c r="G90" s="202"/>
+      <c r="H90" s="203">
         <v>7</v>
       </c>
-      <c r="F90" s="200"/>
-      <c r="G90" s="202">
-        <v>6</v>
-      </c>
-      <c r="H90" s="203"/>
       <c r="I90" s="201"/>
       <c r="J90" s="203">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K90" s="204">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L90" s="203"/>
-      <c r="M90" s="201">
+      <c r="M90" s="201"/>
+      <c r="N90" s="200">
         <v>6</v>
       </c>
-      <c r="N90" s="200"/>
       <c r="O90" s="201">
         <v>6</v>
       </c>
       <c r="P90" s="200"/>
-      <c r="Q90" s="202"/>
-      <c r="R90" s="205">
-        <v>7</v>
-      </c>
-      <c r="S90" s="207">
+      <c r="Q90" s="202">
+        <v>6</v>
+      </c>
+      <c r="R90" s="205"/>
+      <c r="S90" s="206">
         <f>SUM(C91:R91)</f>
         <v>6</v>
       </c>
@@ -12525,7 +12528,7 @@
       <c r="Y90" s="200"/>
       <c r="Z90" s="202"/>
       <c r="AA90" s="203"/>
-      <c r="AB90" s="207">
+      <c r="AB90" s="206">
         <f>SUM(T91:AA91)</f>
         <v>0</v>
       </c>
@@ -12533,21 +12536,21 @@
       <c r="AD90" s="203"/>
       <c r="AE90" s="204"/>
       <c r="AF90" s="203"/>
-      <c r="AG90" s="207">
+      <c r="AG90" s="206">
         <f>SUM(AC91:AF91)</f>
         <v>0</v>
       </c>
-      <c r="AH90" s="212"/>
-      <c r="AI90" s="208"/>
-      <c r="AJ90" s="207">
+      <c r="AH90" s="211"/>
+      <c r="AI90" s="207"/>
+      <c r="AJ90" s="206">
         <f>AH91</f>
         <v>0</v>
       </c>
-      <c r="AK90" s="209">
+      <c r="AK90" s="208">
         <f>MAX($AL$10:$AL$97) - AL90</f>
-        <v>4</v>
-      </c>
-      <c r="AL90" s="207">
+        <v>5</v>
+      </c>
+      <c r="AL90" s="206">
         <f>$S90+$AB90+$AG90+$AJ90</f>
         <v>6</v>
       </c>
@@ -12570,7 +12573,7 @@
       <c r="F91" s="135"/>
       <c r="G91" s="133">
         <f>(IF($G90&lt;&gt;"",($G$6*$O$104)+IF($G$6=4,($O$102)+IF($G90=$G$6+$H$6,$O$103,0),0),0)+IF($H90&lt;&gt;"",($H$6*$O$104)+IF($H$6=4,($O$102)+IF($H90=$G$6+$H$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H91" s="135"/>
       <c r="I91" s="136">
@@ -12585,7 +12588,7 @@
       <c r="L91" s="135"/>
       <c r="M91" s="133">
         <f>(IF($M90&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M90=$M$6+$N$6,$O$103,0),0),0)+IF($N90&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N90=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N91" s="135"/>
       <c r="O91" s="136">
@@ -12877,51 +12880,51 @@
       <c r="B94" s="88" t="s">
         <v>64</v>
       </c>
-      <c r="C94" s="229">
+      <c r="C94" s="227">
         <v>7</v>
       </c>
-      <c r="D94" s="230"/>
-      <c r="E94" s="245">
+      <c r="D94" s="228"/>
+      <c r="E94" s="236">
         <v>6</v>
       </c>
-      <c r="F94" s="230"/>
-      <c r="G94" s="246"/>
-      <c r="H94" s="233">
+      <c r="F94" s="228"/>
+      <c r="G94" s="237"/>
+      <c r="H94" s="231">
         <v>6</v>
       </c>
-      <c r="I94" s="245"/>
-      <c r="J94" s="233">
+      <c r="I94" s="236"/>
+      <c r="J94" s="231">
         <v>7</v>
       </c>
-      <c r="K94" s="234">
+      <c r="K94" s="232">
         <v>5</v>
       </c>
-      <c r="L94" s="233"/>
-      <c r="M94" s="231">
+      <c r="L94" s="231"/>
+      <c r="M94" s="229">
         <v>7</v>
       </c>
-      <c r="N94" s="230"/>
-      <c r="O94" s="231">
+      <c r="N94" s="228"/>
+      <c r="O94" s="229">
         <v>6</v>
       </c>
-      <c r="P94" s="230"/>
-      <c r="Q94" s="232">
+      <c r="P94" s="228"/>
+      <c r="Q94" s="230">
         <v>6</v>
       </c>
-      <c r="R94" s="235"/>
+      <c r="R94" s="233"/>
       <c r="S94" s="130">
         <f>SUM(C95:R95)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T94" s="46"/>
       <c r="U94" s="47"/>
-      <c r="V94" s="247"/>
+      <c r="V94" s="238"/>
       <c r="W94" s="47"/>
       <c r="X94" s="49"/>
       <c r="Y94" s="128"/>
       <c r="Z94" s="48"/>
       <c r="AA94" s="47"/>
-      <c r="AB94" s="221">
+      <c r="AB94" s="219">
         <f>SUM(T95:AA95)</f>
         <v>0</v>
       </c>
@@ -12929,7 +12932,7 @@
       <c r="AD94" s="47"/>
       <c r="AE94" s="49"/>
       <c r="AF94" s="47"/>
-      <c r="AG94" s="221">
+      <c r="AG94" s="219">
         <f>SUM(AC95:AF95)</f>
         <v>0</v>
       </c>
@@ -12943,9 +12946,9 @@
         <f>MAX($AL$10:$AL$97) - AL94</f>
         <v>6</v>
       </c>
-      <c r="AL94" s="221">
+      <c r="AL94" s="219">
         <f>$S94+$AB94+$AG94+$AJ94</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="95" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -12981,7 +12984,7 @@
       <c r="L95" s="135"/>
       <c r="M95" s="133">
         <f>(IF($M94&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M94=$M$6+$N$6,$O$103,0),0),0)+IF($N94&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N94=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N95" s="135"/>
       <c r="O95" s="136">
@@ -13263,72 +13266,72 @@
         <f>SUM(C97:AI97)</f>
         <v>0</v>
       </c>
-      <c r="AL97" s="219"/>
+      <c r="AL97" s="218"/>
     </row>
     <row r="98" spans="1:38" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A98" s="65"/>
       <c r="B98" s="55"/>
-      <c r="C98" s="224">
+      <c r="C98" s="222">
         <f t="shared" ref="C98:R98" si="0">COUNT(C10,C14,C18,C22,C26,C30,C34, C38, C42,C46,C50,C54,C58,C62,C66,C70,C74,C78,C82,C90,C94,C86)</f>
         <v>22</v>
       </c>
-      <c r="D98" s="222">
+      <c r="D98" s="220">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E98" s="223">
+      <c r="E98" s="221">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="F98" s="222">
+      <c r="F98" s="220">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G98" s="223">
+      <c r="G98" s="221">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="H98" s="222">
+      <c r="H98" s="220">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="I98" s="223">
+      <c r="I98" s="221">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="J98" s="222">
+      <c r="J98" s="220">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="K98" s="223">
+      <c r="K98" s="221">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="L98" s="222">
+      <c r="L98" s="220">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M98" s="223">
+      <c r="M98" s="221">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="N98" s="222">
+      <c r="N98" s="220">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="O98" s="223">
+      <c r="O98" s="221">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="P98" s="222">
+      <c r="P98" s="220">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="Q98" s="223">
+      <c r="Q98" s="221">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="R98" s="225">
+      <c r="R98" s="223">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -13398,12 +13401,12 @@
     <row r="100" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B100" s="43"/>
       <c r="N100" s="26"/>
-      <c r="O100" s="284" t="s">
+      <c r="O100" s="241" t="s">
         <v>17</v>
       </c>
-      <c r="P100" s="285"/>
-      <c r="Q100" s="285"/>
-      <c r="R100" s="286"/>
+      <c r="P100" s="242"/>
+      <c r="Q100" s="242"/>
+      <c r="R100" s="243"/>
       <c r="AG100" s="30"/>
       <c r="AH100" s="30"/>
       <c r="AI100" s="30"/>
@@ -13412,21 +13415,21 @@
     </row>
     <row r="101" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="33"/>
-      <c r="B101" s="272" t="s">
+      <c r="B101" s="270" t="s">
         <v>16</v>
       </c>
-      <c r="C101" s="273"/>
-      <c r="D101" s="273"/>
-      <c r="E101" s="273"/>
-      <c r="F101" s="273"/>
-      <c r="G101" s="273"/>
-      <c r="H101" s="273"/>
-      <c r="I101" s="273"/>
-      <c r="J101" s="273"/>
-      <c r="K101" s="273"/>
-      <c r="L101" s="273"/>
-      <c r="M101" s="273"/>
-      <c r="N101" s="274"/>
+      <c r="C101" s="271"/>
+      <c r="D101" s="271"/>
+      <c r="E101" s="271"/>
+      <c r="F101" s="271"/>
+      <c r="G101" s="271"/>
+      <c r="H101" s="271"/>
+      <c r="I101" s="271"/>
+      <c r="J101" s="271"/>
+      <c r="K101" s="271"/>
+      <c r="L101" s="271"/>
+      <c r="M101" s="271"/>
+      <c r="N101" s="272"/>
       <c r="O101" s="21">
         <v>1</v>
       </c>
@@ -13439,45 +13442,45 @@
       <c r="R101" s="22">
         <v>4</v>
       </c>
-      <c r="U101" s="287" t="s">
+      <c r="U101" s="244" t="s">
         <v>26</v>
       </c>
-      <c r="V101" s="288"/>
-      <c r="W101" s="288"/>
-      <c r="X101" s="288"/>
-      <c r="Y101" s="288"/>
-      <c r="Z101" s="288"/>
-      <c r="AA101" s="288"/>
-      <c r="AB101" s="288"/>
-      <c r="AC101" s="288"/>
-      <c r="AD101" s="289"/>
+      <c r="V101" s="245"/>
+      <c r="W101" s="245"/>
+      <c r="X101" s="245"/>
+      <c r="Y101" s="245"/>
+      <c r="Z101" s="245"/>
+      <c r="AA101" s="245"/>
+      <c r="AB101" s="245"/>
+      <c r="AC101" s="245"/>
+      <c r="AD101" s="246"/>
       <c r="AE101" s="28"/>
       <c r="AF101" s="28"/>
-      <c r="AG101" s="290" t="s">
+      <c r="AG101" s="247" t="s">
         <v>24</v>
       </c>
-      <c r="AH101" s="291"/>
-      <c r="AI101" s="291"/>
-      <c r="AJ101" s="291"/>
-      <c r="AK101" s="292"/>
+      <c r="AH101" s="248"/>
+      <c r="AI101" s="248"/>
+      <c r="AJ101" s="248"/>
+      <c r="AK101" s="249"/>
     </row>
     <row r="102" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A102" s="34"/>
-      <c r="B102" s="251" t="s">
+      <c r="B102" s="277" t="s">
         <v>6</v>
       </c>
-      <c r="C102" s="252"/>
-      <c r="D102" s="252"/>
-      <c r="E102" s="252"/>
-      <c r="F102" s="252"/>
-      <c r="G102" s="252"/>
-      <c r="H102" s="252"/>
-      <c r="I102" s="252"/>
-      <c r="J102" s="252"/>
-      <c r="K102" s="252"/>
-      <c r="L102" s="252"/>
-      <c r="M102" s="252"/>
-      <c r="N102" s="253"/>
+      <c r="C102" s="278"/>
+      <c r="D102" s="278"/>
+      <c r="E102" s="278"/>
+      <c r="F102" s="278"/>
+      <c r="G102" s="278"/>
+      <c r="H102" s="278"/>
+      <c r="I102" s="278"/>
+      <c r="J102" s="278"/>
+      <c r="K102" s="278"/>
+      <c r="L102" s="278"/>
+      <c r="M102" s="278"/>
+      <c r="N102" s="279"/>
       <c r="O102" s="20">
         <v>5</v>
       </c>
@@ -13490,49 +13493,49 @@
       <c r="R102" s="23">
         <v>20</v>
       </c>
-      <c r="U102" s="277" t="s">
+      <c r="U102" s="275" t="s">
         <v>20</v>
       </c>
-      <c r="V102" s="278"/>
-      <c r="W102" s="278"/>
-      <c r="X102" s="278"/>
-      <c r="Y102" s="278"/>
-      <c r="Z102" s="278"/>
-      <c r="AA102" s="278"/>
-      <c r="AB102" s="275">
+      <c r="V102" s="276"/>
+      <c r="W102" s="276"/>
+      <c r="X102" s="276"/>
+      <c r="Y102" s="276"/>
+      <c r="Z102" s="276"/>
+      <c r="AA102" s="276"/>
+      <c r="AB102" s="273">
         <v>22</v>
       </c>
-      <c r="AC102" s="275"/>
-      <c r="AD102" s="276"/>
+      <c r="AC102" s="273"/>
+      <c r="AD102" s="274"/>
       <c r="AE102" s="29"/>
       <c r="AF102" s="29"/>
-      <c r="AG102" s="258" t="s">
+      <c r="AG102" s="289" t="s">
         <v>21</v>
       </c>
-      <c r="AH102" s="259"/>
-      <c r="AI102" s="259"/>
-      <c r="AJ102" s="260"/>
-      <c r="AK102" s="226">
+      <c r="AH102" s="290"/>
+      <c r="AI102" s="290"/>
+      <c r="AJ102" s="291"/>
+      <c r="AK102" s="224">
         <v>230</v>
       </c>
     </row>
     <row r="103" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="34"/>
-      <c r="B103" s="251" t="s">
+      <c r="B103" s="277" t="s">
         <v>5</v>
       </c>
-      <c r="C103" s="252"/>
-      <c r="D103" s="252"/>
-      <c r="E103" s="252"/>
-      <c r="F103" s="252"/>
-      <c r="G103" s="252"/>
-      <c r="H103" s="252"/>
-      <c r="I103" s="252"/>
-      <c r="J103" s="252"/>
-      <c r="K103" s="252"/>
-      <c r="L103" s="252"/>
-      <c r="M103" s="252"/>
-      <c r="N103" s="253"/>
+      <c r="C103" s="278"/>
+      <c r="D103" s="278"/>
+      <c r="E103" s="278"/>
+      <c r="F103" s="278"/>
+      <c r="G103" s="278"/>
+      <c r="H103" s="278"/>
+      <c r="I103" s="278"/>
+      <c r="J103" s="278"/>
+      <c r="K103" s="278"/>
+      <c r="L103" s="278"/>
+      <c r="M103" s="278"/>
+      <c r="N103" s="279"/>
       <c r="O103" s="20">
         <v>2</v>
       </c>
@@ -13545,49 +13548,49 @@
       <c r="R103" s="23">
         <v>8</v>
       </c>
-      <c r="U103" s="256" t="s">
+      <c r="U103" s="284" t="s">
         <v>18</v>
       </c>
-      <c r="V103" s="257"/>
-      <c r="W103" s="257"/>
-      <c r="X103" s="257"/>
-      <c r="Y103" s="257"/>
-      <c r="Z103" s="257"/>
-      <c r="AA103" s="257"/>
-      <c r="AB103" s="282">
+      <c r="V103" s="285"/>
+      <c r="W103" s="285"/>
+      <c r="X103" s="285"/>
+      <c r="Y103" s="285"/>
+      <c r="Z103" s="285"/>
+      <c r="AA103" s="285"/>
+      <c r="AB103" s="286">
         <v>20</v>
       </c>
-      <c r="AC103" s="282"/>
-      <c r="AD103" s="283"/>
+      <c r="AC103" s="286"/>
+      <c r="AD103" s="287"/>
       <c r="AE103" s="29"/>
       <c r="AF103" s="29"/>
-      <c r="AG103" s="261" t="s">
+      <c r="AG103" s="292" t="s">
         <v>22</v>
       </c>
-      <c r="AH103" s="252"/>
-      <c r="AI103" s="252"/>
-      <c r="AJ103" s="253"/>
+      <c r="AH103" s="278"/>
+      <c r="AI103" s="278"/>
+      <c r="AJ103" s="279"/>
       <c r="AK103" s="36">
         <v>115</v>
       </c>
     </row>
     <row r="104" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="35"/>
-      <c r="B104" s="265" t="s">
+      <c r="B104" s="263" t="s">
         <v>4</v>
       </c>
-      <c r="C104" s="266"/>
-      <c r="D104" s="266"/>
-      <c r="E104" s="266"/>
-      <c r="F104" s="266"/>
-      <c r="G104" s="266"/>
-      <c r="H104" s="266"/>
-      <c r="I104" s="266"/>
-      <c r="J104" s="266"/>
-      <c r="K104" s="266"/>
-      <c r="L104" s="266"/>
-      <c r="M104" s="266"/>
-      <c r="N104" s="267"/>
+      <c r="C104" s="264"/>
+      <c r="D104" s="264"/>
+      <c r="E104" s="264"/>
+      <c r="F104" s="264"/>
+      <c r="G104" s="264"/>
+      <c r="H104" s="264"/>
+      <c r="I104" s="264"/>
+      <c r="J104" s="264"/>
+      <c r="K104" s="264"/>
+      <c r="L104" s="264"/>
+      <c r="M104" s="264"/>
+      <c r="N104" s="265"/>
       <c r="O104" s="3">
         <v>1</v>
       </c>
@@ -13600,52 +13603,52 @@
       <c r="R104" s="24">
         <v>1</v>
       </c>
-      <c r="U104" s="279" t="s">
+      <c r="U104" s="280" t="s">
         <v>19</v>
       </c>
-      <c r="V104" s="255"/>
-      <c r="W104" s="255"/>
-      <c r="X104" s="255"/>
-      <c r="Y104" s="255"/>
-      <c r="Z104" s="255"/>
-      <c r="AA104" s="255"/>
-      <c r="AB104" s="280">
+      <c r="V104" s="281"/>
+      <c r="W104" s="281"/>
+      <c r="X104" s="281"/>
+      <c r="Y104" s="281"/>
+      <c r="Z104" s="281"/>
+      <c r="AA104" s="281"/>
+      <c r="AB104" s="282">
         <f>AB102*AB103</f>
         <v>440</v>
       </c>
-      <c r="AC104" s="280"/>
-      <c r="AD104" s="281"/>
+      <c r="AC104" s="282"/>
+      <c r="AD104" s="283"/>
       <c r="AE104" s="29"/>
       <c r="AF104" s="29"/>
-      <c r="AG104" s="261" t="s">
+      <c r="AG104" s="292" t="s">
         <v>25</v>
       </c>
-      <c r="AH104" s="252"/>
-      <c r="AI104" s="252"/>
-      <c r="AJ104" s="253"/>
+      <c r="AH104" s="278"/>
+      <c r="AI104" s="278"/>
+      <c r="AJ104" s="279"/>
       <c r="AK104" s="36">
         <v>65</v>
       </c>
     </row>
     <row r="105" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG105" s="256" t="s">
+      <c r="AG105" s="284" t="s">
         <v>23</v>
       </c>
-      <c r="AH105" s="257"/>
-      <c r="AI105" s="257"/>
-      <c r="AJ105" s="257"/>
-      <c r="AK105" s="228">
+      <c r="AH105" s="285"/>
+      <c r="AI105" s="285"/>
+      <c r="AJ105" s="285"/>
+      <c r="AK105" s="226">
         <v>30</v>
       </c>
     </row>
     <row r="106" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG106" s="254" t="s">
+      <c r="AG106" s="288" t="s">
         <v>19</v>
       </c>
-      <c r="AH106" s="255"/>
-      <c r="AI106" s="255"/>
-      <c r="AJ106" s="255"/>
-      <c r="AK106" s="227">
+      <c r="AH106" s="281"/>
+      <c r="AI106" s="281"/>
+      <c r="AJ106" s="281"/>
+      <c r="AK106" s="225">
         <f>SUM(AK102:AK105)</f>
         <v>440</v>
       </c>
@@ -13656,6 +13659,28 @@
     <sortCondition ref="B10:B94"/>
   </sortState>
   <mergeCells count="38">
+    <mergeCell ref="B103:N103"/>
+    <mergeCell ref="AG106:AJ106"/>
+    <mergeCell ref="AG105:AJ105"/>
+    <mergeCell ref="AG102:AJ102"/>
+    <mergeCell ref="AG104:AJ104"/>
+    <mergeCell ref="AG103:AJ103"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="B104:N104"/>
+    <mergeCell ref="C1:O1"/>
+    <mergeCell ref="P1:AJ1"/>
+    <mergeCell ref="C3:O3"/>
+    <mergeCell ref="P3:AJ3"/>
+    <mergeCell ref="C2:P2"/>
+    <mergeCell ref="Q2:AJ2"/>
+    <mergeCell ref="B101:N101"/>
+    <mergeCell ref="AB102:AD102"/>
+    <mergeCell ref="U102:AA102"/>
+    <mergeCell ref="B102:N102"/>
+    <mergeCell ref="U104:AA104"/>
+    <mergeCell ref="AB104:AD104"/>
+    <mergeCell ref="U103:AA103"/>
+    <mergeCell ref="AB103:AD103"/>
     <mergeCell ref="O100:R100"/>
     <mergeCell ref="U101:AD101"/>
     <mergeCell ref="AG101:AK101"/>
@@ -13672,28 +13697,6 @@
     <mergeCell ref="C5:J5"/>
     <mergeCell ref="K5:R5"/>
     <mergeCell ref="S5:S9"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="B104:N104"/>
-    <mergeCell ref="C1:O1"/>
-    <mergeCell ref="P1:AJ1"/>
-    <mergeCell ref="C3:O3"/>
-    <mergeCell ref="P3:AJ3"/>
-    <mergeCell ref="C2:P2"/>
-    <mergeCell ref="Q2:AJ2"/>
-    <mergeCell ref="B101:N101"/>
-    <mergeCell ref="AB102:AD102"/>
-    <mergeCell ref="U102:AA102"/>
-    <mergeCell ref="B102:N102"/>
-    <mergeCell ref="U104:AA104"/>
-    <mergeCell ref="AB104:AD104"/>
-    <mergeCell ref="U103:AA103"/>
-    <mergeCell ref="AB103:AD103"/>
-    <mergeCell ref="B103:N103"/>
-    <mergeCell ref="AG106:AJ106"/>
-    <mergeCell ref="AG105:AJ105"/>
-    <mergeCell ref="AG102:AJ102"/>
-    <mergeCell ref="AG104:AJ104"/>
-    <mergeCell ref="AG103:AJ103"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <conditionalFormatting sqref="AH18:AI18 AH10:AI10 AH14:AI14 T10:AA10 AC10:AF10 C10:R10 C14:R14 T14:AA14 AC14:AF14 T18:AA18 AC18:AF18 AH30:AI30 C30:R30 T30:AA30 AC30:AF30 AH26:AI26 C26:R26 T26:AA26 AC26:AF26 AH62:AI62 C62:R62 T62:AA62 AC62:AF62 AH42:AI42 C42:R42 T42:AA42 AC42:AF42 AH22:AI22 C22:R22 T22:AA22 AC22:AF22 AH38:AI38 C38:R38 T38:AA38 AC38:AF38 AH34:AI34 C34:R34 T34:AA34 AC34:AF34 AH66:AI66 C66:R66 T66:AA66 AC66:AF66 C18:R18">
@@ -14325,7 +14328,7 @@
   <dimension ref="A1:AJ31"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14390,7 +14393,9 @@
       <c r="D3" s="85">
         <v>1</v>
       </c>
-      <c r="E3" s="85"/>
+      <c r="E3" s="85">
+        <v>1</v>
+      </c>
       <c r="F3" s="85"/>
       <c r="G3" s="85"/>
       <c r="H3" s="85"/>
@@ -14432,14 +14437,16 @@
       <c r="D4" s="85">
         <v>5</v>
       </c>
-      <c r="E4" s="85"/>
+      <c r="E4" s="85">
+        <v>3</v>
+      </c>
       <c r="F4" s="85"/>
       <c r="G4" s="85"/>
       <c r="H4" s="85"/>
       <c r="I4" s="85"/>
       <c r="J4" s="77">
         <f>IF(C4&gt;C3,1,0)+IF(D4&gt;D3,1,0)+IF(E4&gt;E3,1,0)+IF(F4&gt;F3,1,0)+IF(G4&gt;G3,1,0)+IF(H4&gt;H3,1,0)+IF(I4&gt;I3,1,0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K4" s="14"/>
       <c r="L4" s="4"/>
@@ -14840,14 +14847,16 @@
       <c r="D13" s="86">
         <v>3</v>
       </c>
-      <c r="E13" s="85"/>
+      <c r="E13" s="85">
+        <v>4</v>
+      </c>
       <c r="F13" s="85"/>
       <c r="G13" s="86"/>
       <c r="H13" s="86"/>
       <c r="I13" s="86"/>
       <c r="J13" s="77">
         <f>IF(C13&gt;C14,1,0)+IF(D13&gt;D14,1,0)+IF(E13&gt;E14,1,0)+IF(F13&gt;F14,1,0)+IF(G13&gt;G14,1,0)+IF(H13&gt;H14,1,0)+IF(I13&gt;I14,1,0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K13" s="16"/>
       <c r="L13" s="4"/>
@@ -14886,7 +14895,9 @@
       <c r="D14" s="86">
         <v>1</v>
       </c>
-      <c r="E14" s="85"/>
+      <c r="E14" s="85">
+        <v>1</v>
+      </c>
       <c r="F14" s="85"/>
       <c r="G14" s="86"/>
       <c r="H14" s="86"/>
@@ -15135,14 +15146,16 @@
       <c r="D20" s="85">
         <v>3</v>
       </c>
-      <c r="E20" s="85"/>
+      <c r="E20" s="85">
+        <v>6</v>
+      </c>
       <c r="F20" s="85"/>
       <c r="G20" s="85"/>
       <c r="H20" s="85"/>
       <c r="I20" s="86"/>
       <c r="J20" s="77">
         <f>IF(C20&gt;C21,1,0)+IF(D20&gt;D21,1,0)+IF(E20&gt;E21,1,0)+IF(F20&gt;F21,1,0)+IF(G20&gt;G21,1,0)+IF(H20&gt;H21,1,0)+IF(I20&gt;I21,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" s="16"/>
       <c r="L20" s="13"/>
@@ -15189,7 +15202,9 @@
       <c r="D21" s="85">
         <v>4</v>
       </c>
-      <c r="E21" s="85"/>
+      <c r="E21" s="85">
+        <v>3</v>
+      </c>
       <c r="F21" s="85"/>
       <c r="G21" s="85"/>
       <c r="H21" s="85"/>
@@ -15465,7 +15480,9 @@
       <c r="D27" s="85">
         <v>3</v>
       </c>
-      <c r="E27" s="86"/>
+      <c r="E27" s="86">
+        <v>3</v>
+      </c>
       <c r="F27" s="86"/>
       <c r="G27" s="85"/>
       <c r="H27" s="86"/>
@@ -15508,14 +15525,16 @@
       <c r="D28" s="85">
         <v>5</v>
       </c>
-      <c r="E28" s="85"/>
+      <c r="E28" s="85">
+        <v>6</v>
+      </c>
       <c r="F28" s="86"/>
       <c r="G28" s="85"/>
       <c r="H28" s="86"/>
       <c r="I28" s="85"/>
       <c r="J28" s="77">
         <f>IF(C28&gt;C27,1,0)+IF(D28&gt;D27,1,0)+IF(E28&gt;E27,1,0)+IF(F28&gt;F27,1,0)+IF(G28&gt;G27,1,0)+IF(H28&gt;H27,1,0)+IF(I28&gt;I27,1,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M28" s="1"/>
       <c r="O28" s="52"/>

</xml_diff>

<commit_message>
Updated games of 2019-04-17
</commit_message>
<xml_diff>
--- a/laval.xlsx
+++ b/laval.xlsx
@@ -2462,30 +2462,150 @@
     <xf numFmtId="0" fontId="19" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="106" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="105" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="87" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="95" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="86" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="88" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2537,151 +2657,31 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="86" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="87" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="88" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="95" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="106" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="105" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3905,217 +3905,217 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="C1" s="272"/>
-      <c r="D1" s="272"/>
-      <c r="E1" s="272"/>
-      <c r="F1" s="272"/>
-      <c r="G1" s="272"/>
-      <c r="H1" s="272"/>
-      <c r="I1" s="272"/>
-      <c r="J1" s="272"/>
-      <c r="K1" s="272"/>
-      <c r="L1" s="272"/>
-      <c r="M1" s="272"/>
-      <c r="N1" s="272"/>
-      <c r="O1" s="272"/>
-      <c r="P1" s="273"/>
-      <c r="Q1" s="273"/>
-      <c r="R1" s="273"/>
-      <c r="S1" s="273"/>
-      <c r="T1" s="273"/>
-      <c r="U1" s="273"/>
-      <c r="V1" s="273"/>
-      <c r="W1" s="273"/>
-      <c r="X1" s="273"/>
-      <c r="Y1" s="273"/>
-      <c r="Z1" s="273"/>
-      <c r="AA1" s="273"/>
-      <c r="AB1" s="273"/>
-      <c r="AC1" s="273"/>
-      <c r="AD1" s="273"/>
-      <c r="AE1" s="273"/>
-      <c r="AF1" s="273"/>
-      <c r="AG1" s="273"/>
-      <c r="AH1" s="273"/>
-      <c r="AI1" s="273"/>
-      <c r="AJ1" s="273"/>
+      <c r="C1" s="271"/>
+      <c r="D1" s="271"/>
+      <c r="E1" s="271"/>
+      <c r="F1" s="271"/>
+      <c r="G1" s="271"/>
+      <c r="H1" s="271"/>
+      <c r="I1" s="271"/>
+      <c r="J1" s="271"/>
+      <c r="K1" s="271"/>
+      <c r="L1" s="271"/>
+      <c r="M1" s="271"/>
+      <c r="N1" s="271"/>
+      <c r="O1" s="271"/>
+      <c r="P1" s="272"/>
+      <c r="Q1" s="272"/>
+      <c r="R1" s="272"/>
+      <c r="S1" s="272"/>
+      <c r="T1" s="272"/>
+      <c r="U1" s="272"/>
+      <c r="V1" s="272"/>
+      <c r="W1" s="272"/>
+      <c r="X1" s="272"/>
+      <c r="Y1" s="272"/>
+      <c r="Z1" s="272"/>
+      <c r="AA1" s="272"/>
+      <c r="AB1" s="272"/>
+      <c r="AC1" s="272"/>
+      <c r="AD1" s="272"/>
+      <c r="AE1" s="272"/>
+      <c r="AF1" s="272"/>
+      <c r="AG1" s="272"/>
+      <c r="AH1" s="272"/>
+      <c r="AI1" s="272"/>
+      <c r="AJ1" s="272"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="41"/>
-      <c r="C2" s="274" t="s">
+      <c r="C2" s="273" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="274"/>
-      <c r="E2" s="274"/>
-      <c r="F2" s="274"/>
-      <c r="G2" s="274"/>
-      <c r="H2" s="274"/>
-      <c r="I2" s="274"/>
-      <c r="J2" s="274"/>
-      <c r="K2" s="274"/>
-      <c r="L2" s="274"/>
-      <c r="M2" s="274"/>
-      <c r="N2" s="274"/>
-      <c r="O2" s="274"/>
-      <c r="P2" s="274"/>
-      <c r="Q2" s="275" t="s">
+      <c r="D2" s="273"/>
+      <c r="E2" s="273"/>
+      <c r="F2" s="273"/>
+      <c r="G2" s="273"/>
+      <c r="H2" s="273"/>
+      <c r="I2" s="273"/>
+      <c r="J2" s="273"/>
+      <c r="K2" s="273"/>
+      <c r="L2" s="273"/>
+      <c r="M2" s="273"/>
+      <c r="N2" s="273"/>
+      <c r="O2" s="273"/>
+      <c r="P2" s="273"/>
+      <c r="Q2" s="274" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="273"/>
-      <c r="S2" s="273"/>
-      <c r="T2" s="273"/>
-      <c r="U2" s="273"/>
-      <c r="V2" s="273"/>
-      <c r="W2" s="273"/>
-      <c r="X2" s="273"/>
-      <c r="Y2" s="273"/>
-      <c r="Z2" s="273"/>
-      <c r="AA2" s="273"/>
-      <c r="AB2" s="273"/>
-      <c r="AC2" s="273"/>
-      <c r="AD2" s="273"/>
-      <c r="AE2" s="273"/>
-      <c r="AF2" s="273"/>
-      <c r="AG2" s="273"/>
-      <c r="AH2" s="273"/>
-      <c r="AI2" s="273"/>
-      <c r="AJ2" s="273"/>
+      <c r="R2" s="272"/>
+      <c r="S2" s="272"/>
+      <c r="T2" s="272"/>
+      <c r="U2" s="272"/>
+      <c r="V2" s="272"/>
+      <c r="W2" s="272"/>
+      <c r="X2" s="272"/>
+      <c r="Y2" s="272"/>
+      <c r="Z2" s="272"/>
+      <c r="AA2" s="272"/>
+      <c r="AB2" s="272"/>
+      <c r="AC2" s="272"/>
+      <c r="AD2" s="272"/>
+      <c r="AE2" s="272"/>
+      <c r="AF2" s="272"/>
+      <c r="AG2" s="272"/>
+      <c r="AH2" s="272"/>
+      <c r="AI2" s="272"/>
+      <c r="AJ2" s="272"/>
     </row>
     <row r="3" spans="1:38" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="272"/>
-      <c r="D3" s="272"/>
-      <c r="E3" s="272"/>
-      <c r="F3" s="272"/>
-      <c r="G3" s="272"/>
-      <c r="H3" s="272"/>
-      <c r="I3" s="272"/>
-      <c r="J3" s="272"/>
-      <c r="K3" s="272"/>
-      <c r="L3" s="272"/>
-      <c r="M3" s="272"/>
-      <c r="N3" s="272"/>
-      <c r="O3" s="272"/>
-      <c r="P3" s="273"/>
-      <c r="Q3" s="273"/>
-      <c r="R3" s="273"/>
-      <c r="S3" s="273"/>
-      <c r="T3" s="273"/>
-      <c r="U3" s="273"/>
-      <c r="V3" s="273"/>
-      <c r="W3" s="273"/>
-      <c r="X3" s="273"/>
-      <c r="Y3" s="273"/>
-      <c r="Z3" s="273"/>
-      <c r="AA3" s="273"/>
-      <c r="AB3" s="273"/>
-      <c r="AC3" s="273"/>
-      <c r="AD3" s="273"/>
-      <c r="AE3" s="273"/>
-      <c r="AF3" s="273"/>
-      <c r="AG3" s="273"/>
-      <c r="AH3" s="273"/>
-      <c r="AI3" s="273"/>
-      <c r="AJ3" s="273"/>
+      <c r="C3" s="271"/>
+      <c r="D3" s="271"/>
+      <c r="E3" s="271"/>
+      <c r="F3" s="271"/>
+      <c r="G3" s="271"/>
+      <c r="H3" s="271"/>
+      <c r="I3" s="271"/>
+      <c r="J3" s="271"/>
+      <c r="K3" s="271"/>
+      <c r="L3" s="271"/>
+      <c r="M3" s="271"/>
+      <c r="N3" s="271"/>
+      <c r="O3" s="271"/>
+      <c r="P3" s="272"/>
+      <c r="Q3" s="272"/>
+      <c r="R3" s="272"/>
+      <c r="S3" s="272"/>
+      <c r="T3" s="272"/>
+      <c r="U3" s="272"/>
+      <c r="V3" s="272"/>
+      <c r="W3" s="272"/>
+      <c r="X3" s="272"/>
+      <c r="Y3" s="272"/>
+      <c r="Z3" s="272"/>
+      <c r="AA3" s="272"/>
+      <c r="AB3" s="272"/>
+      <c r="AC3" s="272"/>
+      <c r="AD3" s="272"/>
+      <c r="AE3" s="272"/>
+      <c r="AF3" s="272"/>
+      <c r="AG3" s="272"/>
+      <c r="AH3" s="272"/>
+      <c r="AI3" s="272"/>
+      <c r="AJ3" s="272"/>
     </row>
     <row r="4" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="256" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="257"/>
-      <c r="E4" s="257"/>
-      <c r="F4" s="257"/>
-      <c r="G4" s="257"/>
-      <c r="H4" s="257"/>
-      <c r="I4" s="257"/>
-      <c r="J4" s="257"/>
-      <c r="K4" s="257"/>
-      <c r="L4" s="257"/>
-      <c r="M4" s="257"/>
-      <c r="N4" s="257"/>
-      <c r="O4" s="257"/>
-      <c r="P4" s="257"/>
-      <c r="Q4" s="257"/>
-      <c r="R4" s="257"/>
-      <c r="S4" s="258"/>
-      <c r="T4" s="256" t="s">
+      <c r="C4" s="296" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="297"/>
+      <c r="E4" s="297"/>
+      <c r="F4" s="297"/>
+      <c r="G4" s="297"/>
+      <c r="H4" s="297"/>
+      <c r="I4" s="297"/>
+      <c r="J4" s="297"/>
+      <c r="K4" s="297"/>
+      <c r="L4" s="297"/>
+      <c r="M4" s="297"/>
+      <c r="N4" s="297"/>
+      <c r="O4" s="297"/>
+      <c r="P4" s="297"/>
+      <c r="Q4" s="297"/>
+      <c r="R4" s="297"/>
+      <c r="S4" s="298"/>
+      <c r="T4" s="296" t="s">
         <v>1</v>
       </c>
-      <c r="U4" s="257"/>
-      <c r="V4" s="257"/>
-      <c r="W4" s="257"/>
-      <c r="X4" s="257"/>
-      <c r="Y4" s="257"/>
-      <c r="Z4" s="257"/>
-      <c r="AA4" s="257"/>
-      <c r="AB4" s="258"/>
-      <c r="AC4" s="256" t="s">
+      <c r="U4" s="297"/>
+      <c r="V4" s="297"/>
+      <c r="W4" s="297"/>
+      <c r="X4" s="297"/>
+      <c r="Y4" s="297"/>
+      <c r="Z4" s="297"/>
+      <c r="AA4" s="297"/>
+      <c r="AB4" s="298"/>
+      <c r="AC4" s="296" t="s">
         <v>2</v>
       </c>
-      <c r="AD4" s="257"/>
-      <c r="AE4" s="257"/>
-      <c r="AF4" s="257"/>
-      <c r="AG4" s="267"/>
-      <c r="AH4" s="256" t="s">
+      <c r="AD4" s="297"/>
+      <c r="AE4" s="297"/>
+      <c r="AF4" s="297"/>
+      <c r="AG4" s="305"/>
+      <c r="AH4" s="296" t="s">
         <v>10</v>
       </c>
-      <c r="AI4" s="257"/>
-      <c r="AJ4" s="258"/>
+      <c r="AI4" s="297"/>
+      <c r="AJ4" s="298"/>
     </row>
     <row r="5" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="268" t="s">
+      <c r="C5" s="265" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="264"/>
-      <c r="E5" s="264"/>
-      <c r="F5" s="264"/>
-      <c r="G5" s="264"/>
-      <c r="H5" s="264"/>
-      <c r="I5" s="264"/>
-      <c r="J5" s="265"/>
-      <c r="K5" s="263" t="s">
+      <c r="D5" s="266"/>
+      <c r="E5" s="266"/>
+      <c r="F5" s="266"/>
+      <c r="G5" s="266"/>
+      <c r="H5" s="266"/>
+      <c r="I5" s="266"/>
+      <c r="J5" s="267"/>
+      <c r="K5" s="303" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="264"/>
-      <c r="M5" s="264"/>
-      <c r="N5" s="264"/>
-      <c r="O5" s="264"/>
-      <c r="P5" s="264"/>
-      <c r="Q5" s="264"/>
-      <c r="R5" s="265"/>
-      <c r="S5" s="259" t="s">
+      <c r="L5" s="266"/>
+      <c r="M5" s="266"/>
+      <c r="N5" s="266"/>
+      <c r="O5" s="266"/>
+      <c r="P5" s="266"/>
+      <c r="Q5" s="266"/>
+      <c r="R5" s="267"/>
+      <c r="S5" s="299" t="s">
         <v>12</v>
       </c>
-      <c r="T5" s="268" t="s">
+      <c r="T5" s="265" t="s">
         <v>9</v>
       </c>
-      <c r="U5" s="264"/>
-      <c r="V5" s="264"/>
-      <c r="W5" s="265"/>
-      <c r="X5" s="263" t="s">
+      <c r="U5" s="266"/>
+      <c r="V5" s="266"/>
+      <c r="W5" s="267"/>
+      <c r="X5" s="303" t="s">
         <v>8</v>
       </c>
-      <c r="Y5" s="264"/>
-      <c r="Z5" s="264"/>
-      <c r="AA5" s="265"/>
-      <c r="AB5" s="259" t="s">
+      <c r="Y5" s="266"/>
+      <c r="Z5" s="266"/>
+      <c r="AA5" s="267"/>
+      <c r="AB5" s="299" t="s">
         <v>13</v>
       </c>
-      <c r="AC5" s="266" t="s">
+      <c r="AC5" s="304" t="s">
         <v>9</v>
       </c>
-      <c r="AD5" s="265"/>
-      <c r="AE5" s="263" t="s">
+      <c r="AD5" s="267"/>
+      <c r="AE5" s="303" t="s">
         <v>8</v>
       </c>
-      <c r="AF5" s="265"/>
-      <c r="AG5" s="259" t="s">
+      <c r="AF5" s="267"/>
+      <c r="AG5" s="299" t="s">
         <v>14</v>
       </c>
       <c r="AH5" s="56"/>
       <c r="AI5" s="25"/>
-      <c r="AJ5" s="259" t="s">
+      <c r="AJ5" s="299" t="s">
         <v>15</v>
       </c>
       <c r="AK5" s="4"/>
@@ -4127,13 +4127,13 @@
         <f>Résultats!$J$3</f>
         <v>0</v>
       </c>
-      <c r="D6" s="303">
+      <c r="D6" s="244">
         <f>Résultats!$J$4</f>
         <v>4</v>
       </c>
       <c r="E6" s="172">
         <f>Résultats!$J$6</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" s="109">
         <f>Résultats!$J$7</f>
@@ -4147,7 +4147,7 @@
         <f>Résultats!$J$11</f>
         <v>1</v>
       </c>
-      <c r="I6" s="299">
+      <c r="I6" s="240">
         <f>Résultats!$J$13</f>
         <v>4</v>
       </c>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="L6" s="108">
         <f>Résultats!$J$18</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M6" s="172">
         <f>Résultats!$J$20</f>
@@ -4177,7 +4177,7 @@
       </c>
       <c r="P6" s="109">
         <f>Résultats!$J$25</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q6" s="111">
         <f>Résultats!$J$27</f>
@@ -4187,7 +4187,7 @@
         <f>Résultats!$J$28</f>
         <v>3</v>
       </c>
-      <c r="S6" s="260"/>
+      <c r="S6" s="300"/>
       <c r="T6" s="169">
         <f>Résultats!$V$6</f>
         <v>0</v>
@@ -4220,7 +4220,7 @@
         <f>Résultats!$V$25</f>
         <v>0</v>
       </c>
-      <c r="AB6" s="260"/>
+      <c r="AB6" s="300"/>
       <c r="AC6" s="111">
         <f>Résultats!$AH$8</f>
         <v>0</v>
@@ -4237,7 +4237,7 @@
         <f>Résultats!$AH$23</f>
         <v>0</v>
       </c>
-      <c r="AG6" s="260"/>
+      <c r="AG6" s="300"/>
       <c r="AH6" s="212">
         <f>Résultats!$AH$15</f>
         <v>0</v>
@@ -4246,7 +4246,7 @@
         <f>Résultats!$AH$16</f>
         <v>0</v>
       </c>
-      <c r="AJ6" s="260"/>
+      <c r="AJ6" s="300"/>
       <c r="AK6" s="37"/>
     </row>
     <row r="7" spans="1:38" s="39" customFormat="1" ht="58.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -4257,12 +4257,12 @@
 +IF(ISBLANK($D10),0,($D$6*PT_VICTOIRE_R1)+IF($D$6=4,PT_PREDICTION_EQUIPE_R1+IF($D10=$C$6+$D$6,PT_PREDICTION_NB_PARTIES_R1,0),0))</f>
         <v>0</v>
       </c>
-      <c r="D7" s="304"/>
+      <c r="D7" s="245"/>
       <c r="E7" s="173"/>
       <c r="F7" s="118"/>
       <c r="G7" s="119"/>
       <c r="H7" s="117"/>
-      <c r="I7" s="300"/>
+      <c r="I7" s="241"/>
       <c r="J7" s="117"/>
       <c r="K7" s="120"/>
       <c r="L7" s="117"/>
@@ -4272,7 +4272,7 @@
       <c r="P7" s="118"/>
       <c r="Q7" s="119"/>
       <c r="R7" s="117"/>
-      <c r="S7" s="260"/>
+      <c r="S7" s="300"/>
       <c r="T7" s="170"/>
       <c r="U7" s="117"/>
       <c r="V7" s="173"/>
@@ -4281,15 +4281,15 @@
       <c r="Y7" s="118"/>
       <c r="Z7" s="119"/>
       <c r="AA7" s="117"/>
-      <c r="AB7" s="260"/>
+      <c r="AB7" s="300"/>
       <c r="AC7" s="119"/>
       <c r="AD7" s="117"/>
       <c r="AE7" s="120"/>
       <c r="AF7" s="117"/>
-      <c r="AG7" s="260"/>
+      <c r="AG7" s="300"/>
       <c r="AH7" s="212"/>
       <c r="AI7" s="112"/>
-      <c r="AJ7" s="260"/>
+      <c r="AJ7" s="300"/>
       <c r="AK7" s="37"/>
     </row>
     <row r="8" spans="1:38" s="39" customFormat="1" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4299,7 +4299,7 @@
         <f>Résultats!$B$3</f>
         <v>TAMPA BAY</v>
       </c>
-      <c r="D8" s="305" t="str">
+      <c r="D8" s="246" t="str">
         <f>Résultats!$B$4</f>
         <v>COLUMBUS</v>
       </c>
@@ -4319,7 +4319,7 @@
         <f>Résultats!$B$11</f>
         <v>CAROLINE</v>
       </c>
-      <c r="I8" s="301" t="str">
+      <c r="I8" s="242" t="str">
         <f>Résultats!$B$13</f>
         <v>NEW YORK I.</v>
       </c>
@@ -4359,7 +4359,7 @@
         <f>Résultats!$B$28</f>
         <v>VEGAS</v>
       </c>
-      <c r="S8" s="260"/>
+      <c r="S8" s="300"/>
       <c r="T8" s="171" t="str">
         <f>Résultats!$N$6</f>
         <v xml:space="preserve"> </v>
@@ -4392,7 +4392,7 @@
         <f>Résultats!$N$25</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AB8" s="260"/>
+      <c r="AB8" s="300"/>
       <c r="AC8" s="177" t="str">
         <f>Résultats!$Z$8</f>
         <v xml:space="preserve"> </v>
@@ -4409,7 +4409,7 @@
         <f>Résultats!$Z$23</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AG8" s="260"/>
+      <c r="AG8" s="300"/>
       <c r="AH8" s="213" t="str">
         <f>Résultats!$Z$15</f>
         <v xml:space="preserve"> </v>
@@ -4418,7 +4418,7 @@
         <f>Résultats!$Z$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ8" s="260"/>
+      <c r="AJ8" s="300"/>
       <c r="AK8" s="37"/>
     </row>
     <row r="9" spans="1:38" s="39" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4432,7 +4432,7 @@
         <f>Résultats!$A$3</f>
         <v>A1</v>
       </c>
-      <c r="D9" s="306" t="str">
+      <c r="D9" s="247" t="str">
         <f>Résultats!$A$4</f>
         <v>WC2</v>
       </c>
@@ -4452,7 +4452,7 @@
         <f>Résultats!$A$11</f>
         <v>WC1</v>
       </c>
-      <c r="I9" s="302" t="str">
+      <c r="I9" s="243" t="str">
         <f>Résultats!$A$13</f>
         <v>M2</v>
       </c>
@@ -4492,7 +4492,7 @@
         <f>Résultats!$A$28</f>
         <v>P3</v>
       </c>
-      <c r="S9" s="262"/>
+      <c r="S9" s="302"/>
       <c r="T9" s="179" t="str">
         <f>Résultats!$M$6</f>
         <v xml:space="preserve"> </v>
@@ -4525,7 +4525,7 @@
         <f>Résultats!$M$25</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AB9" s="261"/>
+      <c r="AB9" s="301"/>
       <c r="AC9" s="183" t="str">
         <f>Résultats!$Y$8</f>
         <v xml:space="preserve"> </v>
@@ -4542,7 +4542,7 @@
         <f>Résultats!$Y$23</f>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="AG9" s="261"/>
+      <c r="AG9" s="301"/>
       <c r="AH9" s="215" t="str">
         <f>Résultats!$Y$15</f>
         <v xml:space="preserve"> </v>
@@ -4551,7 +4551,7 @@
         <f>Résultats!$Y$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ9" s="262"/>
+      <c r="AJ9" s="302"/>
       <c r="AK9" s="114" t="s">
         <v>51</v>
       </c>
@@ -4601,7 +4601,7 @@
       </c>
       <c r="S10" s="194">
         <f>SUM(C11:R11)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="T10" s="187"/>
       <c r="U10" s="189"/>
@@ -4635,7 +4635,7 @@
       </c>
       <c r="AL10" s="194">
         <f>$S10+$AB10+$AG10+$AJ10</f>
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -4651,7 +4651,7 @@
       <c r="D11" s="134"/>
       <c r="E11" s="132">
         <f>(IF($E10&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E10=$E$6+$F$6,$O$103,0),0),0)+IF($F10&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F10=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11" s="134"/>
       <c r="G11" s="132">
@@ -4958,7 +4958,7 @@
     <row r="14" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="122">
         <f>RANK(AL14,$AL$10:$AL$97,)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" s="88" t="s">
         <v>71</v>
@@ -4997,7 +4997,7 @@
       </c>
       <c r="S14" s="129">
         <f>SUM(C15:R15)</f>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="T14" s="46"/>
       <c r="U14" s="47"/>
@@ -5012,7 +5012,7 @@
         <v>0</v>
       </c>
       <c r="AC14" s="48"/>
-      <c r="AD14" s="307"/>
+      <c r="AD14" s="248"/>
       <c r="AE14" s="49"/>
       <c r="AF14" s="47"/>
       <c r="AG14" s="129">
@@ -5027,11 +5027,11 @@
       </c>
       <c r="AK14" s="116">
         <f>MAX($AL$10:$AL$97) - AL14</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL14" s="129">
         <f>$S14+$AB14+$AG14+$AJ14</f>
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5047,7 +5047,7 @@
       <c r="D15" s="150"/>
       <c r="E15" s="132">
         <f>(IF($E14&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E14=$E$6+$F$6,$O$103,0),0),0)+IF($F14&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F14=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" s="150"/>
       <c r="G15" s="132">
@@ -5072,7 +5072,7 @@
       <c r="N15" s="150"/>
       <c r="O15" s="126">
         <f>(IF($O14&lt;&gt;"",($O$6*$O$104)+IF($O$6=4,($O$102)+IF($O14=$O$6+$P$6,$O$103,0),0),0)+IF($P14&lt;&gt;"",($P$6*$O$104)+IF($P$6=4,($O$102)+IF($P14=$O$6+$P$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P15" s="150"/>
       <c r="Q15" s="126">
@@ -5100,7 +5100,7 @@
       <c r="AJ15" s="128"/>
       <c r="AK15" s="96">
         <f>MAX($AL$10:$AL$97) - AL15</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AL15" s="128"/>
     </row>
@@ -5394,9 +5394,9 @@
         <v>7</v>
       </c>
       <c r="R18" s="204"/>
-      <c r="S18" s="309">
+      <c r="S18" s="250">
         <f>SUM(C19:R19)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="T18" s="198"/>
       <c r="U18" s="202"/>
@@ -5430,7 +5430,7 @@
       </c>
       <c r="AL18" s="205">
         <f>$S18+$AB18+$AG18+$AJ18</f>
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5446,7 +5446,7 @@
       <c r="D19" s="150"/>
       <c r="E19" s="126">
         <f>(IF($E18&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E18=$E$6+$F$6,$O$103,0),0),0)+IF($F18&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F18=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F19" s="150"/>
       <c r="G19" s="126">
@@ -5499,7 +5499,7 @@
       <c r="AJ19" s="154"/>
       <c r="AK19" s="162">
         <f>MAX($AL$10:$AL$97) - AL19</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AL19" s="128"/>
     </row>
@@ -5795,7 +5795,7 @@
       <c r="R22" s="50"/>
       <c r="S22" s="116">
         <f>SUM(C23:R23)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="T22" s="46"/>
       <c r="U22" s="47"/>
@@ -5829,7 +5829,7 @@
       </c>
       <c r="AL22" s="129">
         <f>$S22+$AB22+$AG22+$AJ22</f>
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5845,7 +5845,7 @@
       <c r="D23" s="163"/>
       <c r="E23" s="132">
         <f>(IF($E22&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E22=$E$6+$F$6,$O$103,0),0),0)+IF($F22&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F22=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F23" s="163"/>
       <c r="G23" s="132">
@@ -5898,7 +5898,7 @@
       <c r="AJ23" s="154"/>
       <c r="AK23" s="162">
         <f>MAX($AL$10:$AL$97) - AL23</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AL23" s="128"/>
     </row>
@@ -6194,7 +6194,7 @@
       </c>
       <c r="S26" s="205">
         <f>SUM(C27:R27)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T26" s="198"/>
       <c r="U26" s="202"/>
@@ -6228,7 +6228,7 @@
       </c>
       <c r="AL26" s="205">
         <f>$S26+$AB26+$AG26+$AJ26</f>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6259,7 +6259,7 @@
       <c r="J27" s="151"/>
       <c r="K27" s="152">
         <f>(IF($K26&lt;&gt;"",($K$6*$O$104)+IF($K$6=4,($O$102)+IF($K26=$K$6+$L$6,$O$103,0),0),0)+IF($L26&lt;&gt;"",($L$6*$O$104)+IF($L$6=4,($O$102)+IF($L26=$K$6+$L$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L27" s="150"/>
       <c r="M27" s="126">
@@ -6297,7 +6297,7 @@
       <c r="AJ27" s="154"/>
       <c r="AK27" s="162">
         <f>MAX($AL$10:$AL$97) - AL27</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AL27" s="128"/>
     </row>
@@ -6623,7 +6623,7 @@
       </c>
       <c r="AK30" s="116">
         <f>MAX($AL$10:$AL$97) - AL30</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AL30" s="129">
         <f>$S30+$AB30+$AG30+$AJ30</f>
@@ -6696,7 +6696,7 @@
       <c r="AJ31" s="128"/>
       <c r="AK31" s="96">
         <f>MAX($AL$10:$AL$97) - AL31</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AL31" s="128"/>
     </row>
@@ -6956,18 +6956,18 @@
         <v>6</v>
       </c>
       <c r="B34" s="211" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="C34" s="198">
+        <v>4</v>
+      </c>
+      <c r="D34" s="199"/>
+      <c r="E34" s="200">
+        <v>4</v>
+      </c>
+      <c r="F34" s="199"/>
+      <c r="G34" s="201">
         <v>6</v>
-      </c>
-      <c r="D34" s="199"/>
-      <c r="E34" s="200"/>
-      <c r="F34" s="199">
-        <v>7</v>
-      </c>
-      <c r="G34" s="201">
-        <v>7</v>
       </c>
       <c r="H34" s="202"/>
       <c r="I34" s="200"/>
@@ -6979,11 +6979,11 @@
       </c>
       <c r="L34" s="202"/>
       <c r="M34" s="200">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="N34" s="199"/>
       <c r="O34" s="200">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P34" s="199"/>
       <c r="Q34" s="201"/>
@@ -7000,14 +7000,14 @@
       <c r="W34" s="202"/>
       <c r="X34" s="203"/>
       <c r="Y34" s="199"/>
-      <c r="Z34" s="201"/>
+      <c r="Z34" s="208"/>
       <c r="AA34" s="202"/>
       <c r="AB34" s="205">
         <f>SUM(T35:AA35)</f>
         <v>0</v>
       </c>
       <c r="AC34" s="201"/>
-      <c r="AD34" s="202"/>
+      <c r="AD34" s="234"/>
       <c r="AE34" s="203"/>
       <c r="AF34" s="202"/>
       <c r="AG34" s="205">
@@ -7022,7 +7022,7 @@
       </c>
       <c r="AK34" s="207">
         <f>MAX($AL$10:$AL$97) - AL34</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AL34" s="205">
         <f>$S34+$AB34+$AG34+$AJ34</f>
@@ -7095,7 +7095,7 @@
       <c r="AJ35" s="128"/>
       <c r="AK35" s="96">
         <f>MAX($AL$10:$AL$97) - AL35</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AL35" s="128"/>
     </row>
@@ -7355,10 +7355,10 @@
         <v>6</v>
       </c>
       <c r="B38" s="88" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C38" s="46">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D38" s="45"/>
       <c r="E38" s="44"/>
@@ -7366,34 +7366,34 @@
         <v>7</v>
       </c>
       <c r="G38" s="48">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H38" s="47"/>
       <c r="I38" s="44"/>
       <c r="J38" s="47">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K38" s="49">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L38" s="47"/>
       <c r="M38" s="44">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N38" s="45"/>
       <c r="O38" s="44">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P38" s="45"/>
       <c r="Q38" s="48"/>
       <c r="R38" s="50">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S38" s="129">
         <f>SUM(C39:R39)</f>
         <v>12</v>
       </c>
-      <c r="T38" s="237"/>
+      <c r="T38" s="46"/>
       <c r="U38" s="47"/>
       <c r="V38" s="44"/>
       <c r="W38" s="47"/>
@@ -7421,7 +7421,7 @@
       </c>
       <c r="AK38" s="116">
         <f>MAX($AL$10:$AL$97) - AL38</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AL38" s="129">
         <f>$S38+$AB38+$AG38+$AJ38</f>
@@ -7494,7 +7494,7 @@
       <c r="AJ39" s="128"/>
       <c r="AK39" s="96">
         <f>MAX($AL$10:$AL$97) - AL39</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AL39" s="128"/>
     </row>
@@ -7751,46 +7751,46 @@
     <row r="42" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="186">
         <f>RANK(AL42,$AL$10:$AL$97,)</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B42" s="211" t="s">
-        <v>67</v>
-      </c>
-      <c r="C42" s="198">
-        <v>4</v>
-      </c>
-      <c r="D42" s="199"/>
-      <c r="E42" s="200">
-        <v>4</v>
-      </c>
-      <c r="F42" s="199"/>
-      <c r="G42" s="201">
+        <v>68</v>
+      </c>
+      <c r="C42" s="306">
+        <v>5</v>
+      </c>
+      <c r="D42" s="307"/>
+      <c r="E42" s="308">
         <v>6</v>
       </c>
-      <c r="H42" s="202"/>
-      <c r="I42" s="200"/>
-      <c r="J42" s="202">
+      <c r="F42" s="307"/>
+      <c r="G42" s="309">
+        <v>5</v>
+      </c>
+      <c r="H42" s="310"/>
+      <c r="I42" s="308"/>
+      <c r="J42" s="310">
         <v>6</v>
       </c>
-      <c r="K42" s="203">
+      <c r="K42" s="311">
         <v>6</v>
       </c>
-      <c r="L42" s="202"/>
-      <c r="M42" s="200">
-        <v>5</v>
-      </c>
-      <c r="N42" s="199"/>
-      <c r="O42" s="200">
+      <c r="L42" s="310"/>
+      <c r="M42" s="308">
+        <v>7</v>
+      </c>
+      <c r="N42" s="307"/>
+      <c r="O42" s="308">
         <v>6</v>
       </c>
-      <c r="P42" s="199"/>
-      <c r="Q42" s="201"/>
-      <c r="R42" s="204">
+      <c r="P42" s="307"/>
+      <c r="Q42" s="309"/>
+      <c r="R42" s="312">
         <v>6</v>
       </c>
       <c r="S42" s="205">
         <f>SUM(C43:R43)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="T42" s="198"/>
       <c r="U42" s="202"/>
@@ -7798,14 +7798,14 @@
       <c r="W42" s="202"/>
       <c r="X42" s="203"/>
       <c r="Y42" s="199"/>
-      <c r="Z42" s="208"/>
+      <c r="Z42" s="201"/>
       <c r="AA42" s="202"/>
       <c r="AB42" s="205">
         <f>SUM(T43:AA43)</f>
         <v>0</v>
       </c>
       <c r="AC42" s="201"/>
-      <c r="AD42" s="234"/>
+      <c r="AD42" s="202"/>
       <c r="AE42" s="203"/>
       <c r="AF42" s="202"/>
       <c r="AG42" s="205">
@@ -7824,7 +7824,7 @@
       </c>
       <c r="AL42" s="205">
         <f>$S42+$AB42+$AG42+$AJ42</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7840,7 +7840,7 @@
       <c r="D43" s="80"/>
       <c r="E43" s="121">
         <f>(IF($E42&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E42=$E$6+$F$6,$O$103,0),0),0)+IF($F42&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F42=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F43" s="80"/>
       <c r="G43" s="81">
@@ -7893,7 +7893,7 @@
       <c r="AJ43" s="128"/>
       <c r="AK43" s="116">
         <f>MAX($AL$10:$AL$97) - AL43</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AL43" s="128"/>
     </row>
@@ -8150,48 +8150,48 @@
     <row r="46" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="122">
         <f>RANK(AL46,$AL$10:$AL$97,)</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B46" s="88" t="s">
-        <v>68</v>
-      </c>
-      <c r="C46" s="239">
+        <v>78</v>
+      </c>
+      <c r="C46" s="46">
         <v>5</v>
       </c>
-      <c r="D46" s="240"/>
-      <c r="E46" s="241">
+      <c r="D46" s="45"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="45">
+        <v>7</v>
+      </c>
+      <c r="G46" s="48">
         <v>6</v>
       </c>
-      <c r="F46" s="240"/>
-      <c r="G46" s="242">
+      <c r="H46" s="47"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="47">
+        <v>7</v>
+      </c>
+      <c r="K46" s="49">
         <v>5</v>
       </c>
-      <c r="H46" s="243"/>
-      <c r="I46" s="241"/>
-      <c r="J46" s="243">
+      <c r="L46" s="47"/>
+      <c r="M46" s="44">
         <v>6</v>
       </c>
-      <c r="K46" s="244">
-        <v>6</v>
-      </c>
-      <c r="L46" s="243"/>
-      <c r="M46" s="241">
+      <c r="N46" s="45"/>
+      <c r="O46" s="44">
         <v>7</v>
       </c>
-      <c r="N46" s="240"/>
-      <c r="O46" s="241">
-        <v>6</v>
-      </c>
-      <c r="P46" s="240"/>
-      <c r="Q46" s="242"/>
-      <c r="R46" s="245">
-        <v>6</v>
+      <c r="P46" s="45"/>
+      <c r="Q46" s="48"/>
+      <c r="R46" s="50">
+        <v>7</v>
       </c>
       <c r="S46" s="129">
         <f>SUM(C47:R47)</f>
-        <v>11</v>
-      </c>
-      <c r="T46" s="46"/>
+        <v>12</v>
+      </c>
+      <c r="T46" s="237"/>
       <c r="U46" s="47"/>
       <c r="V46" s="44"/>
       <c r="W46" s="47"/>
@@ -8223,7 +8223,7 @@
       </c>
       <c r="AL46" s="129">
         <f>$S46+$AB46+$AG46+$AJ46</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -8239,7 +8239,7 @@
       <c r="D47" s="80"/>
       <c r="E47" s="81">
         <f>(IF($E46&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E46=$E$6+$F$6,$O$103,0),0),0)+IF($F46&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F46=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F47" s="80"/>
       <c r="G47" s="81">
@@ -8292,7 +8292,7 @@
       <c r="AJ47" s="128"/>
       <c r="AK47" s="116">
         <f>MAX($AL$10:$AL$97) - AL47</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AL47" s="128"/>
     </row>
@@ -8549,7 +8549,7 @@
     <row r="50" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="186">
         <f>RANK(AL50,$AL$10:$AL$97,)</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B50" s="211" t="s">
         <v>85</v>
@@ -8588,7 +8588,7 @@
       </c>
       <c r="S50" s="205">
         <f>SUM(C51:R51)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="T50" s="198"/>
       <c r="U50" s="202"/>
@@ -8622,7 +8622,7 @@
       </c>
       <c r="AL50" s="205">
         <f>$S50+$AB50+$AG50+$AJ50</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -8638,7 +8638,7 @@
       <c r="D51" s="134"/>
       <c r="E51" s="132">
         <f>(IF($E50&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E50=$E$6+$F$6,$O$103,0),0),0)+IF($F50&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F50=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F51" s="134"/>
       <c r="G51" s="132">
@@ -8945,7 +8945,7 @@
     <row r="54" spans="1:38" s="27" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="122">
         <f>RANK(AL54,$AL$10:$AL$97,)</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B54" s="88" t="s">
         <v>82</v>
@@ -8984,7 +8984,7 @@
       </c>
       <c r="S54" s="129">
         <f>SUM(C55:R55)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="T54" s="46"/>
       <c r="U54" s="47"/>
@@ -9018,7 +9018,7 @@
       </c>
       <c r="AL54" s="129">
         <f>$S54+$AB54+$AG54+$AJ54</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -9034,7 +9034,7 @@
       <c r="D55" s="134"/>
       <c r="E55" s="132">
         <f>(IF($E54&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E54=$E$6+$F$6,$O$103,0),0),0)+IF($F54&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F54=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F55" s="134"/>
       <c r="G55" s="132">
@@ -9341,7 +9341,7 @@
     <row r="58" spans="1:38" s="27" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="186">
         <f>RANK(AL58,$AL$10:$AL$97,)</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B58" s="211" t="s">
         <v>80</v>
@@ -9380,7 +9380,7 @@
       </c>
       <c r="S58" s="205">
         <f>SUM(C59:R59)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="T58" s="198"/>
       <c r="U58" s="202"/>
@@ -9414,7 +9414,7 @@
       </c>
       <c r="AL58" s="205">
         <f>$S58+$AB58+$AG58+$AJ58</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -9430,7 +9430,7 @@
       <c r="D59" s="134"/>
       <c r="E59" s="132">
         <f>(IF($E58&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E58=$E$6+$F$6,$O$103,0),0),0)+IF($F58&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F58=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F59" s="134"/>
       <c r="G59" s="132">
@@ -9737,7 +9737,7 @@
     <row r="62" spans="1:38" s="27" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="122">
         <f>RANK(AL62,$AL$10:$AL$97,)</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B62" s="88" t="s">
         <v>74</v>
@@ -9776,7 +9776,7 @@
       </c>
       <c r="S62" s="129">
         <f>SUM(C63:R63)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="T62" s="46"/>
       <c r="U62" s="47"/>
@@ -9810,7 +9810,7 @@
       </c>
       <c r="AL62" s="129">
         <f>$S62+$AB62+$AG62+$AJ62</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -9826,7 +9826,7 @@
       <c r="D63" s="134"/>
       <c r="E63" s="132">
         <f>(IF($E62&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E62=$E$6+$F$6,$O$103,0),0),0)+IF($F62&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F62=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F63" s="134"/>
       <c r="G63" s="132">
@@ -10133,7 +10133,7 @@
     <row r="66" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="186">
         <f>RANK(AL66,$AL$10:$AL$97,)</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B66" s="211" t="s">
         <v>75</v>
@@ -10172,7 +10172,7 @@
       </c>
       <c r="S66" s="205">
         <f>SUM(C67:R67)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="T66" s="198"/>
       <c r="U66" s="202"/>
@@ -10206,7 +10206,7 @@
       </c>
       <c r="AL66" s="205">
         <f>$S66+$AB66+$AG66+$AJ66</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="67" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -10222,7 +10222,7 @@
       <c r="D67" s="134"/>
       <c r="E67" s="132">
         <f>(IF($E66&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E66=$E$6+$F$6,$O$103,0),0),0)+IF($F66&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F66=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F67" s="134"/>
       <c r="G67" s="132">
@@ -10529,7 +10529,7 @@
     <row r="70" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="122">
         <f>RANK(AL70,$AL$10:$AL$97,)</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B70" s="88" t="s">
         <v>76</v>
@@ -10568,7 +10568,7 @@
       </c>
       <c r="S70" s="129">
         <f>SUM(C71:R71)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="T70" s="46"/>
       <c r="U70" s="47"/>
@@ -10602,7 +10602,7 @@
       </c>
       <c r="AL70" s="129">
         <f>$S70+$AB70+$AG70+$AJ70</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -10618,7 +10618,7 @@
       <c r="D71" s="134"/>
       <c r="E71" s="132">
         <f>(IF($E70&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E70=$E$6+$F$6,$O$103,0),0),0)+IF($F70&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F70=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F71" s="134"/>
       <c r="G71" s="132">
@@ -10964,7 +10964,7 @@
       </c>
       <c r="S74" s="205">
         <f>SUM(C75:R75)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T74" s="198"/>
       <c r="U74" s="202"/>
@@ -10998,7 +10998,7 @@
       </c>
       <c r="AL74" s="205">
         <f>$S74+$AB74+$AG74+$AJ74</f>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="75" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11014,7 +11014,7 @@
       <c r="D75" s="134"/>
       <c r="E75" s="132">
         <f>(IF($E74&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E74=$E$6+$F$6,$O$103,0),0),0)+IF($F74&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F74=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F75" s="134"/>
       <c r="G75" s="132">
@@ -11360,7 +11360,7 @@
       <c r="R78" s="50"/>
       <c r="S78" s="129">
         <f>SUM(C79:R79)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="T78" s="46"/>
       <c r="U78" s="47"/>
@@ -11382,7 +11382,7 @@
         <f>SUM(AC79:AF79)</f>
         <v>0</v>
       </c>
-      <c r="AH78" s="308"/>
+      <c r="AH78" s="249"/>
       <c r="AI78" s="58"/>
       <c r="AJ78" s="129">
         <f>AH79</f>
@@ -11394,7 +11394,7 @@
       </c>
       <c r="AL78" s="129">
         <f>$S78+$AB78+$AG78+$AJ78</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="79" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11410,7 +11410,7 @@
       <c r="D79" s="134"/>
       <c r="E79" s="132">
         <f>(IF($E78&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E78=$E$6+$F$6,$O$103,0),0),0)+IF($F78&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F78=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F79" s="134"/>
       <c r="G79" s="132">
@@ -11756,7 +11756,7 @@
       <c r="R82" s="204"/>
       <c r="S82" s="205">
         <f>SUM(C83:R83)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="T82" s="198"/>
       <c r="U82" s="202"/>
@@ -11790,7 +11790,7 @@
       </c>
       <c r="AL82" s="205">
         <f>$S82+$AB82+$AG82+$AJ82</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="83" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11806,7 +11806,7 @@
       <c r="D83" s="134"/>
       <c r="E83" s="132">
         <f>(IF($E82&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E82=$E$6+$F$6,$O$103,0),0),0)+IF($F82&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F82=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F83" s="134"/>
       <c r="G83" s="132">
@@ -12152,7 +12152,7 @@
       <c r="R86" s="50"/>
       <c r="S86" s="129">
         <f>SUM(C87:R87)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="T86" s="46"/>
       <c r="U86" s="47"/>
@@ -12186,7 +12186,7 @@
       </c>
       <c r="AL86" s="129">
         <f>$S86+$AB86+$AG86+$AJ86</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="87" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -12202,7 +12202,7 @@
       <c r="D87" s="134"/>
       <c r="E87" s="132">
         <f>(IF($E86&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E86=$E$6+$F$6,$O$103,0),0),0)+IF($F86&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F86=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F87" s="134"/>
       <c r="G87" s="132">
@@ -12518,15 +12518,15 @@
         <v>7</v>
       </c>
       <c r="D90" s="199"/>
-      <c r="E90" s="310">
+      <c r="E90" s="251">
         <v>6</v>
       </c>
       <c r="F90" s="199"/>
-      <c r="G90" s="311"/>
+      <c r="G90" s="252"/>
       <c r="H90" s="202">
         <v>6</v>
       </c>
-      <c r="I90" s="310"/>
+      <c r="I90" s="251"/>
       <c r="J90" s="202">
         <v>7</v>
       </c>
@@ -12548,14 +12548,14 @@
       <c r="R90" s="204"/>
       <c r="S90" s="205">
         <f>SUM(C91:R91)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="T90" s="198"/>
       <c r="U90" s="202"/>
-      <c r="V90" s="312"/>
+      <c r="V90" s="253"/>
       <c r="W90" s="202"/>
       <c r="X90" s="203"/>
-      <c r="Y90" s="246"/>
+      <c r="Y90" s="239"/>
       <c r="Z90" s="201"/>
       <c r="AA90" s="202"/>
       <c r="AB90" s="205">
@@ -12582,7 +12582,7 @@
       </c>
       <c r="AL90" s="205">
         <f>$S90+$AB90+$AG90+$AJ90</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="91" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -12598,7 +12598,7 @@
       <c r="D91" s="134"/>
       <c r="E91" s="132">
         <f>(IF($E90&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E90=$E$6+$F$6,$O$103,0),0),0)+IF($F90&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F90=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F91" s="134"/>
       <c r="G91" s="132">
@@ -12944,7 +12944,7 @@
       <c r="R94" s="232"/>
       <c r="S94" s="129">
         <f>SUM(C95:R95)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="T94" s="46"/>
       <c r="U94" s="47"/>
@@ -12978,7 +12978,7 @@
       </c>
       <c r="AL94" s="218">
         <f>$S94+$AB94+$AG94+$AJ94</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="95" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -12994,7 +12994,7 @@
       <c r="D95" s="134"/>
       <c r="E95" s="132">
         <f>(IF($E94&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E94=$E$6+$F$6,$O$103,0),0),0)+IF($F94&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F94=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F95" s="134"/>
       <c r="G95" s="132">
@@ -13431,12 +13431,12 @@
     <row r="100" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B100" s="43"/>
       <c r="N100" s="26"/>
-      <c r="O100" s="247" t="s">
+      <c r="O100" s="287" t="s">
         <v>17</v>
       </c>
-      <c r="P100" s="248"/>
-      <c r="Q100" s="248"/>
-      <c r="R100" s="249"/>
+      <c r="P100" s="288"/>
+      <c r="Q100" s="288"/>
+      <c r="R100" s="289"/>
       <c r="AG100" s="30"/>
       <c r="AH100" s="30"/>
       <c r="AI100" s="30"/>
@@ -13445,21 +13445,21 @@
     </row>
     <row r="101" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="33"/>
-      <c r="B101" s="276" t="s">
+      <c r="B101" s="275" t="s">
         <v>16</v>
       </c>
-      <c r="C101" s="277"/>
-      <c r="D101" s="277"/>
-      <c r="E101" s="277"/>
-      <c r="F101" s="277"/>
-      <c r="G101" s="277"/>
-      <c r="H101" s="277"/>
-      <c r="I101" s="277"/>
-      <c r="J101" s="277"/>
-      <c r="K101" s="277"/>
-      <c r="L101" s="277"/>
-      <c r="M101" s="277"/>
-      <c r="N101" s="278"/>
+      <c r="C101" s="276"/>
+      <c r="D101" s="276"/>
+      <c r="E101" s="276"/>
+      <c r="F101" s="276"/>
+      <c r="G101" s="276"/>
+      <c r="H101" s="276"/>
+      <c r="I101" s="276"/>
+      <c r="J101" s="276"/>
+      <c r="K101" s="276"/>
+      <c r="L101" s="276"/>
+      <c r="M101" s="276"/>
+      <c r="N101" s="277"/>
       <c r="O101" s="21">
         <v>1</v>
       </c>
@@ -13472,45 +13472,45 @@
       <c r="R101" s="22">
         <v>4</v>
       </c>
-      <c r="U101" s="250" t="s">
+      <c r="U101" s="290" t="s">
         <v>26</v>
       </c>
-      <c r="V101" s="251"/>
-      <c r="W101" s="251"/>
-      <c r="X101" s="251"/>
-      <c r="Y101" s="251"/>
-      <c r="Z101" s="251"/>
-      <c r="AA101" s="251"/>
-      <c r="AB101" s="251"/>
-      <c r="AC101" s="251"/>
-      <c r="AD101" s="252"/>
+      <c r="V101" s="291"/>
+      <c r="W101" s="291"/>
+      <c r="X101" s="291"/>
+      <c r="Y101" s="291"/>
+      <c r="Z101" s="291"/>
+      <c r="AA101" s="291"/>
+      <c r="AB101" s="291"/>
+      <c r="AC101" s="291"/>
+      <c r="AD101" s="292"/>
       <c r="AE101" s="28"/>
       <c r="AF101" s="28"/>
-      <c r="AG101" s="253" t="s">
+      <c r="AG101" s="293" t="s">
         <v>24</v>
       </c>
-      <c r="AH101" s="254"/>
-      <c r="AI101" s="254"/>
-      <c r="AJ101" s="254"/>
-      <c r="AK101" s="255"/>
+      <c r="AH101" s="294"/>
+      <c r="AI101" s="294"/>
+      <c r="AJ101" s="294"/>
+      <c r="AK101" s="295"/>
     </row>
     <row r="102" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A102" s="34"/>
-      <c r="B102" s="283" t="s">
+      <c r="B102" s="254" t="s">
         <v>6</v>
       </c>
-      <c r="C102" s="284"/>
-      <c r="D102" s="284"/>
-      <c r="E102" s="284"/>
-      <c r="F102" s="284"/>
-      <c r="G102" s="284"/>
-      <c r="H102" s="284"/>
-      <c r="I102" s="284"/>
-      <c r="J102" s="284"/>
-      <c r="K102" s="284"/>
-      <c r="L102" s="284"/>
-      <c r="M102" s="284"/>
-      <c r="N102" s="285"/>
+      <c r="C102" s="255"/>
+      <c r="D102" s="255"/>
+      <c r="E102" s="255"/>
+      <c r="F102" s="255"/>
+      <c r="G102" s="255"/>
+      <c r="H102" s="255"/>
+      <c r="I102" s="255"/>
+      <c r="J102" s="255"/>
+      <c r="K102" s="255"/>
+      <c r="L102" s="255"/>
+      <c r="M102" s="255"/>
+      <c r="N102" s="256"/>
       <c r="O102" s="20">
         <v>5</v>
       </c>
@@ -13523,49 +13523,49 @@
       <c r="R102" s="23">
         <v>20</v>
       </c>
-      <c r="U102" s="281" t="s">
+      <c r="U102" s="280" t="s">
         <v>20</v>
       </c>
-      <c r="V102" s="282"/>
-      <c r="W102" s="282"/>
-      <c r="X102" s="282"/>
-      <c r="Y102" s="282"/>
-      <c r="Z102" s="282"/>
-      <c r="AA102" s="282"/>
-      <c r="AB102" s="279">
+      <c r="V102" s="281"/>
+      <c r="W102" s="281"/>
+      <c r="X102" s="281"/>
+      <c r="Y102" s="281"/>
+      <c r="Z102" s="281"/>
+      <c r="AA102" s="281"/>
+      <c r="AB102" s="278">
         <v>22</v>
       </c>
-      <c r="AC102" s="279"/>
-      <c r="AD102" s="280"/>
+      <c r="AC102" s="278"/>
+      <c r="AD102" s="279"/>
       <c r="AE102" s="29"/>
       <c r="AF102" s="29"/>
-      <c r="AG102" s="295" t="s">
+      <c r="AG102" s="261" t="s">
         <v>21</v>
       </c>
-      <c r="AH102" s="296"/>
-      <c r="AI102" s="296"/>
-      <c r="AJ102" s="297"/>
+      <c r="AH102" s="262"/>
+      <c r="AI102" s="262"/>
+      <c r="AJ102" s="263"/>
       <c r="AK102" s="223">
         <v>230</v>
       </c>
     </row>
     <row r="103" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="34"/>
-      <c r="B103" s="283" t="s">
+      <c r="B103" s="254" t="s">
         <v>5</v>
       </c>
-      <c r="C103" s="284"/>
-      <c r="D103" s="284"/>
-      <c r="E103" s="284"/>
-      <c r="F103" s="284"/>
-      <c r="G103" s="284"/>
-      <c r="H103" s="284"/>
-      <c r="I103" s="284"/>
-      <c r="J103" s="284"/>
-      <c r="K103" s="284"/>
-      <c r="L103" s="284"/>
-      <c r="M103" s="284"/>
-      <c r="N103" s="285"/>
+      <c r="C103" s="255"/>
+      <c r="D103" s="255"/>
+      <c r="E103" s="255"/>
+      <c r="F103" s="255"/>
+      <c r="G103" s="255"/>
+      <c r="H103" s="255"/>
+      <c r="I103" s="255"/>
+      <c r="J103" s="255"/>
+      <c r="K103" s="255"/>
+      <c r="L103" s="255"/>
+      <c r="M103" s="255"/>
+      <c r="N103" s="256"/>
       <c r="O103" s="20">
         <v>2</v>
       </c>
@@ -13578,49 +13578,49 @@
       <c r="R103" s="23">
         <v>8</v>
       </c>
-      <c r="U103" s="290" t="s">
+      <c r="U103" s="259" t="s">
         <v>18</v>
       </c>
-      <c r="V103" s="291"/>
-      <c r="W103" s="291"/>
-      <c r="X103" s="291"/>
-      <c r="Y103" s="291"/>
-      <c r="Z103" s="291"/>
-      <c r="AA103" s="291"/>
-      <c r="AB103" s="292">
+      <c r="V103" s="260"/>
+      <c r="W103" s="260"/>
+      <c r="X103" s="260"/>
+      <c r="Y103" s="260"/>
+      <c r="Z103" s="260"/>
+      <c r="AA103" s="260"/>
+      <c r="AB103" s="285">
         <v>20</v>
       </c>
-      <c r="AC103" s="292"/>
-      <c r="AD103" s="293"/>
+      <c r="AC103" s="285"/>
+      <c r="AD103" s="286"/>
       <c r="AE103" s="29"/>
       <c r="AF103" s="29"/>
-      <c r="AG103" s="298" t="s">
+      <c r="AG103" s="264" t="s">
         <v>22</v>
       </c>
-      <c r="AH103" s="284"/>
-      <c r="AI103" s="284"/>
-      <c r="AJ103" s="285"/>
+      <c r="AH103" s="255"/>
+      <c r="AI103" s="255"/>
+      <c r="AJ103" s="256"/>
       <c r="AK103" s="36">
         <v>115</v>
       </c>
     </row>
     <row r="104" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="35"/>
-      <c r="B104" s="269" t="s">
+      <c r="B104" s="268" t="s">
         <v>4</v>
       </c>
-      <c r="C104" s="270"/>
-      <c r="D104" s="270"/>
-      <c r="E104" s="270"/>
-      <c r="F104" s="270"/>
-      <c r="G104" s="270"/>
-      <c r="H104" s="270"/>
-      <c r="I104" s="270"/>
-      <c r="J104" s="270"/>
-      <c r="K104" s="270"/>
-      <c r="L104" s="270"/>
-      <c r="M104" s="270"/>
-      <c r="N104" s="271"/>
+      <c r="C104" s="269"/>
+      <c r="D104" s="269"/>
+      <c r="E104" s="269"/>
+      <c r="F104" s="269"/>
+      <c r="G104" s="269"/>
+      <c r="H104" s="269"/>
+      <c r="I104" s="269"/>
+      <c r="J104" s="269"/>
+      <c r="K104" s="269"/>
+      <c r="L104" s="269"/>
+      <c r="M104" s="269"/>
+      <c r="N104" s="270"/>
       <c r="O104" s="3">
         <v>1</v>
       </c>
@@ -13633,51 +13633,51 @@
       <c r="R104" s="24">
         <v>1</v>
       </c>
-      <c r="U104" s="286" t="s">
+      <c r="U104" s="282" t="s">
         <v>19</v>
       </c>
-      <c r="V104" s="287"/>
-      <c r="W104" s="287"/>
-      <c r="X104" s="287"/>
-      <c r="Y104" s="287"/>
-      <c r="Z104" s="287"/>
-      <c r="AA104" s="287"/>
-      <c r="AB104" s="288">
+      <c r="V104" s="258"/>
+      <c r="W104" s="258"/>
+      <c r="X104" s="258"/>
+      <c r="Y104" s="258"/>
+      <c r="Z104" s="258"/>
+      <c r="AA104" s="258"/>
+      <c r="AB104" s="283">
         <f>AB102*AB103</f>
         <v>440</v>
       </c>
-      <c r="AC104" s="288"/>
-      <c r="AD104" s="289"/>
+      <c r="AC104" s="283"/>
+      <c r="AD104" s="284"/>
       <c r="AE104" s="29"/>
       <c r="AF104" s="29"/>
-      <c r="AG104" s="298" t="s">
+      <c r="AG104" s="264" t="s">
         <v>25</v>
       </c>
-      <c r="AH104" s="284"/>
-      <c r="AI104" s="284"/>
-      <c r="AJ104" s="285"/>
+      <c r="AH104" s="255"/>
+      <c r="AI104" s="255"/>
+      <c r="AJ104" s="256"/>
       <c r="AK104" s="36">
         <v>65</v>
       </c>
     </row>
     <row r="105" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG105" s="290" t="s">
+      <c r="AG105" s="259" t="s">
         <v>23</v>
       </c>
-      <c r="AH105" s="291"/>
-      <c r="AI105" s="291"/>
-      <c r="AJ105" s="291"/>
+      <c r="AH105" s="260"/>
+      <c r="AI105" s="260"/>
+      <c r="AJ105" s="260"/>
       <c r="AK105" s="225">
         <v>30</v>
       </c>
     </row>
     <row r="106" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG106" s="294" t="s">
+      <c r="AG106" s="257" t="s">
         <v>19</v>
       </c>
-      <c r="AH106" s="287"/>
-      <c r="AI106" s="287"/>
-      <c r="AJ106" s="287"/>
+      <c r="AH106" s="258"/>
+      <c r="AI106" s="258"/>
+      <c r="AJ106" s="258"/>
       <c r="AK106" s="224">
         <f>SUM(AK102:AK105)</f>
         <v>440</v>
@@ -13689,12 +13689,22 @@
     <sortCondition ref="B10:B94"/>
   </sortState>
   <mergeCells count="38">
-    <mergeCell ref="B103:N103"/>
-    <mergeCell ref="AG106:AJ106"/>
-    <mergeCell ref="AG105:AJ105"/>
-    <mergeCell ref="AG102:AJ102"/>
-    <mergeCell ref="AG104:AJ104"/>
-    <mergeCell ref="AG103:AJ103"/>
+    <mergeCell ref="O100:R100"/>
+    <mergeCell ref="U101:AD101"/>
+    <mergeCell ref="AG101:AK101"/>
+    <mergeCell ref="AH4:AJ4"/>
+    <mergeCell ref="AG5:AG9"/>
+    <mergeCell ref="AJ5:AJ9"/>
+    <mergeCell ref="X5:AA5"/>
+    <mergeCell ref="AB5:AB9"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="C4:S4"/>
+    <mergeCell ref="T4:AB4"/>
+    <mergeCell ref="AC4:AG4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="K5:R5"/>
+    <mergeCell ref="S5:S9"/>
     <mergeCell ref="T5:W5"/>
     <mergeCell ref="B104:N104"/>
     <mergeCell ref="C1:O1"/>
@@ -13711,22 +13721,12 @@
     <mergeCell ref="AB104:AD104"/>
     <mergeCell ref="U103:AA103"/>
     <mergeCell ref="AB103:AD103"/>
-    <mergeCell ref="O100:R100"/>
-    <mergeCell ref="U101:AD101"/>
-    <mergeCell ref="AG101:AK101"/>
-    <mergeCell ref="AH4:AJ4"/>
-    <mergeCell ref="AG5:AG9"/>
-    <mergeCell ref="AJ5:AJ9"/>
-    <mergeCell ref="X5:AA5"/>
-    <mergeCell ref="AB5:AB9"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="C4:S4"/>
-    <mergeCell ref="T4:AB4"/>
-    <mergeCell ref="AC4:AG4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="K5:R5"/>
-    <mergeCell ref="S5:S9"/>
+    <mergeCell ref="B103:N103"/>
+    <mergeCell ref="AG106:AJ106"/>
+    <mergeCell ref="AG105:AJ105"/>
+    <mergeCell ref="AG102:AJ102"/>
+    <mergeCell ref="AG104:AJ104"/>
+    <mergeCell ref="AG103:AJ103"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <conditionalFormatting sqref="AH18:AI18 AH10:AI10 AH14:AI14 T10:AA10 AC10:AF10 C10:R10 C14:R14 T14:AA14 AC14:AF14 T18:AA18 AC18:AF18 AH30:AI30 C30:R30 T30:AA30 AC30:AF30 AH26:AI26 C26:R26 T26:AA26 AC26:AF26 AH62:AI62 C62:R62 T62:AA62 AC62:AF62 AH42:AI42 C42:R42 T42:AA42 AC42:AF42 AH22:AI22 C22:R22 T22:AA22 AC22:AF22 AH38:AI38 C38:R38 T38:AA38 AC38:AF38 AH34:AI34 C34:R34 T34:AA34 AC34:AF34 AH66:AI66 C66:R66 T66:AA66 AC66:AF66 C18:R18">
@@ -14383,7 +14383,7 @@
   <dimension ref="A1:AJ31"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14575,13 +14575,15 @@
       <c r="E6" s="85">
         <v>2</v>
       </c>
-      <c r="F6" s="85"/>
+      <c r="F6" s="85">
+        <v>6</v>
+      </c>
       <c r="G6" s="85"/>
       <c r="H6" s="85"/>
       <c r="I6" s="85"/>
       <c r="J6" s="77">
         <f>IF(C6&gt;C7,1,0)+IF(D6&gt;D7,1,0)+IF(E6&gt;E7,1,0)+IF(F6&gt;F7,1,0)+IF(G6&gt;G7,1,0)+IF(H6&gt;H7,1,0)+IF(I6&gt;I7,1,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K6" s="16"/>
       <c r="L6" s="13"/>
@@ -14629,7 +14631,9 @@
       <c r="E7" s="85">
         <v>3</v>
       </c>
-      <c r="F7" s="85"/>
+      <c r="F7" s="85">
+        <v>4</v>
+      </c>
       <c r="G7" s="85"/>
       <c r="H7" s="85"/>
       <c r="I7" s="85"/>
@@ -15096,7 +15100,9 @@
       <c r="E17" s="85">
         <v>2</v>
       </c>
-      <c r="F17" s="86"/>
+      <c r="F17" s="86">
+        <v>2</v>
+      </c>
       <c r="G17" s="85"/>
       <c r="H17" s="85"/>
       <c r="I17" s="85"/>
@@ -15144,13 +15150,15 @@
       <c r="E18" s="85">
         <v>6</v>
       </c>
-      <c r="F18" s="86"/>
+      <c r="F18" s="86">
+        <v>3</v>
+      </c>
       <c r="G18" s="85"/>
       <c r="H18" s="85"/>
       <c r="I18" s="85"/>
       <c r="J18" s="77">
         <f>IF(C18&gt;C17,1,0)+IF(D18&gt;D17,1,0)+IF(E18&gt;E17,1,0)+IF(F18&gt;F17,1,0)+IF(G18&gt;G17,1,0)+IF(H18&gt;H17,1,0)+IF(I18&gt;I17,1,0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K18" s="14"/>
       <c r="L18" s="4"/>
@@ -15427,7 +15435,9 @@
       <c r="E24" s="85">
         <v>3</v>
       </c>
-      <c r="F24" s="85"/>
+      <c r="F24" s="85">
+        <v>1</v>
+      </c>
       <c r="G24" s="85"/>
       <c r="H24" s="85"/>
       <c r="I24" s="86"/>
@@ -15482,13 +15492,15 @@
       <c r="E25" s="85">
         <v>2</v>
       </c>
-      <c r="F25" s="85"/>
+      <c r="F25" s="85">
+        <v>5</v>
+      </c>
       <c r="G25" s="85"/>
       <c r="H25" s="85"/>
       <c r="I25" s="86"/>
       <c r="J25" s="77">
         <f>IF(C25&gt;C24,1,0)+IF(D25&gt;D24,1,0)+IF(E25&gt;E24,1,0)+IF(F25&gt;F24,1,0)+IF(G25&gt;G24,1,0)+IF(H25&gt;H24,1,0)+IF(I25&gt;I24,1,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K25" s="14"/>
       <c r="L25" s="4"/>

</xml_diff>

<commit_message>
Updated games of 2014-03-18
</commit_message>
<xml_diff>
--- a/laval.xlsx
+++ b/laval.xlsx
@@ -1960,7 +1960,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="313">
+  <cellXfs count="314">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2453,9 +2453,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2492,12 +2489,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2507,6 +2498,135 @@
     <xf numFmtId="0" fontId="19" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="113" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="114" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="95" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2516,18 +2636,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="86" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="87" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="88" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="87" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="95" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2540,148 +2675,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="86" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="88" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="113" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="114" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="95" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2693,6 +2696,146 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="101">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="1"/>
@@ -3431,146 +3574,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -3882,7 +3885,7 @@
   <dimension ref="A1:AL106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="AM99" sqref="AM99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3905,217 +3908,217 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="C1" s="271"/>
-      <c r="D1" s="271"/>
-      <c r="E1" s="271"/>
-      <c r="F1" s="271"/>
-      <c r="G1" s="271"/>
-      <c r="H1" s="271"/>
-      <c r="I1" s="271"/>
-      <c r="J1" s="271"/>
-      <c r="K1" s="271"/>
-      <c r="L1" s="271"/>
-      <c r="M1" s="271"/>
-      <c r="N1" s="271"/>
-      <c r="O1" s="271"/>
-      <c r="P1" s="272"/>
-      <c r="Q1" s="272"/>
-      <c r="R1" s="272"/>
-      <c r="S1" s="272"/>
-      <c r="T1" s="272"/>
-      <c r="U1" s="272"/>
-      <c r="V1" s="272"/>
-      <c r="W1" s="272"/>
-      <c r="X1" s="272"/>
-      <c r="Y1" s="272"/>
-      <c r="Z1" s="272"/>
-      <c r="AA1" s="272"/>
-      <c r="AB1" s="272"/>
-      <c r="AC1" s="272"/>
-      <c r="AD1" s="272"/>
-      <c r="AE1" s="272"/>
-      <c r="AF1" s="272"/>
-      <c r="AG1" s="272"/>
-      <c r="AH1" s="272"/>
-      <c r="AI1" s="272"/>
-      <c r="AJ1" s="272"/>
+      <c r="C1" s="283"/>
+      <c r="D1" s="283"/>
+      <c r="E1" s="283"/>
+      <c r="F1" s="283"/>
+      <c r="G1" s="283"/>
+      <c r="H1" s="283"/>
+      <c r="I1" s="283"/>
+      <c r="J1" s="283"/>
+      <c r="K1" s="283"/>
+      <c r="L1" s="283"/>
+      <c r="M1" s="283"/>
+      <c r="N1" s="283"/>
+      <c r="O1" s="283"/>
+      <c r="P1" s="284"/>
+      <c r="Q1" s="284"/>
+      <c r="R1" s="284"/>
+      <c r="S1" s="284"/>
+      <c r="T1" s="284"/>
+      <c r="U1" s="284"/>
+      <c r="V1" s="284"/>
+      <c r="W1" s="284"/>
+      <c r="X1" s="284"/>
+      <c r="Y1" s="284"/>
+      <c r="Z1" s="284"/>
+      <c r="AA1" s="284"/>
+      <c r="AB1" s="284"/>
+      <c r="AC1" s="284"/>
+      <c r="AD1" s="284"/>
+      <c r="AE1" s="284"/>
+      <c r="AF1" s="284"/>
+      <c r="AG1" s="284"/>
+      <c r="AH1" s="284"/>
+      <c r="AI1" s="284"/>
+      <c r="AJ1" s="284"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="41"/>
-      <c r="C2" s="273" t="s">
+      <c r="C2" s="285" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="273"/>
-      <c r="E2" s="273"/>
-      <c r="F2" s="273"/>
-      <c r="G2" s="273"/>
-      <c r="H2" s="273"/>
-      <c r="I2" s="273"/>
-      <c r="J2" s="273"/>
-      <c r="K2" s="273"/>
-      <c r="L2" s="273"/>
-      <c r="M2" s="273"/>
-      <c r="N2" s="273"/>
-      <c r="O2" s="273"/>
-      <c r="P2" s="273"/>
-      <c r="Q2" s="274" t="s">
+      <c r="D2" s="285"/>
+      <c r="E2" s="285"/>
+      <c r="F2" s="285"/>
+      <c r="G2" s="285"/>
+      <c r="H2" s="285"/>
+      <c r="I2" s="285"/>
+      <c r="J2" s="285"/>
+      <c r="K2" s="285"/>
+      <c r="L2" s="285"/>
+      <c r="M2" s="285"/>
+      <c r="N2" s="285"/>
+      <c r="O2" s="285"/>
+      <c r="P2" s="285"/>
+      <c r="Q2" s="286" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="272"/>
-      <c r="S2" s="272"/>
-      <c r="T2" s="272"/>
-      <c r="U2" s="272"/>
-      <c r="V2" s="272"/>
-      <c r="W2" s="272"/>
-      <c r="X2" s="272"/>
-      <c r="Y2" s="272"/>
-      <c r="Z2" s="272"/>
-      <c r="AA2" s="272"/>
-      <c r="AB2" s="272"/>
-      <c r="AC2" s="272"/>
-      <c r="AD2" s="272"/>
-      <c r="AE2" s="272"/>
-      <c r="AF2" s="272"/>
-      <c r="AG2" s="272"/>
-      <c r="AH2" s="272"/>
-      <c r="AI2" s="272"/>
-      <c r="AJ2" s="272"/>
+      <c r="R2" s="284"/>
+      <c r="S2" s="284"/>
+      <c r="T2" s="284"/>
+      <c r="U2" s="284"/>
+      <c r="V2" s="284"/>
+      <c r="W2" s="284"/>
+      <c r="X2" s="284"/>
+      <c r="Y2" s="284"/>
+      <c r="Z2" s="284"/>
+      <c r="AA2" s="284"/>
+      <c r="AB2" s="284"/>
+      <c r="AC2" s="284"/>
+      <c r="AD2" s="284"/>
+      <c r="AE2" s="284"/>
+      <c r="AF2" s="284"/>
+      <c r="AG2" s="284"/>
+      <c r="AH2" s="284"/>
+      <c r="AI2" s="284"/>
+      <c r="AJ2" s="284"/>
     </row>
     <row r="3" spans="1:38" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="271"/>
-      <c r="D3" s="271"/>
-      <c r="E3" s="271"/>
-      <c r="F3" s="271"/>
-      <c r="G3" s="271"/>
-      <c r="H3" s="271"/>
-      <c r="I3" s="271"/>
-      <c r="J3" s="271"/>
-      <c r="K3" s="271"/>
-      <c r="L3" s="271"/>
-      <c r="M3" s="271"/>
-      <c r="N3" s="271"/>
-      <c r="O3" s="271"/>
-      <c r="P3" s="272"/>
-      <c r="Q3" s="272"/>
-      <c r="R3" s="272"/>
-      <c r="S3" s="272"/>
-      <c r="T3" s="272"/>
-      <c r="U3" s="272"/>
-      <c r="V3" s="272"/>
-      <c r="W3" s="272"/>
-      <c r="X3" s="272"/>
-      <c r="Y3" s="272"/>
-      <c r="Z3" s="272"/>
-      <c r="AA3" s="272"/>
-      <c r="AB3" s="272"/>
-      <c r="AC3" s="272"/>
-      <c r="AD3" s="272"/>
-      <c r="AE3" s="272"/>
-      <c r="AF3" s="272"/>
-      <c r="AG3" s="272"/>
-      <c r="AH3" s="272"/>
-      <c r="AI3" s="272"/>
-      <c r="AJ3" s="272"/>
+      <c r="C3" s="283"/>
+      <c r="D3" s="283"/>
+      <c r="E3" s="283"/>
+      <c r="F3" s="283"/>
+      <c r="G3" s="283"/>
+      <c r="H3" s="283"/>
+      <c r="I3" s="283"/>
+      <c r="J3" s="283"/>
+      <c r="K3" s="283"/>
+      <c r="L3" s="283"/>
+      <c r="M3" s="283"/>
+      <c r="N3" s="283"/>
+      <c r="O3" s="283"/>
+      <c r="P3" s="284"/>
+      <c r="Q3" s="284"/>
+      <c r="R3" s="284"/>
+      <c r="S3" s="284"/>
+      <c r="T3" s="284"/>
+      <c r="U3" s="284"/>
+      <c r="V3" s="284"/>
+      <c r="W3" s="284"/>
+      <c r="X3" s="284"/>
+      <c r="Y3" s="284"/>
+      <c r="Z3" s="284"/>
+      <c r="AA3" s="284"/>
+      <c r="AB3" s="284"/>
+      <c r="AC3" s="284"/>
+      <c r="AD3" s="284"/>
+      <c r="AE3" s="284"/>
+      <c r="AF3" s="284"/>
+      <c r="AG3" s="284"/>
+      <c r="AH3" s="284"/>
+      <c r="AI3" s="284"/>
+      <c r="AJ3" s="284"/>
     </row>
     <row r="4" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="296" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="297"/>
-      <c r="E4" s="297"/>
-      <c r="F4" s="297"/>
-      <c r="G4" s="297"/>
-      <c r="H4" s="297"/>
-      <c r="I4" s="297"/>
-      <c r="J4" s="297"/>
-      <c r="K4" s="297"/>
-      <c r="L4" s="297"/>
-      <c r="M4" s="297"/>
-      <c r="N4" s="297"/>
-      <c r="O4" s="297"/>
-      <c r="P4" s="297"/>
-      <c r="Q4" s="297"/>
-      <c r="R4" s="297"/>
-      <c r="S4" s="298"/>
-      <c r="T4" s="296" t="s">
+      <c r="C4" s="267" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="268"/>
+      <c r="E4" s="268"/>
+      <c r="F4" s="268"/>
+      <c r="G4" s="268"/>
+      <c r="H4" s="268"/>
+      <c r="I4" s="268"/>
+      <c r="J4" s="268"/>
+      <c r="K4" s="268"/>
+      <c r="L4" s="268"/>
+      <c r="M4" s="268"/>
+      <c r="N4" s="268"/>
+      <c r="O4" s="268"/>
+      <c r="P4" s="268"/>
+      <c r="Q4" s="268"/>
+      <c r="R4" s="268"/>
+      <c r="S4" s="269"/>
+      <c r="T4" s="267" t="s">
         <v>1</v>
       </c>
-      <c r="U4" s="297"/>
-      <c r="V4" s="297"/>
-      <c r="W4" s="297"/>
-      <c r="X4" s="297"/>
-      <c r="Y4" s="297"/>
-      <c r="Z4" s="297"/>
-      <c r="AA4" s="297"/>
-      <c r="AB4" s="298"/>
-      <c r="AC4" s="296" t="s">
+      <c r="U4" s="268"/>
+      <c r="V4" s="268"/>
+      <c r="W4" s="268"/>
+      <c r="X4" s="268"/>
+      <c r="Y4" s="268"/>
+      <c r="Z4" s="268"/>
+      <c r="AA4" s="268"/>
+      <c r="AB4" s="269"/>
+      <c r="AC4" s="267" t="s">
         <v>2</v>
       </c>
-      <c r="AD4" s="297"/>
-      <c r="AE4" s="297"/>
-      <c r="AF4" s="297"/>
-      <c r="AG4" s="305"/>
-      <c r="AH4" s="296" t="s">
+      <c r="AD4" s="268"/>
+      <c r="AE4" s="268"/>
+      <c r="AF4" s="268"/>
+      <c r="AG4" s="278"/>
+      <c r="AH4" s="267" t="s">
         <v>10</v>
       </c>
-      <c r="AI4" s="297"/>
-      <c r="AJ4" s="298"/>
+      <c r="AI4" s="268"/>
+      <c r="AJ4" s="269"/>
     </row>
     <row r="5" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="265" t="s">
+      <c r="C5" s="279" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="266"/>
-      <c r="E5" s="266"/>
-      <c r="F5" s="266"/>
-      <c r="G5" s="266"/>
-      <c r="H5" s="266"/>
-      <c r="I5" s="266"/>
-      <c r="J5" s="267"/>
-      <c r="K5" s="303" t="s">
+      <c r="D5" s="275"/>
+      <c r="E5" s="275"/>
+      <c r="F5" s="275"/>
+      <c r="G5" s="275"/>
+      <c r="H5" s="275"/>
+      <c r="I5" s="275"/>
+      <c r="J5" s="276"/>
+      <c r="K5" s="274" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="266"/>
-      <c r="M5" s="266"/>
-      <c r="N5" s="266"/>
-      <c r="O5" s="266"/>
-      <c r="P5" s="266"/>
-      <c r="Q5" s="266"/>
-      <c r="R5" s="267"/>
-      <c r="S5" s="299" t="s">
+      <c r="L5" s="275"/>
+      <c r="M5" s="275"/>
+      <c r="N5" s="275"/>
+      <c r="O5" s="275"/>
+      <c r="P5" s="275"/>
+      <c r="Q5" s="275"/>
+      <c r="R5" s="276"/>
+      <c r="S5" s="270" t="s">
         <v>12</v>
       </c>
-      <c r="T5" s="265" t="s">
+      <c r="T5" s="279" t="s">
         <v>9</v>
       </c>
-      <c r="U5" s="266"/>
-      <c r="V5" s="266"/>
-      <c r="W5" s="267"/>
-      <c r="X5" s="303" t="s">
+      <c r="U5" s="275"/>
+      <c r="V5" s="275"/>
+      <c r="W5" s="276"/>
+      <c r="X5" s="274" t="s">
         <v>8</v>
       </c>
-      <c r="Y5" s="266"/>
-      <c r="Z5" s="266"/>
-      <c r="AA5" s="267"/>
-      <c r="AB5" s="299" t="s">
+      <c r="Y5" s="275"/>
+      <c r="Z5" s="275"/>
+      <c r="AA5" s="276"/>
+      <c r="AB5" s="270" t="s">
         <v>13</v>
       </c>
-      <c r="AC5" s="304" t="s">
+      <c r="AC5" s="277" t="s">
         <v>9</v>
       </c>
-      <c r="AD5" s="267"/>
-      <c r="AE5" s="303" t="s">
+      <c r="AD5" s="276"/>
+      <c r="AE5" s="274" t="s">
         <v>8</v>
       </c>
-      <c r="AF5" s="267"/>
-      <c r="AG5" s="299" t="s">
+      <c r="AF5" s="276"/>
+      <c r="AG5" s="270" t="s">
         <v>14</v>
       </c>
       <c r="AH5" s="56"/>
       <c r="AI5" s="25"/>
-      <c r="AJ5" s="299" t="s">
+      <c r="AJ5" s="270" t="s">
         <v>15</v>
       </c>
       <c r="AK5" s="4"/>
@@ -4127,7 +4130,7 @@
         <f>Résultats!$J$3</f>
         <v>0</v>
       </c>
-      <c r="D6" s="244">
+      <c r="D6" s="243">
         <f>Résultats!$J$4</f>
         <v>4</v>
       </c>
@@ -4145,9 +4148,9 @@
       </c>
       <c r="H6" s="109">
         <f>Résultats!$J$11</f>
-        <v>1</v>
-      </c>
-      <c r="I6" s="240">
+        <v>2</v>
+      </c>
+      <c r="I6" s="239">
         <f>Résultats!$J$13</f>
         <v>4</v>
       </c>
@@ -4169,7 +4172,7 @@
       </c>
       <c r="N6" s="109">
         <f>Résultats!$J$21</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O6" s="172">
         <f>Résultats!$J$24</f>
@@ -4181,13 +4184,13 @@
       </c>
       <c r="Q6" s="111">
         <f>Résultats!$J$27</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R6" s="108">
         <f>Résultats!$J$28</f>
         <v>3</v>
       </c>
-      <c r="S6" s="300"/>
+      <c r="S6" s="271"/>
       <c r="T6" s="169">
         <f>Résultats!$V$6</f>
         <v>0</v>
@@ -4220,7 +4223,7 @@
         <f>Résultats!$V$25</f>
         <v>0</v>
       </c>
-      <c r="AB6" s="300"/>
+      <c r="AB6" s="271"/>
       <c r="AC6" s="111">
         <f>Résultats!$AH$8</f>
         <v>0</v>
@@ -4237,7 +4240,7 @@
         <f>Résultats!$AH$23</f>
         <v>0</v>
       </c>
-      <c r="AG6" s="300"/>
+      <c r="AG6" s="271"/>
       <c r="AH6" s="212">
         <f>Résultats!$AH$15</f>
         <v>0</v>
@@ -4246,7 +4249,7 @@
         <f>Résultats!$AH$16</f>
         <v>0</v>
       </c>
-      <c r="AJ6" s="300"/>
+      <c r="AJ6" s="271"/>
       <c r="AK6" s="37"/>
     </row>
     <row r="7" spans="1:38" s="39" customFormat="1" ht="58.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -4257,12 +4260,12 @@
 +IF(ISBLANK($D10),0,($D$6*PT_VICTOIRE_R1)+IF($D$6=4,PT_PREDICTION_EQUIPE_R1+IF($D10=$C$6+$D$6,PT_PREDICTION_NB_PARTIES_R1,0),0))</f>
         <v>0</v>
       </c>
-      <c r="D7" s="245"/>
+      <c r="D7" s="244"/>
       <c r="E7" s="173"/>
       <c r="F7" s="118"/>
       <c r="G7" s="119"/>
       <c r="H7" s="117"/>
-      <c r="I7" s="241"/>
+      <c r="I7" s="240"/>
       <c r="J7" s="117"/>
       <c r="K7" s="120"/>
       <c r="L7" s="117"/>
@@ -4272,7 +4275,7 @@
       <c r="P7" s="118"/>
       <c r="Q7" s="119"/>
       <c r="R7" s="117"/>
-      <c r="S7" s="300"/>
+      <c r="S7" s="271"/>
       <c r="T7" s="170"/>
       <c r="U7" s="117"/>
       <c r="V7" s="173"/>
@@ -4281,15 +4284,15 @@
       <c r="Y7" s="118"/>
       <c r="Z7" s="119"/>
       <c r="AA7" s="117"/>
-      <c r="AB7" s="300"/>
+      <c r="AB7" s="271"/>
       <c r="AC7" s="119"/>
       <c r="AD7" s="117"/>
       <c r="AE7" s="120"/>
       <c r="AF7" s="117"/>
-      <c r="AG7" s="300"/>
+      <c r="AG7" s="271"/>
       <c r="AH7" s="212"/>
       <c r="AI7" s="112"/>
-      <c r="AJ7" s="300"/>
+      <c r="AJ7" s="271"/>
       <c r="AK7" s="37"/>
     </row>
     <row r="8" spans="1:38" s="39" customFormat="1" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4299,7 +4302,7 @@
         <f>Résultats!$B$3</f>
         <v>TAMPA BAY</v>
       </c>
-      <c r="D8" s="246" t="str">
+      <c r="D8" s="245" t="str">
         <f>Résultats!$B$4</f>
         <v>COLUMBUS</v>
       </c>
@@ -4319,7 +4322,7 @@
         <f>Résultats!$B$11</f>
         <v>CAROLINE</v>
       </c>
-      <c r="I8" s="242" t="str">
+      <c r="I8" s="241" t="str">
         <f>Résultats!$B$13</f>
         <v>NEW YORK I.</v>
       </c>
@@ -4359,7 +4362,7 @@
         <f>Résultats!$B$28</f>
         <v>VEGAS</v>
       </c>
-      <c r="S8" s="300"/>
+      <c r="S8" s="271"/>
       <c r="T8" s="171" t="str">
         <f>Résultats!$N$6</f>
         <v xml:space="preserve"> </v>
@@ -4392,7 +4395,7 @@
         <f>Résultats!$N$25</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AB8" s="300"/>
+      <c r="AB8" s="271"/>
       <c r="AC8" s="177" t="str">
         <f>Résultats!$Z$8</f>
         <v xml:space="preserve"> </v>
@@ -4409,7 +4412,7 @@
         <f>Résultats!$Z$23</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AG8" s="300"/>
+      <c r="AG8" s="271"/>
       <c r="AH8" s="213" t="str">
         <f>Résultats!$Z$15</f>
         <v xml:space="preserve"> </v>
@@ -4418,7 +4421,7 @@
         <f>Résultats!$Z$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ8" s="300"/>
+      <c r="AJ8" s="271"/>
       <c r="AK8" s="37"/>
     </row>
     <row r="9" spans="1:38" s="39" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4432,7 +4435,7 @@
         <f>Résultats!$A$3</f>
         <v>A1</v>
       </c>
-      <c r="D9" s="247" t="str">
+      <c r="D9" s="246" t="str">
         <f>Résultats!$A$4</f>
         <v>WC2</v>
       </c>
@@ -4452,7 +4455,7 @@
         <f>Résultats!$A$11</f>
         <v>WC1</v>
       </c>
-      <c r="I9" s="243" t="str">
+      <c r="I9" s="242" t="str">
         <f>Résultats!$A$13</f>
         <v>M2</v>
       </c>
@@ -4492,7 +4495,7 @@
         <f>Résultats!$A$28</f>
         <v>P3</v>
       </c>
-      <c r="S9" s="302"/>
+      <c r="S9" s="273"/>
       <c r="T9" s="179" t="str">
         <f>Résultats!$M$6</f>
         <v xml:space="preserve"> </v>
@@ -4525,7 +4528,7 @@
         <f>Résultats!$M$25</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AB9" s="301"/>
+      <c r="AB9" s="272"/>
       <c r="AC9" s="183" t="str">
         <f>Résultats!$Y$8</f>
         <v xml:space="preserve"> </v>
@@ -4542,7 +4545,7 @@
         <f>Résultats!$Y$23</f>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="AG9" s="301"/>
+      <c r="AG9" s="272"/>
       <c r="AH9" s="215" t="str">
         <f>Résultats!$Y$15</f>
         <v xml:space="preserve"> </v>
@@ -4551,7 +4554,7 @@
         <f>Résultats!$Y$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ9" s="302"/>
+      <c r="AJ9" s="273"/>
       <c r="AK9" s="114" t="s">
         <v>51</v>
       </c>
@@ -4608,7 +4611,7 @@
       <c r="V10" s="191"/>
       <c r="W10" s="189"/>
       <c r="X10" s="190"/>
-      <c r="Y10" s="238"/>
+      <c r="Y10" s="237"/>
       <c r="Z10" s="192"/>
       <c r="AA10" s="193"/>
       <c r="AB10" s="194">
@@ -5012,7 +5015,7 @@
         <v>0</v>
       </c>
       <c r="AC14" s="48"/>
-      <c r="AD14" s="248"/>
+      <c r="AD14" s="247"/>
       <c r="AE14" s="49"/>
       <c r="AF14" s="47"/>
       <c r="AG14" s="129">
@@ -5357,46 +5360,46 @@
     <row r="18" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="186">
         <f>RANK(AL18,$AL$10:$AL$97,)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B18" s="211" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C18" s="198">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18" s="199"/>
       <c r="E18" s="200">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F18" s="199"/>
       <c r="G18" s="201">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H18" s="202"/>
       <c r="I18" s="200">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J18" s="202"/>
       <c r="K18" s="203">
         <v>5</v>
       </c>
       <c r="L18" s="202"/>
-      <c r="M18" s="200">
+      <c r="M18" s="200"/>
+      <c r="N18" s="199">
+        <v>7</v>
+      </c>
+      <c r="O18" s="200">
         <v>6</v>
-      </c>
-      <c r="N18" s="199"/>
-      <c r="O18" s="200">
-        <v>5</v>
       </c>
       <c r="P18" s="199"/>
       <c r="Q18" s="201">
         <v>7</v>
       </c>
       <c r="R18" s="204"/>
-      <c r="S18" s="250">
+      <c r="S18" s="312">
         <f>SUM(C19:R19)</f>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="T18" s="198"/>
       <c r="U18" s="202"/>
@@ -5404,7 +5407,7 @@
       <c r="W18" s="202"/>
       <c r="X18" s="203"/>
       <c r="Y18" s="199"/>
-      <c r="Z18" s="208"/>
+      <c r="Z18" s="201"/>
       <c r="AA18" s="204"/>
       <c r="AB18" s="205">
         <f>SUM(T19:AA19)</f>
@@ -5426,11 +5429,11 @@
       </c>
       <c r="AK18" s="207">
         <f>MAX($AL$10:$AL$97) - AL18</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AL18" s="205">
         <f>$S18+$AB18+$AG18+$AJ18</f>
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5466,7 +5469,7 @@
       <c r="L19" s="150"/>
       <c r="M19" s="126">
         <f>(IF($M18&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M18=$M$6+$N$6,$O$103,0),0),0)+IF($N18&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N18=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N19" s="150"/>
       <c r="O19" s="126">
@@ -5476,7 +5479,7 @@
       <c r="P19" s="150"/>
       <c r="Q19" s="126">
         <f>(IF($Q18&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q18=$Q$6+$R$6,$O$103,0),0),0)+IF($R18&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R18=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R19" s="153"/>
       <c r="S19" s="154"/>
@@ -5756,46 +5759,46 @@
     <row r="22" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="122">
         <f>RANK(AL22,$AL$10:$AL$97,)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B22" s="88" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C22" s="46">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D22" s="45"/>
       <c r="E22" s="44">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F22" s="45"/>
       <c r="G22" s="48">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H22" s="47"/>
       <c r="I22" s="44">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J22" s="47"/>
       <c r="K22" s="49">
         <v>5</v>
       </c>
       <c r="L22" s="47"/>
-      <c r="M22" s="44"/>
-      <c r="N22" s="45">
-        <v>7</v>
-      </c>
+      <c r="M22" s="44">
+        <v>6</v>
+      </c>
+      <c r="N22" s="45"/>
       <c r="O22" s="44">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P22" s="45"/>
       <c r="Q22" s="48">
         <v>7</v>
       </c>
       <c r="R22" s="50"/>
-      <c r="S22" s="116">
+      <c r="S22" s="129">
         <f>SUM(C23:R23)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="T22" s="46"/>
       <c r="U22" s="47"/>
@@ -5803,7 +5806,7 @@
       <c r="W22" s="47"/>
       <c r="X22" s="49"/>
       <c r="Y22" s="45"/>
-      <c r="Z22" s="48"/>
+      <c r="Z22" s="310"/>
       <c r="AA22" s="50"/>
       <c r="AB22" s="129">
         <f>SUM(T23:AA23)</f>
@@ -5825,11 +5828,11 @@
       </c>
       <c r="AK22" s="116">
         <f>MAX($AL$10:$AL$97) - AL22</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AL22" s="129">
         <f>$S22+$AB22+$AG22+$AJ22</f>
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5875,7 +5878,7 @@
       <c r="P23" s="163"/>
       <c r="Q23" s="132">
         <f>(IF($Q22&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q22=$Q$6+$R$6,$O$103,0),0),0)+IF($R22&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R22=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R23" s="166"/>
       <c r="S23" s="154"/>
@@ -6194,7 +6197,7 @@
       </c>
       <c r="S26" s="205">
         <f>SUM(C27:R27)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="T26" s="198"/>
       <c r="U26" s="202"/>
@@ -6224,11 +6227,11 @@
       </c>
       <c r="AK26" s="207">
         <f>MAX($AL$10:$AL$97) - AL26</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AL26" s="205">
         <f>$S26+$AB26+$AG26+$AJ26</f>
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6264,7 +6267,7 @@
       <c r="L27" s="150"/>
       <c r="M27" s="126">
         <f>(IF($M26&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M26=$M$6+$N$6,$O$103,0),0),0)+IF($N26&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N26=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N27" s="150"/>
       <c r="O27" s="126">
@@ -6557,34 +6560,34 @@
         <v>6</v>
       </c>
       <c r="B30" s="88" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="C30" s="46">
         <v>5</v>
       </c>
       <c r="D30" s="45"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="45">
-        <v>7</v>
-      </c>
+      <c r="E30" s="44">
+        <v>5</v>
+      </c>
+      <c r="F30" s="45"/>
       <c r="G30" s="48">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H30" s="47"/>
       <c r="I30" s="44"/>
       <c r="J30" s="47">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K30" s="49">
+        <v>5</v>
+      </c>
+      <c r="L30" s="47"/>
+      <c r="M30" s="44"/>
+      <c r="N30" s="45">
         <v>6</v>
       </c>
-      <c r="L30" s="47"/>
-      <c r="M30" s="44">
-        <v>6</v>
-      </c>
-      <c r="N30" s="45"/>
       <c r="O30" s="44">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P30" s="45"/>
       <c r="Q30" s="48"/>
@@ -6593,14 +6596,14 @@
       </c>
       <c r="S30" s="129">
         <f>SUM(C31:R31)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="T30" s="46"/>
       <c r="U30" s="47"/>
       <c r="V30" s="44"/>
       <c r="W30" s="47"/>
       <c r="X30" s="49"/>
-      <c r="Y30" s="127"/>
+      <c r="Y30" s="45"/>
       <c r="Z30" s="48"/>
       <c r="AA30" s="47"/>
       <c r="AB30" s="129">
@@ -6615,7 +6618,7 @@
         <f>SUM(AC31:AF31)</f>
         <v>0</v>
       </c>
-      <c r="AH30" s="107"/>
+      <c r="AH30" s="311"/>
       <c r="AI30" s="57"/>
       <c r="AJ30" s="129">
         <f>AH31</f>
@@ -6623,11 +6626,11 @@
       </c>
       <c r="AK30" s="116">
         <f>MAX($AL$10:$AL$97) - AL30</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AL30" s="129">
         <f>$S30+$AB30+$AG30+$AJ30</f>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6663,7 +6666,7 @@
       <c r="L31" s="80"/>
       <c r="M31" s="81">
         <f>(IF($M30&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M30=$M$6+$N$6,$O$103,0),0),0)+IF($N30&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N30=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N31" s="80"/>
       <c r="O31" s="81">
@@ -6956,34 +6959,34 @@
         <v>6</v>
       </c>
       <c r="B34" s="211" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C34" s="198">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D34" s="199"/>
       <c r="E34" s="200">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F34" s="199"/>
-      <c r="G34" s="201">
-        <v>6</v>
-      </c>
-      <c r="H34" s="202"/>
+      <c r="G34" s="201"/>
+      <c r="H34" s="202">
+        <v>7</v>
+      </c>
       <c r="I34" s="200"/>
       <c r="J34" s="202">
         <v>6</v>
       </c>
       <c r="K34" s="203">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L34" s="202"/>
-      <c r="M34" s="200">
+      <c r="M34" s="200"/>
+      <c r="N34" s="199">
+        <v>7</v>
+      </c>
+      <c r="O34" s="200">
         <v>5</v>
-      </c>
-      <c r="N34" s="199"/>
-      <c r="O34" s="200">
-        <v>6</v>
       </c>
       <c r="P34" s="199"/>
       <c r="Q34" s="201"/>
@@ -6992,7 +6995,7 @@
       </c>
       <c r="S34" s="205">
         <f>SUM(C35:R35)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="T34" s="198"/>
       <c r="U34" s="202"/>
@@ -7007,7 +7010,7 @@
         <v>0</v>
       </c>
       <c r="AC34" s="201"/>
-      <c r="AD34" s="234"/>
+      <c r="AD34" s="202"/>
       <c r="AE34" s="203"/>
       <c r="AF34" s="202"/>
       <c r="AG34" s="205">
@@ -7022,11 +7025,11 @@
       </c>
       <c r="AK34" s="207">
         <f>MAX($AL$10:$AL$97) - AL34</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AL34" s="205">
         <f>$S34+$AB34+$AG34+$AJ34</f>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7062,7 +7065,7 @@
       <c r="L35" s="80"/>
       <c r="M35" s="81">
         <f>(IF($M34&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M34=$M$6+$N$6,$O$103,0),0),0)+IF($N34&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N34=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N35" s="80"/>
       <c r="O35" s="81">
@@ -7355,34 +7358,34 @@
         <v>6</v>
       </c>
       <c r="B38" s="88" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C38" s="46">
+        <v>5</v>
+      </c>
+      <c r="D38" s="45"/>
+      <c r="E38" s="44">
         <v>6</v>
       </c>
-      <c r="D38" s="45"/>
-      <c r="E38" s="44"/>
-      <c r="F38" s="45">
-        <v>7</v>
-      </c>
+      <c r="F38" s="45"/>
       <c r="G38" s="48">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H38" s="47"/>
       <c r="I38" s="44"/>
       <c r="J38" s="47">
+        <v>7</v>
+      </c>
+      <c r="K38" s="49">
+        <v>5</v>
+      </c>
+      <c r="L38" s="47"/>
+      <c r="M38" s="44"/>
+      <c r="N38" s="45">
         <v>6</v>
       </c>
-      <c r="K38" s="49">
-        <v>6</v>
-      </c>
-      <c r="L38" s="47"/>
-      <c r="M38" s="44">
+      <c r="O38" s="44">
         <v>7</v>
-      </c>
-      <c r="N38" s="45"/>
-      <c r="O38" s="44">
-        <v>5</v>
       </c>
       <c r="P38" s="45"/>
       <c r="Q38" s="48"/>
@@ -7391,7 +7394,7 @@
       </c>
       <c r="S38" s="129">
         <f>SUM(C39:R39)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="T38" s="46"/>
       <c r="U38" s="47"/>
@@ -7421,11 +7424,11 @@
       </c>
       <c r="AK38" s="116">
         <f>MAX($AL$10:$AL$97) - AL38</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AL38" s="129">
         <f>$S38+$AB38+$AG38+$AJ38</f>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7461,7 +7464,7 @@
       <c r="L39" s="80"/>
       <c r="M39" s="81">
         <f>(IF($M38&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M38=$M$6+$N$6,$O$103,0),0),0)+IF($N38&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N38=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N39" s="80"/>
       <c r="O39" s="81">
@@ -7751,43 +7754,43 @@
     <row r="42" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="186">
         <f>RANK(AL42,$AL$10:$AL$97,)</f>
+        <v>9</v>
+      </c>
+      <c r="B42" s="211" t="s">
+        <v>77</v>
+      </c>
+      <c r="C42" s="198">
+        <v>5</v>
+      </c>
+      <c r="D42" s="199"/>
+      <c r="E42" s="200">
         <v>6</v>
       </c>
-      <c r="B42" s="211" t="s">
-        <v>68</v>
-      </c>
-      <c r="C42" s="306">
+      <c r="F42" s="199"/>
+      <c r="G42" s="201"/>
+      <c r="H42" s="202">
+        <v>7</v>
+      </c>
+      <c r="I42" s="200"/>
+      <c r="J42" s="202">
+        <v>6</v>
+      </c>
+      <c r="K42" s="203">
         <v>5</v>
       </c>
-      <c r="D42" s="307"/>
-      <c r="E42" s="308">
+      <c r="L42" s="202"/>
+      <c r="M42" s="200"/>
+      <c r="N42" s="199">
         <v>6</v>
       </c>
-      <c r="F42" s="307"/>
-      <c r="G42" s="309">
-        <v>5</v>
-      </c>
-      <c r="H42" s="310"/>
-      <c r="I42" s="308"/>
-      <c r="J42" s="310">
+      <c r="O42" s="200">
         <v>6</v>
       </c>
-      <c r="K42" s="311">
+      <c r="P42" s="199"/>
+      <c r="Q42" s="201">
         <v>6</v>
       </c>
-      <c r="L42" s="310"/>
-      <c r="M42" s="308">
-        <v>7</v>
-      </c>
-      <c r="N42" s="307"/>
-      <c r="O42" s="308">
-        <v>6</v>
-      </c>
-      <c r="P42" s="307"/>
-      <c r="Q42" s="309"/>
-      <c r="R42" s="312">
-        <v>6</v>
-      </c>
+      <c r="R42" s="204"/>
       <c r="S42" s="205">
         <f>SUM(C43:R43)</f>
         <v>12</v>
@@ -7860,7 +7863,7 @@
       <c r="L43" s="80"/>
       <c r="M43" s="81">
         <f>(IF($M42&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M42=$M$6+$N$6,$O$103,0),0),0)+IF($N42&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N42=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N43" s="80"/>
       <c r="O43" s="81">
@@ -7870,7 +7873,7 @@
       <c r="P43" s="80"/>
       <c r="Q43" s="81">
         <f>(IF($Q42&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q42=$Q$6+$R$6,$O$103,0),0),0)+IF($R42&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R42=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R43" s="84"/>
       <c r="S43" s="128"/>
@@ -8150,10 +8153,10 @@
     <row r="46" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="122">
         <f>RANK(AL46,$AL$10:$AL$97,)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B46" s="88" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C46" s="46">
         <v>5</v>
@@ -8164,7 +8167,7 @@
         <v>7</v>
       </c>
       <c r="G46" s="48">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H46" s="47"/>
       <c r="I46" s="44"/>
@@ -8172,7 +8175,7 @@
         <v>7</v>
       </c>
       <c r="K46" s="49">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L46" s="47"/>
       <c r="M46" s="44">
@@ -8185,18 +8188,18 @@
       <c r="P46" s="45"/>
       <c r="Q46" s="48"/>
       <c r="R46" s="50">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S46" s="129">
         <f>SUM(C47:R47)</f>
         <v>12</v>
       </c>
-      <c r="T46" s="237"/>
+      <c r="T46" s="46"/>
       <c r="U46" s="47"/>
       <c r="V46" s="44"/>
       <c r="W46" s="47"/>
       <c r="X46" s="49"/>
-      <c r="Y46" s="45"/>
+      <c r="Y46" s="127"/>
       <c r="Z46" s="48"/>
       <c r="AA46" s="47"/>
       <c r="AB46" s="129">
@@ -8549,21 +8552,21 @@
     <row r="50" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="186">
         <f>RANK(AL50,$AL$10:$AL$97,)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B50" s="211" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="C50" s="198">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D50" s="199"/>
       <c r="E50" s="200">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F50" s="199"/>
       <c r="G50" s="201">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H50" s="202"/>
       <c r="I50" s="200"/>
@@ -8571,15 +8574,15 @@
         <v>6</v>
       </c>
       <c r="K50" s="203">
+        <v>6</v>
+      </c>
+      <c r="L50" s="202"/>
+      <c r="M50" s="200">
         <v>5</v>
       </c>
-      <c r="L50" s="202"/>
-      <c r="M50" s="200"/>
-      <c r="N50" s="199">
+      <c r="N50" s="199"/>
+      <c r="O50" s="200">
         <v>6</v>
-      </c>
-      <c r="O50" s="200">
-        <v>5</v>
       </c>
       <c r="P50" s="199"/>
       <c r="Q50" s="201"/>
@@ -8596,21 +8599,21 @@
       <c r="W50" s="202"/>
       <c r="X50" s="203"/>
       <c r="Y50" s="199"/>
-      <c r="Z50" s="201"/>
+      <c r="Z50" s="208"/>
       <c r="AA50" s="202"/>
       <c r="AB50" s="205">
         <f>SUM(T51:AA51)</f>
         <v>0</v>
       </c>
       <c r="AC50" s="201"/>
-      <c r="AD50" s="202"/>
+      <c r="AD50" s="234"/>
       <c r="AE50" s="203"/>
       <c r="AF50" s="202"/>
       <c r="AG50" s="205">
         <f>SUM(AC51:AF51)</f>
         <v>0</v>
       </c>
-      <c r="AH50" s="236"/>
+      <c r="AH50" s="209"/>
       <c r="AI50" s="196"/>
       <c r="AJ50" s="205">
         <f>AH51</f>
@@ -8945,29 +8948,29 @@
     <row r="54" spans="1:38" s="27" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="122">
         <f>RANK(AL54,$AL$10:$AL$97,)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B54" s="88" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C54" s="46">
         <v>6</v>
       </c>
       <c r="D54" s="45"/>
-      <c r="E54" s="44">
-        <v>6</v>
-      </c>
-      <c r="F54" s="45"/>
+      <c r="E54" s="44"/>
+      <c r="F54" s="45">
+        <v>7</v>
+      </c>
       <c r="G54" s="48">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H54" s="47"/>
       <c r="I54" s="44"/>
       <c r="J54" s="47">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K54" s="49">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L54" s="47"/>
       <c r="M54" s="44">
@@ -8975,7 +8978,7 @@
       </c>
       <c r="N54" s="45"/>
       <c r="O54" s="44">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P54" s="45"/>
       <c r="Q54" s="48"/>
@@ -9341,41 +9344,41 @@
     <row r="58" spans="1:38" s="27" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="186">
         <f>RANK(AL58,$AL$10:$AL$97,)</f>
+        <v>9</v>
+      </c>
+      <c r="B58" s="211" t="s">
+        <v>68</v>
+      </c>
+      <c r="C58" s="251">
+        <v>5</v>
+      </c>
+      <c r="D58" s="252"/>
+      <c r="E58" s="253">
         <v>6</v>
       </c>
-      <c r="B58" s="211" t="s">
-        <v>80</v>
-      </c>
-      <c r="C58" s="198">
+      <c r="F58" s="252"/>
+      <c r="G58" s="254">
         <v>5</v>
       </c>
-      <c r="D58" s="199"/>
-      <c r="E58" s="200">
+      <c r="H58" s="255"/>
+      <c r="I58" s="253"/>
+      <c r="J58" s="255">
         <v>6</v>
       </c>
-      <c r="F58" s="199"/>
-      <c r="G58" s="201">
+      <c r="K58" s="256">
         <v>6</v>
       </c>
-      <c r="H58" s="202"/>
-      <c r="I58" s="200"/>
-      <c r="J58" s="202">
+      <c r="L58" s="255"/>
+      <c r="M58" s="253">
+        <v>7</v>
+      </c>
+      <c r="N58" s="252"/>
+      <c r="O58" s="253">
         <v>6</v>
       </c>
-      <c r="K58" s="203">
-        <v>7</v>
-      </c>
-      <c r="L58" s="202"/>
-      <c r="M58" s="200">
-        <v>6</v>
-      </c>
-      <c r="N58" s="199"/>
-      <c r="O58" s="200">
-        <v>5</v>
-      </c>
-      <c r="P58" s="199"/>
-      <c r="Q58" s="201"/>
-      <c r="R58" s="204">
+      <c r="P58" s="252"/>
+      <c r="Q58" s="254"/>
+      <c r="R58" s="257">
         <v>6</v>
       </c>
       <c r="S58" s="205">
@@ -9737,19 +9740,19 @@
     <row r="62" spans="1:38" s="27" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="122">
         <f>RANK(AL62,$AL$10:$AL$97,)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B62" s="88" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C62" s="46">
         <v>5</v>
       </c>
       <c r="D62" s="45"/>
-      <c r="E62" s="44">
-        <v>6</v>
-      </c>
-      <c r="F62" s="45"/>
+      <c r="E62" s="44"/>
+      <c r="F62" s="45">
+        <v>7</v>
+      </c>
       <c r="G62" s="48">
         <v>6</v>
       </c>
@@ -9762,23 +9765,23 @@
         <v>5</v>
       </c>
       <c r="L62" s="47"/>
-      <c r="M62" s="44"/>
-      <c r="N62" s="45">
+      <c r="M62" s="44">
         <v>6</v>
       </c>
+      <c r="N62" s="45"/>
       <c r="O62" s="44">
         <v>7</v>
       </c>
       <c r="P62" s="45"/>
       <c r="Q62" s="48"/>
       <c r="R62" s="50">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S62" s="129">
         <f>SUM(C63:R63)</f>
         <v>12</v>
       </c>
-      <c r="T62" s="46"/>
+      <c r="T62" s="236"/>
       <c r="U62" s="47"/>
       <c r="V62" s="44"/>
       <c r="W62" s="47"/>
@@ -10133,21 +10136,21 @@
     <row r="66" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="186">
         <f>RANK(AL66,$AL$10:$AL$97,)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B66" s="211" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C66" s="198">
         <v>5</v>
       </c>
       <c r="D66" s="199"/>
       <c r="E66" s="200">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F66" s="199"/>
       <c r="G66" s="201">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H66" s="202"/>
       <c r="I66" s="200"/>
@@ -10155,21 +10158,21 @@
         <v>6</v>
       </c>
       <c r="K66" s="203">
+        <v>5</v>
+      </c>
+      <c r="L66" s="202"/>
+      <c r="M66" s="200"/>
+      <c r="N66" s="199">
         <v>6</v>
       </c>
-      <c r="L66" s="202"/>
-      <c r="M66" s="200">
+      <c r="O66" s="200">
         <v>7</v>
       </c>
-      <c r="N66" s="199"/>
-      <c r="O66" s="200">
+      <c r="P66" s="199"/>
+      <c r="Q66" s="201">
         <v>6</v>
       </c>
-      <c r="P66" s="199"/>
-      <c r="Q66" s="201"/>
-      <c r="R66" s="204">
-        <v>7</v>
-      </c>
+      <c r="R66" s="204"/>
       <c r="S66" s="205">
         <f>SUM(C67:R67)</f>
         <v>12</v>
@@ -10180,7 +10183,7 @@
       <c r="W66" s="202"/>
       <c r="X66" s="203"/>
       <c r="Y66" s="199"/>
-      <c r="Z66" s="208"/>
+      <c r="Z66" s="201"/>
       <c r="AA66" s="202"/>
       <c r="AB66" s="205">
         <f>SUM(T67:AA67)</f>
@@ -10194,7 +10197,7 @@
         <f>SUM(AC67:AF67)</f>
         <v>0</v>
       </c>
-      <c r="AH66" s="210"/>
+      <c r="AH66" s="313"/>
       <c r="AI66" s="206"/>
       <c r="AJ66" s="205">
         <f>AH67</f>
@@ -10242,7 +10245,7 @@
       <c r="L67" s="134"/>
       <c r="M67" s="132">
         <f>(IF($M66&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M66=$M$6+$N$6,$O$103,0),0),0)+IF($N66&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N66=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N67" s="134"/>
       <c r="O67" s="135">
@@ -10252,7 +10255,7 @@
       <c r="P67" s="134"/>
       <c r="Q67" s="135">
         <f>(IF($Q66&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q66=$Q$6+$R$6,$O$103,0),0),0)+IF($R66&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R66=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R67" s="138"/>
       <c r="S67" s="128"/>
@@ -10529,17 +10532,17 @@
     <row r="70" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="122">
         <f>RANK(AL70,$AL$10:$AL$97,)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B70" s="88" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C70" s="46">
         <v>6</v>
       </c>
       <c r="D70" s="45"/>
       <c r="E70" s="44">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F70" s="45"/>
       <c r="G70" s="48">
@@ -10551,11 +10554,11 @@
         <v>7</v>
       </c>
       <c r="K70" s="49">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L70" s="47"/>
       <c r="M70" s="44">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N70" s="45"/>
       <c r="O70" s="44">
@@ -10564,7 +10567,7 @@
       <c r="P70" s="45"/>
       <c r="Q70" s="48"/>
       <c r="R70" s="50">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S70" s="129">
         <f>SUM(C71:R71)</f>
@@ -10925,10 +10928,10 @@
     <row r="74" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="186">
         <f>RANK(AL74,$AL$10:$AL$97,)</f>
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B74" s="211" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="C74" s="198">
         <v>5</v>
@@ -10938,22 +10941,22 @@
         <v>6</v>
       </c>
       <c r="F74" s="199"/>
-      <c r="G74" s="201"/>
-      <c r="H74" s="202">
-        <v>7</v>
-      </c>
+      <c r="G74" s="201">
+        <v>6</v>
+      </c>
+      <c r="H74" s="202"/>
       <c r="I74" s="200"/>
       <c r="J74" s="202">
         <v>6</v>
       </c>
       <c r="K74" s="203">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L74" s="202"/>
-      <c r="M74" s="200"/>
-      <c r="N74" s="199">
-        <v>7</v>
-      </c>
+      <c r="M74" s="200">
+        <v>6</v>
+      </c>
+      <c r="N74" s="199"/>
       <c r="O74" s="200">
         <v>5</v>
       </c>
@@ -10964,7 +10967,7 @@
       </c>
       <c r="S74" s="205">
         <f>SUM(C75:R75)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="T74" s="198"/>
       <c r="U74" s="202"/>
@@ -10972,7 +10975,7 @@
       <c r="W74" s="202"/>
       <c r="X74" s="203"/>
       <c r="Y74" s="199"/>
-      <c r="Z74" s="208"/>
+      <c r="Z74" s="201"/>
       <c r="AA74" s="202"/>
       <c r="AB74" s="205">
         <f>SUM(T75:AA75)</f>
@@ -10994,11 +10997,11 @@
       </c>
       <c r="AK74" s="207">
         <f>MAX($AL$10:$AL$97) - AL74</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AL74" s="205">
         <f>$S74+$AB74+$AG74+$AJ74</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11019,7 +11022,7 @@
       <c r="F75" s="134"/>
       <c r="G75" s="132">
         <f>(IF($G74&lt;&gt;"",($G$6*$O$104)+IF($G$6=4,($O$102)+IF($G74=$G$6+$H$6,$O$103,0),0),0)+IF($H74&lt;&gt;"",($H$6*$O$104)+IF($H$6=4,($O$102)+IF($H74=$G$6+$H$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H75" s="134"/>
       <c r="I75" s="135">
@@ -11321,21 +11324,21 @@
     <row r="78" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="122">
         <f>RANK(AL78,$AL$10:$AL$97,)</f>
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B78" s="88" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="C78" s="46">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D78" s="45"/>
       <c r="E78" s="44">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F78" s="45"/>
       <c r="G78" s="48">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H78" s="47"/>
       <c r="I78" s="44"/>
@@ -11343,24 +11346,24 @@
         <v>6</v>
       </c>
       <c r="K78" s="49">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L78" s="47"/>
       <c r="M78" s="44"/>
       <c r="N78" s="45">
+        <v>7</v>
+      </c>
+      <c r="O78" s="44">
         <v>6</v>
-      </c>
-      <c r="O78" s="44">
-        <v>7</v>
       </c>
       <c r="P78" s="45"/>
       <c r="Q78" s="48">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R78" s="50"/>
       <c r="S78" s="129">
         <f>SUM(C79:R79)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="T78" s="46"/>
       <c r="U78" s="47"/>
@@ -11368,7 +11371,7 @@
       <c r="W78" s="47"/>
       <c r="X78" s="49"/>
       <c r="Y78" s="45"/>
-      <c r="Z78" s="48"/>
+      <c r="Z78" s="310"/>
       <c r="AA78" s="47"/>
       <c r="AB78" s="129">
         <f>SUM(T79:AA79)</f>
@@ -11382,7 +11385,7 @@
         <f>SUM(AC79:AF79)</f>
         <v>0</v>
       </c>
-      <c r="AH78" s="249"/>
+      <c r="AH78" s="105"/>
       <c r="AI78" s="58"/>
       <c r="AJ78" s="129">
         <f>AH79</f>
@@ -11390,11 +11393,11 @@
       </c>
       <c r="AK78" s="116">
         <f>MAX($AL$10:$AL$97) - AL78</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AL78" s="129">
         <f>$S78+$AB78+$AG78+$AJ78</f>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="79" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11430,7 +11433,7 @@
       <c r="L79" s="134"/>
       <c r="M79" s="132">
         <f>(IF($M78&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M78=$M$6+$N$6,$O$103,0),0),0)+IF($N78&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N78=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N79" s="134"/>
       <c r="O79" s="135">
@@ -11440,7 +11443,7 @@
       <c r="P79" s="134"/>
       <c r="Q79" s="135">
         <f>(IF($Q78&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q78=$Q$6+$R$6,$O$103,0),0),0)+IF($R78&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R78=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R79" s="138"/>
       <c r="S79" s="128"/>
@@ -11717,21 +11720,21 @@
     <row r="82" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="186">
         <f>RANK(AL82,$AL$10:$AL$97,)</f>
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B82" s="211" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C82" s="198">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D82" s="199"/>
       <c r="E82" s="200">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F82" s="199"/>
       <c r="G82" s="201">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H82" s="202"/>
       <c r="I82" s="200"/>
@@ -11742,21 +11745,21 @@
         <v>6</v>
       </c>
       <c r="L82" s="202"/>
-      <c r="M82" s="200"/>
-      <c r="N82" s="199">
+      <c r="M82" s="200">
         <v>7</v>
       </c>
+      <c r="N82" s="199"/>
       <c r="O82" s="200">
         <v>6</v>
       </c>
       <c r="P82" s="199"/>
-      <c r="Q82" s="201">
+      <c r="Q82" s="201"/>
+      <c r="R82" s="204">
         <v>7</v>
       </c>
-      <c r="R82" s="204"/>
       <c r="S82" s="205">
         <f>SUM(C83:R83)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="T82" s="198"/>
       <c r="U82" s="202"/>
@@ -11786,11 +11789,11 @@
       </c>
       <c r="AK82" s="207">
         <f>MAX($AL$10:$AL$97) - AL82</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AL82" s="205">
         <f>$S82+$AB82+$AG82+$AJ82</f>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11836,7 +11839,7 @@
       <c r="P83" s="134"/>
       <c r="Q83" s="135">
         <f>(IF($Q82&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q82=$Q$6+$R$6,$O$103,0),0),0)+IF($R82&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R82=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R83" s="138"/>
       <c r="S83" s="128"/>
@@ -12113,10 +12116,10 @@
     <row r="86" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="122">
         <f>RANK(AL86,$AL$10:$AL$97,)</f>
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B86" s="88" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C86" s="46">
         <v>6</v>
@@ -12127,12 +12130,12 @@
       </c>
       <c r="F86" s="45"/>
       <c r="G86" s="48">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H86" s="47"/>
       <c r="I86" s="44"/>
       <c r="J86" s="47">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K86" s="49">
         <v>7</v>
@@ -12143,16 +12146,16 @@
       </c>
       <c r="N86" s="45"/>
       <c r="O86" s="44">
+        <v>6</v>
+      </c>
+      <c r="P86" s="45"/>
+      <c r="Q86" s="48"/>
+      <c r="R86" s="50">
         <v>7</v>
       </c>
-      <c r="P86" s="45"/>
-      <c r="Q86" s="48">
-        <v>5</v>
-      </c>
-      <c r="R86" s="50"/>
       <c r="S86" s="129">
         <f>SUM(C87:R87)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="T86" s="46"/>
       <c r="U86" s="47"/>
@@ -12182,11 +12185,11 @@
       </c>
       <c r="AK86" s="116">
         <f>MAX($AL$10:$AL$97) - AL86</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AL86" s="129">
         <f>$S86+$AB86+$AG86+$AJ86</f>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="87" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -12232,7 +12235,7 @@
       <c r="P87" s="134"/>
       <c r="Q87" s="135">
         <f>(IF($Q86&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q86=$Q$6+$R$6,$O$103,0),0),0)+IF($R86&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R86=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R87" s="138"/>
       <c r="S87" s="128"/>
@@ -12518,15 +12521,15 @@
         <v>7</v>
       </c>
       <c r="D90" s="199"/>
-      <c r="E90" s="251">
+      <c r="E90" s="248">
         <v>6</v>
       </c>
       <c r="F90" s="199"/>
-      <c r="G90" s="252"/>
+      <c r="G90" s="249"/>
       <c r="H90" s="202">
         <v>6</v>
       </c>
-      <c r="I90" s="251"/>
+      <c r="I90" s="248"/>
       <c r="J90" s="202">
         <v>7</v>
       </c>
@@ -12548,14 +12551,14 @@
       <c r="R90" s="204"/>
       <c r="S90" s="205">
         <f>SUM(C91:R91)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="T90" s="198"/>
       <c r="U90" s="202"/>
-      <c r="V90" s="253"/>
+      <c r="V90" s="250"/>
       <c r="W90" s="202"/>
       <c r="X90" s="203"/>
-      <c r="Y90" s="239"/>
+      <c r="Y90" s="238"/>
       <c r="Z90" s="201"/>
       <c r="AA90" s="202"/>
       <c r="AB90" s="205">
@@ -12578,11 +12581,11 @@
       </c>
       <c r="AK90" s="207">
         <f>MAX($AL$10:$AL$97) - AL90</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AL90" s="205">
         <f>$S90+$AB90+$AG90+$AJ90</f>
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="91" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -12603,7 +12606,7 @@
       <c r="F91" s="134"/>
       <c r="G91" s="132">
         <f>(IF($G90&lt;&gt;"",($G$6*$O$104)+IF($G$6=4,($O$102)+IF($G90=$G$6+$H$6,$O$103,0),0),0)+IF($H90&lt;&gt;"",($H$6*$O$104)+IF($H$6=4,($O$102)+IF($H90=$G$6+$H$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H91" s="134"/>
       <c r="I91" s="135">
@@ -12628,7 +12631,7 @@
       <c r="P91" s="134"/>
       <c r="Q91" s="135">
         <f>(IF($Q90&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q90=$Q$6+$R$6,$O$103,0),0),0)+IF($R90&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R90=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R91" s="138"/>
       <c r="S91" s="128"/>
@@ -12908,43 +12911,43 @@
         <v>21</v>
       </c>
       <c r="B94" s="88" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C94" s="226">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D94" s="227"/>
       <c r="E94" s="228">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F94" s="227"/>
-      <c r="G94" s="229"/>
-      <c r="H94" s="230">
-        <v>7</v>
-      </c>
+      <c r="G94" s="229">
+        <v>5</v>
+      </c>
+      <c r="H94" s="230"/>
       <c r="I94" s="228"/>
       <c r="J94" s="230">
+        <v>5</v>
+      </c>
+      <c r="K94" s="231">
+        <v>7</v>
+      </c>
+      <c r="L94" s="230"/>
+      <c r="M94" s="228">
         <v>6</v>
       </c>
-      <c r="K94" s="231">
-        <v>5</v>
-      </c>
-      <c r="L94" s="230"/>
-      <c r="M94" s="228"/>
-      <c r="N94" s="227">
-        <v>6</v>
-      </c>
+      <c r="N94" s="227"/>
       <c r="O94" s="228">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P94" s="227"/>
       <c r="Q94" s="229">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R94" s="232"/>
       <c r="S94" s="129">
         <f>SUM(C95:R95)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="T94" s="46"/>
       <c r="U94" s="47"/>
@@ -12974,11 +12977,11 @@
       </c>
       <c r="AK94" s="116">
         <f>MAX($AL$10:$AL$97) - AL94</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AL94" s="218">
         <f>$S94+$AB94+$AG94+$AJ94</f>
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="95" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -12999,7 +13002,7 @@
       <c r="F95" s="134"/>
       <c r="G95" s="132">
         <f>(IF($G94&lt;&gt;"",($G$6*$O$104)+IF($G$6=4,($O$102)+IF($G94=$G$6+$H$6,$O$103,0),0),0)+IF($H94&lt;&gt;"",($H$6*$O$104)+IF($H$6=4,($O$102)+IF($H94=$G$6+$H$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H95" s="134"/>
       <c r="I95" s="135">
@@ -13024,7 +13027,7 @@
       <c r="P95" s="134"/>
       <c r="Q95" s="135">
         <f>(IF($Q94&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q94=$Q$6+$R$6,$O$103,0),0),0)+IF($R94&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R94=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R95" s="138"/>
       <c r="S95" s="128"/>
@@ -13431,12 +13434,12 @@
     <row r="100" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B100" s="43"/>
       <c r="N100" s="26"/>
-      <c r="O100" s="287" t="s">
+      <c r="O100" s="258" t="s">
         <v>17</v>
       </c>
-      <c r="P100" s="288"/>
-      <c r="Q100" s="288"/>
-      <c r="R100" s="289"/>
+      <c r="P100" s="259"/>
+      <c r="Q100" s="259"/>
+      <c r="R100" s="260"/>
       <c r="AG100" s="30"/>
       <c r="AH100" s="30"/>
       <c r="AI100" s="30"/>
@@ -13445,21 +13448,21 @@
     </row>
     <row r="101" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="33"/>
-      <c r="B101" s="275" t="s">
+      <c r="B101" s="287" t="s">
         <v>16</v>
       </c>
-      <c r="C101" s="276"/>
-      <c r="D101" s="276"/>
-      <c r="E101" s="276"/>
-      <c r="F101" s="276"/>
-      <c r="G101" s="276"/>
-      <c r="H101" s="276"/>
-      <c r="I101" s="276"/>
-      <c r="J101" s="276"/>
-      <c r="K101" s="276"/>
-      <c r="L101" s="276"/>
-      <c r="M101" s="276"/>
-      <c r="N101" s="277"/>
+      <c r="C101" s="288"/>
+      <c r="D101" s="288"/>
+      <c r="E101" s="288"/>
+      <c r="F101" s="288"/>
+      <c r="G101" s="288"/>
+      <c r="H101" s="288"/>
+      <c r="I101" s="288"/>
+      <c r="J101" s="288"/>
+      <c r="K101" s="288"/>
+      <c r="L101" s="288"/>
+      <c r="M101" s="288"/>
+      <c r="N101" s="289"/>
       <c r="O101" s="21">
         <v>1</v>
       </c>
@@ -13472,45 +13475,45 @@
       <c r="R101" s="22">
         <v>4</v>
       </c>
-      <c r="U101" s="290" t="s">
+      <c r="U101" s="261" t="s">
         <v>26</v>
       </c>
-      <c r="V101" s="291"/>
-      <c r="W101" s="291"/>
-      <c r="X101" s="291"/>
-      <c r="Y101" s="291"/>
-      <c r="Z101" s="291"/>
-      <c r="AA101" s="291"/>
-      <c r="AB101" s="291"/>
-      <c r="AC101" s="291"/>
-      <c r="AD101" s="292"/>
+      <c r="V101" s="262"/>
+      <c r="W101" s="262"/>
+      <c r="X101" s="262"/>
+      <c r="Y101" s="262"/>
+      <c r="Z101" s="262"/>
+      <c r="AA101" s="262"/>
+      <c r="AB101" s="262"/>
+      <c r="AC101" s="262"/>
+      <c r="AD101" s="263"/>
       <c r="AE101" s="28"/>
       <c r="AF101" s="28"/>
-      <c r="AG101" s="293" t="s">
+      <c r="AG101" s="264" t="s">
         <v>24</v>
       </c>
-      <c r="AH101" s="294"/>
-      <c r="AI101" s="294"/>
-      <c r="AJ101" s="294"/>
-      <c r="AK101" s="295"/>
+      <c r="AH101" s="265"/>
+      <c r="AI101" s="265"/>
+      <c r="AJ101" s="265"/>
+      <c r="AK101" s="266"/>
     </row>
     <row r="102" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A102" s="34"/>
-      <c r="B102" s="254" t="s">
+      <c r="B102" s="294" t="s">
         <v>6</v>
       </c>
-      <c r="C102" s="255"/>
-      <c r="D102" s="255"/>
-      <c r="E102" s="255"/>
-      <c r="F102" s="255"/>
-      <c r="G102" s="255"/>
-      <c r="H102" s="255"/>
-      <c r="I102" s="255"/>
-      <c r="J102" s="255"/>
-      <c r="K102" s="255"/>
-      <c r="L102" s="255"/>
-      <c r="M102" s="255"/>
-      <c r="N102" s="256"/>
+      <c r="C102" s="295"/>
+      <c r="D102" s="295"/>
+      <c r="E102" s="295"/>
+      <c r="F102" s="295"/>
+      <c r="G102" s="295"/>
+      <c r="H102" s="295"/>
+      <c r="I102" s="295"/>
+      <c r="J102" s="295"/>
+      <c r="K102" s="295"/>
+      <c r="L102" s="295"/>
+      <c r="M102" s="295"/>
+      <c r="N102" s="296"/>
       <c r="O102" s="20">
         <v>5</v>
       </c>
@@ -13523,49 +13526,49 @@
       <c r="R102" s="23">
         <v>20</v>
       </c>
-      <c r="U102" s="280" t="s">
+      <c r="U102" s="292" t="s">
         <v>20</v>
       </c>
-      <c r="V102" s="281"/>
-      <c r="W102" s="281"/>
-      <c r="X102" s="281"/>
-      <c r="Y102" s="281"/>
-      <c r="Z102" s="281"/>
-      <c r="AA102" s="281"/>
-      <c r="AB102" s="278">
+      <c r="V102" s="293"/>
+      <c r="W102" s="293"/>
+      <c r="X102" s="293"/>
+      <c r="Y102" s="293"/>
+      <c r="Z102" s="293"/>
+      <c r="AA102" s="293"/>
+      <c r="AB102" s="290">
         <v>22</v>
       </c>
-      <c r="AC102" s="278"/>
-      <c r="AD102" s="279"/>
+      <c r="AC102" s="290"/>
+      <c r="AD102" s="291"/>
       <c r="AE102" s="29"/>
       <c r="AF102" s="29"/>
-      <c r="AG102" s="261" t="s">
+      <c r="AG102" s="306" t="s">
         <v>21</v>
       </c>
-      <c r="AH102" s="262"/>
-      <c r="AI102" s="262"/>
-      <c r="AJ102" s="263"/>
+      <c r="AH102" s="307"/>
+      <c r="AI102" s="307"/>
+      <c r="AJ102" s="308"/>
       <c r="AK102" s="223">
         <v>230</v>
       </c>
     </row>
     <row r="103" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="34"/>
-      <c r="B103" s="254" t="s">
+      <c r="B103" s="294" t="s">
         <v>5</v>
       </c>
-      <c r="C103" s="255"/>
-      <c r="D103" s="255"/>
-      <c r="E103" s="255"/>
-      <c r="F103" s="255"/>
-      <c r="G103" s="255"/>
-      <c r="H103" s="255"/>
-      <c r="I103" s="255"/>
-      <c r="J103" s="255"/>
-      <c r="K103" s="255"/>
-      <c r="L103" s="255"/>
-      <c r="M103" s="255"/>
-      <c r="N103" s="256"/>
+      <c r="C103" s="295"/>
+      <c r="D103" s="295"/>
+      <c r="E103" s="295"/>
+      <c r="F103" s="295"/>
+      <c r="G103" s="295"/>
+      <c r="H103" s="295"/>
+      <c r="I103" s="295"/>
+      <c r="J103" s="295"/>
+      <c r="K103" s="295"/>
+      <c r="L103" s="295"/>
+      <c r="M103" s="295"/>
+      <c r="N103" s="296"/>
       <c r="O103" s="20">
         <v>2</v>
       </c>
@@ -13578,49 +13581,49 @@
       <c r="R103" s="23">
         <v>8</v>
       </c>
-      <c r="U103" s="259" t="s">
+      <c r="U103" s="301" t="s">
         <v>18</v>
       </c>
-      <c r="V103" s="260"/>
-      <c r="W103" s="260"/>
-      <c r="X103" s="260"/>
-      <c r="Y103" s="260"/>
-      <c r="Z103" s="260"/>
-      <c r="AA103" s="260"/>
-      <c r="AB103" s="285">
+      <c r="V103" s="302"/>
+      <c r="W103" s="302"/>
+      <c r="X103" s="302"/>
+      <c r="Y103" s="302"/>
+      <c r="Z103" s="302"/>
+      <c r="AA103" s="302"/>
+      <c r="AB103" s="303">
         <v>20</v>
       </c>
-      <c r="AC103" s="285"/>
-      <c r="AD103" s="286"/>
+      <c r="AC103" s="303"/>
+      <c r="AD103" s="304"/>
       <c r="AE103" s="29"/>
       <c r="AF103" s="29"/>
-      <c r="AG103" s="264" t="s">
+      <c r="AG103" s="309" t="s">
         <v>22</v>
       </c>
-      <c r="AH103" s="255"/>
-      <c r="AI103" s="255"/>
-      <c r="AJ103" s="256"/>
+      <c r="AH103" s="295"/>
+      <c r="AI103" s="295"/>
+      <c r="AJ103" s="296"/>
       <c r="AK103" s="36">
         <v>115</v>
       </c>
     </row>
     <row r="104" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="35"/>
-      <c r="B104" s="268" t="s">
+      <c r="B104" s="280" t="s">
         <v>4</v>
       </c>
-      <c r="C104" s="269"/>
-      <c r="D104" s="269"/>
-      <c r="E104" s="269"/>
-      <c r="F104" s="269"/>
-      <c r="G104" s="269"/>
-      <c r="H104" s="269"/>
-      <c r="I104" s="269"/>
-      <c r="J104" s="269"/>
-      <c r="K104" s="269"/>
-      <c r="L104" s="269"/>
-      <c r="M104" s="269"/>
-      <c r="N104" s="270"/>
+      <c r="C104" s="281"/>
+      <c r="D104" s="281"/>
+      <c r="E104" s="281"/>
+      <c r="F104" s="281"/>
+      <c r="G104" s="281"/>
+      <c r="H104" s="281"/>
+      <c r="I104" s="281"/>
+      <c r="J104" s="281"/>
+      <c r="K104" s="281"/>
+      <c r="L104" s="281"/>
+      <c r="M104" s="281"/>
+      <c r="N104" s="282"/>
       <c r="O104" s="3">
         <v>1</v>
       </c>
@@ -13633,51 +13636,51 @@
       <c r="R104" s="24">
         <v>1</v>
       </c>
-      <c r="U104" s="282" t="s">
+      <c r="U104" s="297" t="s">
         <v>19</v>
       </c>
-      <c r="V104" s="258"/>
-      <c r="W104" s="258"/>
-      <c r="X104" s="258"/>
-      <c r="Y104" s="258"/>
-      <c r="Z104" s="258"/>
-      <c r="AA104" s="258"/>
-      <c r="AB104" s="283">
+      <c r="V104" s="298"/>
+      <c r="W104" s="298"/>
+      <c r="X104" s="298"/>
+      <c r="Y104" s="298"/>
+      <c r="Z104" s="298"/>
+      <c r="AA104" s="298"/>
+      <c r="AB104" s="299">
         <f>AB102*AB103</f>
         <v>440</v>
       </c>
-      <c r="AC104" s="283"/>
-      <c r="AD104" s="284"/>
+      <c r="AC104" s="299"/>
+      <c r="AD104" s="300"/>
       <c r="AE104" s="29"/>
       <c r="AF104" s="29"/>
-      <c r="AG104" s="264" t="s">
+      <c r="AG104" s="309" t="s">
         <v>25</v>
       </c>
-      <c r="AH104" s="255"/>
-      <c r="AI104" s="255"/>
-      <c r="AJ104" s="256"/>
+      <c r="AH104" s="295"/>
+      <c r="AI104" s="295"/>
+      <c r="AJ104" s="296"/>
       <c r="AK104" s="36">
         <v>65</v>
       </c>
     </row>
     <row r="105" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG105" s="259" t="s">
+      <c r="AG105" s="301" t="s">
         <v>23</v>
       </c>
-      <c r="AH105" s="260"/>
-      <c r="AI105" s="260"/>
-      <c r="AJ105" s="260"/>
+      <c r="AH105" s="302"/>
+      <c r="AI105" s="302"/>
+      <c r="AJ105" s="302"/>
       <c r="AK105" s="225">
         <v>30</v>
       </c>
     </row>
     <row r="106" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG106" s="257" t="s">
+      <c r="AG106" s="305" t="s">
         <v>19</v>
       </c>
-      <c r="AH106" s="258"/>
-      <c r="AI106" s="258"/>
-      <c r="AJ106" s="258"/>
+      <c r="AH106" s="298"/>
+      <c r="AI106" s="298"/>
+      <c r="AJ106" s="298"/>
       <c r="AK106" s="224">
         <f>SUM(AK102:AK105)</f>
         <v>440</v>
@@ -13689,6 +13692,28 @@
     <sortCondition ref="B10:B94"/>
   </sortState>
   <mergeCells count="38">
+    <mergeCell ref="B103:N103"/>
+    <mergeCell ref="AG106:AJ106"/>
+    <mergeCell ref="AG105:AJ105"/>
+    <mergeCell ref="AG102:AJ102"/>
+    <mergeCell ref="AG104:AJ104"/>
+    <mergeCell ref="AG103:AJ103"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="B104:N104"/>
+    <mergeCell ref="C1:O1"/>
+    <mergeCell ref="P1:AJ1"/>
+    <mergeCell ref="C3:O3"/>
+    <mergeCell ref="P3:AJ3"/>
+    <mergeCell ref="C2:P2"/>
+    <mergeCell ref="Q2:AJ2"/>
+    <mergeCell ref="B101:N101"/>
+    <mergeCell ref="AB102:AD102"/>
+    <mergeCell ref="U102:AA102"/>
+    <mergeCell ref="B102:N102"/>
+    <mergeCell ref="U104:AA104"/>
+    <mergeCell ref="AB104:AD104"/>
+    <mergeCell ref="U103:AA103"/>
+    <mergeCell ref="AB103:AD103"/>
     <mergeCell ref="O100:R100"/>
     <mergeCell ref="U101:AD101"/>
     <mergeCell ref="AG101:AK101"/>
@@ -13705,342 +13730,320 @@
     <mergeCell ref="C5:J5"/>
     <mergeCell ref="K5:R5"/>
     <mergeCell ref="S5:S9"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="B104:N104"/>
-    <mergeCell ref="C1:O1"/>
-    <mergeCell ref="P1:AJ1"/>
-    <mergeCell ref="C3:O3"/>
-    <mergeCell ref="P3:AJ3"/>
-    <mergeCell ref="C2:P2"/>
-    <mergeCell ref="Q2:AJ2"/>
-    <mergeCell ref="B101:N101"/>
-    <mergeCell ref="AB102:AD102"/>
-    <mergeCell ref="U102:AA102"/>
-    <mergeCell ref="B102:N102"/>
-    <mergeCell ref="U104:AA104"/>
-    <mergeCell ref="AB104:AD104"/>
-    <mergeCell ref="U103:AA103"/>
-    <mergeCell ref="AB103:AD103"/>
-    <mergeCell ref="B103:N103"/>
-    <mergeCell ref="AG106:AJ106"/>
-    <mergeCell ref="AG105:AJ105"/>
-    <mergeCell ref="AG102:AJ102"/>
-    <mergeCell ref="AG104:AJ104"/>
-    <mergeCell ref="AG103:AJ103"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <conditionalFormatting sqref="AH18:AI18 AH10:AI10 AH14:AI14 T10:AA10 AC10:AF10 C10:R10 C14:R14 T14:AA14 AC14:AF14 T18:AA18 AC18:AF18 AH30:AI30 C30:R30 T30:AA30 AC30:AF30 AH26:AI26 C26:R26 T26:AA26 AC26:AF26 AH62:AI62 C62:R62 T62:AA62 AC62:AF62 AH42:AI42 C42:R42 T42:AA42 AC42:AF42 AH22:AI22 C22:R22 T22:AA22 AC22:AF22 AH38:AI38 C38:R38 T38:AA38 AC38:AF38 AH34:AI34 C34:R34 T34:AA34 AC34:AF34 AH66:AI66 C66:R66 T66:AA66 AC66:AF66 C18:R18">
-    <cfRule type="cellIs" dxfId="80" priority="183" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="100" priority="183" stopIfTrue="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:R10">
-    <cfRule type="cellIs" dxfId="79" priority="179" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="99" priority="179" stopIfTrue="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:R14">
-    <cfRule type="cellIs" dxfId="78" priority="178" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="98" priority="178" stopIfTrue="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:R18">
-    <cfRule type="cellIs" dxfId="77" priority="177" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="97" priority="177" stopIfTrue="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:R22">
-    <cfRule type="cellIs" dxfId="76" priority="176" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="96" priority="176" stopIfTrue="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:R26">
-    <cfRule type="cellIs" dxfId="75" priority="175" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="95" priority="175" stopIfTrue="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:R30">
-    <cfRule type="cellIs" dxfId="74" priority="174" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="94" priority="174" stopIfTrue="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34:R34">
-    <cfRule type="cellIs" dxfId="73" priority="173" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="93" priority="173" stopIfTrue="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:R38">
-    <cfRule type="cellIs" dxfId="72" priority="172" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="92" priority="172" stopIfTrue="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42:R42">
-    <cfRule type="cellIs" dxfId="71" priority="171" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="91" priority="171" stopIfTrue="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH54:AI54 C54:R54 T54:AA54 AC54:AF54">
-    <cfRule type="cellIs" dxfId="70" priority="170" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="90" priority="170" stopIfTrue="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH46:AI46 C46:R46 T46:AA46 AC46:AF46">
-    <cfRule type="cellIs" dxfId="69" priority="169" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="89" priority="169" stopIfTrue="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:R46">
-    <cfRule type="cellIs" dxfId="68" priority="168" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="88" priority="168" stopIfTrue="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH50:AI50 C50:R50 T50:AA50 AC50:AF50">
-    <cfRule type="cellIs" dxfId="67" priority="167" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="87" priority="167" stopIfTrue="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50:R50">
-    <cfRule type="cellIs" dxfId="66" priority="166" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="86" priority="166" stopIfTrue="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH58:AI58 C58:R58 T58:AA58 AC58:AF58">
-    <cfRule type="cellIs" dxfId="65" priority="165" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="85" priority="165" stopIfTrue="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R18">
-    <cfRule type="cellIs" dxfId="64" priority="164" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="84" priority="164" stopIfTrue="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH70:AI70 C70:R70 T70:AA70 AC70:AF70">
-    <cfRule type="cellIs" dxfId="63" priority="163" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="83" priority="163" stopIfTrue="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH74:AI74 C74:R74 T74:AA74 AC74:AF74">
-    <cfRule type="cellIs" dxfId="62" priority="162" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="82" priority="162" stopIfTrue="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH78:AI78 C78:R78 T78:AA78 AC78:AF78">
-    <cfRule type="cellIs" dxfId="61" priority="161" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="81" priority="161" stopIfTrue="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10:S15 AB10:AB15 AG10:AG15 AJ10:AJ15 AJ26:AJ27 AG26:AG27 AB26:AB27 S26:S27 AJ22:AJ23 AG22:AG23 AB22:AB23 S22:S23 AJ18:AJ19 AG18:AG19 AB18:AB19 S18:S19 S38:S39 AB38:AB39 AG38:AG39 AJ38:AJ39 S30:S31 AB30:AB31 AG30:AG31 AJ30:AJ31 AJ42:AJ43 AG42:AG43 AB42:AB43 S42:S43 S46:S47 AB46:AB47 AG46:AG47 AJ46:AJ47 AJ50 AG50 AB50 S50 S58 AB58 AG58 AJ58 S54 AB54 AG54 AJ54 AJ62 AG62 AB62 S62 S66 AB66 AG66 AJ66 AJ70 AG70 AB70 S70 S74 AB74 AG74 AJ74 AJ78 AG78 AB78 S78 AJ34:AJ35 AG34:AG35 AB34:AB35 S34:S35">
-    <cfRule type="cellIs" dxfId="60" priority="156" operator="notEqual">
+    <cfRule type="cellIs" dxfId="80" priority="156" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL10:AL23 AL26:AL27 AL38:AL39 AL30:AL31 AL42:AL43 AL46:AL47 AL50 AL58 AL54 AL62 AL66 AL70 AL74 AL78 AL34:AL35">
-    <cfRule type="cellIs" dxfId="59" priority="155" operator="notEqual">
+    <cfRule type="cellIs" dxfId="79" priority="155" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ24:AJ25">
-    <cfRule type="cellIs" dxfId="58" priority="152" operator="notEqual">
+    <cfRule type="cellIs" dxfId="78" priority="152" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL24:AL25">
-    <cfRule type="cellIs" dxfId="57" priority="153" operator="notEqual">
+    <cfRule type="cellIs" dxfId="77" priority="153" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ20:AJ21">
-    <cfRule type="cellIs" dxfId="56" priority="151" operator="notEqual">
+    <cfRule type="cellIs" dxfId="76" priority="151" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ16:AJ17">
-    <cfRule type="cellIs" dxfId="55" priority="150" operator="notEqual">
+    <cfRule type="cellIs" dxfId="75" priority="150" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ28:AJ29">
-    <cfRule type="cellIs" dxfId="54" priority="146" operator="notEqual">
+    <cfRule type="cellIs" dxfId="74" priority="146" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL28:AL29">
-    <cfRule type="cellIs" dxfId="53" priority="147" operator="notEqual">
+    <cfRule type="cellIs" dxfId="73" priority="147" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL36:AL37">
-    <cfRule type="cellIs" dxfId="52" priority="145" operator="notEqual">
+    <cfRule type="cellIs" dxfId="72" priority="145" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL40:AL41">
-    <cfRule type="cellIs" dxfId="51" priority="143" operator="notEqual">
+    <cfRule type="cellIs" dxfId="71" priority="143" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL44:AL45">
-    <cfRule type="cellIs" dxfId="50" priority="141" operator="notEqual">
+    <cfRule type="cellIs" dxfId="70" priority="141" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL48:AL49">
-    <cfRule type="cellIs" dxfId="49" priority="139" operator="notEqual">
+    <cfRule type="cellIs" dxfId="69" priority="139" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S20:S21 AB20:AB21 AG20:AG21">
-    <cfRule type="cellIs" dxfId="48" priority="116" operator="notEqual">
+    <cfRule type="cellIs" dxfId="68" priority="116" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S24:S25 AB24:AB25 AG24:AG25">
-    <cfRule type="cellIs" dxfId="47" priority="115" operator="notEqual">
+    <cfRule type="cellIs" dxfId="67" priority="115" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S16:S17 AB16:AB17 AG16:AG17">
-    <cfRule type="cellIs" dxfId="46" priority="117" operator="notEqual">
+    <cfRule type="cellIs" dxfId="66" priority="117" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S28:S29 AB28:AB29 AG28:AG29">
-    <cfRule type="cellIs" dxfId="45" priority="114" operator="notEqual">
+    <cfRule type="cellIs" dxfId="65" priority="114" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ32:AJ33">
-    <cfRule type="cellIs" dxfId="44" priority="112" operator="notEqual">
+    <cfRule type="cellIs" dxfId="64" priority="112" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL32:AL33">
-    <cfRule type="cellIs" dxfId="43" priority="113" operator="notEqual">
+    <cfRule type="cellIs" dxfId="63" priority="113" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S32:S33 AB32:AB33 AG32:AG33">
-    <cfRule type="cellIs" dxfId="42" priority="111" operator="notEqual">
+    <cfRule type="cellIs" dxfId="62" priority="111" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ36:AJ37">
-    <cfRule type="cellIs" dxfId="41" priority="110" operator="notEqual">
+    <cfRule type="cellIs" dxfId="61" priority="110" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S36:S37 AB36:AB37 AG36:AG37">
-    <cfRule type="cellIs" dxfId="40" priority="109" operator="notEqual">
+    <cfRule type="cellIs" dxfId="60" priority="109" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ40:AJ41">
-    <cfRule type="cellIs" dxfId="39" priority="108" operator="notEqual">
+    <cfRule type="cellIs" dxfId="59" priority="108" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S40:S41 AB40:AB41 AG40:AG41">
-    <cfRule type="cellIs" dxfId="38" priority="107" operator="notEqual">
+    <cfRule type="cellIs" dxfId="58" priority="107" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ44:AJ45">
-    <cfRule type="cellIs" dxfId="37" priority="106" operator="notEqual">
+    <cfRule type="cellIs" dxfId="57" priority="106" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S44:S45 AB44:AB45 AG44:AG45">
-    <cfRule type="cellIs" dxfId="36" priority="105" operator="notEqual">
+    <cfRule type="cellIs" dxfId="56" priority="105" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ48:AJ49">
-    <cfRule type="cellIs" dxfId="35" priority="104" operator="notEqual">
+    <cfRule type="cellIs" dxfId="55" priority="104" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S48:S49 AB48:AB49 AG48:AG49">
-    <cfRule type="cellIs" dxfId="34" priority="103" operator="notEqual">
+    <cfRule type="cellIs" dxfId="54" priority="103" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S51:S53 AB51:AB53 AG51:AG53 AJ51:AJ53">
-    <cfRule type="cellIs" dxfId="33" priority="84" operator="notEqual">
+    <cfRule type="cellIs" dxfId="53" priority="84" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL51:AL53">
-    <cfRule type="cellIs" dxfId="32" priority="83" operator="notEqual">
+    <cfRule type="cellIs" dxfId="52" priority="83" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S55:S57 AB55:AB57 AG55:AG57 AJ55:AJ57">
-    <cfRule type="cellIs" dxfId="31" priority="82" operator="notEqual">
+    <cfRule type="cellIs" dxfId="51" priority="82" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL55:AL57">
-    <cfRule type="cellIs" dxfId="30" priority="81" operator="notEqual">
+    <cfRule type="cellIs" dxfId="50" priority="81" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S59:S61 AB59:AB61 AG59:AG61 AJ59:AJ61">
-    <cfRule type="cellIs" dxfId="29" priority="80" operator="notEqual">
+    <cfRule type="cellIs" dxfId="49" priority="80" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL59:AL61">
-    <cfRule type="cellIs" dxfId="28" priority="79" operator="notEqual">
+    <cfRule type="cellIs" dxfId="48" priority="79" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S63:S65 AB63:AB65 AG63:AG65 AJ63:AJ65">
-    <cfRule type="cellIs" dxfId="27" priority="78" operator="notEqual">
+    <cfRule type="cellIs" dxfId="47" priority="78" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL63:AL65">
-    <cfRule type="cellIs" dxfId="26" priority="77" operator="notEqual">
+    <cfRule type="cellIs" dxfId="46" priority="77" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S67:S69 AB67:AB69 AG67:AG69 AJ67:AJ69">
-    <cfRule type="cellIs" dxfId="25" priority="76" operator="notEqual">
+    <cfRule type="cellIs" dxfId="45" priority="76" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL67:AL69">
-    <cfRule type="cellIs" dxfId="24" priority="75" operator="notEqual">
+    <cfRule type="cellIs" dxfId="44" priority="75" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S71:S73 AB71:AB73 AG71:AG73 AJ71:AJ73">
-    <cfRule type="cellIs" dxfId="23" priority="74" operator="notEqual">
+    <cfRule type="cellIs" dxfId="43" priority="74" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL71:AL73">
-    <cfRule type="cellIs" dxfId="22" priority="73" operator="notEqual">
+    <cfRule type="cellIs" dxfId="42" priority="73" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S75:S77 AB75:AB77 AG75:AG77 AJ75:AJ77">
-    <cfRule type="cellIs" dxfId="21" priority="72" operator="notEqual">
+    <cfRule type="cellIs" dxfId="41" priority="72" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL75:AL77">
-    <cfRule type="cellIs" dxfId="20" priority="71" operator="notEqual">
+    <cfRule type="cellIs" dxfId="40" priority="71" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S79:S81 AB79:AB81 AG79:AG81 AJ79:AJ81">
-    <cfRule type="cellIs" dxfId="19" priority="70" operator="notEqual">
+    <cfRule type="cellIs" dxfId="39" priority="70" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL79:AL81">
-    <cfRule type="cellIs" dxfId="18" priority="69" operator="notEqual">
+    <cfRule type="cellIs" dxfId="38" priority="69" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14059,92 +14062,92 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH82:AI82 C82:R82 T82:AA82 AC82:AF82">
-    <cfRule type="cellIs" dxfId="17" priority="58" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="37" priority="58" stopIfTrue="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH90:AI90 C90:R90 T90:AA90 AC90:AF90">
-    <cfRule type="cellIs" dxfId="16" priority="57" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="36" priority="57" stopIfTrue="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S82 AB82 AG82 AJ82 AJ90 AG90 AB90 S90">
-    <cfRule type="cellIs" dxfId="15" priority="56" operator="notEqual">
+    <cfRule type="cellIs" dxfId="35" priority="56" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL82 AL90">
-    <cfRule type="cellIs" dxfId="14" priority="55" operator="notEqual">
+    <cfRule type="cellIs" dxfId="34" priority="55" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S83:S85 AB83:AB85 AG83:AG85 AJ83:AJ85">
-    <cfRule type="cellIs" dxfId="13" priority="54" operator="notEqual">
+    <cfRule type="cellIs" dxfId="33" priority="54" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL83:AL85">
-    <cfRule type="cellIs" dxfId="12" priority="53" operator="notEqual">
+    <cfRule type="cellIs" dxfId="32" priority="53" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S91:S93 AB91:AB93 AG91:AG93 AJ91:AJ93">
-    <cfRule type="cellIs" dxfId="11" priority="52" operator="notEqual">
+    <cfRule type="cellIs" dxfId="31" priority="52" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL91:AL93">
-    <cfRule type="cellIs" dxfId="10" priority="51" operator="notEqual">
+    <cfRule type="cellIs" dxfId="30" priority="51" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH94:AI94 C94:R94 T94:AA94 AC94:AF94">
-    <cfRule type="cellIs" dxfId="9" priority="50" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="29" priority="50" stopIfTrue="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S94 AB94 AG94 AJ94">
-    <cfRule type="cellIs" dxfId="8" priority="48" operator="notEqual">
+    <cfRule type="cellIs" dxfId="28" priority="48" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL94">
-    <cfRule type="cellIs" dxfId="7" priority="47" operator="notEqual">
+    <cfRule type="cellIs" dxfId="27" priority="47" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S95:S97 AB95:AB97 AG95:AG97 AJ95:AJ97">
-    <cfRule type="cellIs" dxfId="6" priority="46" operator="notEqual">
+    <cfRule type="cellIs" dxfId="26" priority="46" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL95:AL97">
-    <cfRule type="cellIs" dxfId="5" priority="45" operator="notEqual">
+    <cfRule type="cellIs" dxfId="25" priority="45" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH86:AI86 C86:R86 T86:AA86 AC86:AF86">
-    <cfRule type="cellIs" dxfId="4" priority="14" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="24" priority="14" stopIfTrue="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S86 AB86 AG86 AJ86">
-    <cfRule type="cellIs" dxfId="3" priority="13" operator="notEqual">
+    <cfRule type="cellIs" dxfId="23" priority="13" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL86">
-    <cfRule type="cellIs" dxfId="2" priority="12" operator="notEqual">
+    <cfRule type="cellIs" dxfId="22" priority="12" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S87:S89 AB87:AB89 AG87:AG89 AJ87:AJ89">
-    <cfRule type="cellIs" dxfId="1" priority="11" operator="notEqual">
+    <cfRule type="cellIs" dxfId="21" priority="11" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL87:AL89">
-    <cfRule type="cellIs" dxfId="0" priority="10" operator="notEqual">
+    <cfRule type="cellIs" dxfId="20" priority="10" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14383,7 +14386,7 @@
   <dimension ref="A1:AJ31"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14774,7 +14777,9 @@
         <v>4</v>
       </c>
       <c r="E10" s="85"/>
-      <c r="F10" s="85"/>
+      <c r="F10" s="85">
+        <v>1</v>
+      </c>
       <c r="G10" s="86"/>
       <c r="H10" s="85"/>
       <c r="I10" s="86"/>
@@ -14831,13 +14836,15 @@
       <c r="E11" s="85">
         <v>5</v>
       </c>
-      <c r="F11" s="85"/>
+      <c r="F11" s="85">
+        <v>2</v>
+      </c>
       <c r="G11" s="86"/>
       <c r="H11" s="85"/>
       <c r="I11" s="86"/>
       <c r="J11" s="77">
         <f>IF(C11&gt;C10,1,0)+IF(D11&gt;D10,1,0)+IF(E11&gt;E10,1,0)+IF(F11&gt;F10,1,0)+IF(G11&gt;G10,1,0)+IF(H11&gt;H10,1,0)+IF(I11&gt;I10,1,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K11" s="14"/>
       <c r="L11" s="4"/>
@@ -15235,7 +15242,9 @@
       <c r="F20" s="85">
         <v>2</v>
       </c>
-      <c r="G20" s="85"/>
+      <c r="G20" s="85">
+        <v>2</v>
+      </c>
       <c r="H20" s="85"/>
       <c r="I20" s="86"/>
       <c r="J20" s="77">
@@ -15293,12 +15302,14 @@
       <c r="F21" s="85">
         <v>1</v>
       </c>
-      <c r="G21" s="85"/>
+      <c r="G21" s="85">
+        <v>3</v>
+      </c>
       <c r="H21" s="85"/>
       <c r="I21" s="86"/>
       <c r="J21" s="77">
         <f>IF(C21&gt;C20,1,0)+IF(D21&gt;D20,1,0)+IF(E21&gt;E20,1,0)+IF(F21&gt;F20,1,0)+IF(G21&gt;G20,1,0)+IF(H21&gt;H20,1,0)+IF(I21&gt;I20,1,0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K21" s="55"/>
       <c r="L21" s="4"/>
@@ -15581,12 +15592,14 @@
       <c r="F27" s="86">
         <v>0</v>
       </c>
-      <c r="G27" s="85"/>
+      <c r="G27" s="85">
+        <v>5</v>
+      </c>
       <c r="H27" s="86"/>
       <c r="I27" s="85"/>
       <c r="J27" s="77">
         <f>IF(C27&gt;C28,1,0)+IF(D27&gt;D28,1,0)+IF(E27&gt;E28,1,0)+IF(F27&gt;F28,1,0)+IF(G27&gt;G28,1,0)+IF(H27&gt;H28,1,0)+IF(I27&gt;I28,1,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K27" s="16"/>
       <c r="L27" s="4"/>
@@ -15628,7 +15641,9 @@
       <c r="F28" s="86">
         <v>5</v>
       </c>
-      <c r="G28" s="85"/>
+      <c r="G28" s="85">
+        <v>2</v>
+      </c>
       <c r="H28" s="86"/>
       <c r="I28" s="85"/>
       <c r="J28" s="77">
@@ -15719,102 +15734,102 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C3:I3 C6:I6 O20:U20 C13:I13 AA8:AG8 AA15:AG15 O10:U10 O6:Q6 C10:I10 C24 C20:E20 C17:I17 O24:U24 AA22:AG22 F24:I24 G20:I20 C27:I27 S6:U6">
-    <cfRule type="cellIs" dxfId="100" priority="27" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="27" stopIfTrue="1" operator="greaterThan">
       <formula>C4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:I4 C7:I7 O21:U21 C14:I14 AA9:AG9 AA16:AG16 O11:U11 O7:Q7 C11:I11 C25 C21:E21 C18:I18 O25:U25 AA23:AG23 F25:I25 G21:I21 C28:I28 S7:U7">
-    <cfRule type="cellIs" dxfId="99" priority="28" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="28" stopIfTrue="1" operator="greaterThan">
       <formula>C3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:I3 C6:I6 O20:U20 C13:I13 AA8:AG8 AA15:AG15 O10:U10 O6:Q6 C10:I10 C24 C20:E20 C17:I17 O24:U24 AA22:AG22 F24:I24 G20:I20 C27:I27 S6:U6">
-    <cfRule type="cellIs" dxfId="98" priority="18" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="18" stopIfTrue="1" operator="greaterThan">
       <formula>C4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:I4 C7:I7 O21:U21 C14:I14 AA9:AG9 AA16:AG16 O11:U11 O7:Q7 C11:I11 C25 C21:E21 C18:I18 O25:U25 AA23:AG23 F25:I25 G21:I21 C28:I28 S7:U7">
-    <cfRule type="cellIs" dxfId="97" priority="17" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="17" stopIfTrue="1" operator="greaterThan">
       <formula>C3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24">
-    <cfRule type="cellIs" dxfId="96" priority="15" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="15" stopIfTrue="1" operator="greaterThan">
       <formula>D25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25">
-    <cfRule type="cellIs" dxfId="95" priority="16" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="16" stopIfTrue="1" operator="greaterThan">
       <formula>D24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24">
-    <cfRule type="cellIs" dxfId="94" priority="14" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="14" stopIfTrue="1" operator="greaterThan">
       <formula>D25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25">
-    <cfRule type="cellIs" dxfId="93" priority="13" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="13" stopIfTrue="1" operator="greaterThan">
       <formula>D24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="92" priority="11" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="11" stopIfTrue="1" operator="greaterThan">
       <formula>E25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="91" priority="12" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="12" stopIfTrue="1" operator="greaterThan">
       <formula>E24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="90" priority="10" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="10" stopIfTrue="1" operator="greaterThan">
       <formula>E25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="89" priority="9" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="9" stopIfTrue="1" operator="greaterThan">
       <formula>E24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20">
-    <cfRule type="cellIs" dxfId="88" priority="7" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="greaterThan">
       <formula>F21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21">
-    <cfRule type="cellIs" dxfId="87" priority="8" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="8" stopIfTrue="1" operator="greaterThan">
       <formula>F20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20">
-    <cfRule type="cellIs" dxfId="86" priority="6" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="6" stopIfTrue="1" operator="greaterThan">
       <formula>F21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21">
-    <cfRule type="cellIs" dxfId="85" priority="5" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="greaterThan">
       <formula>F20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R6">
-    <cfRule type="cellIs" dxfId="84" priority="3" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="greaterThan">
       <formula>R7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7">
-    <cfRule type="cellIs" dxfId="83" priority="4" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="greaterThan">
       <formula>R6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R6">
-    <cfRule type="cellIs" dxfId="82" priority="2" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="greaterThan">
       <formula>R7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7">
-    <cfRule type="cellIs" dxfId="81" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>R6</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated games of 2019-04-21
</commit_message>
<xml_diff>
--- a/laval.xlsx
+++ b/laval.xlsx
@@ -2489,30 +2489,132 @@
     <xf numFmtId="0" fontId="19" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="107" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="87" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="95" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="86" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="88" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2564,137 +2666,35 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="86" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="87" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="88" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="95" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="107" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3894,7 +3894,7 @@
   <dimension ref="A1:AL106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="AM8" sqref="AM8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3917,217 +3917,217 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="C1" s="281"/>
-      <c r="D1" s="281"/>
-      <c r="E1" s="281"/>
-      <c r="F1" s="281"/>
-      <c r="G1" s="281"/>
-      <c r="H1" s="281"/>
-      <c r="I1" s="281"/>
-      <c r="J1" s="281"/>
-      <c r="K1" s="281"/>
-      <c r="L1" s="281"/>
-      <c r="M1" s="281"/>
-      <c r="N1" s="281"/>
-      <c r="O1" s="281"/>
-      <c r="P1" s="282"/>
-      <c r="Q1" s="282"/>
-      <c r="R1" s="282"/>
-      <c r="S1" s="282"/>
-      <c r="T1" s="282"/>
-      <c r="U1" s="282"/>
-      <c r="V1" s="282"/>
-      <c r="W1" s="282"/>
-      <c r="X1" s="282"/>
-      <c r="Y1" s="282"/>
-      <c r="Z1" s="282"/>
-      <c r="AA1" s="282"/>
-      <c r="AB1" s="282"/>
-      <c r="AC1" s="282"/>
-      <c r="AD1" s="282"/>
-      <c r="AE1" s="282"/>
-      <c r="AF1" s="282"/>
-      <c r="AG1" s="282"/>
-      <c r="AH1" s="282"/>
-      <c r="AI1" s="282"/>
-      <c r="AJ1" s="282"/>
+      <c r="C1" s="274"/>
+      <c r="D1" s="274"/>
+      <c r="E1" s="274"/>
+      <c r="F1" s="274"/>
+      <c r="G1" s="274"/>
+      <c r="H1" s="274"/>
+      <c r="I1" s="274"/>
+      <c r="J1" s="274"/>
+      <c r="K1" s="274"/>
+      <c r="L1" s="274"/>
+      <c r="M1" s="274"/>
+      <c r="N1" s="274"/>
+      <c r="O1" s="274"/>
+      <c r="P1" s="275"/>
+      <c r="Q1" s="275"/>
+      <c r="R1" s="275"/>
+      <c r="S1" s="275"/>
+      <c r="T1" s="275"/>
+      <c r="U1" s="275"/>
+      <c r="V1" s="275"/>
+      <c r="W1" s="275"/>
+      <c r="X1" s="275"/>
+      <c r="Y1" s="275"/>
+      <c r="Z1" s="275"/>
+      <c r="AA1" s="275"/>
+      <c r="AB1" s="275"/>
+      <c r="AC1" s="275"/>
+      <c r="AD1" s="275"/>
+      <c r="AE1" s="275"/>
+      <c r="AF1" s="275"/>
+      <c r="AG1" s="275"/>
+      <c r="AH1" s="275"/>
+      <c r="AI1" s="275"/>
+      <c r="AJ1" s="275"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="41"/>
-      <c r="C2" s="283" t="s">
+      <c r="C2" s="276" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="283"/>
-      <c r="E2" s="283"/>
-      <c r="F2" s="283"/>
-      <c r="G2" s="283"/>
-      <c r="H2" s="283"/>
-      <c r="I2" s="283"/>
-      <c r="J2" s="283"/>
-      <c r="K2" s="283"/>
-      <c r="L2" s="283"/>
-      <c r="M2" s="283"/>
-      <c r="N2" s="283"/>
-      <c r="O2" s="283"/>
-      <c r="P2" s="283"/>
-      <c r="Q2" s="284" t="s">
+      <c r="D2" s="276"/>
+      <c r="E2" s="276"/>
+      <c r="F2" s="276"/>
+      <c r="G2" s="276"/>
+      <c r="H2" s="276"/>
+      <c r="I2" s="276"/>
+      <c r="J2" s="276"/>
+      <c r="K2" s="276"/>
+      <c r="L2" s="276"/>
+      <c r="M2" s="276"/>
+      <c r="N2" s="276"/>
+      <c r="O2" s="276"/>
+      <c r="P2" s="276"/>
+      <c r="Q2" s="277" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="282"/>
-      <c r="S2" s="282"/>
-      <c r="T2" s="282"/>
-      <c r="U2" s="282"/>
-      <c r="V2" s="282"/>
-      <c r="W2" s="282"/>
-      <c r="X2" s="282"/>
-      <c r="Y2" s="282"/>
-      <c r="Z2" s="282"/>
-      <c r="AA2" s="282"/>
-      <c r="AB2" s="282"/>
-      <c r="AC2" s="282"/>
-      <c r="AD2" s="282"/>
-      <c r="AE2" s="282"/>
-      <c r="AF2" s="282"/>
-      <c r="AG2" s="282"/>
-      <c r="AH2" s="282"/>
-      <c r="AI2" s="282"/>
-      <c r="AJ2" s="282"/>
+      <c r="R2" s="275"/>
+      <c r="S2" s="275"/>
+      <c r="T2" s="275"/>
+      <c r="U2" s="275"/>
+      <c r="V2" s="275"/>
+      <c r="W2" s="275"/>
+      <c r="X2" s="275"/>
+      <c r="Y2" s="275"/>
+      <c r="Z2" s="275"/>
+      <c r="AA2" s="275"/>
+      <c r="AB2" s="275"/>
+      <c r="AC2" s="275"/>
+      <c r="AD2" s="275"/>
+      <c r="AE2" s="275"/>
+      <c r="AF2" s="275"/>
+      <c r="AG2" s="275"/>
+      <c r="AH2" s="275"/>
+      <c r="AI2" s="275"/>
+      <c r="AJ2" s="275"/>
     </row>
     <row r="3" spans="1:38" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="281"/>
-      <c r="D3" s="281"/>
-      <c r="E3" s="281"/>
-      <c r="F3" s="281"/>
-      <c r="G3" s="281"/>
-      <c r="H3" s="281"/>
-      <c r="I3" s="281"/>
-      <c r="J3" s="281"/>
-      <c r="K3" s="281"/>
-      <c r="L3" s="281"/>
-      <c r="M3" s="281"/>
-      <c r="N3" s="281"/>
-      <c r="O3" s="281"/>
-      <c r="P3" s="282"/>
-      <c r="Q3" s="282"/>
-      <c r="R3" s="282"/>
-      <c r="S3" s="282"/>
-      <c r="T3" s="282"/>
-      <c r="U3" s="282"/>
-      <c r="V3" s="282"/>
-      <c r="W3" s="282"/>
-      <c r="X3" s="282"/>
-      <c r="Y3" s="282"/>
-      <c r="Z3" s="282"/>
-      <c r="AA3" s="282"/>
-      <c r="AB3" s="282"/>
-      <c r="AC3" s="282"/>
-      <c r="AD3" s="282"/>
-      <c r="AE3" s="282"/>
-      <c r="AF3" s="282"/>
-      <c r="AG3" s="282"/>
-      <c r="AH3" s="282"/>
-      <c r="AI3" s="282"/>
-      <c r="AJ3" s="282"/>
+      <c r="C3" s="274"/>
+      <c r="D3" s="274"/>
+      <c r="E3" s="274"/>
+      <c r="F3" s="274"/>
+      <c r="G3" s="274"/>
+      <c r="H3" s="274"/>
+      <c r="I3" s="274"/>
+      <c r="J3" s="274"/>
+      <c r="K3" s="274"/>
+      <c r="L3" s="274"/>
+      <c r="M3" s="274"/>
+      <c r="N3" s="274"/>
+      <c r="O3" s="274"/>
+      <c r="P3" s="275"/>
+      <c r="Q3" s="275"/>
+      <c r="R3" s="275"/>
+      <c r="S3" s="275"/>
+      <c r="T3" s="275"/>
+      <c r="U3" s="275"/>
+      <c r="V3" s="275"/>
+      <c r="W3" s="275"/>
+      <c r="X3" s="275"/>
+      <c r="Y3" s="275"/>
+      <c r="Z3" s="275"/>
+      <c r="AA3" s="275"/>
+      <c r="AB3" s="275"/>
+      <c r="AC3" s="275"/>
+      <c r="AD3" s="275"/>
+      <c r="AE3" s="275"/>
+      <c r="AF3" s="275"/>
+      <c r="AG3" s="275"/>
+      <c r="AH3" s="275"/>
+      <c r="AI3" s="275"/>
+      <c r="AJ3" s="275"/>
     </row>
     <row r="4" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="265" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="266"/>
-      <c r="E4" s="266"/>
-      <c r="F4" s="266"/>
-      <c r="G4" s="266"/>
-      <c r="H4" s="266"/>
-      <c r="I4" s="266"/>
-      <c r="J4" s="266"/>
-      <c r="K4" s="266"/>
-      <c r="L4" s="266"/>
-      <c r="M4" s="266"/>
-      <c r="N4" s="266"/>
-      <c r="O4" s="266"/>
-      <c r="P4" s="266"/>
-      <c r="Q4" s="266"/>
-      <c r="R4" s="266"/>
-      <c r="S4" s="267"/>
-      <c r="T4" s="265" t="s">
+      <c r="C4" s="299" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="300"/>
+      <c r="E4" s="300"/>
+      <c r="F4" s="300"/>
+      <c r="G4" s="300"/>
+      <c r="H4" s="300"/>
+      <c r="I4" s="300"/>
+      <c r="J4" s="300"/>
+      <c r="K4" s="300"/>
+      <c r="L4" s="300"/>
+      <c r="M4" s="300"/>
+      <c r="N4" s="300"/>
+      <c r="O4" s="300"/>
+      <c r="P4" s="300"/>
+      <c r="Q4" s="300"/>
+      <c r="R4" s="300"/>
+      <c r="S4" s="301"/>
+      <c r="T4" s="299" t="s">
         <v>1</v>
       </c>
-      <c r="U4" s="266"/>
-      <c r="V4" s="266"/>
-      <c r="W4" s="266"/>
-      <c r="X4" s="266"/>
-      <c r="Y4" s="266"/>
-      <c r="Z4" s="266"/>
-      <c r="AA4" s="266"/>
-      <c r="AB4" s="267"/>
-      <c r="AC4" s="265" t="s">
+      <c r="U4" s="300"/>
+      <c r="V4" s="300"/>
+      <c r="W4" s="300"/>
+      <c r="X4" s="300"/>
+      <c r="Y4" s="300"/>
+      <c r="Z4" s="300"/>
+      <c r="AA4" s="300"/>
+      <c r="AB4" s="301"/>
+      <c r="AC4" s="299" t="s">
         <v>2</v>
       </c>
-      <c r="AD4" s="266"/>
-      <c r="AE4" s="266"/>
-      <c r="AF4" s="266"/>
-      <c r="AG4" s="276"/>
-      <c r="AH4" s="265" t="s">
+      <c r="AD4" s="300"/>
+      <c r="AE4" s="300"/>
+      <c r="AF4" s="300"/>
+      <c r="AG4" s="308"/>
+      <c r="AH4" s="299" t="s">
         <v>10</v>
       </c>
-      <c r="AI4" s="266"/>
-      <c r="AJ4" s="267"/>
+      <c r="AI4" s="300"/>
+      <c r="AJ4" s="301"/>
     </row>
     <row r="5" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="277" t="s">
+      <c r="C5" s="268" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="273"/>
-      <c r="E5" s="273"/>
-      <c r="F5" s="273"/>
-      <c r="G5" s="273"/>
-      <c r="H5" s="273"/>
-      <c r="I5" s="273"/>
-      <c r="J5" s="274"/>
-      <c r="K5" s="272" t="s">
+      <c r="D5" s="269"/>
+      <c r="E5" s="269"/>
+      <c r="F5" s="269"/>
+      <c r="G5" s="269"/>
+      <c r="H5" s="269"/>
+      <c r="I5" s="269"/>
+      <c r="J5" s="270"/>
+      <c r="K5" s="306" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="273"/>
-      <c r="M5" s="273"/>
-      <c r="N5" s="273"/>
-      <c r="O5" s="273"/>
-      <c r="P5" s="273"/>
-      <c r="Q5" s="273"/>
-      <c r="R5" s="274"/>
-      <c r="S5" s="268" t="s">
+      <c r="L5" s="269"/>
+      <c r="M5" s="269"/>
+      <c r="N5" s="269"/>
+      <c r="O5" s="269"/>
+      <c r="P5" s="269"/>
+      <c r="Q5" s="269"/>
+      <c r="R5" s="270"/>
+      <c r="S5" s="302" t="s">
         <v>12</v>
       </c>
-      <c r="T5" s="277" t="s">
+      <c r="T5" s="268" t="s">
         <v>9</v>
       </c>
-      <c r="U5" s="273"/>
-      <c r="V5" s="273"/>
-      <c r="W5" s="274"/>
-      <c r="X5" s="272" t="s">
+      <c r="U5" s="269"/>
+      <c r="V5" s="269"/>
+      <c r="W5" s="270"/>
+      <c r="X5" s="306" t="s">
         <v>8</v>
       </c>
-      <c r="Y5" s="273"/>
-      <c r="Z5" s="273"/>
-      <c r="AA5" s="274"/>
-      <c r="AB5" s="268" t="s">
+      <c r="Y5" s="269"/>
+      <c r="Z5" s="269"/>
+      <c r="AA5" s="270"/>
+      <c r="AB5" s="302" t="s">
         <v>13</v>
       </c>
-      <c r="AC5" s="275" t="s">
+      <c r="AC5" s="307" t="s">
         <v>9</v>
       </c>
-      <c r="AD5" s="274"/>
-      <c r="AE5" s="272" t="s">
+      <c r="AD5" s="270"/>
+      <c r="AE5" s="306" t="s">
         <v>8</v>
       </c>
-      <c r="AF5" s="274"/>
-      <c r="AG5" s="268" t="s">
+      <c r="AF5" s="270"/>
+      <c r="AG5" s="302" t="s">
         <v>14</v>
       </c>
       <c r="AH5" s="56"/>
       <c r="AI5" s="25"/>
-      <c r="AJ5" s="268" t="s">
+      <c r="AJ5" s="302" t="s">
         <v>15</v>
       </c>
       <c r="AK5" s="4"/>
@@ -4145,7 +4145,7 @@
       </c>
       <c r="E6" s="172">
         <f>Résultats!$J$6</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F6" s="109">
         <f>Résultats!$J$7</f>
@@ -4179,7 +4179,7 @@
         <f>Résultats!$J$20</f>
         <v>2</v>
       </c>
-      <c r="N6" s="313">
+      <c r="N6" s="253">
         <f>Résultats!$J$21</f>
         <v>4</v>
       </c>
@@ -4193,13 +4193,13 @@
       </c>
       <c r="Q6" s="111">
         <f>Résultats!$J$27</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R6" s="108">
         <f>Résultats!$J$28</f>
         <v>3</v>
       </c>
-      <c r="S6" s="269"/>
+      <c r="S6" s="303"/>
       <c r="T6" s="169">
         <f>Résultats!$V$6</f>
         <v>0</v>
@@ -4232,7 +4232,7 @@
         <f>Résultats!$V$25</f>
         <v>0</v>
       </c>
-      <c r="AB6" s="269"/>
+      <c r="AB6" s="303"/>
       <c r="AC6" s="111">
         <f>Résultats!$AH$8</f>
         <v>0</v>
@@ -4249,7 +4249,7 @@
         <f>Résultats!$AH$23</f>
         <v>0</v>
       </c>
-      <c r="AG6" s="269"/>
+      <c r="AG6" s="303"/>
       <c r="AH6" s="212">
         <f>Résultats!$AH$15</f>
         <v>0</v>
@@ -4258,7 +4258,7 @@
         <f>Résultats!$AH$16</f>
         <v>0</v>
       </c>
-      <c r="AJ6" s="269"/>
+      <c r="AJ6" s="303"/>
       <c r="AK6" s="37"/>
     </row>
     <row r="7" spans="1:38" s="39" customFormat="1" ht="58.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -4279,12 +4279,12 @@
       <c r="K7" s="120"/>
       <c r="L7" s="243"/>
       <c r="M7" s="173"/>
-      <c r="N7" s="314"/>
+      <c r="N7" s="254"/>
       <c r="O7" s="173"/>
       <c r="P7" s="118"/>
       <c r="Q7" s="119"/>
       <c r="R7" s="117"/>
-      <c r="S7" s="269"/>
+      <c r="S7" s="303"/>
       <c r="T7" s="170"/>
       <c r="U7" s="117"/>
       <c r="V7" s="173"/>
@@ -4293,15 +4293,15 @@
       <c r="Y7" s="118"/>
       <c r="Z7" s="119"/>
       <c r="AA7" s="117"/>
-      <c r="AB7" s="269"/>
+      <c r="AB7" s="303"/>
       <c r="AC7" s="119"/>
       <c r="AD7" s="117"/>
       <c r="AE7" s="120"/>
       <c r="AF7" s="117"/>
-      <c r="AG7" s="269"/>
+      <c r="AG7" s="303"/>
       <c r="AH7" s="212"/>
       <c r="AI7" s="112"/>
-      <c r="AJ7" s="269"/>
+      <c r="AJ7" s="303"/>
       <c r="AK7" s="37"/>
     </row>
     <row r="8" spans="1:38" s="39" customFormat="1" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4351,7 +4351,7 @@
         <f>Résultats!$B$20</f>
         <v>WINNIPEG</v>
       </c>
-      <c r="N8" s="315" t="str">
+      <c r="N8" s="255" t="str">
         <f>Résultats!$B$21</f>
         <v>ST-LOUIS</v>
       </c>
@@ -4371,7 +4371,7 @@
         <f>Résultats!$B$28</f>
         <v>VEGAS</v>
       </c>
-      <c r="S8" s="269"/>
+      <c r="S8" s="303"/>
       <c r="T8" s="171" t="str">
         <f>Résultats!$N$6</f>
         <v xml:space="preserve"> </v>
@@ -4404,7 +4404,7 @@
         <f>Résultats!$N$25</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AB8" s="269"/>
+      <c r="AB8" s="303"/>
       <c r="AC8" s="177" t="str">
         <f>Résultats!$Z$8</f>
         <v xml:space="preserve"> </v>
@@ -4421,7 +4421,7 @@
         <f>Résultats!$Z$23</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AG8" s="269"/>
+      <c r="AG8" s="303"/>
       <c r="AH8" s="213" t="str">
         <f>Résultats!$Z$15</f>
         <v xml:space="preserve"> </v>
@@ -4430,7 +4430,7 @@
         <f>Résultats!$Z$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ8" s="269"/>
+      <c r="AJ8" s="303"/>
       <c r="AK8" s="37"/>
     </row>
     <row r="9" spans="1:38" s="39" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4484,7 +4484,7 @@
         <f>Résultats!$A$20</f>
         <v>C2</v>
       </c>
-      <c r="N9" s="316" t="str">
+      <c r="N9" s="256" t="str">
         <f>Résultats!$A$21</f>
         <v>C3</v>
       </c>
@@ -4504,7 +4504,7 @@
         <f>Résultats!$A$28</f>
         <v>P3</v>
       </c>
-      <c r="S9" s="271"/>
+      <c r="S9" s="305"/>
       <c r="T9" s="179" t="str">
         <f>Résultats!$M$6</f>
         <v xml:space="preserve"> </v>
@@ -4537,7 +4537,7 @@
         <f>Résultats!$M$25</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AB9" s="270"/>
+      <c r="AB9" s="304"/>
       <c r="AC9" s="183" t="str">
         <f>Résultats!$Y$8</f>
         <v xml:space="preserve"> </v>
@@ -4554,7 +4554,7 @@
         <f>Résultats!$Y$23</f>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="AG9" s="270"/>
+      <c r="AG9" s="304"/>
       <c r="AH9" s="215" t="str">
         <f>Résultats!$Y$15</f>
         <v xml:space="preserve"> </v>
@@ -4563,7 +4563,7 @@
         <f>Résultats!$Y$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ9" s="271"/>
+      <c r="AJ9" s="305"/>
       <c r="AK9" s="114" t="s">
         <v>51</v>
       </c>
@@ -5009,7 +5009,7 @@
       <c r="R14" s="50"/>
       <c r="S14" s="129">
         <f>SUM(C15:R15)</f>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="T14" s="46"/>
       <c r="U14" s="47"/>
@@ -5039,11 +5039,11 @@
       </c>
       <c r="AK14" s="116">
         <f>MAX($AL$10:$AL$97) - AL14</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AL14" s="129">
         <f>$S14+$AB14+$AG14+$AJ14</f>
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5059,7 +5059,7 @@
       <c r="D15" s="150"/>
       <c r="E15" s="132">
         <f>(IF($E14&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E14=$E$6+$F$6,$O$103,0),0),0)+IF($F14&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F14=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F15" s="150"/>
       <c r="G15" s="132">
@@ -5089,7 +5089,7 @@
       <c r="P15" s="150"/>
       <c r="Q15" s="126">
         <f>(IF($Q14&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q14=$Q$6+$R$6,$O$103,0),0),0)+IF($R14&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R14=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R15" s="153"/>
       <c r="S15" s="154"/>
@@ -5406,9 +5406,9 @@
       <c r="R18" s="204">
         <v>7</v>
       </c>
-      <c r="S18" s="255">
+      <c r="S18" s="248">
         <f>SUM(C19:R19)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T18" s="198"/>
       <c r="U18" s="202"/>
@@ -5438,11 +5438,11 @@
       </c>
       <c r="AK18" s="207">
         <f>MAX($AL$10:$AL$97) - AL18</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AL18" s="205">
         <f>$S18+$AB18+$AG18+$AJ18</f>
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5458,7 +5458,7 @@
       <c r="D19" s="150"/>
       <c r="E19" s="126">
         <f>(IF($E18&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E18=$E$6+$F$6,$O$103,0),0),0)+IF($F18&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F18=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F19" s="150"/>
       <c r="G19" s="126">
@@ -5807,7 +5807,7 @@
       </c>
       <c r="S22" s="129">
         <f>SUM(C23:R23)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="T22" s="46"/>
       <c r="U22" s="47"/>
@@ -5837,11 +5837,11 @@
       </c>
       <c r="AK22" s="116">
         <f>MAX($AL$10:$AL$97) - AL22</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AL22" s="129">
         <f>$S22+$AB22+$AG22+$AJ22</f>
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5857,7 +5857,7 @@
       <c r="D23" s="163"/>
       <c r="E23" s="132">
         <f>(IF($E22&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E22=$E$6+$F$6,$O$103,0),0),0)+IF($F22&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F22=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F23" s="163"/>
       <c r="G23" s="132">
@@ -6170,43 +6170,43 @@
         <v>4</v>
       </c>
       <c r="B26" s="211" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="C26" s="198">
         <v>5</v>
       </c>
       <c r="D26" s="199"/>
       <c r="E26" s="200">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F26" s="199"/>
       <c r="G26" s="201">
         <v>5</v>
       </c>
       <c r="H26" s="202"/>
-      <c r="I26" s="200"/>
-      <c r="J26" s="202">
+      <c r="I26" s="200">
         <v>6</v>
       </c>
+      <c r="J26" s="202"/>
       <c r="K26" s="203">
         <v>5</v>
       </c>
       <c r="L26" s="202"/>
-      <c r="M26" s="200"/>
-      <c r="N26" s="199">
+      <c r="M26" s="200">
         <v>6</v>
       </c>
+      <c r="N26" s="199"/>
       <c r="O26" s="200">
         <v>5</v>
       </c>
       <c r="P26" s="199"/>
-      <c r="Q26" s="201"/>
-      <c r="R26" s="204">
-        <v>6</v>
-      </c>
+      <c r="Q26" s="201">
+        <v>7</v>
+      </c>
+      <c r="R26" s="204"/>
       <c r="S26" s="205">
         <f>SUM(C27:R27)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="T26" s="198"/>
       <c r="U26" s="202"/>
@@ -6214,7 +6214,7 @@
       <c r="W26" s="202"/>
       <c r="X26" s="203"/>
       <c r="Y26" s="199"/>
-      <c r="Z26" s="201"/>
+      <c r="Z26" s="208"/>
       <c r="AA26" s="204"/>
       <c r="AB26" s="205">
         <f>SUM(T27:AA27)</f>
@@ -6228,7 +6228,7 @@
         <f>SUM(AC27:AF27)</f>
         <v>0</v>
       </c>
-      <c r="AH26" s="308"/>
+      <c r="AH26" s="195"/>
       <c r="AI26" s="196"/>
       <c r="AJ26" s="205">
         <f>AH27</f>
@@ -6236,11 +6236,11 @@
       </c>
       <c r="AK26" s="207">
         <f>MAX($AL$10:$AL$97) - AL26</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AL26" s="205">
         <f>$S26+$AB26+$AG26+$AJ26</f>
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6256,7 +6256,7 @@
       <c r="D27" s="150"/>
       <c r="E27" s="126">
         <f>(IF($E26&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E26=$E$6+$F$6,$O$103,0),0),0)+IF($F26&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F26=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F27" s="150"/>
       <c r="G27" s="126">
@@ -6266,7 +6266,7 @@
       <c r="H27" s="150"/>
       <c r="I27" s="126">
         <f>(IF($I26&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I26=$I$6+$J$6,$O$103,0),0),0)+IF($J26&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J26=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J27" s="151"/>
       <c r="K27" s="152">
@@ -6276,7 +6276,7 @@
       <c r="L27" s="150"/>
       <c r="M27" s="126">
         <f>(IF($M26&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M26=$M$6+$N$6,$O$103,0),0),0)+IF($N26&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N26=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="N27" s="150"/>
       <c r="O27" s="126">
@@ -6358,7 +6358,7 @@
         <f>IF(ISBLANK(I26),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" s="124">
         <f>IF(ISBLANK(J26),
@@ -6388,7 +6388,7 @@
         <f>IF(ISBLANK(N26),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O28" s="124">
         <f>IF(ISBLANK(O26),
@@ -6513,7 +6513,7 @@
         <f>IF(N28 = 0,
 0,
 IF(N26 = (M$6+N$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O29" s="124">
         <f>IF(O28 = 0,
@@ -6559,7 +6559,7 @@
       <c r="AJ29" s="147"/>
       <c r="AK29" s="148">
         <f>SUM(C29:AI29)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL29" s="130"/>
     </row>
@@ -6569,23 +6569,23 @@
         <v>4</v>
       </c>
       <c r="B30" s="88" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="C30" s="46">
         <v>5</v>
       </c>
       <c r="D30" s="45"/>
       <c r="E30" s="44">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F30" s="45"/>
       <c r="G30" s="48">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H30" s="47"/>
       <c r="I30" s="44"/>
       <c r="J30" s="47">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K30" s="49">
         <v>5</v>
@@ -6596,7 +6596,7 @@
         <v>6</v>
       </c>
       <c r="O30" s="44">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P30" s="45"/>
       <c r="Q30" s="48"/>
@@ -6605,7 +6605,7 @@
       </c>
       <c r="S30" s="129">
         <f>SUM(C31:R31)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="T30" s="46"/>
       <c r="U30" s="47"/>
@@ -6627,7 +6627,7 @@
         <f>SUM(AC31:AF31)</f>
         <v>0</v>
       </c>
-      <c r="AH30" s="107"/>
+      <c r="AH30" s="249"/>
       <c r="AI30" s="57"/>
       <c r="AJ30" s="129">
         <f>AH31</f>
@@ -6635,11 +6635,11 @@
       </c>
       <c r="AK30" s="116">
         <f>MAX($AL$10:$AL$97) - AL30</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AL30" s="129">
         <f>$S30+$AB30+$AG30+$AJ30</f>
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6655,7 +6655,7 @@
       <c r="D31" s="80"/>
       <c r="E31" s="81">
         <f>(IF($E30&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E30=$E$6+$F$6,$O$103,0),0),0)+IF($F30&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F30=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F31" s="80"/>
       <c r="G31" s="81">
@@ -6965,10 +6965,10 @@
     <row r="34" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="186">
         <f>RANK(AL34,$AL$10:$AL$97,)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B34" s="211" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C34" s="198">
         <v>5</v>
@@ -6979,32 +6979,32 @@
       </c>
       <c r="F34" s="199"/>
       <c r="G34" s="201">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H34" s="202"/>
-      <c r="I34" s="200">
+      <c r="I34" s="200"/>
+      <c r="J34" s="202">
         <v>6</v>
       </c>
-      <c r="J34" s="202"/>
       <c r="K34" s="203">
         <v>5</v>
       </c>
       <c r="L34" s="202"/>
-      <c r="M34" s="200">
+      <c r="M34" s="200"/>
+      <c r="N34" s="199">
         <v>6</v>
       </c>
-      <c r="N34" s="199"/>
       <c r="O34" s="200">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P34" s="199"/>
       <c r="Q34" s="201">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="R34" s="204"/>
       <c r="S34" s="205">
         <f>SUM(C35:R35)</f>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="T34" s="198"/>
       <c r="U34" s="202"/>
@@ -7012,7 +7012,7 @@
       <c r="W34" s="202"/>
       <c r="X34" s="203"/>
       <c r="Y34" s="199"/>
-      <c r="Z34" s="208"/>
+      <c r="Z34" s="201"/>
       <c r="AA34" s="202"/>
       <c r="AB34" s="205">
         <f>SUM(T35:AA35)</f>
@@ -7026,7 +7026,7 @@
         <f>SUM(AC35:AF35)</f>
         <v>0</v>
       </c>
-      <c r="AH34" s="209"/>
+      <c r="AH34" s="309"/>
       <c r="AI34" s="196"/>
       <c r="AJ34" s="205">
         <f>AH35</f>
@@ -7034,11 +7034,11 @@
       </c>
       <c r="AK34" s="207">
         <f>MAX($AL$10:$AL$97) - AL34</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="AL34" s="205">
         <f>$S34+$AB34+$AG34+$AJ34</f>
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7054,7 +7054,7 @@
       <c r="D35" s="80"/>
       <c r="E35" s="81">
         <f>(IF($E34&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E34=$E$6+$F$6,$O$103,0),0),0)+IF($F34&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F34=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F35" s="80"/>
       <c r="G35" s="81">
@@ -7064,7 +7064,7 @@
       <c r="H35" s="80"/>
       <c r="I35" s="81">
         <f>(IF($I34&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I34=$I$6+$J$6,$O$103,0),0),0)+IF($J34&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J34=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J35" s="82"/>
       <c r="K35" s="83">
@@ -7074,7 +7074,7 @@
       <c r="L35" s="80"/>
       <c r="M35" s="81">
         <f>(IF($M34&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M34=$M$6+$N$6,$O$103,0),0),0)+IF($N34&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N34=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="N35" s="80"/>
       <c r="O35" s="81">
@@ -7084,7 +7084,7 @@
       <c r="P35" s="80"/>
       <c r="Q35" s="81">
         <f>(IF($Q34&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q34=$Q$6+$R$6,$O$103,0),0),0)+IF($R34&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R34=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R35" s="84"/>
       <c r="S35" s="128"/>
@@ -7156,7 +7156,7 @@
         <f>IF(ISBLANK(I34),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J36" s="124">
         <f>IF(ISBLANK(J34),
@@ -7186,7 +7186,7 @@
         <f>IF(ISBLANK(N34),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O36" s="124">
         <f>IF(ISBLANK(O34),
@@ -7311,7 +7311,7 @@
         <f>IF(N36 = 0,
 0,
 IF(N34 = (M$6+N$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O37" s="124">
         <f>IF(O36 = 0,
@@ -7357,33 +7357,33 @@
       <c r="AJ37" s="147"/>
       <c r="AK37" s="148">
         <f>SUM(C37:AI37)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL37" s="130"/>
     </row>
     <row r="38" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="122">
         <f>RANK(AL38,$AL$10:$AL$97,)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B38" s="88" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C38" s="46">
         <v>5</v>
       </c>
       <c r="D38" s="45"/>
       <c r="E38" s="44">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F38" s="45"/>
       <c r="G38" s="48">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H38" s="47"/>
       <c r="I38" s="44"/>
       <c r="J38" s="47">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K38" s="49">
         <v>5</v>
@@ -7397,13 +7397,13 @@
         <v>7</v>
       </c>
       <c r="P38" s="45"/>
-      <c r="Q38" s="48">
+      <c r="Q38" s="48"/>
+      <c r="R38" s="50">
         <v>6</v>
       </c>
-      <c r="R38" s="50"/>
       <c r="S38" s="129">
         <f>SUM(C39:R39)</f>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="T38" s="46"/>
       <c r="U38" s="47"/>
@@ -7425,7 +7425,7 @@
         <f>SUM(AC39:AF39)</f>
         <v>0</v>
       </c>
-      <c r="AH38" s="309"/>
+      <c r="AH38" s="107"/>
       <c r="AI38" s="57"/>
       <c r="AJ38" s="129">
         <f>AH39</f>
@@ -7433,11 +7433,11 @@
       </c>
       <c r="AK38" s="116">
         <f>MAX($AL$10:$AL$97) - AL38</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="AL38" s="129">
         <f>$S38+$AB38+$AG38+$AJ38</f>
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7453,7 +7453,7 @@
       <c r="D39" s="80"/>
       <c r="E39" s="121">
         <f>(IF($E38&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E38=$E$6+$F$6,$O$103,0),0),0)+IF($F38&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F38=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F39" s="80"/>
       <c r="G39" s="125">
@@ -7483,7 +7483,7 @@
       <c r="P39" s="80"/>
       <c r="Q39" s="81">
         <f>(IF($Q38&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q38=$Q$6+$R$6,$O$103,0),0),0)+IF($R38&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R38=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R39" s="84"/>
       <c r="S39" s="128"/>
@@ -7802,7 +7802,7 @@
       <c r="R42" s="204"/>
       <c r="S42" s="205">
         <f>SUM(C43:R43)</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="T42" s="198"/>
       <c r="U42" s="202"/>
@@ -7832,11 +7832,11 @@
       </c>
       <c r="AK42" s="207">
         <f>MAX($AL$10:$AL$97) - AL42</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AL42" s="205">
         <f>$S42+$AB42+$AG42+$AJ42</f>
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7852,7 +7852,7 @@
       <c r="D43" s="80"/>
       <c r="E43" s="121">
         <f>(IF($E42&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E42=$E$6+$F$6,$O$103,0),0),0)+IF($F42&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F42=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F43" s="80"/>
       <c r="G43" s="81">
@@ -7882,7 +7882,7 @@
       <c r="P43" s="80"/>
       <c r="Q43" s="81">
         <f>(IF($Q42&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q42=$Q$6+$R$6,$O$103,0),0),0)+IF($R42&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R42=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R43" s="84"/>
       <c r="S43" s="128"/>
@@ -8201,7 +8201,7 @@
       <c r="R46" s="50"/>
       <c r="S46" s="129">
         <f>SUM(C47:R47)</f>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="T46" s="46"/>
       <c r="U46" s="47"/>
@@ -8231,11 +8231,11 @@
       </c>
       <c r="AK46" s="116">
         <f>MAX($AL$10:$AL$97) - AL46</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AL46" s="129">
         <f>$S46+$AB46+$AG46+$AJ46</f>
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="47" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -8251,7 +8251,7 @@
       <c r="D47" s="80"/>
       <c r="E47" s="81">
         <f>(IF($E46&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E46=$E$6+$F$6,$O$103,0),0),0)+IF($F46&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F46=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F47" s="80"/>
       <c r="G47" s="81">
@@ -8281,7 +8281,7 @@
       <c r="P47" s="80"/>
       <c r="Q47" s="81">
         <f>(IF($Q46&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q46=$Q$6+$R$6,$O$103,0),0),0)+IF($R46&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R46=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R47" s="84"/>
       <c r="S47" s="128"/>
@@ -8561,7 +8561,7 @@
     <row r="50" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="186">
         <f>RANK(AL50,$AL$10:$AL$97,)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B50" s="211" t="s">
         <v>73</v>
@@ -8600,7 +8600,7 @@
       </c>
       <c r="S50" s="205">
         <f>SUM(C51:R51)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="T50" s="198"/>
       <c r="U50" s="202"/>
@@ -8630,11 +8630,11 @@
       </c>
       <c r="AK50" s="207">
         <f>MAX($AL$10:$AL$97) - AL50</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AL50" s="205">
         <f>$S50+$AB50+$AG50+$AJ50</f>
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="51" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -8650,7 +8650,7 @@
       <c r="D51" s="134"/>
       <c r="E51" s="132">
         <f>(IF($E50&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E50=$E$6+$F$6,$O$103,0),0),0)+IF($F50&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F50=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F51" s="134"/>
       <c r="G51" s="132">
@@ -9356,18 +9356,18 @@
         <v>12</v>
       </c>
       <c r="B58" s="211" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="C58" s="198">
+        <v>4</v>
+      </c>
+      <c r="D58" s="199"/>
+      <c r="E58" s="200">
+        <v>4</v>
+      </c>
+      <c r="F58" s="199"/>
+      <c r="G58" s="201">
         <v>6</v>
-      </c>
-      <c r="D58" s="199"/>
-      <c r="E58" s="200"/>
-      <c r="F58" s="199">
-        <v>7</v>
-      </c>
-      <c r="G58" s="201">
-        <v>7</v>
       </c>
       <c r="H58" s="202"/>
       <c r="I58" s="200"/>
@@ -9379,11 +9379,11 @@
       </c>
       <c r="L58" s="202"/>
       <c r="M58" s="200">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="N58" s="199"/>
       <c r="O58" s="200">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P58" s="199"/>
       <c r="Q58" s="201"/>
@@ -9400,14 +9400,14 @@
       <c r="W58" s="202"/>
       <c r="X58" s="203"/>
       <c r="Y58" s="199"/>
-      <c r="Z58" s="201"/>
+      <c r="Z58" s="208"/>
       <c r="AA58" s="202"/>
       <c r="AB58" s="205">
         <f>SUM(T59:AA59)</f>
         <v>0</v>
       </c>
       <c r="AC58" s="201"/>
-      <c r="AD58" s="202"/>
+      <c r="AD58" s="234"/>
       <c r="AE58" s="203"/>
       <c r="AF58" s="202"/>
       <c r="AG58" s="205">
@@ -9752,10 +9752,10 @@
         <v>12</v>
       </c>
       <c r="B62" s="88" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C62" s="46">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D62" s="45"/>
       <c r="E62" s="44"/>
@@ -9763,34 +9763,34 @@
         <v>7</v>
       </c>
       <c r="G62" s="48">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H62" s="47"/>
       <c r="I62" s="44"/>
       <c r="J62" s="47">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K62" s="49">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L62" s="47"/>
       <c r="M62" s="44">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N62" s="45"/>
       <c r="O62" s="44">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P62" s="45"/>
       <c r="Q62" s="48"/>
       <c r="R62" s="50">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S62" s="129">
         <f>SUM(C63:R63)</f>
         <v>14</v>
       </c>
-      <c r="T62" s="236"/>
+      <c r="T62" s="46"/>
       <c r="U62" s="47"/>
       <c r="V62" s="44"/>
       <c r="W62" s="47"/>
@@ -10145,46 +10145,46 @@
     <row r="66" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="186">
         <f>RANK(AL66,$AL$10:$AL$97,)</f>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B66" s="211" t="s">
-        <v>67</v>
-      </c>
-      <c r="C66" s="198">
-        <v>4</v>
-      </c>
-      <c r="D66" s="199"/>
-      <c r="E66" s="200">
-        <v>4</v>
-      </c>
-      <c r="F66" s="199"/>
-      <c r="G66" s="201">
+        <v>68</v>
+      </c>
+      <c r="C66" s="310">
+        <v>5</v>
+      </c>
+      <c r="D66" s="311"/>
+      <c r="E66" s="312">
         <v>6</v>
       </c>
-      <c r="H66" s="202"/>
-      <c r="I66" s="200"/>
-      <c r="J66" s="202">
+      <c r="F66" s="311"/>
+      <c r="G66" s="313">
+        <v>5</v>
+      </c>
+      <c r="H66" s="314"/>
+      <c r="I66" s="312"/>
+      <c r="J66" s="314">
         <v>6</v>
       </c>
-      <c r="K66" s="203">
+      <c r="K66" s="315">
         <v>6</v>
       </c>
-      <c r="L66" s="202"/>
-      <c r="M66" s="200">
-        <v>5</v>
-      </c>
-      <c r="N66" s="199"/>
-      <c r="O66" s="200">
+      <c r="L66" s="314"/>
+      <c r="M66" s="312">
+        <v>7</v>
+      </c>
+      <c r="N66" s="311"/>
+      <c r="O66" s="312">
         <v>6</v>
       </c>
-      <c r="P66" s="199"/>
-      <c r="Q66" s="201"/>
-      <c r="R66" s="204">
+      <c r="P66" s="311"/>
+      <c r="Q66" s="313"/>
+      <c r="R66" s="316">
         <v>6</v>
       </c>
       <c r="S66" s="205">
         <f>SUM(C67:R67)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T66" s="198"/>
       <c r="U66" s="202"/>
@@ -10192,14 +10192,14 @@
       <c r="W66" s="202"/>
       <c r="X66" s="203"/>
       <c r="Y66" s="199"/>
-      <c r="Z66" s="208"/>
+      <c r="Z66" s="201"/>
       <c r="AA66" s="202"/>
       <c r="AB66" s="205">
         <f>SUM(T67:AA67)</f>
         <v>0</v>
       </c>
       <c r="AC66" s="201"/>
-      <c r="AD66" s="234"/>
+      <c r="AD66" s="202"/>
       <c r="AE66" s="203"/>
       <c r="AF66" s="202"/>
       <c r="AG66" s="205">
@@ -10214,11 +10214,11 @@
       </c>
       <c r="AK66" s="207">
         <f>MAX($AL$10:$AL$97) - AL66</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AL66" s="205">
         <f>$S66+$AB66+$AG66+$AJ66</f>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="67" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -10234,7 +10234,7 @@
       <c r="D67" s="134"/>
       <c r="E67" s="132">
         <f>(IF($E66&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E66=$E$6+$F$6,$O$103,0),0),0)+IF($F66&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F66=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F67" s="134"/>
       <c r="G67" s="132">
@@ -10541,48 +10541,48 @@
     <row r="70" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="122">
         <f>RANK(AL70,$AL$10:$AL$97,)</f>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B70" s="88" t="s">
-        <v>68</v>
-      </c>
-      <c r="C70" s="248">
+        <v>78</v>
+      </c>
+      <c r="C70" s="46">
         <v>5</v>
       </c>
-      <c r="D70" s="249"/>
-      <c r="E70" s="250">
+      <c r="D70" s="45"/>
+      <c r="E70" s="44"/>
+      <c r="F70" s="45">
+        <v>7</v>
+      </c>
+      <c r="G70" s="48">
         <v>6</v>
       </c>
-      <c r="F70" s="249"/>
-      <c r="G70" s="251">
+      <c r="H70" s="47"/>
+      <c r="I70" s="44"/>
+      <c r="J70" s="47">
+        <v>7</v>
+      </c>
+      <c r="K70" s="49">
         <v>5</v>
       </c>
-      <c r="H70" s="252"/>
-      <c r="I70" s="250"/>
-      <c r="J70" s="252">
+      <c r="L70" s="47"/>
+      <c r="M70" s="44">
         <v>6</v>
       </c>
-      <c r="K70" s="253">
-        <v>6</v>
-      </c>
-      <c r="L70" s="252"/>
-      <c r="M70" s="250">
+      <c r="N70" s="45"/>
+      <c r="O70" s="44">
         <v>7</v>
       </c>
-      <c r="N70" s="249"/>
-      <c r="O70" s="250">
-        <v>6</v>
-      </c>
-      <c r="P70" s="249"/>
-      <c r="Q70" s="251"/>
-      <c r="R70" s="254">
-        <v>6</v>
+      <c r="P70" s="45"/>
+      <c r="Q70" s="48"/>
+      <c r="R70" s="50">
+        <v>7</v>
       </c>
       <c r="S70" s="129">
         <f>SUM(C71:R71)</f>
-        <v>13</v>
-      </c>
-      <c r="T70" s="46"/>
+        <v>14</v>
+      </c>
+      <c r="T70" s="236"/>
       <c r="U70" s="47"/>
       <c r="V70" s="44"/>
       <c r="W70" s="47"/>
@@ -10610,11 +10610,11 @@
       </c>
       <c r="AK70" s="116">
         <f>MAX($AL$10:$AL$97) - AL70</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AL70" s="129">
         <f>$S70+$AB70+$AG70+$AJ70</f>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -10630,7 +10630,7 @@
       <c r="D71" s="134"/>
       <c r="E71" s="132">
         <f>(IF($E70&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E70=$E$6+$F$6,$O$103,0),0),0)+IF($F70&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F70=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F71" s="134"/>
       <c r="G71" s="132">
@@ -10937,7 +10937,7 @@
     <row r="74" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="186">
         <f>RANK(AL74,$AL$10:$AL$97,)</f>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B74" s="211" t="s">
         <v>82</v>
@@ -10976,7 +10976,7 @@
       </c>
       <c r="S74" s="205">
         <f>SUM(C75:R75)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T74" s="198"/>
       <c r="U74" s="202"/>
@@ -11006,11 +11006,11 @@
       </c>
       <c r="AK74" s="207">
         <f>MAX($AL$10:$AL$97) - AL74</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AL74" s="205">
         <f>$S74+$AB74+$AG74+$AJ74</f>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11026,7 +11026,7 @@
       <c r="D75" s="134"/>
       <c r="E75" s="132">
         <f>(IF($E74&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E74=$E$6+$F$6,$O$103,0),0),0)+IF($F74&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F74=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F75" s="134"/>
       <c r="G75" s="132">
@@ -11333,7 +11333,7 @@
     <row r="78" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="122">
         <f>RANK(AL78,$AL$10:$AL$97,)</f>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B78" s="88" t="s">
         <v>80</v>
@@ -11372,7 +11372,7 @@
       </c>
       <c r="S78" s="129">
         <f>SUM(C79:R79)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T78" s="46"/>
       <c r="U78" s="47"/>
@@ -11402,11 +11402,11 @@
       </c>
       <c r="AK78" s="116">
         <f>MAX($AL$10:$AL$97) - AL78</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AL78" s="129">
         <f>$S78+$AB78+$AG78+$AJ78</f>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11422,7 +11422,7 @@
       <c r="D79" s="134"/>
       <c r="E79" s="132">
         <f>(IF($E78&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E78=$E$6+$F$6,$O$103,0),0),0)+IF($F78&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F78=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F79" s="134"/>
       <c r="G79" s="132">
@@ -11729,7 +11729,7 @@
     <row r="82" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="186">
         <f>RANK(AL82,$AL$10:$AL$97,)</f>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B82" s="211" t="s">
         <v>75</v>
@@ -11768,7 +11768,7 @@
       </c>
       <c r="S82" s="205">
         <f>SUM(C83:R83)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T82" s="198"/>
       <c r="U82" s="202"/>
@@ -11798,11 +11798,11 @@
       </c>
       <c r="AK82" s="207">
         <f>MAX($AL$10:$AL$97) - AL82</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AL82" s="205">
         <f>$S82+$AB82+$AG82+$AJ82</f>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="83" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11818,7 +11818,7 @@
       <c r="D83" s="134"/>
       <c r="E83" s="132">
         <f>(IF($E82&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E82=$E$6+$F$6,$O$103,0),0),0)+IF($F82&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F82=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F83" s="134"/>
       <c r="G83" s="132">
@@ -12125,10 +12125,10 @@
     <row r="86" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="122">
         <f>RANK(AL86,$AL$10:$AL$97,)</f>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B86" s="88" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="C86" s="46">
         <v>6</v>
@@ -12139,12 +12139,12 @@
       </c>
       <c r="F86" s="45"/>
       <c r="G86" s="48">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H86" s="47"/>
       <c r="I86" s="44"/>
       <c r="J86" s="47">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="K86" s="49">
         <v>7</v>
@@ -12155,16 +12155,16 @@
       </c>
       <c r="N86" s="45"/>
       <c r="O86" s="44">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P86" s="45"/>
-      <c r="Q86" s="48"/>
-      <c r="R86" s="50">
-        <v>7</v>
-      </c>
+      <c r="Q86" s="48">
+        <v>5</v>
+      </c>
+      <c r="R86" s="50"/>
       <c r="S86" s="129">
         <f>SUM(C87:R87)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T86" s="46"/>
       <c r="U86" s="47"/>
@@ -12194,11 +12194,11 @@
       </c>
       <c r="AK86" s="116">
         <f>MAX($AL$10:$AL$97) - AL86</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AL86" s="129">
         <f>$S86+$AB86+$AG86+$AJ86</f>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="87" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -12214,7 +12214,7 @@
       <c r="D87" s="134"/>
       <c r="E87" s="132">
         <f>(IF($E86&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E86=$E$6+$F$6,$O$103,0),0),0)+IF($F86&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F86=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F87" s="134"/>
       <c r="G87" s="132">
@@ -12521,10 +12521,10 @@
     <row r="90" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="186">
         <f>RANK(AL90,$AL$10:$AL$97,)</f>
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B90" s="211" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C90" s="198">
         <v>6</v>
@@ -12535,12 +12535,12 @@
       </c>
       <c r="F90" s="199"/>
       <c r="G90" s="201">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H90" s="202"/>
       <c r="I90" s="200"/>
       <c r="J90" s="202">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K90" s="203">
         <v>7</v>
@@ -12551,16 +12551,16 @@
       </c>
       <c r="N90" s="199"/>
       <c r="O90" s="200">
+        <v>6</v>
+      </c>
+      <c r="P90" s="199"/>
+      <c r="Q90" s="201"/>
+      <c r="R90" s="204">
         <v>7</v>
       </c>
-      <c r="P90" s="199"/>
-      <c r="Q90" s="201">
-        <v>5</v>
-      </c>
-      <c r="R90" s="204"/>
       <c r="S90" s="205">
         <f>SUM(C91:R91)</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="T90" s="198"/>
       <c r="U90" s="202"/>
@@ -12590,11 +12590,11 @@
       </c>
       <c r="AK90" s="207">
         <f>MAX($AL$10:$AL$97) - AL90</f>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AL90" s="205">
         <f>$S90+$AB90+$AG90+$AJ90</f>
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -12610,7 +12610,7 @@
       <c r="D91" s="134"/>
       <c r="E91" s="132">
         <f>(IF($E90&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E90=$E$6+$F$6,$O$103,0),0),0)+IF($F90&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F90=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F91" s="134"/>
       <c r="G91" s="132">
@@ -12640,7 +12640,7 @@
       <c r="P91" s="134"/>
       <c r="Q91" s="135">
         <f>(IF($Q90&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q90=$Q$6+$R$6,$O$103,0),0),0)+IF($R90&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R90=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R91" s="138"/>
       <c r="S91" s="128"/>
@@ -12926,15 +12926,15 @@
         <v>7</v>
       </c>
       <c r="D94" s="227"/>
-      <c r="E94" s="310">
+      <c r="E94" s="250">
         <v>6</v>
       </c>
       <c r="F94" s="227"/>
-      <c r="G94" s="311"/>
+      <c r="G94" s="251"/>
       <c r="H94" s="230">
         <v>6</v>
       </c>
-      <c r="I94" s="310"/>
+      <c r="I94" s="250"/>
       <c r="J94" s="230">
         <v>7</v>
       </c>
@@ -12956,11 +12956,11 @@
       <c r="R94" s="232"/>
       <c r="S94" s="129">
         <f>SUM(C95:R95)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="T94" s="46"/>
       <c r="U94" s="47"/>
-      <c r="V94" s="312"/>
+      <c r="V94" s="252"/>
       <c r="W94" s="47"/>
       <c r="X94" s="49"/>
       <c r="Y94" s="127"/>
@@ -12986,11 +12986,11 @@
       </c>
       <c r="AK94" s="116">
         <f>MAX($AL$10:$AL$97) - AL94</f>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AL94" s="218">
         <f>$S94+$AB94+$AG94+$AJ94</f>
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="95" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -13006,7 +13006,7 @@
       <c r="D95" s="134"/>
       <c r="E95" s="132">
         <f>(IF($E94&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E94=$E$6+$F$6,$O$103,0),0),0)+IF($F94&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F94=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F95" s="134"/>
       <c r="G95" s="132">
@@ -13036,7 +13036,7 @@
       <c r="P95" s="134"/>
       <c r="Q95" s="135">
         <f>(IF($Q94&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q94=$Q$6+$R$6,$O$103,0),0),0)+IF($R94&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R94=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R95" s="138"/>
       <c r="S95" s="128"/>
@@ -13443,12 +13443,12 @@
     <row r="100" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B100" s="43"/>
       <c r="N100" s="26"/>
-      <c r="O100" s="256" t="s">
+      <c r="O100" s="290" t="s">
         <v>17</v>
       </c>
-      <c r="P100" s="257"/>
-      <c r="Q100" s="257"/>
-      <c r="R100" s="258"/>
+      <c r="P100" s="291"/>
+      <c r="Q100" s="291"/>
+      <c r="R100" s="292"/>
       <c r="AG100" s="30"/>
       <c r="AH100" s="30"/>
       <c r="AI100" s="30"/>
@@ -13457,21 +13457,21 @@
     </row>
     <row r="101" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="33"/>
-      <c r="B101" s="285" t="s">
+      <c r="B101" s="278" t="s">
         <v>16</v>
       </c>
-      <c r="C101" s="286"/>
-      <c r="D101" s="286"/>
-      <c r="E101" s="286"/>
-      <c r="F101" s="286"/>
-      <c r="G101" s="286"/>
-      <c r="H101" s="286"/>
-      <c r="I101" s="286"/>
-      <c r="J101" s="286"/>
-      <c r="K101" s="286"/>
-      <c r="L101" s="286"/>
-      <c r="M101" s="286"/>
-      <c r="N101" s="287"/>
+      <c r="C101" s="279"/>
+      <c r="D101" s="279"/>
+      <c r="E101" s="279"/>
+      <c r="F101" s="279"/>
+      <c r="G101" s="279"/>
+      <c r="H101" s="279"/>
+      <c r="I101" s="279"/>
+      <c r="J101" s="279"/>
+      <c r="K101" s="279"/>
+      <c r="L101" s="279"/>
+      <c r="M101" s="279"/>
+      <c r="N101" s="280"/>
       <c r="O101" s="21">
         <v>1</v>
       </c>
@@ -13484,45 +13484,45 @@
       <c r="R101" s="22">
         <v>4</v>
       </c>
-      <c r="U101" s="259" t="s">
+      <c r="U101" s="293" t="s">
         <v>26</v>
       </c>
-      <c r="V101" s="260"/>
-      <c r="W101" s="260"/>
-      <c r="X101" s="260"/>
-      <c r="Y101" s="260"/>
-      <c r="Z101" s="260"/>
-      <c r="AA101" s="260"/>
-      <c r="AB101" s="260"/>
-      <c r="AC101" s="260"/>
-      <c r="AD101" s="261"/>
+      <c r="V101" s="294"/>
+      <c r="W101" s="294"/>
+      <c r="X101" s="294"/>
+      <c r="Y101" s="294"/>
+      <c r="Z101" s="294"/>
+      <c r="AA101" s="294"/>
+      <c r="AB101" s="294"/>
+      <c r="AC101" s="294"/>
+      <c r="AD101" s="295"/>
       <c r="AE101" s="28"/>
       <c r="AF101" s="28"/>
-      <c r="AG101" s="262" t="s">
+      <c r="AG101" s="296" t="s">
         <v>24</v>
       </c>
-      <c r="AH101" s="263"/>
-      <c r="AI101" s="263"/>
-      <c r="AJ101" s="263"/>
-      <c r="AK101" s="264"/>
+      <c r="AH101" s="297"/>
+      <c r="AI101" s="297"/>
+      <c r="AJ101" s="297"/>
+      <c r="AK101" s="298"/>
     </row>
     <row r="102" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A102" s="34"/>
-      <c r="B102" s="292" t="s">
+      <c r="B102" s="257" t="s">
         <v>6</v>
       </c>
-      <c r="C102" s="293"/>
-      <c r="D102" s="293"/>
-      <c r="E102" s="293"/>
-      <c r="F102" s="293"/>
-      <c r="G102" s="293"/>
-      <c r="H102" s="293"/>
-      <c r="I102" s="293"/>
-      <c r="J102" s="293"/>
-      <c r="K102" s="293"/>
-      <c r="L102" s="293"/>
-      <c r="M102" s="293"/>
-      <c r="N102" s="294"/>
+      <c r="C102" s="258"/>
+      <c r="D102" s="258"/>
+      <c r="E102" s="258"/>
+      <c r="F102" s="258"/>
+      <c r="G102" s="258"/>
+      <c r="H102" s="258"/>
+      <c r="I102" s="258"/>
+      <c r="J102" s="258"/>
+      <c r="K102" s="258"/>
+      <c r="L102" s="258"/>
+      <c r="M102" s="258"/>
+      <c r="N102" s="259"/>
       <c r="O102" s="20">
         <v>5</v>
       </c>
@@ -13535,49 +13535,49 @@
       <c r="R102" s="23">
         <v>20</v>
       </c>
-      <c r="U102" s="290" t="s">
+      <c r="U102" s="283" t="s">
         <v>20</v>
       </c>
-      <c r="V102" s="291"/>
-      <c r="W102" s="291"/>
-      <c r="X102" s="291"/>
-      <c r="Y102" s="291"/>
-      <c r="Z102" s="291"/>
-      <c r="AA102" s="291"/>
-      <c r="AB102" s="288">
+      <c r="V102" s="284"/>
+      <c r="W102" s="284"/>
+      <c r="X102" s="284"/>
+      <c r="Y102" s="284"/>
+      <c r="Z102" s="284"/>
+      <c r="AA102" s="284"/>
+      <c r="AB102" s="281">
         <v>22</v>
       </c>
-      <c r="AC102" s="288"/>
-      <c r="AD102" s="289"/>
+      <c r="AC102" s="281"/>
+      <c r="AD102" s="282"/>
       <c r="AE102" s="29"/>
       <c r="AF102" s="29"/>
-      <c r="AG102" s="304" t="s">
+      <c r="AG102" s="264" t="s">
         <v>21</v>
       </c>
-      <c r="AH102" s="305"/>
-      <c r="AI102" s="305"/>
-      <c r="AJ102" s="306"/>
+      <c r="AH102" s="265"/>
+      <c r="AI102" s="265"/>
+      <c r="AJ102" s="266"/>
       <c r="AK102" s="223">
         <v>230</v>
       </c>
     </row>
     <row r="103" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="34"/>
-      <c r="B103" s="292" t="s">
+      <c r="B103" s="257" t="s">
         <v>5</v>
       </c>
-      <c r="C103" s="293"/>
-      <c r="D103" s="293"/>
-      <c r="E103" s="293"/>
-      <c r="F103" s="293"/>
-      <c r="G103" s="293"/>
-      <c r="H103" s="293"/>
-      <c r="I103" s="293"/>
-      <c r="J103" s="293"/>
-      <c r="K103" s="293"/>
-      <c r="L103" s="293"/>
-      <c r="M103" s="293"/>
-      <c r="N103" s="294"/>
+      <c r="C103" s="258"/>
+      <c r="D103" s="258"/>
+      <c r="E103" s="258"/>
+      <c r="F103" s="258"/>
+      <c r="G103" s="258"/>
+      <c r="H103" s="258"/>
+      <c r="I103" s="258"/>
+      <c r="J103" s="258"/>
+      <c r="K103" s="258"/>
+      <c r="L103" s="258"/>
+      <c r="M103" s="258"/>
+      <c r="N103" s="259"/>
       <c r="O103" s="20">
         <v>2</v>
       </c>
@@ -13590,49 +13590,49 @@
       <c r="R103" s="23">
         <v>8</v>
       </c>
-      <c r="U103" s="299" t="s">
+      <c r="U103" s="262" t="s">
         <v>18</v>
       </c>
-      <c r="V103" s="300"/>
-      <c r="W103" s="300"/>
-      <c r="X103" s="300"/>
-      <c r="Y103" s="300"/>
-      <c r="Z103" s="300"/>
-      <c r="AA103" s="300"/>
-      <c r="AB103" s="301">
+      <c r="V103" s="263"/>
+      <c r="W103" s="263"/>
+      <c r="X103" s="263"/>
+      <c r="Y103" s="263"/>
+      <c r="Z103" s="263"/>
+      <c r="AA103" s="263"/>
+      <c r="AB103" s="288">
         <v>20</v>
       </c>
-      <c r="AC103" s="301"/>
-      <c r="AD103" s="302"/>
+      <c r="AC103" s="288"/>
+      <c r="AD103" s="289"/>
       <c r="AE103" s="29"/>
       <c r="AF103" s="29"/>
-      <c r="AG103" s="307" t="s">
+      <c r="AG103" s="267" t="s">
         <v>22</v>
       </c>
-      <c r="AH103" s="293"/>
-      <c r="AI103" s="293"/>
-      <c r="AJ103" s="294"/>
+      <c r="AH103" s="258"/>
+      <c r="AI103" s="258"/>
+      <c r="AJ103" s="259"/>
       <c r="AK103" s="36">
         <v>115</v>
       </c>
     </row>
     <row r="104" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="35"/>
-      <c r="B104" s="278" t="s">
+      <c r="B104" s="271" t="s">
         <v>4</v>
       </c>
-      <c r="C104" s="279"/>
-      <c r="D104" s="279"/>
-      <c r="E104" s="279"/>
-      <c r="F104" s="279"/>
-      <c r="G104" s="279"/>
-      <c r="H104" s="279"/>
-      <c r="I104" s="279"/>
-      <c r="J104" s="279"/>
-      <c r="K104" s="279"/>
-      <c r="L104" s="279"/>
-      <c r="M104" s="279"/>
-      <c r="N104" s="280"/>
+      <c r="C104" s="272"/>
+      <c r="D104" s="272"/>
+      <c r="E104" s="272"/>
+      <c r="F104" s="272"/>
+      <c r="G104" s="272"/>
+      <c r="H104" s="272"/>
+      <c r="I104" s="272"/>
+      <c r="J104" s="272"/>
+      <c r="K104" s="272"/>
+      <c r="L104" s="272"/>
+      <c r="M104" s="272"/>
+      <c r="N104" s="273"/>
       <c r="O104" s="3">
         <v>1</v>
       </c>
@@ -13645,51 +13645,51 @@
       <c r="R104" s="24">
         <v>1</v>
       </c>
-      <c r="U104" s="295" t="s">
+      <c r="U104" s="285" t="s">
         <v>19</v>
       </c>
-      <c r="V104" s="296"/>
-      <c r="W104" s="296"/>
-      <c r="X104" s="296"/>
-      <c r="Y104" s="296"/>
-      <c r="Z104" s="296"/>
-      <c r="AA104" s="296"/>
-      <c r="AB104" s="297">
+      <c r="V104" s="261"/>
+      <c r="W104" s="261"/>
+      <c r="X104" s="261"/>
+      <c r="Y104" s="261"/>
+      <c r="Z104" s="261"/>
+      <c r="AA104" s="261"/>
+      <c r="AB104" s="286">
         <f>AB102*AB103</f>
         <v>440</v>
       </c>
-      <c r="AC104" s="297"/>
-      <c r="AD104" s="298"/>
+      <c r="AC104" s="286"/>
+      <c r="AD104" s="287"/>
       <c r="AE104" s="29"/>
       <c r="AF104" s="29"/>
-      <c r="AG104" s="307" t="s">
+      <c r="AG104" s="267" t="s">
         <v>25</v>
       </c>
-      <c r="AH104" s="293"/>
-      <c r="AI104" s="293"/>
-      <c r="AJ104" s="294"/>
+      <c r="AH104" s="258"/>
+      <c r="AI104" s="258"/>
+      <c r="AJ104" s="259"/>
       <c r="AK104" s="36">
         <v>65</v>
       </c>
     </row>
     <row r="105" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG105" s="299" t="s">
+      <c r="AG105" s="262" t="s">
         <v>23</v>
       </c>
-      <c r="AH105" s="300"/>
-      <c r="AI105" s="300"/>
-      <c r="AJ105" s="300"/>
+      <c r="AH105" s="263"/>
+      <c r="AI105" s="263"/>
+      <c r="AJ105" s="263"/>
       <c r="AK105" s="225">
         <v>30</v>
       </c>
     </row>
     <row r="106" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG106" s="303" t="s">
+      <c r="AG106" s="260" t="s">
         <v>19</v>
       </c>
-      <c r="AH106" s="296"/>
-      <c r="AI106" s="296"/>
-      <c r="AJ106" s="296"/>
+      <c r="AH106" s="261"/>
+      <c r="AI106" s="261"/>
+      <c r="AJ106" s="261"/>
       <c r="AK106" s="224">
         <f>SUM(AK102:AK105)</f>
         <v>440</v>
@@ -13701,12 +13701,22 @@
     <sortCondition ref="B10:B94"/>
   </sortState>
   <mergeCells count="38">
-    <mergeCell ref="B103:N103"/>
-    <mergeCell ref="AG106:AJ106"/>
-    <mergeCell ref="AG105:AJ105"/>
-    <mergeCell ref="AG102:AJ102"/>
-    <mergeCell ref="AG104:AJ104"/>
-    <mergeCell ref="AG103:AJ103"/>
+    <mergeCell ref="O100:R100"/>
+    <mergeCell ref="U101:AD101"/>
+    <mergeCell ref="AG101:AK101"/>
+    <mergeCell ref="AH4:AJ4"/>
+    <mergeCell ref="AG5:AG9"/>
+    <mergeCell ref="AJ5:AJ9"/>
+    <mergeCell ref="X5:AA5"/>
+    <mergeCell ref="AB5:AB9"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="C4:S4"/>
+    <mergeCell ref="T4:AB4"/>
+    <mergeCell ref="AC4:AG4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="K5:R5"/>
+    <mergeCell ref="S5:S9"/>
     <mergeCell ref="T5:W5"/>
     <mergeCell ref="B104:N104"/>
     <mergeCell ref="C1:O1"/>
@@ -13723,22 +13733,12 @@
     <mergeCell ref="AB104:AD104"/>
     <mergeCell ref="U103:AA103"/>
     <mergeCell ref="AB103:AD103"/>
-    <mergeCell ref="O100:R100"/>
-    <mergeCell ref="U101:AD101"/>
-    <mergeCell ref="AG101:AK101"/>
-    <mergeCell ref="AH4:AJ4"/>
-    <mergeCell ref="AG5:AG9"/>
-    <mergeCell ref="AJ5:AJ9"/>
-    <mergeCell ref="X5:AA5"/>
-    <mergeCell ref="AB5:AB9"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="C4:S4"/>
-    <mergeCell ref="T4:AB4"/>
-    <mergeCell ref="AC4:AG4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="K5:R5"/>
-    <mergeCell ref="S5:S9"/>
+    <mergeCell ref="B103:N103"/>
+    <mergeCell ref="AG106:AJ106"/>
+    <mergeCell ref="AG105:AJ105"/>
+    <mergeCell ref="AG102:AJ102"/>
+    <mergeCell ref="AG104:AJ104"/>
+    <mergeCell ref="AG103:AJ103"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <conditionalFormatting sqref="AH18:AI18 AH10:AI10 AH14:AI14 T10:AA10 AC10:AF10 C10:R10 C14:R14 T14:AA14 AC14:AF14 T18:AA18 AC18:AF18 AH30:AI30 C30:R30 T30:AA30 AC30:AF30 AH26:AI26 C26:R26 T26:AA26 AC26:AF26 AH62:AI62 C62:R62 T62:AA62 AC62:AF62 AH42:AI42 C42:R42 T42:AA42 AC42:AF42 AH22:AI22 C22:R22 T22:AA22 AC22:AF22 AH38:AI38 C38:R38 T38:AA38 AC38:AF38 AH34:AI34 C34:R34 T34:AA34 AC34:AF34 AH66:AI66 C66:R66 T66:AA66 AC66:AF66 C18:R18">
@@ -14395,7 +14395,7 @@
   <dimension ref="A1:AJ31"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14593,11 +14593,13 @@
       <c r="G6" s="85">
         <v>1</v>
       </c>
-      <c r="H6" s="85"/>
+      <c r="H6" s="85">
+        <v>4</v>
+      </c>
       <c r="I6" s="85"/>
       <c r="J6" s="77">
         <f>IF(C6&gt;C7,1,0)+IF(D6&gt;D7,1,0)+IF(E6&gt;E7,1,0)+IF(F6&gt;F7,1,0)+IF(G6&gt;G7,1,0)+IF(H6&gt;H7,1,0)+IF(I6&gt;I7,1,0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K6" s="16"/>
       <c r="L6" s="13"/>
@@ -14651,7 +14653,9 @@
       <c r="G7" s="85">
         <v>2</v>
       </c>
-      <c r="H7" s="85"/>
+      <c r="H7" s="85">
+        <v>2</v>
+      </c>
       <c r="I7" s="85"/>
       <c r="J7" s="77">
         <f>IF(C7&gt;C6,1,0)+IF(D7&gt;D6,1,0)+IF(E7&gt;E6,1,0)+IF(F7&gt;F6,1,0)+IF(G7&gt;G6,1,0)+IF(H7&gt;H6,1,0)+IF(I7&gt;I6,1,0)</f>
@@ -15624,11 +15628,13 @@
       <c r="G27" s="85">
         <v>5</v>
       </c>
-      <c r="H27" s="86"/>
+      <c r="H27" s="86">
+        <v>2</v>
+      </c>
       <c r="I27" s="85"/>
       <c r="J27" s="77">
         <f>IF(C27&gt;C28,1,0)+IF(D27&gt;D28,1,0)+IF(E27&gt;E28,1,0)+IF(F27&gt;F28,1,0)+IF(G27&gt;G28,1,0)+IF(H27&gt;H28,1,0)+IF(I27&gt;I28,1,0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K27" s="16"/>
       <c r="L27" s="4"/>
@@ -15673,7 +15679,9 @@
       <c r="G28" s="85">
         <v>2</v>
       </c>
-      <c r="H28" s="86"/>
+      <c r="H28" s="86">
+        <v>1</v>
+      </c>
       <c r="I28" s="85"/>
       <c r="J28" s="77">
         <f>IF(C28&gt;C27,1,0)+IF(D28&gt;D27,1,0)+IF(E28&gt;E27,1,0)+IF(F28&gt;F27,1,0)+IF(G28&gt;G27,1,0)+IF(H28&gt;H27,1,0)+IF(I28&gt;I27,1,0)</f>

</xml_diff>

<commit_message>
Updated games of 2019-04-22
</commit_message>
<xml_diff>
--- a/laval.xlsx
+++ b/laval.xlsx
@@ -2447,15 +2447,9 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2495,12 +2489,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2516,6 +2504,117 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="113" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="114" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="95" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2525,18 +2624,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="86" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="87" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="88" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="87" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="95" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2549,151 +2663,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="86" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="88" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="113" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="114" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="95" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3917,217 +3917,217 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="C1" s="274"/>
-      <c r="D1" s="274"/>
-      <c r="E1" s="274"/>
-      <c r="F1" s="274"/>
-      <c r="G1" s="274"/>
-      <c r="H1" s="274"/>
-      <c r="I1" s="274"/>
-      <c r="J1" s="274"/>
-      <c r="K1" s="274"/>
-      <c r="L1" s="274"/>
-      <c r="M1" s="274"/>
-      <c r="N1" s="274"/>
-      <c r="O1" s="274"/>
-      <c r="P1" s="275"/>
-      <c r="Q1" s="275"/>
-      <c r="R1" s="275"/>
-      <c r="S1" s="275"/>
-      <c r="T1" s="275"/>
-      <c r="U1" s="275"/>
-      <c r="V1" s="275"/>
-      <c r="W1" s="275"/>
-      <c r="X1" s="275"/>
-      <c r="Y1" s="275"/>
-      <c r="Z1" s="275"/>
-      <c r="AA1" s="275"/>
-      <c r="AB1" s="275"/>
-      <c r="AC1" s="275"/>
-      <c r="AD1" s="275"/>
-      <c r="AE1" s="275"/>
-      <c r="AF1" s="275"/>
-      <c r="AG1" s="275"/>
-      <c r="AH1" s="275"/>
-      <c r="AI1" s="275"/>
-      <c r="AJ1" s="275"/>
+      <c r="C1" s="279"/>
+      <c r="D1" s="279"/>
+      <c r="E1" s="279"/>
+      <c r="F1" s="279"/>
+      <c r="G1" s="279"/>
+      <c r="H1" s="279"/>
+      <c r="I1" s="279"/>
+      <c r="J1" s="279"/>
+      <c r="K1" s="279"/>
+      <c r="L1" s="279"/>
+      <c r="M1" s="279"/>
+      <c r="N1" s="279"/>
+      <c r="O1" s="279"/>
+      <c r="P1" s="280"/>
+      <c r="Q1" s="280"/>
+      <c r="R1" s="280"/>
+      <c r="S1" s="280"/>
+      <c r="T1" s="280"/>
+      <c r="U1" s="280"/>
+      <c r="V1" s="280"/>
+      <c r="W1" s="280"/>
+      <c r="X1" s="280"/>
+      <c r="Y1" s="280"/>
+      <c r="Z1" s="280"/>
+      <c r="AA1" s="280"/>
+      <c r="AB1" s="280"/>
+      <c r="AC1" s="280"/>
+      <c r="AD1" s="280"/>
+      <c r="AE1" s="280"/>
+      <c r="AF1" s="280"/>
+      <c r="AG1" s="280"/>
+      <c r="AH1" s="280"/>
+      <c r="AI1" s="280"/>
+      <c r="AJ1" s="280"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="41"/>
-      <c r="C2" s="276" t="s">
+      <c r="C2" s="281" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="276"/>
-      <c r="E2" s="276"/>
-      <c r="F2" s="276"/>
-      <c r="G2" s="276"/>
-      <c r="H2" s="276"/>
-      <c r="I2" s="276"/>
-      <c r="J2" s="276"/>
-      <c r="K2" s="276"/>
-      <c r="L2" s="276"/>
-      <c r="M2" s="276"/>
-      <c r="N2" s="276"/>
-      <c r="O2" s="276"/>
-      <c r="P2" s="276"/>
-      <c r="Q2" s="277" t="s">
+      <c r="D2" s="281"/>
+      <c r="E2" s="281"/>
+      <c r="F2" s="281"/>
+      <c r="G2" s="281"/>
+      <c r="H2" s="281"/>
+      <c r="I2" s="281"/>
+      <c r="J2" s="281"/>
+      <c r="K2" s="281"/>
+      <c r="L2" s="281"/>
+      <c r="M2" s="281"/>
+      <c r="N2" s="281"/>
+      <c r="O2" s="281"/>
+      <c r="P2" s="281"/>
+      <c r="Q2" s="282" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="275"/>
-      <c r="S2" s="275"/>
-      <c r="T2" s="275"/>
-      <c r="U2" s="275"/>
-      <c r="V2" s="275"/>
-      <c r="W2" s="275"/>
-      <c r="X2" s="275"/>
-      <c r="Y2" s="275"/>
-      <c r="Z2" s="275"/>
-      <c r="AA2" s="275"/>
-      <c r="AB2" s="275"/>
-      <c r="AC2" s="275"/>
-      <c r="AD2" s="275"/>
-      <c r="AE2" s="275"/>
-      <c r="AF2" s="275"/>
-      <c r="AG2" s="275"/>
-      <c r="AH2" s="275"/>
-      <c r="AI2" s="275"/>
-      <c r="AJ2" s="275"/>
+      <c r="R2" s="280"/>
+      <c r="S2" s="280"/>
+      <c r="T2" s="280"/>
+      <c r="U2" s="280"/>
+      <c r="V2" s="280"/>
+      <c r="W2" s="280"/>
+      <c r="X2" s="280"/>
+      <c r="Y2" s="280"/>
+      <c r="Z2" s="280"/>
+      <c r="AA2" s="280"/>
+      <c r="AB2" s="280"/>
+      <c r="AC2" s="280"/>
+      <c r="AD2" s="280"/>
+      <c r="AE2" s="280"/>
+      <c r="AF2" s="280"/>
+      <c r="AG2" s="280"/>
+      <c r="AH2" s="280"/>
+      <c r="AI2" s="280"/>
+      <c r="AJ2" s="280"/>
     </row>
     <row r="3" spans="1:38" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="274"/>
-      <c r="D3" s="274"/>
-      <c r="E3" s="274"/>
-      <c r="F3" s="274"/>
-      <c r="G3" s="274"/>
-      <c r="H3" s="274"/>
-      <c r="I3" s="274"/>
-      <c r="J3" s="274"/>
-      <c r="K3" s="274"/>
-      <c r="L3" s="274"/>
-      <c r="M3" s="274"/>
-      <c r="N3" s="274"/>
-      <c r="O3" s="274"/>
-      <c r="P3" s="275"/>
-      <c r="Q3" s="275"/>
-      <c r="R3" s="275"/>
-      <c r="S3" s="275"/>
-      <c r="T3" s="275"/>
-      <c r="U3" s="275"/>
-      <c r="V3" s="275"/>
-      <c r="W3" s="275"/>
-      <c r="X3" s="275"/>
-      <c r="Y3" s="275"/>
-      <c r="Z3" s="275"/>
-      <c r="AA3" s="275"/>
-      <c r="AB3" s="275"/>
-      <c r="AC3" s="275"/>
-      <c r="AD3" s="275"/>
-      <c r="AE3" s="275"/>
-      <c r="AF3" s="275"/>
-      <c r="AG3" s="275"/>
-      <c r="AH3" s="275"/>
-      <c r="AI3" s="275"/>
-      <c r="AJ3" s="275"/>
+      <c r="C3" s="279"/>
+      <c r="D3" s="279"/>
+      <c r="E3" s="279"/>
+      <c r="F3" s="279"/>
+      <c r="G3" s="279"/>
+      <c r="H3" s="279"/>
+      <c r="I3" s="279"/>
+      <c r="J3" s="279"/>
+      <c r="K3" s="279"/>
+      <c r="L3" s="279"/>
+      <c r="M3" s="279"/>
+      <c r="N3" s="279"/>
+      <c r="O3" s="279"/>
+      <c r="P3" s="280"/>
+      <c r="Q3" s="280"/>
+      <c r="R3" s="280"/>
+      <c r="S3" s="280"/>
+      <c r="T3" s="280"/>
+      <c r="U3" s="280"/>
+      <c r="V3" s="280"/>
+      <c r="W3" s="280"/>
+      <c r="X3" s="280"/>
+      <c r="Y3" s="280"/>
+      <c r="Z3" s="280"/>
+      <c r="AA3" s="280"/>
+      <c r="AB3" s="280"/>
+      <c r="AC3" s="280"/>
+      <c r="AD3" s="280"/>
+      <c r="AE3" s="280"/>
+      <c r="AF3" s="280"/>
+      <c r="AG3" s="280"/>
+      <c r="AH3" s="280"/>
+      <c r="AI3" s="280"/>
+      <c r="AJ3" s="280"/>
     </row>
     <row r="4" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="299" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="300"/>
-      <c r="E4" s="300"/>
-      <c r="F4" s="300"/>
-      <c r="G4" s="300"/>
-      <c r="H4" s="300"/>
-      <c r="I4" s="300"/>
-      <c r="J4" s="300"/>
-      <c r="K4" s="300"/>
-      <c r="L4" s="300"/>
-      <c r="M4" s="300"/>
-      <c r="N4" s="300"/>
-      <c r="O4" s="300"/>
-      <c r="P4" s="300"/>
-      <c r="Q4" s="300"/>
-      <c r="R4" s="300"/>
-      <c r="S4" s="301"/>
-      <c r="T4" s="299" t="s">
+      <c r="C4" s="263" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="264"/>
+      <c r="E4" s="264"/>
+      <c r="F4" s="264"/>
+      <c r="G4" s="264"/>
+      <c r="H4" s="264"/>
+      <c r="I4" s="264"/>
+      <c r="J4" s="264"/>
+      <c r="K4" s="264"/>
+      <c r="L4" s="264"/>
+      <c r="M4" s="264"/>
+      <c r="N4" s="264"/>
+      <c r="O4" s="264"/>
+      <c r="P4" s="264"/>
+      <c r="Q4" s="264"/>
+      <c r="R4" s="264"/>
+      <c r="S4" s="265"/>
+      <c r="T4" s="263" t="s">
         <v>1</v>
       </c>
-      <c r="U4" s="300"/>
-      <c r="V4" s="300"/>
-      <c r="W4" s="300"/>
-      <c r="X4" s="300"/>
-      <c r="Y4" s="300"/>
-      <c r="Z4" s="300"/>
-      <c r="AA4" s="300"/>
-      <c r="AB4" s="301"/>
-      <c r="AC4" s="299" t="s">
+      <c r="U4" s="264"/>
+      <c r="V4" s="264"/>
+      <c r="W4" s="264"/>
+      <c r="X4" s="264"/>
+      <c r="Y4" s="264"/>
+      <c r="Z4" s="264"/>
+      <c r="AA4" s="264"/>
+      <c r="AB4" s="265"/>
+      <c r="AC4" s="263" t="s">
         <v>2</v>
       </c>
-      <c r="AD4" s="300"/>
-      <c r="AE4" s="300"/>
-      <c r="AF4" s="300"/>
-      <c r="AG4" s="308"/>
-      <c r="AH4" s="299" t="s">
+      <c r="AD4" s="264"/>
+      <c r="AE4" s="264"/>
+      <c r="AF4" s="264"/>
+      <c r="AG4" s="274"/>
+      <c r="AH4" s="263" t="s">
         <v>10</v>
       </c>
-      <c r="AI4" s="300"/>
-      <c r="AJ4" s="301"/>
+      <c r="AI4" s="264"/>
+      <c r="AJ4" s="265"/>
     </row>
     <row r="5" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="268" t="s">
+      <c r="C5" s="275" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="269"/>
-      <c r="E5" s="269"/>
-      <c r="F5" s="269"/>
-      <c r="G5" s="269"/>
-      <c r="H5" s="269"/>
-      <c r="I5" s="269"/>
-      <c r="J5" s="270"/>
-      <c r="K5" s="306" t="s">
+      <c r="D5" s="271"/>
+      <c r="E5" s="271"/>
+      <c r="F5" s="271"/>
+      <c r="G5" s="271"/>
+      <c r="H5" s="271"/>
+      <c r="I5" s="271"/>
+      <c r="J5" s="272"/>
+      <c r="K5" s="270" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="269"/>
-      <c r="M5" s="269"/>
-      <c r="N5" s="269"/>
-      <c r="O5" s="269"/>
-      <c r="P5" s="269"/>
-      <c r="Q5" s="269"/>
-      <c r="R5" s="270"/>
-      <c r="S5" s="302" t="s">
+      <c r="L5" s="271"/>
+      <c r="M5" s="271"/>
+      <c r="N5" s="271"/>
+      <c r="O5" s="271"/>
+      <c r="P5" s="271"/>
+      <c r="Q5" s="271"/>
+      <c r="R5" s="272"/>
+      <c r="S5" s="266" t="s">
         <v>12</v>
       </c>
-      <c r="T5" s="268" t="s">
+      <c r="T5" s="275" t="s">
         <v>9</v>
       </c>
-      <c r="U5" s="269"/>
-      <c r="V5" s="269"/>
-      <c r="W5" s="270"/>
-      <c r="X5" s="306" t="s">
+      <c r="U5" s="271"/>
+      <c r="V5" s="271"/>
+      <c r="W5" s="272"/>
+      <c r="X5" s="270" t="s">
         <v>8</v>
       </c>
-      <c r="Y5" s="269"/>
-      <c r="Z5" s="269"/>
-      <c r="AA5" s="270"/>
-      <c r="AB5" s="302" t="s">
+      <c r="Y5" s="271"/>
+      <c r="Z5" s="271"/>
+      <c r="AA5" s="272"/>
+      <c r="AB5" s="266" t="s">
         <v>13</v>
       </c>
-      <c r="AC5" s="307" t="s">
+      <c r="AC5" s="273" t="s">
         <v>9</v>
       </c>
-      <c r="AD5" s="270"/>
-      <c r="AE5" s="306" t="s">
+      <c r="AD5" s="272"/>
+      <c r="AE5" s="270" t="s">
         <v>8</v>
       </c>
-      <c r="AF5" s="270"/>
-      <c r="AG5" s="302" t="s">
+      <c r="AF5" s="272"/>
+      <c r="AG5" s="266" t="s">
         <v>14</v>
       </c>
       <c r="AH5" s="56"/>
       <c r="AI5" s="25"/>
-      <c r="AJ5" s="302" t="s">
+      <c r="AJ5" s="266" t="s">
         <v>15</v>
       </c>
       <c r="AK5" s="4"/>
@@ -4139,7 +4139,7 @@
         <f>Résultats!$J$3</f>
         <v>0</v>
       </c>
-      <c r="D6" s="242">
+      <c r="D6" s="240">
         <f>Résultats!$J$4</f>
         <v>4</v>
       </c>
@@ -4157,9 +4157,9 @@
       </c>
       <c r="H6" s="109">
         <f>Résultats!$J$11</f>
-        <v>2</v>
-      </c>
-      <c r="I6" s="238">
+        <v>3</v>
+      </c>
+      <c r="I6" s="236">
         <f>Résultats!$J$13</f>
         <v>4</v>
       </c>
@@ -4171,7 +4171,7 @@
         <f>Résultats!$J$17</f>
         <v>1</v>
       </c>
-      <c r="L6" s="242">
+      <c r="L6" s="240">
         <f>Résultats!$J$18</f>
         <v>4</v>
       </c>
@@ -4179,7 +4179,7 @@
         <f>Résultats!$J$20</f>
         <v>2</v>
       </c>
-      <c r="N6" s="253">
+      <c r="N6" s="249">
         <f>Résultats!$J$21</f>
         <v>4</v>
       </c>
@@ -4187,9 +4187,9 @@
         <f>Résultats!$J$24</f>
         <v>2</v>
       </c>
-      <c r="P6" s="109">
+      <c r="P6" s="249">
         <f>Résultats!$J$25</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q6" s="111">
         <f>Résultats!$J$27</f>
@@ -4199,7 +4199,7 @@
         <f>Résultats!$J$28</f>
         <v>3</v>
       </c>
-      <c r="S6" s="303"/>
+      <c r="S6" s="267"/>
       <c r="T6" s="169">
         <f>Résultats!$V$6</f>
         <v>0</v>
@@ -4232,7 +4232,7 @@
         <f>Résultats!$V$25</f>
         <v>0</v>
       </c>
-      <c r="AB6" s="303"/>
+      <c r="AB6" s="267"/>
       <c r="AC6" s="111">
         <f>Résultats!$AH$8</f>
         <v>0</v>
@@ -4249,7 +4249,7 @@
         <f>Résultats!$AH$23</f>
         <v>0</v>
       </c>
-      <c r="AG6" s="303"/>
+      <c r="AG6" s="267"/>
       <c r="AH6" s="212">
         <f>Résultats!$AH$15</f>
         <v>0</v>
@@ -4258,7 +4258,7 @@
         <f>Résultats!$AH$16</f>
         <v>0</v>
       </c>
-      <c r="AJ6" s="303"/>
+      <c r="AJ6" s="267"/>
       <c r="AK6" s="37"/>
     </row>
     <row r="7" spans="1:38" s="39" customFormat="1" ht="58.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -4269,22 +4269,22 @@
 +IF(ISBLANK($D10),0,($D$6*PT_VICTOIRE_R1)+IF($D$6=4,PT_PREDICTION_EQUIPE_R1+IF($D10=$C$6+$D$6,PT_PREDICTION_NB_PARTIES_R1,0),0))</f>
         <v>0</v>
       </c>
-      <c r="D7" s="243"/>
+      <c r="D7" s="241"/>
       <c r="E7" s="173"/>
       <c r="F7" s="118"/>
       <c r="G7" s="119"/>
       <c r="H7" s="117"/>
-      <c r="I7" s="239"/>
+      <c r="I7" s="237"/>
       <c r="J7" s="117"/>
       <c r="K7" s="120"/>
-      <c r="L7" s="243"/>
+      <c r="L7" s="241"/>
       <c r="M7" s="173"/>
-      <c r="N7" s="254"/>
+      <c r="N7" s="250"/>
       <c r="O7" s="173"/>
-      <c r="P7" s="118"/>
+      <c r="P7" s="250"/>
       <c r="Q7" s="119"/>
       <c r="R7" s="117"/>
-      <c r="S7" s="303"/>
+      <c r="S7" s="267"/>
       <c r="T7" s="170"/>
       <c r="U7" s="117"/>
       <c r="V7" s="173"/>
@@ -4293,15 +4293,15 @@
       <c r="Y7" s="118"/>
       <c r="Z7" s="119"/>
       <c r="AA7" s="117"/>
-      <c r="AB7" s="303"/>
+      <c r="AB7" s="267"/>
       <c r="AC7" s="119"/>
       <c r="AD7" s="117"/>
       <c r="AE7" s="120"/>
       <c r="AF7" s="117"/>
-      <c r="AG7" s="303"/>
+      <c r="AG7" s="267"/>
       <c r="AH7" s="212"/>
       <c r="AI7" s="112"/>
-      <c r="AJ7" s="303"/>
+      <c r="AJ7" s="267"/>
       <c r="AK7" s="37"/>
     </row>
     <row r="8" spans="1:38" s="39" customFormat="1" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4311,7 +4311,7 @@
         <f>Résultats!$B$3</f>
         <v>TAMPA BAY</v>
       </c>
-      <c r="D8" s="244" t="str">
+      <c r="D8" s="242" t="str">
         <f>Résultats!$B$4</f>
         <v>COLUMBUS</v>
       </c>
@@ -4331,7 +4331,7 @@
         <f>Résultats!$B$11</f>
         <v>CAROLINE</v>
       </c>
-      <c r="I8" s="240" t="str">
+      <c r="I8" s="238" t="str">
         <f>Résultats!$B$13</f>
         <v>NEW YORK I.</v>
       </c>
@@ -4343,7 +4343,7 @@
         <f>Résultats!$B$17</f>
         <v>CALGARY</v>
       </c>
-      <c r="L8" s="244" t="str">
+      <c r="L8" s="242" t="str">
         <f>Résultats!$B$18</f>
         <v>COLORADO</v>
       </c>
@@ -4351,7 +4351,7 @@
         <f>Résultats!$B$20</f>
         <v>WINNIPEG</v>
       </c>
-      <c r="N8" s="255" t="str">
+      <c r="N8" s="251" t="str">
         <f>Résultats!$B$21</f>
         <v>ST-LOUIS</v>
       </c>
@@ -4359,7 +4359,7 @@
         <f>Résultats!$B$24</f>
         <v>NASHVILLE</v>
       </c>
-      <c r="P8" s="176" t="str">
+      <c r="P8" s="251" t="str">
         <f>Résultats!$B$25</f>
         <v>DALLAS</v>
       </c>
@@ -4371,7 +4371,7 @@
         <f>Résultats!$B$28</f>
         <v>VEGAS</v>
       </c>
-      <c r="S8" s="303"/>
+      <c r="S8" s="267"/>
       <c r="T8" s="171" t="str">
         <f>Résultats!$N$6</f>
         <v xml:space="preserve"> </v>
@@ -4404,7 +4404,7 @@
         <f>Résultats!$N$25</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AB8" s="303"/>
+      <c r="AB8" s="267"/>
       <c r="AC8" s="177" t="str">
         <f>Résultats!$Z$8</f>
         <v xml:space="preserve"> </v>
@@ -4421,7 +4421,7 @@
         <f>Résultats!$Z$23</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AG8" s="303"/>
+      <c r="AG8" s="267"/>
       <c r="AH8" s="213" t="str">
         <f>Résultats!$Z$15</f>
         <v xml:space="preserve"> </v>
@@ -4430,7 +4430,7 @@
         <f>Résultats!$Z$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ8" s="303"/>
+      <c r="AJ8" s="267"/>
       <c r="AK8" s="37"/>
     </row>
     <row r="9" spans="1:38" s="39" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4444,7 +4444,7 @@
         <f>Résultats!$A$3</f>
         <v>A1</v>
       </c>
-      <c r="D9" s="245" t="str">
+      <c r="D9" s="243" t="str">
         <f>Résultats!$A$4</f>
         <v>WC2</v>
       </c>
@@ -4464,7 +4464,7 @@
         <f>Résultats!$A$11</f>
         <v>WC1</v>
       </c>
-      <c r="I9" s="241" t="str">
+      <c r="I9" s="239" t="str">
         <f>Résultats!$A$13</f>
         <v>M2</v>
       </c>
@@ -4476,7 +4476,7 @@
         <f>Résultats!$A$17</f>
         <v>C1</v>
       </c>
-      <c r="L9" s="245" t="str">
+      <c r="L9" s="243" t="str">
         <f>Résultats!$A$18</f>
         <v>WC2</v>
       </c>
@@ -4484,7 +4484,7 @@
         <f>Résultats!$A$20</f>
         <v>C2</v>
       </c>
-      <c r="N9" s="256" t="str">
+      <c r="N9" s="252" t="str">
         <f>Résultats!$A$21</f>
         <v>C3</v>
       </c>
@@ -4492,7 +4492,7 @@
         <f>Résultats!$A$24</f>
         <v>P1</v>
       </c>
-      <c r="P9" s="182" t="str">
+      <c r="P9" s="252" t="str">
         <f>Résultats!$A$25</f>
         <v>WC1</v>
       </c>
@@ -4504,7 +4504,7 @@
         <f>Résultats!$A$28</f>
         <v>P3</v>
       </c>
-      <c r="S9" s="305"/>
+      <c r="S9" s="269"/>
       <c r="T9" s="179" t="str">
         <f>Résultats!$M$6</f>
         <v xml:space="preserve"> </v>
@@ -4537,7 +4537,7 @@
         <f>Résultats!$M$25</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AB9" s="304"/>
+      <c r="AB9" s="268"/>
       <c r="AC9" s="183" t="str">
         <f>Résultats!$Y$8</f>
         <v xml:space="preserve"> </v>
@@ -4554,7 +4554,7 @@
         <f>Résultats!$Y$23</f>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="AG9" s="304"/>
+      <c r="AG9" s="268"/>
       <c r="AH9" s="215" t="str">
         <f>Résultats!$Y$15</f>
         <v xml:space="preserve"> </v>
@@ -4563,7 +4563,7 @@
         <f>Résultats!$Y$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ9" s="305"/>
+      <c r="AJ9" s="269"/>
       <c r="AK9" s="114" t="s">
         <v>51</v>
       </c>
@@ -4621,7 +4621,7 @@
       <c r="W10" s="189"/>
       <c r="X10" s="190"/>
       <c r="Y10" s="188"/>
-      <c r="Z10" s="247"/>
+      <c r="Z10" s="245"/>
       <c r="AA10" s="193"/>
       <c r="AB10" s="194">
         <f>SUM(T11:AA11)</f>
@@ -4973,14 +4973,14 @@
         <v>2</v>
       </c>
       <c r="B14" s="88" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C14" s="46">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D14" s="45"/>
       <c r="E14" s="44">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F14" s="45"/>
       <c r="G14" s="48">
@@ -4988,25 +4988,25 @@
       </c>
       <c r="H14" s="47"/>
       <c r="I14" s="44">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J14" s="47"/>
       <c r="K14" s="49">
+        <v>4</v>
+      </c>
+      <c r="L14" s="47"/>
+      <c r="M14" s="44">
         <v>5</v>
       </c>
-      <c r="L14" s="47"/>
-      <c r="M14" s="44"/>
-      <c r="N14" s="45">
+      <c r="N14" s="45"/>
+      <c r="O14" s="44"/>
+      <c r="P14" s="45">
         <v>7</v>
       </c>
-      <c r="O14" s="44">
-        <v>6</v>
-      </c>
-      <c r="P14" s="45"/>
-      <c r="Q14" s="48">
+      <c r="Q14" s="48"/>
+      <c r="R14" s="50">
         <v>7</v>
       </c>
-      <c r="R14" s="50"/>
       <c r="S14" s="129">
         <f>SUM(C15:R15)</f>
         <v>30</v>
@@ -5016,7 +5016,7 @@
       <c r="V14" s="44"/>
       <c r="W14" s="47"/>
       <c r="X14" s="49"/>
-      <c r="Y14" s="45"/>
+      <c r="Y14" s="127"/>
       <c r="Z14" s="48"/>
       <c r="AA14" s="50"/>
       <c r="AB14" s="129">
@@ -5024,7 +5024,7 @@
         <v>0</v>
       </c>
       <c r="AC14" s="48"/>
-      <c r="AD14" s="47"/>
+      <c r="AD14" s="308"/>
       <c r="AE14" s="49"/>
       <c r="AF14" s="47"/>
       <c r="AG14" s="129">
@@ -5079,12 +5079,12 @@
       <c r="L15" s="150"/>
       <c r="M15" s="132">
         <f>(IF($M14&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M14=$M$6+$N$6,$O$103,0),0),0)+IF($N14&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N14=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="N15" s="150"/>
       <c r="O15" s="126">
         <f>(IF($O14&lt;&gt;"",($O$6*$O$104)+IF($O$6=4,($O$102)+IF($O14=$O$6+$P$6,$O$103,0),0),0)+IF($P14&lt;&gt;"",($P$6*$O$104)+IF($P$6=4,($O$102)+IF($P14=$O$6+$P$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="P15" s="150"/>
       <c r="Q15" s="126">
@@ -5191,7 +5191,7 @@
         <f>IF(ISBLANK(N14),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O16" s="124">
         <f>IF(ISBLANK(O14),
@@ -5203,7 +5203,7 @@
         <f>IF(ISBLANK(P14),
 0,
 IF(P$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q16" s="124">
         <f>IF(ISBLANK(Q14),
@@ -5369,17 +5369,17 @@
     <row r="18" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="186">
         <f>RANK(AL18,$AL$10:$AL$97,)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B18" s="211" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C18" s="198">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18" s="199"/>
       <c r="E18" s="200">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F18" s="199"/>
       <c r="G18" s="201">
@@ -5387,35 +5387,35 @@
       </c>
       <c r="H18" s="202"/>
       <c r="I18" s="200">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J18" s="202"/>
       <c r="K18" s="203">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L18" s="202"/>
-      <c r="M18" s="200">
-        <v>5</v>
-      </c>
-      <c r="N18" s="199"/>
-      <c r="O18" s="200"/>
-      <c r="P18" s="199">
+      <c r="M18" s="200"/>
+      <c r="N18" s="199">
         <v>7</v>
       </c>
-      <c r="Q18" s="201"/>
-      <c r="R18" s="204">
+      <c r="O18" s="200">
+        <v>6</v>
+      </c>
+      <c r="P18" s="199"/>
+      <c r="Q18" s="201">
         <v>7</v>
       </c>
-      <c r="S18" s="248">
+      <c r="R18" s="204"/>
+      <c r="S18" s="246">
         <f>SUM(C19:R19)</f>
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="T18" s="198"/>
       <c r="U18" s="202"/>
       <c r="V18" s="200"/>
       <c r="W18" s="202"/>
       <c r="X18" s="203"/>
-      <c r="Y18" s="237"/>
+      <c r="Y18" s="199"/>
       <c r="Z18" s="201"/>
       <c r="AA18" s="204"/>
       <c r="AB18" s="205">
@@ -5423,7 +5423,7 @@
         <v>0</v>
       </c>
       <c r="AC18" s="201"/>
-      <c r="AD18" s="234"/>
+      <c r="AD18" s="202"/>
       <c r="AE18" s="203"/>
       <c r="AF18" s="202"/>
       <c r="AG18" s="205">
@@ -5438,11 +5438,11 @@
       </c>
       <c r="AK18" s="207">
         <f>MAX($AL$10:$AL$97) - AL18</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="AL18" s="205">
         <f>$S18+$AB18+$AG18+$AJ18</f>
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5478,12 +5478,12 @@
       <c r="L19" s="150"/>
       <c r="M19" s="126">
         <f>(IF($M18&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M18=$M$6+$N$6,$O$103,0),0),0)+IF($N18&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N18=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="N19" s="150"/>
       <c r="O19" s="126">
         <f>(IF($O18&lt;&gt;"",($O$6*$O$104)+IF($O$6=4,($O$102)+IF($O18=$O$6+$P$6,$O$103,0),0),0)+IF($P18&lt;&gt;"",($P$6*$O$104)+IF($P$6=4,($O$102)+IF($P18=$O$6+$P$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P19" s="150"/>
       <c r="Q19" s="126">
@@ -5590,7 +5590,7 @@
         <f>IF(ISBLANK(N18),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O20" s="124">
         <f>IF(ISBLANK(O18),
@@ -5636,7 +5636,7 @@
       <c r="AJ20" s="147"/>
       <c r="AK20" s="148">
         <f>SUM(C20:AI20)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL20" s="130"/>
     </row>
@@ -5829,7 +5829,7 @@
         <f>SUM(AC23:AF23)</f>
         <v>0</v>
       </c>
-      <c r="AH22" s="235"/>
+      <c r="AH22" s="234"/>
       <c r="AI22" s="57"/>
       <c r="AJ22" s="129">
         <f>AH23</f>
@@ -6170,38 +6170,38 @@
         <v>4</v>
       </c>
       <c r="B26" s="211" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="C26" s="198">
         <v>5</v>
       </c>
       <c r="D26" s="199"/>
       <c r="E26" s="200">
+        <v>6</v>
+      </c>
+      <c r="F26" s="199"/>
+      <c r="G26" s="201"/>
+      <c r="H26" s="202">
         <v>7</v>
       </c>
-      <c r="F26" s="199"/>
-      <c r="G26" s="201">
-        <v>5</v>
-      </c>
-      <c r="H26" s="202"/>
-      <c r="I26" s="200">
+      <c r="I26" s="200"/>
+      <c r="J26" s="202">
         <v>6</v>
       </c>
-      <c r="J26" s="202"/>
       <c r="K26" s="203">
         <v>5</v>
       </c>
       <c r="L26" s="202"/>
-      <c r="M26" s="200">
+      <c r="M26" s="200"/>
+      <c r="N26" s="199">
         <v>6</v>
       </c>
-      <c r="N26" s="199"/>
       <c r="O26" s="200">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P26" s="199"/>
       <c r="Q26" s="201">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="R26" s="204"/>
       <c r="S26" s="205">
@@ -6214,7 +6214,7 @@
       <c r="W26" s="202"/>
       <c r="X26" s="203"/>
       <c r="Y26" s="199"/>
-      <c r="Z26" s="208"/>
+      <c r="Z26" s="201"/>
       <c r="AA26" s="204"/>
       <c r="AB26" s="205">
         <f>SUM(T27:AA27)</f>
@@ -6266,7 +6266,7 @@
       <c r="H27" s="150"/>
       <c r="I27" s="126">
         <f>(IF($I26&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I26=$I$6+$J$6,$O$103,0),0),0)+IF($J26&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J26=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J27" s="151"/>
       <c r="K27" s="152">
@@ -6276,7 +6276,7 @@
       <c r="L27" s="150"/>
       <c r="M27" s="126">
         <f>(IF($M26&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M26=$M$6+$N$6,$O$103,0),0),0)+IF($N26&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N26=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="N27" s="150"/>
       <c r="O27" s="126">
@@ -6358,7 +6358,7 @@
         <f>IF(ISBLANK(I26),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" s="124">
         <f>IF(ISBLANK(J26),
@@ -6388,7 +6388,7 @@
         <f>IF(ISBLANK(N26),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O28" s="124">
         <f>IF(ISBLANK(O26),
@@ -6513,7 +6513,7 @@
         <f>IF(N28 = 0,
 0,
 IF(N26 = (M$6+N$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O29" s="124">
         <f>IF(O28 = 0,
@@ -6559,7 +6559,7 @@
       <c r="AJ29" s="147"/>
       <c r="AK29" s="148">
         <f>SUM(C29:AI29)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL29" s="130"/>
     </row>
@@ -6569,40 +6569,40 @@
         <v>4</v>
       </c>
       <c r="B30" s="88" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="C30" s="46">
         <v>5</v>
       </c>
       <c r="D30" s="45"/>
       <c r="E30" s="44">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F30" s="45"/>
       <c r="G30" s="48">
         <v>5</v>
       </c>
       <c r="H30" s="47"/>
-      <c r="I30" s="44"/>
-      <c r="J30" s="47">
+      <c r="I30" s="44">
         <v>6</v>
       </c>
+      <c r="J30" s="47"/>
       <c r="K30" s="49">
         <v>5</v>
       </c>
       <c r="L30" s="47"/>
-      <c r="M30" s="44"/>
-      <c r="N30" s="45">
+      <c r="M30" s="44">
         <v>6</v>
       </c>
+      <c r="N30" s="45"/>
       <c r="O30" s="44">
         <v>5</v>
       </c>
       <c r="P30" s="45"/>
-      <c r="Q30" s="48"/>
-      <c r="R30" s="50">
-        <v>6</v>
-      </c>
+      <c r="Q30" s="48">
+        <v>7</v>
+      </c>
+      <c r="R30" s="50"/>
       <c r="S30" s="129">
         <f>SUM(C31:R31)</f>
         <v>23</v>
@@ -6613,7 +6613,7 @@
       <c r="W30" s="47"/>
       <c r="X30" s="49"/>
       <c r="Y30" s="45"/>
-      <c r="Z30" s="48"/>
+      <c r="Z30" s="244"/>
       <c r="AA30" s="47"/>
       <c r="AB30" s="129">
         <f>SUM(T31:AA31)</f>
@@ -6627,7 +6627,7 @@
         <f>SUM(AC31:AF31)</f>
         <v>0</v>
       </c>
-      <c r="AH30" s="249"/>
+      <c r="AH30" s="107"/>
       <c r="AI30" s="57"/>
       <c r="AJ30" s="129">
         <f>AH31</f>
@@ -6665,7 +6665,7 @@
       <c r="H31" s="80"/>
       <c r="I31" s="81">
         <f>(IF($I30&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I30=$I$6+$J$6,$O$103,0),0),0)+IF($J30&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J30=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J31" s="82"/>
       <c r="K31" s="83">
@@ -6675,7 +6675,7 @@
       <c r="L31" s="80"/>
       <c r="M31" s="81">
         <f>(IF($M30&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M30=$M$6+$N$6,$O$103,0),0),0)+IF($N30&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N30=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="N31" s="80"/>
       <c r="O31" s="81">
@@ -6757,7 +6757,7 @@
         <f>IF(ISBLANK(I30),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J32" s="124">
         <f>IF(ISBLANK(J30),
@@ -6787,7 +6787,7 @@
         <f>IF(ISBLANK(N30),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O32" s="124">
         <f>IF(ISBLANK(O30),
@@ -6912,7 +6912,7 @@
         <f>IF(N32 = 0,
 0,
 IF(N30 = (M$6+N$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O33" s="124">
         <f>IF(O32 = 0,
@@ -6958,7 +6958,7 @@
       <c r="AJ33" s="147"/>
       <c r="AK33" s="148">
         <f>SUM(C33:AI33)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL33" s="130"/>
     </row>
@@ -6968,18 +6968,18 @@
         <v>4</v>
       </c>
       <c r="B34" s="211" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="C34" s="198">
         <v>5</v>
       </c>
       <c r="D34" s="199"/>
       <c r="E34" s="200">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F34" s="199"/>
       <c r="G34" s="201">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H34" s="202"/>
       <c r="I34" s="200"/>
@@ -6995,13 +6995,13 @@
         <v>6</v>
       </c>
       <c r="O34" s="200">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P34" s="199"/>
-      <c r="Q34" s="201">
+      <c r="Q34" s="201"/>
+      <c r="R34" s="204">
         <v>6</v>
       </c>
-      <c r="R34" s="204"/>
       <c r="S34" s="205">
         <f>SUM(C35:R35)</f>
         <v>23</v>
@@ -7026,7 +7026,7 @@
         <f>SUM(AC35:AF35)</f>
         <v>0</v>
       </c>
-      <c r="AH34" s="309"/>
+      <c r="AH34" s="253"/>
       <c r="AI34" s="196"/>
       <c r="AJ34" s="205">
         <f>AH35</f>
@@ -7367,23 +7367,23 @@
         <v>4</v>
       </c>
       <c r="B38" s="88" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C38" s="46">
         <v>5</v>
       </c>
       <c r="D38" s="45"/>
       <c r="E38" s="44">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F38" s="45"/>
       <c r="G38" s="48">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H38" s="47"/>
       <c r="I38" s="44"/>
       <c r="J38" s="47">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K38" s="49">
         <v>5</v>
@@ -7397,10 +7397,10 @@
         <v>7</v>
       </c>
       <c r="P38" s="45"/>
-      <c r="Q38" s="48"/>
-      <c r="R38" s="50">
+      <c r="Q38" s="48">
         <v>6</v>
       </c>
+      <c r="R38" s="50"/>
       <c r="S38" s="129">
         <f>SUM(C39:R39)</f>
         <v>23</v>
@@ -7425,7 +7425,7 @@
         <f>SUM(AC39:AF39)</f>
         <v>0</v>
       </c>
-      <c r="AH38" s="107"/>
+      <c r="AH38" s="247"/>
       <c r="AI38" s="57"/>
       <c r="AJ38" s="129">
         <f>AH39</f>
@@ -7763,10 +7763,10 @@
     <row r="42" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="186">
         <f>RANK(AL42,$AL$10:$AL$97,)</f>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B42" s="211" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C42" s="198">
         <v>5</v>
@@ -7776,13 +7776,13 @@
         <v>6</v>
       </c>
       <c r="F42" s="199"/>
-      <c r="G42" s="201"/>
-      <c r="H42" s="202">
-        <v>7</v>
-      </c>
+      <c r="G42" s="201">
+        <v>6</v>
+      </c>
+      <c r="H42" s="202"/>
       <c r="I42" s="200"/>
       <c r="J42" s="202">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K42" s="203">
         <v>5</v>
@@ -7793,16 +7793,16 @@
         <v>6</v>
       </c>
       <c r="O42" s="200">
+        <v>7</v>
+      </c>
+      <c r="P42" s="199"/>
+      <c r="Q42" s="201"/>
+      <c r="R42" s="204">
         <v>6</v>
       </c>
-      <c r="P42" s="199"/>
-      <c r="Q42" s="201">
-        <v>6</v>
-      </c>
-      <c r="R42" s="204"/>
       <c r="S42" s="205">
         <f>SUM(C43:R43)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="T42" s="198"/>
       <c r="U42" s="202"/>
@@ -7832,11 +7832,11 @@
       </c>
       <c r="AK42" s="207">
         <f>MAX($AL$10:$AL$97) - AL42</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AL42" s="205">
         <f>$S42+$AB42+$AG42+$AJ42</f>
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7857,7 +7857,7 @@
       <c r="F43" s="80"/>
       <c r="G43" s="81">
         <f>(IF($G42&lt;&gt;"",($G$6*$O$104)+IF($G$6=4,($O$102)+IF($G42=$G$6+$H$6,$O$103,0),0),0)+IF($H42&lt;&gt;"",($H$6*$O$104)+IF($H$6=4,($O$102)+IF($H42=$G$6+$H$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H43" s="80"/>
       <c r="I43" s="121">
@@ -8209,7 +8209,7 @@
       <c r="W46" s="47"/>
       <c r="X46" s="49"/>
       <c r="Y46" s="45"/>
-      <c r="Z46" s="246"/>
+      <c r="Z46" s="244"/>
       <c r="AA46" s="47"/>
       <c r="AB46" s="129">
         <f>SUM(T47:AA47)</f>
@@ -8561,7 +8561,7 @@
     <row r="50" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="186">
         <f>RANK(AL50,$AL$10:$AL$97,)</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B50" s="211" t="s">
         <v>73</v>
@@ -8600,7 +8600,7 @@
       </c>
       <c r="S50" s="205">
         <f>SUM(C51:R51)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="T50" s="198"/>
       <c r="U50" s="202"/>
@@ -8630,11 +8630,11 @@
       </c>
       <c r="AK50" s="207">
         <f>MAX($AL$10:$AL$97) - AL50</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AL50" s="205">
         <f>$S50+$AB50+$AG50+$AJ50</f>
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="51" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -8655,7 +8655,7 @@
       <c r="F51" s="134"/>
       <c r="G51" s="132">
         <f>(IF($G50&lt;&gt;"",($G$6*$O$104)+IF($G$6=4,($O$102)+IF($G50=$G$6+$H$6,$O$103,0),0),0)+IF($H50&lt;&gt;"",($H$6*$O$104)+IF($H$6=4,($O$102)+IF($H50=$G$6+$H$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H51" s="134"/>
       <c r="I51" s="135">
@@ -8960,47 +8960,47 @@
         <v>12</v>
       </c>
       <c r="B54" s="88" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C54" s="46">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D54" s="45"/>
-      <c r="E54" s="44"/>
-      <c r="F54" s="45">
-        <v>7</v>
-      </c>
-      <c r="G54" s="48">
-        <v>4</v>
-      </c>
-      <c r="H54" s="47"/>
-      <c r="I54" s="44"/>
+      <c r="E54" s="306">
+        <v>6</v>
+      </c>
+      <c r="F54" s="45"/>
+      <c r="G54" s="307"/>
+      <c r="H54" s="47">
+        <v>6</v>
+      </c>
+      <c r="I54" s="306"/>
       <c r="J54" s="47">
         <v>7</v>
       </c>
       <c r="K54" s="49">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L54" s="47"/>
       <c r="M54" s="44">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N54" s="45"/>
       <c r="O54" s="44">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P54" s="45"/>
-      <c r="Q54" s="48"/>
-      <c r="R54" s="50">
+      <c r="Q54" s="48">
         <v>6</v>
       </c>
+      <c r="R54" s="50"/>
       <c r="S54" s="129">
         <f>SUM(C55:R55)</f>
         <v>14</v>
       </c>
       <c r="T54" s="46"/>
       <c r="U54" s="47"/>
-      <c r="V54" s="44"/>
+      <c r="V54" s="248"/>
       <c r="W54" s="47"/>
       <c r="X54" s="49"/>
       <c r="Y54" s="127"/>
@@ -9356,34 +9356,34 @@
         <v>12</v>
       </c>
       <c r="B58" s="211" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C58" s="198">
+        <v>5</v>
+      </c>
+      <c r="D58" s="199"/>
+      <c r="E58" s="200"/>
+      <c r="F58" s="199">
+        <v>7</v>
+      </c>
+      <c r="G58" s="201">
         <v>4</v>
-      </c>
-      <c r="D58" s="199"/>
-      <c r="E58" s="200">
-        <v>4</v>
-      </c>
-      <c r="F58" s="199"/>
-      <c r="G58" s="201">
-        <v>6</v>
       </c>
       <c r="H58" s="202"/>
       <c r="I58" s="200"/>
       <c r="J58" s="202">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K58" s="203">
         <v>6</v>
       </c>
       <c r="L58" s="202"/>
       <c r="M58" s="200">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N58" s="199"/>
       <c r="O58" s="200">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P58" s="199"/>
       <c r="Q58" s="201"/>
@@ -9399,15 +9399,15 @@
       <c r="V58" s="200"/>
       <c r="W58" s="202"/>
       <c r="X58" s="203"/>
-      <c r="Y58" s="199"/>
-      <c r="Z58" s="208"/>
+      <c r="Y58" s="235"/>
+      <c r="Z58" s="201"/>
       <c r="AA58" s="202"/>
       <c r="AB58" s="205">
         <f>SUM(T59:AA59)</f>
         <v>0</v>
       </c>
       <c r="AC58" s="201"/>
-      <c r="AD58" s="234"/>
+      <c r="AD58" s="202"/>
       <c r="AE58" s="203"/>
       <c r="AF58" s="202"/>
       <c r="AG58" s="205">
@@ -9752,18 +9752,18 @@
         <v>12</v>
       </c>
       <c r="B62" s="88" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="C62" s="46">
+        <v>4</v>
+      </c>
+      <c r="D62" s="45"/>
+      <c r="E62" s="44">
+        <v>4</v>
+      </c>
+      <c r="F62" s="45"/>
+      <c r="G62" s="48">
         <v>6</v>
-      </c>
-      <c r="D62" s="45"/>
-      <c r="E62" s="44"/>
-      <c r="F62" s="45">
-        <v>7</v>
-      </c>
-      <c r="G62" s="48">
-        <v>7</v>
       </c>
       <c r="H62" s="47"/>
       <c r="I62" s="44"/>
@@ -9775,11 +9775,11 @@
       </c>
       <c r="L62" s="47"/>
       <c r="M62" s="44">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="N62" s="45"/>
       <c r="O62" s="44">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P62" s="45"/>
       <c r="Q62" s="48"/>
@@ -9796,14 +9796,14 @@
       <c r="W62" s="47"/>
       <c r="X62" s="49"/>
       <c r="Y62" s="45"/>
-      <c r="Z62" s="48"/>
+      <c r="Z62" s="244"/>
       <c r="AA62" s="47"/>
       <c r="AB62" s="129">
         <f>SUM(T63:AA63)</f>
         <v>0</v>
       </c>
       <c r="AC62" s="48"/>
-      <c r="AD62" s="47"/>
+      <c r="AD62" s="308"/>
       <c r="AE62" s="49"/>
       <c r="AF62" s="47"/>
       <c r="AG62" s="129">
@@ -10148,38 +10148,38 @@
         <v>12</v>
       </c>
       <c r="B66" s="211" t="s">
-        <v>68</v>
-      </c>
-      <c r="C66" s="310">
+        <v>84</v>
+      </c>
+      <c r="C66" s="198">
+        <v>6</v>
+      </c>
+      <c r="D66" s="199"/>
+      <c r="E66" s="200"/>
+      <c r="F66" s="199">
+        <v>7</v>
+      </c>
+      <c r="G66" s="201">
+        <v>7</v>
+      </c>
+      <c r="H66" s="202"/>
+      <c r="I66" s="200"/>
+      <c r="J66" s="202">
+        <v>6</v>
+      </c>
+      <c r="K66" s="203">
+        <v>6</v>
+      </c>
+      <c r="L66" s="202"/>
+      <c r="M66" s="200">
+        <v>7</v>
+      </c>
+      <c r="N66" s="199"/>
+      <c r="O66" s="200">
         <v>5</v>
       </c>
-      <c r="D66" s="311"/>
-      <c r="E66" s="312">
-        <v>6</v>
-      </c>
-      <c r="F66" s="311"/>
-      <c r="G66" s="313">
-        <v>5</v>
-      </c>
-      <c r="H66" s="314"/>
-      <c r="I66" s="312"/>
-      <c r="J66" s="314">
-        <v>6</v>
-      </c>
-      <c r="K66" s="315">
-        <v>6</v>
-      </c>
-      <c r="L66" s="314"/>
-      <c r="M66" s="312">
-        <v>7</v>
-      </c>
-      <c r="N66" s="311"/>
-      <c r="O66" s="312">
-        <v>6</v>
-      </c>
-      <c r="P66" s="311"/>
-      <c r="Q66" s="313"/>
-      <c r="R66" s="316">
+      <c r="P66" s="199"/>
+      <c r="Q66" s="201"/>
+      <c r="R66" s="204">
         <v>6</v>
       </c>
       <c r="S66" s="205">
@@ -10544,45 +10544,45 @@
         <v>12</v>
       </c>
       <c r="B70" s="88" t="s">
-        <v>78</v>
-      </c>
-      <c r="C70" s="46">
+        <v>68</v>
+      </c>
+      <c r="C70" s="309">
         <v>5</v>
       </c>
-      <c r="D70" s="45"/>
-      <c r="E70" s="44"/>
-      <c r="F70" s="45">
+      <c r="D70" s="310"/>
+      <c r="E70" s="311">
+        <v>6</v>
+      </c>
+      <c r="F70" s="310"/>
+      <c r="G70" s="312">
+        <v>5</v>
+      </c>
+      <c r="H70" s="313"/>
+      <c r="I70" s="311"/>
+      <c r="J70" s="313">
+        <v>6</v>
+      </c>
+      <c r="K70" s="314">
+        <v>6</v>
+      </c>
+      <c r="L70" s="313"/>
+      <c r="M70" s="311">
         <v>7</v>
       </c>
-      <c r="G70" s="48">
+      <c r="N70" s="310"/>
+      <c r="O70" s="311">
         <v>6</v>
       </c>
-      <c r="H70" s="47"/>
-      <c r="I70" s="44"/>
-      <c r="J70" s="47">
-        <v>7</v>
-      </c>
-      <c r="K70" s="49">
-        <v>5</v>
-      </c>
-      <c r="L70" s="47"/>
-      <c r="M70" s="44">
+      <c r="P70" s="310"/>
+      <c r="Q70" s="312"/>
+      <c r="R70" s="315">
         <v>6</v>
-      </c>
-      <c r="N70" s="45"/>
-      <c r="O70" s="44">
-        <v>7</v>
-      </c>
-      <c r="P70" s="45"/>
-      <c r="Q70" s="48"/>
-      <c r="R70" s="50">
-        <v>7</v>
       </c>
       <c r="S70" s="129">
         <f>SUM(C71:R71)</f>
         <v>14</v>
       </c>
-      <c r="T70" s="236"/>
+      <c r="T70" s="46"/>
       <c r="U70" s="47"/>
       <c r="V70" s="44"/>
       <c r="W70" s="47"/>
@@ -10940,16 +10940,16 @@
         <v>12</v>
       </c>
       <c r="B74" s="211" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C74" s="198">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D74" s="199"/>
-      <c r="E74" s="200">
-        <v>6</v>
-      </c>
-      <c r="F74" s="199"/>
+      <c r="E74" s="200"/>
+      <c r="F74" s="199">
+        <v>7</v>
+      </c>
       <c r="G74" s="201">
         <v>6</v>
       </c>
@@ -10963,22 +10963,22 @@
       </c>
       <c r="L74" s="202"/>
       <c r="M74" s="200">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N74" s="199"/>
       <c r="O74" s="200">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P74" s="199"/>
       <c r="Q74" s="201"/>
       <c r="R74" s="204">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S74" s="205">
         <f>SUM(C75:R75)</f>
         <v>14</v>
       </c>
-      <c r="T74" s="198"/>
+      <c r="T74" s="316"/>
       <c r="U74" s="202"/>
       <c r="V74" s="200"/>
       <c r="W74" s="202"/>
@@ -11336,10 +11336,10 @@
         <v>12</v>
       </c>
       <c r="B78" s="88" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C78" s="46">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D78" s="45"/>
       <c r="E78" s="44">
@@ -11352,18 +11352,18 @@
       <c r="H78" s="47"/>
       <c r="I78" s="44"/>
       <c r="J78" s="47">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K78" s="49">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L78" s="47"/>
       <c r="M78" s="44">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N78" s="45"/>
       <c r="O78" s="44">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P78" s="45"/>
       <c r="Q78" s="48"/>
@@ -11732,7 +11732,7 @@
         <v>12</v>
       </c>
       <c r="B82" s="211" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C82" s="198">
         <v>5</v>
@@ -11751,20 +11751,20 @@
         <v>6</v>
       </c>
       <c r="K82" s="203">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L82" s="202"/>
       <c r="M82" s="200">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N82" s="199"/>
       <c r="O82" s="200">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P82" s="199"/>
       <c r="Q82" s="201"/>
       <c r="R82" s="204">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S82" s="205">
         <f>SUM(C83:R83)</f>
@@ -11776,7 +11776,7 @@
       <c r="W82" s="202"/>
       <c r="X82" s="203"/>
       <c r="Y82" s="199"/>
-      <c r="Z82" s="208"/>
+      <c r="Z82" s="201"/>
       <c r="AA82" s="202"/>
       <c r="AB82" s="205">
         <f>SUM(T83:AA83)</f>
@@ -12128,40 +12128,40 @@
         <v>12</v>
       </c>
       <c r="B86" s="88" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C86" s="46">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D86" s="45"/>
       <c r="E86" s="44">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F86" s="45"/>
       <c r="G86" s="48">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H86" s="47"/>
       <c r="I86" s="44"/>
       <c r="J86" s="47">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K86" s="49">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L86" s="47"/>
       <c r="M86" s="44">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N86" s="45"/>
       <c r="O86" s="44">
+        <v>6</v>
+      </c>
+      <c r="P86" s="45"/>
+      <c r="Q86" s="48"/>
+      <c r="R86" s="50">
         <v>7</v>
       </c>
-      <c r="P86" s="45"/>
-      <c r="Q86" s="48">
-        <v>5</v>
-      </c>
-      <c r="R86" s="50"/>
       <c r="S86" s="129">
         <f>SUM(C87:R87)</f>
         <v>14</v>
@@ -12172,7 +12172,7 @@
       <c r="W86" s="47"/>
       <c r="X86" s="49"/>
       <c r="Y86" s="45"/>
-      <c r="Z86" s="48"/>
+      <c r="Z86" s="244"/>
       <c r="AA86" s="47"/>
       <c r="AB86" s="129">
         <f>SUM(T87:AA87)</f>
@@ -12524,7 +12524,7 @@
         <v>12</v>
       </c>
       <c r="B90" s="211" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="C90" s="198">
         <v>6</v>
@@ -12535,12 +12535,12 @@
       </c>
       <c r="F90" s="199"/>
       <c r="G90" s="201">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H90" s="202"/>
       <c r="I90" s="200"/>
       <c r="J90" s="202">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="K90" s="203">
         <v>7</v>
@@ -12551,13 +12551,13 @@
       </c>
       <c r="N90" s="199"/>
       <c r="O90" s="200">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P90" s="199"/>
-      <c r="Q90" s="201"/>
-      <c r="R90" s="204">
-        <v>7</v>
-      </c>
+      <c r="Q90" s="201">
+        <v>5</v>
+      </c>
+      <c r="R90" s="204"/>
       <c r="S90" s="205">
         <f>SUM(C91:R91)</f>
         <v>14</v>
@@ -12917,53 +12917,53 @@
     <row r="94" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A94" s="122">
         <f>RANK(AL94,$AL$10:$AL$97,)</f>
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B94" s="88" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C94" s="226">
+        <v>6</v>
+      </c>
+      <c r="D94" s="227"/>
+      <c r="E94" s="228">
         <v>7</v>
       </c>
-      <c r="D94" s="227"/>
-      <c r="E94" s="250">
+      <c r="F94" s="227"/>
+      <c r="G94" s="229">
         <v>6</v>
       </c>
-      <c r="F94" s="227"/>
-      <c r="G94" s="251"/>
-      <c r="H94" s="230">
-        <v>6</v>
-      </c>
-      <c r="I94" s="250"/>
+      <c r="H94" s="230"/>
+      <c r="I94" s="228"/>
       <c r="J94" s="230">
         <v>7</v>
       </c>
       <c r="K94" s="231">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L94" s="230"/>
       <c r="M94" s="228">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N94" s="227"/>
       <c r="O94" s="228">
         <v>6</v>
       </c>
       <c r="P94" s="227"/>
-      <c r="Q94" s="229">
-        <v>6</v>
-      </c>
-      <c r="R94" s="232"/>
+      <c r="Q94" s="229"/>
+      <c r="R94" s="232">
+        <v>7</v>
+      </c>
       <c r="S94" s="129">
         <f>SUM(C95:R95)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T94" s="46"/>
       <c r="U94" s="47"/>
-      <c r="V94" s="252"/>
+      <c r="V94" s="44"/>
       <c r="W94" s="47"/>
       <c r="X94" s="49"/>
-      <c r="Y94" s="127"/>
+      <c r="Y94" s="45"/>
       <c r="Z94" s="48"/>
       <c r="AA94" s="47"/>
       <c r="AB94" s="218">
@@ -12986,11 +12986,11 @@
       </c>
       <c r="AK94" s="116">
         <f>MAX($AL$10:$AL$97) - AL94</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AL94" s="218">
         <f>$S94+$AB94+$AG94+$AJ94</f>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -13011,7 +13011,7 @@
       <c r="F95" s="134"/>
       <c r="G95" s="132">
         <f>(IF($G94&lt;&gt;"",($G$6*$O$104)+IF($G$6=4,($O$102)+IF($G94=$G$6+$H$6,$O$103,0),0),0)+IF($H94&lt;&gt;"",($H$6*$O$104)+IF($H$6=4,($O$102)+IF($H94=$G$6+$H$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H95" s="134"/>
       <c r="I95" s="135">
@@ -13443,12 +13443,12 @@
     <row r="100" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B100" s="43"/>
       <c r="N100" s="26"/>
-      <c r="O100" s="290" t="s">
+      <c r="O100" s="254" t="s">
         <v>17</v>
       </c>
-      <c r="P100" s="291"/>
-      <c r="Q100" s="291"/>
-      <c r="R100" s="292"/>
+      <c r="P100" s="255"/>
+      <c r="Q100" s="255"/>
+      <c r="R100" s="256"/>
       <c r="AG100" s="30"/>
       <c r="AH100" s="30"/>
       <c r="AI100" s="30"/>
@@ -13457,21 +13457,21 @@
     </row>
     <row r="101" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="33"/>
-      <c r="B101" s="278" t="s">
+      <c r="B101" s="283" t="s">
         <v>16</v>
       </c>
-      <c r="C101" s="279"/>
-      <c r="D101" s="279"/>
-      <c r="E101" s="279"/>
-      <c r="F101" s="279"/>
-      <c r="G101" s="279"/>
-      <c r="H101" s="279"/>
-      <c r="I101" s="279"/>
-      <c r="J101" s="279"/>
-      <c r="K101" s="279"/>
-      <c r="L101" s="279"/>
-      <c r="M101" s="279"/>
-      <c r="N101" s="280"/>
+      <c r="C101" s="284"/>
+      <c r="D101" s="284"/>
+      <c r="E101" s="284"/>
+      <c r="F101" s="284"/>
+      <c r="G101" s="284"/>
+      <c r="H101" s="284"/>
+      <c r="I101" s="284"/>
+      <c r="J101" s="284"/>
+      <c r="K101" s="284"/>
+      <c r="L101" s="284"/>
+      <c r="M101" s="284"/>
+      <c r="N101" s="285"/>
       <c r="O101" s="21">
         <v>1</v>
       </c>
@@ -13484,45 +13484,45 @@
       <c r="R101" s="22">
         <v>4</v>
       </c>
-      <c r="U101" s="293" t="s">
+      <c r="U101" s="257" t="s">
         <v>26</v>
       </c>
-      <c r="V101" s="294"/>
-      <c r="W101" s="294"/>
-      <c r="X101" s="294"/>
-      <c r="Y101" s="294"/>
-      <c r="Z101" s="294"/>
-      <c r="AA101" s="294"/>
-      <c r="AB101" s="294"/>
-      <c r="AC101" s="294"/>
-      <c r="AD101" s="295"/>
+      <c r="V101" s="258"/>
+      <c r="W101" s="258"/>
+      <c r="X101" s="258"/>
+      <c r="Y101" s="258"/>
+      <c r="Z101" s="258"/>
+      <c r="AA101" s="258"/>
+      <c r="AB101" s="258"/>
+      <c r="AC101" s="258"/>
+      <c r="AD101" s="259"/>
       <c r="AE101" s="28"/>
       <c r="AF101" s="28"/>
-      <c r="AG101" s="296" t="s">
+      <c r="AG101" s="260" t="s">
         <v>24</v>
       </c>
-      <c r="AH101" s="297"/>
-      <c r="AI101" s="297"/>
-      <c r="AJ101" s="297"/>
-      <c r="AK101" s="298"/>
+      <c r="AH101" s="261"/>
+      <c r="AI101" s="261"/>
+      <c r="AJ101" s="261"/>
+      <c r="AK101" s="262"/>
     </row>
     <row r="102" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A102" s="34"/>
-      <c r="B102" s="257" t="s">
+      <c r="B102" s="290" t="s">
         <v>6</v>
       </c>
-      <c r="C102" s="258"/>
-      <c r="D102" s="258"/>
-      <c r="E102" s="258"/>
-      <c r="F102" s="258"/>
-      <c r="G102" s="258"/>
-      <c r="H102" s="258"/>
-      <c r="I102" s="258"/>
-      <c r="J102" s="258"/>
-      <c r="K102" s="258"/>
-      <c r="L102" s="258"/>
-      <c r="M102" s="258"/>
-      <c r="N102" s="259"/>
+      <c r="C102" s="291"/>
+      <c r="D102" s="291"/>
+      <c r="E102" s="291"/>
+      <c r="F102" s="291"/>
+      <c r="G102" s="291"/>
+      <c r="H102" s="291"/>
+      <c r="I102" s="291"/>
+      <c r="J102" s="291"/>
+      <c r="K102" s="291"/>
+      <c r="L102" s="291"/>
+      <c r="M102" s="291"/>
+      <c r="N102" s="292"/>
       <c r="O102" s="20">
         <v>5</v>
       </c>
@@ -13535,49 +13535,49 @@
       <c r="R102" s="23">
         <v>20</v>
       </c>
-      <c r="U102" s="283" t="s">
+      <c r="U102" s="288" t="s">
         <v>20</v>
       </c>
-      <c r="V102" s="284"/>
-      <c r="W102" s="284"/>
-      <c r="X102" s="284"/>
-      <c r="Y102" s="284"/>
-      <c r="Z102" s="284"/>
-      <c r="AA102" s="284"/>
-      <c r="AB102" s="281">
+      <c r="V102" s="289"/>
+      <c r="W102" s="289"/>
+      <c r="X102" s="289"/>
+      <c r="Y102" s="289"/>
+      <c r="Z102" s="289"/>
+      <c r="AA102" s="289"/>
+      <c r="AB102" s="286">
         <v>22</v>
       </c>
-      <c r="AC102" s="281"/>
-      <c r="AD102" s="282"/>
+      <c r="AC102" s="286"/>
+      <c r="AD102" s="287"/>
       <c r="AE102" s="29"/>
       <c r="AF102" s="29"/>
-      <c r="AG102" s="264" t="s">
+      <c r="AG102" s="302" t="s">
         <v>21</v>
       </c>
-      <c r="AH102" s="265"/>
-      <c r="AI102" s="265"/>
-      <c r="AJ102" s="266"/>
+      <c r="AH102" s="303"/>
+      <c r="AI102" s="303"/>
+      <c r="AJ102" s="304"/>
       <c r="AK102" s="223">
         <v>230</v>
       </c>
     </row>
     <row r="103" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="34"/>
-      <c r="B103" s="257" t="s">
+      <c r="B103" s="290" t="s">
         <v>5</v>
       </c>
-      <c r="C103" s="258"/>
-      <c r="D103" s="258"/>
-      <c r="E103" s="258"/>
-      <c r="F103" s="258"/>
-      <c r="G103" s="258"/>
-      <c r="H103" s="258"/>
-      <c r="I103" s="258"/>
-      <c r="J103" s="258"/>
-      <c r="K103" s="258"/>
-      <c r="L103" s="258"/>
-      <c r="M103" s="258"/>
-      <c r="N103" s="259"/>
+      <c r="C103" s="291"/>
+      <c r="D103" s="291"/>
+      <c r="E103" s="291"/>
+      <c r="F103" s="291"/>
+      <c r="G103" s="291"/>
+      <c r="H103" s="291"/>
+      <c r="I103" s="291"/>
+      <c r="J103" s="291"/>
+      <c r="K103" s="291"/>
+      <c r="L103" s="291"/>
+      <c r="M103" s="291"/>
+      <c r="N103" s="292"/>
       <c r="O103" s="20">
         <v>2</v>
       </c>
@@ -13590,49 +13590,49 @@
       <c r="R103" s="23">
         <v>8</v>
       </c>
-      <c r="U103" s="262" t="s">
+      <c r="U103" s="297" t="s">
         <v>18</v>
       </c>
-      <c r="V103" s="263"/>
-      <c r="W103" s="263"/>
-      <c r="X103" s="263"/>
-      <c r="Y103" s="263"/>
-      <c r="Z103" s="263"/>
-      <c r="AA103" s="263"/>
-      <c r="AB103" s="288">
+      <c r="V103" s="298"/>
+      <c r="W103" s="298"/>
+      <c r="X103" s="298"/>
+      <c r="Y103" s="298"/>
+      <c r="Z103" s="298"/>
+      <c r="AA103" s="298"/>
+      <c r="AB103" s="299">
         <v>20</v>
       </c>
-      <c r="AC103" s="288"/>
-      <c r="AD103" s="289"/>
+      <c r="AC103" s="299"/>
+      <c r="AD103" s="300"/>
       <c r="AE103" s="29"/>
       <c r="AF103" s="29"/>
-      <c r="AG103" s="267" t="s">
+      <c r="AG103" s="305" t="s">
         <v>22</v>
       </c>
-      <c r="AH103" s="258"/>
-      <c r="AI103" s="258"/>
-      <c r="AJ103" s="259"/>
+      <c r="AH103" s="291"/>
+      <c r="AI103" s="291"/>
+      <c r="AJ103" s="292"/>
       <c r="AK103" s="36">
         <v>115</v>
       </c>
     </row>
     <row r="104" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="35"/>
-      <c r="B104" s="271" t="s">
+      <c r="B104" s="276" t="s">
         <v>4</v>
       </c>
-      <c r="C104" s="272"/>
-      <c r="D104" s="272"/>
-      <c r="E104" s="272"/>
-      <c r="F104" s="272"/>
-      <c r="G104" s="272"/>
-      <c r="H104" s="272"/>
-      <c r="I104" s="272"/>
-      <c r="J104" s="272"/>
-      <c r="K104" s="272"/>
-      <c r="L104" s="272"/>
-      <c r="M104" s="272"/>
-      <c r="N104" s="273"/>
+      <c r="C104" s="277"/>
+      <c r="D104" s="277"/>
+      <c r="E104" s="277"/>
+      <c r="F104" s="277"/>
+      <c r="G104" s="277"/>
+      <c r="H104" s="277"/>
+      <c r="I104" s="277"/>
+      <c r="J104" s="277"/>
+      <c r="K104" s="277"/>
+      <c r="L104" s="277"/>
+      <c r="M104" s="277"/>
+      <c r="N104" s="278"/>
       <c r="O104" s="3">
         <v>1</v>
       </c>
@@ -13645,51 +13645,51 @@
       <c r="R104" s="24">
         <v>1</v>
       </c>
-      <c r="U104" s="285" t="s">
+      <c r="U104" s="293" t="s">
         <v>19</v>
       </c>
-      <c r="V104" s="261"/>
-      <c r="W104" s="261"/>
-      <c r="X104" s="261"/>
-      <c r="Y104" s="261"/>
-      <c r="Z104" s="261"/>
-      <c r="AA104" s="261"/>
-      <c r="AB104" s="286">
+      <c r="V104" s="294"/>
+      <c r="W104" s="294"/>
+      <c r="X104" s="294"/>
+      <c r="Y104" s="294"/>
+      <c r="Z104" s="294"/>
+      <c r="AA104" s="294"/>
+      <c r="AB104" s="295">
         <f>AB102*AB103</f>
         <v>440</v>
       </c>
-      <c r="AC104" s="286"/>
-      <c r="AD104" s="287"/>
+      <c r="AC104" s="295"/>
+      <c r="AD104" s="296"/>
       <c r="AE104" s="29"/>
       <c r="AF104" s="29"/>
-      <c r="AG104" s="267" t="s">
+      <c r="AG104" s="305" t="s">
         <v>25</v>
       </c>
-      <c r="AH104" s="258"/>
-      <c r="AI104" s="258"/>
-      <c r="AJ104" s="259"/>
+      <c r="AH104" s="291"/>
+      <c r="AI104" s="291"/>
+      <c r="AJ104" s="292"/>
       <c r="AK104" s="36">
         <v>65</v>
       </c>
     </row>
     <row r="105" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG105" s="262" t="s">
+      <c r="AG105" s="297" t="s">
         <v>23</v>
       </c>
-      <c r="AH105" s="263"/>
-      <c r="AI105" s="263"/>
-      <c r="AJ105" s="263"/>
+      <c r="AH105" s="298"/>
+      <c r="AI105" s="298"/>
+      <c r="AJ105" s="298"/>
       <c r="AK105" s="225">
         <v>30</v>
       </c>
     </row>
     <row r="106" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG106" s="260" t="s">
+      <c r="AG106" s="301" t="s">
         <v>19</v>
       </c>
-      <c r="AH106" s="261"/>
-      <c r="AI106" s="261"/>
-      <c r="AJ106" s="261"/>
+      <c r="AH106" s="294"/>
+      <c r="AI106" s="294"/>
+      <c r="AJ106" s="294"/>
       <c r="AK106" s="224">
         <f>SUM(AK102:AK105)</f>
         <v>440</v>
@@ -13701,6 +13701,28 @@
     <sortCondition ref="B10:B94"/>
   </sortState>
   <mergeCells count="38">
+    <mergeCell ref="B103:N103"/>
+    <mergeCell ref="AG106:AJ106"/>
+    <mergeCell ref="AG105:AJ105"/>
+    <mergeCell ref="AG102:AJ102"/>
+    <mergeCell ref="AG104:AJ104"/>
+    <mergeCell ref="AG103:AJ103"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="B104:N104"/>
+    <mergeCell ref="C1:O1"/>
+    <mergeCell ref="P1:AJ1"/>
+    <mergeCell ref="C3:O3"/>
+    <mergeCell ref="P3:AJ3"/>
+    <mergeCell ref="C2:P2"/>
+    <mergeCell ref="Q2:AJ2"/>
+    <mergeCell ref="B101:N101"/>
+    <mergeCell ref="AB102:AD102"/>
+    <mergeCell ref="U102:AA102"/>
+    <mergeCell ref="B102:N102"/>
+    <mergeCell ref="U104:AA104"/>
+    <mergeCell ref="AB104:AD104"/>
+    <mergeCell ref="U103:AA103"/>
+    <mergeCell ref="AB103:AD103"/>
     <mergeCell ref="O100:R100"/>
     <mergeCell ref="U101:AD101"/>
     <mergeCell ref="AG101:AK101"/>
@@ -13717,28 +13739,6 @@
     <mergeCell ref="C5:J5"/>
     <mergeCell ref="K5:R5"/>
     <mergeCell ref="S5:S9"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="B104:N104"/>
-    <mergeCell ref="C1:O1"/>
-    <mergeCell ref="P1:AJ1"/>
-    <mergeCell ref="C3:O3"/>
-    <mergeCell ref="P3:AJ3"/>
-    <mergeCell ref="C2:P2"/>
-    <mergeCell ref="Q2:AJ2"/>
-    <mergeCell ref="B101:N101"/>
-    <mergeCell ref="AB102:AD102"/>
-    <mergeCell ref="U102:AA102"/>
-    <mergeCell ref="B102:N102"/>
-    <mergeCell ref="U104:AA104"/>
-    <mergeCell ref="AB104:AD104"/>
-    <mergeCell ref="U103:AA103"/>
-    <mergeCell ref="AB103:AD103"/>
-    <mergeCell ref="B103:N103"/>
-    <mergeCell ref="AG106:AJ106"/>
-    <mergeCell ref="AG105:AJ105"/>
-    <mergeCell ref="AG102:AJ102"/>
-    <mergeCell ref="AG104:AJ104"/>
-    <mergeCell ref="AG103:AJ103"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <conditionalFormatting sqref="AH18:AI18 AH10:AI10 AH14:AI14 T10:AA10 AC10:AF10 C10:R10 C14:R14 T14:AA14 AC14:AF14 T18:AA18 AC18:AF18 AH30:AI30 C30:R30 T30:AA30 AC30:AF30 AH26:AI26 C26:R26 T26:AA26 AC26:AF26 AH62:AI62 C62:R62 T62:AA62 AC62:AF62 AH42:AI42 C42:R42 T42:AA42 AC42:AF42 AH22:AI22 C22:R22 T22:AA22 AC22:AF22 AH38:AI38 C38:R38 T38:AA38 AC38:AF38 AH34:AI34 C34:R34 T34:AA34 AC34:AF34 AH66:AI66 C66:R66 T66:AA66 AC66:AF66 C18:R18">
@@ -14395,7 +14395,7 @@
   <dimension ref="A1:AJ31"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14800,7 +14800,9 @@
       <c r="G10" s="86">
         <v>6</v>
       </c>
-      <c r="H10" s="85"/>
+      <c r="H10" s="85">
+        <v>2</v>
+      </c>
       <c r="I10" s="86"/>
       <c r="J10" s="77">
         <f>IF(C10&gt;C11,1,0)+IF(D10&gt;D11,1,0)+IF(E10&gt;E11,1,0)+IF(F10&gt;F11,1,0)+IF(G10&gt;G11,1,0)+IF(H10&gt;H11,1,0)+IF(I10&gt;I11,1,0)</f>
@@ -14861,11 +14863,13 @@
       <c r="G11" s="86">
         <v>0</v>
       </c>
-      <c r="H11" s="85"/>
+      <c r="H11" s="85">
+        <v>5</v>
+      </c>
       <c r="I11" s="86"/>
       <c r="J11" s="77">
         <f>IF(C11&gt;C10,1,0)+IF(D11&gt;D10,1,0)+IF(E11&gt;E10,1,0)+IF(F11&gt;F10,1,0)+IF(G11&gt;G10,1,0)+IF(H11&gt;H10,1,0)+IF(I11&gt;I10,1,0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K11" s="14"/>
       <c r="L11" s="4"/>
@@ -15481,7 +15485,9 @@
       <c r="G24" s="85">
         <v>3</v>
       </c>
-      <c r="H24" s="85"/>
+      <c r="H24" s="85">
+        <v>2</v>
+      </c>
       <c r="I24" s="86"/>
       <c r="J24" s="77">
         <f>IF(C24&gt;C25,1,0)+IF(D24&gt;D25,1,0)+IF(E24&gt;E25,1,0)+IF(F24&gt;F25,1,0)+IF(G24&gt;G25,1,0)+IF(H24&gt;H25,1,0)+IF(I24&gt;I25,1,0)</f>
@@ -15540,11 +15546,13 @@
       <c r="G25" s="85">
         <v>5</v>
       </c>
-      <c r="H25" s="85"/>
+      <c r="H25" s="85">
+        <v>4</v>
+      </c>
       <c r="I25" s="86"/>
       <c r="J25" s="77">
         <f>IF(C25&gt;C24,1,0)+IF(D25&gt;D24,1,0)+IF(E25&gt;E24,1,0)+IF(F25&gt;F24,1,0)+IF(G25&gt;G24,1,0)+IF(H25&gt;H24,1,0)+IF(I25&gt;I24,1,0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K25" s="14"/>
       <c r="L25" s="4"/>

</xml_diff>

<commit_message>
Updated games of 2019-04-23
</commit_message>
<xml_diff>
--- a/laval.xlsx
+++ b/laval.xlsx
@@ -1960,7 +1960,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="317">
+  <cellXfs count="325">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2447,9 +2447,6 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2480,18 +2477,9 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -2507,6 +2495,126 @@
     <xf numFmtId="0" fontId="19" fillId="7" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="87" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="95" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="86" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="88" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2558,142 +2666,58 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="86" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="87" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="88" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="108" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="95" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3917,217 +3941,217 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="C1" s="279"/>
-      <c r="D1" s="279"/>
-      <c r="E1" s="279"/>
-      <c r="F1" s="279"/>
-      <c r="G1" s="279"/>
-      <c r="H1" s="279"/>
-      <c r="I1" s="279"/>
-      <c r="J1" s="279"/>
-      <c r="K1" s="279"/>
-      <c r="L1" s="279"/>
-      <c r="M1" s="279"/>
-      <c r="N1" s="279"/>
-      <c r="O1" s="279"/>
-      <c r="P1" s="280"/>
-      <c r="Q1" s="280"/>
-      <c r="R1" s="280"/>
-      <c r="S1" s="280"/>
-      <c r="T1" s="280"/>
-      <c r="U1" s="280"/>
-      <c r="V1" s="280"/>
-      <c r="W1" s="280"/>
-      <c r="X1" s="280"/>
-      <c r="Y1" s="280"/>
-      <c r="Z1" s="280"/>
-      <c r="AA1" s="280"/>
-      <c r="AB1" s="280"/>
-      <c r="AC1" s="280"/>
-      <c r="AD1" s="280"/>
-      <c r="AE1" s="280"/>
-      <c r="AF1" s="280"/>
-      <c r="AG1" s="280"/>
-      <c r="AH1" s="280"/>
-      <c r="AI1" s="280"/>
-      <c r="AJ1" s="280"/>
+      <c r="C1" s="274"/>
+      <c r="D1" s="274"/>
+      <c r="E1" s="274"/>
+      <c r="F1" s="274"/>
+      <c r="G1" s="274"/>
+      <c r="H1" s="274"/>
+      <c r="I1" s="274"/>
+      <c r="J1" s="274"/>
+      <c r="K1" s="274"/>
+      <c r="L1" s="274"/>
+      <c r="M1" s="274"/>
+      <c r="N1" s="274"/>
+      <c r="O1" s="274"/>
+      <c r="P1" s="275"/>
+      <c r="Q1" s="275"/>
+      <c r="R1" s="275"/>
+      <c r="S1" s="275"/>
+      <c r="T1" s="275"/>
+      <c r="U1" s="275"/>
+      <c r="V1" s="275"/>
+      <c r="W1" s="275"/>
+      <c r="X1" s="275"/>
+      <c r="Y1" s="275"/>
+      <c r="Z1" s="275"/>
+      <c r="AA1" s="275"/>
+      <c r="AB1" s="275"/>
+      <c r="AC1" s="275"/>
+      <c r="AD1" s="275"/>
+      <c r="AE1" s="275"/>
+      <c r="AF1" s="275"/>
+      <c r="AG1" s="275"/>
+      <c r="AH1" s="275"/>
+      <c r="AI1" s="275"/>
+      <c r="AJ1" s="275"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="41"/>
-      <c r="C2" s="281" t="s">
+      <c r="C2" s="276" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="281"/>
-      <c r="E2" s="281"/>
-      <c r="F2" s="281"/>
-      <c r="G2" s="281"/>
-      <c r="H2" s="281"/>
-      <c r="I2" s="281"/>
-      <c r="J2" s="281"/>
-      <c r="K2" s="281"/>
-      <c r="L2" s="281"/>
-      <c r="M2" s="281"/>
-      <c r="N2" s="281"/>
-      <c r="O2" s="281"/>
-      <c r="P2" s="281"/>
-      <c r="Q2" s="282" t="s">
+      <c r="D2" s="276"/>
+      <c r="E2" s="276"/>
+      <c r="F2" s="276"/>
+      <c r="G2" s="276"/>
+      <c r="H2" s="276"/>
+      <c r="I2" s="276"/>
+      <c r="J2" s="276"/>
+      <c r="K2" s="276"/>
+      <c r="L2" s="276"/>
+      <c r="M2" s="276"/>
+      <c r="N2" s="276"/>
+      <c r="O2" s="276"/>
+      <c r="P2" s="276"/>
+      <c r="Q2" s="277" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="280"/>
-      <c r="S2" s="280"/>
-      <c r="T2" s="280"/>
-      <c r="U2" s="280"/>
-      <c r="V2" s="280"/>
-      <c r="W2" s="280"/>
-      <c r="X2" s="280"/>
-      <c r="Y2" s="280"/>
-      <c r="Z2" s="280"/>
-      <c r="AA2" s="280"/>
-      <c r="AB2" s="280"/>
-      <c r="AC2" s="280"/>
-      <c r="AD2" s="280"/>
-      <c r="AE2" s="280"/>
-      <c r="AF2" s="280"/>
-      <c r="AG2" s="280"/>
-      <c r="AH2" s="280"/>
-      <c r="AI2" s="280"/>
-      <c r="AJ2" s="280"/>
+      <c r="R2" s="275"/>
+      <c r="S2" s="275"/>
+      <c r="T2" s="275"/>
+      <c r="U2" s="275"/>
+      <c r="V2" s="275"/>
+      <c r="W2" s="275"/>
+      <c r="X2" s="275"/>
+      <c r="Y2" s="275"/>
+      <c r="Z2" s="275"/>
+      <c r="AA2" s="275"/>
+      <c r="AB2" s="275"/>
+      <c r="AC2" s="275"/>
+      <c r="AD2" s="275"/>
+      <c r="AE2" s="275"/>
+      <c r="AF2" s="275"/>
+      <c r="AG2" s="275"/>
+      <c r="AH2" s="275"/>
+      <c r="AI2" s="275"/>
+      <c r="AJ2" s="275"/>
     </row>
     <row r="3" spans="1:38" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="279"/>
-      <c r="D3" s="279"/>
-      <c r="E3" s="279"/>
-      <c r="F3" s="279"/>
-      <c r="G3" s="279"/>
-      <c r="H3" s="279"/>
-      <c r="I3" s="279"/>
-      <c r="J3" s="279"/>
-      <c r="K3" s="279"/>
-      <c r="L3" s="279"/>
-      <c r="M3" s="279"/>
-      <c r="N3" s="279"/>
-      <c r="O3" s="279"/>
-      <c r="P3" s="280"/>
-      <c r="Q3" s="280"/>
-      <c r="R3" s="280"/>
-      <c r="S3" s="280"/>
-      <c r="T3" s="280"/>
-      <c r="U3" s="280"/>
-      <c r="V3" s="280"/>
-      <c r="W3" s="280"/>
-      <c r="X3" s="280"/>
-      <c r="Y3" s="280"/>
-      <c r="Z3" s="280"/>
-      <c r="AA3" s="280"/>
-      <c r="AB3" s="280"/>
-      <c r="AC3" s="280"/>
-      <c r="AD3" s="280"/>
-      <c r="AE3" s="280"/>
-      <c r="AF3" s="280"/>
-      <c r="AG3" s="280"/>
-      <c r="AH3" s="280"/>
-      <c r="AI3" s="280"/>
-      <c r="AJ3" s="280"/>
+      <c r="C3" s="274"/>
+      <c r="D3" s="274"/>
+      <c r="E3" s="274"/>
+      <c r="F3" s="274"/>
+      <c r="G3" s="274"/>
+      <c r="H3" s="274"/>
+      <c r="I3" s="274"/>
+      <c r="J3" s="274"/>
+      <c r="K3" s="274"/>
+      <c r="L3" s="274"/>
+      <c r="M3" s="274"/>
+      <c r="N3" s="274"/>
+      <c r="O3" s="274"/>
+      <c r="P3" s="275"/>
+      <c r="Q3" s="275"/>
+      <c r="R3" s="275"/>
+      <c r="S3" s="275"/>
+      <c r="T3" s="275"/>
+      <c r="U3" s="275"/>
+      <c r="V3" s="275"/>
+      <c r="W3" s="275"/>
+      <c r="X3" s="275"/>
+      <c r="Y3" s="275"/>
+      <c r="Z3" s="275"/>
+      <c r="AA3" s="275"/>
+      <c r="AB3" s="275"/>
+      <c r="AC3" s="275"/>
+      <c r="AD3" s="275"/>
+      <c r="AE3" s="275"/>
+      <c r="AF3" s="275"/>
+      <c r="AG3" s="275"/>
+      <c r="AH3" s="275"/>
+      <c r="AI3" s="275"/>
+      <c r="AJ3" s="275"/>
     </row>
     <row r="4" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="263" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="264"/>
-      <c r="E4" s="264"/>
-      <c r="F4" s="264"/>
-      <c r="G4" s="264"/>
-      <c r="H4" s="264"/>
-      <c r="I4" s="264"/>
-      <c r="J4" s="264"/>
-      <c r="K4" s="264"/>
-      <c r="L4" s="264"/>
-      <c r="M4" s="264"/>
-      <c r="N4" s="264"/>
-      <c r="O4" s="264"/>
-      <c r="P4" s="264"/>
-      <c r="Q4" s="264"/>
-      <c r="R4" s="264"/>
-      <c r="S4" s="265"/>
-      <c r="T4" s="263" t="s">
+      <c r="C4" s="299" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="300"/>
+      <c r="E4" s="300"/>
+      <c r="F4" s="300"/>
+      <c r="G4" s="300"/>
+      <c r="H4" s="300"/>
+      <c r="I4" s="300"/>
+      <c r="J4" s="300"/>
+      <c r="K4" s="300"/>
+      <c r="L4" s="300"/>
+      <c r="M4" s="300"/>
+      <c r="N4" s="300"/>
+      <c r="O4" s="300"/>
+      <c r="P4" s="300"/>
+      <c r="Q4" s="300"/>
+      <c r="R4" s="300"/>
+      <c r="S4" s="301"/>
+      <c r="T4" s="299" t="s">
         <v>1</v>
       </c>
-      <c r="U4" s="264"/>
-      <c r="V4" s="264"/>
-      <c r="W4" s="264"/>
-      <c r="X4" s="264"/>
-      <c r="Y4" s="264"/>
-      <c r="Z4" s="264"/>
-      <c r="AA4" s="264"/>
-      <c r="AB4" s="265"/>
-      <c r="AC4" s="263" t="s">
+      <c r="U4" s="300"/>
+      <c r="V4" s="300"/>
+      <c r="W4" s="300"/>
+      <c r="X4" s="300"/>
+      <c r="Y4" s="300"/>
+      <c r="Z4" s="300"/>
+      <c r="AA4" s="300"/>
+      <c r="AB4" s="301"/>
+      <c r="AC4" s="299" t="s">
         <v>2</v>
       </c>
-      <c r="AD4" s="264"/>
-      <c r="AE4" s="264"/>
-      <c r="AF4" s="264"/>
-      <c r="AG4" s="274"/>
-      <c r="AH4" s="263" t="s">
+      <c r="AD4" s="300"/>
+      <c r="AE4" s="300"/>
+      <c r="AF4" s="300"/>
+      <c r="AG4" s="308"/>
+      <c r="AH4" s="299" t="s">
         <v>10</v>
       </c>
-      <c r="AI4" s="264"/>
-      <c r="AJ4" s="265"/>
+      <c r="AI4" s="300"/>
+      <c r="AJ4" s="301"/>
     </row>
     <row r="5" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="275" t="s">
+      <c r="C5" s="268" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="271"/>
-      <c r="E5" s="271"/>
-      <c r="F5" s="271"/>
-      <c r="G5" s="271"/>
-      <c r="H5" s="271"/>
-      <c r="I5" s="271"/>
-      <c r="J5" s="272"/>
-      <c r="K5" s="270" t="s">
+      <c r="D5" s="269"/>
+      <c r="E5" s="269"/>
+      <c r="F5" s="269"/>
+      <c r="G5" s="269"/>
+      <c r="H5" s="269"/>
+      <c r="I5" s="269"/>
+      <c r="J5" s="270"/>
+      <c r="K5" s="306" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="271"/>
-      <c r="M5" s="271"/>
-      <c r="N5" s="271"/>
-      <c r="O5" s="271"/>
-      <c r="P5" s="271"/>
-      <c r="Q5" s="271"/>
-      <c r="R5" s="272"/>
-      <c r="S5" s="266" t="s">
+      <c r="L5" s="269"/>
+      <c r="M5" s="269"/>
+      <c r="N5" s="269"/>
+      <c r="O5" s="269"/>
+      <c r="P5" s="269"/>
+      <c r="Q5" s="269"/>
+      <c r="R5" s="270"/>
+      <c r="S5" s="302" t="s">
         <v>12</v>
       </c>
-      <c r="T5" s="275" t="s">
+      <c r="T5" s="268" t="s">
         <v>9</v>
       </c>
-      <c r="U5" s="271"/>
-      <c r="V5" s="271"/>
-      <c r="W5" s="272"/>
-      <c r="X5" s="270" t="s">
+      <c r="U5" s="269"/>
+      <c r="V5" s="269"/>
+      <c r="W5" s="270"/>
+      <c r="X5" s="306" t="s">
         <v>8</v>
       </c>
-      <c r="Y5" s="271"/>
-      <c r="Z5" s="271"/>
-      <c r="AA5" s="272"/>
-      <c r="AB5" s="266" t="s">
+      <c r="Y5" s="269"/>
+      <c r="Z5" s="269"/>
+      <c r="AA5" s="270"/>
+      <c r="AB5" s="302" t="s">
         <v>13</v>
       </c>
-      <c r="AC5" s="273" t="s">
+      <c r="AC5" s="307" t="s">
         <v>9</v>
       </c>
-      <c r="AD5" s="272"/>
-      <c r="AE5" s="270" t="s">
+      <c r="AD5" s="270"/>
+      <c r="AE5" s="306" t="s">
         <v>8</v>
       </c>
-      <c r="AF5" s="272"/>
-      <c r="AG5" s="266" t="s">
+      <c r="AF5" s="270"/>
+      <c r="AG5" s="302" t="s">
         <v>14</v>
       </c>
       <c r="AH5" s="56"/>
       <c r="AI5" s="25"/>
-      <c r="AJ5" s="266" t="s">
+      <c r="AJ5" s="302" t="s">
         <v>15</v>
       </c>
       <c r="AK5" s="4"/>
@@ -4139,13 +4163,13 @@
         <f>Résultats!$J$3</f>
         <v>0</v>
       </c>
-      <c r="D6" s="240">
+      <c r="D6" s="239">
         <f>Résultats!$J$4</f>
         <v>4</v>
       </c>
-      <c r="E6" s="172">
+      <c r="E6" s="235">
         <f>Résultats!$J$6</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F6" s="109">
         <f>Résultats!$J$7</f>
@@ -4159,7 +4183,7 @@
         <f>Résultats!$J$11</f>
         <v>3</v>
       </c>
-      <c r="I6" s="236">
+      <c r="I6" s="235">
         <f>Résultats!$J$13</f>
         <v>4</v>
       </c>
@@ -4171,7 +4195,7 @@
         <f>Résultats!$J$17</f>
         <v>1</v>
       </c>
-      <c r="L6" s="240">
+      <c r="L6" s="239">
         <f>Résultats!$J$18</f>
         <v>4</v>
       </c>
@@ -4179,7 +4203,7 @@
         <f>Résultats!$J$20</f>
         <v>2</v>
       </c>
-      <c r="N6" s="249">
+      <c r="N6" s="245">
         <f>Résultats!$J$21</f>
         <v>4</v>
       </c>
@@ -4187,19 +4211,19 @@
         <f>Résultats!$J$24</f>
         <v>2</v>
       </c>
-      <c r="P6" s="249">
+      <c r="P6" s="245">
         <f>Résultats!$J$25</f>
         <v>4</v>
       </c>
-      <c r="Q6" s="111">
+      <c r="Q6" s="315">
         <f>Résultats!$J$27</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R6" s="108">
         <f>Résultats!$J$28</f>
         <v>3</v>
       </c>
-      <c r="S6" s="267"/>
+      <c r="S6" s="303"/>
       <c r="T6" s="169">
         <f>Résultats!$V$6</f>
         <v>0</v>
@@ -4232,7 +4256,7 @@
         <f>Résultats!$V$25</f>
         <v>0</v>
       </c>
-      <c r="AB6" s="267"/>
+      <c r="AB6" s="303"/>
       <c r="AC6" s="111">
         <f>Résultats!$AH$8</f>
         <v>0</v>
@@ -4249,7 +4273,7 @@
         <f>Résultats!$AH$23</f>
         <v>0</v>
       </c>
-      <c r="AG6" s="267"/>
+      <c r="AG6" s="303"/>
       <c r="AH6" s="212">
         <f>Résultats!$AH$15</f>
         <v>0</v>
@@ -4258,7 +4282,7 @@
         <f>Résultats!$AH$16</f>
         <v>0</v>
       </c>
-      <c r="AJ6" s="267"/>
+      <c r="AJ6" s="303"/>
       <c r="AK6" s="37"/>
     </row>
     <row r="7" spans="1:38" s="39" customFormat="1" ht="58.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -4269,22 +4293,22 @@
 +IF(ISBLANK($D10),0,($D$6*PT_VICTOIRE_R1)+IF($D$6=4,PT_PREDICTION_EQUIPE_R1+IF($D10=$C$6+$D$6,PT_PREDICTION_NB_PARTIES_R1,0),0))</f>
         <v>0</v>
       </c>
-      <c r="D7" s="241"/>
-      <c r="E7" s="173"/>
+      <c r="D7" s="240"/>
+      <c r="E7" s="236"/>
       <c r="F7" s="118"/>
       <c r="G7" s="119"/>
       <c r="H7" s="117"/>
-      <c r="I7" s="237"/>
+      <c r="I7" s="236"/>
       <c r="J7" s="117"/>
       <c r="K7" s="120"/>
-      <c r="L7" s="241"/>
+      <c r="L7" s="240"/>
       <c r="M7" s="173"/>
-      <c r="N7" s="250"/>
+      <c r="N7" s="246"/>
       <c r="O7" s="173"/>
-      <c r="P7" s="250"/>
-      <c r="Q7" s="119"/>
+      <c r="P7" s="246"/>
+      <c r="Q7" s="316"/>
       <c r="R7" s="117"/>
-      <c r="S7" s="267"/>
+      <c r="S7" s="303"/>
       <c r="T7" s="170"/>
       <c r="U7" s="117"/>
       <c r="V7" s="173"/>
@@ -4293,15 +4317,15 @@
       <c r="Y7" s="118"/>
       <c r="Z7" s="119"/>
       <c r="AA7" s="117"/>
-      <c r="AB7" s="267"/>
+      <c r="AB7" s="303"/>
       <c r="AC7" s="119"/>
       <c r="AD7" s="117"/>
       <c r="AE7" s="120"/>
       <c r="AF7" s="117"/>
-      <c r="AG7" s="267"/>
+      <c r="AG7" s="303"/>
       <c r="AH7" s="212"/>
       <c r="AI7" s="112"/>
-      <c r="AJ7" s="267"/>
+      <c r="AJ7" s="303"/>
       <c r="AK7" s="37"/>
     </row>
     <row r="8" spans="1:38" s="39" customFormat="1" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4311,11 +4335,11 @@
         <f>Résultats!$B$3</f>
         <v>TAMPA BAY</v>
       </c>
-      <c r="D8" s="242" t="str">
+      <c r="D8" s="241" t="str">
         <f>Résultats!$B$4</f>
         <v>COLUMBUS</v>
       </c>
-      <c r="E8" s="175" t="str">
+      <c r="E8" s="237" t="str">
         <f>Résultats!$B$6</f>
         <v>BOSTON</v>
       </c>
@@ -4331,7 +4355,7 @@
         <f>Résultats!$B$11</f>
         <v>CAROLINE</v>
       </c>
-      <c r="I8" s="238" t="str">
+      <c r="I8" s="237" t="str">
         <f>Résultats!$B$13</f>
         <v>NEW YORK I.</v>
       </c>
@@ -4343,7 +4367,7 @@
         <f>Résultats!$B$17</f>
         <v>CALGARY</v>
       </c>
-      <c r="L8" s="242" t="str">
+      <c r="L8" s="241" t="str">
         <f>Résultats!$B$18</f>
         <v>COLORADO</v>
       </c>
@@ -4351,7 +4375,7 @@
         <f>Résultats!$B$20</f>
         <v>WINNIPEG</v>
       </c>
-      <c r="N8" s="251" t="str">
+      <c r="N8" s="247" t="str">
         <f>Résultats!$B$21</f>
         <v>ST-LOUIS</v>
       </c>
@@ -4359,11 +4383,11 @@
         <f>Résultats!$B$24</f>
         <v>NASHVILLE</v>
       </c>
-      <c r="P8" s="251" t="str">
+      <c r="P8" s="247" t="str">
         <f>Résultats!$B$25</f>
         <v>DALLAS</v>
       </c>
-      <c r="Q8" s="177" t="str">
+      <c r="Q8" s="317" t="str">
         <f>Résultats!$B$27</f>
         <v>SAN JOSE</v>
       </c>
@@ -4371,14 +4395,14 @@
         <f>Résultats!$B$28</f>
         <v>VEGAS</v>
       </c>
-      <c r="S8" s="267"/>
+      <c r="S8" s="303"/>
       <c r="T8" s="171" t="str">
         <f>Résultats!$N$6</f>
-        <v xml:space="preserve"> </v>
+        <v>BOSTON</v>
       </c>
       <c r="U8" s="174" t="str">
         <f>Résultats!$N$7</f>
-        <v xml:space="preserve"> </v>
+        <v>COLUMBUS</v>
       </c>
       <c r="V8" s="175" t="str">
         <f>Résultats!$N$10</f>
@@ -4390,21 +4414,21 @@
       </c>
       <c r="X8" s="178" t="str">
         <f>Résultats!$N$20</f>
-        <v xml:space="preserve"> </v>
+        <v>ST-LOUIS</v>
       </c>
       <c r="Y8" s="176" t="str">
         <f>Résultats!$N$21</f>
-        <v xml:space="preserve"> </v>
+        <v>COLORADO</v>
       </c>
       <c r="Z8" s="177" t="str">
         <f>Résultats!$N$24</f>
-        <v xml:space="preserve"> </v>
+        <v>VEGAS</v>
       </c>
       <c r="AA8" s="174" t="str">
         <f>Résultats!$N$25</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="AB8" s="267"/>
+        <v>DALLAS</v>
+      </c>
+      <c r="AB8" s="303"/>
       <c r="AC8" s="177" t="str">
         <f>Résultats!$Z$8</f>
         <v xml:space="preserve"> </v>
@@ -4421,7 +4445,7 @@
         <f>Résultats!$Z$23</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AG8" s="267"/>
+      <c r="AG8" s="303"/>
       <c r="AH8" s="213" t="str">
         <f>Résultats!$Z$15</f>
         <v xml:space="preserve"> </v>
@@ -4430,7 +4454,7 @@
         <f>Résultats!$Z$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ8" s="267"/>
+      <c r="AJ8" s="303"/>
       <c r="AK8" s="37"/>
     </row>
     <row r="9" spans="1:38" s="39" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4444,11 +4468,11 @@
         <f>Résultats!$A$3</f>
         <v>A1</v>
       </c>
-      <c r="D9" s="243" t="str">
+      <c r="D9" s="242" t="str">
         <f>Résultats!$A$4</f>
         <v>WC2</v>
       </c>
-      <c r="E9" s="181" t="str">
+      <c r="E9" s="238" t="str">
         <f>Résultats!$A$6</f>
         <v>A2</v>
       </c>
@@ -4464,7 +4488,7 @@
         <f>Résultats!$A$11</f>
         <v>WC1</v>
       </c>
-      <c r="I9" s="239" t="str">
+      <c r="I9" s="238" t="str">
         <f>Résultats!$A$13</f>
         <v>M2</v>
       </c>
@@ -4476,7 +4500,7 @@
         <f>Résultats!$A$17</f>
         <v>C1</v>
       </c>
-      <c r="L9" s="243" t="str">
+      <c r="L9" s="242" t="str">
         <f>Résultats!$A$18</f>
         <v>WC2</v>
       </c>
@@ -4484,7 +4508,7 @@
         <f>Résultats!$A$20</f>
         <v>C2</v>
       </c>
-      <c r="N9" s="252" t="str">
+      <c r="N9" s="248" t="str">
         <f>Résultats!$A$21</f>
         <v>C3</v>
       </c>
@@ -4492,11 +4516,11 @@
         <f>Résultats!$A$24</f>
         <v>P1</v>
       </c>
-      <c r="P9" s="252" t="str">
+      <c r="P9" s="248" t="str">
         <f>Résultats!$A$25</f>
         <v>WC1</v>
       </c>
-      <c r="Q9" s="183" t="str">
+      <c r="Q9" s="318" t="str">
         <f>Résultats!$A$27</f>
         <v>P2</v>
       </c>
@@ -4504,14 +4528,14 @@
         <f>Résultats!$A$28</f>
         <v>P3</v>
       </c>
-      <c r="S9" s="269"/>
+      <c r="S9" s="305"/>
       <c r="T9" s="179" t="str">
         <f>Résultats!$M$6</f>
-        <v xml:space="preserve"> </v>
+        <v>A2</v>
       </c>
       <c r="U9" s="180" t="str">
         <f>Résultats!$M$7</f>
-        <v xml:space="preserve"> </v>
+        <v>WC2</v>
       </c>
       <c r="V9" s="181" t="str">
         <f>Résultats!$M$10</f>
@@ -4523,21 +4547,21 @@
       </c>
       <c r="X9" s="184" t="str">
         <f>Résultats!$M$20</f>
-        <v xml:space="preserve"> </v>
+        <v>C3</v>
       </c>
       <c r="Y9" s="182" t="str">
         <f>Résultats!$M$21</f>
-        <v xml:space="preserve"> </v>
+        <v>WC2</v>
       </c>
       <c r="Z9" s="183" t="str">
         <f>Résultats!$M$24</f>
-        <v xml:space="preserve"> </v>
+        <v>P3</v>
       </c>
       <c r="AA9" s="185" t="str">
         <f>Résultats!$M$25</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="AB9" s="268"/>
+        <v>WC1</v>
+      </c>
+      <c r="AB9" s="304"/>
       <c r="AC9" s="183" t="str">
         <f>Résultats!$Y$8</f>
         <v xml:space="preserve"> </v>
@@ -4554,7 +4578,7 @@
         <f>Résultats!$Y$23</f>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="AG9" s="268"/>
+      <c r="AG9" s="304"/>
       <c r="AH9" s="215" t="str">
         <f>Résultats!$Y$15</f>
         <v xml:space="preserve"> </v>
@@ -4563,7 +4587,7 @@
         <f>Résultats!$Y$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ9" s="269"/>
+      <c r="AJ9" s="305"/>
       <c r="AK9" s="114" t="s">
         <v>51</v>
       </c>
@@ -4577,43 +4601,43 @@
         <v>1</v>
       </c>
       <c r="B10" s="211" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C10" s="187">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D10" s="188"/>
-      <c r="E10" s="191"/>
-      <c r="F10" s="188">
-        <v>7</v>
-      </c>
+      <c r="E10" s="191">
+        <v>5</v>
+      </c>
+      <c r="F10" s="188"/>
       <c r="G10" s="192">
         <v>6</v>
       </c>
       <c r="H10" s="189"/>
-      <c r="I10" s="191"/>
-      <c r="J10" s="189">
-        <v>6</v>
-      </c>
-      <c r="K10" s="190"/>
-      <c r="L10" s="189">
-        <v>6</v>
-      </c>
+      <c r="I10" s="191">
+        <v>7</v>
+      </c>
+      <c r="J10" s="189"/>
+      <c r="K10" s="190">
+        <v>5</v>
+      </c>
+      <c r="L10" s="189"/>
       <c r="M10" s="191"/>
       <c r="N10" s="188">
+        <v>7</v>
+      </c>
+      <c r="O10" s="191">
         <v>6</v>
       </c>
-      <c r="O10" s="191">
-        <v>5</v>
-      </c>
       <c r="P10" s="188"/>
-      <c r="Q10" s="192"/>
-      <c r="R10" s="193">
-        <v>6</v>
-      </c>
+      <c r="Q10" s="323">
+        <v>7</v>
+      </c>
+      <c r="R10" s="193"/>
       <c r="S10" s="194">
         <f>SUM(C11:R11)</f>
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="T10" s="187"/>
       <c r="U10" s="189"/>
@@ -4621,7 +4645,7 @@
       <c r="W10" s="189"/>
       <c r="X10" s="190"/>
       <c r="Y10" s="188"/>
-      <c r="Z10" s="245"/>
+      <c r="Z10" s="192"/>
       <c r="AA10" s="193"/>
       <c r="AB10" s="194">
         <f>SUM(T11:AA11)</f>
@@ -4647,7 +4671,7 @@
       </c>
       <c r="AL10" s="194">
         <f>$S10+$AB10+$AG10+$AJ10</f>
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -4663,7 +4687,7 @@
       <c r="D11" s="134"/>
       <c r="E11" s="132">
         <f>(IF($E10&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E10=$E$6+$F$6,$O$103,0),0),0)+IF($F10&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F10=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F11" s="134"/>
       <c r="G11" s="132">
@@ -4673,17 +4697,17 @@
       <c r="H11" s="134"/>
       <c r="I11" s="135">
         <f>(IF($I10&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I10=$I$6+$J$6,$O$103,0),0),0)+IF($J10&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J10=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J11" s="136"/>
       <c r="K11" s="137">
         <f>(IF($K10&lt;&gt;"",($K$6*$O$104)+IF($K$6=4,($O$102)+IF($K10=$K$6+$L$6,$O$103,0),0),0)+IF($L10&lt;&gt;"",($L$6*$O$104)+IF($L$6=4,($O$102)+IF($L10=$K$6+$L$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="L11" s="134"/>
       <c r="M11" s="132">
         <f>(IF($M10&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M10=$M$6+$N$6,$O$103,0),0),0)+IF($N10&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N10=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="N11" s="134"/>
       <c r="O11" s="135">
@@ -4691,9 +4715,9 @@
         <v>2</v>
       </c>
       <c r="P11" s="134"/>
-      <c r="Q11" s="135">
+      <c r="Q11" s="132">
         <f>(IF($Q10&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q10=$Q$6+$R$6,$O$103,0),0),0)+IF($R10&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R10=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="R11" s="138"/>
       <c r="S11" s="128"/>
@@ -4738,7 +4762,7 @@
         <f>IF(ISBLANK(E10),
 0,
 IF(E$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="124">
         <f>IF(ISBLANK(F10),
@@ -4762,7 +4786,7 @@
         <f>IF(ISBLANK(I10),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" s="124">
         <f>IF(ISBLANK(J10),
@@ -4780,7 +4804,7 @@
         <f>IF(ISBLANK(L10),
 0,
 IF(L$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M12" s="124">
         <f>IF(ISBLANK(M10),
@@ -4806,11 +4830,11 @@
 IF(P$6 = 4, 1, 0))</f>
         <v>0</v>
       </c>
-      <c r="Q12" s="124">
+      <c r="Q12" s="146">
         <f>IF(ISBLANK(Q10),
 0,
 IF(Q$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R12" s="124">
         <f>IF(ISBLANK(R10),
@@ -4838,7 +4862,7 @@
       <c r="AJ12" s="147"/>
       <c r="AK12" s="148">
         <f>SUM(C12:AI12)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AL12" s="130"/>
     </row>
@@ -4917,7 +4941,7 @@
         <f>IF(N12 = 0,
 0,
 IF(N10 = (M$6+N$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O13" s="124">
         <f>IF(O12 = 0,
@@ -4931,11 +4955,11 @@
 IF(P10 = (O$6+P$6),1,0))</f>
         <v>0</v>
       </c>
-      <c r="Q13" s="124">
+      <c r="Q13" s="146">
         <f>IF(Q12 = 0,
 0,
 IF(Q10 = (Q$6+R$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R13" s="124">
         <f>IF(R12 = 0,
@@ -4973,18 +4997,18 @@
         <v>2</v>
       </c>
       <c r="B14" s="88" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C14" s="46">
         <v>5</v>
       </c>
       <c r="D14" s="45"/>
-      <c r="E14" s="44">
+      <c r="E14" s="319">
         <v>7</v>
       </c>
       <c r="F14" s="45"/>
       <c r="G14" s="48">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H14" s="47"/>
       <c r="I14" s="44">
@@ -4992,39 +5016,39 @@
       </c>
       <c r="J14" s="47"/>
       <c r="K14" s="49">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L14" s="47"/>
       <c r="M14" s="44">
+        <v>6</v>
+      </c>
+      <c r="N14" s="45"/>
+      <c r="O14" s="44">
         <v>5</v>
       </c>
-      <c r="N14" s="45"/>
-      <c r="O14" s="44"/>
-      <c r="P14" s="45">
+      <c r="P14" s="45"/>
+      <c r="Q14" s="324">
         <v>7</v>
       </c>
-      <c r="Q14" s="48"/>
-      <c r="R14" s="50">
-        <v>7</v>
-      </c>
+      <c r="R14" s="50"/>
       <c r="S14" s="129">
         <f>SUM(C15:R15)</f>
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="T14" s="46"/>
       <c r="U14" s="47"/>
       <c r="V14" s="44"/>
       <c r="W14" s="47"/>
       <c r="X14" s="49"/>
-      <c r="Y14" s="127"/>
-      <c r="Z14" s="48"/>
+      <c r="Y14" s="45"/>
+      <c r="Z14" s="243"/>
       <c r="AA14" s="50"/>
       <c r="AB14" s="129">
         <f>SUM(T15:AA15)</f>
         <v>0</v>
       </c>
       <c r="AC14" s="48"/>
-      <c r="AD14" s="308"/>
+      <c r="AD14" s="47"/>
       <c r="AE14" s="49"/>
       <c r="AF14" s="47"/>
       <c r="AG14" s="129">
@@ -5039,11 +5063,11 @@
       </c>
       <c r="AK14" s="116">
         <f>MAX($AL$10:$AL$97) - AL14</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AL14" s="129">
         <f>$S14+$AB14+$AG14+$AJ14</f>
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5059,7 +5083,7 @@
       <c r="D15" s="150"/>
       <c r="E15" s="132">
         <f>(IF($E14&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E14=$E$6+$F$6,$O$103,0),0),0)+IF($F14&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F14=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F15" s="150"/>
       <c r="G15" s="132">
@@ -5084,12 +5108,12 @@
       <c r="N15" s="150"/>
       <c r="O15" s="126">
         <f>(IF($O14&lt;&gt;"",($O$6*$O$104)+IF($O$6=4,($O$102)+IF($O14=$O$6+$P$6,$O$103,0),0),0)+IF($P14&lt;&gt;"",($P$6*$O$104)+IF($P$6=4,($O$102)+IF($P14=$O$6+$P$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="P15" s="150"/>
       <c r="Q15" s="126">
         <f>(IF($Q14&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q14=$Q$6+$R$6,$O$103,0),0),0)+IF($R14&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R14=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="R15" s="153"/>
       <c r="S15" s="154"/>
@@ -5112,7 +5136,7 @@
       <c r="AJ15" s="128"/>
       <c r="AK15" s="96">
         <f>MAX($AL$10:$AL$97) - AL15</f>
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="AL15" s="128"/>
     </row>
@@ -5133,11 +5157,11 @@
 IF(D$6 = 4, 1, 0))</f>
         <v>0</v>
       </c>
-      <c r="E16" s="124">
+      <c r="E16" s="146">
         <f>IF(ISBLANK(E14),
 0,
 IF(E$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="124">
         <f>IF(ISBLANK(F14),
@@ -5203,13 +5227,13 @@
         <f>IF(ISBLANK(P14),
 0,
 IF(P$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q16" s="124">
         <f>IF(ISBLANK(Q14),
 0,
 IF(Q$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R16" s="124">
         <f>IF(ISBLANK(R14),
@@ -5237,7 +5261,7 @@
       <c r="AJ16" s="147"/>
       <c r="AK16" s="148">
         <f>SUM(C16:AI16)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL16" s="130"/>
     </row>
@@ -5258,11 +5282,11 @@
 IF(D14 = (C$6+D$6),1,0))</f>
         <v>0</v>
       </c>
-      <c r="E17" s="124">
+      <c r="E17" s="146">
         <f>IF(E16 = 0,
 0,
 IF(E14 = (E$6+F$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="124">
         <f>IF(F16 = 0,
@@ -5334,7 +5358,7 @@
         <f>IF(Q16 = 0,
 0,
 IF(Q14 = (Q$6+R$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R17" s="124">
         <f>IF(R16 = 0,
@@ -5362,24 +5386,24 @@
       <c r="AJ17" s="147"/>
       <c r="AK17" s="148">
         <f>SUM(C17:AI17)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL17" s="130"/>
     </row>
     <row r="18" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="186">
         <f>RANK(AL18,$AL$10:$AL$97,)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B18" s="211" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C18" s="198">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D18" s="199"/>
-      <c r="E18" s="200">
-        <v>5</v>
+      <c r="E18" s="320">
+        <v>7</v>
       </c>
       <c r="F18" s="199"/>
       <c r="G18" s="201">
@@ -5387,35 +5411,35 @@
       </c>
       <c r="H18" s="202"/>
       <c r="I18" s="200">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J18" s="202"/>
       <c r="K18" s="203">
+        <v>4</v>
+      </c>
+      <c r="L18" s="202"/>
+      <c r="M18" s="200">
         <v>5</v>
       </c>
-      <c r="L18" s="202"/>
-      <c r="M18" s="200"/>
-      <c r="N18" s="199">
+      <c r="N18" s="199"/>
+      <c r="O18" s="200"/>
+      <c r="P18" s="199">
         <v>7</v>
       </c>
-      <c r="O18" s="200">
-        <v>6</v>
-      </c>
-      <c r="P18" s="199"/>
-      <c r="Q18" s="201">
+      <c r="Q18" s="201"/>
+      <c r="R18" s="204">
         <v>7</v>
       </c>
-      <c r="R18" s="204"/>
-      <c r="S18" s="246">
+      <c r="S18" s="244">
         <f>SUM(C19:R19)</f>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="T18" s="198"/>
       <c r="U18" s="202"/>
       <c r="V18" s="200"/>
       <c r="W18" s="202"/>
       <c r="X18" s="203"/>
-      <c r="Y18" s="199"/>
+      <c r="Y18" s="234"/>
       <c r="Z18" s="201"/>
       <c r="AA18" s="204"/>
       <c r="AB18" s="205">
@@ -5423,7 +5447,7 @@
         <v>0</v>
       </c>
       <c r="AC18" s="201"/>
-      <c r="AD18" s="202"/>
+      <c r="AD18" s="311"/>
       <c r="AE18" s="203"/>
       <c r="AF18" s="202"/>
       <c r="AG18" s="205">
@@ -5438,11 +5462,11 @@
       </c>
       <c r="AK18" s="207">
         <f>MAX($AL$10:$AL$97) - AL18</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AL18" s="205">
         <f>$S18+$AB18+$AG18+$AJ18</f>
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5456,9 +5480,9 @@
         <v>0</v>
       </c>
       <c r="D19" s="150"/>
-      <c r="E19" s="126">
+      <c r="E19" s="132">
         <f>(IF($E18&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E18=$E$6+$F$6,$O$103,0),0),0)+IF($F18&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F18=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F19" s="150"/>
       <c r="G19" s="126">
@@ -5478,12 +5502,12 @@
       <c r="L19" s="150"/>
       <c r="M19" s="126">
         <f>(IF($M18&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M18=$M$6+$N$6,$O$103,0),0),0)+IF($N18&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N18=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="N19" s="150"/>
       <c r="O19" s="126">
         <f>(IF($O18&lt;&gt;"",($O$6*$O$104)+IF($O$6=4,($O$102)+IF($O18=$O$6+$P$6,$O$103,0),0),0)+IF($P18&lt;&gt;"",($P$6*$O$104)+IF($P$6=4,($O$102)+IF($P18=$O$6+$P$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="P19" s="150"/>
       <c r="Q19" s="126">
@@ -5511,7 +5535,7 @@
       <c r="AJ19" s="154"/>
       <c r="AK19" s="162">
         <f>MAX($AL$10:$AL$97) - AL19</f>
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="AL19" s="128"/>
     </row>
@@ -5532,11 +5556,11 @@
 IF(D$6 = 4, 1, 0))</f>
         <v>0</v>
       </c>
-      <c r="E20" s="124">
+      <c r="E20" s="146">
         <f>IF(ISBLANK(E18),
 0,
 IF(E$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="124">
         <f>IF(ISBLANK(F18),
@@ -5590,7 +5614,7 @@
         <f>IF(ISBLANK(N18),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O20" s="124">
         <f>IF(ISBLANK(O18),
@@ -5602,7 +5626,7 @@
         <f>IF(ISBLANK(P18),
 0,
 IF(P$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q20" s="124">
         <f>IF(ISBLANK(Q18),
@@ -5636,7 +5660,7 @@
       <c r="AJ20" s="147"/>
       <c r="AK20" s="148">
         <f>SUM(C20:AI20)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL20" s="130"/>
     </row>
@@ -5657,11 +5681,11 @@
 IF(D18 = (C$6+D$6),1,0))</f>
         <v>0</v>
       </c>
-      <c r="E21" s="124">
+      <c r="E21" s="146">
         <f>IF(E20 = 0,
 0,
 IF(E18 = (E$6+F$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="124">
         <f>IF(F20 = 0,
@@ -5761,7 +5785,7 @@
       <c r="AJ21" s="147"/>
       <c r="AK21" s="148">
         <f>SUM(C21:AI21)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL21" s="130"/>
     </row>
@@ -5771,50 +5795,50 @@
         <v>4</v>
       </c>
       <c r="B22" s="88" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C22" s="46">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D22" s="45"/>
-      <c r="E22" s="44">
-        <v>4</v>
+      <c r="E22" s="319">
+        <v>7</v>
       </c>
       <c r="F22" s="45"/>
       <c r="G22" s="48">
+        <v>4</v>
+      </c>
+      <c r="H22" s="47"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="47">
         <v>6</v>
       </c>
-      <c r="H22" s="47"/>
-      <c r="I22" s="44">
+      <c r="K22" s="49">
+        <v>5</v>
+      </c>
+      <c r="L22" s="47"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="321">
         <v>6</v>
       </c>
-      <c r="J22" s="47"/>
-      <c r="K22" s="49">
+      <c r="O22" s="44">
         <v>7</v>
       </c>
-      <c r="L22" s="47"/>
-      <c r="M22" s="44">
-        <v>5</v>
-      </c>
-      <c r="N22" s="45"/>
-      <c r="O22" s="44">
-        <v>4</v>
-      </c>
       <c r="P22" s="45"/>
-      <c r="Q22" s="48"/>
-      <c r="R22" s="50">
+      <c r="Q22" s="48">
         <v>6</v>
       </c>
+      <c r="R22" s="50"/>
       <c r="S22" s="129">
         <f>SUM(C23:R23)</f>
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="T22" s="46"/>
       <c r="U22" s="47"/>
       <c r="V22" s="44"/>
       <c r="W22" s="47"/>
       <c r="X22" s="49"/>
-      <c r="Y22" s="127"/>
+      <c r="Y22" s="45"/>
       <c r="Z22" s="48"/>
       <c r="AA22" s="50"/>
       <c r="AB22" s="129">
@@ -5829,7 +5853,7 @@
         <f>SUM(AC23:AF23)</f>
         <v>0</v>
       </c>
-      <c r="AH22" s="234"/>
+      <c r="AH22" s="309"/>
       <c r="AI22" s="57"/>
       <c r="AJ22" s="129">
         <f>AH23</f>
@@ -5837,11 +5861,11 @@
       </c>
       <c r="AK22" s="116">
         <f>MAX($AL$10:$AL$97) - AL22</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AL22" s="129">
         <f>$S22+$AB22+$AG22+$AJ22</f>
-        <v>23</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5857,7 +5881,7 @@
       <c r="D23" s="163"/>
       <c r="E23" s="132">
         <f>(IF($E22&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E22=$E$6+$F$6,$O$103,0),0),0)+IF($F22&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F22=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F23" s="163"/>
       <c r="G23" s="132">
@@ -5867,7 +5891,7 @@
       <c r="H23" s="163"/>
       <c r="I23" s="132">
         <f>(IF($I22&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I22=$I$6+$J$6,$O$103,0),0),0)+IF($J22&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J22=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J23" s="164"/>
       <c r="K23" s="165">
@@ -5877,7 +5901,7 @@
       <c r="L23" s="163"/>
       <c r="M23" s="132">
         <f>(IF($M22&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M22=$M$6+$N$6,$O$103,0),0),0)+IF($N22&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N22=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="N23" s="163"/>
       <c r="O23" s="132">
@@ -5887,7 +5911,7 @@
       <c r="P23" s="163"/>
       <c r="Q23" s="132">
         <f>(IF($Q22&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q22=$Q$6+$R$6,$O$103,0),0),0)+IF($R22&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R22=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="R23" s="166"/>
       <c r="S23" s="154"/>
@@ -5910,7 +5934,7 @@
       <c r="AJ23" s="154"/>
       <c r="AK23" s="162">
         <f>MAX($AL$10:$AL$97) - AL23</f>
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="AL23" s="128"/>
     </row>
@@ -5935,7 +5959,7 @@
         <f>IF(ISBLANK(E22),
 0,
 IF(E$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" s="124">
         <f>IF(ISBLANK(F22),
@@ -5959,7 +5983,7 @@
         <f>IF(ISBLANK(I22),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" s="124">
         <f>IF(ISBLANK(J22),
@@ -5985,11 +6009,11 @@
 IF(M$6= 4, 1, 0))</f>
         <v>0</v>
       </c>
-      <c r="N24" s="124">
+      <c r="N24" s="146">
         <f>IF(ISBLANK(N22),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O24" s="124">
         <f>IF(ISBLANK(O22),
@@ -6007,7 +6031,7 @@
         <f>IF(ISBLANK(Q22),
 0,
 IF(Q$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R24" s="124">
         <f>IF(ISBLANK(R22),
@@ -6035,7 +6059,7 @@
       <c r="AJ24" s="147"/>
       <c r="AK24" s="148">
         <f>SUM(C24:AI24)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AL24" s="130"/>
     </row>
@@ -6060,7 +6084,7 @@
         <f>IF(E24 = 0,
 0,
 IF(E22 = (E$6+F$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="124">
         <f>IF(F24 = 0,
@@ -6110,11 +6134,11 @@
 IF(M22 = (M$6+N$6),1,0))</f>
         <v>0</v>
       </c>
-      <c r="N25" s="124">
+      <c r="N25" s="146">
         <f>IF(N24 = 0,
 0,
 IF(N22 = (M$6+N$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O25" s="124">
         <f>IF(O24 = 0,
@@ -6160,14 +6184,14 @@
       <c r="AJ25" s="147"/>
       <c r="AK25" s="148">
         <f>SUM(C25:AI25)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL25" s="130"/>
     </row>
     <row r="26" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="186">
         <f>RANK(AL26,$AL$10:$AL$97,)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B26" s="211" t="s">
         <v>77</v>
@@ -6193,7 +6217,7 @@
       </c>
       <c r="L26" s="202"/>
       <c r="M26" s="200"/>
-      <c r="N26" s="199">
+      <c r="N26" s="322">
         <v>6</v>
       </c>
       <c r="O26" s="200">
@@ -6206,7 +6230,7 @@
       <c r="R26" s="204"/>
       <c r="S26" s="205">
         <f>SUM(C27:R27)</f>
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="T26" s="198"/>
       <c r="U26" s="202"/>
@@ -6236,11 +6260,11 @@
       </c>
       <c r="AK26" s="207">
         <f>MAX($AL$10:$AL$97) - AL26</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AL26" s="205">
         <f>$S26+$AB26+$AG26+$AJ26</f>
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6256,7 +6280,7 @@
       <c r="D27" s="150"/>
       <c r="E27" s="126">
         <f>(IF($E26&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E26=$E$6+$F$6,$O$103,0),0),0)+IF($F26&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F26=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F27" s="150"/>
       <c r="G27" s="126">
@@ -6286,7 +6310,7 @@
       <c r="P27" s="150"/>
       <c r="Q27" s="126">
         <f>(IF($Q26&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q26=$Q$6+$R$6,$O$103,0),0),0)+IF($R26&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R26=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="R27" s="153"/>
       <c r="S27" s="154"/>
@@ -6309,7 +6333,7 @@
       <c r="AJ27" s="154"/>
       <c r="AK27" s="162">
         <f>MAX($AL$10:$AL$97) - AL27</f>
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="AL27" s="128"/>
     </row>
@@ -6334,7 +6358,7 @@
         <f>IF(ISBLANK(E26),
 0,
 IF(E$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" s="124">
         <f>IF(ISBLANK(F26),
@@ -6406,7 +6430,7 @@
         <f>IF(ISBLANK(Q26),
 0,
 IF(Q$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R28" s="124">
         <f>IF(ISBLANK(R26),
@@ -6434,7 +6458,7 @@
       <c r="AJ28" s="147"/>
       <c r="AK28" s="148">
         <f>SUM(C28:AI28)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AL28" s="130"/>
     </row>
@@ -6566,46 +6590,46 @@
     <row r="30" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="122">
         <f>RANK(AL30,$AL$10:$AL$97,)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B30" s="88" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="C30" s="46">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D30" s="45"/>
       <c r="E30" s="44">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F30" s="45"/>
       <c r="G30" s="48">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H30" s="47"/>
-      <c r="I30" s="44">
+      <c r="I30" s="44"/>
+      <c r="J30" s="47">
         <v>6</v>
       </c>
-      <c r="J30" s="47"/>
       <c r="K30" s="49">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L30" s="47"/>
-      <c r="M30" s="44">
+      <c r="M30" s="44"/>
+      <c r="N30" s="45">
+        <v>7</v>
+      </c>
+      <c r="O30" s="44">
         <v>6</v>
       </c>
-      <c r="N30" s="45"/>
-      <c r="O30" s="44">
-        <v>5</v>
-      </c>
       <c r="P30" s="45"/>
-      <c r="Q30" s="48">
+      <c r="Q30" s="324">
         <v>7</v>
       </c>
       <c r="R30" s="50"/>
       <c r="S30" s="129">
         <f>SUM(C31:R31)</f>
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="T30" s="46"/>
       <c r="U30" s="47"/>
@@ -6613,7 +6637,7 @@
       <c r="W30" s="47"/>
       <c r="X30" s="49"/>
       <c r="Y30" s="45"/>
-      <c r="Z30" s="244"/>
+      <c r="Z30" s="243"/>
       <c r="AA30" s="47"/>
       <c r="AB30" s="129">
         <f>SUM(T31:AA31)</f>
@@ -6635,11 +6659,11 @@
       </c>
       <c r="AK30" s="116">
         <f>MAX($AL$10:$AL$97) - AL30</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AL30" s="129">
         <f>$S30+$AB30+$AG30+$AJ30</f>
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6655,7 +6679,7 @@
       <c r="D31" s="80"/>
       <c r="E31" s="81">
         <f>(IF($E30&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E30=$E$6+$F$6,$O$103,0),0),0)+IF($F30&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F30=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F31" s="80"/>
       <c r="G31" s="81">
@@ -6665,7 +6689,7 @@
       <c r="H31" s="80"/>
       <c r="I31" s="81">
         <f>(IF($I30&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I30=$I$6+$J$6,$O$103,0),0),0)+IF($J30&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J30=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J31" s="82"/>
       <c r="K31" s="83">
@@ -6675,7 +6699,7 @@
       <c r="L31" s="80"/>
       <c r="M31" s="81">
         <f>(IF($M30&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M30=$M$6+$N$6,$O$103,0),0),0)+IF($N30&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N30=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="N31" s="80"/>
       <c r="O31" s="81">
@@ -6685,7 +6709,7 @@
       <c r="P31" s="80"/>
       <c r="Q31" s="81">
         <f>(IF($Q30&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q30=$Q$6+$R$6,$O$103,0),0),0)+IF($R30&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R30=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="R31" s="84"/>
       <c r="S31" s="128"/>
@@ -6708,7 +6732,7 @@
       <c r="AJ31" s="128"/>
       <c r="AK31" s="96">
         <f>MAX($AL$10:$AL$97) - AL31</f>
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="AL31" s="128"/>
     </row>
@@ -6733,7 +6757,7 @@
         <f>IF(ISBLANK(E30),
 0,
 IF(E$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" s="124">
         <f>IF(ISBLANK(F30),
@@ -6757,7 +6781,7 @@
         <f>IF(ISBLANK(I30),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J32" s="124">
         <f>IF(ISBLANK(J30),
@@ -6787,7 +6811,7 @@
         <f>IF(ISBLANK(N30),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O32" s="124">
         <f>IF(ISBLANK(O30),
@@ -6805,7 +6829,7 @@
         <f>IF(ISBLANK(Q30),
 0,
 IF(Q$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R32" s="124">
         <f>IF(ISBLANK(R30),
@@ -6833,7 +6857,7 @@
       <c r="AJ32" s="147"/>
       <c r="AK32" s="148">
         <f>SUM(C32:AI32)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AL32" s="130"/>
     </row>
@@ -6930,7 +6954,7 @@
         <f>IF(Q32 = 0,
 0,
 IF(Q30 = (Q$6+R$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R33" s="124">
         <f>IF(R32 = 0,
@@ -6958,40 +6982,40 @@
       <c r="AJ33" s="147"/>
       <c r="AK33" s="148">
         <f>SUM(C33:AI33)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL33" s="130"/>
     </row>
     <row r="34" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="186">
         <f>RANK(AL34,$AL$10:$AL$97,)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B34" s="211" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C34" s="198">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D34" s="199"/>
-      <c r="E34" s="200">
-        <v>5</v>
-      </c>
-      <c r="F34" s="199"/>
+      <c r="E34" s="200"/>
+      <c r="F34" s="199">
+        <v>7</v>
+      </c>
       <c r="G34" s="201">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H34" s="202"/>
       <c r="I34" s="200"/>
       <c r="J34" s="202">
         <v>6</v>
       </c>
-      <c r="K34" s="203">
-        <v>5</v>
-      </c>
-      <c r="L34" s="202"/>
+      <c r="K34" s="203"/>
+      <c r="L34" s="202">
+        <v>6</v>
+      </c>
       <c r="M34" s="200"/>
-      <c r="N34" s="199">
+      <c r="N34" s="322">
         <v>6</v>
       </c>
       <c r="O34" s="200">
@@ -7004,7 +7028,7 @@
       </c>
       <c r="S34" s="205">
         <f>SUM(C35:R35)</f>
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="T34" s="198"/>
       <c r="U34" s="202"/>
@@ -7012,7 +7036,7 @@
       <c r="W34" s="202"/>
       <c r="X34" s="203"/>
       <c r="Y34" s="199"/>
-      <c r="Z34" s="201"/>
+      <c r="Z34" s="208"/>
       <c r="AA34" s="202"/>
       <c r="AB34" s="205">
         <f>SUM(T35:AA35)</f>
@@ -7026,7 +7050,7 @@
         <f>SUM(AC35:AF35)</f>
         <v>0</v>
       </c>
-      <c r="AH34" s="253"/>
+      <c r="AH34" s="209"/>
       <c r="AI34" s="196"/>
       <c r="AJ34" s="205">
         <f>AH35</f>
@@ -7034,11 +7058,11 @@
       </c>
       <c r="AK34" s="207">
         <f>MAX($AL$10:$AL$97) - AL34</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="AL34" s="205">
         <f>$S34+$AB34+$AG34+$AJ34</f>
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7069,7 +7093,7 @@
       <c r="J35" s="82"/>
       <c r="K35" s="83">
         <f>(IF($K34&lt;&gt;"",($K$6*$O$104)+IF($K$6=4,($O$102)+IF($K34=$K$6+$L$6,$O$103,0),0),0)+IF($L34&lt;&gt;"",($L$6*$O$104)+IF($L$6=4,($O$102)+IF($L34=$K$6+$L$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="L35" s="80"/>
       <c r="M35" s="81">
@@ -7107,7 +7131,7 @@
       <c r="AJ35" s="128"/>
       <c r="AK35" s="96">
         <f>MAX($AL$10:$AL$97) - AL35</f>
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="AL35" s="128"/>
     </row>
@@ -7174,7 +7198,7 @@
         <f>IF(ISBLANK(L34),
 0,
 IF(L$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M36" s="124">
         <f>IF(ISBLANK(M34),
@@ -7232,7 +7256,7 @@
       <c r="AJ36" s="147"/>
       <c r="AK36" s="148">
         <f>SUM(C36:AI36)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL36" s="130"/>
     </row>
@@ -7364,53 +7388,53 @@
     <row r="38" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="122">
         <f>RANK(AL38,$AL$10:$AL$97,)</f>
+        <v>8</v>
+      </c>
+      <c r="B38" s="88" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" s="46">
         <v>4</v>
-      </c>
-      <c r="B38" s="88" t="s">
-        <v>70</v>
-      </c>
-      <c r="C38" s="46">
-        <v>5</v>
       </c>
       <c r="D38" s="45"/>
       <c r="E38" s="44">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F38" s="45"/>
       <c r="G38" s="48">
+        <v>6</v>
+      </c>
+      <c r="H38" s="47"/>
+      <c r="I38" s="44">
+        <v>6</v>
+      </c>
+      <c r="J38" s="47"/>
+      <c r="K38" s="49">
+        <v>7</v>
+      </c>
+      <c r="L38" s="47"/>
+      <c r="M38" s="44">
+        <v>5</v>
+      </c>
+      <c r="N38" s="45"/>
+      <c r="O38" s="44">
         <v>4</v>
       </c>
-      <c r="H38" s="47"/>
-      <c r="I38" s="44"/>
-      <c r="J38" s="47">
+      <c r="P38" s="45"/>
+      <c r="Q38" s="48"/>
+      <c r="R38" s="50">
         <v>6</v>
       </c>
-      <c r="K38" s="49">
-        <v>5</v>
-      </c>
-      <c r="L38" s="47"/>
-      <c r="M38" s="44"/>
-      <c r="N38" s="45">
-        <v>6</v>
-      </c>
-      <c r="O38" s="44">
-        <v>7</v>
-      </c>
-      <c r="P38" s="45"/>
-      <c r="Q38" s="48">
-        <v>6</v>
-      </c>
-      <c r="R38" s="50"/>
       <c r="S38" s="129">
         <f>SUM(C39:R39)</f>
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="T38" s="46"/>
       <c r="U38" s="47"/>
       <c r="V38" s="44"/>
       <c r="W38" s="47"/>
       <c r="X38" s="49"/>
-      <c r="Y38" s="45"/>
+      <c r="Y38" s="127"/>
       <c r="Z38" s="48"/>
       <c r="AA38" s="47"/>
       <c r="AB38" s="129">
@@ -7425,7 +7449,7 @@
         <f>SUM(AC39:AF39)</f>
         <v>0</v>
       </c>
-      <c r="AH38" s="247"/>
+      <c r="AH38" s="107"/>
       <c r="AI38" s="57"/>
       <c r="AJ38" s="129">
         <f>AH39</f>
@@ -7433,11 +7457,11 @@
       </c>
       <c r="AK38" s="116">
         <f>MAX($AL$10:$AL$97) - AL38</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="AL38" s="129">
         <f>$S38+$AB38+$AG38+$AJ38</f>
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7453,7 +7477,7 @@
       <c r="D39" s="80"/>
       <c r="E39" s="121">
         <f>(IF($E38&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E38=$E$6+$F$6,$O$103,0),0),0)+IF($F38&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F38=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F39" s="80"/>
       <c r="G39" s="125">
@@ -7463,7 +7487,7 @@
       <c r="H39" s="80"/>
       <c r="I39" s="121">
         <f>(IF($I38&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I38=$I$6+$J$6,$O$103,0),0),0)+IF($J38&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J38=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J39" s="82"/>
       <c r="K39" s="83">
@@ -7473,7 +7497,7 @@
       <c r="L39" s="80"/>
       <c r="M39" s="81">
         <f>(IF($M38&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M38=$M$6+$N$6,$O$103,0),0),0)+IF($N38&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N38=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="N39" s="80"/>
       <c r="O39" s="81">
@@ -7506,7 +7530,7 @@
       <c r="AJ39" s="128"/>
       <c r="AK39" s="96">
         <f>MAX($AL$10:$AL$97) - AL39</f>
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="AL39" s="128"/>
     </row>
@@ -7531,7 +7555,7 @@
         <f>IF(ISBLANK(E38),
 0,
 IF(E$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F40" s="124">
         <f>IF(ISBLANK(F38),
@@ -7555,7 +7579,7 @@
         <f>IF(ISBLANK(I38),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J40" s="124">
         <f>IF(ISBLANK(J38),
@@ -7585,7 +7609,7 @@
         <f>IF(ISBLANK(N38),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O40" s="124">
         <f>IF(ISBLANK(O38),
@@ -7631,7 +7655,7 @@
       <c r="AJ40" s="147"/>
       <c r="AK40" s="148">
         <f>SUM(C40:AI40)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL40" s="130"/>
     </row>
@@ -7710,7 +7734,7 @@
         <f>IF(N40 = 0,
 0,
 IF(N38 = (M$6+N$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O41" s="124">
         <f>IF(O40 = 0,
@@ -7756,44 +7780,44 @@
       <c r="AJ41" s="147"/>
       <c r="AK41" s="148">
         <f>SUM(C41:AI41)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL41" s="130"/>
     </row>
     <row r="42" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="186">
         <f>RANK(AL42,$AL$10:$AL$97,)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B42" s="211" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="C42" s="198">
         <v>5</v>
       </c>
       <c r="D42" s="199"/>
       <c r="E42" s="200">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F42" s="199"/>
       <c r="G42" s="201">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H42" s="202"/>
       <c r="I42" s="200"/>
       <c r="J42" s="202">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K42" s="203">
         <v>5</v>
       </c>
       <c r="L42" s="202"/>
       <c r="M42" s="200"/>
-      <c r="N42" s="199">
+      <c r="N42" s="322">
         <v>6</v>
       </c>
       <c r="O42" s="200">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P42" s="199"/>
       <c r="Q42" s="201"/>
@@ -7802,7 +7826,7 @@
       </c>
       <c r="S42" s="205">
         <f>SUM(C43:R43)</f>
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="T42" s="198"/>
       <c r="U42" s="202"/>
@@ -7824,7 +7848,7 @@
         <f>SUM(AC43:AF43)</f>
         <v>0</v>
       </c>
-      <c r="AH42" s="209"/>
+      <c r="AH42" s="249"/>
       <c r="AI42" s="196"/>
       <c r="AJ42" s="205">
         <f>AH43</f>
@@ -7832,11 +7856,11 @@
       </c>
       <c r="AK42" s="207">
         <f>MAX($AL$10:$AL$97) - AL42</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="AL42" s="205">
         <f>$S42+$AB42+$AG42+$AJ42</f>
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="43" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7852,7 +7876,7 @@
       <c r="D43" s="80"/>
       <c r="E43" s="121">
         <f>(IF($E42&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E42=$E$6+$F$6,$O$103,0),0),0)+IF($F42&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F42=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F43" s="80"/>
       <c r="G43" s="81">
@@ -7874,7 +7898,7 @@
         <f>(IF($M42&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M42=$M$6+$N$6,$O$103,0),0),0)+IF($N42&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N42=$M$6+$N$6,$O$103,0),0),0))</f>
         <v>11</v>
       </c>
-      <c r="N43" s="80"/>
+      <c r="N43" s="163"/>
       <c r="O43" s="81">
         <f>(IF($O42&lt;&gt;"",($O$6*$O$104)+IF($O$6=4,($O$102)+IF($O42=$O$6+$P$6,$O$103,0),0),0)+IF($P42&lt;&gt;"",($P$6*$O$104)+IF($P$6=4,($O$102)+IF($P42=$O$6+$P$6,$O$103,0),0),0))</f>
         <v>2</v>
@@ -7905,7 +7929,7 @@
       <c r="AJ43" s="128"/>
       <c r="AK43" s="116">
         <f>MAX($AL$10:$AL$97) - AL43</f>
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="AL43" s="128"/>
     </row>
@@ -7930,7 +7954,7 @@
         <f>IF(ISBLANK(E42),
 0,
 IF(E$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F44" s="124">
         <f>IF(ISBLANK(F42),
@@ -7980,7 +8004,7 @@
 IF(M$6= 4, 1, 0))</f>
         <v>0</v>
       </c>
-      <c r="N44" s="124">
+      <c r="N44" s="146">
         <f>IF(ISBLANK(N42),
 0,
 IF(N$6 = 4, 1, 0))</f>
@@ -8030,7 +8054,7 @@
       <c r="AJ44" s="147"/>
       <c r="AK44" s="148">
         <f>SUM(C44:AI44)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL44" s="130"/>
     </row>
@@ -8105,7 +8129,7 @@
 IF(M42 = (M$6+N$6),1,0))</f>
         <v>0</v>
       </c>
-      <c r="N45" s="124">
+      <c r="N45" s="146">
         <f>IF(N44 = 0,
 0,
 IF(N42 = (M$6+N$6),1,0))</f>
@@ -8162,46 +8186,46 @@
     <row r="46" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="122">
         <f>RANK(AL46,$AL$10:$AL$97,)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B46" s="88" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C46" s="46">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D46" s="45"/>
       <c r="E46" s="44">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F46" s="45"/>
       <c r="G46" s="48">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H46" s="47"/>
       <c r="I46" s="44"/>
       <c r="J46" s="47">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K46" s="49">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L46" s="47"/>
       <c r="M46" s="44"/>
-      <c r="N46" s="45">
+      <c r="N46" s="321">
+        <v>6</v>
+      </c>
+      <c r="O46" s="44">
         <v>7</v>
       </c>
-      <c r="O46" s="44">
+      <c r="P46" s="45"/>
+      <c r="Q46" s="48"/>
+      <c r="R46" s="50">
         <v>6</v>
       </c>
-      <c r="P46" s="45"/>
-      <c r="Q46" s="48">
-        <v>7</v>
-      </c>
-      <c r="R46" s="50"/>
       <c r="S46" s="129">
         <f>SUM(C47:R47)</f>
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="T46" s="46"/>
       <c r="U46" s="47"/>
@@ -8209,7 +8233,7 @@
       <c r="W46" s="47"/>
       <c r="X46" s="49"/>
       <c r="Y46" s="45"/>
-      <c r="Z46" s="244"/>
+      <c r="Z46" s="48"/>
       <c r="AA46" s="47"/>
       <c r="AB46" s="129">
         <f>SUM(T47:AA47)</f>
@@ -8231,11 +8255,11 @@
       </c>
       <c r="AK46" s="116">
         <f>MAX($AL$10:$AL$97) - AL46</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="AL46" s="129">
         <f>$S46+$AB46+$AG46+$AJ46</f>
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="47" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -8251,7 +8275,7 @@
       <c r="D47" s="80"/>
       <c r="E47" s="81">
         <f>(IF($E46&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E46=$E$6+$F$6,$O$103,0),0),0)+IF($F46&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F46=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F47" s="80"/>
       <c r="G47" s="81">
@@ -8271,7 +8295,7 @@
       <c r="L47" s="80"/>
       <c r="M47" s="81">
         <f>(IF($M46&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M46=$M$6+$N$6,$O$103,0),0),0)+IF($N46&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N46=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="N47" s="80"/>
       <c r="O47" s="81">
@@ -8304,7 +8328,7 @@
       <c r="AJ47" s="128"/>
       <c r="AK47" s="116">
         <f>MAX($AL$10:$AL$97) - AL47</f>
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="AL47" s="128"/>
     </row>
@@ -8329,7 +8353,7 @@
         <f>IF(ISBLANK(E46),
 0,
 IF(E$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F48" s="124">
         <f>IF(ISBLANK(F46),
@@ -8429,7 +8453,7 @@
       <c r="AJ48" s="147"/>
       <c r="AK48" s="148">
         <f>SUM(C48:AI48)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL48" s="130"/>
     </row>
@@ -8508,7 +8532,7 @@
         <f>IF(N48 = 0,
 0,
 IF(N46 = (M$6+N$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O49" s="124">
         <f>IF(O48 = 0,
@@ -8554,53 +8578,53 @@
       <c r="AJ49" s="147"/>
       <c r="AK49" s="148">
         <f>SUM(C49:AI49)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL49" s="130"/>
     </row>
     <row r="50" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="186">
         <f>RANK(AL50,$AL$10:$AL$97,)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B50" s="211" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C50" s="198">
+        <v>6</v>
+      </c>
+      <c r="D50" s="199"/>
+      <c r="E50" s="320">
+        <v>7</v>
+      </c>
+      <c r="F50" s="199"/>
+      <c r="G50" s="201">
         <v>5</v>
       </c>
-      <c r="D50" s="199"/>
-      <c r="E50" s="200">
-        <v>6</v>
-      </c>
-      <c r="F50" s="199"/>
-      <c r="G50" s="201"/>
-      <c r="H50" s="202">
-        <v>7</v>
-      </c>
+      <c r="H50" s="202"/>
       <c r="I50" s="200"/>
       <c r="J50" s="202">
+        <v>5</v>
+      </c>
+      <c r="K50" s="203">
+        <v>7</v>
+      </c>
+      <c r="L50" s="202"/>
+      <c r="M50" s="200">
         <v>6</v>
       </c>
-      <c r="K50" s="203">
+      <c r="N50" s="199"/>
+      <c r="O50" s="200">
+        <v>7</v>
+      </c>
+      <c r="P50" s="199"/>
+      <c r="Q50" s="201">
         <v>5</v>
       </c>
-      <c r="L50" s="202"/>
-      <c r="M50" s="200"/>
-      <c r="N50" s="199">
-        <v>7</v>
-      </c>
-      <c r="O50" s="200">
-        <v>5</v>
-      </c>
-      <c r="P50" s="199"/>
-      <c r="Q50" s="201"/>
-      <c r="R50" s="204">
-        <v>6</v>
-      </c>
+      <c r="R50" s="204"/>
       <c r="S50" s="205">
         <f>SUM(C51:R51)</f>
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="T50" s="198"/>
       <c r="U50" s="202"/>
@@ -8608,7 +8632,7 @@
       <c r="W50" s="202"/>
       <c r="X50" s="203"/>
       <c r="Y50" s="199"/>
-      <c r="Z50" s="208"/>
+      <c r="Z50" s="201"/>
       <c r="AA50" s="202"/>
       <c r="AB50" s="205">
         <f>SUM(T51:AA51)</f>
@@ -8630,11 +8654,11 @@
       </c>
       <c r="AK50" s="207">
         <f>MAX($AL$10:$AL$97) - AL50</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="AL50" s="205">
         <f>$S50+$AB50+$AG50+$AJ50</f>
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="51" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -8650,7 +8674,7 @@
       <c r="D51" s="134"/>
       <c r="E51" s="132">
         <f>(IF($E50&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E50=$E$6+$F$6,$O$103,0),0),0)+IF($F50&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F50=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F51" s="134"/>
       <c r="G51" s="132">
@@ -8670,7 +8694,7 @@
       <c r="L51" s="134"/>
       <c r="M51" s="132">
         <f>(IF($M50&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M50=$M$6+$N$6,$O$103,0),0),0)+IF($N50&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N50=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="N51" s="134"/>
       <c r="O51" s="135">
@@ -8680,7 +8704,7 @@
       <c r="P51" s="134"/>
       <c r="Q51" s="135">
         <f>(IF($Q50&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q50=$Q$6+$R$6,$O$103,0),0),0)+IF($R50&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R50=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="R51" s="138"/>
       <c r="S51" s="128"/>
@@ -8725,7 +8749,7 @@
         <f>IF(ISBLANK(E50),
 0,
 IF(E$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F52" s="124">
         <f>IF(ISBLANK(F50),
@@ -8779,7 +8803,7 @@
         <f>IF(ISBLANK(N50),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O52" s="124">
         <f>IF(ISBLANK(O50),
@@ -8797,7 +8821,7 @@
         <f>IF(ISBLANK(Q50),
 0,
 IF(Q$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R52" s="124">
         <f>IF(ISBLANK(R50),
@@ -8825,7 +8849,7 @@
       <c r="AJ52" s="147"/>
       <c r="AK52" s="148">
         <f>SUM(C52:AI52)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL52" s="130"/>
     </row>
@@ -8850,7 +8874,7 @@
         <f>IF(E52 = 0,
 0,
 IF(E50 = (E$6+F$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F53" s="124">
         <f>IF(F52 = 0,
@@ -8950,7 +8974,7 @@
       <c r="AJ53" s="147"/>
       <c r="AK53" s="148">
         <f>SUM(C53:AI53)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL53" s="130"/>
     </row>
@@ -8960,51 +8984,51 @@
         <v>12</v>
       </c>
       <c r="B54" s="88" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C54" s="46">
+        <v>5</v>
+      </c>
+      <c r="D54" s="45"/>
+      <c r="E54" s="44">
+        <v>6</v>
+      </c>
+      <c r="F54" s="45"/>
+      <c r="G54" s="48"/>
+      <c r="H54" s="47">
         <v>7</v>
       </c>
-      <c r="D54" s="45"/>
-      <c r="E54" s="306">
+      <c r="I54" s="44"/>
+      <c r="J54" s="47">
         <v>6</v>
-      </c>
-      <c r="F54" s="45"/>
-      <c r="G54" s="307"/>
-      <c r="H54" s="47">
-        <v>6</v>
-      </c>
-      <c r="I54" s="306"/>
-      <c r="J54" s="47">
-        <v>7</v>
       </c>
       <c r="K54" s="49">
         <v>5</v>
       </c>
       <c r="L54" s="47"/>
-      <c r="M54" s="44">
+      <c r="M54" s="44"/>
+      <c r="N54" s="45">
         <v>7</v>
       </c>
-      <c r="N54" s="45"/>
       <c r="O54" s="44">
+        <v>5</v>
+      </c>
+      <c r="P54" s="45"/>
+      <c r="Q54" s="48"/>
+      <c r="R54" s="50">
         <v>6</v>
       </c>
-      <c r="P54" s="45"/>
-      <c r="Q54" s="48">
-        <v>6</v>
-      </c>
-      <c r="R54" s="50"/>
       <c r="S54" s="129">
         <f>SUM(C55:R55)</f>
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="T54" s="46"/>
       <c r="U54" s="47"/>
-      <c r="V54" s="248"/>
+      <c r="V54" s="44"/>
       <c r="W54" s="47"/>
       <c r="X54" s="49"/>
-      <c r="Y54" s="127"/>
-      <c r="Z54" s="48"/>
+      <c r="Y54" s="45"/>
+      <c r="Z54" s="243"/>
       <c r="AA54" s="47"/>
       <c r="AB54" s="129">
         <f>SUM(T55:AA55)</f>
@@ -9030,7 +9054,7 @@
       </c>
       <c r="AL54" s="129">
         <f>$S54+$AB54+$AG54+$AJ54</f>
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="55" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -9046,7 +9070,7 @@
       <c r="D55" s="134"/>
       <c r="E55" s="132">
         <f>(IF($E54&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E54=$E$6+$F$6,$O$103,0),0),0)+IF($F54&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F54=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F55" s="134"/>
       <c r="G55" s="132">
@@ -9066,7 +9090,7 @@
       <c r="L55" s="134"/>
       <c r="M55" s="132">
         <f>(IF($M54&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M54=$M$6+$N$6,$O$103,0),0),0)+IF($N54&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N54=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="N55" s="134"/>
       <c r="O55" s="135">
@@ -9121,7 +9145,7 @@
         <f>IF(ISBLANK(E54),
 0,
 IF(E$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F56" s="124">
         <f>IF(ISBLANK(F54),
@@ -9175,7 +9199,7 @@
         <f>IF(ISBLANK(N54),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O56" s="124">
         <f>IF(ISBLANK(O54),
@@ -9221,7 +9245,7 @@
       <c r="AJ56" s="147"/>
       <c r="AK56" s="148">
         <f>SUM(C56:AI56)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL56" s="130"/>
     </row>
@@ -9353,53 +9377,53 @@
     <row r="58" spans="1:38" s="27" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="186">
         <f>RANK(AL58,$AL$10:$AL$97,)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B58" s="211" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C58" s="198">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D58" s="199"/>
-      <c r="E58" s="200"/>
-      <c r="F58" s="199">
-        <v>7</v>
-      </c>
-      <c r="G58" s="201">
-        <v>4</v>
-      </c>
-      <c r="H58" s="202"/>
-      <c r="I58" s="200"/>
+      <c r="E58" s="312">
+        <v>6</v>
+      </c>
+      <c r="F58" s="199"/>
+      <c r="G58" s="313"/>
+      <c r="H58" s="202">
+        <v>6</v>
+      </c>
+      <c r="I58" s="312"/>
       <c r="J58" s="202">
         <v>7</v>
       </c>
       <c r="K58" s="203">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L58" s="202"/>
       <c r="M58" s="200">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N58" s="199"/>
       <c r="O58" s="200">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P58" s="199"/>
-      <c r="Q58" s="201"/>
-      <c r="R58" s="204">
+      <c r="Q58" s="201">
         <v>6</v>
       </c>
+      <c r="R58" s="204"/>
       <c r="S58" s="205">
         <f>SUM(C59:R59)</f>
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="T58" s="198"/>
       <c r="U58" s="202"/>
-      <c r="V58" s="200"/>
+      <c r="V58" s="314"/>
       <c r="W58" s="202"/>
       <c r="X58" s="203"/>
-      <c r="Y58" s="235"/>
+      <c r="Y58" s="234"/>
       <c r="Z58" s="201"/>
       <c r="AA58" s="202"/>
       <c r="AB58" s="205">
@@ -9422,11 +9446,11 @@
       </c>
       <c r="AK58" s="207">
         <f>MAX($AL$10:$AL$97) - AL58</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AL58" s="205">
         <f>$S58+$AB58+$AG58+$AJ58</f>
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="59" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -9442,7 +9466,7 @@
       <c r="D59" s="134"/>
       <c r="E59" s="132">
         <f>(IF($E58&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E58=$E$6+$F$6,$O$103,0),0),0)+IF($F58&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F58=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F59" s="134"/>
       <c r="G59" s="132">
@@ -9472,7 +9496,7 @@
       <c r="P59" s="134"/>
       <c r="Q59" s="135">
         <f>(IF($Q58&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q58=$Q$6+$R$6,$O$103,0),0),0)+IF($R58&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R58=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="R59" s="138"/>
       <c r="S59" s="128"/>
@@ -9517,7 +9541,7 @@
         <f>IF(ISBLANK(E58),
 0,
 IF(E$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F60" s="124">
         <f>IF(ISBLANK(F58),
@@ -9589,7 +9613,7 @@
         <f>IF(ISBLANK(Q58),
 0,
 IF(Q$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R60" s="124">
         <f>IF(ISBLANK(R58),
@@ -9617,7 +9641,7 @@
       <c r="AJ60" s="147"/>
       <c r="AK60" s="148">
         <f>SUM(C60:AI60)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL60" s="130"/>
     </row>
@@ -9749,17 +9773,17 @@
     <row r="62" spans="1:38" s="27" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="122">
         <f>RANK(AL62,$AL$10:$AL$97,)</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B62" s="88" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="C62" s="46">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D62" s="45"/>
-      <c r="E62" s="44">
-        <v>4</v>
+      <c r="E62" s="319">
+        <v>7</v>
       </c>
       <c r="F62" s="45"/>
       <c r="G62" s="48">
@@ -9768,14 +9792,14 @@
       <c r="H62" s="47"/>
       <c r="I62" s="44"/>
       <c r="J62" s="47">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K62" s="49">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L62" s="47"/>
       <c r="M62" s="44">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N62" s="45"/>
       <c r="O62" s="44">
@@ -9784,11 +9808,11 @@
       <c r="P62" s="45"/>
       <c r="Q62" s="48"/>
       <c r="R62" s="50">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S62" s="129">
         <f>SUM(C63:R63)</f>
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="T62" s="46"/>
       <c r="U62" s="47"/>
@@ -9796,14 +9820,14 @@
       <c r="W62" s="47"/>
       <c r="X62" s="49"/>
       <c r="Y62" s="45"/>
-      <c r="Z62" s="244"/>
+      <c r="Z62" s="48"/>
       <c r="AA62" s="47"/>
       <c r="AB62" s="129">
         <f>SUM(T63:AA63)</f>
         <v>0</v>
       </c>
       <c r="AC62" s="48"/>
-      <c r="AD62" s="308"/>
+      <c r="AD62" s="47"/>
       <c r="AE62" s="49"/>
       <c r="AF62" s="47"/>
       <c r="AG62" s="129">
@@ -9818,11 +9842,11 @@
       </c>
       <c r="AK62" s="116">
         <f>MAX($AL$10:$AL$97) - AL62</f>
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="AL62" s="129">
         <f>$S62+$AB62+$AG62+$AJ62</f>
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="63" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -9838,7 +9862,7 @@
       <c r="D63" s="134"/>
       <c r="E63" s="132">
         <f>(IF($E62&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E62=$E$6+$F$6,$O$103,0),0),0)+IF($F62&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F62=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F63" s="134"/>
       <c r="G63" s="132">
@@ -9913,7 +9937,7 @@
         <f>IF(ISBLANK(E62),
 0,
 IF(E$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F64" s="124">
         <f>IF(ISBLANK(F62),
@@ -10013,7 +10037,7 @@
       <c r="AJ64" s="147"/>
       <c r="AK64" s="148">
         <f>SUM(C64:AI64)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL64" s="130"/>
     </row>
@@ -10038,7 +10062,7 @@
         <f>IF(E64 = 0,
 0,
 IF(E62 = (E$6+F$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F65" s="124">
         <f>IF(F64 = 0,
@@ -10138,28 +10162,28 @@
       <c r="AJ65" s="147"/>
       <c r="AK65" s="148">
         <f>SUM(C65:AI65)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL65" s="130"/>
     </row>
     <row r="66" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="186">
         <f>RANK(AL66,$AL$10:$AL$97,)</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B66" s="211" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="C66" s="198">
+        <v>4</v>
+      </c>
+      <c r="D66" s="199"/>
+      <c r="E66" s="200">
+        <v>4</v>
+      </c>
+      <c r="F66" s="199"/>
+      <c r="G66" s="201">
         <v>6</v>
-      </c>
-      <c r="D66" s="199"/>
-      <c r="E66" s="200"/>
-      <c r="F66" s="199">
-        <v>7</v>
-      </c>
-      <c r="G66" s="201">
-        <v>7</v>
       </c>
       <c r="H66" s="202"/>
       <c r="I66" s="200"/>
@@ -10171,11 +10195,11 @@
       </c>
       <c r="L66" s="202"/>
       <c r="M66" s="200">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="N66" s="199"/>
       <c r="O66" s="200">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P66" s="199"/>
       <c r="Q66" s="201"/>
@@ -10184,7 +10208,7 @@
       </c>
       <c r="S66" s="205">
         <f>SUM(C67:R67)</f>
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="T66" s="198"/>
       <c r="U66" s="202"/>
@@ -10192,14 +10216,14 @@
       <c r="W66" s="202"/>
       <c r="X66" s="203"/>
       <c r="Y66" s="199"/>
-      <c r="Z66" s="201"/>
+      <c r="Z66" s="208"/>
       <c r="AA66" s="202"/>
       <c r="AB66" s="205">
         <f>SUM(T67:AA67)</f>
         <v>0</v>
       </c>
       <c r="AC66" s="201"/>
-      <c r="AD66" s="202"/>
+      <c r="AD66" s="311"/>
       <c r="AE66" s="203"/>
       <c r="AF66" s="202"/>
       <c r="AG66" s="205">
@@ -10214,11 +10238,11 @@
       </c>
       <c r="AK66" s="207">
         <f>MAX($AL$10:$AL$97) - AL66</f>
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="AL66" s="205">
         <f>$S66+$AB66+$AG66+$AJ66</f>
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="67" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -10234,7 +10258,7 @@
       <c r="D67" s="134"/>
       <c r="E67" s="132">
         <f>(IF($E66&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E66=$E$6+$F$6,$O$103,0),0),0)+IF($F66&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F66=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F67" s="134"/>
       <c r="G67" s="132">
@@ -10309,7 +10333,7 @@
         <f>IF(ISBLANK(E66),
 0,
 IF(E$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F68" s="124">
         <f>IF(ISBLANK(F66),
@@ -10409,7 +10433,7 @@
       <c r="AJ68" s="147"/>
       <c r="AK68" s="148">
         <f>SUM(C68:AI68)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL68" s="130"/>
     </row>
@@ -10541,46 +10565,46 @@
     <row r="70" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="122">
         <f>RANK(AL70,$AL$10:$AL$97,)</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B70" s="88" t="s">
         <v>68</v>
       </c>
-      <c r="C70" s="309">
+      <c r="C70" s="250">
         <v>5</v>
       </c>
-      <c r="D70" s="310"/>
-      <c r="E70" s="311">
+      <c r="D70" s="251"/>
+      <c r="E70" s="252">
         <v>6</v>
       </c>
-      <c r="F70" s="310"/>
-      <c r="G70" s="312">
+      <c r="F70" s="251"/>
+      <c r="G70" s="253">
         <v>5</v>
       </c>
-      <c r="H70" s="313"/>
-      <c r="I70" s="311"/>
-      <c r="J70" s="313">
+      <c r="H70" s="254"/>
+      <c r="I70" s="252"/>
+      <c r="J70" s="254">
         <v>6</v>
       </c>
-      <c r="K70" s="314">
+      <c r="K70" s="255">
         <v>6</v>
       </c>
-      <c r="L70" s="313"/>
-      <c r="M70" s="311">
+      <c r="L70" s="254"/>
+      <c r="M70" s="252">
         <v>7</v>
       </c>
-      <c r="N70" s="310"/>
-      <c r="O70" s="311">
+      <c r="N70" s="251"/>
+      <c r="O70" s="252">
         <v>6</v>
       </c>
-      <c r="P70" s="310"/>
-      <c r="Q70" s="312"/>
-      <c r="R70" s="315">
+      <c r="P70" s="251"/>
+      <c r="Q70" s="253"/>
+      <c r="R70" s="256">
         <v>6</v>
       </c>
       <c r="S70" s="129">
         <f>SUM(C71:R71)</f>
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="T70" s="46"/>
       <c r="U70" s="47"/>
@@ -10610,11 +10634,11 @@
       </c>
       <c r="AK70" s="116">
         <f>MAX($AL$10:$AL$97) - AL70</f>
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="AL70" s="129">
         <f>$S70+$AB70+$AG70+$AJ70</f>
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="71" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -10630,7 +10654,7 @@
       <c r="D71" s="134"/>
       <c r="E71" s="132">
         <f>(IF($E70&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E70=$E$6+$F$6,$O$103,0),0),0)+IF($F70&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F70=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F71" s="134"/>
       <c r="G71" s="132">
@@ -10705,7 +10729,7 @@
         <f>IF(ISBLANK(E70),
 0,
 IF(E$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F72" s="124">
         <f>IF(ISBLANK(F70),
@@ -10805,7 +10829,7 @@
       <c r="AJ72" s="147"/>
       <c r="AK72" s="148">
         <f>SUM(C72:AI72)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL72" s="130"/>
     </row>
@@ -10937,19 +10961,19 @@
     <row r="74" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="186">
         <f>RANK(AL74,$AL$10:$AL$97,)</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B74" s="211" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C74" s="198">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D74" s="199"/>
-      <c r="E74" s="200"/>
-      <c r="F74" s="199">
-        <v>7</v>
-      </c>
+      <c r="E74" s="200">
+        <v>6</v>
+      </c>
+      <c r="F74" s="199"/>
       <c r="G74" s="201">
         <v>6</v>
       </c>
@@ -10963,22 +10987,22 @@
       </c>
       <c r="L74" s="202"/>
       <c r="M74" s="200">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N74" s="199"/>
       <c r="O74" s="200">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P74" s="199"/>
       <c r="Q74" s="201"/>
       <c r="R74" s="204">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S74" s="205">
         <f>SUM(C75:R75)</f>
-        <v>14</v>
-      </c>
-      <c r="T74" s="316"/>
+        <v>20</v>
+      </c>
+      <c r="T74" s="198"/>
       <c r="U74" s="202"/>
       <c r="V74" s="200"/>
       <c r="W74" s="202"/>
@@ -11006,11 +11030,11 @@
       </c>
       <c r="AK74" s="207">
         <f>MAX($AL$10:$AL$97) - AL74</f>
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="AL74" s="205">
         <f>$S74+$AB74+$AG74+$AJ74</f>
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="75" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11026,7 +11050,7 @@
       <c r="D75" s="134"/>
       <c r="E75" s="132">
         <f>(IF($E74&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E74=$E$6+$F$6,$O$103,0),0),0)+IF($F74&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F74=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F75" s="134"/>
       <c r="G75" s="132">
@@ -11101,7 +11125,7 @@
         <f>IF(ISBLANK(E74),
 0,
 IF(E$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F76" s="124">
         <f>IF(ISBLANK(F74),
@@ -11201,7 +11225,7 @@
       <c r="AJ76" s="147"/>
       <c r="AK76" s="148">
         <f>SUM(C76:AI76)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL76" s="130"/>
     </row>
@@ -11333,13 +11357,13 @@
     <row r="78" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="122">
         <f>RANK(AL78,$AL$10:$AL$97,)</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B78" s="88" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C78" s="46">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D78" s="45"/>
       <c r="E78" s="44">
@@ -11352,18 +11376,18 @@
       <c r="H78" s="47"/>
       <c r="I78" s="44"/>
       <c r="J78" s="47">
+        <v>6</v>
+      </c>
+      <c r="K78" s="49">
         <v>7</v>
-      </c>
-      <c r="K78" s="49">
-        <v>5</v>
       </c>
       <c r="L78" s="47"/>
       <c r="M78" s="44">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N78" s="45"/>
       <c r="O78" s="44">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P78" s="45"/>
       <c r="Q78" s="48"/>
@@ -11372,7 +11396,7 @@
       </c>
       <c r="S78" s="129">
         <f>SUM(C79:R79)</f>
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="T78" s="46"/>
       <c r="U78" s="47"/>
@@ -11402,11 +11426,11 @@
       </c>
       <c r="AK78" s="116">
         <f>MAX($AL$10:$AL$97) - AL78</f>
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="AL78" s="129">
         <f>$S78+$AB78+$AG78+$AJ78</f>
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="79" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11422,7 +11446,7 @@
       <c r="D79" s="134"/>
       <c r="E79" s="132">
         <f>(IF($E78&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E78=$E$6+$F$6,$O$103,0),0),0)+IF($F78&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F78=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F79" s="134"/>
       <c r="G79" s="132">
@@ -11497,7 +11521,7 @@
         <f>IF(ISBLANK(E78),
 0,
 IF(E$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F80" s="124">
         <f>IF(ISBLANK(F78),
@@ -11597,7 +11621,7 @@
       <c r="AJ80" s="147"/>
       <c r="AK80" s="148">
         <f>SUM(C80:AI80)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL80" s="130"/>
     </row>
@@ -11729,10 +11753,10 @@
     <row r="82" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="186">
         <f>RANK(AL82,$AL$10:$AL$97,)</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B82" s="211" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C82" s="198">
         <v>5</v>
@@ -11751,24 +11775,24 @@
         <v>6</v>
       </c>
       <c r="K82" s="203">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L82" s="202"/>
       <c r="M82" s="200">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N82" s="199"/>
       <c r="O82" s="200">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P82" s="199"/>
       <c r="Q82" s="201"/>
       <c r="R82" s="204">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S82" s="205">
         <f>SUM(C83:R83)</f>
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="T82" s="198"/>
       <c r="U82" s="202"/>
@@ -11776,7 +11800,7 @@
       <c r="W82" s="202"/>
       <c r="X82" s="203"/>
       <c r="Y82" s="199"/>
-      <c r="Z82" s="201"/>
+      <c r="Z82" s="208"/>
       <c r="AA82" s="202"/>
       <c r="AB82" s="205">
         <f>SUM(T83:AA83)</f>
@@ -11798,11 +11822,11 @@
       </c>
       <c r="AK82" s="207">
         <f>MAX($AL$10:$AL$97) - AL82</f>
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="AL82" s="205">
         <f>$S82+$AB82+$AG82+$AJ82</f>
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="83" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11818,7 +11842,7 @@
       <c r="D83" s="134"/>
       <c r="E83" s="132">
         <f>(IF($E82&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E82=$E$6+$F$6,$O$103,0),0),0)+IF($F82&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F82=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F83" s="134"/>
       <c r="G83" s="132">
@@ -11893,7 +11917,7 @@
         <f>IF(ISBLANK(E82),
 0,
 IF(E$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F84" s="124">
         <f>IF(ISBLANK(F82),
@@ -11993,7 +12017,7 @@
       <c r="AJ84" s="147"/>
       <c r="AK84" s="148">
         <f>SUM(C84:AI84)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL84" s="130"/>
     </row>
@@ -12125,42 +12149,42 @@
     <row r="86" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="122">
         <f>RANK(AL86,$AL$10:$AL$97,)</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B86" s="88" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C86" s="46">
         <v>5</v>
       </c>
       <c r="D86" s="45"/>
-      <c r="E86" s="44">
-        <v>6</v>
-      </c>
-      <c r="F86" s="45"/>
+      <c r="E86" s="44"/>
+      <c r="F86" s="45">
+        <v>7</v>
+      </c>
       <c r="G86" s="48">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H86" s="47"/>
       <c r="I86" s="44"/>
       <c r="J86" s="47">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K86" s="49">
         <v>6</v>
       </c>
       <c r="L86" s="47"/>
       <c r="M86" s="44">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N86" s="45"/>
       <c r="O86" s="44">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P86" s="45"/>
       <c r="Q86" s="48"/>
       <c r="R86" s="50">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S86" s="129">
         <f>SUM(C87:R87)</f>
@@ -12171,8 +12195,8 @@
       <c r="V86" s="44"/>
       <c r="W86" s="47"/>
       <c r="X86" s="49"/>
-      <c r="Y86" s="45"/>
-      <c r="Z86" s="244"/>
+      <c r="Y86" s="127"/>
+      <c r="Z86" s="48"/>
       <c r="AA86" s="47"/>
       <c r="AB86" s="129">
         <f>SUM(T87:AA87)</f>
@@ -12194,7 +12218,7 @@
       </c>
       <c r="AK86" s="116">
         <f>MAX($AL$10:$AL$97) - AL86</f>
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="AL86" s="129">
         <f>$S86+$AB86+$AG86+$AJ86</f>
@@ -12521,43 +12545,43 @@
     <row r="90" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="186">
         <f>RANK(AL90,$AL$10:$AL$97,)</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B90" s="211" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C90" s="198">
         <v>6</v>
       </c>
       <c r="D90" s="199"/>
-      <c r="E90" s="200">
+      <c r="E90" s="200"/>
+      <c r="F90" s="199">
         <v>7</v>
       </c>
-      <c r="F90" s="199"/>
       <c r="G90" s="201">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H90" s="202"/>
       <c r="I90" s="200"/>
       <c r="J90" s="202">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K90" s="203">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L90" s="202"/>
       <c r="M90" s="200">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N90" s="199"/>
       <c r="O90" s="200">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P90" s="199"/>
-      <c r="Q90" s="201">
-        <v>5</v>
-      </c>
-      <c r="R90" s="204"/>
+      <c r="Q90" s="201"/>
+      <c r="R90" s="204">
+        <v>6</v>
+      </c>
       <c r="S90" s="205">
         <f>SUM(C91:R91)</f>
         <v>14</v>
@@ -12590,7 +12614,7 @@
       </c>
       <c r="AK90" s="207">
         <f>MAX($AL$10:$AL$97) - AL90</f>
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="AL90" s="205">
         <f>$S90+$AB90+$AG90+$AJ90</f>
@@ -12917,19 +12941,19 @@
     <row r="94" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A94" s="122">
         <f>RANK(AL94,$AL$10:$AL$97,)</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B94" s="88" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C94" s="226">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D94" s="227"/>
-      <c r="E94" s="228">
+      <c r="E94" s="228"/>
+      <c r="F94" s="227">
         <v>7</v>
       </c>
-      <c r="F94" s="227"/>
       <c r="G94" s="229">
         <v>6</v>
       </c>
@@ -12939,7 +12963,7 @@
         <v>7</v>
       </c>
       <c r="K94" s="231">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L94" s="230"/>
       <c r="M94" s="228">
@@ -12947,7 +12971,7 @@
       </c>
       <c r="N94" s="227"/>
       <c r="O94" s="228">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P94" s="227"/>
       <c r="Q94" s="229"/>
@@ -12958,7 +12982,7 @@
         <f>SUM(C95:R95)</f>
         <v>14</v>
       </c>
-      <c r="T94" s="46"/>
+      <c r="T94" s="310"/>
       <c r="U94" s="47"/>
       <c r="V94" s="44"/>
       <c r="W94" s="47"/>
@@ -12986,7 +13010,7 @@
       </c>
       <c r="AK94" s="116">
         <f>MAX($AL$10:$AL$97) - AL94</f>
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="AL94" s="218">
         <f>$S94+$AB94+$AG94+$AJ94</f>
@@ -13443,12 +13467,12 @@
     <row r="100" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B100" s="43"/>
       <c r="N100" s="26"/>
-      <c r="O100" s="254" t="s">
+      <c r="O100" s="290" t="s">
         <v>17</v>
       </c>
-      <c r="P100" s="255"/>
-      <c r="Q100" s="255"/>
-      <c r="R100" s="256"/>
+      <c r="P100" s="291"/>
+      <c r="Q100" s="291"/>
+      <c r="R100" s="292"/>
       <c r="AG100" s="30"/>
       <c r="AH100" s="30"/>
       <c r="AI100" s="30"/>
@@ -13457,21 +13481,21 @@
     </row>
     <row r="101" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="33"/>
-      <c r="B101" s="283" t="s">
+      <c r="B101" s="278" t="s">
         <v>16</v>
       </c>
-      <c r="C101" s="284"/>
-      <c r="D101" s="284"/>
-      <c r="E101" s="284"/>
-      <c r="F101" s="284"/>
-      <c r="G101" s="284"/>
-      <c r="H101" s="284"/>
-      <c r="I101" s="284"/>
-      <c r="J101" s="284"/>
-      <c r="K101" s="284"/>
-      <c r="L101" s="284"/>
-      <c r="M101" s="284"/>
-      <c r="N101" s="285"/>
+      <c r="C101" s="279"/>
+      <c r="D101" s="279"/>
+      <c r="E101" s="279"/>
+      <c r="F101" s="279"/>
+      <c r="G101" s="279"/>
+      <c r="H101" s="279"/>
+      <c r="I101" s="279"/>
+      <c r="J101" s="279"/>
+      <c r="K101" s="279"/>
+      <c r="L101" s="279"/>
+      <c r="M101" s="279"/>
+      <c r="N101" s="280"/>
       <c r="O101" s="21">
         <v>1</v>
       </c>
@@ -13484,45 +13508,45 @@
       <c r="R101" s="22">
         <v>4</v>
       </c>
-      <c r="U101" s="257" t="s">
+      <c r="U101" s="293" t="s">
         <v>26</v>
       </c>
-      <c r="V101" s="258"/>
-      <c r="W101" s="258"/>
-      <c r="X101" s="258"/>
-      <c r="Y101" s="258"/>
-      <c r="Z101" s="258"/>
-      <c r="AA101" s="258"/>
-      <c r="AB101" s="258"/>
-      <c r="AC101" s="258"/>
-      <c r="AD101" s="259"/>
+      <c r="V101" s="294"/>
+      <c r="W101" s="294"/>
+      <c r="X101" s="294"/>
+      <c r="Y101" s="294"/>
+      <c r="Z101" s="294"/>
+      <c r="AA101" s="294"/>
+      <c r="AB101" s="294"/>
+      <c r="AC101" s="294"/>
+      <c r="AD101" s="295"/>
       <c r="AE101" s="28"/>
       <c r="AF101" s="28"/>
-      <c r="AG101" s="260" t="s">
+      <c r="AG101" s="296" t="s">
         <v>24</v>
       </c>
-      <c r="AH101" s="261"/>
-      <c r="AI101" s="261"/>
-      <c r="AJ101" s="261"/>
-      <c r="AK101" s="262"/>
+      <c r="AH101" s="297"/>
+      <c r="AI101" s="297"/>
+      <c r="AJ101" s="297"/>
+      <c r="AK101" s="298"/>
     </row>
     <row r="102" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A102" s="34"/>
-      <c r="B102" s="290" t="s">
+      <c r="B102" s="257" t="s">
         <v>6</v>
       </c>
-      <c r="C102" s="291"/>
-      <c r="D102" s="291"/>
-      <c r="E102" s="291"/>
-      <c r="F102" s="291"/>
-      <c r="G102" s="291"/>
-      <c r="H102" s="291"/>
-      <c r="I102" s="291"/>
-      <c r="J102" s="291"/>
-      <c r="K102" s="291"/>
-      <c r="L102" s="291"/>
-      <c r="M102" s="291"/>
-      <c r="N102" s="292"/>
+      <c r="C102" s="258"/>
+      <c r="D102" s="258"/>
+      <c r="E102" s="258"/>
+      <c r="F102" s="258"/>
+      <c r="G102" s="258"/>
+      <c r="H102" s="258"/>
+      <c r="I102" s="258"/>
+      <c r="J102" s="258"/>
+      <c r="K102" s="258"/>
+      <c r="L102" s="258"/>
+      <c r="M102" s="258"/>
+      <c r="N102" s="259"/>
       <c r="O102" s="20">
         <v>5</v>
       </c>
@@ -13535,49 +13559,49 @@
       <c r="R102" s="23">
         <v>20</v>
       </c>
-      <c r="U102" s="288" t="s">
+      <c r="U102" s="283" t="s">
         <v>20</v>
       </c>
-      <c r="V102" s="289"/>
-      <c r="W102" s="289"/>
-      <c r="X102" s="289"/>
-      <c r="Y102" s="289"/>
-      <c r="Z102" s="289"/>
-      <c r="AA102" s="289"/>
-      <c r="AB102" s="286">
+      <c r="V102" s="284"/>
+      <c r="W102" s="284"/>
+      <c r="X102" s="284"/>
+      <c r="Y102" s="284"/>
+      <c r="Z102" s="284"/>
+      <c r="AA102" s="284"/>
+      <c r="AB102" s="281">
         <v>22</v>
       </c>
-      <c r="AC102" s="286"/>
-      <c r="AD102" s="287"/>
+      <c r="AC102" s="281"/>
+      <c r="AD102" s="282"/>
       <c r="AE102" s="29"/>
       <c r="AF102" s="29"/>
-      <c r="AG102" s="302" t="s">
+      <c r="AG102" s="264" t="s">
         <v>21</v>
       </c>
-      <c r="AH102" s="303"/>
-      <c r="AI102" s="303"/>
-      <c r="AJ102" s="304"/>
+      <c r="AH102" s="265"/>
+      <c r="AI102" s="265"/>
+      <c r="AJ102" s="266"/>
       <c r="AK102" s="223">
         <v>230</v>
       </c>
     </row>
     <row r="103" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="34"/>
-      <c r="B103" s="290" t="s">
+      <c r="B103" s="257" t="s">
         <v>5</v>
       </c>
-      <c r="C103" s="291"/>
-      <c r="D103" s="291"/>
-      <c r="E103" s="291"/>
-      <c r="F103" s="291"/>
-      <c r="G103" s="291"/>
-      <c r="H103" s="291"/>
-      <c r="I103" s="291"/>
-      <c r="J103" s="291"/>
-      <c r="K103" s="291"/>
-      <c r="L103" s="291"/>
-      <c r="M103" s="291"/>
-      <c r="N103" s="292"/>
+      <c r="C103" s="258"/>
+      <c r="D103" s="258"/>
+      <c r="E103" s="258"/>
+      <c r="F103" s="258"/>
+      <c r="G103" s="258"/>
+      <c r="H103" s="258"/>
+      <c r="I103" s="258"/>
+      <c r="J103" s="258"/>
+      <c r="K103" s="258"/>
+      <c r="L103" s="258"/>
+      <c r="M103" s="258"/>
+      <c r="N103" s="259"/>
       <c r="O103" s="20">
         <v>2</v>
       </c>
@@ -13590,49 +13614,49 @@
       <c r="R103" s="23">
         <v>8</v>
       </c>
-      <c r="U103" s="297" t="s">
+      <c r="U103" s="262" t="s">
         <v>18</v>
       </c>
-      <c r="V103" s="298"/>
-      <c r="W103" s="298"/>
-      <c r="X103" s="298"/>
-      <c r="Y103" s="298"/>
-      <c r="Z103" s="298"/>
-      <c r="AA103" s="298"/>
-      <c r="AB103" s="299">
+      <c r="V103" s="263"/>
+      <c r="W103" s="263"/>
+      <c r="X103" s="263"/>
+      <c r="Y103" s="263"/>
+      <c r="Z103" s="263"/>
+      <c r="AA103" s="263"/>
+      <c r="AB103" s="288">
         <v>20</v>
       </c>
-      <c r="AC103" s="299"/>
-      <c r="AD103" s="300"/>
+      <c r="AC103" s="288"/>
+      <c r="AD103" s="289"/>
       <c r="AE103" s="29"/>
       <c r="AF103" s="29"/>
-      <c r="AG103" s="305" t="s">
+      <c r="AG103" s="267" t="s">
         <v>22</v>
       </c>
-      <c r="AH103" s="291"/>
-      <c r="AI103" s="291"/>
-      <c r="AJ103" s="292"/>
+      <c r="AH103" s="258"/>
+      <c r="AI103" s="258"/>
+      <c r="AJ103" s="259"/>
       <c r="AK103" s="36">
         <v>115</v>
       </c>
     </row>
     <row r="104" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="35"/>
-      <c r="B104" s="276" t="s">
+      <c r="B104" s="271" t="s">
         <v>4</v>
       </c>
-      <c r="C104" s="277"/>
-      <c r="D104" s="277"/>
-      <c r="E104" s="277"/>
-      <c r="F104" s="277"/>
-      <c r="G104" s="277"/>
-      <c r="H104" s="277"/>
-      <c r="I104" s="277"/>
-      <c r="J104" s="277"/>
-      <c r="K104" s="277"/>
-      <c r="L104" s="277"/>
-      <c r="M104" s="277"/>
-      <c r="N104" s="278"/>
+      <c r="C104" s="272"/>
+      <c r="D104" s="272"/>
+      <c r="E104" s="272"/>
+      <c r="F104" s="272"/>
+      <c r="G104" s="272"/>
+      <c r="H104" s="272"/>
+      <c r="I104" s="272"/>
+      <c r="J104" s="272"/>
+      <c r="K104" s="272"/>
+      <c r="L104" s="272"/>
+      <c r="M104" s="272"/>
+      <c r="N104" s="273"/>
       <c r="O104" s="3">
         <v>1</v>
       </c>
@@ -13645,51 +13669,51 @@
       <c r="R104" s="24">
         <v>1</v>
       </c>
-      <c r="U104" s="293" t="s">
+      <c r="U104" s="285" t="s">
         <v>19</v>
       </c>
-      <c r="V104" s="294"/>
-      <c r="W104" s="294"/>
-      <c r="X104" s="294"/>
-      <c r="Y104" s="294"/>
-      <c r="Z104" s="294"/>
-      <c r="AA104" s="294"/>
-      <c r="AB104" s="295">
+      <c r="V104" s="261"/>
+      <c r="W104" s="261"/>
+      <c r="X104" s="261"/>
+      <c r="Y104" s="261"/>
+      <c r="Z104" s="261"/>
+      <c r="AA104" s="261"/>
+      <c r="AB104" s="286">
         <f>AB102*AB103</f>
         <v>440</v>
       </c>
-      <c r="AC104" s="295"/>
-      <c r="AD104" s="296"/>
+      <c r="AC104" s="286"/>
+      <c r="AD104" s="287"/>
       <c r="AE104" s="29"/>
       <c r="AF104" s="29"/>
-      <c r="AG104" s="305" t="s">
+      <c r="AG104" s="267" t="s">
         <v>25</v>
       </c>
-      <c r="AH104" s="291"/>
-      <c r="AI104" s="291"/>
-      <c r="AJ104" s="292"/>
+      <c r="AH104" s="258"/>
+      <c r="AI104" s="258"/>
+      <c r="AJ104" s="259"/>
       <c r="AK104" s="36">
         <v>65</v>
       </c>
     </row>
     <row r="105" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG105" s="297" t="s">
+      <c r="AG105" s="262" t="s">
         <v>23</v>
       </c>
-      <c r="AH105" s="298"/>
-      <c r="AI105" s="298"/>
-      <c r="AJ105" s="298"/>
+      <c r="AH105" s="263"/>
+      <c r="AI105" s="263"/>
+      <c r="AJ105" s="263"/>
       <c r="AK105" s="225">
         <v>30</v>
       </c>
     </row>
     <row r="106" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG106" s="301" t="s">
+      <c r="AG106" s="260" t="s">
         <v>19</v>
       </c>
-      <c r="AH106" s="294"/>
-      <c r="AI106" s="294"/>
-      <c r="AJ106" s="294"/>
+      <c r="AH106" s="261"/>
+      <c r="AI106" s="261"/>
+      <c r="AJ106" s="261"/>
       <c r="AK106" s="224">
         <f>SUM(AK102:AK105)</f>
         <v>440</v>
@@ -13701,12 +13725,22 @@
     <sortCondition ref="B10:B94"/>
   </sortState>
   <mergeCells count="38">
-    <mergeCell ref="B103:N103"/>
-    <mergeCell ref="AG106:AJ106"/>
-    <mergeCell ref="AG105:AJ105"/>
-    <mergeCell ref="AG102:AJ102"/>
-    <mergeCell ref="AG104:AJ104"/>
-    <mergeCell ref="AG103:AJ103"/>
+    <mergeCell ref="O100:R100"/>
+    <mergeCell ref="U101:AD101"/>
+    <mergeCell ref="AG101:AK101"/>
+    <mergeCell ref="AH4:AJ4"/>
+    <mergeCell ref="AG5:AG9"/>
+    <mergeCell ref="AJ5:AJ9"/>
+    <mergeCell ref="X5:AA5"/>
+    <mergeCell ref="AB5:AB9"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="C4:S4"/>
+    <mergeCell ref="T4:AB4"/>
+    <mergeCell ref="AC4:AG4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="K5:R5"/>
+    <mergeCell ref="S5:S9"/>
     <mergeCell ref="T5:W5"/>
     <mergeCell ref="B104:N104"/>
     <mergeCell ref="C1:O1"/>
@@ -13723,22 +13757,12 @@
     <mergeCell ref="AB104:AD104"/>
     <mergeCell ref="U103:AA103"/>
     <mergeCell ref="AB103:AD103"/>
-    <mergeCell ref="O100:R100"/>
-    <mergeCell ref="U101:AD101"/>
-    <mergeCell ref="AG101:AK101"/>
-    <mergeCell ref="AH4:AJ4"/>
-    <mergeCell ref="AG5:AG9"/>
-    <mergeCell ref="AJ5:AJ9"/>
-    <mergeCell ref="X5:AA5"/>
-    <mergeCell ref="AB5:AB9"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="C4:S4"/>
-    <mergeCell ref="T4:AB4"/>
-    <mergeCell ref="AC4:AG4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="K5:R5"/>
-    <mergeCell ref="S5:S9"/>
+    <mergeCell ref="B103:N103"/>
+    <mergeCell ref="AG106:AJ106"/>
+    <mergeCell ref="AG105:AJ105"/>
+    <mergeCell ref="AG102:AJ102"/>
+    <mergeCell ref="AG104:AJ104"/>
+    <mergeCell ref="AG103:AJ103"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <conditionalFormatting sqref="AH18:AI18 AH10:AI10 AH14:AI14 T10:AA10 AC10:AF10 C10:R10 C14:R14 T14:AA14 AC14:AF14 T18:AA18 AC18:AF18 AH30:AI30 C30:R30 T30:AA30 AC30:AF30 AH26:AI26 C26:R26 T26:AA26 AC26:AF26 AH62:AI62 C62:R62 T62:AA62 AC62:AF62 AH42:AI42 C42:R42 T42:AA42 AC42:AF42 AH22:AI22 C22:R22 T22:AA22 AC22:AF22 AH38:AI38 C38:R38 T38:AA38 AC38:AF38 AH34:AI34 C34:R34 T34:AA34 AC34:AF34 AH66:AI66 C66:R66 T66:AA66 AC66:AF66 C18:R18">
@@ -14394,20 +14418,20 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:AJ31"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="2.7109375" style="19" customWidth="1"/>
     <col min="6" max="6" width="3" style="19" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="2.7109375" style="19" customWidth="1"/>
     <col min="10" max="10" width="2.7109375" style="2" customWidth="1"/>
     <col min="11" max="12" width="2.7109375" customWidth="1"/>
-    <col min="13" max="13" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="21" width="2.7109375" style="18" customWidth="1"/>
     <col min="22" max="24" width="2.7109375" customWidth="1"/>
@@ -14596,18 +14620,20 @@
       <c r="H6" s="85">
         <v>4</v>
       </c>
-      <c r="I6" s="85"/>
+      <c r="I6" s="85">
+        <v>5</v>
+      </c>
       <c r="J6" s="77">
         <f>IF(C6&gt;C7,1,0)+IF(D6&gt;D7,1,0)+IF(E6&gt;E7,1,0)+IF(F6&gt;F7,1,0)+IF(G6&gt;G7,1,0)+IF(H6&gt;H7,1,0)+IF(I6&gt;I7,1,0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K6" s="16"/>
       <c r="L6" s="13"/>
       <c r="M6" s="76" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="N6" s="87" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="O6" s="85"/>
       <c r="P6" s="85"/>
@@ -14656,7 +14682,9 @@
       <c r="H7" s="85">
         <v>2</v>
       </c>
-      <c r="I7" s="85"/>
+      <c r="I7" s="85">
+        <v>1</v>
+      </c>
       <c r="J7" s="77">
         <f>IF(C7&gt;C6,1,0)+IF(D7&gt;D6,1,0)+IF(E7&gt;E6,1,0)+IF(F7&gt;F6,1,0)+IF(G7&gt;G6,1,0)+IF(H7&gt;H6,1,0)+IF(I7&gt;I6,1,0)</f>
         <v>3</v>
@@ -14664,10 +14692,10 @@
       <c r="K7" s="55"/>
       <c r="L7" s="4"/>
       <c r="M7" s="76" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="N7" s="87" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="O7" s="85"/>
       <c r="P7" s="85"/>
@@ -15285,10 +15313,10 @@
       <c r="K20" s="16"/>
       <c r="L20" s="13"/>
       <c r="M20" s="76" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="N20" s="87" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O20" s="85"/>
       <c r="P20" s="85"/>
@@ -15347,10 +15375,10 @@
       <c r="K21" s="55"/>
       <c r="L21" s="4"/>
       <c r="M21" s="76" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="N21" s="87" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="O21" s="85"/>
       <c r="P21" s="85"/>
@@ -15496,10 +15524,10 @@
       <c r="K24" s="13"/>
       <c r="L24" s="13"/>
       <c r="M24" s="76" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="N24" s="87" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="O24" s="85"/>
       <c r="P24" s="86"/>
@@ -15557,10 +15585,10 @@
       <c r="K25" s="14"/>
       <c r="L25" s="4"/>
       <c r="M25" s="76" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="N25" s="87" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O25" s="85"/>
       <c r="P25" s="86"/>
@@ -15639,10 +15667,12 @@
       <c r="H27" s="86">
         <v>2</v>
       </c>
-      <c r="I27" s="85"/>
+      <c r="I27" s="85">
+        <v>5</v>
+      </c>
       <c r="J27" s="77">
         <f>IF(C27&gt;C28,1,0)+IF(D27&gt;D28,1,0)+IF(E27&gt;E28,1,0)+IF(F27&gt;F28,1,0)+IF(G27&gt;G28,1,0)+IF(H27&gt;H28,1,0)+IF(I27&gt;I28,1,0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K27" s="16"/>
       <c r="L27" s="4"/>
@@ -15690,7 +15720,9 @@
       <c r="H28" s="86">
         <v>1</v>
       </c>
-      <c r="I28" s="85"/>
+      <c r="I28" s="85">
+        <v>4</v>
+      </c>
       <c r="J28" s="77">
         <f>IF(C28&gt;C27,1,0)+IF(D28&gt;D27,1,0)+IF(E28&gt;E27,1,0)+IF(F28&gt;F27,1,0)+IF(G28&gt;G27,1,0)+IF(H28&gt;H27,1,0)+IF(I28&gt;I27,1,0)</f>
         <v>3</v>

</xml_diff>

<commit_message>
Fixed 2nd round teams
</commit_message>
<xml_diff>
--- a/laval.xlsx
+++ b/laval.xlsx
@@ -2516,6 +2516,162 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="108" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="113" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="114" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="95" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2525,18 +2681,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="86" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="87" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="88" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="87" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="95" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2548,177 +2719,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="86" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="88" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="113" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="114" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="95" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="108" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3941,217 +3941,217 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="C1" s="274"/>
-      <c r="D1" s="274"/>
-      <c r="E1" s="274"/>
-      <c r="F1" s="274"/>
-      <c r="G1" s="274"/>
-      <c r="H1" s="274"/>
-      <c r="I1" s="274"/>
-      <c r="J1" s="274"/>
-      <c r="K1" s="274"/>
-      <c r="L1" s="274"/>
-      <c r="M1" s="274"/>
-      <c r="N1" s="274"/>
-      <c r="O1" s="274"/>
-      <c r="P1" s="275"/>
-      <c r="Q1" s="275"/>
-      <c r="R1" s="275"/>
-      <c r="S1" s="275"/>
-      <c r="T1" s="275"/>
-      <c r="U1" s="275"/>
-      <c r="V1" s="275"/>
-      <c r="W1" s="275"/>
-      <c r="X1" s="275"/>
-      <c r="Y1" s="275"/>
-      <c r="Z1" s="275"/>
-      <c r="AA1" s="275"/>
-      <c r="AB1" s="275"/>
-      <c r="AC1" s="275"/>
-      <c r="AD1" s="275"/>
-      <c r="AE1" s="275"/>
-      <c r="AF1" s="275"/>
-      <c r="AG1" s="275"/>
-      <c r="AH1" s="275"/>
-      <c r="AI1" s="275"/>
-      <c r="AJ1" s="275"/>
+      <c r="C1" s="298"/>
+      <c r="D1" s="298"/>
+      <c r="E1" s="298"/>
+      <c r="F1" s="298"/>
+      <c r="G1" s="298"/>
+      <c r="H1" s="298"/>
+      <c r="I1" s="298"/>
+      <c r="J1" s="298"/>
+      <c r="K1" s="298"/>
+      <c r="L1" s="298"/>
+      <c r="M1" s="298"/>
+      <c r="N1" s="298"/>
+      <c r="O1" s="298"/>
+      <c r="P1" s="299"/>
+      <c r="Q1" s="299"/>
+      <c r="R1" s="299"/>
+      <c r="S1" s="299"/>
+      <c r="T1" s="299"/>
+      <c r="U1" s="299"/>
+      <c r="V1" s="299"/>
+      <c r="W1" s="299"/>
+      <c r="X1" s="299"/>
+      <c r="Y1" s="299"/>
+      <c r="Z1" s="299"/>
+      <c r="AA1" s="299"/>
+      <c r="AB1" s="299"/>
+      <c r="AC1" s="299"/>
+      <c r="AD1" s="299"/>
+      <c r="AE1" s="299"/>
+      <c r="AF1" s="299"/>
+      <c r="AG1" s="299"/>
+      <c r="AH1" s="299"/>
+      <c r="AI1" s="299"/>
+      <c r="AJ1" s="299"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="41"/>
-      <c r="C2" s="276" t="s">
+      <c r="C2" s="300" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="276"/>
-      <c r="E2" s="276"/>
-      <c r="F2" s="276"/>
-      <c r="G2" s="276"/>
-      <c r="H2" s="276"/>
-      <c r="I2" s="276"/>
-      <c r="J2" s="276"/>
-      <c r="K2" s="276"/>
-      <c r="L2" s="276"/>
-      <c r="M2" s="276"/>
-      <c r="N2" s="276"/>
-      <c r="O2" s="276"/>
-      <c r="P2" s="276"/>
-      <c r="Q2" s="277" t="s">
+      <c r="D2" s="300"/>
+      <c r="E2" s="300"/>
+      <c r="F2" s="300"/>
+      <c r="G2" s="300"/>
+      <c r="H2" s="300"/>
+      <c r="I2" s="300"/>
+      <c r="J2" s="300"/>
+      <c r="K2" s="300"/>
+      <c r="L2" s="300"/>
+      <c r="M2" s="300"/>
+      <c r="N2" s="300"/>
+      <c r="O2" s="300"/>
+      <c r="P2" s="300"/>
+      <c r="Q2" s="301" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="275"/>
-      <c r="S2" s="275"/>
-      <c r="T2" s="275"/>
-      <c r="U2" s="275"/>
-      <c r="V2" s="275"/>
-      <c r="W2" s="275"/>
-      <c r="X2" s="275"/>
-      <c r="Y2" s="275"/>
-      <c r="Z2" s="275"/>
-      <c r="AA2" s="275"/>
-      <c r="AB2" s="275"/>
-      <c r="AC2" s="275"/>
-      <c r="AD2" s="275"/>
-      <c r="AE2" s="275"/>
-      <c r="AF2" s="275"/>
-      <c r="AG2" s="275"/>
-      <c r="AH2" s="275"/>
-      <c r="AI2" s="275"/>
-      <c r="AJ2" s="275"/>
+      <c r="R2" s="299"/>
+      <c r="S2" s="299"/>
+      <c r="T2" s="299"/>
+      <c r="U2" s="299"/>
+      <c r="V2" s="299"/>
+      <c r="W2" s="299"/>
+      <c r="X2" s="299"/>
+      <c r="Y2" s="299"/>
+      <c r="Z2" s="299"/>
+      <c r="AA2" s="299"/>
+      <c r="AB2" s="299"/>
+      <c r="AC2" s="299"/>
+      <c r="AD2" s="299"/>
+      <c r="AE2" s="299"/>
+      <c r="AF2" s="299"/>
+      <c r="AG2" s="299"/>
+      <c r="AH2" s="299"/>
+      <c r="AI2" s="299"/>
+      <c r="AJ2" s="299"/>
     </row>
     <row r="3" spans="1:38" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="274"/>
-      <c r="D3" s="274"/>
-      <c r="E3" s="274"/>
-      <c r="F3" s="274"/>
-      <c r="G3" s="274"/>
-      <c r="H3" s="274"/>
-      <c r="I3" s="274"/>
-      <c r="J3" s="274"/>
-      <c r="K3" s="274"/>
-      <c r="L3" s="274"/>
-      <c r="M3" s="274"/>
-      <c r="N3" s="274"/>
-      <c r="O3" s="274"/>
-      <c r="P3" s="275"/>
-      <c r="Q3" s="275"/>
-      <c r="R3" s="275"/>
-      <c r="S3" s="275"/>
-      <c r="T3" s="275"/>
-      <c r="U3" s="275"/>
-      <c r="V3" s="275"/>
-      <c r="W3" s="275"/>
-      <c r="X3" s="275"/>
-      <c r="Y3" s="275"/>
-      <c r="Z3" s="275"/>
-      <c r="AA3" s="275"/>
-      <c r="AB3" s="275"/>
-      <c r="AC3" s="275"/>
-      <c r="AD3" s="275"/>
-      <c r="AE3" s="275"/>
-      <c r="AF3" s="275"/>
-      <c r="AG3" s="275"/>
-      <c r="AH3" s="275"/>
-      <c r="AI3" s="275"/>
-      <c r="AJ3" s="275"/>
+      <c r="C3" s="298"/>
+      <c r="D3" s="298"/>
+      <c r="E3" s="298"/>
+      <c r="F3" s="298"/>
+      <c r="G3" s="298"/>
+      <c r="H3" s="298"/>
+      <c r="I3" s="298"/>
+      <c r="J3" s="298"/>
+      <c r="K3" s="298"/>
+      <c r="L3" s="298"/>
+      <c r="M3" s="298"/>
+      <c r="N3" s="298"/>
+      <c r="O3" s="298"/>
+      <c r="P3" s="299"/>
+      <c r="Q3" s="299"/>
+      <c r="R3" s="299"/>
+      <c r="S3" s="299"/>
+      <c r="T3" s="299"/>
+      <c r="U3" s="299"/>
+      <c r="V3" s="299"/>
+      <c r="W3" s="299"/>
+      <c r="X3" s="299"/>
+      <c r="Y3" s="299"/>
+      <c r="Z3" s="299"/>
+      <c r="AA3" s="299"/>
+      <c r="AB3" s="299"/>
+      <c r="AC3" s="299"/>
+      <c r="AD3" s="299"/>
+      <c r="AE3" s="299"/>
+      <c r="AF3" s="299"/>
+      <c r="AG3" s="299"/>
+      <c r="AH3" s="299"/>
+      <c r="AI3" s="299"/>
+      <c r="AJ3" s="299"/>
     </row>
     <row r="4" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="299" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="300"/>
-      <c r="E4" s="300"/>
-      <c r="F4" s="300"/>
-      <c r="G4" s="300"/>
-      <c r="H4" s="300"/>
-      <c r="I4" s="300"/>
-      <c r="J4" s="300"/>
-      <c r="K4" s="300"/>
-      <c r="L4" s="300"/>
-      <c r="M4" s="300"/>
-      <c r="N4" s="300"/>
-      <c r="O4" s="300"/>
-      <c r="P4" s="300"/>
-      <c r="Q4" s="300"/>
-      <c r="R4" s="300"/>
-      <c r="S4" s="301"/>
-      <c r="T4" s="299" t="s">
+      <c r="C4" s="282" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="283"/>
+      <c r="E4" s="283"/>
+      <c r="F4" s="283"/>
+      <c r="G4" s="283"/>
+      <c r="H4" s="283"/>
+      <c r="I4" s="283"/>
+      <c r="J4" s="283"/>
+      <c r="K4" s="283"/>
+      <c r="L4" s="283"/>
+      <c r="M4" s="283"/>
+      <c r="N4" s="283"/>
+      <c r="O4" s="283"/>
+      <c r="P4" s="283"/>
+      <c r="Q4" s="283"/>
+      <c r="R4" s="283"/>
+      <c r="S4" s="284"/>
+      <c r="T4" s="282" t="s">
         <v>1</v>
       </c>
-      <c r="U4" s="300"/>
-      <c r="V4" s="300"/>
-      <c r="W4" s="300"/>
-      <c r="X4" s="300"/>
-      <c r="Y4" s="300"/>
-      <c r="Z4" s="300"/>
-      <c r="AA4" s="300"/>
-      <c r="AB4" s="301"/>
-      <c r="AC4" s="299" t="s">
+      <c r="U4" s="283"/>
+      <c r="V4" s="283"/>
+      <c r="W4" s="283"/>
+      <c r="X4" s="283"/>
+      <c r="Y4" s="283"/>
+      <c r="Z4" s="283"/>
+      <c r="AA4" s="283"/>
+      <c r="AB4" s="284"/>
+      <c r="AC4" s="282" t="s">
         <v>2</v>
       </c>
-      <c r="AD4" s="300"/>
-      <c r="AE4" s="300"/>
-      <c r="AF4" s="300"/>
-      <c r="AG4" s="308"/>
-      <c r="AH4" s="299" t="s">
+      <c r="AD4" s="283"/>
+      <c r="AE4" s="283"/>
+      <c r="AF4" s="283"/>
+      <c r="AG4" s="293"/>
+      <c r="AH4" s="282" t="s">
         <v>10</v>
       </c>
-      <c r="AI4" s="300"/>
-      <c r="AJ4" s="301"/>
+      <c r="AI4" s="283"/>
+      <c r="AJ4" s="284"/>
     </row>
     <row r="5" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="268" t="s">
+      <c r="C5" s="294" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="269"/>
-      <c r="E5" s="269"/>
-      <c r="F5" s="269"/>
-      <c r="G5" s="269"/>
-      <c r="H5" s="269"/>
-      <c r="I5" s="269"/>
-      <c r="J5" s="270"/>
-      <c r="K5" s="306" t="s">
+      <c r="D5" s="290"/>
+      <c r="E5" s="290"/>
+      <c r="F5" s="290"/>
+      <c r="G5" s="290"/>
+      <c r="H5" s="290"/>
+      <c r="I5" s="290"/>
+      <c r="J5" s="291"/>
+      <c r="K5" s="289" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="269"/>
-      <c r="M5" s="269"/>
-      <c r="N5" s="269"/>
-      <c r="O5" s="269"/>
-      <c r="P5" s="269"/>
-      <c r="Q5" s="269"/>
-      <c r="R5" s="270"/>
-      <c r="S5" s="302" t="s">
+      <c r="L5" s="290"/>
+      <c r="M5" s="290"/>
+      <c r="N5" s="290"/>
+      <c r="O5" s="290"/>
+      <c r="P5" s="290"/>
+      <c r="Q5" s="290"/>
+      <c r="R5" s="291"/>
+      <c r="S5" s="285" t="s">
         <v>12</v>
       </c>
-      <c r="T5" s="268" t="s">
+      <c r="T5" s="294" t="s">
         <v>9</v>
       </c>
-      <c r="U5" s="269"/>
-      <c r="V5" s="269"/>
-      <c r="W5" s="270"/>
-      <c r="X5" s="306" t="s">
+      <c r="U5" s="290"/>
+      <c r="V5" s="290"/>
+      <c r="W5" s="291"/>
+      <c r="X5" s="289" t="s">
         <v>8</v>
       </c>
-      <c r="Y5" s="269"/>
-      <c r="Z5" s="269"/>
-      <c r="AA5" s="270"/>
-      <c r="AB5" s="302" t="s">
+      <c r="Y5" s="290"/>
+      <c r="Z5" s="290"/>
+      <c r="AA5" s="291"/>
+      <c r="AB5" s="285" t="s">
         <v>13</v>
       </c>
-      <c r="AC5" s="307" t="s">
+      <c r="AC5" s="292" t="s">
         <v>9</v>
       </c>
-      <c r="AD5" s="270"/>
-      <c r="AE5" s="306" t="s">
+      <c r="AD5" s="291"/>
+      <c r="AE5" s="289" t="s">
         <v>8</v>
       </c>
-      <c r="AF5" s="270"/>
-      <c r="AG5" s="302" t="s">
+      <c r="AF5" s="291"/>
+      <c r="AG5" s="285" t="s">
         <v>14</v>
       </c>
       <c r="AH5" s="56"/>
       <c r="AI5" s="25"/>
-      <c r="AJ5" s="302" t="s">
+      <c r="AJ5" s="285" t="s">
         <v>15</v>
       </c>
       <c r="AK5" s="4"/>
@@ -4215,7 +4215,7 @@
         <f>Résultats!$J$25</f>
         <v>4</v>
       </c>
-      <c r="Q6" s="315">
+      <c r="Q6" s="263">
         <f>Résultats!$J$27</f>
         <v>4</v>
       </c>
@@ -4223,7 +4223,7 @@
         <f>Résultats!$J$28</f>
         <v>3</v>
       </c>
-      <c r="S6" s="303"/>
+      <c r="S6" s="286"/>
       <c r="T6" s="169">
         <f>Résultats!$V$6</f>
         <v>0</v>
@@ -4256,7 +4256,7 @@
         <f>Résultats!$V$25</f>
         <v>0</v>
       </c>
-      <c r="AB6" s="303"/>
+      <c r="AB6" s="286"/>
       <c r="AC6" s="111">
         <f>Résultats!$AH$8</f>
         <v>0</v>
@@ -4273,7 +4273,7 @@
         <f>Résultats!$AH$23</f>
         <v>0</v>
       </c>
-      <c r="AG6" s="303"/>
+      <c r="AG6" s="286"/>
       <c r="AH6" s="212">
         <f>Résultats!$AH$15</f>
         <v>0</v>
@@ -4282,7 +4282,7 @@
         <f>Résultats!$AH$16</f>
         <v>0</v>
       </c>
-      <c r="AJ6" s="303"/>
+      <c r="AJ6" s="286"/>
       <c r="AK6" s="37"/>
     </row>
     <row r="7" spans="1:38" s="39" customFormat="1" ht="58.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -4306,9 +4306,9 @@
       <c r="N7" s="246"/>
       <c r="O7" s="173"/>
       <c r="P7" s="246"/>
-      <c r="Q7" s="316"/>
+      <c r="Q7" s="264"/>
       <c r="R7" s="117"/>
-      <c r="S7" s="303"/>
+      <c r="S7" s="286"/>
       <c r="T7" s="170"/>
       <c r="U7" s="117"/>
       <c r="V7" s="173"/>
@@ -4317,15 +4317,15 @@
       <c r="Y7" s="118"/>
       <c r="Z7" s="119"/>
       <c r="AA7" s="117"/>
-      <c r="AB7" s="303"/>
+      <c r="AB7" s="286"/>
       <c r="AC7" s="119"/>
       <c r="AD7" s="117"/>
       <c r="AE7" s="120"/>
       <c r="AF7" s="117"/>
-      <c r="AG7" s="303"/>
+      <c r="AG7" s="286"/>
       <c r="AH7" s="212"/>
       <c r="AI7" s="112"/>
-      <c r="AJ7" s="303"/>
+      <c r="AJ7" s="286"/>
       <c r="AK7" s="37"/>
     </row>
     <row r="8" spans="1:38" s="39" customFormat="1" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4387,7 +4387,7 @@
         <f>Résultats!$B$25</f>
         <v>DALLAS</v>
       </c>
-      <c r="Q8" s="317" t="str">
+      <c r="Q8" s="265" t="str">
         <f>Résultats!$B$27</f>
         <v>SAN JOSE</v>
       </c>
@@ -4395,7 +4395,7 @@
         <f>Résultats!$B$28</f>
         <v>VEGAS</v>
       </c>
-      <c r="S8" s="303"/>
+      <c r="S8" s="286"/>
       <c r="T8" s="171" t="str">
         <f>Résultats!$N$6</f>
         <v>BOSTON</v>
@@ -4422,13 +4422,13 @@
       </c>
       <c r="Z8" s="177" t="str">
         <f>Résultats!$N$24</f>
-        <v>VEGAS</v>
+        <v>SAN JOSE</v>
       </c>
       <c r="AA8" s="174" t="str">
         <f>Résultats!$N$25</f>
         <v>DALLAS</v>
       </c>
-      <c r="AB8" s="303"/>
+      <c r="AB8" s="286"/>
       <c r="AC8" s="177" t="str">
         <f>Résultats!$Z$8</f>
         <v xml:space="preserve"> </v>
@@ -4445,7 +4445,7 @@
         <f>Résultats!$Z$23</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AG8" s="303"/>
+      <c r="AG8" s="286"/>
       <c r="AH8" s="213" t="str">
         <f>Résultats!$Z$15</f>
         <v xml:space="preserve"> </v>
@@ -4454,7 +4454,7 @@
         <f>Résultats!$Z$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ8" s="303"/>
+      <c r="AJ8" s="286"/>
       <c r="AK8" s="37"/>
     </row>
     <row r="9" spans="1:38" s="39" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4520,7 +4520,7 @@
         <f>Résultats!$A$25</f>
         <v>WC1</v>
       </c>
-      <c r="Q9" s="318" t="str">
+      <c r="Q9" s="266" t="str">
         <f>Résultats!$A$27</f>
         <v>P2</v>
       </c>
@@ -4528,7 +4528,7 @@
         <f>Résultats!$A$28</f>
         <v>P3</v>
       </c>
-      <c r="S9" s="305"/>
+      <c r="S9" s="288"/>
       <c r="T9" s="179" t="str">
         <f>Résultats!$M$6</f>
         <v>A2</v>
@@ -4555,13 +4555,13 @@
       </c>
       <c r="Z9" s="183" t="str">
         <f>Résultats!$M$24</f>
-        <v>P3</v>
+        <v>P2</v>
       </c>
       <c r="AA9" s="185" t="str">
         <f>Résultats!$M$25</f>
         <v>WC1</v>
       </c>
-      <c r="AB9" s="304"/>
+      <c r="AB9" s="287"/>
       <c r="AC9" s="183" t="str">
         <f>Résultats!$Y$8</f>
         <v xml:space="preserve"> </v>
@@ -4578,7 +4578,7 @@
         <f>Résultats!$Y$23</f>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="AG9" s="304"/>
+      <c r="AG9" s="287"/>
       <c r="AH9" s="215" t="str">
         <f>Résultats!$Y$15</f>
         <v xml:space="preserve"> </v>
@@ -4587,7 +4587,7 @@
         <f>Résultats!$Y$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ9" s="305"/>
+      <c r="AJ9" s="288"/>
       <c r="AK9" s="114" t="s">
         <v>51</v>
       </c>
@@ -4631,7 +4631,7 @@
         <v>6</v>
       </c>
       <c r="P10" s="188"/>
-      <c r="Q10" s="323">
+      <c r="Q10" s="271">
         <v>7</v>
       </c>
       <c r="R10" s="193"/>
@@ -5003,7 +5003,7 @@
         <v>5</v>
       </c>
       <c r="D14" s="45"/>
-      <c r="E14" s="319">
+      <c r="E14" s="267">
         <v>7</v>
       </c>
       <c r="F14" s="45"/>
@@ -5027,7 +5027,7 @@
         <v>5</v>
       </c>
       <c r="P14" s="45"/>
-      <c r="Q14" s="324">
+      <c r="Q14" s="272">
         <v>7</v>
       </c>
       <c r="R14" s="50"/>
@@ -5402,7 +5402,7 @@
         <v>5</v>
       </c>
       <c r="D18" s="199"/>
-      <c r="E18" s="320">
+      <c r="E18" s="268">
         <v>7</v>
       </c>
       <c r="F18" s="199"/>
@@ -5447,7 +5447,7 @@
         <v>0</v>
       </c>
       <c r="AC18" s="201"/>
-      <c r="AD18" s="311"/>
+      <c r="AD18" s="259"/>
       <c r="AE18" s="203"/>
       <c r="AF18" s="202"/>
       <c r="AG18" s="205">
@@ -5801,7 +5801,7 @@
         <v>5</v>
       </c>
       <c r="D22" s="45"/>
-      <c r="E22" s="319">
+      <c r="E22" s="267">
         <v>7</v>
       </c>
       <c r="F22" s="45"/>
@@ -5818,7 +5818,7 @@
       </c>
       <c r="L22" s="47"/>
       <c r="M22" s="44"/>
-      <c r="N22" s="321">
+      <c r="N22" s="269">
         <v>6</v>
       </c>
       <c r="O22" s="44">
@@ -5853,7 +5853,7 @@
         <f>SUM(AC23:AF23)</f>
         <v>0</v>
       </c>
-      <c r="AH22" s="309"/>
+      <c r="AH22" s="257"/>
       <c r="AI22" s="57"/>
       <c r="AJ22" s="129">
         <f>AH23</f>
@@ -6217,7 +6217,7 @@
       </c>
       <c r="L26" s="202"/>
       <c r="M26" s="200"/>
-      <c r="N26" s="322">
+      <c r="N26" s="270">
         <v>6</v>
       </c>
       <c r="O26" s="200">
@@ -6623,7 +6623,7 @@
         <v>6</v>
       </c>
       <c r="P30" s="45"/>
-      <c r="Q30" s="324">
+      <c r="Q30" s="272">
         <v>7</v>
       </c>
       <c r="R30" s="50"/>
@@ -7015,7 +7015,7 @@
         <v>6</v>
       </c>
       <c r="M34" s="200"/>
-      <c r="N34" s="322">
+      <c r="N34" s="270">
         <v>6</v>
       </c>
       <c r="O34" s="200">
@@ -7813,7 +7813,7 @@
       </c>
       <c r="L42" s="202"/>
       <c r="M42" s="200"/>
-      <c r="N42" s="322">
+      <c r="N42" s="270">
         <v>6</v>
       </c>
       <c r="O42" s="200">
@@ -8212,7 +8212,7 @@
       </c>
       <c r="L46" s="47"/>
       <c r="M46" s="44"/>
-      <c r="N46" s="321">
+      <c r="N46" s="269">
         <v>6</v>
       </c>
       <c r="O46" s="44">
@@ -8594,7 +8594,7 @@
         <v>6</v>
       </c>
       <c r="D50" s="199"/>
-      <c r="E50" s="320">
+      <c r="E50" s="268">
         <v>7</v>
       </c>
       <c r="F50" s="199"/>
@@ -9386,15 +9386,15 @@
         <v>7</v>
       </c>
       <c r="D58" s="199"/>
-      <c r="E58" s="312">
+      <c r="E58" s="260">
         <v>6</v>
       </c>
       <c r="F58" s="199"/>
-      <c r="G58" s="313"/>
+      <c r="G58" s="261"/>
       <c r="H58" s="202">
         <v>6</v>
       </c>
-      <c r="I58" s="312"/>
+      <c r="I58" s="260"/>
       <c r="J58" s="202">
         <v>7</v>
       </c>
@@ -9420,7 +9420,7 @@
       </c>
       <c r="T58" s="198"/>
       <c r="U58" s="202"/>
-      <c r="V58" s="314"/>
+      <c r="V58" s="262"/>
       <c r="W58" s="202"/>
       <c r="X58" s="203"/>
       <c r="Y58" s="234"/>
@@ -9782,7 +9782,7 @@
         <v>6</v>
       </c>
       <c r="D62" s="45"/>
-      <c r="E62" s="319">
+      <c r="E62" s="267">
         <v>7</v>
       </c>
       <c r="F62" s="45"/>
@@ -10223,7 +10223,7 @@
         <v>0</v>
       </c>
       <c r="AC66" s="201"/>
-      <c r="AD66" s="311"/>
+      <c r="AD66" s="259"/>
       <c r="AE66" s="203"/>
       <c r="AF66" s="202"/>
       <c r="AG66" s="205">
@@ -12982,7 +12982,7 @@
         <f>SUM(C95:R95)</f>
         <v>14</v>
       </c>
-      <c r="T94" s="310"/>
+      <c r="T94" s="258"/>
       <c r="U94" s="47"/>
       <c r="V94" s="44"/>
       <c r="W94" s="47"/>
@@ -13467,12 +13467,12 @@
     <row r="100" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B100" s="43"/>
       <c r="N100" s="26"/>
-      <c r="O100" s="290" t="s">
+      <c r="O100" s="273" t="s">
         <v>17</v>
       </c>
-      <c r="P100" s="291"/>
-      <c r="Q100" s="291"/>
-      <c r="R100" s="292"/>
+      <c r="P100" s="274"/>
+      <c r="Q100" s="274"/>
+      <c r="R100" s="275"/>
       <c r="AG100" s="30"/>
       <c r="AH100" s="30"/>
       <c r="AI100" s="30"/>
@@ -13481,21 +13481,21 @@
     </row>
     <row r="101" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="33"/>
-      <c r="B101" s="278" t="s">
+      <c r="B101" s="302" t="s">
         <v>16</v>
       </c>
-      <c r="C101" s="279"/>
-      <c r="D101" s="279"/>
-      <c r="E101" s="279"/>
-      <c r="F101" s="279"/>
-      <c r="G101" s="279"/>
-      <c r="H101" s="279"/>
-      <c r="I101" s="279"/>
-      <c r="J101" s="279"/>
-      <c r="K101" s="279"/>
-      <c r="L101" s="279"/>
-      <c r="M101" s="279"/>
-      <c r="N101" s="280"/>
+      <c r="C101" s="303"/>
+      <c r="D101" s="303"/>
+      <c r="E101" s="303"/>
+      <c r="F101" s="303"/>
+      <c r="G101" s="303"/>
+      <c r="H101" s="303"/>
+      <c r="I101" s="303"/>
+      <c r="J101" s="303"/>
+      <c r="K101" s="303"/>
+      <c r="L101" s="303"/>
+      <c r="M101" s="303"/>
+      <c r="N101" s="304"/>
       <c r="O101" s="21">
         <v>1</v>
       </c>
@@ -13508,45 +13508,45 @@
       <c r="R101" s="22">
         <v>4</v>
       </c>
-      <c r="U101" s="293" t="s">
+      <c r="U101" s="276" t="s">
         <v>26</v>
       </c>
-      <c r="V101" s="294"/>
-      <c r="W101" s="294"/>
-      <c r="X101" s="294"/>
-      <c r="Y101" s="294"/>
-      <c r="Z101" s="294"/>
-      <c r="AA101" s="294"/>
-      <c r="AB101" s="294"/>
-      <c r="AC101" s="294"/>
-      <c r="AD101" s="295"/>
+      <c r="V101" s="277"/>
+      <c r="W101" s="277"/>
+      <c r="X101" s="277"/>
+      <c r="Y101" s="277"/>
+      <c r="Z101" s="277"/>
+      <c r="AA101" s="277"/>
+      <c r="AB101" s="277"/>
+      <c r="AC101" s="277"/>
+      <c r="AD101" s="278"/>
       <c r="AE101" s="28"/>
       <c r="AF101" s="28"/>
-      <c r="AG101" s="296" t="s">
+      <c r="AG101" s="279" t="s">
         <v>24</v>
       </c>
-      <c r="AH101" s="297"/>
-      <c r="AI101" s="297"/>
-      <c r="AJ101" s="297"/>
-      <c r="AK101" s="298"/>
+      <c r="AH101" s="280"/>
+      <c r="AI101" s="280"/>
+      <c r="AJ101" s="280"/>
+      <c r="AK101" s="281"/>
     </row>
     <row r="102" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A102" s="34"/>
-      <c r="B102" s="257" t="s">
+      <c r="B102" s="309" t="s">
         <v>6</v>
       </c>
-      <c r="C102" s="258"/>
-      <c r="D102" s="258"/>
-      <c r="E102" s="258"/>
-      <c r="F102" s="258"/>
-      <c r="G102" s="258"/>
-      <c r="H102" s="258"/>
-      <c r="I102" s="258"/>
-      <c r="J102" s="258"/>
-      <c r="K102" s="258"/>
-      <c r="L102" s="258"/>
-      <c r="M102" s="258"/>
-      <c r="N102" s="259"/>
+      <c r="C102" s="310"/>
+      <c r="D102" s="310"/>
+      <c r="E102" s="310"/>
+      <c r="F102" s="310"/>
+      <c r="G102" s="310"/>
+      <c r="H102" s="310"/>
+      <c r="I102" s="310"/>
+      <c r="J102" s="310"/>
+      <c r="K102" s="310"/>
+      <c r="L102" s="310"/>
+      <c r="M102" s="310"/>
+      <c r="N102" s="311"/>
       <c r="O102" s="20">
         <v>5</v>
       </c>
@@ -13559,49 +13559,49 @@
       <c r="R102" s="23">
         <v>20</v>
       </c>
-      <c r="U102" s="283" t="s">
+      <c r="U102" s="307" t="s">
         <v>20</v>
       </c>
-      <c r="V102" s="284"/>
-      <c r="W102" s="284"/>
-      <c r="X102" s="284"/>
-      <c r="Y102" s="284"/>
-      <c r="Z102" s="284"/>
-      <c r="AA102" s="284"/>
-      <c r="AB102" s="281">
+      <c r="V102" s="308"/>
+      <c r="W102" s="308"/>
+      <c r="X102" s="308"/>
+      <c r="Y102" s="308"/>
+      <c r="Z102" s="308"/>
+      <c r="AA102" s="308"/>
+      <c r="AB102" s="305">
         <v>22</v>
       </c>
-      <c r="AC102" s="281"/>
-      <c r="AD102" s="282"/>
+      <c r="AC102" s="305"/>
+      <c r="AD102" s="306"/>
       <c r="AE102" s="29"/>
       <c r="AF102" s="29"/>
-      <c r="AG102" s="264" t="s">
+      <c r="AG102" s="321" t="s">
         <v>21</v>
       </c>
-      <c r="AH102" s="265"/>
-      <c r="AI102" s="265"/>
-      <c r="AJ102" s="266"/>
+      <c r="AH102" s="322"/>
+      <c r="AI102" s="322"/>
+      <c r="AJ102" s="323"/>
       <c r="AK102" s="223">
         <v>230</v>
       </c>
     </row>
     <row r="103" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="34"/>
-      <c r="B103" s="257" t="s">
+      <c r="B103" s="309" t="s">
         <v>5</v>
       </c>
-      <c r="C103" s="258"/>
-      <c r="D103" s="258"/>
-      <c r="E103" s="258"/>
-      <c r="F103" s="258"/>
-      <c r="G103" s="258"/>
-      <c r="H103" s="258"/>
-      <c r="I103" s="258"/>
-      <c r="J103" s="258"/>
-      <c r="K103" s="258"/>
-      <c r="L103" s="258"/>
-      <c r="M103" s="258"/>
-      <c r="N103" s="259"/>
+      <c r="C103" s="310"/>
+      <c r="D103" s="310"/>
+      <c r="E103" s="310"/>
+      <c r="F103" s="310"/>
+      <c r="G103" s="310"/>
+      <c r="H103" s="310"/>
+      <c r="I103" s="310"/>
+      <c r="J103" s="310"/>
+      <c r="K103" s="310"/>
+      <c r="L103" s="310"/>
+      <c r="M103" s="310"/>
+      <c r="N103" s="311"/>
       <c r="O103" s="20">
         <v>2</v>
       </c>
@@ -13614,49 +13614,49 @@
       <c r="R103" s="23">
         <v>8</v>
       </c>
-      <c r="U103" s="262" t="s">
+      <c r="U103" s="316" t="s">
         <v>18</v>
       </c>
-      <c r="V103" s="263"/>
-      <c r="W103" s="263"/>
-      <c r="X103" s="263"/>
-      <c r="Y103" s="263"/>
-      <c r="Z103" s="263"/>
-      <c r="AA103" s="263"/>
-      <c r="AB103" s="288">
+      <c r="V103" s="317"/>
+      <c r="W103" s="317"/>
+      <c r="X103" s="317"/>
+      <c r="Y103" s="317"/>
+      <c r="Z103" s="317"/>
+      <c r="AA103" s="317"/>
+      <c r="AB103" s="318">
         <v>20</v>
       </c>
-      <c r="AC103" s="288"/>
-      <c r="AD103" s="289"/>
+      <c r="AC103" s="318"/>
+      <c r="AD103" s="319"/>
       <c r="AE103" s="29"/>
       <c r="AF103" s="29"/>
-      <c r="AG103" s="267" t="s">
+      <c r="AG103" s="324" t="s">
         <v>22</v>
       </c>
-      <c r="AH103" s="258"/>
-      <c r="AI103" s="258"/>
-      <c r="AJ103" s="259"/>
+      <c r="AH103" s="310"/>
+      <c r="AI103" s="310"/>
+      <c r="AJ103" s="311"/>
       <c r="AK103" s="36">
         <v>115</v>
       </c>
     </row>
     <row r="104" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="35"/>
-      <c r="B104" s="271" t="s">
+      <c r="B104" s="295" t="s">
         <v>4</v>
       </c>
-      <c r="C104" s="272"/>
-      <c r="D104" s="272"/>
-      <c r="E104" s="272"/>
-      <c r="F104" s="272"/>
-      <c r="G104" s="272"/>
-      <c r="H104" s="272"/>
-      <c r="I104" s="272"/>
-      <c r="J104" s="272"/>
-      <c r="K104" s="272"/>
-      <c r="L104" s="272"/>
-      <c r="M104" s="272"/>
-      <c r="N104" s="273"/>
+      <c r="C104" s="296"/>
+      <c r="D104" s="296"/>
+      <c r="E104" s="296"/>
+      <c r="F104" s="296"/>
+      <c r="G104" s="296"/>
+      <c r="H104" s="296"/>
+      <c r="I104" s="296"/>
+      <c r="J104" s="296"/>
+      <c r="K104" s="296"/>
+      <c r="L104" s="296"/>
+      <c r="M104" s="296"/>
+      <c r="N104" s="297"/>
       <c r="O104" s="3">
         <v>1</v>
       </c>
@@ -13669,51 +13669,51 @@
       <c r="R104" s="24">
         <v>1</v>
       </c>
-      <c r="U104" s="285" t="s">
+      <c r="U104" s="312" t="s">
         <v>19</v>
       </c>
-      <c r="V104" s="261"/>
-      <c r="W104" s="261"/>
-      <c r="X104" s="261"/>
-      <c r="Y104" s="261"/>
-      <c r="Z104" s="261"/>
-      <c r="AA104" s="261"/>
-      <c r="AB104" s="286">
+      <c r="V104" s="313"/>
+      <c r="W104" s="313"/>
+      <c r="X104" s="313"/>
+      <c r="Y104" s="313"/>
+      <c r="Z104" s="313"/>
+      <c r="AA104" s="313"/>
+      <c r="AB104" s="314">
         <f>AB102*AB103</f>
         <v>440</v>
       </c>
-      <c r="AC104" s="286"/>
-      <c r="AD104" s="287"/>
+      <c r="AC104" s="314"/>
+      <c r="AD104" s="315"/>
       <c r="AE104" s="29"/>
       <c r="AF104" s="29"/>
-      <c r="AG104" s="267" t="s">
+      <c r="AG104" s="324" t="s">
         <v>25</v>
       </c>
-      <c r="AH104" s="258"/>
-      <c r="AI104" s="258"/>
-      <c r="AJ104" s="259"/>
+      <c r="AH104" s="310"/>
+      <c r="AI104" s="310"/>
+      <c r="AJ104" s="311"/>
       <c r="AK104" s="36">
         <v>65</v>
       </c>
     </row>
     <row r="105" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG105" s="262" t="s">
+      <c r="AG105" s="316" t="s">
         <v>23</v>
       </c>
-      <c r="AH105" s="263"/>
-      <c r="AI105" s="263"/>
-      <c r="AJ105" s="263"/>
+      <c r="AH105" s="317"/>
+      <c r="AI105" s="317"/>
+      <c r="AJ105" s="317"/>
       <c r="AK105" s="225">
         <v>30</v>
       </c>
     </row>
     <row r="106" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG106" s="260" t="s">
+      <c r="AG106" s="320" t="s">
         <v>19</v>
       </c>
-      <c r="AH106" s="261"/>
-      <c r="AI106" s="261"/>
-      <c r="AJ106" s="261"/>
+      <c r="AH106" s="313"/>
+      <c r="AI106" s="313"/>
+      <c r="AJ106" s="313"/>
       <c r="AK106" s="224">
         <f>SUM(AK102:AK105)</f>
         <v>440</v>
@@ -13725,6 +13725,28 @@
     <sortCondition ref="B10:B94"/>
   </sortState>
   <mergeCells count="38">
+    <mergeCell ref="B103:N103"/>
+    <mergeCell ref="AG106:AJ106"/>
+    <mergeCell ref="AG105:AJ105"/>
+    <mergeCell ref="AG102:AJ102"/>
+    <mergeCell ref="AG104:AJ104"/>
+    <mergeCell ref="AG103:AJ103"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="B104:N104"/>
+    <mergeCell ref="C1:O1"/>
+    <mergeCell ref="P1:AJ1"/>
+    <mergeCell ref="C3:O3"/>
+    <mergeCell ref="P3:AJ3"/>
+    <mergeCell ref="C2:P2"/>
+    <mergeCell ref="Q2:AJ2"/>
+    <mergeCell ref="B101:N101"/>
+    <mergeCell ref="AB102:AD102"/>
+    <mergeCell ref="U102:AA102"/>
+    <mergeCell ref="B102:N102"/>
+    <mergeCell ref="U104:AA104"/>
+    <mergeCell ref="AB104:AD104"/>
+    <mergeCell ref="U103:AA103"/>
+    <mergeCell ref="AB103:AD103"/>
     <mergeCell ref="O100:R100"/>
     <mergeCell ref="U101:AD101"/>
     <mergeCell ref="AG101:AK101"/>
@@ -13741,28 +13763,6 @@
     <mergeCell ref="C5:J5"/>
     <mergeCell ref="K5:R5"/>
     <mergeCell ref="S5:S9"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="B104:N104"/>
-    <mergeCell ref="C1:O1"/>
-    <mergeCell ref="P1:AJ1"/>
-    <mergeCell ref="C3:O3"/>
-    <mergeCell ref="P3:AJ3"/>
-    <mergeCell ref="C2:P2"/>
-    <mergeCell ref="Q2:AJ2"/>
-    <mergeCell ref="B101:N101"/>
-    <mergeCell ref="AB102:AD102"/>
-    <mergeCell ref="U102:AA102"/>
-    <mergeCell ref="B102:N102"/>
-    <mergeCell ref="U104:AA104"/>
-    <mergeCell ref="AB104:AD104"/>
-    <mergeCell ref="U103:AA103"/>
-    <mergeCell ref="AB103:AD103"/>
-    <mergeCell ref="B103:N103"/>
-    <mergeCell ref="AG106:AJ106"/>
-    <mergeCell ref="AG105:AJ105"/>
-    <mergeCell ref="AG102:AJ102"/>
-    <mergeCell ref="AG104:AJ104"/>
-    <mergeCell ref="AG103:AJ103"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <conditionalFormatting sqref="AH18:AI18 AH10:AI10 AH14:AI14 T10:AA10 AC10:AF10 C10:R10 C14:R14 T14:AA14 AC14:AF14 T18:AA18 AC18:AF18 AH30:AI30 C30:R30 T30:AA30 AC30:AF30 AH26:AI26 C26:R26 T26:AA26 AC26:AF26 AH62:AI62 C62:R62 T62:AA62 AC62:AF62 AH42:AI42 C42:R42 T42:AA42 AC42:AF42 AH22:AI22 C22:R22 T22:AA22 AC22:AF22 AH38:AI38 C38:R38 T38:AA38 AC38:AF38 AH34:AI34 C34:R34 T34:AA34 AC34:AF34 AH66:AI66 C66:R66 T66:AA66 AC66:AF66 C18:R18">
@@ -14419,7 +14419,7 @@
   <dimension ref="A1:AJ31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15524,10 +15524,10 @@
       <c r="K24" s="13"/>
       <c r="L24" s="13"/>
       <c r="M24" s="76" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N24" s="87" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="O24" s="85"/>
       <c r="P24" s="86"/>

</xml_diff>

<commit_message>
Fixed 2nd page width
</commit_message>
<xml_diff>
--- a/laval.xlsx
+++ b/laval.xlsx
@@ -2564,6 +2564,105 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="87" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="95" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="86" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="88" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2615,110 +2714,11 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="86" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="87" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="88" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="95" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3941,217 +3941,217 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="C1" s="298"/>
-      <c r="D1" s="298"/>
-      <c r="E1" s="298"/>
-      <c r="F1" s="298"/>
-      <c r="G1" s="298"/>
-      <c r="H1" s="298"/>
-      <c r="I1" s="298"/>
-      <c r="J1" s="298"/>
-      <c r="K1" s="298"/>
-      <c r="L1" s="298"/>
-      <c r="M1" s="298"/>
-      <c r="N1" s="298"/>
-      <c r="O1" s="298"/>
-      <c r="P1" s="299"/>
-      <c r="Q1" s="299"/>
-      <c r="R1" s="299"/>
-      <c r="S1" s="299"/>
-      <c r="T1" s="299"/>
-      <c r="U1" s="299"/>
-      <c r="V1" s="299"/>
-      <c r="W1" s="299"/>
-      <c r="X1" s="299"/>
-      <c r="Y1" s="299"/>
-      <c r="Z1" s="299"/>
-      <c r="AA1" s="299"/>
-      <c r="AB1" s="299"/>
-      <c r="AC1" s="299"/>
-      <c r="AD1" s="299"/>
-      <c r="AE1" s="299"/>
-      <c r="AF1" s="299"/>
-      <c r="AG1" s="299"/>
-      <c r="AH1" s="299"/>
-      <c r="AI1" s="299"/>
-      <c r="AJ1" s="299"/>
+      <c r="C1" s="290"/>
+      <c r="D1" s="290"/>
+      <c r="E1" s="290"/>
+      <c r="F1" s="290"/>
+      <c r="G1" s="290"/>
+      <c r="H1" s="290"/>
+      <c r="I1" s="290"/>
+      <c r="J1" s="290"/>
+      <c r="K1" s="290"/>
+      <c r="L1" s="290"/>
+      <c r="M1" s="290"/>
+      <c r="N1" s="290"/>
+      <c r="O1" s="290"/>
+      <c r="P1" s="291"/>
+      <c r="Q1" s="291"/>
+      <c r="R1" s="291"/>
+      <c r="S1" s="291"/>
+      <c r="T1" s="291"/>
+      <c r="U1" s="291"/>
+      <c r="V1" s="291"/>
+      <c r="W1" s="291"/>
+      <c r="X1" s="291"/>
+      <c r="Y1" s="291"/>
+      <c r="Z1" s="291"/>
+      <c r="AA1" s="291"/>
+      <c r="AB1" s="291"/>
+      <c r="AC1" s="291"/>
+      <c r="AD1" s="291"/>
+      <c r="AE1" s="291"/>
+      <c r="AF1" s="291"/>
+      <c r="AG1" s="291"/>
+      <c r="AH1" s="291"/>
+      <c r="AI1" s="291"/>
+      <c r="AJ1" s="291"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="41"/>
-      <c r="C2" s="300" t="s">
+      <c r="C2" s="292" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="300"/>
-      <c r="E2" s="300"/>
-      <c r="F2" s="300"/>
-      <c r="G2" s="300"/>
-      <c r="H2" s="300"/>
-      <c r="I2" s="300"/>
-      <c r="J2" s="300"/>
-      <c r="K2" s="300"/>
-      <c r="L2" s="300"/>
-      <c r="M2" s="300"/>
-      <c r="N2" s="300"/>
-      <c r="O2" s="300"/>
-      <c r="P2" s="300"/>
-      <c r="Q2" s="301" t="s">
+      <c r="D2" s="292"/>
+      <c r="E2" s="292"/>
+      <c r="F2" s="292"/>
+      <c r="G2" s="292"/>
+      <c r="H2" s="292"/>
+      <c r="I2" s="292"/>
+      <c r="J2" s="292"/>
+      <c r="K2" s="292"/>
+      <c r="L2" s="292"/>
+      <c r="M2" s="292"/>
+      <c r="N2" s="292"/>
+      <c r="O2" s="292"/>
+      <c r="P2" s="292"/>
+      <c r="Q2" s="293" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="299"/>
-      <c r="S2" s="299"/>
-      <c r="T2" s="299"/>
-      <c r="U2" s="299"/>
-      <c r="V2" s="299"/>
-      <c r="W2" s="299"/>
-      <c r="X2" s="299"/>
-      <c r="Y2" s="299"/>
-      <c r="Z2" s="299"/>
-      <c r="AA2" s="299"/>
-      <c r="AB2" s="299"/>
-      <c r="AC2" s="299"/>
-      <c r="AD2" s="299"/>
-      <c r="AE2" s="299"/>
-      <c r="AF2" s="299"/>
-      <c r="AG2" s="299"/>
-      <c r="AH2" s="299"/>
-      <c r="AI2" s="299"/>
-      <c r="AJ2" s="299"/>
+      <c r="R2" s="291"/>
+      <c r="S2" s="291"/>
+      <c r="T2" s="291"/>
+      <c r="U2" s="291"/>
+      <c r="V2" s="291"/>
+      <c r="W2" s="291"/>
+      <c r="X2" s="291"/>
+      <c r="Y2" s="291"/>
+      <c r="Z2" s="291"/>
+      <c r="AA2" s="291"/>
+      <c r="AB2" s="291"/>
+      <c r="AC2" s="291"/>
+      <c r="AD2" s="291"/>
+      <c r="AE2" s="291"/>
+      <c r="AF2" s="291"/>
+      <c r="AG2" s="291"/>
+      <c r="AH2" s="291"/>
+      <c r="AI2" s="291"/>
+      <c r="AJ2" s="291"/>
     </row>
     <row r="3" spans="1:38" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="298"/>
-      <c r="D3" s="298"/>
-      <c r="E3" s="298"/>
-      <c r="F3" s="298"/>
-      <c r="G3" s="298"/>
-      <c r="H3" s="298"/>
-      <c r="I3" s="298"/>
-      <c r="J3" s="298"/>
-      <c r="K3" s="298"/>
-      <c r="L3" s="298"/>
-      <c r="M3" s="298"/>
-      <c r="N3" s="298"/>
-      <c r="O3" s="298"/>
-      <c r="P3" s="299"/>
-      <c r="Q3" s="299"/>
-      <c r="R3" s="299"/>
-      <c r="S3" s="299"/>
-      <c r="T3" s="299"/>
-      <c r="U3" s="299"/>
-      <c r="V3" s="299"/>
-      <c r="W3" s="299"/>
-      <c r="X3" s="299"/>
-      <c r="Y3" s="299"/>
-      <c r="Z3" s="299"/>
-      <c r="AA3" s="299"/>
-      <c r="AB3" s="299"/>
-      <c r="AC3" s="299"/>
-      <c r="AD3" s="299"/>
-      <c r="AE3" s="299"/>
-      <c r="AF3" s="299"/>
-      <c r="AG3" s="299"/>
-      <c r="AH3" s="299"/>
-      <c r="AI3" s="299"/>
-      <c r="AJ3" s="299"/>
+      <c r="C3" s="290"/>
+      <c r="D3" s="290"/>
+      <c r="E3" s="290"/>
+      <c r="F3" s="290"/>
+      <c r="G3" s="290"/>
+      <c r="H3" s="290"/>
+      <c r="I3" s="290"/>
+      <c r="J3" s="290"/>
+      <c r="K3" s="290"/>
+      <c r="L3" s="290"/>
+      <c r="M3" s="290"/>
+      <c r="N3" s="290"/>
+      <c r="O3" s="290"/>
+      <c r="P3" s="291"/>
+      <c r="Q3" s="291"/>
+      <c r="R3" s="291"/>
+      <c r="S3" s="291"/>
+      <c r="T3" s="291"/>
+      <c r="U3" s="291"/>
+      <c r="V3" s="291"/>
+      <c r="W3" s="291"/>
+      <c r="X3" s="291"/>
+      <c r="Y3" s="291"/>
+      <c r="Z3" s="291"/>
+      <c r="AA3" s="291"/>
+      <c r="AB3" s="291"/>
+      <c r="AC3" s="291"/>
+      <c r="AD3" s="291"/>
+      <c r="AE3" s="291"/>
+      <c r="AF3" s="291"/>
+      <c r="AG3" s="291"/>
+      <c r="AH3" s="291"/>
+      <c r="AI3" s="291"/>
+      <c r="AJ3" s="291"/>
     </row>
     <row r="4" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="282" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="283"/>
-      <c r="E4" s="283"/>
-      <c r="F4" s="283"/>
-      <c r="G4" s="283"/>
-      <c r="H4" s="283"/>
-      <c r="I4" s="283"/>
-      <c r="J4" s="283"/>
-      <c r="K4" s="283"/>
-      <c r="L4" s="283"/>
-      <c r="M4" s="283"/>
-      <c r="N4" s="283"/>
-      <c r="O4" s="283"/>
-      <c r="P4" s="283"/>
-      <c r="Q4" s="283"/>
-      <c r="R4" s="283"/>
-      <c r="S4" s="284"/>
-      <c r="T4" s="282" t="s">
+      <c r="C4" s="315" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="316"/>
+      <c r="E4" s="316"/>
+      <c r="F4" s="316"/>
+      <c r="G4" s="316"/>
+      <c r="H4" s="316"/>
+      <c r="I4" s="316"/>
+      <c r="J4" s="316"/>
+      <c r="K4" s="316"/>
+      <c r="L4" s="316"/>
+      <c r="M4" s="316"/>
+      <c r="N4" s="316"/>
+      <c r="O4" s="316"/>
+      <c r="P4" s="316"/>
+      <c r="Q4" s="316"/>
+      <c r="R4" s="316"/>
+      <c r="S4" s="317"/>
+      <c r="T4" s="315" t="s">
         <v>1</v>
       </c>
-      <c r="U4" s="283"/>
-      <c r="V4" s="283"/>
-      <c r="W4" s="283"/>
-      <c r="X4" s="283"/>
-      <c r="Y4" s="283"/>
-      <c r="Z4" s="283"/>
-      <c r="AA4" s="283"/>
-      <c r="AB4" s="284"/>
-      <c r="AC4" s="282" t="s">
+      <c r="U4" s="316"/>
+      <c r="V4" s="316"/>
+      <c r="W4" s="316"/>
+      <c r="X4" s="316"/>
+      <c r="Y4" s="316"/>
+      <c r="Z4" s="316"/>
+      <c r="AA4" s="316"/>
+      <c r="AB4" s="317"/>
+      <c r="AC4" s="315" t="s">
         <v>2</v>
       </c>
-      <c r="AD4" s="283"/>
-      <c r="AE4" s="283"/>
-      <c r="AF4" s="283"/>
-      <c r="AG4" s="293"/>
-      <c r="AH4" s="282" t="s">
+      <c r="AD4" s="316"/>
+      <c r="AE4" s="316"/>
+      <c r="AF4" s="316"/>
+      <c r="AG4" s="324"/>
+      <c r="AH4" s="315" t="s">
         <v>10</v>
       </c>
-      <c r="AI4" s="283"/>
-      <c r="AJ4" s="284"/>
+      <c r="AI4" s="316"/>
+      <c r="AJ4" s="317"/>
     </row>
     <row r="5" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="294" t="s">
+      <c r="C5" s="284" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="290"/>
-      <c r="E5" s="290"/>
-      <c r="F5" s="290"/>
-      <c r="G5" s="290"/>
-      <c r="H5" s="290"/>
-      <c r="I5" s="290"/>
-      <c r="J5" s="291"/>
-      <c r="K5" s="289" t="s">
+      <c r="D5" s="285"/>
+      <c r="E5" s="285"/>
+      <c r="F5" s="285"/>
+      <c r="G5" s="285"/>
+      <c r="H5" s="285"/>
+      <c r="I5" s="285"/>
+      <c r="J5" s="286"/>
+      <c r="K5" s="322" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="290"/>
-      <c r="M5" s="290"/>
-      <c r="N5" s="290"/>
-      <c r="O5" s="290"/>
-      <c r="P5" s="290"/>
-      <c r="Q5" s="290"/>
-      <c r="R5" s="291"/>
-      <c r="S5" s="285" t="s">
+      <c r="L5" s="285"/>
+      <c r="M5" s="285"/>
+      <c r="N5" s="285"/>
+      <c r="O5" s="285"/>
+      <c r="P5" s="285"/>
+      <c r="Q5" s="285"/>
+      <c r="R5" s="286"/>
+      <c r="S5" s="318" t="s">
         <v>12</v>
       </c>
-      <c r="T5" s="294" t="s">
+      <c r="T5" s="284" t="s">
         <v>9</v>
       </c>
-      <c r="U5" s="290"/>
-      <c r="V5" s="290"/>
-      <c r="W5" s="291"/>
-      <c r="X5" s="289" t="s">
+      <c r="U5" s="285"/>
+      <c r="V5" s="285"/>
+      <c r="W5" s="286"/>
+      <c r="X5" s="322" t="s">
         <v>8</v>
       </c>
-      <c r="Y5" s="290"/>
-      <c r="Z5" s="290"/>
-      <c r="AA5" s="291"/>
-      <c r="AB5" s="285" t="s">
+      <c r="Y5" s="285"/>
+      <c r="Z5" s="285"/>
+      <c r="AA5" s="286"/>
+      <c r="AB5" s="318" t="s">
         <v>13</v>
       </c>
-      <c r="AC5" s="292" t="s">
+      <c r="AC5" s="323" t="s">
         <v>9</v>
       </c>
-      <c r="AD5" s="291"/>
-      <c r="AE5" s="289" t="s">
+      <c r="AD5" s="286"/>
+      <c r="AE5" s="322" t="s">
         <v>8</v>
       </c>
-      <c r="AF5" s="291"/>
-      <c r="AG5" s="285" t="s">
+      <c r="AF5" s="286"/>
+      <c r="AG5" s="318" t="s">
         <v>14</v>
       </c>
       <c r="AH5" s="56"/>
       <c r="AI5" s="25"/>
-      <c r="AJ5" s="285" t="s">
+      <c r="AJ5" s="318" t="s">
         <v>15</v>
       </c>
       <c r="AK5" s="4"/>
@@ -4223,7 +4223,7 @@
         <f>Résultats!$J$28</f>
         <v>3</v>
       </c>
-      <c r="S6" s="286"/>
+      <c r="S6" s="319"/>
       <c r="T6" s="169">
         <f>Résultats!$V$6</f>
         <v>0</v>
@@ -4256,7 +4256,7 @@
         <f>Résultats!$V$25</f>
         <v>0</v>
       </c>
-      <c r="AB6" s="286"/>
+      <c r="AB6" s="319"/>
       <c r="AC6" s="111">
         <f>Résultats!$AH$8</f>
         <v>0</v>
@@ -4273,7 +4273,7 @@
         <f>Résultats!$AH$23</f>
         <v>0</v>
       </c>
-      <c r="AG6" s="286"/>
+      <c r="AG6" s="319"/>
       <c r="AH6" s="212">
         <f>Résultats!$AH$15</f>
         <v>0</v>
@@ -4282,7 +4282,7 @@
         <f>Résultats!$AH$16</f>
         <v>0</v>
       </c>
-      <c r="AJ6" s="286"/>
+      <c r="AJ6" s="319"/>
       <c r="AK6" s="37"/>
     </row>
     <row r="7" spans="1:38" s="39" customFormat="1" ht="58.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -4308,7 +4308,7 @@
       <c r="P7" s="246"/>
       <c r="Q7" s="264"/>
       <c r="R7" s="117"/>
-      <c r="S7" s="286"/>
+      <c r="S7" s="319"/>
       <c r="T7" s="170"/>
       <c r="U7" s="117"/>
       <c r="V7" s="173"/>
@@ -4317,15 +4317,15 @@
       <c r="Y7" s="118"/>
       <c r="Z7" s="119"/>
       <c r="AA7" s="117"/>
-      <c r="AB7" s="286"/>
+      <c r="AB7" s="319"/>
       <c r="AC7" s="119"/>
       <c r="AD7" s="117"/>
       <c r="AE7" s="120"/>
       <c r="AF7" s="117"/>
-      <c r="AG7" s="286"/>
+      <c r="AG7" s="319"/>
       <c r="AH7" s="212"/>
       <c r="AI7" s="112"/>
-      <c r="AJ7" s="286"/>
+      <c r="AJ7" s="319"/>
       <c r="AK7" s="37"/>
     </row>
     <row r="8" spans="1:38" s="39" customFormat="1" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4395,7 +4395,7 @@
         <f>Résultats!$B$28</f>
         <v>VEGAS</v>
       </c>
-      <c r="S8" s="286"/>
+      <c r="S8" s="319"/>
       <c r="T8" s="171" t="str">
         <f>Résultats!$N$6</f>
         <v>BOSTON</v>
@@ -4428,7 +4428,7 @@
         <f>Résultats!$N$25</f>
         <v>DALLAS</v>
       </c>
-      <c r="AB8" s="286"/>
+      <c r="AB8" s="319"/>
       <c r="AC8" s="177" t="str">
         <f>Résultats!$Z$8</f>
         <v xml:space="preserve"> </v>
@@ -4445,7 +4445,7 @@
         <f>Résultats!$Z$23</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AG8" s="286"/>
+      <c r="AG8" s="319"/>
       <c r="AH8" s="213" t="str">
         <f>Résultats!$Z$15</f>
         <v xml:space="preserve"> </v>
@@ -4454,7 +4454,7 @@
         <f>Résultats!$Z$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ8" s="286"/>
+      <c r="AJ8" s="319"/>
       <c r="AK8" s="37"/>
     </row>
     <row r="9" spans="1:38" s="39" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4528,7 +4528,7 @@
         <f>Résultats!$A$28</f>
         <v>P3</v>
       </c>
-      <c r="S9" s="288"/>
+      <c r="S9" s="321"/>
       <c r="T9" s="179" t="str">
         <f>Résultats!$M$6</f>
         <v>A2</v>
@@ -4561,7 +4561,7 @@
         <f>Résultats!$M$25</f>
         <v>WC1</v>
       </c>
-      <c r="AB9" s="287"/>
+      <c r="AB9" s="320"/>
       <c r="AC9" s="183" t="str">
         <f>Résultats!$Y$8</f>
         <v xml:space="preserve"> </v>
@@ -4578,7 +4578,7 @@
         <f>Résultats!$Y$23</f>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="AG9" s="287"/>
+      <c r="AG9" s="320"/>
       <c r="AH9" s="215" t="str">
         <f>Résultats!$Y$15</f>
         <v xml:space="preserve"> </v>
@@ -4587,7 +4587,7 @@
         <f>Résultats!$Y$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ9" s="288"/>
+      <c r="AJ9" s="321"/>
       <c r="AK9" s="114" t="s">
         <v>51</v>
       </c>
@@ -13467,12 +13467,12 @@
     <row r="100" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B100" s="43"/>
       <c r="N100" s="26"/>
-      <c r="O100" s="273" t="s">
+      <c r="O100" s="306" t="s">
         <v>17</v>
       </c>
-      <c r="P100" s="274"/>
-      <c r="Q100" s="274"/>
-      <c r="R100" s="275"/>
+      <c r="P100" s="307"/>
+      <c r="Q100" s="307"/>
+      <c r="R100" s="308"/>
       <c r="AG100" s="30"/>
       <c r="AH100" s="30"/>
       <c r="AI100" s="30"/>
@@ -13481,21 +13481,21 @@
     </row>
     <row r="101" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="33"/>
-      <c r="B101" s="302" t="s">
+      <c r="B101" s="294" t="s">
         <v>16</v>
       </c>
-      <c r="C101" s="303"/>
-      <c r="D101" s="303"/>
-      <c r="E101" s="303"/>
-      <c r="F101" s="303"/>
-      <c r="G101" s="303"/>
-      <c r="H101" s="303"/>
-      <c r="I101" s="303"/>
-      <c r="J101" s="303"/>
-      <c r="K101" s="303"/>
-      <c r="L101" s="303"/>
-      <c r="M101" s="303"/>
-      <c r="N101" s="304"/>
+      <c r="C101" s="295"/>
+      <c r="D101" s="295"/>
+      <c r="E101" s="295"/>
+      <c r="F101" s="295"/>
+      <c r="G101" s="295"/>
+      <c r="H101" s="295"/>
+      <c r="I101" s="295"/>
+      <c r="J101" s="295"/>
+      <c r="K101" s="295"/>
+      <c r="L101" s="295"/>
+      <c r="M101" s="295"/>
+      <c r="N101" s="296"/>
       <c r="O101" s="21">
         <v>1</v>
       </c>
@@ -13508,45 +13508,45 @@
       <c r="R101" s="22">
         <v>4</v>
       </c>
-      <c r="U101" s="276" t="s">
+      <c r="U101" s="309" t="s">
         <v>26</v>
       </c>
-      <c r="V101" s="277"/>
-      <c r="W101" s="277"/>
-      <c r="X101" s="277"/>
-      <c r="Y101" s="277"/>
-      <c r="Z101" s="277"/>
-      <c r="AA101" s="277"/>
-      <c r="AB101" s="277"/>
-      <c r="AC101" s="277"/>
-      <c r="AD101" s="278"/>
+      <c r="V101" s="310"/>
+      <c r="W101" s="310"/>
+      <c r="X101" s="310"/>
+      <c r="Y101" s="310"/>
+      <c r="Z101" s="310"/>
+      <c r="AA101" s="310"/>
+      <c r="AB101" s="310"/>
+      <c r="AC101" s="310"/>
+      <c r="AD101" s="311"/>
       <c r="AE101" s="28"/>
       <c r="AF101" s="28"/>
-      <c r="AG101" s="279" t="s">
+      <c r="AG101" s="312" t="s">
         <v>24</v>
       </c>
-      <c r="AH101" s="280"/>
-      <c r="AI101" s="280"/>
-      <c r="AJ101" s="280"/>
-      <c r="AK101" s="281"/>
+      <c r="AH101" s="313"/>
+      <c r="AI101" s="313"/>
+      <c r="AJ101" s="313"/>
+      <c r="AK101" s="314"/>
     </row>
     <row r="102" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A102" s="34"/>
-      <c r="B102" s="309" t="s">
+      <c r="B102" s="273" t="s">
         <v>6</v>
       </c>
-      <c r="C102" s="310"/>
-      <c r="D102" s="310"/>
-      <c r="E102" s="310"/>
-      <c r="F102" s="310"/>
-      <c r="G102" s="310"/>
-      <c r="H102" s="310"/>
-      <c r="I102" s="310"/>
-      <c r="J102" s="310"/>
-      <c r="K102" s="310"/>
-      <c r="L102" s="310"/>
-      <c r="M102" s="310"/>
-      <c r="N102" s="311"/>
+      <c r="C102" s="274"/>
+      <c r="D102" s="274"/>
+      <c r="E102" s="274"/>
+      <c r="F102" s="274"/>
+      <c r="G102" s="274"/>
+      <c r="H102" s="274"/>
+      <c r="I102" s="274"/>
+      <c r="J102" s="274"/>
+      <c r="K102" s="274"/>
+      <c r="L102" s="274"/>
+      <c r="M102" s="274"/>
+      <c r="N102" s="275"/>
       <c r="O102" s="20">
         <v>5</v>
       </c>
@@ -13559,49 +13559,49 @@
       <c r="R102" s="23">
         <v>20</v>
       </c>
-      <c r="U102" s="307" t="s">
+      <c r="U102" s="299" t="s">
         <v>20</v>
       </c>
-      <c r="V102" s="308"/>
-      <c r="W102" s="308"/>
-      <c r="X102" s="308"/>
-      <c r="Y102" s="308"/>
-      <c r="Z102" s="308"/>
-      <c r="AA102" s="308"/>
-      <c r="AB102" s="305">
+      <c r="V102" s="300"/>
+      <c r="W102" s="300"/>
+      <c r="X102" s="300"/>
+      <c r="Y102" s="300"/>
+      <c r="Z102" s="300"/>
+      <c r="AA102" s="300"/>
+      <c r="AB102" s="297">
         <v>22</v>
       </c>
-      <c r="AC102" s="305"/>
-      <c r="AD102" s="306"/>
+      <c r="AC102" s="297"/>
+      <c r="AD102" s="298"/>
       <c r="AE102" s="29"/>
       <c r="AF102" s="29"/>
-      <c r="AG102" s="321" t="s">
+      <c r="AG102" s="280" t="s">
         <v>21</v>
       </c>
-      <c r="AH102" s="322"/>
-      <c r="AI102" s="322"/>
-      <c r="AJ102" s="323"/>
+      <c r="AH102" s="281"/>
+      <c r="AI102" s="281"/>
+      <c r="AJ102" s="282"/>
       <c r="AK102" s="223">
         <v>230</v>
       </c>
     </row>
     <row r="103" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="34"/>
-      <c r="B103" s="309" t="s">
+      <c r="B103" s="273" t="s">
         <v>5</v>
       </c>
-      <c r="C103" s="310"/>
-      <c r="D103" s="310"/>
-      <c r="E103" s="310"/>
-      <c r="F103" s="310"/>
-      <c r="G103" s="310"/>
-      <c r="H103" s="310"/>
-      <c r="I103" s="310"/>
-      <c r="J103" s="310"/>
-      <c r="K103" s="310"/>
-      <c r="L103" s="310"/>
-      <c r="M103" s="310"/>
-      <c r="N103" s="311"/>
+      <c r="C103" s="274"/>
+      <c r="D103" s="274"/>
+      <c r="E103" s="274"/>
+      <c r="F103" s="274"/>
+      <c r="G103" s="274"/>
+      <c r="H103" s="274"/>
+      <c r="I103" s="274"/>
+      <c r="J103" s="274"/>
+      <c r="K103" s="274"/>
+      <c r="L103" s="274"/>
+      <c r="M103" s="274"/>
+      <c r="N103" s="275"/>
       <c r="O103" s="20">
         <v>2</v>
       </c>
@@ -13614,49 +13614,49 @@
       <c r="R103" s="23">
         <v>8</v>
       </c>
-      <c r="U103" s="316" t="s">
+      <c r="U103" s="278" t="s">
         <v>18</v>
       </c>
-      <c r="V103" s="317"/>
-      <c r="W103" s="317"/>
-      <c r="X103" s="317"/>
-      <c r="Y103" s="317"/>
-      <c r="Z103" s="317"/>
-      <c r="AA103" s="317"/>
-      <c r="AB103" s="318">
+      <c r="V103" s="279"/>
+      <c r="W103" s="279"/>
+      <c r="X103" s="279"/>
+      <c r="Y103" s="279"/>
+      <c r="Z103" s="279"/>
+      <c r="AA103" s="279"/>
+      <c r="AB103" s="304">
         <v>20</v>
       </c>
-      <c r="AC103" s="318"/>
-      <c r="AD103" s="319"/>
+      <c r="AC103" s="304"/>
+      <c r="AD103" s="305"/>
       <c r="AE103" s="29"/>
       <c r="AF103" s="29"/>
-      <c r="AG103" s="324" t="s">
+      <c r="AG103" s="283" t="s">
         <v>22</v>
       </c>
-      <c r="AH103" s="310"/>
-      <c r="AI103" s="310"/>
-      <c r="AJ103" s="311"/>
+      <c r="AH103" s="274"/>
+      <c r="AI103" s="274"/>
+      <c r="AJ103" s="275"/>
       <c r="AK103" s="36">
         <v>115</v>
       </c>
     </row>
     <row r="104" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="35"/>
-      <c r="B104" s="295" t="s">
+      <c r="B104" s="287" t="s">
         <v>4</v>
       </c>
-      <c r="C104" s="296"/>
-      <c r="D104" s="296"/>
-      <c r="E104" s="296"/>
-      <c r="F104" s="296"/>
-      <c r="G104" s="296"/>
-      <c r="H104" s="296"/>
-      <c r="I104" s="296"/>
-      <c r="J104" s="296"/>
-      <c r="K104" s="296"/>
-      <c r="L104" s="296"/>
-      <c r="M104" s="296"/>
-      <c r="N104" s="297"/>
+      <c r="C104" s="288"/>
+      <c r="D104" s="288"/>
+      <c r="E104" s="288"/>
+      <c r="F104" s="288"/>
+      <c r="G104" s="288"/>
+      <c r="H104" s="288"/>
+      <c r="I104" s="288"/>
+      <c r="J104" s="288"/>
+      <c r="K104" s="288"/>
+      <c r="L104" s="288"/>
+      <c r="M104" s="288"/>
+      <c r="N104" s="289"/>
       <c r="O104" s="3">
         <v>1</v>
       </c>
@@ -13669,51 +13669,51 @@
       <c r="R104" s="24">
         <v>1</v>
       </c>
-      <c r="U104" s="312" t="s">
+      <c r="U104" s="301" t="s">
         <v>19</v>
       </c>
-      <c r="V104" s="313"/>
-      <c r="W104" s="313"/>
-      <c r="X104" s="313"/>
-      <c r="Y104" s="313"/>
-      <c r="Z104" s="313"/>
-      <c r="AA104" s="313"/>
-      <c r="AB104" s="314">
+      <c r="V104" s="277"/>
+      <c r="W104" s="277"/>
+      <c r="X104" s="277"/>
+      <c r="Y104" s="277"/>
+      <c r="Z104" s="277"/>
+      <c r="AA104" s="277"/>
+      <c r="AB104" s="302">
         <f>AB102*AB103</f>
         <v>440</v>
       </c>
-      <c r="AC104" s="314"/>
-      <c r="AD104" s="315"/>
+      <c r="AC104" s="302"/>
+      <c r="AD104" s="303"/>
       <c r="AE104" s="29"/>
       <c r="AF104" s="29"/>
-      <c r="AG104" s="324" t="s">
+      <c r="AG104" s="283" t="s">
         <v>25</v>
       </c>
-      <c r="AH104" s="310"/>
-      <c r="AI104" s="310"/>
-      <c r="AJ104" s="311"/>
+      <c r="AH104" s="274"/>
+      <c r="AI104" s="274"/>
+      <c r="AJ104" s="275"/>
       <c r="AK104" s="36">
         <v>65</v>
       </c>
     </row>
     <row r="105" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG105" s="316" t="s">
+      <c r="AG105" s="278" t="s">
         <v>23</v>
       </c>
-      <c r="AH105" s="317"/>
-      <c r="AI105" s="317"/>
-      <c r="AJ105" s="317"/>
+      <c r="AH105" s="279"/>
+      <c r="AI105" s="279"/>
+      <c r="AJ105" s="279"/>
       <c r="AK105" s="225">
         <v>30</v>
       </c>
     </row>
     <row r="106" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG106" s="320" t="s">
+      <c r="AG106" s="276" t="s">
         <v>19</v>
       </c>
-      <c r="AH106" s="313"/>
-      <c r="AI106" s="313"/>
-      <c r="AJ106" s="313"/>
+      <c r="AH106" s="277"/>
+      <c r="AI106" s="277"/>
+      <c r="AJ106" s="277"/>
       <c r="AK106" s="224">
         <f>SUM(AK102:AK105)</f>
         <v>440</v>
@@ -13725,12 +13725,22 @@
     <sortCondition ref="B10:B94"/>
   </sortState>
   <mergeCells count="38">
-    <mergeCell ref="B103:N103"/>
-    <mergeCell ref="AG106:AJ106"/>
-    <mergeCell ref="AG105:AJ105"/>
-    <mergeCell ref="AG102:AJ102"/>
-    <mergeCell ref="AG104:AJ104"/>
-    <mergeCell ref="AG103:AJ103"/>
+    <mergeCell ref="O100:R100"/>
+    <mergeCell ref="U101:AD101"/>
+    <mergeCell ref="AG101:AK101"/>
+    <mergeCell ref="AH4:AJ4"/>
+    <mergeCell ref="AG5:AG9"/>
+    <mergeCell ref="AJ5:AJ9"/>
+    <mergeCell ref="X5:AA5"/>
+    <mergeCell ref="AB5:AB9"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="C4:S4"/>
+    <mergeCell ref="T4:AB4"/>
+    <mergeCell ref="AC4:AG4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="K5:R5"/>
+    <mergeCell ref="S5:S9"/>
     <mergeCell ref="T5:W5"/>
     <mergeCell ref="B104:N104"/>
     <mergeCell ref="C1:O1"/>
@@ -13747,22 +13757,12 @@
     <mergeCell ref="AB104:AD104"/>
     <mergeCell ref="U103:AA103"/>
     <mergeCell ref="AB103:AD103"/>
-    <mergeCell ref="O100:R100"/>
-    <mergeCell ref="U101:AD101"/>
-    <mergeCell ref="AG101:AK101"/>
-    <mergeCell ref="AH4:AJ4"/>
-    <mergeCell ref="AG5:AG9"/>
-    <mergeCell ref="AJ5:AJ9"/>
-    <mergeCell ref="X5:AA5"/>
-    <mergeCell ref="AB5:AB9"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="C4:S4"/>
-    <mergeCell ref="T4:AB4"/>
-    <mergeCell ref="AC4:AG4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="K5:R5"/>
-    <mergeCell ref="S5:S9"/>
+    <mergeCell ref="B103:N103"/>
+    <mergeCell ref="AG106:AJ106"/>
+    <mergeCell ref="AG105:AJ105"/>
+    <mergeCell ref="AG102:AJ102"/>
+    <mergeCell ref="AG104:AJ104"/>
+    <mergeCell ref="AG103:AJ103"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <conditionalFormatting sqref="AH18:AI18 AH10:AI10 AH14:AI14 T10:AA10 AC10:AF10 C10:R10 C14:R14 T14:AA14 AC14:AF14 T18:AA18 AC18:AF18 AH30:AI30 C30:R30 T30:AA30 AC30:AF30 AH26:AI26 C26:R26 T26:AA26 AC26:AF26 AH62:AI62 C62:R62 T62:AA62 AC62:AF62 AH42:AI42 C42:R42 T42:AA42 AC42:AF42 AH22:AI22 C22:R22 T22:AA22 AC22:AF22 AH38:AI38 C38:R38 T38:AA38 AC38:AF38 AH34:AI34 C34:R34 T34:AA34 AC34:AF34 AH66:AI66 C66:R66 T66:AA66 AC66:AF66 C18:R18">
@@ -14419,20 +14419,20 @@
   <dimension ref="A1:AJ31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+      <selection activeCell="N1" activeCellId="1" sqref="B1:B1048576 N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="1" customWidth="1"/>
     <col min="3" max="5" width="2.7109375" style="19" customWidth="1"/>
     <col min="6" max="6" width="3" style="19" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="2.7109375" style="19" customWidth="1"/>
     <col min="10" max="10" width="2.7109375" style="2" customWidth="1"/>
     <col min="11" max="12" width="2.7109375" customWidth="1"/>
     <col min="13" max="13" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" style="1" customWidth="1"/>
     <col min="15" max="21" width="2.7109375" style="18" customWidth="1"/>
     <col min="22" max="24" width="2.7109375" customWidth="1"/>
     <col min="25" max="25" width="3.85546875" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Updated games of 2019-04-24
</commit_message>
<xml_diff>
--- a/laval.xlsx
+++ b/laval.xlsx
@@ -1960,7 +1960,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="325">
+  <cellXfs count="329">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2447,9 +2447,6 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -2516,24 +2513,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -2564,6 +2549,114 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="113" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="114" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="95" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2573,18 +2666,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="86" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="87" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="88" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="87" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="95" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2597,127 +2705,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="86" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="88" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="113" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="114" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="95" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3918,7 +3930,7 @@
   <dimension ref="A1:AL106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="AK8" sqref="AK8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3941,166 +3953,166 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="C1" s="290"/>
-      <c r="D1" s="290"/>
-      <c r="E1" s="290"/>
-      <c r="F1" s="290"/>
-      <c r="G1" s="290"/>
-      <c r="H1" s="290"/>
-      <c r="I1" s="290"/>
-      <c r="J1" s="290"/>
-      <c r="K1" s="290"/>
-      <c r="L1" s="290"/>
-      <c r="M1" s="290"/>
-      <c r="N1" s="290"/>
-      <c r="O1" s="290"/>
-      <c r="P1" s="291"/>
-      <c r="Q1" s="291"/>
-      <c r="R1" s="291"/>
-      <c r="S1" s="291"/>
-      <c r="T1" s="291"/>
-      <c r="U1" s="291"/>
-      <c r="V1" s="291"/>
-      <c r="W1" s="291"/>
-      <c r="X1" s="291"/>
-      <c r="Y1" s="291"/>
-      <c r="Z1" s="291"/>
-      <c r="AA1" s="291"/>
-      <c r="AB1" s="291"/>
-      <c r="AC1" s="291"/>
-      <c r="AD1" s="291"/>
-      <c r="AE1" s="291"/>
-      <c r="AF1" s="291"/>
-      <c r="AG1" s="291"/>
-      <c r="AH1" s="291"/>
-      <c r="AI1" s="291"/>
-      <c r="AJ1" s="291"/>
+      <c r="C1" s="293"/>
+      <c r="D1" s="293"/>
+      <c r="E1" s="293"/>
+      <c r="F1" s="293"/>
+      <c r="G1" s="293"/>
+      <c r="H1" s="293"/>
+      <c r="I1" s="293"/>
+      <c r="J1" s="293"/>
+      <c r="K1" s="293"/>
+      <c r="L1" s="293"/>
+      <c r="M1" s="293"/>
+      <c r="N1" s="293"/>
+      <c r="O1" s="293"/>
+      <c r="P1" s="294"/>
+      <c r="Q1" s="294"/>
+      <c r="R1" s="294"/>
+      <c r="S1" s="294"/>
+      <c r="T1" s="294"/>
+      <c r="U1" s="294"/>
+      <c r="V1" s="294"/>
+      <c r="W1" s="294"/>
+      <c r="X1" s="294"/>
+      <c r="Y1" s="294"/>
+      <c r="Z1" s="294"/>
+      <c r="AA1" s="294"/>
+      <c r="AB1" s="294"/>
+      <c r="AC1" s="294"/>
+      <c r="AD1" s="294"/>
+      <c r="AE1" s="294"/>
+      <c r="AF1" s="294"/>
+      <c r="AG1" s="294"/>
+      <c r="AH1" s="294"/>
+      <c r="AI1" s="294"/>
+      <c r="AJ1" s="294"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="41"/>
-      <c r="C2" s="292" t="s">
+      <c r="C2" s="295" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="292"/>
-      <c r="E2" s="292"/>
-      <c r="F2" s="292"/>
-      <c r="G2" s="292"/>
-      <c r="H2" s="292"/>
-      <c r="I2" s="292"/>
-      <c r="J2" s="292"/>
-      <c r="K2" s="292"/>
-      <c r="L2" s="292"/>
-      <c r="M2" s="292"/>
-      <c r="N2" s="292"/>
-      <c r="O2" s="292"/>
-      <c r="P2" s="292"/>
-      <c r="Q2" s="293" t="s">
+      <c r="D2" s="295"/>
+      <c r="E2" s="295"/>
+      <c r="F2" s="295"/>
+      <c r="G2" s="295"/>
+      <c r="H2" s="295"/>
+      <c r="I2" s="295"/>
+      <c r="J2" s="295"/>
+      <c r="K2" s="295"/>
+      <c r="L2" s="295"/>
+      <c r="M2" s="295"/>
+      <c r="N2" s="295"/>
+      <c r="O2" s="295"/>
+      <c r="P2" s="295"/>
+      <c r="Q2" s="296" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="291"/>
-      <c r="S2" s="291"/>
-      <c r="T2" s="291"/>
-      <c r="U2" s="291"/>
-      <c r="V2" s="291"/>
-      <c r="W2" s="291"/>
-      <c r="X2" s="291"/>
-      <c r="Y2" s="291"/>
-      <c r="Z2" s="291"/>
-      <c r="AA2" s="291"/>
-      <c r="AB2" s="291"/>
-      <c r="AC2" s="291"/>
-      <c r="AD2" s="291"/>
-      <c r="AE2" s="291"/>
-      <c r="AF2" s="291"/>
-      <c r="AG2" s="291"/>
-      <c r="AH2" s="291"/>
-      <c r="AI2" s="291"/>
-      <c r="AJ2" s="291"/>
+      <c r="R2" s="294"/>
+      <c r="S2" s="294"/>
+      <c r="T2" s="294"/>
+      <c r="U2" s="294"/>
+      <c r="V2" s="294"/>
+      <c r="W2" s="294"/>
+      <c r="X2" s="294"/>
+      <c r="Y2" s="294"/>
+      <c r="Z2" s="294"/>
+      <c r="AA2" s="294"/>
+      <c r="AB2" s="294"/>
+      <c r="AC2" s="294"/>
+      <c r="AD2" s="294"/>
+      <c r="AE2" s="294"/>
+      <c r="AF2" s="294"/>
+      <c r="AG2" s="294"/>
+      <c r="AH2" s="294"/>
+      <c r="AI2" s="294"/>
+      <c r="AJ2" s="294"/>
     </row>
     <row r="3" spans="1:38" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="290"/>
-      <c r="D3" s="290"/>
-      <c r="E3" s="290"/>
-      <c r="F3" s="290"/>
-      <c r="G3" s="290"/>
-      <c r="H3" s="290"/>
-      <c r="I3" s="290"/>
-      <c r="J3" s="290"/>
-      <c r="K3" s="290"/>
-      <c r="L3" s="290"/>
-      <c r="M3" s="290"/>
-      <c r="N3" s="290"/>
-      <c r="O3" s="290"/>
-      <c r="P3" s="291"/>
-      <c r="Q3" s="291"/>
-      <c r="R3" s="291"/>
-      <c r="S3" s="291"/>
-      <c r="T3" s="291"/>
-      <c r="U3" s="291"/>
-      <c r="V3" s="291"/>
-      <c r="W3" s="291"/>
-      <c r="X3" s="291"/>
-      <c r="Y3" s="291"/>
-      <c r="Z3" s="291"/>
-      <c r="AA3" s="291"/>
-      <c r="AB3" s="291"/>
-      <c r="AC3" s="291"/>
-      <c r="AD3" s="291"/>
-      <c r="AE3" s="291"/>
-      <c r="AF3" s="291"/>
-      <c r="AG3" s="291"/>
-      <c r="AH3" s="291"/>
-      <c r="AI3" s="291"/>
-      <c r="AJ3" s="291"/>
+      <c r="C3" s="293"/>
+      <c r="D3" s="293"/>
+      <c r="E3" s="293"/>
+      <c r="F3" s="293"/>
+      <c r="G3" s="293"/>
+      <c r="H3" s="293"/>
+      <c r="I3" s="293"/>
+      <c r="J3" s="293"/>
+      <c r="K3" s="293"/>
+      <c r="L3" s="293"/>
+      <c r="M3" s="293"/>
+      <c r="N3" s="293"/>
+      <c r="O3" s="293"/>
+      <c r="P3" s="294"/>
+      <c r="Q3" s="294"/>
+      <c r="R3" s="294"/>
+      <c r="S3" s="294"/>
+      <c r="T3" s="294"/>
+      <c r="U3" s="294"/>
+      <c r="V3" s="294"/>
+      <c r="W3" s="294"/>
+      <c r="X3" s="294"/>
+      <c r="Y3" s="294"/>
+      <c r="Z3" s="294"/>
+      <c r="AA3" s="294"/>
+      <c r="AB3" s="294"/>
+      <c r="AC3" s="294"/>
+      <c r="AD3" s="294"/>
+      <c r="AE3" s="294"/>
+      <c r="AF3" s="294"/>
+      <c r="AG3" s="294"/>
+      <c r="AH3" s="294"/>
+      <c r="AI3" s="294"/>
+      <c r="AJ3" s="294"/>
     </row>
     <row r="4" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="315" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="316"/>
-      <c r="E4" s="316"/>
-      <c r="F4" s="316"/>
-      <c r="G4" s="316"/>
-      <c r="H4" s="316"/>
-      <c r="I4" s="316"/>
-      <c r="J4" s="316"/>
-      <c r="K4" s="316"/>
-      <c r="L4" s="316"/>
-      <c r="M4" s="316"/>
-      <c r="N4" s="316"/>
-      <c r="O4" s="316"/>
-      <c r="P4" s="316"/>
-      <c r="Q4" s="316"/>
-      <c r="R4" s="316"/>
-      <c r="S4" s="317"/>
-      <c r="T4" s="315" t="s">
+      <c r="C4" s="277" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="278"/>
+      <c r="E4" s="278"/>
+      <c r="F4" s="278"/>
+      <c r="G4" s="278"/>
+      <c r="H4" s="278"/>
+      <c r="I4" s="278"/>
+      <c r="J4" s="278"/>
+      <c r="K4" s="278"/>
+      <c r="L4" s="278"/>
+      <c r="M4" s="278"/>
+      <c r="N4" s="278"/>
+      <c r="O4" s="278"/>
+      <c r="P4" s="278"/>
+      <c r="Q4" s="278"/>
+      <c r="R4" s="278"/>
+      <c r="S4" s="279"/>
+      <c r="T4" s="277" t="s">
         <v>1</v>
       </c>
-      <c r="U4" s="316"/>
-      <c r="V4" s="316"/>
-      <c r="W4" s="316"/>
-      <c r="X4" s="316"/>
-      <c r="Y4" s="316"/>
-      <c r="Z4" s="316"/>
-      <c r="AA4" s="316"/>
-      <c r="AB4" s="317"/>
-      <c r="AC4" s="315" t="s">
+      <c r="U4" s="278"/>
+      <c r="V4" s="278"/>
+      <c r="W4" s="278"/>
+      <c r="X4" s="278"/>
+      <c r="Y4" s="278"/>
+      <c r="Z4" s="278"/>
+      <c r="AA4" s="278"/>
+      <c r="AB4" s="279"/>
+      <c r="AC4" s="277" t="s">
         <v>2</v>
       </c>
-      <c r="AD4" s="316"/>
-      <c r="AE4" s="316"/>
-      <c r="AF4" s="316"/>
-      <c r="AG4" s="324"/>
-      <c r="AH4" s="315" t="s">
+      <c r="AD4" s="278"/>
+      <c r="AE4" s="278"/>
+      <c r="AF4" s="278"/>
+      <c r="AG4" s="288"/>
+      <c r="AH4" s="277" t="s">
         <v>10</v>
       </c>
-      <c r="AI4" s="316"/>
-      <c r="AJ4" s="317"/>
+      <c r="AI4" s="278"/>
+      <c r="AJ4" s="279"/>
     </row>
     <row r="5" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="284" t="s">
+      <c r="C5" s="289" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="285"/>
@@ -4110,7 +4122,7 @@
       <c r="H5" s="285"/>
       <c r="I5" s="285"/>
       <c r="J5" s="286"/>
-      <c r="K5" s="322" t="s">
+      <c r="K5" s="284" t="s">
         <v>8</v>
       </c>
       <c r="L5" s="285"/>
@@ -4120,38 +4132,38 @@
       <c r="P5" s="285"/>
       <c r="Q5" s="285"/>
       <c r="R5" s="286"/>
-      <c r="S5" s="318" t="s">
+      <c r="S5" s="280" t="s">
         <v>12</v>
       </c>
-      <c r="T5" s="284" t="s">
+      <c r="T5" s="289" t="s">
         <v>9</v>
       </c>
       <c r="U5" s="285"/>
       <c r="V5" s="285"/>
       <c r="W5" s="286"/>
-      <c r="X5" s="322" t="s">
+      <c r="X5" s="284" t="s">
         <v>8</v>
       </c>
       <c r="Y5" s="285"/>
       <c r="Z5" s="285"/>
       <c r="AA5" s="286"/>
-      <c r="AB5" s="318" t="s">
+      <c r="AB5" s="280" t="s">
         <v>13</v>
       </c>
-      <c r="AC5" s="323" t="s">
+      <c r="AC5" s="287" t="s">
         <v>9</v>
       </c>
       <c r="AD5" s="286"/>
-      <c r="AE5" s="322" t="s">
+      <c r="AE5" s="284" t="s">
         <v>8</v>
       </c>
       <c r="AF5" s="286"/>
-      <c r="AG5" s="318" t="s">
+      <c r="AG5" s="280" t="s">
         <v>14</v>
       </c>
       <c r="AH5" s="56"/>
       <c r="AI5" s="25"/>
-      <c r="AJ5" s="318" t="s">
+      <c r="AJ5" s="280" t="s">
         <v>15</v>
       </c>
       <c r="AK5" s="4"/>
@@ -4163,11 +4175,11 @@
         <f>Résultats!$J$3</f>
         <v>0</v>
       </c>
-      <c r="D6" s="239">
+      <c r="D6" s="238">
         <f>Résultats!$J$4</f>
         <v>4</v>
       </c>
-      <c r="E6" s="235">
+      <c r="E6" s="234">
         <f>Résultats!$J$6</f>
         <v>4</v>
       </c>
@@ -4179,11 +4191,11 @@
         <f>Résultats!$J$10</f>
         <v>3</v>
       </c>
-      <c r="H6" s="109">
+      <c r="H6" s="244">
         <f>Résultats!$J$11</f>
-        <v>3</v>
-      </c>
-      <c r="I6" s="235">
+        <v>4</v>
+      </c>
+      <c r="I6" s="234">
         <f>Résultats!$J$13</f>
         <v>4</v>
       </c>
@@ -4195,7 +4207,7 @@
         <f>Résultats!$J$17</f>
         <v>1</v>
       </c>
-      <c r="L6" s="239">
+      <c r="L6" s="238">
         <f>Résultats!$J$18</f>
         <v>4</v>
       </c>
@@ -4203,7 +4215,7 @@
         <f>Résultats!$J$20</f>
         <v>2</v>
       </c>
-      <c r="N6" s="245">
+      <c r="N6" s="244">
         <f>Résultats!$J$21</f>
         <v>4</v>
       </c>
@@ -4211,11 +4223,11 @@
         <f>Résultats!$J$24</f>
         <v>2</v>
       </c>
-      <c r="P6" s="245">
+      <c r="P6" s="244">
         <f>Résultats!$J$25</f>
         <v>4</v>
       </c>
-      <c r="Q6" s="263">
+      <c r="Q6" s="258">
         <f>Résultats!$J$27</f>
         <v>4</v>
       </c>
@@ -4223,7 +4235,7 @@
         <f>Résultats!$J$28</f>
         <v>3</v>
       </c>
-      <c r="S6" s="319"/>
+      <c r="S6" s="281"/>
       <c r="T6" s="169">
         <f>Résultats!$V$6</f>
         <v>0</v>
@@ -4256,7 +4268,7 @@
         <f>Résultats!$V$25</f>
         <v>0</v>
       </c>
-      <c r="AB6" s="319"/>
+      <c r="AB6" s="281"/>
       <c r="AC6" s="111">
         <f>Résultats!$AH$8</f>
         <v>0</v>
@@ -4273,7 +4285,7 @@
         <f>Résultats!$AH$23</f>
         <v>0</v>
       </c>
-      <c r="AG6" s="319"/>
+      <c r="AG6" s="281"/>
       <c r="AH6" s="212">
         <f>Résultats!$AH$15</f>
         <v>0</v>
@@ -4282,7 +4294,7 @@
         <f>Résultats!$AH$16</f>
         <v>0</v>
       </c>
-      <c r="AJ6" s="319"/>
+      <c r="AJ6" s="281"/>
       <c r="AK6" s="37"/>
     </row>
     <row r="7" spans="1:38" s="39" customFormat="1" ht="58.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -4293,22 +4305,22 @@
 +IF(ISBLANK($D10),0,($D$6*PT_VICTOIRE_R1)+IF($D$6=4,PT_PREDICTION_EQUIPE_R1+IF($D10=$C$6+$D$6,PT_PREDICTION_NB_PARTIES_R1,0),0))</f>
         <v>0</v>
       </c>
-      <c r="D7" s="240"/>
-      <c r="E7" s="236"/>
+      <c r="D7" s="239"/>
+      <c r="E7" s="235"/>
       <c r="F7" s="118"/>
       <c r="G7" s="119"/>
-      <c r="H7" s="117"/>
-      <c r="I7" s="236"/>
+      <c r="H7" s="239"/>
+      <c r="I7" s="235"/>
       <c r="J7" s="117"/>
       <c r="K7" s="120"/>
-      <c r="L7" s="240"/>
+      <c r="L7" s="239"/>
       <c r="M7" s="173"/>
-      <c r="N7" s="246"/>
+      <c r="N7" s="245"/>
       <c r="O7" s="173"/>
-      <c r="P7" s="246"/>
-      <c r="Q7" s="264"/>
+      <c r="P7" s="245"/>
+      <c r="Q7" s="259"/>
       <c r="R7" s="117"/>
-      <c r="S7" s="319"/>
+      <c r="S7" s="281"/>
       <c r="T7" s="170"/>
       <c r="U7" s="117"/>
       <c r="V7" s="173"/>
@@ -4317,15 +4329,15 @@
       <c r="Y7" s="118"/>
       <c r="Z7" s="119"/>
       <c r="AA7" s="117"/>
-      <c r="AB7" s="319"/>
+      <c r="AB7" s="281"/>
       <c r="AC7" s="119"/>
       <c r="AD7" s="117"/>
       <c r="AE7" s="120"/>
       <c r="AF7" s="117"/>
-      <c r="AG7" s="319"/>
+      <c r="AG7" s="281"/>
       <c r="AH7" s="212"/>
       <c r="AI7" s="112"/>
-      <c r="AJ7" s="319"/>
+      <c r="AJ7" s="281"/>
       <c r="AK7" s="37"/>
     </row>
     <row r="8" spans="1:38" s="39" customFormat="1" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4335,11 +4347,11 @@
         <f>Résultats!$B$3</f>
         <v>TAMPA BAY</v>
       </c>
-      <c r="D8" s="241" t="str">
+      <c r="D8" s="240" t="str">
         <f>Résultats!$B$4</f>
         <v>COLUMBUS</v>
       </c>
-      <c r="E8" s="237" t="str">
+      <c r="E8" s="236" t="str">
         <f>Résultats!$B$6</f>
         <v>BOSTON</v>
       </c>
@@ -4351,11 +4363,11 @@
         <f>Résultats!$B$10</f>
         <v>WASHINGTON</v>
       </c>
-      <c r="H8" s="174" t="str">
+      <c r="H8" s="240" t="str">
         <f>Résultats!$B$11</f>
         <v>CAROLINE</v>
       </c>
-      <c r="I8" s="237" t="str">
+      <c r="I8" s="236" t="str">
         <f>Résultats!$B$13</f>
         <v>NEW YORK I.</v>
       </c>
@@ -4367,7 +4379,7 @@
         <f>Résultats!$B$17</f>
         <v>CALGARY</v>
       </c>
-      <c r="L8" s="241" t="str">
+      <c r="L8" s="240" t="str">
         <f>Résultats!$B$18</f>
         <v>COLORADO</v>
       </c>
@@ -4375,7 +4387,7 @@
         <f>Résultats!$B$20</f>
         <v>WINNIPEG</v>
       </c>
-      <c r="N8" s="247" t="str">
+      <c r="N8" s="246" t="str">
         <f>Résultats!$B$21</f>
         <v>ST-LOUIS</v>
       </c>
@@ -4383,11 +4395,11 @@
         <f>Résultats!$B$24</f>
         <v>NASHVILLE</v>
       </c>
-      <c r="P8" s="247" t="str">
+      <c r="P8" s="246" t="str">
         <f>Résultats!$B$25</f>
         <v>DALLAS</v>
       </c>
-      <c r="Q8" s="265" t="str">
+      <c r="Q8" s="260" t="str">
         <f>Résultats!$B$27</f>
         <v>SAN JOSE</v>
       </c>
@@ -4395,7 +4407,7 @@
         <f>Résultats!$B$28</f>
         <v>VEGAS</v>
       </c>
-      <c r="S8" s="319"/>
+      <c r="S8" s="281"/>
       <c r="T8" s="171" t="str">
         <f>Résultats!$N$6</f>
         <v>BOSTON</v>
@@ -4406,11 +4418,11 @@
       </c>
       <c r="V8" s="175" t="str">
         <f>Résultats!$N$10</f>
-        <v xml:space="preserve"> </v>
+        <v>NEW YORK I.</v>
       </c>
       <c r="W8" s="174" t="str">
         <f>Résultats!$N$11</f>
-        <v xml:space="preserve"> </v>
+        <v>CAROLINE</v>
       </c>
       <c r="X8" s="178" t="str">
         <f>Résultats!$N$20</f>
@@ -4428,7 +4440,7 @@
         <f>Résultats!$N$25</f>
         <v>DALLAS</v>
       </c>
-      <c r="AB8" s="319"/>
+      <c r="AB8" s="281"/>
       <c r="AC8" s="177" t="str">
         <f>Résultats!$Z$8</f>
         <v xml:space="preserve"> </v>
@@ -4445,7 +4457,7 @@
         <f>Résultats!$Z$23</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AG8" s="319"/>
+      <c r="AG8" s="281"/>
       <c r="AH8" s="213" t="str">
         <f>Résultats!$Z$15</f>
         <v xml:space="preserve"> </v>
@@ -4454,7 +4466,7 @@
         <f>Résultats!$Z$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ8" s="319"/>
+      <c r="AJ8" s="281"/>
       <c r="AK8" s="37"/>
     </row>
     <row r="9" spans="1:38" s="39" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4468,11 +4480,11 @@
         <f>Résultats!$A$3</f>
         <v>A1</v>
       </c>
-      <c r="D9" s="242" t="str">
+      <c r="D9" s="241" t="str">
         <f>Résultats!$A$4</f>
         <v>WC2</v>
       </c>
-      <c r="E9" s="238" t="str">
+      <c r="E9" s="237" t="str">
         <f>Résultats!$A$6</f>
         <v>A2</v>
       </c>
@@ -4484,11 +4496,11 @@
         <f>Résultats!$A$10</f>
         <v>M1</v>
       </c>
-      <c r="H9" s="180" t="str">
+      <c r="H9" s="241" t="str">
         <f>Résultats!$A$11</f>
         <v>WC1</v>
       </c>
-      <c r="I9" s="238" t="str">
+      <c r="I9" s="237" t="str">
         <f>Résultats!$A$13</f>
         <v>M2</v>
       </c>
@@ -4500,7 +4512,7 @@
         <f>Résultats!$A$17</f>
         <v>C1</v>
       </c>
-      <c r="L9" s="242" t="str">
+      <c r="L9" s="241" t="str">
         <f>Résultats!$A$18</f>
         <v>WC2</v>
       </c>
@@ -4508,7 +4520,7 @@
         <f>Résultats!$A$20</f>
         <v>C2</v>
       </c>
-      <c r="N9" s="248" t="str">
+      <c r="N9" s="247" t="str">
         <f>Résultats!$A$21</f>
         <v>C3</v>
       </c>
@@ -4516,11 +4528,11 @@
         <f>Résultats!$A$24</f>
         <v>P1</v>
       </c>
-      <c r="P9" s="248" t="str">
+      <c r="P9" s="247" t="str">
         <f>Résultats!$A$25</f>
         <v>WC1</v>
       </c>
-      <c r="Q9" s="266" t="str">
+      <c r="Q9" s="261" t="str">
         <f>Résultats!$A$27</f>
         <v>P2</v>
       </c>
@@ -4528,7 +4540,7 @@
         <f>Résultats!$A$28</f>
         <v>P3</v>
       </c>
-      <c r="S9" s="321"/>
+      <c r="S9" s="283"/>
       <c r="T9" s="179" t="str">
         <f>Résultats!$M$6</f>
         <v>A2</v>
@@ -4539,11 +4551,11 @@
       </c>
       <c r="V9" s="181" t="str">
         <f>Résultats!$M$10</f>
-        <v xml:space="preserve"> </v>
+        <v>M2</v>
       </c>
       <c r="W9" s="180" t="str">
         <f>Résultats!$M$11</f>
-        <v xml:space="preserve"> </v>
+        <v>WC1</v>
       </c>
       <c r="X9" s="184" t="str">
         <f>Résultats!$M$20</f>
@@ -4561,7 +4573,7 @@
         <f>Résultats!$M$25</f>
         <v>WC1</v>
       </c>
-      <c r="AB9" s="320"/>
+      <c r="AB9" s="282"/>
       <c r="AC9" s="183" t="str">
         <f>Résultats!$Y$8</f>
         <v xml:space="preserve"> </v>
@@ -4578,7 +4590,7 @@
         <f>Résultats!$Y$23</f>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="AG9" s="320"/>
+      <c r="AG9" s="282"/>
       <c r="AH9" s="215" t="str">
         <f>Résultats!$Y$15</f>
         <v xml:space="preserve"> </v>
@@ -4587,7 +4599,7 @@
         <f>Résultats!$Y$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ9" s="321"/>
+      <c r="AJ9" s="283"/>
       <c r="AK9" s="114" t="s">
         <v>51</v>
       </c>
@@ -4631,7 +4643,7 @@
         <v>6</v>
       </c>
       <c r="P10" s="188"/>
-      <c r="Q10" s="271">
+      <c r="Q10" s="266">
         <v>7</v>
       </c>
       <c r="R10" s="193"/>
@@ -4997,43 +5009,43 @@
         <v>2</v>
       </c>
       <c r="B14" s="88" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="C14" s="46">
         <v>5</v>
       </c>
       <c r="D14" s="45"/>
-      <c r="E14" s="267">
+      <c r="E14" s="44">
+        <v>6</v>
+      </c>
+      <c r="F14" s="45"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="327">
         <v>7</v>
       </c>
-      <c r="F14" s="45"/>
-      <c r="G14" s="48">
-        <v>5</v>
-      </c>
-      <c r="H14" s="47"/>
-      <c r="I14" s="44">
+      <c r="I14" s="44"/>
+      <c r="J14" s="47">
         <v>6</v>
       </c>
-      <c r="J14" s="47"/>
       <c r="K14" s="49">
         <v>5</v>
       </c>
       <c r="L14" s="47"/>
-      <c r="M14" s="44">
+      <c r="M14" s="44"/>
+      <c r="N14" s="264">
         <v>6</v>
       </c>
-      <c r="N14" s="45"/>
       <c r="O14" s="44">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P14" s="45"/>
-      <c r="Q14" s="272">
-        <v>7</v>
+      <c r="Q14" s="48">
+        <v>6</v>
       </c>
       <c r="R14" s="50"/>
       <c r="S14" s="129">
         <f>SUM(C15:R15)</f>
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="T14" s="46"/>
       <c r="U14" s="47"/>
@@ -5041,7 +5053,7 @@
       <c r="W14" s="47"/>
       <c r="X14" s="49"/>
       <c r="Y14" s="45"/>
-      <c r="Z14" s="243"/>
+      <c r="Z14" s="48"/>
       <c r="AA14" s="50"/>
       <c r="AB14" s="129">
         <f>SUM(T15:AA15)</f>
@@ -5063,11 +5075,11 @@
       </c>
       <c r="AK14" s="116">
         <f>MAX($AL$10:$AL$97) - AL14</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AL14" s="129">
         <f>$S14+$AB14+$AG14+$AJ14</f>
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5083,17 +5095,17 @@
       <c r="D15" s="150"/>
       <c r="E15" s="132">
         <f>(IF($E14&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E14=$E$6+$F$6,$O$103,0),0),0)+IF($F14&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F14=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F15" s="150"/>
       <c r="G15" s="132">
         <f>(IF($G14&lt;&gt;"",($G$6*$O$104)+IF($G$6=4,($O$102)+IF($G14=$G$6+$H$6,$O$103,0),0),0)+IF($H14&lt;&gt;"",($H$6*$O$104)+IF($H$6=4,($O$102)+IF($H14=$G$6+$H$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="H15" s="150"/>
       <c r="I15" s="126">
         <f>(IF($I14&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I14=$I$6+$J$6,$O$103,0),0),0)+IF($J14&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J14=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J15" s="151"/>
       <c r="K15" s="152">
@@ -5103,7 +5115,7 @@
       <c r="L15" s="150"/>
       <c r="M15" s="132">
         <f>(IF($M14&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M14=$M$6+$N$6,$O$103,0),0),0)+IF($N14&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N14=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="N15" s="150"/>
       <c r="O15" s="126">
@@ -5113,7 +5125,7 @@
       <c r="P15" s="150"/>
       <c r="Q15" s="126">
         <f>(IF($Q14&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q14=$Q$6+$R$6,$O$103,0),0),0)+IF($R14&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R14=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="R15" s="153"/>
       <c r="S15" s="154"/>
@@ -5179,13 +5191,13 @@
         <f>IF(ISBLANK(H14),
 0,
 IF(H$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" s="124">
         <f>IF(ISBLANK(I14),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" s="124">
         <f>IF(ISBLANK(J14),
@@ -5215,7 +5227,7 @@
         <f>IF(ISBLANK(N14),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O16" s="124">
         <f>IF(ISBLANK(O14),
@@ -5261,7 +5273,7 @@
       <c r="AJ16" s="147"/>
       <c r="AK16" s="148">
         <f>SUM(C16:AI16)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AL16" s="130"/>
     </row>
@@ -5286,7 +5298,7 @@
         <f>IF(E16 = 0,
 0,
 IF(E14 = (E$6+F$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" s="124">
         <f>IF(F16 = 0,
@@ -5304,7 +5316,7 @@
         <f>IF(H16 = 0,
 0,
 IF(H14 = (G$6+H$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="124">
         <f>IF(I16 = 0,
@@ -5340,7 +5352,7 @@
         <f>IF(N16 = 0,
 0,
 IF(N14 = (M$6+N$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O17" s="124">
         <f>IF(O16 = 0,
@@ -5358,7 +5370,7 @@
         <f>IF(Q16 = 0,
 0,
 IF(Q14 = (Q$6+R$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R17" s="124">
         <f>IF(R16 = 0,
@@ -5396,18 +5408,18 @@
         <v>3</v>
       </c>
       <c r="B18" s="211" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C18" s="198">
         <v>5</v>
       </c>
       <c r="D18" s="199"/>
-      <c r="E18" s="268">
+      <c r="E18" s="263">
         <v>7</v>
       </c>
       <c r="F18" s="199"/>
       <c r="G18" s="201">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H18" s="202"/>
       <c r="I18" s="200">
@@ -5415,39 +5427,39 @@
       </c>
       <c r="J18" s="202"/>
       <c r="K18" s="203">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L18" s="202"/>
       <c r="M18" s="200">
+        <v>6</v>
+      </c>
+      <c r="N18" s="199"/>
+      <c r="O18" s="200">
         <v>5</v>
       </c>
-      <c r="N18" s="199"/>
-      <c r="O18" s="200"/>
-      <c r="P18" s="199">
+      <c r="P18" s="199"/>
+      <c r="Q18" s="325">
         <v>7</v>
       </c>
-      <c r="Q18" s="201"/>
-      <c r="R18" s="204">
-        <v>7</v>
-      </c>
-      <c r="S18" s="244">
+      <c r="R18" s="204"/>
+      <c r="S18" s="243">
         <f>SUM(C19:R19)</f>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="T18" s="198"/>
       <c r="U18" s="202"/>
       <c r="V18" s="200"/>
       <c r="W18" s="202"/>
       <c r="X18" s="203"/>
-      <c r="Y18" s="234"/>
-      <c r="Z18" s="201"/>
+      <c r="Y18" s="199"/>
+      <c r="Z18" s="208"/>
       <c r="AA18" s="204"/>
       <c r="AB18" s="205">
         <f>SUM(T19:AA19)</f>
         <v>0</v>
       </c>
       <c r="AC18" s="201"/>
-      <c r="AD18" s="259"/>
+      <c r="AD18" s="202"/>
       <c r="AE18" s="203"/>
       <c r="AF18" s="202"/>
       <c r="AG18" s="205">
@@ -5462,11 +5474,11 @@
       </c>
       <c r="AK18" s="207">
         <f>MAX($AL$10:$AL$97) - AL18</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AL18" s="205">
         <f>$S18+$AB18+$AG18+$AJ18</f>
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5507,12 +5519,12 @@
       <c r="N19" s="150"/>
       <c r="O19" s="126">
         <f>(IF($O18&lt;&gt;"",($O$6*$O$104)+IF($O$6=4,($O$102)+IF($O18=$O$6+$P$6,$O$103,0),0),0)+IF($P18&lt;&gt;"",($P$6*$O$104)+IF($P$6=4,($O$102)+IF($P18=$O$6+$P$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="P19" s="150"/>
       <c r="Q19" s="126">
         <f>(IF($Q18&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q18=$Q$6+$R$6,$O$103,0),0),0)+IF($R18&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R18=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="R19" s="153"/>
       <c r="S19" s="154"/>
@@ -5626,13 +5638,13 @@
         <f>IF(ISBLANK(P18),
 0,
 IF(P$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q20" s="124">
         <f>IF(ISBLANK(Q18),
 0,
 IF(Q$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R20" s="124">
         <f>IF(ISBLANK(R18),
@@ -5757,7 +5769,7 @@
         <f>IF(Q20 = 0,
 0,
 IF(Q18 = (Q$6+R$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R21" s="124">
         <f>IF(R20 = 0,
@@ -5785,7 +5797,7 @@
       <c r="AJ21" s="147"/>
       <c r="AK21" s="148">
         <f>SUM(C21:AI21)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL21" s="130"/>
     </row>
@@ -5795,50 +5807,50 @@
         <v>4</v>
       </c>
       <c r="B22" s="88" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C22" s="46">
         <v>5</v>
       </c>
       <c r="D22" s="45"/>
-      <c r="E22" s="267">
+      <c r="E22" s="262">
         <v>7</v>
       </c>
       <c r="F22" s="45"/>
       <c r="G22" s="48">
+        <v>6</v>
+      </c>
+      <c r="H22" s="47"/>
+      <c r="I22" s="44">
+        <v>6</v>
+      </c>
+      <c r="J22" s="47"/>
+      <c r="K22" s="49">
         <v>4</v>
       </c>
-      <c r="H22" s="47"/>
-      <c r="I22" s="44"/>
-      <c r="J22" s="47">
-        <v>6</v>
-      </c>
-      <c r="K22" s="49">
+      <c r="L22" s="47"/>
+      <c r="M22" s="44">
         <v>5</v>
       </c>
-      <c r="L22" s="47"/>
-      <c r="M22" s="44"/>
-      <c r="N22" s="269">
-        <v>6</v>
-      </c>
-      <c r="O22" s="44">
+      <c r="N22" s="45"/>
+      <c r="O22" s="44"/>
+      <c r="P22" s="45">
         <v>7</v>
       </c>
-      <c r="P22" s="45"/>
-      <c r="Q22" s="48">
-        <v>6</v>
-      </c>
-      <c r="R22" s="50"/>
+      <c r="Q22" s="48"/>
+      <c r="R22" s="50">
+        <v>7</v>
+      </c>
       <c r="S22" s="129">
         <f>SUM(C23:R23)</f>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="T22" s="46"/>
       <c r="U22" s="47"/>
       <c r="V22" s="44"/>
       <c r="W22" s="47"/>
       <c r="X22" s="49"/>
-      <c r="Y22" s="45"/>
+      <c r="Y22" s="127"/>
       <c r="Z22" s="48"/>
       <c r="AA22" s="50"/>
       <c r="AB22" s="129">
@@ -5846,14 +5858,14 @@
         <v>0</v>
       </c>
       <c r="AC22" s="48"/>
-      <c r="AD22" s="47"/>
+      <c r="AD22" s="321"/>
       <c r="AE22" s="49"/>
       <c r="AF22" s="47"/>
       <c r="AG22" s="129">
         <f>SUM(AC23:AF23)</f>
         <v>0</v>
       </c>
-      <c r="AH22" s="257"/>
+      <c r="AH22" s="320"/>
       <c r="AI22" s="57"/>
       <c r="AJ22" s="129">
         <f>AH23</f>
@@ -5861,11 +5873,11 @@
       </c>
       <c r="AK22" s="116">
         <f>MAX($AL$10:$AL$97) - AL22</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AL22" s="129">
         <f>$S22+$AB22+$AG22+$AJ22</f>
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5891,7 +5903,7 @@
       <c r="H23" s="163"/>
       <c r="I23" s="132">
         <f>(IF($I22&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I22=$I$6+$J$6,$O$103,0),0),0)+IF($J22&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J22=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J23" s="164"/>
       <c r="K23" s="165">
@@ -5901,17 +5913,17 @@
       <c r="L23" s="163"/>
       <c r="M23" s="132">
         <f>(IF($M22&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M22=$M$6+$N$6,$O$103,0),0),0)+IF($N22&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N22=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="N23" s="163"/>
       <c r="O23" s="132">
         <f>(IF($O22&lt;&gt;"",($O$6*$O$104)+IF($O$6=4,($O$102)+IF($O22=$O$6+$P$6,$O$103,0),0),0)+IF($P22&lt;&gt;"",($P$6*$O$104)+IF($P$6=4,($O$102)+IF($P22=$O$6+$P$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="P23" s="163"/>
       <c r="Q23" s="132">
         <f>(IF($Q22&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q22=$Q$6+$R$6,$O$103,0),0),0)+IF($R22&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R22=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="R23" s="166"/>
       <c r="S23" s="154"/>
@@ -5983,7 +5995,7 @@
         <f>IF(ISBLANK(I22),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" s="124">
         <f>IF(ISBLANK(J22),
@@ -6013,7 +6025,7 @@
         <f>IF(ISBLANK(N22),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O24" s="124">
         <f>IF(ISBLANK(O22),
@@ -6025,13 +6037,13 @@
         <f>IF(ISBLANK(P22),
 0,
 IF(P$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q24" s="124">
         <f>IF(ISBLANK(Q22),
 0,
 IF(Q$6= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R24" s="124">
         <f>IF(ISBLANK(R22),
@@ -6138,7 +6150,7 @@
         <f>IF(N24 = 0,
 0,
 IF(N22 = (M$6+N$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O25" s="124">
         <f>IF(O24 = 0,
@@ -6184,7 +6196,7 @@
       <c r="AJ25" s="147"/>
       <c r="AK25" s="148">
         <f>SUM(C25:AI25)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AL25" s="130"/>
     </row>
@@ -6194,20 +6206,20 @@
         <v>5</v>
       </c>
       <c r="B26" s="211" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C26" s="198">
         <v>5</v>
       </c>
       <c r="D26" s="199"/>
-      <c r="E26" s="200">
-        <v>6</v>
+      <c r="E26" s="263">
+        <v>7</v>
       </c>
       <c r="F26" s="199"/>
-      <c r="G26" s="201"/>
-      <c r="H26" s="202">
-        <v>7</v>
-      </c>
+      <c r="G26" s="201">
+        <v>4</v>
+      </c>
+      <c r="H26" s="202"/>
       <c r="I26" s="200"/>
       <c r="J26" s="202">
         <v>6</v>
@@ -6217,11 +6229,11 @@
       </c>
       <c r="L26" s="202"/>
       <c r="M26" s="200"/>
-      <c r="N26" s="270">
+      <c r="N26" s="265">
         <v>6</v>
       </c>
       <c r="O26" s="200">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P26" s="199"/>
       <c r="Q26" s="201">
@@ -6230,7 +6242,7 @@
       <c r="R26" s="204"/>
       <c r="S26" s="205">
         <f>SUM(C27:R27)</f>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="T26" s="198"/>
       <c r="U26" s="202"/>
@@ -6252,7 +6264,7 @@
         <f>SUM(AC27:AF27)</f>
         <v>0</v>
       </c>
-      <c r="AH26" s="195"/>
+      <c r="AH26" s="326"/>
       <c r="AI26" s="196"/>
       <c r="AJ26" s="205">
         <f>AH27</f>
@@ -6260,11 +6272,11 @@
       </c>
       <c r="AK26" s="207">
         <f>MAX($AL$10:$AL$97) - AL26</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AL26" s="205">
         <f>$S26+$AB26+$AG26+$AJ26</f>
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6280,7 +6292,7 @@
       <c r="D27" s="150"/>
       <c r="E27" s="126">
         <f>(IF($E26&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E26=$E$6+$F$6,$O$103,0),0),0)+IF($F26&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F26=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F27" s="150"/>
       <c r="G27" s="126">
@@ -6483,7 +6495,7 @@
         <f>IF(E28 = 0,
 0,
 IF(E26 = (E$6+F$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29" s="124">
         <f>IF(F28 = 0,
@@ -6583,14 +6595,14 @@
       <c r="AJ29" s="147"/>
       <c r="AK29" s="148">
         <f>SUM(C29:AI29)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL29" s="130"/>
     </row>
     <row r="30" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="122">
         <f>RANK(AL30,$AL$10:$AL$97,)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B30" s="88" t="s">
         <v>81</v>
@@ -6623,7 +6635,7 @@
         <v>6</v>
       </c>
       <c r="P30" s="45"/>
-      <c r="Q30" s="272">
+      <c r="Q30" s="267">
         <v>7</v>
       </c>
       <c r="R30" s="50"/>
@@ -6637,7 +6649,7 @@
       <c r="W30" s="47"/>
       <c r="X30" s="49"/>
       <c r="Y30" s="45"/>
-      <c r="Z30" s="243"/>
+      <c r="Z30" s="242"/>
       <c r="AA30" s="47"/>
       <c r="AB30" s="129">
         <f>SUM(T31:AA31)</f>
@@ -6989,34 +7001,34 @@
     <row r="34" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="186">
         <f>RANK(AL34,$AL$10:$AL$97,)</f>
+        <v>6</v>
+      </c>
+      <c r="B34" s="211" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="198">
+        <v>5</v>
+      </c>
+      <c r="D34" s="199"/>
+      <c r="E34" s="200">
+        <v>6</v>
+      </c>
+      <c r="F34" s="199"/>
+      <c r="G34" s="201"/>
+      <c r="H34" s="328">
         <v>7</v>
       </c>
-      <c r="B34" s="211" t="s">
-        <v>79</v>
-      </c>
-      <c r="C34" s="198">
-        <v>6</v>
-      </c>
-      <c r="D34" s="199"/>
-      <c r="E34" s="200"/>
-      <c r="F34" s="199">
-        <v>7</v>
-      </c>
-      <c r="G34" s="201">
-        <v>6</v>
-      </c>
-      <c r="H34" s="202"/>
       <c r="I34" s="200"/>
       <c r="J34" s="202">
         <v>6</v>
       </c>
-      <c r="K34" s="203"/>
-      <c r="L34" s="202">
-        <v>6</v>
-      </c>
+      <c r="K34" s="203">
+        <v>5</v>
+      </c>
+      <c r="L34" s="202"/>
       <c r="M34" s="200"/>
-      <c r="N34" s="270">
-        <v>6</v>
+      <c r="N34" s="199">
+        <v>7</v>
       </c>
       <c r="O34" s="200">
         <v>5</v>
@@ -7028,7 +7040,7 @@
       </c>
       <c r="S34" s="205">
         <f>SUM(C35:R35)</f>
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="T34" s="198"/>
       <c r="U34" s="202"/>
@@ -7058,11 +7070,11 @@
       </c>
       <c r="AK34" s="207">
         <f>MAX($AL$10:$AL$97) - AL34</f>
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="AL34" s="205">
         <f>$S34+$AB34+$AG34+$AJ34</f>
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7078,12 +7090,12 @@
       <c r="D35" s="80"/>
       <c r="E35" s="81">
         <f>(IF($E34&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E34=$E$6+$F$6,$O$103,0),0),0)+IF($F34&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F34=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F35" s="80"/>
       <c r="G35" s="81">
         <f>(IF($G34&lt;&gt;"",($G$6*$O$104)+IF($G$6=4,($O$102)+IF($G34=$G$6+$H$6,$O$103,0),0),0)+IF($H34&lt;&gt;"",($H$6*$O$104)+IF($H$6=4,($O$102)+IF($H34=$G$6+$H$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="H35" s="80"/>
       <c r="I35" s="81">
@@ -7093,12 +7105,12 @@
       <c r="J35" s="82"/>
       <c r="K35" s="83">
         <f>(IF($K34&lt;&gt;"",($K$6*$O$104)+IF($K$6=4,($O$102)+IF($K34=$K$6+$L$6,$O$103,0),0),0)+IF($L34&lt;&gt;"",($L$6*$O$104)+IF($L$6=4,($O$102)+IF($L34=$K$6+$L$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="L35" s="80"/>
       <c r="M35" s="81">
         <f>(IF($M34&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M34=$M$6+$N$6,$O$103,0),0),0)+IF($N34&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N34=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="N35" s="80"/>
       <c r="O35" s="81">
@@ -7156,7 +7168,7 @@
         <f>IF(ISBLANK(E34),
 0,
 IF(E$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F36" s="124">
         <f>IF(ISBLANK(F34),
@@ -7174,7 +7186,7 @@
         <f>IF(ISBLANK(H34),
 0,
 IF(H$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I36" s="124">
         <f>IF(ISBLANK(I34),
@@ -7198,7 +7210,7 @@
         <f>IF(ISBLANK(L34),
 0,
 IF(L$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M36" s="124">
         <f>IF(ISBLANK(M34),
@@ -7256,7 +7268,7 @@
       <c r="AJ36" s="147"/>
       <c r="AK36" s="148">
         <f>SUM(C36:AI36)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL36" s="130"/>
     </row>
@@ -7299,7 +7311,7 @@
         <f>IF(H36 = 0,
 0,
 IF(H34 = (G$6+H$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37" s="124">
         <f>IF(I36 = 0,
@@ -7335,7 +7347,7 @@
         <f>IF(N36 = 0,
 0,
 IF(N34 = (M$6+N$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O37" s="124">
         <f>IF(O36 = 0,
@@ -7391,47 +7403,47 @@
         <v>8</v>
       </c>
       <c r="B38" s="88" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C38" s="46">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D38" s="45"/>
-      <c r="E38" s="44">
-        <v>4</v>
+      <c r="E38" s="322">
+        <v>6</v>
       </c>
       <c r="F38" s="45"/>
-      <c r="G38" s="48">
+      <c r="G38" s="323"/>
+      <c r="H38" s="47">
         <v>6</v>
       </c>
-      <c r="H38" s="47"/>
-      <c r="I38" s="44">
-        <v>6</v>
-      </c>
-      <c r="J38" s="47"/>
+      <c r="I38" s="322"/>
+      <c r="J38" s="47">
+        <v>7</v>
+      </c>
       <c r="K38" s="49">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L38" s="47"/>
       <c r="M38" s="44">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N38" s="45"/>
       <c r="O38" s="44">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P38" s="45"/>
-      <c r="Q38" s="48"/>
-      <c r="R38" s="50">
+      <c r="Q38" s="48">
         <v>6</v>
       </c>
+      <c r="R38" s="50"/>
       <c r="S38" s="129">
         <f>SUM(C39:R39)</f>
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="T38" s="46"/>
       <c r="U38" s="47"/>
-      <c r="V38" s="44"/>
+      <c r="V38" s="324"/>
       <c r="W38" s="47"/>
       <c r="X38" s="49"/>
       <c r="Y38" s="127"/>
@@ -7457,11 +7469,11 @@
       </c>
       <c r="AK38" s="116">
         <f>MAX($AL$10:$AL$97) - AL38</f>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="AL38" s="129">
         <f>$S38+$AB38+$AG38+$AJ38</f>
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7482,12 +7494,12 @@
       <c r="F39" s="80"/>
       <c r="G39" s="125">
         <f>(IF($G38&lt;&gt;"",($G$6*$O$104)+IF($G$6=4,($O$102)+IF($G38=$G$6+$H$6,$O$103,0),0),0)+IF($H38&lt;&gt;"",($H$6*$O$104)+IF($H$6=4,($O$102)+IF($H38=$G$6+$H$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H39" s="80"/>
       <c r="I39" s="121">
         <f>(IF($I38&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I38=$I$6+$J$6,$O$103,0),0),0)+IF($J38&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J38=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J39" s="82"/>
       <c r="K39" s="83">
@@ -7507,7 +7519,7 @@
       <c r="P39" s="80"/>
       <c r="Q39" s="81">
         <f>(IF($Q38&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q38=$Q$6+$R$6,$O$103,0),0),0)+IF($R38&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R38=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="R39" s="84"/>
       <c r="S39" s="128"/>
@@ -7573,13 +7585,13 @@
         <f>IF(ISBLANK(H38),
 0,
 IF(H$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40" s="124">
         <f>IF(ISBLANK(I38),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J40" s="124">
         <f>IF(ISBLANK(J38),
@@ -7627,7 +7639,7 @@
         <f>IF(ISBLANK(Q38),
 0,
 IF(Q$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R40" s="124">
         <f>IF(ISBLANK(R38),
@@ -7655,7 +7667,7 @@
       <c r="AJ40" s="147"/>
       <c r="AK40" s="148">
         <f>SUM(C40:AI40)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL40" s="130"/>
     </row>
@@ -7787,33 +7799,33 @@
     <row r="42" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="186">
         <f>RANK(AL42,$AL$10:$AL$97,)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B42" s="211" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C42" s="198">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D42" s="199"/>
-      <c r="E42" s="200">
-        <v>5</v>
-      </c>
-      <c r="F42" s="199"/>
+      <c r="E42" s="200"/>
+      <c r="F42" s="199">
+        <v>7</v>
+      </c>
       <c r="G42" s="201">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H42" s="202"/>
       <c r="I42" s="200"/>
       <c r="J42" s="202">
         <v>6</v>
       </c>
-      <c r="K42" s="203">
-        <v>5</v>
-      </c>
-      <c r="L42" s="202"/>
+      <c r="K42" s="203"/>
+      <c r="L42" s="202">
+        <v>6</v>
+      </c>
       <c r="M42" s="200"/>
-      <c r="N42" s="270">
+      <c r="N42" s="265">
         <v>6</v>
       </c>
       <c r="O42" s="200">
@@ -7826,7 +7838,7 @@
       </c>
       <c r="S42" s="205">
         <f>SUM(C43:R43)</f>
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="T42" s="198"/>
       <c r="U42" s="202"/>
@@ -7834,7 +7846,7 @@
       <c r="W42" s="202"/>
       <c r="X42" s="203"/>
       <c r="Y42" s="199"/>
-      <c r="Z42" s="201"/>
+      <c r="Z42" s="208"/>
       <c r="AA42" s="202"/>
       <c r="AB42" s="205">
         <f>SUM(T43:AA43)</f>
@@ -7848,7 +7860,7 @@
         <f>SUM(AC43:AF43)</f>
         <v>0</v>
       </c>
-      <c r="AH42" s="249"/>
+      <c r="AH42" s="209"/>
       <c r="AI42" s="196"/>
       <c r="AJ42" s="205">
         <f>AH43</f>
@@ -7856,11 +7868,11 @@
       </c>
       <c r="AK42" s="207">
         <f>MAX($AL$10:$AL$97) - AL42</f>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AL42" s="205">
         <f>$S42+$AB42+$AG42+$AJ42</f>
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="43" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7876,7 +7888,7 @@
       <c r="D43" s="80"/>
       <c r="E43" s="121">
         <f>(IF($E42&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E42=$E$6+$F$6,$O$103,0),0),0)+IF($F42&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F42=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F43" s="80"/>
       <c r="G43" s="81">
@@ -7891,7 +7903,7 @@
       <c r="J43" s="82"/>
       <c r="K43" s="83">
         <f>(IF($K42&lt;&gt;"",($K$6*$O$104)+IF($K$6=4,($O$102)+IF($K42=$K$6+$L$6,$O$103,0),0),0)+IF($L42&lt;&gt;"",($L$6*$O$104)+IF($L$6=4,($O$102)+IF($L42=$K$6+$L$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="L43" s="80"/>
       <c r="M43" s="81">
@@ -7954,7 +7966,7 @@
         <f>IF(ISBLANK(E42),
 0,
 IF(E$6= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44" s="124">
         <f>IF(ISBLANK(F42),
@@ -7996,7 +8008,7 @@
         <f>IF(ISBLANK(L42),
 0,
 IF(L$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M44" s="124">
         <f>IF(ISBLANK(M42),
@@ -8186,37 +8198,37 @@
     <row r="46" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="122">
         <f>RANK(AL46,$AL$10:$AL$97,)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B46" s="88" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C46" s="46">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D46" s="45"/>
       <c r="E46" s="44">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F46" s="45"/>
       <c r="G46" s="48">
         <v>6</v>
       </c>
       <c r="H46" s="47"/>
-      <c r="I46" s="44"/>
-      <c r="J46" s="47">
+      <c r="I46" s="44">
+        <v>6</v>
+      </c>
+      <c r="J46" s="47"/>
+      <c r="K46" s="49">
         <v>7</v>
       </c>
-      <c r="K46" s="49">
+      <c r="L46" s="47"/>
+      <c r="M46" s="44">
         <v>5</v>
       </c>
-      <c r="L46" s="47"/>
-      <c r="M46" s="44"/>
-      <c r="N46" s="269">
-        <v>6</v>
-      </c>
+      <c r="N46" s="45"/>
       <c r="O46" s="44">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="P46" s="45"/>
       <c r="Q46" s="48"/>
@@ -8232,7 +8244,7 @@
       <c r="V46" s="44"/>
       <c r="W46" s="47"/>
       <c r="X46" s="49"/>
-      <c r="Y46" s="45"/>
+      <c r="Y46" s="127"/>
       <c r="Z46" s="48"/>
       <c r="AA46" s="47"/>
       <c r="AB46" s="129">
@@ -8285,7 +8297,7 @@
       <c r="H47" s="80"/>
       <c r="I47" s="81">
         <f>(IF($I46&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I46=$I$6+$J$6,$O$103,0),0),0)+IF($J46&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J46=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J47" s="82"/>
       <c r="K47" s="83">
@@ -8295,7 +8307,7 @@
       <c r="L47" s="80"/>
       <c r="M47" s="81">
         <f>(IF($M46&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M46=$M$6+$N$6,$O$103,0),0),0)+IF($N46&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N46=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="N47" s="80"/>
       <c r="O47" s="81">
@@ -8377,7 +8389,7 @@
         <f>IF(ISBLANK(I46),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J48" s="124">
         <f>IF(ISBLANK(J46),
@@ -8407,7 +8419,7 @@
         <f>IF(ISBLANK(N46),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O48" s="124">
         <f>IF(ISBLANK(O46),
@@ -8532,7 +8544,7 @@
         <f>IF(N48 = 0,
 0,
 IF(N46 = (M$6+N$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O49" s="124">
         <f>IF(O48 = 0,
@@ -8578,24 +8590,24 @@
       <c r="AJ49" s="147"/>
       <c r="AK49" s="148">
         <f>SUM(C49:AI49)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL49" s="130"/>
     </row>
     <row r="50" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="186">
         <f>RANK(AL50,$AL$10:$AL$97,)</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B50" s="211" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C50" s="198">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D50" s="199"/>
-      <c r="E50" s="268">
-        <v>7</v>
+      <c r="E50" s="200">
+        <v>5</v>
       </c>
       <c r="F50" s="199"/>
       <c r="G50" s="201">
@@ -8604,27 +8616,27 @@
       <c r="H50" s="202"/>
       <c r="I50" s="200"/>
       <c r="J50" s="202">
+        <v>6</v>
+      </c>
+      <c r="K50" s="203">
         <v>5</v>
       </c>
-      <c r="K50" s="203">
-        <v>7</v>
-      </c>
       <c r="L50" s="202"/>
-      <c r="M50" s="200">
+      <c r="M50" s="200"/>
+      <c r="N50" s="265">
         <v>6</v>
       </c>
-      <c r="N50" s="199"/>
       <c r="O50" s="200">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P50" s="199"/>
-      <c r="Q50" s="201">
-        <v>5</v>
-      </c>
-      <c r="R50" s="204"/>
+      <c r="Q50" s="201"/>
+      <c r="R50" s="204">
+        <v>6</v>
+      </c>
       <c r="S50" s="205">
         <f>SUM(C51:R51)</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T50" s="198"/>
       <c r="U50" s="202"/>
@@ -8646,7 +8658,7 @@
         <f>SUM(AC51:AF51)</f>
         <v>0</v>
       </c>
-      <c r="AH50" s="209"/>
+      <c r="AH50" s="248"/>
       <c r="AI50" s="196"/>
       <c r="AJ50" s="205">
         <f>AH51</f>
@@ -8654,11 +8666,11 @@
       </c>
       <c r="AK50" s="207">
         <f>MAX($AL$10:$AL$97) - AL50</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AL50" s="205">
         <f>$S50+$AB50+$AG50+$AJ50</f>
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="51" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -8674,7 +8686,7 @@
       <c r="D51" s="134"/>
       <c r="E51" s="132">
         <f>(IF($E50&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E50=$E$6+$F$6,$O$103,0),0),0)+IF($F50&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F50=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F51" s="134"/>
       <c r="G51" s="132">
@@ -8694,7 +8706,7 @@
       <c r="L51" s="134"/>
       <c r="M51" s="132">
         <f>(IF($M50&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M50=$M$6+$N$6,$O$103,0),0),0)+IF($N50&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N50=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="N51" s="134"/>
       <c r="O51" s="135">
@@ -8704,7 +8716,7 @@
       <c r="P51" s="134"/>
       <c r="Q51" s="135">
         <f>(IF($Q50&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q50=$Q$6+$R$6,$O$103,0),0),0)+IF($R50&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R50=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="R51" s="138"/>
       <c r="S51" s="128"/>
@@ -8803,7 +8815,7 @@
         <f>IF(ISBLANK(N50),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O52" s="124">
         <f>IF(ISBLANK(O50),
@@ -8821,7 +8833,7 @@
         <f>IF(ISBLANK(Q50),
 0,
 IF(Q$6= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R52" s="124">
         <f>IF(ISBLANK(R50),
@@ -8874,7 +8886,7 @@
         <f>IF(E52 = 0,
 0,
 IF(E50 = (E$6+F$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F53" s="124">
         <f>IF(F52 = 0,
@@ -8928,7 +8940,7 @@
         <f>IF(N52 = 0,
 0,
 IF(N50 = (M$6+N$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O53" s="124">
         <f>IF(O52 = 0,
@@ -8981,10 +8993,10 @@
     <row r="54" spans="1:38" s="27" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="122">
         <f>RANK(AL54,$AL$10:$AL$97,)</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B54" s="88" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C54" s="46">
         <v>5</v>
@@ -8994,24 +9006,24 @@
         <v>6</v>
       </c>
       <c r="F54" s="45"/>
-      <c r="G54" s="48"/>
-      <c r="H54" s="47">
-        <v>7</v>
-      </c>
+      <c r="G54" s="48">
+        <v>6</v>
+      </c>
+      <c r="H54" s="47"/>
       <c r="I54" s="44"/>
       <c r="J54" s="47">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K54" s="49">
         <v>5</v>
       </c>
       <c r="L54" s="47"/>
       <c r="M54" s="44"/>
-      <c r="N54" s="45">
+      <c r="N54" s="264">
+        <v>6</v>
+      </c>
+      <c r="O54" s="44">
         <v>7</v>
-      </c>
-      <c r="O54" s="44">
-        <v>5</v>
       </c>
       <c r="P54" s="45"/>
       <c r="Q54" s="48"/>
@@ -9020,7 +9032,7 @@
       </c>
       <c r="S54" s="129">
         <f>SUM(C55:R55)</f>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="T54" s="46"/>
       <c r="U54" s="47"/>
@@ -9028,7 +9040,7 @@
       <c r="W54" s="47"/>
       <c r="X54" s="49"/>
       <c r="Y54" s="45"/>
-      <c r="Z54" s="243"/>
+      <c r="Z54" s="48"/>
       <c r="AA54" s="47"/>
       <c r="AB54" s="129">
         <f>SUM(T55:AA55)</f>
@@ -9050,11 +9062,11 @@
       </c>
       <c r="AK54" s="116">
         <f>MAX($AL$10:$AL$97) - AL54</f>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="AL54" s="129">
         <f>$S54+$AB54+$AG54+$AJ54</f>
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="55" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -9090,7 +9102,7 @@
       <c r="L55" s="134"/>
       <c r="M55" s="132">
         <f>(IF($M54&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M54=$M$6+$N$6,$O$103,0),0),0)+IF($N54&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N54=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="N55" s="134"/>
       <c r="O55" s="135">
@@ -9324,7 +9336,7 @@
         <f>IF(N56 = 0,
 0,
 IF(N54 = (M$6+N$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O57" s="124">
         <f>IF(O56 = 0,
@@ -9370,7 +9382,7 @@
       <c r="AJ57" s="147"/>
       <c r="AK57" s="148">
         <f>SUM(C57:AI57)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL57" s="130"/>
     </row>
@@ -9380,50 +9392,50 @@
         <v>13</v>
       </c>
       <c r="B58" s="211" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="C58" s="198">
+        <v>6</v>
+      </c>
+      <c r="D58" s="199"/>
+      <c r="E58" s="263">
         <v>7</v>
       </c>
-      <c r="D58" s="199"/>
-      <c r="E58" s="260">
-        <v>6</v>
-      </c>
       <c r="F58" s="199"/>
-      <c r="G58" s="261"/>
-      <c r="H58" s="202">
-        <v>6</v>
-      </c>
-      <c r="I58" s="260"/>
+      <c r="G58" s="201">
+        <v>5</v>
+      </c>
+      <c r="H58" s="202"/>
+      <c r="I58" s="200"/>
       <c r="J58" s="202">
+        <v>5</v>
+      </c>
+      <c r="K58" s="203">
         <v>7</v>
-      </c>
-      <c r="K58" s="203">
-        <v>5</v>
       </c>
       <c r="L58" s="202"/>
       <c r="M58" s="200">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N58" s="199"/>
       <c r="O58" s="200">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P58" s="199"/>
       <c r="Q58" s="201">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R58" s="204"/>
       <c r="S58" s="205">
         <f>SUM(C59:R59)</f>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="T58" s="198"/>
       <c r="U58" s="202"/>
-      <c r="V58" s="262"/>
+      <c r="V58" s="200"/>
       <c r="W58" s="202"/>
       <c r="X58" s="203"/>
-      <c r="Y58" s="234"/>
+      <c r="Y58" s="199"/>
       <c r="Z58" s="201"/>
       <c r="AA58" s="202"/>
       <c r="AB58" s="205">
@@ -9446,11 +9458,11 @@
       </c>
       <c r="AK58" s="207">
         <f>MAX($AL$10:$AL$97) - AL58</f>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="AL58" s="205">
         <f>$S58+$AB58+$AG58+$AJ58</f>
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="59" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -9466,7 +9478,7 @@
       <c r="D59" s="134"/>
       <c r="E59" s="132">
         <f>(IF($E58&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E58=$E$6+$F$6,$O$103,0),0),0)+IF($F58&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F58=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F59" s="134"/>
       <c r="G59" s="132">
@@ -9666,7 +9678,7 @@
         <f>IF(E60 = 0,
 0,
 IF(E58 = (E$6+F$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F61" s="124">
         <f>IF(F60 = 0,
@@ -9766,7 +9778,7 @@
       <c r="AJ61" s="147"/>
       <c r="AK61" s="148">
         <f>SUM(C61:AI61)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL61" s="130"/>
     </row>
@@ -9782,7 +9794,7 @@
         <v>6</v>
       </c>
       <c r="D62" s="45"/>
-      <c r="E62" s="267">
+      <c r="E62" s="262">
         <v>7</v>
       </c>
       <c r="F62" s="45"/>
@@ -10223,7 +10235,7 @@
         <v>0</v>
       </c>
       <c r="AC66" s="201"/>
-      <c r="AD66" s="259"/>
+      <c r="AD66" s="257"/>
       <c r="AE66" s="203"/>
       <c r="AF66" s="202"/>
       <c r="AG66" s="205">
@@ -10570,36 +10582,36 @@
       <c r="B70" s="88" t="s">
         <v>68</v>
       </c>
-      <c r="C70" s="250">
+      <c r="C70" s="249">
         <v>5</v>
       </c>
-      <c r="D70" s="251"/>
-      <c r="E70" s="252">
+      <c r="D70" s="250"/>
+      <c r="E70" s="251">
         <v>6</v>
       </c>
-      <c r="F70" s="251"/>
-      <c r="G70" s="253">
+      <c r="F70" s="250"/>
+      <c r="G70" s="252">
         <v>5</v>
       </c>
-      <c r="H70" s="254"/>
-      <c r="I70" s="252"/>
-      <c r="J70" s="254">
+      <c r="H70" s="253"/>
+      <c r="I70" s="251"/>
+      <c r="J70" s="253">
         <v>6</v>
       </c>
-      <c r="K70" s="255">
+      <c r="K70" s="254">
         <v>6</v>
       </c>
-      <c r="L70" s="254"/>
-      <c r="M70" s="252">
+      <c r="L70" s="253"/>
+      <c r="M70" s="251">
         <v>7</v>
       </c>
-      <c r="N70" s="251"/>
-      <c r="O70" s="252">
+      <c r="N70" s="250"/>
+      <c r="O70" s="251">
         <v>6</v>
       </c>
-      <c r="P70" s="251"/>
-      <c r="Q70" s="253"/>
-      <c r="R70" s="256">
+      <c r="P70" s="250"/>
+      <c r="Q70" s="252"/>
+      <c r="R70" s="255">
         <v>6</v>
       </c>
       <c r="S70" s="129">
@@ -12982,7 +12994,7 @@
         <f>SUM(C95:R95)</f>
         <v>14</v>
       </c>
-      <c r="T94" s="258"/>
+      <c r="T94" s="256"/>
       <c r="U94" s="47"/>
       <c r="V94" s="44"/>
       <c r="W94" s="47"/>
@@ -13467,12 +13479,12 @@
     <row r="100" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B100" s="43"/>
       <c r="N100" s="26"/>
-      <c r="O100" s="306" t="s">
+      <c r="O100" s="268" t="s">
         <v>17</v>
       </c>
-      <c r="P100" s="307"/>
-      <c r="Q100" s="307"/>
-      <c r="R100" s="308"/>
+      <c r="P100" s="269"/>
+      <c r="Q100" s="269"/>
+      <c r="R100" s="270"/>
       <c r="AG100" s="30"/>
       <c r="AH100" s="30"/>
       <c r="AI100" s="30"/>
@@ -13481,21 +13493,21 @@
     </row>
     <row r="101" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="33"/>
-      <c r="B101" s="294" t="s">
+      <c r="B101" s="297" t="s">
         <v>16</v>
       </c>
-      <c r="C101" s="295"/>
-      <c r="D101" s="295"/>
-      <c r="E101" s="295"/>
-      <c r="F101" s="295"/>
-      <c r="G101" s="295"/>
-      <c r="H101" s="295"/>
-      <c r="I101" s="295"/>
-      <c r="J101" s="295"/>
-      <c r="K101" s="295"/>
-      <c r="L101" s="295"/>
-      <c r="M101" s="295"/>
-      <c r="N101" s="296"/>
+      <c r="C101" s="298"/>
+      <c r="D101" s="298"/>
+      <c r="E101" s="298"/>
+      <c r="F101" s="298"/>
+      <c r="G101" s="298"/>
+      <c r="H101" s="298"/>
+      <c r="I101" s="298"/>
+      <c r="J101" s="298"/>
+      <c r="K101" s="298"/>
+      <c r="L101" s="298"/>
+      <c r="M101" s="298"/>
+      <c r="N101" s="299"/>
       <c r="O101" s="21">
         <v>1</v>
       </c>
@@ -13508,45 +13520,45 @@
       <c r="R101" s="22">
         <v>4</v>
       </c>
-      <c r="U101" s="309" t="s">
+      <c r="U101" s="271" t="s">
         <v>26</v>
       </c>
-      <c r="V101" s="310"/>
-      <c r="W101" s="310"/>
-      <c r="X101" s="310"/>
-      <c r="Y101" s="310"/>
-      <c r="Z101" s="310"/>
-      <c r="AA101" s="310"/>
-      <c r="AB101" s="310"/>
-      <c r="AC101" s="310"/>
-      <c r="AD101" s="311"/>
+      <c r="V101" s="272"/>
+      <c r="W101" s="272"/>
+      <c r="X101" s="272"/>
+      <c r="Y101" s="272"/>
+      <c r="Z101" s="272"/>
+      <c r="AA101" s="272"/>
+      <c r="AB101" s="272"/>
+      <c r="AC101" s="272"/>
+      <c r="AD101" s="273"/>
       <c r="AE101" s="28"/>
       <c r="AF101" s="28"/>
-      <c r="AG101" s="312" t="s">
+      <c r="AG101" s="274" t="s">
         <v>24</v>
       </c>
-      <c r="AH101" s="313"/>
-      <c r="AI101" s="313"/>
-      <c r="AJ101" s="313"/>
-      <c r="AK101" s="314"/>
+      <c r="AH101" s="275"/>
+      <c r="AI101" s="275"/>
+      <c r="AJ101" s="275"/>
+      <c r="AK101" s="276"/>
     </row>
     <row r="102" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A102" s="34"/>
-      <c r="B102" s="273" t="s">
+      <c r="B102" s="304" t="s">
         <v>6</v>
       </c>
-      <c r="C102" s="274"/>
-      <c r="D102" s="274"/>
-      <c r="E102" s="274"/>
-      <c r="F102" s="274"/>
-      <c r="G102" s="274"/>
-      <c r="H102" s="274"/>
-      <c r="I102" s="274"/>
-      <c r="J102" s="274"/>
-      <c r="K102" s="274"/>
-      <c r="L102" s="274"/>
-      <c r="M102" s="274"/>
-      <c r="N102" s="275"/>
+      <c r="C102" s="305"/>
+      <c r="D102" s="305"/>
+      <c r="E102" s="305"/>
+      <c r="F102" s="305"/>
+      <c r="G102" s="305"/>
+      <c r="H102" s="305"/>
+      <c r="I102" s="305"/>
+      <c r="J102" s="305"/>
+      <c r="K102" s="305"/>
+      <c r="L102" s="305"/>
+      <c r="M102" s="305"/>
+      <c r="N102" s="306"/>
       <c r="O102" s="20">
         <v>5</v>
       </c>
@@ -13559,49 +13571,49 @@
       <c r="R102" s="23">
         <v>20</v>
       </c>
-      <c r="U102" s="299" t="s">
+      <c r="U102" s="302" t="s">
         <v>20</v>
       </c>
-      <c r="V102" s="300"/>
-      <c r="W102" s="300"/>
-      <c r="X102" s="300"/>
-      <c r="Y102" s="300"/>
-      <c r="Z102" s="300"/>
-      <c r="AA102" s="300"/>
-      <c r="AB102" s="297">
+      <c r="V102" s="303"/>
+      <c r="W102" s="303"/>
+      <c r="X102" s="303"/>
+      <c r="Y102" s="303"/>
+      <c r="Z102" s="303"/>
+      <c r="AA102" s="303"/>
+      <c r="AB102" s="300">
         <v>22</v>
       </c>
-      <c r="AC102" s="297"/>
-      <c r="AD102" s="298"/>
+      <c r="AC102" s="300"/>
+      <c r="AD102" s="301"/>
       <c r="AE102" s="29"/>
       <c r="AF102" s="29"/>
-      <c r="AG102" s="280" t="s">
+      <c r="AG102" s="316" t="s">
         <v>21</v>
       </c>
-      <c r="AH102" s="281"/>
-      <c r="AI102" s="281"/>
-      <c r="AJ102" s="282"/>
+      <c r="AH102" s="317"/>
+      <c r="AI102" s="317"/>
+      <c r="AJ102" s="318"/>
       <c r="AK102" s="223">
         <v>230</v>
       </c>
     </row>
     <row r="103" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="34"/>
-      <c r="B103" s="273" t="s">
+      <c r="B103" s="304" t="s">
         <v>5</v>
       </c>
-      <c r="C103" s="274"/>
-      <c r="D103" s="274"/>
-      <c r="E103" s="274"/>
-      <c r="F103" s="274"/>
-      <c r="G103" s="274"/>
-      <c r="H103" s="274"/>
-      <c r="I103" s="274"/>
-      <c r="J103" s="274"/>
-      <c r="K103" s="274"/>
-      <c r="L103" s="274"/>
-      <c r="M103" s="274"/>
-      <c r="N103" s="275"/>
+      <c r="C103" s="305"/>
+      <c r="D103" s="305"/>
+      <c r="E103" s="305"/>
+      <c r="F103" s="305"/>
+      <c r="G103" s="305"/>
+      <c r="H103" s="305"/>
+      <c r="I103" s="305"/>
+      <c r="J103" s="305"/>
+      <c r="K103" s="305"/>
+      <c r="L103" s="305"/>
+      <c r="M103" s="305"/>
+      <c r="N103" s="306"/>
       <c r="O103" s="20">
         <v>2</v>
       </c>
@@ -13614,49 +13626,49 @@
       <c r="R103" s="23">
         <v>8</v>
       </c>
-      <c r="U103" s="278" t="s">
+      <c r="U103" s="311" t="s">
         <v>18</v>
       </c>
-      <c r="V103" s="279"/>
-      <c r="W103" s="279"/>
-      <c r="X103" s="279"/>
-      <c r="Y103" s="279"/>
-      <c r="Z103" s="279"/>
-      <c r="AA103" s="279"/>
-      <c r="AB103" s="304">
+      <c r="V103" s="312"/>
+      <c r="W103" s="312"/>
+      <c r="X103" s="312"/>
+      <c r="Y103" s="312"/>
+      <c r="Z103" s="312"/>
+      <c r="AA103" s="312"/>
+      <c r="AB103" s="313">
         <v>20</v>
       </c>
-      <c r="AC103" s="304"/>
-      <c r="AD103" s="305"/>
+      <c r="AC103" s="313"/>
+      <c r="AD103" s="314"/>
       <c r="AE103" s="29"/>
       <c r="AF103" s="29"/>
-      <c r="AG103" s="283" t="s">
+      <c r="AG103" s="319" t="s">
         <v>22</v>
       </c>
-      <c r="AH103" s="274"/>
-      <c r="AI103" s="274"/>
-      <c r="AJ103" s="275"/>
+      <c r="AH103" s="305"/>
+      <c r="AI103" s="305"/>
+      <c r="AJ103" s="306"/>
       <c r="AK103" s="36">
         <v>115</v>
       </c>
     </row>
     <row r="104" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="35"/>
-      <c r="B104" s="287" t="s">
+      <c r="B104" s="290" t="s">
         <v>4</v>
       </c>
-      <c r="C104" s="288"/>
-      <c r="D104" s="288"/>
-      <c r="E104" s="288"/>
-      <c r="F104" s="288"/>
-      <c r="G104" s="288"/>
-      <c r="H104" s="288"/>
-      <c r="I104" s="288"/>
-      <c r="J104" s="288"/>
-      <c r="K104" s="288"/>
-      <c r="L104" s="288"/>
-      <c r="M104" s="288"/>
-      <c r="N104" s="289"/>
+      <c r="C104" s="291"/>
+      <c r="D104" s="291"/>
+      <c r="E104" s="291"/>
+      <c r="F104" s="291"/>
+      <c r="G104" s="291"/>
+      <c r="H104" s="291"/>
+      <c r="I104" s="291"/>
+      <c r="J104" s="291"/>
+      <c r="K104" s="291"/>
+      <c r="L104" s="291"/>
+      <c r="M104" s="291"/>
+      <c r="N104" s="292"/>
       <c r="O104" s="3">
         <v>1</v>
       </c>
@@ -13669,51 +13681,51 @@
       <c r="R104" s="24">
         <v>1</v>
       </c>
-      <c r="U104" s="301" t="s">
+      <c r="U104" s="307" t="s">
         <v>19</v>
       </c>
-      <c r="V104" s="277"/>
-      <c r="W104" s="277"/>
-      <c r="X104" s="277"/>
-      <c r="Y104" s="277"/>
-      <c r="Z104" s="277"/>
-      <c r="AA104" s="277"/>
-      <c r="AB104" s="302">
+      <c r="V104" s="308"/>
+      <c r="W104" s="308"/>
+      <c r="X104" s="308"/>
+      <c r="Y104" s="308"/>
+      <c r="Z104" s="308"/>
+      <c r="AA104" s="308"/>
+      <c r="AB104" s="309">
         <f>AB102*AB103</f>
         <v>440</v>
       </c>
-      <c r="AC104" s="302"/>
-      <c r="AD104" s="303"/>
+      <c r="AC104" s="309"/>
+      <c r="AD104" s="310"/>
       <c r="AE104" s="29"/>
       <c r="AF104" s="29"/>
-      <c r="AG104" s="283" t="s">
+      <c r="AG104" s="319" t="s">
         <v>25</v>
       </c>
-      <c r="AH104" s="274"/>
-      <c r="AI104" s="274"/>
-      <c r="AJ104" s="275"/>
+      <c r="AH104" s="305"/>
+      <c r="AI104" s="305"/>
+      <c r="AJ104" s="306"/>
       <c r="AK104" s="36">
         <v>65</v>
       </c>
     </row>
     <row r="105" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG105" s="278" t="s">
+      <c r="AG105" s="311" t="s">
         <v>23</v>
       </c>
-      <c r="AH105" s="279"/>
-      <c r="AI105" s="279"/>
-      <c r="AJ105" s="279"/>
+      <c r="AH105" s="312"/>
+      <c r="AI105" s="312"/>
+      <c r="AJ105" s="312"/>
       <c r="AK105" s="225">
         <v>30</v>
       </c>
     </row>
     <row r="106" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG106" s="276" t="s">
+      <c r="AG106" s="315" t="s">
         <v>19</v>
       </c>
-      <c r="AH106" s="277"/>
-      <c r="AI106" s="277"/>
-      <c r="AJ106" s="277"/>
+      <c r="AH106" s="308"/>
+      <c r="AI106" s="308"/>
+      <c r="AJ106" s="308"/>
       <c r="AK106" s="224">
         <f>SUM(AK102:AK105)</f>
         <v>440</v>
@@ -13725,6 +13737,28 @@
     <sortCondition ref="B10:B94"/>
   </sortState>
   <mergeCells count="38">
+    <mergeCell ref="B103:N103"/>
+    <mergeCell ref="AG106:AJ106"/>
+    <mergeCell ref="AG105:AJ105"/>
+    <mergeCell ref="AG102:AJ102"/>
+    <mergeCell ref="AG104:AJ104"/>
+    <mergeCell ref="AG103:AJ103"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="B104:N104"/>
+    <mergeCell ref="C1:O1"/>
+    <mergeCell ref="P1:AJ1"/>
+    <mergeCell ref="C3:O3"/>
+    <mergeCell ref="P3:AJ3"/>
+    <mergeCell ref="C2:P2"/>
+    <mergeCell ref="Q2:AJ2"/>
+    <mergeCell ref="B101:N101"/>
+    <mergeCell ref="AB102:AD102"/>
+    <mergeCell ref="U102:AA102"/>
+    <mergeCell ref="B102:N102"/>
+    <mergeCell ref="U104:AA104"/>
+    <mergeCell ref="AB104:AD104"/>
+    <mergeCell ref="U103:AA103"/>
+    <mergeCell ref="AB103:AD103"/>
     <mergeCell ref="O100:R100"/>
     <mergeCell ref="U101:AD101"/>
     <mergeCell ref="AG101:AK101"/>
@@ -13741,28 +13775,6 @@
     <mergeCell ref="C5:J5"/>
     <mergeCell ref="K5:R5"/>
     <mergeCell ref="S5:S9"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="B104:N104"/>
-    <mergeCell ref="C1:O1"/>
-    <mergeCell ref="P1:AJ1"/>
-    <mergeCell ref="C3:O3"/>
-    <mergeCell ref="P3:AJ3"/>
-    <mergeCell ref="C2:P2"/>
-    <mergeCell ref="Q2:AJ2"/>
-    <mergeCell ref="B101:N101"/>
-    <mergeCell ref="AB102:AD102"/>
-    <mergeCell ref="U102:AA102"/>
-    <mergeCell ref="B102:N102"/>
-    <mergeCell ref="U104:AA104"/>
-    <mergeCell ref="AB104:AD104"/>
-    <mergeCell ref="U103:AA103"/>
-    <mergeCell ref="AB103:AD103"/>
-    <mergeCell ref="B103:N103"/>
-    <mergeCell ref="AG106:AJ106"/>
-    <mergeCell ref="AG105:AJ105"/>
-    <mergeCell ref="AG102:AJ102"/>
-    <mergeCell ref="AG104:AJ104"/>
-    <mergeCell ref="AG103:AJ103"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <conditionalFormatting sqref="AH18:AI18 AH10:AI10 AH14:AI14 T10:AA10 AC10:AF10 C10:R10 C14:R14 T14:AA14 AC14:AF14 T18:AA18 AC18:AF18 AH30:AI30 C30:R30 T30:AA30 AC30:AF30 AH26:AI26 C26:R26 T26:AA26 AC26:AF26 AH62:AI62 C62:R62 T62:AA62 AC62:AF62 AH42:AI42 C42:R42 T42:AA42 AC42:AF42 AH22:AI22 C22:R22 T22:AA22 AC22:AF22 AH38:AI38 C38:R38 T38:AA38 AC38:AF38 AH34:AI34 C34:R34 T34:AA34 AC34:AF34 AH66:AI66 C66:R66 T66:AA66 AC66:AF66 C18:R18">
@@ -14419,7 +14431,7 @@
   <dimension ref="A1:AJ31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N1" activeCellId="1" sqref="B1:B1048576 N1:N1048576"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14831,7 +14843,9 @@
       <c r="H10" s="85">
         <v>2</v>
       </c>
-      <c r="I10" s="86"/>
+      <c r="I10" s="86">
+        <v>3</v>
+      </c>
       <c r="J10" s="77">
         <f>IF(C10&gt;C11,1,0)+IF(D10&gt;D11,1,0)+IF(E10&gt;E11,1,0)+IF(F10&gt;F11,1,0)+IF(G10&gt;G11,1,0)+IF(H10&gt;H11,1,0)+IF(I10&gt;I11,1,0)</f>
         <v>3</v>
@@ -14839,10 +14853,10 @@
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
       <c r="M10" s="76" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="N10" s="87" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="O10" s="85"/>
       <c r="P10" s="85"/>
@@ -14894,18 +14908,20 @@
       <c r="H11" s="85">
         <v>5</v>
       </c>
-      <c r="I11" s="86"/>
+      <c r="I11" s="86">
+        <v>4</v>
+      </c>
       <c r="J11" s="77">
         <f>IF(C11&gt;C10,1,0)+IF(D11&gt;D10,1,0)+IF(E11&gt;E10,1,0)+IF(F11&gt;F10,1,0)+IF(G11&gt;G10,1,0)+IF(H11&gt;H10,1,0)+IF(I11&gt;I10,1,0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K11" s="14"/>
       <c r="L11" s="4"/>
       <c r="M11" s="76" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="N11" s="87" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="O11" s="85"/>
       <c r="P11" s="85"/>

</xml_diff>

<commit_message>
added missing picks round 2
</commit_message>
<xml_diff>
--- a/laval.xlsx
+++ b/laval.xlsx
@@ -2436,9 +2436,6 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -2490,6 +2487,138 @@
     <xf numFmtId="1" fontId="5" fillId="0" borderId="112" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2499,18 +2628,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="83" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="85" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="92" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2523,154 +2667,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="83" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="85" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3871,7 +3871,7 @@
   <dimension ref="A1:AL106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3895,217 +3895,217 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="C1" s="268"/>
-      <c r="D1" s="268"/>
-      <c r="E1" s="268"/>
-      <c r="F1" s="268"/>
-      <c r="G1" s="268"/>
-      <c r="H1" s="268"/>
-      <c r="I1" s="268"/>
-      <c r="J1" s="268"/>
-      <c r="K1" s="268"/>
-      <c r="L1" s="268"/>
-      <c r="M1" s="268"/>
-      <c r="N1" s="268"/>
-      <c r="O1" s="268"/>
-      <c r="P1" s="269"/>
-      <c r="Q1" s="269"/>
-      <c r="R1" s="269"/>
-      <c r="S1" s="269"/>
-      <c r="T1" s="269"/>
-      <c r="U1" s="269"/>
-      <c r="V1" s="269"/>
-      <c r="W1" s="269"/>
-      <c r="X1" s="269"/>
-      <c r="Y1" s="269"/>
-      <c r="Z1" s="269"/>
-      <c r="AA1" s="269"/>
-      <c r="AB1" s="269"/>
-      <c r="AC1" s="269"/>
-      <c r="AD1" s="269"/>
-      <c r="AE1" s="269"/>
-      <c r="AF1" s="269"/>
-      <c r="AG1" s="269"/>
-      <c r="AH1" s="269"/>
-      <c r="AI1" s="269"/>
-      <c r="AJ1" s="269"/>
+      <c r="C1" s="283"/>
+      <c r="D1" s="283"/>
+      <c r="E1" s="283"/>
+      <c r="F1" s="283"/>
+      <c r="G1" s="283"/>
+      <c r="H1" s="283"/>
+      <c r="I1" s="283"/>
+      <c r="J1" s="283"/>
+      <c r="K1" s="283"/>
+      <c r="L1" s="283"/>
+      <c r="M1" s="283"/>
+      <c r="N1" s="283"/>
+      <c r="O1" s="283"/>
+      <c r="P1" s="284"/>
+      <c r="Q1" s="284"/>
+      <c r="R1" s="284"/>
+      <c r="S1" s="284"/>
+      <c r="T1" s="284"/>
+      <c r="U1" s="284"/>
+      <c r="V1" s="284"/>
+      <c r="W1" s="284"/>
+      <c r="X1" s="284"/>
+      <c r="Y1" s="284"/>
+      <c r="Z1" s="284"/>
+      <c r="AA1" s="284"/>
+      <c r="AB1" s="284"/>
+      <c r="AC1" s="284"/>
+      <c r="AD1" s="284"/>
+      <c r="AE1" s="284"/>
+      <c r="AF1" s="284"/>
+      <c r="AG1" s="284"/>
+      <c r="AH1" s="284"/>
+      <c r="AI1" s="284"/>
+      <c r="AJ1" s="284"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="41"/>
-      <c r="C2" s="270" t="s">
+      <c r="C2" s="285" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="270"/>
-      <c r="E2" s="270"/>
-      <c r="F2" s="270"/>
-      <c r="G2" s="270"/>
-      <c r="H2" s="270"/>
-      <c r="I2" s="270"/>
-      <c r="J2" s="270"/>
-      <c r="K2" s="270"/>
-      <c r="L2" s="270"/>
-      <c r="M2" s="270"/>
-      <c r="N2" s="270"/>
-      <c r="O2" s="270"/>
-      <c r="P2" s="270"/>
-      <c r="Q2" s="271" t="s">
+      <c r="D2" s="285"/>
+      <c r="E2" s="285"/>
+      <c r="F2" s="285"/>
+      <c r="G2" s="285"/>
+      <c r="H2" s="285"/>
+      <c r="I2" s="285"/>
+      <c r="J2" s="285"/>
+      <c r="K2" s="285"/>
+      <c r="L2" s="285"/>
+      <c r="M2" s="285"/>
+      <c r="N2" s="285"/>
+      <c r="O2" s="285"/>
+      <c r="P2" s="285"/>
+      <c r="Q2" s="286" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="269"/>
-      <c r="S2" s="269"/>
-      <c r="T2" s="269"/>
-      <c r="U2" s="269"/>
-      <c r="V2" s="269"/>
-      <c r="W2" s="269"/>
-      <c r="X2" s="269"/>
-      <c r="Y2" s="269"/>
-      <c r="Z2" s="269"/>
-      <c r="AA2" s="269"/>
-      <c r="AB2" s="269"/>
-      <c r="AC2" s="269"/>
-      <c r="AD2" s="269"/>
-      <c r="AE2" s="269"/>
-      <c r="AF2" s="269"/>
-      <c r="AG2" s="269"/>
-      <c r="AH2" s="269"/>
-      <c r="AI2" s="269"/>
-      <c r="AJ2" s="269"/>
+      <c r="R2" s="284"/>
+      <c r="S2" s="284"/>
+      <c r="T2" s="284"/>
+      <c r="U2" s="284"/>
+      <c r="V2" s="284"/>
+      <c r="W2" s="284"/>
+      <c r="X2" s="284"/>
+      <c r="Y2" s="284"/>
+      <c r="Z2" s="284"/>
+      <c r="AA2" s="284"/>
+      <c r="AB2" s="284"/>
+      <c r="AC2" s="284"/>
+      <c r="AD2" s="284"/>
+      <c r="AE2" s="284"/>
+      <c r="AF2" s="284"/>
+      <c r="AG2" s="284"/>
+      <c r="AH2" s="284"/>
+      <c r="AI2" s="284"/>
+      <c r="AJ2" s="284"/>
     </row>
     <row r="3" spans="1:38" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="268"/>
-      <c r="D3" s="268"/>
-      <c r="E3" s="268"/>
-      <c r="F3" s="268"/>
-      <c r="G3" s="268"/>
-      <c r="H3" s="268"/>
-      <c r="I3" s="268"/>
-      <c r="J3" s="268"/>
-      <c r="K3" s="268"/>
-      <c r="L3" s="268"/>
-      <c r="M3" s="268"/>
-      <c r="N3" s="268"/>
-      <c r="O3" s="268"/>
-      <c r="P3" s="269"/>
-      <c r="Q3" s="269"/>
-      <c r="R3" s="269"/>
-      <c r="S3" s="269"/>
-      <c r="T3" s="269"/>
-      <c r="U3" s="269"/>
-      <c r="V3" s="269"/>
-      <c r="W3" s="269"/>
-      <c r="X3" s="269"/>
-      <c r="Y3" s="269"/>
-      <c r="Z3" s="269"/>
-      <c r="AA3" s="269"/>
-      <c r="AB3" s="269"/>
-      <c r="AC3" s="269"/>
-      <c r="AD3" s="269"/>
-      <c r="AE3" s="269"/>
-      <c r="AF3" s="269"/>
-      <c r="AG3" s="269"/>
-      <c r="AH3" s="269"/>
-      <c r="AI3" s="269"/>
-      <c r="AJ3" s="269"/>
+      <c r="C3" s="283"/>
+      <c r="D3" s="283"/>
+      <c r="E3" s="283"/>
+      <c r="F3" s="283"/>
+      <c r="G3" s="283"/>
+      <c r="H3" s="283"/>
+      <c r="I3" s="283"/>
+      <c r="J3" s="283"/>
+      <c r="K3" s="283"/>
+      <c r="L3" s="283"/>
+      <c r="M3" s="283"/>
+      <c r="N3" s="283"/>
+      <c r="O3" s="283"/>
+      <c r="P3" s="284"/>
+      <c r="Q3" s="284"/>
+      <c r="R3" s="284"/>
+      <c r="S3" s="284"/>
+      <c r="T3" s="284"/>
+      <c r="U3" s="284"/>
+      <c r="V3" s="284"/>
+      <c r="W3" s="284"/>
+      <c r="X3" s="284"/>
+      <c r="Y3" s="284"/>
+      <c r="Z3" s="284"/>
+      <c r="AA3" s="284"/>
+      <c r="AB3" s="284"/>
+      <c r="AC3" s="284"/>
+      <c r="AD3" s="284"/>
+      <c r="AE3" s="284"/>
+      <c r="AF3" s="284"/>
+      <c r="AG3" s="284"/>
+      <c r="AH3" s="284"/>
+      <c r="AI3" s="284"/>
+      <c r="AJ3" s="284"/>
     </row>
     <row r="4" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="293" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="294"/>
-      <c r="E4" s="294"/>
-      <c r="F4" s="294"/>
-      <c r="G4" s="294"/>
-      <c r="H4" s="294"/>
-      <c r="I4" s="294"/>
-      <c r="J4" s="294"/>
-      <c r="K4" s="294"/>
-      <c r="L4" s="294"/>
-      <c r="M4" s="294"/>
-      <c r="N4" s="294"/>
-      <c r="O4" s="294"/>
-      <c r="P4" s="294"/>
-      <c r="Q4" s="294"/>
-      <c r="R4" s="294"/>
-      <c r="S4" s="295"/>
-      <c r="T4" s="293" t="s">
+      <c r="C4" s="267" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="268"/>
+      <c r="E4" s="268"/>
+      <c r="F4" s="268"/>
+      <c r="G4" s="268"/>
+      <c r="H4" s="268"/>
+      <c r="I4" s="268"/>
+      <c r="J4" s="268"/>
+      <c r="K4" s="268"/>
+      <c r="L4" s="268"/>
+      <c r="M4" s="268"/>
+      <c r="N4" s="268"/>
+      <c r="O4" s="268"/>
+      <c r="P4" s="268"/>
+      <c r="Q4" s="268"/>
+      <c r="R4" s="268"/>
+      <c r="S4" s="269"/>
+      <c r="T4" s="267" t="s">
         <v>1</v>
       </c>
-      <c r="U4" s="294"/>
-      <c r="V4" s="294"/>
-      <c r="W4" s="294"/>
-      <c r="X4" s="294"/>
-      <c r="Y4" s="294"/>
-      <c r="Z4" s="294"/>
-      <c r="AA4" s="294"/>
-      <c r="AB4" s="295"/>
-      <c r="AC4" s="293" t="s">
+      <c r="U4" s="268"/>
+      <c r="V4" s="268"/>
+      <c r="W4" s="268"/>
+      <c r="X4" s="268"/>
+      <c r="Y4" s="268"/>
+      <c r="Z4" s="268"/>
+      <c r="AA4" s="268"/>
+      <c r="AB4" s="269"/>
+      <c r="AC4" s="267" t="s">
         <v>2</v>
       </c>
-      <c r="AD4" s="294"/>
-      <c r="AE4" s="294"/>
-      <c r="AF4" s="294"/>
-      <c r="AG4" s="302"/>
-      <c r="AH4" s="293" t="s">
+      <c r="AD4" s="268"/>
+      <c r="AE4" s="268"/>
+      <c r="AF4" s="268"/>
+      <c r="AG4" s="278"/>
+      <c r="AH4" s="267" t="s">
         <v>10</v>
       </c>
-      <c r="AI4" s="294"/>
-      <c r="AJ4" s="295"/>
+      <c r="AI4" s="268"/>
+      <c r="AJ4" s="269"/>
     </row>
     <row r="5" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="262" t="s">
+      <c r="C5" s="279" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="263"/>
-      <c r="E5" s="263"/>
-      <c r="F5" s="263"/>
-      <c r="G5" s="263"/>
-      <c r="H5" s="263"/>
-      <c r="I5" s="263"/>
-      <c r="J5" s="264"/>
-      <c r="K5" s="300" t="s">
+      <c r="D5" s="275"/>
+      <c r="E5" s="275"/>
+      <c r="F5" s="275"/>
+      <c r="G5" s="275"/>
+      <c r="H5" s="275"/>
+      <c r="I5" s="275"/>
+      <c r="J5" s="276"/>
+      <c r="K5" s="274" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="263"/>
-      <c r="M5" s="263"/>
-      <c r="N5" s="263"/>
-      <c r="O5" s="263"/>
-      <c r="P5" s="263"/>
-      <c r="Q5" s="263"/>
-      <c r="R5" s="264"/>
-      <c r="S5" s="296" t="s">
+      <c r="L5" s="275"/>
+      <c r="M5" s="275"/>
+      <c r="N5" s="275"/>
+      <c r="O5" s="275"/>
+      <c r="P5" s="275"/>
+      <c r="Q5" s="275"/>
+      <c r="R5" s="276"/>
+      <c r="S5" s="270" t="s">
         <v>12</v>
       </c>
-      <c r="T5" s="262" t="s">
+      <c r="T5" s="279" t="s">
         <v>9</v>
       </c>
-      <c r="U5" s="263"/>
-      <c r="V5" s="263"/>
-      <c r="W5" s="264"/>
-      <c r="X5" s="300" t="s">
+      <c r="U5" s="275"/>
+      <c r="V5" s="275"/>
+      <c r="W5" s="276"/>
+      <c r="X5" s="274" t="s">
         <v>8</v>
       </c>
-      <c r="Y5" s="263"/>
-      <c r="Z5" s="263"/>
-      <c r="AA5" s="264"/>
-      <c r="AB5" s="296" t="s">
+      <c r="Y5" s="275"/>
+      <c r="Z5" s="275"/>
+      <c r="AA5" s="276"/>
+      <c r="AB5" s="270" t="s">
         <v>13</v>
       </c>
-      <c r="AC5" s="301" t="s">
+      <c r="AC5" s="277" t="s">
         <v>9</v>
       </c>
-      <c r="AD5" s="264"/>
-      <c r="AE5" s="300" t="s">
+      <c r="AD5" s="276"/>
+      <c r="AE5" s="274" t="s">
         <v>8</v>
       </c>
-      <c r="AF5" s="264"/>
-      <c r="AG5" s="296" t="s">
+      <c r="AF5" s="276"/>
+      <c r="AG5" s="270" t="s">
         <v>14</v>
       </c>
       <c r="AH5" s="56"/>
       <c r="AI5" s="25"/>
-      <c r="AJ5" s="296" t="s">
+      <c r="AJ5" s="270" t="s">
         <v>15</v>
       </c>
       <c r="AK5" s="4"/>
@@ -4169,7 +4169,7 @@
         <f>Résultats!$J$25</f>
         <v>4</v>
       </c>
-      <c r="Q6" s="234">
+      <c r="Q6" s="233">
         <f>Résultats!$J$27</f>
         <v>4</v>
       </c>
@@ -4177,7 +4177,7 @@
         <f>Résultats!$J$28</f>
         <v>3</v>
       </c>
-      <c r="S6" s="297"/>
+      <c r="S6" s="271"/>
       <c r="T6" s="156">
         <f>Résultats!$V$6</f>
         <v>1</v>
@@ -4210,7 +4210,7 @@
         <f>Résultats!$V$25</f>
         <v>0</v>
       </c>
-      <c r="AB6" s="297"/>
+      <c r="AB6" s="271"/>
       <c r="AC6" s="106">
         <f>Résultats!$AH$8</f>
         <v>0</v>
@@ -4227,7 +4227,7 @@
         <f>Résultats!$AH$23</f>
         <v>0</v>
       </c>
-      <c r="AG6" s="297"/>
+      <c r="AG6" s="271"/>
       <c r="AH6" s="198">
         <f>Résultats!$AH$15</f>
         <v>0</v>
@@ -4236,7 +4236,7 @@
         <f>Résultats!$AH$16</f>
         <v>0</v>
       </c>
-      <c r="AJ6" s="297"/>
+      <c r="AJ6" s="271"/>
       <c r="AK6" s="37"/>
     </row>
     <row r="7" spans="1:38" s="39" customFormat="1" ht="58.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -4260,9 +4260,9 @@
       <c r="N7" s="230"/>
       <c r="O7" s="160"/>
       <c r="P7" s="230"/>
-      <c r="Q7" s="235"/>
+      <c r="Q7" s="234"/>
       <c r="R7" s="112"/>
-      <c r="S7" s="297"/>
+      <c r="S7" s="271"/>
       <c r="T7" s="157"/>
       <c r="U7" s="112"/>
       <c r="V7" s="160"/>
@@ -4271,15 +4271,15 @@
       <c r="Y7" s="113"/>
       <c r="Z7" s="114"/>
       <c r="AA7" s="112"/>
-      <c r="AB7" s="297"/>
+      <c r="AB7" s="271"/>
       <c r="AC7" s="114"/>
       <c r="AD7" s="112"/>
       <c r="AE7" s="115"/>
       <c r="AF7" s="112"/>
-      <c r="AG7" s="297"/>
+      <c r="AG7" s="271"/>
       <c r="AH7" s="198"/>
       <c r="AI7" s="107"/>
-      <c r="AJ7" s="297"/>
+      <c r="AJ7" s="271"/>
       <c r="AK7" s="37"/>
     </row>
     <row r="8" spans="1:38" s="39" customFormat="1" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4341,7 +4341,7 @@
         <f>Résultats!$B$25</f>
         <v>DALLAS</v>
       </c>
-      <c r="Q8" s="236" t="str">
+      <c r="Q8" s="235" t="str">
         <f>Résultats!$B$27</f>
         <v>SAN JOSE</v>
       </c>
@@ -4349,7 +4349,7 @@
         <f>Résultats!$B$28</f>
         <v>VEGAS</v>
       </c>
-      <c r="S8" s="297"/>
+      <c r="S8" s="271"/>
       <c r="T8" s="158" t="str">
         <f>Résultats!$N$6</f>
         <v>BOSTON</v>
@@ -4382,7 +4382,7 @@
         <f>Résultats!$N$25</f>
         <v>DALLAS</v>
       </c>
-      <c r="AB8" s="297"/>
+      <c r="AB8" s="271"/>
       <c r="AC8" s="164" t="str">
         <f>Résultats!$Z$8</f>
         <v xml:space="preserve"> </v>
@@ -4399,7 +4399,7 @@
         <f>Résultats!$Z$23</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AG8" s="297"/>
+      <c r="AG8" s="271"/>
       <c r="AH8" s="199" t="str">
         <f>Résultats!$Z$15</f>
         <v xml:space="preserve"> </v>
@@ -4408,7 +4408,7 @@
         <f>Résultats!$Z$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ8" s="297"/>
+      <c r="AJ8" s="271"/>
       <c r="AK8" s="37"/>
     </row>
     <row r="9" spans="1:38" s="39" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4474,7 +4474,7 @@
         <f>Résultats!$A$25</f>
         <v>WC1</v>
       </c>
-      <c r="Q9" s="237" t="str">
+      <c r="Q9" s="236" t="str">
         <f>Résultats!$A$27</f>
         <v>P2</v>
       </c>
@@ -4482,7 +4482,7 @@
         <f>Résultats!$A$28</f>
         <v>P3</v>
       </c>
-      <c r="S9" s="299"/>
+      <c r="S9" s="273"/>
       <c r="T9" s="166" t="str">
         <f>Résultats!$M$6</f>
         <v>A2</v>
@@ -4515,7 +4515,7 @@
         <f>Résultats!$M$25</f>
         <v>WC1</v>
       </c>
-      <c r="AB9" s="298"/>
+      <c r="AB9" s="272"/>
       <c r="AC9" s="170" t="str">
         <f>Résultats!$Y$8</f>
         <v xml:space="preserve"> </v>
@@ -4532,7 +4532,7 @@
         <f>Résultats!$Y$23</f>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="AG9" s="298"/>
+      <c r="AG9" s="272"/>
       <c r="AH9" s="201" t="str">
         <f>Résultats!$Y$15</f>
         <v xml:space="preserve"> </v>
@@ -4541,7 +4541,7 @@
         <f>Résultats!$Y$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ9" s="299"/>
+      <c r="AJ9" s="273"/>
       <c r="AK9" s="109" t="s">
         <v>51</v>
       </c>
@@ -4585,7 +4585,7 @@
         <v>6</v>
       </c>
       <c r="P10" s="175"/>
-      <c r="Q10" s="242">
+      <c r="Q10" s="241">
         <v>7</v>
       </c>
       <c r="R10" s="180"/>
@@ -5062,7 +5062,7 @@
       </c>
       <c r="F14" s="45"/>
       <c r="G14" s="48"/>
-      <c r="H14" s="248">
+      <c r="H14" s="247">
         <v>7</v>
       </c>
       <c r="I14" s="44"/>
@@ -5074,7 +5074,7 @@
       </c>
       <c r="L14" s="47"/>
       <c r="M14" s="44"/>
-      <c r="N14" s="240">
+      <c r="N14" s="239">
         <v>6</v>
       </c>
       <c r="O14" s="44">
@@ -5556,7 +5556,7 @@
         <v>5</v>
       </c>
       <c r="D18" s="186"/>
-      <c r="E18" s="239">
+      <c r="E18" s="238">
         <v>7</v>
       </c>
       <c r="F18" s="186"/>
@@ -5580,7 +5580,7 @@
         <v>5</v>
       </c>
       <c r="P18" s="186"/>
-      <c r="Q18" s="247">
+      <c r="Q18" s="246">
         <v>7</v>
       </c>
       <c r="R18" s="191"/>
@@ -6049,73 +6049,73 @@
         <v>4</v>
       </c>
       <c r="B22" s="84" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C22" s="46">
         <v>5</v>
       </c>
       <c r="D22" s="45"/>
-      <c r="E22" s="238">
+      <c r="E22" s="237">
         <v>7</v>
       </c>
       <c r="F22" s="45"/>
       <c r="G22" s="48">
+        <v>6</v>
+      </c>
+      <c r="H22" s="47"/>
+      <c r="I22" s="44">
+        <v>6</v>
+      </c>
+      <c r="J22" s="47"/>
+      <c r="K22" s="49">
         <v>4</v>
       </c>
-      <c r="H22" s="47"/>
-      <c r="I22" s="44"/>
-      <c r="J22" s="47">
-        <v>6</v>
-      </c>
-      <c r="K22" s="49">
+      <c r="L22" s="47"/>
+      <c r="M22" s="44">
         <v>5</v>
       </c>
-      <c r="L22" s="47"/>
-      <c r="M22" s="44"/>
-      <c r="N22" s="240">
-        <v>6</v>
-      </c>
-      <c r="O22" s="44">
+      <c r="N22" s="45"/>
+      <c r="O22" s="44"/>
+      <c r="P22" s="45">
         <v>7</v>
       </c>
-      <c r="P22" s="45"/>
-      <c r="Q22" s="48">
-        <v>6</v>
-      </c>
-      <c r="R22" s="50"/>
+      <c r="Q22" s="48"/>
+      <c r="R22" s="50">
+        <v>7</v>
+      </c>
       <c r="S22" s="122">
         <f>SUM(C23:R23)</f>
-        <v>37</v>
-      </c>
-      <c r="T22" s="46">
+        <v>38</v>
+      </c>
+      <c r="T22" s="46"/>
+      <c r="U22" s="47">
         <v>6</v>
       </c>
-      <c r="U22" s="47"/>
-      <c r="V22" s="44"/>
-      <c r="W22" s="47">
-        <v>6</v>
-      </c>
-      <c r="X22" s="49">
+      <c r="V22" s="44">
         <v>5</v>
       </c>
-      <c r="Y22" s="45"/>
-      <c r="Z22" s="48"/>
-      <c r="AA22" s="50">
+      <c r="W22" s="47"/>
+      <c r="X22" s="49"/>
+      <c r="Y22" s="45">
+        <v>5</v>
+      </c>
+      <c r="Z22" s="48">
         <v>7</v>
       </c>
+      <c r="AA22" s="50"/>
       <c r="AB22" s="122">
         <f>SUM(T23:AA23)</f>
         <v>1</v>
       </c>
       <c r="AC22" s="48"/>
-      <c r="AD22" s="47"/>
+      <c r="AD22" s="243"/>
       <c r="AE22" s="49"/>
       <c r="AF22" s="47"/>
       <c r="AG22" s="122">
         <f>SUM(AC23:AF23)</f>
         <v>0</v>
       </c>
-      <c r="AH22" s="303"/>
+      <c r="AH22" s="310"/>
       <c r="AI22" s="57"/>
       <c r="AJ22" s="122">
         <f>AH23</f>
@@ -6123,11 +6123,11 @@
       </c>
       <c r="AK22" s="111">
         <f>MAX($AL$10:$AL$97) - AL22</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AL22" s="122">
         <f>$S22+$AB22+$AG22+$AJ22</f>
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6153,7 +6153,7 @@
       <c r="H23" s="151"/>
       <c r="I23" s="125">
         <f>(IF($I22&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I22=$I$6+$J$6,$O$103,0),0),0)+IF($J22&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J22=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J23" s="152"/>
       <c r="K23" s="153">
@@ -6163,23 +6163,23 @@
       <c r="L23" s="151"/>
       <c r="M23" s="125">
         <f>(IF($M22&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M22=$M$6+$N$6,$O$103,0),0),0)+IF($N22&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N22=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="N23" s="151"/>
       <c r="O23" s="125">
         <f>(IF($O22&lt;&gt;"",($O$6*$O$104)+IF($O$6=4,($O$102)+IF($O22=$O$6+$P$6,$O$103,0),0),0)+IF($P22&lt;&gt;"",($P$6*$O$104)+IF($P$6=4,($O$102)+IF($P22=$O$6+$P$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="P23" s="151"/>
       <c r="Q23" s="125">
         <f>(IF($Q22&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q22=$Q$6+$R$6,$O$103,0),0),0)+IF($R22&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R22=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="R23" s="154"/>
       <c r="S23" s="144"/>
       <c r="T23" s="126">
         <f>(IF($T22&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T22=$T$6+$U$6,$P$103,0),0),0)+IF($U22&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U22=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U23" s="126"/>
       <c r="V23" s="126">
@@ -6194,7 +6194,7 @@
       <c r="Y23" s="59"/>
       <c r="Z23" s="126">
         <f>(IF($Z22&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z22=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA22&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA22=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA23" s="62"/>
       <c r="AB23" s="144"/>
@@ -6257,7 +6257,7 @@
         <f>IF(ISBLANK(I22),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" s="118">
         <f>IF(ISBLANK(J22),
@@ -6287,7 +6287,7 @@
         <f>IF(ISBLANK(N22),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O24" s="118">
         <f>IF(ISBLANK(O22),
@@ -6299,13 +6299,13 @@
         <f>IF(ISBLANK(P22),
 0,
 IF(P$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q24" s="118">
         <f>IF(ISBLANK(Q22),
 0,
 IF(Q$6= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R24" s="118">
         <f>IF(ISBLANK(R22),
@@ -6452,7 +6452,7 @@
         <f>IF(N24 = 0,
 0,
 IF(N22 = (M$6+N$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O25" s="118">
         <f>IF(O24 = 0,
@@ -6538,79 +6538,83 @@
       <c r="AJ25" s="138"/>
       <c r="AK25" s="139">
         <f>SUM(C25:AI25)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AL25" s="123"/>
     </row>
     <row r="26" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="173">
         <f>RANK(AL26,$AL$10:$AL$97,)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B26" s="197" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C26" s="185">
         <v>5</v>
       </c>
       <c r="D26" s="186"/>
-      <c r="E26" s="239">
+      <c r="E26" s="238">
         <v>7</v>
       </c>
       <c r="F26" s="186"/>
       <c r="G26" s="188">
+        <v>4</v>
+      </c>
+      <c r="H26" s="189"/>
+      <c r="I26" s="187"/>
+      <c r="J26" s="189">
         <v>6</v>
       </c>
-      <c r="H26" s="189"/>
-      <c r="I26" s="187">
+      <c r="K26" s="190">
+        <v>5</v>
+      </c>
+      <c r="L26" s="189"/>
+      <c r="M26" s="187"/>
+      <c r="N26" s="240">
         <v>6</v>
       </c>
-      <c r="J26" s="189"/>
-      <c r="K26" s="190">
-        <v>4</v>
-      </c>
-      <c r="L26" s="189"/>
-      <c r="M26" s="187">
-        <v>5</v>
-      </c>
-      <c r="N26" s="186"/>
-      <c r="O26" s="187"/>
-      <c r="P26" s="186">
+      <c r="O26" s="187">
         <v>7</v>
       </c>
-      <c r="Q26" s="188"/>
-      <c r="R26" s="191">
-        <v>7</v>
-      </c>
+      <c r="P26" s="186"/>
+      <c r="Q26" s="188">
+        <v>6</v>
+      </c>
+      <c r="R26" s="191"/>
       <c r="S26" s="192">
         <f>SUM(C27:R27)</f>
-        <v>38</v>
-      </c>
-      <c r="T26" s="185"/>
-      <c r="U26" s="189">
+        <v>37</v>
+      </c>
+      <c r="T26" s="185">
         <v>6</v>
       </c>
-      <c r="V26" s="187">
+      <c r="U26" s="189"/>
+      <c r="V26" s="187"/>
+      <c r="W26" s="189">
+        <v>6</v>
+      </c>
+      <c r="X26" s="190">
         <v>5</v>
       </c>
-      <c r="W26" s="189"/>
-      <c r="X26" s="190"/>
       <c r="Y26" s="186"/>
       <c r="Z26" s="188"/>
-      <c r="AA26" s="191"/>
+      <c r="AA26" s="191">
+        <v>7</v>
+      </c>
       <c r="AB26" s="192">
         <f>SUM(T27:AA27)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC26" s="188"/>
-      <c r="AD26" s="233"/>
+      <c r="AD26" s="189"/>
       <c r="AE26" s="190"/>
       <c r="AF26" s="189"/>
       <c r="AG26" s="192">
         <f>SUM(AC27:AF27)</f>
         <v>0</v>
       </c>
-      <c r="AH26" s="182"/>
+      <c r="AH26" s="311"/>
       <c r="AI26" s="183"/>
       <c r="AJ26" s="192">
         <f>AH27</f>
@@ -6648,7 +6652,7 @@
       <c r="H27" s="140"/>
       <c r="I27" s="120">
         <f>(IF($I26&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I26=$I$6+$J$6,$O$103,0),0),0)+IF($J26&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J26=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J27" s="141"/>
       <c r="K27" s="142">
@@ -6658,23 +6662,23 @@
       <c r="L27" s="140"/>
       <c r="M27" s="120">
         <f>(IF($M26&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M26=$M$6+$N$6,$O$103,0),0),0)+IF($N26&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N26=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="N27" s="140"/>
       <c r="O27" s="120">
         <f>(IF($O26&lt;&gt;"",($O$6*$O$104)+IF($O$6=4,($O$102)+IF($O26=$O$6+$P$6,$O$103,0),0),0)+IF($P26&lt;&gt;"",($P$6*$O$104)+IF($P$6=4,($O$102)+IF($P26=$O$6+$P$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="P27" s="140"/>
       <c r="Q27" s="120">
         <f>(IF($Q26&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q26=$Q$6+$R$6,$O$103,0),0),0)+IF($R26&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R26=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="R27" s="143"/>
       <c r="S27" s="144"/>
       <c r="T27" s="126">
         <f>(IF($T26&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T26=$T$6+$U$6,$P$103,0),0),0)+IF($U26&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U26=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U27" s="126"/>
       <c r="V27" s="126">
@@ -6752,7 +6756,7 @@
         <f>IF(ISBLANK(I26),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" s="118">
         <f>IF(ISBLANK(J26),
@@ -6782,7 +6786,7 @@
         <f>IF(ISBLANK(N26),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O28" s="118">
         <f>IF(ISBLANK(O26),
@@ -6794,13 +6798,13 @@
         <f>IF(ISBLANK(P26),
 0,
 IF(P$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q28" s="118">
         <f>IF(ISBLANK(Q26),
 0,
 IF(Q$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R28" s="118">
         <f>IF(ISBLANK(R26),
@@ -6947,7 +6951,7 @@
         <f>IF(N28 = 0,
 0,
 IF(N26 = (M$6+N$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O29" s="118">
         <f>IF(O28 = 0,
@@ -7033,7 +7037,7 @@
       <c r="AJ29" s="138"/>
       <c r="AK29" s="139">
         <f>SUM(C29:AI29)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL29" s="123"/>
     </row>
@@ -7073,7 +7077,7 @@
         <v>6</v>
       </c>
       <c r="P30" s="45"/>
-      <c r="Q30" s="243">
+      <c r="Q30" s="242">
         <v>7</v>
       </c>
       <c r="R30" s="50"/>
@@ -7553,7 +7557,7 @@
       </c>
       <c r="F34" s="186"/>
       <c r="G34" s="188"/>
-      <c r="H34" s="249">
+      <c r="H34" s="248">
         <v>7</v>
       </c>
       <c r="I34" s="187"/>
@@ -8047,15 +8051,15 @@
         <v>7</v>
       </c>
       <c r="D38" s="45"/>
-      <c r="E38" s="245">
+      <c r="E38" s="244">
         <v>6</v>
       </c>
       <c r="F38" s="45"/>
-      <c r="G38" s="246"/>
+      <c r="G38" s="245"/>
       <c r="H38" s="47">
         <v>6</v>
       </c>
-      <c r="I38" s="245"/>
+      <c r="I38" s="244"/>
       <c r="J38" s="47">
         <v>7</v>
       </c>
@@ -9062,7 +9066,7 @@
       </c>
       <c r="L46" s="47"/>
       <c r="M46" s="44"/>
-      <c r="N46" s="240">
+      <c r="N46" s="239">
         <v>6</v>
       </c>
       <c r="O46" s="44">
@@ -9105,7 +9109,7 @@
         <f>SUM(AC47:AF47)</f>
         <v>0</v>
       </c>
-      <c r="AH46" s="304"/>
+      <c r="AH46" s="250"/>
       <c r="AI46" s="57"/>
       <c r="AJ46" s="122">
         <f>AH47</f>
@@ -9561,7 +9565,7 @@
         <v>6</v>
       </c>
       <c r="M50" s="187"/>
-      <c r="N50" s="241">
+      <c r="N50" s="240">
         <v>6</v>
       </c>
       <c r="O50" s="187">
@@ -10057,7 +10061,7 @@
       </c>
       <c r="L54" s="47"/>
       <c r="M54" s="44"/>
-      <c r="N54" s="240">
+      <c r="N54" s="239">
         <v>6</v>
       </c>
       <c r="O54" s="44">
@@ -10536,7 +10540,7 @@
         <v>6</v>
       </c>
       <c r="D58" s="186"/>
-      <c r="E58" s="239">
+      <c r="E58" s="238">
         <v>7</v>
       </c>
       <c r="F58" s="186"/>
@@ -11032,7 +11036,7 @@
         <v>6</v>
       </c>
       <c r="D62" s="45"/>
-      <c r="E62" s="238">
+      <c r="E62" s="237">
         <v>7</v>
       </c>
       <c r="F62" s="45"/>
@@ -12077,7 +12081,7 @@
         <v>1</v>
       </c>
       <c r="AC70" s="48"/>
-      <c r="AD70" s="244"/>
+      <c r="AD70" s="243"/>
       <c r="AE70" s="49"/>
       <c r="AF70" s="47"/>
       <c r="AG70" s="122">
@@ -12516,36 +12520,36 @@
       <c r="B74" s="197" t="s">
         <v>68</v>
       </c>
-      <c r="C74" s="305">
+      <c r="C74" s="251">
         <v>5</v>
       </c>
-      <c r="D74" s="306"/>
-      <c r="E74" s="307">
+      <c r="D74" s="252"/>
+      <c r="E74" s="253">
         <v>6</v>
       </c>
-      <c r="F74" s="306"/>
-      <c r="G74" s="308">
+      <c r="F74" s="252"/>
+      <c r="G74" s="254">
         <v>5</v>
       </c>
-      <c r="H74" s="309"/>
-      <c r="I74" s="307"/>
-      <c r="J74" s="309">
+      <c r="H74" s="255"/>
+      <c r="I74" s="253"/>
+      <c r="J74" s="255">
         <v>6</v>
       </c>
-      <c r="K74" s="310">
+      <c r="K74" s="256">
         <v>6</v>
       </c>
-      <c r="L74" s="309"/>
-      <c r="M74" s="307">
+      <c r="L74" s="255"/>
+      <c r="M74" s="253">
         <v>7</v>
       </c>
-      <c r="N74" s="306"/>
-      <c r="O74" s="307">
+      <c r="N74" s="252"/>
+      <c r="O74" s="253">
         <v>6</v>
       </c>
-      <c r="P74" s="306"/>
-      <c r="Q74" s="308"/>
-      <c r="R74" s="311">
+      <c r="P74" s="252"/>
+      <c r="Q74" s="254"/>
+      <c r="R74" s="257">
         <v>6</v>
       </c>
       <c r="S74" s="192">
@@ -15515,7 +15519,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="J98" s="250">
+      <c r="J98" s="249">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
@@ -15564,7 +15568,7 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="W98" s="250">
+      <c r="W98" s="249">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -15574,11 +15578,11 @@
       </c>
       <c r="Y98" s="205">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Z98" s="207">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AA98" s="208">
         <f t="shared" si="0"/>
@@ -15617,12 +15621,12 @@
     <row r="100" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B100" s="43"/>
       <c r="N100" s="26"/>
-      <c r="O100" s="284" t="s">
+      <c r="O100" s="258" t="s">
         <v>17</v>
       </c>
-      <c r="P100" s="285"/>
-      <c r="Q100" s="285"/>
-      <c r="R100" s="286"/>
+      <c r="P100" s="259"/>
+      <c r="Q100" s="259"/>
+      <c r="R100" s="260"/>
       <c r="AG100" s="30"/>
       <c r="AH100" s="30"/>
       <c r="AI100" s="30"/>
@@ -15631,21 +15635,21 @@
     </row>
     <row r="101" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="33"/>
-      <c r="B101" s="272" t="s">
+      <c r="B101" s="287" t="s">
         <v>16</v>
       </c>
-      <c r="C101" s="273"/>
-      <c r="D101" s="273"/>
-      <c r="E101" s="273"/>
-      <c r="F101" s="273"/>
-      <c r="G101" s="273"/>
-      <c r="H101" s="273"/>
-      <c r="I101" s="273"/>
-      <c r="J101" s="273"/>
-      <c r="K101" s="273"/>
-      <c r="L101" s="273"/>
-      <c r="M101" s="273"/>
-      <c r="N101" s="274"/>
+      <c r="C101" s="288"/>
+      <c r="D101" s="288"/>
+      <c r="E101" s="288"/>
+      <c r="F101" s="288"/>
+      <c r="G101" s="288"/>
+      <c r="H101" s="288"/>
+      <c r="I101" s="288"/>
+      <c r="J101" s="288"/>
+      <c r="K101" s="288"/>
+      <c r="L101" s="288"/>
+      <c r="M101" s="288"/>
+      <c r="N101" s="289"/>
       <c r="O101" s="21">
         <v>1</v>
       </c>
@@ -15658,45 +15662,45 @@
       <c r="R101" s="22">
         <v>4</v>
       </c>
-      <c r="U101" s="287" t="s">
+      <c r="U101" s="261" t="s">
         <v>26</v>
       </c>
-      <c r="V101" s="288"/>
-      <c r="W101" s="288"/>
-      <c r="X101" s="288"/>
-      <c r="Y101" s="288"/>
-      <c r="Z101" s="288"/>
-      <c r="AA101" s="288"/>
-      <c r="AB101" s="288"/>
-      <c r="AC101" s="288"/>
-      <c r="AD101" s="289"/>
+      <c r="V101" s="262"/>
+      <c r="W101" s="262"/>
+      <c r="X101" s="262"/>
+      <c r="Y101" s="262"/>
+      <c r="Z101" s="262"/>
+      <c r="AA101" s="262"/>
+      <c r="AB101" s="262"/>
+      <c r="AC101" s="262"/>
+      <c r="AD101" s="263"/>
       <c r="AE101" s="28"/>
       <c r="AF101" s="28"/>
-      <c r="AG101" s="290" t="s">
+      <c r="AG101" s="264" t="s">
         <v>24</v>
       </c>
-      <c r="AH101" s="291"/>
-      <c r="AI101" s="291"/>
-      <c r="AJ101" s="291"/>
-      <c r="AK101" s="292"/>
+      <c r="AH101" s="265"/>
+      <c r="AI101" s="265"/>
+      <c r="AJ101" s="265"/>
+      <c r="AK101" s="266"/>
     </row>
     <row r="102" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A102" s="34"/>
-      <c r="B102" s="251" t="s">
+      <c r="B102" s="294" t="s">
         <v>6</v>
       </c>
-      <c r="C102" s="252"/>
-      <c r="D102" s="252"/>
-      <c r="E102" s="252"/>
-      <c r="F102" s="252"/>
-      <c r="G102" s="252"/>
-      <c r="H102" s="252"/>
-      <c r="I102" s="252"/>
-      <c r="J102" s="252"/>
-      <c r="K102" s="252"/>
-      <c r="L102" s="252"/>
-      <c r="M102" s="252"/>
-      <c r="N102" s="253"/>
+      <c r="C102" s="295"/>
+      <c r="D102" s="295"/>
+      <c r="E102" s="295"/>
+      <c r="F102" s="295"/>
+      <c r="G102" s="295"/>
+      <c r="H102" s="295"/>
+      <c r="I102" s="295"/>
+      <c r="J102" s="295"/>
+      <c r="K102" s="295"/>
+      <c r="L102" s="295"/>
+      <c r="M102" s="295"/>
+      <c r="N102" s="296"/>
       <c r="O102" s="20">
         <v>5</v>
       </c>
@@ -15709,49 +15713,49 @@
       <c r="R102" s="23">
         <v>20</v>
       </c>
-      <c r="U102" s="277" t="s">
+      <c r="U102" s="292" t="s">
         <v>20</v>
       </c>
-      <c r="V102" s="278"/>
-      <c r="W102" s="278"/>
-      <c r="X102" s="278"/>
-      <c r="Y102" s="278"/>
-      <c r="Z102" s="278"/>
-      <c r="AA102" s="278"/>
-      <c r="AB102" s="275">
+      <c r="V102" s="293"/>
+      <c r="W102" s="293"/>
+      <c r="X102" s="293"/>
+      <c r="Y102" s="293"/>
+      <c r="Z102" s="293"/>
+      <c r="AA102" s="293"/>
+      <c r="AB102" s="290">
         <v>22</v>
       </c>
-      <c r="AC102" s="275"/>
-      <c r="AD102" s="276"/>
+      <c r="AC102" s="290"/>
+      <c r="AD102" s="291"/>
       <c r="AE102" s="29"/>
       <c r="AF102" s="29"/>
-      <c r="AG102" s="258" t="s">
+      <c r="AG102" s="306" t="s">
         <v>21</v>
       </c>
-      <c r="AH102" s="259"/>
-      <c r="AI102" s="259"/>
-      <c r="AJ102" s="260"/>
+      <c r="AH102" s="307"/>
+      <c r="AI102" s="307"/>
+      <c r="AJ102" s="308"/>
       <c r="AK102" s="209">
         <v>230</v>
       </c>
     </row>
     <row r="103" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="34"/>
-      <c r="B103" s="251" t="s">
+      <c r="B103" s="294" t="s">
         <v>5</v>
       </c>
-      <c r="C103" s="252"/>
-      <c r="D103" s="252"/>
-      <c r="E103" s="252"/>
-      <c r="F103" s="252"/>
-      <c r="G103" s="252"/>
-      <c r="H103" s="252"/>
-      <c r="I103" s="252"/>
-      <c r="J103" s="252"/>
-      <c r="K103" s="252"/>
-      <c r="L103" s="252"/>
-      <c r="M103" s="252"/>
-      <c r="N103" s="253"/>
+      <c r="C103" s="295"/>
+      <c r="D103" s="295"/>
+      <c r="E103" s="295"/>
+      <c r="F103" s="295"/>
+      <c r="G103" s="295"/>
+      <c r="H103" s="295"/>
+      <c r="I103" s="295"/>
+      <c r="J103" s="295"/>
+      <c r="K103" s="295"/>
+      <c r="L103" s="295"/>
+      <c r="M103" s="295"/>
+      <c r="N103" s="296"/>
       <c r="O103" s="20">
         <v>2</v>
       </c>
@@ -15764,49 +15768,49 @@
       <c r="R103" s="23">
         <v>8</v>
       </c>
-      <c r="U103" s="256" t="s">
+      <c r="U103" s="301" t="s">
         <v>18</v>
       </c>
-      <c r="V103" s="257"/>
-      <c r="W103" s="257"/>
-      <c r="X103" s="257"/>
-      <c r="Y103" s="257"/>
-      <c r="Z103" s="257"/>
-      <c r="AA103" s="257"/>
-      <c r="AB103" s="282">
+      <c r="V103" s="302"/>
+      <c r="W103" s="302"/>
+      <c r="X103" s="302"/>
+      <c r="Y103" s="302"/>
+      <c r="Z103" s="302"/>
+      <c r="AA103" s="302"/>
+      <c r="AB103" s="303">
         <v>20</v>
       </c>
-      <c r="AC103" s="282"/>
-      <c r="AD103" s="283"/>
+      <c r="AC103" s="303"/>
+      <c r="AD103" s="304"/>
       <c r="AE103" s="29"/>
       <c r="AF103" s="29"/>
-      <c r="AG103" s="261" t="s">
+      <c r="AG103" s="309" t="s">
         <v>22</v>
       </c>
-      <c r="AH103" s="252"/>
-      <c r="AI103" s="252"/>
-      <c r="AJ103" s="253"/>
+      <c r="AH103" s="295"/>
+      <c r="AI103" s="295"/>
+      <c r="AJ103" s="296"/>
       <c r="AK103" s="36">
         <v>115</v>
       </c>
     </row>
     <row r="104" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="35"/>
-      <c r="B104" s="265" t="s">
+      <c r="B104" s="280" t="s">
         <v>4</v>
       </c>
-      <c r="C104" s="266"/>
-      <c r="D104" s="266"/>
-      <c r="E104" s="266"/>
-      <c r="F104" s="266"/>
-      <c r="G104" s="266"/>
-      <c r="H104" s="266"/>
-      <c r="I104" s="266"/>
-      <c r="J104" s="266"/>
-      <c r="K104" s="266"/>
-      <c r="L104" s="266"/>
-      <c r="M104" s="266"/>
-      <c r="N104" s="267"/>
+      <c r="C104" s="281"/>
+      <c r="D104" s="281"/>
+      <c r="E104" s="281"/>
+      <c r="F104" s="281"/>
+      <c r="G104" s="281"/>
+      <c r="H104" s="281"/>
+      <c r="I104" s="281"/>
+      <c r="J104" s="281"/>
+      <c r="K104" s="281"/>
+      <c r="L104" s="281"/>
+      <c r="M104" s="281"/>
+      <c r="N104" s="282"/>
       <c r="O104" s="3">
         <v>1</v>
       </c>
@@ -15819,51 +15823,51 @@
       <c r="R104" s="24">
         <v>1</v>
       </c>
-      <c r="U104" s="279" t="s">
+      <c r="U104" s="297" t="s">
         <v>19</v>
       </c>
-      <c r="V104" s="255"/>
-      <c r="W104" s="255"/>
-      <c r="X104" s="255"/>
-      <c r="Y104" s="255"/>
-      <c r="Z104" s="255"/>
-      <c r="AA104" s="255"/>
-      <c r="AB104" s="280">
+      <c r="V104" s="298"/>
+      <c r="W104" s="298"/>
+      <c r="X104" s="298"/>
+      <c r="Y104" s="298"/>
+      <c r="Z104" s="298"/>
+      <c r="AA104" s="298"/>
+      <c r="AB104" s="299">
         <f>AB102*AB103</f>
         <v>440</v>
       </c>
-      <c r="AC104" s="280"/>
-      <c r="AD104" s="281"/>
+      <c r="AC104" s="299"/>
+      <c r="AD104" s="300"/>
       <c r="AE104" s="29"/>
       <c r="AF104" s="29"/>
-      <c r="AG104" s="261" t="s">
+      <c r="AG104" s="309" t="s">
         <v>25</v>
       </c>
-      <c r="AH104" s="252"/>
-      <c r="AI104" s="252"/>
-      <c r="AJ104" s="253"/>
+      <c r="AH104" s="295"/>
+      <c r="AI104" s="295"/>
+      <c r="AJ104" s="296"/>
       <c r="AK104" s="36">
         <v>65</v>
       </c>
     </row>
     <row r="105" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG105" s="256" t="s">
+      <c r="AG105" s="301" t="s">
         <v>23</v>
       </c>
-      <c r="AH105" s="257"/>
-      <c r="AI105" s="257"/>
-      <c r="AJ105" s="257"/>
+      <c r="AH105" s="302"/>
+      <c r="AI105" s="302"/>
+      <c r="AJ105" s="302"/>
       <c r="AK105" s="211">
         <v>30</v>
       </c>
     </row>
     <row r="106" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG106" s="254" t="s">
+      <c r="AG106" s="305" t="s">
         <v>19</v>
       </c>
-      <c r="AH106" s="255"/>
-      <c r="AI106" s="255"/>
-      <c r="AJ106" s="255"/>
+      <c r="AH106" s="298"/>
+      <c r="AI106" s="298"/>
+      <c r="AJ106" s="298"/>
       <c r="AK106" s="210">
         <f>SUM(AK102:AK105)</f>
         <v>440</v>
@@ -15875,6 +15879,28 @@
     <sortCondition ref="B10:B94"/>
   </sortState>
   <mergeCells count="38">
+    <mergeCell ref="B103:N103"/>
+    <mergeCell ref="AG106:AJ106"/>
+    <mergeCell ref="AG105:AJ105"/>
+    <mergeCell ref="AG102:AJ102"/>
+    <mergeCell ref="AG104:AJ104"/>
+    <mergeCell ref="AG103:AJ103"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="B104:N104"/>
+    <mergeCell ref="C1:O1"/>
+    <mergeCell ref="P1:AJ1"/>
+    <mergeCell ref="C3:O3"/>
+    <mergeCell ref="P3:AJ3"/>
+    <mergeCell ref="C2:P2"/>
+    <mergeCell ref="Q2:AJ2"/>
+    <mergeCell ref="B101:N101"/>
+    <mergeCell ref="AB102:AD102"/>
+    <mergeCell ref="U102:AA102"/>
+    <mergeCell ref="B102:N102"/>
+    <mergeCell ref="U104:AA104"/>
+    <mergeCell ref="AB104:AD104"/>
+    <mergeCell ref="U103:AA103"/>
+    <mergeCell ref="AB103:AD103"/>
     <mergeCell ref="O100:R100"/>
     <mergeCell ref="U101:AD101"/>
     <mergeCell ref="AG101:AK101"/>
@@ -15891,28 +15917,6 @@
     <mergeCell ref="C5:J5"/>
     <mergeCell ref="K5:R5"/>
     <mergeCell ref="S5:S9"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="B104:N104"/>
-    <mergeCell ref="C1:O1"/>
-    <mergeCell ref="P1:AJ1"/>
-    <mergeCell ref="C3:O3"/>
-    <mergeCell ref="P3:AJ3"/>
-    <mergeCell ref="C2:P2"/>
-    <mergeCell ref="Q2:AJ2"/>
-    <mergeCell ref="B101:N101"/>
-    <mergeCell ref="AB102:AD102"/>
-    <mergeCell ref="U102:AA102"/>
-    <mergeCell ref="B102:N102"/>
-    <mergeCell ref="U104:AA104"/>
-    <mergeCell ref="AB104:AD104"/>
-    <mergeCell ref="U103:AA103"/>
-    <mergeCell ref="AB103:AD103"/>
-    <mergeCell ref="B103:N103"/>
-    <mergeCell ref="AG106:AJ106"/>
-    <mergeCell ref="AG105:AJ105"/>
-    <mergeCell ref="AG102:AJ102"/>
-    <mergeCell ref="AG104:AJ104"/>
-    <mergeCell ref="AG103:AJ103"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <conditionalFormatting sqref="AH18:AI18 AH10:AI10 AH14:AI14 T10:AA10 AC10:AF10 C10:R10 C14:R14 T14:AA14 AC14:AF14 T18:AA18 AC18:AF18 AH30:AI30 C30:R30 T30:AA30 AC30:AF30 AH26:AI26 C26:R26 T26:AA26 AC26:AF26 AH62:AI62 C62:R62 T62:AA62 AC62:AF62 AH42:AI42 C42:R42 T42:AA42 AC42:AF42 AH22:AI22 C22:R22 T22:AA22 AC22:AF22 AH38:AI38 C38:R38 T38:AA38 AC38:AF38 AH34:AI34 C34:R34 T34:AA34 AC34:AF34 AH66:AI66 C66:R66 T66:AA66 AC66:AF66 C18:R18">

</xml_diff>

<commit_message>
Updated games for last days
</commit_message>
<xml_diff>
--- a/laval.xlsx
+++ b/laval.xlsx
@@ -1934,7 +1934,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="312">
+  <cellXfs count="309">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2463,12 +2463,6 @@
     <xf numFmtId="0" fontId="14" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2481,15 +2475,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="112" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2511,6 +2499,105 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="92" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="82" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="83" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="85" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2562,115 +2649,19 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="83" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="85" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="92" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="82" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3871,7 +3862,7 @@
   <dimension ref="A1:AL106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3895,217 +3886,217 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="C1" s="283"/>
-      <c r="D1" s="283"/>
-      <c r="E1" s="283"/>
-      <c r="F1" s="283"/>
-      <c r="G1" s="283"/>
-      <c r="H1" s="283"/>
-      <c r="I1" s="283"/>
-      <c r="J1" s="283"/>
-      <c r="K1" s="283"/>
-      <c r="L1" s="283"/>
-      <c r="M1" s="283"/>
-      <c r="N1" s="283"/>
-      <c r="O1" s="283"/>
-      <c r="P1" s="284"/>
-      <c r="Q1" s="284"/>
-      <c r="R1" s="284"/>
-      <c r="S1" s="284"/>
-      <c r="T1" s="284"/>
-      <c r="U1" s="284"/>
-      <c r="V1" s="284"/>
-      <c r="W1" s="284"/>
-      <c r="X1" s="284"/>
-      <c r="Y1" s="284"/>
-      <c r="Z1" s="284"/>
-      <c r="AA1" s="284"/>
-      <c r="AB1" s="284"/>
-      <c r="AC1" s="284"/>
-      <c r="AD1" s="284"/>
-      <c r="AE1" s="284"/>
-      <c r="AF1" s="284"/>
-      <c r="AG1" s="284"/>
-      <c r="AH1" s="284"/>
-      <c r="AI1" s="284"/>
-      <c r="AJ1" s="284"/>
+      <c r="C1" s="271"/>
+      <c r="D1" s="271"/>
+      <c r="E1" s="271"/>
+      <c r="F1" s="271"/>
+      <c r="G1" s="271"/>
+      <c r="H1" s="271"/>
+      <c r="I1" s="271"/>
+      <c r="J1" s="271"/>
+      <c r="K1" s="271"/>
+      <c r="L1" s="271"/>
+      <c r="M1" s="271"/>
+      <c r="N1" s="271"/>
+      <c r="O1" s="271"/>
+      <c r="P1" s="272"/>
+      <c r="Q1" s="272"/>
+      <c r="R1" s="272"/>
+      <c r="S1" s="272"/>
+      <c r="T1" s="272"/>
+      <c r="U1" s="272"/>
+      <c r="V1" s="272"/>
+      <c r="W1" s="272"/>
+      <c r="X1" s="272"/>
+      <c r="Y1" s="272"/>
+      <c r="Z1" s="272"/>
+      <c r="AA1" s="272"/>
+      <c r="AB1" s="272"/>
+      <c r="AC1" s="272"/>
+      <c r="AD1" s="272"/>
+      <c r="AE1" s="272"/>
+      <c r="AF1" s="272"/>
+      <c r="AG1" s="272"/>
+      <c r="AH1" s="272"/>
+      <c r="AI1" s="272"/>
+      <c r="AJ1" s="272"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="41"/>
-      <c r="C2" s="285" t="s">
+      <c r="C2" s="273" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="285"/>
-      <c r="E2" s="285"/>
-      <c r="F2" s="285"/>
-      <c r="G2" s="285"/>
-      <c r="H2" s="285"/>
-      <c r="I2" s="285"/>
-      <c r="J2" s="285"/>
-      <c r="K2" s="285"/>
-      <c r="L2" s="285"/>
-      <c r="M2" s="285"/>
-      <c r="N2" s="285"/>
-      <c r="O2" s="285"/>
-      <c r="P2" s="285"/>
-      <c r="Q2" s="286" t="s">
+      <c r="D2" s="273"/>
+      <c r="E2" s="273"/>
+      <c r="F2" s="273"/>
+      <c r="G2" s="273"/>
+      <c r="H2" s="273"/>
+      <c r="I2" s="273"/>
+      <c r="J2" s="273"/>
+      <c r="K2" s="273"/>
+      <c r="L2" s="273"/>
+      <c r="M2" s="273"/>
+      <c r="N2" s="273"/>
+      <c r="O2" s="273"/>
+      <c r="P2" s="273"/>
+      <c r="Q2" s="274" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="284"/>
-      <c r="S2" s="284"/>
-      <c r="T2" s="284"/>
-      <c r="U2" s="284"/>
-      <c r="V2" s="284"/>
-      <c r="W2" s="284"/>
-      <c r="X2" s="284"/>
-      <c r="Y2" s="284"/>
-      <c r="Z2" s="284"/>
-      <c r="AA2" s="284"/>
-      <c r="AB2" s="284"/>
-      <c r="AC2" s="284"/>
-      <c r="AD2" s="284"/>
-      <c r="AE2" s="284"/>
-      <c r="AF2" s="284"/>
-      <c r="AG2" s="284"/>
-      <c r="AH2" s="284"/>
-      <c r="AI2" s="284"/>
-      <c r="AJ2" s="284"/>
+      <c r="R2" s="272"/>
+      <c r="S2" s="272"/>
+      <c r="T2" s="272"/>
+      <c r="U2" s="272"/>
+      <c r="V2" s="272"/>
+      <c r="W2" s="272"/>
+      <c r="X2" s="272"/>
+      <c r="Y2" s="272"/>
+      <c r="Z2" s="272"/>
+      <c r="AA2" s="272"/>
+      <c r="AB2" s="272"/>
+      <c r="AC2" s="272"/>
+      <c r="AD2" s="272"/>
+      <c r="AE2" s="272"/>
+      <c r="AF2" s="272"/>
+      <c r="AG2" s="272"/>
+      <c r="AH2" s="272"/>
+      <c r="AI2" s="272"/>
+      <c r="AJ2" s="272"/>
     </row>
     <row r="3" spans="1:38" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="283"/>
-      <c r="D3" s="283"/>
-      <c r="E3" s="283"/>
-      <c r="F3" s="283"/>
-      <c r="G3" s="283"/>
-      <c r="H3" s="283"/>
-      <c r="I3" s="283"/>
-      <c r="J3" s="283"/>
-      <c r="K3" s="283"/>
-      <c r="L3" s="283"/>
-      <c r="M3" s="283"/>
-      <c r="N3" s="283"/>
-      <c r="O3" s="283"/>
-      <c r="P3" s="284"/>
-      <c r="Q3" s="284"/>
-      <c r="R3" s="284"/>
-      <c r="S3" s="284"/>
-      <c r="T3" s="284"/>
-      <c r="U3" s="284"/>
-      <c r="V3" s="284"/>
-      <c r="W3" s="284"/>
-      <c r="X3" s="284"/>
-      <c r="Y3" s="284"/>
-      <c r="Z3" s="284"/>
-      <c r="AA3" s="284"/>
-      <c r="AB3" s="284"/>
-      <c r="AC3" s="284"/>
-      <c r="AD3" s="284"/>
-      <c r="AE3" s="284"/>
-      <c r="AF3" s="284"/>
-      <c r="AG3" s="284"/>
-      <c r="AH3" s="284"/>
-      <c r="AI3" s="284"/>
-      <c r="AJ3" s="284"/>
+      <c r="C3" s="271"/>
+      <c r="D3" s="271"/>
+      <c r="E3" s="271"/>
+      <c r="F3" s="271"/>
+      <c r="G3" s="271"/>
+      <c r="H3" s="271"/>
+      <c r="I3" s="271"/>
+      <c r="J3" s="271"/>
+      <c r="K3" s="271"/>
+      <c r="L3" s="271"/>
+      <c r="M3" s="271"/>
+      <c r="N3" s="271"/>
+      <c r="O3" s="271"/>
+      <c r="P3" s="272"/>
+      <c r="Q3" s="272"/>
+      <c r="R3" s="272"/>
+      <c r="S3" s="272"/>
+      <c r="T3" s="272"/>
+      <c r="U3" s="272"/>
+      <c r="V3" s="272"/>
+      <c r="W3" s="272"/>
+      <c r="X3" s="272"/>
+      <c r="Y3" s="272"/>
+      <c r="Z3" s="272"/>
+      <c r="AA3" s="272"/>
+      <c r="AB3" s="272"/>
+      <c r="AC3" s="272"/>
+      <c r="AD3" s="272"/>
+      <c r="AE3" s="272"/>
+      <c r="AF3" s="272"/>
+      <c r="AG3" s="272"/>
+      <c r="AH3" s="272"/>
+      <c r="AI3" s="272"/>
+      <c r="AJ3" s="272"/>
     </row>
     <row r="4" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="267" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="268"/>
-      <c r="E4" s="268"/>
-      <c r="F4" s="268"/>
-      <c r="G4" s="268"/>
-      <c r="H4" s="268"/>
-      <c r="I4" s="268"/>
-      <c r="J4" s="268"/>
-      <c r="K4" s="268"/>
-      <c r="L4" s="268"/>
-      <c r="M4" s="268"/>
-      <c r="N4" s="268"/>
-      <c r="O4" s="268"/>
-      <c r="P4" s="268"/>
-      <c r="Q4" s="268"/>
-      <c r="R4" s="268"/>
-      <c r="S4" s="269"/>
-      <c r="T4" s="267" t="s">
-        <v>1</v>
-      </c>
-      <c r="U4" s="268"/>
-      <c r="V4" s="268"/>
-      <c r="W4" s="268"/>
-      <c r="X4" s="268"/>
-      <c r="Y4" s="268"/>
-      <c r="Z4" s="268"/>
-      <c r="AA4" s="268"/>
-      <c r="AB4" s="269"/>
-      <c r="AC4" s="267" t="s">
+      <c r="C4" s="296" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="297"/>
+      <c r="E4" s="297"/>
+      <c r="F4" s="297"/>
+      <c r="G4" s="297"/>
+      <c r="H4" s="297"/>
+      <c r="I4" s="297"/>
+      <c r="J4" s="297"/>
+      <c r="K4" s="297"/>
+      <c r="L4" s="297"/>
+      <c r="M4" s="297"/>
+      <c r="N4" s="297"/>
+      <c r="O4" s="297"/>
+      <c r="P4" s="297"/>
+      <c r="Q4" s="297"/>
+      <c r="R4" s="297"/>
+      <c r="S4" s="298"/>
+      <c r="T4" s="296" t="s">
+        <v>1</v>
+      </c>
+      <c r="U4" s="297"/>
+      <c r="V4" s="297"/>
+      <c r="W4" s="297"/>
+      <c r="X4" s="297"/>
+      <c r="Y4" s="297"/>
+      <c r="Z4" s="297"/>
+      <c r="AA4" s="297"/>
+      <c r="AB4" s="298"/>
+      <c r="AC4" s="296" t="s">
         <v>2</v>
       </c>
-      <c r="AD4" s="268"/>
-      <c r="AE4" s="268"/>
-      <c r="AF4" s="268"/>
-      <c r="AG4" s="278"/>
-      <c r="AH4" s="267" t="s">
+      <c r="AD4" s="297"/>
+      <c r="AE4" s="297"/>
+      <c r="AF4" s="297"/>
+      <c r="AG4" s="305"/>
+      <c r="AH4" s="296" t="s">
         <v>10</v>
       </c>
-      <c r="AI4" s="268"/>
-      <c r="AJ4" s="269"/>
+      <c r="AI4" s="297"/>
+      <c r="AJ4" s="298"/>
     </row>
     <row r="5" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="279" t="s">
+      <c r="C5" s="265" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="275"/>
-      <c r="E5" s="275"/>
-      <c r="F5" s="275"/>
-      <c r="G5" s="275"/>
-      <c r="H5" s="275"/>
-      <c r="I5" s="275"/>
-      <c r="J5" s="276"/>
-      <c r="K5" s="274" t="s">
+      <c r="D5" s="266"/>
+      <c r="E5" s="266"/>
+      <c r="F5" s="266"/>
+      <c r="G5" s="266"/>
+      <c r="H5" s="266"/>
+      <c r="I5" s="266"/>
+      <c r="J5" s="267"/>
+      <c r="K5" s="303" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="275"/>
-      <c r="M5" s="275"/>
-      <c r="N5" s="275"/>
-      <c r="O5" s="275"/>
-      <c r="P5" s="275"/>
-      <c r="Q5" s="275"/>
-      <c r="R5" s="276"/>
-      <c r="S5" s="270" t="s">
+      <c r="L5" s="266"/>
+      <c r="M5" s="266"/>
+      <c r="N5" s="266"/>
+      <c r="O5" s="266"/>
+      <c r="P5" s="266"/>
+      <c r="Q5" s="266"/>
+      <c r="R5" s="267"/>
+      <c r="S5" s="299" t="s">
         <v>12</v>
       </c>
-      <c r="T5" s="279" t="s">
+      <c r="T5" s="265" t="s">
         <v>9</v>
       </c>
-      <c r="U5" s="275"/>
-      <c r="V5" s="275"/>
-      <c r="W5" s="276"/>
-      <c r="X5" s="274" t="s">
+      <c r="U5" s="266"/>
+      <c r="V5" s="266"/>
+      <c r="W5" s="267"/>
+      <c r="X5" s="303" t="s">
         <v>8</v>
       </c>
-      <c r="Y5" s="275"/>
-      <c r="Z5" s="275"/>
-      <c r="AA5" s="276"/>
-      <c r="AB5" s="270" t="s">
+      <c r="Y5" s="266"/>
+      <c r="Z5" s="266"/>
+      <c r="AA5" s="267"/>
+      <c r="AB5" s="299" t="s">
         <v>13</v>
       </c>
-      <c r="AC5" s="277" t="s">
+      <c r="AC5" s="304" t="s">
         <v>9</v>
       </c>
-      <c r="AD5" s="276"/>
-      <c r="AE5" s="274" t="s">
+      <c r="AD5" s="267"/>
+      <c r="AE5" s="303" t="s">
         <v>8</v>
       </c>
-      <c r="AF5" s="276"/>
-      <c r="AG5" s="270" t="s">
+      <c r="AF5" s="267"/>
+      <c r="AG5" s="299" t="s">
         <v>14</v>
       </c>
       <c r="AH5" s="56"/>
       <c r="AI5" s="25"/>
-      <c r="AJ5" s="270" t="s">
+      <c r="AJ5" s="299" t="s">
         <v>15</v>
       </c>
       <c r="AK5" s="4"/>
@@ -4177,14 +4168,14 @@
         <f>Résultats!$J$28</f>
         <v>3</v>
       </c>
-      <c r="S6" s="271"/>
+      <c r="S6" s="300"/>
       <c r="T6" s="156">
         <f>Résultats!$V$6</f>
         <v>1</v>
       </c>
       <c r="U6" s="103">
         <f>Résultats!$V$7</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V6" s="159">
         <f>Résultats!$V$10</f>
@@ -4192,15 +4183,15 @@
       </c>
       <c r="W6" s="103">
         <f>Résultats!$V$11</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X6" s="105">
         <f>Résultats!$V$20</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y6" s="104">
         <f>Résultats!$V$21</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z6" s="106">
         <f>Résultats!$V$24</f>
@@ -4208,9 +4199,9 @@
       </c>
       <c r="AA6" s="103">
         <f>Résultats!$V$25</f>
-        <v>0</v>
-      </c>
-      <c r="AB6" s="271"/>
+        <v>1</v>
+      </c>
+      <c r="AB6" s="300"/>
       <c r="AC6" s="106">
         <f>Résultats!$AH$8</f>
         <v>0</v>
@@ -4227,7 +4218,7 @@
         <f>Résultats!$AH$23</f>
         <v>0</v>
       </c>
-      <c r="AG6" s="271"/>
+      <c r="AG6" s="300"/>
       <c r="AH6" s="198">
         <f>Résultats!$AH$15</f>
         <v>0</v>
@@ -4236,7 +4227,7 @@
         <f>Résultats!$AH$16</f>
         <v>0</v>
       </c>
-      <c r="AJ6" s="271"/>
+      <c r="AJ6" s="300"/>
       <c r="AK6" s="37"/>
     </row>
     <row r="7" spans="1:38" s="39" customFormat="1" ht="58.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -4262,7 +4253,7 @@
       <c r="P7" s="230"/>
       <c r="Q7" s="234"/>
       <c r="R7" s="112"/>
-      <c r="S7" s="271"/>
+      <c r="S7" s="300"/>
       <c r="T7" s="157"/>
       <c r="U7" s="112"/>
       <c r="V7" s="160"/>
@@ -4271,15 +4262,15 @@
       <c r="Y7" s="113"/>
       <c r="Z7" s="114"/>
       <c r="AA7" s="112"/>
-      <c r="AB7" s="271"/>
+      <c r="AB7" s="300"/>
       <c r="AC7" s="114"/>
       <c r="AD7" s="112"/>
       <c r="AE7" s="115"/>
       <c r="AF7" s="112"/>
-      <c r="AG7" s="271"/>
+      <c r="AG7" s="300"/>
       <c r="AH7" s="198"/>
       <c r="AI7" s="107"/>
-      <c r="AJ7" s="271"/>
+      <c r="AJ7" s="300"/>
       <c r="AK7" s="37"/>
     </row>
     <row r="8" spans="1:38" s="39" customFormat="1" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4349,7 +4340,7 @@
         <f>Résultats!$B$28</f>
         <v>VEGAS</v>
       </c>
-      <c r="S8" s="271"/>
+      <c r="S8" s="300"/>
       <c r="T8" s="158" t="str">
         <f>Résultats!$N$6</f>
         <v>BOSTON</v>
@@ -4382,7 +4373,7 @@
         <f>Résultats!$N$25</f>
         <v>DALLAS</v>
       </c>
-      <c r="AB8" s="271"/>
+      <c r="AB8" s="300"/>
       <c r="AC8" s="164" t="str">
         <f>Résultats!$Z$8</f>
         <v xml:space="preserve"> </v>
@@ -4399,7 +4390,7 @@
         <f>Résultats!$Z$23</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AG8" s="271"/>
+      <c r="AG8" s="300"/>
       <c r="AH8" s="199" t="str">
         <f>Résultats!$Z$15</f>
         <v xml:space="preserve"> </v>
@@ -4408,7 +4399,7 @@
         <f>Résultats!$Z$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ8" s="271"/>
+      <c r="AJ8" s="300"/>
       <c r="AK8" s="37"/>
     </row>
     <row r="9" spans="1:38" s="39" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4482,7 +4473,7 @@
         <f>Résultats!$A$28</f>
         <v>P3</v>
       </c>
-      <c r="S9" s="273"/>
+      <c r="S9" s="302"/>
       <c r="T9" s="166" t="str">
         <f>Résultats!$M$6</f>
         <v>A2</v>
@@ -4515,7 +4506,7 @@
         <f>Résultats!$M$25</f>
         <v>WC1</v>
       </c>
-      <c r="AB9" s="272"/>
+      <c r="AB9" s="301"/>
       <c r="AC9" s="170" t="str">
         <f>Résultats!$Y$8</f>
         <v xml:space="preserve"> </v>
@@ -4532,7 +4523,7 @@
         <f>Résultats!$Y$23</f>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="AG9" s="272"/>
+      <c r="AG9" s="301"/>
       <c r="AH9" s="201" t="str">
         <f>Résultats!$Y$15</f>
         <v xml:space="preserve"> </v>
@@ -4541,7 +4532,7 @@
         <f>Résultats!$Y$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ9" s="273"/>
+      <c r="AJ9" s="302"/>
       <c r="AK9" s="109" t="s">
         <v>51</v>
       </c>
@@ -4611,7 +4602,7 @@
       <c r="AA10" s="180"/>
       <c r="AB10" s="181">
         <f>SUM(T11:AA11)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AC10" s="179"/>
       <c r="AD10" s="176"/>
@@ -4633,7 +4624,7 @@
       </c>
       <c r="AL10" s="181">
         <f>$S10+$AB10+$AG10+$AJ10</f>
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -4685,7 +4676,7 @@
       <c r="S11" s="121"/>
       <c r="T11" s="126">
         <f>(IF($T10&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T10=$T$6+$U$6,$P$103,0),0),0)+IF($U10&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U10=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U11" s="126"/>
       <c r="V11" s="126">
@@ -4695,7 +4686,7 @@
       <c r="W11" s="126"/>
       <c r="X11" s="126">
         <f>(IF($X10&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X10=$X$6+$Y$6,$P$103,0),0),0)+IF($Y10&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y10=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y11" s="59"/>
       <c r="Z11" s="126">
@@ -5062,7 +5053,7 @@
       </c>
       <c r="F14" s="45"/>
       <c r="G14" s="48"/>
-      <c r="H14" s="247">
+      <c r="H14" s="245">
         <v>7</v>
       </c>
       <c r="I14" s="44"/>
@@ -5107,7 +5098,7 @@
       </c>
       <c r="AB14" s="122">
         <f>SUM(T15:AA15)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AC14" s="48"/>
       <c r="AD14" s="47"/>
@@ -5125,11 +5116,11 @@
       </c>
       <c r="AK14" s="111">
         <f>MAX($AL$10:$AL$97) - AL14</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AL14" s="122">
         <f>$S14+$AB14+$AG14+$AJ14</f>
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5181,7 +5172,7 @@
       <c r="S15" s="144"/>
       <c r="T15" s="126">
         <f>(IF($T14&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T14=$T$6+$U$6,$P$103,0),0),0)+IF($U14&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U14=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U15" s="126"/>
       <c r="V15" s="126">
@@ -5191,12 +5182,12 @@
       <c r="W15" s="126"/>
       <c r="X15" s="126">
         <f>(IF($X14&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X14=$X$6+$Y$6,$P$103,0),0),0)+IF($Y14&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y14=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y15" s="59"/>
       <c r="Z15" s="126">
         <f>(IF($Z14&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z14=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA14&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA14=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA15" s="62"/>
       <c r="AB15" s="144"/>
@@ -5210,7 +5201,7 @@
       <c r="AJ15" s="121"/>
       <c r="AK15" s="92">
         <f>MAX($AL$10:$AL$97) - AL15</f>
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="AL15" s="121"/>
     </row>
@@ -5580,7 +5571,7 @@
         <v>5</v>
       </c>
       <c r="P18" s="186"/>
-      <c r="Q18" s="246">
+      <c r="Q18" s="244">
         <v>7</v>
       </c>
       <c r="R18" s="191"/>
@@ -5606,7 +5597,7 @@
       <c r="AA18" s="191"/>
       <c r="AB18" s="192">
         <f>SUM(T19:AA19)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AC18" s="188"/>
       <c r="AD18" s="189"/>
@@ -5628,7 +5619,7 @@
       </c>
       <c r="AL18" s="192">
         <f>$S18+$AB18+$AG18+$AJ18</f>
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5680,7 +5671,7 @@
       <c r="S19" s="144"/>
       <c r="T19" s="126">
         <f>(IF($T18&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T18=$T$6+$U$6,$P$103,0),0),0)+IF($U18&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U18=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U19" s="126"/>
       <c r="V19" s="126">
@@ -5690,7 +5681,7 @@
       <c r="W19" s="126"/>
       <c r="X19" s="126">
         <f>(IF($X18&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X18=$X$6+$Y$6,$P$103,0),0),0)+IF($Y18&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y18=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y19" s="59"/>
       <c r="Z19" s="126">
@@ -5709,7 +5700,7 @@
       <c r="AJ19" s="144"/>
       <c r="AK19" s="150">
         <f>MAX($AL$10:$AL$97) - AL19</f>
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="AL19" s="121"/>
     </row>
@@ -6046,10 +6037,10 @@
     <row r="22" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="117">
         <f>RANK(AL22,$AL$10:$AL$97,)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B22" s="84" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C22" s="46">
         <v>5</v>
@@ -6060,62 +6051,62 @@
       </c>
       <c r="F22" s="45"/>
       <c r="G22" s="48">
+        <v>4</v>
+      </c>
+      <c r="H22" s="47"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="47">
         <v>6</v>
       </c>
-      <c r="H22" s="47"/>
-      <c r="I22" s="44">
+      <c r="K22" s="49">
+        <v>5</v>
+      </c>
+      <c r="L22" s="47"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="239">
         <v>6</v>
       </c>
-      <c r="J22" s="47"/>
-      <c r="K22" s="49">
-        <v>4</v>
-      </c>
-      <c r="L22" s="47"/>
-      <c r="M22" s="44">
-        <v>5</v>
-      </c>
-      <c r="N22" s="45"/>
-      <c r="O22" s="44"/>
-      <c r="P22" s="45">
+      <c r="O22" s="44">
         <v>7</v>
       </c>
-      <c r="Q22" s="48"/>
-      <c r="R22" s="50">
-        <v>7</v>
-      </c>
+      <c r="P22" s="45"/>
+      <c r="Q22" s="48">
+        <v>6</v>
+      </c>
+      <c r="R22" s="50"/>
       <c r="S22" s="122">
         <f>SUM(C23:R23)</f>
-        <v>38</v>
-      </c>
-      <c r="T22" s="46"/>
-      <c r="U22" s="47">
+        <v>37</v>
+      </c>
+      <c r="T22" s="46">
         <v>6</v>
       </c>
-      <c r="V22" s="44">
+      <c r="U22" s="47"/>
+      <c r="V22" s="44"/>
+      <c r="W22" s="47">
+        <v>6</v>
+      </c>
+      <c r="X22" s="49">
         <v>5</v>
       </c>
-      <c r="W22" s="47"/>
-      <c r="X22" s="49"/>
-      <c r="Y22" s="45">
-        <v>5</v>
-      </c>
-      <c r="Z22" s="48">
+      <c r="Y22" s="45"/>
+      <c r="Z22" s="48"/>
+      <c r="AA22" s="50">
         <v>7</v>
       </c>
-      <c r="AA22" s="50"/>
       <c r="AB22" s="122">
         <f>SUM(T23:AA23)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AC22" s="48"/>
-      <c r="AD22" s="243"/>
+      <c r="AD22" s="47"/>
       <c r="AE22" s="49"/>
       <c r="AF22" s="47"/>
       <c r="AG22" s="122">
         <f>SUM(AC23:AF23)</f>
         <v>0</v>
       </c>
-      <c r="AH22" s="310"/>
+      <c r="AH22" s="306"/>
       <c r="AI22" s="57"/>
       <c r="AJ22" s="122">
         <f>AH23</f>
@@ -6123,11 +6114,11 @@
       </c>
       <c r="AK22" s="111">
         <f>MAX($AL$10:$AL$97) - AL22</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AL22" s="122">
         <f>$S22+$AB22+$AG22+$AJ22</f>
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6153,7 +6144,7 @@
       <c r="H23" s="151"/>
       <c r="I23" s="125">
         <f>(IF($I22&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I22=$I$6+$J$6,$O$103,0),0),0)+IF($J22&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J22=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J23" s="152"/>
       <c r="K23" s="153">
@@ -6163,33 +6154,33 @@
       <c r="L23" s="151"/>
       <c r="M23" s="125">
         <f>(IF($M22&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M22=$M$6+$N$6,$O$103,0),0),0)+IF($N22&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N22=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="N23" s="151"/>
       <c r="O23" s="125">
         <f>(IF($O22&lt;&gt;"",($O$6*$O$104)+IF($O$6=4,($O$102)+IF($O22=$O$6+$P$6,$O$103,0),0),0)+IF($P22&lt;&gt;"",($P$6*$O$104)+IF($P$6=4,($O$102)+IF($P22=$O$6+$P$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="P23" s="151"/>
       <c r="Q23" s="125">
         <f>(IF($Q22&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q22=$Q$6+$R$6,$O$103,0),0),0)+IF($R22&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R22=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="R23" s="154"/>
       <c r="S23" s="144"/>
       <c r="T23" s="126">
         <f>(IF($T22&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T22=$T$6+$U$6,$P$103,0),0),0)+IF($U22&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U22=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U23" s="126"/>
       <c r="V23" s="126">
         <f>(IF($V22&lt;&gt;"",($V$6*$P$104)+IF($V$6=4,($P$102)+IF($V22=$V$6+$W$6,$P$103,0),0),0)+IF($W22&lt;&gt;"",($W$6*$P$104)+IF($W$6=4,($P$102)+IF($W22=$V$6+$W$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W23" s="126"/>
       <c r="X23" s="126">
         <f>(IF($X22&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X22=$X$6+$Y$6,$P$103,0),0),0)+IF($Y22&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y22=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y23" s="59"/>
       <c r="Z23" s="126">
@@ -6208,7 +6199,7 @@
       <c r="AJ23" s="144"/>
       <c r="AK23" s="150">
         <f>MAX($AL$10:$AL$97) - AL23</f>
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="AL23" s="121"/>
     </row>
@@ -6257,7 +6248,7 @@
         <f>IF(ISBLANK(I22),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" s="118">
         <f>IF(ISBLANK(J22),
@@ -6287,7 +6278,7 @@
         <f>IF(ISBLANK(N22),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O24" s="118">
         <f>IF(ISBLANK(O22),
@@ -6299,13 +6290,13 @@
         <f>IF(ISBLANK(P22),
 0,
 IF(P$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q24" s="118">
         <f>IF(ISBLANK(Q22),
 0,
 IF(Q$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R24" s="118">
         <f>IF(ISBLANK(R22),
@@ -6452,7 +6443,7 @@
         <f>IF(N24 = 0,
 0,
 IF(N22 = (M$6+N$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O25" s="118">
         <f>IF(O24 = 0,
@@ -6538,7 +6529,7 @@
       <c r="AJ25" s="138"/>
       <c r="AK25" s="139">
         <f>SUM(C25:AI25)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL25" s="123"/>
     </row>
@@ -6548,7 +6539,7 @@
         <v>5</v>
       </c>
       <c r="B26" s="197" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C26" s="185">
         <v>5</v>
@@ -6559,62 +6550,62 @@
       </c>
       <c r="F26" s="186"/>
       <c r="G26" s="188">
+        <v>6</v>
+      </c>
+      <c r="H26" s="189"/>
+      <c r="I26" s="187">
+        <v>6</v>
+      </c>
+      <c r="J26" s="189"/>
+      <c r="K26" s="190">
         <v>4</v>
       </c>
-      <c r="H26" s="189"/>
-      <c r="I26" s="187"/>
-      <c r="J26" s="189">
-        <v>6</v>
-      </c>
-      <c r="K26" s="190">
+      <c r="L26" s="189"/>
+      <c r="M26" s="187">
         <v>5</v>
       </c>
-      <c r="L26" s="189"/>
-      <c r="M26" s="187"/>
-      <c r="N26" s="240">
-        <v>6</v>
-      </c>
-      <c r="O26" s="187">
+      <c r="N26" s="186"/>
+      <c r="O26" s="187"/>
+      <c r="P26" s="186">
         <v>7</v>
       </c>
-      <c r="P26" s="186"/>
-      <c r="Q26" s="188">
-        <v>6</v>
-      </c>
-      <c r="R26" s="191"/>
+      <c r="Q26" s="188"/>
+      <c r="R26" s="191">
+        <v>7</v>
+      </c>
       <c r="S26" s="192">
         <f>SUM(C27:R27)</f>
-        <v>37</v>
-      </c>
-      <c r="T26" s="185">
+        <v>38</v>
+      </c>
+      <c r="T26" s="185"/>
+      <c r="U26" s="189">
         <v>6</v>
       </c>
-      <c r="U26" s="189"/>
-      <c r="V26" s="187"/>
-      <c r="W26" s="189">
-        <v>6</v>
-      </c>
-      <c r="X26" s="190">
+      <c r="V26" s="187">
         <v>5</v>
       </c>
-      <c r="Y26" s="186"/>
-      <c r="Z26" s="188"/>
-      <c r="AA26" s="191">
+      <c r="W26" s="189"/>
+      <c r="X26" s="190"/>
+      <c r="Y26" s="186">
+        <v>5</v>
+      </c>
+      <c r="Z26" s="188">
         <v>7</v>
       </c>
+      <c r="AA26" s="191"/>
       <c r="AB26" s="192">
         <f>SUM(T27:AA27)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AC26" s="188"/>
-      <c r="AD26" s="189"/>
+      <c r="AD26" s="307"/>
       <c r="AE26" s="190"/>
       <c r="AF26" s="189"/>
       <c r="AG26" s="192">
         <f>SUM(AC27:AF27)</f>
         <v>0</v>
       </c>
-      <c r="AH26" s="311"/>
+      <c r="AH26" s="182"/>
       <c r="AI26" s="183"/>
       <c r="AJ26" s="192">
         <f>AH27</f>
@@ -6622,11 +6613,11 @@
       </c>
       <c r="AK26" s="194">
         <f>MAX($AL$10:$AL$97) - AL26</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AL26" s="192">
         <f>$S26+$AB26+$AG26+$AJ26</f>
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6652,7 +6643,7 @@
       <c r="H27" s="140"/>
       <c r="I27" s="120">
         <f>(IF($I26&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I26=$I$6+$J$6,$O$103,0),0),0)+IF($J26&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J26=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J27" s="141"/>
       <c r="K27" s="142">
@@ -6662,17 +6653,17 @@
       <c r="L27" s="140"/>
       <c r="M27" s="120">
         <f>(IF($M26&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M26=$M$6+$N$6,$O$103,0),0),0)+IF($N26&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N26=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="N27" s="140"/>
       <c r="O27" s="120">
         <f>(IF($O26&lt;&gt;"",($O$6*$O$104)+IF($O$6=4,($O$102)+IF($O26=$O$6+$P$6,$O$103,0),0),0)+IF($P26&lt;&gt;"",($P$6*$O$104)+IF($P$6=4,($O$102)+IF($P26=$O$6+$P$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="P27" s="140"/>
       <c r="Q27" s="120">
         <f>(IF($Q26&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q26=$Q$6+$R$6,$O$103,0),0),0)+IF($R26&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R26=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="R27" s="143"/>
       <c r="S27" s="144"/>
@@ -6688,12 +6679,12 @@
       <c r="W27" s="126"/>
       <c r="X27" s="126">
         <f>(IF($X26&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X26=$X$6+$Y$6,$P$103,0),0),0)+IF($Y26&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y26=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y27" s="59"/>
       <c r="Z27" s="126">
         <f>(IF($Z26&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z26=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA26&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA26=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA27" s="62"/>
       <c r="AB27" s="155"/>
@@ -6707,7 +6698,7 @@
       <c r="AJ27" s="144"/>
       <c r="AK27" s="150">
         <f>MAX($AL$10:$AL$97) - AL27</f>
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="AL27" s="121"/>
     </row>
@@ -6756,7 +6747,7 @@
         <f>IF(ISBLANK(I26),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" s="118">
         <f>IF(ISBLANK(J26),
@@ -6786,7 +6777,7 @@
         <f>IF(ISBLANK(N26),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O28" s="118">
         <f>IF(ISBLANK(O26),
@@ -6798,13 +6789,13 @@
         <f>IF(ISBLANK(P26),
 0,
 IF(P$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q28" s="118">
         <f>IF(ISBLANK(Q26),
 0,
 IF(Q$6= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R28" s="118">
         <f>IF(ISBLANK(R26),
@@ -6951,7 +6942,7 @@
         <f>IF(N28 = 0,
 0,
 IF(N26 = (M$6+N$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O29" s="118">
         <f>IF(O28 = 0,
@@ -7037,7 +7028,7 @@
       <c r="AJ29" s="138"/>
       <c r="AK29" s="139">
         <f>SUM(C29:AI29)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AL29" s="123"/>
     </row>
@@ -7047,26 +7038,26 @@
         <v>6</v>
       </c>
       <c r="B30" s="84" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C30" s="46">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D30" s="45"/>
       <c r="E30" s="44">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F30" s="45"/>
-      <c r="G30" s="48">
+      <c r="G30" s="48"/>
+      <c r="H30" s="245">
         <v>7</v>
       </c>
-      <c r="H30" s="47"/>
       <c r="I30" s="44"/>
       <c r="J30" s="47">
         <v>6</v>
       </c>
       <c r="K30" s="49">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L30" s="47"/>
       <c r="M30" s="44"/>
@@ -7074,13 +7065,13 @@
         <v>7</v>
       </c>
       <c r="O30" s="44">
+        <v>5</v>
+      </c>
+      <c r="P30" s="45"/>
+      <c r="Q30" s="48"/>
+      <c r="R30" s="50">
         <v>6</v>
       </c>
-      <c r="P30" s="45"/>
-      <c r="Q30" s="242">
-        <v>7</v>
-      </c>
-      <c r="R30" s="50"/>
       <c r="S30" s="122">
         <f>SUM(C31:R31)</f>
         <v>35</v>
@@ -7089,21 +7080,21 @@
       <c r="U30" s="47">
         <v>7</v>
       </c>
-      <c r="V30" s="44">
+      <c r="V30" s="44"/>
+      <c r="W30" s="47">
+        <v>7</v>
+      </c>
+      <c r="X30" s="49">
         <v>6</v>
       </c>
-      <c r="W30" s="47"/>
-      <c r="X30" s="49"/>
-      <c r="Y30" s="45">
-        <v>7</v>
-      </c>
+      <c r="Y30" s="45"/>
       <c r="Z30" s="48">
         <v>6</v>
       </c>
       <c r="AA30" s="47"/>
       <c r="AB30" s="122">
         <f>SUM(T31:AA31)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AC30" s="48"/>
       <c r="AD30" s="47"/>
@@ -7121,11 +7112,11 @@
       </c>
       <c r="AK30" s="111">
         <f>MAX($AL$10:$AL$97) - AL30</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AL30" s="122">
         <f>$S30+$AB30+$AG30+$AJ30</f>
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7146,7 +7137,7 @@
       <c r="F31" s="76"/>
       <c r="G31" s="77">
         <f>(IF($G30&lt;&gt;"",($G$6*$O$104)+IF($G$6=4,($O$102)+IF($G30=$G$6+$H$6,$O$103,0),0),0)+IF($H30&lt;&gt;"",($H$6*$O$104)+IF($H$6=4,($O$102)+IF($H30=$G$6+$H$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="H31" s="76"/>
       <c r="I31" s="77">
@@ -7171,23 +7162,23 @@
       <c r="P31" s="76"/>
       <c r="Q31" s="77">
         <f>(IF($Q30&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q30=$Q$6+$R$6,$O$103,0),0),0)+IF($R30&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R30=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="R31" s="80"/>
       <c r="S31" s="121"/>
       <c r="T31" s="126">
         <f>(IF($T30&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T30=$T$6+$U$6,$P$103,0),0),0)+IF($U30&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U30=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U31" s="126"/>
       <c r="V31" s="126">
         <f>(IF($V30&lt;&gt;"",($V$6*$P$104)+IF($V$6=4,($P$102)+IF($V30=$V$6+$W$6,$P$103,0),0),0)+IF($W30&lt;&gt;"",($W$6*$P$104)+IF($W$6=4,($P$102)+IF($W30=$V$6+$W$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W31" s="126"/>
       <c r="X31" s="126">
         <f>(IF($X30&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X30=$X$6+$Y$6,$P$103,0),0),0)+IF($Y30&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y30=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y31" s="59"/>
       <c r="Z31" s="126">
@@ -7206,7 +7197,7 @@
       <c r="AJ31" s="121"/>
       <c r="AK31" s="92">
         <f>MAX($AL$10:$AL$97) - AL31</f>
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="AL31" s="121"/>
     </row>
@@ -7249,7 +7240,7 @@
         <f>IF(ISBLANK(H30),
 0,
 IF(H$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32" s="118">
         <f>IF(ISBLANK(I30),
@@ -7303,7 +7294,7 @@
         <f>IF(ISBLANK(Q30),
 0,
 IF(Q$6= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R32" s="118">
         <f>IF(ISBLANK(R30),
@@ -7414,7 +7405,7 @@
         <f>IF(H32 = 0,
 0,
 IF(H30 = (G$6+H$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33" s="118">
         <f>IF(I32 = 0,
@@ -7468,7 +7459,7 @@
         <f>IF(Q32 = 0,
 0,
 IF(Q30 = (Q$6+R$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R33" s="118">
         <f>IF(R32 = 0,
@@ -7543,29 +7534,29 @@
     <row r="34" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="173">
         <f>RANK(AL34,$AL$10:$AL$97,)</f>
+        <v>7</v>
+      </c>
+      <c r="B34" s="197" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" s="185">
         <v>6</v>
-      </c>
-      <c r="B34" s="197" t="s">
-        <v>73</v>
-      </c>
-      <c r="C34" s="185">
-        <v>5</v>
       </c>
       <c r="D34" s="186"/>
       <c r="E34" s="187">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F34" s="186"/>
-      <c r="G34" s="188"/>
-      <c r="H34" s="248">
+      <c r="G34" s="188">
         <v>7</v>
       </c>
+      <c r="H34" s="189"/>
       <c r="I34" s="187"/>
       <c r="J34" s="189">
         <v>6</v>
       </c>
       <c r="K34" s="190">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L34" s="189"/>
       <c r="M34" s="187"/>
@@ -7573,13 +7564,13 @@
         <v>7</v>
       </c>
       <c r="O34" s="187">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P34" s="186"/>
-      <c r="Q34" s="188"/>
-      <c r="R34" s="191">
-        <v>6</v>
-      </c>
+      <c r="Q34" s="244">
+        <v>7</v>
+      </c>
+      <c r="R34" s="191"/>
       <c r="S34" s="192">
         <f>SUM(C35:R35)</f>
         <v>35</v>
@@ -7588,21 +7579,21 @@
       <c r="U34" s="189">
         <v>7</v>
       </c>
-      <c r="V34" s="187"/>
-      <c r="W34" s="189">
+      <c r="V34" s="187">
+        <v>6</v>
+      </c>
+      <c r="W34" s="189"/>
+      <c r="X34" s="190"/>
+      <c r="Y34" s="186">
         <v>7</v>
       </c>
-      <c r="X34" s="190">
-        <v>6</v>
-      </c>
-      <c r="Y34" s="186"/>
       <c r="Z34" s="188">
         <v>6</v>
       </c>
       <c r="AA34" s="189"/>
       <c r="AB34" s="192">
         <f>SUM(T35:AA35)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AC34" s="188"/>
       <c r="AD34" s="189"/>
@@ -7624,7 +7615,7 @@
       </c>
       <c r="AL34" s="192">
         <f>$S34+$AB34+$AG34+$AJ34</f>
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7645,7 +7636,7 @@
       <c r="F35" s="76"/>
       <c r="G35" s="77">
         <f>(IF($G34&lt;&gt;"",($G$6*$O$104)+IF($G$6=4,($O$102)+IF($G34=$G$6+$H$6,$O$103,0),0),0)+IF($H34&lt;&gt;"",($H$6*$O$104)+IF($H$6=4,($O$102)+IF($H34=$G$6+$H$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="H35" s="76"/>
       <c r="I35" s="77">
@@ -7670,13 +7661,13 @@
       <c r="P35" s="76"/>
       <c r="Q35" s="77">
         <f>(IF($Q34&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q34=$Q$6+$R$6,$O$103,0),0),0)+IF($R34&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R34=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="R35" s="80"/>
       <c r="S35" s="121"/>
       <c r="T35" s="126">
         <f>(IF($T34&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T34=$T$6+$U$6,$P$103,0),0),0)+IF($U34&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U34=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U35" s="126"/>
       <c r="V35" s="126">
@@ -7686,7 +7677,7 @@
       <c r="W35" s="126"/>
       <c r="X35" s="126">
         <f>(IF($X34&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X34=$X$6+$Y$6,$P$103,0),0),0)+IF($Y34&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y34=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y35" s="59"/>
       <c r="Z35" s="126">
@@ -7705,7 +7696,7 @@
       <c r="AJ35" s="121"/>
       <c r="AK35" s="92">
         <f>MAX($AL$10:$AL$97) - AL35</f>
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="AL35" s="121"/>
     </row>
@@ -7748,7 +7739,7 @@
         <f>IF(ISBLANK(H34),
 0,
 IF(H$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I36" s="118">
         <f>IF(ISBLANK(I34),
@@ -7802,7 +7793,7 @@
         <f>IF(ISBLANK(Q34),
 0,
 IF(Q$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R36" s="118">
         <f>IF(ISBLANK(R34),
@@ -7913,7 +7904,7 @@
         <f>IF(H36 = 0,
 0,
 IF(H34 = (G$6+H$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I37" s="118">
         <f>IF(I36 = 0,
@@ -7967,7 +7958,7 @@
         <f>IF(Q36 = 0,
 0,
 IF(Q34 = (Q$6+R$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R37" s="118">
         <f>IF(R36 = 0,
@@ -8051,15 +8042,15 @@
         <v>7</v>
       </c>
       <c r="D38" s="45"/>
-      <c r="E38" s="244">
+      <c r="E38" s="242">
         <v>6</v>
       </c>
       <c r="F38" s="45"/>
-      <c r="G38" s="245"/>
+      <c r="G38" s="243"/>
       <c r="H38" s="47">
         <v>6</v>
       </c>
-      <c r="I38" s="244"/>
+      <c r="I38" s="242"/>
       <c r="J38" s="47">
         <v>7</v>
       </c>
@@ -8101,7 +8092,7 @@
       <c r="AA38" s="47"/>
       <c r="AB38" s="122">
         <f>SUM(T39:AA39)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AC38" s="48"/>
       <c r="AD38" s="47"/>
@@ -8119,11 +8110,11 @@
       </c>
       <c r="AK38" s="111">
         <f>MAX($AL$10:$AL$97) - AL38</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AL38" s="122">
         <f>$S38+$AB38+$AG38+$AJ38</f>
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -8175,17 +8166,17 @@
       <c r="S39" s="121"/>
       <c r="T39" s="126">
         <f>(IF($T38&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T38=$T$6+$U$6,$P$103,0),0),0)+IF($U38&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U38=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U39" s="126"/>
       <c r="V39" s="126">
         <f>(IF($V38&lt;&gt;"",($V$6*$P$104)+IF($V$6=4,($P$102)+IF($V38=$V$6+$W$6,$P$103,0),0),0)+IF($W38&lt;&gt;"",($W$6*$P$104)+IF($W$6=4,($P$102)+IF($W38=$V$6+$W$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W39" s="126"/>
       <c r="X39" s="126">
         <f>(IF($X38&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X38=$X$6+$Y$6,$P$103,0),0),0)+IF($Y38&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y38=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y39" s="59"/>
       <c r="Z39" s="126">
@@ -8204,7 +8195,7 @@
       <c r="AJ39" s="121"/>
       <c r="AK39" s="92">
         <f>MAX($AL$10:$AL$97) - AL39</f>
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="AL39" s="121"/>
     </row>
@@ -8544,34 +8535,34 @@
         <v>9</v>
       </c>
       <c r="B42" s="197" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C42" s="185">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D42" s="186"/>
-      <c r="E42" s="187">
-        <v>4</v>
-      </c>
-      <c r="F42" s="186"/>
+      <c r="E42" s="187"/>
+      <c r="F42" s="186">
+        <v>7</v>
+      </c>
       <c r="G42" s="188">
         <v>6</v>
       </c>
       <c r="H42" s="189"/>
-      <c r="I42" s="187">
+      <c r="I42" s="187"/>
+      <c r="J42" s="189">
         <v>6</v>
       </c>
-      <c r="J42" s="189"/>
-      <c r="K42" s="190">
-        <v>7</v>
-      </c>
-      <c r="L42" s="189"/>
-      <c r="M42" s="187">
+      <c r="K42" s="190"/>
+      <c r="L42" s="189">
+        <v>6</v>
+      </c>
+      <c r="M42" s="187"/>
+      <c r="N42" s="240">
+        <v>6</v>
+      </c>
+      <c r="O42" s="187">
         <v>5</v>
-      </c>
-      <c r="N42" s="186"/>
-      <c r="O42" s="187">
-        <v>4</v>
       </c>
       <c r="P42" s="186"/>
       <c r="Q42" s="188"/>
@@ -8580,27 +8571,27 @@
       </c>
       <c r="S42" s="192">
         <f>SUM(C43:R43)</f>
-        <v>29</v>
-      </c>
-      <c r="T42" s="185">
+        <v>31</v>
+      </c>
+      <c r="T42" s="185"/>
+      <c r="U42" s="189">
+        <v>5</v>
+      </c>
+      <c r="V42" s="187">
         <v>6</v>
       </c>
-      <c r="U42" s="189"/>
-      <c r="V42" s="187">
-        <v>5</v>
-      </c>
       <c r="W42" s="189"/>
-      <c r="X42" s="190"/>
-      <c r="Y42" s="186">
-        <v>7</v>
-      </c>
-      <c r="Z42" s="188">
+      <c r="X42" s="190">
         <v>6</v>
       </c>
-      <c r="AA42" s="189"/>
+      <c r="Y42" s="186"/>
+      <c r="Z42" s="188"/>
+      <c r="AA42" s="189">
+        <v>6</v>
+      </c>
       <c r="AB42" s="192">
         <f>SUM(T43:AA43)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AC42" s="188"/>
       <c r="AD42" s="189"/>
@@ -8618,11 +8609,11 @@
       </c>
       <c r="AK42" s="194">
         <f>MAX($AL$10:$AL$97) - AL42</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AL42" s="192">
         <f>$S42+$AB42+$AG42+$AJ42</f>
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="43" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -8638,7 +8629,7 @@
       <c r="D43" s="76"/>
       <c r="E43" s="116">
         <f>(IF($E42&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E42=$E$6+$F$6,$O$103,0),0),0)+IF($F42&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F42=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F43" s="76"/>
       <c r="G43" s="77">
@@ -8648,17 +8639,17 @@
       <c r="H43" s="76"/>
       <c r="I43" s="116">
         <f>(IF($I42&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I42=$I$6+$J$6,$O$103,0),0),0)+IF($J42&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J42=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J43" s="78"/>
       <c r="K43" s="79">
         <f>(IF($K42&lt;&gt;"",($K$6*$O$104)+IF($K$6=4,($O$102)+IF($K42=$K$6+$L$6,$O$103,0),0),0)+IF($L42&lt;&gt;"",($L$6*$O$104)+IF($L$6=4,($O$102)+IF($L42=$K$6+$L$6,$O$103,0),0),0))</f>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="L43" s="76"/>
       <c r="M43" s="77">
         <f>(IF($M42&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M42=$M$6+$N$6,$O$103,0),0),0)+IF($N42&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N42=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="N43" s="151"/>
       <c r="O43" s="77">
@@ -8684,7 +8675,7 @@
       <c r="W43" s="126"/>
       <c r="X43" s="126">
         <f>(IF($X42&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X42=$X$6+$Y$6,$P$103,0),0),0)+IF($Y42&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y42=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y43" s="59"/>
       <c r="Z43" s="126">
@@ -8703,7 +8694,7 @@
       <c r="AJ43" s="121"/>
       <c r="AK43" s="111">
         <f>MAX($AL$10:$AL$97) - AL43</f>
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="AL43" s="121"/>
     </row>
@@ -8728,7 +8719,7 @@
         <f>IF(ISBLANK(E42),
 0,
 IF(E$6= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44" s="118">
         <f>IF(ISBLANK(F42),
@@ -8752,7 +8743,7 @@
         <f>IF(ISBLANK(I42),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J44" s="118">
         <f>IF(ISBLANK(J42),
@@ -8770,7 +8761,7 @@
         <f>IF(ISBLANK(L42),
 0,
 IF(L$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M44" s="118">
         <f>IF(ISBLANK(M42),
@@ -8782,7 +8773,7 @@
         <f>IF(ISBLANK(N42),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O44" s="118">
         <f>IF(ISBLANK(O42),
@@ -8947,7 +8938,7 @@
         <f>IF(N44 = 0,
 0,
 IF(N42 = (M$6+N$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O45" s="118">
         <f>IF(O44 = 0,
@@ -9033,44 +9024,44 @@
       <c r="AJ45" s="138"/>
       <c r="AK45" s="139">
         <f>SUM(C45:AI45)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL45" s="123"/>
     </row>
     <row r="46" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="117">
         <f>RANK(AL46,$AL$10:$AL$97,)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B46" s="84" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="C46" s="46">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D46" s="45"/>
       <c r="E46" s="44">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" s="45"/>
       <c r="G46" s="48">
+        <v>6</v>
+      </c>
+      <c r="H46" s="47"/>
+      <c r="I46" s="44">
+        <v>6</v>
+      </c>
+      <c r="J46" s="47"/>
+      <c r="K46" s="49">
+        <v>7</v>
+      </c>
+      <c r="L46" s="47"/>
+      <c r="M46" s="44">
         <v>5</v>
       </c>
-      <c r="H46" s="47"/>
-      <c r="I46" s="44"/>
-      <c r="J46" s="47">
-        <v>6</v>
-      </c>
-      <c r="K46" s="49">
-        <v>5</v>
-      </c>
-      <c r="L46" s="47"/>
-      <c r="M46" s="44"/>
-      <c r="N46" s="239">
-        <v>6</v>
-      </c>
+      <c r="N46" s="45"/>
       <c r="O46" s="44">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P46" s="45"/>
       <c r="Q46" s="48"/>
@@ -9089,17 +9080,17 @@
         <v>5</v>
       </c>
       <c r="W46" s="47"/>
-      <c r="X46" s="49">
+      <c r="X46" s="49"/>
+      <c r="Y46" s="45">
         <v>7</v>
       </c>
-      <c r="Y46" s="45"/>
       <c r="Z46" s="48">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA46" s="47"/>
       <c r="AB46" s="122">
         <f>SUM(T47:AA47)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AC46" s="48"/>
       <c r="AD46" s="47"/>
@@ -9109,7 +9100,7 @@
         <f>SUM(AC47:AF47)</f>
         <v>0</v>
       </c>
-      <c r="AH46" s="250"/>
+      <c r="AH46" s="102"/>
       <c r="AI46" s="57"/>
       <c r="AJ46" s="122">
         <f>AH47</f>
@@ -9117,11 +9108,11 @@
       </c>
       <c r="AK46" s="111">
         <f>MAX($AL$10:$AL$97) - AL46</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AL46" s="122">
         <f>$S46+$AB46+$AG46+$AJ46</f>
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -9147,7 +9138,7 @@
       <c r="H47" s="76"/>
       <c r="I47" s="77">
         <f>(IF($I46&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I46=$I$6+$J$6,$O$103,0),0),0)+IF($J46&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J46=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J47" s="78"/>
       <c r="K47" s="79">
@@ -9157,7 +9148,7 @@
       <c r="L47" s="76"/>
       <c r="M47" s="77">
         <f>(IF($M46&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M46=$M$6+$N$6,$O$103,0),0),0)+IF($N46&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N46=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="N47" s="76"/>
       <c r="O47" s="77">
@@ -9183,7 +9174,7 @@
       <c r="W47" s="126"/>
       <c r="X47" s="126">
         <f>(IF($X46&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X46=$X$6+$Y$6,$P$103,0),0),0)+IF($Y46&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y46=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y47" s="59"/>
       <c r="Z47" s="126">
@@ -9202,7 +9193,7 @@
       <c r="AJ47" s="121"/>
       <c r="AK47" s="111">
         <f>MAX($AL$10:$AL$97) - AL47</f>
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="AL47" s="121"/>
     </row>
@@ -9251,7 +9242,7 @@
         <f>IF(ISBLANK(I46),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J48" s="118">
         <f>IF(ISBLANK(J46),
@@ -9281,7 +9272,7 @@
         <f>IF(ISBLANK(N46),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O48" s="118">
         <f>IF(ISBLANK(O46),
@@ -9446,7 +9437,7 @@
         <f>IF(N48 = 0,
 0,
 IF(N46 = (M$6+N$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O49" s="118">
         <f>IF(O48 = 0,
@@ -9532,38 +9523,38 @@
       <c r="AJ49" s="138"/>
       <c r="AK49" s="139">
         <f>SUM(C49:AI49)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL49" s="123"/>
     </row>
     <row r="50" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="173">
         <f>RANK(AL50,$AL$10:$AL$97,)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B50" s="197" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C50" s="185">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D50" s="186"/>
-      <c r="E50" s="187"/>
-      <c r="F50" s="186">
-        <v>7</v>
-      </c>
+      <c r="E50" s="187">
+        <v>5</v>
+      </c>
+      <c r="F50" s="186"/>
       <c r="G50" s="188">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H50" s="189"/>
       <c r="I50" s="187"/>
       <c r="J50" s="189">
         <v>6</v>
       </c>
-      <c r="K50" s="190"/>
-      <c r="L50" s="189">
-        <v>6</v>
-      </c>
+      <c r="K50" s="190">
+        <v>5</v>
+      </c>
+      <c r="L50" s="189"/>
       <c r="M50" s="187"/>
       <c r="N50" s="240">
         <v>6</v>
@@ -9578,27 +9569,27 @@
       </c>
       <c r="S50" s="192">
         <f>SUM(C51:R51)</f>
-        <v>31</v>
-      </c>
-      <c r="T50" s="185"/>
-      <c r="U50" s="189">
+        <v>29</v>
+      </c>
+      <c r="T50" s="185">
+        <v>6</v>
+      </c>
+      <c r="U50" s="189"/>
+      <c r="V50" s="187">
         <v>5</v>
-      </c>
-      <c r="V50" s="187">
-        <v>6</v>
       </c>
       <c r="W50" s="189"/>
       <c r="X50" s="190">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Y50" s="186"/>
-      <c r="Z50" s="188"/>
-      <c r="AA50" s="189">
-        <v>6</v>
-      </c>
+      <c r="Z50" s="188">
+        <v>7</v>
+      </c>
+      <c r="AA50" s="189"/>
       <c r="AB50" s="192">
         <f>SUM(T51:AA51)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AC50" s="188"/>
       <c r="AD50" s="189"/>
@@ -9608,7 +9599,7 @@
         <f>SUM(AC51:AF51)</f>
         <v>0</v>
       </c>
-      <c r="AH50" s="195"/>
+      <c r="AH50" s="308"/>
       <c r="AI50" s="183"/>
       <c r="AJ50" s="192">
         <f>AH51</f>
@@ -9616,11 +9607,11 @@
       </c>
       <c r="AK50" s="194">
         <f>MAX($AL$10:$AL$97) - AL50</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AL50" s="192">
         <f>$S50+$AB50+$AG50+$AJ50</f>
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -9636,7 +9627,7 @@
       <c r="D51" s="127"/>
       <c r="E51" s="125">
         <f>(IF($E50&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E50=$E$6+$F$6,$O$103,0),0),0)+IF($F50&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F50=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F51" s="127"/>
       <c r="G51" s="125">
@@ -9651,7 +9642,7 @@
       <c r="J51" s="129"/>
       <c r="K51" s="130">
         <f>(IF($K50&lt;&gt;"",($K$6*$O$104)+IF($K$6=4,($O$102)+IF($K50=$K$6+$L$6,$O$103,0),0),0)+IF($L50&lt;&gt;"",($L$6*$O$104)+IF($L$6=4,($O$102)+IF($L50=$K$6+$L$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="L51" s="127"/>
       <c r="M51" s="125">
@@ -9672,7 +9663,7 @@
       <c r="S51" s="121"/>
       <c r="T51" s="126">
         <f>(IF($T50&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T50=$T$6+$U$6,$P$103,0),0),0)+IF($U50&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U50=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U51" s="126"/>
       <c r="V51" s="126">
@@ -9682,12 +9673,12 @@
       <c r="W51" s="126"/>
       <c r="X51" s="126">
         <f>(IF($X50&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X50=$X$6+$Y$6,$P$103,0),0),0)+IF($Y50&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y50=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y51" s="59"/>
       <c r="Z51" s="126">
         <f>(IF($Z50&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z50=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA50&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA50=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA51" s="62"/>
       <c r="AB51" s="121"/>
@@ -9723,7 +9714,7 @@
         <f>IF(ISBLANK(E50),
 0,
 IF(E$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F52" s="118">
         <f>IF(ISBLANK(F50),
@@ -9765,7 +9756,7 @@
         <f>IF(ISBLANK(L50),
 0,
 IF(L$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M52" s="118">
         <f>IF(ISBLANK(M50),
@@ -10035,7 +10026,7 @@
     <row r="54" spans="1:38" s="27" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="117">
         <f>RANK(AL54,$AL$10:$AL$97,)</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B54" s="84" t="s">
         <v>74</v>
@@ -10094,7 +10085,7 @@
       <c r="AA54" s="47"/>
       <c r="AB54" s="122">
         <f>SUM(T55:AA55)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AC54" s="48"/>
       <c r="AD54" s="47"/>
@@ -10116,7 +10107,7 @@
       </c>
       <c r="AL54" s="122">
         <f>$S54+$AB54+$AG54+$AJ54</f>
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="55" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -10168,7 +10159,7 @@
       <c r="S55" s="121"/>
       <c r="T55" s="126">
         <f>(IF($T54&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T54=$T$6+$U$6,$P$103,0),0),0)+IF($U54&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U54=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U55" s="126"/>
       <c r="V55" s="126">
@@ -10178,7 +10169,7 @@
       <c r="W55" s="126"/>
       <c r="X55" s="126">
         <f>(IF($X54&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X54=$X$6+$Y$6,$P$103,0),0),0)+IF($Y54&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y54=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y55" s="59"/>
       <c r="Z55" s="126">
@@ -10590,7 +10581,7 @@
       <c r="AA58" s="189"/>
       <c r="AB58" s="192">
         <f>SUM(T59:AA59)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AC58" s="188"/>
       <c r="AD58" s="189"/>
@@ -10612,7 +10603,7 @@
       </c>
       <c r="AL58" s="192">
         <f>$S58+$AB58+$AG58+$AJ58</f>
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="59" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -10664,7 +10655,7 @@
       <c r="S59" s="121"/>
       <c r="T59" s="126">
         <f>(IF($T58&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T58=$T$6+$U$6,$P$103,0),0),0)+IF($U58&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U58=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U59" s="126"/>
       <c r="V59" s="126">
@@ -10674,7 +10665,7 @@
       <c r="W59" s="126"/>
       <c r="X59" s="126">
         <f>(IF($X58&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X58=$X$6+$Y$6,$P$103,0),0),0)+IF($Y58&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y58=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y59" s="59"/>
       <c r="Z59" s="126">
@@ -11086,7 +11077,7 @@
       <c r="AA62" s="47"/>
       <c r="AB62" s="122">
         <f>SUM(T63:AA63)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AC62" s="48"/>
       <c r="AD62" s="47"/>
@@ -11104,11 +11095,11 @@
       </c>
       <c r="AK62" s="111">
         <f>MAX($AL$10:$AL$97) - AL62</f>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AL62" s="122">
         <f>$S62+$AB62+$AG62+$AJ62</f>
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="63" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11160,17 +11151,17 @@
       <c r="S63" s="121"/>
       <c r="T63" s="126">
         <f>(IF($T62&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T62=$T$6+$U$6,$P$103,0),0),0)+IF($U62&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U62=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U63" s="126"/>
       <c r="V63" s="126">
         <f>(IF($V62&lt;&gt;"",($V$6*$P$104)+IF($V$6=4,($P$102)+IF($V62=$V$6+$W$6,$P$103,0),0),0)+IF($W62&lt;&gt;"",($W$6*$P$104)+IF($W$6=4,($P$102)+IF($W62=$V$6+$W$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W63" s="126"/>
       <c r="X63" s="126">
         <f>(IF($X62&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X62=$X$6+$Y$6,$P$103,0),0),0)+IF($Y62&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y62=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y63" s="59"/>
       <c r="Z63" s="126">
@@ -11526,14 +11517,14 @@
         <v>15</v>
       </c>
       <c r="B66" s="197" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C66" s="185">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D66" s="186"/>
       <c r="E66" s="187">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F66" s="186"/>
       <c r="G66" s="188">
@@ -11549,7 +11540,7 @@
       </c>
       <c r="L66" s="189"/>
       <c r="M66" s="187">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="N66" s="186"/>
       <c r="O66" s="187">
@@ -11558,34 +11549,34 @@
       <c r="P66" s="186"/>
       <c r="Q66" s="188"/>
       <c r="R66" s="191">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S66" s="192">
         <f>SUM(C67:R67)</f>
         <v>20</v>
       </c>
-      <c r="T66" s="185">
+      <c r="T66" s="185"/>
+      <c r="U66" s="189">
+        <v>6</v>
+      </c>
+      <c r="V66" s="187"/>
+      <c r="W66" s="189">
         <v>7</v>
       </c>
-      <c r="U66" s="189"/>
-      <c r="V66" s="187">
+      <c r="X66" s="190"/>
+      <c r="Y66" s="186">
         <v>7</v>
       </c>
-      <c r="W66" s="189"/>
-      <c r="X66" s="190">
-        <v>7</v>
-      </c>
-      <c r="Y66" s="186"/>
       <c r="Z66" s="188">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA66" s="189"/>
       <c r="AB66" s="192">
         <f>SUM(T67:AA67)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AC66" s="188"/>
-      <c r="AD66" s="189"/>
+      <c r="AD66" s="307"/>
       <c r="AE66" s="190"/>
       <c r="AF66" s="189"/>
       <c r="AG66" s="192">
@@ -11600,11 +11591,11 @@
       </c>
       <c r="AK66" s="194">
         <f>MAX($AL$10:$AL$97) - AL66</f>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AL66" s="192">
         <f>$S66+$AB66+$AG66+$AJ66</f>
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="67" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11661,12 +11652,12 @@
       <c r="U67" s="126"/>
       <c r="V67" s="126">
         <f>(IF($V66&lt;&gt;"",($V$6*$P$104)+IF($V$6=4,($P$102)+IF($V66=$V$6+$W$6,$P$103,0),0),0)+IF($W66&lt;&gt;"",($W$6*$P$104)+IF($W$6=4,($P$102)+IF($W66=$V$6+$W$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W67" s="126"/>
       <c r="X67" s="126">
         <f>(IF($X66&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X66=$X$6+$Y$6,$P$103,0),0),0)+IF($Y66&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y66=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y67" s="59"/>
       <c r="Z67" s="126">
@@ -12019,17 +12010,17 @@
     <row r="70" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="117">
         <f>RANK(AL70,$AL$10:$AL$97,)</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B70" s="84" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="C70" s="46">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D70" s="45"/>
       <c r="E70" s="44">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F70" s="45"/>
       <c r="G70" s="48">
@@ -12038,14 +12029,14 @@
       <c r="H70" s="47"/>
       <c r="I70" s="44"/>
       <c r="J70" s="47">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K70" s="49">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L70" s="47"/>
       <c r="M70" s="44">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N70" s="45"/>
       <c r="O70" s="44">
@@ -12066,22 +12057,22 @@
       </c>
       <c r="V70" s="44"/>
       <c r="W70" s="47">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="X70" s="49"/>
       <c r="Y70" s="45">
         <v>7</v>
       </c>
-      <c r="Z70" s="48">
+      <c r="Z70" s="48"/>
+      <c r="AA70" s="47">
         <v>6</v>
       </c>
-      <c r="AA70" s="47"/>
       <c r="AB70" s="122">
         <f>SUM(T71:AA71)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AC70" s="48"/>
-      <c r="AD70" s="243"/>
+      <c r="AD70" s="47"/>
       <c r="AE70" s="49"/>
       <c r="AF70" s="47"/>
       <c r="AG70" s="122">
@@ -12096,11 +12087,11 @@
       </c>
       <c r="AK70" s="111">
         <f>MAX($AL$10:$AL$97) - AL70</f>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="AL70" s="122">
         <f>$S70+$AB70+$AG70+$AJ70</f>
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="71" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -12152,17 +12143,17 @@
       <c r="S71" s="121"/>
       <c r="T71" s="126">
         <f>(IF($T70&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T70=$T$6+$U$6,$P$103,0),0),0)+IF($U70&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U70=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U71" s="126"/>
       <c r="V71" s="126">
         <f>(IF($V70&lt;&gt;"",($V$6*$P$104)+IF($V$6=4,($P$102)+IF($V70=$V$6+$W$6,$P$103,0),0),0)+IF($W70&lt;&gt;"",($W$6*$P$104)+IF($W$6=4,($P$102)+IF($W70=$V$6+$W$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W71" s="126"/>
       <c r="X71" s="126">
         <f>(IF($X70&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X70=$X$6+$Y$6,$P$103,0),0),0)+IF($Y70&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y70=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y71" s="59"/>
       <c r="Z71" s="126">
@@ -12515,41 +12506,41 @@
     <row r="74" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="173">
         <f>RANK(AL74,$AL$10:$AL$97,)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B74" s="197" t="s">
         <v>68</v>
       </c>
-      <c r="C74" s="251">
+      <c r="C74" s="247">
         <v>5</v>
       </c>
-      <c r="D74" s="252"/>
-      <c r="E74" s="253">
+      <c r="D74" s="248"/>
+      <c r="E74" s="249">
         <v>6</v>
       </c>
-      <c r="F74" s="252"/>
-      <c r="G74" s="254">
+      <c r="F74" s="248"/>
+      <c r="G74" s="250">
         <v>5</v>
       </c>
-      <c r="H74" s="255"/>
-      <c r="I74" s="253"/>
-      <c r="J74" s="255">
+      <c r="H74" s="251"/>
+      <c r="I74" s="249"/>
+      <c r="J74" s="251">
         <v>6</v>
       </c>
-      <c r="K74" s="256">
+      <c r="K74" s="252">
         <v>6</v>
       </c>
-      <c r="L74" s="255"/>
-      <c r="M74" s="253">
+      <c r="L74" s="251"/>
+      <c r="M74" s="249">
         <v>7</v>
       </c>
-      <c r="N74" s="252"/>
-      <c r="O74" s="253">
+      <c r="N74" s="248"/>
+      <c r="O74" s="249">
         <v>6</v>
       </c>
-      <c r="P74" s="252"/>
-      <c r="Q74" s="254"/>
-      <c r="R74" s="257">
+      <c r="P74" s="248"/>
+      <c r="Q74" s="250"/>
+      <c r="R74" s="253">
         <v>6</v>
       </c>
       <c r="S74" s="192">
@@ -12574,7 +12565,7 @@
       <c r="AA74" s="189"/>
       <c r="AB74" s="192">
         <f>SUM(T75:AA75)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AC74" s="188"/>
       <c r="AD74" s="189"/>
@@ -12596,7 +12587,7 @@
       </c>
       <c r="AL74" s="192">
         <f>$S74+$AB74+$AG74+$AJ74</f>
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="75" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -12648,7 +12639,7 @@
       <c r="S75" s="121"/>
       <c r="T75" s="126">
         <f>(IF($T74&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T74=$T$6+$U$6,$P$103,0),0),0)+IF($U74&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U74=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U75" s="126"/>
       <c r="V75" s="126">
@@ -12658,7 +12649,7 @@
       <c r="W75" s="126"/>
       <c r="X75" s="126">
         <f>(IF($X74&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X74=$X$6+$Y$6,$P$103,0),0),0)+IF($Y74&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y74=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y75" s="59"/>
       <c r="Z75" s="126">
@@ -13011,13 +13002,13 @@
     <row r="78" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="117">
         <f>RANK(AL78,$AL$10:$AL$97,)</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B78" s="84" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C78" s="46">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D78" s="45"/>
       <c r="E78" s="44">
@@ -13030,18 +13021,18 @@
       <c r="H78" s="47"/>
       <c r="I78" s="44"/>
       <c r="J78" s="47">
+        <v>6</v>
+      </c>
+      <c r="K78" s="49">
         <v>7</v>
-      </c>
-      <c r="K78" s="49">
-        <v>5</v>
       </c>
       <c r="L78" s="47"/>
       <c r="M78" s="44">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N78" s="45"/>
       <c r="O78" s="44">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P78" s="45"/>
       <c r="Q78" s="48"/>
@@ -13056,13 +13047,13 @@
       <c r="U78" s="47">
         <v>6</v>
       </c>
-      <c r="V78" s="44"/>
-      <c r="W78" s="47">
+      <c r="V78" s="44">
         <v>6</v>
       </c>
+      <c r="W78" s="47"/>
       <c r="X78" s="49"/>
       <c r="Y78" s="45">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="Z78" s="48"/>
       <c r="AA78" s="47">
@@ -13070,7 +13061,7 @@
       </c>
       <c r="AB78" s="122">
         <f>SUM(T79:AA79)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AC78" s="48"/>
       <c r="AD78" s="47"/>
@@ -13088,11 +13079,11 @@
       </c>
       <c r="AK78" s="111">
         <f>MAX($AL$10:$AL$97) - AL78</f>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AL78" s="122">
         <f>$S78+$AB78+$AG78+$AJ78</f>
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="79" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -13144,7 +13135,7 @@
       <c r="S79" s="121"/>
       <c r="T79" s="126">
         <f>(IF($T78&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T78=$T$6+$U$6,$P$103,0),0),0)+IF($U78&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U78=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U79" s="126"/>
       <c r="V79" s="126">
@@ -13154,12 +13145,12 @@
       <c r="W79" s="126"/>
       <c r="X79" s="126">
         <f>(IF($X78&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X78=$X$6+$Y$6,$P$103,0),0),0)+IF($Y78&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y78=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y79" s="59"/>
       <c r="Z79" s="126">
         <f>(IF($Z78&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z78=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA78&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA78=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA79" s="62"/>
       <c r="AB79" s="121"/>
@@ -13507,10 +13498,10 @@
     <row r="82" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="173">
         <f>RANK(AL82,$AL$10:$AL$97,)</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B82" s="197" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C82" s="185">
         <v>5</v>
@@ -13529,44 +13520,44 @@
         <v>6</v>
       </c>
       <c r="K82" s="190">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L82" s="189"/>
       <c r="M82" s="187">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N82" s="186"/>
       <c r="O82" s="187">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P82" s="186"/>
       <c r="Q82" s="188"/>
       <c r="R82" s="191">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S82" s="192">
         <f>SUM(C83:R83)</f>
         <v>20</v>
       </c>
-      <c r="T82" s="185"/>
-      <c r="U82" s="189">
-        <v>6</v>
-      </c>
+      <c r="T82" s="185">
+        <v>7</v>
+      </c>
+      <c r="U82" s="189"/>
       <c r="V82" s="187">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="W82" s="189"/>
-      <c r="X82" s="190"/>
-      <c r="Y82" s="186">
-        <v>5</v>
-      </c>
-      <c r="Z82" s="188"/>
-      <c r="AA82" s="189">
-        <v>6</v>
-      </c>
+      <c r="X82" s="190">
+        <v>7</v>
+      </c>
+      <c r="Y82" s="186"/>
+      <c r="Z82" s="188">
+        <v>7</v>
+      </c>
+      <c r="AA82" s="189"/>
       <c r="AB82" s="192">
         <f>SUM(T83:AA83)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AC82" s="188"/>
       <c r="AD82" s="189"/>
@@ -13584,11 +13575,11 @@
       </c>
       <c r="AK82" s="194">
         <f>MAX($AL$10:$AL$97) - AL82</f>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AL82" s="192">
         <f>$S82+$AB82+$AG82+$AJ82</f>
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="83" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -13640,7 +13631,7 @@
       <c r="S83" s="121"/>
       <c r="T83" s="126">
         <f>(IF($T82&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T82=$T$6+$U$6,$P$103,0),0),0)+IF($U82&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U82=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U83" s="126"/>
       <c r="V83" s="126">
@@ -13650,12 +13641,12 @@
       <c r="W83" s="126"/>
       <c r="X83" s="126">
         <f>(IF($X82&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X82=$X$6+$Y$6,$P$103,0),0),0)+IF($Y82&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y82=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y83" s="59"/>
       <c r="Z83" s="126">
         <f>(IF($Z82&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z82=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA82&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA82=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA83" s="62"/>
       <c r="AB83" s="121"/>
@@ -14062,7 +14053,7 @@
       <c r="AA86" s="47"/>
       <c r="AB86" s="122">
         <f>SUM(T87:AA87)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AC86" s="48"/>
       <c r="AD86" s="47"/>
@@ -14084,7 +14075,7 @@
       </c>
       <c r="AL86" s="122">
         <f>$S86+$AB86+$AG86+$AJ86</f>
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="87" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -14136,7 +14127,7 @@
       <c r="S87" s="121"/>
       <c r="T87" s="126">
         <f>(IF($T86&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T86=$T$6+$U$6,$P$103,0),0),0)+IF($U86&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U86=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U87" s="126"/>
       <c r="V87" s="126">
@@ -14146,7 +14137,7 @@
       <c r="W87" s="126"/>
       <c r="X87" s="126">
         <f>(IF($X86&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X86=$X$6+$Y$6,$P$103,0),0),0)+IF($Y86&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y86=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y87" s="59"/>
       <c r="Z87" s="126">
@@ -14558,7 +14549,7 @@
       <c r="AA90" s="189"/>
       <c r="AB90" s="192">
         <f>SUM(T91:AA91)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AC90" s="188"/>
       <c r="AD90" s="189"/>
@@ -14580,7 +14571,7 @@
       </c>
       <c r="AL90" s="192">
         <f>$S90+$AB90+$AG90+$AJ90</f>
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="91" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -14632,7 +14623,7 @@
       <c r="S91" s="121"/>
       <c r="T91" s="126">
         <f>(IF($T90&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T90=$T$6+$U$6,$P$103,0),0),0)+IF($U90&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U90=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U91" s="126"/>
       <c r="V91" s="126">
@@ -14642,7 +14633,7 @@
       <c r="W91" s="126"/>
       <c r="X91" s="126">
         <f>(IF($X90&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X90=$X$6+$Y$6,$P$103,0),0),0)+IF($Y90&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y90=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y91" s="59"/>
       <c r="Z91" s="126">
@@ -15054,7 +15045,7 @@
       <c r="AA94" s="47"/>
       <c r="AB94" s="204">
         <f>SUM(T95:AA95)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AC94" s="48"/>
       <c r="AD94" s="47"/>
@@ -15076,7 +15067,7 @@
       </c>
       <c r="AL94" s="204">
         <f>$S94+$AB94+$AG94+$AJ94</f>
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="95" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -15128,7 +15119,7 @@
       <c r="S95" s="121"/>
       <c r="T95" s="126">
         <f>(IF($T94&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T94=$T$6+$U$6,$P$103,0),0),0)+IF($U94&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U94=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U95" s="126"/>
       <c r="V95" s="126">
@@ -15138,7 +15129,7 @@
       <c r="W95" s="126"/>
       <c r="X95" s="126">
         <f>(IF($X94&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X94=$X$6+$Y$6,$P$103,0),0),0)+IF($Y94&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y94=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y95" s="59"/>
       <c r="Z95" s="126">
@@ -15519,7 +15510,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="J98" s="249">
+      <c r="J98" s="246">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
@@ -15568,7 +15559,7 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="W98" s="249">
+      <c r="W98" s="246">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -15621,12 +15612,12 @@
     <row r="100" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B100" s="43"/>
       <c r="N100" s="26"/>
-      <c r="O100" s="258" t="s">
+      <c r="O100" s="287" t="s">
         <v>17</v>
       </c>
-      <c r="P100" s="259"/>
-      <c r="Q100" s="259"/>
-      <c r="R100" s="260"/>
+      <c r="P100" s="288"/>
+      <c r="Q100" s="288"/>
+      <c r="R100" s="289"/>
       <c r="AG100" s="30"/>
       <c r="AH100" s="30"/>
       <c r="AI100" s="30"/>
@@ -15635,21 +15626,21 @@
     </row>
     <row r="101" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="33"/>
-      <c r="B101" s="287" t="s">
+      <c r="B101" s="275" t="s">
         <v>16</v>
       </c>
-      <c r="C101" s="288"/>
-      <c r="D101" s="288"/>
-      <c r="E101" s="288"/>
-      <c r="F101" s="288"/>
-      <c r="G101" s="288"/>
-      <c r="H101" s="288"/>
-      <c r="I101" s="288"/>
-      <c r="J101" s="288"/>
-      <c r="K101" s="288"/>
-      <c r="L101" s="288"/>
-      <c r="M101" s="288"/>
-      <c r="N101" s="289"/>
+      <c r="C101" s="276"/>
+      <c r="D101" s="276"/>
+      <c r="E101" s="276"/>
+      <c r="F101" s="276"/>
+      <c r="G101" s="276"/>
+      <c r="H101" s="276"/>
+      <c r="I101" s="276"/>
+      <c r="J101" s="276"/>
+      <c r="K101" s="276"/>
+      <c r="L101" s="276"/>
+      <c r="M101" s="276"/>
+      <c r="N101" s="277"/>
       <c r="O101" s="21">
         <v>1</v>
       </c>
@@ -15662,45 +15653,45 @@
       <c r="R101" s="22">
         <v>4</v>
       </c>
-      <c r="U101" s="261" t="s">
+      <c r="U101" s="290" t="s">
         <v>26</v>
       </c>
-      <c r="V101" s="262"/>
-      <c r="W101" s="262"/>
-      <c r="X101" s="262"/>
-      <c r="Y101" s="262"/>
-      <c r="Z101" s="262"/>
-      <c r="AA101" s="262"/>
-      <c r="AB101" s="262"/>
-      <c r="AC101" s="262"/>
-      <c r="AD101" s="263"/>
+      <c r="V101" s="291"/>
+      <c r="W101" s="291"/>
+      <c r="X101" s="291"/>
+      <c r="Y101" s="291"/>
+      <c r="Z101" s="291"/>
+      <c r="AA101" s="291"/>
+      <c r="AB101" s="291"/>
+      <c r="AC101" s="291"/>
+      <c r="AD101" s="292"/>
       <c r="AE101" s="28"/>
       <c r="AF101" s="28"/>
-      <c r="AG101" s="264" t="s">
+      <c r="AG101" s="293" t="s">
         <v>24</v>
       </c>
-      <c r="AH101" s="265"/>
-      <c r="AI101" s="265"/>
-      <c r="AJ101" s="265"/>
-      <c r="AK101" s="266"/>
+      <c r="AH101" s="294"/>
+      <c r="AI101" s="294"/>
+      <c r="AJ101" s="294"/>
+      <c r="AK101" s="295"/>
     </row>
     <row r="102" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A102" s="34"/>
-      <c r="B102" s="294" t="s">
+      <c r="B102" s="254" t="s">
         <v>6</v>
       </c>
-      <c r="C102" s="295"/>
-      <c r="D102" s="295"/>
-      <c r="E102" s="295"/>
-      <c r="F102" s="295"/>
-      <c r="G102" s="295"/>
-      <c r="H102" s="295"/>
-      <c r="I102" s="295"/>
-      <c r="J102" s="295"/>
-      <c r="K102" s="295"/>
-      <c r="L102" s="295"/>
-      <c r="M102" s="295"/>
-      <c r="N102" s="296"/>
+      <c r="C102" s="255"/>
+      <c r="D102" s="255"/>
+      <c r="E102" s="255"/>
+      <c r="F102" s="255"/>
+      <c r="G102" s="255"/>
+      <c r="H102" s="255"/>
+      <c r="I102" s="255"/>
+      <c r="J102" s="255"/>
+      <c r="K102" s="255"/>
+      <c r="L102" s="255"/>
+      <c r="M102" s="255"/>
+      <c r="N102" s="256"/>
       <c r="O102" s="20">
         <v>5</v>
       </c>
@@ -15713,49 +15704,49 @@
       <c r="R102" s="23">
         <v>20</v>
       </c>
-      <c r="U102" s="292" t="s">
+      <c r="U102" s="280" t="s">
         <v>20</v>
       </c>
-      <c r="V102" s="293"/>
-      <c r="W102" s="293"/>
-      <c r="X102" s="293"/>
-      <c r="Y102" s="293"/>
-      <c r="Z102" s="293"/>
-      <c r="AA102" s="293"/>
-      <c r="AB102" s="290">
+      <c r="V102" s="281"/>
+      <c r="W102" s="281"/>
+      <c r="X102" s="281"/>
+      <c r="Y102" s="281"/>
+      <c r="Z102" s="281"/>
+      <c r="AA102" s="281"/>
+      <c r="AB102" s="278">
         <v>22</v>
       </c>
-      <c r="AC102" s="290"/>
-      <c r="AD102" s="291"/>
+      <c r="AC102" s="278"/>
+      <c r="AD102" s="279"/>
       <c r="AE102" s="29"/>
       <c r="AF102" s="29"/>
-      <c r="AG102" s="306" t="s">
+      <c r="AG102" s="261" t="s">
         <v>21</v>
       </c>
-      <c r="AH102" s="307"/>
-      <c r="AI102" s="307"/>
-      <c r="AJ102" s="308"/>
+      <c r="AH102" s="262"/>
+      <c r="AI102" s="262"/>
+      <c r="AJ102" s="263"/>
       <c r="AK102" s="209">
         <v>230</v>
       </c>
     </row>
     <row r="103" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="34"/>
-      <c r="B103" s="294" t="s">
+      <c r="B103" s="254" t="s">
         <v>5</v>
       </c>
-      <c r="C103" s="295"/>
-      <c r="D103" s="295"/>
-      <c r="E103" s="295"/>
-      <c r="F103" s="295"/>
-      <c r="G103" s="295"/>
-      <c r="H103" s="295"/>
-      <c r="I103" s="295"/>
-      <c r="J103" s="295"/>
-      <c r="K103" s="295"/>
-      <c r="L103" s="295"/>
-      <c r="M103" s="295"/>
-      <c r="N103" s="296"/>
+      <c r="C103" s="255"/>
+      <c r="D103" s="255"/>
+      <c r="E103" s="255"/>
+      <c r="F103" s="255"/>
+      <c r="G103" s="255"/>
+      <c r="H103" s="255"/>
+      <c r="I103" s="255"/>
+      <c r="J103" s="255"/>
+      <c r="K103" s="255"/>
+      <c r="L103" s="255"/>
+      <c r="M103" s="255"/>
+      <c r="N103" s="256"/>
       <c r="O103" s="20">
         <v>2</v>
       </c>
@@ -15768,49 +15759,49 @@
       <c r="R103" s="23">
         <v>8</v>
       </c>
-      <c r="U103" s="301" t="s">
+      <c r="U103" s="259" t="s">
         <v>18</v>
       </c>
-      <c r="V103" s="302"/>
-      <c r="W103" s="302"/>
-      <c r="X103" s="302"/>
-      <c r="Y103" s="302"/>
-      <c r="Z103" s="302"/>
-      <c r="AA103" s="302"/>
-      <c r="AB103" s="303">
+      <c r="V103" s="260"/>
+      <c r="W103" s="260"/>
+      <c r="X103" s="260"/>
+      <c r="Y103" s="260"/>
+      <c r="Z103" s="260"/>
+      <c r="AA103" s="260"/>
+      <c r="AB103" s="285">
         <v>20</v>
       </c>
-      <c r="AC103" s="303"/>
-      <c r="AD103" s="304"/>
+      <c r="AC103" s="285"/>
+      <c r="AD103" s="286"/>
       <c r="AE103" s="29"/>
       <c r="AF103" s="29"/>
-      <c r="AG103" s="309" t="s">
+      <c r="AG103" s="264" t="s">
         <v>22</v>
       </c>
-      <c r="AH103" s="295"/>
-      <c r="AI103" s="295"/>
-      <c r="AJ103" s="296"/>
+      <c r="AH103" s="255"/>
+      <c r="AI103" s="255"/>
+      <c r="AJ103" s="256"/>
       <c r="AK103" s="36">
         <v>115</v>
       </c>
     </row>
     <row r="104" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="35"/>
-      <c r="B104" s="280" t="s">
+      <c r="B104" s="268" t="s">
         <v>4</v>
       </c>
-      <c r="C104" s="281"/>
-      <c r="D104" s="281"/>
-      <c r="E104" s="281"/>
-      <c r="F104" s="281"/>
-      <c r="G104" s="281"/>
-      <c r="H104" s="281"/>
-      <c r="I104" s="281"/>
-      <c r="J104" s="281"/>
-      <c r="K104" s="281"/>
-      <c r="L104" s="281"/>
-      <c r="M104" s="281"/>
-      <c r="N104" s="282"/>
+      <c r="C104" s="269"/>
+      <c r="D104" s="269"/>
+      <c r="E104" s="269"/>
+      <c r="F104" s="269"/>
+      <c r="G104" s="269"/>
+      <c r="H104" s="269"/>
+      <c r="I104" s="269"/>
+      <c r="J104" s="269"/>
+      <c r="K104" s="269"/>
+      <c r="L104" s="269"/>
+      <c r="M104" s="269"/>
+      <c r="N104" s="270"/>
       <c r="O104" s="3">
         <v>1</v>
       </c>
@@ -15823,51 +15814,51 @@
       <c r="R104" s="24">
         <v>1</v>
       </c>
-      <c r="U104" s="297" t="s">
+      <c r="U104" s="282" t="s">
         <v>19</v>
       </c>
-      <c r="V104" s="298"/>
-      <c r="W104" s="298"/>
-      <c r="X104" s="298"/>
-      <c r="Y104" s="298"/>
-      <c r="Z104" s="298"/>
-      <c r="AA104" s="298"/>
-      <c r="AB104" s="299">
+      <c r="V104" s="258"/>
+      <c r="W104" s="258"/>
+      <c r="X104" s="258"/>
+      <c r="Y104" s="258"/>
+      <c r="Z104" s="258"/>
+      <c r="AA104" s="258"/>
+      <c r="AB104" s="283">
         <f>AB102*AB103</f>
         <v>440</v>
       </c>
-      <c r="AC104" s="299"/>
-      <c r="AD104" s="300"/>
+      <c r="AC104" s="283"/>
+      <c r="AD104" s="284"/>
       <c r="AE104" s="29"/>
       <c r="AF104" s="29"/>
-      <c r="AG104" s="309" t="s">
+      <c r="AG104" s="264" t="s">
         <v>25</v>
       </c>
-      <c r="AH104" s="295"/>
-      <c r="AI104" s="295"/>
-      <c r="AJ104" s="296"/>
+      <c r="AH104" s="255"/>
+      <c r="AI104" s="255"/>
+      <c r="AJ104" s="256"/>
       <c r="AK104" s="36">
         <v>65</v>
       </c>
     </row>
     <row r="105" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG105" s="301" t="s">
+      <c r="AG105" s="259" t="s">
         <v>23</v>
       </c>
-      <c r="AH105" s="302"/>
-      <c r="AI105" s="302"/>
-      <c r="AJ105" s="302"/>
+      <c r="AH105" s="260"/>
+      <c r="AI105" s="260"/>
+      <c r="AJ105" s="260"/>
       <c r="AK105" s="211">
         <v>30</v>
       </c>
     </row>
     <row r="106" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG106" s="305" t="s">
+      <c r="AG106" s="257" t="s">
         <v>19</v>
       </c>
-      <c r="AH106" s="298"/>
-      <c r="AI106" s="298"/>
-      <c r="AJ106" s="298"/>
+      <c r="AH106" s="258"/>
+      <c r="AI106" s="258"/>
+      <c r="AJ106" s="258"/>
       <c r="AK106" s="210">
         <f>SUM(AK102:AK105)</f>
         <v>440</v>
@@ -15879,12 +15870,22 @@
     <sortCondition ref="B10:B94"/>
   </sortState>
   <mergeCells count="38">
-    <mergeCell ref="B103:N103"/>
-    <mergeCell ref="AG106:AJ106"/>
-    <mergeCell ref="AG105:AJ105"/>
-    <mergeCell ref="AG102:AJ102"/>
-    <mergeCell ref="AG104:AJ104"/>
-    <mergeCell ref="AG103:AJ103"/>
+    <mergeCell ref="O100:R100"/>
+    <mergeCell ref="U101:AD101"/>
+    <mergeCell ref="AG101:AK101"/>
+    <mergeCell ref="AH4:AJ4"/>
+    <mergeCell ref="AG5:AG9"/>
+    <mergeCell ref="AJ5:AJ9"/>
+    <mergeCell ref="X5:AA5"/>
+    <mergeCell ref="AB5:AB9"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="C4:S4"/>
+    <mergeCell ref="T4:AB4"/>
+    <mergeCell ref="AC4:AG4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="K5:R5"/>
+    <mergeCell ref="S5:S9"/>
     <mergeCell ref="T5:W5"/>
     <mergeCell ref="B104:N104"/>
     <mergeCell ref="C1:O1"/>
@@ -15901,22 +15902,12 @@
     <mergeCell ref="AB104:AD104"/>
     <mergeCell ref="U103:AA103"/>
     <mergeCell ref="AB103:AD103"/>
-    <mergeCell ref="O100:R100"/>
-    <mergeCell ref="U101:AD101"/>
-    <mergeCell ref="AG101:AK101"/>
-    <mergeCell ref="AH4:AJ4"/>
-    <mergeCell ref="AG5:AG9"/>
-    <mergeCell ref="AJ5:AJ9"/>
-    <mergeCell ref="X5:AA5"/>
-    <mergeCell ref="AB5:AB9"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="C4:S4"/>
-    <mergeCell ref="T4:AB4"/>
-    <mergeCell ref="AC4:AG4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="K5:R5"/>
-    <mergeCell ref="S5:S9"/>
+    <mergeCell ref="B103:N103"/>
+    <mergeCell ref="AG106:AJ106"/>
+    <mergeCell ref="AG105:AJ105"/>
+    <mergeCell ref="AG102:AJ102"/>
+    <mergeCell ref="AG104:AJ104"/>
+    <mergeCell ref="AG103:AJ103"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <conditionalFormatting sqref="AH18:AI18 AH10:AI10 AH14:AI14 T10:AA10 AC10:AF10 C10:R10 C14:R14 T14:AA14 AC14:AF14 T18:AA18 AC18:AF18 AH30:AI30 C30:R30 T30:AA30 AC30:AF30 AH26:AI26 C26:R26 T26:AA26 AC26:AF26 AH62:AI62 C62:R62 T62:AA62 AC62:AF62 AH42:AI42 C42:R42 T42:AA42 AC42:AF42 AH22:AI22 C22:R22 T22:AA22 AC22:AF22 AH38:AI38 C38:R38 T38:AA38 AC38:AF38 AH34:AI34 C34:R34 T34:AA34 AC34:AF34 AH66:AI66 C66:R66 T66:AA66 AC66:AF66 C18:R18">
@@ -16673,7 +16664,7 @@
   <dimension ref="A1:AJ31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16892,7 +16883,9 @@
       <c r="O6" s="81">
         <v>3</v>
       </c>
-      <c r="P6" s="81"/>
+      <c r="P6" s="81">
+        <v>2</v>
+      </c>
       <c r="Q6" s="81"/>
       <c r="R6" s="81"/>
       <c r="S6" s="81"/>
@@ -16956,7 +16949,9 @@
       <c r="O7" s="81">
         <v>2</v>
       </c>
-      <c r="P7" s="81"/>
+      <c r="P7" s="81">
+        <v>3</v>
+      </c>
       <c r="Q7" s="81"/>
       <c r="R7" s="81"/>
       <c r="S7" s="81"/>
@@ -16964,7 +16959,7 @@
       <c r="U7" s="81"/>
       <c r="V7" s="73">
         <f>IF(O7&gt;O6,1,0)+IF(P7&gt;P6,1,0)+IF(Q7&gt;Q6,1,0)+IF(R7&gt;R6,1,0)+IF(S7&gt;S6,1,0)+IF(T7&gt;T6,1,0)+IF(U7&gt;U6,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W7" s="14"/>
       <c r="X7" s="4"/>
@@ -17104,8 +17099,12 @@
       <c r="N10" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="O10" s="81"/>
-      <c r="P10" s="81"/>
+      <c r="O10" s="81">
+        <v>0</v>
+      </c>
+      <c r="P10" s="81">
+        <v>1</v>
+      </c>
       <c r="Q10" s="81"/>
       <c r="R10" s="81"/>
       <c r="S10" s="81"/>
@@ -17169,8 +17168,12 @@
       <c r="N11" s="83" t="s">
         <v>57</v>
       </c>
-      <c r="O11" s="81"/>
-      <c r="P11" s="81"/>
+      <c r="O11" s="81">
+        <v>1</v>
+      </c>
+      <c r="P11" s="81">
+        <v>2</v>
+      </c>
       <c r="Q11" s="81"/>
       <c r="R11" s="81"/>
       <c r="S11" s="81"/>
@@ -17178,7 +17181,7 @@
       <c r="U11" s="81"/>
       <c r="V11" s="73">
         <f>IF(O11&gt;O10,1,0)+IF(P11&gt;P10,1,0)+IF(Q11&gt;Q10,1,0)+IF(R11&gt;R10,1,0)+IF(S11&gt;S10,1,0)+IF(T11&gt;T10,1,0)+IF(U11&gt;U10,1,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y11" s="93"/>
       <c r="Z11" s="86"/>
@@ -17580,8 +17583,12 @@
       <c r="N20" s="83" t="s">
         <v>48</v>
       </c>
-      <c r="O20" s="81"/>
-      <c r="P20" s="81"/>
+      <c r="O20" s="81">
+        <v>5</v>
+      </c>
+      <c r="P20" s="81">
+        <v>3</v>
+      </c>
       <c r="Q20" s="81"/>
       <c r="R20" s="81"/>
       <c r="S20" s="81"/>
@@ -17589,7 +17596,7 @@
       <c r="U20" s="81"/>
       <c r="V20" s="73">
         <f>IF(O20&gt;O21,1,0)+IF(P20&gt;P21,1,0)+IF(Q20&gt;Q21,1,0)+IF(R20&gt;R21,1,0)+IF(S20&gt;S21,1,0)+IF(T20&gt;T21,1,0)+IF(U20&gt;U21,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W20" s="13"/>
       <c r="Y20" s="93"/>
@@ -17642,8 +17649,12 @@
       <c r="N21" s="83" t="s">
         <v>45</v>
       </c>
-      <c r="O21" s="81"/>
-      <c r="P21" s="81"/>
+      <c r="O21" s="81">
+        <v>2</v>
+      </c>
+      <c r="P21" s="81">
+        <v>4</v>
+      </c>
       <c r="Q21" s="81"/>
       <c r="R21" s="81"/>
       <c r="S21" s="81"/>
@@ -17651,7 +17662,7 @@
       <c r="U21" s="81"/>
       <c r="V21" s="73">
         <f>IF(O21&gt;O20,1,0)+IF(P21&gt;P20,1,0)+IF(Q21&gt;Q20,1,0)+IF(R21&gt;R20,1,0)+IF(S21&gt;S20,1,0)+IF(T21&gt;T20,1,0)+IF(U21&gt;U20,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W21" s="14"/>
       <c r="X21" s="4"/>
@@ -17794,7 +17805,9 @@
       <c r="O24" s="81">
         <v>3</v>
       </c>
-      <c r="P24" s="82"/>
+      <c r="P24" s="82">
+        <v>2</v>
+      </c>
       <c r="Q24" s="82"/>
       <c r="R24" s="82"/>
       <c r="S24" s="82"/>
@@ -17857,7 +17870,9 @@
       <c r="O25" s="81">
         <v>2</v>
       </c>
-      <c r="P25" s="82"/>
+      <c r="P25" s="82">
+        <v>4</v>
+      </c>
       <c r="Q25" s="82"/>
       <c r="R25" s="82"/>
       <c r="S25" s="82"/>
@@ -17865,7 +17880,7 @@
       <c r="U25" s="81"/>
       <c r="V25" s="73">
         <f>IF(O25&gt;O24,1,0)+IF(P25&gt;P24,1,0)+IF(Q25&gt;Q24,1,0)+IF(R25&gt;R24,1,0)+IF(S25&gt;S24,1,0)+IF(T25&gt;T24,1,0)+IF(U25&gt;U24,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y25" s="86"/>
       <c r="Z25" s="86"/>

</xml_diff>

<commit_message>
Updated games of 2019-04-29
</commit_message>
<xml_diff>
--- a/laval.xlsx
+++ b/laval.xlsx
@@ -2499,6 +2499,123 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2508,18 +2625,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="83" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="85" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="92" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2531,138 +2663,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="83" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="85" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3886,217 +3886,217 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="C1" s="271"/>
-      <c r="D1" s="271"/>
-      <c r="E1" s="271"/>
-      <c r="F1" s="271"/>
-      <c r="G1" s="271"/>
-      <c r="H1" s="271"/>
-      <c r="I1" s="271"/>
-      <c r="J1" s="271"/>
-      <c r="K1" s="271"/>
-      <c r="L1" s="271"/>
-      <c r="M1" s="271"/>
-      <c r="N1" s="271"/>
-      <c r="O1" s="271"/>
-      <c r="P1" s="272"/>
-      <c r="Q1" s="272"/>
-      <c r="R1" s="272"/>
-      <c r="S1" s="272"/>
-      <c r="T1" s="272"/>
-      <c r="U1" s="272"/>
-      <c r="V1" s="272"/>
-      <c r="W1" s="272"/>
-      <c r="X1" s="272"/>
-      <c r="Y1" s="272"/>
-      <c r="Z1" s="272"/>
-      <c r="AA1" s="272"/>
-      <c r="AB1" s="272"/>
-      <c r="AC1" s="272"/>
-      <c r="AD1" s="272"/>
-      <c r="AE1" s="272"/>
-      <c r="AF1" s="272"/>
-      <c r="AG1" s="272"/>
-      <c r="AH1" s="272"/>
-      <c r="AI1" s="272"/>
-      <c r="AJ1" s="272"/>
+      <c r="C1" s="282"/>
+      <c r="D1" s="282"/>
+      <c r="E1" s="282"/>
+      <c r="F1" s="282"/>
+      <c r="G1" s="282"/>
+      <c r="H1" s="282"/>
+      <c r="I1" s="282"/>
+      <c r="J1" s="282"/>
+      <c r="K1" s="282"/>
+      <c r="L1" s="282"/>
+      <c r="M1" s="282"/>
+      <c r="N1" s="282"/>
+      <c r="O1" s="282"/>
+      <c r="P1" s="283"/>
+      <c r="Q1" s="283"/>
+      <c r="R1" s="283"/>
+      <c r="S1" s="283"/>
+      <c r="T1" s="283"/>
+      <c r="U1" s="283"/>
+      <c r="V1" s="283"/>
+      <c r="W1" s="283"/>
+      <c r="X1" s="283"/>
+      <c r="Y1" s="283"/>
+      <c r="Z1" s="283"/>
+      <c r="AA1" s="283"/>
+      <c r="AB1" s="283"/>
+      <c r="AC1" s="283"/>
+      <c r="AD1" s="283"/>
+      <c r="AE1" s="283"/>
+      <c r="AF1" s="283"/>
+      <c r="AG1" s="283"/>
+      <c r="AH1" s="283"/>
+      <c r="AI1" s="283"/>
+      <c r="AJ1" s="283"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="41"/>
-      <c r="C2" s="273" t="s">
+      <c r="C2" s="284" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="273"/>
-      <c r="E2" s="273"/>
-      <c r="F2" s="273"/>
-      <c r="G2" s="273"/>
-      <c r="H2" s="273"/>
-      <c r="I2" s="273"/>
-      <c r="J2" s="273"/>
-      <c r="K2" s="273"/>
-      <c r="L2" s="273"/>
-      <c r="M2" s="273"/>
-      <c r="N2" s="273"/>
-      <c r="O2" s="273"/>
-      <c r="P2" s="273"/>
-      <c r="Q2" s="274" t="s">
+      <c r="D2" s="284"/>
+      <c r="E2" s="284"/>
+      <c r="F2" s="284"/>
+      <c r="G2" s="284"/>
+      <c r="H2" s="284"/>
+      <c r="I2" s="284"/>
+      <c r="J2" s="284"/>
+      <c r="K2" s="284"/>
+      <c r="L2" s="284"/>
+      <c r="M2" s="284"/>
+      <c r="N2" s="284"/>
+      <c r="O2" s="284"/>
+      <c r="P2" s="284"/>
+      <c r="Q2" s="285" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="272"/>
-      <c r="S2" s="272"/>
-      <c r="T2" s="272"/>
-      <c r="U2" s="272"/>
-      <c r="V2" s="272"/>
-      <c r="W2" s="272"/>
-      <c r="X2" s="272"/>
-      <c r="Y2" s="272"/>
-      <c r="Z2" s="272"/>
-      <c r="AA2" s="272"/>
-      <c r="AB2" s="272"/>
-      <c r="AC2" s="272"/>
-      <c r="AD2" s="272"/>
-      <c r="AE2" s="272"/>
-      <c r="AF2" s="272"/>
-      <c r="AG2" s="272"/>
-      <c r="AH2" s="272"/>
-      <c r="AI2" s="272"/>
-      <c r="AJ2" s="272"/>
+      <c r="R2" s="283"/>
+      <c r="S2" s="283"/>
+      <c r="T2" s="283"/>
+      <c r="U2" s="283"/>
+      <c r="V2" s="283"/>
+      <c r="W2" s="283"/>
+      <c r="X2" s="283"/>
+      <c r="Y2" s="283"/>
+      <c r="Z2" s="283"/>
+      <c r="AA2" s="283"/>
+      <c r="AB2" s="283"/>
+      <c r="AC2" s="283"/>
+      <c r="AD2" s="283"/>
+      <c r="AE2" s="283"/>
+      <c r="AF2" s="283"/>
+      <c r="AG2" s="283"/>
+      <c r="AH2" s="283"/>
+      <c r="AI2" s="283"/>
+      <c r="AJ2" s="283"/>
     </row>
     <row r="3" spans="1:38" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="271"/>
-      <c r="D3" s="271"/>
-      <c r="E3" s="271"/>
-      <c r="F3" s="271"/>
-      <c r="G3" s="271"/>
-      <c r="H3" s="271"/>
-      <c r="I3" s="271"/>
-      <c r="J3" s="271"/>
-      <c r="K3" s="271"/>
-      <c r="L3" s="271"/>
-      <c r="M3" s="271"/>
-      <c r="N3" s="271"/>
-      <c r="O3" s="271"/>
-      <c r="P3" s="272"/>
-      <c r="Q3" s="272"/>
-      <c r="R3" s="272"/>
-      <c r="S3" s="272"/>
-      <c r="T3" s="272"/>
-      <c r="U3" s="272"/>
-      <c r="V3" s="272"/>
-      <c r="W3" s="272"/>
-      <c r="X3" s="272"/>
-      <c r="Y3" s="272"/>
-      <c r="Z3" s="272"/>
-      <c r="AA3" s="272"/>
-      <c r="AB3" s="272"/>
-      <c r="AC3" s="272"/>
-      <c r="AD3" s="272"/>
-      <c r="AE3" s="272"/>
-      <c r="AF3" s="272"/>
-      <c r="AG3" s="272"/>
-      <c r="AH3" s="272"/>
-      <c r="AI3" s="272"/>
-      <c r="AJ3" s="272"/>
+      <c r="C3" s="282"/>
+      <c r="D3" s="282"/>
+      <c r="E3" s="282"/>
+      <c r="F3" s="282"/>
+      <c r="G3" s="282"/>
+      <c r="H3" s="282"/>
+      <c r="I3" s="282"/>
+      <c r="J3" s="282"/>
+      <c r="K3" s="282"/>
+      <c r="L3" s="282"/>
+      <c r="M3" s="282"/>
+      <c r="N3" s="282"/>
+      <c r="O3" s="282"/>
+      <c r="P3" s="283"/>
+      <c r="Q3" s="283"/>
+      <c r="R3" s="283"/>
+      <c r="S3" s="283"/>
+      <c r="T3" s="283"/>
+      <c r="U3" s="283"/>
+      <c r="V3" s="283"/>
+      <c r="W3" s="283"/>
+      <c r="X3" s="283"/>
+      <c r="Y3" s="283"/>
+      <c r="Z3" s="283"/>
+      <c r="AA3" s="283"/>
+      <c r="AB3" s="283"/>
+      <c r="AC3" s="283"/>
+      <c r="AD3" s="283"/>
+      <c r="AE3" s="283"/>
+      <c r="AF3" s="283"/>
+      <c r="AG3" s="283"/>
+      <c r="AH3" s="283"/>
+      <c r="AI3" s="283"/>
+      <c r="AJ3" s="283"/>
     </row>
     <row r="4" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="296" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="297"/>
-      <c r="E4" s="297"/>
-      <c r="F4" s="297"/>
-      <c r="G4" s="297"/>
-      <c r="H4" s="297"/>
-      <c r="I4" s="297"/>
-      <c r="J4" s="297"/>
-      <c r="K4" s="297"/>
-      <c r="L4" s="297"/>
-      <c r="M4" s="297"/>
-      <c r="N4" s="297"/>
-      <c r="O4" s="297"/>
-      <c r="P4" s="297"/>
-      <c r="Q4" s="297"/>
-      <c r="R4" s="297"/>
-      <c r="S4" s="298"/>
-      <c r="T4" s="296" t="s">
+      <c r="C4" s="266" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="267"/>
+      <c r="E4" s="267"/>
+      <c r="F4" s="267"/>
+      <c r="G4" s="267"/>
+      <c r="H4" s="267"/>
+      <c r="I4" s="267"/>
+      <c r="J4" s="267"/>
+      <c r="K4" s="267"/>
+      <c r="L4" s="267"/>
+      <c r="M4" s="267"/>
+      <c r="N4" s="267"/>
+      <c r="O4" s="267"/>
+      <c r="P4" s="267"/>
+      <c r="Q4" s="267"/>
+      <c r="R4" s="267"/>
+      <c r="S4" s="268"/>
+      <c r="T4" s="266" t="s">
         <v>1</v>
       </c>
-      <c r="U4" s="297"/>
-      <c r="V4" s="297"/>
-      <c r="W4" s="297"/>
-      <c r="X4" s="297"/>
-      <c r="Y4" s="297"/>
-      <c r="Z4" s="297"/>
-      <c r="AA4" s="297"/>
-      <c r="AB4" s="298"/>
-      <c r="AC4" s="296" t="s">
+      <c r="U4" s="267"/>
+      <c r="V4" s="267"/>
+      <c r="W4" s="267"/>
+      <c r="X4" s="267"/>
+      <c r="Y4" s="267"/>
+      <c r="Z4" s="267"/>
+      <c r="AA4" s="267"/>
+      <c r="AB4" s="268"/>
+      <c r="AC4" s="266" t="s">
         <v>2</v>
       </c>
-      <c r="AD4" s="297"/>
-      <c r="AE4" s="297"/>
-      <c r="AF4" s="297"/>
-      <c r="AG4" s="305"/>
-      <c r="AH4" s="296" t="s">
+      <c r="AD4" s="267"/>
+      <c r="AE4" s="267"/>
+      <c r="AF4" s="267"/>
+      <c r="AG4" s="277"/>
+      <c r="AH4" s="266" t="s">
         <v>10</v>
       </c>
-      <c r="AI4" s="297"/>
-      <c r="AJ4" s="298"/>
+      <c r="AI4" s="267"/>
+      <c r="AJ4" s="268"/>
     </row>
     <row r="5" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="265" t="s">
+      <c r="C5" s="278" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="266"/>
-      <c r="E5" s="266"/>
-      <c r="F5" s="266"/>
-      <c r="G5" s="266"/>
-      <c r="H5" s="266"/>
-      <c r="I5" s="266"/>
-      <c r="J5" s="267"/>
-      <c r="K5" s="303" t="s">
+      <c r="D5" s="274"/>
+      <c r="E5" s="274"/>
+      <c r="F5" s="274"/>
+      <c r="G5" s="274"/>
+      <c r="H5" s="274"/>
+      <c r="I5" s="274"/>
+      <c r="J5" s="275"/>
+      <c r="K5" s="273" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="266"/>
-      <c r="M5" s="266"/>
-      <c r="N5" s="266"/>
-      <c r="O5" s="266"/>
-      <c r="P5" s="266"/>
-      <c r="Q5" s="266"/>
-      <c r="R5" s="267"/>
-      <c r="S5" s="299" t="s">
+      <c r="L5" s="274"/>
+      <c r="M5" s="274"/>
+      <c r="N5" s="274"/>
+      <c r="O5" s="274"/>
+      <c r="P5" s="274"/>
+      <c r="Q5" s="274"/>
+      <c r="R5" s="275"/>
+      <c r="S5" s="269" t="s">
         <v>12</v>
       </c>
-      <c r="T5" s="265" t="s">
+      <c r="T5" s="278" t="s">
         <v>9</v>
       </c>
-      <c r="U5" s="266"/>
-      <c r="V5" s="266"/>
-      <c r="W5" s="267"/>
-      <c r="X5" s="303" t="s">
+      <c r="U5" s="274"/>
+      <c r="V5" s="274"/>
+      <c r="W5" s="275"/>
+      <c r="X5" s="273" t="s">
         <v>8</v>
       </c>
-      <c r="Y5" s="266"/>
-      <c r="Z5" s="266"/>
-      <c r="AA5" s="267"/>
-      <c r="AB5" s="299" t="s">
+      <c r="Y5" s="274"/>
+      <c r="Z5" s="274"/>
+      <c r="AA5" s="275"/>
+      <c r="AB5" s="269" t="s">
         <v>13</v>
       </c>
-      <c r="AC5" s="304" t="s">
+      <c r="AC5" s="276" t="s">
         <v>9</v>
       </c>
-      <c r="AD5" s="267"/>
-      <c r="AE5" s="303" t="s">
+      <c r="AD5" s="275"/>
+      <c r="AE5" s="273" t="s">
         <v>8</v>
       </c>
-      <c r="AF5" s="267"/>
-      <c r="AG5" s="299" t="s">
+      <c r="AF5" s="275"/>
+      <c r="AG5" s="269" t="s">
         <v>14</v>
       </c>
       <c r="AH5" s="56"/>
       <c r="AI5" s="25"/>
-      <c r="AJ5" s="299" t="s">
+      <c r="AJ5" s="269" t="s">
         <v>15</v>
       </c>
       <c r="AK5" s="4"/>
@@ -4168,7 +4168,7 @@
         <f>Résultats!$J$28</f>
         <v>3</v>
       </c>
-      <c r="S6" s="300"/>
+      <c r="S6" s="270"/>
       <c r="T6" s="156">
         <f>Résultats!$V$6</f>
         <v>1</v>
@@ -4195,13 +4195,13 @@
       </c>
       <c r="Z6" s="106">
         <f>Résultats!$V$24</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA6" s="103">
         <f>Résultats!$V$25</f>
         <v>1</v>
       </c>
-      <c r="AB6" s="300"/>
+      <c r="AB6" s="270"/>
       <c r="AC6" s="106">
         <f>Résultats!$AH$8</f>
         <v>0</v>
@@ -4218,7 +4218,7 @@
         <f>Résultats!$AH$23</f>
         <v>0</v>
       </c>
-      <c r="AG6" s="300"/>
+      <c r="AG6" s="270"/>
       <c r="AH6" s="198">
         <f>Résultats!$AH$15</f>
         <v>0</v>
@@ -4227,7 +4227,7 @@
         <f>Résultats!$AH$16</f>
         <v>0</v>
       </c>
-      <c r="AJ6" s="300"/>
+      <c r="AJ6" s="270"/>
       <c r="AK6" s="37"/>
     </row>
     <row r="7" spans="1:38" s="39" customFormat="1" ht="58.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -4253,7 +4253,7 @@
       <c r="P7" s="230"/>
       <c r="Q7" s="234"/>
       <c r="R7" s="112"/>
-      <c r="S7" s="300"/>
+      <c r="S7" s="270"/>
       <c r="T7" s="157"/>
       <c r="U7" s="112"/>
       <c r="V7" s="160"/>
@@ -4262,15 +4262,15 @@
       <c r="Y7" s="113"/>
       <c r="Z7" s="114"/>
       <c r="AA7" s="112"/>
-      <c r="AB7" s="300"/>
+      <c r="AB7" s="270"/>
       <c r="AC7" s="114"/>
       <c r="AD7" s="112"/>
       <c r="AE7" s="115"/>
       <c r="AF7" s="112"/>
-      <c r="AG7" s="300"/>
+      <c r="AG7" s="270"/>
       <c r="AH7" s="198"/>
       <c r="AI7" s="107"/>
-      <c r="AJ7" s="300"/>
+      <c r="AJ7" s="270"/>
       <c r="AK7" s="37"/>
     </row>
     <row r="8" spans="1:38" s="39" customFormat="1" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4340,7 +4340,7 @@
         <f>Résultats!$B$28</f>
         <v>VEGAS</v>
       </c>
-      <c r="S8" s="300"/>
+      <c r="S8" s="270"/>
       <c r="T8" s="158" t="str">
         <f>Résultats!$N$6</f>
         <v>BOSTON</v>
@@ -4373,7 +4373,7 @@
         <f>Résultats!$N$25</f>
         <v>DALLAS</v>
       </c>
-      <c r="AB8" s="300"/>
+      <c r="AB8" s="270"/>
       <c r="AC8" s="164" t="str">
         <f>Résultats!$Z$8</f>
         <v xml:space="preserve"> </v>
@@ -4390,7 +4390,7 @@
         <f>Résultats!$Z$23</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AG8" s="300"/>
+      <c r="AG8" s="270"/>
       <c r="AH8" s="199" t="str">
         <f>Résultats!$Z$15</f>
         <v xml:space="preserve"> </v>
@@ -4399,7 +4399,7 @@
         <f>Résultats!$Z$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ8" s="300"/>
+      <c r="AJ8" s="270"/>
       <c r="AK8" s="37"/>
     </row>
     <row r="9" spans="1:38" s="39" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4473,7 +4473,7 @@
         <f>Résultats!$A$28</f>
         <v>P3</v>
       </c>
-      <c r="S9" s="302"/>
+      <c r="S9" s="272"/>
       <c r="T9" s="166" t="str">
         <f>Résultats!$M$6</f>
         <v>A2</v>
@@ -4506,7 +4506,7 @@
         <f>Résultats!$M$25</f>
         <v>WC1</v>
       </c>
-      <c r="AB9" s="301"/>
+      <c r="AB9" s="271"/>
       <c r="AC9" s="170" t="str">
         <f>Résultats!$Y$8</f>
         <v xml:space="preserve"> </v>
@@ -4523,7 +4523,7 @@
         <f>Résultats!$Y$23</f>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="AG9" s="301"/>
+      <c r="AG9" s="271"/>
       <c r="AH9" s="201" t="str">
         <f>Résultats!$Y$15</f>
         <v xml:space="preserve"> </v>
@@ -4532,7 +4532,7 @@
         <f>Résultats!$Y$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ9" s="302"/>
+      <c r="AJ9" s="272"/>
       <c r="AK9" s="109" t="s">
         <v>51</v>
       </c>
@@ -4602,7 +4602,7 @@
       <c r="AA10" s="180"/>
       <c r="AB10" s="181">
         <f>SUM(T11:AA11)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AC10" s="179"/>
       <c r="AD10" s="176"/>
@@ -4624,7 +4624,7 @@
       </c>
       <c r="AL10" s="181">
         <f>$S10+$AB10+$AG10+$AJ10</f>
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -4691,7 +4691,7 @@
       <c r="Y11" s="59"/>
       <c r="Z11" s="126">
         <f>(IF($Z10&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z10=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA10&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA10=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA11" s="62"/>
       <c r="AB11" s="121"/>
@@ -5116,7 +5116,7 @@
       </c>
       <c r="AK14" s="111">
         <f>MAX($AL$10:$AL$97) - AL14</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL14" s="122">
         <f>$S14+$AB14+$AG14+$AJ14</f>
@@ -5201,7 +5201,7 @@
       <c r="AJ15" s="121"/>
       <c r="AK15" s="92">
         <f>MAX($AL$10:$AL$97) - AL15</f>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AL15" s="121"/>
     </row>
@@ -5597,7 +5597,7 @@
       <c r="AA18" s="191"/>
       <c r="AB18" s="192">
         <f>SUM(T19:AA19)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AC18" s="188"/>
       <c r="AD18" s="189"/>
@@ -5619,7 +5619,7 @@
       </c>
       <c r="AL18" s="192">
         <f>$S18+$AB18+$AG18+$AJ18</f>
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5686,7 +5686,7 @@
       <c r="Y19" s="59"/>
       <c r="Z19" s="126">
         <f>(IF($Z18&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z18=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA18&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA18=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA19" s="62"/>
       <c r="AB19" s="144"/>
@@ -5700,7 +5700,7 @@
       <c r="AJ19" s="144"/>
       <c r="AK19" s="150">
         <f>MAX($AL$10:$AL$97) - AL19</f>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AL19" s="121"/>
     </row>
@@ -6037,7 +6037,7 @@
     <row r="22" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="117">
         <f>RANK(AL22,$AL$10:$AL$97,)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B22" s="84" t="s">
         <v>70</v>
@@ -6106,7 +6106,7 @@
         <f>SUM(AC23:AF23)</f>
         <v>0</v>
       </c>
-      <c r="AH22" s="306"/>
+      <c r="AH22" s="254"/>
       <c r="AI22" s="57"/>
       <c r="AJ22" s="122">
         <f>AH23</f>
@@ -6114,7 +6114,7 @@
       </c>
       <c r="AK22" s="111">
         <f>MAX($AL$10:$AL$97) - AL22</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AL22" s="122">
         <f>$S22+$AB22+$AG22+$AJ22</f>
@@ -6199,7 +6199,7 @@
       <c r="AJ23" s="144"/>
       <c r="AK23" s="150">
         <f>MAX($AL$10:$AL$97) - AL23</f>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AL23" s="121"/>
     </row>
@@ -6536,7 +6536,7 @@
     <row r="26" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="173">
         <f>RANK(AL26,$AL$10:$AL$97,)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B26" s="197" t="s">
         <v>71</v>
@@ -6595,10 +6595,10 @@
       <c r="AA26" s="191"/>
       <c r="AB26" s="192">
         <f>SUM(T27:AA27)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AC26" s="188"/>
-      <c r="AD26" s="307"/>
+      <c r="AD26" s="255"/>
       <c r="AE26" s="190"/>
       <c r="AF26" s="189"/>
       <c r="AG26" s="192">
@@ -6617,7 +6617,7 @@
       </c>
       <c r="AL26" s="192">
         <f>$S26+$AB26+$AG26+$AJ26</f>
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6684,7 +6684,7 @@
       <c r="Y27" s="59"/>
       <c r="Z27" s="126">
         <f>(IF($Z26&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z26=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA26&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA26=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA27" s="62"/>
       <c r="AB27" s="155"/>
@@ -6698,7 +6698,7 @@
       <c r="AJ27" s="144"/>
       <c r="AK27" s="150">
         <f>MAX($AL$10:$AL$97) - AL27</f>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AL27" s="121"/>
     </row>
@@ -7094,7 +7094,7 @@
       <c r="AA30" s="47"/>
       <c r="AB30" s="122">
         <f>SUM(T31:AA31)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC30" s="48"/>
       <c r="AD30" s="47"/>
@@ -7116,7 +7116,7 @@
       </c>
       <c r="AL30" s="122">
         <f>$S30+$AB30+$AG30+$AJ30</f>
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7183,7 +7183,7 @@
       <c r="Y31" s="59"/>
       <c r="Z31" s="126">
         <f>(IF($Z30&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z30=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA30&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA30=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA31" s="62"/>
       <c r="AB31" s="121"/>
@@ -7197,7 +7197,7 @@
       <c r="AJ31" s="121"/>
       <c r="AK31" s="92">
         <f>MAX($AL$10:$AL$97) - AL31</f>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AL31" s="121"/>
     </row>
@@ -7593,7 +7593,7 @@
       <c r="AA34" s="189"/>
       <c r="AB34" s="192">
         <f>SUM(T35:AA35)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AC34" s="188"/>
       <c r="AD34" s="189"/>
@@ -7615,7 +7615,7 @@
       </c>
       <c r="AL34" s="192">
         <f>$S34+$AB34+$AG34+$AJ34</f>
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7682,7 +7682,7 @@
       <c r="Y35" s="59"/>
       <c r="Z35" s="126">
         <f>(IF($Z34&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z34=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA34&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA34=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA35" s="62"/>
       <c r="AB35" s="121"/>
@@ -7696,7 +7696,7 @@
       <c r="AJ35" s="121"/>
       <c r="AK35" s="92">
         <f>MAX($AL$10:$AL$97) - AL35</f>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AL35" s="121"/>
     </row>
@@ -8092,7 +8092,7 @@
       <c r="AA38" s="47"/>
       <c r="AB38" s="122">
         <f>SUM(T39:AA39)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC38" s="48"/>
       <c r="AD38" s="47"/>
@@ -8114,7 +8114,7 @@
       </c>
       <c r="AL38" s="122">
         <f>$S38+$AB38+$AG38+$AJ38</f>
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -8181,7 +8181,7 @@
       <c r="Y39" s="59"/>
       <c r="Z39" s="126">
         <f>(IF($Z38&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z38=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA38&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA38=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA39" s="62"/>
       <c r="AB39" s="121"/>
@@ -8195,7 +8195,7 @@
       <c r="AJ39" s="121"/>
       <c r="AK39" s="92">
         <f>MAX($AL$10:$AL$97) - AL39</f>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AL39" s="121"/>
     </row>
@@ -8609,7 +8609,7 @@
       </c>
       <c r="AK42" s="194">
         <f>MAX($AL$10:$AL$97) - AL42</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AL42" s="192">
         <f>$S42+$AB42+$AG42+$AJ42</f>
@@ -8694,7 +8694,7 @@
       <c r="AJ43" s="121"/>
       <c r="AK43" s="111">
         <f>MAX($AL$10:$AL$97) - AL43</f>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AL43" s="121"/>
     </row>
@@ -9090,7 +9090,7 @@
       <c r="AA46" s="47"/>
       <c r="AB46" s="122">
         <f>SUM(T47:AA47)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AC46" s="48"/>
       <c r="AD46" s="47"/>
@@ -9112,7 +9112,7 @@
       </c>
       <c r="AL46" s="122">
         <f>$S46+$AB46+$AG46+$AJ46</f>
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="47" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -9179,7 +9179,7 @@
       <c r="Y47" s="59"/>
       <c r="Z47" s="126">
         <f>(IF($Z46&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z46=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA46&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA46=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA47" s="62"/>
       <c r="AB47" s="121"/>
@@ -9193,7 +9193,7 @@
       <c r="AJ47" s="121"/>
       <c r="AK47" s="111">
         <f>MAX($AL$10:$AL$97) - AL47</f>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AL47" s="121"/>
     </row>
@@ -9589,7 +9589,7 @@
       <c r="AA50" s="189"/>
       <c r="AB50" s="192">
         <f>SUM(T51:AA51)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AC50" s="188"/>
       <c r="AD50" s="189"/>
@@ -9599,7 +9599,7 @@
         <f>SUM(AC51:AF51)</f>
         <v>0</v>
       </c>
-      <c r="AH50" s="308"/>
+      <c r="AH50" s="256"/>
       <c r="AI50" s="183"/>
       <c r="AJ50" s="192">
         <f>AH51</f>
@@ -9611,7 +9611,7 @@
       </c>
       <c r="AL50" s="192">
         <f>$S50+$AB50+$AG50+$AJ50</f>
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="51" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -9678,7 +9678,7 @@
       <c r="Y51" s="59"/>
       <c r="Z51" s="126">
         <f>(IF($Z50&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z50=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA50&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA50=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA51" s="62"/>
       <c r="AB51" s="121"/>
@@ -10085,7 +10085,7 @@
       <c r="AA54" s="47"/>
       <c r="AB54" s="122">
         <f>SUM(T55:AA55)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AC54" s="48"/>
       <c r="AD54" s="47"/>
@@ -10107,7 +10107,7 @@
       </c>
       <c r="AL54" s="122">
         <f>$S54+$AB54+$AG54+$AJ54</f>
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="55" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -10174,7 +10174,7 @@
       <c r="Y55" s="59"/>
       <c r="Z55" s="126">
         <f>(IF($Z54&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z54=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA54&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA54=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA55" s="62"/>
       <c r="AB55" s="121"/>
@@ -10581,7 +10581,7 @@
       <c r="AA58" s="189"/>
       <c r="AB58" s="192">
         <f>SUM(T59:AA59)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AC58" s="188"/>
       <c r="AD58" s="189"/>
@@ -10603,7 +10603,7 @@
       </c>
       <c r="AL58" s="192">
         <f>$S58+$AB58+$AG58+$AJ58</f>
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="59" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -10670,7 +10670,7 @@
       <c r="Y59" s="59"/>
       <c r="Z59" s="126">
         <f>(IF($Z58&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z58=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA58&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA58=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA59" s="62"/>
       <c r="AB59" s="121"/>
@@ -11077,7 +11077,7 @@
       <c r="AA62" s="47"/>
       <c r="AB62" s="122">
         <f>SUM(T63:AA63)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC62" s="48"/>
       <c r="AD62" s="47"/>
@@ -11099,7 +11099,7 @@
       </c>
       <c r="AL62" s="122">
         <f>$S62+$AB62+$AG62+$AJ62</f>
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="63" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11166,7 +11166,7 @@
       <c r="Y63" s="59"/>
       <c r="Z63" s="126">
         <f>(IF($Z62&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z62=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA62&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA62=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA63" s="62"/>
       <c r="AB63" s="121"/>
@@ -11573,10 +11573,10 @@
       <c r="AA66" s="189"/>
       <c r="AB66" s="192">
         <f>SUM(T67:AA67)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC66" s="188"/>
-      <c r="AD66" s="307"/>
+      <c r="AD66" s="255"/>
       <c r="AE66" s="190"/>
       <c r="AF66" s="189"/>
       <c r="AG66" s="192">
@@ -11595,7 +11595,7 @@
       </c>
       <c r="AL66" s="192">
         <f>$S66+$AB66+$AG66+$AJ66</f>
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="67" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11662,7 +11662,7 @@
       <c r="Y67" s="59"/>
       <c r="Z67" s="126">
         <f>(IF($Z66&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z66=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA66&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA66=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA67" s="62"/>
       <c r="AB67" s="121"/>
@@ -12010,7 +12010,7 @@
     <row r="70" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="117">
         <f>RANK(AL70,$AL$10:$AL$97,)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B70" s="84" t="s">
         <v>82</v>
@@ -12087,7 +12087,7 @@
       </c>
       <c r="AK70" s="111">
         <f>MAX($AL$10:$AL$97) - AL70</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AL70" s="122">
         <f>$S70+$AB70+$AG70+$AJ70</f>
@@ -12565,7 +12565,7 @@
       <c r="AA74" s="189"/>
       <c r="AB74" s="192">
         <f>SUM(T75:AA75)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AC74" s="188"/>
       <c r="AD74" s="189"/>
@@ -12587,7 +12587,7 @@
       </c>
       <c r="AL74" s="192">
         <f>$S74+$AB74+$AG74+$AJ74</f>
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="75" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -12654,7 +12654,7 @@
       <c r="Y75" s="59"/>
       <c r="Z75" s="126">
         <f>(IF($Z74&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z74=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA74&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA74=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA75" s="62"/>
       <c r="AB75" s="121"/>
@@ -13005,7 +13005,7 @@
         <v>17</v>
       </c>
       <c r="B78" s="84" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C78" s="46">
         <v>5</v>
@@ -13024,44 +13024,44 @@
         <v>6</v>
       </c>
       <c r="K78" s="49">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L78" s="47"/>
       <c r="M78" s="44">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N78" s="45"/>
       <c r="O78" s="44">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P78" s="45"/>
       <c r="Q78" s="48"/>
       <c r="R78" s="50">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S78" s="122">
         <f>SUM(C79:R79)</f>
         <v>20</v>
       </c>
-      <c r="T78" s="46"/>
-      <c r="U78" s="47">
-        <v>6</v>
-      </c>
+      <c r="T78" s="46">
+        <v>7</v>
+      </c>
+      <c r="U78" s="47"/>
       <c r="V78" s="44">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="W78" s="47"/>
-      <c r="X78" s="49"/>
-      <c r="Y78" s="45">
-        <v>5</v>
-      </c>
-      <c r="Z78" s="48"/>
-      <c r="AA78" s="47">
-        <v>6</v>
-      </c>
+      <c r="X78" s="49">
+        <v>7</v>
+      </c>
+      <c r="Y78" s="45"/>
+      <c r="Z78" s="48">
+        <v>7</v>
+      </c>
+      <c r="AA78" s="47"/>
       <c r="AB78" s="122">
         <f>SUM(T79:AA79)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AC78" s="48"/>
       <c r="AD78" s="47"/>
@@ -13083,7 +13083,7 @@
       </c>
       <c r="AL78" s="122">
         <f>$S78+$AB78+$AG78+$AJ78</f>
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="79" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -13150,7 +13150,7 @@
       <c r="Y79" s="59"/>
       <c r="Z79" s="126">
         <f>(IF($Z78&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z78=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA78&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA78=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA79" s="62"/>
       <c r="AB79" s="121"/>
@@ -13498,10 +13498,10 @@
     <row r="82" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="173">
         <f>RANK(AL82,$AL$10:$AL$97,)</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B82" s="197" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C82" s="185">
         <v>5</v>
@@ -13520,41 +13520,41 @@
         <v>6</v>
       </c>
       <c r="K82" s="190">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L82" s="189"/>
       <c r="M82" s="187">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N82" s="186"/>
       <c r="O82" s="187">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P82" s="186"/>
       <c r="Q82" s="188"/>
       <c r="R82" s="191">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S82" s="192">
         <f>SUM(C83:R83)</f>
         <v>20</v>
       </c>
-      <c r="T82" s="185">
-        <v>7</v>
-      </c>
-      <c r="U82" s="189"/>
+      <c r="T82" s="185"/>
+      <c r="U82" s="189">
+        <v>6</v>
+      </c>
       <c r="V82" s="187">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="W82" s="189"/>
-      <c r="X82" s="190">
-        <v>7</v>
-      </c>
-      <c r="Y82" s="186"/>
-      <c r="Z82" s="188">
-        <v>7</v>
-      </c>
-      <c r="AA82" s="189"/>
+      <c r="X82" s="190"/>
+      <c r="Y82" s="186">
+        <v>5</v>
+      </c>
+      <c r="Z82" s="188"/>
+      <c r="AA82" s="189">
+        <v>6</v>
+      </c>
       <c r="AB82" s="192">
         <f>SUM(T83:AA83)</f>
         <v>3</v>
@@ -13575,7 +13575,7 @@
       </c>
       <c r="AK82" s="194">
         <f>MAX($AL$10:$AL$97) - AL82</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AL82" s="192">
         <f>$S82+$AB82+$AG82+$AJ82</f>
@@ -14053,7 +14053,7 @@
       <c r="AA86" s="47"/>
       <c r="AB86" s="122">
         <f>SUM(T87:AA87)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AC86" s="48"/>
       <c r="AD86" s="47"/>
@@ -14075,7 +14075,7 @@
       </c>
       <c r="AL86" s="122">
         <f>$S86+$AB86+$AG86+$AJ86</f>
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="87" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -14142,7 +14142,7 @@
       <c r="Y87" s="59"/>
       <c r="Z87" s="126">
         <f>(IF($Z86&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z86=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA86&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA86=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA87" s="62"/>
       <c r="AB87" s="121"/>
@@ -14549,7 +14549,7 @@
       <c r="AA90" s="189"/>
       <c r="AB90" s="192">
         <f>SUM(T91:AA91)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AC90" s="188"/>
       <c r="AD90" s="189"/>
@@ -14571,7 +14571,7 @@
       </c>
       <c r="AL90" s="192">
         <f>$S90+$AB90+$AG90+$AJ90</f>
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="91" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -14638,7 +14638,7 @@
       <c r="Y91" s="59"/>
       <c r="Z91" s="126">
         <f>(IF($Z90&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z90=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA90&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA90=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA91" s="62"/>
       <c r="AB91" s="121"/>
@@ -15045,7 +15045,7 @@
       <c r="AA94" s="47"/>
       <c r="AB94" s="204">
         <f>SUM(T95:AA95)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AC94" s="48"/>
       <c r="AD94" s="47"/>
@@ -15067,7 +15067,7 @@
       </c>
       <c r="AL94" s="204">
         <f>$S94+$AB94+$AG94+$AJ94</f>
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="95" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -15134,7 +15134,7 @@
       <c r="Y95" s="59"/>
       <c r="Z95" s="126">
         <f>(IF($Z94&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z94=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA94&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA94=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA95" s="62"/>
       <c r="AB95" s="121"/>
@@ -15612,12 +15612,12 @@
     <row r="100" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B100" s="43"/>
       <c r="N100" s="26"/>
-      <c r="O100" s="287" t="s">
+      <c r="O100" s="257" t="s">
         <v>17</v>
       </c>
-      <c r="P100" s="288"/>
-      <c r="Q100" s="288"/>
-      <c r="R100" s="289"/>
+      <c r="P100" s="258"/>
+      <c r="Q100" s="258"/>
+      <c r="R100" s="259"/>
       <c r="AG100" s="30"/>
       <c r="AH100" s="30"/>
       <c r="AI100" s="30"/>
@@ -15626,21 +15626,21 @@
     </row>
     <row r="101" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="33"/>
-      <c r="B101" s="275" t="s">
+      <c r="B101" s="286" t="s">
         <v>16</v>
       </c>
-      <c r="C101" s="276"/>
-      <c r="D101" s="276"/>
-      <c r="E101" s="276"/>
-      <c r="F101" s="276"/>
-      <c r="G101" s="276"/>
-      <c r="H101" s="276"/>
-      <c r="I101" s="276"/>
-      <c r="J101" s="276"/>
-      <c r="K101" s="276"/>
-      <c r="L101" s="276"/>
-      <c r="M101" s="276"/>
-      <c r="N101" s="277"/>
+      <c r="C101" s="287"/>
+      <c r="D101" s="287"/>
+      <c r="E101" s="287"/>
+      <c r="F101" s="287"/>
+      <c r="G101" s="287"/>
+      <c r="H101" s="287"/>
+      <c r="I101" s="287"/>
+      <c r="J101" s="287"/>
+      <c r="K101" s="287"/>
+      <c r="L101" s="287"/>
+      <c r="M101" s="287"/>
+      <c r="N101" s="288"/>
       <c r="O101" s="21">
         <v>1</v>
       </c>
@@ -15653,45 +15653,45 @@
       <c r="R101" s="22">
         <v>4</v>
       </c>
-      <c r="U101" s="290" t="s">
+      <c r="U101" s="260" t="s">
         <v>26</v>
       </c>
-      <c r="V101" s="291"/>
-      <c r="W101" s="291"/>
-      <c r="X101" s="291"/>
-      <c r="Y101" s="291"/>
-      <c r="Z101" s="291"/>
-      <c r="AA101" s="291"/>
-      <c r="AB101" s="291"/>
-      <c r="AC101" s="291"/>
-      <c r="AD101" s="292"/>
+      <c r="V101" s="261"/>
+      <c r="W101" s="261"/>
+      <c r="X101" s="261"/>
+      <c r="Y101" s="261"/>
+      <c r="Z101" s="261"/>
+      <c r="AA101" s="261"/>
+      <c r="AB101" s="261"/>
+      <c r="AC101" s="261"/>
+      <c r="AD101" s="262"/>
       <c r="AE101" s="28"/>
       <c r="AF101" s="28"/>
-      <c r="AG101" s="293" t="s">
+      <c r="AG101" s="263" t="s">
         <v>24</v>
       </c>
-      <c r="AH101" s="294"/>
-      <c r="AI101" s="294"/>
-      <c r="AJ101" s="294"/>
-      <c r="AK101" s="295"/>
+      <c r="AH101" s="264"/>
+      <c r="AI101" s="264"/>
+      <c r="AJ101" s="264"/>
+      <c r="AK101" s="265"/>
     </row>
     <row r="102" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A102" s="34"/>
-      <c r="B102" s="254" t="s">
+      <c r="B102" s="293" t="s">
         <v>6</v>
       </c>
-      <c r="C102" s="255"/>
-      <c r="D102" s="255"/>
-      <c r="E102" s="255"/>
-      <c r="F102" s="255"/>
-      <c r="G102" s="255"/>
-      <c r="H102" s="255"/>
-      <c r="I102" s="255"/>
-      <c r="J102" s="255"/>
-      <c r="K102" s="255"/>
-      <c r="L102" s="255"/>
-      <c r="M102" s="255"/>
-      <c r="N102" s="256"/>
+      <c r="C102" s="294"/>
+      <c r="D102" s="294"/>
+      <c r="E102" s="294"/>
+      <c r="F102" s="294"/>
+      <c r="G102" s="294"/>
+      <c r="H102" s="294"/>
+      <c r="I102" s="294"/>
+      <c r="J102" s="294"/>
+      <c r="K102" s="294"/>
+      <c r="L102" s="294"/>
+      <c r="M102" s="294"/>
+      <c r="N102" s="295"/>
       <c r="O102" s="20">
         <v>5</v>
       </c>
@@ -15704,49 +15704,49 @@
       <c r="R102" s="23">
         <v>20</v>
       </c>
-      <c r="U102" s="280" t="s">
+      <c r="U102" s="291" t="s">
         <v>20</v>
       </c>
-      <c r="V102" s="281"/>
-      <c r="W102" s="281"/>
-      <c r="X102" s="281"/>
-      <c r="Y102" s="281"/>
-      <c r="Z102" s="281"/>
-      <c r="AA102" s="281"/>
-      <c r="AB102" s="278">
+      <c r="V102" s="292"/>
+      <c r="W102" s="292"/>
+      <c r="X102" s="292"/>
+      <c r="Y102" s="292"/>
+      <c r="Z102" s="292"/>
+      <c r="AA102" s="292"/>
+      <c r="AB102" s="289">
         <v>22</v>
       </c>
-      <c r="AC102" s="278"/>
-      <c r="AD102" s="279"/>
+      <c r="AC102" s="289"/>
+      <c r="AD102" s="290"/>
       <c r="AE102" s="29"/>
       <c r="AF102" s="29"/>
-      <c r="AG102" s="261" t="s">
+      <c r="AG102" s="305" t="s">
         <v>21</v>
       </c>
-      <c r="AH102" s="262"/>
-      <c r="AI102" s="262"/>
-      <c r="AJ102" s="263"/>
+      <c r="AH102" s="306"/>
+      <c r="AI102" s="306"/>
+      <c r="AJ102" s="307"/>
       <c r="AK102" s="209">
         <v>230</v>
       </c>
     </row>
     <row r="103" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="34"/>
-      <c r="B103" s="254" t="s">
+      <c r="B103" s="293" t="s">
         <v>5</v>
       </c>
-      <c r="C103" s="255"/>
-      <c r="D103" s="255"/>
-      <c r="E103" s="255"/>
-      <c r="F103" s="255"/>
-      <c r="G103" s="255"/>
-      <c r="H103" s="255"/>
-      <c r="I103" s="255"/>
-      <c r="J103" s="255"/>
-      <c r="K103" s="255"/>
-      <c r="L103" s="255"/>
-      <c r="M103" s="255"/>
-      <c r="N103" s="256"/>
+      <c r="C103" s="294"/>
+      <c r="D103" s="294"/>
+      <c r="E103" s="294"/>
+      <c r="F103" s="294"/>
+      <c r="G103" s="294"/>
+      <c r="H103" s="294"/>
+      <c r="I103" s="294"/>
+      <c r="J103" s="294"/>
+      <c r="K103" s="294"/>
+      <c r="L103" s="294"/>
+      <c r="M103" s="294"/>
+      <c r="N103" s="295"/>
       <c r="O103" s="20">
         <v>2</v>
       </c>
@@ -15759,49 +15759,49 @@
       <c r="R103" s="23">
         <v>8</v>
       </c>
-      <c r="U103" s="259" t="s">
+      <c r="U103" s="300" t="s">
         <v>18</v>
       </c>
-      <c r="V103" s="260"/>
-      <c r="W103" s="260"/>
-      <c r="X103" s="260"/>
-      <c r="Y103" s="260"/>
-      <c r="Z103" s="260"/>
-      <c r="AA103" s="260"/>
-      <c r="AB103" s="285">
+      <c r="V103" s="301"/>
+      <c r="W103" s="301"/>
+      <c r="X103" s="301"/>
+      <c r="Y103" s="301"/>
+      <c r="Z103" s="301"/>
+      <c r="AA103" s="301"/>
+      <c r="AB103" s="302">
         <v>20</v>
       </c>
-      <c r="AC103" s="285"/>
-      <c r="AD103" s="286"/>
+      <c r="AC103" s="302"/>
+      <c r="AD103" s="303"/>
       <c r="AE103" s="29"/>
       <c r="AF103" s="29"/>
-      <c r="AG103" s="264" t="s">
+      <c r="AG103" s="308" t="s">
         <v>22</v>
       </c>
-      <c r="AH103" s="255"/>
-      <c r="AI103" s="255"/>
-      <c r="AJ103" s="256"/>
+      <c r="AH103" s="294"/>
+      <c r="AI103" s="294"/>
+      <c r="AJ103" s="295"/>
       <c r="AK103" s="36">
         <v>115</v>
       </c>
     </row>
     <row r="104" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="35"/>
-      <c r="B104" s="268" t="s">
+      <c r="B104" s="279" t="s">
         <v>4</v>
       </c>
-      <c r="C104" s="269"/>
-      <c r="D104" s="269"/>
-      <c r="E104" s="269"/>
-      <c r="F104" s="269"/>
-      <c r="G104" s="269"/>
-      <c r="H104" s="269"/>
-      <c r="I104" s="269"/>
-      <c r="J104" s="269"/>
-      <c r="K104" s="269"/>
-      <c r="L104" s="269"/>
-      <c r="M104" s="269"/>
-      <c r="N104" s="270"/>
+      <c r="C104" s="280"/>
+      <c r="D104" s="280"/>
+      <c r="E104" s="280"/>
+      <c r="F104" s="280"/>
+      <c r="G104" s="280"/>
+      <c r="H104" s="280"/>
+      <c r="I104" s="280"/>
+      <c r="J104" s="280"/>
+      <c r="K104" s="280"/>
+      <c r="L104" s="280"/>
+      <c r="M104" s="280"/>
+      <c r="N104" s="281"/>
       <c r="O104" s="3">
         <v>1</v>
       </c>
@@ -15814,51 +15814,51 @@
       <c r="R104" s="24">
         <v>1</v>
       </c>
-      <c r="U104" s="282" t="s">
+      <c r="U104" s="296" t="s">
         <v>19</v>
       </c>
-      <c r="V104" s="258"/>
-      <c r="W104" s="258"/>
-      <c r="X104" s="258"/>
-      <c r="Y104" s="258"/>
-      <c r="Z104" s="258"/>
-      <c r="AA104" s="258"/>
-      <c r="AB104" s="283">
+      <c r="V104" s="297"/>
+      <c r="W104" s="297"/>
+      <c r="X104" s="297"/>
+      <c r="Y104" s="297"/>
+      <c r="Z104" s="297"/>
+      <c r="AA104" s="297"/>
+      <c r="AB104" s="298">
         <f>AB102*AB103</f>
         <v>440</v>
       </c>
-      <c r="AC104" s="283"/>
-      <c r="AD104" s="284"/>
+      <c r="AC104" s="298"/>
+      <c r="AD104" s="299"/>
       <c r="AE104" s="29"/>
       <c r="AF104" s="29"/>
-      <c r="AG104" s="264" t="s">
+      <c r="AG104" s="308" t="s">
         <v>25</v>
       </c>
-      <c r="AH104" s="255"/>
-      <c r="AI104" s="255"/>
-      <c r="AJ104" s="256"/>
+      <c r="AH104" s="294"/>
+      <c r="AI104" s="294"/>
+      <c r="AJ104" s="295"/>
       <c r="AK104" s="36">
         <v>65</v>
       </c>
     </row>
     <row r="105" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG105" s="259" t="s">
+      <c r="AG105" s="300" t="s">
         <v>23</v>
       </c>
-      <c r="AH105" s="260"/>
-      <c r="AI105" s="260"/>
-      <c r="AJ105" s="260"/>
+      <c r="AH105" s="301"/>
+      <c r="AI105" s="301"/>
+      <c r="AJ105" s="301"/>
       <c r="AK105" s="211">
         <v>30</v>
       </c>
     </row>
     <row r="106" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG106" s="257" t="s">
+      <c r="AG106" s="304" t="s">
         <v>19</v>
       </c>
-      <c r="AH106" s="258"/>
-      <c r="AI106" s="258"/>
-      <c r="AJ106" s="258"/>
+      <c r="AH106" s="297"/>
+      <c r="AI106" s="297"/>
+      <c r="AJ106" s="297"/>
       <c r="AK106" s="210">
         <f>SUM(AK102:AK105)</f>
         <v>440</v>
@@ -15870,6 +15870,28 @@
     <sortCondition ref="B10:B94"/>
   </sortState>
   <mergeCells count="38">
+    <mergeCell ref="B103:N103"/>
+    <mergeCell ref="AG106:AJ106"/>
+    <mergeCell ref="AG105:AJ105"/>
+    <mergeCell ref="AG102:AJ102"/>
+    <mergeCell ref="AG104:AJ104"/>
+    <mergeCell ref="AG103:AJ103"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="B104:N104"/>
+    <mergeCell ref="C1:O1"/>
+    <mergeCell ref="P1:AJ1"/>
+    <mergeCell ref="C3:O3"/>
+    <mergeCell ref="P3:AJ3"/>
+    <mergeCell ref="C2:P2"/>
+    <mergeCell ref="Q2:AJ2"/>
+    <mergeCell ref="B101:N101"/>
+    <mergeCell ref="AB102:AD102"/>
+    <mergeCell ref="U102:AA102"/>
+    <mergeCell ref="B102:N102"/>
+    <mergeCell ref="U104:AA104"/>
+    <mergeCell ref="AB104:AD104"/>
+    <mergeCell ref="U103:AA103"/>
+    <mergeCell ref="AB103:AD103"/>
     <mergeCell ref="O100:R100"/>
     <mergeCell ref="U101:AD101"/>
     <mergeCell ref="AG101:AK101"/>
@@ -15886,28 +15908,6 @@
     <mergeCell ref="C5:J5"/>
     <mergeCell ref="K5:R5"/>
     <mergeCell ref="S5:S9"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="B104:N104"/>
-    <mergeCell ref="C1:O1"/>
-    <mergeCell ref="P1:AJ1"/>
-    <mergeCell ref="C3:O3"/>
-    <mergeCell ref="P3:AJ3"/>
-    <mergeCell ref="C2:P2"/>
-    <mergeCell ref="Q2:AJ2"/>
-    <mergeCell ref="B101:N101"/>
-    <mergeCell ref="AB102:AD102"/>
-    <mergeCell ref="U102:AA102"/>
-    <mergeCell ref="B102:N102"/>
-    <mergeCell ref="U104:AA104"/>
-    <mergeCell ref="AB104:AD104"/>
-    <mergeCell ref="U103:AA103"/>
-    <mergeCell ref="AB103:AD103"/>
-    <mergeCell ref="B103:N103"/>
-    <mergeCell ref="AG106:AJ106"/>
-    <mergeCell ref="AG105:AJ105"/>
-    <mergeCell ref="AG102:AJ102"/>
-    <mergeCell ref="AG104:AJ104"/>
-    <mergeCell ref="AG103:AJ103"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <conditionalFormatting sqref="AH18:AI18 AH10:AI10 AH14:AI14 T10:AA10 AC10:AF10 C10:R10 C14:R14 T14:AA14 AC14:AF14 T18:AA18 AC18:AF18 AH30:AI30 C30:R30 T30:AA30 AC30:AF30 AH26:AI26 C26:R26 T26:AA26 AC26:AF26 AH62:AI62 C62:R62 T62:AA62 AC62:AF62 AH42:AI42 C42:R42 T42:AA42 AC42:AF42 AH22:AI22 C22:R22 T22:AA22 AC22:AF22 AH38:AI38 C38:R38 T38:AA38 AC38:AF38 AH34:AI34 C34:R34 T34:AA34 AC34:AF34 AH66:AI66 C66:R66 T66:AA66 AC66:AF66 C18:R18">
@@ -16664,7 +16664,7 @@
   <dimension ref="A1:AJ31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17808,14 +17808,16 @@
       <c r="P24" s="82">
         <v>2</v>
       </c>
-      <c r="Q24" s="82"/>
+      <c r="Q24" s="82">
+        <v>4</v>
+      </c>
       <c r="R24" s="82"/>
       <c r="S24" s="82"/>
       <c r="T24" s="82"/>
       <c r="U24" s="81"/>
       <c r="V24" s="73">
         <f>IF(O24&gt;O25,1,0)+IF(P24&gt;P25,1,0)+IF(Q24&gt;Q25,1,0)+IF(R24&gt;R25,1,0)+IF(S24&gt;S25,1,0)+IF(T24&gt;T25,1,0)+IF(U24&gt;U25,1,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W24" s="16"/>
       <c r="X24" s="4"/>
@@ -17873,7 +17875,9 @@
       <c r="P25" s="82">
         <v>4</v>
       </c>
-      <c r="Q25" s="82"/>
+      <c r="Q25" s="82">
+        <v>3</v>
+      </c>
       <c r="R25" s="82"/>
       <c r="S25" s="82"/>
       <c r="T25" s="82"/>

</xml_diff>

<commit_message>
Update games of 2019-04-30 and fixed JCP
</commit_message>
<xml_diff>
--- a/laval.xlsx
+++ b/laval.xlsx
@@ -1934,7 +1934,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="309">
+  <cellXfs count="310">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2463,12 +2463,6 @@
     <xf numFmtId="0" fontId="14" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2478,34 +2472,109 @@
     <xf numFmtId="1" fontId="5" fillId="0" borderId="112" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="92" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="82" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="83" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="85" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2559,110 +2628,44 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="83" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="85" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="92" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="82" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3886,217 +3889,217 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="C1" s="282"/>
-      <c r="D1" s="282"/>
-      <c r="E1" s="282"/>
-      <c r="F1" s="282"/>
-      <c r="G1" s="282"/>
-      <c r="H1" s="282"/>
-      <c r="I1" s="282"/>
-      <c r="J1" s="282"/>
-      <c r="K1" s="282"/>
-      <c r="L1" s="282"/>
-      <c r="M1" s="282"/>
-      <c r="N1" s="282"/>
-      <c r="O1" s="282"/>
-      <c r="P1" s="283"/>
-      <c r="Q1" s="283"/>
-      <c r="R1" s="283"/>
-      <c r="S1" s="283"/>
-      <c r="T1" s="283"/>
-      <c r="U1" s="283"/>
-      <c r="V1" s="283"/>
-      <c r="W1" s="283"/>
-      <c r="X1" s="283"/>
-      <c r="Y1" s="283"/>
-      <c r="Z1" s="283"/>
-      <c r="AA1" s="283"/>
-      <c r="AB1" s="283"/>
-      <c r="AC1" s="283"/>
-      <c r="AD1" s="283"/>
-      <c r="AE1" s="283"/>
-      <c r="AF1" s="283"/>
-      <c r="AG1" s="283"/>
-      <c r="AH1" s="283"/>
-      <c r="AI1" s="283"/>
-      <c r="AJ1" s="283"/>
+      <c r="C1" s="264"/>
+      <c r="D1" s="264"/>
+      <c r="E1" s="264"/>
+      <c r="F1" s="264"/>
+      <c r="G1" s="264"/>
+      <c r="H1" s="264"/>
+      <c r="I1" s="264"/>
+      <c r="J1" s="264"/>
+      <c r="K1" s="264"/>
+      <c r="L1" s="264"/>
+      <c r="M1" s="264"/>
+      <c r="N1" s="264"/>
+      <c r="O1" s="264"/>
+      <c r="P1" s="265"/>
+      <c r="Q1" s="265"/>
+      <c r="R1" s="265"/>
+      <c r="S1" s="265"/>
+      <c r="T1" s="265"/>
+      <c r="U1" s="265"/>
+      <c r="V1" s="265"/>
+      <c r="W1" s="265"/>
+      <c r="X1" s="265"/>
+      <c r="Y1" s="265"/>
+      <c r="Z1" s="265"/>
+      <c r="AA1" s="265"/>
+      <c r="AB1" s="265"/>
+      <c r="AC1" s="265"/>
+      <c r="AD1" s="265"/>
+      <c r="AE1" s="265"/>
+      <c r="AF1" s="265"/>
+      <c r="AG1" s="265"/>
+      <c r="AH1" s="265"/>
+      <c r="AI1" s="265"/>
+      <c r="AJ1" s="265"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="41"/>
-      <c r="C2" s="284" t="s">
+      <c r="C2" s="266" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="284"/>
-      <c r="E2" s="284"/>
-      <c r="F2" s="284"/>
-      <c r="G2" s="284"/>
-      <c r="H2" s="284"/>
-      <c r="I2" s="284"/>
-      <c r="J2" s="284"/>
-      <c r="K2" s="284"/>
-      <c r="L2" s="284"/>
-      <c r="M2" s="284"/>
-      <c r="N2" s="284"/>
-      <c r="O2" s="284"/>
-      <c r="P2" s="284"/>
-      <c r="Q2" s="285" t="s">
+      <c r="D2" s="266"/>
+      <c r="E2" s="266"/>
+      <c r="F2" s="266"/>
+      <c r="G2" s="266"/>
+      <c r="H2" s="266"/>
+      <c r="I2" s="266"/>
+      <c r="J2" s="266"/>
+      <c r="K2" s="266"/>
+      <c r="L2" s="266"/>
+      <c r="M2" s="266"/>
+      <c r="N2" s="266"/>
+      <c r="O2" s="266"/>
+      <c r="P2" s="266"/>
+      <c r="Q2" s="267" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="283"/>
-      <c r="S2" s="283"/>
-      <c r="T2" s="283"/>
-      <c r="U2" s="283"/>
-      <c r="V2" s="283"/>
-      <c r="W2" s="283"/>
-      <c r="X2" s="283"/>
-      <c r="Y2" s="283"/>
-      <c r="Z2" s="283"/>
-      <c r="AA2" s="283"/>
-      <c r="AB2" s="283"/>
-      <c r="AC2" s="283"/>
-      <c r="AD2" s="283"/>
-      <c r="AE2" s="283"/>
-      <c r="AF2" s="283"/>
-      <c r="AG2" s="283"/>
-      <c r="AH2" s="283"/>
-      <c r="AI2" s="283"/>
-      <c r="AJ2" s="283"/>
+      <c r="R2" s="265"/>
+      <c r="S2" s="265"/>
+      <c r="T2" s="265"/>
+      <c r="U2" s="265"/>
+      <c r="V2" s="265"/>
+      <c r="W2" s="265"/>
+      <c r="X2" s="265"/>
+      <c r="Y2" s="265"/>
+      <c r="Z2" s="265"/>
+      <c r="AA2" s="265"/>
+      <c r="AB2" s="265"/>
+      <c r="AC2" s="265"/>
+      <c r="AD2" s="265"/>
+      <c r="AE2" s="265"/>
+      <c r="AF2" s="265"/>
+      <c r="AG2" s="265"/>
+      <c r="AH2" s="265"/>
+      <c r="AI2" s="265"/>
+      <c r="AJ2" s="265"/>
     </row>
     <row r="3" spans="1:38" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="282"/>
-      <c r="D3" s="282"/>
-      <c r="E3" s="282"/>
-      <c r="F3" s="282"/>
-      <c r="G3" s="282"/>
-      <c r="H3" s="282"/>
-      <c r="I3" s="282"/>
-      <c r="J3" s="282"/>
-      <c r="K3" s="282"/>
-      <c r="L3" s="282"/>
-      <c r="M3" s="282"/>
-      <c r="N3" s="282"/>
-      <c r="O3" s="282"/>
-      <c r="P3" s="283"/>
-      <c r="Q3" s="283"/>
-      <c r="R3" s="283"/>
-      <c r="S3" s="283"/>
-      <c r="T3" s="283"/>
-      <c r="U3" s="283"/>
-      <c r="V3" s="283"/>
-      <c r="W3" s="283"/>
-      <c r="X3" s="283"/>
-      <c r="Y3" s="283"/>
-      <c r="Z3" s="283"/>
-      <c r="AA3" s="283"/>
-      <c r="AB3" s="283"/>
-      <c r="AC3" s="283"/>
-      <c r="AD3" s="283"/>
-      <c r="AE3" s="283"/>
-      <c r="AF3" s="283"/>
-      <c r="AG3" s="283"/>
-      <c r="AH3" s="283"/>
-      <c r="AI3" s="283"/>
-      <c r="AJ3" s="283"/>
+      <c r="C3" s="264"/>
+      <c r="D3" s="264"/>
+      <c r="E3" s="264"/>
+      <c r="F3" s="264"/>
+      <c r="G3" s="264"/>
+      <c r="H3" s="264"/>
+      <c r="I3" s="264"/>
+      <c r="J3" s="264"/>
+      <c r="K3" s="264"/>
+      <c r="L3" s="264"/>
+      <c r="M3" s="264"/>
+      <c r="N3" s="264"/>
+      <c r="O3" s="264"/>
+      <c r="P3" s="265"/>
+      <c r="Q3" s="265"/>
+      <c r="R3" s="265"/>
+      <c r="S3" s="265"/>
+      <c r="T3" s="265"/>
+      <c r="U3" s="265"/>
+      <c r="V3" s="265"/>
+      <c r="W3" s="265"/>
+      <c r="X3" s="265"/>
+      <c r="Y3" s="265"/>
+      <c r="Z3" s="265"/>
+      <c r="AA3" s="265"/>
+      <c r="AB3" s="265"/>
+      <c r="AC3" s="265"/>
+      <c r="AD3" s="265"/>
+      <c r="AE3" s="265"/>
+      <c r="AF3" s="265"/>
+      <c r="AG3" s="265"/>
+      <c r="AH3" s="265"/>
+      <c r="AI3" s="265"/>
+      <c r="AJ3" s="265"/>
     </row>
     <row r="4" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="266" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="267"/>
-      <c r="E4" s="267"/>
-      <c r="F4" s="267"/>
-      <c r="G4" s="267"/>
-      <c r="H4" s="267"/>
-      <c r="I4" s="267"/>
-      <c r="J4" s="267"/>
-      <c r="K4" s="267"/>
-      <c r="L4" s="267"/>
-      <c r="M4" s="267"/>
-      <c r="N4" s="267"/>
-      <c r="O4" s="267"/>
-      <c r="P4" s="267"/>
-      <c r="Q4" s="267"/>
-      <c r="R4" s="267"/>
-      <c r="S4" s="268"/>
-      <c r="T4" s="266" t="s">
+      <c r="C4" s="289" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="290"/>
+      <c r="E4" s="290"/>
+      <c r="F4" s="290"/>
+      <c r="G4" s="290"/>
+      <c r="H4" s="290"/>
+      <c r="I4" s="290"/>
+      <c r="J4" s="290"/>
+      <c r="K4" s="290"/>
+      <c r="L4" s="290"/>
+      <c r="M4" s="290"/>
+      <c r="N4" s="290"/>
+      <c r="O4" s="290"/>
+      <c r="P4" s="290"/>
+      <c r="Q4" s="290"/>
+      <c r="R4" s="290"/>
+      <c r="S4" s="291"/>
+      <c r="T4" s="289" t="s">
         <v>1</v>
       </c>
-      <c r="U4" s="267"/>
-      <c r="V4" s="267"/>
-      <c r="W4" s="267"/>
-      <c r="X4" s="267"/>
-      <c r="Y4" s="267"/>
-      <c r="Z4" s="267"/>
-      <c r="AA4" s="267"/>
-      <c r="AB4" s="268"/>
-      <c r="AC4" s="266" t="s">
+      <c r="U4" s="290"/>
+      <c r="V4" s="290"/>
+      <c r="W4" s="290"/>
+      <c r="X4" s="290"/>
+      <c r="Y4" s="290"/>
+      <c r="Z4" s="290"/>
+      <c r="AA4" s="290"/>
+      <c r="AB4" s="291"/>
+      <c r="AC4" s="289" t="s">
         <v>2</v>
       </c>
-      <c r="AD4" s="267"/>
-      <c r="AE4" s="267"/>
-      <c r="AF4" s="267"/>
-      <c r="AG4" s="277"/>
-      <c r="AH4" s="266" t="s">
+      <c r="AD4" s="290"/>
+      <c r="AE4" s="290"/>
+      <c r="AF4" s="290"/>
+      <c r="AG4" s="298"/>
+      <c r="AH4" s="289" t="s">
         <v>10</v>
       </c>
-      <c r="AI4" s="267"/>
-      <c r="AJ4" s="268"/>
+      <c r="AI4" s="290"/>
+      <c r="AJ4" s="291"/>
     </row>
     <row r="5" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="278" t="s">
+      <c r="C5" s="258" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="274"/>
-      <c r="E5" s="274"/>
-      <c r="F5" s="274"/>
-      <c r="G5" s="274"/>
-      <c r="H5" s="274"/>
-      <c r="I5" s="274"/>
-      <c r="J5" s="275"/>
-      <c r="K5" s="273" t="s">
+      <c r="D5" s="259"/>
+      <c r="E5" s="259"/>
+      <c r="F5" s="259"/>
+      <c r="G5" s="259"/>
+      <c r="H5" s="259"/>
+      <c r="I5" s="259"/>
+      <c r="J5" s="260"/>
+      <c r="K5" s="296" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="274"/>
-      <c r="M5" s="274"/>
-      <c r="N5" s="274"/>
-      <c r="O5" s="274"/>
-      <c r="P5" s="274"/>
-      <c r="Q5" s="274"/>
-      <c r="R5" s="275"/>
-      <c r="S5" s="269" t="s">
+      <c r="L5" s="259"/>
+      <c r="M5" s="259"/>
+      <c r="N5" s="259"/>
+      <c r="O5" s="259"/>
+      <c r="P5" s="259"/>
+      <c r="Q5" s="259"/>
+      <c r="R5" s="260"/>
+      <c r="S5" s="292" t="s">
         <v>12</v>
       </c>
-      <c r="T5" s="278" t="s">
+      <c r="T5" s="258" t="s">
         <v>9</v>
       </c>
-      <c r="U5" s="274"/>
-      <c r="V5" s="274"/>
-      <c r="W5" s="275"/>
-      <c r="X5" s="273" t="s">
+      <c r="U5" s="259"/>
+      <c r="V5" s="259"/>
+      <c r="W5" s="260"/>
+      <c r="X5" s="296" t="s">
         <v>8</v>
       </c>
-      <c r="Y5" s="274"/>
-      <c r="Z5" s="274"/>
-      <c r="AA5" s="275"/>
-      <c r="AB5" s="269" t="s">
+      <c r="Y5" s="259"/>
+      <c r="Z5" s="259"/>
+      <c r="AA5" s="260"/>
+      <c r="AB5" s="292" t="s">
         <v>13</v>
       </c>
-      <c r="AC5" s="276" t="s">
+      <c r="AC5" s="297" t="s">
         <v>9</v>
       </c>
-      <c r="AD5" s="275"/>
-      <c r="AE5" s="273" t="s">
+      <c r="AD5" s="260"/>
+      <c r="AE5" s="296" t="s">
         <v>8</v>
       </c>
-      <c r="AF5" s="275"/>
-      <c r="AG5" s="269" t="s">
+      <c r="AF5" s="260"/>
+      <c r="AG5" s="292" t="s">
         <v>14</v>
       </c>
       <c r="AH5" s="56"/>
       <c r="AI5" s="25"/>
-      <c r="AJ5" s="269" t="s">
+      <c r="AJ5" s="292" t="s">
         <v>15</v>
       </c>
       <c r="AK5" s="4"/>
@@ -4168,14 +4171,14 @@
         <f>Résultats!$J$28</f>
         <v>3</v>
       </c>
-      <c r="S6" s="270"/>
+      <c r="S6" s="293"/>
       <c r="T6" s="156">
         <f>Résultats!$V$6</f>
         <v>1</v>
       </c>
       <c r="U6" s="103">
         <f>Résultats!$V$7</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V6" s="159">
         <f>Résultats!$V$10</f>
@@ -4187,7 +4190,7 @@
       </c>
       <c r="X6" s="105">
         <f>Résultats!$V$20</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y6" s="104">
         <f>Résultats!$V$21</f>
@@ -4201,7 +4204,7 @@
         <f>Résultats!$V$25</f>
         <v>1</v>
       </c>
-      <c r="AB6" s="270"/>
+      <c r="AB6" s="293"/>
       <c r="AC6" s="106">
         <f>Résultats!$AH$8</f>
         <v>0</v>
@@ -4218,7 +4221,7 @@
         <f>Résultats!$AH$23</f>
         <v>0</v>
       </c>
-      <c r="AG6" s="270"/>
+      <c r="AG6" s="293"/>
       <c r="AH6" s="198">
         <f>Résultats!$AH$15</f>
         <v>0</v>
@@ -4227,7 +4230,7 @@
         <f>Résultats!$AH$16</f>
         <v>0</v>
       </c>
-      <c r="AJ6" s="270"/>
+      <c r="AJ6" s="293"/>
       <c r="AK6" s="37"/>
     </row>
     <row r="7" spans="1:38" s="39" customFormat="1" ht="58.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -4253,7 +4256,7 @@
       <c r="P7" s="230"/>
       <c r="Q7" s="234"/>
       <c r="R7" s="112"/>
-      <c r="S7" s="270"/>
+      <c r="S7" s="293"/>
       <c r="T7" s="157"/>
       <c r="U7" s="112"/>
       <c r="V7" s="160"/>
@@ -4262,15 +4265,15 @@
       <c r="Y7" s="113"/>
       <c r="Z7" s="114"/>
       <c r="AA7" s="112"/>
-      <c r="AB7" s="270"/>
+      <c r="AB7" s="293"/>
       <c r="AC7" s="114"/>
       <c r="AD7" s="112"/>
       <c r="AE7" s="115"/>
       <c r="AF7" s="112"/>
-      <c r="AG7" s="270"/>
+      <c r="AG7" s="293"/>
       <c r="AH7" s="198"/>
       <c r="AI7" s="107"/>
-      <c r="AJ7" s="270"/>
+      <c r="AJ7" s="293"/>
       <c r="AK7" s="37"/>
     </row>
     <row r="8" spans="1:38" s="39" customFormat="1" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4340,7 +4343,7 @@
         <f>Résultats!$B$28</f>
         <v>VEGAS</v>
       </c>
-      <c r="S8" s="270"/>
+      <c r="S8" s="293"/>
       <c r="T8" s="158" t="str">
         <f>Résultats!$N$6</f>
         <v>BOSTON</v>
@@ -4373,7 +4376,7 @@
         <f>Résultats!$N$25</f>
         <v>DALLAS</v>
       </c>
-      <c r="AB8" s="270"/>
+      <c r="AB8" s="293"/>
       <c r="AC8" s="164" t="str">
         <f>Résultats!$Z$8</f>
         <v xml:space="preserve"> </v>
@@ -4390,7 +4393,7 @@
         <f>Résultats!$Z$23</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AG8" s="270"/>
+      <c r="AG8" s="293"/>
       <c r="AH8" s="199" t="str">
         <f>Résultats!$Z$15</f>
         <v xml:space="preserve"> </v>
@@ -4399,7 +4402,7 @@
         <f>Résultats!$Z$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ8" s="270"/>
+      <c r="AJ8" s="293"/>
       <c r="AK8" s="37"/>
     </row>
     <row r="9" spans="1:38" s="39" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4473,7 +4476,7 @@
         <f>Résultats!$A$28</f>
         <v>P3</v>
       </c>
-      <c r="S9" s="272"/>
+      <c r="S9" s="295"/>
       <c r="T9" s="166" t="str">
         <f>Résultats!$M$6</f>
         <v>A2</v>
@@ -4506,7 +4509,7 @@
         <f>Résultats!$M$25</f>
         <v>WC1</v>
       </c>
-      <c r="AB9" s="271"/>
+      <c r="AB9" s="294"/>
       <c r="AC9" s="170" t="str">
         <f>Résultats!$Y$8</f>
         <v xml:space="preserve"> </v>
@@ -4523,7 +4526,7 @@
         <f>Résultats!$Y$23</f>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="AG9" s="271"/>
+      <c r="AG9" s="294"/>
       <c r="AH9" s="201" t="str">
         <f>Résultats!$Y$15</f>
         <v xml:space="preserve"> </v>
@@ -4532,7 +4535,7 @@
         <f>Résultats!$Y$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ9" s="272"/>
+      <c r="AJ9" s="295"/>
       <c r="AK9" s="109" t="s">
         <v>51</v>
       </c>
@@ -4602,7 +4605,7 @@
       <c r="AA10" s="180"/>
       <c r="AB10" s="181">
         <f>SUM(T11:AA11)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AC10" s="179"/>
       <c r="AD10" s="176"/>
@@ -4624,7 +4627,7 @@
       </c>
       <c r="AL10" s="181">
         <f>$S10+$AB10+$AG10+$AJ10</f>
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -4676,7 +4679,7 @@
       <c r="S11" s="121"/>
       <c r="T11" s="126">
         <f>(IF($T10&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T10=$T$6+$U$6,$P$103,0),0),0)+IF($U10&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U10=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U11" s="126"/>
       <c r="V11" s="126">
@@ -5053,7 +5056,7 @@
       </c>
       <c r="F14" s="45"/>
       <c r="G14" s="48"/>
-      <c r="H14" s="245">
+      <c r="H14" s="243">
         <v>7</v>
       </c>
       <c r="I14" s="44"/>
@@ -5098,7 +5101,7 @@
       </c>
       <c r="AB14" s="122">
         <f>SUM(T15:AA15)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AC14" s="48"/>
       <c r="AD14" s="47"/>
@@ -5116,11 +5119,11 @@
       </c>
       <c r="AK14" s="111">
         <f>MAX($AL$10:$AL$97) - AL14</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AL14" s="122">
         <f>$S14+$AB14+$AG14+$AJ14</f>
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5172,7 +5175,7 @@
       <c r="S15" s="144"/>
       <c r="T15" s="126">
         <f>(IF($T14&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T14=$T$6+$U$6,$P$103,0),0),0)+IF($U14&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U14=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U15" s="126"/>
       <c r="V15" s="126">
@@ -5182,7 +5185,7 @@
       <c r="W15" s="126"/>
       <c r="X15" s="126">
         <f>(IF($X14&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X14=$X$6+$Y$6,$P$103,0),0),0)+IF($Y14&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y14=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y15" s="59"/>
       <c r="Z15" s="126">
@@ -5201,7 +5204,7 @@
       <c r="AJ15" s="121"/>
       <c r="AK15" s="92">
         <f>MAX($AL$10:$AL$97) - AL15</f>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AL15" s="121"/>
     </row>
@@ -5571,7 +5574,7 @@
         <v>5</v>
       </c>
       <c r="P18" s="186"/>
-      <c r="Q18" s="244">
+      <c r="Q18" s="242">
         <v>7</v>
       </c>
       <c r="R18" s="191"/>
@@ -5597,7 +5600,7 @@
       <c r="AA18" s="191"/>
       <c r="AB18" s="192">
         <f>SUM(T19:AA19)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AC18" s="188"/>
       <c r="AD18" s="189"/>
@@ -5619,7 +5622,7 @@
       </c>
       <c r="AL18" s="192">
         <f>$S18+$AB18+$AG18+$AJ18</f>
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5671,7 +5674,7 @@
       <c r="S19" s="144"/>
       <c r="T19" s="126">
         <f>(IF($T18&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T18=$T$6+$U$6,$P$103,0),0),0)+IF($U18&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U18=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U19" s="126"/>
       <c r="V19" s="126">
@@ -5700,7 +5703,7 @@
       <c r="AJ19" s="144"/>
       <c r="AK19" s="150">
         <f>MAX($AL$10:$AL$97) - AL19</f>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AL19" s="121"/>
     </row>
@@ -6096,7 +6099,7 @@
       </c>
       <c r="AB22" s="122">
         <f>SUM(T23:AA23)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC22" s="48"/>
       <c r="AD22" s="47"/>
@@ -6106,7 +6109,7 @@
         <f>SUM(AC23:AF23)</f>
         <v>0</v>
       </c>
-      <c r="AH22" s="254"/>
+      <c r="AH22" s="245"/>
       <c r="AI22" s="57"/>
       <c r="AJ22" s="122">
         <f>AH23</f>
@@ -6118,7 +6121,7 @@
       </c>
       <c r="AL22" s="122">
         <f>$S22+$AB22+$AG22+$AJ22</f>
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6180,7 +6183,7 @@
       <c r="W23" s="126"/>
       <c r="X23" s="126">
         <f>(IF($X22&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X22=$X$6+$Y$6,$P$103,0),0),0)+IF($Y22&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y22=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y23" s="59"/>
       <c r="Z23" s="126">
@@ -6199,7 +6202,7 @@
       <c r="AJ23" s="144"/>
       <c r="AK23" s="150">
         <f>MAX($AL$10:$AL$97) - AL23</f>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AL23" s="121"/>
     </row>
@@ -6595,10 +6598,10 @@
       <c r="AA26" s="191"/>
       <c r="AB26" s="192">
         <f>SUM(T27:AA27)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AC26" s="188"/>
-      <c r="AD26" s="255"/>
+      <c r="AD26" s="246"/>
       <c r="AE26" s="190"/>
       <c r="AF26" s="189"/>
       <c r="AG26" s="192">
@@ -6617,7 +6620,7 @@
       </c>
       <c r="AL26" s="192">
         <f>$S26+$AB26+$AG26+$AJ26</f>
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6669,7 +6672,7 @@
       <c r="S27" s="144"/>
       <c r="T27" s="126">
         <f>(IF($T26&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T26=$T$6+$U$6,$P$103,0),0),0)+IF($U26&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U26=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U27" s="126"/>
       <c r="V27" s="126">
@@ -6698,7 +6701,7 @@
       <c r="AJ27" s="144"/>
       <c r="AK27" s="150">
         <f>MAX($AL$10:$AL$97) - AL27</f>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AL27" s="121"/>
     </row>
@@ -7035,7 +7038,7 @@
     <row r="30" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="117">
         <f>RANK(AL30,$AL$10:$AL$97,)</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B30" s="84" t="s">
         <v>73</v>
@@ -7049,7 +7052,7 @@
       </c>
       <c r="F30" s="45"/>
       <c r="G30" s="48"/>
-      <c r="H30" s="245">
+      <c r="H30" s="243">
         <v>7</v>
       </c>
       <c r="I30" s="44"/>
@@ -7094,7 +7097,7 @@
       <c r="AA30" s="47"/>
       <c r="AB30" s="122">
         <f>SUM(T31:AA31)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AC30" s="48"/>
       <c r="AD30" s="47"/>
@@ -7112,11 +7115,11 @@
       </c>
       <c r="AK30" s="111">
         <f>MAX($AL$10:$AL$97) - AL30</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AL30" s="122">
         <f>$S30+$AB30+$AG30+$AJ30</f>
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7168,7 +7171,7 @@
       <c r="S31" s="121"/>
       <c r="T31" s="126">
         <f>(IF($T30&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T30=$T$6+$U$6,$P$103,0),0),0)+IF($U30&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U30=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U31" s="126"/>
       <c r="V31" s="126">
@@ -7178,7 +7181,7 @@
       <c r="W31" s="126"/>
       <c r="X31" s="126">
         <f>(IF($X30&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X30=$X$6+$Y$6,$P$103,0),0),0)+IF($Y30&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y30=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y31" s="59"/>
       <c r="Z31" s="126">
@@ -7197,7 +7200,7 @@
       <c r="AJ31" s="121"/>
       <c r="AK31" s="92">
         <f>MAX($AL$10:$AL$97) - AL31</f>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AL31" s="121"/>
     </row>
@@ -7537,63 +7540,63 @@
         <v>7</v>
       </c>
       <c r="B34" s="197" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="C34" s="185">
+        <v>7</v>
+      </c>
+      <c r="D34" s="186"/>
+      <c r="E34" s="308">
         <v>6</v>
       </c>
-      <c r="D34" s="186"/>
-      <c r="E34" s="187">
+      <c r="F34" s="186"/>
+      <c r="G34" s="309"/>
+      <c r="H34" s="189">
+        <v>6</v>
+      </c>
+      <c r="I34" s="308"/>
+      <c r="J34" s="189">
+        <v>7</v>
+      </c>
+      <c r="K34" s="190">
         <v>5</v>
       </c>
-      <c r="F34" s="186"/>
-      <c r="G34" s="188">
+      <c r="L34" s="189"/>
+      <c r="M34" s="187">
         <v>7</v>
       </c>
-      <c r="H34" s="189"/>
-      <c r="I34" s="187"/>
-      <c r="J34" s="189">
-        <v>6</v>
-      </c>
-      <c r="K34" s="190">
-        <v>6</v>
-      </c>
-      <c r="L34" s="189"/>
-      <c r="M34" s="187"/>
-      <c r="N34" s="186">
-        <v>7</v>
-      </c>
+      <c r="N34" s="186"/>
       <c r="O34" s="187">
         <v>6</v>
       </c>
       <c r="P34" s="186"/>
-      <c r="Q34" s="244">
-        <v>7</v>
+      <c r="Q34" s="188">
+        <v>6</v>
       </c>
       <c r="R34" s="191"/>
       <c r="S34" s="192">
         <f>SUM(C35:R35)</f>
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="T34" s="185"/>
       <c r="U34" s="189">
         <v>7</v>
       </c>
-      <c r="V34" s="187">
+      <c r="V34" s="187"/>
+      <c r="W34" s="189">
         <v>6</v>
       </c>
-      <c r="W34" s="189"/>
-      <c r="X34" s="190"/>
-      <c r="Y34" s="186">
+      <c r="X34" s="190">
         <v>7</v>
       </c>
+      <c r="Y34" s="186"/>
       <c r="Z34" s="188">
         <v>6</v>
       </c>
       <c r="AA34" s="189"/>
       <c r="AB34" s="192">
         <f>SUM(T35:AA35)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AC34" s="188"/>
       <c r="AD34" s="189"/>
@@ -7615,7 +7618,7 @@
       </c>
       <c r="AL34" s="192">
         <f>$S34+$AB34+$AG34+$AJ34</f>
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7636,7 +7639,7 @@
       <c r="F35" s="76"/>
       <c r="G35" s="77">
         <f>(IF($G34&lt;&gt;"",($G$6*$O$104)+IF($G$6=4,($O$102)+IF($G34=$G$6+$H$6,$O$103,0),0),0)+IF($H34&lt;&gt;"",($H$6*$O$104)+IF($H$6=4,($O$102)+IF($H34=$G$6+$H$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H35" s="76"/>
       <c r="I35" s="77">
@@ -7651,7 +7654,7 @@
       <c r="L35" s="76"/>
       <c r="M35" s="77">
         <f>(IF($M34&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M34=$M$6+$N$6,$O$103,0),0),0)+IF($N34&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N34=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="N35" s="76"/>
       <c r="O35" s="77">
@@ -7661,23 +7664,23 @@
       <c r="P35" s="76"/>
       <c r="Q35" s="77">
         <f>(IF($Q34&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q34=$Q$6+$R$6,$O$103,0),0),0)+IF($R34&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R34=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="R35" s="80"/>
       <c r="S35" s="121"/>
       <c r="T35" s="126">
         <f>(IF($T34&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T34=$T$6+$U$6,$P$103,0),0),0)+IF($U34&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U34=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U35" s="126"/>
       <c r="V35" s="126">
         <f>(IF($V34&lt;&gt;"",($V$6*$P$104)+IF($V$6=4,($P$102)+IF($V34=$V$6+$W$6,$P$103,0),0),0)+IF($W34&lt;&gt;"",($W$6*$P$104)+IF($W$6=4,($P$102)+IF($W34=$V$6+$W$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W35" s="126"/>
       <c r="X35" s="126">
         <f>(IF($X34&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X34=$X$6+$Y$6,$P$103,0),0),0)+IF($Y34&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y34=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y35" s="59"/>
       <c r="Z35" s="126">
@@ -7696,7 +7699,7 @@
       <c r="AJ35" s="121"/>
       <c r="AK35" s="92">
         <f>MAX($AL$10:$AL$97) - AL35</f>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AL35" s="121"/>
     </row>
@@ -7739,7 +7742,7 @@
         <f>IF(ISBLANK(H34),
 0,
 IF(H$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I36" s="118">
         <f>IF(ISBLANK(I34),
@@ -7775,7 +7778,7 @@
         <f>IF(ISBLANK(N34),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O36" s="118">
         <f>IF(ISBLANK(O34),
@@ -7958,7 +7961,7 @@
         <f>IF(Q36 = 0,
 0,
 IF(Q34 = (Q$6+R$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R37" s="118">
         <f>IF(R36 = 0,
@@ -8026,73 +8029,73 @@
       <c r="AJ37" s="138"/>
       <c r="AK37" s="139">
         <f>SUM(C37:AI37)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL37" s="123"/>
     </row>
     <row r="38" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="117">
         <f>RANK(AL38,$AL$10:$AL$97,)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B38" s="84" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C38" s="46">
+        <v>6</v>
+      </c>
+      <c r="D38" s="45"/>
+      <c r="E38" s="44">
+        <v>5</v>
+      </c>
+      <c r="F38" s="45"/>
+      <c r="G38" s="48">
         <v>7</v>
       </c>
-      <c r="D38" s="45"/>
-      <c r="E38" s="242">
+      <c r="H38" s="47"/>
+      <c r="I38" s="44"/>
+      <c r="J38" s="47">
         <v>6</v>
       </c>
-      <c r="F38" s="45"/>
-      <c r="G38" s="243"/>
-      <c r="H38" s="47">
+      <c r="K38" s="49">
         <v>6</v>
       </c>
-      <c r="I38" s="242"/>
-      <c r="J38" s="47">
+      <c r="L38" s="47"/>
+      <c r="M38" s="44"/>
+      <c r="N38" s="45">
         <v>7</v>
       </c>
-      <c r="K38" s="49">
-        <v>5</v>
-      </c>
-      <c r="L38" s="47"/>
-      <c r="M38" s="44">
-        <v>7</v>
-      </c>
-      <c r="N38" s="45"/>
       <c r="O38" s="44">
         <v>6</v>
       </c>
       <c r="P38" s="45"/>
-      <c r="Q38" s="48">
-        <v>6</v>
+      <c r="Q38" s="299">
+        <v>7</v>
       </c>
       <c r="R38" s="50"/>
       <c r="S38" s="122">
         <f>SUM(C39:R39)</f>
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="T38" s="46"/>
       <c r="U38" s="47">
         <v>7</v>
       </c>
-      <c r="V38" s="44"/>
-      <c r="W38" s="47">
+      <c r="V38" s="44">
         <v>6</v>
       </c>
-      <c r="X38" s="49">
+      <c r="W38" s="47"/>
+      <c r="X38" s="49"/>
+      <c r="Y38" s="45">
         <v>7</v>
       </c>
-      <c r="Y38" s="45"/>
       <c r="Z38" s="48">
         <v>6</v>
       </c>
       <c r="AA38" s="47"/>
       <c r="AB38" s="122">
         <f>SUM(T39:AA39)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AC38" s="48"/>
       <c r="AD38" s="47"/>
@@ -8110,11 +8113,11 @@
       </c>
       <c r="AK38" s="111">
         <f>MAX($AL$10:$AL$97) - AL38</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AL38" s="122">
         <f>$S38+$AB38+$AG38+$AJ38</f>
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -8135,7 +8138,7 @@
       <c r="F39" s="76"/>
       <c r="G39" s="119">
         <f>(IF($G38&lt;&gt;"",($G$6*$O$104)+IF($G$6=4,($O$102)+IF($G38=$G$6+$H$6,$O$103,0),0),0)+IF($H38&lt;&gt;"",($H$6*$O$104)+IF($H$6=4,($O$102)+IF($H38=$G$6+$H$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H39" s="76"/>
       <c r="I39" s="116">
@@ -8150,7 +8153,7 @@
       <c r="L39" s="76"/>
       <c r="M39" s="77">
         <f>(IF($M38&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M38=$M$6+$N$6,$O$103,0),0),0)+IF($N38&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N38=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="N39" s="76"/>
       <c r="O39" s="77">
@@ -8160,18 +8163,18 @@
       <c r="P39" s="76"/>
       <c r="Q39" s="77">
         <f>(IF($Q38&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q38=$Q$6+$R$6,$O$103,0),0),0)+IF($R38&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R38=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="R39" s="80"/>
       <c r="S39" s="121"/>
       <c r="T39" s="126">
         <f>(IF($T38&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T38=$T$6+$U$6,$P$103,0),0),0)+IF($U38&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U38=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U39" s="126"/>
       <c r="V39" s="126">
         <f>(IF($V38&lt;&gt;"",($V$6*$P$104)+IF($V$6=4,($P$102)+IF($V38=$V$6+$W$6,$P$103,0),0),0)+IF($W38&lt;&gt;"",($W$6*$P$104)+IF($W$6=4,($P$102)+IF($W38=$V$6+$W$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W39" s="126"/>
       <c r="X39" s="126">
@@ -8195,7 +8198,7 @@
       <c r="AJ39" s="121"/>
       <c r="AK39" s="92">
         <f>MAX($AL$10:$AL$97) - AL39</f>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AL39" s="121"/>
     </row>
@@ -8238,7 +8241,7 @@
         <f>IF(ISBLANK(H38),
 0,
 IF(H$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I40" s="118">
         <f>IF(ISBLANK(I38),
@@ -8274,7 +8277,7 @@
         <f>IF(ISBLANK(N38),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O40" s="118">
         <f>IF(ISBLANK(O38),
@@ -8457,7 +8460,7 @@
         <f>IF(Q40 = 0,
 0,
 IF(Q38 = (Q$6+R$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R41" s="118">
         <f>IF(R40 = 0,
@@ -8525,7 +8528,7 @@
       <c r="AJ41" s="138"/>
       <c r="AK41" s="139">
         <f>SUM(C41:AI41)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL41" s="123"/>
     </row>
@@ -8591,7 +8594,7 @@
       </c>
       <c r="AB42" s="192">
         <f>SUM(T43:AA43)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AC42" s="188"/>
       <c r="AD42" s="189"/>
@@ -8609,11 +8612,11 @@
       </c>
       <c r="AK42" s="194">
         <f>MAX($AL$10:$AL$97) - AL42</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AL42" s="192">
         <f>$S42+$AB42+$AG42+$AJ42</f>
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -8665,7 +8668,7 @@
       <c r="S43" s="121"/>
       <c r="T43" s="126">
         <f>(IF($T42&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T42=$T$6+$U$6,$P$103,0),0),0)+IF($U42&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U42=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U43" s="126"/>
       <c r="V43" s="126">
@@ -8675,7 +8678,7 @@
       <c r="W43" s="126"/>
       <c r="X43" s="126">
         <f>(IF($X42&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X42=$X$6+$Y$6,$P$103,0),0),0)+IF($Y42&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y42=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y43" s="59"/>
       <c r="Z43" s="126">
@@ -8694,7 +8697,7 @@
       <c r="AJ43" s="121"/>
       <c r="AK43" s="111">
         <f>MAX($AL$10:$AL$97) - AL43</f>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AL43" s="121"/>
     </row>
@@ -9034,34 +9037,34 @@
         <v>10</v>
       </c>
       <c r="B46" s="84" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="C46" s="46">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D46" s="45"/>
       <c r="E46" s="44">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F46" s="45"/>
       <c r="G46" s="48">
+        <v>5</v>
+      </c>
+      <c r="H46" s="47"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="47">
         <v>6</v>
       </c>
-      <c r="H46" s="47"/>
-      <c r="I46" s="44">
+      <c r="K46" s="49">
+        <v>5</v>
+      </c>
+      <c r="L46" s="47"/>
+      <c r="M46" s="44"/>
+      <c r="N46" s="239">
         <v>6</v>
       </c>
-      <c r="J46" s="47"/>
-      <c r="K46" s="49">
-        <v>7</v>
-      </c>
-      <c r="L46" s="47"/>
-      <c r="M46" s="44">
+      <c r="O46" s="44">
         <v>5</v>
-      </c>
-      <c r="N46" s="45"/>
-      <c r="O46" s="44">
-        <v>4</v>
       </c>
       <c r="P46" s="45"/>
       <c r="Q46" s="48"/>
@@ -9072,25 +9075,25 @@
         <f>SUM(C47:R47)</f>
         <v>29</v>
       </c>
-      <c r="T46" s="46">
+      <c r="T46" s="46"/>
+      <c r="U46" s="47">
         <v>6</v>
       </c>
-      <c r="U46" s="47"/>
       <c r="V46" s="44">
         <v>5</v>
       </c>
       <c r="W46" s="47"/>
-      <c r="X46" s="49"/>
-      <c r="Y46" s="45">
+      <c r="X46" s="49">
         <v>7</v>
       </c>
+      <c r="Y46" s="45"/>
       <c r="Z46" s="48">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AA46" s="47"/>
       <c r="AB46" s="122">
         <f>SUM(T47:AA47)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AC46" s="48"/>
       <c r="AD46" s="47"/>
@@ -9100,7 +9103,7 @@
         <f>SUM(AC47:AF47)</f>
         <v>0</v>
       </c>
-      <c r="AH46" s="102"/>
+      <c r="AH46" s="300"/>
       <c r="AI46" s="57"/>
       <c r="AJ46" s="122">
         <f>AH47</f>
@@ -9108,11 +9111,11 @@
       </c>
       <c r="AK46" s="111">
         <f>MAX($AL$10:$AL$97) - AL46</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AL46" s="122">
         <f>$S46+$AB46+$AG46+$AJ46</f>
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -9138,7 +9141,7 @@
       <c r="H47" s="76"/>
       <c r="I47" s="77">
         <f>(IF($I46&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I46=$I$6+$J$6,$O$103,0),0),0)+IF($J46&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J46=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J47" s="78"/>
       <c r="K47" s="79">
@@ -9148,7 +9151,7 @@
       <c r="L47" s="76"/>
       <c r="M47" s="77">
         <f>(IF($M46&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M46=$M$6+$N$6,$O$103,0),0),0)+IF($N46&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N46=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="N47" s="76"/>
       <c r="O47" s="77">
@@ -9164,7 +9167,7 @@
       <c r="S47" s="121"/>
       <c r="T47" s="126">
         <f>(IF($T46&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T46=$T$6+$U$6,$P$103,0),0),0)+IF($U46&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U46=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U47" s="126"/>
       <c r="V47" s="126">
@@ -9174,7 +9177,7 @@
       <c r="W47" s="126"/>
       <c r="X47" s="126">
         <f>(IF($X46&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X46=$X$6+$Y$6,$P$103,0),0),0)+IF($Y46&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y46=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y47" s="59"/>
       <c r="Z47" s="126">
@@ -9193,7 +9196,7 @@
       <c r="AJ47" s="121"/>
       <c r="AK47" s="111">
         <f>MAX($AL$10:$AL$97) - AL47</f>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AL47" s="121"/>
     </row>
@@ -9242,7 +9245,7 @@
         <f>IF(ISBLANK(I46),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J48" s="118">
         <f>IF(ISBLANK(J46),
@@ -9272,7 +9275,7 @@
         <f>IF(ISBLANK(N46),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O48" s="118">
         <f>IF(ISBLANK(O46),
@@ -9437,7 +9440,7 @@
         <f>IF(N48 = 0,
 0,
 IF(N46 = (M$6+N$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O49" s="118">
         <f>IF(O48 = 0,
@@ -9523,33 +9526,33 @@
       <c r="AJ49" s="138"/>
       <c r="AK49" s="139">
         <f>SUM(C49:AI49)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL49" s="123"/>
     </row>
     <row r="50" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="173">
         <f>RANK(AL50,$AL$10:$AL$97,)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B50" s="197" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C50" s="185">
         <v>5</v>
       </c>
       <c r="D50" s="186"/>
       <c r="E50" s="187">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F50" s="186"/>
       <c r="G50" s="188">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H50" s="189"/>
       <c r="I50" s="187"/>
       <c r="J50" s="189">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K50" s="190">
         <v>5</v>
@@ -9560,7 +9563,7 @@
         <v>6</v>
       </c>
       <c r="O50" s="187">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P50" s="186"/>
       <c r="Q50" s="188"/>
@@ -9571,25 +9574,25 @@
         <f>SUM(C51:R51)</f>
         <v>29</v>
       </c>
-      <c r="T50" s="185">
+      <c r="T50" s="185"/>
+      <c r="U50" s="189">
         <v>6</v>
       </c>
-      <c r="U50" s="189"/>
       <c r="V50" s="187">
         <v>5</v>
       </c>
       <c r="W50" s="189"/>
-      <c r="X50" s="190">
-        <v>7</v>
-      </c>
-      <c r="Y50" s="186"/>
+      <c r="X50" s="190"/>
+      <c r="Y50" s="186">
+        <v>5</v>
+      </c>
       <c r="Z50" s="188">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA50" s="189"/>
       <c r="AB50" s="192">
         <f>SUM(T51:AA51)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AC50" s="188"/>
       <c r="AD50" s="189"/>
@@ -9599,7 +9602,7 @@
         <f>SUM(AC51:AF51)</f>
         <v>0</v>
       </c>
-      <c r="AH50" s="256"/>
+      <c r="AH50" s="195"/>
       <c r="AI50" s="183"/>
       <c r="AJ50" s="192">
         <f>AH51</f>
@@ -9611,7 +9614,7 @@
       </c>
       <c r="AL50" s="192">
         <f>$S50+$AB50+$AG50+$AJ50</f>
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="51" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -9663,7 +9666,7 @@
       <c r="S51" s="121"/>
       <c r="T51" s="126">
         <f>(IF($T50&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T50=$T$6+$U$6,$P$103,0),0),0)+IF($U50&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U50=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U51" s="126"/>
       <c r="V51" s="126">
@@ -10026,46 +10029,46 @@
     <row r="54" spans="1:38" s="27" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="117">
         <f>RANK(AL54,$AL$10:$AL$97,)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B54" s="84" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="C54" s="46">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D54" s="45"/>
-      <c r="E54" s="44">
-        <v>6</v>
+      <c r="E54" s="237">
+        <v>7</v>
       </c>
       <c r="F54" s="45"/>
       <c r="G54" s="48">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H54" s="47"/>
       <c r="I54" s="44"/>
       <c r="J54" s="47">
+        <v>5</v>
+      </c>
+      <c r="K54" s="49">
         <v>7</v>
       </c>
-      <c r="K54" s="49">
-        <v>5</v>
-      </c>
       <c r="L54" s="47"/>
-      <c r="M54" s="44"/>
-      <c r="N54" s="239">
+      <c r="M54" s="44">
         <v>6</v>
       </c>
+      <c r="N54" s="45"/>
       <c r="O54" s="44">
         <v>7</v>
       </c>
       <c r="P54" s="45"/>
-      <c r="Q54" s="48"/>
-      <c r="R54" s="50">
-        <v>6</v>
-      </c>
+      <c r="Q54" s="48">
+        <v>5</v>
+      </c>
+      <c r="R54" s="50"/>
       <c r="S54" s="122">
         <f>SUM(C55:R55)</f>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="T54" s="46"/>
       <c r="U54" s="47">
@@ -10075,17 +10078,17 @@
         <v>5</v>
       </c>
       <c r="W54" s="47"/>
-      <c r="X54" s="49"/>
-      <c r="Y54" s="45">
-        <v>5</v>
-      </c>
+      <c r="X54" s="49">
+        <v>4</v>
+      </c>
+      <c r="Y54" s="45"/>
       <c r="Z54" s="48">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AA54" s="47"/>
       <c r="AB54" s="122">
         <f>SUM(T55:AA55)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AC54" s="48"/>
       <c r="AD54" s="47"/>
@@ -10107,7 +10110,7 @@
       </c>
       <c r="AL54" s="122">
         <f>$S54+$AB54+$AG54+$AJ54</f>
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="55" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -10123,7 +10126,7 @@
       <c r="D55" s="127"/>
       <c r="E55" s="125">
         <f>(IF($E54&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E54=$E$6+$F$6,$O$103,0),0),0)+IF($F54&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F54=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F55" s="127"/>
       <c r="G55" s="125">
@@ -10143,7 +10146,7 @@
       <c r="L55" s="127"/>
       <c r="M55" s="125">
         <f>(IF($M54&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M54=$M$6+$N$6,$O$103,0),0),0)+IF($N54&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N54=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="N55" s="127"/>
       <c r="O55" s="128">
@@ -10153,13 +10156,13 @@
       <c r="P55" s="127"/>
       <c r="Q55" s="128">
         <f>(IF($Q54&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q54=$Q$6+$R$6,$O$103,0),0),0)+IF($R54&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R54=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="R55" s="131"/>
       <c r="S55" s="121"/>
       <c r="T55" s="126">
         <f>(IF($T54&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T54=$T$6+$U$6,$P$103,0),0),0)+IF($U54&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U54=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U55" s="126"/>
       <c r="V55" s="126">
@@ -10169,7 +10172,7 @@
       <c r="W55" s="126"/>
       <c r="X55" s="126">
         <f>(IF($X54&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X54=$X$6+$Y$6,$P$103,0),0),0)+IF($Y54&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y54=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y55" s="59"/>
       <c r="Z55" s="126">
@@ -10264,7 +10267,7 @@
         <f>IF(ISBLANK(N54),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O56" s="118">
         <f>IF(ISBLANK(O54),
@@ -10282,7 +10285,7 @@
         <f>IF(ISBLANK(Q54),
 0,
 IF(Q$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R56" s="118">
         <f>IF(ISBLANK(R54),
@@ -10375,7 +10378,7 @@
         <f>IF(E56 = 0,
 0,
 IF(E54 = (E$6+F$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F57" s="118">
         <f>IF(F56 = 0,
@@ -10429,7 +10432,7 @@
         <f>IF(N56 = 0,
 0,
 IF(N54 = (M$6+N$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O57" s="118">
         <f>IF(O56 = 0,
@@ -10525,58 +10528,58 @@
         <v>13</v>
       </c>
       <c r="B58" s="197" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="C58" s="185">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D58" s="186"/>
-      <c r="E58" s="238">
-        <v>7</v>
+      <c r="E58" s="187">
+        <v>4</v>
       </c>
       <c r="F58" s="186"/>
       <c r="G58" s="188">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H58" s="189"/>
-      <c r="I58" s="187"/>
-      <c r="J58" s="189">
-        <v>5</v>
-      </c>
+      <c r="I58" s="187">
+        <v>6</v>
+      </c>
+      <c r="J58" s="189"/>
       <c r="K58" s="190">
         <v>7</v>
       </c>
       <c r="L58" s="189"/>
       <c r="M58" s="187">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N58" s="186"/>
       <c r="O58" s="187">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="P58" s="186"/>
-      <c r="Q58" s="188">
-        <v>5</v>
-      </c>
-      <c r="R58" s="191"/>
+      <c r="Q58" s="188"/>
+      <c r="R58" s="191">
+        <v>6</v>
+      </c>
       <c r="S58" s="192">
         <f>SUM(C59:R59)</f>
-        <v>28</v>
-      </c>
-      <c r="T58" s="185"/>
-      <c r="U58" s="189">
+        <v>29</v>
+      </c>
+      <c r="T58" s="185">
         <v>6</v>
       </c>
+      <c r="U58" s="189"/>
       <c r="V58" s="187">
         <v>5</v>
       </c>
       <c r="W58" s="189"/>
-      <c r="X58" s="190">
-        <v>4</v>
-      </c>
-      <c r="Y58" s="186"/>
+      <c r="X58" s="190"/>
+      <c r="Y58" s="186">
+        <v>7</v>
+      </c>
       <c r="Z58" s="188">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA58" s="189"/>
       <c r="AB58" s="192">
@@ -10603,7 +10606,7 @@
       </c>
       <c r="AL58" s="192">
         <f>$S58+$AB58+$AG58+$AJ58</f>
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="59" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -10619,7 +10622,7 @@
       <c r="D59" s="127"/>
       <c r="E59" s="125">
         <f>(IF($E58&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E58=$E$6+$F$6,$O$103,0),0),0)+IF($F58&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F58=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F59" s="127"/>
       <c r="G59" s="125">
@@ -10629,7 +10632,7 @@
       <c r="H59" s="127"/>
       <c r="I59" s="128">
         <f>(IF($I58&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I58=$I$6+$J$6,$O$103,0),0),0)+IF($J58&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J58=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J59" s="129"/>
       <c r="K59" s="130">
@@ -10649,7 +10652,7 @@
       <c r="P59" s="127"/>
       <c r="Q59" s="128">
         <f>(IF($Q58&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q58=$Q$6+$R$6,$O$103,0),0),0)+IF($R58&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R58=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="R59" s="131"/>
       <c r="S59" s="121"/>
@@ -10730,7 +10733,7 @@
         <f>IF(ISBLANK(I58),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J60" s="118">
         <f>IF(ISBLANK(J58),
@@ -10778,7 +10781,7 @@
         <f>IF(ISBLANK(Q58),
 0,
 IF(Q$6= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R60" s="118">
         <f>IF(ISBLANK(R58),
@@ -10871,7 +10874,7 @@
         <f>IF(E60 = 0,
 0,
 IF(E58 = (E$6+F$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F61" s="118">
         <f>IF(F60 = 0,
@@ -11011,7 +11014,7 @@
       <c r="AJ61" s="138"/>
       <c r="AK61" s="139">
         <f>SUM(C61:AI61)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL61" s="123"/>
     </row>
@@ -11077,7 +11080,7 @@
       <c r="AA62" s="47"/>
       <c r="AB62" s="122">
         <f>SUM(T63:AA63)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AC62" s="48"/>
       <c r="AD62" s="47"/>
@@ -11095,11 +11098,11 @@
       </c>
       <c r="AK62" s="111">
         <f>MAX($AL$10:$AL$97) - AL62</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AL62" s="122">
         <f>$S62+$AB62+$AG62+$AJ62</f>
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="63" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11151,7 +11154,7 @@
       <c r="S63" s="121"/>
       <c r="T63" s="126">
         <f>(IF($T62&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T62=$T$6+$U$6,$P$103,0),0),0)+IF($U62&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U62=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U63" s="126"/>
       <c r="V63" s="126">
@@ -11161,7 +11164,7 @@
       <c r="W63" s="126"/>
       <c r="X63" s="126">
         <f>(IF($X62&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X62=$X$6+$Y$6,$P$103,0),0),0)+IF($Y62&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y62=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y63" s="59"/>
       <c r="Z63" s="126">
@@ -11573,10 +11576,10 @@
       <c r="AA66" s="189"/>
       <c r="AB66" s="192">
         <f>SUM(T67:AA67)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AC66" s="188"/>
-      <c r="AD66" s="255"/>
+      <c r="AD66" s="246"/>
       <c r="AE66" s="190"/>
       <c r="AF66" s="189"/>
       <c r="AG66" s="192">
@@ -11595,7 +11598,7 @@
       </c>
       <c r="AL66" s="192">
         <f>$S66+$AB66+$AG66+$AJ66</f>
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="67" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11647,7 +11650,7 @@
       <c r="S67" s="121"/>
       <c r="T67" s="126">
         <f>(IF($T66&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T66=$T$6+$U$6,$P$103,0),0),0)+IF($U66&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U66=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U67" s="126"/>
       <c r="V67" s="126">
@@ -12013,38 +12016,38 @@
         <v>16</v>
       </c>
       <c r="B70" s="84" t="s">
-        <v>82</v>
-      </c>
-      <c r="C70" s="46">
+        <v>68</v>
+      </c>
+      <c r="C70" s="301">
+        <v>5</v>
+      </c>
+      <c r="D70" s="302"/>
+      <c r="E70" s="303">
         <v>6</v>
       </c>
-      <c r="D70" s="45"/>
-      <c r="E70" s="44">
+      <c r="F70" s="302"/>
+      <c r="G70" s="304">
+        <v>5</v>
+      </c>
+      <c r="H70" s="305"/>
+      <c r="I70" s="303"/>
+      <c r="J70" s="305">
         <v>6</v>
       </c>
-      <c r="F70" s="45"/>
-      <c r="G70" s="48">
+      <c r="K70" s="306">
         <v>6</v>
       </c>
-      <c r="H70" s="47"/>
-      <c r="I70" s="44"/>
-      <c r="J70" s="47">
+      <c r="L70" s="305"/>
+      <c r="M70" s="303">
         <v>7</v>
       </c>
-      <c r="K70" s="49">
-        <v>5</v>
-      </c>
-      <c r="L70" s="47"/>
-      <c r="M70" s="44">
-        <v>7</v>
-      </c>
-      <c r="N70" s="45"/>
-      <c r="O70" s="44">
+      <c r="N70" s="302"/>
+      <c r="O70" s="303">
         <v>6</v>
       </c>
-      <c r="P70" s="45"/>
-      <c r="Q70" s="48"/>
-      <c r="R70" s="50">
+      <c r="P70" s="302"/>
+      <c r="Q70" s="304"/>
+      <c r="R70" s="307">
         <v>6</v>
       </c>
       <c r="S70" s="122">
@@ -12055,21 +12058,21 @@
       <c r="U70" s="47">
         <v>6</v>
       </c>
-      <c r="V70" s="44"/>
-      <c r="W70" s="47">
+      <c r="V70" s="44">
+        <v>7</v>
+      </c>
+      <c r="W70" s="47"/>
+      <c r="X70" s="49">
         <v>6</v>
       </c>
-      <c r="X70" s="49"/>
-      <c r="Y70" s="45">
+      <c r="Y70" s="45"/>
+      <c r="Z70" s="48">
         <v>7</v>
       </c>
-      <c r="Z70" s="48"/>
-      <c r="AA70" s="47">
-        <v>6</v>
-      </c>
+      <c r="AA70" s="47"/>
       <c r="AB70" s="122">
         <f>SUM(T71:AA71)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC70" s="48"/>
       <c r="AD70" s="47"/>
@@ -12091,7 +12094,7 @@
       </c>
       <c r="AL70" s="122">
         <f>$S70+$AB70+$AG70+$AJ70</f>
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="71" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -12143,22 +12146,22 @@
       <c r="S71" s="121"/>
       <c r="T71" s="126">
         <f>(IF($T70&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T70=$T$6+$U$6,$P$103,0),0),0)+IF($U70&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U70=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U71" s="126"/>
       <c r="V71" s="126">
         <f>(IF($V70&lt;&gt;"",($V$6*$P$104)+IF($V$6=4,($P$102)+IF($V70=$V$6+$W$6,$P$103,0),0),0)+IF($W70&lt;&gt;"",($W$6*$P$104)+IF($W$6=4,($P$102)+IF($W70=$V$6+$W$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W71" s="126"/>
       <c r="X71" s="126">
         <f>(IF($X70&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X70=$X$6+$Y$6,$P$103,0),0),0)+IF($Y70&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y70=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y71" s="59"/>
       <c r="Z71" s="126">
         <f>(IF($Z70&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z70=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA70&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA70=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA71" s="62"/>
       <c r="AB71" s="121"/>
@@ -12506,41 +12509,41 @@
     <row r="74" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="173">
         <f>RANK(AL74,$AL$10:$AL$97,)</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B74" s="197" t="s">
-        <v>68</v>
-      </c>
-      <c r="C74" s="247">
+        <v>82</v>
+      </c>
+      <c r="C74" s="185">
+        <v>6</v>
+      </c>
+      <c r="D74" s="186"/>
+      <c r="E74" s="187">
+        <v>6</v>
+      </c>
+      <c r="F74" s="186"/>
+      <c r="G74" s="188">
+        <v>6</v>
+      </c>
+      <c r="H74" s="189"/>
+      <c r="I74" s="187"/>
+      <c r="J74" s="189">
+        <v>7</v>
+      </c>
+      <c r="K74" s="190">
         <v>5</v>
       </c>
-      <c r="D74" s="248"/>
-      <c r="E74" s="249">
+      <c r="L74" s="189"/>
+      <c r="M74" s="187">
+        <v>7</v>
+      </c>
+      <c r="N74" s="186"/>
+      <c r="O74" s="187">
         <v>6</v>
       </c>
-      <c r="F74" s="248"/>
-      <c r="G74" s="250">
-        <v>5</v>
-      </c>
-      <c r="H74" s="251"/>
-      <c r="I74" s="249"/>
-      <c r="J74" s="251">
-        <v>6</v>
-      </c>
-      <c r="K74" s="252">
-        <v>6</v>
-      </c>
-      <c r="L74" s="251"/>
-      <c r="M74" s="249">
-        <v>7</v>
-      </c>
-      <c r="N74" s="248"/>
-      <c r="O74" s="249">
-        <v>6</v>
-      </c>
-      <c r="P74" s="248"/>
-      <c r="Q74" s="250"/>
-      <c r="R74" s="253">
+      <c r="P74" s="186"/>
+      <c r="Q74" s="188"/>
+      <c r="R74" s="191">
         <v>6</v>
       </c>
       <c r="S74" s="192">
@@ -12551,21 +12554,21 @@
       <c r="U74" s="189">
         <v>6</v>
       </c>
-      <c r="V74" s="187">
+      <c r="V74" s="187"/>
+      <c r="W74" s="189">
+        <v>6</v>
+      </c>
+      <c r="X74" s="190"/>
+      <c r="Y74" s="186">
         <v>7</v>
       </c>
-      <c r="W74" s="189"/>
-      <c r="X74" s="190">
+      <c r="Z74" s="188"/>
+      <c r="AA74" s="189">
         <v>6</v>
       </c>
-      <c r="Y74" s="186"/>
-      <c r="Z74" s="188">
-        <v>7</v>
-      </c>
-      <c r="AA74" s="189"/>
       <c r="AB74" s="192">
         <f>SUM(T75:AA75)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AC74" s="188"/>
       <c r="AD74" s="189"/>
@@ -12583,11 +12586,11 @@
       </c>
       <c r="AK74" s="194">
         <f>MAX($AL$10:$AL$97) - AL74</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AL74" s="192">
         <f>$S74+$AB74+$AG74+$AJ74</f>
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="75" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -12639,12 +12642,12 @@
       <c r="S75" s="121"/>
       <c r="T75" s="126">
         <f>(IF($T74&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T74=$T$6+$U$6,$P$103,0),0),0)+IF($U74&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U74=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U75" s="126"/>
       <c r="V75" s="126">
         <f>(IF($V74&lt;&gt;"",($V$6*$P$104)+IF($V$6=4,($P$102)+IF($V74=$V$6+$W$6,$P$103,0),0),0)+IF($W74&lt;&gt;"",($W$6*$P$104)+IF($W$6=4,($P$102)+IF($W74=$V$6+$W$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W75" s="126"/>
       <c r="X75" s="126">
@@ -12654,7 +12657,7 @@
       <c r="Y75" s="59"/>
       <c r="Z75" s="126">
         <f>(IF($Z74&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z74=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA74&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA74=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA75" s="62"/>
       <c r="AB75" s="121"/>
@@ -13002,7 +13005,7 @@
     <row r="78" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="117">
         <f>RANK(AL78,$AL$10:$AL$97,)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B78" s="84" t="s">
         <v>75</v>
@@ -13061,7 +13064,7 @@
       <c r="AA78" s="47"/>
       <c r="AB78" s="122">
         <f>SUM(T79:AA79)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AC78" s="48"/>
       <c r="AD78" s="47"/>
@@ -13083,7 +13086,7 @@
       </c>
       <c r="AL78" s="122">
         <f>$S78+$AB78+$AG78+$AJ78</f>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="79" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -13145,7 +13148,7 @@
       <c r="W79" s="126"/>
       <c r="X79" s="126">
         <f>(IF($X78&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X78=$X$6+$Y$6,$P$103,0),0),0)+IF($Y78&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y78=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y79" s="59"/>
       <c r="Z79" s="126">
@@ -13557,7 +13560,7 @@
       </c>
       <c r="AB82" s="192">
         <f>SUM(T83:AA83)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AC82" s="188"/>
       <c r="AD82" s="189"/>
@@ -13579,7 +13582,7 @@
       </c>
       <c r="AL82" s="192">
         <f>$S82+$AB82+$AG82+$AJ82</f>
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="83" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -13631,7 +13634,7 @@
       <c r="S83" s="121"/>
       <c r="T83" s="126">
         <f>(IF($T82&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T82=$T$6+$U$6,$P$103,0),0),0)+IF($U82&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U82=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U83" s="126"/>
       <c r="V83" s="126">
@@ -14053,7 +14056,7 @@
       <c r="AA86" s="47"/>
       <c r="AB86" s="122">
         <f>SUM(T87:AA87)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AC86" s="48"/>
       <c r="AD86" s="47"/>
@@ -14071,11 +14074,11 @@
       </c>
       <c r="AK86" s="111">
         <f>MAX($AL$10:$AL$97) - AL86</f>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AL86" s="122">
         <f>$S86+$AB86+$AG86+$AJ86</f>
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="87" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -14127,7 +14130,7 @@
       <c r="S87" s="121"/>
       <c r="T87" s="126">
         <f>(IF($T86&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T86=$T$6+$U$6,$P$103,0),0),0)+IF($U86&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U86=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U87" s="126"/>
       <c r="V87" s="126">
@@ -14137,7 +14140,7 @@
       <c r="W87" s="126"/>
       <c r="X87" s="126">
         <f>(IF($X86&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X86=$X$6+$Y$6,$P$103,0),0),0)+IF($Y86&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y86=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y87" s="59"/>
       <c r="Z87" s="126">
@@ -14493,10 +14496,10 @@
         <v>20</v>
       </c>
       <c r="B90" s="197" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C90" s="185">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D90" s="186"/>
       <c r="E90" s="187"/>
@@ -14504,28 +14507,28 @@
         <v>7</v>
       </c>
       <c r="G90" s="188">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H90" s="189"/>
       <c r="I90" s="187"/>
       <c r="J90" s="189">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K90" s="190">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L90" s="189"/>
       <c r="M90" s="187">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N90" s="186"/>
       <c r="O90" s="187">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P90" s="186"/>
       <c r="Q90" s="188"/>
       <c r="R90" s="191">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S90" s="192">
         <f>SUM(C91:R91)</f>
@@ -14536,20 +14539,20 @@
         <v>7</v>
       </c>
       <c r="V90" s="187">
+        <v>7</v>
+      </c>
+      <c r="W90" s="189"/>
+      <c r="X90" s="190">
         <v>6</v>
       </c>
-      <c r="W90" s="189"/>
-      <c r="X90" s="190"/>
-      <c r="Y90" s="186">
-        <v>6</v>
-      </c>
+      <c r="Y90" s="186"/>
       <c r="Z90" s="188">
         <v>6</v>
       </c>
       <c r="AA90" s="189"/>
       <c r="AB90" s="192">
         <f>SUM(T91:AA91)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AC90" s="188"/>
       <c r="AD90" s="189"/>
@@ -14567,11 +14570,11 @@
       </c>
       <c r="AK90" s="194">
         <f>MAX($AL$10:$AL$97) - AL90</f>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AL90" s="192">
         <f>$S90+$AB90+$AG90+$AJ90</f>
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="91" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -14623,7 +14626,7 @@
       <c r="S91" s="121"/>
       <c r="T91" s="126">
         <f>(IF($T90&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T90=$T$6+$U$6,$P$103,0),0),0)+IF($U90&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U90=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U91" s="126"/>
       <c r="V91" s="126">
@@ -14633,7 +14636,7 @@
       <c r="W91" s="126"/>
       <c r="X91" s="126">
         <f>(IF($X90&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X90=$X$6+$Y$6,$P$103,0),0),0)+IF($Y90&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y90=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y91" s="59"/>
       <c r="Z91" s="126">
@@ -14986,13 +14989,13 @@
     <row r="94" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A94" s="117">
         <f>RANK(AL94,$AL$10:$AL$97,)</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B94" s="84" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C94" s="212">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D94" s="213"/>
       <c r="E94" s="214"/>
@@ -15000,28 +15003,28 @@
         <v>7</v>
       </c>
       <c r="G94" s="215">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H94" s="216"/>
       <c r="I94" s="214"/>
       <c r="J94" s="216">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K94" s="217">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L94" s="216"/>
       <c r="M94" s="214">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N94" s="213"/>
       <c r="O94" s="214">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P94" s="213"/>
       <c r="Q94" s="215"/>
       <c r="R94" s="218">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S94" s="122">
         <f>SUM(C95:R95)</f>
@@ -15032,20 +15035,20 @@
         <v>7</v>
       </c>
       <c r="V94" s="44">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="W94" s="47"/>
-      <c r="X94" s="49">
+      <c r="X94" s="49"/>
+      <c r="Y94" s="45">
         <v>6</v>
       </c>
-      <c r="Y94" s="45"/>
       <c r="Z94" s="48">
         <v>6</v>
       </c>
       <c r="AA94" s="47"/>
       <c r="AB94" s="204">
         <f>SUM(T95:AA95)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AC94" s="48"/>
       <c r="AD94" s="47"/>
@@ -15067,7 +15070,7 @@
       </c>
       <c r="AL94" s="204">
         <f>$S94+$AB94+$AG94+$AJ94</f>
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="95" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -15119,7 +15122,7 @@
       <c r="S95" s="121"/>
       <c r="T95" s="126">
         <f>(IF($T94&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T94=$T$6+$U$6,$P$103,0),0),0)+IF($U94&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U94=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U95" s="126"/>
       <c r="V95" s="126">
@@ -15510,7 +15513,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="J98" s="246">
+      <c r="J98" s="244">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
@@ -15549,17 +15552,17 @@
       <c r="S98" s="68"/>
       <c r="T98" s="207">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U98" s="205">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="V98" s="207">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="W98" s="246">
+      <c r="W98" s="244">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -15612,12 +15615,12 @@
     <row r="100" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B100" s="43"/>
       <c r="N100" s="26"/>
-      <c r="O100" s="257" t="s">
+      <c r="O100" s="280" t="s">
         <v>17</v>
       </c>
-      <c r="P100" s="258"/>
-      <c r="Q100" s="258"/>
-      <c r="R100" s="259"/>
+      <c r="P100" s="281"/>
+      <c r="Q100" s="281"/>
+      <c r="R100" s="282"/>
       <c r="AG100" s="30"/>
       <c r="AH100" s="30"/>
       <c r="AI100" s="30"/>
@@ -15626,21 +15629,21 @@
     </row>
     <row r="101" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="33"/>
-      <c r="B101" s="286" t="s">
+      <c r="B101" s="268" t="s">
         <v>16</v>
       </c>
-      <c r="C101" s="287"/>
-      <c r="D101" s="287"/>
-      <c r="E101" s="287"/>
-      <c r="F101" s="287"/>
-      <c r="G101" s="287"/>
-      <c r="H101" s="287"/>
-      <c r="I101" s="287"/>
-      <c r="J101" s="287"/>
-      <c r="K101" s="287"/>
-      <c r="L101" s="287"/>
-      <c r="M101" s="287"/>
-      <c r="N101" s="288"/>
+      <c r="C101" s="269"/>
+      <c r="D101" s="269"/>
+      <c r="E101" s="269"/>
+      <c r="F101" s="269"/>
+      <c r="G101" s="269"/>
+      <c r="H101" s="269"/>
+      <c r="I101" s="269"/>
+      <c r="J101" s="269"/>
+      <c r="K101" s="269"/>
+      <c r="L101" s="269"/>
+      <c r="M101" s="269"/>
+      <c r="N101" s="270"/>
       <c r="O101" s="21">
         <v>1</v>
       </c>
@@ -15653,45 +15656,45 @@
       <c r="R101" s="22">
         <v>4</v>
       </c>
-      <c r="U101" s="260" t="s">
+      <c r="U101" s="283" t="s">
         <v>26</v>
       </c>
-      <c r="V101" s="261"/>
-      <c r="W101" s="261"/>
-      <c r="X101" s="261"/>
-      <c r="Y101" s="261"/>
-      <c r="Z101" s="261"/>
-      <c r="AA101" s="261"/>
-      <c r="AB101" s="261"/>
-      <c r="AC101" s="261"/>
-      <c r="AD101" s="262"/>
+      <c r="V101" s="284"/>
+      <c r="W101" s="284"/>
+      <c r="X101" s="284"/>
+      <c r="Y101" s="284"/>
+      <c r="Z101" s="284"/>
+      <c r="AA101" s="284"/>
+      <c r="AB101" s="284"/>
+      <c r="AC101" s="284"/>
+      <c r="AD101" s="285"/>
       <c r="AE101" s="28"/>
       <c r="AF101" s="28"/>
-      <c r="AG101" s="263" t="s">
+      <c r="AG101" s="286" t="s">
         <v>24</v>
       </c>
-      <c r="AH101" s="264"/>
-      <c r="AI101" s="264"/>
-      <c r="AJ101" s="264"/>
-      <c r="AK101" s="265"/>
+      <c r="AH101" s="287"/>
+      <c r="AI101" s="287"/>
+      <c r="AJ101" s="287"/>
+      <c r="AK101" s="288"/>
     </row>
     <row r="102" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A102" s="34"/>
-      <c r="B102" s="293" t="s">
+      <c r="B102" s="247" t="s">
         <v>6</v>
       </c>
-      <c r="C102" s="294"/>
-      <c r="D102" s="294"/>
-      <c r="E102" s="294"/>
-      <c r="F102" s="294"/>
-      <c r="G102" s="294"/>
-      <c r="H102" s="294"/>
-      <c r="I102" s="294"/>
-      <c r="J102" s="294"/>
-      <c r="K102" s="294"/>
-      <c r="L102" s="294"/>
-      <c r="M102" s="294"/>
-      <c r="N102" s="295"/>
+      <c r="C102" s="248"/>
+      <c r="D102" s="248"/>
+      <c r="E102" s="248"/>
+      <c r="F102" s="248"/>
+      <c r="G102" s="248"/>
+      <c r="H102" s="248"/>
+      <c r="I102" s="248"/>
+      <c r="J102" s="248"/>
+      <c r="K102" s="248"/>
+      <c r="L102" s="248"/>
+      <c r="M102" s="248"/>
+      <c r="N102" s="249"/>
       <c r="O102" s="20">
         <v>5</v>
       </c>
@@ -15704,49 +15707,49 @@
       <c r="R102" s="23">
         <v>20</v>
       </c>
-      <c r="U102" s="291" t="s">
+      <c r="U102" s="273" t="s">
         <v>20</v>
       </c>
-      <c r="V102" s="292"/>
-      <c r="W102" s="292"/>
-      <c r="X102" s="292"/>
-      <c r="Y102" s="292"/>
-      <c r="Z102" s="292"/>
-      <c r="AA102" s="292"/>
-      <c r="AB102" s="289">
+      <c r="V102" s="274"/>
+      <c r="W102" s="274"/>
+      <c r="X102" s="274"/>
+      <c r="Y102" s="274"/>
+      <c r="Z102" s="274"/>
+      <c r="AA102" s="274"/>
+      <c r="AB102" s="271">
         <v>22</v>
       </c>
-      <c r="AC102" s="289"/>
-      <c r="AD102" s="290"/>
+      <c r="AC102" s="271"/>
+      <c r="AD102" s="272"/>
       <c r="AE102" s="29"/>
       <c r="AF102" s="29"/>
-      <c r="AG102" s="305" t="s">
+      <c r="AG102" s="254" t="s">
         <v>21</v>
       </c>
-      <c r="AH102" s="306"/>
-      <c r="AI102" s="306"/>
-      <c r="AJ102" s="307"/>
+      <c r="AH102" s="255"/>
+      <c r="AI102" s="255"/>
+      <c r="AJ102" s="256"/>
       <c r="AK102" s="209">
         <v>230</v>
       </c>
     </row>
     <row r="103" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="34"/>
-      <c r="B103" s="293" t="s">
+      <c r="B103" s="247" t="s">
         <v>5</v>
       </c>
-      <c r="C103" s="294"/>
-      <c r="D103" s="294"/>
-      <c r="E103" s="294"/>
-      <c r="F103" s="294"/>
-      <c r="G103" s="294"/>
-      <c r="H103" s="294"/>
-      <c r="I103" s="294"/>
-      <c r="J103" s="294"/>
-      <c r="K103" s="294"/>
-      <c r="L103" s="294"/>
-      <c r="M103" s="294"/>
-      <c r="N103" s="295"/>
+      <c r="C103" s="248"/>
+      <c r="D103" s="248"/>
+      <c r="E103" s="248"/>
+      <c r="F103" s="248"/>
+      <c r="G103" s="248"/>
+      <c r="H103" s="248"/>
+      <c r="I103" s="248"/>
+      <c r="J103" s="248"/>
+      <c r="K103" s="248"/>
+      <c r="L103" s="248"/>
+      <c r="M103" s="248"/>
+      <c r="N103" s="249"/>
       <c r="O103" s="20">
         <v>2</v>
       </c>
@@ -15759,49 +15762,49 @@
       <c r="R103" s="23">
         <v>8</v>
       </c>
-      <c r="U103" s="300" t="s">
+      <c r="U103" s="252" t="s">
         <v>18</v>
       </c>
-      <c r="V103" s="301"/>
-      <c r="W103" s="301"/>
-      <c r="X103" s="301"/>
-      <c r="Y103" s="301"/>
-      <c r="Z103" s="301"/>
-      <c r="AA103" s="301"/>
-      <c r="AB103" s="302">
+      <c r="V103" s="253"/>
+      <c r="W103" s="253"/>
+      <c r="X103" s="253"/>
+      <c r="Y103" s="253"/>
+      <c r="Z103" s="253"/>
+      <c r="AA103" s="253"/>
+      <c r="AB103" s="278">
         <v>20</v>
       </c>
-      <c r="AC103" s="302"/>
-      <c r="AD103" s="303"/>
+      <c r="AC103" s="278"/>
+      <c r="AD103" s="279"/>
       <c r="AE103" s="29"/>
       <c r="AF103" s="29"/>
-      <c r="AG103" s="308" t="s">
+      <c r="AG103" s="257" t="s">
         <v>22</v>
       </c>
-      <c r="AH103" s="294"/>
-      <c r="AI103" s="294"/>
-      <c r="AJ103" s="295"/>
+      <c r="AH103" s="248"/>
+      <c r="AI103" s="248"/>
+      <c r="AJ103" s="249"/>
       <c r="AK103" s="36">
         <v>115</v>
       </c>
     </row>
     <row r="104" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="35"/>
-      <c r="B104" s="279" t="s">
+      <c r="B104" s="261" t="s">
         <v>4</v>
       </c>
-      <c r="C104" s="280"/>
-      <c r="D104" s="280"/>
-      <c r="E104" s="280"/>
-      <c r="F104" s="280"/>
-      <c r="G104" s="280"/>
-      <c r="H104" s="280"/>
-      <c r="I104" s="280"/>
-      <c r="J104" s="280"/>
-      <c r="K104" s="280"/>
-      <c r="L104" s="280"/>
-      <c r="M104" s="280"/>
-      <c r="N104" s="281"/>
+      <c r="C104" s="262"/>
+      <c r="D104" s="262"/>
+      <c r="E104" s="262"/>
+      <c r="F104" s="262"/>
+      <c r="G104" s="262"/>
+      <c r="H104" s="262"/>
+      <c r="I104" s="262"/>
+      <c r="J104" s="262"/>
+      <c r="K104" s="262"/>
+      <c r="L104" s="262"/>
+      <c r="M104" s="262"/>
+      <c r="N104" s="263"/>
       <c r="O104" s="3">
         <v>1</v>
       </c>
@@ -15814,51 +15817,51 @@
       <c r="R104" s="24">
         <v>1</v>
       </c>
-      <c r="U104" s="296" t="s">
+      <c r="U104" s="275" t="s">
         <v>19</v>
       </c>
-      <c r="V104" s="297"/>
-      <c r="W104" s="297"/>
-      <c r="X104" s="297"/>
-      <c r="Y104" s="297"/>
-      <c r="Z104" s="297"/>
-      <c r="AA104" s="297"/>
-      <c r="AB104" s="298">
+      <c r="V104" s="251"/>
+      <c r="W104" s="251"/>
+      <c r="X104" s="251"/>
+      <c r="Y104" s="251"/>
+      <c r="Z104" s="251"/>
+      <c r="AA104" s="251"/>
+      <c r="AB104" s="276">
         <f>AB102*AB103</f>
         <v>440</v>
       </c>
-      <c r="AC104" s="298"/>
-      <c r="AD104" s="299"/>
+      <c r="AC104" s="276"/>
+      <c r="AD104" s="277"/>
       <c r="AE104" s="29"/>
       <c r="AF104" s="29"/>
-      <c r="AG104" s="308" t="s">
+      <c r="AG104" s="257" t="s">
         <v>25</v>
       </c>
-      <c r="AH104" s="294"/>
-      <c r="AI104" s="294"/>
-      <c r="AJ104" s="295"/>
+      <c r="AH104" s="248"/>
+      <c r="AI104" s="248"/>
+      <c r="AJ104" s="249"/>
       <c r="AK104" s="36">
         <v>65</v>
       </c>
     </row>
     <row r="105" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG105" s="300" t="s">
+      <c r="AG105" s="252" t="s">
         <v>23</v>
       </c>
-      <c r="AH105" s="301"/>
-      <c r="AI105" s="301"/>
-      <c r="AJ105" s="301"/>
+      <c r="AH105" s="253"/>
+      <c r="AI105" s="253"/>
+      <c r="AJ105" s="253"/>
       <c r="AK105" s="211">
         <v>30</v>
       </c>
     </row>
     <row r="106" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG106" s="304" t="s">
+      <c r="AG106" s="250" t="s">
         <v>19</v>
       </c>
-      <c r="AH106" s="297"/>
-      <c r="AI106" s="297"/>
-      <c r="AJ106" s="297"/>
+      <c r="AH106" s="251"/>
+      <c r="AI106" s="251"/>
+      <c r="AJ106" s="251"/>
       <c r="AK106" s="210">
         <f>SUM(AK102:AK105)</f>
         <v>440</v>
@@ -15870,12 +15873,22 @@
     <sortCondition ref="B10:B94"/>
   </sortState>
   <mergeCells count="38">
-    <mergeCell ref="B103:N103"/>
-    <mergeCell ref="AG106:AJ106"/>
-    <mergeCell ref="AG105:AJ105"/>
-    <mergeCell ref="AG102:AJ102"/>
-    <mergeCell ref="AG104:AJ104"/>
-    <mergeCell ref="AG103:AJ103"/>
+    <mergeCell ref="O100:R100"/>
+    <mergeCell ref="U101:AD101"/>
+    <mergeCell ref="AG101:AK101"/>
+    <mergeCell ref="AH4:AJ4"/>
+    <mergeCell ref="AG5:AG9"/>
+    <mergeCell ref="AJ5:AJ9"/>
+    <mergeCell ref="X5:AA5"/>
+    <mergeCell ref="AB5:AB9"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="C4:S4"/>
+    <mergeCell ref="T4:AB4"/>
+    <mergeCell ref="AC4:AG4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="K5:R5"/>
+    <mergeCell ref="S5:S9"/>
     <mergeCell ref="T5:W5"/>
     <mergeCell ref="B104:N104"/>
     <mergeCell ref="C1:O1"/>
@@ -15892,22 +15905,12 @@
     <mergeCell ref="AB104:AD104"/>
     <mergeCell ref="U103:AA103"/>
     <mergeCell ref="AB103:AD103"/>
-    <mergeCell ref="O100:R100"/>
-    <mergeCell ref="U101:AD101"/>
-    <mergeCell ref="AG101:AK101"/>
-    <mergeCell ref="AH4:AJ4"/>
-    <mergeCell ref="AG5:AG9"/>
-    <mergeCell ref="AJ5:AJ9"/>
-    <mergeCell ref="X5:AA5"/>
-    <mergeCell ref="AB5:AB9"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="C4:S4"/>
-    <mergeCell ref="T4:AB4"/>
-    <mergeCell ref="AC4:AG4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="K5:R5"/>
-    <mergeCell ref="S5:S9"/>
+    <mergeCell ref="B103:N103"/>
+    <mergeCell ref="AG106:AJ106"/>
+    <mergeCell ref="AG105:AJ105"/>
+    <mergeCell ref="AG102:AJ102"/>
+    <mergeCell ref="AG104:AJ104"/>
+    <mergeCell ref="AG103:AJ103"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <conditionalFormatting sqref="AH18:AI18 AH10:AI10 AH14:AI14 T10:AA10 AC10:AF10 C10:R10 C14:R14 T14:AA14 AC14:AF14 T18:AA18 AC18:AF18 AH30:AI30 C30:R30 T30:AA30 AC30:AF30 AH26:AI26 C26:R26 T26:AA26 AC26:AF26 AH62:AI62 C62:R62 T62:AA62 AC62:AF62 AH42:AI42 C42:R42 T42:AA42 AC42:AF42 AH22:AI22 C22:R22 T22:AA22 AC22:AF22 AH38:AI38 C38:R38 T38:AA38 AC38:AF38 AH34:AI34 C34:R34 T34:AA34 AC34:AF34 AH66:AI66 C66:R66 T66:AA66 AC66:AF66 C18:R18">
@@ -16664,7 +16667,7 @@
   <dimension ref="A1:AJ31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16886,7 +16889,9 @@
       <c r="P6" s="81">
         <v>2</v>
       </c>
-      <c r="Q6" s="81"/>
+      <c r="Q6" s="81">
+        <v>1</v>
+      </c>
       <c r="R6" s="81"/>
       <c r="S6" s="81"/>
       <c r="T6" s="81"/>
@@ -16952,14 +16957,16 @@
       <c r="P7" s="81">
         <v>3</v>
       </c>
-      <c r="Q7" s="81"/>
+      <c r="Q7" s="81">
+        <v>2</v>
+      </c>
       <c r="R7" s="81"/>
       <c r="S7" s="81"/>
       <c r="T7" s="81"/>
       <c r="U7" s="81"/>
       <c r="V7" s="73">
         <f>IF(O7&gt;O6,1,0)+IF(P7&gt;P6,1,0)+IF(Q7&gt;Q6,1,0)+IF(R7&gt;R6,1,0)+IF(S7&gt;S6,1,0)+IF(T7&gt;T6,1,0)+IF(U7&gt;U6,1,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W7" s="14"/>
       <c r="X7" s="4"/>
@@ -17589,14 +17596,16 @@
       <c r="P20" s="81">
         <v>3</v>
       </c>
-      <c r="Q20" s="81"/>
+      <c r="Q20" s="81">
+        <v>4</v>
+      </c>
       <c r="R20" s="81"/>
       <c r="S20" s="81"/>
       <c r="T20" s="81"/>
       <c r="U20" s="81"/>
       <c r="V20" s="73">
         <f>IF(O20&gt;O21,1,0)+IF(P20&gt;P21,1,0)+IF(Q20&gt;Q21,1,0)+IF(R20&gt;R21,1,0)+IF(S20&gt;S21,1,0)+IF(T20&gt;T21,1,0)+IF(U20&gt;U21,1,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W20" s="13"/>
       <c r="Y20" s="93"/>
@@ -17655,7 +17664,9 @@
       <c r="P21" s="81">
         <v>4</v>
       </c>
-      <c r="Q21" s="81"/>
+      <c r="Q21" s="81">
+        <v>2</v>
+      </c>
       <c r="R21" s="81"/>
       <c r="S21" s="81"/>
       <c r="T21" s="81"/>

</xml_diff>

<commit_message>
Updated games of 2019-05-01
</commit_message>
<xml_diff>
--- a/laval.xlsx
+++ b/laval.xlsx
@@ -466,13 +466,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1934,7 +1934,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="310">
+  <cellXfs count="311">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2262,81 +2262,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -2394,89 +2319,176 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="103" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="103" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="104" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="104" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="105" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="105" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="112" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2487,18 +2499,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="83" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="85" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="92" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2511,160 +2538,136 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="83" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="85" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3889,217 +3892,217 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="C1" s="264"/>
-      <c r="D1" s="264"/>
-      <c r="E1" s="264"/>
-      <c r="F1" s="264"/>
-      <c r="G1" s="264"/>
-      <c r="H1" s="264"/>
-      <c r="I1" s="264"/>
-      <c r="J1" s="264"/>
-      <c r="K1" s="264"/>
-      <c r="L1" s="264"/>
-      <c r="M1" s="264"/>
-      <c r="N1" s="264"/>
-      <c r="O1" s="264"/>
-      <c r="P1" s="265"/>
-      <c r="Q1" s="265"/>
-      <c r="R1" s="265"/>
-      <c r="S1" s="265"/>
-      <c r="T1" s="265"/>
-      <c r="U1" s="265"/>
-      <c r="V1" s="265"/>
-      <c r="W1" s="265"/>
-      <c r="X1" s="265"/>
-      <c r="Y1" s="265"/>
-      <c r="Z1" s="265"/>
-      <c r="AA1" s="265"/>
-      <c r="AB1" s="265"/>
-      <c r="AC1" s="265"/>
-      <c r="AD1" s="265"/>
-      <c r="AE1" s="265"/>
-      <c r="AF1" s="265"/>
-      <c r="AG1" s="265"/>
-      <c r="AH1" s="265"/>
-      <c r="AI1" s="265"/>
-      <c r="AJ1" s="265"/>
+      <c r="C1" s="240"/>
+      <c r="D1" s="240"/>
+      <c r="E1" s="240"/>
+      <c r="F1" s="240"/>
+      <c r="G1" s="240"/>
+      <c r="H1" s="240"/>
+      <c r="I1" s="240"/>
+      <c r="J1" s="240"/>
+      <c r="K1" s="240"/>
+      <c r="L1" s="240"/>
+      <c r="M1" s="240"/>
+      <c r="N1" s="240"/>
+      <c r="O1" s="240"/>
+      <c r="P1" s="241"/>
+      <c r="Q1" s="241"/>
+      <c r="R1" s="241"/>
+      <c r="S1" s="241"/>
+      <c r="T1" s="241"/>
+      <c r="U1" s="241"/>
+      <c r="V1" s="241"/>
+      <c r="W1" s="241"/>
+      <c r="X1" s="241"/>
+      <c r="Y1" s="241"/>
+      <c r="Z1" s="241"/>
+      <c r="AA1" s="241"/>
+      <c r="AB1" s="241"/>
+      <c r="AC1" s="241"/>
+      <c r="AD1" s="241"/>
+      <c r="AE1" s="241"/>
+      <c r="AF1" s="241"/>
+      <c r="AG1" s="241"/>
+      <c r="AH1" s="241"/>
+      <c r="AI1" s="241"/>
+      <c r="AJ1" s="241"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="41"/>
-      <c r="C2" s="266" t="s">
+      <c r="C2" s="242" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="266"/>
-      <c r="E2" s="266"/>
-      <c r="F2" s="266"/>
-      <c r="G2" s="266"/>
-      <c r="H2" s="266"/>
-      <c r="I2" s="266"/>
-      <c r="J2" s="266"/>
-      <c r="K2" s="266"/>
-      <c r="L2" s="266"/>
-      <c r="M2" s="266"/>
-      <c r="N2" s="266"/>
-      <c r="O2" s="266"/>
-      <c r="P2" s="266"/>
-      <c r="Q2" s="267" t="s">
+      <c r="D2" s="242"/>
+      <c r="E2" s="242"/>
+      <c r="F2" s="242"/>
+      <c r="G2" s="242"/>
+      <c r="H2" s="242"/>
+      <c r="I2" s="242"/>
+      <c r="J2" s="242"/>
+      <c r="K2" s="242"/>
+      <c r="L2" s="242"/>
+      <c r="M2" s="242"/>
+      <c r="N2" s="242"/>
+      <c r="O2" s="242"/>
+      <c r="P2" s="242"/>
+      <c r="Q2" s="243" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="265"/>
-      <c r="S2" s="265"/>
-      <c r="T2" s="265"/>
-      <c r="U2" s="265"/>
-      <c r="V2" s="265"/>
-      <c r="W2" s="265"/>
-      <c r="X2" s="265"/>
-      <c r="Y2" s="265"/>
-      <c r="Z2" s="265"/>
-      <c r="AA2" s="265"/>
-      <c r="AB2" s="265"/>
-      <c r="AC2" s="265"/>
-      <c r="AD2" s="265"/>
-      <c r="AE2" s="265"/>
-      <c r="AF2" s="265"/>
-      <c r="AG2" s="265"/>
-      <c r="AH2" s="265"/>
-      <c r="AI2" s="265"/>
-      <c r="AJ2" s="265"/>
+      <c r="R2" s="241"/>
+      <c r="S2" s="241"/>
+      <c r="T2" s="241"/>
+      <c r="U2" s="241"/>
+      <c r="V2" s="241"/>
+      <c r="W2" s="241"/>
+      <c r="X2" s="241"/>
+      <c r="Y2" s="241"/>
+      <c r="Z2" s="241"/>
+      <c r="AA2" s="241"/>
+      <c r="AB2" s="241"/>
+      <c r="AC2" s="241"/>
+      <c r="AD2" s="241"/>
+      <c r="AE2" s="241"/>
+      <c r="AF2" s="241"/>
+      <c r="AG2" s="241"/>
+      <c r="AH2" s="241"/>
+      <c r="AI2" s="241"/>
+      <c r="AJ2" s="241"/>
     </row>
     <row r="3" spans="1:38" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="264"/>
-      <c r="D3" s="264"/>
-      <c r="E3" s="264"/>
-      <c r="F3" s="264"/>
-      <c r="G3" s="264"/>
-      <c r="H3" s="264"/>
-      <c r="I3" s="264"/>
-      <c r="J3" s="264"/>
-      <c r="K3" s="264"/>
-      <c r="L3" s="264"/>
-      <c r="M3" s="264"/>
-      <c r="N3" s="264"/>
-      <c r="O3" s="264"/>
-      <c r="P3" s="265"/>
-      <c r="Q3" s="265"/>
-      <c r="R3" s="265"/>
-      <c r="S3" s="265"/>
-      <c r="T3" s="265"/>
-      <c r="U3" s="265"/>
-      <c r="V3" s="265"/>
-      <c r="W3" s="265"/>
-      <c r="X3" s="265"/>
-      <c r="Y3" s="265"/>
-      <c r="Z3" s="265"/>
-      <c r="AA3" s="265"/>
-      <c r="AB3" s="265"/>
-      <c r="AC3" s="265"/>
-      <c r="AD3" s="265"/>
-      <c r="AE3" s="265"/>
-      <c r="AF3" s="265"/>
-      <c r="AG3" s="265"/>
-      <c r="AH3" s="265"/>
-      <c r="AI3" s="265"/>
-      <c r="AJ3" s="265"/>
+      <c r="C3" s="240"/>
+      <c r="D3" s="240"/>
+      <c r="E3" s="240"/>
+      <c r="F3" s="240"/>
+      <c r="G3" s="240"/>
+      <c r="H3" s="240"/>
+      <c r="I3" s="240"/>
+      <c r="J3" s="240"/>
+      <c r="K3" s="240"/>
+      <c r="L3" s="240"/>
+      <c r="M3" s="240"/>
+      <c r="N3" s="240"/>
+      <c r="O3" s="240"/>
+      <c r="P3" s="241"/>
+      <c r="Q3" s="241"/>
+      <c r="R3" s="241"/>
+      <c r="S3" s="241"/>
+      <c r="T3" s="241"/>
+      <c r="U3" s="241"/>
+      <c r="V3" s="241"/>
+      <c r="W3" s="241"/>
+      <c r="X3" s="241"/>
+      <c r="Y3" s="241"/>
+      <c r="Z3" s="241"/>
+      <c r="AA3" s="241"/>
+      <c r="AB3" s="241"/>
+      <c r="AC3" s="241"/>
+      <c r="AD3" s="241"/>
+      <c r="AE3" s="241"/>
+      <c r="AF3" s="241"/>
+      <c r="AG3" s="241"/>
+      <c r="AH3" s="241"/>
+      <c r="AI3" s="241"/>
+      <c r="AJ3" s="241"/>
     </row>
     <row r="4" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="289" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="290"/>
-      <c r="E4" s="290"/>
-      <c r="F4" s="290"/>
-      <c r="G4" s="290"/>
-      <c r="H4" s="290"/>
-      <c r="I4" s="290"/>
-      <c r="J4" s="290"/>
-      <c r="K4" s="290"/>
-      <c r="L4" s="290"/>
-      <c r="M4" s="290"/>
-      <c r="N4" s="290"/>
-      <c r="O4" s="290"/>
-      <c r="P4" s="290"/>
-      <c r="Q4" s="290"/>
-      <c r="R4" s="290"/>
-      <c r="S4" s="291"/>
-      <c r="T4" s="289" t="s">
+      <c r="C4" s="224" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="225"/>
+      <c r="E4" s="225"/>
+      <c r="F4" s="225"/>
+      <c r="G4" s="225"/>
+      <c r="H4" s="225"/>
+      <c r="I4" s="225"/>
+      <c r="J4" s="225"/>
+      <c r="K4" s="225"/>
+      <c r="L4" s="225"/>
+      <c r="M4" s="225"/>
+      <c r="N4" s="225"/>
+      <c r="O4" s="225"/>
+      <c r="P4" s="225"/>
+      <c r="Q4" s="225"/>
+      <c r="R4" s="225"/>
+      <c r="S4" s="226"/>
+      <c r="T4" s="224" t="s">
         <v>1</v>
       </c>
-      <c r="U4" s="290"/>
-      <c r="V4" s="290"/>
-      <c r="W4" s="290"/>
-      <c r="X4" s="290"/>
-      <c r="Y4" s="290"/>
-      <c r="Z4" s="290"/>
-      <c r="AA4" s="290"/>
-      <c r="AB4" s="291"/>
-      <c r="AC4" s="289" t="s">
+      <c r="U4" s="225"/>
+      <c r="V4" s="225"/>
+      <c r="W4" s="225"/>
+      <c r="X4" s="225"/>
+      <c r="Y4" s="225"/>
+      <c r="Z4" s="225"/>
+      <c r="AA4" s="225"/>
+      <c r="AB4" s="226"/>
+      <c r="AC4" s="224" t="s">
         <v>2</v>
       </c>
-      <c r="AD4" s="290"/>
-      <c r="AE4" s="290"/>
-      <c r="AF4" s="290"/>
-      <c r="AG4" s="298"/>
-      <c r="AH4" s="289" t="s">
+      <c r="AD4" s="225"/>
+      <c r="AE4" s="225"/>
+      <c r="AF4" s="225"/>
+      <c r="AG4" s="235"/>
+      <c r="AH4" s="224" t="s">
         <v>10</v>
       </c>
-      <c r="AI4" s="290"/>
-      <c r="AJ4" s="291"/>
+      <c r="AI4" s="225"/>
+      <c r="AJ4" s="226"/>
     </row>
     <row r="5" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="258" t="s">
+      <c r="C5" s="236" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="259"/>
-      <c r="E5" s="259"/>
-      <c r="F5" s="259"/>
-      <c r="G5" s="259"/>
-      <c r="H5" s="259"/>
-      <c r="I5" s="259"/>
-      <c r="J5" s="260"/>
-      <c r="K5" s="296" t="s">
+      <c r="D5" s="232"/>
+      <c r="E5" s="232"/>
+      <c r="F5" s="232"/>
+      <c r="G5" s="232"/>
+      <c r="H5" s="232"/>
+      <c r="I5" s="232"/>
+      <c r="J5" s="233"/>
+      <c r="K5" s="231" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="259"/>
-      <c r="M5" s="259"/>
-      <c r="N5" s="259"/>
-      <c r="O5" s="259"/>
-      <c r="P5" s="259"/>
-      <c r="Q5" s="259"/>
-      <c r="R5" s="260"/>
-      <c r="S5" s="292" t="s">
+      <c r="L5" s="232"/>
+      <c r="M5" s="232"/>
+      <c r="N5" s="232"/>
+      <c r="O5" s="232"/>
+      <c r="P5" s="232"/>
+      <c r="Q5" s="232"/>
+      <c r="R5" s="233"/>
+      <c r="S5" s="227" t="s">
         <v>12</v>
       </c>
-      <c r="T5" s="258" t="s">
+      <c r="T5" s="236" t="s">
         <v>9</v>
       </c>
-      <c r="U5" s="259"/>
-      <c r="V5" s="259"/>
-      <c r="W5" s="260"/>
-      <c r="X5" s="296" t="s">
+      <c r="U5" s="232"/>
+      <c r="V5" s="232"/>
+      <c r="W5" s="233"/>
+      <c r="X5" s="231" t="s">
         <v>8</v>
       </c>
-      <c r="Y5" s="259"/>
-      <c r="Z5" s="259"/>
-      <c r="AA5" s="260"/>
-      <c r="AB5" s="292" t="s">
+      <c r="Y5" s="232"/>
+      <c r="Z5" s="232"/>
+      <c r="AA5" s="233"/>
+      <c r="AB5" s="227" t="s">
         <v>13</v>
       </c>
-      <c r="AC5" s="297" t="s">
+      <c r="AC5" s="234" t="s">
         <v>9</v>
       </c>
-      <c r="AD5" s="260"/>
-      <c r="AE5" s="296" t="s">
+      <c r="AD5" s="233"/>
+      <c r="AE5" s="231" t="s">
         <v>8</v>
       </c>
-      <c r="AF5" s="260"/>
-      <c r="AG5" s="292" t="s">
+      <c r="AF5" s="233"/>
+      <c r="AG5" s="227" t="s">
         <v>14</v>
       </c>
       <c r="AH5" s="56"/>
       <c r="AI5" s="25"/>
-      <c r="AJ5" s="292" t="s">
+      <c r="AJ5" s="227" t="s">
         <v>15</v>
       </c>
       <c r="AK5" s="4"/>
@@ -4111,11 +4114,11 @@
         <f>Résultats!$J$3</f>
         <v>0</v>
       </c>
-      <c r="D6" s="224">
+      <c r="D6" s="198">
         <f>Résultats!$J$4</f>
         <v>4</v>
       </c>
-      <c r="E6" s="220">
+      <c r="E6" s="194">
         <f>Résultats!$J$6</f>
         <v>4</v>
       </c>
@@ -4127,11 +4130,11 @@
         <f>Résultats!$J$10</f>
         <v>3</v>
       </c>
-      <c r="H6" s="229">
+      <c r="H6" s="202">
         <f>Résultats!$J$11</f>
         <v>4</v>
       </c>
-      <c r="I6" s="220">
+      <c r="I6" s="194">
         <f>Résultats!$J$13</f>
         <v>4</v>
       </c>
@@ -4143,7 +4146,7 @@
         <f>Résultats!$J$17</f>
         <v>1</v>
       </c>
-      <c r="L6" s="224">
+      <c r="L6" s="198">
         <f>Résultats!$J$18</f>
         <v>4</v>
       </c>
@@ -4151,7 +4154,7 @@
         <f>Résultats!$J$20</f>
         <v>2</v>
       </c>
-      <c r="N6" s="229">
+      <c r="N6" s="202">
         <f>Résultats!$J$21</f>
         <v>4</v>
       </c>
@@ -4159,11 +4162,11 @@
         <f>Résultats!$J$24</f>
         <v>2</v>
       </c>
-      <c r="P6" s="229">
+      <c r="P6" s="202">
         <f>Résultats!$J$25</f>
         <v>4</v>
       </c>
-      <c r="Q6" s="233">
+      <c r="Q6" s="206">
         <f>Résultats!$J$27</f>
         <v>4</v>
       </c>
@@ -4171,7 +4174,7 @@
         <f>Résultats!$J$28</f>
         <v>3</v>
       </c>
-      <c r="S6" s="293"/>
+      <c r="S6" s="228"/>
       <c r="T6" s="156">
         <f>Résultats!$V$6</f>
         <v>1</v>
@@ -4186,7 +4189,7 @@
       </c>
       <c r="W6" s="103">
         <f>Résultats!$V$11</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X6" s="105">
         <f>Résultats!$V$20</f>
@@ -4202,9 +4205,9 @@
       </c>
       <c r="AA6" s="103">
         <f>Résultats!$V$25</f>
-        <v>1</v>
-      </c>
-      <c r="AB6" s="293"/>
+        <v>2</v>
+      </c>
+      <c r="AB6" s="228"/>
       <c r="AC6" s="106">
         <f>Résultats!$AH$8</f>
         <v>0</v>
@@ -4221,8 +4224,8 @@
         <f>Résultats!$AH$23</f>
         <v>0</v>
       </c>
-      <c r="AG6" s="293"/>
-      <c r="AH6" s="198">
+      <c r="AG6" s="228"/>
+      <c r="AH6" s="173">
         <f>Résultats!$AH$15</f>
         <v>0</v>
       </c>
@@ -4230,7 +4233,7 @@
         <f>Résultats!$AH$16</f>
         <v>0</v>
       </c>
-      <c r="AJ6" s="293"/>
+      <c r="AJ6" s="228"/>
       <c r="AK6" s="37"/>
     </row>
     <row r="7" spans="1:38" s="39" customFormat="1" ht="58.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -4241,22 +4244,22 @@
 +IF(ISBLANK($D10),0,($D$6*PT_VICTOIRE_R1)+IF($D$6=4,PT_PREDICTION_EQUIPE_R1+IF($D10=$C$6+$D$6,PT_PREDICTION_NB_PARTIES_R1,0),0))</f>
         <v>0</v>
       </c>
-      <c r="D7" s="225"/>
-      <c r="E7" s="221"/>
+      <c r="D7" s="199"/>
+      <c r="E7" s="195"/>
       <c r="F7" s="113"/>
       <c r="G7" s="114"/>
-      <c r="H7" s="225"/>
-      <c r="I7" s="221"/>
+      <c r="H7" s="199"/>
+      <c r="I7" s="195"/>
       <c r="J7" s="112"/>
       <c r="K7" s="115"/>
-      <c r="L7" s="225"/>
+      <c r="L7" s="199"/>
       <c r="M7" s="160"/>
-      <c r="N7" s="230"/>
+      <c r="N7" s="203"/>
       <c r="O7" s="160"/>
-      <c r="P7" s="230"/>
-      <c r="Q7" s="234"/>
+      <c r="P7" s="203"/>
+      <c r="Q7" s="207"/>
       <c r="R7" s="112"/>
-      <c r="S7" s="293"/>
+      <c r="S7" s="228"/>
       <c r="T7" s="157"/>
       <c r="U7" s="112"/>
       <c r="V7" s="160"/>
@@ -4265,15 +4268,15 @@
       <c r="Y7" s="113"/>
       <c r="Z7" s="114"/>
       <c r="AA7" s="112"/>
-      <c r="AB7" s="293"/>
+      <c r="AB7" s="228"/>
       <c r="AC7" s="114"/>
       <c r="AD7" s="112"/>
       <c r="AE7" s="115"/>
       <c r="AF7" s="112"/>
-      <c r="AG7" s="293"/>
-      <c r="AH7" s="198"/>
+      <c r="AG7" s="228"/>
+      <c r="AH7" s="173"/>
       <c r="AI7" s="107"/>
-      <c r="AJ7" s="293"/>
+      <c r="AJ7" s="228"/>
       <c r="AK7" s="37"/>
     </row>
     <row r="8" spans="1:38" s="39" customFormat="1" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4283,11 +4286,11 @@
         <f>Résultats!$B$3</f>
         <v>TAMPA BAY</v>
       </c>
-      <c r="D8" s="226" t="str">
+      <c r="D8" s="200" t="str">
         <f>Résultats!$B$4</f>
         <v>COLUMBUS</v>
       </c>
-      <c r="E8" s="222" t="str">
+      <c r="E8" s="196" t="str">
         <f>Résultats!$B$6</f>
         <v>BOSTON</v>
       </c>
@@ -4299,11 +4302,11 @@
         <f>Résultats!$B$10</f>
         <v>WASHINGTON</v>
       </c>
-      <c r="H8" s="226" t="str">
+      <c r="H8" s="200" t="str">
         <f>Résultats!$B$11</f>
         <v>CAROLINE</v>
       </c>
-      <c r="I8" s="222" t="str">
+      <c r="I8" s="196" t="str">
         <f>Résultats!$B$13</f>
         <v>NEW YORK I.</v>
       </c>
@@ -4315,7 +4318,7 @@
         <f>Résultats!$B$17</f>
         <v>CALGARY</v>
       </c>
-      <c r="L8" s="226" t="str">
+      <c r="L8" s="200" t="str">
         <f>Résultats!$B$18</f>
         <v>COLORADO</v>
       </c>
@@ -4323,7 +4326,7 @@
         <f>Résultats!$B$20</f>
         <v>WINNIPEG</v>
       </c>
-      <c r="N8" s="231" t="str">
+      <c r="N8" s="204" t="str">
         <f>Résultats!$B$21</f>
         <v>ST-LOUIS</v>
       </c>
@@ -4331,11 +4334,11 @@
         <f>Résultats!$B$24</f>
         <v>NASHVILLE</v>
       </c>
-      <c r="P8" s="231" t="str">
+      <c r="P8" s="204" t="str">
         <f>Résultats!$B$25</f>
         <v>DALLAS</v>
       </c>
-      <c r="Q8" s="235" t="str">
+      <c r="Q8" s="208" t="str">
         <f>Résultats!$B$27</f>
         <v>SAN JOSE</v>
       </c>
@@ -4343,7 +4346,7 @@
         <f>Résultats!$B$28</f>
         <v>VEGAS</v>
       </c>
-      <c r="S8" s="293"/>
+      <c r="S8" s="228"/>
       <c r="T8" s="158" t="str">
         <f>Résultats!$N$6</f>
         <v>BOSTON</v>
@@ -4376,7 +4379,7 @@
         <f>Résultats!$N$25</f>
         <v>DALLAS</v>
       </c>
-      <c r="AB8" s="293"/>
+      <c r="AB8" s="228"/>
       <c r="AC8" s="164" t="str">
         <f>Résultats!$Z$8</f>
         <v xml:space="preserve"> </v>
@@ -4393,16 +4396,16 @@
         <f>Résultats!$Z$23</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AG8" s="293"/>
-      <c r="AH8" s="199" t="str">
+      <c r="AG8" s="228"/>
+      <c r="AH8" s="174" t="str">
         <f>Résultats!$Z$15</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AI8" s="200" t="str">
+      <c r="AI8" s="175" t="str">
         <f>Résultats!$Z$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ8" s="293"/>
+      <c r="AJ8" s="228"/>
       <c r="AK8" s="37"/>
     </row>
     <row r="9" spans="1:38" s="39" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4416,11 +4419,11 @@
         <f>Résultats!$A$3</f>
         <v>A1</v>
       </c>
-      <c r="D9" s="227" t="str">
+      <c r="D9" s="201" t="str">
         <f>Résultats!$A$4</f>
         <v>WC2</v>
       </c>
-      <c r="E9" s="223" t="str">
+      <c r="E9" s="197" t="str">
         <f>Résultats!$A$6</f>
         <v>A2</v>
       </c>
@@ -4432,11 +4435,11 @@
         <f>Résultats!$A$10</f>
         <v>M1</v>
       </c>
-      <c r="H9" s="227" t="str">
+      <c r="H9" s="201" t="str">
         <f>Résultats!$A$11</f>
         <v>WC1</v>
       </c>
-      <c r="I9" s="223" t="str">
+      <c r="I9" s="197" t="str">
         <f>Résultats!$A$13</f>
         <v>M2</v>
       </c>
@@ -4448,7 +4451,7 @@
         <f>Résultats!$A$17</f>
         <v>C1</v>
       </c>
-      <c r="L9" s="227" t="str">
+      <c r="L9" s="201" t="str">
         <f>Résultats!$A$18</f>
         <v>WC2</v>
       </c>
@@ -4456,7 +4459,7 @@
         <f>Résultats!$A$20</f>
         <v>C2</v>
       </c>
-      <c r="N9" s="232" t="str">
+      <c r="N9" s="205" t="str">
         <f>Résultats!$A$21</f>
         <v>C3</v>
       </c>
@@ -4464,11 +4467,11 @@
         <f>Résultats!$A$24</f>
         <v>P1</v>
       </c>
-      <c r="P9" s="232" t="str">
+      <c r="P9" s="205" t="str">
         <f>Résultats!$A$25</f>
         <v>WC1</v>
       </c>
-      <c r="Q9" s="236" t="str">
+      <c r="Q9" s="209" t="str">
         <f>Résultats!$A$27</f>
         <v>P2</v>
       </c>
@@ -4476,7 +4479,7 @@
         <f>Résultats!$A$28</f>
         <v>P3</v>
       </c>
-      <c r="S9" s="295"/>
+      <c r="S9" s="230"/>
       <c r="T9" s="166" t="str">
         <f>Résultats!$M$6</f>
         <v>A2</v>
@@ -4509,7 +4512,7 @@
         <f>Résultats!$M$25</f>
         <v>WC1</v>
       </c>
-      <c r="AB9" s="294"/>
+      <c r="AB9" s="229"/>
       <c r="AC9" s="170" t="str">
         <f>Résultats!$Y$8</f>
         <v xml:space="preserve"> </v>
@@ -4526,16 +4529,16 @@
         <f>Résultats!$Y$23</f>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="AG9" s="294"/>
-      <c r="AH9" s="201" t="str">
+      <c r="AG9" s="229"/>
+      <c r="AH9" s="176" t="str">
         <f>Résultats!$Y$15</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AI9" s="202" t="str">
+      <c r="AI9" s="177" t="str">
         <f>Résultats!$Y$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ9" s="295"/>
+      <c r="AJ9" s="230"/>
       <c r="AK9" s="109" t="s">
         <v>51</v>
       </c>
@@ -4544,88 +4547,88 @@
       </c>
     </row>
     <row r="10" spans="1:38" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="173">
+      <c r="A10" s="269">
         <f>RANK(AL10,$AL$10:$AL$97,)</f>
         <v>1</v>
       </c>
-      <c r="B10" s="197" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" s="174">
-        <v>4</v>
-      </c>
-      <c r="D10" s="175"/>
-      <c r="E10" s="178">
+      <c r="B10" s="270" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="271">
         <v>5</v>
       </c>
-      <c r="F10" s="175"/>
-      <c r="G10" s="179">
+      <c r="D10" s="272"/>
+      <c r="E10" s="273">
         <v>6</v>
       </c>
-      <c r="H10" s="176"/>
-      <c r="I10" s="178">
+      <c r="F10" s="272"/>
+      <c r="G10" s="274"/>
+      <c r="H10" s="275">
         <v>7</v>
       </c>
-      <c r="J10" s="176"/>
-      <c r="K10" s="177">
+      <c r="I10" s="273"/>
+      <c r="J10" s="276">
+        <v>6</v>
+      </c>
+      <c r="K10" s="277">
         <v>5</v>
       </c>
-      <c r="L10" s="176"/>
-      <c r="M10" s="178"/>
-      <c r="N10" s="175">
+      <c r="L10" s="276"/>
+      <c r="M10" s="273"/>
+      <c r="N10" s="278">
+        <v>6</v>
+      </c>
+      <c r="O10" s="273">
+        <v>6</v>
+      </c>
+      <c r="P10" s="272"/>
+      <c r="Q10" s="274">
+        <v>6</v>
+      </c>
+      <c r="R10" s="279"/>
+      <c r="S10" s="280">
+        <f>SUM(C11:R11)</f>
+        <v>43</v>
+      </c>
+      <c r="T10" s="271"/>
+      <c r="U10" s="276">
+        <v>6</v>
+      </c>
+      <c r="V10" s="273">
+        <v>6</v>
+      </c>
+      <c r="W10" s="276"/>
+      <c r="X10" s="277">
+        <v>5</v>
+      </c>
+      <c r="Y10" s="272"/>
+      <c r="Z10" s="274"/>
+      <c r="AA10" s="279">
         <v>7</v>
       </c>
-      <c r="O10" s="178">
+      <c r="AB10" s="280">
+        <f>SUM(T11:AA11)</f>
         <v>6</v>
       </c>
-      <c r="P10" s="175"/>
-      <c r="Q10" s="241">
-        <v>7</v>
-      </c>
-      <c r="R10" s="180"/>
-      <c r="S10" s="181">
-        <f>SUM(C11:R11)</f>
-        <v>44</v>
-      </c>
-      <c r="T10" s="174"/>
-      <c r="U10" s="176">
-        <v>6</v>
-      </c>
-      <c r="V10" s="178">
-        <v>6</v>
-      </c>
-      <c r="W10" s="176"/>
-      <c r="X10" s="177"/>
-      <c r="Y10" s="175">
-        <v>6</v>
-      </c>
-      <c r="Z10" s="179">
-        <v>6</v>
-      </c>
-      <c r="AA10" s="180"/>
-      <c r="AB10" s="181">
-        <f>SUM(T11:AA11)</f>
-        <v>5</v>
-      </c>
-      <c r="AC10" s="179"/>
-      <c r="AD10" s="176"/>
-      <c r="AE10" s="177"/>
-      <c r="AF10" s="176"/>
-      <c r="AG10" s="181">
+      <c r="AC10" s="274"/>
+      <c r="AD10" s="276"/>
+      <c r="AE10" s="277"/>
+      <c r="AF10" s="276"/>
+      <c r="AG10" s="280">
         <f>SUM(AC11:AF11)</f>
         <v>0</v>
       </c>
-      <c r="AH10" s="182"/>
-      <c r="AI10" s="183"/>
-      <c r="AJ10" s="181">
+      <c r="AH10" s="281"/>
+      <c r="AI10" s="282"/>
+      <c r="AJ10" s="280">
         <f>AH11</f>
         <v>0</v>
       </c>
-      <c r="AK10" s="184">
+      <c r="AK10" s="283">
         <f>MAX($AL$10:$AL$97) - AL10</f>
         <v>0</v>
       </c>
-      <c r="AL10" s="181">
+      <c r="AL10" s="280">
         <f>$S10+$AB10+$AG10+$AJ10</f>
         <v>49</v>
       </c>
@@ -4648,12 +4651,12 @@
       <c r="F11" s="127"/>
       <c r="G11" s="125">
         <f>(IF($G10&lt;&gt;"",($G$6*$O$104)+IF($G$6=4,($O$102)+IF($G10=$G$6+$H$6,$O$103,0),0),0)+IF($H10&lt;&gt;"",($H$6*$O$104)+IF($H$6=4,($O$102)+IF($H10=$G$6+$H$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="H11" s="127"/>
       <c r="I11" s="128">
         <f>(IF($I10&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I10=$I$6+$J$6,$O$103,0),0),0)+IF($J10&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J10=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J11" s="129"/>
       <c r="K11" s="130">
@@ -4663,7 +4666,7 @@
       <c r="L11" s="127"/>
       <c r="M11" s="125">
         <f>(IF($M10&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M10=$M$6+$N$6,$O$103,0),0),0)+IF($N10&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N10=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="N11" s="127"/>
       <c r="O11" s="128">
@@ -4673,7 +4676,7 @@
       <c r="P11" s="127"/>
       <c r="Q11" s="125">
         <f>(IF($Q10&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q10=$Q$6+$R$6,$O$103,0),0),0)+IF($R10&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R10=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="R11" s="131"/>
       <c r="S11" s="121"/>
@@ -4689,7 +4692,7 @@
       <c r="W11" s="126"/>
       <c r="X11" s="126">
         <f>(IF($X10&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X10=$X$6+$Y$6,$P$103,0),0),0)+IF($Y10&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y10=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y11" s="59"/>
       <c r="Z11" s="126">
@@ -4748,13 +4751,13 @@
         <f>IF(ISBLANK(H10),
 0,
 IF(H$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="118">
         <f>IF(ISBLANK(I10),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" s="118">
         <f>IF(ISBLANK(J10),
@@ -4913,7 +4916,7 @@
         <f>IF(H12 = 0,
 0,
 IF(H10 = (G$6+H$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" s="118">
         <f>IF(I12 = 0,
@@ -4949,7 +4952,7 @@
         <f>IF(N12 = 0,
 0,
 IF(N10 = (M$6+N$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O13" s="118">
         <f>IF(O12 = 0,
@@ -4967,7 +4970,7 @@
         <f>IF(Q12 = 0,
 0,
 IF(Q10 = (Q$6+R$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R13" s="118">
         <f>IF(R12 = 0,
@@ -5035,53 +5038,53 @@
       <c r="AJ13" s="138"/>
       <c r="AK13" s="139">
         <f>SUM(C13:AI13)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL13" s="123"/>
     </row>
     <row r="14" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="117">
         <f>RANK(AL14,$AL$10:$AL$97,)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" s="84" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C14" s="46">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D14" s="45"/>
       <c r="E14" s="44">
+        <v>5</v>
+      </c>
+      <c r="F14" s="45"/>
+      <c r="G14" s="48">
         <v>6</v>
       </c>
-      <c r="F14" s="45"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="243">
+      <c r="H14" s="47"/>
+      <c r="I14" s="44">
         <v>7</v>
       </c>
-      <c r="I14" s="44"/>
-      <c r="J14" s="47">
-        <v>6</v>
-      </c>
+      <c r="J14" s="47"/>
       <c r="K14" s="49">
         <v>5</v>
       </c>
       <c r="L14" s="47"/>
       <c r="M14" s="44"/>
-      <c r="N14" s="239">
-        <v>6</v>
+      <c r="N14" s="45">
+        <v>7</v>
       </c>
       <c r="O14" s="44">
         <v>6</v>
       </c>
       <c r="P14" s="45"/>
-      <c r="Q14" s="48">
-        <v>6</v>
+      <c r="Q14" s="213">
+        <v>7</v>
       </c>
       <c r="R14" s="50"/>
       <c r="S14" s="122">
         <f>SUM(C15:R15)</f>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="T14" s="46"/>
       <c r="U14" s="47">
@@ -5091,14 +5094,14 @@
         <v>6</v>
       </c>
       <c r="W14" s="47"/>
-      <c r="X14" s="49">
-        <v>5</v>
-      </c>
-      <c r="Y14" s="45"/>
-      <c r="Z14" s="48"/>
-      <c r="AA14" s="50">
-        <v>7</v>
-      </c>
+      <c r="X14" s="49"/>
+      <c r="Y14" s="45">
+        <v>6</v>
+      </c>
+      <c r="Z14" s="48">
+        <v>6</v>
+      </c>
+      <c r="AA14" s="50"/>
       <c r="AB14" s="122">
         <f>SUM(T15:AA15)</f>
         <v>5</v>
@@ -5119,11 +5122,11 @@
       </c>
       <c r="AK14" s="111">
         <f>MAX($AL$10:$AL$97) - AL14</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL14" s="122">
         <f>$S14+$AB14+$AG14+$AJ14</f>
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5144,12 +5147,12 @@
       <c r="F15" s="140"/>
       <c r="G15" s="125">
         <f>(IF($G14&lt;&gt;"",($G$6*$O$104)+IF($G$6=4,($O$102)+IF($G14=$G$6+$H$6,$O$103,0),0),0)+IF($H14&lt;&gt;"",($H$6*$O$104)+IF($H$6=4,($O$102)+IF($H14=$G$6+$H$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="H15" s="140"/>
       <c r="I15" s="120">
         <f>(IF($I14&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I14=$I$6+$J$6,$O$103,0),0),0)+IF($J14&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J14=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J15" s="141"/>
       <c r="K15" s="142">
@@ -5159,7 +5162,7 @@
       <c r="L15" s="140"/>
       <c r="M15" s="125">
         <f>(IF($M14&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M14=$M$6+$N$6,$O$103,0),0),0)+IF($N14&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N14=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="N15" s="140"/>
       <c r="O15" s="120">
@@ -5169,7 +5172,7 @@
       <c r="P15" s="140"/>
       <c r="Q15" s="120">
         <f>(IF($Q14&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q14=$Q$6+$R$6,$O$103,0),0),0)+IF($R14&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R14=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="R15" s="143"/>
       <c r="S15" s="144"/>
@@ -5185,12 +5188,12 @@
       <c r="W15" s="126"/>
       <c r="X15" s="126">
         <f>(IF($X14&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X14=$X$6+$Y$6,$P$103,0),0),0)+IF($Y14&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y14=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y15" s="59"/>
       <c r="Z15" s="126">
         <f>(IF($Z14&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z14=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA14&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA14=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA15" s="62"/>
       <c r="AB15" s="144"/>
@@ -5247,13 +5250,13 @@
         <f>IF(ISBLANK(H14),
 0,
 IF(H$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" s="118">
         <f>IF(ISBLANK(I14),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" s="118">
         <f>IF(ISBLANK(J14),
@@ -5412,7 +5415,7 @@
         <f>IF(H16 = 0,
 0,
 IF(H14 = (G$6+H$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" s="118">
         <f>IF(I16 = 0,
@@ -5448,7 +5451,7 @@
         <f>IF(N16 = 0,
 0,
 IF(N14 = (M$6+N$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O17" s="118">
         <f>IF(O16 = 0,
@@ -5466,7 +5469,7 @@
         <f>IF(Q16 = 0,
 0,
 IF(Q14 = (Q$6+R$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R17" s="118">
         <f>IF(R16 = 0,
@@ -5534,95 +5537,95 @@
       <c r="AJ17" s="138"/>
       <c r="AK17" s="139">
         <f>SUM(C17:AI17)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AL17" s="123"/>
     </row>
     <row r="18" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="173">
+      <c r="A18" s="269">
         <f>RANK(AL18,$AL$10:$AL$97,)</f>
         <v>3</v>
       </c>
-      <c r="B18" s="197" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="185">
+      <c r="B18" s="270" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="284">
         <v>5</v>
       </c>
-      <c r="D18" s="186"/>
-      <c r="E18" s="238">
+      <c r="D18" s="285"/>
+      <c r="E18" s="286">
         <v>7</v>
       </c>
-      <c r="F18" s="186"/>
-      <c r="G18" s="188">
+      <c r="F18" s="285"/>
+      <c r="G18" s="287">
+        <v>4</v>
+      </c>
+      <c r="H18" s="288"/>
+      <c r="I18" s="289"/>
+      <c r="J18" s="288">
+        <v>6</v>
+      </c>
+      <c r="K18" s="290">
         <v>5</v>
       </c>
-      <c r="H18" s="189"/>
-      <c r="I18" s="187">
+      <c r="L18" s="288"/>
+      <c r="M18" s="289"/>
+      <c r="N18" s="291">
         <v>6</v>
       </c>
-      <c r="J18" s="189"/>
-      <c r="K18" s="190">
+      <c r="O18" s="289">
+        <v>7</v>
+      </c>
+      <c r="P18" s="285"/>
+      <c r="Q18" s="287">
+        <v>6</v>
+      </c>
+      <c r="R18" s="292"/>
+      <c r="S18" s="293">
+        <f>SUM(C19:R19)</f>
+        <v>37</v>
+      </c>
+      <c r="T18" s="284">
+        <v>6</v>
+      </c>
+      <c r="U18" s="288"/>
+      <c r="V18" s="289"/>
+      <c r="W18" s="288">
+        <v>6</v>
+      </c>
+      <c r="X18" s="290">
         <v>5</v>
       </c>
-      <c r="L18" s="189"/>
-      <c r="M18" s="187">
-        <v>6</v>
-      </c>
-      <c r="N18" s="186"/>
-      <c r="O18" s="187">
-        <v>5</v>
-      </c>
-      <c r="P18" s="186"/>
-      <c r="Q18" s="242">
+      <c r="Y18" s="285"/>
+      <c r="Z18" s="287"/>
+      <c r="AA18" s="292">
         <v>7</v>
       </c>
-      <c r="R18" s="191"/>
-      <c r="S18" s="228">
-        <f>SUM(C19:R19)</f>
-        <v>39</v>
-      </c>
-      <c r="T18" s="185"/>
-      <c r="U18" s="189">
-        <v>6</v>
-      </c>
-      <c r="V18" s="187">
-        <v>6</v>
-      </c>
-      <c r="W18" s="189"/>
-      <c r="X18" s="190"/>
-      <c r="Y18" s="186">
-        <v>6</v>
-      </c>
-      <c r="Z18" s="188">
-        <v>7</v>
-      </c>
-      <c r="AA18" s="191"/>
-      <c r="AB18" s="192">
+      <c r="AB18" s="294">
         <f>SUM(T19:AA19)</f>
-        <v>5</v>
-      </c>
-      <c r="AC18" s="188"/>
-      <c r="AD18" s="189"/>
-      <c r="AE18" s="190"/>
-      <c r="AF18" s="189"/>
-      <c r="AG18" s="192">
+        <v>8</v>
+      </c>
+      <c r="AC18" s="287"/>
+      <c r="AD18" s="288"/>
+      <c r="AE18" s="290"/>
+      <c r="AF18" s="288"/>
+      <c r="AG18" s="294">
         <f>SUM(AC19:AF19)</f>
         <v>0</v>
       </c>
-      <c r="AH18" s="219"/>
-      <c r="AI18" s="193"/>
-      <c r="AJ18" s="192">
+      <c r="AH18" s="295"/>
+      <c r="AI18" s="296"/>
+      <c r="AJ18" s="294">
         <f>AH19</f>
         <v>0</v>
       </c>
-      <c r="AK18" s="194">
+      <c r="AK18" s="297">
         <f>MAX($AL$10:$AL$97) - AL18</f>
-        <v>5</v>
-      </c>
-      <c r="AL18" s="192">
+        <v>4</v>
+      </c>
+      <c r="AL18" s="294">
         <f>$S18+$AB18+$AG18+$AJ18</f>
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5648,7 +5651,7 @@
       <c r="H19" s="140"/>
       <c r="I19" s="120">
         <f>(IF($I18&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I18=$I$6+$J$6,$O$103,0),0),0)+IF($J18&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J18=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J19" s="141"/>
       <c r="K19" s="142">
@@ -5658,7 +5661,7 @@
       <c r="L19" s="140"/>
       <c r="M19" s="120">
         <f>(IF($M18&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M18=$M$6+$N$6,$O$103,0),0),0)+IF($N18&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N18=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="N19" s="140"/>
       <c r="O19" s="120">
@@ -5668,23 +5671,23 @@
       <c r="P19" s="140"/>
       <c r="Q19" s="120">
         <f>(IF($Q18&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q18=$Q$6+$R$6,$O$103,0),0),0)+IF($R18&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R18=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="R19" s="143"/>
       <c r="S19" s="144"/>
       <c r="T19" s="126">
         <f>(IF($T18&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T18=$T$6+$U$6,$P$103,0),0),0)+IF($U18&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U18=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U19" s="126"/>
       <c r="V19" s="126">
         <f>(IF($V18&lt;&gt;"",($V$6*$P$104)+IF($V$6=4,($P$102)+IF($V18=$V$6+$W$6,$P$103,0),0),0)+IF($W18&lt;&gt;"",($W$6*$P$104)+IF($W$6=4,($P$102)+IF($W18=$V$6+$W$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W19" s="126"/>
       <c r="X19" s="126">
         <f>(IF($X18&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X18=$X$6+$Y$6,$P$103,0),0),0)+IF($Y18&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y18=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y19" s="59"/>
       <c r="Z19" s="126">
@@ -5752,7 +5755,7 @@
         <f>IF(ISBLANK(I18),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" s="118">
         <f>IF(ISBLANK(J18),
@@ -5782,7 +5785,7 @@
         <f>IF(ISBLANK(N18),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O20" s="118">
         <f>IF(ISBLANK(O18),
@@ -5947,7 +5950,7 @@
         <f>IF(N20 = 0,
 0,
 IF(N18 = (M$6+N$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O21" s="118">
         <f>IF(O20 = 0,
@@ -5965,7 +5968,7 @@
         <f>IF(Q20 = 0,
 0,
 IF(Q18 = (Q$6+R$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R21" s="118">
         <f>IF(R20 = 0,
@@ -6043,63 +6046,63 @@
         <v>4</v>
       </c>
       <c r="B22" s="84" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C22" s="46">
         <v>5</v>
       </c>
       <c r="D22" s="45"/>
-      <c r="E22" s="237">
+      <c r="E22" s="210">
         <v>7</v>
       </c>
       <c r="F22" s="45"/>
       <c r="G22" s="48">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H22" s="47"/>
-      <c r="I22" s="44"/>
-      <c r="J22" s="47">
+      <c r="I22" s="44">
         <v>6</v>
       </c>
+      <c r="J22" s="47"/>
       <c r="K22" s="49">
         <v>5</v>
       </c>
       <c r="L22" s="47"/>
-      <c r="M22" s="44"/>
-      <c r="N22" s="239">
+      <c r="M22" s="44">
         <v>6</v>
       </c>
+      <c r="N22" s="45"/>
       <c r="O22" s="44">
+        <v>5</v>
+      </c>
+      <c r="P22" s="45"/>
+      <c r="Q22" s="213">
         <v>7</v>
-      </c>
-      <c r="P22" s="45"/>
-      <c r="Q22" s="48">
-        <v>6</v>
       </c>
       <c r="R22" s="50"/>
       <c r="S22" s="122">
         <f>SUM(C23:R23)</f>
-        <v>37</v>
-      </c>
-      <c r="T22" s="46">
+        <v>39</v>
+      </c>
+      <c r="T22" s="46"/>
+      <c r="U22" s="47">
         <v>6</v>
       </c>
-      <c r="U22" s="47"/>
-      <c r="V22" s="44"/>
-      <c r="W22" s="47">
+      <c r="V22" s="44">
         <v>6</v>
       </c>
-      <c r="X22" s="49">
-        <v>5</v>
-      </c>
-      <c r="Y22" s="45"/>
-      <c r="Z22" s="48"/>
-      <c r="AA22" s="50">
+      <c r="W22" s="47"/>
+      <c r="X22" s="49"/>
+      <c r="Y22" s="45">
+        <v>6</v>
+      </c>
+      <c r="Z22" s="48">
         <v>7</v>
       </c>
+      <c r="AA22" s="50"/>
       <c r="AB22" s="122">
         <f>SUM(T23:AA23)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AC22" s="48"/>
       <c r="AD22" s="47"/>
@@ -6109,7 +6112,7 @@
         <f>SUM(AC23:AF23)</f>
         <v>0</v>
       </c>
-      <c r="AH22" s="245"/>
+      <c r="AH22" s="267"/>
       <c r="AI22" s="57"/>
       <c r="AJ22" s="122">
         <f>AH23</f>
@@ -6117,11 +6120,11 @@
       </c>
       <c r="AK22" s="111">
         <f>MAX($AL$10:$AL$97) - AL22</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AL22" s="122">
         <f>$S22+$AB22+$AG22+$AJ22</f>
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6147,7 +6150,7 @@
       <c r="H23" s="151"/>
       <c r="I23" s="125">
         <f>(IF($I22&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I22=$I$6+$J$6,$O$103,0),0),0)+IF($J22&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J22=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J23" s="152"/>
       <c r="K23" s="153">
@@ -6157,7 +6160,7 @@
       <c r="L23" s="151"/>
       <c r="M23" s="125">
         <f>(IF($M22&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M22=$M$6+$N$6,$O$103,0),0),0)+IF($N22&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N22=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="N23" s="151"/>
       <c r="O23" s="125">
@@ -6167,28 +6170,28 @@
       <c r="P23" s="151"/>
       <c r="Q23" s="125">
         <f>(IF($Q22&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q22=$Q$6+$R$6,$O$103,0),0),0)+IF($R22&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R22=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="R23" s="154"/>
       <c r="S23" s="144"/>
       <c r="T23" s="126">
         <f>(IF($T22&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T22=$T$6+$U$6,$P$103,0),0),0)+IF($U22&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U22=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U23" s="126"/>
       <c r="V23" s="126">
         <f>(IF($V22&lt;&gt;"",($V$6*$P$104)+IF($V$6=4,($P$102)+IF($V22=$V$6+$W$6,$P$103,0),0),0)+IF($W22&lt;&gt;"",($W$6*$P$104)+IF($W$6=4,($P$102)+IF($W22=$V$6+$W$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W23" s="126"/>
       <c r="X23" s="126">
         <f>(IF($X22&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X22=$X$6+$Y$6,$P$103,0),0),0)+IF($Y22&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y22=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y23" s="59"/>
       <c r="Z23" s="126">
         <f>(IF($Z22&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z22=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA22&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA22=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA23" s="62"/>
       <c r="AB23" s="144"/>
@@ -6251,7 +6254,7 @@
         <f>IF(ISBLANK(I22),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" s="118">
         <f>IF(ISBLANK(J22),
@@ -6281,7 +6284,7 @@
         <f>IF(ISBLANK(N22),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O24" s="118">
         <f>IF(ISBLANK(O22),
@@ -6446,7 +6449,7 @@
         <f>IF(N24 = 0,
 0,
 IF(N22 = (M$6+N$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O25" s="118">
         <f>IF(O24 = 0,
@@ -6464,7 +6467,7 @@
         <f>IF(Q24 = 0,
 0,
 IF(Q22 = (Q$6+R$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R25" s="118">
         <f>IF(R24 = 0,
@@ -6537,90 +6540,90 @@
       <c r="AL25" s="123"/>
     </row>
     <row r="26" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="173">
+      <c r="A26" s="269">
         <f>RANK(AL26,$AL$10:$AL$97,)</f>
         <v>4</v>
       </c>
-      <c r="B26" s="197" t="s">
-        <v>71</v>
-      </c>
-      <c r="C26" s="185">
+      <c r="B26" s="270" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="284">
         <v>5</v>
       </c>
-      <c r="D26" s="186"/>
-      <c r="E26" s="238">
+      <c r="D26" s="285"/>
+      <c r="E26" s="289">
+        <v>6</v>
+      </c>
+      <c r="F26" s="285"/>
+      <c r="G26" s="287"/>
+      <c r="H26" s="298">
         <v>7</v>
       </c>
-      <c r="F26" s="186"/>
-      <c r="G26" s="188">
+      <c r="I26" s="289"/>
+      <c r="J26" s="288">
         <v>6</v>
       </c>
-      <c r="H26" s="189"/>
-      <c r="I26" s="187">
+      <c r="K26" s="290">
+        <v>5</v>
+      </c>
+      <c r="L26" s="288"/>
+      <c r="M26" s="289"/>
+      <c r="N26" s="285">
+        <v>7</v>
+      </c>
+      <c r="O26" s="289">
+        <v>5</v>
+      </c>
+      <c r="P26" s="285"/>
+      <c r="Q26" s="287"/>
+      <c r="R26" s="292">
         <v>6</v>
       </c>
-      <c r="J26" s="189"/>
-      <c r="K26" s="190">
-        <v>4</v>
-      </c>
-      <c r="L26" s="189"/>
-      <c r="M26" s="187">
+      <c r="S26" s="294">
+        <f>SUM(C27:R27)</f>
+        <v>35</v>
+      </c>
+      <c r="T26" s="284"/>
+      <c r="U26" s="288">
+        <v>7</v>
+      </c>
+      <c r="V26" s="289"/>
+      <c r="W26" s="288">
+        <v>7</v>
+      </c>
+      <c r="X26" s="290">
+        <v>6</v>
+      </c>
+      <c r="Y26" s="285"/>
+      <c r="Z26" s="287">
+        <v>6</v>
+      </c>
+      <c r="AA26" s="292"/>
+      <c r="AB26" s="294">
+        <f>SUM(T27:AA27)</f>
+        <v>9</v>
+      </c>
+      <c r="AC26" s="287"/>
+      <c r="AD26" s="288"/>
+      <c r="AE26" s="290"/>
+      <c r="AF26" s="288"/>
+      <c r="AG26" s="294">
+        <f>SUM(AC27:AF27)</f>
+        <v>0</v>
+      </c>
+      <c r="AH26" s="281"/>
+      <c r="AI26" s="282"/>
+      <c r="AJ26" s="294">
+        <f>AH27</f>
+        <v>0</v>
+      </c>
+      <c r="AK26" s="297">
+        <f>MAX($AL$10:$AL$97) - AL26</f>
         <v>5</v>
       </c>
-      <c r="N26" s="186"/>
-      <c r="O26" s="187"/>
-      <c r="P26" s="186">
-        <v>7</v>
-      </c>
-      <c r="Q26" s="188"/>
-      <c r="R26" s="191">
-        <v>7</v>
-      </c>
-      <c r="S26" s="192">
-        <f>SUM(C27:R27)</f>
-        <v>38</v>
-      </c>
-      <c r="T26" s="185"/>
-      <c r="U26" s="189">
-        <v>6</v>
-      </c>
-      <c r="V26" s="187">
-        <v>5</v>
-      </c>
-      <c r="W26" s="189"/>
-      <c r="X26" s="190"/>
-      <c r="Y26" s="186">
-        <v>5</v>
-      </c>
-      <c r="Z26" s="188">
-        <v>7</v>
-      </c>
-      <c r="AA26" s="191"/>
-      <c r="AB26" s="192">
-        <f>SUM(T27:AA27)</f>
-        <v>5</v>
-      </c>
-      <c r="AC26" s="188"/>
-      <c r="AD26" s="246"/>
-      <c r="AE26" s="190"/>
-      <c r="AF26" s="189"/>
-      <c r="AG26" s="192">
-        <f>SUM(AC27:AF27)</f>
-        <v>0</v>
-      </c>
-      <c r="AH26" s="182"/>
-      <c r="AI26" s="183"/>
-      <c r="AJ26" s="192">
-        <f>AH27</f>
-        <v>0</v>
-      </c>
-      <c r="AK26" s="194">
-        <f>MAX($AL$10:$AL$97) - AL26</f>
-        <v>6</v>
-      </c>
-      <c r="AL26" s="192">
+      <c r="AL26" s="294">
         <f>$S26+$AB26+$AG26+$AJ26</f>
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6636,17 +6639,17 @@
       <c r="D27" s="140"/>
       <c r="E27" s="120">
         <f>(IF($E26&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E26=$E$6+$F$6,$O$103,0),0),0)+IF($F26&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F26=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F27" s="140"/>
       <c r="G27" s="120">
         <f>(IF($G26&lt;&gt;"",($G$6*$O$104)+IF($G$6=4,($O$102)+IF($G26=$G$6+$H$6,$O$103,0),0),0)+IF($H26&lt;&gt;"",($H$6*$O$104)+IF($H$6=4,($O$102)+IF($H26=$G$6+$H$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="H27" s="140"/>
       <c r="I27" s="120">
         <f>(IF($I26&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I26=$I$6+$J$6,$O$103,0),0),0)+IF($J26&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J26=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J27" s="141"/>
       <c r="K27" s="142">
@@ -6656,12 +6659,12 @@
       <c r="L27" s="140"/>
       <c r="M27" s="120">
         <f>(IF($M26&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M26=$M$6+$N$6,$O$103,0),0),0)+IF($N26&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N26=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="N27" s="140"/>
       <c r="O27" s="120">
         <f>(IF($O26&lt;&gt;"",($O$6*$O$104)+IF($O$6=4,($O$102)+IF($O26=$O$6+$P$6,$O$103,0),0),0)+IF($P26&lt;&gt;"",($P$6*$O$104)+IF($P$6=4,($O$102)+IF($P26=$O$6+$P$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="P27" s="140"/>
       <c r="Q27" s="120">
@@ -6677,12 +6680,12 @@
       <c r="U27" s="126"/>
       <c r="V27" s="126">
         <f>(IF($V26&lt;&gt;"",($V$6*$P$104)+IF($V$6=4,($P$102)+IF($V26=$V$6+$W$6,$P$103,0),0),0)+IF($W26&lt;&gt;"",($W$6*$P$104)+IF($W$6=4,($P$102)+IF($W26=$V$6+$W$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W27" s="126"/>
       <c r="X27" s="126">
         <f>(IF($X26&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X26=$X$6+$Y$6,$P$103,0),0),0)+IF($Y26&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y26=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y27" s="59"/>
       <c r="Z27" s="126">
@@ -6744,13 +6747,13 @@
         <f>IF(ISBLANK(H26),
 0,
 IF(H$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28" s="118">
         <f>IF(ISBLANK(I26),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" s="118">
         <f>IF(ISBLANK(J26),
@@ -6780,7 +6783,7 @@
         <f>IF(ISBLANK(N26),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O28" s="118">
         <f>IF(ISBLANK(O26),
@@ -6792,7 +6795,7 @@
         <f>IF(ISBLANK(P26),
 0,
 IF(P$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q28" s="118">
         <f>IF(ISBLANK(Q26),
@@ -6891,7 +6894,7 @@
         <f>IF(E28 = 0,
 0,
 IF(E26 = (E$6+F$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29" s="118">
         <f>IF(F28 = 0,
@@ -6909,7 +6912,7 @@
         <f>IF(H28 = 0,
 0,
 IF(H26 = (G$6+H$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29" s="118">
         <f>IF(I28 = 0,
@@ -7038,69 +7041,69 @@
     <row r="30" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="117">
         <f>RANK(AL30,$AL$10:$AL$97,)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B30" s="84" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C30" s="46">
         <v>5</v>
       </c>
       <c r="D30" s="45"/>
-      <c r="E30" s="44">
+      <c r="E30" s="210">
+        <v>7</v>
+      </c>
+      <c r="F30" s="45"/>
+      <c r="G30" s="48">
         <v>6</v>
       </c>
-      <c r="F30" s="45"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="243">
+      <c r="H30" s="47"/>
+      <c r="I30" s="44">
+        <v>6</v>
+      </c>
+      <c r="J30" s="47"/>
+      <c r="K30" s="49">
+        <v>4</v>
+      </c>
+      <c r="L30" s="47"/>
+      <c r="M30" s="44">
+        <v>5</v>
+      </c>
+      <c r="N30" s="45"/>
+      <c r="O30" s="44"/>
+      <c r="P30" s="45">
         <v>7</v>
       </c>
-      <c r="I30" s="44"/>
-      <c r="J30" s="47">
-        <v>6</v>
-      </c>
-      <c r="K30" s="49">
-        <v>5</v>
-      </c>
-      <c r="L30" s="47"/>
-      <c r="M30" s="44"/>
-      <c r="N30" s="45">
-        <v>7</v>
-      </c>
-      <c r="O30" s="44">
-        <v>5</v>
-      </c>
-      <c r="P30" s="45"/>
       <c r="Q30" s="48"/>
       <c r="R30" s="50">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S30" s="122">
         <f>SUM(C31:R31)</f>
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="T30" s="46"/>
       <c r="U30" s="47">
+        <v>6</v>
+      </c>
+      <c r="V30" s="44">
+        <v>5</v>
+      </c>
+      <c r="W30" s="47"/>
+      <c r="X30" s="49"/>
+      <c r="Y30" s="45">
+        <v>5</v>
+      </c>
+      <c r="Z30" s="48">
         <v>7</v>
-      </c>
-      <c r="V30" s="44"/>
-      <c r="W30" s="47">
-        <v>7</v>
-      </c>
-      <c r="X30" s="49">
-        <v>6</v>
-      </c>
-      <c r="Y30" s="45"/>
-      <c r="Z30" s="48">
-        <v>6</v>
       </c>
       <c r="AA30" s="47"/>
       <c r="AB30" s="122">
         <f>SUM(T31:AA31)</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AC30" s="48"/>
-      <c r="AD30" s="47"/>
+      <c r="AD30" s="268"/>
       <c r="AE30" s="49"/>
       <c r="AF30" s="47"/>
       <c r="AG30" s="122">
@@ -7135,17 +7138,17 @@
       <c r="D31" s="76"/>
       <c r="E31" s="77">
         <f>(IF($E30&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E30=$E$6+$F$6,$O$103,0),0),0)+IF($F30&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F30=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F31" s="76"/>
       <c r="G31" s="77">
         <f>(IF($G30&lt;&gt;"",($G$6*$O$104)+IF($G$6=4,($O$102)+IF($G30=$G$6+$H$6,$O$103,0),0),0)+IF($H30&lt;&gt;"",($H$6*$O$104)+IF($H$6=4,($O$102)+IF($H30=$G$6+$H$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="H31" s="76"/>
       <c r="I31" s="77">
         <f>(IF($I30&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I30=$I$6+$J$6,$O$103,0),0),0)+IF($J30&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J30=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J31" s="78"/>
       <c r="K31" s="79">
@@ -7155,12 +7158,12 @@
       <c r="L31" s="76"/>
       <c r="M31" s="77">
         <f>(IF($M30&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M30=$M$6+$N$6,$O$103,0),0),0)+IF($N30&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N30=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="N31" s="76"/>
       <c r="O31" s="77">
         <f>(IF($O30&lt;&gt;"",($O$6*$O$104)+IF($O$6=4,($O$102)+IF($O30=$O$6+$P$6,$O$103,0),0),0)+IF($P30&lt;&gt;"",($P$6*$O$104)+IF($P$6=4,($O$102)+IF($P30=$O$6+$P$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="P31" s="76"/>
       <c r="Q31" s="77">
@@ -7176,12 +7179,12 @@
       <c r="U31" s="126"/>
       <c r="V31" s="126">
         <f>(IF($V30&lt;&gt;"",($V$6*$P$104)+IF($V$6=4,($P$102)+IF($V30=$V$6+$W$6,$P$103,0),0),0)+IF($W30&lt;&gt;"",($W$6*$P$104)+IF($W$6=4,($P$102)+IF($W30=$V$6+$W$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W31" s="126"/>
       <c r="X31" s="126">
         <f>(IF($X30&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X30=$X$6+$Y$6,$P$103,0),0),0)+IF($Y30&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y30=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y31" s="59"/>
       <c r="Z31" s="126">
@@ -7243,13 +7246,13 @@
         <f>IF(ISBLANK(H30),
 0,
 IF(H$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I32" s="118">
         <f>IF(ISBLANK(I30),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J32" s="118">
         <f>IF(ISBLANK(J30),
@@ -7279,7 +7282,7 @@
         <f>IF(ISBLANK(N30),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O32" s="118">
         <f>IF(ISBLANK(O30),
@@ -7291,7 +7294,7 @@
         <f>IF(ISBLANK(P30),
 0,
 IF(P$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q32" s="118">
         <f>IF(ISBLANK(Q30),
@@ -7390,7 +7393,7 @@
         <f>IF(E32 = 0,
 0,
 IF(E30 = (E$6+F$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33" s="118">
         <f>IF(F32 = 0,
@@ -7408,7 +7411,7 @@
         <f>IF(H32 = 0,
 0,
 IF(H30 = (G$6+H$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I33" s="118">
         <f>IF(I32 = 0,
@@ -7535,90 +7538,90 @@
       <c r="AL33" s="123"/>
     </row>
     <row r="34" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="173">
+      <c r="A34" s="269">
         <f>RANK(AL34,$AL$10:$AL$97,)</f>
         <v>7</v>
       </c>
-      <c r="B34" s="197" t="s">
+      <c r="B34" s="270" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="185">
+      <c r="C34" s="284">
         <v>7</v>
       </c>
-      <c r="D34" s="186"/>
-      <c r="E34" s="308">
+      <c r="D34" s="285"/>
+      <c r="E34" s="299">
         <v>6</v>
       </c>
-      <c r="F34" s="186"/>
-      <c r="G34" s="309"/>
-      <c r="H34" s="189">
+      <c r="F34" s="285"/>
+      <c r="G34" s="300"/>
+      <c r="H34" s="288">
         <v>6</v>
       </c>
-      <c r="I34" s="308"/>
-      <c r="J34" s="189">
+      <c r="I34" s="299"/>
+      <c r="J34" s="288">
         <v>7</v>
       </c>
-      <c r="K34" s="190">
+      <c r="K34" s="290">
         <v>5</v>
       </c>
-      <c r="L34" s="189"/>
-      <c r="M34" s="187">
+      <c r="L34" s="288"/>
+      <c r="M34" s="289">
         <v>7</v>
       </c>
-      <c r="N34" s="186"/>
-      <c r="O34" s="187">
+      <c r="N34" s="285"/>
+      <c r="O34" s="289">
         <v>6</v>
       </c>
-      <c r="P34" s="186"/>
-      <c r="Q34" s="188">
+      <c r="P34" s="285"/>
+      <c r="Q34" s="287">
         <v>6</v>
       </c>
-      <c r="R34" s="191"/>
-      <c r="S34" s="192">
+      <c r="R34" s="292"/>
+      <c r="S34" s="294">
         <f>SUM(C35:R35)</f>
         <v>32</v>
       </c>
-      <c r="T34" s="185"/>
-      <c r="U34" s="189">
+      <c r="T34" s="284"/>
+      <c r="U34" s="288">
         <v>7</v>
       </c>
-      <c r="V34" s="187"/>
-      <c r="W34" s="189">
+      <c r="V34" s="289"/>
+      <c r="W34" s="288">
         <v>6</v>
       </c>
-      <c r="X34" s="190">
+      <c r="X34" s="290">
         <v>7</v>
       </c>
-      <c r="Y34" s="186"/>
-      <c r="Z34" s="188">
+      <c r="Y34" s="285"/>
+      <c r="Z34" s="287">
         <v>6</v>
       </c>
-      <c r="AA34" s="189"/>
-      <c r="AB34" s="192">
+      <c r="AA34" s="288"/>
+      <c r="AB34" s="294">
         <f>SUM(T35:AA35)</f>
+        <v>9</v>
+      </c>
+      <c r="AC34" s="287"/>
+      <c r="AD34" s="288"/>
+      <c r="AE34" s="290"/>
+      <c r="AF34" s="288"/>
+      <c r="AG34" s="294">
+        <f>SUM(AC35:AF35)</f>
+        <v>0</v>
+      </c>
+      <c r="AH34" s="301"/>
+      <c r="AI34" s="282"/>
+      <c r="AJ34" s="294">
+        <f>AH35</f>
+        <v>0</v>
+      </c>
+      <c r="AK34" s="297">
+        <f>MAX($AL$10:$AL$97) - AL34</f>
         <v>8</v>
       </c>
-      <c r="AC34" s="188"/>
-      <c r="AD34" s="189"/>
-      <c r="AE34" s="190"/>
-      <c r="AF34" s="189"/>
-      <c r="AG34" s="192">
-        <f>SUM(AC35:AF35)</f>
-        <v>0</v>
-      </c>
-      <c r="AH34" s="195"/>
-      <c r="AI34" s="183"/>
-      <c r="AJ34" s="192">
-        <f>AH35</f>
-        <v>0</v>
-      </c>
-      <c r="AK34" s="194">
-        <f>MAX($AL$10:$AL$97) - AL34</f>
-        <v>9</v>
-      </c>
-      <c r="AL34" s="192">
+      <c r="AL34" s="294">
         <f>$S34+$AB34+$AG34+$AJ34</f>
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7675,7 +7678,7 @@
       <c r="U35" s="126"/>
       <c r="V35" s="126">
         <f>(IF($V34&lt;&gt;"",($V$6*$P$104)+IF($V$6=4,($P$102)+IF($V34=$V$6+$W$6,$P$103,0),0),0)+IF($W34&lt;&gt;"",($W$6*$P$104)+IF($W$6=4,($P$102)+IF($W34=$V$6+$W$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W35" s="126"/>
       <c r="X35" s="126">
@@ -8036,7 +8039,7 @@
     <row r="38" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="117">
         <f>RANK(AL38,$AL$10:$AL$97,)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B38" s="84" t="s">
         <v>81</v>
@@ -8069,7 +8072,7 @@
         <v>6</v>
       </c>
       <c r="P38" s="45"/>
-      <c r="Q38" s="299">
+      <c r="Q38" s="213">
         <v>7</v>
       </c>
       <c r="R38" s="50"/>
@@ -8533,90 +8536,90 @@
       <c r="AL41" s="123"/>
     </row>
     <row r="42" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="173">
+      <c r="A42" s="269">
         <f>RANK(AL42,$AL$10:$AL$97,)</f>
         <v>9</v>
       </c>
-      <c r="B42" s="197" t="s">
+      <c r="B42" s="270" t="s">
         <v>79</v>
       </c>
-      <c r="C42" s="185">
+      <c r="C42" s="284">
         <v>6</v>
       </c>
-      <c r="D42" s="186"/>
-      <c r="E42" s="187"/>
-      <c r="F42" s="186">
+      <c r="D42" s="285"/>
+      <c r="E42" s="289"/>
+      <c r="F42" s="285">
         <v>7</v>
       </c>
-      <c r="G42" s="188">
+      <c r="G42" s="287">
         <v>6</v>
       </c>
-      <c r="H42" s="189"/>
-      <c r="I42" s="187"/>
-      <c r="J42" s="189">
+      <c r="H42" s="288"/>
+      <c r="I42" s="289"/>
+      <c r="J42" s="288">
         <v>6</v>
       </c>
-      <c r="K42" s="190"/>
-      <c r="L42" s="189">
+      <c r="K42" s="290"/>
+      <c r="L42" s="288">
         <v>6</v>
       </c>
-      <c r="M42" s="187"/>
-      <c r="N42" s="240">
+      <c r="M42" s="289"/>
+      <c r="N42" s="291">
         <v>6</v>
       </c>
-      <c r="O42" s="187">
+      <c r="O42" s="289">
         <v>5</v>
       </c>
-      <c r="P42" s="186"/>
-      <c r="Q42" s="188"/>
-      <c r="R42" s="191">
+      <c r="P42" s="285"/>
+      <c r="Q42" s="287"/>
+      <c r="R42" s="292">
         <v>6</v>
       </c>
-      <c r="S42" s="192">
+      <c r="S42" s="294">
         <f>SUM(C43:R43)</f>
         <v>31</v>
       </c>
-      <c r="T42" s="185"/>
-      <c r="U42" s="189">
+      <c r="T42" s="284"/>
+      <c r="U42" s="288">
         <v>5</v>
       </c>
-      <c r="V42" s="187">
+      <c r="V42" s="289">
         <v>6</v>
       </c>
-      <c r="W42" s="189"/>
-      <c r="X42" s="190">
+      <c r="W42" s="288"/>
+      <c r="X42" s="290">
         <v>6</v>
       </c>
-      <c r="Y42" s="186"/>
-      <c r="Z42" s="188"/>
-      <c r="AA42" s="189">
+      <c r="Y42" s="285"/>
+      <c r="Z42" s="287"/>
+      <c r="AA42" s="288">
         <v>6</v>
       </c>
-      <c r="AB42" s="192">
+      <c r="AB42" s="294">
         <f>SUM(T43:AA43)</f>
-        <v>5</v>
-      </c>
-      <c r="AC42" s="188"/>
-      <c r="AD42" s="189"/>
-      <c r="AE42" s="190"/>
-      <c r="AF42" s="189"/>
-      <c r="AG42" s="192">
+        <v>6</v>
+      </c>
+      <c r="AC42" s="287"/>
+      <c r="AD42" s="288"/>
+      <c r="AE42" s="290"/>
+      <c r="AF42" s="288"/>
+      <c r="AG42" s="294">
         <f>SUM(AC43:AF43)</f>
         <v>0</v>
       </c>
-      <c r="AH42" s="195"/>
-      <c r="AI42" s="183"/>
-      <c r="AJ42" s="192">
+      <c r="AH42" s="301"/>
+      <c r="AI42" s="282"/>
+      <c r="AJ42" s="294">
         <f>AH43</f>
         <v>0</v>
       </c>
-      <c r="AK42" s="194">
+      <c r="AK42" s="297">
         <f>MAX($AL$10:$AL$97) - AL42</f>
-        <v>13</v>
-      </c>
-      <c r="AL42" s="192">
+        <v>12</v>
+      </c>
+      <c r="AL42" s="294">
         <f>$S42+$AB42+$AG42+$AJ42</f>
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -8683,7 +8686,7 @@
       <c r="Y43" s="59"/>
       <c r="Z43" s="126">
         <f>(IF($Z42&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z42=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA42&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA42=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA43" s="62"/>
       <c r="AB43" s="121"/>
@@ -9060,7 +9063,7 @@
       </c>
       <c r="L46" s="47"/>
       <c r="M46" s="44"/>
-      <c r="N46" s="239">
+      <c r="N46" s="211">
         <v>6</v>
       </c>
       <c r="O46" s="44">
@@ -9103,7 +9106,7 @@
         <f>SUM(AC47:AF47)</f>
         <v>0</v>
       </c>
-      <c r="AH46" s="300"/>
+      <c r="AH46" s="214"/>
       <c r="AI46" s="57"/>
       <c r="AJ46" s="122">
         <f>AH47</f>
@@ -9531,88 +9534,88 @@
       <c r="AL49" s="123"/>
     </row>
     <row r="50" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="173">
+      <c r="A50" s="269">
         <f>RANK(AL50,$AL$10:$AL$97,)</f>
         <v>11</v>
       </c>
-      <c r="B50" s="197" t="s">
+      <c r="B50" s="270" t="s">
         <v>74</v>
       </c>
-      <c r="C50" s="185">
+      <c r="C50" s="284">
         <v>5</v>
       </c>
-      <c r="D50" s="186"/>
-      <c r="E50" s="187">
+      <c r="D50" s="285"/>
+      <c r="E50" s="289">
         <v>6</v>
       </c>
-      <c r="F50" s="186"/>
-      <c r="G50" s="188">
+      <c r="F50" s="285"/>
+      <c r="G50" s="287">
         <v>6</v>
       </c>
-      <c r="H50" s="189"/>
-      <c r="I50" s="187"/>
-      <c r="J50" s="189">
+      <c r="H50" s="288"/>
+      <c r="I50" s="289"/>
+      <c r="J50" s="288">
         <v>7</v>
       </c>
-      <c r="K50" s="190">
+      <c r="K50" s="290">
         <v>5</v>
       </c>
-      <c r="L50" s="189"/>
-      <c r="M50" s="187"/>
-      <c r="N50" s="240">
+      <c r="L50" s="288"/>
+      <c r="M50" s="289"/>
+      <c r="N50" s="291">
         <v>6</v>
       </c>
-      <c r="O50" s="187">
+      <c r="O50" s="289">
         <v>7</v>
       </c>
-      <c r="P50" s="186"/>
-      <c r="Q50" s="188"/>
-      <c r="R50" s="191">
+      <c r="P50" s="285"/>
+      <c r="Q50" s="287"/>
+      <c r="R50" s="292">
         <v>6</v>
       </c>
-      <c r="S50" s="192">
+      <c r="S50" s="294">
         <f>SUM(C51:R51)</f>
         <v>29</v>
       </c>
-      <c r="T50" s="185"/>
-      <c r="U50" s="189">
+      <c r="T50" s="284"/>
+      <c r="U50" s="288">
         <v>6</v>
       </c>
-      <c r="V50" s="187">
+      <c r="V50" s="289">
         <v>5</v>
       </c>
-      <c r="W50" s="189"/>
-      <c r="X50" s="190"/>
-      <c r="Y50" s="186">
+      <c r="W50" s="288"/>
+      <c r="X50" s="290"/>
+      <c r="Y50" s="285">
         <v>5</v>
       </c>
-      <c r="Z50" s="188">
+      <c r="Z50" s="287">
         <v>6</v>
       </c>
-      <c r="AA50" s="189"/>
-      <c r="AB50" s="192">
+      <c r="AA50" s="288"/>
+      <c r="AB50" s="294">
         <f>SUM(T51:AA51)</f>
         <v>5</v>
       </c>
-      <c r="AC50" s="188"/>
-      <c r="AD50" s="189"/>
-      <c r="AE50" s="190"/>
-      <c r="AF50" s="189"/>
-      <c r="AG50" s="192">
+      <c r="AC50" s="287"/>
+      <c r="AD50" s="288"/>
+      <c r="AE50" s="290"/>
+      <c r="AF50" s="288"/>
+      <c r="AG50" s="294">
         <f>SUM(AC51:AF51)</f>
         <v>0</v>
       </c>
-      <c r="AH50" s="195"/>
-      <c r="AI50" s="183"/>
-      <c r="AJ50" s="192">
+      <c r="AH50" s="301"/>
+      <c r="AI50" s="282"/>
+      <c r="AJ50" s="294">
         <f>AH51</f>
         <v>0</v>
       </c>
-      <c r="AK50" s="194">
+      <c r="AK50" s="297">
         <f>MAX($AL$10:$AL$97) - AL50</f>
         <v>15</v>
       </c>
-      <c r="AL50" s="192">
+      <c r="AL50" s="294">
         <f>$S50+$AB50+$AG50+$AJ50</f>
         <v>34</v>
       </c>
@@ -10038,7 +10041,7 @@
         <v>6</v>
       </c>
       <c r="D54" s="45"/>
-      <c r="E54" s="237">
+      <c r="E54" s="210">
         <v>7</v>
       </c>
       <c r="F54" s="45"/>
@@ -10523,88 +10526,88 @@
       <c r="AL57" s="123"/>
     </row>
     <row r="58" spans="1:38" s="27" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="173">
+      <c r="A58" s="269">
         <f>RANK(AL58,$AL$10:$AL$97,)</f>
         <v>13</v>
       </c>
-      <c r="B58" s="197" t="s">
+      <c r="B58" s="270" t="s">
         <v>65</v>
       </c>
-      <c r="C58" s="185">
+      <c r="C58" s="284">
         <v>4</v>
       </c>
-      <c r="D58" s="186"/>
-      <c r="E58" s="187">
+      <c r="D58" s="285"/>
+      <c r="E58" s="289">
         <v>4</v>
       </c>
-      <c r="F58" s="186"/>
-      <c r="G58" s="188">
+      <c r="F58" s="285"/>
+      <c r="G58" s="287">
         <v>6</v>
       </c>
-      <c r="H58" s="189"/>
-      <c r="I58" s="187">
+      <c r="H58" s="288"/>
+      <c r="I58" s="289">
         <v>6</v>
       </c>
-      <c r="J58" s="189"/>
-      <c r="K58" s="190">
+      <c r="J58" s="288"/>
+      <c r="K58" s="290">
         <v>7</v>
       </c>
-      <c r="L58" s="189"/>
-      <c r="M58" s="187">
+      <c r="L58" s="288"/>
+      <c r="M58" s="289">
         <v>5</v>
       </c>
-      <c r="N58" s="186"/>
-      <c r="O58" s="187">
+      <c r="N58" s="285"/>
+      <c r="O58" s="289">
         <v>4</v>
       </c>
-      <c r="P58" s="186"/>
-      <c r="Q58" s="188"/>
-      <c r="R58" s="191">
+      <c r="P58" s="285"/>
+      <c r="Q58" s="287"/>
+      <c r="R58" s="292">
         <v>6</v>
       </c>
-      <c r="S58" s="192">
+      <c r="S58" s="294">
         <f>SUM(C59:R59)</f>
         <v>29</v>
       </c>
-      <c r="T58" s="185">
+      <c r="T58" s="284">
         <v>6</v>
       </c>
-      <c r="U58" s="189"/>
-      <c r="V58" s="187">
+      <c r="U58" s="288"/>
+      <c r="V58" s="289">
         <v>5</v>
       </c>
-      <c r="W58" s="189"/>
-      <c r="X58" s="190"/>
-      <c r="Y58" s="186">
+      <c r="W58" s="288"/>
+      <c r="X58" s="290"/>
+      <c r="Y58" s="285">
         <v>7</v>
       </c>
-      <c r="Z58" s="188">
+      <c r="Z58" s="287">
         <v>6</v>
       </c>
-      <c r="AA58" s="189"/>
-      <c r="AB58" s="192">
+      <c r="AA58" s="288"/>
+      <c r="AB58" s="294">
         <f>SUM(T59:AA59)</f>
         <v>4</v>
       </c>
-      <c r="AC58" s="188"/>
-      <c r="AD58" s="189"/>
-      <c r="AE58" s="190"/>
-      <c r="AF58" s="189"/>
-      <c r="AG58" s="192">
+      <c r="AC58" s="287"/>
+      <c r="AD58" s="288"/>
+      <c r="AE58" s="290"/>
+      <c r="AF58" s="288"/>
+      <c r="AG58" s="294">
         <f>SUM(AC59:AF59)</f>
         <v>0</v>
       </c>
-      <c r="AH58" s="195"/>
-      <c r="AI58" s="183"/>
-      <c r="AJ58" s="192">
+      <c r="AH58" s="301"/>
+      <c r="AI58" s="282"/>
+      <c r="AJ58" s="294">
         <f>AH59</f>
         <v>0</v>
       </c>
-      <c r="AK58" s="194">
+      <c r="AK58" s="297">
         <f>MAX($AL$10:$AL$97) - AL58</f>
         <v>16</v>
       </c>
-      <c r="AL58" s="192">
+      <c r="AL58" s="294">
         <f>$S58+$AB58+$AG58+$AJ58</f>
         <v>33</v>
       </c>
@@ -11030,7 +11033,7 @@
         <v>6</v>
       </c>
       <c r="D62" s="45"/>
-      <c r="E62" s="237">
+      <c r="E62" s="210">
         <v>7</v>
       </c>
       <c r="F62" s="45"/>
@@ -11080,7 +11083,7 @@
       <c r="AA62" s="47"/>
       <c r="AB62" s="122">
         <f>SUM(T63:AA63)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AC62" s="48"/>
       <c r="AD62" s="47"/>
@@ -11098,11 +11101,11 @@
       </c>
       <c r="AK62" s="111">
         <f>MAX($AL$10:$AL$97) - AL62</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AL62" s="122">
         <f>$S62+$AB62+$AG62+$AJ62</f>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="63" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11159,7 +11162,7 @@
       <c r="U63" s="126"/>
       <c r="V63" s="126">
         <f>(IF($V62&lt;&gt;"",($V$6*$P$104)+IF($V$6=4,($P$102)+IF($V62=$V$6+$W$6,$P$103,0),0),0)+IF($W62&lt;&gt;"",($W$6*$P$104)+IF($W$6=4,($P$102)+IF($W62=$V$6+$W$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W63" s="126"/>
       <c r="X63" s="126">
@@ -11515,90 +11518,90 @@
       <c r="AL65" s="123"/>
     </row>
     <row r="66" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="173">
+      <c r="A66" s="269">
         <f>RANK(AL66,$AL$10:$AL$97,)</f>
         <v>15</v>
       </c>
-      <c r="B66" s="197" t="s">
+      <c r="B66" s="270" t="s">
         <v>67</v>
       </c>
-      <c r="C66" s="185">
+      <c r="C66" s="284">
         <v>4</v>
       </c>
-      <c r="D66" s="186"/>
-      <c r="E66" s="187">
+      <c r="D66" s="285"/>
+      <c r="E66" s="289">
         <v>4</v>
       </c>
-      <c r="F66" s="186"/>
-      <c r="G66" s="188">
+      <c r="F66" s="285"/>
+      <c r="G66" s="287">
         <v>6</v>
       </c>
-      <c r="H66" s="189"/>
-      <c r="I66" s="187"/>
-      <c r="J66" s="189">
+      <c r="H66" s="288"/>
+      <c r="I66" s="289"/>
+      <c r="J66" s="288">
         <v>6</v>
       </c>
-      <c r="K66" s="190">
+      <c r="K66" s="290">
         <v>6</v>
       </c>
-      <c r="L66" s="189"/>
-      <c r="M66" s="187">
+      <c r="L66" s="288"/>
+      <c r="M66" s="289">
         <v>5</v>
       </c>
-      <c r="N66" s="186"/>
-      <c r="O66" s="187">
+      <c r="N66" s="285"/>
+      <c r="O66" s="289">
         <v>6</v>
       </c>
-      <c r="P66" s="186"/>
-      <c r="Q66" s="188"/>
-      <c r="R66" s="191">
+      <c r="P66" s="285"/>
+      <c r="Q66" s="287"/>
+      <c r="R66" s="292">
         <v>6</v>
       </c>
-      <c r="S66" s="192">
+      <c r="S66" s="294">
         <f>SUM(C67:R67)</f>
         <v>20</v>
       </c>
-      <c r="T66" s="185"/>
-      <c r="U66" s="189">
+      <c r="T66" s="284"/>
+      <c r="U66" s="288">
         <v>6</v>
       </c>
-      <c r="V66" s="187"/>
-      <c r="W66" s="189">
+      <c r="V66" s="289"/>
+      <c r="W66" s="288">
         <v>7</v>
       </c>
-      <c r="X66" s="190"/>
-      <c r="Y66" s="186">
+      <c r="X66" s="290"/>
+      <c r="Y66" s="285">
         <v>7</v>
       </c>
-      <c r="Z66" s="188">
+      <c r="Z66" s="287">
         <v>6</v>
       </c>
-      <c r="AA66" s="189"/>
-      <c r="AB66" s="192">
+      <c r="AA66" s="288"/>
+      <c r="AB66" s="294">
         <f>SUM(T67:AA67)</f>
-        <v>7</v>
-      </c>
-      <c r="AC66" s="188"/>
-      <c r="AD66" s="246"/>
-      <c r="AE66" s="190"/>
-      <c r="AF66" s="189"/>
-      <c r="AG66" s="192">
+        <v>8</v>
+      </c>
+      <c r="AC66" s="287"/>
+      <c r="AD66" s="302"/>
+      <c r="AE66" s="290"/>
+      <c r="AF66" s="288"/>
+      <c r="AG66" s="294">
         <f>SUM(AC67:AF67)</f>
         <v>0</v>
       </c>
-      <c r="AH66" s="196"/>
-      <c r="AI66" s="193"/>
-      <c r="AJ66" s="192">
+      <c r="AH66" s="303"/>
+      <c r="AI66" s="296"/>
+      <c r="AJ66" s="294">
         <f>AH67</f>
         <v>0</v>
       </c>
-      <c r="AK66" s="194">
+      <c r="AK66" s="297">
         <f>MAX($AL$10:$AL$97) - AL66</f>
-        <v>22</v>
-      </c>
-      <c r="AL66" s="192">
+        <v>21</v>
+      </c>
+      <c r="AL66" s="294">
         <f>$S66+$AB66+$AG66+$AJ66</f>
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="67" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11655,7 +11658,7 @@
       <c r="U67" s="126"/>
       <c r="V67" s="126">
         <f>(IF($V66&lt;&gt;"",($V$6*$P$104)+IF($V$6=4,($P$102)+IF($V66=$V$6+$W$6,$P$103,0),0),0)+IF($W66&lt;&gt;"",($W$6*$P$104)+IF($W$6=4,($P$102)+IF($W66=$V$6+$W$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W67" s="126"/>
       <c r="X67" s="126">
@@ -12013,41 +12016,41 @@
     <row r="70" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="117">
         <f>RANK(AL70,$AL$10:$AL$97,)</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B70" s="84" t="s">
-        <v>68</v>
-      </c>
-      <c r="C70" s="301">
+        <v>82</v>
+      </c>
+      <c r="C70" s="46">
+        <v>6</v>
+      </c>
+      <c r="D70" s="45"/>
+      <c r="E70" s="44">
+        <v>6</v>
+      </c>
+      <c r="F70" s="45"/>
+      <c r="G70" s="48">
+        <v>6</v>
+      </c>
+      <c r="H70" s="47"/>
+      <c r="I70" s="44"/>
+      <c r="J70" s="47">
+        <v>7</v>
+      </c>
+      <c r="K70" s="49">
         <v>5</v>
       </c>
-      <c r="D70" s="302"/>
-      <c r="E70" s="303">
+      <c r="L70" s="47"/>
+      <c r="M70" s="44">
+        <v>7</v>
+      </c>
+      <c r="N70" s="45"/>
+      <c r="O70" s="44">
         <v>6</v>
       </c>
-      <c r="F70" s="302"/>
-      <c r="G70" s="304">
-        <v>5</v>
-      </c>
-      <c r="H70" s="305"/>
-      <c r="I70" s="303"/>
-      <c r="J70" s="305">
-        <v>6</v>
-      </c>
-      <c r="K70" s="306">
-        <v>6</v>
-      </c>
-      <c r="L70" s="305"/>
-      <c r="M70" s="303">
-        <v>7</v>
-      </c>
-      <c r="N70" s="302"/>
-      <c r="O70" s="303">
-        <v>6</v>
-      </c>
-      <c r="P70" s="302"/>
-      <c r="Q70" s="304"/>
-      <c r="R70" s="307">
+      <c r="P70" s="45"/>
+      <c r="Q70" s="48"/>
+      <c r="R70" s="50">
         <v>6</v>
       </c>
       <c r="S70" s="122">
@@ -12058,21 +12061,21 @@
       <c r="U70" s="47">
         <v>6</v>
       </c>
-      <c r="V70" s="44">
+      <c r="V70" s="44"/>
+      <c r="W70" s="47">
+        <v>6</v>
+      </c>
+      <c r="X70" s="49"/>
+      <c r="Y70" s="45">
         <v>7</v>
       </c>
-      <c r="W70" s="47"/>
-      <c r="X70" s="49">
+      <c r="Z70" s="48"/>
+      <c r="AA70" s="47">
         <v>6</v>
       </c>
-      <c r="Y70" s="45"/>
-      <c r="Z70" s="48">
-        <v>7</v>
-      </c>
-      <c r="AA70" s="47"/>
       <c r="AB70" s="122">
         <f>SUM(T71:AA71)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AC70" s="48"/>
       <c r="AD70" s="47"/>
@@ -12090,11 +12093,11 @@
       </c>
       <c r="AK70" s="111">
         <f>MAX($AL$10:$AL$97) - AL70</f>
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AL70" s="122">
         <f>$S70+$AB70+$AG70+$AJ70</f>
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="71" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -12151,12 +12154,12 @@
       <c r="U71" s="126"/>
       <c r="V71" s="126">
         <f>(IF($V70&lt;&gt;"",($V$6*$P$104)+IF($V$6=4,($P$102)+IF($V70=$V$6+$W$6,$P$103,0),0),0)+IF($W70&lt;&gt;"",($W$6*$P$104)+IF($W$6=4,($P$102)+IF($W70=$V$6+$W$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W71" s="126"/>
       <c r="X71" s="126">
         <f>(IF($X70&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X70=$X$6+$Y$6,$P$103,0),0),0)+IF($Y70&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y70=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y71" s="59"/>
       <c r="Z71" s="126">
@@ -12507,88 +12510,88 @@
       <c r="AL73" s="123"/>
     </row>
     <row r="74" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="173">
+      <c r="A74" s="269">
         <f>RANK(AL74,$AL$10:$AL$97,)</f>
-        <v>16</v>
-      </c>
-      <c r="B74" s="197" t="s">
-        <v>82</v>
-      </c>
-      <c r="C74" s="185">
+        <v>17</v>
+      </c>
+      <c r="B74" s="270" t="s">
+        <v>68</v>
+      </c>
+      <c r="C74" s="304">
+        <v>5</v>
+      </c>
+      <c r="D74" s="305"/>
+      <c r="E74" s="306">
         <v>6</v>
       </c>
-      <c r="D74" s="186"/>
-      <c r="E74" s="187">
+      <c r="F74" s="305"/>
+      <c r="G74" s="307">
+        <v>5</v>
+      </c>
+      <c r="H74" s="308"/>
+      <c r="I74" s="306"/>
+      <c r="J74" s="308">
         <v>6</v>
       </c>
-      <c r="F74" s="186"/>
-      <c r="G74" s="188">
+      <c r="K74" s="309">
         <v>6</v>
       </c>
-      <c r="H74" s="189"/>
-      <c r="I74" s="187"/>
-      <c r="J74" s="189">
+      <c r="L74" s="308"/>
+      <c r="M74" s="306">
         <v>7</v>
       </c>
-      <c r="K74" s="190">
-        <v>5</v>
-      </c>
-      <c r="L74" s="189"/>
-      <c r="M74" s="187">
-        <v>7</v>
-      </c>
-      <c r="N74" s="186"/>
-      <c r="O74" s="187">
+      <c r="N74" s="305"/>
+      <c r="O74" s="306">
         <v>6</v>
       </c>
-      <c r="P74" s="186"/>
-      <c r="Q74" s="188"/>
-      <c r="R74" s="191">
+      <c r="P74" s="305"/>
+      <c r="Q74" s="307"/>
+      <c r="R74" s="310">
         <v>6</v>
       </c>
-      <c r="S74" s="192">
+      <c r="S74" s="294">
         <f>SUM(C75:R75)</f>
         <v>20</v>
       </c>
-      <c r="T74" s="185"/>
-      <c r="U74" s="189">
+      <c r="T74" s="284"/>
+      <c r="U74" s="288">
         <v>6</v>
       </c>
-      <c r="V74" s="187"/>
-      <c r="W74" s="189">
+      <c r="V74" s="289">
+        <v>7</v>
+      </c>
+      <c r="W74" s="288"/>
+      <c r="X74" s="290">
         <v>6</v>
       </c>
-      <c r="X74" s="190"/>
-      <c r="Y74" s="186">
+      <c r="Y74" s="285"/>
+      <c r="Z74" s="287">
         <v>7</v>
       </c>
-      <c r="Z74" s="188"/>
-      <c r="AA74" s="189">
-        <v>6</v>
-      </c>
-      <c r="AB74" s="192">
+      <c r="AA74" s="288"/>
+      <c r="AB74" s="294">
         <f>SUM(T75:AA75)</f>
         <v>6</v>
       </c>
-      <c r="AC74" s="188"/>
-      <c r="AD74" s="189"/>
-      <c r="AE74" s="190"/>
-      <c r="AF74" s="189"/>
-      <c r="AG74" s="192">
+      <c r="AC74" s="287"/>
+      <c r="AD74" s="288"/>
+      <c r="AE74" s="290"/>
+      <c r="AF74" s="288"/>
+      <c r="AG74" s="294">
         <f>SUM(AC75:AF75)</f>
         <v>0</v>
       </c>
-      <c r="AH74" s="196"/>
-      <c r="AI74" s="193"/>
-      <c r="AJ74" s="192">
+      <c r="AH74" s="303"/>
+      <c r="AI74" s="296"/>
+      <c r="AJ74" s="294">
         <f>AH75</f>
         <v>0</v>
       </c>
-      <c r="AK74" s="194">
+      <c r="AK74" s="297">
         <f>MAX($AL$10:$AL$97) - AL74</f>
         <v>23</v>
       </c>
-      <c r="AL74" s="192">
+      <c r="AL74" s="294">
         <f>$S74+$AB74+$AG74+$AJ74</f>
         <v>26</v>
       </c>
@@ -12647,17 +12650,17 @@
       <c r="U75" s="126"/>
       <c r="V75" s="126">
         <f>(IF($V74&lt;&gt;"",($V$6*$P$104)+IF($V$6=4,($P$102)+IF($V74=$V$6+$W$6,$P$103,0),0),0)+IF($W74&lt;&gt;"",($W$6*$P$104)+IF($W$6=4,($P$102)+IF($W74=$V$6+$W$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W75" s="126"/>
       <c r="X75" s="126">
         <f>(IF($X74&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X74=$X$6+$Y$6,$P$103,0),0),0)+IF($Y74&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y74=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y75" s="59"/>
       <c r="Z75" s="126">
         <f>(IF($Z74&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z74=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA74&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA74=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA75" s="62"/>
       <c r="AB75" s="121"/>
@@ -13008,7 +13011,7 @@
         <v>18</v>
       </c>
       <c r="B78" s="84" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C78" s="46">
         <v>5</v>
@@ -13027,41 +13030,41 @@
         <v>6</v>
       </c>
       <c r="K78" s="49">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L78" s="47"/>
       <c r="M78" s="44">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N78" s="45"/>
       <c r="O78" s="44">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P78" s="45"/>
       <c r="Q78" s="48"/>
       <c r="R78" s="50">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S78" s="122">
         <f>SUM(C79:R79)</f>
         <v>20</v>
       </c>
-      <c r="T78" s="46">
-        <v>7</v>
-      </c>
-      <c r="U78" s="47"/>
+      <c r="T78" s="46"/>
+      <c r="U78" s="47">
+        <v>6</v>
+      </c>
       <c r="V78" s="44">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="W78" s="47"/>
-      <c r="X78" s="49">
-        <v>7</v>
-      </c>
-      <c r="Y78" s="45"/>
-      <c r="Z78" s="48">
-        <v>7</v>
-      </c>
-      <c r="AA78" s="47"/>
+      <c r="X78" s="49"/>
+      <c r="Y78" s="45">
+        <v>5</v>
+      </c>
+      <c r="Z78" s="48"/>
+      <c r="AA78" s="47">
+        <v>6</v>
+      </c>
       <c r="AB78" s="122">
         <f>SUM(T79:AA79)</f>
         <v>5</v>
@@ -13138,7 +13141,7 @@
       <c r="S79" s="121"/>
       <c r="T79" s="126">
         <f>(IF($T78&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T78=$T$6+$U$6,$P$103,0),0),0)+IF($U78&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U78=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U79" s="126"/>
       <c r="V79" s="126">
@@ -13148,7 +13151,7 @@
       <c r="W79" s="126"/>
       <c r="X79" s="126">
         <f>(IF($X78&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X78=$X$6+$Y$6,$P$103,0),0),0)+IF($Y78&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y78=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y79" s="59"/>
       <c r="Z79" s="126">
@@ -13499,90 +13502,90 @@
       <c r="AL81" s="123"/>
     </row>
     <row r="82" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="173">
+      <c r="A82" s="269">
         <f>RANK(AL82,$AL$10:$AL$97,)</f>
-        <v>19</v>
-      </c>
-      <c r="B82" s="197" t="s">
-        <v>80</v>
-      </c>
-      <c r="C82" s="185">
+        <v>18</v>
+      </c>
+      <c r="B82" s="270" t="s">
+        <v>75</v>
+      </c>
+      <c r="C82" s="284">
         <v>5</v>
       </c>
-      <c r="D82" s="186"/>
-      <c r="E82" s="187">
+      <c r="D82" s="285"/>
+      <c r="E82" s="289">
         <v>6</v>
       </c>
-      <c r="F82" s="186"/>
-      <c r="G82" s="188">
+      <c r="F82" s="285"/>
+      <c r="G82" s="287">
         <v>6</v>
       </c>
-      <c r="H82" s="189"/>
-      <c r="I82" s="187"/>
-      <c r="J82" s="189">
+      <c r="H82" s="288"/>
+      <c r="I82" s="289"/>
+      <c r="J82" s="288">
         <v>6</v>
       </c>
-      <c r="K82" s="190">
+      <c r="K82" s="290">
+        <v>6</v>
+      </c>
+      <c r="L82" s="288"/>
+      <c r="M82" s="289">
         <v>7</v>
       </c>
-      <c r="L82" s="189"/>
-      <c r="M82" s="187">
+      <c r="N82" s="285"/>
+      <c r="O82" s="289">
         <v>6</v>
       </c>
-      <c r="N82" s="186"/>
-      <c r="O82" s="187">
-        <v>5</v>
-      </c>
-      <c r="P82" s="186"/>
-      <c r="Q82" s="188"/>
-      <c r="R82" s="191">
-        <v>6</v>
-      </c>
-      <c r="S82" s="192">
+      <c r="P82" s="285"/>
+      <c r="Q82" s="287"/>
+      <c r="R82" s="292">
+        <v>7</v>
+      </c>
+      <c r="S82" s="294">
         <f>SUM(C83:R83)</f>
         <v>20</v>
       </c>
-      <c r="T82" s="185"/>
-      <c r="U82" s="189">
-        <v>6</v>
-      </c>
-      <c r="V82" s="187">
-        <v>6</v>
-      </c>
-      <c r="W82" s="189"/>
-      <c r="X82" s="190"/>
-      <c r="Y82" s="186">
+      <c r="T82" s="284">
+        <v>7</v>
+      </c>
+      <c r="U82" s="288"/>
+      <c r="V82" s="289">
+        <v>7</v>
+      </c>
+      <c r="W82" s="288"/>
+      <c r="X82" s="290">
+        <v>7</v>
+      </c>
+      <c r="Y82" s="285"/>
+      <c r="Z82" s="287">
+        <v>7</v>
+      </c>
+      <c r="AA82" s="288"/>
+      <c r="AB82" s="294">
+        <f>SUM(T83:AA83)</f>
         <v>5</v>
       </c>
-      <c r="Z82" s="188"/>
-      <c r="AA82" s="189">
-        <v>6</v>
-      </c>
-      <c r="AB82" s="192">
-        <f>SUM(T83:AA83)</f>
-        <v>4</v>
-      </c>
-      <c r="AC82" s="188"/>
-      <c r="AD82" s="189"/>
-      <c r="AE82" s="190"/>
-      <c r="AF82" s="189"/>
-      <c r="AG82" s="192">
+      <c r="AC82" s="287"/>
+      <c r="AD82" s="288"/>
+      <c r="AE82" s="290"/>
+      <c r="AF82" s="288"/>
+      <c r="AG82" s="294">
         <f>SUM(AC83:AF83)</f>
         <v>0</v>
       </c>
-      <c r="AH82" s="196"/>
-      <c r="AI82" s="193"/>
-      <c r="AJ82" s="192">
+      <c r="AH82" s="303"/>
+      <c r="AI82" s="296"/>
+      <c r="AJ82" s="294">
         <f>AH83</f>
         <v>0</v>
       </c>
-      <c r="AK82" s="194">
+      <c r="AK82" s="297">
         <f>MAX($AL$10:$AL$97) - AL82</f>
+        <v>24</v>
+      </c>
+      <c r="AL82" s="294">
+        <f>$S82+$AB82+$AG82+$AJ82</f>
         <v>25</v>
-      </c>
-      <c r="AL82" s="192">
-        <f>$S82+$AB82+$AG82+$AJ82</f>
-        <v>24</v>
       </c>
     </row>
     <row r="83" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -13634,7 +13637,7 @@
       <c r="S83" s="121"/>
       <c r="T83" s="126">
         <f>(IF($T82&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T82=$T$6+$U$6,$P$103,0),0),0)+IF($U82&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U82=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U83" s="126"/>
       <c r="V83" s="126">
@@ -13644,12 +13647,12 @@
       <c r="W83" s="126"/>
       <c r="X83" s="126">
         <f>(IF($X82&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X82=$X$6+$Y$6,$P$103,0),0),0)+IF($Y82&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y82=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y83" s="59"/>
       <c r="Z83" s="126">
         <f>(IF($Z82&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z82=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA82&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA82=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA83" s="62"/>
       <c r="AB83" s="121"/>
@@ -14491,88 +14494,88 @@
       <c r="AL89" s="123"/>
     </row>
     <row r="90" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="173">
+      <c r="A90" s="269">
         <f>RANK(AL90,$AL$10:$AL$97,)</f>
         <v>20</v>
       </c>
-      <c r="B90" s="197" t="s">
+      <c r="B90" s="270" t="s">
         <v>78</v>
       </c>
-      <c r="C90" s="185">
+      <c r="C90" s="284">
         <v>5</v>
       </c>
-      <c r="D90" s="186"/>
-      <c r="E90" s="187"/>
-      <c r="F90" s="186">
+      <c r="D90" s="285"/>
+      <c r="E90" s="289"/>
+      <c r="F90" s="285">
         <v>7</v>
       </c>
-      <c r="G90" s="188">
+      <c r="G90" s="287">
         <v>6</v>
       </c>
-      <c r="H90" s="189"/>
-      <c r="I90" s="187"/>
-      <c r="J90" s="189">
+      <c r="H90" s="288"/>
+      <c r="I90" s="289"/>
+      <c r="J90" s="288">
         <v>7</v>
       </c>
-      <c r="K90" s="190">
+      <c r="K90" s="290">
         <v>5</v>
       </c>
-      <c r="L90" s="189"/>
-      <c r="M90" s="187">
+      <c r="L90" s="288"/>
+      <c r="M90" s="289">
         <v>6</v>
       </c>
-      <c r="N90" s="186"/>
-      <c r="O90" s="187">
+      <c r="N90" s="285"/>
+      <c r="O90" s="289">
         <v>7</v>
       </c>
-      <c r="P90" s="186"/>
-      <c r="Q90" s="188"/>
-      <c r="R90" s="191">
+      <c r="P90" s="285"/>
+      <c r="Q90" s="287"/>
+      <c r="R90" s="292">
         <v>7</v>
       </c>
-      <c r="S90" s="192">
+      <c r="S90" s="294">
         <f>SUM(C91:R91)</f>
         <v>14</v>
       </c>
-      <c r="T90" s="185"/>
-      <c r="U90" s="189">
+      <c r="T90" s="284"/>
+      <c r="U90" s="288">
         <v>7</v>
       </c>
-      <c r="V90" s="187">
+      <c r="V90" s="289">
         <v>7</v>
       </c>
-      <c r="W90" s="189"/>
-      <c r="X90" s="190">
+      <c r="W90" s="288"/>
+      <c r="X90" s="290">
         <v>6</v>
       </c>
-      <c r="Y90" s="186"/>
-      <c r="Z90" s="188">
+      <c r="Y90" s="285"/>
+      <c r="Z90" s="287">
         <v>6</v>
       </c>
-      <c r="AA90" s="189"/>
-      <c r="AB90" s="192">
+      <c r="AA90" s="288"/>
+      <c r="AB90" s="294">
         <f>SUM(T91:AA91)</f>
         <v>6</v>
       </c>
-      <c r="AC90" s="188"/>
-      <c r="AD90" s="189"/>
-      <c r="AE90" s="190"/>
-      <c r="AF90" s="189"/>
-      <c r="AG90" s="192">
+      <c r="AC90" s="287"/>
+      <c r="AD90" s="288"/>
+      <c r="AE90" s="290"/>
+      <c r="AF90" s="288"/>
+      <c r="AG90" s="294">
         <f>SUM(AC91:AF91)</f>
         <v>0</v>
       </c>
-      <c r="AH90" s="196"/>
-      <c r="AI90" s="193"/>
-      <c r="AJ90" s="192">
+      <c r="AH90" s="303"/>
+      <c r="AI90" s="296"/>
+      <c r="AJ90" s="294">
         <f>AH91</f>
         <v>0</v>
       </c>
-      <c r="AK90" s="194">
+      <c r="AK90" s="297">
         <f>MAX($AL$10:$AL$97) - AL90</f>
         <v>29</v>
       </c>
-      <c r="AL90" s="192">
+      <c r="AL90" s="294">
         <f>$S90+$AB90+$AG90+$AJ90</f>
         <v>20</v>
       </c>
@@ -14994,36 +14997,36 @@
       <c r="B94" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="C94" s="212">
+      <c r="C94" s="187">
         <v>6</v>
       </c>
-      <c r="D94" s="213"/>
-      <c r="E94" s="214"/>
-      <c r="F94" s="213">
+      <c r="D94" s="188"/>
+      <c r="E94" s="189"/>
+      <c r="F94" s="188">
         <v>7</v>
       </c>
-      <c r="G94" s="215">
+      <c r="G94" s="190">
         <v>7</v>
       </c>
-      <c r="H94" s="216"/>
-      <c r="I94" s="214"/>
-      <c r="J94" s="216">
+      <c r="H94" s="191"/>
+      <c r="I94" s="189"/>
+      <c r="J94" s="191">
         <v>6</v>
       </c>
-      <c r="K94" s="217">
+      <c r="K94" s="192">
         <v>6</v>
       </c>
-      <c r="L94" s="216"/>
-      <c r="M94" s="214">
+      <c r="L94" s="191"/>
+      <c r="M94" s="189">
         <v>7</v>
       </c>
-      <c r="N94" s="213"/>
-      <c r="O94" s="214">
+      <c r="N94" s="188"/>
+      <c r="O94" s="189">
         <v>5</v>
       </c>
-      <c r="P94" s="213"/>
-      <c r="Q94" s="215"/>
-      <c r="R94" s="218">
+      <c r="P94" s="188"/>
+      <c r="Q94" s="190"/>
+      <c r="R94" s="193">
         <v>6</v>
       </c>
       <c r="S94" s="122">
@@ -15046,7 +15049,7 @@
         <v>6</v>
       </c>
       <c r="AA94" s="47"/>
-      <c r="AB94" s="204">
+      <c r="AB94" s="179">
         <f>SUM(T95:AA95)</f>
         <v>5</v>
       </c>
@@ -15054,7 +15057,7 @@
       <c r="AD94" s="47"/>
       <c r="AE94" s="49"/>
       <c r="AF94" s="47"/>
-      <c r="AG94" s="204">
+      <c r="AG94" s="179">
         <f>SUM(AC95:AF95)</f>
         <v>0</v>
       </c>
@@ -15068,7 +15071,7 @@
         <f>MAX($AL$10:$AL$97) - AL94</f>
         <v>30</v>
       </c>
-      <c r="AL94" s="204">
+      <c r="AL94" s="179">
         <f>$S94+$AB94+$AG94+$AJ94</f>
         <v>19</v>
       </c>
@@ -15480,105 +15483,105 @@
         <f>SUM(C97:AI97)</f>
         <v>0</v>
       </c>
-      <c r="AL97" s="203"/>
+      <c r="AL97" s="178"/>
     </row>
     <row r="98" spans="1:38" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A98" s="63"/>
       <c r="B98" s="55"/>
-      <c r="C98" s="207">
+      <c r="C98" s="182">
         <f t="shared" ref="C98:AA98" si="0">COUNT(C10,C14,C18,C22,C26,C30,C34, C38, C42,C46,C50,C54,C58,C62,C66,C70,C74,C78,C82,C90,C94,C86)</f>
         <v>22</v>
       </c>
-      <c r="D98" s="205">
+      <c r="D98" s="180">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E98" s="207">
+      <c r="E98" s="182">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="F98" s="205">
+      <c r="F98" s="180">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G98" s="207">
+      <c r="G98" s="182">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="H98" s="205">
+      <c r="H98" s="180">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="I98" s="207">
+      <c r="I98" s="182">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="J98" s="244">
+      <c r="J98" s="212">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="K98" s="206">
+      <c r="K98" s="181">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="L98" s="205">
+      <c r="L98" s="180">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M98" s="207">
+      <c r="M98" s="182">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="N98" s="205">
+      <c r="N98" s="180">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="O98" s="207">
+      <c r="O98" s="182">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="P98" s="205">
+      <c r="P98" s="180">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="Q98" s="207">
+      <c r="Q98" s="182">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="R98" s="208">
+      <c r="R98" s="183">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="S98" s="68"/>
-      <c r="T98" s="207">
+      <c r="T98" s="182">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="U98" s="205">
+      <c r="U98" s="180">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="V98" s="207">
+      <c r="V98" s="182">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="W98" s="244">
+      <c r="W98" s="212">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="X98" s="206">
+      <c r="X98" s="181">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="Y98" s="205">
+      <c r="Y98" s="180">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="Z98" s="207">
+      <c r="Z98" s="182">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="AA98" s="208">
+      <c r="AA98" s="183">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -15615,12 +15618,12 @@
     <row r="100" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B100" s="43"/>
       <c r="N100" s="26"/>
-      <c r="O100" s="280" t="s">
+      <c r="O100" s="215" t="s">
         <v>17</v>
       </c>
-      <c r="P100" s="281"/>
-      <c r="Q100" s="281"/>
-      <c r="R100" s="282"/>
+      <c r="P100" s="216"/>
+      <c r="Q100" s="216"/>
+      <c r="R100" s="217"/>
       <c r="AG100" s="30"/>
       <c r="AH100" s="30"/>
       <c r="AI100" s="30"/>
@@ -15629,21 +15632,21 @@
     </row>
     <row r="101" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="33"/>
-      <c r="B101" s="268" t="s">
+      <c r="B101" s="244" t="s">
         <v>16</v>
       </c>
-      <c r="C101" s="269"/>
-      <c r="D101" s="269"/>
-      <c r="E101" s="269"/>
-      <c r="F101" s="269"/>
-      <c r="G101" s="269"/>
-      <c r="H101" s="269"/>
-      <c r="I101" s="269"/>
-      <c r="J101" s="269"/>
-      <c r="K101" s="269"/>
-      <c r="L101" s="269"/>
-      <c r="M101" s="269"/>
-      <c r="N101" s="270"/>
+      <c r="C101" s="245"/>
+      <c r="D101" s="245"/>
+      <c r="E101" s="245"/>
+      <c r="F101" s="245"/>
+      <c r="G101" s="245"/>
+      <c r="H101" s="245"/>
+      <c r="I101" s="245"/>
+      <c r="J101" s="245"/>
+      <c r="K101" s="245"/>
+      <c r="L101" s="245"/>
+      <c r="M101" s="245"/>
+      <c r="N101" s="246"/>
       <c r="O101" s="21">
         <v>1</v>
       </c>
@@ -15656,45 +15659,45 @@
       <c r="R101" s="22">
         <v>4</v>
       </c>
-      <c r="U101" s="283" t="s">
+      <c r="U101" s="218" t="s">
         <v>26</v>
       </c>
-      <c r="V101" s="284"/>
-      <c r="W101" s="284"/>
-      <c r="X101" s="284"/>
-      <c r="Y101" s="284"/>
-      <c r="Z101" s="284"/>
-      <c r="AA101" s="284"/>
-      <c r="AB101" s="284"/>
-      <c r="AC101" s="284"/>
-      <c r="AD101" s="285"/>
+      <c r="V101" s="219"/>
+      <c r="W101" s="219"/>
+      <c r="X101" s="219"/>
+      <c r="Y101" s="219"/>
+      <c r="Z101" s="219"/>
+      <c r="AA101" s="219"/>
+      <c r="AB101" s="219"/>
+      <c r="AC101" s="219"/>
+      <c r="AD101" s="220"/>
       <c r="AE101" s="28"/>
       <c r="AF101" s="28"/>
-      <c r="AG101" s="286" t="s">
+      <c r="AG101" s="221" t="s">
         <v>24</v>
       </c>
-      <c r="AH101" s="287"/>
-      <c r="AI101" s="287"/>
-      <c r="AJ101" s="287"/>
-      <c r="AK101" s="288"/>
+      <c r="AH101" s="222"/>
+      <c r="AI101" s="222"/>
+      <c r="AJ101" s="222"/>
+      <c r="AK101" s="223"/>
     </row>
     <row r="102" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A102" s="34"/>
-      <c r="B102" s="247" t="s">
+      <c r="B102" s="251" t="s">
         <v>6</v>
       </c>
-      <c r="C102" s="248"/>
-      <c r="D102" s="248"/>
-      <c r="E102" s="248"/>
-      <c r="F102" s="248"/>
-      <c r="G102" s="248"/>
-      <c r="H102" s="248"/>
-      <c r="I102" s="248"/>
-      <c r="J102" s="248"/>
-      <c r="K102" s="248"/>
-      <c r="L102" s="248"/>
-      <c r="M102" s="248"/>
-      <c r="N102" s="249"/>
+      <c r="C102" s="252"/>
+      <c r="D102" s="252"/>
+      <c r="E102" s="252"/>
+      <c r="F102" s="252"/>
+      <c r="G102" s="252"/>
+      <c r="H102" s="252"/>
+      <c r="I102" s="252"/>
+      <c r="J102" s="252"/>
+      <c r="K102" s="252"/>
+      <c r="L102" s="252"/>
+      <c r="M102" s="252"/>
+      <c r="N102" s="253"/>
       <c r="O102" s="20">
         <v>5</v>
       </c>
@@ -15707,49 +15710,49 @@
       <c r="R102" s="23">
         <v>20</v>
       </c>
-      <c r="U102" s="273" t="s">
+      <c r="U102" s="249" t="s">
         <v>20</v>
       </c>
-      <c r="V102" s="274"/>
-      <c r="W102" s="274"/>
-      <c r="X102" s="274"/>
-      <c r="Y102" s="274"/>
-      <c r="Z102" s="274"/>
-      <c r="AA102" s="274"/>
-      <c r="AB102" s="271">
+      <c r="V102" s="250"/>
+      <c r="W102" s="250"/>
+      <c r="X102" s="250"/>
+      <c r="Y102" s="250"/>
+      <c r="Z102" s="250"/>
+      <c r="AA102" s="250"/>
+      <c r="AB102" s="247">
         <v>22</v>
       </c>
-      <c r="AC102" s="271"/>
-      <c r="AD102" s="272"/>
+      <c r="AC102" s="247"/>
+      <c r="AD102" s="248"/>
       <c r="AE102" s="29"/>
       <c r="AF102" s="29"/>
-      <c r="AG102" s="254" t="s">
+      <c r="AG102" s="263" t="s">
         <v>21</v>
       </c>
-      <c r="AH102" s="255"/>
-      <c r="AI102" s="255"/>
-      <c r="AJ102" s="256"/>
-      <c r="AK102" s="209">
+      <c r="AH102" s="264"/>
+      <c r="AI102" s="264"/>
+      <c r="AJ102" s="265"/>
+      <c r="AK102" s="184">
         <v>230</v>
       </c>
     </row>
     <row r="103" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="34"/>
-      <c r="B103" s="247" t="s">
+      <c r="B103" s="251" t="s">
         <v>5</v>
       </c>
-      <c r="C103" s="248"/>
-      <c r="D103" s="248"/>
-      <c r="E103" s="248"/>
-      <c r="F103" s="248"/>
-      <c r="G103" s="248"/>
-      <c r="H103" s="248"/>
-      <c r="I103" s="248"/>
-      <c r="J103" s="248"/>
-      <c r="K103" s="248"/>
-      <c r="L103" s="248"/>
-      <c r="M103" s="248"/>
-      <c r="N103" s="249"/>
+      <c r="C103" s="252"/>
+      <c r="D103" s="252"/>
+      <c r="E103" s="252"/>
+      <c r="F103" s="252"/>
+      <c r="G103" s="252"/>
+      <c r="H103" s="252"/>
+      <c r="I103" s="252"/>
+      <c r="J103" s="252"/>
+      <c r="K103" s="252"/>
+      <c r="L103" s="252"/>
+      <c r="M103" s="252"/>
+      <c r="N103" s="253"/>
       <c r="O103" s="20">
         <v>2</v>
       </c>
@@ -15762,49 +15765,49 @@
       <c r="R103" s="23">
         <v>8</v>
       </c>
-      <c r="U103" s="252" t="s">
+      <c r="U103" s="258" t="s">
         <v>18</v>
       </c>
-      <c r="V103" s="253"/>
-      <c r="W103" s="253"/>
-      <c r="X103" s="253"/>
-      <c r="Y103" s="253"/>
-      <c r="Z103" s="253"/>
-      <c r="AA103" s="253"/>
-      <c r="AB103" s="278">
+      <c r="V103" s="259"/>
+      <c r="W103" s="259"/>
+      <c r="X103" s="259"/>
+      <c r="Y103" s="259"/>
+      <c r="Z103" s="259"/>
+      <c r="AA103" s="259"/>
+      <c r="AB103" s="260">
         <v>20</v>
       </c>
-      <c r="AC103" s="278"/>
-      <c r="AD103" s="279"/>
+      <c r="AC103" s="260"/>
+      <c r="AD103" s="261"/>
       <c r="AE103" s="29"/>
       <c r="AF103" s="29"/>
-      <c r="AG103" s="257" t="s">
+      <c r="AG103" s="266" t="s">
         <v>22</v>
       </c>
-      <c r="AH103" s="248"/>
-      <c r="AI103" s="248"/>
-      <c r="AJ103" s="249"/>
+      <c r="AH103" s="252"/>
+      <c r="AI103" s="252"/>
+      <c r="AJ103" s="253"/>
       <c r="AK103" s="36">
         <v>115</v>
       </c>
     </row>
     <row r="104" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="35"/>
-      <c r="B104" s="261" t="s">
+      <c r="B104" s="237" t="s">
         <v>4</v>
       </c>
-      <c r="C104" s="262"/>
-      <c r="D104" s="262"/>
-      <c r="E104" s="262"/>
-      <c r="F104" s="262"/>
-      <c r="G104" s="262"/>
-      <c r="H104" s="262"/>
-      <c r="I104" s="262"/>
-      <c r="J104" s="262"/>
-      <c r="K104" s="262"/>
-      <c r="L104" s="262"/>
-      <c r="M104" s="262"/>
-      <c r="N104" s="263"/>
+      <c r="C104" s="238"/>
+      <c r="D104" s="238"/>
+      <c r="E104" s="238"/>
+      <c r="F104" s="238"/>
+      <c r="G104" s="238"/>
+      <c r="H104" s="238"/>
+      <c r="I104" s="238"/>
+      <c r="J104" s="238"/>
+      <c r="K104" s="238"/>
+      <c r="L104" s="238"/>
+      <c r="M104" s="238"/>
+      <c r="N104" s="239"/>
       <c r="O104" s="3">
         <v>1</v>
       </c>
@@ -15817,52 +15820,52 @@
       <c r="R104" s="24">
         <v>1</v>
       </c>
-      <c r="U104" s="275" t="s">
+      <c r="U104" s="254" t="s">
         <v>19</v>
       </c>
-      <c r="V104" s="251"/>
-      <c r="W104" s="251"/>
-      <c r="X104" s="251"/>
-      <c r="Y104" s="251"/>
-      <c r="Z104" s="251"/>
-      <c r="AA104" s="251"/>
-      <c r="AB104" s="276">
+      <c r="V104" s="255"/>
+      <c r="W104" s="255"/>
+      <c r="X104" s="255"/>
+      <c r="Y104" s="255"/>
+      <c r="Z104" s="255"/>
+      <c r="AA104" s="255"/>
+      <c r="AB104" s="256">
         <f>AB102*AB103</f>
         <v>440</v>
       </c>
-      <c r="AC104" s="276"/>
-      <c r="AD104" s="277"/>
+      <c r="AC104" s="256"/>
+      <c r="AD104" s="257"/>
       <c r="AE104" s="29"/>
       <c r="AF104" s="29"/>
-      <c r="AG104" s="257" t="s">
+      <c r="AG104" s="266" t="s">
         <v>25</v>
       </c>
-      <c r="AH104" s="248"/>
-      <c r="AI104" s="248"/>
-      <c r="AJ104" s="249"/>
+      <c r="AH104" s="252"/>
+      <c r="AI104" s="252"/>
+      <c r="AJ104" s="253"/>
       <c r="AK104" s="36">
         <v>65</v>
       </c>
     </row>
     <row r="105" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG105" s="252" t="s">
+      <c r="AG105" s="258" t="s">
         <v>23</v>
       </c>
-      <c r="AH105" s="253"/>
-      <c r="AI105" s="253"/>
-      <c r="AJ105" s="253"/>
-      <c r="AK105" s="211">
+      <c r="AH105" s="259"/>
+      <c r="AI105" s="259"/>
+      <c r="AJ105" s="259"/>
+      <c r="AK105" s="186">
         <v>30</v>
       </c>
     </row>
     <row r="106" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG106" s="250" t="s">
+      <c r="AG106" s="262" t="s">
         <v>19</v>
       </c>
-      <c r="AH106" s="251"/>
-      <c r="AI106" s="251"/>
-      <c r="AJ106" s="251"/>
-      <c r="AK106" s="210">
+      <c r="AH106" s="255"/>
+      <c r="AI106" s="255"/>
+      <c r="AJ106" s="255"/>
+      <c r="AK106" s="185">
         <f>SUM(AK102:AK105)</f>
         <v>440</v>
       </c>
@@ -15873,6 +15876,28 @@
     <sortCondition ref="B10:B94"/>
   </sortState>
   <mergeCells count="38">
+    <mergeCell ref="B103:N103"/>
+    <mergeCell ref="AG106:AJ106"/>
+    <mergeCell ref="AG105:AJ105"/>
+    <mergeCell ref="AG102:AJ102"/>
+    <mergeCell ref="AG104:AJ104"/>
+    <mergeCell ref="AG103:AJ103"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="B104:N104"/>
+    <mergeCell ref="C1:O1"/>
+    <mergeCell ref="P1:AJ1"/>
+    <mergeCell ref="C3:O3"/>
+    <mergeCell ref="P3:AJ3"/>
+    <mergeCell ref="C2:P2"/>
+    <mergeCell ref="Q2:AJ2"/>
+    <mergeCell ref="B101:N101"/>
+    <mergeCell ref="AB102:AD102"/>
+    <mergeCell ref="U102:AA102"/>
+    <mergeCell ref="B102:N102"/>
+    <mergeCell ref="U104:AA104"/>
+    <mergeCell ref="AB104:AD104"/>
+    <mergeCell ref="U103:AA103"/>
+    <mergeCell ref="AB103:AD103"/>
     <mergeCell ref="O100:R100"/>
     <mergeCell ref="U101:AD101"/>
     <mergeCell ref="AG101:AK101"/>
@@ -15889,28 +15914,6 @@
     <mergeCell ref="C5:J5"/>
     <mergeCell ref="K5:R5"/>
     <mergeCell ref="S5:S9"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="B104:N104"/>
-    <mergeCell ref="C1:O1"/>
-    <mergeCell ref="P1:AJ1"/>
-    <mergeCell ref="C3:O3"/>
-    <mergeCell ref="P3:AJ3"/>
-    <mergeCell ref="C2:P2"/>
-    <mergeCell ref="Q2:AJ2"/>
-    <mergeCell ref="B101:N101"/>
-    <mergeCell ref="AB102:AD102"/>
-    <mergeCell ref="U102:AA102"/>
-    <mergeCell ref="B102:N102"/>
-    <mergeCell ref="U104:AA104"/>
-    <mergeCell ref="AB104:AD104"/>
-    <mergeCell ref="U103:AA103"/>
-    <mergeCell ref="AB103:AD103"/>
-    <mergeCell ref="B103:N103"/>
-    <mergeCell ref="AG106:AJ106"/>
-    <mergeCell ref="AG105:AJ105"/>
-    <mergeCell ref="AG102:AJ102"/>
-    <mergeCell ref="AG104:AJ104"/>
-    <mergeCell ref="AG103:AJ103"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <conditionalFormatting sqref="AH18:AI18 AH10:AI10 AH14:AI14 T10:AA10 AC10:AF10 C10:R10 C14:R14 T14:AA14 AC14:AF14 T18:AA18 AC18:AF18 AH30:AI30 C30:R30 T30:AA30 AC30:AF30 AH26:AI26 C26:R26 T26:AA26 AC26:AF26 AH62:AI62 C62:R62 T62:AA62 AC62:AF62 AH42:AI42 C42:R42 T42:AA42 AC42:AF42 AH22:AI22 C22:R22 T22:AA22 AC22:AF22 AH38:AI38 C38:R38 T38:AA38 AC38:AF38 AH34:AI34 C34:R34 T34:AA34 AC34:AF34 AH66:AI66 C66:R66 T66:AA66 AC66:AF66 C18:R18">
@@ -16667,7 +16670,7 @@
   <dimension ref="A1:AJ31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17112,7 +17115,9 @@
       <c r="P10" s="81">
         <v>1</v>
       </c>
-      <c r="Q10" s="81"/>
+      <c r="Q10" s="81">
+        <v>2</v>
+      </c>
       <c r="R10" s="81"/>
       <c r="S10" s="81"/>
       <c r="T10" s="81"/>
@@ -17181,14 +17186,16 @@
       <c r="P11" s="81">
         <v>2</v>
       </c>
-      <c r="Q11" s="81"/>
+      <c r="Q11" s="81">
+        <v>5</v>
+      </c>
       <c r="R11" s="81"/>
       <c r="S11" s="81"/>
       <c r="T11" s="81"/>
       <c r="U11" s="81"/>
       <c r="V11" s="73">
         <f>IF(O11&gt;O10,1,0)+IF(P11&gt;P10,1,0)+IF(Q11&gt;Q10,1,0)+IF(R11&gt;R10,1,0)+IF(S11&gt;S10,1,0)+IF(T11&gt;T10,1,0)+IF(U11&gt;U10,1,0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y11" s="93"/>
       <c r="Z11" s="86"/>
@@ -17822,7 +17829,9 @@
       <c r="Q24" s="82">
         <v>4</v>
       </c>
-      <c r="R24" s="82"/>
+      <c r="R24" s="82">
+        <v>2</v>
+      </c>
       <c r="S24" s="82"/>
       <c r="T24" s="82"/>
       <c r="U24" s="81"/>
@@ -17889,13 +17898,15 @@
       <c r="Q25" s="82">
         <v>3</v>
       </c>
-      <c r="R25" s="82"/>
+      <c r="R25" s="82">
+        <v>4</v>
+      </c>
       <c r="S25" s="82"/>
       <c r="T25" s="82"/>
       <c r="U25" s="81"/>
       <c r="V25" s="73">
         <f>IF(O25&gt;O24,1,0)+IF(P25&gt;P24,1,0)+IF(Q25&gt;Q24,1,0)+IF(R25&gt;R24,1,0)+IF(S25&gt;S24,1,0)+IF(T25&gt;T24,1,0)+IF(U25&gt;U24,1,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y25" s="86"/>
       <c r="Z25" s="86"/>

</xml_diff>

<commit_message>
Updated games of 2019-05-02
</commit_message>
<xml_diff>
--- a/laval.xlsx
+++ b/laval.xlsx
@@ -472,7 +472,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1934,7 +1934,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="311">
+  <cellXfs count="309">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2379,7 +2379,106 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="92" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="82" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="83" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="85" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2433,115 +2532,13 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="83" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="85" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="92" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="82" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2562,16 +2559,13 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2631,7 +2625,7 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2643,7 +2637,7 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3892,217 +3886,217 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="C1" s="240"/>
-      <c r="D1" s="240"/>
-      <c r="E1" s="240"/>
-      <c r="F1" s="240"/>
-      <c r="G1" s="240"/>
-      <c r="H1" s="240"/>
-      <c r="I1" s="240"/>
-      <c r="J1" s="240"/>
-      <c r="K1" s="240"/>
-      <c r="L1" s="240"/>
-      <c r="M1" s="240"/>
-      <c r="N1" s="240"/>
-      <c r="O1" s="240"/>
-      <c r="P1" s="241"/>
-      <c r="Q1" s="241"/>
-      <c r="R1" s="241"/>
-      <c r="S1" s="241"/>
-      <c r="T1" s="241"/>
-      <c r="U1" s="241"/>
-      <c r="V1" s="241"/>
-      <c r="W1" s="241"/>
-      <c r="X1" s="241"/>
-      <c r="Y1" s="241"/>
-      <c r="Z1" s="241"/>
-      <c r="AA1" s="241"/>
-      <c r="AB1" s="241"/>
-      <c r="AC1" s="241"/>
-      <c r="AD1" s="241"/>
-      <c r="AE1" s="241"/>
-      <c r="AF1" s="241"/>
-      <c r="AG1" s="241"/>
-      <c r="AH1" s="241"/>
-      <c r="AI1" s="241"/>
-      <c r="AJ1" s="241"/>
+      <c r="C1" s="232"/>
+      <c r="D1" s="232"/>
+      <c r="E1" s="232"/>
+      <c r="F1" s="232"/>
+      <c r="G1" s="232"/>
+      <c r="H1" s="232"/>
+      <c r="I1" s="232"/>
+      <c r="J1" s="232"/>
+      <c r="K1" s="232"/>
+      <c r="L1" s="232"/>
+      <c r="M1" s="232"/>
+      <c r="N1" s="232"/>
+      <c r="O1" s="232"/>
+      <c r="P1" s="233"/>
+      <c r="Q1" s="233"/>
+      <c r="R1" s="233"/>
+      <c r="S1" s="233"/>
+      <c r="T1" s="233"/>
+      <c r="U1" s="233"/>
+      <c r="V1" s="233"/>
+      <c r="W1" s="233"/>
+      <c r="X1" s="233"/>
+      <c r="Y1" s="233"/>
+      <c r="Z1" s="233"/>
+      <c r="AA1" s="233"/>
+      <c r="AB1" s="233"/>
+      <c r="AC1" s="233"/>
+      <c r="AD1" s="233"/>
+      <c r="AE1" s="233"/>
+      <c r="AF1" s="233"/>
+      <c r="AG1" s="233"/>
+      <c r="AH1" s="233"/>
+      <c r="AI1" s="233"/>
+      <c r="AJ1" s="233"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="41"/>
-      <c r="C2" s="242" t="s">
+      <c r="C2" s="234" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="242"/>
-      <c r="E2" s="242"/>
-      <c r="F2" s="242"/>
-      <c r="G2" s="242"/>
-      <c r="H2" s="242"/>
-      <c r="I2" s="242"/>
-      <c r="J2" s="242"/>
-      <c r="K2" s="242"/>
-      <c r="L2" s="242"/>
-      <c r="M2" s="242"/>
-      <c r="N2" s="242"/>
-      <c r="O2" s="242"/>
-      <c r="P2" s="242"/>
-      <c r="Q2" s="243" t="s">
+      <c r="D2" s="234"/>
+      <c r="E2" s="234"/>
+      <c r="F2" s="234"/>
+      <c r="G2" s="234"/>
+      <c r="H2" s="234"/>
+      <c r="I2" s="234"/>
+      <c r="J2" s="234"/>
+      <c r="K2" s="234"/>
+      <c r="L2" s="234"/>
+      <c r="M2" s="234"/>
+      <c r="N2" s="234"/>
+      <c r="O2" s="234"/>
+      <c r="P2" s="234"/>
+      <c r="Q2" s="235" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="241"/>
-      <c r="S2" s="241"/>
-      <c r="T2" s="241"/>
-      <c r="U2" s="241"/>
-      <c r="V2" s="241"/>
-      <c r="W2" s="241"/>
-      <c r="X2" s="241"/>
-      <c r="Y2" s="241"/>
-      <c r="Z2" s="241"/>
-      <c r="AA2" s="241"/>
-      <c r="AB2" s="241"/>
-      <c r="AC2" s="241"/>
-      <c r="AD2" s="241"/>
-      <c r="AE2" s="241"/>
-      <c r="AF2" s="241"/>
-      <c r="AG2" s="241"/>
-      <c r="AH2" s="241"/>
-      <c r="AI2" s="241"/>
-      <c r="AJ2" s="241"/>
+      <c r="R2" s="233"/>
+      <c r="S2" s="233"/>
+      <c r="T2" s="233"/>
+      <c r="U2" s="233"/>
+      <c r="V2" s="233"/>
+      <c r="W2" s="233"/>
+      <c r="X2" s="233"/>
+      <c r="Y2" s="233"/>
+      <c r="Z2" s="233"/>
+      <c r="AA2" s="233"/>
+      <c r="AB2" s="233"/>
+      <c r="AC2" s="233"/>
+      <c r="AD2" s="233"/>
+      <c r="AE2" s="233"/>
+      <c r="AF2" s="233"/>
+      <c r="AG2" s="233"/>
+      <c r="AH2" s="233"/>
+      <c r="AI2" s="233"/>
+      <c r="AJ2" s="233"/>
     </row>
     <row r="3" spans="1:38" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="240"/>
-      <c r="D3" s="240"/>
-      <c r="E3" s="240"/>
-      <c r="F3" s="240"/>
-      <c r="G3" s="240"/>
-      <c r="H3" s="240"/>
-      <c r="I3" s="240"/>
-      <c r="J3" s="240"/>
-      <c r="K3" s="240"/>
-      <c r="L3" s="240"/>
-      <c r="M3" s="240"/>
-      <c r="N3" s="240"/>
-      <c r="O3" s="240"/>
-      <c r="P3" s="241"/>
-      <c r="Q3" s="241"/>
-      <c r="R3" s="241"/>
-      <c r="S3" s="241"/>
-      <c r="T3" s="241"/>
-      <c r="U3" s="241"/>
-      <c r="V3" s="241"/>
-      <c r="W3" s="241"/>
-      <c r="X3" s="241"/>
-      <c r="Y3" s="241"/>
-      <c r="Z3" s="241"/>
-      <c r="AA3" s="241"/>
-      <c r="AB3" s="241"/>
-      <c r="AC3" s="241"/>
-      <c r="AD3" s="241"/>
-      <c r="AE3" s="241"/>
-      <c r="AF3" s="241"/>
-      <c r="AG3" s="241"/>
-      <c r="AH3" s="241"/>
-      <c r="AI3" s="241"/>
-      <c r="AJ3" s="241"/>
+      <c r="C3" s="232"/>
+      <c r="D3" s="232"/>
+      <c r="E3" s="232"/>
+      <c r="F3" s="232"/>
+      <c r="G3" s="232"/>
+      <c r="H3" s="232"/>
+      <c r="I3" s="232"/>
+      <c r="J3" s="232"/>
+      <c r="K3" s="232"/>
+      <c r="L3" s="232"/>
+      <c r="M3" s="232"/>
+      <c r="N3" s="232"/>
+      <c r="O3" s="232"/>
+      <c r="P3" s="233"/>
+      <c r="Q3" s="233"/>
+      <c r="R3" s="233"/>
+      <c r="S3" s="233"/>
+      <c r="T3" s="233"/>
+      <c r="U3" s="233"/>
+      <c r="V3" s="233"/>
+      <c r="W3" s="233"/>
+      <c r="X3" s="233"/>
+      <c r="Y3" s="233"/>
+      <c r="Z3" s="233"/>
+      <c r="AA3" s="233"/>
+      <c r="AB3" s="233"/>
+      <c r="AC3" s="233"/>
+      <c r="AD3" s="233"/>
+      <c r="AE3" s="233"/>
+      <c r="AF3" s="233"/>
+      <c r="AG3" s="233"/>
+      <c r="AH3" s="233"/>
+      <c r="AI3" s="233"/>
+      <c r="AJ3" s="233"/>
     </row>
     <row r="4" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="224" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="225"/>
-      <c r="E4" s="225"/>
-      <c r="F4" s="225"/>
-      <c r="G4" s="225"/>
-      <c r="H4" s="225"/>
-      <c r="I4" s="225"/>
-      <c r="J4" s="225"/>
-      <c r="K4" s="225"/>
-      <c r="L4" s="225"/>
-      <c r="M4" s="225"/>
-      <c r="N4" s="225"/>
-      <c r="O4" s="225"/>
-      <c r="P4" s="225"/>
-      <c r="Q4" s="225"/>
-      <c r="R4" s="225"/>
-      <c r="S4" s="226"/>
-      <c r="T4" s="224" t="s">
+      <c r="C4" s="257" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="258"/>
+      <c r="E4" s="258"/>
+      <c r="F4" s="258"/>
+      <c r="G4" s="258"/>
+      <c r="H4" s="258"/>
+      <c r="I4" s="258"/>
+      <c r="J4" s="258"/>
+      <c r="K4" s="258"/>
+      <c r="L4" s="258"/>
+      <c r="M4" s="258"/>
+      <c r="N4" s="258"/>
+      <c r="O4" s="258"/>
+      <c r="P4" s="258"/>
+      <c r="Q4" s="258"/>
+      <c r="R4" s="258"/>
+      <c r="S4" s="259"/>
+      <c r="T4" s="257" t="s">
         <v>1</v>
       </c>
-      <c r="U4" s="225"/>
-      <c r="V4" s="225"/>
-      <c r="W4" s="225"/>
-      <c r="X4" s="225"/>
-      <c r="Y4" s="225"/>
-      <c r="Z4" s="225"/>
-      <c r="AA4" s="225"/>
-      <c r="AB4" s="226"/>
-      <c r="AC4" s="224" t="s">
+      <c r="U4" s="258"/>
+      <c r="V4" s="258"/>
+      <c r="W4" s="258"/>
+      <c r="X4" s="258"/>
+      <c r="Y4" s="258"/>
+      <c r="Z4" s="258"/>
+      <c r="AA4" s="258"/>
+      <c r="AB4" s="259"/>
+      <c r="AC4" s="257" t="s">
         <v>2</v>
       </c>
-      <c r="AD4" s="225"/>
-      <c r="AE4" s="225"/>
-      <c r="AF4" s="225"/>
-      <c r="AG4" s="235"/>
-      <c r="AH4" s="224" t="s">
+      <c r="AD4" s="258"/>
+      <c r="AE4" s="258"/>
+      <c r="AF4" s="258"/>
+      <c r="AG4" s="266"/>
+      <c r="AH4" s="257" t="s">
         <v>10</v>
       </c>
-      <c r="AI4" s="225"/>
-      <c r="AJ4" s="226"/>
+      <c r="AI4" s="258"/>
+      <c r="AJ4" s="259"/>
     </row>
     <row r="5" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="236" t="s">
+      <c r="C5" s="226" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="232"/>
-      <c r="E5" s="232"/>
-      <c r="F5" s="232"/>
-      <c r="G5" s="232"/>
-      <c r="H5" s="232"/>
-      <c r="I5" s="232"/>
-      <c r="J5" s="233"/>
-      <c r="K5" s="231" t="s">
+      <c r="D5" s="227"/>
+      <c r="E5" s="227"/>
+      <c r="F5" s="227"/>
+      <c r="G5" s="227"/>
+      <c r="H5" s="227"/>
+      <c r="I5" s="227"/>
+      <c r="J5" s="228"/>
+      <c r="K5" s="264" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="232"/>
-      <c r="M5" s="232"/>
-      <c r="N5" s="232"/>
-      <c r="O5" s="232"/>
-      <c r="P5" s="232"/>
-      <c r="Q5" s="232"/>
-      <c r="R5" s="233"/>
-      <c r="S5" s="227" t="s">
+      <c r="L5" s="227"/>
+      <c r="M5" s="227"/>
+      <c r="N5" s="227"/>
+      <c r="O5" s="227"/>
+      <c r="P5" s="227"/>
+      <c r="Q5" s="227"/>
+      <c r="R5" s="228"/>
+      <c r="S5" s="260" t="s">
         <v>12</v>
       </c>
-      <c r="T5" s="236" t="s">
+      <c r="T5" s="226" t="s">
         <v>9</v>
       </c>
-      <c r="U5" s="232"/>
-      <c r="V5" s="232"/>
-      <c r="W5" s="233"/>
-      <c r="X5" s="231" t="s">
+      <c r="U5" s="227"/>
+      <c r="V5" s="227"/>
+      <c r="W5" s="228"/>
+      <c r="X5" s="264" t="s">
         <v>8</v>
       </c>
-      <c r="Y5" s="232"/>
-      <c r="Z5" s="232"/>
-      <c r="AA5" s="233"/>
-      <c r="AB5" s="227" t="s">
+      <c r="Y5" s="227"/>
+      <c r="Z5" s="227"/>
+      <c r="AA5" s="228"/>
+      <c r="AB5" s="260" t="s">
         <v>13</v>
       </c>
-      <c r="AC5" s="234" t="s">
+      <c r="AC5" s="265" t="s">
         <v>9</v>
       </c>
-      <c r="AD5" s="233"/>
-      <c r="AE5" s="231" t="s">
+      <c r="AD5" s="228"/>
+      <c r="AE5" s="264" t="s">
         <v>8</v>
       </c>
-      <c r="AF5" s="233"/>
-      <c r="AG5" s="227" t="s">
+      <c r="AF5" s="228"/>
+      <c r="AG5" s="260" t="s">
         <v>14</v>
       </c>
       <c r="AH5" s="56"/>
       <c r="AI5" s="25"/>
-      <c r="AJ5" s="227" t="s">
+      <c r="AJ5" s="260" t="s">
         <v>15</v>
       </c>
       <c r="AK5" s="4"/>
@@ -4174,10 +4168,10 @@
         <f>Résultats!$J$28</f>
         <v>3</v>
       </c>
-      <c r="S6" s="228"/>
+      <c r="S6" s="261"/>
       <c r="T6" s="156">
         <f>Résultats!$V$6</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U6" s="103">
         <f>Résultats!$V$7</f>
@@ -4197,7 +4191,7 @@
       </c>
       <c r="Y6" s="104">
         <f>Résultats!$V$21</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z6" s="106">
         <f>Résultats!$V$24</f>
@@ -4207,7 +4201,7 @@
         <f>Résultats!$V$25</f>
         <v>2</v>
       </c>
-      <c r="AB6" s="228"/>
+      <c r="AB6" s="261"/>
       <c r="AC6" s="106">
         <f>Résultats!$AH$8</f>
         <v>0</v>
@@ -4224,7 +4218,7 @@
         <f>Résultats!$AH$23</f>
         <v>0</v>
       </c>
-      <c r="AG6" s="228"/>
+      <c r="AG6" s="261"/>
       <c r="AH6" s="173">
         <f>Résultats!$AH$15</f>
         <v>0</v>
@@ -4233,7 +4227,7 @@
         <f>Résultats!$AH$16</f>
         <v>0</v>
       </c>
-      <c r="AJ6" s="228"/>
+      <c r="AJ6" s="261"/>
       <c r="AK6" s="37"/>
     </row>
     <row r="7" spans="1:38" s="39" customFormat="1" ht="58.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -4259,7 +4253,7 @@
       <c r="P7" s="203"/>
       <c r="Q7" s="207"/>
       <c r="R7" s="112"/>
-      <c r="S7" s="228"/>
+      <c r="S7" s="261"/>
       <c r="T7" s="157"/>
       <c r="U7" s="112"/>
       <c r="V7" s="160"/>
@@ -4268,15 +4262,15 @@
       <c r="Y7" s="113"/>
       <c r="Z7" s="114"/>
       <c r="AA7" s="112"/>
-      <c r="AB7" s="228"/>
+      <c r="AB7" s="261"/>
       <c r="AC7" s="114"/>
       <c r="AD7" s="112"/>
       <c r="AE7" s="115"/>
       <c r="AF7" s="112"/>
-      <c r="AG7" s="228"/>
+      <c r="AG7" s="261"/>
       <c r="AH7" s="173"/>
       <c r="AI7" s="107"/>
-      <c r="AJ7" s="228"/>
+      <c r="AJ7" s="261"/>
       <c r="AK7" s="37"/>
     </row>
     <row r="8" spans="1:38" s="39" customFormat="1" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4346,7 +4340,7 @@
         <f>Résultats!$B$28</f>
         <v>VEGAS</v>
       </c>
-      <c r="S8" s="228"/>
+      <c r="S8" s="261"/>
       <c r="T8" s="158" t="str">
         <f>Résultats!$N$6</f>
         <v>BOSTON</v>
@@ -4379,7 +4373,7 @@
         <f>Résultats!$N$25</f>
         <v>DALLAS</v>
       </c>
-      <c r="AB8" s="228"/>
+      <c r="AB8" s="261"/>
       <c r="AC8" s="164" t="str">
         <f>Résultats!$Z$8</f>
         <v xml:space="preserve"> </v>
@@ -4396,7 +4390,7 @@
         <f>Résultats!$Z$23</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AG8" s="228"/>
+      <c r="AG8" s="261"/>
       <c r="AH8" s="174" t="str">
         <f>Résultats!$Z$15</f>
         <v xml:space="preserve"> </v>
@@ -4405,7 +4399,7 @@
         <f>Résultats!$Z$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ8" s="228"/>
+      <c r="AJ8" s="261"/>
       <c r="AK8" s="37"/>
     </row>
     <row r="9" spans="1:38" s="39" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4479,7 +4473,7 @@
         <f>Résultats!$A$28</f>
         <v>P3</v>
       </c>
-      <c r="S9" s="230"/>
+      <c r="S9" s="263"/>
       <c r="T9" s="166" t="str">
         <f>Résultats!$M$6</f>
         <v>A2</v>
@@ -4512,7 +4506,7 @@
         <f>Résultats!$M$25</f>
         <v>WC1</v>
       </c>
-      <c r="AB9" s="229"/>
+      <c r="AB9" s="262"/>
       <c r="AC9" s="170" t="str">
         <f>Résultats!$Y$8</f>
         <v xml:space="preserve"> </v>
@@ -4529,7 +4523,7 @@
         <f>Résultats!$Y$23</f>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="AG9" s="229"/>
+      <c r="AG9" s="262"/>
       <c r="AH9" s="176" t="str">
         <f>Résultats!$Y$15</f>
         <v xml:space="preserve"> </v>
@@ -4538,7 +4532,7 @@
         <f>Résultats!$Y$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ9" s="230"/>
+      <c r="AJ9" s="263"/>
       <c r="AK9" s="109" t="s">
         <v>51</v>
       </c>
@@ -4547,90 +4541,90 @@
       </c>
     </row>
     <row r="10" spans="1:38" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="269">
+      <c r="A10" s="268">
         <f>RANK(AL10,$AL$10:$AL$97,)</f>
         <v>1</v>
       </c>
-      <c r="B10" s="270" t="s">
-        <v>77</v>
-      </c>
-      <c r="C10" s="271">
+      <c r="B10" s="269" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="270">
+        <v>4</v>
+      </c>
+      <c r="D10" s="271"/>
+      <c r="E10" s="272">
         <v>5</v>
       </c>
-      <c r="D10" s="272"/>
-      <c r="E10" s="273">
+      <c r="F10" s="271"/>
+      <c r="G10" s="273">
         <v>6</v>
       </c>
-      <c r="F10" s="272"/>
-      <c r="G10" s="274"/>
-      <c r="H10" s="275">
+      <c r="H10" s="274"/>
+      <c r="I10" s="272">
         <v>7</v>
       </c>
-      <c r="I10" s="273"/>
-      <c r="J10" s="276">
+      <c r="J10" s="274"/>
+      <c r="K10" s="275">
+        <v>5</v>
+      </c>
+      <c r="L10" s="274"/>
+      <c r="M10" s="272"/>
+      <c r="N10" s="271">
+        <v>7</v>
+      </c>
+      <c r="O10" s="272">
         <v>6</v>
       </c>
-      <c r="K10" s="277">
-        <v>5</v>
-      </c>
-      <c r="L10" s="276"/>
-      <c r="M10" s="273"/>
-      <c r="N10" s="278">
+      <c r="P10" s="271"/>
+      <c r="Q10" s="276">
+        <v>7</v>
+      </c>
+      <c r="R10" s="277"/>
+      <c r="S10" s="278">
+        <f>SUM(C11:R11)</f>
+        <v>44</v>
+      </c>
+      <c r="T10" s="270"/>
+      <c r="U10" s="274">
         <v>6</v>
       </c>
-      <c r="O10" s="273">
+      <c r="V10" s="272">
         <v>6</v>
       </c>
-      <c r="P10" s="272"/>
-      <c r="Q10" s="274">
+      <c r="W10" s="274"/>
+      <c r="X10" s="275"/>
+      <c r="Y10" s="271">
         <v>6</v>
       </c>
-      <c r="R10" s="279"/>
-      <c r="S10" s="280">
-        <f>SUM(C11:R11)</f>
-        <v>43</v>
-      </c>
-      <c r="T10" s="271"/>
-      <c r="U10" s="276">
+      <c r="Z10" s="273">
         <v>6</v>
       </c>
-      <c r="V10" s="273">
-        <v>6</v>
-      </c>
-      <c r="W10" s="276"/>
-      <c r="X10" s="277">
-        <v>5</v>
-      </c>
-      <c r="Y10" s="272"/>
-      <c r="Z10" s="274"/>
-      <c r="AA10" s="279">
-        <v>7</v>
-      </c>
-      <c r="AB10" s="280">
+      <c r="AA10" s="277"/>
+      <c r="AB10" s="278">
         <f>SUM(T11:AA11)</f>
         <v>6</v>
       </c>
-      <c r="AC10" s="274"/>
-      <c r="AD10" s="276"/>
-      <c r="AE10" s="277"/>
-      <c r="AF10" s="276"/>
-      <c r="AG10" s="280">
+      <c r="AC10" s="273"/>
+      <c r="AD10" s="274"/>
+      <c r="AE10" s="275"/>
+      <c r="AF10" s="274"/>
+      <c r="AG10" s="278">
         <f>SUM(AC11:AF11)</f>
         <v>0</v>
       </c>
-      <c r="AH10" s="281"/>
-      <c r="AI10" s="282"/>
-      <c r="AJ10" s="280">
+      <c r="AH10" s="279"/>
+      <c r="AI10" s="280"/>
+      <c r="AJ10" s="278">
         <f>AH11</f>
         <v>0</v>
       </c>
-      <c r="AK10" s="283">
+      <c r="AK10" s="281">
         <f>MAX($AL$10:$AL$97) - AL10</f>
         <v>0</v>
       </c>
-      <c r="AL10" s="280">
+      <c r="AL10" s="278">
         <f>$S10+$AB10+$AG10+$AJ10</f>
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -4651,12 +4645,12 @@
       <c r="F11" s="127"/>
       <c r="G11" s="125">
         <f>(IF($G10&lt;&gt;"",($G$6*$O$104)+IF($G$6=4,($O$102)+IF($G10=$G$6+$H$6,$O$103,0),0),0)+IF($H10&lt;&gt;"",($H$6*$O$104)+IF($H$6=4,($O$102)+IF($H10=$G$6+$H$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="H11" s="127"/>
       <c r="I11" s="128">
         <f>(IF($I10&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I10=$I$6+$J$6,$O$103,0),0),0)+IF($J10&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J10=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J11" s="129"/>
       <c r="K11" s="130">
@@ -4666,7 +4660,7 @@
       <c r="L11" s="127"/>
       <c r="M11" s="125">
         <f>(IF($M10&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M10=$M$6+$N$6,$O$103,0),0),0)+IF($N10&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N10=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="N11" s="127"/>
       <c r="O11" s="128">
@@ -4676,7 +4670,7 @@
       <c r="P11" s="127"/>
       <c r="Q11" s="125">
         <f>(IF($Q10&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q10=$Q$6+$R$6,$O$103,0),0),0)+IF($R10&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R10=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="R11" s="131"/>
       <c r="S11" s="121"/>
@@ -4751,13 +4745,13 @@
         <f>IF(ISBLANK(H10),
 0,
 IF(H$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12" s="118">
         <f>IF(ISBLANK(I10),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" s="118">
         <f>IF(ISBLANK(J10),
@@ -4916,7 +4910,7 @@
         <f>IF(H12 = 0,
 0,
 IF(H10 = (G$6+H$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" s="118">
         <f>IF(I12 = 0,
@@ -4952,7 +4946,7 @@
         <f>IF(N12 = 0,
 0,
 IF(N10 = (M$6+N$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O13" s="118">
         <f>IF(O12 = 0,
@@ -4970,7 +4964,7 @@
         <f>IF(Q12 = 0,
 0,
 IF(Q10 = (Q$6+R$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R13" s="118">
         <f>IF(R12 = 0,
@@ -5038,53 +5032,53 @@
       <c r="AJ13" s="138"/>
       <c r="AK13" s="139">
         <f>SUM(C13:AI13)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AL13" s="123"/>
     </row>
     <row r="14" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="117">
         <f>RANK(AL14,$AL$10:$AL$97,)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14" s="84" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C14" s="46">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D14" s="45"/>
       <c r="E14" s="44">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F14" s="45"/>
-      <c r="G14" s="48">
+      <c r="G14" s="48"/>
+      <c r="H14" s="267">
+        <v>7</v>
+      </c>
+      <c r="I14" s="44"/>
+      <c r="J14" s="47">
         <v>6</v>
       </c>
-      <c r="H14" s="47"/>
-      <c r="I14" s="44">
-        <v>7</v>
-      </c>
-      <c r="J14" s="47"/>
       <c r="K14" s="49">
         <v>5</v>
       </c>
       <c r="L14" s="47"/>
       <c r="M14" s="44"/>
-      <c r="N14" s="45">
-        <v>7</v>
+      <c r="N14" s="211">
+        <v>6</v>
       </c>
       <c r="O14" s="44">
         <v>6</v>
       </c>
       <c r="P14" s="45"/>
-      <c r="Q14" s="213">
-        <v>7</v>
+      <c r="Q14" s="48">
+        <v>6</v>
       </c>
       <c r="R14" s="50"/>
       <c r="S14" s="122">
         <f>SUM(C15:R15)</f>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T14" s="46"/>
       <c r="U14" s="47">
@@ -5094,17 +5088,17 @@
         <v>6</v>
       </c>
       <c r="W14" s="47"/>
-      <c r="X14" s="49"/>
-      <c r="Y14" s="45">
-        <v>6</v>
-      </c>
-      <c r="Z14" s="48">
-        <v>6</v>
-      </c>
-      <c r="AA14" s="50"/>
+      <c r="X14" s="49">
+        <v>5</v>
+      </c>
+      <c r="Y14" s="45"/>
+      <c r="Z14" s="48"/>
+      <c r="AA14" s="50">
+        <v>7</v>
+      </c>
       <c r="AB14" s="122">
         <f>SUM(T15:AA15)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC14" s="48"/>
       <c r="AD14" s="47"/>
@@ -5122,7 +5116,7 @@
       </c>
       <c r="AK14" s="111">
         <f>MAX($AL$10:$AL$97) - AL14</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL14" s="122">
         <f>$S14+$AB14+$AG14+$AJ14</f>
@@ -5147,12 +5141,12 @@
       <c r="F15" s="140"/>
       <c r="G15" s="125">
         <f>(IF($G14&lt;&gt;"",($G$6*$O$104)+IF($G$6=4,($O$102)+IF($G14=$G$6+$H$6,$O$103,0),0),0)+IF($H14&lt;&gt;"",($H$6*$O$104)+IF($H$6=4,($O$102)+IF($H14=$G$6+$H$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="H15" s="140"/>
       <c r="I15" s="120">
         <f>(IF($I14&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I14=$I$6+$J$6,$O$103,0),0),0)+IF($J14&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J14=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J15" s="141"/>
       <c r="K15" s="142">
@@ -5162,7 +5156,7 @@
       <c r="L15" s="140"/>
       <c r="M15" s="125">
         <f>(IF($M14&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M14=$M$6+$N$6,$O$103,0),0),0)+IF($N14&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N14=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="N15" s="140"/>
       <c r="O15" s="120">
@@ -5172,7 +5166,7 @@
       <c r="P15" s="140"/>
       <c r="Q15" s="120">
         <f>(IF($Q14&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q14=$Q$6+$R$6,$O$103,0),0),0)+IF($R14&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R14=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="R15" s="143"/>
       <c r="S15" s="144"/>
@@ -5188,7 +5182,7 @@
       <c r="W15" s="126"/>
       <c r="X15" s="126">
         <f>(IF($X14&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X14=$X$6+$Y$6,$P$103,0),0),0)+IF($Y14&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y14=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y15" s="59"/>
       <c r="Z15" s="126">
@@ -5207,7 +5201,7 @@
       <c r="AJ15" s="121"/>
       <c r="AK15" s="92">
         <f>MAX($AL$10:$AL$97) - AL15</f>
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AL15" s="121"/>
     </row>
@@ -5250,13 +5244,13 @@
         <f>IF(ISBLANK(H14),
 0,
 IF(H$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" s="118">
         <f>IF(ISBLANK(I14),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" s="118">
         <f>IF(ISBLANK(J14),
@@ -5415,7 +5409,7 @@
         <f>IF(H16 = 0,
 0,
 IF(H14 = (G$6+H$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="118">
         <f>IF(I16 = 0,
@@ -5451,7 +5445,7 @@
         <f>IF(N16 = 0,
 0,
 IF(N14 = (M$6+N$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O17" s="118">
         <f>IF(O16 = 0,
@@ -5469,7 +5463,7 @@
         <f>IF(Q16 = 0,
 0,
 IF(Q14 = (Q$6+R$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R17" s="118">
         <f>IF(R16 = 0,
@@ -5537,95 +5531,95 @@
       <c r="AJ17" s="138"/>
       <c r="AK17" s="139">
         <f>SUM(C17:AI17)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL17" s="123"/>
     </row>
     <row r="18" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="269">
+      <c r="A18" s="268">
         <f>RANK(AL18,$AL$10:$AL$97,)</f>
         <v>3</v>
       </c>
-      <c r="B18" s="270" t="s">
+      <c r="B18" s="269" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="284">
+      <c r="C18" s="282">
         <v>5</v>
       </c>
-      <c r="D18" s="285"/>
-      <c r="E18" s="286">
+      <c r="D18" s="283"/>
+      <c r="E18" s="284">
         <v>7</v>
       </c>
-      <c r="F18" s="285"/>
-      <c r="G18" s="287">
+      <c r="F18" s="283"/>
+      <c r="G18" s="285">
         <v>4</v>
       </c>
-      <c r="H18" s="288"/>
-      <c r="I18" s="289"/>
-      <c r="J18" s="288">
+      <c r="H18" s="286"/>
+      <c r="I18" s="287"/>
+      <c r="J18" s="286">
         <v>6</v>
       </c>
-      <c r="K18" s="290">
+      <c r="K18" s="288">
         <v>5</v>
       </c>
-      <c r="L18" s="288"/>
-      <c r="M18" s="289"/>
-      <c r="N18" s="291">
+      <c r="L18" s="286"/>
+      <c r="M18" s="287"/>
+      <c r="N18" s="289">
         <v>6</v>
       </c>
-      <c r="O18" s="289">
+      <c r="O18" s="287">
         <v>7</v>
       </c>
-      <c r="P18" s="285"/>
-      <c r="Q18" s="287">
+      <c r="P18" s="283"/>
+      <c r="Q18" s="285">
         <v>6</v>
       </c>
-      <c r="R18" s="292"/>
-      <c r="S18" s="293">
+      <c r="R18" s="290"/>
+      <c r="S18" s="291">
         <f>SUM(C19:R19)</f>
         <v>37</v>
       </c>
-      <c r="T18" s="284">
+      <c r="T18" s="282">
         <v>6</v>
       </c>
-      <c r="U18" s="288"/>
-      <c r="V18" s="289"/>
-      <c r="W18" s="288">
+      <c r="U18" s="286"/>
+      <c r="V18" s="287"/>
+      <c r="W18" s="286">
         <v>6</v>
       </c>
-      <c r="X18" s="290">
+      <c r="X18" s="288">
         <v>5</v>
       </c>
-      <c r="Y18" s="285"/>
-      <c r="Z18" s="287"/>
-      <c r="AA18" s="292">
+      <c r="Y18" s="283"/>
+      <c r="Z18" s="285"/>
+      <c r="AA18" s="290">
         <v>7</v>
       </c>
-      <c r="AB18" s="294">
+      <c r="AB18" s="292">
         <f>SUM(T19:AA19)</f>
-        <v>8</v>
-      </c>
-      <c r="AC18" s="287"/>
-      <c r="AD18" s="288"/>
-      <c r="AE18" s="290"/>
-      <c r="AF18" s="288"/>
-      <c r="AG18" s="294">
+        <v>9</v>
+      </c>
+      <c r="AC18" s="285"/>
+      <c r="AD18" s="286"/>
+      <c r="AE18" s="288"/>
+      <c r="AF18" s="286"/>
+      <c r="AG18" s="292">
         <f>SUM(AC19:AF19)</f>
         <v>0</v>
       </c>
-      <c r="AH18" s="295"/>
-      <c r="AI18" s="296"/>
-      <c r="AJ18" s="294">
+      <c r="AH18" s="293"/>
+      <c r="AI18" s="294"/>
+      <c r="AJ18" s="292">
         <f>AH19</f>
         <v>0</v>
       </c>
-      <c r="AK18" s="297">
+      <c r="AK18" s="295">
         <f>MAX($AL$10:$AL$97) - AL18</f>
         <v>4</v>
       </c>
-      <c r="AL18" s="294">
+      <c r="AL18" s="292">
         <f>$S18+$AB18+$AG18+$AJ18</f>
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5677,7 +5671,7 @@
       <c r="S19" s="144"/>
       <c r="T19" s="126">
         <f>(IF($T18&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T18=$T$6+$U$6,$P$103,0),0),0)+IF($U18&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U18=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U19" s="126"/>
       <c r="V19" s="126">
@@ -5706,7 +5700,7 @@
       <c r="AJ19" s="144"/>
       <c r="AK19" s="150">
         <f>MAX($AL$10:$AL$97) - AL19</f>
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AL19" s="121"/>
     </row>
@@ -6102,7 +6096,7 @@
       <c r="AA22" s="50"/>
       <c r="AB22" s="122">
         <f>SUM(T23:AA23)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC22" s="48"/>
       <c r="AD22" s="47"/>
@@ -6112,7 +6106,7 @@
         <f>SUM(AC23:AF23)</f>
         <v>0</v>
       </c>
-      <c r="AH22" s="267"/>
+      <c r="AH22" s="214"/>
       <c r="AI22" s="57"/>
       <c r="AJ22" s="122">
         <f>AH23</f>
@@ -6124,7 +6118,7 @@
       </c>
       <c r="AL22" s="122">
         <f>$S22+$AB22+$AG22+$AJ22</f>
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6186,7 +6180,7 @@
       <c r="W23" s="126"/>
       <c r="X23" s="126">
         <f>(IF($X22&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X22=$X$6+$Y$6,$P$103,0),0),0)+IF($Y22&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y22=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y23" s="59"/>
       <c r="Z23" s="126">
@@ -6205,7 +6199,7 @@
       <c r="AJ23" s="144"/>
       <c r="AK23" s="150">
         <f>MAX($AL$10:$AL$97) - AL23</f>
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AL23" s="121"/>
     </row>
@@ -6540,88 +6534,88 @@
       <c r="AL25" s="123"/>
     </row>
     <row r="26" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="269">
+      <c r="A26" s="268">
         <f>RANK(AL26,$AL$10:$AL$97,)</f>
+        <v>5</v>
+      </c>
+      <c r="B26" s="269" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="282">
+        <v>5</v>
+      </c>
+      <c r="D26" s="283"/>
+      <c r="E26" s="284">
+        <v>7</v>
+      </c>
+      <c r="F26" s="283"/>
+      <c r="G26" s="285">
+        <v>6</v>
+      </c>
+      <c r="H26" s="286"/>
+      <c r="I26" s="287">
+        <v>6</v>
+      </c>
+      <c r="J26" s="286"/>
+      <c r="K26" s="288">
         <v>4</v>
       </c>
-      <c r="B26" s="270" t="s">
-        <v>73</v>
-      </c>
-      <c r="C26" s="284">
+      <c r="L26" s="286"/>
+      <c r="M26" s="287">
         <v>5</v>
       </c>
-      <c r="D26" s="285"/>
-      <c r="E26" s="289">
+      <c r="N26" s="283"/>
+      <c r="O26" s="287"/>
+      <c r="P26" s="283">
+        <v>7</v>
+      </c>
+      <c r="Q26" s="285"/>
+      <c r="R26" s="290">
+        <v>7</v>
+      </c>
+      <c r="S26" s="292">
+        <f>SUM(C27:R27)</f>
+        <v>38</v>
+      </c>
+      <c r="T26" s="282"/>
+      <c r="U26" s="286">
         <v>6</v>
       </c>
-      <c r="F26" s="285"/>
-      <c r="G26" s="287"/>
-      <c r="H26" s="298">
+      <c r="V26" s="287">
+        <v>5</v>
+      </c>
+      <c r="W26" s="286"/>
+      <c r="X26" s="288"/>
+      <c r="Y26" s="283">
+        <v>5</v>
+      </c>
+      <c r="Z26" s="285">
         <v>7</v>
       </c>
-      <c r="I26" s="289"/>
-      <c r="J26" s="288">
+      <c r="AA26" s="290"/>
+      <c r="AB26" s="292">
+        <f>SUM(T27:AA27)</f>
         <v>6</v>
       </c>
-      <c r="K26" s="290">
-        <v>5</v>
-      </c>
-      <c r="L26" s="288"/>
-      <c r="M26" s="289"/>
-      <c r="N26" s="285">
-        <v>7</v>
-      </c>
-      <c r="O26" s="289">
-        <v>5</v>
-      </c>
-      <c r="P26" s="285"/>
-      <c r="Q26" s="287"/>
-      <c r="R26" s="292">
+      <c r="AC26" s="285"/>
+      <c r="AD26" s="296"/>
+      <c r="AE26" s="288"/>
+      <c r="AF26" s="286"/>
+      <c r="AG26" s="292">
+        <f>SUM(AC27:AF27)</f>
+        <v>0</v>
+      </c>
+      <c r="AH26" s="279"/>
+      <c r="AI26" s="280"/>
+      <c r="AJ26" s="292">
+        <f>AH27</f>
+        <v>0</v>
+      </c>
+      <c r="AK26" s="295">
+        <f>MAX($AL$10:$AL$97) - AL26</f>
         <v>6</v>
       </c>
-      <c r="S26" s="294">
-        <f>SUM(C27:R27)</f>
-        <v>35</v>
-      </c>
-      <c r="T26" s="284"/>
-      <c r="U26" s="288">
-        <v>7</v>
-      </c>
-      <c r="V26" s="289"/>
-      <c r="W26" s="288">
-        <v>7</v>
-      </c>
-      <c r="X26" s="290">
-        <v>6</v>
-      </c>
-      <c r="Y26" s="285"/>
-      <c r="Z26" s="287">
-        <v>6</v>
-      </c>
-      <c r="AA26" s="292"/>
-      <c r="AB26" s="294">
-        <f>SUM(T27:AA27)</f>
-        <v>9</v>
-      </c>
-      <c r="AC26" s="287"/>
-      <c r="AD26" s="288"/>
-      <c r="AE26" s="290"/>
-      <c r="AF26" s="288"/>
-      <c r="AG26" s="294">
-        <f>SUM(AC27:AF27)</f>
-        <v>0</v>
-      </c>
-      <c r="AH26" s="281"/>
-      <c r="AI26" s="282"/>
-      <c r="AJ26" s="294">
-        <f>AH27</f>
-        <v>0</v>
-      </c>
-      <c r="AK26" s="297">
-        <f>MAX($AL$10:$AL$97) - AL26</f>
-        <v>5</v>
-      </c>
-      <c r="AL26" s="294">
+      <c r="AL26" s="292">
         <f>$S26+$AB26+$AG26+$AJ26</f>
         <v>44</v>
       </c>
@@ -6639,17 +6633,17 @@
       <c r="D27" s="140"/>
       <c r="E27" s="120">
         <f>(IF($E26&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E26=$E$6+$F$6,$O$103,0),0),0)+IF($F26&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F26=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F27" s="140"/>
       <c r="G27" s="120">
         <f>(IF($G26&lt;&gt;"",($G$6*$O$104)+IF($G$6=4,($O$102)+IF($G26=$G$6+$H$6,$O$103,0),0),0)+IF($H26&lt;&gt;"",($H$6*$O$104)+IF($H$6=4,($O$102)+IF($H26=$G$6+$H$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="H27" s="140"/>
       <c r="I27" s="120">
         <f>(IF($I26&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I26=$I$6+$J$6,$O$103,0),0),0)+IF($J26&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J26=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J27" s="141"/>
       <c r="K27" s="142">
@@ -6659,12 +6653,12 @@
       <c r="L27" s="140"/>
       <c r="M27" s="120">
         <f>(IF($M26&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M26=$M$6+$N$6,$O$103,0),0),0)+IF($N26&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N26=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="N27" s="140"/>
       <c r="O27" s="120">
         <f>(IF($O26&lt;&gt;"",($O$6*$O$104)+IF($O$6=4,($O$102)+IF($O26=$O$6+$P$6,$O$103,0),0),0)+IF($P26&lt;&gt;"",($P$6*$O$104)+IF($P$6=4,($O$102)+IF($P26=$O$6+$P$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="P27" s="140"/>
       <c r="Q27" s="120">
@@ -6680,7 +6674,7 @@
       <c r="U27" s="126"/>
       <c r="V27" s="126">
         <f>(IF($V26&lt;&gt;"",($V$6*$P$104)+IF($V$6=4,($P$102)+IF($V26=$V$6+$W$6,$P$103,0),0),0)+IF($W26&lt;&gt;"",($W$6*$P$104)+IF($W$6=4,($P$102)+IF($W26=$V$6+$W$6,$P$103,0),0),0))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W27" s="126"/>
       <c r="X27" s="126">
@@ -6704,7 +6698,7 @@
       <c r="AJ27" s="144"/>
       <c r="AK27" s="150">
         <f>MAX($AL$10:$AL$97) - AL27</f>
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AL27" s="121"/>
     </row>
@@ -6747,13 +6741,13 @@
         <f>IF(ISBLANK(H26),
 0,
 IF(H$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28" s="118">
         <f>IF(ISBLANK(I26),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" s="118">
         <f>IF(ISBLANK(J26),
@@ -6783,7 +6777,7 @@
         <f>IF(ISBLANK(N26),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O28" s="118">
         <f>IF(ISBLANK(O26),
@@ -6795,7 +6789,7 @@
         <f>IF(ISBLANK(P26),
 0,
 IF(P$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q28" s="118">
         <f>IF(ISBLANK(Q26),
@@ -6894,7 +6888,7 @@
         <f>IF(E28 = 0,
 0,
 IF(E26 = (E$6+F$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29" s="118">
         <f>IF(F28 = 0,
@@ -6912,7 +6906,7 @@
         <f>IF(H28 = 0,
 0,
 IF(H26 = (G$6+H$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I29" s="118">
         <f>IF(I28 = 0,
@@ -7041,69 +7035,69 @@
     <row r="30" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="117">
         <f>RANK(AL30,$AL$10:$AL$97,)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B30" s="84" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C30" s="46">
         <v>5</v>
       </c>
       <c r="D30" s="45"/>
-      <c r="E30" s="210">
+      <c r="E30" s="44">
+        <v>6</v>
+      </c>
+      <c r="F30" s="45"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="267">
         <v>7</v>
       </c>
-      <c r="F30" s="45"/>
-      <c r="G30" s="48">
+      <c r="I30" s="44"/>
+      <c r="J30" s="47">
         <v>6</v>
       </c>
-      <c r="H30" s="47"/>
-      <c r="I30" s="44">
-        <v>6</v>
-      </c>
-      <c r="J30" s="47"/>
       <c r="K30" s="49">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L30" s="47"/>
-      <c r="M30" s="44">
+      <c r="M30" s="44"/>
+      <c r="N30" s="45">
+        <v>7</v>
+      </c>
+      <c r="O30" s="44">
         <v>5</v>
       </c>
-      <c r="N30" s="45"/>
-      <c r="O30" s="44"/>
-      <c r="P30" s="45">
-        <v>7</v>
-      </c>
+      <c r="P30" s="45"/>
       <c r="Q30" s="48"/>
       <c r="R30" s="50">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S30" s="122">
         <f>SUM(C31:R31)</f>
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="T30" s="46"/>
       <c r="U30" s="47">
+        <v>7</v>
+      </c>
+      <c r="V30" s="44"/>
+      <c r="W30" s="47">
+        <v>7</v>
+      </c>
+      <c r="X30" s="49">
         <v>6</v>
       </c>
-      <c r="V30" s="44">
-        <v>5</v>
-      </c>
-      <c r="W30" s="47"/>
-      <c r="X30" s="49"/>
-      <c r="Y30" s="45">
-        <v>5</v>
-      </c>
+      <c r="Y30" s="45"/>
       <c r="Z30" s="48">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA30" s="47"/>
       <c r="AB30" s="122">
         <f>SUM(T31:AA31)</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="AC30" s="48"/>
-      <c r="AD30" s="268"/>
+      <c r="AD30" s="47"/>
       <c r="AE30" s="49"/>
       <c r="AF30" s="47"/>
       <c r="AG30" s="122">
@@ -7122,7 +7116,7 @@
       </c>
       <c r="AL30" s="122">
         <f>$S30+$AB30+$AG30+$AJ30</f>
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7138,17 +7132,17 @@
       <c r="D31" s="76"/>
       <c r="E31" s="77">
         <f>(IF($E30&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E30=$E$6+$F$6,$O$103,0),0),0)+IF($F30&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F30=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F31" s="76"/>
       <c r="G31" s="77">
         <f>(IF($G30&lt;&gt;"",($G$6*$O$104)+IF($G$6=4,($O$102)+IF($G30=$G$6+$H$6,$O$103,0),0),0)+IF($H30&lt;&gt;"",($H$6*$O$104)+IF($H$6=4,($O$102)+IF($H30=$G$6+$H$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="H31" s="76"/>
       <c r="I31" s="77">
         <f>(IF($I30&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I30=$I$6+$J$6,$O$103,0),0),0)+IF($J30&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J30=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J31" s="78"/>
       <c r="K31" s="79">
@@ -7158,12 +7152,12 @@
       <c r="L31" s="76"/>
       <c r="M31" s="77">
         <f>(IF($M30&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M30=$M$6+$N$6,$O$103,0),0),0)+IF($N30&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N30=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="N31" s="76"/>
       <c r="O31" s="77">
         <f>(IF($O30&lt;&gt;"",($O$6*$O$104)+IF($O$6=4,($O$102)+IF($O30=$O$6+$P$6,$O$103,0),0),0)+IF($P30&lt;&gt;"",($P$6*$O$104)+IF($P$6=4,($O$102)+IF($P30=$O$6+$P$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="P31" s="76"/>
       <c r="Q31" s="77">
@@ -7179,12 +7173,12 @@
       <c r="U31" s="126"/>
       <c r="V31" s="126">
         <f>(IF($V30&lt;&gt;"",($V$6*$P$104)+IF($V$6=4,($P$102)+IF($V30=$V$6+$W$6,$P$103,0),0),0)+IF($W30&lt;&gt;"",($W$6*$P$104)+IF($W$6=4,($P$102)+IF($W30=$V$6+$W$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W31" s="126"/>
       <c r="X31" s="126">
         <f>(IF($X30&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X30=$X$6+$Y$6,$P$103,0),0),0)+IF($Y30&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y30=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y31" s="59"/>
       <c r="Z31" s="126">
@@ -7203,7 +7197,7 @@
       <c r="AJ31" s="121"/>
       <c r="AK31" s="92">
         <f>MAX($AL$10:$AL$97) - AL31</f>
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AL31" s="121"/>
     </row>
@@ -7246,13 +7240,13 @@
         <f>IF(ISBLANK(H30),
 0,
 IF(H$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32" s="118">
         <f>IF(ISBLANK(I30),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J32" s="118">
         <f>IF(ISBLANK(J30),
@@ -7282,7 +7276,7 @@
         <f>IF(ISBLANK(N30),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O32" s="118">
         <f>IF(ISBLANK(O30),
@@ -7294,7 +7288,7 @@
         <f>IF(ISBLANK(P30),
 0,
 IF(P$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q32" s="118">
         <f>IF(ISBLANK(Q30),
@@ -7393,7 +7387,7 @@
         <f>IF(E32 = 0,
 0,
 IF(E30 = (E$6+F$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F33" s="118">
         <f>IF(F32 = 0,
@@ -7411,7 +7405,7 @@
         <f>IF(H32 = 0,
 0,
 IF(H30 = (G$6+H$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33" s="118">
         <f>IF(I32 = 0,
@@ -7538,88 +7532,88 @@
       <c r="AL33" s="123"/>
     </row>
     <row r="34" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="269">
+      <c r="A34" s="268">
         <f>RANK(AL34,$AL$10:$AL$97,)</f>
         <v>7</v>
       </c>
-      <c r="B34" s="270" t="s">
+      <c r="B34" s="269" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="284">
+      <c r="C34" s="282">
         <v>7</v>
       </c>
-      <c r="D34" s="285"/>
-      <c r="E34" s="299">
+      <c r="D34" s="283"/>
+      <c r="E34" s="297">
         <v>6</v>
       </c>
-      <c r="F34" s="285"/>
-      <c r="G34" s="300"/>
-      <c r="H34" s="288">
+      <c r="F34" s="283"/>
+      <c r="G34" s="298"/>
+      <c r="H34" s="286">
         <v>6</v>
       </c>
-      <c r="I34" s="299"/>
-      <c r="J34" s="288">
+      <c r="I34" s="297"/>
+      <c r="J34" s="286">
         <v>7</v>
       </c>
-      <c r="K34" s="290">
+      <c r="K34" s="288">
         <v>5</v>
       </c>
-      <c r="L34" s="288"/>
-      <c r="M34" s="289">
+      <c r="L34" s="286"/>
+      <c r="M34" s="287">
         <v>7</v>
       </c>
-      <c r="N34" s="285"/>
-      <c r="O34" s="289">
+      <c r="N34" s="283"/>
+      <c r="O34" s="287">
         <v>6</v>
       </c>
-      <c r="P34" s="285"/>
-      <c r="Q34" s="287">
+      <c r="P34" s="283"/>
+      <c r="Q34" s="285">
         <v>6</v>
       </c>
-      <c r="R34" s="292"/>
-      <c r="S34" s="294">
+      <c r="R34" s="290"/>
+      <c r="S34" s="292">
         <f>SUM(C35:R35)</f>
         <v>32</v>
       </c>
-      <c r="T34" s="284"/>
-      <c r="U34" s="288">
+      <c r="T34" s="282"/>
+      <c r="U34" s="286">
         <v>7</v>
       </c>
-      <c r="V34" s="289"/>
-      <c r="W34" s="288">
+      <c r="V34" s="287"/>
+      <c r="W34" s="286">
         <v>6</v>
       </c>
-      <c r="X34" s="290">
+      <c r="X34" s="288">
         <v>7</v>
       </c>
-      <c r="Y34" s="285"/>
-      <c r="Z34" s="287">
+      <c r="Y34" s="283"/>
+      <c r="Z34" s="285">
         <v>6</v>
       </c>
-      <c r="AA34" s="288"/>
-      <c r="AB34" s="294">
+      <c r="AA34" s="286"/>
+      <c r="AB34" s="292">
         <f>SUM(T35:AA35)</f>
         <v>9</v>
       </c>
-      <c r="AC34" s="287"/>
-      <c r="AD34" s="288"/>
-      <c r="AE34" s="290"/>
-      <c r="AF34" s="288"/>
-      <c r="AG34" s="294">
+      <c r="AC34" s="285"/>
+      <c r="AD34" s="286"/>
+      <c r="AE34" s="288"/>
+      <c r="AF34" s="286"/>
+      <c r="AG34" s="292">
         <f>SUM(AC35:AF35)</f>
         <v>0</v>
       </c>
-      <c r="AH34" s="301"/>
-      <c r="AI34" s="282"/>
-      <c r="AJ34" s="294">
+      <c r="AH34" s="299"/>
+      <c r="AI34" s="280"/>
+      <c r="AJ34" s="292">
         <f>AH35</f>
         <v>0</v>
       </c>
-      <c r="AK34" s="297">
+      <c r="AK34" s="295">
         <f>MAX($AL$10:$AL$97) - AL34</f>
-        <v>8</v>
-      </c>
-      <c r="AL34" s="294">
+        <v>9</v>
+      </c>
+      <c r="AL34" s="292">
         <f>$S34+$AB34+$AG34+$AJ34</f>
         <v>41</v>
       </c>
@@ -7702,7 +7696,7 @@
       <c r="AJ35" s="121"/>
       <c r="AK35" s="92">
         <f>MAX($AL$10:$AL$97) - AL35</f>
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AL35" s="121"/>
     </row>
@@ -8039,7 +8033,7 @@
     <row r="38" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="117">
         <f>RANK(AL38,$AL$10:$AL$97,)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B38" s="84" t="s">
         <v>81</v>
@@ -8098,7 +8092,7 @@
       <c r="AA38" s="47"/>
       <c r="AB38" s="122">
         <f>SUM(T39:AA39)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC38" s="48"/>
       <c r="AD38" s="47"/>
@@ -8120,7 +8114,7 @@
       </c>
       <c r="AL38" s="122">
         <f>$S38+$AB38+$AG38+$AJ38</f>
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -8182,7 +8176,7 @@
       <c r="W39" s="126"/>
       <c r="X39" s="126">
         <f>(IF($X38&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X38=$X$6+$Y$6,$P$103,0),0),0)+IF($Y38&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y38=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y39" s="59"/>
       <c r="Z39" s="126">
@@ -8201,7 +8195,7 @@
       <c r="AJ39" s="121"/>
       <c r="AK39" s="92">
         <f>MAX($AL$10:$AL$97) - AL39</f>
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AL39" s="121"/>
     </row>
@@ -8536,88 +8530,88 @@
       <c r="AL41" s="123"/>
     </row>
     <row r="42" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="269">
+      <c r="A42" s="268">
         <f>RANK(AL42,$AL$10:$AL$97,)</f>
         <v>9</v>
       </c>
-      <c r="B42" s="270" t="s">
+      <c r="B42" s="269" t="s">
         <v>79</v>
       </c>
-      <c r="C42" s="284">
+      <c r="C42" s="282">
         <v>6</v>
       </c>
-      <c r="D42" s="285"/>
-      <c r="E42" s="289"/>
-      <c r="F42" s="285">
+      <c r="D42" s="283"/>
+      <c r="E42" s="287"/>
+      <c r="F42" s="283">
         <v>7</v>
       </c>
-      <c r="G42" s="287">
+      <c r="G42" s="285">
         <v>6</v>
       </c>
-      <c r="H42" s="288"/>
-      <c r="I42" s="289"/>
-      <c r="J42" s="288">
+      <c r="H42" s="286"/>
+      <c r="I42" s="287"/>
+      <c r="J42" s="286">
         <v>6</v>
       </c>
-      <c r="K42" s="290"/>
-      <c r="L42" s="288">
+      <c r="K42" s="288"/>
+      <c r="L42" s="286">
         <v>6</v>
       </c>
-      <c r="M42" s="289"/>
-      <c r="N42" s="291">
+      <c r="M42" s="287"/>
+      <c r="N42" s="289">
         <v>6</v>
       </c>
-      <c r="O42" s="289">
+      <c r="O42" s="287">
         <v>5</v>
       </c>
-      <c r="P42" s="285"/>
-      <c r="Q42" s="287"/>
-      <c r="R42" s="292">
+      <c r="P42" s="283"/>
+      <c r="Q42" s="285"/>
+      <c r="R42" s="290">
         <v>6</v>
       </c>
-      <c r="S42" s="294">
+      <c r="S42" s="292">
         <f>SUM(C43:R43)</f>
         <v>31</v>
       </c>
-      <c r="T42" s="284"/>
-      <c r="U42" s="288">
+      <c r="T42" s="282"/>
+      <c r="U42" s="286">
         <v>5</v>
       </c>
-      <c r="V42" s="289">
+      <c r="V42" s="287">
         <v>6</v>
       </c>
-      <c r="W42" s="288"/>
-      <c r="X42" s="290">
+      <c r="W42" s="286"/>
+      <c r="X42" s="288">
         <v>6</v>
       </c>
-      <c r="Y42" s="285"/>
-      <c r="Z42" s="287"/>
-      <c r="AA42" s="288">
+      <c r="Y42" s="283"/>
+      <c r="Z42" s="285"/>
+      <c r="AA42" s="286">
         <v>6</v>
       </c>
-      <c r="AB42" s="294">
+      <c r="AB42" s="292">
         <f>SUM(T43:AA43)</f>
         <v>6</v>
       </c>
-      <c r="AC42" s="287"/>
-      <c r="AD42" s="288"/>
-      <c r="AE42" s="290"/>
-      <c r="AF42" s="288"/>
-      <c r="AG42" s="294">
+      <c r="AC42" s="285"/>
+      <c r="AD42" s="286"/>
+      <c r="AE42" s="288"/>
+      <c r="AF42" s="286"/>
+      <c r="AG42" s="292">
         <f>SUM(AC43:AF43)</f>
         <v>0</v>
       </c>
-      <c r="AH42" s="301"/>
-      <c r="AI42" s="282"/>
-      <c r="AJ42" s="294">
+      <c r="AH42" s="299"/>
+      <c r="AI42" s="280"/>
+      <c r="AJ42" s="292">
         <f>AH43</f>
         <v>0</v>
       </c>
-      <c r="AK42" s="297">
+      <c r="AK42" s="295">
         <f>MAX($AL$10:$AL$97) - AL42</f>
-        <v>12</v>
-      </c>
-      <c r="AL42" s="294">
+        <v>13</v>
+      </c>
+      <c r="AL42" s="292">
         <f>$S42+$AB42+$AG42+$AJ42</f>
         <v>37</v>
       </c>
@@ -8700,7 +8694,7 @@
       <c r="AJ43" s="121"/>
       <c r="AK43" s="111">
         <f>MAX($AL$10:$AL$97) - AL43</f>
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AL43" s="121"/>
     </row>
@@ -9040,34 +9034,34 @@
         <v>10</v>
       </c>
       <c r="B46" s="84" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="C46" s="46">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D46" s="45"/>
       <c r="E46" s="44">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" s="45"/>
       <c r="G46" s="48">
+        <v>6</v>
+      </c>
+      <c r="H46" s="47"/>
+      <c r="I46" s="44">
+        <v>6</v>
+      </c>
+      <c r="J46" s="47"/>
+      <c r="K46" s="49">
+        <v>7</v>
+      </c>
+      <c r="L46" s="47"/>
+      <c r="M46" s="44">
         <v>5</v>
       </c>
-      <c r="H46" s="47"/>
-      <c r="I46" s="44"/>
-      <c r="J46" s="47">
-        <v>6</v>
-      </c>
-      <c r="K46" s="49">
-        <v>5</v>
-      </c>
-      <c r="L46" s="47"/>
-      <c r="M46" s="44"/>
-      <c r="N46" s="211">
-        <v>6</v>
-      </c>
+      <c r="N46" s="45"/>
       <c r="O46" s="44">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P46" s="45"/>
       <c r="Q46" s="48"/>
@@ -9078,20 +9072,20 @@
         <f>SUM(C47:R47)</f>
         <v>29</v>
       </c>
-      <c r="T46" s="46"/>
-      <c r="U46" s="47">
+      <c r="T46" s="46">
         <v>6</v>
       </c>
+      <c r="U46" s="47"/>
       <c r="V46" s="44">
         <v>5</v>
       </c>
       <c r="W46" s="47"/>
-      <c r="X46" s="49">
+      <c r="X46" s="49"/>
+      <c r="Y46" s="45">
         <v>7</v>
       </c>
-      <c r="Y46" s="45"/>
       <c r="Z46" s="48">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA46" s="47"/>
       <c r="AB46" s="122">
@@ -9106,7 +9100,7 @@
         <f>SUM(AC47:AF47)</f>
         <v>0</v>
       </c>
-      <c r="AH46" s="214"/>
+      <c r="AH46" s="102"/>
       <c r="AI46" s="57"/>
       <c r="AJ46" s="122">
         <f>AH47</f>
@@ -9114,7 +9108,7 @@
       </c>
       <c r="AK46" s="111">
         <f>MAX($AL$10:$AL$97) - AL46</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AL46" s="122">
         <f>$S46+$AB46+$AG46+$AJ46</f>
@@ -9144,7 +9138,7 @@
       <c r="H47" s="76"/>
       <c r="I47" s="77">
         <f>(IF($I46&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I46=$I$6+$J$6,$O$103,0),0),0)+IF($J46&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J46=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J47" s="78"/>
       <c r="K47" s="79">
@@ -9154,7 +9148,7 @@
       <c r="L47" s="76"/>
       <c r="M47" s="77">
         <f>(IF($M46&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M46=$M$6+$N$6,$O$103,0),0),0)+IF($N46&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N46=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="N47" s="76"/>
       <c r="O47" s="77">
@@ -9199,7 +9193,7 @@
       <c r="AJ47" s="121"/>
       <c r="AK47" s="111">
         <f>MAX($AL$10:$AL$97) - AL47</f>
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AL47" s="121"/>
     </row>
@@ -9248,7 +9242,7 @@
         <f>IF(ISBLANK(I46),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J48" s="118">
         <f>IF(ISBLANK(J46),
@@ -9278,7 +9272,7 @@
         <f>IF(ISBLANK(N46),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O48" s="118">
         <f>IF(ISBLANK(O46),
@@ -9443,7 +9437,7 @@
         <f>IF(N48 = 0,
 0,
 IF(N46 = (M$6+N$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O49" s="118">
         <f>IF(O48 = 0,
@@ -9529,95 +9523,95 @@
       <c r="AJ49" s="138"/>
       <c r="AK49" s="139">
         <f>SUM(C49:AI49)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL49" s="123"/>
     </row>
     <row r="50" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="269">
+      <c r="A50" s="268">
         <f>RANK(AL50,$AL$10:$AL$97,)</f>
-        <v>11</v>
-      </c>
-      <c r="B50" s="270" t="s">
-        <v>74</v>
-      </c>
-      <c r="C50" s="284">
+        <v>10</v>
+      </c>
+      <c r="B50" s="269" t="s">
+        <v>85</v>
+      </c>
+      <c r="C50" s="282">
         <v>5</v>
       </c>
-      <c r="D50" s="285"/>
-      <c r="E50" s="289">
+      <c r="D50" s="283"/>
+      <c r="E50" s="287">
+        <v>5</v>
+      </c>
+      <c r="F50" s="283"/>
+      <c r="G50" s="285">
+        <v>5</v>
+      </c>
+      <c r="H50" s="286"/>
+      <c r="I50" s="287"/>
+      <c r="J50" s="286">
         <v>6</v>
       </c>
-      <c r="F50" s="285"/>
-      <c r="G50" s="287">
+      <c r="K50" s="288">
+        <v>5</v>
+      </c>
+      <c r="L50" s="286"/>
+      <c r="M50" s="287"/>
+      <c r="N50" s="289">
         <v>6</v>
       </c>
-      <c r="H50" s="288"/>
-      <c r="I50" s="289"/>
-      <c r="J50" s="288">
-        <v>7</v>
-      </c>
-      <c r="K50" s="290">
+      <c r="O50" s="287">
         <v>5</v>
       </c>
-      <c r="L50" s="288"/>
-      <c r="M50" s="289"/>
-      <c r="N50" s="291">
+      <c r="P50" s="283"/>
+      <c r="Q50" s="285"/>
+      <c r="R50" s="290">
         <v>6</v>
       </c>
-      <c r="O50" s="289">
-        <v>7</v>
-      </c>
-      <c r="P50" s="285"/>
-      <c r="Q50" s="287"/>
-      <c r="R50" s="292">
-        <v>6</v>
-      </c>
-      <c r="S50" s="294">
+      <c r="S50" s="292">
         <f>SUM(C51:R51)</f>
         <v>29</v>
       </c>
-      <c r="T50" s="284"/>
-      <c r="U50" s="288">
+      <c r="T50" s="282"/>
+      <c r="U50" s="286">
         <v>6</v>
       </c>
-      <c r="V50" s="289">
+      <c r="V50" s="287">
         <v>5</v>
       </c>
-      <c r="W50" s="288"/>
-      <c r="X50" s="290"/>
-      <c r="Y50" s="285">
-        <v>5</v>
-      </c>
-      <c r="Z50" s="287">
+      <c r="W50" s="286"/>
+      <c r="X50" s="288">
+        <v>7</v>
+      </c>
+      <c r="Y50" s="283"/>
+      <c r="Z50" s="285">
+        <v>7</v>
+      </c>
+      <c r="AA50" s="286"/>
+      <c r="AB50" s="292">
+        <f>SUM(T51:AA51)</f>
         <v>6</v>
       </c>
-      <c r="AA50" s="288"/>
-      <c r="AB50" s="294">
-        <f>SUM(T51:AA51)</f>
-        <v>5</v>
-      </c>
-      <c r="AC50" s="287"/>
-      <c r="AD50" s="288"/>
-      <c r="AE50" s="290"/>
-      <c r="AF50" s="288"/>
-      <c r="AG50" s="294">
+      <c r="AC50" s="285"/>
+      <c r="AD50" s="286"/>
+      <c r="AE50" s="288"/>
+      <c r="AF50" s="286"/>
+      <c r="AG50" s="292">
         <f>SUM(AC51:AF51)</f>
         <v>0</v>
       </c>
-      <c r="AH50" s="301"/>
-      <c r="AI50" s="282"/>
-      <c r="AJ50" s="294">
+      <c r="AH50" s="300"/>
+      <c r="AI50" s="280"/>
+      <c r="AJ50" s="292">
         <f>AH51</f>
         <v>0</v>
       </c>
-      <c r="AK50" s="297">
+      <c r="AK50" s="295">
         <f>MAX($AL$10:$AL$97) - AL50</f>
         <v>15</v>
       </c>
-      <c r="AL50" s="294">
+      <c r="AL50" s="292">
         <f>$S50+$AB50+$AG50+$AJ50</f>
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -9679,7 +9673,7 @@
       <c r="W51" s="126"/>
       <c r="X51" s="126">
         <f>(IF($X50&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X50=$X$6+$Y$6,$P$103,0),0),0)+IF($Y50&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y50=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y51" s="59"/>
       <c r="Z51" s="126">
@@ -10032,46 +10026,46 @@
     <row r="54" spans="1:38" s="27" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="117">
         <f>RANK(AL54,$AL$10:$AL$97,)</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B54" s="84" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C54" s="46">
+        <v>5</v>
+      </c>
+      <c r="D54" s="45"/>
+      <c r="E54" s="44">
         <v>6</v>
-      </c>
-      <c r="D54" s="45"/>
-      <c r="E54" s="210">
-        <v>7</v>
       </c>
       <c r="F54" s="45"/>
       <c r="G54" s="48">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H54" s="47"/>
       <c r="I54" s="44"/>
       <c r="J54" s="47">
+        <v>7</v>
+      </c>
+      <c r="K54" s="49">
         <v>5</v>
       </c>
-      <c r="K54" s="49">
-        <v>7</v>
-      </c>
       <c r="L54" s="47"/>
-      <c r="M54" s="44">
+      <c r="M54" s="44"/>
+      <c r="N54" s="211">
         <v>6</v>
       </c>
-      <c r="N54" s="45"/>
       <c r="O54" s="44">
         <v>7</v>
       </c>
       <c r="P54" s="45"/>
-      <c r="Q54" s="48">
-        <v>5</v>
-      </c>
-      <c r="R54" s="50"/>
+      <c r="Q54" s="48"/>
+      <c r="R54" s="50">
+        <v>6</v>
+      </c>
       <c r="S54" s="122">
         <f>SUM(C55:R55)</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T54" s="46"/>
       <c r="U54" s="47">
@@ -10081,12 +10075,12 @@
         <v>5</v>
       </c>
       <c r="W54" s="47"/>
-      <c r="X54" s="49">
-        <v>4</v>
-      </c>
-      <c r="Y54" s="45"/>
+      <c r="X54" s="49"/>
+      <c r="Y54" s="45">
+        <v>5</v>
+      </c>
       <c r="Z54" s="48">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA54" s="47"/>
       <c r="AB54" s="122">
@@ -10113,7 +10107,7 @@
       </c>
       <c r="AL54" s="122">
         <f>$S54+$AB54+$AG54+$AJ54</f>
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="55" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -10129,7 +10123,7 @@
       <c r="D55" s="127"/>
       <c r="E55" s="125">
         <f>(IF($E54&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E54=$E$6+$F$6,$O$103,0),0),0)+IF($F54&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F54=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F55" s="127"/>
       <c r="G55" s="125">
@@ -10149,7 +10143,7 @@
       <c r="L55" s="127"/>
       <c r="M55" s="125">
         <f>(IF($M54&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M54=$M$6+$N$6,$O$103,0),0),0)+IF($N54&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N54=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="N55" s="127"/>
       <c r="O55" s="128">
@@ -10159,7 +10153,7 @@
       <c r="P55" s="127"/>
       <c r="Q55" s="128">
         <f>(IF($Q54&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q54=$Q$6+$R$6,$O$103,0),0),0)+IF($R54&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R54=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="R55" s="131"/>
       <c r="S55" s="121"/>
@@ -10270,7 +10264,7 @@
         <f>IF(ISBLANK(N54),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O56" s="118">
         <f>IF(ISBLANK(O54),
@@ -10288,7 +10282,7 @@
         <f>IF(ISBLANK(Q54),
 0,
 IF(Q$6= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R56" s="118">
         <f>IF(ISBLANK(R54),
@@ -10381,7 +10375,7 @@
         <f>IF(E56 = 0,
 0,
 IF(E54 = (E$6+F$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F57" s="118">
         <f>IF(F56 = 0,
@@ -10435,7 +10429,7 @@
         <f>IF(N56 = 0,
 0,
 IF(N54 = (M$6+N$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O57" s="118">
         <f>IF(O56 = 0,
@@ -10526,90 +10520,90 @@
       <c r="AL57" s="123"/>
     </row>
     <row r="58" spans="1:38" s="27" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="269">
+      <c r="A58" s="268">
         <f>RANK(AL58,$AL$10:$AL$97,)</f>
         <v>13</v>
       </c>
-      <c r="B58" s="270" t="s">
-        <v>65</v>
-      </c>
-      <c r="C58" s="284">
+      <c r="B58" s="269" t="s">
+        <v>83</v>
+      </c>
+      <c r="C58" s="282">
+        <v>6</v>
+      </c>
+      <c r="D58" s="283"/>
+      <c r="E58" s="284">
+        <v>7</v>
+      </c>
+      <c r="F58" s="283"/>
+      <c r="G58" s="285">
+        <v>5</v>
+      </c>
+      <c r="H58" s="286"/>
+      <c r="I58" s="287"/>
+      <c r="J58" s="286">
+        <v>5</v>
+      </c>
+      <c r="K58" s="288">
+        <v>7</v>
+      </c>
+      <c r="L58" s="286"/>
+      <c r="M58" s="287">
+        <v>6</v>
+      </c>
+      <c r="N58" s="283"/>
+      <c r="O58" s="287">
+        <v>7</v>
+      </c>
+      <c r="P58" s="283"/>
+      <c r="Q58" s="285">
+        <v>5</v>
+      </c>
+      <c r="R58" s="290"/>
+      <c r="S58" s="292">
+        <f>SUM(C59:R59)</f>
+        <v>28</v>
+      </c>
+      <c r="T58" s="282"/>
+      <c r="U58" s="286">
+        <v>6</v>
+      </c>
+      <c r="V58" s="287">
+        <v>5</v>
+      </c>
+      <c r="W58" s="286"/>
+      <c r="X58" s="288">
         <v>4</v>
       </c>
-      <c r="D58" s="285"/>
-      <c r="E58" s="289">
-        <v>4</v>
-      </c>
-      <c r="F58" s="285"/>
-      <c r="G58" s="287">
+      <c r="Y58" s="283"/>
+      <c r="Z58" s="285">
+        <v>7</v>
+      </c>
+      <c r="AA58" s="286"/>
+      <c r="AB58" s="292">
+        <f>SUM(T59:AA59)</f>
         <v>6</v>
       </c>
-      <c r="H58" s="288"/>
-      <c r="I58" s="289">
-        <v>6</v>
-      </c>
-      <c r="J58" s="288"/>
-      <c r="K58" s="290">
-        <v>7</v>
-      </c>
-      <c r="L58" s="288"/>
-      <c r="M58" s="289">
-        <v>5</v>
-      </c>
-      <c r="N58" s="285"/>
-      <c r="O58" s="289">
-        <v>4</v>
-      </c>
-      <c r="P58" s="285"/>
-      <c r="Q58" s="287"/>
-      <c r="R58" s="292">
-        <v>6</v>
-      </c>
-      <c r="S58" s="294">
-        <f>SUM(C59:R59)</f>
-        <v>29</v>
-      </c>
-      <c r="T58" s="284">
-        <v>6</v>
-      </c>
-      <c r="U58" s="288"/>
-      <c r="V58" s="289">
-        <v>5</v>
-      </c>
-      <c r="W58" s="288"/>
-      <c r="X58" s="290"/>
-      <c r="Y58" s="285">
-        <v>7</v>
-      </c>
-      <c r="Z58" s="287">
-        <v>6</v>
-      </c>
-      <c r="AA58" s="288"/>
-      <c r="AB58" s="294">
-        <f>SUM(T59:AA59)</f>
-        <v>4</v>
-      </c>
-      <c r="AC58" s="287"/>
-      <c r="AD58" s="288"/>
-      <c r="AE58" s="290"/>
-      <c r="AF58" s="288"/>
-      <c r="AG58" s="294">
+      <c r="AC58" s="285"/>
+      <c r="AD58" s="286"/>
+      <c r="AE58" s="288"/>
+      <c r="AF58" s="286"/>
+      <c r="AG58" s="292">
         <f>SUM(AC59:AF59)</f>
         <v>0</v>
       </c>
-      <c r="AH58" s="301"/>
-      <c r="AI58" s="282"/>
-      <c r="AJ58" s="294">
+      <c r="AH58" s="299"/>
+      <c r="AI58" s="280"/>
+      <c r="AJ58" s="292">
         <f>AH59</f>
         <v>0</v>
       </c>
-      <c r="AK58" s="297">
+      <c r="AK58" s="295">
         <f>MAX($AL$10:$AL$97) - AL58</f>
         <v>16</v>
       </c>
-      <c r="AL58" s="294">
+      <c r="AL58" s="292">
         <f>$S58+$AB58+$AG58+$AJ58</f>
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="59" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -10625,7 +10619,7 @@
       <c r="D59" s="127"/>
       <c r="E59" s="125">
         <f>(IF($E58&lt;&gt;"",($E$6*$O$104)+IF($E$6=4,($O$102)+IF($E58=$E$6+$F$6,$O$103,0),0),0)+IF($F58&lt;&gt;"",($F$6*$O$104)+IF($F$6=4,($O$102)+IF($F58=$E$6+$F$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F59" s="127"/>
       <c r="G59" s="125">
@@ -10635,7 +10629,7 @@
       <c r="H59" s="127"/>
       <c r="I59" s="128">
         <f>(IF($I58&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I58=$I$6+$J$6,$O$103,0),0),0)+IF($J58&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J58=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J59" s="129"/>
       <c r="K59" s="130">
@@ -10655,13 +10649,13 @@
       <c r="P59" s="127"/>
       <c r="Q59" s="128">
         <f>(IF($Q58&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q58=$Q$6+$R$6,$O$103,0),0),0)+IF($R58&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R58=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="R59" s="131"/>
       <c r="S59" s="121"/>
       <c r="T59" s="126">
         <f>(IF($T58&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T58=$T$6+$U$6,$P$103,0),0),0)+IF($U58&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U58=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U59" s="126"/>
       <c r="V59" s="126">
@@ -10671,7 +10665,7 @@
       <c r="W59" s="126"/>
       <c r="X59" s="126">
         <f>(IF($X58&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X58=$X$6+$Y$6,$P$103,0),0),0)+IF($Y58&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y58=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y59" s="59"/>
       <c r="Z59" s="126">
@@ -10736,7 +10730,7 @@
         <f>IF(ISBLANK(I58),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J60" s="118">
         <f>IF(ISBLANK(J58),
@@ -10784,7 +10778,7 @@
         <f>IF(ISBLANK(Q58),
 0,
 IF(Q$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R60" s="118">
         <f>IF(ISBLANK(R58),
@@ -10877,7 +10871,7 @@
         <f>IF(E60 = 0,
 0,
 IF(E58 = (E$6+F$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F61" s="118">
         <f>IF(F60 = 0,
@@ -11017,7 +11011,7 @@
       <c r="AJ61" s="138"/>
       <c r="AK61" s="139">
         <f>SUM(C61:AI61)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL61" s="123"/>
     </row>
@@ -11101,7 +11095,7 @@
       </c>
       <c r="AK62" s="111">
         <f>MAX($AL$10:$AL$97) - AL62</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AL62" s="122">
         <f>$S62+$AB62+$AG62+$AJ62</f>
@@ -11518,90 +11512,90 @@
       <c r="AL65" s="123"/>
     </row>
     <row r="66" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="269">
+      <c r="A66" s="268">
         <f>RANK(AL66,$AL$10:$AL$97,)</f>
         <v>15</v>
       </c>
-      <c r="B66" s="270" t="s">
+      <c r="B66" s="269" t="s">
         <v>67</v>
       </c>
-      <c r="C66" s="284">
+      <c r="C66" s="282">
         <v>4</v>
       </c>
-      <c r="D66" s="285"/>
-      <c r="E66" s="289">
+      <c r="D66" s="283"/>
+      <c r="E66" s="287">
         <v>4</v>
       </c>
-      <c r="F66" s="285"/>
-      <c r="G66" s="287">
+      <c r="F66" s="283"/>
+      <c r="G66" s="285">
         <v>6</v>
       </c>
-      <c r="H66" s="288"/>
-      <c r="I66" s="289"/>
-      <c r="J66" s="288">
+      <c r="H66" s="286"/>
+      <c r="I66" s="287"/>
+      <c r="J66" s="286">
         <v>6</v>
       </c>
-      <c r="K66" s="290">
+      <c r="K66" s="288">
         <v>6</v>
       </c>
-      <c r="L66" s="288"/>
-      <c r="M66" s="289">
+      <c r="L66" s="286"/>
+      <c r="M66" s="287">
         <v>5</v>
       </c>
-      <c r="N66" s="285"/>
-      <c r="O66" s="289">
+      <c r="N66" s="283"/>
+      <c r="O66" s="287">
         <v>6</v>
       </c>
-      <c r="P66" s="285"/>
-      <c r="Q66" s="287"/>
-      <c r="R66" s="292">
+      <c r="P66" s="283"/>
+      <c r="Q66" s="285"/>
+      <c r="R66" s="290">
         <v>6</v>
       </c>
-      <c r="S66" s="294">
+      <c r="S66" s="292">
         <f>SUM(C67:R67)</f>
         <v>20</v>
       </c>
-      <c r="T66" s="284"/>
-      <c r="U66" s="288">
+      <c r="T66" s="282"/>
+      <c r="U66" s="286">
         <v>6</v>
       </c>
-      <c r="V66" s="289"/>
-      <c r="W66" s="288">
+      <c r="V66" s="287"/>
+      <c r="W66" s="286">
         <v>7</v>
       </c>
-      <c r="X66" s="290"/>
-      <c r="Y66" s="285">
+      <c r="X66" s="288"/>
+      <c r="Y66" s="283">
         <v>7</v>
       </c>
-      <c r="Z66" s="287">
+      <c r="Z66" s="285">
         <v>6</v>
       </c>
-      <c r="AA66" s="288"/>
-      <c r="AB66" s="294">
+      <c r="AA66" s="286"/>
+      <c r="AB66" s="292">
         <f>SUM(T67:AA67)</f>
-        <v>8</v>
-      </c>
-      <c r="AC66" s="287"/>
-      <c r="AD66" s="302"/>
-      <c r="AE66" s="290"/>
-      <c r="AF66" s="288"/>
-      <c r="AG66" s="294">
+        <v>9</v>
+      </c>
+      <c r="AC66" s="285"/>
+      <c r="AD66" s="296"/>
+      <c r="AE66" s="288"/>
+      <c r="AF66" s="286"/>
+      <c r="AG66" s="292">
         <f>SUM(AC67:AF67)</f>
         <v>0</v>
       </c>
-      <c r="AH66" s="303"/>
-      <c r="AI66" s="296"/>
-      <c r="AJ66" s="294">
+      <c r="AH66" s="301"/>
+      <c r="AI66" s="294"/>
+      <c r="AJ66" s="292">
         <f>AH67</f>
         <v>0</v>
       </c>
-      <c r="AK66" s="297">
+      <c r="AK66" s="295">
         <f>MAX($AL$10:$AL$97) - AL66</f>
         <v>21</v>
       </c>
-      <c r="AL66" s="294">
+      <c r="AL66" s="292">
         <f>$S66+$AB66+$AG66+$AJ66</f>
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="67" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11663,7 +11657,7 @@
       <c r="W67" s="126"/>
       <c r="X67" s="126">
         <f>(IF($X66&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X66=$X$6+$Y$6,$P$103,0),0),0)+IF($Y66&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y66=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y67" s="59"/>
       <c r="Z67" s="126">
@@ -12075,7 +12069,7 @@
       </c>
       <c r="AB70" s="122">
         <f>SUM(T71:AA71)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AC70" s="48"/>
       <c r="AD70" s="47"/>
@@ -12097,7 +12091,7 @@
       </c>
       <c r="AL70" s="122">
         <f>$S70+$AB70+$AG70+$AJ70</f>
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="71" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -12159,7 +12153,7 @@
       <c r="W71" s="126"/>
       <c r="X71" s="126">
         <f>(IF($X70&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X70=$X$6+$Y$6,$P$103,0),0),0)+IF($Y70&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y70=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y71" s="59"/>
       <c r="Z71" s="126">
@@ -12510,88 +12504,88 @@
       <c r="AL73" s="123"/>
     </row>
     <row r="74" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="269">
+      <c r="A74" s="268">
         <f>RANK(AL74,$AL$10:$AL$97,)</f>
         <v>17</v>
       </c>
-      <c r="B74" s="270" t="s">
+      <c r="B74" s="269" t="s">
         <v>68</v>
       </c>
-      <c r="C74" s="304">
+      <c r="C74" s="302">
         <v>5</v>
       </c>
-      <c r="D74" s="305"/>
-      <c r="E74" s="306">
+      <c r="D74" s="303"/>
+      <c r="E74" s="304">
         <v>6</v>
       </c>
-      <c r="F74" s="305"/>
-      <c r="G74" s="307">
+      <c r="F74" s="303"/>
+      <c r="G74" s="305">
         <v>5</v>
       </c>
-      <c r="H74" s="308"/>
-      <c r="I74" s="306"/>
-      <c r="J74" s="308">
+      <c r="H74" s="306"/>
+      <c r="I74" s="304"/>
+      <c r="J74" s="306">
         <v>6</v>
       </c>
-      <c r="K74" s="309">
+      <c r="K74" s="307">
         <v>6</v>
       </c>
-      <c r="L74" s="308"/>
-      <c r="M74" s="306">
+      <c r="L74" s="306"/>
+      <c r="M74" s="304">
         <v>7</v>
       </c>
-      <c r="N74" s="305"/>
-      <c r="O74" s="306">
+      <c r="N74" s="303"/>
+      <c r="O74" s="304">
         <v>6</v>
       </c>
-      <c r="P74" s="305"/>
-      <c r="Q74" s="307"/>
-      <c r="R74" s="310">
+      <c r="P74" s="303"/>
+      <c r="Q74" s="305"/>
+      <c r="R74" s="308">
         <v>6</v>
       </c>
-      <c r="S74" s="294">
+      <c r="S74" s="292">
         <f>SUM(C75:R75)</f>
         <v>20</v>
       </c>
-      <c r="T74" s="284"/>
-      <c r="U74" s="288">
+      <c r="T74" s="282"/>
+      <c r="U74" s="286">
         <v>6</v>
       </c>
-      <c r="V74" s="289">
+      <c r="V74" s="287">
         <v>7</v>
       </c>
-      <c r="W74" s="288"/>
-      <c r="X74" s="290">
+      <c r="W74" s="286"/>
+      <c r="X74" s="288">
         <v>6</v>
       </c>
-      <c r="Y74" s="285"/>
-      <c r="Z74" s="287">
+      <c r="Y74" s="283"/>
+      <c r="Z74" s="285">
         <v>7</v>
       </c>
-      <c r="AA74" s="288"/>
-      <c r="AB74" s="294">
+      <c r="AA74" s="286"/>
+      <c r="AB74" s="292">
         <f>SUM(T75:AA75)</f>
         <v>6</v>
       </c>
-      <c r="AC74" s="287"/>
-      <c r="AD74" s="288"/>
-      <c r="AE74" s="290"/>
-      <c r="AF74" s="288"/>
-      <c r="AG74" s="294">
+      <c r="AC74" s="285"/>
+      <c r="AD74" s="286"/>
+      <c r="AE74" s="288"/>
+      <c r="AF74" s="286"/>
+      <c r="AG74" s="292">
         <f>SUM(AC75:AF75)</f>
         <v>0</v>
       </c>
-      <c r="AH74" s="303"/>
-      <c r="AI74" s="296"/>
-      <c r="AJ74" s="294">
+      <c r="AH74" s="301"/>
+      <c r="AI74" s="294"/>
+      <c r="AJ74" s="292">
         <f>AH75</f>
         <v>0</v>
       </c>
-      <c r="AK74" s="297">
+      <c r="AK74" s="295">
         <f>MAX($AL$10:$AL$97) - AL74</f>
-        <v>23</v>
-      </c>
-      <c r="AL74" s="294">
+        <v>24</v>
+      </c>
+      <c r="AL74" s="292">
         <f>$S74+$AB74+$AG74+$AJ74</f>
         <v>26</v>
       </c>
@@ -13008,7 +13002,7 @@
     <row r="78" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="117">
         <f>RANK(AL78,$AL$10:$AL$97,)</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B78" s="84" t="s">
         <v>80</v>
@@ -13067,7 +13061,7 @@
       </c>
       <c r="AB78" s="122">
         <f>SUM(T79:AA79)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC78" s="48"/>
       <c r="AD78" s="47"/>
@@ -13089,7 +13083,7 @@
       </c>
       <c r="AL78" s="122">
         <f>$S78+$AB78+$AG78+$AJ78</f>
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="79" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -13151,7 +13145,7 @@
       <c r="W79" s="126"/>
       <c r="X79" s="126">
         <f>(IF($X78&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X78=$X$6+$Y$6,$P$103,0),0),0)+IF($Y78&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y78=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y79" s="59"/>
       <c r="Z79" s="126">
@@ -13502,90 +13496,90 @@
       <c r="AL81" s="123"/>
     </row>
     <row r="82" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="269">
+      <c r="A82" s="268">
         <f>RANK(AL82,$AL$10:$AL$97,)</f>
-        <v>18</v>
-      </c>
-      <c r="B82" s="270" t="s">
+        <v>17</v>
+      </c>
+      <c r="B82" s="269" t="s">
         <v>75</v>
       </c>
-      <c r="C82" s="284">
+      <c r="C82" s="282">
         <v>5</v>
       </c>
-      <c r="D82" s="285"/>
-      <c r="E82" s="289">
+      <c r="D82" s="283"/>
+      <c r="E82" s="287">
         <v>6</v>
       </c>
-      <c r="F82" s="285"/>
-      <c r="G82" s="287">
+      <c r="F82" s="283"/>
+      <c r="G82" s="285">
         <v>6</v>
       </c>
-      <c r="H82" s="288"/>
-      <c r="I82" s="289"/>
-      <c r="J82" s="288">
+      <c r="H82" s="286"/>
+      <c r="I82" s="287"/>
+      <c r="J82" s="286">
         <v>6</v>
       </c>
-      <c r="K82" s="290">
+      <c r="K82" s="288">
         <v>6</v>
       </c>
-      <c r="L82" s="288"/>
-      <c r="M82" s="289">
+      <c r="L82" s="286"/>
+      <c r="M82" s="287">
         <v>7</v>
       </c>
-      <c r="N82" s="285"/>
-      <c r="O82" s="289">
+      <c r="N82" s="283"/>
+      <c r="O82" s="287">
         <v>6</v>
       </c>
-      <c r="P82" s="285"/>
-      <c r="Q82" s="287"/>
-      <c r="R82" s="292">
+      <c r="P82" s="283"/>
+      <c r="Q82" s="285"/>
+      <c r="R82" s="290">
         <v>7</v>
       </c>
-      <c r="S82" s="294">
+      <c r="S82" s="292">
         <f>SUM(C83:R83)</f>
         <v>20</v>
       </c>
-      <c r="T82" s="284">
+      <c r="T82" s="282">
         <v>7</v>
       </c>
-      <c r="U82" s="288"/>
-      <c r="V82" s="289">
+      <c r="U82" s="286"/>
+      <c r="V82" s="287">
         <v>7</v>
       </c>
-      <c r="W82" s="288"/>
-      <c r="X82" s="290">
+      <c r="W82" s="286"/>
+      <c r="X82" s="288">
         <v>7</v>
       </c>
-      <c r="Y82" s="285"/>
-      <c r="Z82" s="287">
+      <c r="Y82" s="283"/>
+      <c r="Z82" s="285">
         <v>7</v>
       </c>
-      <c r="AA82" s="288"/>
-      <c r="AB82" s="294">
+      <c r="AA82" s="286"/>
+      <c r="AB82" s="292">
         <f>SUM(T83:AA83)</f>
-        <v>5</v>
-      </c>
-      <c r="AC82" s="287"/>
-      <c r="AD82" s="288"/>
-      <c r="AE82" s="290"/>
-      <c r="AF82" s="288"/>
-      <c r="AG82" s="294">
+        <v>6</v>
+      </c>
+      <c r="AC82" s="285"/>
+      <c r="AD82" s="286"/>
+      <c r="AE82" s="288"/>
+      <c r="AF82" s="286"/>
+      <c r="AG82" s="292">
         <f>SUM(AC83:AF83)</f>
         <v>0</v>
       </c>
-      <c r="AH82" s="303"/>
-      <c r="AI82" s="296"/>
-      <c r="AJ82" s="294">
+      <c r="AH82" s="301"/>
+      <c r="AI82" s="294"/>
+      <c r="AJ82" s="292">
         <f>AH83</f>
         <v>0</v>
       </c>
-      <c r="AK82" s="297">
+      <c r="AK82" s="295">
         <f>MAX($AL$10:$AL$97) - AL82</f>
         <v>24</v>
       </c>
-      <c r="AL82" s="294">
+      <c r="AL82" s="292">
         <f>$S82+$AB82+$AG82+$AJ82</f>
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="83" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -13637,7 +13631,7 @@
       <c r="S83" s="121"/>
       <c r="T83" s="126">
         <f>(IF($T82&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T82=$T$6+$U$6,$P$103,0),0),0)+IF($U82&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U82=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U83" s="126"/>
       <c r="V83" s="126">
@@ -14077,7 +14071,7 @@
       </c>
       <c r="AK86" s="111">
         <f>MAX($AL$10:$AL$97) - AL86</f>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AL86" s="122">
         <f>$S86+$AB86+$AG86+$AJ86</f>
@@ -14494,88 +14488,88 @@
       <c r="AL89" s="123"/>
     </row>
     <row r="90" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="269">
+      <c r="A90" s="268">
         <f>RANK(AL90,$AL$10:$AL$97,)</f>
         <v>20</v>
       </c>
-      <c r="B90" s="270" t="s">
-        <v>78</v>
-      </c>
-      <c r="C90" s="284">
+      <c r="B90" s="269" t="s">
+        <v>84</v>
+      </c>
+      <c r="C90" s="282">
+        <v>6</v>
+      </c>
+      <c r="D90" s="283"/>
+      <c r="E90" s="287"/>
+      <c r="F90" s="283">
+        <v>7</v>
+      </c>
+      <c r="G90" s="285">
+        <v>7</v>
+      </c>
+      <c r="H90" s="286"/>
+      <c r="I90" s="287"/>
+      <c r="J90" s="286">
+        <v>6</v>
+      </c>
+      <c r="K90" s="288">
+        <v>6</v>
+      </c>
+      <c r="L90" s="286"/>
+      <c r="M90" s="287">
+        <v>7</v>
+      </c>
+      <c r="N90" s="283"/>
+      <c r="O90" s="287">
         <v>5</v>
       </c>
-      <c r="D90" s="285"/>
-      <c r="E90" s="289"/>
-      <c r="F90" s="285">
-        <v>7</v>
-      </c>
-      <c r="G90" s="287">
+      <c r="P90" s="283"/>
+      <c r="Q90" s="285"/>
+      <c r="R90" s="290">
         <v>6</v>
       </c>
-      <c r="H90" s="288"/>
-      <c r="I90" s="289"/>
-      <c r="J90" s="288">
-        <v>7</v>
-      </c>
-      <c r="K90" s="290">
-        <v>5</v>
-      </c>
-      <c r="L90" s="288"/>
-      <c r="M90" s="289">
-        <v>6</v>
-      </c>
-      <c r="N90" s="285"/>
-      <c r="O90" s="289">
-        <v>7</v>
-      </c>
-      <c r="P90" s="285"/>
-      <c r="Q90" s="287"/>
-      <c r="R90" s="292">
-        <v>7</v>
-      </c>
-      <c r="S90" s="294">
+      <c r="S90" s="292">
         <f>SUM(C91:R91)</f>
         <v>14</v>
       </c>
-      <c r="T90" s="284"/>
-      <c r="U90" s="288">
+      <c r="T90" s="282"/>
+      <c r="U90" s="286">
         <v>7</v>
       </c>
-      <c r="V90" s="289">
-        <v>7</v>
-      </c>
-      <c r="W90" s="288"/>
-      <c r="X90" s="290">
+      <c r="V90" s="287">
         <v>6</v>
       </c>
-      <c r="Y90" s="285"/>
-      <c r="Z90" s="287">
+      <c r="W90" s="286"/>
+      <c r="X90" s="288"/>
+      <c r="Y90" s="283">
         <v>6</v>
       </c>
-      <c r="AA90" s="288"/>
-      <c r="AB90" s="294">
+      <c r="Z90" s="285">
+        <v>6</v>
+      </c>
+      <c r="AA90" s="286"/>
+      <c r="AB90" s="292">
         <f>SUM(T91:AA91)</f>
         <v>6</v>
       </c>
-      <c r="AC90" s="287"/>
-      <c r="AD90" s="288"/>
-      <c r="AE90" s="290"/>
-      <c r="AF90" s="288"/>
-      <c r="AG90" s="294">
+      <c r="AC90" s="285"/>
+      <c r="AD90" s="286"/>
+      <c r="AE90" s="288"/>
+      <c r="AF90" s="286"/>
+      <c r="AG90" s="292">
         <f>SUM(AC91:AF91)</f>
         <v>0</v>
       </c>
-      <c r="AH90" s="303"/>
-      <c r="AI90" s="296"/>
-      <c r="AJ90" s="294">
+      <c r="AH90" s="301"/>
+      <c r="AI90" s="294"/>
+      <c r="AJ90" s="292">
         <f>AH91</f>
         <v>0</v>
       </c>
-      <c r="AK90" s="297">
+      <c r="AK90" s="295">
         <f>MAX($AL$10:$AL$97) - AL90</f>
-        <v>29</v>
-      </c>
-      <c r="AL90" s="294">
+        <v>30</v>
+      </c>
+      <c r="AL90" s="292">
         <f>$S90+$AB90+$AG90+$AJ90</f>
         <v>20</v>
       </c>
@@ -14992,13 +14986,13 @@
     <row r="94" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A94" s="117">
         <f>RANK(AL94,$AL$10:$AL$97,)</f>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B94" s="84" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C94" s="187">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D94" s="188"/>
       <c r="E94" s="189"/>
@@ -15006,28 +15000,28 @@
         <v>7</v>
       </c>
       <c r="G94" s="190">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H94" s="191"/>
       <c r="I94" s="189"/>
       <c r="J94" s="191">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K94" s="192">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L94" s="191"/>
       <c r="M94" s="189">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N94" s="188"/>
       <c r="O94" s="189">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P94" s="188"/>
       <c r="Q94" s="190"/>
       <c r="R94" s="193">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S94" s="122">
         <f>SUM(C95:R95)</f>
@@ -15038,20 +15032,20 @@
         <v>7</v>
       </c>
       <c r="V94" s="44">
+        <v>7</v>
+      </c>
+      <c r="W94" s="47"/>
+      <c r="X94" s="49">
         <v>6</v>
       </c>
-      <c r="W94" s="47"/>
-      <c r="X94" s="49"/>
-      <c r="Y94" s="45">
-        <v>6</v>
-      </c>
+      <c r="Y94" s="45"/>
       <c r="Z94" s="48">
         <v>6</v>
       </c>
       <c r="AA94" s="47"/>
       <c r="AB94" s="179">
         <f>SUM(T95:AA95)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC94" s="48"/>
       <c r="AD94" s="47"/>
@@ -15073,7 +15067,7 @@
       </c>
       <c r="AL94" s="179">
         <f>$S94+$AB94+$AG94+$AJ94</f>
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="95" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -15135,7 +15129,7 @@
       <c r="W95" s="126"/>
       <c r="X95" s="126">
         <f>(IF($X94&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X94=$X$6+$Y$6,$P$103,0),0),0)+IF($Y94&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y94=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y95" s="59"/>
       <c r="Z95" s="126">
@@ -15618,12 +15612,12 @@
     <row r="100" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B100" s="43"/>
       <c r="N100" s="26"/>
-      <c r="O100" s="215" t="s">
+      <c r="O100" s="248" t="s">
         <v>17</v>
       </c>
-      <c r="P100" s="216"/>
-      <c r="Q100" s="216"/>
-      <c r="R100" s="217"/>
+      <c r="P100" s="249"/>
+      <c r="Q100" s="249"/>
+      <c r="R100" s="250"/>
       <c r="AG100" s="30"/>
       <c r="AH100" s="30"/>
       <c r="AI100" s="30"/>
@@ -15632,21 +15626,21 @@
     </row>
     <row r="101" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="33"/>
-      <c r="B101" s="244" t="s">
+      <c r="B101" s="236" t="s">
         <v>16</v>
       </c>
-      <c r="C101" s="245"/>
-      <c r="D101" s="245"/>
-      <c r="E101" s="245"/>
-      <c r="F101" s="245"/>
-      <c r="G101" s="245"/>
-      <c r="H101" s="245"/>
-      <c r="I101" s="245"/>
-      <c r="J101" s="245"/>
-      <c r="K101" s="245"/>
-      <c r="L101" s="245"/>
-      <c r="M101" s="245"/>
-      <c r="N101" s="246"/>
+      <c r="C101" s="237"/>
+      <c r="D101" s="237"/>
+      <c r="E101" s="237"/>
+      <c r="F101" s="237"/>
+      <c r="G101" s="237"/>
+      <c r="H101" s="237"/>
+      <c r="I101" s="237"/>
+      <c r="J101" s="237"/>
+      <c r="K101" s="237"/>
+      <c r="L101" s="237"/>
+      <c r="M101" s="237"/>
+      <c r="N101" s="238"/>
       <c r="O101" s="21">
         <v>1</v>
       </c>
@@ -15659,45 +15653,45 @@
       <c r="R101" s="22">
         <v>4</v>
       </c>
-      <c r="U101" s="218" t="s">
+      <c r="U101" s="251" t="s">
         <v>26</v>
       </c>
-      <c r="V101" s="219"/>
-      <c r="W101" s="219"/>
-      <c r="X101" s="219"/>
-      <c r="Y101" s="219"/>
-      <c r="Z101" s="219"/>
-      <c r="AA101" s="219"/>
-      <c r="AB101" s="219"/>
-      <c r="AC101" s="219"/>
-      <c r="AD101" s="220"/>
+      <c r="V101" s="252"/>
+      <c r="W101" s="252"/>
+      <c r="X101" s="252"/>
+      <c r="Y101" s="252"/>
+      <c r="Z101" s="252"/>
+      <c r="AA101" s="252"/>
+      <c r="AB101" s="252"/>
+      <c r="AC101" s="252"/>
+      <c r="AD101" s="253"/>
       <c r="AE101" s="28"/>
       <c r="AF101" s="28"/>
-      <c r="AG101" s="221" t="s">
+      <c r="AG101" s="254" t="s">
         <v>24</v>
       </c>
-      <c r="AH101" s="222"/>
-      <c r="AI101" s="222"/>
-      <c r="AJ101" s="222"/>
-      <c r="AK101" s="223"/>
+      <c r="AH101" s="255"/>
+      <c r="AI101" s="255"/>
+      <c r="AJ101" s="255"/>
+      <c r="AK101" s="256"/>
     </row>
     <row r="102" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A102" s="34"/>
-      <c r="B102" s="251" t="s">
+      <c r="B102" s="215" t="s">
         <v>6</v>
       </c>
-      <c r="C102" s="252"/>
-      <c r="D102" s="252"/>
-      <c r="E102" s="252"/>
-      <c r="F102" s="252"/>
-      <c r="G102" s="252"/>
-      <c r="H102" s="252"/>
-      <c r="I102" s="252"/>
-      <c r="J102" s="252"/>
-      <c r="K102" s="252"/>
-      <c r="L102" s="252"/>
-      <c r="M102" s="252"/>
-      <c r="N102" s="253"/>
+      <c r="C102" s="216"/>
+      <c r="D102" s="216"/>
+      <c r="E102" s="216"/>
+      <c r="F102" s="216"/>
+      <c r="G102" s="216"/>
+      <c r="H102" s="216"/>
+      <c r="I102" s="216"/>
+      <c r="J102" s="216"/>
+      <c r="K102" s="216"/>
+      <c r="L102" s="216"/>
+      <c r="M102" s="216"/>
+      <c r="N102" s="217"/>
       <c r="O102" s="20">
         <v>5</v>
       </c>
@@ -15710,49 +15704,49 @@
       <c r="R102" s="23">
         <v>20</v>
       </c>
-      <c r="U102" s="249" t="s">
+      <c r="U102" s="241" t="s">
         <v>20</v>
       </c>
-      <c r="V102" s="250"/>
-      <c r="W102" s="250"/>
-      <c r="X102" s="250"/>
-      <c r="Y102" s="250"/>
-      <c r="Z102" s="250"/>
-      <c r="AA102" s="250"/>
-      <c r="AB102" s="247">
+      <c r="V102" s="242"/>
+      <c r="W102" s="242"/>
+      <c r="X102" s="242"/>
+      <c r="Y102" s="242"/>
+      <c r="Z102" s="242"/>
+      <c r="AA102" s="242"/>
+      <c r="AB102" s="239">
         <v>22</v>
       </c>
-      <c r="AC102" s="247"/>
-      <c r="AD102" s="248"/>
+      <c r="AC102" s="239"/>
+      <c r="AD102" s="240"/>
       <c r="AE102" s="29"/>
       <c r="AF102" s="29"/>
-      <c r="AG102" s="263" t="s">
+      <c r="AG102" s="222" t="s">
         <v>21</v>
       </c>
-      <c r="AH102" s="264"/>
-      <c r="AI102" s="264"/>
-      <c r="AJ102" s="265"/>
+      <c r="AH102" s="223"/>
+      <c r="AI102" s="223"/>
+      <c r="AJ102" s="224"/>
       <c r="AK102" s="184">
         <v>230</v>
       </c>
     </row>
     <row r="103" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="34"/>
-      <c r="B103" s="251" t="s">
+      <c r="B103" s="215" t="s">
         <v>5</v>
       </c>
-      <c r="C103" s="252"/>
-      <c r="D103" s="252"/>
-      <c r="E103" s="252"/>
-      <c r="F103" s="252"/>
-      <c r="G103" s="252"/>
-      <c r="H103" s="252"/>
-      <c r="I103" s="252"/>
-      <c r="J103" s="252"/>
-      <c r="K103" s="252"/>
-      <c r="L103" s="252"/>
-      <c r="M103" s="252"/>
-      <c r="N103" s="253"/>
+      <c r="C103" s="216"/>
+      <c r="D103" s="216"/>
+      <c r="E103" s="216"/>
+      <c r="F103" s="216"/>
+      <c r="G103" s="216"/>
+      <c r="H103" s="216"/>
+      <c r="I103" s="216"/>
+      <c r="J103" s="216"/>
+      <c r="K103" s="216"/>
+      <c r="L103" s="216"/>
+      <c r="M103" s="216"/>
+      <c r="N103" s="217"/>
       <c r="O103" s="20">
         <v>2</v>
       </c>
@@ -15765,49 +15759,49 @@
       <c r="R103" s="23">
         <v>8</v>
       </c>
-      <c r="U103" s="258" t="s">
+      <c r="U103" s="220" t="s">
         <v>18</v>
       </c>
-      <c r="V103" s="259"/>
-      <c r="W103" s="259"/>
-      <c r="X103" s="259"/>
-      <c r="Y103" s="259"/>
-      <c r="Z103" s="259"/>
-      <c r="AA103" s="259"/>
-      <c r="AB103" s="260">
+      <c r="V103" s="221"/>
+      <c r="W103" s="221"/>
+      <c r="X103" s="221"/>
+      <c r="Y103" s="221"/>
+      <c r="Z103" s="221"/>
+      <c r="AA103" s="221"/>
+      <c r="AB103" s="246">
         <v>20</v>
       </c>
-      <c r="AC103" s="260"/>
-      <c r="AD103" s="261"/>
+      <c r="AC103" s="246"/>
+      <c r="AD103" s="247"/>
       <c r="AE103" s="29"/>
       <c r="AF103" s="29"/>
-      <c r="AG103" s="266" t="s">
+      <c r="AG103" s="225" t="s">
         <v>22</v>
       </c>
-      <c r="AH103" s="252"/>
-      <c r="AI103" s="252"/>
-      <c r="AJ103" s="253"/>
+      <c r="AH103" s="216"/>
+      <c r="AI103" s="216"/>
+      <c r="AJ103" s="217"/>
       <c r="AK103" s="36">
         <v>115</v>
       </c>
     </row>
     <row r="104" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="35"/>
-      <c r="B104" s="237" t="s">
+      <c r="B104" s="229" t="s">
         <v>4</v>
       </c>
-      <c r="C104" s="238"/>
-      <c r="D104" s="238"/>
-      <c r="E104" s="238"/>
-      <c r="F104" s="238"/>
-      <c r="G104" s="238"/>
-      <c r="H104" s="238"/>
-      <c r="I104" s="238"/>
-      <c r="J104" s="238"/>
-      <c r="K104" s="238"/>
-      <c r="L104" s="238"/>
-      <c r="M104" s="238"/>
-      <c r="N104" s="239"/>
+      <c r="C104" s="230"/>
+      <c r="D104" s="230"/>
+      <c r="E104" s="230"/>
+      <c r="F104" s="230"/>
+      <c r="G104" s="230"/>
+      <c r="H104" s="230"/>
+      <c r="I104" s="230"/>
+      <c r="J104" s="230"/>
+      <c r="K104" s="230"/>
+      <c r="L104" s="230"/>
+      <c r="M104" s="230"/>
+      <c r="N104" s="231"/>
       <c r="O104" s="3">
         <v>1</v>
       </c>
@@ -15820,51 +15814,51 @@
       <c r="R104" s="24">
         <v>1</v>
       </c>
-      <c r="U104" s="254" t="s">
+      <c r="U104" s="243" t="s">
         <v>19</v>
       </c>
-      <c r="V104" s="255"/>
-      <c r="W104" s="255"/>
-      <c r="X104" s="255"/>
-      <c r="Y104" s="255"/>
-      <c r="Z104" s="255"/>
-      <c r="AA104" s="255"/>
-      <c r="AB104" s="256">
+      <c r="V104" s="219"/>
+      <c r="W104" s="219"/>
+      <c r="X104" s="219"/>
+      <c r="Y104" s="219"/>
+      <c r="Z104" s="219"/>
+      <c r="AA104" s="219"/>
+      <c r="AB104" s="244">
         <f>AB102*AB103</f>
         <v>440</v>
       </c>
-      <c r="AC104" s="256"/>
-      <c r="AD104" s="257"/>
+      <c r="AC104" s="244"/>
+      <c r="AD104" s="245"/>
       <c r="AE104" s="29"/>
       <c r="AF104" s="29"/>
-      <c r="AG104" s="266" t="s">
+      <c r="AG104" s="225" t="s">
         <v>25</v>
       </c>
-      <c r="AH104" s="252"/>
-      <c r="AI104" s="252"/>
-      <c r="AJ104" s="253"/>
+      <c r="AH104" s="216"/>
+      <c r="AI104" s="216"/>
+      <c r="AJ104" s="217"/>
       <c r="AK104" s="36">
         <v>65</v>
       </c>
     </row>
     <row r="105" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG105" s="258" t="s">
+      <c r="AG105" s="220" t="s">
         <v>23</v>
       </c>
-      <c r="AH105" s="259"/>
-      <c r="AI105" s="259"/>
-      <c r="AJ105" s="259"/>
+      <c r="AH105" s="221"/>
+      <c r="AI105" s="221"/>
+      <c r="AJ105" s="221"/>
       <c r="AK105" s="186">
         <v>30</v>
       </c>
     </row>
     <row r="106" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG106" s="262" t="s">
+      <c r="AG106" s="218" t="s">
         <v>19</v>
       </c>
-      <c r="AH106" s="255"/>
-      <c r="AI106" s="255"/>
-      <c r="AJ106" s="255"/>
+      <c r="AH106" s="219"/>
+      <c r="AI106" s="219"/>
+      <c r="AJ106" s="219"/>
       <c r="AK106" s="185">
         <f>SUM(AK102:AK105)</f>
         <v>440</v>
@@ -15876,12 +15870,22 @@
     <sortCondition ref="B10:B94"/>
   </sortState>
   <mergeCells count="38">
-    <mergeCell ref="B103:N103"/>
-    <mergeCell ref="AG106:AJ106"/>
-    <mergeCell ref="AG105:AJ105"/>
-    <mergeCell ref="AG102:AJ102"/>
-    <mergeCell ref="AG104:AJ104"/>
-    <mergeCell ref="AG103:AJ103"/>
+    <mergeCell ref="O100:R100"/>
+    <mergeCell ref="U101:AD101"/>
+    <mergeCell ref="AG101:AK101"/>
+    <mergeCell ref="AH4:AJ4"/>
+    <mergeCell ref="AG5:AG9"/>
+    <mergeCell ref="AJ5:AJ9"/>
+    <mergeCell ref="X5:AA5"/>
+    <mergeCell ref="AB5:AB9"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="C4:S4"/>
+    <mergeCell ref="T4:AB4"/>
+    <mergeCell ref="AC4:AG4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="K5:R5"/>
+    <mergeCell ref="S5:S9"/>
     <mergeCell ref="T5:W5"/>
     <mergeCell ref="B104:N104"/>
     <mergeCell ref="C1:O1"/>
@@ -15898,22 +15902,12 @@
     <mergeCell ref="AB104:AD104"/>
     <mergeCell ref="U103:AA103"/>
     <mergeCell ref="AB103:AD103"/>
-    <mergeCell ref="O100:R100"/>
-    <mergeCell ref="U101:AD101"/>
-    <mergeCell ref="AG101:AK101"/>
-    <mergeCell ref="AH4:AJ4"/>
-    <mergeCell ref="AG5:AG9"/>
-    <mergeCell ref="AJ5:AJ9"/>
-    <mergeCell ref="X5:AA5"/>
-    <mergeCell ref="AB5:AB9"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="C4:S4"/>
-    <mergeCell ref="T4:AB4"/>
-    <mergeCell ref="AC4:AG4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="K5:R5"/>
-    <mergeCell ref="S5:S9"/>
+    <mergeCell ref="B103:N103"/>
+    <mergeCell ref="AG106:AJ106"/>
+    <mergeCell ref="AG105:AJ105"/>
+    <mergeCell ref="AG102:AJ102"/>
+    <mergeCell ref="AG104:AJ104"/>
+    <mergeCell ref="AG103:AJ103"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <conditionalFormatting sqref="AH18:AI18 AH10:AI10 AH14:AI14 T10:AA10 AC10:AF10 C10:R10 C14:R14 T14:AA14 AC14:AF14 T18:AA18 AC18:AF18 AH30:AI30 C30:R30 T30:AA30 AC30:AF30 AH26:AI26 C26:R26 T26:AA26 AC26:AF26 AH62:AI62 C62:R62 T62:AA62 AC62:AF62 AH42:AI42 C42:R42 T42:AA42 AC42:AF42 AH22:AI22 C22:R22 T22:AA22 AC22:AF22 AH38:AI38 C38:R38 T38:AA38 AC38:AF38 AH34:AI34 C34:R34 T34:AA34 AC34:AF34 AH66:AI66 C66:R66 T66:AA66 AC66:AF66 C18:R18">
@@ -16670,7 +16664,7 @@
   <dimension ref="A1:AJ31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16895,13 +16889,15 @@
       <c r="Q6" s="81">
         <v>1</v>
       </c>
-      <c r="R6" s="81"/>
+      <c r="R6" s="81">
+        <v>4</v>
+      </c>
       <c r="S6" s="81"/>
       <c r="T6" s="81"/>
       <c r="U6" s="81"/>
       <c r="V6" s="73">
         <f>IF(O6&gt;O7,1,0)+IF(P6&gt;P7,1,0)+IF(Q6&gt;Q7,1,0)+IF(R6&gt;R7,1,0)+IF(S6&gt;S7,1,0)+IF(T6&gt;T7,1,0)+IF(U6&gt;U7,1,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W6" s="13"/>
       <c r="Y6" s="86"/>
@@ -16963,7 +16959,9 @@
       <c r="Q7" s="81">
         <v>2</v>
       </c>
-      <c r="R7" s="81"/>
+      <c r="R7" s="81">
+        <v>1</v>
+      </c>
       <c r="S7" s="81"/>
       <c r="T7" s="81"/>
       <c r="U7" s="81"/>
@@ -17606,7 +17604,9 @@
       <c r="Q20" s="81">
         <v>4</v>
       </c>
-      <c r="R20" s="81"/>
+      <c r="R20" s="81">
+        <v>0</v>
+      </c>
       <c r="S20" s="81"/>
       <c r="T20" s="81"/>
       <c r="U20" s="81"/>
@@ -17674,13 +17674,15 @@
       <c r="Q21" s="81">
         <v>2</v>
       </c>
-      <c r="R21" s="81"/>
+      <c r="R21" s="81">
+        <v>3</v>
+      </c>
       <c r="S21" s="81"/>
       <c r="T21" s="81"/>
       <c r="U21" s="81"/>
       <c r="V21" s="73">
         <f>IF(O21&gt;O20,1,0)+IF(P21&gt;P20,1,0)+IF(Q21&gt;Q20,1,0)+IF(R21&gt;R20,1,0)+IF(S21&gt;S20,1,0)+IF(T21&gt;T20,1,0)+IF(U21&gt;U20,1,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W21" s="14"/>
       <c r="X21" s="4"/>

</xml_diff>

<commit_message>
Updated games of 2019-05-03
</commit_message>
<xml_diff>
--- a/laval.xlsx
+++ b/laval.xlsx
@@ -1934,7 +1934,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="314">
+  <cellXfs count="312">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2478,25 +2478,121 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="92" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="82" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="83" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="85" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2550,133 +2646,31 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="83" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="85" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="92" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="82" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2687,7 +2681,615 @@
     <cellStyle name="Monétaire" xfId="4" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="101">
+  <dxfs count="159">
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2869,13 +3471,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color theme="1"/>
       </font>
@@ -2892,33 +3487,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2983,16 +3551,22 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor indexed="13"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor indexed="13"/>
+          <bgColor rgb="FF00FFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3901,217 +4475,217 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="C1" s="279"/>
-      <c r="D1" s="279"/>
-      <c r="E1" s="279"/>
-      <c r="F1" s="279"/>
-      <c r="G1" s="279"/>
-      <c r="H1" s="279"/>
-      <c r="I1" s="279"/>
-      <c r="J1" s="279"/>
-      <c r="K1" s="279"/>
-      <c r="L1" s="279"/>
-      <c r="M1" s="279"/>
-      <c r="N1" s="279"/>
-      <c r="O1" s="279"/>
-      <c r="P1" s="280"/>
-      <c r="Q1" s="280"/>
-      <c r="R1" s="280"/>
-      <c r="S1" s="280"/>
-      <c r="T1" s="280"/>
-      <c r="U1" s="280"/>
-      <c r="V1" s="280"/>
-      <c r="W1" s="280"/>
-      <c r="X1" s="280"/>
-      <c r="Y1" s="280"/>
-      <c r="Z1" s="280"/>
-      <c r="AA1" s="280"/>
-      <c r="AB1" s="280"/>
-      <c r="AC1" s="280"/>
-      <c r="AD1" s="280"/>
-      <c r="AE1" s="280"/>
-      <c r="AF1" s="280"/>
-      <c r="AG1" s="280"/>
-      <c r="AH1" s="280"/>
-      <c r="AI1" s="280"/>
-      <c r="AJ1" s="280"/>
+      <c r="C1" s="270"/>
+      <c r="D1" s="270"/>
+      <c r="E1" s="270"/>
+      <c r="F1" s="270"/>
+      <c r="G1" s="270"/>
+      <c r="H1" s="270"/>
+      <c r="I1" s="270"/>
+      <c r="J1" s="270"/>
+      <c r="K1" s="270"/>
+      <c r="L1" s="270"/>
+      <c r="M1" s="270"/>
+      <c r="N1" s="270"/>
+      <c r="O1" s="270"/>
+      <c r="P1" s="271"/>
+      <c r="Q1" s="271"/>
+      <c r="R1" s="271"/>
+      <c r="S1" s="271"/>
+      <c r="T1" s="271"/>
+      <c r="U1" s="271"/>
+      <c r="V1" s="271"/>
+      <c r="W1" s="271"/>
+      <c r="X1" s="271"/>
+      <c r="Y1" s="271"/>
+      <c r="Z1" s="271"/>
+      <c r="AA1" s="271"/>
+      <c r="AB1" s="271"/>
+      <c r="AC1" s="271"/>
+      <c r="AD1" s="271"/>
+      <c r="AE1" s="271"/>
+      <c r="AF1" s="271"/>
+      <c r="AG1" s="271"/>
+      <c r="AH1" s="271"/>
+      <c r="AI1" s="271"/>
+      <c r="AJ1" s="271"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="41"/>
-      <c r="C2" s="281" t="s">
+      <c r="C2" s="272" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="281"/>
-      <c r="E2" s="281"/>
-      <c r="F2" s="281"/>
-      <c r="G2" s="281"/>
-      <c r="H2" s="281"/>
-      <c r="I2" s="281"/>
-      <c r="J2" s="281"/>
-      <c r="K2" s="281"/>
-      <c r="L2" s="281"/>
-      <c r="M2" s="281"/>
-      <c r="N2" s="281"/>
-      <c r="O2" s="281"/>
-      <c r="P2" s="281"/>
-      <c r="Q2" s="282" t="s">
+      <c r="D2" s="272"/>
+      <c r="E2" s="272"/>
+      <c r="F2" s="272"/>
+      <c r="G2" s="272"/>
+      <c r="H2" s="272"/>
+      <c r="I2" s="272"/>
+      <c r="J2" s="272"/>
+      <c r="K2" s="272"/>
+      <c r="L2" s="272"/>
+      <c r="M2" s="272"/>
+      <c r="N2" s="272"/>
+      <c r="O2" s="272"/>
+      <c r="P2" s="272"/>
+      <c r="Q2" s="273" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="280"/>
-      <c r="S2" s="280"/>
-      <c r="T2" s="280"/>
-      <c r="U2" s="280"/>
-      <c r="V2" s="280"/>
-      <c r="W2" s="280"/>
-      <c r="X2" s="280"/>
-      <c r="Y2" s="280"/>
-      <c r="Z2" s="280"/>
-      <c r="AA2" s="280"/>
-      <c r="AB2" s="280"/>
-      <c r="AC2" s="280"/>
-      <c r="AD2" s="280"/>
-      <c r="AE2" s="280"/>
-      <c r="AF2" s="280"/>
-      <c r="AG2" s="280"/>
-      <c r="AH2" s="280"/>
-      <c r="AI2" s="280"/>
-      <c r="AJ2" s="280"/>
+      <c r="R2" s="271"/>
+      <c r="S2" s="271"/>
+      <c r="T2" s="271"/>
+      <c r="U2" s="271"/>
+      <c r="V2" s="271"/>
+      <c r="W2" s="271"/>
+      <c r="X2" s="271"/>
+      <c r="Y2" s="271"/>
+      <c r="Z2" s="271"/>
+      <c r="AA2" s="271"/>
+      <c r="AB2" s="271"/>
+      <c r="AC2" s="271"/>
+      <c r="AD2" s="271"/>
+      <c r="AE2" s="271"/>
+      <c r="AF2" s="271"/>
+      <c r="AG2" s="271"/>
+      <c r="AH2" s="271"/>
+      <c r="AI2" s="271"/>
+      <c r="AJ2" s="271"/>
     </row>
     <row r="3" spans="1:38" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="279"/>
-      <c r="D3" s="279"/>
-      <c r="E3" s="279"/>
-      <c r="F3" s="279"/>
-      <c r="G3" s="279"/>
-      <c r="H3" s="279"/>
-      <c r="I3" s="279"/>
-      <c r="J3" s="279"/>
-      <c r="K3" s="279"/>
-      <c r="L3" s="279"/>
-      <c r="M3" s="279"/>
-      <c r="N3" s="279"/>
-      <c r="O3" s="279"/>
-      <c r="P3" s="280"/>
-      <c r="Q3" s="280"/>
-      <c r="R3" s="280"/>
-      <c r="S3" s="280"/>
-      <c r="T3" s="280"/>
-      <c r="U3" s="280"/>
-      <c r="V3" s="280"/>
-      <c r="W3" s="280"/>
-      <c r="X3" s="280"/>
-      <c r="Y3" s="280"/>
-      <c r="Z3" s="280"/>
-      <c r="AA3" s="280"/>
-      <c r="AB3" s="280"/>
-      <c r="AC3" s="280"/>
-      <c r="AD3" s="280"/>
-      <c r="AE3" s="280"/>
-      <c r="AF3" s="280"/>
-      <c r="AG3" s="280"/>
-      <c r="AH3" s="280"/>
-      <c r="AI3" s="280"/>
-      <c r="AJ3" s="280"/>
+      <c r="C3" s="270"/>
+      <c r="D3" s="270"/>
+      <c r="E3" s="270"/>
+      <c r="F3" s="270"/>
+      <c r="G3" s="270"/>
+      <c r="H3" s="270"/>
+      <c r="I3" s="270"/>
+      <c r="J3" s="270"/>
+      <c r="K3" s="270"/>
+      <c r="L3" s="270"/>
+      <c r="M3" s="270"/>
+      <c r="N3" s="270"/>
+      <c r="O3" s="270"/>
+      <c r="P3" s="271"/>
+      <c r="Q3" s="271"/>
+      <c r="R3" s="271"/>
+      <c r="S3" s="271"/>
+      <c r="T3" s="271"/>
+      <c r="U3" s="271"/>
+      <c r="V3" s="271"/>
+      <c r="W3" s="271"/>
+      <c r="X3" s="271"/>
+      <c r="Y3" s="271"/>
+      <c r="Z3" s="271"/>
+      <c r="AA3" s="271"/>
+      <c r="AB3" s="271"/>
+      <c r="AC3" s="271"/>
+      <c r="AD3" s="271"/>
+      <c r="AE3" s="271"/>
+      <c r="AF3" s="271"/>
+      <c r="AG3" s="271"/>
+      <c r="AH3" s="271"/>
+      <c r="AI3" s="271"/>
+      <c r="AJ3" s="271"/>
     </row>
     <row r="4" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="263" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="264"/>
-      <c r="E4" s="264"/>
-      <c r="F4" s="264"/>
-      <c r="G4" s="264"/>
-      <c r="H4" s="264"/>
-      <c r="I4" s="264"/>
-      <c r="J4" s="264"/>
-      <c r="K4" s="264"/>
-      <c r="L4" s="264"/>
-      <c r="M4" s="264"/>
-      <c r="N4" s="264"/>
-      <c r="O4" s="264"/>
-      <c r="P4" s="264"/>
-      <c r="Q4" s="264"/>
-      <c r="R4" s="264"/>
-      <c r="S4" s="265"/>
-      <c r="T4" s="263" t="s">
+      <c r="C4" s="295" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="296"/>
+      <c r="E4" s="296"/>
+      <c r="F4" s="296"/>
+      <c r="G4" s="296"/>
+      <c r="H4" s="296"/>
+      <c r="I4" s="296"/>
+      <c r="J4" s="296"/>
+      <c r="K4" s="296"/>
+      <c r="L4" s="296"/>
+      <c r="M4" s="296"/>
+      <c r="N4" s="296"/>
+      <c r="O4" s="296"/>
+      <c r="P4" s="296"/>
+      <c r="Q4" s="296"/>
+      <c r="R4" s="296"/>
+      <c r="S4" s="297"/>
+      <c r="T4" s="295" t="s">
         <v>1</v>
       </c>
-      <c r="U4" s="264"/>
-      <c r="V4" s="264"/>
-      <c r="W4" s="264"/>
-      <c r="X4" s="264"/>
-      <c r="Y4" s="264"/>
-      <c r="Z4" s="264"/>
-      <c r="AA4" s="264"/>
-      <c r="AB4" s="265"/>
-      <c r="AC4" s="263" t="s">
+      <c r="U4" s="296"/>
+      <c r="V4" s="296"/>
+      <c r="W4" s="296"/>
+      <c r="X4" s="296"/>
+      <c r="Y4" s="296"/>
+      <c r="Z4" s="296"/>
+      <c r="AA4" s="296"/>
+      <c r="AB4" s="297"/>
+      <c r="AC4" s="295" t="s">
         <v>2</v>
       </c>
-      <c r="AD4" s="264"/>
-      <c r="AE4" s="264"/>
-      <c r="AF4" s="264"/>
-      <c r="AG4" s="274"/>
-      <c r="AH4" s="263" t="s">
+      <c r="AD4" s="296"/>
+      <c r="AE4" s="296"/>
+      <c r="AF4" s="296"/>
+      <c r="AG4" s="304"/>
+      <c r="AH4" s="295" t="s">
         <v>10</v>
       </c>
-      <c r="AI4" s="264"/>
-      <c r="AJ4" s="265"/>
+      <c r="AI4" s="296"/>
+      <c r="AJ4" s="297"/>
     </row>
     <row r="5" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="275" t="s">
+      <c r="C5" s="264" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="271"/>
-      <c r="E5" s="271"/>
-      <c r="F5" s="271"/>
-      <c r="G5" s="271"/>
-      <c r="H5" s="271"/>
-      <c r="I5" s="271"/>
-      <c r="J5" s="272"/>
-      <c r="K5" s="270" t="s">
+      <c r="D5" s="265"/>
+      <c r="E5" s="265"/>
+      <c r="F5" s="265"/>
+      <c r="G5" s="265"/>
+      <c r="H5" s="265"/>
+      <c r="I5" s="265"/>
+      <c r="J5" s="266"/>
+      <c r="K5" s="302" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="271"/>
-      <c r="M5" s="271"/>
-      <c r="N5" s="271"/>
-      <c r="O5" s="271"/>
-      <c r="P5" s="271"/>
-      <c r="Q5" s="271"/>
-      <c r="R5" s="272"/>
-      <c r="S5" s="266" t="s">
+      <c r="L5" s="265"/>
+      <c r="M5" s="265"/>
+      <c r="N5" s="265"/>
+      <c r="O5" s="265"/>
+      <c r="P5" s="265"/>
+      <c r="Q5" s="265"/>
+      <c r="R5" s="266"/>
+      <c r="S5" s="298" t="s">
         <v>12</v>
       </c>
-      <c r="T5" s="275" t="s">
+      <c r="T5" s="264" t="s">
         <v>9</v>
       </c>
-      <c r="U5" s="271"/>
-      <c r="V5" s="271"/>
-      <c r="W5" s="272"/>
-      <c r="X5" s="270" t="s">
+      <c r="U5" s="265"/>
+      <c r="V5" s="265"/>
+      <c r="W5" s="266"/>
+      <c r="X5" s="302" t="s">
         <v>8</v>
       </c>
-      <c r="Y5" s="271"/>
-      <c r="Z5" s="271"/>
-      <c r="AA5" s="272"/>
-      <c r="AB5" s="266" t="s">
+      <c r="Y5" s="265"/>
+      <c r="Z5" s="265"/>
+      <c r="AA5" s="266"/>
+      <c r="AB5" s="298" t="s">
         <v>13</v>
       </c>
-      <c r="AC5" s="273" t="s">
+      <c r="AC5" s="303" t="s">
         <v>9</v>
       </c>
-      <c r="AD5" s="272"/>
-      <c r="AE5" s="270" t="s">
+      <c r="AD5" s="266"/>
+      <c r="AE5" s="302" t="s">
         <v>8</v>
       </c>
-      <c r="AF5" s="272"/>
-      <c r="AG5" s="266" t="s">
+      <c r="AF5" s="266"/>
+      <c r="AG5" s="298" t="s">
         <v>14</v>
       </c>
       <c r="AH5" s="56"/>
       <c r="AI5" s="25"/>
-      <c r="AJ5" s="266" t="s">
+      <c r="AJ5" s="298" t="s">
         <v>15</v>
       </c>
       <c r="AK5" s="4"/>
@@ -4183,7 +4757,7 @@
         <f>Résultats!$J$28</f>
         <v>3</v>
       </c>
-      <c r="S6" s="267"/>
+      <c r="S6" s="299"/>
       <c r="T6" s="156">
         <f>Résultats!$V$6</f>
         <v>2</v>
@@ -4214,9 +4788,9 @@
       </c>
       <c r="AA6" s="103">
         <f>Résultats!$V$25</f>
-        <v>2</v>
-      </c>
-      <c r="AB6" s="267"/>
+        <v>3</v>
+      </c>
+      <c r="AB6" s="299"/>
       <c r="AC6" s="106">
         <f>Résultats!$AH$8</f>
         <v>0</v>
@@ -4233,7 +4807,7 @@
         <f>Résultats!$AH$23</f>
         <v>0</v>
       </c>
-      <c r="AG6" s="267"/>
+      <c r="AG6" s="299"/>
       <c r="AH6" s="173">
         <f>Résultats!$AH$15</f>
         <v>0</v>
@@ -4242,7 +4816,7 @@
         <f>Résultats!$AH$16</f>
         <v>0</v>
       </c>
-      <c r="AJ6" s="267"/>
+      <c r="AJ6" s="299"/>
       <c r="AK6" s="37"/>
     </row>
     <row r="7" spans="1:38" s="39" customFormat="1" ht="58.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -4268,7 +4842,7 @@
       <c r="P7" s="203"/>
       <c r="Q7" s="207"/>
       <c r="R7" s="112"/>
-      <c r="S7" s="267"/>
+      <c r="S7" s="299"/>
       <c r="T7" s="157"/>
       <c r="U7" s="112"/>
       <c r="V7" s="160"/>
@@ -4277,15 +4851,15 @@
       <c r="Y7" s="113"/>
       <c r="Z7" s="114"/>
       <c r="AA7" s="112"/>
-      <c r="AB7" s="267"/>
+      <c r="AB7" s="299"/>
       <c r="AC7" s="114"/>
       <c r="AD7" s="112"/>
       <c r="AE7" s="115"/>
       <c r="AF7" s="112"/>
-      <c r="AG7" s="267"/>
+      <c r="AG7" s="299"/>
       <c r="AH7" s="173"/>
       <c r="AI7" s="107"/>
-      <c r="AJ7" s="267"/>
+      <c r="AJ7" s="299"/>
       <c r="AK7" s="37"/>
     </row>
     <row r="8" spans="1:38" s="39" customFormat="1" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4355,7 +4929,7 @@
         <f>Résultats!$B$28</f>
         <v>VEGAS</v>
       </c>
-      <c r="S8" s="267"/>
+      <c r="S8" s="299"/>
       <c r="T8" s="158" t="str">
         <f>Résultats!$N$6</f>
         <v>BOSTON</v>
@@ -4388,7 +4962,7 @@
         <f>Résultats!$N$25</f>
         <v>DALLAS</v>
       </c>
-      <c r="AB8" s="267"/>
+      <c r="AB8" s="299"/>
       <c r="AC8" s="164" t="str">
         <f>Résultats!$Z$8</f>
         <v xml:space="preserve"> </v>
@@ -4405,7 +4979,7 @@
         <f>Résultats!$Z$23</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AG8" s="267"/>
+      <c r="AG8" s="299"/>
       <c r="AH8" s="174" t="str">
         <f>Résultats!$Z$15</f>
         <v xml:space="preserve"> </v>
@@ -4414,7 +4988,7 @@
         <f>Résultats!$Z$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ8" s="267"/>
+      <c r="AJ8" s="299"/>
       <c r="AK8" s="37"/>
     </row>
     <row r="9" spans="1:38" s="39" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4488,7 +5062,7 @@
         <f>Résultats!$A$28</f>
         <v>P3</v>
       </c>
-      <c r="S9" s="269"/>
+      <c r="S9" s="301"/>
       <c r="T9" s="166" t="str">
         <f>Résultats!$M$6</f>
         <v>A2</v>
@@ -4521,7 +5095,7 @@
         <f>Résultats!$M$25</f>
         <v>WC1</v>
       </c>
-      <c r="AB9" s="268"/>
+      <c r="AB9" s="300"/>
       <c r="AC9" s="170" t="str">
         <f>Résultats!$Y$8</f>
         <v xml:space="preserve"> </v>
@@ -4538,7 +5112,7 @@
         <f>Résultats!$Y$23</f>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="AG9" s="268"/>
+      <c r="AG9" s="300"/>
       <c r="AH9" s="176" t="str">
         <f>Résultats!$Y$15</f>
         <v xml:space="preserve"> </v>
@@ -4547,7 +5121,7 @@
         <f>Résultats!$Y$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ9" s="269"/>
+      <c r="AJ9" s="301"/>
       <c r="AK9" s="109" t="s">
         <v>51</v>
       </c>
@@ -4567,7 +5141,7 @@
         <v>5</v>
       </c>
       <c r="D10" s="219"/>
-      <c r="E10" s="306">
+      <c r="E10" s="247">
         <v>7</v>
       </c>
       <c r="F10" s="219"/>
@@ -4584,7 +5158,7 @@
       </c>
       <c r="L10" s="222"/>
       <c r="M10" s="220"/>
-      <c r="N10" s="307">
+      <c r="N10" s="248">
         <v>6</v>
       </c>
       <c r="O10" s="220">
@@ -4617,7 +5191,7 @@
       </c>
       <c r="AB10" s="225">
         <f>SUM(T11:AA11)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AC10" s="221"/>
       <c r="AD10" s="222"/>
@@ -4627,7 +5201,7 @@
         <f>SUM(AC11:AF11)</f>
         <v>0</v>
       </c>
-      <c r="AH10" s="309"/>
+      <c r="AH10" s="250"/>
       <c r="AI10" s="227"/>
       <c r="AJ10" s="225">
         <f>AH11</f>
@@ -4639,7 +5213,7 @@
       </c>
       <c r="AL10" s="225">
         <f>$S10+$AB10+$AG10+$AJ10</f>
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -4706,7 +5280,7 @@
       <c r="Y11" s="59"/>
       <c r="Z11" s="126">
         <f>(IF($Z10&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z10=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA10&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA10=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA11" s="62"/>
       <c r="AB11" s="121"/>
@@ -5131,7 +5705,7 @@
       </c>
       <c r="AK14" s="111">
         <f>MAX($AL$10:$AL$97) - AL14</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL14" s="122">
         <f>$S14+$AB14+$AG14+$AJ14</f>
@@ -5216,7 +5790,7 @@
       <c r="AJ15" s="121"/>
       <c r="AK15" s="92">
         <f>MAX($AL$10:$AL$97) - AL15</f>
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AL15" s="121"/>
     </row>
@@ -5622,7 +6196,7 @@
         <f>SUM(AC19:AF19)</f>
         <v>0</v>
       </c>
-      <c r="AH18" s="310"/>
+      <c r="AH18" s="251"/>
       <c r="AI18" s="240"/>
       <c r="AJ18" s="239">
         <f>AH19</f>
@@ -5630,7 +6204,7 @@
       </c>
       <c r="AK18" s="241">
         <f>MAX($AL$10:$AL$97) - AL18</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AL18" s="239">
         <f>$S18+$AB18+$AG18+$AJ18</f>
@@ -5715,7 +6289,7 @@
       <c r="AJ19" s="144"/>
       <c r="AK19" s="150">
         <f>MAX($AL$10:$AL$97) - AL19</f>
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AL19" s="121"/>
     </row>
@@ -6055,43 +6629,43 @@
         <v>4</v>
       </c>
       <c r="B22" s="84" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C22" s="46">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D22" s="45"/>
       <c r="E22" s="44">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F22" s="45"/>
-      <c r="G22" s="48">
+      <c r="G22" s="48"/>
+      <c r="H22" s="215">
+        <v>7</v>
+      </c>
+      <c r="I22" s="44"/>
+      <c r="J22" s="47">
         <v>6</v>
       </c>
-      <c r="H22" s="47"/>
-      <c r="I22" s="44">
-        <v>7</v>
-      </c>
-      <c r="J22" s="47"/>
       <c r="K22" s="49">
         <v>5</v>
       </c>
       <c r="L22" s="47"/>
       <c r="M22" s="44"/>
-      <c r="N22" s="45">
-        <v>7</v>
+      <c r="N22" s="211">
+        <v>6</v>
       </c>
       <c r="O22" s="44">
         <v>6</v>
       </c>
       <c r="P22" s="45"/>
-      <c r="Q22" s="213">
-        <v>7</v>
+      <c r="Q22" s="48">
+        <v>6</v>
       </c>
       <c r="R22" s="50"/>
       <c r="S22" s="122">
         <f>SUM(C23:R23)</f>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T22" s="46"/>
       <c r="U22" s="47">
@@ -6101,17 +6675,17 @@
         <v>6</v>
       </c>
       <c r="W22" s="47"/>
-      <c r="X22" s="49"/>
-      <c r="Y22" s="45">
-        <v>6</v>
-      </c>
-      <c r="Z22" s="48">
-        <v>6</v>
-      </c>
-      <c r="AA22" s="50"/>
+      <c r="X22" s="49">
+        <v>5</v>
+      </c>
+      <c r="Y22" s="45"/>
+      <c r="Z22" s="48"/>
+      <c r="AA22" s="50">
+        <v>7</v>
+      </c>
       <c r="AB22" s="122">
         <f>SUM(T23:AA23)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AC22" s="48"/>
       <c r="AD22" s="47"/>
@@ -6129,7 +6703,7 @@
       </c>
       <c r="AK22" s="111">
         <f>MAX($AL$10:$AL$97) - AL22</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AL22" s="122">
         <f>$S22+$AB22+$AG22+$AJ22</f>
@@ -6154,12 +6728,12 @@
       <c r="F23" s="151"/>
       <c r="G23" s="125">
         <f>(IF($G22&lt;&gt;"",($G$6*$O$104)+IF($G$6=4,($O$102)+IF($G22=$G$6+$H$6,$O$103,0),0),0)+IF($H22&lt;&gt;"",($H$6*$O$104)+IF($H$6=4,($O$102)+IF($H22=$G$6+$H$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="H23" s="151"/>
       <c r="I23" s="125">
         <f>(IF($I22&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I22=$I$6+$J$6,$O$103,0),0),0)+IF($J22&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J22=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J23" s="152"/>
       <c r="K23" s="153">
@@ -6169,7 +6743,7 @@
       <c r="L23" s="151"/>
       <c r="M23" s="125">
         <f>(IF($M22&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M22=$M$6+$N$6,$O$103,0),0),0)+IF($N22&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N22=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="N23" s="151"/>
       <c r="O23" s="125">
@@ -6179,7 +6753,7 @@
       <c r="P23" s="151"/>
       <c r="Q23" s="125">
         <f>(IF($Q22&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q22=$Q$6+$R$6,$O$103,0),0),0)+IF($R22&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R22=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="R23" s="154"/>
       <c r="S23" s="144"/>
@@ -6200,7 +6774,7 @@
       <c r="Y23" s="59"/>
       <c r="Z23" s="126">
         <f>(IF($Z22&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z22=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA22&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA22=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA23" s="62"/>
       <c r="AB23" s="144"/>
@@ -6214,7 +6788,7 @@
       <c r="AJ23" s="144"/>
       <c r="AK23" s="150">
         <f>MAX($AL$10:$AL$97) - AL23</f>
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AL23" s="121"/>
     </row>
@@ -6257,13 +6831,13 @@
         <f>IF(ISBLANK(H22),
 0,
 IF(H$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" s="118">
         <f>IF(ISBLANK(I22),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" s="118">
         <f>IF(ISBLANK(J22),
@@ -6422,7 +6996,7 @@
         <f>IF(H24 = 0,
 0,
 IF(H22 = (G$6+H$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25" s="118">
         <f>IF(I24 = 0,
@@ -6458,7 +7032,7 @@
         <f>IF(N24 = 0,
 0,
 IF(N22 = (M$6+N$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O25" s="118">
         <f>IF(O24 = 0,
@@ -6476,7 +7050,7 @@
         <f>IF(Q24 = 0,
 0,
 IF(Q22 = (Q$6+R$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R25" s="118">
         <f>IF(R24 = 0,
@@ -6544,53 +7118,53 @@
       <c r="AJ25" s="138"/>
       <c r="AK25" s="139">
         <f>SUM(C25:AI25)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL25" s="123"/>
     </row>
     <row r="26" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="216">
         <f>RANK(AL26,$AL$10:$AL$97,)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B26" s="217" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C26" s="229">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D26" s="230"/>
       <c r="E26" s="234">
+        <v>5</v>
+      </c>
+      <c r="F26" s="230"/>
+      <c r="G26" s="232">
         <v>6</v>
       </c>
-      <c r="F26" s="230"/>
-      <c r="G26" s="232"/>
-      <c r="H26" s="313">
+      <c r="H26" s="233"/>
+      <c r="I26" s="234">
         <v>7</v>
       </c>
-      <c r="I26" s="234"/>
-      <c r="J26" s="233">
-        <v>6</v>
-      </c>
+      <c r="J26" s="233"/>
       <c r="K26" s="235">
         <v>5</v>
       </c>
       <c r="L26" s="233"/>
       <c r="M26" s="234"/>
-      <c r="N26" s="236">
-        <v>6</v>
+      <c r="N26" s="230">
+        <v>7</v>
       </c>
       <c r="O26" s="234">
         <v>6</v>
       </c>
       <c r="P26" s="230"/>
-      <c r="Q26" s="232">
-        <v>6</v>
+      <c r="Q26" s="249">
+        <v>7</v>
       </c>
       <c r="R26" s="237"/>
       <c r="S26" s="239">
         <f>SUM(C27:R27)</f>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="T26" s="229"/>
       <c r="U26" s="233">
@@ -6600,14 +7174,14 @@
         <v>6</v>
       </c>
       <c r="W26" s="233"/>
-      <c r="X26" s="235">
-        <v>5</v>
-      </c>
-      <c r="Y26" s="230"/>
-      <c r="Z26" s="232"/>
-      <c r="AA26" s="237">
-        <v>7</v>
-      </c>
+      <c r="X26" s="235"/>
+      <c r="Y26" s="230">
+        <v>6</v>
+      </c>
+      <c r="Z26" s="232">
+        <v>6</v>
+      </c>
+      <c r="AA26" s="237"/>
       <c r="AB26" s="239">
         <f>SUM(T27:AA27)</f>
         <v>6</v>
@@ -6632,7 +7206,7 @@
       </c>
       <c r="AL26" s="239">
         <f>$S26+$AB26+$AG26+$AJ26</f>
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6653,12 +7227,12 @@
       <c r="F27" s="140"/>
       <c r="G27" s="120">
         <f>(IF($G26&lt;&gt;"",($G$6*$O$104)+IF($G$6=4,($O$102)+IF($G26=$G$6+$H$6,$O$103,0),0),0)+IF($H26&lt;&gt;"",($H$6*$O$104)+IF($H$6=4,($O$102)+IF($H26=$G$6+$H$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="H27" s="140"/>
       <c r="I27" s="120">
         <f>(IF($I26&lt;&gt;"",($I$6*$O$104)+IF($I$6=4,($O$102)+IF($I26=$I$6+$J$6,$O$103,0),0),0)+IF($J26&lt;&gt;"",($J$6*$O$104)+IF($J$6=4,($O$102)+IF($J26=$I$6+$J$6,$O$103,0),0),0))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J27" s="141"/>
       <c r="K27" s="142">
@@ -6668,7 +7242,7 @@
       <c r="L27" s="140"/>
       <c r="M27" s="120">
         <f>(IF($M26&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M26=$M$6+$N$6,$O$103,0),0),0)+IF($N26&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N26=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="N27" s="140"/>
       <c r="O27" s="120">
@@ -6678,7 +7252,7 @@
       <c r="P27" s="140"/>
       <c r="Q27" s="120">
         <f>(IF($Q26&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q26=$Q$6+$R$6,$O$103,0),0),0)+IF($R26&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R26=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="R27" s="143"/>
       <c r="S27" s="144"/>
@@ -6713,7 +7287,7 @@
       <c r="AJ27" s="144"/>
       <c r="AK27" s="150">
         <f>MAX($AL$10:$AL$97) - AL27</f>
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AL27" s="121"/>
     </row>
@@ -6756,13 +7330,13 @@
         <f>IF(ISBLANK(H26),
 0,
 IF(H$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28" s="118">
         <f>IF(ISBLANK(I26),
 0,
 IF(I$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" s="118">
         <f>IF(ISBLANK(J26),
@@ -6921,7 +7495,7 @@
         <f>IF(H28 = 0,
 0,
 IF(H26 = (G$6+H$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I29" s="118">
         <f>IF(I28 = 0,
@@ -6957,7 +7531,7 @@
         <f>IF(N28 = 0,
 0,
 IF(N26 = (M$6+N$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O29" s="118">
         <f>IF(O28 = 0,
@@ -6975,7 +7549,7 @@
         <f>IF(Q28 = 0,
 0,
 IF(Q26 = (Q$6+R$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R29" s="118">
         <f>IF(R28 = 0,
@@ -7043,7 +7617,7 @@
       <c r="AJ29" s="138"/>
       <c r="AK29" s="139">
         <f>SUM(C29:AI29)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AL29" s="123"/>
     </row>
@@ -7127,7 +7701,7 @@
       </c>
       <c r="AK30" s="111">
         <f>MAX($AL$10:$AL$97) - AL30</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AL30" s="122">
         <f>$S30+$AB30+$AG30+$AJ30</f>
@@ -7212,7 +7786,7 @@
       <c r="AJ31" s="121"/>
       <c r="AK31" s="92">
         <f>MAX($AL$10:$AL$97) - AL31</f>
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AL31" s="121"/>
     </row>
@@ -7626,7 +8200,7 @@
       </c>
       <c r="AK34" s="241">
         <f>MAX($AL$10:$AL$97) - AL34</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AL34" s="239">
         <f>$S34+$AB34+$AG34+$AJ34</f>
@@ -7711,7 +8285,7 @@
       <c r="AJ35" s="121"/>
       <c r="AK35" s="92">
         <f>MAX($AL$10:$AL$97) - AL35</f>
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AL35" s="121"/>
     </row>
@@ -8125,7 +8699,7 @@
       </c>
       <c r="AK38" s="111">
         <f>MAX($AL$10:$AL$97) - AL38</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AL38" s="122">
         <f>$S38+$AB38+$AG38+$AJ38</f>
@@ -8210,7 +8784,7 @@
       <c r="AJ39" s="121"/>
       <c r="AK39" s="92">
         <f>MAX($AL$10:$AL$97) - AL39</f>
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AL39" s="121"/>
     </row>
@@ -8550,63 +9124,63 @@
         <v>9</v>
       </c>
       <c r="B42" s="217" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C42" s="229">
         <v>6</v>
       </c>
       <c r="D42" s="230"/>
       <c r="E42" s="234">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F42" s="230"/>
       <c r="G42" s="232">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H42" s="233"/>
       <c r="I42" s="234"/>
       <c r="J42" s="233">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K42" s="235">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L42" s="233"/>
-      <c r="M42" s="234"/>
-      <c r="N42" s="230">
+      <c r="M42" s="234">
         <v>7</v>
       </c>
+      <c r="N42" s="230"/>
       <c r="O42" s="234">
         <v>6</v>
       </c>
       <c r="P42" s="230"/>
-      <c r="Q42" s="308">
-        <v>7</v>
-      </c>
-      <c r="R42" s="237"/>
+      <c r="Q42" s="232"/>
+      <c r="R42" s="237">
+        <v>6</v>
+      </c>
       <c r="S42" s="239">
         <f>SUM(C43:R43)</f>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="T42" s="229"/>
       <c r="U42" s="233">
-        <v>7</v>
-      </c>
-      <c r="V42" s="234">
         <v>6</v>
       </c>
-      <c r="W42" s="233"/>
+      <c r="V42" s="234"/>
+      <c r="W42" s="233">
+        <v>6</v>
+      </c>
       <c r="X42" s="235"/>
       <c r="Y42" s="230">
         <v>7</v>
       </c>
-      <c r="Z42" s="232">
+      <c r="Z42" s="232"/>
+      <c r="AA42" s="233">
         <v>6</v>
       </c>
-      <c r="AA42" s="233"/>
       <c r="AB42" s="239">
         <f>SUM(T43:AA43)</f>
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="AC42" s="232"/>
       <c r="AD42" s="233"/>
@@ -8624,7 +9198,7 @@
       </c>
       <c r="AK42" s="241">
         <f>MAX($AL$10:$AL$97) - AL42</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AL42" s="239">
         <f>$S42+$AB42+$AG42+$AJ42</f>
@@ -8664,7 +9238,7 @@
       <c r="L43" s="76"/>
       <c r="M43" s="77">
         <f>(IF($M42&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M42=$M$6+$N$6,$O$103,0),0),0)+IF($N42&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N42=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="N43" s="151"/>
       <c r="O43" s="77">
@@ -8674,7 +9248,7 @@
       <c r="P43" s="76"/>
       <c r="Q43" s="77">
         <f>(IF($Q42&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q42=$Q$6+$R$6,$O$103,0),0),0)+IF($R42&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R42=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="R43" s="80"/>
       <c r="S43" s="121"/>
@@ -8685,7 +9259,7 @@
       <c r="U43" s="126"/>
       <c r="V43" s="126">
         <f>(IF($V42&lt;&gt;"",($V$6*$P$104)+IF($V$6=4,($P$102)+IF($V42=$V$6+$W$6,$P$103,0),0),0)+IF($W42&lt;&gt;"",($W$6*$P$104)+IF($W$6=4,($P$102)+IF($W42=$V$6+$W$6,$P$103,0),0),0))</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="W43" s="126"/>
       <c r="X43" s="126">
@@ -8695,7 +9269,7 @@
       <c r="Y43" s="59"/>
       <c r="Z43" s="126">
         <f>(IF($Z42&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z42=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA42&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA42=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA43" s="62"/>
       <c r="AB43" s="121"/>
@@ -8709,7 +9283,7 @@
       <c r="AJ43" s="121"/>
       <c r="AK43" s="111">
         <f>MAX($AL$10:$AL$97) - AL43</f>
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AL43" s="121"/>
     </row>
@@ -8788,7 +9362,7 @@
         <f>IF(ISBLANK(N42),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O44" s="118">
         <f>IF(ISBLANK(O42),
@@ -8806,7 +9380,7 @@
         <f>IF(ISBLANK(Q42),
 0,
 IF(Q$6= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R44" s="118">
         <f>IF(ISBLANK(R42),
@@ -8837,7 +9411,7 @@
         <f>IF(ISBLANK(W42),
 0,
 IF(W$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X44" s="118">
         <f>IF(ISBLANK(X42),
@@ -8874,7 +9448,7 @@
       <c r="AJ44" s="138"/>
       <c r="AK44" s="139">
         <f>SUM(C44:AI44)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AL44" s="123"/>
     </row>
@@ -8971,7 +9545,7 @@
         <f>IF(Q44 = 0,
 0,
 IF(Q42 = (Q$6+R$6),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R45" s="118">
         <f>IF(R44 = 0,
@@ -9039,28 +9613,28 @@
       <c r="AJ45" s="138"/>
       <c r="AK45" s="139">
         <f>SUM(C45:AI45)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL45" s="123"/>
     </row>
     <row r="46" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="117">
         <f>RANK(AL46,$AL$10:$AL$97,)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B46" s="84" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="C46" s="46">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D46" s="45"/>
       <c r="E46" s="44">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F46" s="45"/>
       <c r="G46" s="48">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H46" s="47"/>
       <c r="I46" s="44"/>
@@ -9071,30 +9645,30 @@
         <v>6</v>
       </c>
       <c r="L46" s="47"/>
-      <c r="M46" s="44">
-        <v>5</v>
-      </c>
-      <c r="N46" s="45"/>
+      <c r="M46" s="44"/>
+      <c r="N46" s="45">
+        <v>7</v>
+      </c>
       <c r="O46" s="44">
         <v>6</v>
       </c>
       <c r="P46" s="45"/>
-      <c r="Q46" s="48"/>
-      <c r="R46" s="50">
-        <v>6</v>
-      </c>
+      <c r="Q46" s="213">
+        <v>7</v>
+      </c>
+      <c r="R46" s="50"/>
       <c r="S46" s="122">
         <f>SUM(C47:R47)</f>
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="T46" s="46"/>
       <c r="U46" s="47">
+        <v>7</v>
+      </c>
+      <c r="V46" s="44">
         <v>6</v>
       </c>
-      <c r="V46" s="44"/>
-      <c r="W46" s="47">
-        <v>7</v>
-      </c>
+      <c r="W46" s="47"/>
       <c r="X46" s="49"/>
       <c r="Y46" s="45">
         <v>7</v>
@@ -9105,10 +9679,10 @@
       <c r="AA46" s="47"/>
       <c r="AB46" s="122">
         <f>SUM(T47:AA47)</f>
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="AC46" s="48"/>
-      <c r="AD46" s="311"/>
+      <c r="AD46" s="47"/>
       <c r="AE46" s="49"/>
       <c r="AF46" s="47"/>
       <c r="AG46" s="122">
@@ -9127,7 +9701,7 @@
       </c>
       <c r="AL46" s="122">
         <f>$S46+$AB46+$AG46+$AJ46</f>
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -9163,7 +9737,7 @@
       <c r="L47" s="76"/>
       <c r="M47" s="77">
         <f>(IF($M46&lt;&gt;"",($M$6*$O$104)+IF($M$6=4,($O$102)+IF($M46=$M$6+$N$6,$O$103,0),0),0)+IF($N46&lt;&gt;"",($N$6*$O$104)+IF($N$6=4,($O$102)+IF($N46=$M$6+$N$6,$O$103,0),0),0))</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="N47" s="76"/>
       <c r="O47" s="77">
@@ -9173,7 +9747,7 @@
       <c r="P47" s="76"/>
       <c r="Q47" s="77">
         <f>(IF($Q46&lt;&gt;"",($Q$6*$O$104)+IF($Q$6=4,($O$102)+IF($Q46=$Q$6+$R$6,$O$103,0),0),0)+IF($R46&lt;&gt;"",($R$6*$O$104)+IF($R$6=4,($O$102)+IF($R46=$Q$6+$R$6,$O$103,0),0),0))</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="R47" s="80"/>
       <c r="S47" s="121"/>
@@ -9184,7 +9758,7 @@
       <c r="U47" s="126"/>
       <c r="V47" s="126">
         <f>(IF($V46&lt;&gt;"",($V$6*$P$104)+IF($V$6=4,($P$102)+IF($V46=$V$6+$W$6,$P$103,0),0),0)+IF($W46&lt;&gt;"",($W$6*$P$104)+IF($W$6=4,($P$102)+IF($W46=$V$6+$W$6,$P$103,0),0),0))</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="W47" s="126"/>
       <c r="X47" s="126">
@@ -9208,7 +9782,7 @@
       <c r="AJ47" s="121"/>
       <c r="AK47" s="111">
         <f>MAX($AL$10:$AL$97) - AL47</f>
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AL47" s="121"/>
     </row>
@@ -9287,7 +9861,7 @@
         <f>IF(ISBLANK(N46),
 0,
 IF(N$6 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O48" s="118">
         <f>IF(ISBLANK(O46),
@@ -9305,7 +9879,7 @@
         <f>IF(ISBLANK(Q46),
 0,
 IF(Q$6= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R48" s="118">
         <f>IF(ISBLANK(R46),
@@ -9336,7 +9910,7 @@
         <f>IF(ISBLANK(W46),
 0,
 IF(W$6 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X48" s="118">
         <f>IF(ISBLANK(X46),
@@ -9373,7 +9947,7 @@
       <c r="AJ48" s="138"/>
       <c r="AK48" s="139">
         <f>SUM(C48:AI48)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL48" s="123"/>
     </row>
@@ -9470,7 +10044,7 @@
         <f>IF(Q48 = 0,
 0,
 IF(Q46 = (Q$6+R$6),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R49" s="118">
         <f>IF(R48 = 0,
@@ -9538,24 +10112,24 @@
       <c r="AJ49" s="138"/>
       <c r="AK49" s="139">
         <f>SUM(C49:AI49)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL49" s="123"/>
     </row>
     <row r="50" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="216">
         <f>RANK(AL50,$AL$10:$AL$97,)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B50" s="217" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="C50" s="229">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D50" s="230"/>
       <c r="E50" s="234">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F50" s="230"/>
       <c r="G50" s="232">
@@ -9564,14 +10138,14 @@
       <c r="H50" s="233"/>
       <c r="I50" s="234"/>
       <c r="J50" s="233">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K50" s="235">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L50" s="233"/>
       <c r="M50" s="234">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="N50" s="230"/>
       <c r="O50" s="234">
@@ -9592,22 +10166,22 @@
       </c>
       <c r="V50" s="234"/>
       <c r="W50" s="233">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="X50" s="235"/>
       <c r="Y50" s="230">
         <v>7</v>
       </c>
-      <c r="Z50" s="232"/>
-      <c r="AA50" s="233">
+      <c r="Z50" s="232">
         <v>6</v>
       </c>
+      <c r="AA50" s="233"/>
       <c r="AB50" s="239">
         <f>SUM(T51:AA51)</f>
         <v>20</v>
       </c>
       <c r="AC50" s="232"/>
-      <c r="AD50" s="233"/>
+      <c r="AD50" s="242"/>
       <c r="AE50" s="235"/>
       <c r="AF50" s="233"/>
       <c r="AG50" s="239">
@@ -9622,7 +10196,7 @@
       </c>
       <c r="AK50" s="241">
         <f>MAX($AL$10:$AL$97) - AL50</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AL50" s="239">
         <f>$S50+$AB50+$AG50+$AJ50</f>
@@ -10100,7 +10674,7 @@
       </c>
       <c r="AB54" s="122">
         <f>SUM(T55:AA55)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AC54" s="48"/>
       <c r="AD54" s="47"/>
@@ -10122,7 +10696,7 @@
       </c>
       <c r="AL54" s="122">
         <f>$S54+$AB54+$AG54+$AJ54</f>
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="55" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -10189,7 +10763,7 @@
       <c r="Y55" s="59"/>
       <c r="Z55" s="126">
         <f>(IF($Z54&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z54=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA54&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA54=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA55" s="62"/>
       <c r="AB55" s="121"/>
@@ -10614,7 +11188,7 @@
       </c>
       <c r="AK58" s="241">
         <f>MAX($AL$10:$AL$97) - AL58</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AL58" s="239">
         <f>$S58+$AB58+$AG58+$AJ58</f>
@@ -11102,7 +11676,7 @@
         <f>SUM(AC63:AF63)</f>
         <v>0</v>
       </c>
-      <c r="AH62" s="312"/>
+      <c r="AH62" s="252"/>
       <c r="AI62" s="57"/>
       <c r="AJ62" s="122">
         <f>AH63</f>
@@ -11110,7 +11684,7 @@
       </c>
       <c r="AK62" s="111">
         <f>MAX($AL$10:$AL$97) - AL62</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AL62" s="122">
         <f>$S62+$AB62+$AG62+$AJ62</f>
@@ -11606,7 +12180,7 @@
       </c>
       <c r="AK66" s="241">
         <f>MAX($AL$10:$AL$97) - AL66</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AL66" s="239">
         <f>$S66+$AB66+$AG66+$AJ66</f>
@@ -12102,7 +12676,7 @@
       </c>
       <c r="AK70" s="111">
         <f>MAX($AL$10:$AL$97) - AL70</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AL70" s="122">
         <f>$S70+$AB70+$AG70+$AJ70</f>
@@ -12524,38 +13098,38 @@
         <v>17</v>
       </c>
       <c r="B74" s="217" t="s">
-        <v>68</v>
-      </c>
-      <c r="C74" s="247">
+        <v>80</v>
+      </c>
+      <c r="C74" s="229">
         <v>5</v>
       </c>
-      <c r="D74" s="248"/>
-      <c r="E74" s="249">
+      <c r="D74" s="230"/>
+      <c r="E74" s="234">
         <v>6</v>
       </c>
-      <c r="F74" s="248"/>
-      <c r="G74" s="250">
+      <c r="F74" s="230"/>
+      <c r="G74" s="232">
+        <v>6</v>
+      </c>
+      <c r="H74" s="233"/>
+      <c r="I74" s="234"/>
+      <c r="J74" s="233">
+        <v>6</v>
+      </c>
+      <c r="K74" s="235">
+        <v>7</v>
+      </c>
+      <c r="L74" s="233"/>
+      <c r="M74" s="234">
+        <v>6</v>
+      </c>
+      <c r="N74" s="230"/>
+      <c r="O74" s="234">
         <v>5</v>
       </c>
-      <c r="H74" s="251"/>
-      <c r="I74" s="249"/>
-      <c r="J74" s="251">
-        <v>6</v>
-      </c>
-      <c r="K74" s="252">
-        <v>6</v>
-      </c>
-      <c r="L74" s="251"/>
-      <c r="M74" s="249">
-        <v>7</v>
-      </c>
-      <c r="N74" s="248"/>
-      <c r="O74" s="249">
-        <v>6</v>
-      </c>
-      <c r="P74" s="248"/>
-      <c r="Q74" s="250"/>
-      <c r="R74" s="253">
+      <c r="P74" s="230"/>
+      <c r="Q74" s="232"/>
+      <c r="R74" s="237">
         <v>6</v>
       </c>
       <c r="S74" s="239">
@@ -12567,20 +13141,20 @@
         <v>6</v>
       </c>
       <c r="V74" s="234">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="W74" s="233"/>
-      <c r="X74" s="235">
+      <c r="X74" s="235"/>
+      <c r="Y74" s="230">
+        <v>5</v>
+      </c>
+      <c r="Z74" s="232"/>
+      <c r="AA74" s="233">
         <v>6</v>
       </c>
-      <c r="Y74" s="230"/>
-      <c r="Z74" s="232">
-        <v>7</v>
-      </c>
-      <c r="AA74" s="233"/>
       <c r="AB74" s="239">
         <f>SUM(T75:AA75)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AC74" s="232"/>
       <c r="AD74" s="233"/>
@@ -12602,7 +13176,7 @@
       </c>
       <c r="AL74" s="239">
         <f>$S74+$AB74+$AG74+$AJ74</f>
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="75" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -12669,7 +13243,7 @@
       <c r="Y75" s="59"/>
       <c r="Z75" s="126">
         <f>(IF($Z74&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z74=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA74&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA74=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA75" s="62"/>
       <c r="AB75" s="121"/>
@@ -13017,41 +13591,41 @@
     <row r="78" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="117">
         <f>RANK(AL78,$AL$10:$AL$97,)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B78" s="84" t="s">
-        <v>80</v>
-      </c>
-      <c r="C78" s="46">
+        <v>68</v>
+      </c>
+      <c r="C78" s="305">
         <v>5</v>
       </c>
-      <c r="D78" s="45"/>
-      <c r="E78" s="44">
+      <c r="D78" s="306"/>
+      <c r="E78" s="307">
         <v>6</v>
       </c>
-      <c r="F78" s="45"/>
-      <c r="G78" s="48">
+      <c r="F78" s="306"/>
+      <c r="G78" s="308">
+        <v>5</v>
+      </c>
+      <c r="H78" s="309"/>
+      <c r="I78" s="307"/>
+      <c r="J78" s="309">
         <v>6</v>
       </c>
-      <c r="H78" s="47"/>
-      <c r="I78" s="44"/>
-      <c r="J78" s="47">
+      <c r="K78" s="310">
         <v>6</v>
       </c>
-      <c r="K78" s="49">
+      <c r="L78" s="309"/>
+      <c r="M78" s="307">
         <v>7</v>
       </c>
-      <c r="L78" s="47"/>
-      <c r="M78" s="44">
+      <c r="N78" s="306"/>
+      <c r="O78" s="307">
         <v>6</v>
       </c>
-      <c r="N78" s="45"/>
-      <c r="O78" s="44">
-        <v>5</v>
-      </c>
-      <c r="P78" s="45"/>
-      <c r="Q78" s="48"/>
-      <c r="R78" s="50">
+      <c r="P78" s="306"/>
+      <c r="Q78" s="308"/>
+      <c r="R78" s="311">
         <v>6</v>
       </c>
       <c r="S78" s="122">
@@ -13063,17 +13637,17 @@
         <v>6</v>
       </c>
       <c r="V78" s="44">
+        <v>7</v>
+      </c>
+      <c r="W78" s="47"/>
+      <c r="X78" s="49">
         <v>6</v>
       </c>
-      <c r="W78" s="47"/>
-      <c r="X78" s="49"/>
-      <c r="Y78" s="45">
-        <v>5</v>
-      </c>
-      <c r="Z78" s="48"/>
-      <c r="AA78" s="47">
-        <v>6</v>
-      </c>
+      <c r="Y78" s="45"/>
+      <c r="Z78" s="48">
+        <v>7</v>
+      </c>
+      <c r="AA78" s="47"/>
       <c r="AB78" s="122">
         <f>SUM(T79:AA79)</f>
         <v>6</v>
@@ -13094,7 +13668,7 @@
       </c>
       <c r="AK78" s="111">
         <f>MAX($AL$10:$AL$97) - AL78</f>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AL78" s="122">
         <f>$S78+$AB78+$AG78+$AJ78</f>
@@ -13513,7 +14087,7 @@
     <row r="82" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="216">
         <f>RANK(AL82,$AL$10:$AL$97,)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B82" s="217" t="s">
         <v>75</v>
@@ -13590,7 +14164,7 @@
       </c>
       <c r="AK82" s="241">
         <f>MAX($AL$10:$AL$97) - AL82</f>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AL82" s="239">
         <f>$S82+$AB82+$AG82+$AJ82</f>
@@ -14086,7 +14660,7 @@
       </c>
       <c r="AK86" s="111">
         <f>MAX($AL$10:$AL$97) - AL86</f>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AL86" s="122">
         <f>$S86+$AB86+$AG86+$AJ86</f>
@@ -14582,7 +15156,7 @@
       </c>
       <c r="AK90" s="241">
         <f>MAX($AL$10:$AL$97) - AL90</f>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AL90" s="239">
         <f>$S90+$AB90+$AG90+$AJ90</f>
@@ -15078,7 +15652,7 @@
       </c>
       <c r="AK94" s="111">
         <f>MAX($AL$10:$AL$97) - AL94</f>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AL94" s="179">
         <f>$S94+$AB94+$AG94+$AJ94</f>
@@ -15627,12 +16201,12 @@
     <row r="100" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B100" s="43"/>
       <c r="N100" s="26"/>
-      <c r="O100" s="254" t="s">
+      <c r="O100" s="286" t="s">
         <v>17</v>
       </c>
-      <c r="P100" s="255"/>
-      <c r="Q100" s="255"/>
-      <c r="R100" s="256"/>
+      <c r="P100" s="287"/>
+      <c r="Q100" s="287"/>
+      <c r="R100" s="288"/>
       <c r="AG100" s="30"/>
       <c r="AH100" s="30"/>
       <c r="AI100" s="30"/>
@@ -15641,21 +16215,21 @@
     </row>
     <row r="101" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="33"/>
-      <c r="B101" s="283" t="s">
+      <c r="B101" s="274" t="s">
         <v>16</v>
       </c>
-      <c r="C101" s="284"/>
-      <c r="D101" s="284"/>
-      <c r="E101" s="284"/>
-      <c r="F101" s="284"/>
-      <c r="G101" s="284"/>
-      <c r="H101" s="284"/>
-      <c r="I101" s="284"/>
-      <c r="J101" s="284"/>
-      <c r="K101" s="284"/>
-      <c r="L101" s="284"/>
-      <c r="M101" s="284"/>
-      <c r="N101" s="285"/>
+      <c r="C101" s="275"/>
+      <c r="D101" s="275"/>
+      <c r="E101" s="275"/>
+      <c r="F101" s="275"/>
+      <c r="G101" s="275"/>
+      <c r="H101" s="275"/>
+      <c r="I101" s="275"/>
+      <c r="J101" s="275"/>
+      <c r="K101" s="275"/>
+      <c r="L101" s="275"/>
+      <c r="M101" s="275"/>
+      <c r="N101" s="276"/>
       <c r="O101" s="21">
         <v>1</v>
       </c>
@@ -15668,45 +16242,45 @@
       <c r="R101" s="22">
         <v>4</v>
       </c>
-      <c r="U101" s="257" t="s">
+      <c r="U101" s="289" t="s">
         <v>26</v>
       </c>
-      <c r="V101" s="258"/>
-      <c r="W101" s="258"/>
-      <c r="X101" s="258"/>
-      <c r="Y101" s="258"/>
-      <c r="Z101" s="258"/>
-      <c r="AA101" s="258"/>
-      <c r="AB101" s="258"/>
-      <c r="AC101" s="258"/>
-      <c r="AD101" s="259"/>
+      <c r="V101" s="290"/>
+      <c r="W101" s="290"/>
+      <c r="X101" s="290"/>
+      <c r="Y101" s="290"/>
+      <c r="Z101" s="290"/>
+      <c r="AA101" s="290"/>
+      <c r="AB101" s="290"/>
+      <c r="AC101" s="290"/>
+      <c r="AD101" s="291"/>
       <c r="AE101" s="28"/>
       <c r="AF101" s="28"/>
-      <c r="AG101" s="260" t="s">
+      <c r="AG101" s="292" t="s">
         <v>24</v>
       </c>
-      <c r="AH101" s="261"/>
-      <c r="AI101" s="261"/>
-      <c r="AJ101" s="261"/>
-      <c r="AK101" s="262"/>
+      <c r="AH101" s="293"/>
+      <c r="AI101" s="293"/>
+      <c r="AJ101" s="293"/>
+      <c r="AK101" s="294"/>
     </row>
     <row r="102" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A102" s="34"/>
-      <c r="B102" s="290" t="s">
+      <c r="B102" s="253" t="s">
         <v>6</v>
       </c>
-      <c r="C102" s="291"/>
-      <c r="D102" s="291"/>
-      <c r="E102" s="291"/>
-      <c r="F102" s="291"/>
-      <c r="G102" s="291"/>
-      <c r="H102" s="291"/>
-      <c r="I102" s="291"/>
-      <c r="J102" s="291"/>
-      <c r="K102" s="291"/>
-      <c r="L102" s="291"/>
-      <c r="M102" s="291"/>
-      <c r="N102" s="292"/>
+      <c r="C102" s="254"/>
+      <c r="D102" s="254"/>
+      <c r="E102" s="254"/>
+      <c r="F102" s="254"/>
+      <c r="G102" s="254"/>
+      <c r="H102" s="254"/>
+      <c r="I102" s="254"/>
+      <c r="J102" s="254"/>
+      <c r="K102" s="254"/>
+      <c r="L102" s="254"/>
+      <c r="M102" s="254"/>
+      <c r="N102" s="255"/>
       <c r="O102" s="20">
         <v>5</v>
       </c>
@@ -15719,49 +16293,49 @@
       <c r="R102" s="23">
         <v>20</v>
       </c>
-      <c r="U102" s="288" t="s">
+      <c r="U102" s="279" t="s">
         <v>20</v>
       </c>
-      <c r="V102" s="289"/>
-      <c r="W102" s="289"/>
-      <c r="X102" s="289"/>
-      <c r="Y102" s="289"/>
-      <c r="Z102" s="289"/>
-      <c r="AA102" s="289"/>
-      <c r="AB102" s="286">
+      <c r="V102" s="280"/>
+      <c r="W102" s="280"/>
+      <c r="X102" s="280"/>
+      <c r="Y102" s="280"/>
+      <c r="Z102" s="280"/>
+      <c r="AA102" s="280"/>
+      <c r="AB102" s="277">
         <v>22</v>
       </c>
-      <c r="AC102" s="286"/>
-      <c r="AD102" s="287"/>
+      <c r="AC102" s="277"/>
+      <c r="AD102" s="278"/>
       <c r="AE102" s="29"/>
       <c r="AF102" s="29"/>
-      <c r="AG102" s="302" t="s">
+      <c r="AG102" s="260" t="s">
         <v>21</v>
       </c>
-      <c r="AH102" s="303"/>
-      <c r="AI102" s="303"/>
-      <c r="AJ102" s="304"/>
+      <c r="AH102" s="261"/>
+      <c r="AI102" s="261"/>
+      <c r="AJ102" s="262"/>
       <c r="AK102" s="184">
         <v>230</v>
       </c>
     </row>
     <row r="103" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="34"/>
-      <c r="B103" s="290" t="s">
+      <c r="B103" s="253" t="s">
         <v>5</v>
       </c>
-      <c r="C103" s="291"/>
-      <c r="D103" s="291"/>
-      <c r="E103" s="291"/>
-      <c r="F103" s="291"/>
-      <c r="G103" s="291"/>
-      <c r="H103" s="291"/>
-      <c r="I103" s="291"/>
-      <c r="J103" s="291"/>
-      <c r="K103" s="291"/>
-      <c r="L103" s="291"/>
-      <c r="M103" s="291"/>
-      <c r="N103" s="292"/>
+      <c r="C103" s="254"/>
+      <c r="D103" s="254"/>
+      <c r="E103" s="254"/>
+      <c r="F103" s="254"/>
+      <c r="G103" s="254"/>
+      <c r="H103" s="254"/>
+      <c r="I103" s="254"/>
+      <c r="J103" s="254"/>
+      <c r="K103" s="254"/>
+      <c r="L103" s="254"/>
+      <c r="M103" s="254"/>
+      <c r="N103" s="255"/>
       <c r="O103" s="20">
         <v>2</v>
       </c>
@@ -15774,49 +16348,49 @@
       <c r="R103" s="23">
         <v>8</v>
       </c>
-      <c r="U103" s="297" t="s">
+      <c r="U103" s="258" t="s">
         <v>18</v>
       </c>
-      <c r="V103" s="298"/>
-      <c r="W103" s="298"/>
-      <c r="X103" s="298"/>
-      <c r="Y103" s="298"/>
-      <c r="Z103" s="298"/>
-      <c r="AA103" s="298"/>
-      <c r="AB103" s="299">
+      <c r="V103" s="259"/>
+      <c r="W103" s="259"/>
+      <c r="X103" s="259"/>
+      <c r="Y103" s="259"/>
+      <c r="Z103" s="259"/>
+      <c r="AA103" s="259"/>
+      <c r="AB103" s="284">
         <v>20</v>
       </c>
-      <c r="AC103" s="299"/>
-      <c r="AD103" s="300"/>
+      <c r="AC103" s="284"/>
+      <c r="AD103" s="285"/>
       <c r="AE103" s="29"/>
       <c r="AF103" s="29"/>
-      <c r="AG103" s="305" t="s">
+      <c r="AG103" s="263" t="s">
         <v>22</v>
       </c>
-      <c r="AH103" s="291"/>
-      <c r="AI103" s="291"/>
-      <c r="AJ103" s="292"/>
+      <c r="AH103" s="254"/>
+      <c r="AI103" s="254"/>
+      <c r="AJ103" s="255"/>
       <c r="AK103" s="36">
         <v>115</v>
       </c>
     </row>
     <row r="104" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="35"/>
-      <c r="B104" s="276" t="s">
+      <c r="B104" s="267" t="s">
         <v>4</v>
       </c>
-      <c r="C104" s="277"/>
-      <c r="D104" s="277"/>
-      <c r="E104" s="277"/>
-      <c r="F104" s="277"/>
-      <c r="G104" s="277"/>
-      <c r="H104" s="277"/>
-      <c r="I104" s="277"/>
-      <c r="J104" s="277"/>
-      <c r="K104" s="277"/>
-      <c r="L104" s="277"/>
-      <c r="M104" s="277"/>
-      <c r="N104" s="278"/>
+      <c r="C104" s="268"/>
+      <c r="D104" s="268"/>
+      <c r="E104" s="268"/>
+      <c r="F104" s="268"/>
+      <c r="G104" s="268"/>
+      <c r="H104" s="268"/>
+      <c r="I104" s="268"/>
+      <c r="J104" s="268"/>
+      <c r="K104" s="268"/>
+      <c r="L104" s="268"/>
+      <c r="M104" s="268"/>
+      <c r="N104" s="269"/>
       <c r="O104" s="3">
         <v>1</v>
       </c>
@@ -15829,51 +16403,51 @@
       <c r="R104" s="24">
         <v>1</v>
       </c>
-      <c r="U104" s="293" t="s">
+      <c r="U104" s="281" t="s">
         <v>19</v>
       </c>
-      <c r="V104" s="294"/>
-      <c r="W104" s="294"/>
-      <c r="X104" s="294"/>
-      <c r="Y104" s="294"/>
-      <c r="Z104" s="294"/>
-      <c r="AA104" s="294"/>
-      <c r="AB104" s="295">
+      <c r="V104" s="257"/>
+      <c r="W104" s="257"/>
+      <c r="X104" s="257"/>
+      <c r="Y104" s="257"/>
+      <c r="Z104" s="257"/>
+      <c r="AA104" s="257"/>
+      <c r="AB104" s="282">
         <f>AB102*AB103</f>
         <v>440</v>
       </c>
-      <c r="AC104" s="295"/>
-      <c r="AD104" s="296"/>
+      <c r="AC104" s="282"/>
+      <c r="AD104" s="283"/>
       <c r="AE104" s="29"/>
       <c r="AF104" s="29"/>
-      <c r="AG104" s="305" t="s">
+      <c r="AG104" s="263" t="s">
         <v>25</v>
       </c>
-      <c r="AH104" s="291"/>
-      <c r="AI104" s="291"/>
-      <c r="AJ104" s="292"/>
+      <c r="AH104" s="254"/>
+      <c r="AI104" s="254"/>
+      <c r="AJ104" s="255"/>
       <c r="AK104" s="36">
         <v>65</v>
       </c>
     </row>
     <row r="105" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG105" s="297" t="s">
+      <c r="AG105" s="258" t="s">
         <v>23</v>
       </c>
-      <c r="AH105" s="298"/>
-      <c r="AI105" s="298"/>
-      <c r="AJ105" s="298"/>
+      <c r="AH105" s="259"/>
+      <c r="AI105" s="259"/>
+      <c r="AJ105" s="259"/>
       <c r="AK105" s="186">
         <v>30</v>
       </c>
     </row>
     <row r="106" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG106" s="301" t="s">
+      <c r="AG106" s="256" t="s">
         <v>19</v>
       </c>
-      <c r="AH106" s="294"/>
-      <c r="AI106" s="294"/>
-      <c r="AJ106" s="294"/>
+      <c r="AH106" s="257"/>
+      <c r="AI106" s="257"/>
+      <c r="AJ106" s="257"/>
       <c r="AK106" s="185">
         <f>SUM(AK102:AK105)</f>
         <v>440</v>
@@ -15885,12 +16459,22 @@
     <sortCondition ref="B10:B94"/>
   </sortState>
   <mergeCells count="38">
-    <mergeCell ref="B103:N103"/>
-    <mergeCell ref="AG106:AJ106"/>
-    <mergeCell ref="AG105:AJ105"/>
-    <mergeCell ref="AG102:AJ102"/>
-    <mergeCell ref="AG104:AJ104"/>
-    <mergeCell ref="AG103:AJ103"/>
+    <mergeCell ref="O100:R100"/>
+    <mergeCell ref="U101:AD101"/>
+    <mergeCell ref="AG101:AK101"/>
+    <mergeCell ref="AH4:AJ4"/>
+    <mergeCell ref="AG5:AG9"/>
+    <mergeCell ref="AJ5:AJ9"/>
+    <mergeCell ref="X5:AA5"/>
+    <mergeCell ref="AB5:AB9"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="C4:S4"/>
+    <mergeCell ref="T4:AB4"/>
+    <mergeCell ref="AC4:AG4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="K5:R5"/>
+    <mergeCell ref="S5:S9"/>
     <mergeCell ref="T5:W5"/>
     <mergeCell ref="B104:N104"/>
     <mergeCell ref="C1:O1"/>
@@ -15907,341 +16491,231 @@
     <mergeCell ref="AB104:AD104"/>
     <mergeCell ref="U103:AA103"/>
     <mergeCell ref="AB103:AD103"/>
-    <mergeCell ref="O100:R100"/>
-    <mergeCell ref="U101:AD101"/>
-    <mergeCell ref="AG101:AK101"/>
-    <mergeCell ref="AH4:AJ4"/>
-    <mergeCell ref="AG5:AG9"/>
-    <mergeCell ref="AJ5:AJ9"/>
-    <mergeCell ref="X5:AA5"/>
-    <mergeCell ref="AB5:AB9"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="C4:S4"/>
-    <mergeCell ref="T4:AB4"/>
-    <mergeCell ref="AC4:AG4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="K5:R5"/>
-    <mergeCell ref="S5:S9"/>
+    <mergeCell ref="B103:N103"/>
+    <mergeCell ref="AG106:AJ106"/>
+    <mergeCell ref="AG105:AJ105"/>
+    <mergeCell ref="AG102:AJ102"/>
+    <mergeCell ref="AG104:AJ104"/>
+    <mergeCell ref="AG103:AJ103"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
-  <conditionalFormatting sqref="AH18:AI18 AH10:AI10 AH14:AI14 T10:AA10 AC10:AF10 C10:R10 C14:R14 T14:AA14 AC14:AF14 T18:AA18 AC18:AF18 AH30:AI30 C30:R30 T30:AA30 AC30:AF30 AH26:AI26 C26:R26 T26:AA26 AC26:AF26 AH62:AI62 C62:R62 T62:AA62 AC62:AF62 AH42:AI42 C42:R42 T42:AA42 AC42:AF42 AH22:AI22 C22:R22 T22:AA22 AC22:AF22 AH38:AI38 C38:R38 T38:AA38 AC38:AF38 AH34:AI34 C34:R34 T34:AA34 AC34:AF34 AH66:AI66 C66:R66 T66:AA66 AC66:AF66 C18:R18">
-    <cfRule type="cellIs" dxfId="100" priority="199" stopIfTrue="1" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C10:R10">
-    <cfRule type="cellIs" dxfId="99" priority="195" stopIfTrue="1" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14:R14">
-    <cfRule type="cellIs" dxfId="98" priority="194" stopIfTrue="1" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C18:R18">
-    <cfRule type="cellIs" dxfId="97" priority="193" stopIfTrue="1" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C22:R22">
-    <cfRule type="cellIs" dxfId="96" priority="192" stopIfTrue="1" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C26:R26">
-    <cfRule type="cellIs" dxfId="95" priority="191" stopIfTrue="1" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30:R30">
-    <cfRule type="cellIs" dxfId="94" priority="190" stopIfTrue="1" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34:R34">
-    <cfRule type="cellIs" dxfId="93" priority="189" stopIfTrue="1" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:R38">
-    <cfRule type="cellIs" dxfId="92" priority="188" stopIfTrue="1" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C42:R42">
-    <cfRule type="cellIs" dxfId="91" priority="187" stopIfTrue="1" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH54:AI54 C54:R54 T54:AA54 AC54:AF54">
-    <cfRule type="cellIs" dxfId="90" priority="186" stopIfTrue="1" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH46:AI46 C46:R46 T46:AA46 AC46:AF46">
-    <cfRule type="cellIs" dxfId="89" priority="185" stopIfTrue="1" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C46:R46">
-    <cfRule type="cellIs" dxfId="88" priority="184" stopIfTrue="1" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH50:AI50 C50:R50 T50:AA50 AC50:AF50">
-    <cfRule type="cellIs" dxfId="87" priority="183" stopIfTrue="1" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50:R50">
-    <cfRule type="cellIs" dxfId="86" priority="182" stopIfTrue="1" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH58:AI58 C58:R58 T58:AA58 AC58:AF58">
-    <cfRule type="cellIs" dxfId="85" priority="181" stopIfTrue="1" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R18">
-    <cfRule type="cellIs" dxfId="84" priority="180" stopIfTrue="1" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH70:AI70 C70:R70 T70:AA70 AC70:AF70">
-    <cfRule type="cellIs" dxfId="83" priority="179" stopIfTrue="1" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH74:AI74 C74:R74 T74:AA74 AC74:AF74">
-    <cfRule type="cellIs" dxfId="82" priority="178" stopIfTrue="1" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH78:AI78 C78:R78 T78:AA78 AC78:AF78">
-    <cfRule type="cellIs" dxfId="81" priority="177" stopIfTrue="1" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="S10:S15 AB10:AB15 AG10:AG15 AJ10:AJ15 AJ26:AJ27 AG26:AG27 AB26:AB27 S26:S27 AJ22:AJ23 AG22:AG23 AB22:AB23 S22:S23 AJ18:AJ19 AG18:AG19 AB18:AB19 S18:S19 S38:S39 AB38:AB39 AG38:AG39 AJ38:AJ39 S30:S31 AB30:AB31 AG30:AG31 AJ30:AJ31 AJ42:AJ43 AG42:AG43 AB42:AB43 S42:S43 S46:S47 AB46:AB47 AG46:AG47 AJ46:AJ47 AJ50 AG50 AB50 S50 S58 AB58 AG58 AJ58 S54 AB54 AG54 AJ54 AJ62 AG62 AB62 S62 S66 AB66 AG66 AJ66 AJ70 AG70 AB70 S70 S74 AB74 AG74 AJ74 AJ78 AG78 AB78 S78 AJ34:AJ35 AG34:AG35 AB34:AB35 S34:S35">
-    <cfRule type="cellIs" dxfId="80" priority="172" operator="notEqual">
+    <cfRule type="cellIs" dxfId="138" priority="174" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL10:AL23 AL26:AL27 AL38:AL39 AL30:AL31 AL42:AL43 AL46:AL47 AL50 AL58 AL54 AL62 AL66 AL70 AL74 AL78 AL34:AL35">
-    <cfRule type="cellIs" dxfId="79" priority="171" operator="notEqual">
+    <cfRule type="cellIs" dxfId="137" priority="173" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ24:AJ25">
-    <cfRule type="cellIs" dxfId="78" priority="168" operator="notEqual">
+    <cfRule type="cellIs" dxfId="136" priority="170" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL24:AL25">
-    <cfRule type="cellIs" dxfId="77" priority="169" operator="notEqual">
+    <cfRule type="cellIs" dxfId="135" priority="171" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ20:AJ21">
-    <cfRule type="cellIs" dxfId="76" priority="167" operator="notEqual">
+    <cfRule type="cellIs" dxfId="134" priority="169" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ16:AJ17">
-    <cfRule type="cellIs" dxfId="75" priority="166" operator="notEqual">
+    <cfRule type="cellIs" dxfId="133" priority="168" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ28:AJ29">
-    <cfRule type="cellIs" dxfId="74" priority="162" operator="notEqual">
+    <cfRule type="cellIs" dxfId="132" priority="164" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL28:AL29">
-    <cfRule type="cellIs" dxfId="73" priority="163" operator="notEqual">
+    <cfRule type="cellIs" dxfId="131" priority="165" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL36:AL37">
-    <cfRule type="cellIs" dxfId="72" priority="161" operator="notEqual">
+    <cfRule type="cellIs" dxfId="130" priority="163" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL40:AL41">
-    <cfRule type="cellIs" dxfId="71" priority="159" operator="notEqual">
+    <cfRule type="cellIs" dxfId="129" priority="161" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL44:AL45">
-    <cfRule type="cellIs" dxfId="70" priority="157" operator="notEqual">
+    <cfRule type="cellIs" dxfId="128" priority="159" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL48:AL49">
-    <cfRule type="cellIs" dxfId="69" priority="155" operator="notEqual">
+    <cfRule type="cellIs" dxfId="127" priority="157" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S20:S21 AB20:AB21 AG20:AG21">
-    <cfRule type="cellIs" dxfId="68" priority="132" operator="notEqual">
+    <cfRule type="cellIs" dxfId="126" priority="134" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S24:S25 AB24:AB25 AG24:AG25">
-    <cfRule type="cellIs" dxfId="67" priority="131" operator="notEqual">
+    <cfRule type="cellIs" dxfId="125" priority="133" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S16:S17 AB16:AB17 AG16:AG17">
-    <cfRule type="cellIs" dxfId="66" priority="133" operator="notEqual">
+    <cfRule type="cellIs" dxfId="124" priority="135" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S28:S29 AB28:AB29 AG28:AG29">
-    <cfRule type="cellIs" dxfId="65" priority="130" operator="notEqual">
+    <cfRule type="cellIs" dxfId="123" priority="132" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ32:AJ33">
-    <cfRule type="cellIs" dxfId="64" priority="128" operator="notEqual">
+    <cfRule type="cellIs" dxfId="122" priority="130" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL32:AL33">
-    <cfRule type="cellIs" dxfId="63" priority="129" operator="notEqual">
+    <cfRule type="cellIs" dxfId="121" priority="131" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S32:S33 AB32:AB33 AG32:AG33">
-    <cfRule type="cellIs" dxfId="62" priority="127" operator="notEqual">
+    <cfRule type="cellIs" dxfId="120" priority="129" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ36:AJ37">
-    <cfRule type="cellIs" dxfId="61" priority="126" operator="notEqual">
+    <cfRule type="cellIs" dxfId="119" priority="128" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S36:S37 AB36:AB37 AG36:AG37">
-    <cfRule type="cellIs" dxfId="60" priority="125" operator="notEqual">
+    <cfRule type="cellIs" dxfId="118" priority="127" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ40:AJ41">
-    <cfRule type="cellIs" dxfId="59" priority="124" operator="notEqual">
+    <cfRule type="cellIs" dxfId="117" priority="126" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S40:S41 AB40:AB41 AG40:AG41">
-    <cfRule type="cellIs" dxfId="58" priority="123" operator="notEqual">
+    <cfRule type="cellIs" dxfId="116" priority="125" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ44:AJ45">
-    <cfRule type="cellIs" dxfId="57" priority="122" operator="notEqual">
+    <cfRule type="cellIs" dxfId="115" priority="124" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S44:S45 AB44:AB45 AG44:AG45">
-    <cfRule type="cellIs" dxfId="56" priority="121" operator="notEqual">
+    <cfRule type="cellIs" dxfId="114" priority="123" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ48:AJ49">
-    <cfRule type="cellIs" dxfId="55" priority="120" operator="notEqual">
+    <cfRule type="cellIs" dxfId="113" priority="122" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S48:S49 AB48:AB49 AG48:AG49">
-    <cfRule type="cellIs" dxfId="54" priority="119" operator="notEqual">
+    <cfRule type="cellIs" dxfId="112" priority="121" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S51:S53 AB51:AB53 AG51:AG53 AJ51:AJ53">
-    <cfRule type="cellIs" dxfId="53" priority="100" operator="notEqual">
+    <cfRule type="cellIs" dxfId="111" priority="102" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL51:AL53">
-    <cfRule type="cellIs" dxfId="52" priority="99" operator="notEqual">
+    <cfRule type="cellIs" dxfId="110" priority="101" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S55:S57 AB55:AB57 AG55:AG57 AJ55:AJ57">
-    <cfRule type="cellIs" dxfId="51" priority="98" operator="notEqual">
+    <cfRule type="cellIs" dxfId="109" priority="100" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL55:AL57">
-    <cfRule type="cellIs" dxfId="50" priority="97" operator="notEqual">
+    <cfRule type="cellIs" dxfId="108" priority="99" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S59:S61 AB59:AB61 AG59:AG61 AJ59:AJ61">
-    <cfRule type="cellIs" dxfId="49" priority="96" operator="notEqual">
+    <cfRule type="cellIs" dxfId="107" priority="98" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL59:AL61">
-    <cfRule type="cellIs" dxfId="48" priority="95" operator="notEqual">
+    <cfRule type="cellIs" dxfId="106" priority="97" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S63:S65 AB63:AB65 AG63:AG65 AJ63:AJ65">
-    <cfRule type="cellIs" dxfId="47" priority="94" operator="notEqual">
+    <cfRule type="cellIs" dxfId="105" priority="96" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL63:AL65">
-    <cfRule type="cellIs" dxfId="46" priority="93" operator="notEqual">
+    <cfRule type="cellIs" dxfId="104" priority="95" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S67:S69 AB67:AB69 AG67:AG69 AJ67:AJ69">
-    <cfRule type="cellIs" dxfId="45" priority="92" operator="notEqual">
+    <cfRule type="cellIs" dxfId="103" priority="94" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL67:AL69">
-    <cfRule type="cellIs" dxfId="44" priority="91" operator="notEqual">
+    <cfRule type="cellIs" dxfId="102" priority="93" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S71:S73 AB71:AB73 AG71:AG73 AJ71:AJ73">
-    <cfRule type="cellIs" dxfId="43" priority="90" operator="notEqual">
+    <cfRule type="cellIs" dxfId="101" priority="92" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL71:AL73">
-    <cfRule type="cellIs" dxfId="42" priority="89" operator="notEqual">
+    <cfRule type="cellIs" dxfId="100" priority="91" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S75:S77 AB75:AB77 AG75:AG77 AJ75:AJ77">
-    <cfRule type="cellIs" dxfId="41" priority="88" operator="notEqual">
+    <cfRule type="cellIs" dxfId="99" priority="90" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL75:AL77">
-    <cfRule type="cellIs" dxfId="40" priority="87" operator="notEqual">
+    <cfRule type="cellIs" dxfId="98" priority="89" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S79:S81 AB79:AB81 AG79:AG81 AJ79:AJ81">
-    <cfRule type="cellIs" dxfId="39" priority="86" operator="notEqual">
+    <cfRule type="cellIs" dxfId="97" priority="88" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL79:AL81">
-    <cfRule type="cellIs" dxfId="38" priority="85" operator="notEqual">
+    <cfRule type="cellIs" dxfId="96" priority="87" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98:D98">
-    <cfRule type="dataBar" priority="25">
+    <cfRule type="dataBar" priority="27">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -16254,98 +16728,78 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH82:AI82 C82:R82 T82:AA82 AC82:AF82">
-    <cfRule type="cellIs" dxfId="37" priority="74" stopIfTrue="1" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH90:AI90 C90:R90 T90:AA90 AC90:AF90">
-    <cfRule type="cellIs" dxfId="36" priority="73" stopIfTrue="1" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="S82 AB82 AG82 AJ82 AJ90 AG90 AB90 S90">
-    <cfRule type="cellIs" dxfId="35" priority="72" operator="notEqual">
+    <cfRule type="cellIs" dxfId="95" priority="74" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL82 AL90">
-    <cfRule type="cellIs" dxfId="34" priority="71" operator="notEqual">
+    <cfRule type="cellIs" dxfId="94" priority="73" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S83:S85 AB83:AB85 AG83:AG85 AJ83:AJ85">
-    <cfRule type="cellIs" dxfId="33" priority="70" operator="notEqual">
+    <cfRule type="cellIs" dxfId="93" priority="72" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL83:AL85">
-    <cfRule type="cellIs" dxfId="32" priority="69" operator="notEqual">
+    <cfRule type="cellIs" dxfId="92" priority="71" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S91:S93 AB91:AB93 AG91:AG93 AJ91:AJ93">
-    <cfRule type="cellIs" dxfId="31" priority="68" operator="notEqual">
+    <cfRule type="cellIs" dxfId="91" priority="70" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL91:AL93">
-    <cfRule type="cellIs" dxfId="30" priority="67" operator="notEqual">
+    <cfRule type="cellIs" dxfId="90" priority="69" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH94:AI94 C94:R94 T94:AA94 AC94:AF94">
-    <cfRule type="cellIs" dxfId="29" priority="66" stopIfTrue="1" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="S94 AB94 AG94 AJ94">
-    <cfRule type="cellIs" dxfId="28" priority="64" operator="notEqual">
+    <cfRule type="cellIs" dxfId="89" priority="66" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL94">
-    <cfRule type="cellIs" dxfId="27" priority="63" operator="notEqual">
+    <cfRule type="cellIs" dxfId="88" priority="65" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S95:S97 AB95:AB97 AG95:AG97 AJ95:AJ97">
-    <cfRule type="cellIs" dxfId="26" priority="62" operator="notEqual">
+    <cfRule type="cellIs" dxfId="87" priority="64" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL95:AL97">
-    <cfRule type="cellIs" dxfId="25" priority="61" operator="notEqual">
+    <cfRule type="cellIs" dxfId="86" priority="63" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH86:AI86 C86:R86 T86:AA86 AC86:AF86">
-    <cfRule type="cellIs" dxfId="24" priority="30" stopIfTrue="1" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="S86 AB86 AG86 AJ86">
-    <cfRule type="cellIs" dxfId="23" priority="29" operator="notEqual">
+    <cfRule type="cellIs" dxfId="85" priority="31" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL86">
-    <cfRule type="cellIs" dxfId="22" priority="28" operator="notEqual">
+    <cfRule type="cellIs" dxfId="84" priority="30" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S87:S89 AB87:AB89 AG87:AG89 AJ87:AJ89">
-    <cfRule type="cellIs" dxfId="21" priority="27" operator="notEqual">
+    <cfRule type="cellIs" dxfId="83" priority="29" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL87:AL89">
-    <cfRule type="cellIs" dxfId="20" priority="26" operator="notEqual">
+    <cfRule type="cellIs" dxfId="82" priority="28" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK10:AK94">
-    <cfRule type="dataBar" priority="17">
+    <cfRule type="dataBar" priority="19">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -16359,7 +16813,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E98:F98">
-    <cfRule type="dataBar" priority="15">
+    <cfRule type="dataBar" priority="17">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -16373,7 +16827,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G98:H98">
-    <cfRule type="dataBar" priority="14">
+    <cfRule type="dataBar" priority="16">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -16387,7 +16841,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I98:J98">
-    <cfRule type="dataBar" priority="13">
+    <cfRule type="dataBar" priority="15">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -16401,7 +16855,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K98:L98">
-    <cfRule type="dataBar" priority="12">
+    <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -16415,7 +16869,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M98:N98">
-    <cfRule type="dataBar" priority="11">
+    <cfRule type="dataBar" priority="13">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -16429,7 +16883,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O98:P98">
-    <cfRule type="dataBar" priority="10">
+    <cfRule type="dataBar" priority="12">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -16443,7 +16897,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q98:R98">
-    <cfRule type="dataBar" priority="9">
+    <cfRule type="dataBar" priority="11">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -16457,7 +16911,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T98:U98">
-    <cfRule type="dataBar" priority="4">
+    <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -16471,7 +16925,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V98:W98">
-    <cfRule type="dataBar" priority="3">
+    <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -16485,7 +16939,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X98:Y98">
-    <cfRule type="dataBar" priority="2">
+    <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -16499,7 +16953,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z98:AA98">
-    <cfRule type="dataBar" priority="1">
+    <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -16510,6 +16964,11 @@
           <x14:id>{B0535630-473C-4E46-A99F-93A267D87F22}</x14:id>
         </ext>
       </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10:R94 T10:AA94 AC10:AF94 AH10:AI94">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -16679,7 +17138,7 @@
   <dimension ref="A1:AJ31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17853,7 +18312,9 @@
       <c r="R24" s="82">
         <v>2</v>
       </c>
-      <c r="S24" s="82"/>
+      <c r="S24" s="82">
+        <v>1</v>
+      </c>
       <c r="T24" s="82"/>
       <c r="U24" s="81"/>
       <c r="V24" s="73">
@@ -17922,12 +18383,14 @@
       <c r="R25" s="82">
         <v>4</v>
       </c>
-      <c r="S25" s="82"/>
+      <c r="S25" s="82">
+        <v>2</v>
+      </c>
       <c r="T25" s="82"/>
       <c r="U25" s="81"/>
       <c r="V25" s="73">
         <f>IF(O25&gt;O24,1,0)+IF(P25&gt;P24,1,0)+IF(Q25&gt;Q24,1,0)+IF(R25&gt;R24,1,0)+IF(S25&gt;S24,1,0)+IF(T25&gt;T24,1,0)+IF(U25&gt;U24,1,0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y25" s="86"/>
       <c r="Z25" s="86"/>
@@ -18139,102 +18602,102 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C3:I3 C6:I6 O20:U20 C13:I13 AA8:AG8 AA15:AG15 O10:U10 O6:Q6 C10:I10 C24 C20:E20 C17:I17 O24:U24 AA22:AG22 F24:I24 G20:I20 C27:I27 S6:U6">
-    <cfRule type="cellIs" dxfId="19" priority="27" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="158" priority="27" stopIfTrue="1" operator="greaterThan">
       <formula>C4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:I4 C7:I7 O21:U21 C14:I14 AA9:AG9 AA16:AG16 O11:U11 O7:Q7 C11:I11 C25 C21:E21 C18:I18 O25:U25 AA23:AG23 F25:I25 G21:I21 C28:I28 S7:U7">
-    <cfRule type="cellIs" dxfId="18" priority="28" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="157" priority="28" stopIfTrue="1" operator="greaterThan">
       <formula>C3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:I3 C6:I6 O20:U20 C13:I13 AA8:AG8 AA15:AG15 O10:U10 O6:Q6 C10:I10 C24 C20:E20 C17:I17 O24:U24 AA22:AG22 F24:I24 G20:I20 C27:I27 S6:U6">
-    <cfRule type="cellIs" dxfId="17" priority="18" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="156" priority="18" stopIfTrue="1" operator="greaterThan">
       <formula>C4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:I4 C7:I7 O21:U21 C14:I14 AA9:AG9 AA16:AG16 O11:U11 O7:Q7 C11:I11 C25 C21:E21 C18:I18 O25:U25 AA23:AG23 F25:I25 G21:I21 C28:I28 S7:U7">
-    <cfRule type="cellIs" dxfId="16" priority="17" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="155" priority="17" stopIfTrue="1" operator="greaterThan">
       <formula>C3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24">
-    <cfRule type="cellIs" dxfId="15" priority="15" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="154" priority="15" stopIfTrue="1" operator="greaterThan">
       <formula>D25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25">
-    <cfRule type="cellIs" dxfId="14" priority="16" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="153" priority="16" stopIfTrue="1" operator="greaterThan">
       <formula>D24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24">
-    <cfRule type="cellIs" dxfId="13" priority="14" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="152" priority="14" stopIfTrue="1" operator="greaterThan">
       <formula>D25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25">
-    <cfRule type="cellIs" dxfId="12" priority="13" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="151" priority="13" stopIfTrue="1" operator="greaterThan">
       <formula>D24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="11" priority="11" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="150" priority="11" stopIfTrue="1" operator="greaterThan">
       <formula>E25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="10" priority="12" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="149" priority="12" stopIfTrue="1" operator="greaterThan">
       <formula>E24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="9" priority="10" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="148" priority="10" stopIfTrue="1" operator="greaterThan">
       <formula>E25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="8" priority="9" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="147" priority="9" stopIfTrue="1" operator="greaterThan">
       <formula>E24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20">
-    <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="146" priority="7" stopIfTrue="1" operator="greaterThan">
       <formula>F21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21">
-    <cfRule type="cellIs" dxfId="6" priority="8" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="145" priority="8" stopIfTrue="1" operator="greaterThan">
       <formula>F20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20">
-    <cfRule type="cellIs" dxfId="5" priority="6" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="144" priority="6" stopIfTrue="1" operator="greaterThan">
       <formula>F21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21">
-    <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="143" priority="5" stopIfTrue="1" operator="greaterThan">
       <formula>F20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R6">
-    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="142" priority="3" stopIfTrue="1" operator="greaterThan">
       <formula>R7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7">
-    <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="141" priority="4" stopIfTrue="1" operator="greaterThan">
       <formula>R6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R6">
-    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="140" priority="2" stopIfTrue="1" operator="greaterThan">
       <formula>R7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7">
-    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="139" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>R6</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated games of 2019-05-04
</commit_message>
<xml_diff>
--- a/laval.xlsx
+++ b/laval.xlsx
@@ -2496,6 +2496,135 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2505,18 +2634,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="83" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="85" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="92" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2528,150 +2672,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="83" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="85" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2681,612 +2681,11 @@
     <cellStyle name="Monétaire" xfId="4" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="159">
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="78">
     <dxf>
       <fill>
         <patternFill>
           <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3424,9 +2823,12 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor indexed="13"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4000,146 +3402,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -4475,217 +3737,217 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="C1" s="270"/>
-      <c r="D1" s="270"/>
-      <c r="E1" s="270"/>
-      <c r="F1" s="270"/>
-      <c r="G1" s="270"/>
-      <c r="H1" s="270"/>
-      <c r="I1" s="270"/>
-      <c r="J1" s="270"/>
-      <c r="K1" s="270"/>
-      <c r="L1" s="270"/>
-      <c r="M1" s="270"/>
-      <c r="N1" s="270"/>
-      <c r="O1" s="270"/>
-      <c r="P1" s="271"/>
-      <c r="Q1" s="271"/>
-      <c r="R1" s="271"/>
-      <c r="S1" s="271"/>
-      <c r="T1" s="271"/>
-      <c r="U1" s="271"/>
-      <c r="V1" s="271"/>
-      <c r="W1" s="271"/>
-      <c r="X1" s="271"/>
-      <c r="Y1" s="271"/>
-      <c r="Z1" s="271"/>
-      <c r="AA1" s="271"/>
-      <c r="AB1" s="271"/>
-      <c r="AC1" s="271"/>
-      <c r="AD1" s="271"/>
-      <c r="AE1" s="271"/>
-      <c r="AF1" s="271"/>
-      <c r="AG1" s="271"/>
-      <c r="AH1" s="271"/>
-      <c r="AI1" s="271"/>
-      <c r="AJ1" s="271"/>
+      <c r="C1" s="285"/>
+      <c r="D1" s="285"/>
+      <c r="E1" s="285"/>
+      <c r="F1" s="285"/>
+      <c r="G1" s="285"/>
+      <c r="H1" s="285"/>
+      <c r="I1" s="285"/>
+      <c r="J1" s="285"/>
+      <c r="K1" s="285"/>
+      <c r="L1" s="285"/>
+      <c r="M1" s="285"/>
+      <c r="N1" s="285"/>
+      <c r="O1" s="285"/>
+      <c r="P1" s="286"/>
+      <c r="Q1" s="286"/>
+      <c r="R1" s="286"/>
+      <c r="S1" s="286"/>
+      <c r="T1" s="286"/>
+      <c r="U1" s="286"/>
+      <c r="V1" s="286"/>
+      <c r="W1" s="286"/>
+      <c r="X1" s="286"/>
+      <c r="Y1" s="286"/>
+      <c r="Z1" s="286"/>
+      <c r="AA1" s="286"/>
+      <c r="AB1" s="286"/>
+      <c r="AC1" s="286"/>
+      <c r="AD1" s="286"/>
+      <c r="AE1" s="286"/>
+      <c r="AF1" s="286"/>
+      <c r="AG1" s="286"/>
+      <c r="AH1" s="286"/>
+      <c r="AI1" s="286"/>
+      <c r="AJ1" s="286"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="41"/>
-      <c r="C2" s="272" t="s">
+      <c r="C2" s="287" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="272"/>
-      <c r="E2" s="272"/>
-      <c r="F2" s="272"/>
-      <c r="G2" s="272"/>
-      <c r="H2" s="272"/>
-      <c r="I2" s="272"/>
-      <c r="J2" s="272"/>
-      <c r="K2" s="272"/>
-      <c r="L2" s="272"/>
-      <c r="M2" s="272"/>
-      <c r="N2" s="272"/>
-      <c r="O2" s="272"/>
-      <c r="P2" s="272"/>
-      <c r="Q2" s="273" t="s">
+      <c r="D2" s="287"/>
+      <c r="E2" s="287"/>
+      <c r="F2" s="287"/>
+      <c r="G2" s="287"/>
+      <c r="H2" s="287"/>
+      <c r="I2" s="287"/>
+      <c r="J2" s="287"/>
+      <c r="K2" s="287"/>
+      <c r="L2" s="287"/>
+      <c r="M2" s="287"/>
+      <c r="N2" s="287"/>
+      <c r="O2" s="287"/>
+      <c r="P2" s="287"/>
+      <c r="Q2" s="288" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="271"/>
-      <c r="S2" s="271"/>
-      <c r="T2" s="271"/>
-      <c r="U2" s="271"/>
-      <c r="V2" s="271"/>
-      <c r="W2" s="271"/>
-      <c r="X2" s="271"/>
-      <c r="Y2" s="271"/>
-      <c r="Z2" s="271"/>
-      <c r="AA2" s="271"/>
-      <c r="AB2" s="271"/>
-      <c r="AC2" s="271"/>
-      <c r="AD2" s="271"/>
-      <c r="AE2" s="271"/>
-      <c r="AF2" s="271"/>
-      <c r="AG2" s="271"/>
-      <c r="AH2" s="271"/>
-      <c r="AI2" s="271"/>
-      <c r="AJ2" s="271"/>
+      <c r="R2" s="286"/>
+      <c r="S2" s="286"/>
+      <c r="T2" s="286"/>
+      <c r="U2" s="286"/>
+      <c r="V2" s="286"/>
+      <c r="W2" s="286"/>
+      <c r="X2" s="286"/>
+      <c r="Y2" s="286"/>
+      <c r="Z2" s="286"/>
+      <c r="AA2" s="286"/>
+      <c r="AB2" s="286"/>
+      <c r="AC2" s="286"/>
+      <c r="AD2" s="286"/>
+      <c r="AE2" s="286"/>
+      <c r="AF2" s="286"/>
+      <c r="AG2" s="286"/>
+      <c r="AH2" s="286"/>
+      <c r="AI2" s="286"/>
+      <c r="AJ2" s="286"/>
     </row>
     <row r="3" spans="1:38" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="270"/>
-      <c r="D3" s="270"/>
-      <c r="E3" s="270"/>
-      <c r="F3" s="270"/>
-      <c r="G3" s="270"/>
-      <c r="H3" s="270"/>
-      <c r="I3" s="270"/>
-      <c r="J3" s="270"/>
-      <c r="K3" s="270"/>
-      <c r="L3" s="270"/>
-      <c r="M3" s="270"/>
-      <c r="N3" s="270"/>
-      <c r="O3" s="270"/>
-      <c r="P3" s="271"/>
-      <c r="Q3" s="271"/>
-      <c r="R3" s="271"/>
-      <c r="S3" s="271"/>
-      <c r="T3" s="271"/>
-      <c r="U3" s="271"/>
-      <c r="V3" s="271"/>
-      <c r="W3" s="271"/>
-      <c r="X3" s="271"/>
-      <c r="Y3" s="271"/>
-      <c r="Z3" s="271"/>
-      <c r="AA3" s="271"/>
-      <c r="AB3" s="271"/>
-      <c r="AC3" s="271"/>
-      <c r="AD3" s="271"/>
-      <c r="AE3" s="271"/>
-      <c r="AF3" s="271"/>
-      <c r="AG3" s="271"/>
-      <c r="AH3" s="271"/>
-      <c r="AI3" s="271"/>
-      <c r="AJ3" s="271"/>
+      <c r="C3" s="285"/>
+      <c r="D3" s="285"/>
+      <c r="E3" s="285"/>
+      <c r="F3" s="285"/>
+      <c r="G3" s="285"/>
+      <c r="H3" s="285"/>
+      <c r="I3" s="285"/>
+      <c r="J3" s="285"/>
+      <c r="K3" s="285"/>
+      <c r="L3" s="285"/>
+      <c r="M3" s="285"/>
+      <c r="N3" s="285"/>
+      <c r="O3" s="285"/>
+      <c r="P3" s="286"/>
+      <c r="Q3" s="286"/>
+      <c r="R3" s="286"/>
+      <c r="S3" s="286"/>
+      <c r="T3" s="286"/>
+      <c r="U3" s="286"/>
+      <c r="V3" s="286"/>
+      <c r="W3" s="286"/>
+      <c r="X3" s="286"/>
+      <c r="Y3" s="286"/>
+      <c r="Z3" s="286"/>
+      <c r="AA3" s="286"/>
+      <c r="AB3" s="286"/>
+      <c r="AC3" s="286"/>
+      <c r="AD3" s="286"/>
+      <c r="AE3" s="286"/>
+      <c r="AF3" s="286"/>
+      <c r="AG3" s="286"/>
+      <c r="AH3" s="286"/>
+      <c r="AI3" s="286"/>
+      <c r="AJ3" s="286"/>
     </row>
     <row r="4" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="295" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="296"/>
-      <c r="E4" s="296"/>
-      <c r="F4" s="296"/>
-      <c r="G4" s="296"/>
-      <c r="H4" s="296"/>
-      <c r="I4" s="296"/>
-      <c r="J4" s="296"/>
-      <c r="K4" s="296"/>
-      <c r="L4" s="296"/>
-      <c r="M4" s="296"/>
-      <c r="N4" s="296"/>
-      <c r="O4" s="296"/>
-      <c r="P4" s="296"/>
-      <c r="Q4" s="296"/>
-      <c r="R4" s="296"/>
-      <c r="S4" s="297"/>
-      <c r="T4" s="295" t="s">
+      <c r="C4" s="269" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="270"/>
+      <c r="E4" s="270"/>
+      <c r="F4" s="270"/>
+      <c r="G4" s="270"/>
+      <c r="H4" s="270"/>
+      <c r="I4" s="270"/>
+      <c r="J4" s="270"/>
+      <c r="K4" s="270"/>
+      <c r="L4" s="270"/>
+      <c r="M4" s="270"/>
+      <c r="N4" s="270"/>
+      <c r="O4" s="270"/>
+      <c r="P4" s="270"/>
+      <c r="Q4" s="270"/>
+      <c r="R4" s="270"/>
+      <c r="S4" s="271"/>
+      <c r="T4" s="269" t="s">
         <v>1</v>
       </c>
-      <c r="U4" s="296"/>
-      <c r="V4" s="296"/>
-      <c r="W4" s="296"/>
-      <c r="X4" s="296"/>
-      <c r="Y4" s="296"/>
-      <c r="Z4" s="296"/>
-      <c r="AA4" s="296"/>
-      <c r="AB4" s="297"/>
-      <c r="AC4" s="295" t="s">
+      <c r="U4" s="270"/>
+      <c r="V4" s="270"/>
+      <c r="W4" s="270"/>
+      <c r="X4" s="270"/>
+      <c r="Y4" s="270"/>
+      <c r="Z4" s="270"/>
+      <c r="AA4" s="270"/>
+      <c r="AB4" s="271"/>
+      <c r="AC4" s="269" t="s">
         <v>2</v>
       </c>
-      <c r="AD4" s="296"/>
-      <c r="AE4" s="296"/>
-      <c r="AF4" s="296"/>
-      <c r="AG4" s="304"/>
-      <c r="AH4" s="295" t="s">
+      <c r="AD4" s="270"/>
+      <c r="AE4" s="270"/>
+      <c r="AF4" s="270"/>
+      <c r="AG4" s="280"/>
+      <c r="AH4" s="269" t="s">
         <v>10</v>
       </c>
-      <c r="AI4" s="296"/>
-      <c r="AJ4" s="297"/>
+      <c r="AI4" s="270"/>
+      <c r="AJ4" s="271"/>
     </row>
     <row r="5" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="264" t="s">
+      <c r="C5" s="281" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="265"/>
-      <c r="E5" s="265"/>
-      <c r="F5" s="265"/>
-      <c r="G5" s="265"/>
-      <c r="H5" s="265"/>
-      <c r="I5" s="265"/>
-      <c r="J5" s="266"/>
-      <c r="K5" s="302" t="s">
+      <c r="D5" s="277"/>
+      <c r="E5" s="277"/>
+      <c r="F5" s="277"/>
+      <c r="G5" s="277"/>
+      <c r="H5" s="277"/>
+      <c r="I5" s="277"/>
+      <c r="J5" s="278"/>
+      <c r="K5" s="276" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="265"/>
-      <c r="M5" s="265"/>
-      <c r="N5" s="265"/>
-      <c r="O5" s="265"/>
-      <c r="P5" s="265"/>
-      <c r="Q5" s="265"/>
-      <c r="R5" s="266"/>
-      <c r="S5" s="298" t="s">
+      <c r="L5" s="277"/>
+      <c r="M5" s="277"/>
+      <c r="N5" s="277"/>
+      <c r="O5" s="277"/>
+      <c r="P5" s="277"/>
+      <c r="Q5" s="277"/>
+      <c r="R5" s="278"/>
+      <c r="S5" s="272" t="s">
         <v>12</v>
       </c>
-      <c r="T5" s="264" t="s">
+      <c r="T5" s="281" t="s">
         <v>9</v>
       </c>
-      <c r="U5" s="265"/>
-      <c r="V5" s="265"/>
-      <c r="W5" s="266"/>
-      <c r="X5" s="302" t="s">
+      <c r="U5" s="277"/>
+      <c r="V5" s="277"/>
+      <c r="W5" s="278"/>
+      <c r="X5" s="276" t="s">
         <v>8</v>
       </c>
-      <c r="Y5" s="265"/>
-      <c r="Z5" s="265"/>
-      <c r="AA5" s="266"/>
-      <c r="AB5" s="298" t="s">
+      <c r="Y5" s="277"/>
+      <c r="Z5" s="277"/>
+      <c r="AA5" s="278"/>
+      <c r="AB5" s="272" t="s">
         <v>13</v>
       </c>
-      <c r="AC5" s="303" t="s">
+      <c r="AC5" s="279" t="s">
         <v>9</v>
       </c>
-      <c r="AD5" s="266"/>
-      <c r="AE5" s="302" t="s">
+      <c r="AD5" s="278"/>
+      <c r="AE5" s="276" t="s">
         <v>8</v>
       </c>
-      <c r="AF5" s="266"/>
-      <c r="AG5" s="298" t="s">
+      <c r="AF5" s="278"/>
+      <c r="AG5" s="272" t="s">
         <v>14</v>
       </c>
       <c r="AH5" s="56"/>
       <c r="AI5" s="25"/>
-      <c r="AJ5" s="298" t="s">
+      <c r="AJ5" s="272" t="s">
         <v>15</v>
       </c>
       <c r="AK5" s="4"/>
@@ -4757,10 +4019,10 @@
         <f>Résultats!$J$28</f>
         <v>3</v>
       </c>
-      <c r="S6" s="299"/>
+      <c r="S6" s="273"/>
       <c r="T6" s="156">
         <f>Résultats!$V$6</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U6" s="103">
         <f>Résultats!$V$7</f>
@@ -4776,7 +4038,7 @@
       </c>
       <c r="X6" s="105">
         <f>Résultats!$V$20</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y6" s="104">
         <f>Résultats!$V$21</f>
@@ -4790,7 +4052,7 @@
         <f>Résultats!$V$25</f>
         <v>3</v>
       </c>
-      <c r="AB6" s="299"/>
+      <c r="AB6" s="273"/>
       <c r="AC6" s="106">
         <f>Résultats!$AH$8</f>
         <v>0</v>
@@ -4807,7 +4069,7 @@
         <f>Résultats!$AH$23</f>
         <v>0</v>
       </c>
-      <c r="AG6" s="299"/>
+      <c r="AG6" s="273"/>
       <c r="AH6" s="173">
         <f>Résultats!$AH$15</f>
         <v>0</v>
@@ -4816,7 +4078,7 @@
         <f>Résultats!$AH$16</f>
         <v>0</v>
       </c>
-      <c r="AJ6" s="299"/>
+      <c r="AJ6" s="273"/>
       <c r="AK6" s="37"/>
     </row>
     <row r="7" spans="1:38" s="39" customFormat="1" ht="58.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -4842,7 +4104,7 @@
       <c r="P7" s="203"/>
       <c r="Q7" s="207"/>
       <c r="R7" s="112"/>
-      <c r="S7" s="299"/>
+      <c r="S7" s="273"/>
       <c r="T7" s="157"/>
       <c r="U7" s="112"/>
       <c r="V7" s="160"/>
@@ -4851,15 +4113,15 @@
       <c r="Y7" s="113"/>
       <c r="Z7" s="114"/>
       <c r="AA7" s="112"/>
-      <c r="AB7" s="299"/>
+      <c r="AB7" s="273"/>
       <c r="AC7" s="114"/>
       <c r="AD7" s="112"/>
       <c r="AE7" s="115"/>
       <c r="AF7" s="112"/>
-      <c r="AG7" s="299"/>
+      <c r="AG7" s="273"/>
       <c r="AH7" s="173"/>
       <c r="AI7" s="107"/>
-      <c r="AJ7" s="299"/>
+      <c r="AJ7" s="273"/>
       <c r="AK7" s="37"/>
     </row>
     <row r="8" spans="1:38" s="39" customFormat="1" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4929,7 +4191,7 @@
         <f>Résultats!$B$28</f>
         <v>VEGAS</v>
       </c>
-      <c r="S8" s="299"/>
+      <c r="S8" s="273"/>
       <c r="T8" s="158" t="str">
         <f>Résultats!$N$6</f>
         <v>BOSTON</v>
@@ -4962,7 +4224,7 @@
         <f>Résultats!$N$25</f>
         <v>DALLAS</v>
       </c>
-      <c r="AB8" s="299"/>
+      <c r="AB8" s="273"/>
       <c r="AC8" s="164" t="str">
         <f>Résultats!$Z$8</f>
         <v xml:space="preserve"> </v>
@@ -4979,7 +4241,7 @@
         <f>Résultats!$Z$23</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AG8" s="299"/>
+      <c r="AG8" s="273"/>
       <c r="AH8" s="174" t="str">
         <f>Résultats!$Z$15</f>
         <v xml:space="preserve"> </v>
@@ -4988,7 +4250,7 @@
         <f>Résultats!$Z$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ8" s="299"/>
+      <c r="AJ8" s="273"/>
       <c r="AK8" s="37"/>
     </row>
     <row r="9" spans="1:38" s="39" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5062,7 +4324,7 @@
         <f>Résultats!$A$28</f>
         <v>P3</v>
       </c>
-      <c r="S9" s="301"/>
+      <c r="S9" s="275"/>
       <c r="T9" s="166" t="str">
         <f>Résultats!$M$6</f>
         <v>A2</v>
@@ -5095,7 +4357,7 @@
         <f>Résultats!$M$25</f>
         <v>WC1</v>
       </c>
-      <c r="AB9" s="300"/>
+      <c r="AB9" s="274"/>
       <c r="AC9" s="170" t="str">
         <f>Résultats!$Y$8</f>
         <v xml:space="preserve"> </v>
@@ -5112,7 +4374,7 @@
         <f>Résultats!$Y$23</f>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="AG9" s="300"/>
+      <c r="AG9" s="274"/>
       <c r="AH9" s="176" t="str">
         <f>Résultats!$Y$15</f>
         <v xml:space="preserve"> </v>
@@ -5121,7 +4383,7 @@
         <f>Résultats!$Y$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ9" s="301"/>
+      <c r="AJ9" s="275"/>
       <c r="AK9" s="109" t="s">
         <v>51</v>
       </c>
@@ -5191,7 +4453,7 @@
       </c>
       <c r="AB10" s="225">
         <f>SUM(T11:AA11)</f>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="AC10" s="221"/>
       <c r="AD10" s="222"/>
@@ -5213,7 +4475,7 @@
       </c>
       <c r="AL10" s="225">
         <f>$S10+$AB10+$AG10+$AJ10</f>
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -5265,7 +4527,7 @@
       <c r="S11" s="121"/>
       <c r="T11" s="126">
         <f>(IF($T10&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T10=$T$6+$U$6,$P$103,0),0),0)+IF($U10&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U10=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U11" s="126"/>
       <c r="V11" s="126">
@@ -5275,7 +4537,7 @@
       <c r="W11" s="126"/>
       <c r="X11" s="126">
         <f>(IF($X10&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X10=$X$6+$Y$6,$P$103,0),0),0)+IF($Y10&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y10=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y11" s="59"/>
       <c r="Z11" s="126">
@@ -5687,7 +4949,7 @@
       <c r="AA14" s="50"/>
       <c r="AB14" s="122">
         <f>SUM(T15:AA15)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AC14" s="48"/>
       <c r="AD14" s="47"/>
@@ -5705,11 +4967,11 @@
       </c>
       <c r="AK14" s="111">
         <f>MAX($AL$10:$AL$97) - AL14</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AL14" s="122">
         <f>$S14+$AB14+$AG14+$AJ14</f>
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5771,7 +5033,7 @@
       <c r="W15" s="126"/>
       <c r="X15" s="126">
         <f>(IF($X14&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X14=$X$6+$Y$6,$P$103,0),0),0)+IF($Y14&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y14=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y15" s="59"/>
       <c r="Z15" s="126">
@@ -5790,7 +5052,7 @@
       <c r="AJ15" s="121"/>
       <c r="AK15" s="92">
         <f>MAX($AL$10:$AL$97) - AL15</f>
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AL15" s="121"/>
     </row>
@@ -6186,7 +5448,7 @@
       <c r="AA18" s="237"/>
       <c r="AB18" s="239">
         <f>SUM(T19:AA19)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AC18" s="232"/>
       <c r="AD18" s="233"/>
@@ -6204,11 +5466,11 @@
       </c>
       <c r="AK18" s="241">
         <f>MAX($AL$10:$AL$97) - AL18</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AL18" s="239">
         <f>$S18+$AB18+$AG18+$AJ18</f>
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6270,7 +5532,7 @@
       <c r="W19" s="126"/>
       <c r="X19" s="126">
         <f>(IF($X18&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X18=$X$6+$Y$6,$P$103,0),0),0)+IF($Y18&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y18=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y19" s="59"/>
       <c r="Z19" s="126">
@@ -6289,7 +5551,7 @@
       <c r="AJ19" s="144"/>
       <c r="AK19" s="150">
         <f>MAX($AL$10:$AL$97) - AL19</f>
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AL19" s="121"/>
     </row>
@@ -6685,7 +5947,7 @@
       </c>
       <c r="AB22" s="122">
         <f>SUM(T23:AA23)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AC22" s="48"/>
       <c r="AD22" s="47"/>
@@ -6703,11 +5965,11 @@
       </c>
       <c r="AK22" s="111">
         <f>MAX($AL$10:$AL$97) - AL22</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AL22" s="122">
         <f>$S22+$AB22+$AG22+$AJ22</f>
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6769,7 +6031,7 @@
       <c r="W23" s="126"/>
       <c r="X23" s="126">
         <f>(IF($X22&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X22=$X$6+$Y$6,$P$103,0),0),0)+IF($Y22&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y22=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y23" s="59"/>
       <c r="Z23" s="126">
@@ -6788,7 +6050,7 @@
       <c r="AJ23" s="144"/>
       <c r="AK23" s="150">
         <f>MAX($AL$10:$AL$97) - AL23</f>
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AL23" s="121"/>
     </row>
@@ -7125,7 +6387,7 @@
     <row r="26" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="216">
         <f>RANK(AL26,$AL$10:$AL$97,)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B26" s="217" t="s">
         <v>72</v>
@@ -7202,7 +6464,7 @@
       </c>
       <c r="AK26" s="241">
         <f>MAX($AL$10:$AL$97) - AL26</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AL26" s="239">
         <f>$S26+$AB26+$AG26+$AJ26</f>
@@ -7287,7 +6549,7 @@
       <c r="AJ27" s="144"/>
       <c r="AK27" s="150">
         <f>MAX($AL$10:$AL$97) - AL27</f>
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AL27" s="121"/>
     </row>
@@ -7701,7 +6963,7 @@
       </c>
       <c r="AK30" s="111">
         <f>MAX($AL$10:$AL$97) - AL30</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="AL30" s="122">
         <f>$S30+$AB30+$AG30+$AJ30</f>
@@ -7786,7 +7048,7 @@
       <c r="AJ31" s="121"/>
       <c r="AK31" s="92">
         <f>MAX($AL$10:$AL$97) - AL31</f>
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AL31" s="121"/>
     </row>
@@ -8200,7 +7462,7 @@
       </c>
       <c r="AK34" s="241">
         <f>MAX($AL$10:$AL$97) - AL34</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="AL34" s="239">
         <f>$S34+$AB34+$AG34+$AJ34</f>
@@ -8285,7 +7547,7 @@
       <c r="AJ35" s="121"/>
       <c r="AK35" s="92">
         <f>MAX($AL$10:$AL$97) - AL35</f>
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AL35" s="121"/>
     </row>
@@ -8681,7 +7943,7 @@
       <c r="AA38" s="47"/>
       <c r="AB38" s="122">
         <f>SUM(T39:AA39)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AC38" s="48"/>
       <c r="AD38" s="47"/>
@@ -8699,11 +7961,11 @@
       </c>
       <c r="AK38" s="111">
         <f>MAX($AL$10:$AL$97) - AL38</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AL38" s="122">
         <f>$S38+$AB38+$AG38+$AJ38</f>
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -8765,7 +8027,7 @@
       <c r="W39" s="126"/>
       <c r="X39" s="126">
         <f>(IF($X38&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X38=$X$6+$Y$6,$P$103,0),0),0)+IF($Y38&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y38=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y39" s="59"/>
       <c r="Z39" s="126">
@@ -8784,7 +8046,7 @@
       <c r="AJ39" s="121"/>
       <c r="AK39" s="92">
         <f>MAX($AL$10:$AL$97) - AL39</f>
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AL39" s="121"/>
     </row>
@@ -9198,7 +8460,7 @@
       </c>
       <c r="AK42" s="241">
         <f>MAX($AL$10:$AL$97) - AL42</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AL42" s="239">
         <f>$S42+$AB42+$AG42+$AJ42</f>
@@ -9283,7 +8545,7 @@
       <c r="AJ43" s="121"/>
       <c r="AK43" s="111">
         <f>MAX($AL$10:$AL$97) - AL43</f>
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AL43" s="121"/>
     </row>
@@ -9697,7 +8959,7 @@
       </c>
       <c r="AK46" s="111">
         <f>MAX($AL$10:$AL$97) - AL46</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AL46" s="122">
         <f>$S46+$AB46+$AG46+$AJ46</f>
@@ -9782,7 +9044,7 @@
       <c r="AJ47" s="121"/>
       <c r="AK47" s="111">
         <f>MAX($AL$10:$AL$97) - AL47</f>
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AL47" s="121"/>
     </row>
@@ -10196,7 +9458,7 @@
       </c>
       <c r="AK50" s="241">
         <f>MAX($AL$10:$AL$97) - AL50</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="AL50" s="239">
         <f>$S50+$AB50+$AG50+$AJ50</f>
@@ -10674,7 +9936,7 @@
       </c>
       <c r="AB54" s="122">
         <f>SUM(T55:AA55)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AC54" s="48"/>
       <c r="AD54" s="47"/>
@@ -10692,11 +9954,11 @@
       </c>
       <c r="AK54" s="111">
         <f>MAX($AL$10:$AL$97) - AL54</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AL54" s="122">
         <f>$S54+$AB54+$AG54+$AJ54</f>
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="55" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -10758,7 +10020,7 @@
       <c r="W55" s="126"/>
       <c r="X55" s="126">
         <f>(IF($X54&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X54=$X$6+$Y$6,$P$103,0),0),0)+IF($Y54&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y54=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y55" s="59"/>
       <c r="Z55" s="126">
@@ -11170,7 +10432,7 @@
       <c r="AA58" s="233"/>
       <c r="AB58" s="239">
         <f>SUM(T59:AA59)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AC58" s="232"/>
       <c r="AD58" s="233"/>
@@ -11188,11 +10450,11 @@
       </c>
       <c r="AK58" s="241">
         <f>MAX($AL$10:$AL$97) - AL58</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AL58" s="239">
         <f>$S58+$AB58+$AG58+$AJ58</f>
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="59" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11244,7 +10506,7 @@
       <c r="S59" s="121"/>
       <c r="T59" s="126">
         <f>(IF($T58&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T58=$T$6+$U$6,$P$103,0),0),0)+IF($U58&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U58=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U59" s="126"/>
       <c r="V59" s="126">
@@ -11666,7 +10928,7 @@
       <c r="AA62" s="47"/>
       <c r="AB62" s="122">
         <f>SUM(T63:AA63)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AC62" s="48"/>
       <c r="AD62" s="47"/>
@@ -11684,11 +10946,11 @@
       </c>
       <c r="AK62" s="111">
         <f>MAX($AL$10:$AL$97) - AL62</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AL62" s="122">
         <f>$S62+$AB62+$AG62+$AJ62</f>
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="63" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11750,7 +11012,7 @@
       <c r="W63" s="126"/>
       <c r="X63" s="126">
         <f>(IF($X62&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X62=$X$6+$Y$6,$P$103,0),0),0)+IF($Y62&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y62=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y63" s="59"/>
       <c r="Z63" s="126">
@@ -12103,7 +11365,7 @@
     <row r="66" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="216">
         <f>RANK(AL66,$AL$10:$AL$97,)</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B66" s="217" t="s">
         <v>74</v>
@@ -12180,7 +11442,7 @@
       </c>
       <c r="AK66" s="241">
         <f>MAX($AL$10:$AL$97) - AL66</f>
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="AL66" s="239">
         <f>$S66+$AB66+$AG66+$AJ66</f>
@@ -12599,7 +11861,7 @@
     <row r="70" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="117">
         <f>RANK(AL70,$AL$10:$AL$97,)</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B70" s="84" t="s">
         <v>83</v>
@@ -12658,7 +11920,7 @@
       <c r="AA70" s="47"/>
       <c r="AB70" s="122">
         <f>SUM(T71:AA71)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AC70" s="48"/>
       <c r="AD70" s="47"/>
@@ -12676,11 +11938,11 @@
       </c>
       <c r="AK70" s="111">
         <f>MAX($AL$10:$AL$97) - AL70</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AL70" s="122">
         <f>$S70+$AB70+$AG70+$AJ70</f>
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="71" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -12742,7 +12004,7 @@
       <c r="W71" s="126"/>
       <c r="X71" s="126">
         <f>(IF($X70&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X70=$X$6+$Y$6,$P$103,0),0),0)+IF($Y70&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y70=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y71" s="59"/>
       <c r="Z71" s="126">
@@ -13098,7 +12360,7 @@
         <v>17</v>
       </c>
       <c r="B74" s="217" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C74" s="229">
         <v>5</v>
@@ -13117,44 +12379,44 @@
         <v>6</v>
       </c>
       <c r="K74" s="235">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L74" s="233"/>
       <c r="M74" s="234">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N74" s="230"/>
       <c r="O74" s="234">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P74" s="230"/>
       <c r="Q74" s="232"/>
       <c r="R74" s="237">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S74" s="239">
         <f>SUM(C75:R75)</f>
         <v>20</v>
       </c>
-      <c r="T74" s="229"/>
-      <c r="U74" s="233">
-        <v>6</v>
-      </c>
+      <c r="T74" s="229">
+        <v>7</v>
+      </c>
+      <c r="U74" s="233"/>
       <c r="V74" s="234">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="W74" s="233"/>
-      <c r="X74" s="235"/>
-      <c r="Y74" s="230">
-        <v>5</v>
-      </c>
-      <c r="Z74" s="232"/>
-      <c r="AA74" s="233">
-        <v>6</v>
-      </c>
+      <c r="X74" s="235">
+        <v>7</v>
+      </c>
+      <c r="Y74" s="230"/>
+      <c r="Z74" s="232">
+        <v>7</v>
+      </c>
+      <c r="AA74" s="233"/>
       <c r="AB74" s="239">
         <f>SUM(T75:AA75)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AC74" s="232"/>
       <c r="AD74" s="233"/>
@@ -13172,11 +12434,11 @@
       </c>
       <c r="AK74" s="241">
         <f>MAX($AL$10:$AL$97) - AL74</f>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AL74" s="239">
         <f>$S74+$AB74+$AG74+$AJ74</f>
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="75" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -13228,7 +12490,7 @@
       <c r="S75" s="121"/>
       <c r="T75" s="126">
         <f>(IF($T74&lt;&gt;"",($T$6*$P$104)+IF($T$6=4,($P$102)+IF($T74=$T$6+$U$6,$P$103,0),0),0)+IF($U74&lt;&gt;"",($U$6*$P$104)+IF($U$6=4,($P$102)+IF($U74=$T$6+$U$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U75" s="126"/>
       <c r="V75" s="126">
@@ -13238,12 +12500,12 @@
       <c r="W75" s="126"/>
       <c r="X75" s="126">
         <f>(IF($X74&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X74=$X$6+$Y$6,$P$103,0),0),0)+IF($Y74&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y74=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y75" s="59"/>
       <c r="Z75" s="126">
         <f>(IF($Z74&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z74=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA74&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA74=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AA75" s="62"/>
       <c r="AB75" s="121"/>
@@ -13596,36 +12858,36 @@
       <c r="B78" s="84" t="s">
         <v>68</v>
       </c>
-      <c r="C78" s="305">
+      <c r="C78" s="253">
         <v>5</v>
       </c>
-      <c r="D78" s="306"/>
-      <c r="E78" s="307">
+      <c r="D78" s="254"/>
+      <c r="E78" s="255">
         <v>6</v>
       </c>
-      <c r="F78" s="306"/>
-      <c r="G78" s="308">
+      <c r="F78" s="254"/>
+      <c r="G78" s="256">
         <v>5</v>
       </c>
-      <c r="H78" s="309"/>
-      <c r="I78" s="307"/>
-      <c r="J78" s="309">
+      <c r="H78" s="257"/>
+      <c r="I78" s="255"/>
+      <c r="J78" s="257">
         <v>6</v>
       </c>
-      <c r="K78" s="310">
+      <c r="K78" s="258">
         <v>6</v>
       </c>
-      <c r="L78" s="309"/>
-      <c r="M78" s="307">
+      <c r="L78" s="257"/>
+      <c r="M78" s="255">
         <v>7</v>
       </c>
-      <c r="N78" s="306"/>
-      <c r="O78" s="307">
+      <c r="N78" s="254"/>
+      <c r="O78" s="255">
         <v>6</v>
       </c>
-      <c r="P78" s="306"/>
-      <c r="Q78" s="308"/>
-      <c r="R78" s="311">
+      <c r="P78" s="254"/>
+      <c r="Q78" s="256"/>
+      <c r="R78" s="259">
         <v>6</v>
       </c>
       <c r="S78" s="122">
@@ -13650,7 +12912,7 @@
       <c r="AA78" s="47"/>
       <c r="AB78" s="122">
         <f>SUM(T79:AA79)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AC78" s="48"/>
       <c r="AD78" s="47"/>
@@ -13668,11 +12930,11 @@
       </c>
       <c r="AK78" s="111">
         <f>MAX($AL$10:$AL$97) - AL78</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AL78" s="122">
         <f>$S78+$AB78+$AG78+$AJ78</f>
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="79" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -13734,7 +12996,7 @@
       <c r="W79" s="126"/>
       <c r="X79" s="126">
         <f>(IF($X78&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X78=$X$6+$Y$6,$P$103,0),0),0)+IF($Y78&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y78=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y79" s="59"/>
       <c r="Z79" s="126">
@@ -14090,7 +13352,7 @@
         <v>18</v>
       </c>
       <c r="B82" s="217" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C82" s="229">
         <v>5</v>
@@ -14109,44 +13371,44 @@
         <v>6</v>
       </c>
       <c r="K82" s="235">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L82" s="233"/>
       <c r="M82" s="234">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N82" s="230"/>
       <c r="O82" s="234">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P82" s="230"/>
       <c r="Q82" s="232"/>
       <c r="R82" s="237">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S82" s="239">
         <f>SUM(C83:R83)</f>
         <v>20</v>
       </c>
-      <c r="T82" s="229">
-        <v>7</v>
-      </c>
-      <c r="U82" s="233"/>
+      <c r="T82" s="229"/>
+      <c r="U82" s="233">
+        <v>6</v>
+      </c>
       <c r="V82" s="234">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="W82" s="233"/>
-      <c r="X82" s="235">
-        <v>7</v>
-      </c>
-      <c r="Y82" s="230"/>
-      <c r="Z82" s="232">
-        <v>7</v>
-      </c>
-      <c r="AA82" s="233"/>
+      <c r="X82" s="235"/>
+      <c r="Y82" s="230">
+        <v>5</v>
+      </c>
+      <c r="Z82" s="232"/>
+      <c r="AA82" s="233">
+        <v>6</v>
+      </c>
       <c r="AB82" s="239">
         <f>SUM(T83:AA83)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AC82" s="232"/>
       <c r="AD82" s="233"/>
@@ -14164,11 +13426,11 @@
       </c>
       <c r="AK82" s="241">
         <f>MAX($AL$10:$AL$97) - AL82</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AL82" s="239">
         <f>$S82+$AB82+$AG82+$AJ82</f>
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="83" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -14235,7 +13497,7 @@
       <c r="Y83" s="59"/>
       <c r="Z83" s="126">
         <f>(IF($Z82&lt;&gt;"",($Z$6*$P$104)+IF($Z$6=4,($P$102)+IF($Z82=$Z$6+$AA$6,$P$103,0),0),0)+IF($AA82&lt;&gt;"",($AA$6*$P$104)+IF($AA$6=4,($P$102)+IF($AA82=$Z$6+$AA$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA83" s="62"/>
       <c r="AB83" s="121"/>
@@ -14642,7 +13904,7 @@
       <c r="AA86" s="47"/>
       <c r="AB86" s="122">
         <f>SUM(T87:AA87)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AC86" s="48"/>
       <c r="AD86" s="47"/>
@@ -14660,11 +13922,11 @@
       </c>
       <c r="AK86" s="111">
         <f>MAX($AL$10:$AL$97) - AL86</f>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AL86" s="122">
         <f>$S86+$AB86+$AG86+$AJ86</f>
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="87" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -14726,7 +13988,7 @@
       <c r="W87" s="126"/>
       <c r="X87" s="126">
         <f>(IF($X86&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X86=$X$6+$Y$6,$P$103,0),0),0)+IF($Y86&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y86=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y87" s="59"/>
       <c r="Z87" s="126">
@@ -15082,10 +14344,10 @@
         <v>20</v>
       </c>
       <c r="B90" s="217" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C90" s="229">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D90" s="230"/>
       <c r="E90" s="234"/>
@@ -15093,28 +14355,28 @@
         <v>7</v>
       </c>
       <c r="G90" s="232">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H90" s="233"/>
       <c r="I90" s="234"/>
       <c r="J90" s="233">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K90" s="235">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L90" s="233"/>
       <c r="M90" s="234">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N90" s="230"/>
       <c r="O90" s="234">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P90" s="230"/>
       <c r="Q90" s="232"/>
       <c r="R90" s="237">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S90" s="239">
         <f>SUM(C91:R91)</f>
@@ -15125,20 +14387,20 @@
         <v>7</v>
       </c>
       <c r="V90" s="234">
+        <v>7</v>
+      </c>
+      <c r="W90" s="233"/>
+      <c r="X90" s="235">
         <v>6</v>
       </c>
-      <c r="W90" s="233"/>
-      <c r="X90" s="235"/>
-      <c r="Y90" s="230">
-        <v>6</v>
-      </c>
+      <c r="Y90" s="230"/>
       <c r="Z90" s="232">
         <v>6</v>
       </c>
       <c r="AA90" s="233"/>
       <c r="AB90" s="239">
         <f>SUM(T91:AA91)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AC90" s="232"/>
       <c r="AD90" s="233"/>
@@ -15156,11 +14418,11 @@
       </c>
       <c r="AK90" s="241">
         <f>MAX($AL$10:$AL$97) - AL90</f>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AL90" s="239">
         <f>$S90+$AB90+$AG90+$AJ90</f>
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="91" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -15222,7 +14484,7 @@
       <c r="W91" s="126"/>
       <c r="X91" s="126">
         <f>(IF($X90&lt;&gt;"",($X$6*$P$104)+IF($X$6=4,($P$102)+IF($X90=$X$6+$Y$6,$P$103,0),0),0)+IF($Y90&lt;&gt;"",($Y$6*$P$104)+IF($Y$6=4,($P$102)+IF($Y90=$X$6+$Y$6,$P$103,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y91" s="59"/>
       <c r="Z91" s="126">
@@ -15575,13 +14837,13 @@
     <row r="94" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A94" s="117">
         <f>RANK(AL94,$AL$10:$AL$97,)</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B94" s="84" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C94" s="187">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D94" s="188"/>
       <c r="E94" s="189"/>
@@ -15589,28 +14851,28 @@
         <v>7</v>
       </c>
       <c r="G94" s="190">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H94" s="191"/>
       <c r="I94" s="189"/>
       <c r="J94" s="191">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K94" s="192">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L94" s="191"/>
       <c r="M94" s="189">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N94" s="188"/>
       <c r="O94" s="189">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P94" s="188"/>
       <c r="Q94" s="190"/>
       <c r="R94" s="193">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S94" s="122">
         <f>SUM(C95:R95)</f>
@@ -15621,13 +14883,13 @@
         <v>7</v>
       </c>
       <c r="V94" s="44">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="W94" s="47"/>
-      <c r="X94" s="49">
+      <c r="X94" s="49"/>
+      <c r="Y94" s="45">
         <v>6</v>
       </c>
-      <c r="Y94" s="45"/>
       <c r="Z94" s="48">
         <v>6</v>
       </c>
@@ -15652,7 +14914,7 @@
       </c>
       <c r="AK94" s="111">
         <f>MAX($AL$10:$AL$97) - AL94</f>
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="AL94" s="179">
         <f>$S94+$AB94+$AG94+$AJ94</f>
@@ -16201,12 +15463,12 @@
     <row r="100" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B100" s="43"/>
       <c r="N100" s="26"/>
-      <c r="O100" s="286" t="s">
+      <c r="O100" s="260" t="s">
         <v>17</v>
       </c>
-      <c r="P100" s="287"/>
-      <c r="Q100" s="287"/>
-      <c r="R100" s="288"/>
+      <c r="P100" s="261"/>
+      <c r="Q100" s="261"/>
+      <c r="R100" s="262"/>
       <c r="AG100" s="30"/>
       <c r="AH100" s="30"/>
       <c r="AI100" s="30"/>
@@ -16215,21 +15477,21 @@
     </row>
     <row r="101" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="33"/>
-      <c r="B101" s="274" t="s">
+      <c r="B101" s="289" t="s">
         <v>16</v>
       </c>
-      <c r="C101" s="275"/>
-      <c r="D101" s="275"/>
-      <c r="E101" s="275"/>
-      <c r="F101" s="275"/>
-      <c r="G101" s="275"/>
-      <c r="H101" s="275"/>
-      <c r="I101" s="275"/>
-      <c r="J101" s="275"/>
-      <c r="K101" s="275"/>
-      <c r="L101" s="275"/>
-      <c r="M101" s="275"/>
-      <c r="N101" s="276"/>
+      <c r="C101" s="290"/>
+      <c r="D101" s="290"/>
+      <c r="E101" s="290"/>
+      <c r="F101" s="290"/>
+      <c r="G101" s="290"/>
+      <c r="H101" s="290"/>
+      <c r="I101" s="290"/>
+      <c r="J101" s="290"/>
+      <c r="K101" s="290"/>
+      <c r="L101" s="290"/>
+      <c r="M101" s="290"/>
+      <c r="N101" s="291"/>
       <c r="O101" s="21">
         <v>1</v>
       </c>
@@ -16242,45 +15504,45 @@
       <c r="R101" s="22">
         <v>4</v>
       </c>
-      <c r="U101" s="289" t="s">
+      <c r="U101" s="263" t="s">
         <v>26</v>
       </c>
-      <c r="V101" s="290"/>
-      <c r="W101" s="290"/>
-      <c r="X101" s="290"/>
-      <c r="Y101" s="290"/>
-      <c r="Z101" s="290"/>
-      <c r="AA101" s="290"/>
-      <c r="AB101" s="290"/>
-      <c r="AC101" s="290"/>
-      <c r="AD101" s="291"/>
+      <c r="V101" s="264"/>
+      <c r="W101" s="264"/>
+      <c r="X101" s="264"/>
+      <c r="Y101" s="264"/>
+      <c r="Z101" s="264"/>
+      <c r="AA101" s="264"/>
+      <c r="AB101" s="264"/>
+      <c r="AC101" s="264"/>
+      <c r="AD101" s="265"/>
       <c r="AE101" s="28"/>
       <c r="AF101" s="28"/>
-      <c r="AG101" s="292" t="s">
+      <c r="AG101" s="266" t="s">
         <v>24</v>
       </c>
-      <c r="AH101" s="293"/>
-      <c r="AI101" s="293"/>
-      <c r="AJ101" s="293"/>
-      <c r="AK101" s="294"/>
+      <c r="AH101" s="267"/>
+      <c r="AI101" s="267"/>
+      <c r="AJ101" s="267"/>
+      <c r="AK101" s="268"/>
     </row>
     <row r="102" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A102" s="34"/>
-      <c r="B102" s="253" t="s">
+      <c r="B102" s="296" t="s">
         <v>6</v>
       </c>
-      <c r="C102" s="254"/>
-      <c r="D102" s="254"/>
-      <c r="E102" s="254"/>
-      <c r="F102" s="254"/>
-      <c r="G102" s="254"/>
-      <c r="H102" s="254"/>
-      <c r="I102" s="254"/>
-      <c r="J102" s="254"/>
-      <c r="K102" s="254"/>
-      <c r="L102" s="254"/>
-      <c r="M102" s="254"/>
-      <c r="N102" s="255"/>
+      <c r="C102" s="297"/>
+      <c r="D102" s="297"/>
+      <c r="E102" s="297"/>
+      <c r="F102" s="297"/>
+      <c r="G102" s="297"/>
+      <c r="H102" s="297"/>
+      <c r="I102" s="297"/>
+      <c r="J102" s="297"/>
+      <c r="K102" s="297"/>
+      <c r="L102" s="297"/>
+      <c r="M102" s="297"/>
+      <c r="N102" s="298"/>
       <c r="O102" s="20">
         <v>5</v>
       </c>
@@ -16293,49 +15555,49 @@
       <c r="R102" s="23">
         <v>20</v>
       </c>
-      <c r="U102" s="279" t="s">
+      <c r="U102" s="294" t="s">
         <v>20</v>
       </c>
-      <c r="V102" s="280"/>
-      <c r="W102" s="280"/>
-      <c r="X102" s="280"/>
-      <c r="Y102" s="280"/>
-      <c r="Z102" s="280"/>
-      <c r="AA102" s="280"/>
-      <c r="AB102" s="277">
+      <c r="V102" s="295"/>
+      <c r="W102" s="295"/>
+      <c r="X102" s="295"/>
+      <c r="Y102" s="295"/>
+      <c r="Z102" s="295"/>
+      <c r="AA102" s="295"/>
+      <c r="AB102" s="292">
         <v>22</v>
       </c>
-      <c r="AC102" s="277"/>
-      <c r="AD102" s="278"/>
+      <c r="AC102" s="292"/>
+      <c r="AD102" s="293"/>
       <c r="AE102" s="29"/>
       <c r="AF102" s="29"/>
-      <c r="AG102" s="260" t="s">
+      <c r="AG102" s="308" t="s">
         <v>21</v>
       </c>
-      <c r="AH102" s="261"/>
-      <c r="AI102" s="261"/>
-      <c r="AJ102" s="262"/>
+      <c r="AH102" s="309"/>
+      <c r="AI102" s="309"/>
+      <c r="AJ102" s="310"/>
       <c r="AK102" s="184">
         <v>230</v>
       </c>
     </row>
     <row r="103" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="34"/>
-      <c r="B103" s="253" t="s">
+      <c r="B103" s="296" t="s">
         <v>5</v>
       </c>
-      <c r="C103" s="254"/>
-      <c r="D103" s="254"/>
-      <c r="E103" s="254"/>
-      <c r="F103" s="254"/>
-      <c r="G103" s="254"/>
-      <c r="H103" s="254"/>
-      <c r="I103" s="254"/>
-      <c r="J103" s="254"/>
-      <c r="K103" s="254"/>
-      <c r="L103" s="254"/>
-      <c r="M103" s="254"/>
-      <c r="N103" s="255"/>
+      <c r="C103" s="297"/>
+      <c r="D103" s="297"/>
+      <c r="E103" s="297"/>
+      <c r="F103" s="297"/>
+      <c r="G103" s="297"/>
+      <c r="H103" s="297"/>
+      <c r="I103" s="297"/>
+      <c r="J103" s="297"/>
+      <c r="K103" s="297"/>
+      <c r="L103" s="297"/>
+      <c r="M103" s="297"/>
+      <c r="N103" s="298"/>
       <c r="O103" s="20">
         <v>2</v>
       </c>
@@ -16348,49 +15610,49 @@
       <c r="R103" s="23">
         <v>8</v>
       </c>
-      <c r="U103" s="258" t="s">
+      <c r="U103" s="303" t="s">
         <v>18</v>
       </c>
-      <c r="V103" s="259"/>
-      <c r="W103" s="259"/>
-      <c r="X103" s="259"/>
-      <c r="Y103" s="259"/>
-      <c r="Z103" s="259"/>
-      <c r="AA103" s="259"/>
-      <c r="AB103" s="284">
+      <c r="V103" s="304"/>
+      <c r="W103" s="304"/>
+      <c r="X103" s="304"/>
+      <c r="Y103" s="304"/>
+      <c r="Z103" s="304"/>
+      <c r="AA103" s="304"/>
+      <c r="AB103" s="305">
         <v>20</v>
       </c>
-      <c r="AC103" s="284"/>
-      <c r="AD103" s="285"/>
+      <c r="AC103" s="305"/>
+      <c r="AD103" s="306"/>
       <c r="AE103" s="29"/>
       <c r="AF103" s="29"/>
-      <c r="AG103" s="263" t="s">
+      <c r="AG103" s="311" t="s">
         <v>22</v>
       </c>
-      <c r="AH103" s="254"/>
-      <c r="AI103" s="254"/>
-      <c r="AJ103" s="255"/>
+      <c r="AH103" s="297"/>
+      <c r="AI103" s="297"/>
+      <c r="AJ103" s="298"/>
       <c r="AK103" s="36">
         <v>115</v>
       </c>
     </row>
     <row r="104" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="35"/>
-      <c r="B104" s="267" t="s">
+      <c r="B104" s="282" t="s">
         <v>4</v>
       </c>
-      <c r="C104" s="268"/>
-      <c r="D104" s="268"/>
-      <c r="E104" s="268"/>
-      <c r="F104" s="268"/>
-      <c r="G104" s="268"/>
-      <c r="H104" s="268"/>
-      <c r="I104" s="268"/>
-      <c r="J104" s="268"/>
-      <c r="K104" s="268"/>
-      <c r="L104" s="268"/>
-      <c r="M104" s="268"/>
-      <c r="N104" s="269"/>
+      <c r="C104" s="283"/>
+      <c r="D104" s="283"/>
+      <c r="E104" s="283"/>
+      <c r="F104" s="283"/>
+      <c r="G104" s="283"/>
+      <c r="H104" s="283"/>
+      <c r="I104" s="283"/>
+      <c r="J104" s="283"/>
+      <c r="K104" s="283"/>
+      <c r="L104" s="283"/>
+      <c r="M104" s="283"/>
+      <c r="N104" s="284"/>
       <c r="O104" s="3">
         <v>1</v>
       </c>
@@ -16403,51 +15665,51 @@
       <c r="R104" s="24">
         <v>1</v>
       </c>
-      <c r="U104" s="281" t="s">
+      <c r="U104" s="299" t="s">
         <v>19</v>
       </c>
-      <c r="V104" s="257"/>
-      <c r="W104" s="257"/>
-      <c r="X104" s="257"/>
-      <c r="Y104" s="257"/>
-      <c r="Z104" s="257"/>
-      <c r="AA104" s="257"/>
-      <c r="AB104" s="282">
+      <c r="V104" s="300"/>
+      <c r="W104" s="300"/>
+      <c r="X104" s="300"/>
+      <c r="Y104" s="300"/>
+      <c r="Z104" s="300"/>
+      <c r="AA104" s="300"/>
+      <c r="AB104" s="301">
         <f>AB102*AB103</f>
         <v>440</v>
       </c>
-      <c r="AC104" s="282"/>
-      <c r="AD104" s="283"/>
+      <c r="AC104" s="301"/>
+      <c r="AD104" s="302"/>
       <c r="AE104" s="29"/>
       <c r="AF104" s="29"/>
-      <c r="AG104" s="263" t="s">
+      <c r="AG104" s="311" t="s">
         <v>25</v>
       </c>
-      <c r="AH104" s="254"/>
-      <c r="AI104" s="254"/>
-      <c r="AJ104" s="255"/>
+      <c r="AH104" s="297"/>
+      <c r="AI104" s="297"/>
+      <c r="AJ104" s="298"/>
       <c r="AK104" s="36">
         <v>65</v>
       </c>
     </row>
     <row r="105" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG105" s="258" t="s">
+      <c r="AG105" s="303" t="s">
         <v>23</v>
       </c>
-      <c r="AH105" s="259"/>
-      <c r="AI105" s="259"/>
-      <c r="AJ105" s="259"/>
+      <c r="AH105" s="304"/>
+      <c r="AI105" s="304"/>
+      <c r="AJ105" s="304"/>
       <c r="AK105" s="186">
         <v>30</v>
       </c>
     </row>
     <row r="106" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG106" s="256" t="s">
+      <c r="AG106" s="307" t="s">
         <v>19</v>
       </c>
-      <c r="AH106" s="257"/>
-      <c r="AI106" s="257"/>
-      <c r="AJ106" s="257"/>
+      <c r="AH106" s="300"/>
+      <c r="AI106" s="300"/>
+      <c r="AJ106" s="300"/>
       <c r="AK106" s="185">
         <f>SUM(AK102:AK105)</f>
         <v>440</v>
@@ -16459,6 +15721,28 @@
     <sortCondition ref="B10:B94"/>
   </sortState>
   <mergeCells count="38">
+    <mergeCell ref="B103:N103"/>
+    <mergeCell ref="AG106:AJ106"/>
+    <mergeCell ref="AG105:AJ105"/>
+    <mergeCell ref="AG102:AJ102"/>
+    <mergeCell ref="AG104:AJ104"/>
+    <mergeCell ref="AG103:AJ103"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="B104:N104"/>
+    <mergeCell ref="C1:O1"/>
+    <mergeCell ref="P1:AJ1"/>
+    <mergeCell ref="C3:O3"/>
+    <mergeCell ref="P3:AJ3"/>
+    <mergeCell ref="C2:P2"/>
+    <mergeCell ref="Q2:AJ2"/>
+    <mergeCell ref="B101:N101"/>
+    <mergeCell ref="AB102:AD102"/>
+    <mergeCell ref="U102:AA102"/>
+    <mergeCell ref="B102:N102"/>
+    <mergeCell ref="U104:AA104"/>
+    <mergeCell ref="AB104:AD104"/>
+    <mergeCell ref="U103:AA103"/>
+    <mergeCell ref="AB103:AD103"/>
     <mergeCell ref="O100:R100"/>
     <mergeCell ref="U101:AD101"/>
     <mergeCell ref="AG101:AK101"/>
@@ -16475,242 +15759,220 @@
     <mergeCell ref="C5:J5"/>
     <mergeCell ref="K5:R5"/>
     <mergeCell ref="S5:S9"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="B104:N104"/>
-    <mergeCell ref="C1:O1"/>
-    <mergeCell ref="P1:AJ1"/>
-    <mergeCell ref="C3:O3"/>
-    <mergeCell ref="P3:AJ3"/>
-    <mergeCell ref="C2:P2"/>
-    <mergeCell ref="Q2:AJ2"/>
-    <mergeCell ref="B101:N101"/>
-    <mergeCell ref="AB102:AD102"/>
-    <mergeCell ref="U102:AA102"/>
-    <mergeCell ref="B102:N102"/>
-    <mergeCell ref="U104:AA104"/>
-    <mergeCell ref="AB104:AD104"/>
-    <mergeCell ref="U103:AA103"/>
-    <mergeCell ref="AB103:AD103"/>
-    <mergeCell ref="B103:N103"/>
-    <mergeCell ref="AG106:AJ106"/>
-    <mergeCell ref="AG105:AJ105"/>
-    <mergeCell ref="AG102:AJ102"/>
-    <mergeCell ref="AG104:AJ104"/>
-    <mergeCell ref="AG103:AJ103"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <conditionalFormatting sqref="S10:S15 AB10:AB15 AG10:AG15 AJ10:AJ15 AJ26:AJ27 AG26:AG27 AB26:AB27 S26:S27 AJ22:AJ23 AG22:AG23 AB22:AB23 S22:S23 AJ18:AJ19 AG18:AG19 AB18:AB19 S18:S19 S38:S39 AB38:AB39 AG38:AG39 AJ38:AJ39 S30:S31 AB30:AB31 AG30:AG31 AJ30:AJ31 AJ42:AJ43 AG42:AG43 AB42:AB43 S42:S43 S46:S47 AB46:AB47 AG46:AG47 AJ46:AJ47 AJ50 AG50 AB50 S50 S58 AB58 AG58 AJ58 S54 AB54 AG54 AJ54 AJ62 AG62 AB62 S62 S66 AB66 AG66 AJ66 AJ70 AG70 AB70 S70 S74 AB74 AG74 AJ74 AJ78 AG78 AB78 S78 AJ34:AJ35 AG34:AG35 AB34:AB35 S34:S35">
-    <cfRule type="cellIs" dxfId="138" priority="174" operator="notEqual">
+    <cfRule type="cellIs" dxfId="77" priority="174" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL10:AL23 AL26:AL27 AL38:AL39 AL30:AL31 AL42:AL43 AL46:AL47 AL50 AL58 AL54 AL62 AL66 AL70 AL74 AL78 AL34:AL35">
-    <cfRule type="cellIs" dxfId="137" priority="173" operator="notEqual">
+    <cfRule type="cellIs" dxfId="76" priority="173" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ24:AJ25">
-    <cfRule type="cellIs" dxfId="136" priority="170" operator="notEqual">
+    <cfRule type="cellIs" dxfId="75" priority="170" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL24:AL25">
-    <cfRule type="cellIs" dxfId="135" priority="171" operator="notEqual">
+    <cfRule type="cellIs" dxfId="74" priority="171" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ20:AJ21">
-    <cfRule type="cellIs" dxfId="134" priority="169" operator="notEqual">
+    <cfRule type="cellIs" dxfId="73" priority="169" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ16:AJ17">
-    <cfRule type="cellIs" dxfId="133" priority="168" operator="notEqual">
+    <cfRule type="cellIs" dxfId="72" priority="168" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ28:AJ29">
-    <cfRule type="cellIs" dxfId="132" priority="164" operator="notEqual">
+    <cfRule type="cellIs" dxfId="71" priority="164" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL28:AL29">
-    <cfRule type="cellIs" dxfId="131" priority="165" operator="notEqual">
+    <cfRule type="cellIs" dxfId="70" priority="165" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL36:AL37">
-    <cfRule type="cellIs" dxfId="130" priority="163" operator="notEqual">
+    <cfRule type="cellIs" dxfId="69" priority="163" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL40:AL41">
-    <cfRule type="cellIs" dxfId="129" priority="161" operator="notEqual">
+    <cfRule type="cellIs" dxfId="68" priority="161" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL44:AL45">
-    <cfRule type="cellIs" dxfId="128" priority="159" operator="notEqual">
+    <cfRule type="cellIs" dxfId="67" priority="159" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL48:AL49">
-    <cfRule type="cellIs" dxfId="127" priority="157" operator="notEqual">
+    <cfRule type="cellIs" dxfId="66" priority="157" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S20:S21 AB20:AB21 AG20:AG21">
-    <cfRule type="cellIs" dxfId="126" priority="134" operator="notEqual">
+    <cfRule type="cellIs" dxfId="65" priority="134" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S24:S25 AB24:AB25 AG24:AG25">
-    <cfRule type="cellIs" dxfId="125" priority="133" operator="notEqual">
+    <cfRule type="cellIs" dxfId="64" priority="133" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S16:S17 AB16:AB17 AG16:AG17">
-    <cfRule type="cellIs" dxfId="124" priority="135" operator="notEqual">
+    <cfRule type="cellIs" dxfId="63" priority="135" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S28:S29 AB28:AB29 AG28:AG29">
-    <cfRule type="cellIs" dxfId="123" priority="132" operator="notEqual">
+    <cfRule type="cellIs" dxfId="62" priority="132" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ32:AJ33">
-    <cfRule type="cellIs" dxfId="122" priority="130" operator="notEqual">
+    <cfRule type="cellIs" dxfId="61" priority="130" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL32:AL33">
-    <cfRule type="cellIs" dxfId="121" priority="131" operator="notEqual">
+    <cfRule type="cellIs" dxfId="60" priority="131" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S32:S33 AB32:AB33 AG32:AG33">
-    <cfRule type="cellIs" dxfId="120" priority="129" operator="notEqual">
+    <cfRule type="cellIs" dxfId="59" priority="129" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ36:AJ37">
-    <cfRule type="cellIs" dxfId="119" priority="128" operator="notEqual">
+    <cfRule type="cellIs" dxfId="58" priority="128" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S36:S37 AB36:AB37 AG36:AG37">
-    <cfRule type="cellIs" dxfId="118" priority="127" operator="notEqual">
+    <cfRule type="cellIs" dxfId="57" priority="127" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ40:AJ41">
-    <cfRule type="cellIs" dxfId="117" priority="126" operator="notEqual">
+    <cfRule type="cellIs" dxfId="56" priority="126" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S40:S41 AB40:AB41 AG40:AG41">
-    <cfRule type="cellIs" dxfId="116" priority="125" operator="notEqual">
+    <cfRule type="cellIs" dxfId="55" priority="125" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ44:AJ45">
-    <cfRule type="cellIs" dxfId="115" priority="124" operator="notEqual">
+    <cfRule type="cellIs" dxfId="54" priority="124" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S44:S45 AB44:AB45 AG44:AG45">
-    <cfRule type="cellIs" dxfId="114" priority="123" operator="notEqual">
+    <cfRule type="cellIs" dxfId="53" priority="123" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ48:AJ49">
-    <cfRule type="cellIs" dxfId="113" priority="122" operator="notEqual">
+    <cfRule type="cellIs" dxfId="52" priority="122" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S48:S49 AB48:AB49 AG48:AG49">
-    <cfRule type="cellIs" dxfId="112" priority="121" operator="notEqual">
+    <cfRule type="cellIs" dxfId="51" priority="121" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S51:S53 AB51:AB53 AG51:AG53 AJ51:AJ53">
-    <cfRule type="cellIs" dxfId="111" priority="102" operator="notEqual">
+    <cfRule type="cellIs" dxfId="50" priority="102" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL51:AL53">
-    <cfRule type="cellIs" dxfId="110" priority="101" operator="notEqual">
+    <cfRule type="cellIs" dxfId="49" priority="101" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S55:S57 AB55:AB57 AG55:AG57 AJ55:AJ57">
-    <cfRule type="cellIs" dxfId="109" priority="100" operator="notEqual">
+    <cfRule type="cellIs" dxfId="48" priority="100" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL55:AL57">
-    <cfRule type="cellIs" dxfId="108" priority="99" operator="notEqual">
+    <cfRule type="cellIs" dxfId="47" priority="99" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S59:S61 AB59:AB61 AG59:AG61 AJ59:AJ61">
-    <cfRule type="cellIs" dxfId="107" priority="98" operator="notEqual">
+    <cfRule type="cellIs" dxfId="46" priority="98" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL59:AL61">
-    <cfRule type="cellIs" dxfId="106" priority="97" operator="notEqual">
+    <cfRule type="cellIs" dxfId="45" priority="97" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S63:S65 AB63:AB65 AG63:AG65 AJ63:AJ65">
-    <cfRule type="cellIs" dxfId="105" priority="96" operator="notEqual">
+    <cfRule type="cellIs" dxfId="44" priority="96" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL63:AL65">
-    <cfRule type="cellIs" dxfId="104" priority="95" operator="notEqual">
+    <cfRule type="cellIs" dxfId="43" priority="95" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S67:S69 AB67:AB69 AG67:AG69 AJ67:AJ69">
-    <cfRule type="cellIs" dxfId="103" priority="94" operator="notEqual">
+    <cfRule type="cellIs" dxfId="42" priority="94" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL67:AL69">
-    <cfRule type="cellIs" dxfId="102" priority="93" operator="notEqual">
+    <cfRule type="cellIs" dxfId="41" priority="93" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S71:S73 AB71:AB73 AG71:AG73 AJ71:AJ73">
-    <cfRule type="cellIs" dxfId="101" priority="92" operator="notEqual">
+    <cfRule type="cellIs" dxfId="40" priority="92" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL71:AL73">
-    <cfRule type="cellIs" dxfId="100" priority="91" operator="notEqual">
+    <cfRule type="cellIs" dxfId="39" priority="91" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S75:S77 AB75:AB77 AG75:AG77 AJ75:AJ77">
-    <cfRule type="cellIs" dxfId="99" priority="90" operator="notEqual">
+    <cfRule type="cellIs" dxfId="38" priority="90" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL75:AL77">
-    <cfRule type="cellIs" dxfId="98" priority="89" operator="notEqual">
+    <cfRule type="cellIs" dxfId="37" priority="89" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S79:S81 AB79:AB81 AG79:AG81 AJ79:AJ81">
-    <cfRule type="cellIs" dxfId="97" priority="88" operator="notEqual">
+    <cfRule type="cellIs" dxfId="36" priority="88" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL79:AL81">
-    <cfRule type="cellIs" dxfId="96" priority="87" operator="notEqual">
+    <cfRule type="cellIs" dxfId="35" priority="87" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16729,72 +15991,72 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S82 AB82 AG82 AJ82 AJ90 AG90 AB90 S90">
-    <cfRule type="cellIs" dxfId="95" priority="74" operator="notEqual">
+    <cfRule type="cellIs" dxfId="34" priority="74" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL82 AL90">
-    <cfRule type="cellIs" dxfId="94" priority="73" operator="notEqual">
+    <cfRule type="cellIs" dxfId="33" priority="73" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S83:S85 AB83:AB85 AG83:AG85 AJ83:AJ85">
-    <cfRule type="cellIs" dxfId="93" priority="72" operator="notEqual">
+    <cfRule type="cellIs" dxfId="32" priority="72" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL83:AL85">
-    <cfRule type="cellIs" dxfId="92" priority="71" operator="notEqual">
+    <cfRule type="cellIs" dxfId="31" priority="71" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S91:S93 AB91:AB93 AG91:AG93 AJ91:AJ93">
-    <cfRule type="cellIs" dxfId="91" priority="70" operator="notEqual">
+    <cfRule type="cellIs" dxfId="30" priority="70" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL91:AL93">
-    <cfRule type="cellIs" dxfId="90" priority="69" operator="notEqual">
+    <cfRule type="cellIs" dxfId="29" priority="69" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S94 AB94 AG94 AJ94">
-    <cfRule type="cellIs" dxfId="89" priority="66" operator="notEqual">
+    <cfRule type="cellIs" dxfId="28" priority="66" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL94">
-    <cfRule type="cellIs" dxfId="88" priority="65" operator="notEqual">
+    <cfRule type="cellIs" dxfId="27" priority="65" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S95:S97 AB95:AB97 AG95:AG97 AJ95:AJ97">
-    <cfRule type="cellIs" dxfId="87" priority="64" operator="notEqual">
+    <cfRule type="cellIs" dxfId="26" priority="64" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL95:AL97">
-    <cfRule type="cellIs" dxfId="86" priority="63" operator="notEqual">
+    <cfRule type="cellIs" dxfId="25" priority="63" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S86 AB86 AG86 AJ86">
-    <cfRule type="cellIs" dxfId="85" priority="31" operator="notEqual">
+    <cfRule type="cellIs" dxfId="24" priority="31" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL86">
-    <cfRule type="cellIs" dxfId="84" priority="30" operator="notEqual">
+    <cfRule type="cellIs" dxfId="23" priority="30" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S87:S89 AB87:AB89 AG87:AG89 AJ87:AJ89">
-    <cfRule type="cellIs" dxfId="83" priority="29" operator="notEqual">
+    <cfRule type="cellIs" dxfId="22" priority="29" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL87:AL89">
-    <cfRule type="cellIs" dxfId="82" priority="28" operator="notEqual">
+    <cfRule type="cellIs" dxfId="21" priority="28" operator="notEqual">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16967,7 +16229,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:R94 T10:AA94 AC10:AF94 AH10:AI94">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17138,7 +16400,7 @@
   <dimension ref="A1:AJ31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S24" sqref="S24"/>
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17366,12 +16628,14 @@
       <c r="R6" s="81">
         <v>4</v>
       </c>
-      <c r="S6" s="81"/>
+      <c r="S6" s="81">
+        <v>4</v>
+      </c>
       <c r="T6" s="81"/>
       <c r="U6" s="81"/>
       <c r="V6" s="73">
         <f>IF(O6&gt;O7,1,0)+IF(P6&gt;P7,1,0)+IF(Q6&gt;Q7,1,0)+IF(R6&gt;R7,1,0)+IF(S6&gt;S7,1,0)+IF(T6&gt;T7,1,0)+IF(U6&gt;U7,1,0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W6" s="13"/>
       <c r="Y6" s="86"/>
@@ -17436,7 +16700,9 @@
       <c r="R7" s="81">
         <v>1</v>
       </c>
-      <c r="S7" s="81"/>
+      <c r="S7" s="81">
+        <v>3</v>
+      </c>
       <c r="T7" s="81"/>
       <c r="U7" s="81"/>
       <c r="V7" s="73">
@@ -18085,12 +17351,14 @@
       <c r="R20" s="81">
         <v>0</v>
       </c>
-      <c r="S20" s="81"/>
+      <c r="S20" s="81">
+        <v>2</v>
+      </c>
       <c r="T20" s="81"/>
       <c r="U20" s="81"/>
       <c r="V20" s="73">
         <f>IF(O20&gt;O21,1,0)+IF(P20&gt;P21,1,0)+IF(Q20&gt;Q21,1,0)+IF(R20&gt;R21,1,0)+IF(S20&gt;S21,1,0)+IF(T20&gt;T21,1,0)+IF(U20&gt;U21,1,0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W20" s="13"/>
       <c r="Y20" s="93"/>
@@ -18155,7 +17423,9 @@
       <c r="R21" s="81">
         <v>3</v>
       </c>
-      <c r="S21" s="81"/>
+      <c r="S21" s="81">
+        <v>1</v>
+      </c>
       <c r="T21" s="81"/>
       <c r="U21" s="81"/>
       <c r="V21" s="73">
@@ -18602,102 +17872,102 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C3:I3 C6:I6 O20:U20 C13:I13 AA8:AG8 AA15:AG15 O10:U10 O6:Q6 C10:I10 C24 C20:E20 C17:I17 O24:U24 AA22:AG22 F24:I24 G20:I20 C27:I27 S6:U6">
-    <cfRule type="cellIs" dxfId="158" priority="27" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="27" stopIfTrue="1" operator="greaterThan">
       <formula>C4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:I4 C7:I7 O21:U21 C14:I14 AA9:AG9 AA16:AG16 O11:U11 O7:Q7 C11:I11 C25 C21:E21 C18:I18 O25:U25 AA23:AG23 F25:I25 G21:I21 C28:I28 S7:U7">
-    <cfRule type="cellIs" dxfId="157" priority="28" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="28" stopIfTrue="1" operator="greaterThan">
       <formula>C3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:I3 C6:I6 O20:U20 C13:I13 AA8:AG8 AA15:AG15 O10:U10 O6:Q6 C10:I10 C24 C20:E20 C17:I17 O24:U24 AA22:AG22 F24:I24 G20:I20 C27:I27 S6:U6">
-    <cfRule type="cellIs" dxfId="156" priority="18" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="18" stopIfTrue="1" operator="greaterThan">
       <formula>C4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:I4 C7:I7 O21:U21 C14:I14 AA9:AG9 AA16:AG16 O11:U11 O7:Q7 C11:I11 C25 C21:E21 C18:I18 O25:U25 AA23:AG23 F25:I25 G21:I21 C28:I28 S7:U7">
-    <cfRule type="cellIs" dxfId="155" priority="17" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="17" stopIfTrue="1" operator="greaterThan">
       <formula>C3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24">
-    <cfRule type="cellIs" dxfId="154" priority="15" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="15" stopIfTrue="1" operator="greaterThan">
       <formula>D25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25">
-    <cfRule type="cellIs" dxfId="153" priority="16" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="16" stopIfTrue="1" operator="greaterThan">
       <formula>D24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24">
-    <cfRule type="cellIs" dxfId="152" priority="14" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="14" stopIfTrue="1" operator="greaterThan">
       <formula>D25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25">
-    <cfRule type="cellIs" dxfId="151" priority="13" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="13" stopIfTrue="1" operator="greaterThan">
       <formula>D24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="150" priority="11" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="11" stopIfTrue="1" operator="greaterThan">
       <formula>E25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="149" priority="12" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="12" stopIfTrue="1" operator="greaterThan">
       <formula>E24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="148" priority="10" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="10" stopIfTrue="1" operator="greaterThan">
       <formula>E25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="147" priority="9" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="9" stopIfTrue="1" operator="greaterThan">
       <formula>E24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20">
-    <cfRule type="cellIs" dxfId="146" priority="7" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="greaterThan">
       <formula>F21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21">
-    <cfRule type="cellIs" dxfId="145" priority="8" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="8" stopIfTrue="1" operator="greaterThan">
       <formula>F20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20">
-    <cfRule type="cellIs" dxfId="144" priority="6" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="6" stopIfTrue="1" operator="greaterThan">
       <formula>F21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21">
-    <cfRule type="cellIs" dxfId="143" priority="5" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="greaterThan">
       <formula>F20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R6">
-    <cfRule type="cellIs" dxfId="142" priority="3" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="greaterThan">
       <formula>R7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7">
-    <cfRule type="cellIs" dxfId="141" priority="4" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="greaterThan">
       <formula>R6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R6">
-    <cfRule type="cellIs" dxfId="140" priority="2" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="greaterThan">
       <formula>R7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7">
-    <cfRule type="cellIs" dxfId="139" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>R6</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated games of 2019-05-06
</commit_message>
<xml_diff>
--- a/laval.xlsx
+++ b/laval.xlsx
@@ -1940,7 +1940,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="313">
+  <cellXfs count="317">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2499,9 +2499,6 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2523,48 +2520,72 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="92" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="82" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="85" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="92" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="82" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2580,6 +2601,9 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2613,12 +2637,6 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="85" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2655,32 +2673,26 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3746,258 +3758,258 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="C1" s="277"/>
-      <c r="D1" s="277"/>
-      <c r="E1" s="277"/>
-      <c r="F1" s="277"/>
-      <c r="G1" s="277"/>
-      <c r="H1" s="277"/>
-      <c r="I1" s="277"/>
-      <c r="J1" s="277"/>
-      <c r="K1" s="277"/>
-      <c r="L1" s="277"/>
-      <c r="M1" s="277"/>
-      <c r="N1" s="277"/>
-      <c r="O1" s="277"/>
-      <c r="P1" s="278"/>
-      <c r="Q1" s="278"/>
-      <c r="R1" s="278"/>
-      <c r="S1" s="278"/>
-      <c r="T1" s="278"/>
-      <c r="U1" s="278"/>
-      <c r="V1" s="278"/>
-      <c r="W1" s="278"/>
-      <c r="X1" s="278"/>
-      <c r="Y1" s="278"/>
-      <c r="Z1" s="278"/>
-      <c r="AA1" s="278"/>
-      <c r="AB1" s="278"/>
-      <c r="AC1" s="278"/>
-      <c r="AD1" s="278"/>
-      <c r="AE1" s="278"/>
-      <c r="AF1" s="278"/>
-      <c r="AG1" s="278"/>
-      <c r="AH1" s="278"/>
-      <c r="AI1" s="278"/>
-      <c r="AJ1" s="278"/>
+      <c r="C1" s="284"/>
+      <c r="D1" s="284"/>
+      <c r="E1" s="284"/>
+      <c r="F1" s="284"/>
+      <c r="G1" s="284"/>
+      <c r="H1" s="284"/>
+      <c r="I1" s="284"/>
+      <c r="J1" s="284"/>
+      <c r="K1" s="284"/>
+      <c r="L1" s="284"/>
+      <c r="M1" s="284"/>
+      <c r="N1" s="284"/>
+      <c r="O1" s="284"/>
+      <c r="P1" s="285"/>
+      <c r="Q1" s="285"/>
+      <c r="R1" s="285"/>
+      <c r="S1" s="285"/>
+      <c r="T1" s="285"/>
+      <c r="U1" s="285"/>
+      <c r="V1" s="285"/>
+      <c r="W1" s="285"/>
+      <c r="X1" s="285"/>
+      <c r="Y1" s="285"/>
+      <c r="Z1" s="285"/>
+      <c r="AA1" s="285"/>
+      <c r="AB1" s="285"/>
+      <c r="AC1" s="285"/>
+      <c r="AD1" s="285"/>
+      <c r="AE1" s="285"/>
+      <c r="AF1" s="285"/>
+      <c r="AG1" s="285"/>
+      <c r="AH1" s="285"/>
+      <c r="AI1" s="285"/>
+      <c r="AJ1" s="285"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="41"/>
-      <c r="C2" s="312" t="s">
+      <c r="C2" s="286" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="312"/>
-      <c r="E2" s="312"/>
-      <c r="F2" s="312"/>
-      <c r="G2" s="312"/>
-      <c r="H2" s="312"/>
-      <c r="I2" s="312"/>
-      <c r="J2" s="312"/>
-      <c r="K2" s="312"/>
-      <c r="L2" s="312"/>
-      <c r="M2" s="312"/>
-      <c r="N2" s="312"/>
-      <c r="O2" s="312"/>
-      <c r="P2" s="312"/>
-      <c r="Q2" s="279" t="s">
+      <c r="D2" s="286"/>
+      <c r="E2" s="286"/>
+      <c r="F2" s="286"/>
+      <c r="G2" s="286"/>
+      <c r="H2" s="286"/>
+      <c r="I2" s="286"/>
+      <c r="J2" s="286"/>
+      <c r="K2" s="286"/>
+      <c r="L2" s="286"/>
+      <c r="M2" s="286"/>
+      <c r="N2" s="286"/>
+      <c r="O2" s="286"/>
+      <c r="P2" s="286"/>
+      <c r="Q2" s="287" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="278"/>
-      <c r="S2" s="278"/>
-      <c r="T2" s="278"/>
-      <c r="U2" s="278"/>
-      <c r="V2" s="278"/>
-      <c r="W2" s="278"/>
-      <c r="X2" s="278"/>
-      <c r="Y2" s="278"/>
-      <c r="Z2" s="278"/>
-      <c r="AA2" s="278"/>
-      <c r="AB2" s="278"/>
-      <c r="AC2" s="278"/>
-      <c r="AD2" s="278"/>
-      <c r="AE2" s="278"/>
-      <c r="AF2" s="278"/>
-      <c r="AG2" s="278"/>
-      <c r="AH2" s="278"/>
-      <c r="AI2" s="278"/>
-      <c r="AJ2" s="278"/>
+      <c r="R2" s="285"/>
+      <c r="S2" s="285"/>
+      <c r="T2" s="285"/>
+      <c r="U2" s="285"/>
+      <c r="V2" s="285"/>
+      <c r="W2" s="285"/>
+      <c r="X2" s="285"/>
+      <c r="Y2" s="285"/>
+      <c r="Z2" s="285"/>
+      <c r="AA2" s="285"/>
+      <c r="AB2" s="285"/>
+      <c r="AC2" s="285"/>
+      <c r="AD2" s="285"/>
+      <c r="AE2" s="285"/>
+      <c r="AF2" s="285"/>
+      <c r="AG2" s="285"/>
+      <c r="AH2" s="285"/>
+      <c r="AI2" s="285"/>
+      <c r="AJ2" s="285"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A3" s="41"/>
-      <c r="C3" s="312" t="s">
+      <c r="C3" s="286" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="312"/>
-      <c r="E3" s="312"/>
-      <c r="F3" s="312"/>
-      <c r="G3" s="312"/>
-      <c r="H3" s="312"/>
-      <c r="I3" s="312"/>
-      <c r="J3" s="312"/>
-      <c r="K3" s="312"/>
-      <c r="L3" s="312"/>
-      <c r="M3" s="312"/>
-      <c r="N3" s="312"/>
-      <c r="O3" s="312"/>
-      <c r="P3" s="312"/>
-      <c r="Q3" s="279" t="s">
+      <c r="D3" s="286"/>
+      <c r="E3" s="286"/>
+      <c r="F3" s="286"/>
+      <c r="G3" s="286"/>
+      <c r="H3" s="286"/>
+      <c r="I3" s="286"/>
+      <c r="J3" s="286"/>
+      <c r="K3" s="286"/>
+      <c r="L3" s="286"/>
+      <c r="M3" s="286"/>
+      <c r="N3" s="286"/>
+      <c r="O3" s="286"/>
+      <c r="P3" s="286"/>
+      <c r="Q3" s="287" t="s">
         <v>87</v>
       </c>
-      <c r="R3" s="278"/>
-      <c r="S3" s="278"/>
-      <c r="T3" s="278"/>
-      <c r="U3" s="278"/>
-      <c r="V3" s="278"/>
-      <c r="W3" s="278"/>
-      <c r="X3" s="278"/>
-      <c r="Y3" s="278"/>
-      <c r="Z3" s="278"/>
-      <c r="AA3" s="278"/>
-      <c r="AB3" s="278"/>
-      <c r="AC3" s="278"/>
-      <c r="AD3" s="278"/>
-      <c r="AE3" s="278"/>
-      <c r="AF3" s="278"/>
-      <c r="AG3" s="278"/>
-      <c r="AH3" s="278"/>
-      <c r="AI3" s="278"/>
-      <c r="AJ3" s="278"/>
+      <c r="R3" s="285"/>
+      <c r="S3" s="285"/>
+      <c r="T3" s="285"/>
+      <c r="U3" s="285"/>
+      <c r="V3" s="285"/>
+      <c r="W3" s="285"/>
+      <c r="X3" s="285"/>
+      <c r="Y3" s="285"/>
+      <c r="Z3" s="285"/>
+      <c r="AA3" s="285"/>
+      <c r="AB3" s="285"/>
+      <c r="AC3" s="285"/>
+      <c r="AD3" s="285"/>
+      <c r="AE3" s="285"/>
+      <c r="AF3" s="285"/>
+      <c r="AG3" s="285"/>
+      <c r="AH3" s="285"/>
+      <c r="AI3" s="285"/>
+      <c r="AJ3" s="285"/>
     </row>
     <row r="4" spans="1:38" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="277"/>
-      <c r="D4" s="277"/>
-      <c r="E4" s="277"/>
-      <c r="F4" s="277"/>
-      <c r="G4" s="277"/>
-      <c r="H4" s="277"/>
-      <c r="I4" s="277"/>
-      <c r="J4" s="277"/>
-      <c r="K4" s="277"/>
-      <c r="L4" s="277"/>
-      <c r="M4" s="277"/>
-      <c r="N4" s="277"/>
-      <c r="O4" s="277"/>
-      <c r="P4" s="278"/>
-      <c r="Q4" s="278"/>
-      <c r="R4" s="278"/>
-      <c r="S4" s="278"/>
-      <c r="T4" s="278"/>
-      <c r="U4" s="278"/>
-      <c r="V4" s="278"/>
-      <c r="W4" s="278"/>
-      <c r="X4" s="278"/>
-      <c r="Y4" s="278"/>
-      <c r="Z4" s="278"/>
-      <c r="AA4" s="278"/>
-      <c r="AB4" s="278"/>
-      <c r="AC4" s="278"/>
-      <c r="AD4" s="278"/>
-      <c r="AE4" s="278"/>
-      <c r="AF4" s="278"/>
-      <c r="AG4" s="278"/>
-      <c r="AH4" s="278"/>
-      <c r="AI4" s="278"/>
-      <c r="AJ4" s="278"/>
+      <c r="C4" s="284"/>
+      <c r="D4" s="284"/>
+      <c r="E4" s="284"/>
+      <c r="F4" s="284"/>
+      <c r="G4" s="284"/>
+      <c r="H4" s="284"/>
+      <c r="I4" s="284"/>
+      <c r="J4" s="284"/>
+      <c r="K4" s="284"/>
+      <c r="L4" s="284"/>
+      <c r="M4" s="284"/>
+      <c r="N4" s="284"/>
+      <c r="O4" s="284"/>
+      <c r="P4" s="285"/>
+      <c r="Q4" s="285"/>
+      <c r="R4" s="285"/>
+      <c r="S4" s="285"/>
+      <c r="T4" s="285"/>
+      <c r="U4" s="285"/>
+      <c r="V4" s="285"/>
+      <c r="W4" s="285"/>
+      <c r="X4" s="285"/>
+      <c r="Y4" s="285"/>
+      <c r="Z4" s="285"/>
+      <c r="AA4" s="285"/>
+      <c r="AB4" s="285"/>
+      <c r="AC4" s="285"/>
+      <c r="AD4" s="285"/>
+      <c r="AE4" s="285"/>
+      <c r="AF4" s="285"/>
+      <c r="AG4" s="285"/>
+      <c r="AH4" s="285"/>
+      <c r="AI4" s="285"/>
+      <c r="AJ4" s="285"/>
     </row>
     <row r="5" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="301" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="302"/>
-      <c r="E5" s="302"/>
-      <c r="F5" s="302"/>
-      <c r="G5" s="302"/>
-      <c r="H5" s="302"/>
-      <c r="I5" s="302"/>
-      <c r="J5" s="302"/>
-      <c r="K5" s="302"/>
-      <c r="L5" s="302"/>
-      <c r="M5" s="302"/>
-      <c r="N5" s="302"/>
-      <c r="O5" s="302"/>
-      <c r="P5" s="302"/>
-      <c r="Q5" s="302"/>
-      <c r="R5" s="302"/>
-      <c r="S5" s="303"/>
-      <c r="T5" s="301" t="s">
+      <c r="C5" s="307" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="308"/>
+      <c r="E5" s="308"/>
+      <c r="F5" s="308"/>
+      <c r="G5" s="308"/>
+      <c r="H5" s="308"/>
+      <c r="I5" s="308"/>
+      <c r="J5" s="308"/>
+      <c r="K5" s="308"/>
+      <c r="L5" s="308"/>
+      <c r="M5" s="308"/>
+      <c r="N5" s="308"/>
+      <c r="O5" s="308"/>
+      <c r="P5" s="308"/>
+      <c r="Q5" s="308"/>
+      <c r="R5" s="308"/>
+      <c r="S5" s="309"/>
+      <c r="T5" s="307" t="s">
         <v>1</v>
       </c>
-      <c r="U5" s="302"/>
-      <c r="V5" s="302"/>
-      <c r="W5" s="302"/>
-      <c r="X5" s="302"/>
-      <c r="Y5" s="302"/>
-      <c r="Z5" s="302"/>
-      <c r="AA5" s="302"/>
-      <c r="AB5" s="303"/>
-      <c r="AC5" s="301" t="s">
+      <c r="U5" s="308"/>
+      <c r="V5" s="308"/>
+      <c r="W5" s="308"/>
+      <c r="X5" s="308"/>
+      <c r="Y5" s="308"/>
+      <c r="Z5" s="308"/>
+      <c r="AA5" s="308"/>
+      <c r="AB5" s="309"/>
+      <c r="AC5" s="307" t="s">
         <v>2</v>
       </c>
-      <c r="AD5" s="302"/>
-      <c r="AE5" s="302"/>
-      <c r="AF5" s="302"/>
-      <c r="AG5" s="310"/>
-      <c r="AH5" s="301" t="s">
+      <c r="AD5" s="308"/>
+      <c r="AE5" s="308"/>
+      <c r="AF5" s="308"/>
+      <c r="AG5" s="312"/>
+      <c r="AH5" s="307" t="s">
         <v>10</v>
       </c>
-      <c r="AI5" s="302"/>
-      <c r="AJ5" s="303"/>
+      <c r="AI5" s="308"/>
+      <c r="AJ5" s="309"/>
     </row>
     <row r="6" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="32"/>
       <c r="B6" s="4"/>
-      <c r="C6" s="271" t="s">
+      <c r="C6" s="280" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="272"/>
-      <c r="E6" s="272"/>
-      <c r="F6" s="272"/>
-      <c r="G6" s="272"/>
-      <c r="H6" s="272"/>
-      <c r="I6" s="272"/>
-      <c r="J6" s="273"/>
-      <c r="K6" s="308" t="s">
+      <c r="D6" s="275"/>
+      <c r="E6" s="275"/>
+      <c r="F6" s="275"/>
+      <c r="G6" s="275"/>
+      <c r="H6" s="275"/>
+      <c r="I6" s="275"/>
+      <c r="J6" s="276"/>
+      <c r="K6" s="274" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="272"/>
-      <c r="M6" s="272"/>
-      <c r="N6" s="272"/>
-      <c r="O6" s="272"/>
-      <c r="P6" s="272"/>
-      <c r="Q6" s="272"/>
-      <c r="R6" s="273"/>
-      <c r="S6" s="304" t="s">
+      <c r="L6" s="275"/>
+      <c r="M6" s="275"/>
+      <c r="N6" s="275"/>
+      <c r="O6" s="275"/>
+      <c r="P6" s="275"/>
+      <c r="Q6" s="275"/>
+      <c r="R6" s="276"/>
+      <c r="S6" s="277" t="s">
         <v>12</v>
       </c>
-      <c r="T6" s="271" t="s">
+      <c r="T6" s="280" t="s">
         <v>9</v>
       </c>
-      <c r="U6" s="272"/>
-      <c r="V6" s="272"/>
-      <c r="W6" s="273"/>
-      <c r="X6" s="308" t="s">
+      <c r="U6" s="275"/>
+      <c r="V6" s="275"/>
+      <c r="W6" s="276"/>
+      <c r="X6" s="274" t="s">
         <v>8</v>
       </c>
-      <c r="Y6" s="272"/>
-      <c r="Z6" s="272"/>
-      <c r="AA6" s="273"/>
-      <c r="AB6" s="304" t="s">
+      <c r="Y6" s="275"/>
+      <c r="Z6" s="275"/>
+      <c r="AA6" s="276"/>
+      <c r="AB6" s="277" t="s">
         <v>13</v>
       </c>
-      <c r="AC6" s="309" t="s">
+      <c r="AC6" s="311" t="s">
         <v>9</v>
       </c>
-      <c r="AD6" s="273"/>
-      <c r="AE6" s="308" t="s">
+      <c r="AD6" s="276"/>
+      <c r="AE6" s="274" t="s">
         <v>8</v>
       </c>
-      <c r="AF6" s="273"/>
-      <c r="AG6" s="304" t="s">
+      <c r="AF6" s="276"/>
+      <c r="AG6" s="277" t="s">
         <v>14</v>
       </c>
       <c r="AH6" s="56"/>
       <c r="AI6" s="25"/>
-      <c r="AJ6" s="304" t="s">
+      <c r="AJ6" s="277" t="s">
         <v>15</v>
       </c>
       <c r="AK6" s="4"/>
@@ -4069,10 +4081,10 @@
         <f>Résultats!$J$28</f>
         <v>3</v>
       </c>
-      <c r="S7" s="305"/>
-      <c r="T7" s="156">
+      <c r="S7" s="278"/>
+      <c r="T7" s="313">
         <f>Résultats!$V$6</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U7" s="103">
         <f>Résultats!$V$7</f>
@@ -4092,7 +4104,7 @@
       </c>
       <c r="Y7" s="104">
         <f>Résultats!$V$21</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Z7" s="106">
         <f>Résultats!$V$24</f>
@@ -4102,7 +4114,7 @@
         <f>Résultats!$V$25</f>
         <v>3</v>
       </c>
-      <c r="AB7" s="305"/>
+      <c r="AB7" s="278"/>
       <c r="AC7" s="106">
         <f>Résultats!$AH$8</f>
         <v>0</v>
@@ -4119,7 +4131,7 @@
         <f>Résultats!$AH$23</f>
         <v>0</v>
       </c>
-      <c r="AG7" s="305"/>
+      <c r="AG7" s="278"/>
       <c r="AH7" s="173">
         <f>Résultats!$AH$15</f>
         <v>0</v>
@@ -4128,7 +4140,7 @@
         <f>Résultats!$AH$16</f>
         <v>0</v>
       </c>
-      <c r="AJ7" s="305"/>
+      <c r="AJ7" s="278"/>
       <c r="AK7" s="37"/>
     </row>
     <row r="8" spans="1:38" s="39" customFormat="1" ht="58.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -4154,8 +4166,8 @@
       <c r="P8" s="203"/>
       <c r="Q8" s="207"/>
       <c r="R8" s="112"/>
-      <c r="S8" s="305"/>
-      <c r="T8" s="157"/>
+      <c r="S8" s="278"/>
+      <c r="T8" s="314"/>
       <c r="U8" s="112"/>
       <c r="V8" s="160"/>
       <c r="W8" s="199"/>
@@ -4163,15 +4175,15 @@
       <c r="Y8" s="113"/>
       <c r="Z8" s="114"/>
       <c r="AA8" s="112"/>
-      <c r="AB8" s="305"/>
+      <c r="AB8" s="278"/>
       <c r="AC8" s="114"/>
       <c r="AD8" s="112"/>
       <c r="AE8" s="115"/>
       <c r="AF8" s="112"/>
-      <c r="AG8" s="305"/>
+      <c r="AG8" s="278"/>
       <c r="AH8" s="173"/>
       <c r="AI8" s="107"/>
-      <c r="AJ8" s="305"/>
+      <c r="AJ8" s="278"/>
       <c r="AK8" s="37"/>
     </row>
     <row r="9" spans="1:38" s="39" customFormat="1" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4241,8 +4253,8 @@
         <f>Résultats!$B$28</f>
         <v>VEGAS</v>
       </c>
-      <c r="S9" s="305"/>
-      <c r="T9" s="158" t="str">
+      <c r="S9" s="278"/>
+      <c r="T9" s="315" t="str">
         <f>Résultats!$N$6</f>
         <v>BOSTON</v>
       </c>
@@ -4274,7 +4286,7 @@
         <f>Résultats!$N$25</f>
         <v>DALLAS</v>
       </c>
-      <c r="AB9" s="305"/>
+      <c r="AB9" s="278"/>
       <c r="AC9" s="164" t="str">
         <f>Résultats!$Z$8</f>
         <v xml:space="preserve"> </v>
@@ -4291,7 +4303,7 @@
         <f>Résultats!$Z$23</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AG9" s="305"/>
+      <c r="AG9" s="278"/>
       <c r="AH9" s="174" t="str">
         <f>Résultats!$Z$15</f>
         <v xml:space="preserve"> </v>
@@ -4300,7 +4312,7 @@
         <f>Résultats!$Z$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ9" s="305"/>
+      <c r="AJ9" s="278"/>
       <c r="AK9" s="37"/>
     </row>
     <row r="10" spans="1:38" s="39" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4374,8 +4386,8 @@
         <f>Résultats!$A$28</f>
         <v>P3</v>
       </c>
-      <c r="S10" s="307"/>
-      <c r="T10" s="166" t="str">
+      <c r="S10" s="279"/>
+      <c r="T10" s="316" t="str">
         <f>Résultats!$M$6</f>
         <v>A2</v>
       </c>
@@ -4407,7 +4419,7 @@
         <f>Résultats!$M$25</f>
         <v>WC1</v>
       </c>
-      <c r="AB10" s="306"/>
+      <c r="AB10" s="310"/>
       <c r="AC10" s="170" t="str">
         <f>Résultats!$Y$8</f>
         <v xml:space="preserve"> </v>
@@ -4424,7 +4436,7 @@
         <f>Résultats!$Y$23</f>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="AG10" s="306"/>
+      <c r="AG10" s="310"/>
       <c r="AH10" s="176" t="str">
         <f>Résultats!$Y$15</f>
         <v xml:space="preserve"> </v>
@@ -4433,7 +4445,7 @@
         <f>Résultats!$Y$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ10" s="307"/>
+      <c r="AJ10" s="279"/>
       <c r="AK10" s="109" t="s">
         <v>51</v>
       </c>
@@ -4503,7 +4515,7 @@
       </c>
       <c r="AB11" s="225">
         <f>SUM(T12:AA12)</f>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="AC11" s="221"/>
       <c r="AD11" s="222"/>
@@ -4525,7 +4537,7 @@
       </c>
       <c r="AL11" s="225">
         <f>$S11+$AB11+$AG11+$AJ11</f>
-        <v>60</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -4577,7 +4589,7 @@
       <c r="S12" s="121"/>
       <c r="T12" s="126">
         <f>(IF($T11&lt;&gt;"",($T$7*$P$105)+IF($T$7=4,($P$103)+IF($T11=$T$7+$U$7,$P$104,0),0),0)+IF($U11&lt;&gt;"",($U$7*$P$105)+IF($U$7=4,($P$103)+IF($U11=$T$7+$U$7,$P$104,0),0),0))</f>
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="U12" s="126"/>
       <c r="V12" s="126">
@@ -4713,7 +4725,7 @@
         <f>IF(ISBLANK(T11),
 0,
 IF(T$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U13" s="118">
         <f>IF(ISBLANK(U11),
@@ -4768,7 +4780,7 @@
       <c r="AJ13" s="138"/>
       <c r="AK13" s="139">
         <f>SUM(C13:AI13)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AL13" s="123"/>
     </row>
@@ -4878,7 +4890,7 @@
         <f>IF(T13 = 0,
 0,
 IF(T11 = (T$7+U$7),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U14" s="118">
         <f>IF(U13 = 0,
@@ -4933,7 +4945,7 @@
       <c r="AJ14" s="138"/>
       <c r="AK14" s="139">
         <f>SUM(C14:AI14)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL14" s="123"/>
     </row>
@@ -5017,7 +5029,7 @@
       </c>
       <c r="AK15" s="111">
         <f>MAX($AL$11:$AL$98) - AL15</f>
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="AL15" s="122">
         <f>$S15+$AB15+$AG15+$AJ15</f>
@@ -5102,7 +5114,7 @@
       <c r="AJ16" s="121"/>
       <c r="AK16" s="92">
         <f>MAX($AL$11:$AL$98) - AL16</f>
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="AL16" s="121"/>
     </row>
@@ -5516,7 +5528,7 @@
       </c>
       <c r="AK19" s="241">
         <f>MAX($AL$11:$AL$98) - AL19</f>
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="AL19" s="239">
         <f>$S19+$AB19+$AG19+$AJ19</f>
@@ -5601,7 +5613,7 @@
       <c r="AJ20" s="144"/>
       <c r="AK20" s="150">
         <f>MAX($AL$11:$AL$98) - AL20</f>
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="AL20" s="121"/>
     </row>
@@ -5941,63 +5953,63 @@
         <v>4</v>
       </c>
       <c r="B23" s="84" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C23" s="46">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23" s="45"/>
       <c r="E23" s="44">
+        <v>4</v>
+      </c>
+      <c r="F23" s="45"/>
+      <c r="G23" s="48">
         <v>6</v>
       </c>
-      <c r="F23" s="45"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="215">
+      <c r="H23" s="47"/>
+      <c r="I23" s="44">
+        <v>6</v>
+      </c>
+      <c r="J23" s="47"/>
+      <c r="K23" s="49">
         <v>7</v>
       </c>
-      <c r="I23" s="44"/>
-      <c r="J23" s="47">
+      <c r="L23" s="47"/>
+      <c r="M23" s="44">
+        <v>5</v>
+      </c>
+      <c r="N23" s="45"/>
+      <c r="O23" s="44">
+        <v>4</v>
+      </c>
+      <c r="P23" s="45"/>
+      <c r="Q23" s="48"/>
+      <c r="R23" s="50">
         <v>6</v>
       </c>
-      <c r="K23" s="49">
-        <v>5</v>
-      </c>
-      <c r="L23" s="47"/>
-      <c r="M23" s="44"/>
-      <c r="N23" s="211">
-        <v>6</v>
-      </c>
-      <c r="O23" s="44">
-        <v>6</v>
-      </c>
-      <c r="P23" s="45"/>
-      <c r="Q23" s="48">
-        <v>6</v>
-      </c>
-      <c r="R23" s="50"/>
       <c r="S23" s="122">
         <f>SUM(C24:R24)</f>
-        <v>43</v>
-      </c>
-      <c r="T23" s="46"/>
-      <c r="U23" s="47">
+        <v>29</v>
+      </c>
+      <c r="T23" s="46">
         <v>6</v>
       </c>
+      <c r="U23" s="47"/>
       <c r="V23" s="44">
+        <v>5</v>
+      </c>
+      <c r="W23" s="47"/>
+      <c r="X23" s="49"/>
+      <c r="Y23" s="45">
+        <v>7</v>
+      </c>
+      <c r="Z23" s="48">
         <v>6</v>
       </c>
-      <c r="W23" s="47"/>
-      <c r="X23" s="49">
-        <v>5</v>
-      </c>
-      <c r="Y23" s="45"/>
-      <c r="Z23" s="48"/>
-      <c r="AA23" s="50">
-        <v>7</v>
-      </c>
+      <c r="AA23" s="50"/>
       <c r="AB23" s="122">
         <f>SUM(T24:AA24)</f>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="AC23" s="48"/>
       <c r="AD23" s="47"/>
@@ -6015,11 +6027,11 @@
       </c>
       <c r="AK23" s="111">
         <f>MAX($AL$11:$AL$98) - AL23</f>
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="AL23" s="122">
         <f>$S23+$AB23+$AG23+$AJ23</f>
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6040,12 +6052,12 @@
       <c r="F24" s="151"/>
       <c r="G24" s="125">
         <f>(IF($G23&lt;&gt;"",($G$7*$O$105)+IF($G$7=4,($O$103)+IF($G23=$G$7+$H$7,$O$104,0),0),0)+IF($H23&lt;&gt;"",($H$7*$O$105)+IF($H$7=4,($O$103)+IF($H23=$G$7+$H$7,$O$104,0),0),0))</f>
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="H24" s="151"/>
       <c r="I24" s="125">
         <f>(IF($I23&lt;&gt;"",($I$7*$O$105)+IF($I$7=4,($O$103)+IF($I23=$I$7+$J$7,$O$104,0),0),0)+IF($J23&lt;&gt;"",($J$7*$O$105)+IF($J$7=4,($O$103)+IF($J23=$I$7+$J$7,$O$104,0),0),0))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J24" s="152"/>
       <c r="K24" s="153">
@@ -6055,7 +6067,7 @@
       <c r="L24" s="151"/>
       <c r="M24" s="125">
         <f>(IF($M23&lt;&gt;"",($M$7*$O$105)+IF($M$7=4,($O$103)+IF($M23=$M$7+$N$7,$O$104,0),0),0)+IF($N23&lt;&gt;"",($N$7*$O$105)+IF($N$7=4,($O$103)+IF($N23=$M$7+$N$7,$O$104,0),0),0))</f>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="N24" s="151"/>
       <c r="O24" s="125">
@@ -6065,13 +6077,13 @@
       <c r="P24" s="151"/>
       <c r="Q24" s="125">
         <f>(IF($Q23&lt;&gt;"",($Q$7*$O$105)+IF($Q$7=4,($O$103)+IF($Q23=$Q$7+$R$7,$O$104,0),0),0)+IF($R23&lt;&gt;"",($R$7*$O$105)+IF($R$7=4,($O$103)+IF($R23=$Q$7+$R$7,$O$104,0),0),0))</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="R24" s="154"/>
       <c r="S24" s="144"/>
       <c r="T24" s="126">
         <f>(IF($T23&lt;&gt;"",($T$7*$P$105)+IF($T$7=4,($P$103)+IF($T23=$T$7+$U$7,$P$104,0),0),0)+IF($U23&lt;&gt;"",($U$7*$P$105)+IF($U$7=4,($P$103)+IF($U23=$T$7+$U$7,$P$104,0),0),0))</f>
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="U24" s="126"/>
       <c r="V24" s="126">
@@ -6100,7 +6112,7 @@
       <c r="AJ24" s="144"/>
       <c r="AK24" s="150">
         <f>MAX($AL$11:$AL$98) - AL24</f>
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="AL24" s="121"/>
     </row>
@@ -6143,13 +6155,13 @@
         <f>IF(ISBLANK(H23),
 0,
 IF(H$7 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25" s="118">
         <f>IF(ISBLANK(I23),
 0,
 IF(I$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" s="118">
         <f>IF(ISBLANK(J23),
@@ -6179,7 +6191,7 @@
         <f>IF(ISBLANK(N23),
 0,
 IF(N$7 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O25" s="118">
         <f>IF(ISBLANK(O23),
@@ -6197,7 +6209,7 @@
         <f>IF(ISBLANK(Q23),
 0,
 IF(Q$7= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R25" s="118">
         <f>IF(ISBLANK(R23),
@@ -6210,7 +6222,7 @@
         <f>IF(ISBLANK(T23),
 0,
 IF(T$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U25" s="118">
         <f>IF(ISBLANK(U23),
@@ -6265,7 +6277,7 @@
       <c r="AJ25" s="138"/>
       <c r="AK25" s="139">
         <f>SUM(C25:AI25)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AL25" s="123"/>
     </row>
@@ -6308,7 +6320,7 @@
         <f>IF(H25 = 0,
 0,
 IF(H23 = (G$7+H$7),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26" s="118">
         <f>IF(I25 = 0,
@@ -6344,7 +6356,7 @@
         <f>IF(N25 = 0,
 0,
 IF(N23 = (M$7+N$7),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O26" s="118">
         <f>IF(O25 = 0,
@@ -6375,7 +6387,7 @@
         <f>IF(T25 = 0,
 0,
 IF(T23 = (T$7+U$7),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U26" s="118">
         <f>IF(U25 = 0,
@@ -6430,14 +6442,14 @@
       <c r="AJ26" s="138"/>
       <c r="AK26" s="139">
         <f>SUM(C26:AI26)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AL26" s="123"/>
     </row>
     <row r="27" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="216">
         <f>RANK(AL27,$AL$11:$AL$98,)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B27" s="217" t="s">
         <v>72</v>
@@ -6496,7 +6508,7 @@
       <c r="AA27" s="237"/>
       <c r="AB27" s="239">
         <f>SUM(T28:AA28)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AC27" s="232"/>
       <c r="AD27" s="233"/>
@@ -6514,11 +6526,11 @@
       </c>
       <c r="AK27" s="241">
         <f>MAX($AL$11:$AL$98) - AL27</f>
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="AL27" s="239">
         <f>$S27+$AB27+$AG27+$AJ27</f>
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6580,7 +6592,7 @@
       <c r="W28" s="126"/>
       <c r="X28" s="126">
         <f>(IF($X27&lt;&gt;"",($X$7*$P$105)+IF($X$7=4,($P$103)+IF($X27=$X$7+$Y$7,$P$104,0),0),0)+IF($Y27&lt;&gt;"",($Y$7*$P$105)+IF($Y$7=4,($P$103)+IF($Y27=$X$7+$Y$7,$P$104,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y28" s="59"/>
       <c r="Z28" s="126">
@@ -6599,7 +6611,7 @@
       <c r="AJ28" s="144"/>
       <c r="AK28" s="150">
         <f>MAX($AL$11:$AL$98) - AL28</f>
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="AL28" s="121"/>
     </row>
@@ -6939,43 +6951,43 @@
         <v>6</v>
       </c>
       <c r="B31" s="84" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="C31" s="46">
         <v>5</v>
       </c>
       <c r="D31" s="45"/>
-      <c r="E31" s="210">
+      <c r="E31" s="44">
+        <v>6</v>
+      </c>
+      <c r="F31" s="45"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="215">
         <v>7</v>
       </c>
-      <c r="F31" s="45"/>
-      <c r="G31" s="48">
-        <v>5</v>
-      </c>
-      <c r="H31" s="47"/>
-      <c r="I31" s="44">
+      <c r="I31" s="44"/>
+      <c r="J31" s="47">
         <v>6</v>
       </c>
-      <c r="J31" s="47"/>
       <c r="K31" s="49">
         <v>5</v>
       </c>
       <c r="L31" s="47"/>
-      <c r="M31" s="44">
+      <c r="M31" s="44"/>
+      <c r="N31" s="211">
         <v>6</v>
       </c>
-      <c r="N31" s="45"/>
       <c r="O31" s="44">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P31" s="45"/>
-      <c r="Q31" s="213">
-        <v>7</v>
+      <c r="Q31" s="48">
+        <v>6</v>
       </c>
       <c r="R31" s="50"/>
       <c r="S31" s="122">
         <f>SUM(C32:R32)</f>
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="T31" s="46"/>
       <c r="U31" s="47">
@@ -6985,17 +6997,17 @@
         <v>6</v>
       </c>
       <c r="W31" s="47"/>
-      <c r="X31" s="49"/>
-      <c r="Y31" s="45">
-        <v>6</v>
-      </c>
-      <c r="Z31" s="48">
+      <c r="X31" s="49">
+        <v>5</v>
+      </c>
+      <c r="Y31" s="45"/>
+      <c r="Z31" s="48"/>
+      <c r="AA31" s="47">
         <v>7</v>
       </c>
-      <c r="AA31" s="47"/>
       <c r="AB31" s="122">
         <f>SUM(T32:AA32)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AC31" s="48"/>
       <c r="AD31" s="47"/>
@@ -7013,11 +7025,11 @@
       </c>
       <c r="AK31" s="111">
         <f>MAX($AL$11:$AL$98) - AL31</f>
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="AL31" s="122">
         <f>$S31+$AB31+$AG31+$AJ31</f>
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7033,17 +7045,17 @@
       <c r="D32" s="76"/>
       <c r="E32" s="77">
         <f>(IF($E31&lt;&gt;"",($E$7*$O$105)+IF($E$7=4,($O$103)+IF($E31=$E$7+$F$7,$O$104,0),0),0)+IF($F31&lt;&gt;"",($F$7*$O$105)+IF($F$7=4,($O$103)+IF($F31=$E$7+$F$7,$O$104,0),0),0))</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F32" s="76"/>
       <c r="G32" s="77">
         <f>(IF($G31&lt;&gt;"",($G$7*$O$105)+IF($G$7=4,($O$103)+IF($G31=$G$7+$H$7,$O$104,0),0),0)+IF($H31&lt;&gt;"",($H$7*$O$105)+IF($H$7=4,($O$103)+IF($H31=$G$7+$H$7,$O$104,0),0),0))</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="H32" s="76"/>
       <c r="I32" s="77">
         <f>(IF($I31&lt;&gt;"",($I$7*$O$105)+IF($I$7=4,($O$103)+IF($I31=$I$7+$J$7,$O$104,0),0),0)+IF($J31&lt;&gt;"",($J$7*$O$105)+IF($J$7=4,($O$103)+IF($J31=$I$7+$J$7,$O$104,0),0),0))</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J32" s="78"/>
       <c r="K32" s="79">
@@ -7053,7 +7065,7 @@
       <c r="L32" s="76"/>
       <c r="M32" s="77">
         <f>(IF($M31&lt;&gt;"",($M$7*$O$105)+IF($M$7=4,($O$103)+IF($M31=$M$7+$N$7,$O$104,0),0),0)+IF($N31&lt;&gt;"",($N$7*$O$105)+IF($N$7=4,($O$103)+IF($N31=$M$7+$N$7,$O$104,0),0),0))</f>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="N32" s="76"/>
       <c r="O32" s="77">
@@ -7063,7 +7075,7 @@
       <c r="P32" s="76"/>
       <c r="Q32" s="77">
         <f>(IF($Q31&lt;&gt;"",($Q$7*$O$105)+IF($Q$7=4,($O$103)+IF($Q31=$Q$7+$R$7,$O$104,0),0),0)+IF($R31&lt;&gt;"",($R$7*$O$105)+IF($R$7=4,($O$103)+IF($R31=$Q$7+$R$7,$O$104,0),0),0))</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="R32" s="80"/>
       <c r="S32" s="121"/>
@@ -7079,7 +7091,7 @@
       <c r="W32" s="126"/>
       <c r="X32" s="126">
         <f>(IF($X31&lt;&gt;"",($X$7*$P$105)+IF($X$7=4,($P$103)+IF($X31=$X$7+$Y$7,$P$104,0),0),0)+IF($Y31&lt;&gt;"",($Y$7*$P$105)+IF($Y$7=4,($P$103)+IF($Y31=$X$7+$Y$7,$P$104,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y32" s="59"/>
       <c r="Z32" s="126">
@@ -7098,7 +7110,7 @@
       <c r="AJ32" s="121"/>
       <c r="AK32" s="92">
         <f>MAX($AL$11:$AL$98) - AL32</f>
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="AL32" s="121"/>
     </row>
@@ -7141,13 +7153,13 @@
         <f>IF(ISBLANK(H31),
 0,
 IF(H$7 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33" s="118">
         <f>IF(ISBLANK(I31),
 0,
 IF(I$7= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J33" s="118">
         <f>IF(ISBLANK(J31),
@@ -7177,7 +7189,7 @@
         <f>IF(ISBLANK(N31),
 0,
 IF(N$7 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O33" s="118">
         <f>IF(ISBLANK(O31),
@@ -7263,7 +7275,7 @@
       <c r="AJ33" s="138"/>
       <c r="AK33" s="139">
         <f>SUM(C33:AI33)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AL33" s="123"/>
     </row>
@@ -7288,7 +7300,7 @@
         <f>IF(E33 = 0,
 0,
 IF(E31 = (E$7+F$7),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F34" s="118">
         <f>IF(F33 = 0,
@@ -7306,7 +7318,7 @@
         <f>IF(H33 = 0,
 0,
 IF(H31 = (G$7+H$7),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34" s="118">
         <f>IF(I33 = 0,
@@ -7342,7 +7354,7 @@
         <f>IF(N33 = 0,
 0,
 IF(N31 = (M$7+N$7),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O34" s="118">
         <f>IF(O33 = 0,
@@ -7360,7 +7372,7 @@
         <f>IF(Q33 = 0,
 0,
 IF(Q31 = (Q$7+R$7),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R34" s="118">
         <f>IF(R33 = 0,
@@ -7438,7 +7450,7 @@
         <v>7</v>
       </c>
       <c r="B35" s="217" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C35" s="229">
         <v>5</v>
@@ -7449,7 +7461,7 @@
       </c>
       <c r="F35" s="230"/>
       <c r="G35" s="232">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H35" s="233"/>
       <c r="I35" s="234">
@@ -7457,36 +7469,36 @@
       </c>
       <c r="J35" s="233"/>
       <c r="K35" s="235">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L35" s="233"/>
       <c r="M35" s="234">
+        <v>6</v>
+      </c>
+      <c r="N35" s="230"/>
+      <c r="O35" s="234">
         <v>5</v>
       </c>
-      <c r="N35" s="230"/>
-      <c r="O35" s="234"/>
-      <c r="P35" s="230">
+      <c r="P35" s="230"/>
+      <c r="Q35" s="249">
         <v>7</v>
       </c>
-      <c r="Q35" s="232"/>
-      <c r="R35" s="237">
-        <v>7</v>
-      </c>
+      <c r="R35" s="237"/>
       <c r="S35" s="239">
         <f>SUM(C36:R36)</f>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="T35" s="229"/>
       <c r="U35" s="233">
         <v>6</v>
       </c>
       <c r="V35" s="234">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="W35" s="233"/>
       <c r="X35" s="235"/>
       <c r="Y35" s="230">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Z35" s="232">
         <v>7</v>
@@ -7494,10 +7506,10 @@
       <c r="AA35" s="233"/>
       <c r="AB35" s="239">
         <f>SUM(T36:AA36)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AC35" s="232"/>
-      <c r="AD35" s="242"/>
+      <c r="AD35" s="233"/>
       <c r="AE35" s="235"/>
       <c r="AF35" s="233"/>
       <c r="AG35" s="239">
@@ -7512,11 +7524,11 @@
       </c>
       <c r="AK35" s="241">
         <f>MAX($AL$11:$AL$98) - AL35</f>
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="AL35" s="239">
         <f>$S35+$AB35+$AG35+$AJ35</f>
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7557,12 +7569,12 @@
       <c r="N36" s="76"/>
       <c r="O36" s="77">
         <f>(IF($O35&lt;&gt;"",($O$7*$O$105)+IF($O$7=4,($O$103)+IF($O35=$O$7+$P$7,$O$104,0),0),0)+IF($P35&lt;&gt;"",($P$7*$O$105)+IF($P$7=4,($O$103)+IF($P35=$O$7+$P$7,$O$104,0),0),0))</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="P36" s="76"/>
       <c r="Q36" s="77">
         <f>(IF($Q35&lt;&gt;"",($Q$7*$O$105)+IF($Q$7=4,($O$103)+IF($Q35=$Q$7+$R$7,$O$104,0),0),0)+IF($R35&lt;&gt;"",($R$7*$O$105)+IF($R$7=4,($O$103)+IF($R35=$Q$7+$R$7,$O$104,0),0),0))</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="R36" s="80"/>
       <c r="S36" s="121"/>
@@ -7578,7 +7590,7 @@
       <c r="W36" s="126"/>
       <c r="X36" s="126">
         <f>(IF($X35&lt;&gt;"",($X$7*$P$105)+IF($X$7=4,($P$103)+IF($X35=$X$7+$Y$7,$P$104,0),0),0)+IF($Y35&lt;&gt;"",($Y$7*$P$105)+IF($Y$7=4,($P$103)+IF($Y35=$X$7+$Y$7,$P$104,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y36" s="59"/>
       <c r="Z36" s="126">
@@ -7597,7 +7609,7 @@
       <c r="AJ36" s="121"/>
       <c r="AK36" s="92">
         <f>MAX($AL$11:$AL$98) - AL36</f>
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="AL36" s="121"/>
     </row>
@@ -7688,13 +7700,13 @@
         <f>IF(ISBLANK(P35),
 0,
 IF(P$7 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q37" s="118">
         <f>IF(ISBLANK(Q35),
 0,
 IF(Q$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R37" s="118">
         <f>IF(ISBLANK(R35),
@@ -7859,7 +7871,7 @@
         <f>IF(Q37 = 0,
 0,
 IF(Q35 = (Q$7+R$7),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R38" s="118">
         <f>IF(R37 = 0,
@@ -7927,7 +7939,7 @@
       <c r="AJ38" s="138"/>
       <c r="AK38" s="139">
         <f>SUM(C38:AI38)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL38" s="123"/>
     </row>
@@ -7937,10 +7949,10 @@
         <v>8</v>
       </c>
       <c r="B39" s="84" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C39" s="46">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D39" s="45"/>
       <c r="E39" s="210">
@@ -7951,52 +7963,52 @@
         <v>6</v>
       </c>
       <c r="H39" s="47"/>
-      <c r="I39" s="44"/>
-      <c r="J39" s="47">
-        <v>7</v>
-      </c>
+      <c r="I39" s="44">
+        <v>6</v>
+      </c>
+      <c r="J39" s="47"/>
       <c r="K39" s="49">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="L39" s="47"/>
       <c r="M39" s="44">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N39" s="45"/>
-      <c r="O39" s="44">
-        <v>6</v>
-      </c>
-      <c r="P39" s="45"/>
+      <c r="O39" s="44"/>
+      <c r="P39" s="45">
+        <v>7</v>
+      </c>
       <c r="Q39" s="48"/>
       <c r="R39" s="50">
         <v>7</v>
       </c>
       <c r="S39" s="122">
         <f>SUM(C40:R40)</f>
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="T39" s="46"/>
       <c r="U39" s="47">
-        <v>7</v>
-      </c>
-      <c r="V39" s="44"/>
-      <c r="W39" s="47">
-        <v>7</v>
-      </c>
-      <c r="X39" s="49">
-        <v>7</v>
-      </c>
-      <c r="Y39" s="45"/>
+        <v>6</v>
+      </c>
+      <c r="V39" s="44">
+        <v>5</v>
+      </c>
+      <c r="W39" s="47"/>
+      <c r="X39" s="49"/>
+      <c r="Y39" s="45">
+        <v>5</v>
+      </c>
       <c r="Z39" s="48">
         <v>7</v>
       </c>
       <c r="AA39" s="47"/>
       <c r="AB39" s="122">
         <f>SUM(T40:AA40)</f>
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="AC39" s="48"/>
-      <c r="AD39" s="47"/>
+      <c r="AD39" s="259"/>
       <c r="AE39" s="49"/>
       <c r="AF39" s="47"/>
       <c r="AG39" s="122">
@@ -8011,11 +8023,11 @@
       </c>
       <c r="AK39" s="111">
         <f>MAX($AL$11:$AL$98) - AL39</f>
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="AL39" s="122">
         <f>$S39+$AB39+$AG39+$AJ39</f>
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -8041,7 +8053,7 @@
       <c r="H40" s="76"/>
       <c r="I40" s="116">
         <f>(IF($I39&lt;&gt;"",($I$7*$O$105)+IF($I$7=4,($O$103)+IF($I39=$I$7+$J$7,$O$104,0),0),0)+IF($J39&lt;&gt;"",($J$7*$O$105)+IF($J$7=4,($O$103)+IF($J39=$I$7+$J$7,$O$104,0),0),0))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J40" s="78"/>
       <c r="K40" s="79">
@@ -8056,7 +8068,7 @@
       <c r="N40" s="76"/>
       <c r="O40" s="77">
         <f>(IF($O39&lt;&gt;"",($O$7*$O$105)+IF($O$7=4,($O$103)+IF($O39=$O$7+$P$7,$O$104,0),0),0)+IF($P39&lt;&gt;"",($P$7*$O$105)+IF($P$7=4,($O$103)+IF($P39=$O$7+$P$7,$O$104,0),0),0))</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="P40" s="76"/>
       <c r="Q40" s="77">
@@ -8072,7 +8084,7 @@
       <c r="U40" s="126"/>
       <c r="V40" s="126">
         <f>(IF($V39&lt;&gt;"",($V$7*$P$105)+IF($V$7=4,($P$103)+IF($V39=$V$7+$W$7,$P$104,0),0),0)+IF($W39&lt;&gt;"",($W$7*$P$105)+IF($W$7=4,($P$103)+IF($W39=$V$7+$W$7,$P$104,0),0),0))</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="W40" s="126"/>
       <c r="X40" s="126">
@@ -8096,7 +8108,7 @@
       <c r="AJ40" s="121"/>
       <c r="AK40" s="92">
         <f>MAX($AL$11:$AL$98) - AL40</f>
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="AL40" s="121"/>
     </row>
@@ -8145,7 +8157,7 @@
         <f>IF(ISBLANK(I39),
 0,
 IF(I$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J41" s="118">
         <f>IF(ISBLANK(J39),
@@ -8187,7 +8199,7 @@
         <f>IF(ISBLANK(P39),
 0,
 IF(P$7 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q41" s="118">
         <f>IF(ISBLANK(Q39),
@@ -8224,7 +8236,7 @@
         <f>IF(ISBLANK(W39),
 0,
 IF(W$7 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X41" s="118">
         <f>IF(ISBLANK(X39),
@@ -8261,7 +8273,7 @@
       <c r="AJ41" s="138"/>
       <c r="AK41" s="139">
         <f>SUM(C41:AI41)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL41" s="123"/>
     </row>
@@ -8436,63 +8448,63 @@
         <v>9</v>
       </c>
       <c r="B43" s="217" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C43" s="229">
         <v>6</v>
       </c>
       <c r="D43" s="230"/>
-      <c r="E43" s="234">
-        <v>5</v>
+      <c r="E43" s="231">
+        <v>7</v>
       </c>
       <c r="F43" s="230"/>
       <c r="G43" s="232">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H43" s="233"/>
       <c r="I43" s="234"/>
       <c r="J43" s="233">
+        <v>7</v>
+      </c>
+      <c r="K43" s="235">
+        <v>7</v>
+      </c>
+      <c r="L43" s="233"/>
+      <c r="M43" s="234">
         <v>6</v>
       </c>
-      <c r="K43" s="235">
-        <v>6</v>
-      </c>
-      <c r="L43" s="233"/>
-      <c r="M43" s="234"/>
-      <c r="N43" s="230">
-        <v>7</v>
-      </c>
+      <c r="N43" s="230"/>
       <c r="O43" s="234">
         <v>6</v>
       </c>
       <c r="P43" s="230"/>
-      <c r="Q43" s="249">
+      <c r="Q43" s="232"/>
+      <c r="R43" s="237">
         <v>7</v>
       </c>
-      <c r="R43" s="237"/>
       <c r="S43" s="239">
         <f>SUM(C44:R44)</f>
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="T43" s="229"/>
       <c r="U43" s="233">
         <v>7</v>
       </c>
-      <c r="V43" s="234">
-        <v>6</v>
-      </c>
-      <c r="W43" s="233"/>
-      <c r="X43" s="235"/>
-      <c r="Y43" s="230">
+      <c r="V43" s="234"/>
+      <c r="W43" s="233">
         <v>7</v>
       </c>
+      <c r="X43" s="235">
+        <v>7</v>
+      </c>
+      <c r="Y43" s="230"/>
       <c r="Z43" s="232">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AA43" s="233"/>
       <c r="AB43" s="239">
         <f>SUM(T44:AA44)</f>
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="AC43" s="232"/>
       <c r="AD43" s="233"/>
@@ -8510,11 +8522,11 @@
       </c>
       <c r="AK43" s="241">
         <f>MAX($AL$11:$AL$98) - AL43</f>
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="AL43" s="239">
         <f>$S43+$AB43+$AG43+$AJ43</f>
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -8530,7 +8542,7 @@
       <c r="D44" s="76"/>
       <c r="E44" s="116">
         <f>(IF($E43&lt;&gt;"",($E$7*$O$105)+IF($E$7=4,($O$103)+IF($E43=$E$7+$F$7,$O$104,0),0),0)+IF($F43&lt;&gt;"",($F$7*$O$105)+IF($F$7=4,($O$103)+IF($F43=$E$7+$F$7,$O$104,0),0),0))</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F44" s="76"/>
       <c r="G44" s="77">
@@ -8550,7 +8562,7 @@
       <c r="L44" s="76"/>
       <c r="M44" s="77">
         <f>(IF($M43&lt;&gt;"",($M$7*$O$105)+IF($M$7=4,($O$103)+IF($M43=$M$7+$N$7,$O$104,0),0),0)+IF($N43&lt;&gt;"",($N$7*$O$105)+IF($N$7=4,($O$103)+IF($N43=$M$7+$N$7,$O$104,0),0),0))</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="N44" s="151"/>
       <c r="O44" s="77">
@@ -8560,7 +8572,7 @@
       <c r="P44" s="76"/>
       <c r="Q44" s="77">
         <f>(IF($Q43&lt;&gt;"",($Q$7*$O$105)+IF($Q$7=4,($O$103)+IF($Q43=$Q$7+$R$7,$O$104,0),0),0)+IF($R43&lt;&gt;"",($R$7*$O$105)+IF($R$7=4,($O$103)+IF($R43=$Q$7+$R$7,$O$104,0),0),0))</f>
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="R44" s="80"/>
       <c r="S44" s="121"/>
@@ -8571,12 +8583,12 @@
       <c r="U44" s="126"/>
       <c r="V44" s="126">
         <f>(IF($V43&lt;&gt;"",($V$7*$P$105)+IF($V$7=4,($P$103)+IF($V43=$V$7+$W$7,$P$104,0),0),0)+IF($W43&lt;&gt;"",($W$7*$P$105)+IF($W$7=4,($P$103)+IF($W43=$V$7+$W$7,$P$104,0),0),0))</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="W44" s="126"/>
       <c r="X44" s="126">
         <f>(IF($X43&lt;&gt;"",($X$7*$P$105)+IF($X$7=4,($P$103)+IF($X43=$X$7+$Y$7,$P$104,0),0),0)+IF($Y43&lt;&gt;"",($Y$7*$P$105)+IF($Y$7=4,($P$103)+IF($Y43=$X$7+$Y$7,$P$104,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y44" s="59"/>
       <c r="Z44" s="126">
@@ -8595,7 +8607,7 @@
       <c r="AJ44" s="121"/>
       <c r="AK44" s="111">
         <f>MAX($AL$11:$AL$98) - AL44</f>
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="AL44" s="121"/>
     </row>
@@ -8674,7 +8686,7 @@
         <f>IF(ISBLANK(N43),
 0,
 IF(N$7 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O45" s="118">
         <f>IF(ISBLANK(O43),
@@ -8692,7 +8704,7 @@
         <f>IF(ISBLANK(Q43),
 0,
 IF(Q$7= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R45" s="118">
         <f>IF(ISBLANK(R43),
@@ -8723,7 +8735,7 @@
         <f>IF(ISBLANK(W43),
 0,
 IF(W$7 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X45" s="118">
         <f>IF(ISBLANK(X43),
@@ -8760,7 +8772,7 @@
       <c r="AJ45" s="138"/>
       <c r="AK45" s="139">
         <f>SUM(C45:AI45)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AL45" s="123"/>
     </row>
@@ -8785,7 +8797,7 @@
         <f>IF(E45 = 0,
 0,
 IF(E43 = (E$7+F$7),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46" s="118">
         <f>IF(F45 = 0,
@@ -8857,7 +8869,7 @@
         <f>IF(Q45 = 0,
 0,
 IF(Q43 = (Q$7+R$7),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R46" s="118">
         <f>IF(R45 = 0,
@@ -8935,18 +8947,18 @@
         <v>10</v>
       </c>
       <c r="B47" s="84" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="C47" s="46">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D47" s="45"/>
       <c r="E47" s="44">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F47" s="45"/>
       <c r="G47" s="48">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H47" s="47"/>
       <c r="I47" s="44"/>
@@ -8957,30 +8969,30 @@
         <v>6</v>
       </c>
       <c r="L47" s="47"/>
-      <c r="M47" s="44">
-        <v>5</v>
-      </c>
-      <c r="N47" s="45"/>
+      <c r="M47" s="44"/>
+      <c r="N47" s="45">
+        <v>7</v>
+      </c>
       <c r="O47" s="44">
         <v>6</v>
       </c>
       <c r="P47" s="45"/>
-      <c r="Q47" s="48"/>
-      <c r="R47" s="50">
-        <v>6</v>
-      </c>
+      <c r="Q47" s="213">
+        <v>7</v>
+      </c>
+      <c r="R47" s="50"/>
       <c r="S47" s="122">
         <f>SUM(C48:R48)</f>
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="T47" s="46"/>
       <c r="U47" s="47">
+        <v>7</v>
+      </c>
+      <c r="V47" s="44">
         <v>6</v>
       </c>
-      <c r="V47" s="44"/>
-      <c r="W47" s="47">
-        <v>7</v>
-      </c>
+      <c r="W47" s="47"/>
       <c r="X47" s="49"/>
       <c r="Y47" s="45">
         <v>7</v>
@@ -8991,10 +9003,10 @@
       <c r="AA47" s="47"/>
       <c r="AB47" s="122">
         <f>SUM(T48:AA48)</f>
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="AC47" s="48"/>
-      <c r="AD47" s="311"/>
+      <c r="AD47" s="47"/>
       <c r="AE47" s="49"/>
       <c r="AF47" s="47"/>
       <c r="AG47" s="122">
@@ -9009,11 +9021,11 @@
       </c>
       <c r="AK47" s="111">
         <f>MAX($AL$11:$AL$98) - AL47</f>
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="AL47" s="122">
         <f>$S47+$AB47+$AG47+$AJ47</f>
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -9049,7 +9061,7 @@
       <c r="L48" s="76"/>
       <c r="M48" s="77">
         <f>(IF($M47&lt;&gt;"",($M$7*$O$105)+IF($M$7=4,($O$103)+IF($M47=$M$7+$N$7,$O$104,0),0),0)+IF($N47&lt;&gt;"",($N$7*$O$105)+IF($N$7=4,($O$103)+IF($N47=$M$7+$N$7,$O$104,0),0),0))</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="N48" s="76"/>
       <c r="O48" s="77">
@@ -9059,7 +9071,7 @@
       <c r="P48" s="76"/>
       <c r="Q48" s="77">
         <f>(IF($Q47&lt;&gt;"",($Q$7*$O$105)+IF($Q$7=4,($O$103)+IF($Q47=$Q$7+$R$7,$O$104,0),0),0)+IF($R47&lt;&gt;"",($R$7*$O$105)+IF($R$7=4,($O$103)+IF($R47=$Q$7+$R$7,$O$104,0),0),0))</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="R48" s="80"/>
       <c r="S48" s="121"/>
@@ -9070,12 +9082,12 @@
       <c r="U48" s="126"/>
       <c r="V48" s="126">
         <f>(IF($V47&lt;&gt;"",($V$7*$P$105)+IF($V$7=4,($P$103)+IF($V47=$V$7+$W$7,$P$104,0),0),0)+IF($W47&lt;&gt;"",($W$7*$P$105)+IF($W$7=4,($P$103)+IF($W47=$V$7+$W$7,$P$104,0),0),0))</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="W48" s="126"/>
       <c r="X48" s="126">
         <f>(IF($X47&lt;&gt;"",($X$7*$P$105)+IF($X$7=4,($P$103)+IF($X47=$X$7+$Y$7,$P$104,0),0),0)+IF($Y47&lt;&gt;"",($Y$7*$P$105)+IF($Y$7=4,($P$103)+IF($Y47=$X$7+$Y$7,$P$104,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y48" s="59"/>
       <c r="Z48" s="126">
@@ -9094,7 +9106,7 @@
       <c r="AJ48" s="121"/>
       <c r="AK48" s="111">
         <f>MAX($AL$11:$AL$98) - AL48</f>
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="AL48" s="121"/>
     </row>
@@ -9173,7 +9185,7 @@
         <f>IF(ISBLANK(N47),
 0,
 IF(N$7 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O49" s="118">
         <f>IF(ISBLANK(O47),
@@ -9191,7 +9203,7 @@
         <f>IF(ISBLANK(Q47),
 0,
 IF(Q$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R49" s="118">
         <f>IF(ISBLANK(R47),
@@ -9222,7 +9234,7 @@
         <f>IF(ISBLANK(W47),
 0,
 IF(W$7 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X49" s="118">
         <f>IF(ISBLANK(X47),
@@ -9259,7 +9271,7 @@
       <c r="AJ49" s="138"/>
       <c r="AK49" s="139">
         <f>SUM(C49:AI49)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL49" s="123"/>
     </row>
@@ -9356,7 +9368,7 @@
         <f>IF(Q49 = 0,
 0,
 IF(Q47 = (Q$7+R$7),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R50" s="118">
         <f>IF(R49 = 0,
@@ -9424,24 +9436,24 @@
       <c r="AJ50" s="138"/>
       <c r="AK50" s="139">
         <f>SUM(C50:AI50)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL50" s="123"/>
     </row>
     <row r="51" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="216">
         <f>RANK(AL51,$AL$11:$AL$98,)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B51" s="217" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="C51" s="229">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D51" s="230"/>
       <c r="E51" s="234">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F51" s="230"/>
       <c r="G51" s="232">
@@ -9450,14 +9462,14 @@
       <c r="H51" s="233"/>
       <c r="I51" s="234"/>
       <c r="J51" s="233">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K51" s="235">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L51" s="233"/>
       <c r="M51" s="234">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="N51" s="230"/>
       <c r="O51" s="234">
@@ -9478,22 +9490,22 @@
       </c>
       <c r="V51" s="234"/>
       <c r="W51" s="233">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="X51" s="235"/>
       <c r="Y51" s="230">
         <v>7</v>
       </c>
-      <c r="Z51" s="232"/>
-      <c r="AA51" s="233">
+      <c r="Z51" s="232">
         <v>6</v>
       </c>
+      <c r="AA51" s="233"/>
       <c r="AB51" s="239">
         <f>SUM(T52:AA52)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AC51" s="232"/>
-      <c r="AD51" s="233"/>
+      <c r="AD51" s="242"/>
       <c r="AE51" s="235"/>
       <c r="AF51" s="233"/>
       <c r="AG51" s="239">
@@ -9508,11 +9520,11 @@
       </c>
       <c r="AK51" s="241">
         <f>MAX($AL$11:$AL$98) - AL51</f>
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="AL51" s="239">
         <f>$S51+$AB51+$AG51+$AJ51</f>
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -9574,7 +9586,7 @@
       <c r="W52" s="126"/>
       <c r="X52" s="126">
         <f>(IF($X51&lt;&gt;"",($X$7*$P$105)+IF($X$7=4,($P$103)+IF($X51=$X$7+$Y$7,$P$104,0),0),0)+IF($Y51&lt;&gt;"",($Y$7*$P$105)+IF($Y$7=4,($P$103)+IF($Y51=$X$7+$Y$7,$P$104,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y52" s="59"/>
       <c r="Z52" s="126">
@@ -9927,37 +9939,37 @@
     <row r="55" spans="1:38" s="27" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="117">
         <f>RANK(AL55,$AL$11:$AL$98,)</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B55" s="84" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C55" s="46">
         <v>6</v>
       </c>
       <c r="D55" s="45"/>
-      <c r="E55" s="44"/>
-      <c r="F55" s="45">
-        <v>7</v>
-      </c>
+      <c r="E55" s="44">
+        <v>6</v>
+      </c>
+      <c r="F55" s="45"/>
       <c r="G55" s="48">
         <v>6</v>
       </c>
       <c r="H55" s="47"/>
       <c r="I55" s="44"/>
       <c r="J55" s="47">
+        <v>7</v>
+      </c>
+      <c r="K55" s="49">
+        <v>5</v>
+      </c>
+      <c r="L55" s="47"/>
+      <c r="M55" s="44">
+        <v>7</v>
+      </c>
+      <c r="N55" s="45"/>
+      <c r="O55" s="44">
         <v>6</v>
-      </c>
-      <c r="K55" s="49"/>
-      <c r="L55" s="47">
-        <v>6</v>
-      </c>
-      <c r="M55" s="44"/>
-      <c r="N55" s="211">
-        <v>6</v>
-      </c>
-      <c r="O55" s="44">
-        <v>5</v>
       </c>
       <c r="P55" s="45"/>
       <c r="Q55" s="48"/>
@@ -9966,27 +9978,27 @@
       </c>
       <c r="S55" s="122">
         <f>SUM(C56:R56)</f>
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="T55" s="46"/>
       <c r="U55" s="47">
-        <v>5</v>
-      </c>
-      <c r="V55" s="44">
         <v>6</v>
       </c>
-      <c r="W55" s="47"/>
-      <c r="X55" s="49">
+      <c r="V55" s="44"/>
+      <c r="W55" s="47">
         <v>6</v>
       </c>
-      <c r="Y55" s="45"/>
+      <c r="X55" s="49"/>
+      <c r="Y55" s="45">
+        <v>7</v>
+      </c>
       <c r="Z55" s="48"/>
       <c r="AA55" s="47">
         <v>6</v>
       </c>
       <c r="AB55" s="122">
         <f>SUM(T56:AA56)</f>
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="AC55" s="48"/>
       <c r="AD55" s="47"/>
@@ -10004,11 +10016,11 @@
       </c>
       <c r="AK55" s="111">
         <f>MAX($AL$11:$AL$98) - AL55</f>
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="AL55" s="122">
         <f>$S55+$AB55+$AG55+$AJ55</f>
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="56" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -10024,7 +10036,7 @@
       <c r="D56" s="127"/>
       <c r="E56" s="125">
         <f>(IF($E55&lt;&gt;"",($E$7*$O$105)+IF($E$7=4,($O$103)+IF($E55=$E$7+$F$7,$O$104,0),0),0)+IF($F55&lt;&gt;"",($F$7*$O$105)+IF($F$7=4,($O$103)+IF($F55=$E$7+$F$7,$O$104,0),0),0))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F56" s="127"/>
       <c r="G56" s="125">
@@ -10039,12 +10051,12 @@
       <c r="J56" s="129"/>
       <c r="K56" s="130">
         <f>(IF($K55&lt;&gt;"",($K$7*$O$105)+IF($K$7=4,($O$103)+IF($K55=$K$7+$L$7,$O$104,0),0),0)+IF($L55&lt;&gt;"",($L$7*$O$105)+IF($L$7=4,($O$103)+IF($L55=$K$7+$L$7,$O$104,0),0),0))</f>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="L56" s="127"/>
       <c r="M56" s="125">
         <f>(IF($M55&lt;&gt;"",($M$7*$O$105)+IF($M$7=4,($O$103)+IF($M55=$M$7+$N$7,$O$104,0),0),0)+IF($N55&lt;&gt;"",($N$7*$O$105)+IF($N$7=4,($O$103)+IF($N55=$M$7+$N$7,$O$104,0),0),0))</f>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="N56" s="127"/>
       <c r="O56" s="128">
@@ -10065,7 +10077,7 @@
       <c r="U56" s="126"/>
       <c r="V56" s="126">
         <f>(IF($V55&lt;&gt;"",($V$7*$P$105)+IF($V$7=4,($P$103)+IF($V55=$V$7+$W$7,$P$104,0),0),0)+IF($W55&lt;&gt;"",($W$7*$P$105)+IF($W$7=4,($P$103)+IF($W55=$V$7+$W$7,$P$104,0),0),0))</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="W56" s="126"/>
       <c r="X56" s="126">
@@ -10111,7 +10123,7 @@
         <f>IF(ISBLANK(E55),
 0,
 IF(E$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F57" s="118">
         <f>IF(ISBLANK(F55),
@@ -10153,7 +10165,7 @@
         <f>IF(ISBLANK(L55),
 0,
 IF(L$7 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M57" s="118">
         <f>IF(ISBLANK(M55),
@@ -10165,7 +10177,7 @@
         <f>IF(ISBLANK(N55),
 0,
 IF(N$7 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O57" s="118">
         <f>IF(ISBLANK(O55),
@@ -10214,7 +10226,7 @@
         <f>IF(ISBLANK(W55),
 0,
 IF(W$7 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X57" s="118">
         <f>IF(ISBLANK(X55),
@@ -10330,7 +10342,7 @@
         <f>IF(N57 = 0,
 0,
 IF(N55 = (M$7+N$7),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O58" s="118">
         <f>IF(O57 = 0,
@@ -10416,7 +10428,7 @@
       <c r="AJ58" s="138"/>
       <c r="AK58" s="139">
         <f>SUM(C58:AI58)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL58" s="123"/>
     </row>
@@ -10426,63 +10438,63 @@
         <v>13</v>
       </c>
       <c r="B59" s="217" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C59" s="229">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D59" s="230"/>
       <c r="E59" s="234">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F59" s="230"/>
       <c r="G59" s="232">
         <v>6</v>
       </c>
       <c r="H59" s="233"/>
-      <c r="I59" s="234">
+      <c r="I59" s="234"/>
+      <c r="J59" s="233">
         <v>6</v>
       </c>
-      <c r="J59" s="233"/>
       <c r="K59" s="235">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L59" s="233"/>
       <c r="M59" s="234">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N59" s="230"/>
       <c r="O59" s="234">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P59" s="230"/>
       <c r="Q59" s="232"/>
       <c r="R59" s="237">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S59" s="239">
         <f>SUM(C60:R60)</f>
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="T59" s="229">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="U59" s="233"/>
       <c r="V59" s="234">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="W59" s="233"/>
-      <c r="X59" s="235"/>
-      <c r="Y59" s="230">
+      <c r="X59" s="235">
         <v>7</v>
       </c>
+      <c r="Y59" s="230"/>
       <c r="Z59" s="232">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AA59" s="233"/>
       <c r="AB59" s="239">
         <f>SUM(T60:AA60)</f>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="AC59" s="232"/>
       <c r="AD59" s="233"/>
@@ -10500,11 +10512,11 @@
       </c>
       <c r="AK59" s="241">
         <f>MAX($AL$11:$AL$98) - AL59</f>
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="AL59" s="239">
         <f>$S59+$AB59+$AG59+$AJ59</f>
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="60" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -10530,7 +10542,7 @@
       <c r="H60" s="127"/>
       <c r="I60" s="128">
         <f>(IF($I59&lt;&gt;"",($I$7*$O$105)+IF($I$7=4,($O$103)+IF($I59=$I$7+$J$7,$O$104,0),0),0)+IF($J59&lt;&gt;"",($J$7*$O$105)+IF($J$7=4,($O$103)+IF($J59=$I$7+$J$7,$O$104,0),0),0))</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J60" s="129"/>
       <c r="K60" s="130">
@@ -10556,7 +10568,7 @@
       <c r="S60" s="121"/>
       <c r="T60" s="126">
         <f>(IF($T59&lt;&gt;"",($T$7*$P$105)+IF($T$7=4,($P$103)+IF($T59=$T$7+$U$7,$P$104,0),0),0)+IF($U59&lt;&gt;"",($U$7*$P$105)+IF($U$7=4,($P$103)+IF($U59=$T$7+$U$7,$P$104,0),0),0))</f>
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="U60" s="126"/>
       <c r="V60" s="126">
@@ -10566,7 +10578,7 @@
       <c r="W60" s="126"/>
       <c r="X60" s="126">
         <f>(IF($X59&lt;&gt;"",($X$7*$P$105)+IF($X$7=4,($P$103)+IF($X59=$X$7+$Y$7,$P$104,0),0),0)+IF($Y59&lt;&gt;"",($Y$7*$P$105)+IF($Y$7=4,($P$103)+IF($Y59=$X$7+$Y$7,$P$104,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y60" s="59"/>
       <c r="Z60" s="126">
@@ -10631,7 +10643,7 @@
         <f>IF(ISBLANK(I59),
 0,
 IF(I$7= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J61" s="118">
         <f>IF(ISBLANK(J59),
@@ -10692,7 +10704,7 @@
         <f>IF(ISBLANK(T59),
 0,
 IF(T$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U61" s="118">
         <f>IF(ISBLANK(U59),
@@ -10919,31 +10931,31 @@
     <row r="63" spans="1:38" s="27" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="117">
         <f>RANK(AL63,$AL$11:$AL$98,)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B63" s="84" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C63" s="46">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D63" s="45"/>
-      <c r="E63" s="44">
-        <v>5</v>
-      </c>
-      <c r="F63" s="45"/>
+      <c r="E63" s="44"/>
+      <c r="F63" s="45">
+        <v>7</v>
+      </c>
       <c r="G63" s="48">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H63" s="47"/>
       <c r="I63" s="44"/>
       <c r="J63" s="47">
         <v>6</v>
       </c>
-      <c r="K63" s="49">
-        <v>5</v>
-      </c>
-      <c r="L63" s="47"/>
+      <c r="K63" s="49"/>
+      <c r="L63" s="47">
+        <v>6</v>
+      </c>
       <c r="M63" s="44"/>
       <c r="N63" s="211">
         <v>6</v>
@@ -10958,24 +10970,24 @@
       </c>
       <c r="S63" s="122">
         <f>SUM(C64:R64)</f>
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="T63" s="46"/>
       <c r="U63" s="47">
+        <v>5</v>
+      </c>
+      <c r="V63" s="44">
         <v>6</v>
-      </c>
-      <c r="V63" s="44">
-        <v>5</v>
       </c>
       <c r="W63" s="47"/>
       <c r="X63" s="49">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Y63" s="45"/>
-      <c r="Z63" s="48">
-        <v>7</v>
-      </c>
-      <c r="AA63" s="47"/>
+      <c r="Z63" s="48"/>
+      <c r="AA63" s="47">
+        <v>6</v>
+      </c>
       <c r="AB63" s="122">
         <f>SUM(T64:AA64)</f>
         <v>8</v>
@@ -10988,7 +11000,7 @@
         <f>SUM(AC64:AF64)</f>
         <v>0</v>
       </c>
-      <c r="AH63" s="252"/>
+      <c r="AH63" s="102"/>
       <c r="AI63" s="57"/>
       <c r="AJ63" s="122">
         <f>AH64</f>
@@ -10996,11 +11008,11 @@
       </c>
       <c r="AK63" s="111">
         <f>MAX($AL$11:$AL$98) - AL63</f>
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="AL63" s="122">
         <f>$S63+$AB63+$AG63+$AJ63</f>
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="64" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11016,7 +11028,7 @@
       <c r="D64" s="127"/>
       <c r="E64" s="125">
         <f>(IF($E63&lt;&gt;"",($E$7*$O$105)+IF($E$7=4,($O$103)+IF($E63=$E$7+$F$7,$O$104,0),0),0)+IF($F63&lt;&gt;"",($F$7*$O$105)+IF($F$7=4,($O$103)+IF($F63=$E$7+$F$7,$O$104,0),0),0))</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F64" s="127"/>
       <c r="G64" s="125">
@@ -11031,7 +11043,7 @@
       <c r="J64" s="129"/>
       <c r="K64" s="130">
         <f>(IF($K63&lt;&gt;"",($K$7*$O$105)+IF($K$7=4,($O$103)+IF($K63=$K$7+$L$7,$O$104,0),0),0)+IF($L63&lt;&gt;"",($L$7*$O$105)+IF($L$7=4,($O$103)+IF($L63=$K$7+$L$7,$O$104,0),0),0))</f>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="L64" s="127"/>
       <c r="M64" s="125">
@@ -11103,7 +11115,7 @@
         <f>IF(ISBLANK(E63),
 0,
 IF(E$7= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F65" s="118">
         <f>IF(ISBLANK(F63),
@@ -11145,7 +11157,7 @@
         <f>IF(ISBLANK(L63),
 0,
 IF(L$7 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M65" s="118">
         <f>IF(ISBLANK(M63),
@@ -11418,23 +11430,23 @@
         <v>15</v>
       </c>
       <c r="B67" s="217" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="C67" s="229">
         <v>5</v>
       </c>
       <c r="D67" s="230"/>
       <c r="E67" s="234">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F67" s="230"/>
       <c r="G67" s="232">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H67" s="233"/>
       <c r="I67" s="234"/>
       <c r="J67" s="233">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K67" s="235">
         <v>5</v>
@@ -11445,7 +11457,7 @@
         <v>6</v>
       </c>
       <c r="O67" s="234">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P67" s="230"/>
       <c r="Q67" s="232"/>
@@ -11464,17 +11476,17 @@
         <v>5</v>
       </c>
       <c r="W67" s="233"/>
-      <c r="X67" s="235"/>
-      <c r="Y67" s="230">
-        <v>5</v>
-      </c>
+      <c r="X67" s="235">
+        <v>7</v>
+      </c>
+      <c r="Y67" s="230"/>
       <c r="Z67" s="232">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AA67" s="233"/>
       <c r="AB67" s="239">
         <f>SUM(T68:AA68)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AC67" s="232"/>
       <c r="AD67" s="233"/>
@@ -11484,7 +11496,7 @@
         <f>SUM(AC68:AF68)</f>
         <v>0</v>
       </c>
-      <c r="AH67" s="246"/>
+      <c r="AH67" s="260"/>
       <c r="AI67" s="240"/>
       <c r="AJ67" s="239">
         <f>AH68</f>
@@ -11492,11 +11504,11 @@
       </c>
       <c r="AK67" s="241">
         <f>MAX($AL$11:$AL$98) - AL67</f>
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="AL67" s="239">
         <f>$S67+$AB67+$AG67+$AJ67</f>
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="68" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11558,7 +11570,7 @@
       <c r="W68" s="126"/>
       <c r="X68" s="126">
         <f>(IF($X67&lt;&gt;"",($X$7*$P$105)+IF($X$7=4,($P$103)+IF($X67=$X$7+$Y$7,$P$104,0),0),0)+IF($Y67&lt;&gt;"",($Y$7*$P$105)+IF($Y$7=4,($P$103)+IF($Y67=$X$7+$Y$7,$P$104,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y68" s="59"/>
       <c r="Z68" s="126">
@@ -11914,43 +11926,43 @@
         <v>15</v>
       </c>
       <c r="B71" s="84" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C71" s="46">
+        <v>5</v>
+      </c>
+      <c r="D71" s="45"/>
+      <c r="E71" s="44">
         <v>6</v>
-      </c>
-      <c r="D71" s="45"/>
-      <c r="E71" s="210">
-        <v>7</v>
       </c>
       <c r="F71" s="45"/>
       <c r="G71" s="48">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H71" s="47"/>
       <c r="I71" s="44"/>
       <c r="J71" s="47">
+        <v>7</v>
+      </c>
+      <c r="K71" s="49">
         <v>5</v>
       </c>
-      <c r="K71" s="49">
-        <v>7</v>
-      </c>
       <c r="L71" s="47"/>
-      <c r="M71" s="44">
+      <c r="M71" s="44"/>
+      <c r="N71" s="211">
         <v>6</v>
       </c>
-      <c r="N71" s="45"/>
       <c r="O71" s="44">
         <v>7</v>
       </c>
       <c r="P71" s="45"/>
-      <c r="Q71" s="48">
-        <v>5</v>
-      </c>
-      <c r="R71" s="50"/>
+      <c r="Q71" s="48"/>
+      <c r="R71" s="50">
+        <v>6</v>
+      </c>
       <c r="S71" s="122">
         <f>SUM(C72:R72)</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T71" s="46"/>
       <c r="U71" s="47">
@@ -11960,12 +11972,12 @@
         <v>5</v>
       </c>
       <c r="W71" s="47"/>
-      <c r="X71" s="49">
-        <v>4</v>
-      </c>
-      <c r="Y71" s="45"/>
+      <c r="X71" s="49"/>
+      <c r="Y71" s="45">
+        <v>5</v>
+      </c>
       <c r="Z71" s="48">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA71" s="47"/>
       <c r="AB71" s="122">
@@ -11988,11 +12000,11 @@
       </c>
       <c r="AK71" s="111">
         <f>MAX($AL$11:$AL$98) - AL71</f>
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="AL71" s="122">
         <f>$S71+$AB71+$AG71+$AJ71</f>
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="72" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -12008,7 +12020,7 @@
       <c r="D72" s="127"/>
       <c r="E72" s="125">
         <f>(IF($E71&lt;&gt;"",($E$7*$O$105)+IF($E$7=4,($O$103)+IF($E71=$E$7+$F$7,$O$104,0),0),0)+IF($F71&lt;&gt;"",($F$7*$O$105)+IF($F$7=4,($O$103)+IF($F71=$E$7+$F$7,$O$104,0),0),0))</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F72" s="127"/>
       <c r="G72" s="125">
@@ -12028,7 +12040,7 @@
       <c r="L72" s="127"/>
       <c r="M72" s="125">
         <f>(IF($M71&lt;&gt;"",($M$7*$O$105)+IF($M$7=4,($O$103)+IF($M71=$M$7+$N$7,$O$104,0),0),0)+IF($N71&lt;&gt;"",($N$7*$O$105)+IF($N$7=4,($O$103)+IF($N71=$M$7+$N$7,$O$104,0),0),0))</f>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="N72" s="127"/>
       <c r="O72" s="128">
@@ -12038,7 +12050,7 @@
       <c r="P72" s="127"/>
       <c r="Q72" s="128">
         <f>(IF($Q71&lt;&gt;"",($Q$7*$O$105)+IF($Q$7=4,($O$103)+IF($Q71=$Q$7+$R$7,$O$104,0),0),0)+IF($R71&lt;&gt;"",($R$7*$O$105)+IF($R$7=4,($O$103)+IF($R71=$Q$7+$R$7,$O$104,0),0),0))</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="R72" s="131"/>
       <c r="S72" s="121"/>
@@ -12149,7 +12161,7 @@
         <f>IF(ISBLANK(N71),
 0,
 IF(N$7 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O73" s="118">
         <f>IF(ISBLANK(O71),
@@ -12167,7 +12179,7 @@
         <f>IF(ISBLANK(Q71),
 0,
 IF(Q$7= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R73" s="118">
         <f>IF(ISBLANK(R71),
@@ -12260,7 +12272,7 @@
         <f>IF(E73 = 0,
 0,
 IF(E71 = (E$7+F$7),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F74" s="118">
         <f>IF(F73 = 0,
@@ -12314,7 +12326,7 @@
         <f>IF(N73 = 0,
 0,
 IF(N71 = (M$7+N$7),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O74" s="118">
         <f>IF(O73 = 0,
@@ -12410,54 +12422,54 @@
         <v>17</v>
       </c>
       <c r="B75" s="217" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="C75" s="229">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D75" s="230"/>
-      <c r="E75" s="234">
-        <v>6</v>
+      <c r="E75" s="231">
+        <v>7</v>
       </c>
       <c r="F75" s="230"/>
       <c r="G75" s="232">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H75" s="233"/>
       <c r="I75" s="234"/>
       <c r="J75" s="233">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K75" s="235">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L75" s="233"/>
       <c r="M75" s="234">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N75" s="230"/>
       <c r="O75" s="234">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P75" s="230"/>
-      <c r="Q75" s="232"/>
-      <c r="R75" s="237">
-        <v>7</v>
-      </c>
+      <c r="Q75" s="232">
+        <v>5</v>
+      </c>
+      <c r="R75" s="237"/>
       <c r="S75" s="239">
         <f>SUM(C76:R76)</f>
-        <v>20</v>
-      </c>
-      <c r="T75" s="229">
-        <v>7</v>
-      </c>
-      <c r="U75" s="233"/>
+        <v>28</v>
+      </c>
+      <c r="T75" s="229"/>
+      <c r="U75" s="233">
+        <v>6</v>
+      </c>
       <c r="V75" s="234">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="W75" s="233"/>
       <c r="X75" s="235">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="Y75" s="230"/>
       <c r="Z75" s="232">
@@ -12466,7 +12478,7 @@
       <c r="AA75" s="233"/>
       <c r="AB75" s="239">
         <f>SUM(T76:AA76)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AC75" s="232"/>
       <c r="AD75" s="233"/>
@@ -12484,11 +12496,11 @@
       </c>
       <c r="AK75" s="241">
         <f>MAX($AL$11:$AL$98) - AL75</f>
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="AL75" s="239">
         <f>$S75+$AB75+$AG75+$AJ75</f>
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="76" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -12504,7 +12516,7 @@
       <c r="D76" s="127"/>
       <c r="E76" s="125">
         <f>(IF($E75&lt;&gt;"",($E$7*$O$105)+IF($E$7=4,($O$103)+IF($E75=$E$7+$F$7,$O$104,0),0),0)+IF($F75&lt;&gt;"",($F$7*$O$105)+IF($F$7=4,($O$103)+IF($F75=$E$7+$F$7,$O$104,0),0),0))</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F76" s="127"/>
       <c r="G76" s="125">
@@ -12534,13 +12546,13 @@
       <c r="P76" s="127"/>
       <c r="Q76" s="128">
         <f>(IF($Q75&lt;&gt;"",($Q$7*$O$105)+IF($Q$7=4,($O$103)+IF($Q75=$Q$7+$R$7,$O$104,0),0),0)+IF($R75&lt;&gt;"",($R$7*$O$105)+IF($R$7=4,($O$103)+IF($R75=$Q$7+$R$7,$O$104,0),0),0))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="R76" s="131"/>
       <c r="S76" s="121"/>
       <c r="T76" s="126">
         <f>(IF($T75&lt;&gt;"",($T$7*$P$105)+IF($T$7=4,($P$103)+IF($T75=$T$7+$U$7,$P$104,0),0),0)+IF($U75&lt;&gt;"",($U$7*$P$105)+IF($U$7=4,($P$103)+IF($U75=$T$7+$U$7,$P$104,0),0),0))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U76" s="126"/>
       <c r="V76" s="126">
@@ -12663,7 +12675,7 @@
         <f>IF(ISBLANK(Q75),
 0,
 IF(Q$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R77" s="118">
         <f>IF(ISBLANK(R75),
@@ -12731,7 +12743,7 @@
       <c r="AJ77" s="138"/>
       <c r="AK77" s="139">
         <f>SUM(C77:AI77)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL77" s="123"/>
     </row>
@@ -12756,7 +12768,7 @@
         <f>IF(E77 = 0,
 0,
 IF(E75 = (E$7+F$7),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F78" s="118">
         <f>IF(F77 = 0,
@@ -12896,7 +12908,7 @@
       <c r="AJ78" s="138"/>
       <c r="AK78" s="139">
         <f>SUM(C78:AI78)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL78" s="123"/>
     </row>
@@ -12908,36 +12920,36 @@
       <c r="B79" s="84" t="s">
         <v>68</v>
       </c>
-      <c r="C79" s="253">
+      <c r="C79" s="252">
         <v>5</v>
       </c>
-      <c r="D79" s="254"/>
-      <c r="E79" s="255">
+      <c r="D79" s="253"/>
+      <c r="E79" s="254">
         <v>6</v>
       </c>
-      <c r="F79" s="254"/>
-      <c r="G79" s="256">
+      <c r="F79" s="253"/>
+      <c r="G79" s="255">
         <v>5</v>
       </c>
-      <c r="H79" s="257"/>
-      <c r="I79" s="255"/>
-      <c r="J79" s="257">
+      <c r="H79" s="256"/>
+      <c r="I79" s="254"/>
+      <c r="J79" s="256">
         <v>6</v>
       </c>
-      <c r="K79" s="258">
+      <c r="K79" s="257">
         <v>6</v>
       </c>
-      <c r="L79" s="257"/>
-      <c r="M79" s="255">
+      <c r="L79" s="256"/>
+      <c r="M79" s="254">
         <v>7</v>
       </c>
-      <c r="N79" s="254"/>
-      <c r="O79" s="255">
+      <c r="N79" s="253"/>
+      <c r="O79" s="254">
         <v>6</v>
       </c>
-      <c r="P79" s="254"/>
-      <c r="Q79" s="256"/>
-      <c r="R79" s="259">
+      <c r="P79" s="253"/>
+      <c r="Q79" s="255"/>
+      <c r="R79" s="258">
         <v>6</v>
       </c>
       <c r="S79" s="122">
@@ -12980,7 +12992,7 @@
       </c>
       <c r="AK79" s="111">
         <f>MAX($AL$11:$AL$98) - AL79</f>
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="AL79" s="122">
         <f>$S79+$AB79+$AG79+$AJ79</f>
@@ -13399,7 +13411,7 @@
     <row r="83" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="216">
         <f>RANK(AL83,$AL$11:$AL$98,)</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B83" s="217" t="s">
         <v>80</v>
@@ -13458,7 +13470,7 @@
       </c>
       <c r="AB83" s="239">
         <f>SUM(T84:AA84)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AC83" s="232"/>
       <c r="AD83" s="233"/>
@@ -13476,11 +13488,11 @@
       </c>
       <c r="AK83" s="241">
         <f>MAX($AL$11:$AL$98) - AL83</f>
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="AL83" s="239">
         <f>$S83+$AB83+$AG83+$AJ83</f>
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="84" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -13542,7 +13554,7 @@
       <c r="W84" s="126"/>
       <c r="X84" s="126">
         <f>(IF($X83&lt;&gt;"",($X$7*$P$105)+IF($X$7=4,($P$103)+IF($X83=$X$7+$Y$7,$P$104,0),0),0)+IF($Y83&lt;&gt;"",($Y$7*$P$105)+IF($Y$7=4,($P$103)+IF($Y83=$X$7+$Y$7,$P$104,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y84" s="59"/>
       <c r="Z84" s="126">
@@ -13972,7 +13984,7 @@
       </c>
       <c r="AK87" s="111">
         <f>MAX($AL$11:$AL$98) - AL87</f>
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="AL87" s="122">
         <f>$S87+$AB87+$AG87+$AJ87</f>
@@ -14394,10 +14406,10 @@
         <v>20</v>
       </c>
       <c r="B91" s="217" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C91" s="229">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D91" s="230"/>
       <c r="E91" s="234"/>
@@ -14405,28 +14417,28 @@
         <v>7</v>
       </c>
       <c r="G91" s="232">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H91" s="233"/>
       <c r="I91" s="234"/>
       <c r="J91" s="233">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K91" s="235">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L91" s="233"/>
       <c r="M91" s="234">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N91" s="230"/>
       <c r="O91" s="234">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P91" s="230"/>
       <c r="Q91" s="232"/>
       <c r="R91" s="237">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S91" s="239">
         <f>SUM(C92:R92)</f>
@@ -14437,13 +14449,13 @@
         <v>7</v>
       </c>
       <c r="V91" s="234">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="W91" s="233"/>
-      <c r="X91" s="235">
+      <c r="X91" s="235"/>
+      <c r="Y91" s="230">
         <v>6</v>
       </c>
-      <c r="Y91" s="230"/>
       <c r="Z91" s="232">
         <v>6</v>
       </c>
@@ -14468,7 +14480,7 @@
       </c>
       <c r="AK91" s="241">
         <f>MAX($AL$11:$AL$98) - AL91</f>
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="AL91" s="239">
         <f>$S91+$AB91+$AG91+$AJ91</f>
@@ -14887,13 +14899,13 @@
     <row r="95" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A95" s="117">
         <f>RANK(AL95,$AL$11:$AL$98,)</f>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B95" s="84" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C95" s="187">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D95" s="188"/>
       <c r="E95" s="189"/>
@@ -14901,28 +14913,28 @@
         <v>7</v>
       </c>
       <c r="G95" s="190">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H95" s="191"/>
       <c r="I95" s="189"/>
       <c r="J95" s="191">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K95" s="192">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L95" s="191"/>
       <c r="M95" s="189">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N95" s="188"/>
       <c r="O95" s="189">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P95" s="188"/>
       <c r="Q95" s="190"/>
       <c r="R95" s="193">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S95" s="122">
         <f>SUM(C96:R96)</f>
@@ -14933,20 +14945,20 @@
         <v>7</v>
       </c>
       <c r="V95" s="44">
+        <v>7</v>
+      </c>
+      <c r="W95" s="47"/>
+      <c r="X95" s="49">
         <v>6</v>
       </c>
-      <c r="W95" s="47"/>
-      <c r="X95" s="49"/>
-      <c r="Y95" s="45">
-        <v>6</v>
-      </c>
+      <c r="Y95" s="45"/>
       <c r="Z95" s="48">
         <v>6</v>
       </c>
       <c r="AA95" s="47"/>
       <c r="AB95" s="179">
         <f>SUM(T96:AA96)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AC95" s="48"/>
       <c r="AD95" s="47"/>
@@ -14964,11 +14976,11 @@
       </c>
       <c r="AK95" s="111">
         <f>MAX($AL$11:$AL$98) - AL95</f>
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="AL95" s="179">
         <f>$S95+$AB95+$AG95+$AJ95</f>
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="96" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -15030,7 +15042,7 @@
       <c r="W96" s="126"/>
       <c r="X96" s="126">
         <f>(IF($X95&lt;&gt;"",($X$7*$P$105)+IF($X$7=4,($P$103)+IF($X95=$X$7+$Y$7,$P$104,0),0),0)+IF($Y95&lt;&gt;"",($Y$7*$P$105)+IF($Y$7=4,($P$103)+IF($Y95=$X$7+$Y$7,$P$104,0),0),0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y96" s="59"/>
       <c r="Z96" s="126">
@@ -15513,12 +15525,12 @@
     <row r="101" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B101" s="43"/>
       <c r="N101" s="26"/>
-      <c r="O101" s="292" t="s">
+      <c r="O101" s="298" t="s">
         <v>17</v>
       </c>
-      <c r="P101" s="293"/>
-      <c r="Q101" s="293"/>
-      <c r="R101" s="294"/>
+      <c r="P101" s="299"/>
+      <c r="Q101" s="299"/>
+      <c r="R101" s="300"/>
       <c r="AG101" s="30"/>
       <c r="AH101" s="30"/>
       <c r="AI101" s="30"/>
@@ -15527,21 +15539,21 @@
     </row>
     <row r="102" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A102" s="33"/>
-      <c r="B102" s="280" t="s">
+      <c r="B102" s="288" t="s">
         <v>16</v>
       </c>
-      <c r="C102" s="281"/>
-      <c r="D102" s="281"/>
-      <c r="E102" s="281"/>
-      <c r="F102" s="281"/>
-      <c r="G102" s="281"/>
-      <c r="H102" s="281"/>
-      <c r="I102" s="281"/>
-      <c r="J102" s="281"/>
-      <c r="K102" s="281"/>
-      <c r="L102" s="281"/>
-      <c r="M102" s="281"/>
-      <c r="N102" s="282"/>
+      <c r="C102" s="289"/>
+      <c r="D102" s="289"/>
+      <c r="E102" s="289"/>
+      <c r="F102" s="289"/>
+      <c r="G102" s="289"/>
+      <c r="H102" s="289"/>
+      <c r="I102" s="289"/>
+      <c r="J102" s="289"/>
+      <c r="K102" s="289"/>
+      <c r="L102" s="289"/>
+      <c r="M102" s="289"/>
+      <c r="N102" s="290"/>
       <c r="O102" s="21">
         <v>1</v>
       </c>
@@ -15554,45 +15566,45 @@
       <c r="R102" s="22">
         <v>4</v>
       </c>
-      <c r="U102" s="295" t="s">
+      <c r="U102" s="301" t="s">
         <v>26</v>
       </c>
-      <c r="V102" s="296"/>
-      <c r="W102" s="296"/>
-      <c r="X102" s="296"/>
-      <c r="Y102" s="296"/>
-      <c r="Z102" s="296"/>
-      <c r="AA102" s="296"/>
-      <c r="AB102" s="296"/>
-      <c r="AC102" s="296"/>
-      <c r="AD102" s="297"/>
+      <c r="V102" s="302"/>
+      <c r="W102" s="302"/>
+      <c r="X102" s="302"/>
+      <c r="Y102" s="302"/>
+      <c r="Z102" s="302"/>
+      <c r="AA102" s="302"/>
+      <c r="AB102" s="302"/>
+      <c r="AC102" s="302"/>
+      <c r="AD102" s="303"/>
       <c r="AE102" s="28"/>
       <c r="AF102" s="28"/>
-      <c r="AG102" s="298" t="s">
+      <c r="AG102" s="304" t="s">
         <v>24</v>
       </c>
-      <c r="AH102" s="299"/>
-      <c r="AI102" s="299"/>
-      <c r="AJ102" s="299"/>
-      <c r="AK102" s="300"/>
+      <c r="AH102" s="305"/>
+      <c r="AI102" s="305"/>
+      <c r="AJ102" s="305"/>
+      <c r="AK102" s="306"/>
     </row>
     <row r="103" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A103" s="34"/>
-      <c r="B103" s="260" t="s">
+      <c r="B103" s="271" t="s">
         <v>6</v>
       </c>
-      <c r="C103" s="261"/>
-      <c r="D103" s="261"/>
-      <c r="E103" s="261"/>
-      <c r="F103" s="261"/>
-      <c r="G103" s="261"/>
-      <c r="H103" s="261"/>
-      <c r="I103" s="261"/>
-      <c r="J103" s="261"/>
-      <c r="K103" s="261"/>
-      <c r="L103" s="261"/>
-      <c r="M103" s="261"/>
-      <c r="N103" s="262"/>
+      <c r="C103" s="265"/>
+      <c r="D103" s="265"/>
+      <c r="E103" s="265"/>
+      <c r="F103" s="265"/>
+      <c r="G103" s="265"/>
+      <c r="H103" s="265"/>
+      <c r="I103" s="265"/>
+      <c r="J103" s="265"/>
+      <c r="K103" s="265"/>
+      <c r="L103" s="265"/>
+      <c r="M103" s="265"/>
+      <c r="N103" s="266"/>
       <c r="O103" s="20">
         <v>5</v>
       </c>
@@ -15605,49 +15617,49 @@
       <c r="R103" s="23">
         <v>20</v>
       </c>
-      <c r="U103" s="285" t="s">
+      <c r="U103" s="293" t="s">
         <v>20</v>
       </c>
-      <c r="V103" s="286"/>
-      <c r="W103" s="286"/>
-      <c r="X103" s="286"/>
-      <c r="Y103" s="286"/>
-      <c r="Z103" s="286"/>
-      <c r="AA103" s="286"/>
-      <c r="AB103" s="283">
+      <c r="V103" s="294"/>
+      <c r="W103" s="294"/>
+      <c r="X103" s="294"/>
+      <c r="Y103" s="294"/>
+      <c r="Z103" s="294"/>
+      <c r="AA103" s="294"/>
+      <c r="AB103" s="291">
         <v>22</v>
       </c>
-      <c r="AC103" s="283"/>
-      <c r="AD103" s="284"/>
+      <c r="AC103" s="291"/>
+      <c r="AD103" s="292"/>
       <c r="AE103" s="29"/>
       <c r="AF103" s="29"/>
-      <c r="AG103" s="267" t="s">
+      <c r="AG103" s="261" t="s">
         <v>21</v>
       </c>
-      <c r="AH103" s="268"/>
-      <c r="AI103" s="268"/>
-      <c r="AJ103" s="269"/>
+      <c r="AH103" s="262"/>
+      <c r="AI103" s="262"/>
+      <c r="AJ103" s="263"/>
       <c r="AK103" s="184">
         <v>230</v>
       </c>
     </row>
     <row r="104" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="34"/>
-      <c r="B104" s="260" t="s">
+      <c r="B104" s="271" t="s">
         <v>5</v>
       </c>
-      <c r="C104" s="261"/>
-      <c r="D104" s="261"/>
-      <c r="E104" s="261"/>
-      <c r="F104" s="261"/>
-      <c r="G104" s="261"/>
-      <c r="H104" s="261"/>
-      <c r="I104" s="261"/>
-      <c r="J104" s="261"/>
-      <c r="K104" s="261"/>
-      <c r="L104" s="261"/>
-      <c r="M104" s="261"/>
-      <c r="N104" s="262"/>
+      <c r="C104" s="265"/>
+      <c r="D104" s="265"/>
+      <c r="E104" s="265"/>
+      <c r="F104" s="265"/>
+      <c r="G104" s="265"/>
+      <c r="H104" s="265"/>
+      <c r="I104" s="265"/>
+      <c r="J104" s="265"/>
+      <c r="K104" s="265"/>
+      <c r="L104" s="265"/>
+      <c r="M104" s="265"/>
+      <c r="N104" s="266"/>
       <c r="O104" s="20">
         <v>2</v>
       </c>
@@ -15660,49 +15672,49 @@
       <c r="R104" s="23">
         <v>8</v>
       </c>
-      <c r="U104" s="265" t="s">
+      <c r="U104" s="267" t="s">
         <v>18</v>
       </c>
-      <c r="V104" s="266"/>
-      <c r="W104" s="266"/>
-      <c r="X104" s="266"/>
-      <c r="Y104" s="266"/>
-      <c r="Z104" s="266"/>
-      <c r="AA104" s="266"/>
-      <c r="AB104" s="290">
+      <c r="V104" s="268"/>
+      <c r="W104" s="268"/>
+      <c r="X104" s="268"/>
+      <c r="Y104" s="268"/>
+      <c r="Z104" s="268"/>
+      <c r="AA104" s="268"/>
+      <c r="AB104" s="269">
         <v>20</v>
       </c>
-      <c r="AC104" s="290"/>
-      <c r="AD104" s="291"/>
+      <c r="AC104" s="269"/>
+      <c r="AD104" s="270"/>
       <c r="AE104" s="29"/>
       <c r="AF104" s="29"/>
-      <c r="AG104" s="270" t="s">
+      <c r="AG104" s="264" t="s">
         <v>22</v>
       </c>
-      <c r="AH104" s="261"/>
-      <c r="AI104" s="261"/>
-      <c r="AJ104" s="262"/>
+      <c r="AH104" s="265"/>
+      <c r="AI104" s="265"/>
+      <c r="AJ104" s="266"/>
       <c r="AK104" s="36">
         <v>115</v>
       </c>
     </row>
     <row r="105" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A105" s="35"/>
-      <c r="B105" s="274" t="s">
+      <c r="B105" s="281" t="s">
         <v>4</v>
       </c>
-      <c r="C105" s="275"/>
-      <c r="D105" s="275"/>
-      <c r="E105" s="275"/>
-      <c r="F105" s="275"/>
-      <c r="G105" s="275"/>
-      <c r="H105" s="275"/>
-      <c r="I105" s="275"/>
-      <c r="J105" s="275"/>
-      <c r="K105" s="275"/>
-      <c r="L105" s="275"/>
-      <c r="M105" s="275"/>
-      <c r="N105" s="276"/>
+      <c r="C105" s="282"/>
+      <c r="D105" s="282"/>
+      <c r="E105" s="282"/>
+      <c r="F105" s="282"/>
+      <c r="G105" s="282"/>
+      <c r="H105" s="282"/>
+      <c r="I105" s="282"/>
+      <c r="J105" s="282"/>
+      <c r="K105" s="282"/>
+      <c r="L105" s="282"/>
+      <c r="M105" s="282"/>
+      <c r="N105" s="283"/>
       <c r="O105" s="3">
         <v>1</v>
       </c>
@@ -15715,67 +15727,66 @@
       <c r="R105" s="24">
         <v>1</v>
       </c>
-      <c r="U105" s="287" t="s">
+      <c r="U105" s="295" t="s">
         <v>19</v>
       </c>
-      <c r="V105" s="264"/>
-      <c r="W105" s="264"/>
-      <c r="X105" s="264"/>
-      <c r="Y105" s="264"/>
-      <c r="Z105" s="264"/>
-      <c r="AA105" s="264"/>
-      <c r="AB105" s="288">
+      <c r="V105" s="273"/>
+      <c r="W105" s="273"/>
+      <c r="X105" s="273"/>
+      <c r="Y105" s="273"/>
+      <c r="Z105" s="273"/>
+      <c r="AA105" s="273"/>
+      <c r="AB105" s="296">
         <f>AB103*AB104</f>
         <v>440</v>
       </c>
-      <c r="AC105" s="288"/>
-      <c r="AD105" s="289"/>
+      <c r="AC105" s="296"/>
+      <c r="AD105" s="297"/>
       <c r="AE105" s="29"/>
       <c r="AF105" s="29"/>
-      <c r="AG105" s="270" t="s">
+      <c r="AG105" s="264" t="s">
         <v>25</v>
       </c>
-      <c r="AH105" s="261"/>
-      <c r="AI105" s="261"/>
-      <c r="AJ105" s="262"/>
+      <c r="AH105" s="265"/>
+      <c r="AI105" s="265"/>
+      <c r="AJ105" s="266"/>
       <c r="AK105" s="36">
         <v>65</v>
       </c>
     </row>
     <row r="106" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG106" s="265" t="s">
+      <c r="AG106" s="267" t="s">
         <v>23</v>
       </c>
-      <c r="AH106" s="266"/>
-      <c r="AI106" s="266"/>
-      <c r="AJ106" s="266"/>
+      <c r="AH106" s="268"/>
+      <c r="AI106" s="268"/>
+      <c r="AJ106" s="268"/>
       <c r="AK106" s="186">
         <v>30</v>
       </c>
     </row>
     <row r="107" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG107" s="263" t="s">
+      <c r="AG107" s="272" t="s">
         <v>19</v>
       </c>
-      <c r="AH107" s="264"/>
-      <c r="AI107" s="264"/>
-      <c r="AJ107" s="264"/>
+      <c r="AH107" s="273"/>
+      <c r="AI107" s="273"/>
+      <c r="AJ107" s="273"/>
       <c r="AK107" s="185">
         <f>SUM(AK103:AK106)</f>
         <v>440</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A10:AL94">
-    <sortCondition descending="1" ref="AL10:AL94"/>
-    <sortCondition ref="B10:B94"/>
+  <sortState ref="A11:AL95">
+    <sortCondition descending="1" ref="AL11:AL95"/>
+    <sortCondition ref="B11:B95"/>
   </sortState>
   <mergeCells count="40">
-    <mergeCell ref="C2:P2"/>
-    <mergeCell ref="Q2:AJ2"/>
-    <mergeCell ref="O101:R101"/>
-    <mergeCell ref="U102:AD102"/>
-    <mergeCell ref="AG102:AK102"/>
+    <mergeCell ref="C5:S5"/>
+    <mergeCell ref="T5:AB5"/>
+    <mergeCell ref="AC5:AG5"/>
+    <mergeCell ref="C6:J6"/>
     <mergeCell ref="AH5:AJ5"/>
     <mergeCell ref="AG6:AG10"/>
     <mergeCell ref="AJ6:AJ10"/>
@@ -15783,34 +15794,35 @@
     <mergeCell ref="AB6:AB10"/>
     <mergeCell ref="AC6:AD6"/>
     <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="C5:S5"/>
-    <mergeCell ref="T5:AB5"/>
-    <mergeCell ref="AC5:AG5"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="K6:R6"/>
-    <mergeCell ref="S6:S10"/>
-    <mergeCell ref="T6:W6"/>
-    <mergeCell ref="B105:N105"/>
     <mergeCell ref="C1:O1"/>
     <mergeCell ref="P1:AJ1"/>
     <mergeCell ref="C4:O4"/>
     <mergeCell ref="P4:AJ4"/>
     <mergeCell ref="C3:P3"/>
     <mergeCell ref="Q3:AJ3"/>
+    <mergeCell ref="C2:P2"/>
+    <mergeCell ref="Q2:AJ2"/>
+    <mergeCell ref="B104:N104"/>
+    <mergeCell ref="AG107:AJ107"/>
+    <mergeCell ref="AG106:AJ106"/>
+    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="S6:S10"/>
+    <mergeCell ref="T6:W6"/>
+    <mergeCell ref="B105:N105"/>
     <mergeCell ref="B102:N102"/>
     <mergeCell ref="AB103:AD103"/>
     <mergeCell ref="U103:AA103"/>
     <mergeCell ref="B103:N103"/>
     <mergeCell ref="U105:AA105"/>
     <mergeCell ref="AB105:AD105"/>
-    <mergeCell ref="U104:AA104"/>
-    <mergeCell ref="AB104:AD104"/>
-    <mergeCell ref="B104:N104"/>
-    <mergeCell ref="AG107:AJ107"/>
-    <mergeCell ref="AG106:AJ106"/>
+    <mergeCell ref="O101:R101"/>
+    <mergeCell ref="U102:AD102"/>
+    <mergeCell ref="AG102:AK102"/>
     <mergeCell ref="AG103:AJ103"/>
     <mergeCell ref="AG105:AJ105"/>
     <mergeCell ref="AG104:AJ104"/>
+    <mergeCell ref="U104:AA104"/>
+    <mergeCell ref="AB104:AD104"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <conditionalFormatting sqref="S11:S16 AB11:AB16 AG11:AG16 AJ11:AJ16 AJ27:AJ28 AG27:AG28 AB27:AB28 S27:S28 AJ23:AJ24 AG23:AG24 AB23:AB24 S23:S24 AJ19:AJ20 AG19:AG20 AB19:AB20 S19:S20 S39:S40 AB39:AB40 AG39:AG40 AJ39:AJ40 S31:S32 AB31:AB32 AG31:AG32 AJ31:AJ32 AJ43:AJ44 AG43:AG44 AB43:AB44 S43:S44 S47:S48 AB47:AB48 AG47:AG48 AJ47:AJ48 AJ51 AG51 AB51 S51 S59 AB59 AG59 AJ59 S55 AB55 AG55 AJ55 AJ63 AG63 AB63 S63 S67 AB67 AG67 AJ67 AJ71 AG71 AB71 S71 S75 AB75 AG75 AJ75 AJ79 AG79 AB79 S79 AJ35:AJ36 AG35:AG36 AB35:AB36 S35:S36">
@@ -16453,7 +16465,7 @@
   <dimension ref="A1:AJ31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T24" sqref="T24"/>
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16684,11 +16696,13 @@
       <c r="S6" s="81">
         <v>4</v>
       </c>
-      <c r="T6" s="81"/>
+      <c r="T6" s="81">
+        <v>3</v>
+      </c>
       <c r="U6" s="81"/>
       <c r="V6" s="73">
         <f>IF(O6&gt;O7,1,0)+IF(P6&gt;P7,1,0)+IF(Q6&gt;Q7,1,0)+IF(R6&gt;R7,1,0)+IF(S6&gt;S7,1,0)+IF(T6&gt;T7,1,0)+IF(U6&gt;U7,1,0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W6" s="13"/>
       <c r="Y6" s="86"/>
@@ -16756,7 +16770,9 @@
       <c r="S7" s="81">
         <v>3</v>
       </c>
-      <c r="T7" s="81"/>
+      <c r="T7" s="81">
+        <v>0</v>
+      </c>
       <c r="U7" s="81"/>
       <c r="V7" s="73">
         <f>IF(O7&gt;O6,1,0)+IF(P7&gt;P6,1,0)+IF(Q7&gt;Q6,1,0)+IF(R7&gt;R6,1,0)+IF(S7&gt;S6,1,0)+IF(T7&gt;T6,1,0)+IF(U7&gt;U6,1,0)</f>
@@ -17407,7 +17423,9 @@
       <c r="S20" s="81">
         <v>2</v>
       </c>
-      <c r="T20" s="81"/>
+      <c r="T20" s="81">
+        <v>3</v>
+      </c>
       <c r="U20" s="81"/>
       <c r="V20" s="73">
         <f>IF(O20&gt;O21,1,0)+IF(P20&gt;P21,1,0)+IF(Q20&gt;Q21,1,0)+IF(R20&gt;R21,1,0)+IF(S20&gt;S21,1,0)+IF(T20&gt;T21,1,0)+IF(U20&gt;U21,1,0)</f>
@@ -17479,11 +17497,13 @@
       <c r="S21" s="81">
         <v>1</v>
       </c>
-      <c r="T21" s="81"/>
+      <c r="T21" s="81">
+        <v>4</v>
+      </c>
       <c r="U21" s="81"/>
       <c r="V21" s="73">
         <f>IF(O21&gt;O20,1,0)+IF(P21&gt;P20,1,0)+IF(Q21&gt;Q20,1,0)+IF(R21&gt;R20,1,0)+IF(S21&gt;S20,1,0)+IF(T21&gt;T20,1,0)+IF(U21&gt;U20,1,0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W21" s="14"/>
       <c r="X21" s="4"/>

</xml_diff>

<commit_message>
Updated games of 2019-05-07
</commit_message>
<xml_diff>
--- a/laval.xlsx
+++ b/laval.xlsx
@@ -2520,10 +2520,154 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="83" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="92" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2538,161 +2682,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="85" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="83" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3758,258 +3758,258 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="C1" s="284"/>
-      <c r="D1" s="284"/>
-      <c r="E1" s="284"/>
-      <c r="F1" s="284"/>
-      <c r="G1" s="284"/>
-      <c r="H1" s="284"/>
-      <c r="I1" s="284"/>
-      <c r="J1" s="284"/>
-      <c r="K1" s="284"/>
-      <c r="L1" s="284"/>
-      <c r="M1" s="284"/>
-      <c r="N1" s="284"/>
-      <c r="O1" s="284"/>
-      <c r="P1" s="285"/>
-      <c r="Q1" s="285"/>
-      <c r="R1" s="285"/>
-      <c r="S1" s="285"/>
-      <c r="T1" s="285"/>
-      <c r="U1" s="285"/>
-      <c r="V1" s="285"/>
-      <c r="W1" s="285"/>
-      <c r="X1" s="285"/>
-      <c r="Y1" s="285"/>
-      <c r="Z1" s="285"/>
-      <c r="AA1" s="285"/>
-      <c r="AB1" s="285"/>
-      <c r="AC1" s="285"/>
-      <c r="AD1" s="285"/>
-      <c r="AE1" s="285"/>
-      <c r="AF1" s="285"/>
-      <c r="AG1" s="285"/>
-      <c r="AH1" s="285"/>
-      <c r="AI1" s="285"/>
-      <c r="AJ1" s="285"/>
+      <c r="C1" s="276"/>
+      <c r="D1" s="276"/>
+      <c r="E1" s="276"/>
+      <c r="F1" s="276"/>
+      <c r="G1" s="276"/>
+      <c r="H1" s="276"/>
+      <c r="I1" s="276"/>
+      <c r="J1" s="276"/>
+      <c r="K1" s="276"/>
+      <c r="L1" s="276"/>
+      <c r="M1" s="276"/>
+      <c r="N1" s="276"/>
+      <c r="O1" s="276"/>
+      <c r="P1" s="277"/>
+      <c r="Q1" s="277"/>
+      <c r="R1" s="277"/>
+      <c r="S1" s="277"/>
+      <c r="T1" s="277"/>
+      <c r="U1" s="277"/>
+      <c r="V1" s="277"/>
+      <c r="W1" s="277"/>
+      <c r="X1" s="277"/>
+      <c r="Y1" s="277"/>
+      <c r="Z1" s="277"/>
+      <c r="AA1" s="277"/>
+      <c r="AB1" s="277"/>
+      <c r="AC1" s="277"/>
+      <c r="AD1" s="277"/>
+      <c r="AE1" s="277"/>
+      <c r="AF1" s="277"/>
+      <c r="AG1" s="277"/>
+      <c r="AH1" s="277"/>
+      <c r="AI1" s="277"/>
+      <c r="AJ1" s="277"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="41"/>
-      <c r="C2" s="286" t="s">
+      <c r="C2" s="278" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="286"/>
-      <c r="E2" s="286"/>
-      <c r="F2" s="286"/>
-      <c r="G2" s="286"/>
-      <c r="H2" s="286"/>
-      <c r="I2" s="286"/>
-      <c r="J2" s="286"/>
-      <c r="K2" s="286"/>
-      <c r="L2" s="286"/>
-      <c r="M2" s="286"/>
-      <c r="N2" s="286"/>
-      <c r="O2" s="286"/>
-      <c r="P2" s="286"/>
-      <c r="Q2" s="287" t="s">
+      <c r="D2" s="278"/>
+      <c r="E2" s="278"/>
+      <c r="F2" s="278"/>
+      <c r="G2" s="278"/>
+      <c r="H2" s="278"/>
+      <c r="I2" s="278"/>
+      <c r="J2" s="278"/>
+      <c r="K2" s="278"/>
+      <c r="L2" s="278"/>
+      <c r="M2" s="278"/>
+      <c r="N2" s="278"/>
+      <c r="O2" s="278"/>
+      <c r="P2" s="278"/>
+      <c r="Q2" s="279" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="285"/>
-      <c r="S2" s="285"/>
-      <c r="T2" s="285"/>
-      <c r="U2" s="285"/>
-      <c r="V2" s="285"/>
-      <c r="W2" s="285"/>
-      <c r="X2" s="285"/>
-      <c r="Y2" s="285"/>
-      <c r="Z2" s="285"/>
-      <c r="AA2" s="285"/>
-      <c r="AB2" s="285"/>
-      <c r="AC2" s="285"/>
-      <c r="AD2" s="285"/>
-      <c r="AE2" s="285"/>
-      <c r="AF2" s="285"/>
-      <c r="AG2" s="285"/>
-      <c r="AH2" s="285"/>
-      <c r="AI2" s="285"/>
-      <c r="AJ2" s="285"/>
+      <c r="R2" s="277"/>
+      <c r="S2" s="277"/>
+      <c r="T2" s="277"/>
+      <c r="U2" s="277"/>
+      <c r="V2" s="277"/>
+      <c r="W2" s="277"/>
+      <c r="X2" s="277"/>
+      <c r="Y2" s="277"/>
+      <c r="Z2" s="277"/>
+      <c r="AA2" s="277"/>
+      <c r="AB2" s="277"/>
+      <c r="AC2" s="277"/>
+      <c r="AD2" s="277"/>
+      <c r="AE2" s="277"/>
+      <c r="AF2" s="277"/>
+      <c r="AG2" s="277"/>
+      <c r="AH2" s="277"/>
+      <c r="AI2" s="277"/>
+      <c r="AJ2" s="277"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A3" s="41"/>
-      <c r="C3" s="286" t="s">
+      <c r="C3" s="278" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="286"/>
-      <c r="E3" s="286"/>
-      <c r="F3" s="286"/>
-      <c r="G3" s="286"/>
-      <c r="H3" s="286"/>
-      <c r="I3" s="286"/>
-      <c r="J3" s="286"/>
-      <c r="K3" s="286"/>
-      <c r="L3" s="286"/>
-      <c r="M3" s="286"/>
-      <c r="N3" s="286"/>
-      <c r="O3" s="286"/>
-      <c r="P3" s="286"/>
-      <c r="Q3" s="287" t="s">
+      <c r="D3" s="278"/>
+      <c r="E3" s="278"/>
+      <c r="F3" s="278"/>
+      <c r="G3" s="278"/>
+      <c r="H3" s="278"/>
+      <c r="I3" s="278"/>
+      <c r="J3" s="278"/>
+      <c r="K3" s="278"/>
+      <c r="L3" s="278"/>
+      <c r="M3" s="278"/>
+      <c r="N3" s="278"/>
+      <c r="O3" s="278"/>
+      <c r="P3" s="278"/>
+      <c r="Q3" s="279" t="s">
         <v>87</v>
       </c>
-      <c r="R3" s="285"/>
-      <c r="S3" s="285"/>
-      <c r="T3" s="285"/>
-      <c r="U3" s="285"/>
-      <c r="V3" s="285"/>
-      <c r="W3" s="285"/>
-      <c r="X3" s="285"/>
-      <c r="Y3" s="285"/>
-      <c r="Z3" s="285"/>
-      <c r="AA3" s="285"/>
-      <c r="AB3" s="285"/>
-      <c r="AC3" s="285"/>
-      <c r="AD3" s="285"/>
-      <c r="AE3" s="285"/>
-      <c r="AF3" s="285"/>
-      <c r="AG3" s="285"/>
-      <c r="AH3" s="285"/>
-      <c r="AI3" s="285"/>
-      <c r="AJ3" s="285"/>
+      <c r="R3" s="277"/>
+      <c r="S3" s="277"/>
+      <c r="T3" s="277"/>
+      <c r="U3" s="277"/>
+      <c r="V3" s="277"/>
+      <c r="W3" s="277"/>
+      <c r="X3" s="277"/>
+      <c r="Y3" s="277"/>
+      <c r="Z3" s="277"/>
+      <c r="AA3" s="277"/>
+      <c r="AB3" s="277"/>
+      <c r="AC3" s="277"/>
+      <c r="AD3" s="277"/>
+      <c r="AE3" s="277"/>
+      <c r="AF3" s="277"/>
+      <c r="AG3" s="277"/>
+      <c r="AH3" s="277"/>
+      <c r="AI3" s="277"/>
+      <c r="AJ3" s="277"/>
     </row>
     <row r="4" spans="1:38" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="284"/>
-      <c r="D4" s="284"/>
-      <c r="E4" s="284"/>
-      <c r="F4" s="284"/>
-      <c r="G4" s="284"/>
-      <c r="H4" s="284"/>
-      <c r="I4" s="284"/>
-      <c r="J4" s="284"/>
-      <c r="K4" s="284"/>
-      <c r="L4" s="284"/>
-      <c r="M4" s="284"/>
-      <c r="N4" s="284"/>
-      <c r="O4" s="284"/>
-      <c r="P4" s="285"/>
-      <c r="Q4" s="285"/>
-      <c r="R4" s="285"/>
-      <c r="S4" s="285"/>
-      <c r="T4" s="285"/>
-      <c r="U4" s="285"/>
-      <c r="V4" s="285"/>
-      <c r="W4" s="285"/>
-      <c r="X4" s="285"/>
-      <c r="Y4" s="285"/>
-      <c r="Z4" s="285"/>
-      <c r="AA4" s="285"/>
-      <c r="AB4" s="285"/>
-      <c r="AC4" s="285"/>
-      <c r="AD4" s="285"/>
-      <c r="AE4" s="285"/>
-      <c r="AF4" s="285"/>
-      <c r="AG4" s="285"/>
-      <c r="AH4" s="285"/>
-      <c r="AI4" s="285"/>
-      <c r="AJ4" s="285"/>
+      <c r="C4" s="276"/>
+      <c r="D4" s="276"/>
+      <c r="E4" s="276"/>
+      <c r="F4" s="276"/>
+      <c r="G4" s="276"/>
+      <c r="H4" s="276"/>
+      <c r="I4" s="276"/>
+      <c r="J4" s="276"/>
+      <c r="K4" s="276"/>
+      <c r="L4" s="276"/>
+      <c r="M4" s="276"/>
+      <c r="N4" s="276"/>
+      <c r="O4" s="276"/>
+      <c r="P4" s="277"/>
+      <c r="Q4" s="277"/>
+      <c r="R4" s="277"/>
+      <c r="S4" s="277"/>
+      <c r="T4" s="277"/>
+      <c r="U4" s="277"/>
+      <c r="V4" s="277"/>
+      <c r="W4" s="277"/>
+      <c r="X4" s="277"/>
+      <c r="Y4" s="277"/>
+      <c r="Z4" s="277"/>
+      <c r="AA4" s="277"/>
+      <c r="AB4" s="277"/>
+      <c r="AC4" s="277"/>
+      <c r="AD4" s="277"/>
+      <c r="AE4" s="277"/>
+      <c r="AF4" s="277"/>
+      <c r="AG4" s="277"/>
+      <c r="AH4" s="277"/>
+      <c r="AI4" s="277"/>
+      <c r="AJ4" s="277"/>
     </row>
     <row r="5" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="307" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="308"/>
-      <c r="E5" s="308"/>
-      <c r="F5" s="308"/>
-      <c r="G5" s="308"/>
-      <c r="H5" s="308"/>
-      <c r="I5" s="308"/>
-      <c r="J5" s="308"/>
-      <c r="K5" s="308"/>
-      <c r="L5" s="308"/>
-      <c r="M5" s="308"/>
-      <c r="N5" s="308"/>
-      <c r="O5" s="308"/>
-      <c r="P5" s="308"/>
-      <c r="Q5" s="308"/>
-      <c r="R5" s="308"/>
-      <c r="S5" s="309"/>
-      <c r="T5" s="307" t="s">
+      <c r="C5" s="263" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="264"/>
+      <c r="E5" s="264"/>
+      <c r="F5" s="264"/>
+      <c r="G5" s="264"/>
+      <c r="H5" s="264"/>
+      <c r="I5" s="264"/>
+      <c r="J5" s="264"/>
+      <c r="K5" s="264"/>
+      <c r="L5" s="264"/>
+      <c r="M5" s="264"/>
+      <c r="N5" s="264"/>
+      <c r="O5" s="264"/>
+      <c r="P5" s="264"/>
+      <c r="Q5" s="264"/>
+      <c r="R5" s="264"/>
+      <c r="S5" s="265"/>
+      <c r="T5" s="263" t="s">
         <v>1</v>
       </c>
-      <c r="U5" s="308"/>
-      <c r="V5" s="308"/>
-      <c r="W5" s="308"/>
-      <c r="X5" s="308"/>
-      <c r="Y5" s="308"/>
-      <c r="Z5" s="308"/>
-      <c r="AA5" s="308"/>
-      <c r="AB5" s="309"/>
-      <c r="AC5" s="307" t="s">
+      <c r="U5" s="264"/>
+      <c r="V5" s="264"/>
+      <c r="W5" s="264"/>
+      <c r="X5" s="264"/>
+      <c r="Y5" s="264"/>
+      <c r="Z5" s="264"/>
+      <c r="AA5" s="264"/>
+      <c r="AB5" s="265"/>
+      <c r="AC5" s="263" t="s">
         <v>2</v>
       </c>
-      <c r="AD5" s="308"/>
-      <c r="AE5" s="308"/>
-      <c r="AF5" s="308"/>
-      <c r="AG5" s="312"/>
-      <c r="AH5" s="307" t="s">
+      <c r="AD5" s="264"/>
+      <c r="AE5" s="264"/>
+      <c r="AF5" s="264"/>
+      <c r="AG5" s="266"/>
+      <c r="AH5" s="263" t="s">
         <v>10</v>
       </c>
-      <c r="AI5" s="308"/>
-      <c r="AJ5" s="309"/>
+      <c r="AI5" s="264"/>
+      <c r="AJ5" s="265"/>
     </row>
     <row r="6" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="32"/>
       <c r="B6" s="4"/>
-      <c r="C6" s="280" t="s">
+      <c r="C6" s="267" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="275"/>
-      <c r="E6" s="275"/>
-      <c r="F6" s="275"/>
-      <c r="G6" s="275"/>
-      <c r="H6" s="275"/>
-      <c r="I6" s="275"/>
-      <c r="J6" s="276"/>
+      <c r="D6" s="268"/>
+      <c r="E6" s="268"/>
+      <c r="F6" s="268"/>
+      <c r="G6" s="268"/>
+      <c r="H6" s="268"/>
+      <c r="I6" s="268"/>
+      <c r="J6" s="269"/>
       <c r="K6" s="274" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="275"/>
-      <c r="M6" s="275"/>
-      <c r="N6" s="275"/>
-      <c r="O6" s="275"/>
-      <c r="P6" s="275"/>
-      <c r="Q6" s="275"/>
-      <c r="R6" s="276"/>
-      <c r="S6" s="277" t="s">
+      <c r="L6" s="268"/>
+      <c r="M6" s="268"/>
+      <c r="N6" s="268"/>
+      <c r="O6" s="268"/>
+      <c r="P6" s="268"/>
+      <c r="Q6" s="268"/>
+      <c r="R6" s="269"/>
+      <c r="S6" s="270" t="s">
         <v>12</v>
       </c>
-      <c r="T6" s="280" t="s">
+      <c r="T6" s="267" t="s">
         <v>9</v>
       </c>
-      <c r="U6" s="275"/>
-      <c r="V6" s="275"/>
-      <c r="W6" s="276"/>
+      <c r="U6" s="268"/>
+      <c r="V6" s="268"/>
+      <c r="W6" s="269"/>
       <c r="X6" s="274" t="s">
         <v>8</v>
       </c>
-      <c r="Y6" s="275"/>
-      <c r="Z6" s="275"/>
-      <c r="AA6" s="276"/>
-      <c r="AB6" s="277" t="s">
+      <c r="Y6" s="268"/>
+      <c r="Z6" s="268"/>
+      <c r="AA6" s="269"/>
+      <c r="AB6" s="270" t="s">
         <v>13</v>
       </c>
-      <c r="AC6" s="311" t="s">
+      <c r="AC6" s="275" t="s">
         <v>9</v>
       </c>
-      <c r="AD6" s="276"/>
+      <c r="AD6" s="269"/>
       <c r="AE6" s="274" t="s">
         <v>8</v>
       </c>
-      <c r="AF6" s="276"/>
-      <c r="AG6" s="277" t="s">
+      <c r="AF6" s="269"/>
+      <c r="AG6" s="270" t="s">
         <v>14</v>
       </c>
       <c r="AH6" s="56"/>
       <c r="AI6" s="25"/>
-      <c r="AJ6" s="277" t="s">
+      <c r="AJ6" s="270" t="s">
         <v>15</v>
       </c>
       <c r="AK6" s="4"/>
@@ -4081,8 +4081,8 @@
         <f>Résultats!$J$28</f>
         <v>3</v>
       </c>
-      <c r="S7" s="278"/>
-      <c r="T7" s="313">
+      <c r="S7" s="271"/>
+      <c r="T7" s="259">
         <f>Résultats!$V$6</f>
         <v>4</v>
       </c>
@@ -4106,15 +4106,15 @@
         <f>Résultats!$V$21</f>
         <v>3</v>
       </c>
-      <c r="Z7" s="106">
+      <c r="Z7" s="206">
         <f>Résultats!$V$24</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AA7" s="103">
         <f>Résultats!$V$25</f>
         <v>3</v>
       </c>
-      <c r="AB7" s="278"/>
+      <c r="AB7" s="271"/>
       <c r="AC7" s="106">
         <f>Résultats!$AH$8</f>
         <v>0</v>
@@ -4131,7 +4131,7 @@
         <f>Résultats!$AH$23</f>
         <v>0</v>
       </c>
-      <c r="AG7" s="278"/>
+      <c r="AG7" s="271"/>
       <c r="AH7" s="173">
         <f>Résultats!$AH$15</f>
         <v>0</v>
@@ -4140,7 +4140,7 @@
         <f>Résultats!$AH$16</f>
         <v>0</v>
       </c>
-      <c r="AJ7" s="278"/>
+      <c r="AJ7" s="271"/>
       <c r="AK7" s="37"/>
     </row>
     <row r="8" spans="1:38" s="39" customFormat="1" ht="58.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -4166,24 +4166,24 @@
       <c r="P8" s="203"/>
       <c r="Q8" s="207"/>
       <c r="R8" s="112"/>
-      <c r="S8" s="278"/>
-      <c r="T8" s="314"/>
+      <c r="S8" s="271"/>
+      <c r="T8" s="260"/>
       <c r="U8" s="112"/>
       <c r="V8" s="160"/>
       <c r="W8" s="199"/>
       <c r="X8" s="115"/>
       <c r="Y8" s="113"/>
-      <c r="Z8" s="114"/>
+      <c r="Z8" s="207"/>
       <c r="AA8" s="112"/>
-      <c r="AB8" s="278"/>
+      <c r="AB8" s="271"/>
       <c r="AC8" s="114"/>
       <c r="AD8" s="112"/>
       <c r="AE8" s="115"/>
       <c r="AF8" s="112"/>
-      <c r="AG8" s="278"/>
+      <c r="AG8" s="271"/>
       <c r="AH8" s="173"/>
       <c r="AI8" s="107"/>
-      <c r="AJ8" s="278"/>
+      <c r="AJ8" s="271"/>
       <c r="AK8" s="37"/>
     </row>
     <row r="9" spans="1:38" s="39" customFormat="1" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4253,8 +4253,8 @@
         <f>Résultats!$B$28</f>
         <v>VEGAS</v>
       </c>
-      <c r="S9" s="278"/>
-      <c r="T9" s="315" t="str">
+      <c r="S9" s="271"/>
+      <c r="T9" s="261" t="str">
         <f>Résultats!$N$6</f>
         <v>BOSTON</v>
       </c>
@@ -4278,7 +4278,7 @@
         <f>Résultats!$N$21</f>
         <v>COLORADO</v>
       </c>
-      <c r="Z9" s="164" t="str">
+      <c r="Z9" s="208" t="str">
         <f>Résultats!$N$24</f>
         <v>ST-LOUIS</v>
       </c>
@@ -4286,7 +4286,7 @@
         <f>Résultats!$N$25</f>
         <v>DALLAS</v>
       </c>
-      <c r="AB9" s="278"/>
+      <c r="AB9" s="271"/>
       <c r="AC9" s="164" t="str">
         <f>Résultats!$Z$8</f>
         <v xml:space="preserve"> </v>
@@ -4303,7 +4303,7 @@
         <f>Résultats!$Z$23</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AG9" s="278"/>
+      <c r="AG9" s="271"/>
       <c r="AH9" s="174" t="str">
         <f>Résultats!$Z$15</f>
         <v xml:space="preserve"> </v>
@@ -4312,7 +4312,7 @@
         <f>Résultats!$Z$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ9" s="278"/>
+      <c r="AJ9" s="271"/>
       <c r="AK9" s="37"/>
     </row>
     <row r="10" spans="1:38" s="39" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4386,8 +4386,8 @@
         <f>Résultats!$A$28</f>
         <v>P3</v>
       </c>
-      <c r="S10" s="279"/>
-      <c r="T10" s="316" t="str">
+      <c r="S10" s="273"/>
+      <c r="T10" s="262" t="str">
         <f>Résultats!$M$6</f>
         <v>A2</v>
       </c>
@@ -4411,7 +4411,7 @@
         <f>Résultats!$M$21</f>
         <v>WC2</v>
       </c>
-      <c r="Z10" s="170" t="str">
+      <c r="Z10" s="209" t="str">
         <f>Résultats!$M$24</f>
         <v>C3</v>
       </c>
@@ -4419,7 +4419,7 @@
         <f>Résultats!$M$25</f>
         <v>WC1</v>
       </c>
-      <c r="AB10" s="310"/>
+      <c r="AB10" s="272"/>
       <c r="AC10" s="170" t="str">
         <f>Résultats!$Y$8</f>
         <v xml:space="preserve"> </v>
@@ -4436,7 +4436,7 @@
         <f>Résultats!$Y$23</f>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="AG10" s="310"/>
+      <c r="AG10" s="272"/>
       <c r="AH10" s="176" t="str">
         <f>Résultats!$Y$15</f>
         <v xml:space="preserve"> </v>
@@ -4445,7 +4445,7 @@
         <f>Résultats!$Y$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ10" s="279"/>
+      <c r="AJ10" s="273"/>
       <c r="AK10" s="109" t="s">
         <v>51</v>
       </c>
@@ -5011,7 +5011,7 @@
       <c r="AA15" s="50"/>
       <c r="AB15" s="122">
         <f>SUM(T16:AA16)</f>
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="AC15" s="48"/>
       <c r="AD15" s="47"/>
@@ -5029,11 +5029,11 @@
       </c>
       <c r="AK15" s="111">
         <f>MAX($AL$11:$AL$98) - AL15</f>
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="AL15" s="122">
         <f>$S15+$AB15+$AG15+$AJ15</f>
-        <v>57</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5100,7 +5100,7 @@
       <c r="Y16" s="59"/>
       <c r="Z16" s="126">
         <f>(IF($Z15&lt;&gt;"",($Z$7*$P$105)+IF($Z$7=4,($P$103)+IF($Z15=$Z$7+$AA$7,$P$104,0),0),0)+IF($AA15&lt;&gt;"",($AA$7*$P$105)+IF($AA$7=4,($P$103)+IF($AA15=$Z$7+$AA$7,$P$104,0),0),0))</f>
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="AA16" s="62"/>
       <c r="AB16" s="144"/>
@@ -5260,7 +5260,7 @@
         <f>IF(ISBLANK(Z15),
 0,
 IF(Z$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA17" s="118">
         <f>IF(ISBLANK(AA15),
@@ -5279,7 +5279,7 @@
       <c r="AJ17" s="138"/>
       <c r="AK17" s="139">
         <f>SUM(C17:AI17)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AL17" s="123"/>
     </row>
@@ -5510,7 +5510,7 @@
       <c r="AA19" s="237"/>
       <c r="AB19" s="239">
         <f>SUM(T20:AA20)</f>
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="AC19" s="232"/>
       <c r="AD19" s="233"/>
@@ -5528,11 +5528,11 @@
       </c>
       <c r="AK19" s="241">
         <f>MAX($AL$11:$AL$98) - AL19</f>
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="AL19" s="239">
         <f>$S19+$AB19+$AG19+$AJ19</f>
-        <v>54</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5599,7 +5599,7 @@
       <c r="Y20" s="59"/>
       <c r="Z20" s="126">
         <f>(IF($Z19&lt;&gt;"",($Z$7*$P$105)+IF($Z$7=4,($P$103)+IF($Z19=$Z$7+$AA$7,$P$104,0),0),0)+IF($AA19&lt;&gt;"",($AA$7*$P$105)+IF($AA$7=4,($P$103)+IF($AA19=$Z$7+$AA$7,$P$104,0),0),0))</f>
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="AA20" s="62"/>
       <c r="AB20" s="144"/>
@@ -5759,7 +5759,7 @@
         <f>IF(ISBLANK(Z19),
 0,
 IF(Z$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA21" s="118">
         <f>IF(ISBLANK(AA19),
@@ -5778,7 +5778,7 @@
       <c r="AJ21" s="138"/>
       <c r="AK21" s="139">
         <f>SUM(C21:AI21)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AL21" s="123"/>
     </row>
@@ -6009,7 +6009,7 @@
       <c r="AA23" s="50"/>
       <c r="AB23" s="122">
         <f>SUM(T24:AA24)</f>
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="AC23" s="48"/>
       <c r="AD23" s="47"/>
@@ -6027,11 +6027,11 @@
       </c>
       <c r="AK23" s="111">
         <f>MAX($AL$11:$AL$98) - AL23</f>
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="AL23" s="122">
         <f>$S23+$AB23+$AG23+$AJ23</f>
-        <v>53</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6098,7 +6098,7 @@
       <c r="Y24" s="59"/>
       <c r="Z24" s="126">
         <f>(IF($Z23&lt;&gt;"",($Z$7*$P$105)+IF($Z$7=4,($P$103)+IF($Z23=$Z$7+$AA$7,$P$104,0),0),0)+IF($AA23&lt;&gt;"",($AA$7*$P$105)+IF($AA$7=4,($P$103)+IF($AA23=$Z$7+$AA$7,$P$104,0),0),0))</f>
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="AA24" s="62"/>
       <c r="AB24" s="144"/>
@@ -6258,7 +6258,7 @@
         <f>IF(ISBLANK(Z23),
 0,
 IF(Z$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA25" s="118">
         <f>IF(ISBLANK(AA23),
@@ -6277,7 +6277,7 @@
       <c r="AJ25" s="138"/>
       <c r="AK25" s="139">
         <f>SUM(C25:AI25)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AL25" s="123"/>
     </row>
@@ -6508,7 +6508,7 @@
       <c r="AA27" s="237"/>
       <c r="AB27" s="239">
         <f>SUM(T28:AA28)</f>
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="AC27" s="232"/>
       <c r="AD27" s="233"/>
@@ -6526,11 +6526,11 @@
       </c>
       <c r="AK27" s="241">
         <f>MAX($AL$11:$AL$98) - AL27</f>
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="AL27" s="239">
         <f>$S27+$AB27+$AG27+$AJ27</f>
-        <v>52</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6597,7 +6597,7 @@
       <c r="Y28" s="59"/>
       <c r="Z28" s="126">
         <f>(IF($Z27&lt;&gt;"",($Z$7*$P$105)+IF($Z$7=4,($P$103)+IF($Z27=$Z$7+$AA$7,$P$104,0),0),0)+IF($AA27&lt;&gt;"",($AA$7*$P$105)+IF($AA$7=4,($P$103)+IF($AA27=$Z$7+$AA$7,$P$104,0),0),0))</f>
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="AA28" s="62"/>
       <c r="AB28" s="155"/>
@@ -6757,7 +6757,7 @@
         <f>IF(ISBLANK(Z27),
 0,
 IF(Z$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA29" s="118">
         <f>IF(ISBLANK(AA27),
@@ -6776,7 +6776,7 @@
       <c r="AJ29" s="138"/>
       <c r="AK29" s="139">
         <f>SUM(C29:AI29)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AL29" s="123"/>
     </row>
@@ -6951,43 +6951,43 @@
         <v>6</v>
       </c>
       <c r="B31" s="84" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C31" s="46">
         <v>5</v>
       </c>
       <c r="D31" s="45"/>
-      <c r="E31" s="44">
+      <c r="E31" s="210">
+        <v>7</v>
+      </c>
+      <c r="F31" s="45"/>
+      <c r="G31" s="48">
+        <v>5</v>
+      </c>
+      <c r="H31" s="47"/>
+      <c r="I31" s="44">
         <v>6</v>
       </c>
-      <c r="F31" s="45"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="215">
-        <v>7</v>
-      </c>
-      <c r="I31" s="44"/>
-      <c r="J31" s="47">
-        <v>6</v>
-      </c>
+      <c r="J31" s="47"/>
       <c r="K31" s="49">
         <v>5</v>
       </c>
       <c r="L31" s="47"/>
-      <c r="M31" s="44"/>
-      <c r="N31" s="211">
+      <c r="M31" s="44">
         <v>6</v>
       </c>
+      <c r="N31" s="45"/>
       <c r="O31" s="44">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P31" s="45"/>
-      <c r="Q31" s="48">
-        <v>6</v>
+      <c r="Q31" s="213">
+        <v>7</v>
       </c>
       <c r="R31" s="50"/>
       <c r="S31" s="122">
         <f>SUM(C32:R32)</f>
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="T31" s="46"/>
       <c r="U31" s="47">
@@ -6997,17 +6997,17 @@
         <v>6</v>
       </c>
       <c r="W31" s="47"/>
-      <c r="X31" s="49">
-        <v>5</v>
-      </c>
-      <c r="Y31" s="45"/>
-      <c r="Z31" s="48"/>
-      <c r="AA31" s="47">
+      <c r="X31" s="49"/>
+      <c r="Y31" s="45">
+        <v>6</v>
+      </c>
+      <c r="Z31" s="48">
         <v>7</v>
       </c>
+      <c r="AA31" s="47"/>
       <c r="AB31" s="122">
         <f>SUM(T32:AA32)</f>
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="AC31" s="48"/>
       <c r="AD31" s="47"/>
@@ -7025,11 +7025,11 @@
       </c>
       <c r="AK31" s="111">
         <f>MAX($AL$11:$AL$98) - AL31</f>
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="AL31" s="122">
         <f>$S31+$AB31+$AG31+$AJ31</f>
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7045,17 +7045,17 @@
       <c r="D32" s="76"/>
       <c r="E32" s="77">
         <f>(IF($E31&lt;&gt;"",($E$7*$O$105)+IF($E$7=4,($O$103)+IF($E31=$E$7+$F$7,$O$104,0),0),0)+IF($F31&lt;&gt;"",($F$7*$O$105)+IF($F$7=4,($O$103)+IF($F31=$E$7+$F$7,$O$104,0),0),0))</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F32" s="76"/>
       <c r="G32" s="77">
         <f>(IF($G31&lt;&gt;"",($G$7*$O$105)+IF($G$7=4,($O$103)+IF($G31=$G$7+$H$7,$O$104,0),0),0)+IF($H31&lt;&gt;"",($H$7*$O$105)+IF($H$7=4,($O$103)+IF($H31=$G$7+$H$7,$O$104,0),0),0))</f>
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="H32" s="76"/>
       <c r="I32" s="77">
         <f>(IF($I31&lt;&gt;"",($I$7*$O$105)+IF($I$7=4,($O$103)+IF($I31=$I$7+$J$7,$O$104,0),0),0)+IF($J31&lt;&gt;"",($J$7*$O$105)+IF($J$7=4,($O$103)+IF($J31=$I$7+$J$7,$O$104,0),0),0))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J32" s="78"/>
       <c r="K32" s="79">
@@ -7065,7 +7065,7 @@
       <c r="L32" s="76"/>
       <c r="M32" s="77">
         <f>(IF($M31&lt;&gt;"",($M$7*$O$105)+IF($M$7=4,($O$103)+IF($M31=$M$7+$N$7,$O$104,0),0),0)+IF($N31&lt;&gt;"",($N$7*$O$105)+IF($N$7=4,($O$103)+IF($N31=$M$7+$N$7,$O$104,0),0),0))</f>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="N32" s="76"/>
       <c r="O32" s="77">
@@ -7075,7 +7075,7 @@
       <c r="P32" s="76"/>
       <c r="Q32" s="77">
         <f>(IF($Q31&lt;&gt;"",($Q$7*$O$105)+IF($Q$7=4,($O$103)+IF($Q31=$Q$7+$R$7,$O$104,0),0),0)+IF($R31&lt;&gt;"",($R$7*$O$105)+IF($R$7=4,($O$103)+IF($R31=$Q$7+$R$7,$O$104,0),0),0))</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="R32" s="80"/>
       <c r="S32" s="121"/>
@@ -7096,7 +7096,7 @@
       <c r="Y32" s="59"/>
       <c r="Z32" s="126">
         <f>(IF($Z31&lt;&gt;"",($Z$7*$P$105)+IF($Z$7=4,($P$103)+IF($Z31=$Z$7+$AA$7,$P$104,0),0),0)+IF($AA31&lt;&gt;"",($AA$7*$P$105)+IF($AA$7=4,($P$103)+IF($AA31=$Z$7+$AA$7,$P$104,0),0),0))</f>
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="AA32" s="62"/>
       <c r="AB32" s="121"/>
@@ -7153,13 +7153,13 @@
         <f>IF(ISBLANK(H31),
 0,
 IF(H$7 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I33" s="118">
         <f>IF(ISBLANK(I31),
 0,
 IF(I$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J33" s="118">
         <f>IF(ISBLANK(J31),
@@ -7189,7 +7189,7 @@
         <f>IF(ISBLANK(N31),
 0,
 IF(N$7 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O33" s="118">
         <f>IF(ISBLANK(O31),
@@ -7256,7 +7256,7 @@
         <f>IF(ISBLANK(Z31),
 0,
 IF(Z$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA33" s="118">
         <f>IF(ISBLANK(AA31),
@@ -7300,7 +7300,7 @@
         <f>IF(E33 = 0,
 0,
 IF(E31 = (E$7+F$7),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34" s="118">
         <f>IF(F33 = 0,
@@ -7318,7 +7318,7 @@
         <f>IF(H33 = 0,
 0,
 IF(H31 = (G$7+H$7),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I34" s="118">
         <f>IF(I33 = 0,
@@ -7354,7 +7354,7 @@
         <f>IF(N33 = 0,
 0,
 IF(N31 = (M$7+N$7),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O34" s="118">
         <f>IF(O33 = 0,
@@ -7372,7 +7372,7 @@
         <f>IF(Q33 = 0,
 0,
 IF(Q31 = (Q$7+R$7),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R34" s="118">
         <f>IF(R33 = 0,
@@ -7421,7 +7421,7 @@
         <f>IF(Z33 = 0,
 0,
 IF(Z31 = (Z$7+AA$7),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA34" s="118">
         <f>IF(AA33 = 0,
@@ -7440,7 +7440,7 @@
       <c r="AJ34" s="138"/>
       <c r="AK34" s="139">
         <f>SUM(C34:AI34)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL34" s="123"/>
     </row>
@@ -7450,7 +7450,7 @@
         <v>7</v>
       </c>
       <c r="B35" s="217" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C35" s="229">
         <v>5</v>
@@ -7461,7 +7461,7 @@
       </c>
       <c r="F35" s="230"/>
       <c r="G35" s="232">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H35" s="233"/>
       <c r="I35" s="234">
@@ -7469,36 +7469,36 @@
       </c>
       <c r="J35" s="233"/>
       <c r="K35" s="235">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L35" s="233"/>
       <c r="M35" s="234">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N35" s="230"/>
-      <c r="O35" s="234">
-        <v>5</v>
-      </c>
-      <c r="P35" s="230"/>
-      <c r="Q35" s="249">
+      <c r="O35" s="234"/>
+      <c r="P35" s="230">
         <v>7</v>
       </c>
-      <c r="R35" s="237"/>
+      <c r="Q35" s="232"/>
+      <c r="R35" s="237">
+        <v>7</v>
+      </c>
       <c r="S35" s="239">
         <f>SUM(C36:R36)</f>
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T35" s="229"/>
       <c r="U35" s="233">
         <v>6</v>
       </c>
       <c r="V35" s="234">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="W35" s="233"/>
       <c r="X35" s="235"/>
       <c r="Y35" s="230">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Z35" s="232">
         <v>7</v>
@@ -7506,10 +7506,10 @@
       <c r="AA35" s="233"/>
       <c r="AB35" s="239">
         <f>SUM(T36:AA36)</f>
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="AC35" s="232"/>
-      <c r="AD35" s="233"/>
+      <c r="AD35" s="242"/>
       <c r="AE35" s="235"/>
       <c r="AF35" s="233"/>
       <c r="AG35" s="239">
@@ -7524,11 +7524,11 @@
       </c>
       <c r="AK35" s="241">
         <f>MAX($AL$11:$AL$98) - AL35</f>
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="AL35" s="239">
         <f>$S35+$AB35+$AG35+$AJ35</f>
-        <v>47</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7569,12 +7569,12 @@
       <c r="N36" s="76"/>
       <c r="O36" s="77">
         <f>(IF($O35&lt;&gt;"",($O$7*$O$105)+IF($O$7=4,($O$103)+IF($O35=$O$7+$P$7,$O$104,0),0),0)+IF($P35&lt;&gt;"",($P$7*$O$105)+IF($P$7=4,($O$103)+IF($P35=$O$7+$P$7,$O$104,0),0),0))</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="P36" s="76"/>
       <c r="Q36" s="77">
         <f>(IF($Q35&lt;&gt;"",($Q$7*$O$105)+IF($Q$7=4,($O$103)+IF($Q35=$Q$7+$R$7,$O$104,0),0),0)+IF($R35&lt;&gt;"",($R$7*$O$105)+IF($R$7=4,($O$103)+IF($R35=$Q$7+$R$7,$O$104,0),0),0))</f>
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="R36" s="80"/>
       <c r="S36" s="121"/>
@@ -7595,7 +7595,7 @@
       <c r="Y36" s="59"/>
       <c r="Z36" s="126">
         <f>(IF($Z35&lt;&gt;"",($Z$7*$P$105)+IF($Z$7=4,($P$103)+IF($Z35=$Z$7+$AA$7,$P$104,0),0),0)+IF($AA35&lt;&gt;"",($AA$7*$P$105)+IF($AA$7=4,($P$103)+IF($AA35=$Z$7+$AA$7,$P$104,0),0),0))</f>
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="AA36" s="62"/>
       <c r="AB36" s="121"/>
@@ -7700,13 +7700,13 @@
         <f>IF(ISBLANK(P35),
 0,
 IF(P$7 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q37" s="118">
         <f>IF(ISBLANK(Q35),
 0,
 IF(Q$7= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R37" s="118">
         <f>IF(ISBLANK(R35),
@@ -7755,7 +7755,7 @@
         <f>IF(ISBLANK(Z35),
 0,
 IF(Z$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA37" s="118">
         <f>IF(ISBLANK(AA35),
@@ -7774,7 +7774,7 @@
       <c r="AJ37" s="138"/>
       <c r="AK37" s="139">
         <f>SUM(C37:AI37)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AL37" s="123"/>
     </row>
@@ -7871,7 +7871,7 @@
         <f>IF(Q37 = 0,
 0,
 IF(Q35 = (Q$7+R$7),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R38" s="118">
         <f>IF(R37 = 0,
@@ -7920,7 +7920,7 @@
         <f>IF(Z37 = 0,
 0,
 IF(Z35 = (Z$7+AA$7),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA38" s="118">
         <f>IF(AA37 = 0,
@@ -7949,10 +7949,10 @@
         <v>8</v>
       </c>
       <c r="B39" s="84" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C39" s="46">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D39" s="45"/>
       <c r="E39" s="210">
@@ -7963,52 +7963,52 @@
         <v>6</v>
       </c>
       <c r="H39" s="47"/>
-      <c r="I39" s="44">
-        <v>6</v>
-      </c>
-      <c r="J39" s="47"/>
+      <c r="I39" s="44"/>
+      <c r="J39" s="47">
+        <v>7</v>
+      </c>
       <c r="K39" s="49">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="L39" s="47"/>
       <c r="M39" s="44">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N39" s="45"/>
-      <c r="O39" s="44"/>
-      <c r="P39" s="45">
-        <v>7</v>
-      </c>
+      <c r="O39" s="44">
+        <v>6</v>
+      </c>
+      <c r="P39" s="45"/>
       <c r="Q39" s="48"/>
       <c r="R39" s="50">
         <v>7</v>
       </c>
       <c r="S39" s="122">
         <f>SUM(C40:R40)</f>
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="T39" s="46"/>
       <c r="U39" s="47">
-        <v>6</v>
-      </c>
-      <c r="V39" s="44">
-        <v>5</v>
-      </c>
-      <c r="W39" s="47"/>
-      <c r="X39" s="49"/>
-      <c r="Y39" s="45">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="V39" s="44"/>
+      <c r="W39" s="47">
+        <v>7</v>
+      </c>
+      <c r="X39" s="49">
+        <v>7</v>
+      </c>
+      <c r="Y39" s="45"/>
       <c r="Z39" s="48">
         <v>7</v>
       </c>
       <c r="AA39" s="47"/>
       <c r="AB39" s="122">
         <f>SUM(T40:AA40)</f>
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="AC39" s="48"/>
-      <c r="AD39" s="259"/>
+      <c r="AD39" s="47"/>
       <c r="AE39" s="49"/>
       <c r="AF39" s="47"/>
       <c r="AG39" s="122">
@@ -8023,11 +8023,11 @@
       </c>
       <c r="AK39" s="111">
         <f>MAX($AL$11:$AL$98) - AL39</f>
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="AL39" s="122">
         <f>$S39+$AB39+$AG39+$AJ39</f>
-        <v>46</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -8053,7 +8053,7 @@
       <c r="H40" s="76"/>
       <c r="I40" s="116">
         <f>(IF($I39&lt;&gt;"",($I$7*$O$105)+IF($I$7=4,($O$103)+IF($I39=$I$7+$J$7,$O$104,0),0),0)+IF($J39&lt;&gt;"",($J$7*$O$105)+IF($J$7=4,($O$103)+IF($J39=$I$7+$J$7,$O$104,0),0),0))</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J40" s="78"/>
       <c r="K40" s="79">
@@ -8068,7 +8068,7 @@
       <c r="N40" s="76"/>
       <c r="O40" s="77">
         <f>(IF($O39&lt;&gt;"",($O$7*$O$105)+IF($O$7=4,($O$103)+IF($O39=$O$7+$P$7,$O$104,0),0),0)+IF($P39&lt;&gt;"",($P$7*$O$105)+IF($P$7=4,($O$103)+IF($P39=$O$7+$P$7,$O$104,0),0),0))</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="P40" s="76"/>
       <c r="Q40" s="77">
@@ -8084,7 +8084,7 @@
       <c r="U40" s="126"/>
       <c r="V40" s="126">
         <f>(IF($V39&lt;&gt;"",($V$7*$P$105)+IF($V$7=4,($P$103)+IF($V39=$V$7+$W$7,$P$104,0),0),0)+IF($W39&lt;&gt;"",($W$7*$P$105)+IF($W$7=4,($P$103)+IF($W39=$V$7+$W$7,$P$104,0),0),0))</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="W40" s="126"/>
       <c r="X40" s="126">
@@ -8094,7 +8094,7 @@
       <c r="Y40" s="59"/>
       <c r="Z40" s="126">
         <f>(IF($Z39&lt;&gt;"",($Z$7*$P$105)+IF($Z$7=4,($P$103)+IF($Z39=$Z$7+$AA$7,$P$104,0),0),0)+IF($AA39&lt;&gt;"",($AA$7*$P$105)+IF($AA$7=4,($P$103)+IF($AA39=$Z$7+$AA$7,$P$104,0),0),0))</f>
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="AA40" s="62"/>
       <c r="AB40" s="121"/>
@@ -8157,7 +8157,7 @@
         <f>IF(ISBLANK(I39),
 0,
 IF(I$7= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J41" s="118">
         <f>IF(ISBLANK(J39),
@@ -8199,7 +8199,7 @@
         <f>IF(ISBLANK(P39),
 0,
 IF(P$7 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q41" s="118">
         <f>IF(ISBLANK(Q39),
@@ -8236,7 +8236,7 @@
         <f>IF(ISBLANK(W39),
 0,
 IF(W$7 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X41" s="118">
         <f>IF(ISBLANK(X39),
@@ -8254,7 +8254,7 @@
         <f>IF(ISBLANK(Z39),
 0,
 IF(Z$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA41" s="118">
         <f>IF(ISBLANK(AA39),
@@ -8419,7 +8419,7 @@
         <f>IF(Z41 = 0,
 0,
 IF(Z39 = (Z$7+AA$7),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA42" s="118">
         <f>IF(AA41 = 0,
@@ -8438,7 +8438,7 @@
       <c r="AJ42" s="138"/>
       <c r="AK42" s="139">
         <f>SUM(C42:AI42)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL42" s="123"/>
     </row>
@@ -8448,14 +8448,14 @@
         <v>9</v>
       </c>
       <c r="B43" s="217" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C43" s="229">
+        <v>5</v>
+      </c>
+      <c r="D43" s="230"/>
+      <c r="E43" s="234">
         <v>6</v>
-      </c>
-      <c r="D43" s="230"/>
-      <c r="E43" s="231">
-        <v>7</v>
       </c>
       <c r="F43" s="230"/>
       <c r="G43" s="232">
@@ -8464,14 +8464,14 @@
       <c r="H43" s="233"/>
       <c r="I43" s="234"/>
       <c r="J43" s="233">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K43" s="235">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L43" s="233"/>
       <c r="M43" s="234">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N43" s="230"/>
       <c r="O43" s="234">
@@ -8484,16 +8484,16 @@
       </c>
       <c r="S43" s="239">
         <f>SUM(C44:R44)</f>
-        <v>22</v>
-      </c>
-      <c r="T43" s="229"/>
-      <c r="U43" s="233">
+        <v>20</v>
+      </c>
+      <c r="T43" s="229">
         <v>7</v>
       </c>
-      <c r="V43" s="234"/>
-      <c r="W43" s="233">
+      <c r="U43" s="233"/>
+      <c r="V43" s="234">
         <v>7</v>
       </c>
+      <c r="W43" s="233"/>
       <c r="X43" s="235">
         <v>7</v>
       </c>
@@ -8504,7 +8504,7 @@
       <c r="AA43" s="233"/>
       <c r="AB43" s="239">
         <f>SUM(T44:AA44)</f>
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="AC43" s="232"/>
       <c r="AD43" s="233"/>
@@ -8522,11 +8522,11 @@
       </c>
       <c r="AK43" s="241">
         <f>MAX($AL$11:$AL$98) - AL43</f>
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="AL43" s="239">
         <f>$S43+$AB43+$AG43+$AJ43</f>
-        <v>44</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -8542,7 +8542,7 @@
       <c r="D44" s="76"/>
       <c r="E44" s="116">
         <f>(IF($E43&lt;&gt;"",($E$7*$O$105)+IF($E$7=4,($O$103)+IF($E43=$E$7+$F$7,$O$104,0),0),0)+IF($F43&lt;&gt;"",($F$7*$O$105)+IF($F$7=4,($O$103)+IF($F43=$E$7+$F$7,$O$104,0),0),0))</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F44" s="76"/>
       <c r="G44" s="77">
@@ -8578,12 +8578,12 @@
       <c r="S44" s="121"/>
       <c r="T44" s="126">
         <f>(IF($T43&lt;&gt;"",($T$7*$P$105)+IF($T$7=4,($P$103)+IF($T43=$T$7+$U$7,$P$104,0),0),0)+IF($U43&lt;&gt;"",($U$7*$P$105)+IF($U$7=4,($P$103)+IF($U43=$T$7+$U$7,$P$104,0),0),0))</f>
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="U44" s="126"/>
       <c r="V44" s="126">
         <f>(IF($V43&lt;&gt;"",($V$7*$P$105)+IF($V$7=4,($P$103)+IF($V43=$V$7+$W$7,$P$104,0),0),0)+IF($W43&lt;&gt;"",($W$7*$P$105)+IF($W$7=4,($P$103)+IF($W43=$V$7+$W$7,$P$104,0),0),0))</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="W44" s="126"/>
       <c r="X44" s="126">
@@ -8593,7 +8593,7 @@
       <c r="Y44" s="59"/>
       <c r="Z44" s="126">
         <f>(IF($Z43&lt;&gt;"",($Z$7*$P$105)+IF($Z$7=4,($P$103)+IF($Z43=$Z$7+$AA$7,$P$104,0),0),0)+IF($AA43&lt;&gt;"",($AA$7*$P$105)+IF($AA$7=4,($P$103)+IF($AA43=$Z$7+$AA$7,$P$104,0),0),0))</f>
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="AA44" s="62"/>
       <c r="AB44" s="121"/>
@@ -8717,7 +8717,7 @@
         <f>IF(ISBLANK(T43),
 0,
 IF(T$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U45" s="118">
         <f>IF(ISBLANK(U43),
@@ -8735,7 +8735,7 @@
         <f>IF(ISBLANK(W43),
 0,
 IF(W$7 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X45" s="118">
         <f>IF(ISBLANK(X43),
@@ -8753,7 +8753,7 @@
         <f>IF(ISBLANK(Z43),
 0,
 IF(Z$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA45" s="118">
         <f>IF(ISBLANK(AA43),
@@ -8772,7 +8772,7 @@
       <c r="AJ45" s="138"/>
       <c r="AK45" s="139">
         <f>SUM(C45:AI45)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL45" s="123"/>
     </row>
@@ -8797,7 +8797,7 @@
         <f>IF(E45 = 0,
 0,
 IF(E43 = (E$7+F$7),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F46" s="118">
         <f>IF(F45 = 0,
@@ -8918,7 +8918,7 @@
         <f>IF(Z45 = 0,
 0,
 IF(Z43 = (Z$7+AA$7),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA46" s="118">
         <f>IF(AA45 = 0,
@@ -9003,7 +9003,7 @@
       <c r="AA47" s="47"/>
       <c r="AB47" s="122">
         <f>SUM(T48:AA48)</f>
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="AC47" s="48"/>
       <c r="AD47" s="47"/>
@@ -9021,11 +9021,11 @@
       </c>
       <c r="AK47" s="111">
         <f>MAX($AL$11:$AL$98) - AL47</f>
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="AL47" s="122">
         <f>$S47+$AB47+$AG47+$AJ47</f>
-        <v>43</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -9092,7 +9092,7 @@
       <c r="Y48" s="59"/>
       <c r="Z48" s="126">
         <f>(IF($Z47&lt;&gt;"",($Z$7*$P$105)+IF($Z$7=4,($P$103)+IF($Z47=$Z$7+$AA$7,$P$104,0),0),0)+IF($AA47&lt;&gt;"",($AA$7*$P$105)+IF($AA$7=4,($P$103)+IF($AA47=$Z$7+$AA$7,$P$104,0),0),0))</f>
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="AA48" s="62"/>
       <c r="AB48" s="121"/>
@@ -9252,7 +9252,7 @@
         <f>IF(ISBLANK(Z47),
 0,
 IF(Z$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA49" s="118">
         <f>IF(ISBLANK(AA47),
@@ -9271,7 +9271,7 @@
       <c r="AJ49" s="138"/>
       <c r="AK49" s="139">
         <f>SUM(C49:AI49)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AL49" s="123"/>
     </row>
@@ -9502,7 +9502,7 @@
       <c r="AA51" s="233"/>
       <c r="AB51" s="239">
         <f>SUM(T52:AA52)</f>
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="AC51" s="232"/>
       <c r="AD51" s="242"/>
@@ -9520,11 +9520,11 @@
       </c>
       <c r="AK51" s="241">
         <f>MAX($AL$11:$AL$98) - AL51</f>
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="AL51" s="239">
         <f>$S51+$AB51+$AG51+$AJ51</f>
-        <v>42</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -9591,7 +9591,7 @@
       <c r="Y52" s="59"/>
       <c r="Z52" s="126">
         <f>(IF($Z51&lt;&gt;"",($Z$7*$P$105)+IF($Z$7=4,($P$103)+IF($Z51=$Z$7+$AA$7,$P$104,0),0),0)+IF($AA51&lt;&gt;"",($AA$7*$P$105)+IF($AA$7=4,($P$103)+IF($AA51=$Z$7+$AA$7,$P$104,0),0),0))</f>
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="AA52" s="62"/>
       <c r="AB52" s="121"/>
@@ -9748,7 +9748,7 @@
         <f>IF(ISBLANK(Z51),
 0,
 IF(Z$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA53" s="118">
         <f>IF(ISBLANK(AA51),
@@ -9767,7 +9767,7 @@
       <c r="AJ53" s="138"/>
       <c r="AK53" s="139">
         <f>SUM(C53:AI53)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL53" s="123"/>
     </row>
@@ -9939,37 +9939,37 @@
     <row r="55" spans="1:38" s="27" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="117">
         <f>RANK(AL55,$AL$11:$AL$98,)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B55" s="84" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C55" s="46">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D55" s="45"/>
       <c r="E55" s="44">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F55" s="45"/>
       <c r="G55" s="48">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H55" s="47"/>
       <c r="I55" s="44"/>
       <c r="J55" s="47">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K55" s="49">
         <v>5</v>
       </c>
       <c r="L55" s="47"/>
-      <c r="M55" s="44">
-        <v>7</v>
-      </c>
-      <c r="N55" s="45"/>
+      <c r="M55" s="44"/>
+      <c r="N55" s="211">
+        <v>6</v>
+      </c>
       <c r="O55" s="44">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P55" s="45"/>
       <c r="Q55" s="48"/>
@@ -9978,27 +9978,27 @@
       </c>
       <c r="S55" s="122">
         <f>SUM(C56:R56)</f>
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="T55" s="46"/>
       <c r="U55" s="47">
         <v>6</v>
       </c>
-      <c r="V55" s="44"/>
-      <c r="W55" s="47">
-        <v>6</v>
-      </c>
-      <c r="X55" s="49"/>
-      <c r="Y55" s="45">
+      <c r="V55" s="44">
+        <v>5</v>
+      </c>
+      <c r="W55" s="47"/>
+      <c r="X55" s="49">
         <v>7</v>
       </c>
-      <c r="Z55" s="48"/>
-      <c r="AA55" s="47">
-        <v>6</v>
-      </c>
+      <c r="Y55" s="45"/>
+      <c r="Z55" s="48">
+        <v>7</v>
+      </c>
+      <c r="AA55" s="47"/>
       <c r="AB55" s="122">
         <f>SUM(T56:AA56)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AC55" s="48"/>
       <c r="AD55" s="47"/>
@@ -10008,7 +10008,7 @@
         <f>SUM(AC56:AF56)</f>
         <v>0</v>
       </c>
-      <c r="AH55" s="102"/>
+      <c r="AH55" s="315"/>
       <c r="AI55" s="57"/>
       <c r="AJ55" s="122">
         <f>AH56</f>
@@ -10016,11 +10016,11 @@
       </c>
       <c r="AK55" s="111">
         <f>MAX($AL$11:$AL$98) - AL55</f>
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="AL55" s="122">
         <f>$S55+$AB55+$AG55+$AJ55</f>
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="56" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -10056,7 +10056,7 @@
       <c r="L56" s="127"/>
       <c r="M56" s="125">
         <f>(IF($M55&lt;&gt;"",($M$7*$O$105)+IF($M$7=4,($O$103)+IF($M55=$M$7+$N$7,$O$104,0),0),0)+IF($N55&lt;&gt;"",($N$7*$O$105)+IF($N$7=4,($O$103)+IF($N55=$M$7+$N$7,$O$104,0),0),0))</f>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="N56" s="127"/>
       <c r="O56" s="128">
@@ -10077,7 +10077,7 @@
       <c r="U56" s="126"/>
       <c r="V56" s="126">
         <f>(IF($V55&lt;&gt;"",($V$7*$P$105)+IF($V$7=4,($P$103)+IF($V55=$V$7+$W$7,$P$104,0),0),0)+IF($W55&lt;&gt;"",($W$7*$P$105)+IF($W$7=4,($P$103)+IF($W55=$V$7+$W$7,$P$104,0),0),0))</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="W56" s="126"/>
       <c r="X56" s="126">
@@ -10087,7 +10087,7 @@
       <c r="Y56" s="59"/>
       <c r="Z56" s="126">
         <f>(IF($Z55&lt;&gt;"",($Z$7*$P$105)+IF($Z$7=4,($P$103)+IF($Z55=$Z$7+$AA$7,$P$104,0),0),0)+IF($AA55&lt;&gt;"",($AA$7*$P$105)+IF($AA$7=4,($P$103)+IF($AA55=$Z$7+$AA$7,$P$104,0),0),0))</f>
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="AA56" s="62"/>
       <c r="AB56" s="121"/>
@@ -10177,7 +10177,7 @@
         <f>IF(ISBLANK(N55),
 0,
 IF(N$7 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O57" s="118">
         <f>IF(ISBLANK(O55),
@@ -10226,7 +10226,7 @@
         <f>IF(ISBLANK(W55),
 0,
 IF(W$7 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X57" s="118">
         <f>IF(ISBLANK(X55),
@@ -10244,7 +10244,7 @@
         <f>IF(ISBLANK(Z55),
 0,
 IF(Z$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA57" s="118">
         <f>IF(ISBLANK(AA55),
@@ -10263,7 +10263,7 @@
       <c r="AJ57" s="138"/>
       <c r="AK57" s="139">
         <f>SUM(C57:AI57)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL57" s="123"/>
     </row>
@@ -10342,7 +10342,7 @@
         <f>IF(N57 = 0,
 0,
 IF(N55 = (M$7+N$7),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O58" s="118">
         <f>IF(O57 = 0,
@@ -10409,7 +10409,7 @@
         <f>IF(Z57 = 0,
 0,
 IF(Z55 = (Z$7+AA$7),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA58" s="118">
         <f>IF(AA57 = 0,
@@ -10428,7 +10428,7 @@
       <c r="AJ58" s="138"/>
       <c r="AK58" s="139">
         <f>SUM(C58:AI58)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL58" s="123"/>
     </row>
@@ -10438,7 +10438,7 @@
         <v>13</v>
       </c>
       <c r="B59" s="217" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C59" s="229">
         <v>5</v>
@@ -10448,53 +10448,53 @@
         <v>6</v>
       </c>
       <c r="F59" s="230"/>
-      <c r="G59" s="232">
-        <v>6</v>
-      </c>
-      <c r="H59" s="233"/>
+      <c r="G59" s="232"/>
+      <c r="H59" s="316">
+        <v>7</v>
+      </c>
       <c r="I59" s="234"/>
       <c r="J59" s="233">
         <v>6</v>
       </c>
       <c r="K59" s="235">
+        <v>5</v>
+      </c>
+      <c r="L59" s="233"/>
+      <c r="M59" s="234"/>
+      <c r="N59" s="236">
         <v>6</v>
       </c>
-      <c r="L59" s="233"/>
-      <c r="M59" s="234">
-        <v>7</v>
-      </c>
-      <c r="N59" s="230"/>
       <c r="O59" s="234">
         <v>6</v>
       </c>
       <c r="P59" s="230"/>
-      <c r="Q59" s="232"/>
-      <c r="R59" s="237">
-        <v>7</v>
-      </c>
+      <c r="Q59" s="232">
+        <v>6</v>
+      </c>
+      <c r="R59" s="237"/>
       <c r="S59" s="239">
         <f>SUM(C60:R60)</f>
-        <v>20</v>
-      </c>
-      <c r="T59" s="229">
-        <v>7</v>
-      </c>
-      <c r="U59" s="233"/>
+        <v>43</v>
+      </c>
+      <c r="T59" s="229"/>
+      <c r="U59" s="233">
+        <v>6</v>
+      </c>
       <c r="V59" s="234">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="W59" s="233"/>
       <c r="X59" s="235">
+        <v>5</v>
+      </c>
+      <c r="Y59" s="230"/>
+      <c r="Z59" s="232"/>
+      <c r="AA59" s="233">
         <v>7</v>
       </c>
-      <c r="Y59" s="230"/>
-      <c r="Z59" s="232">
-        <v>7</v>
-      </c>
-      <c r="AA59" s="233"/>
       <c r="AB59" s="239">
         <f>SUM(T60:AA60)</f>
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="AC59" s="232"/>
       <c r="AD59" s="233"/>
@@ -10512,11 +10512,11 @@
       </c>
       <c r="AK59" s="241">
         <f>MAX($AL$11:$AL$98) - AL59</f>
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="AL59" s="239">
         <f>$S59+$AB59+$AG59+$AJ59</f>
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="60" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -10537,7 +10537,7 @@
       <c r="F60" s="127"/>
       <c r="G60" s="125">
         <f>(IF($G59&lt;&gt;"",($G$7*$O$105)+IF($G$7=4,($O$103)+IF($G59=$G$7+$H$7,$O$104,0),0),0)+IF($H59&lt;&gt;"",($H$7*$O$105)+IF($H$7=4,($O$103)+IF($H59=$G$7+$H$7,$O$104,0),0),0))</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="H60" s="127"/>
       <c r="I60" s="128">
@@ -10552,7 +10552,7 @@
       <c r="L60" s="127"/>
       <c r="M60" s="125">
         <f>(IF($M59&lt;&gt;"",($M$7*$O$105)+IF($M$7=4,($O$103)+IF($M59=$M$7+$N$7,$O$104,0),0),0)+IF($N59&lt;&gt;"",($N$7*$O$105)+IF($N$7=4,($O$103)+IF($N59=$M$7+$N$7,$O$104,0),0),0))</f>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="N60" s="127"/>
       <c r="O60" s="128">
@@ -10562,13 +10562,13 @@
       <c r="P60" s="127"/>
       <c r="Q60" s="128">
         <f>(IF($Q59&lt;&gt;"",($Q$7*$O$105)+IF($Q$7=4,($O$103)+IF($Q59=$Q$7+$R$7,$O$104,0),0),0)+IF($R59&lt;&gt;"",($R$7*$O$105)+IF($R$7=4,($O$103)+IF($R59=$Q$7+$R$7,$O$104,0),0),0))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="R60" s="131"/>
       <c r="S60" s="121"/>
       <c r="T60" s="126">
         <f>(IF($T59&lt;&gt;"",($T$7*$P$105)+IF($T$7=4,($P$103)+IF($T59=$T$7+$U$7,$P$104,0),0),0)+IF($U59&lt;&gt;"",($U$7*$P$105)+IF($U$7=4,($P$103)+IF($U59=$T$7+$U$7,$P$104,0),0),0))</f>
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="U60" s="126"/>
       <c r="V60" s="126">
@@ -10637,7 +10637,7 @@
         <f>IF(ISBLANK(H59),
 0,
 IF(H$7 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I61" s="118">
         <f>IF(ISBLANK(I59),
@@ -10673,7 +10673,7 @@
         <f>IF(ISBLANK(N59),
 0,
 IF(N$7 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O61" s="118">
         <f>IF(ISBLANK(O59),
@@ -10691,7 +10691,7 @@
         <f>IF(ISBLANK(Q59),
 0,
 IF(Q$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R61" s="118">
         <f>IF(ISBLANK(R59),
@@ -10704,7 +10704,7 @@
         <f>IF(ISBLANK(T59),
 0,
 IF(T$7= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U61" s="118">
         <f>IF(ISBLANK(U59),
@@ -10759,7 +10759,7 @@
       <c r="AJ61" s="138"/>
       <c r="AK61" s="139">
         <f>SUM(C61:AI61)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AL61" s="123"/>
     </row>
@@ -10802,7 +10802,7 @@
         <f>IF(H61 = 0,
 0,
 IF(H59 = (G$7+H$7),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I62" s="118">
         <f>IF(I61 = 0,
@@ -10838,7 +10838,7 @@
         <f>IF(N61 = 0,
 0,
 IF(N59 = (M$7+N$7),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O62" s="118">
         <f>IF(O61 = 0,
@@ -10924,73 +10924,73 @@
       <c r="AJ62" s="138"/>
       <c r="AK62" s="139">
         <f>SUM(C62:AI62)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL62" s="123"/>
     </row>
     <row r="63" spans="1:38" s="27" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="117">
         <f>RANK(AL63,$AL$11:$AL$98,)</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B63" s="84" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C63" s="46">
         <v>6</v>
       </c>
       <c r="D63" s="45"/>
-      <c r="E63" s="44"/>
-      <c r="F63" s="45">
+      <c r="E63" s="210">
         <v>7</v>
       </c>
+      <c r="F63" s="45"/>
       <c r="G63" s="48">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H63" s="47"/>
       <c r="I63" s="44"/>
       <c r="J63" s="47">
+        <v>5</v>
+      </c>
+      <c r="K63" s="49">
+        <v>7</v>
+      </c>
+      <c r="L63" s="47"/>
+      <c r="M63" s="44">
         <v>6</v>
       </c>
-      <c r="K63" s="49"/>
-      <c r="L63" s="47">
-        <v>6</v>
-      </c>
-      <c r="M63" s="44"/>
-      <c r="N63" s="211">
-        <v>6</v>
-      </c>
+      <c r="N63" s="45"/>
       <c r="O63" s="44">
+        <v>7</v>
+      </c>
+      <c r="P63" s="45"/>
+      <c r="Q63" s="48">
         <v>5</v>
       </c>
-      <c r="P63" s="45"/>
-      <c r="Q63" s="48"/>
-      <c r="R63" s="50">
-        <v>6</v>
-      </c>
+      <c r="R63" s="50"/>
       <c r="S63" s="122">
         <f>SUM(C64:R64)</f>
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="T63" s="46"/>
       <c r="U63" s="47">
+        <v>6</v>
+      </c>
+      <c r="V63" s="44">
         <v>5</v>
-      </c>
-      <c r="V63" s="44">
-        <v>6</v>
       </c>
       <c r="W63" s="47"/>
       <c r="X63" s="49">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Y63" s="45"/>
-      <c r="Z63" s="48"/>
-      <c r="AA63" s="47">
-        <v>6</v>
-      </c>
+      <c r="Z63" s="48">
+        <v>7</v>
+      </c>
+      <c r="AA63" s="47"/>
       <c r="AB63" s="122">
         <f>SUM(T64:AA64)</f>
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="AC63" s="48"/>
       <c r="AD63" s="47"/>
@@ -11008,11 +11008,11 @@
       </c>
       <c r="AK63" s="111">
         <f>MAX($AL$11:$AL$98) - AL63</f>
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="AL63" s="122">
         <f>$S63+$AB63+$AG63+$AJ63</f>
-        <v>39</v>
+        <v>51</v>
       </c>
     </row>
     <row r="64" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11028,7 +11028,7 @@
       <c r="D64" s="127"/>
       <c r="E64" s="125">
         <f>(IF($E63&lt;&gt;"",($E$7*$O$105)+IF($E$7=4,($O$103)+IF($E63=$E$7+$F$7,$O$104,0),0),0)+IF($F63&lt;&gt;"",($F$7*$O$105)+IF($F$7=4,($O$103)+IF($F63=$E$7+$F$7,$O$104,0),0),0))</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F64" s="127"/>
       <c r="G64" s="125">
@@ -11043,12 +11043,12 @@
       <c r="J64" s="129"/>
       <c r="K64" s="130">
         <f>(IF($K63&lt;&gt;"",($K$7*$O$105)+IF($K$7=4,($O$103)+IF($K63=$K$7+$L$7,$O$104,0),0),0)+IF($L63&lt;&gt;"",($L$7*$O$105)+IF($L$7=4,($O$103)+IF($L63=$K$7+$L$7,$O$104,0),0),0))</f>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="L64" s="127"/>
       <c r="M64" s="125">
         <f>(IF($M63&lt;&gt;"",($M$7*$O$105)+IF($M$7=4,($O$103)+IF($M63=$M$7+$N$7,$O$104,0),0),0)+IF($N63&lt;&gt;"",($N$7*$O$105)+IF($N$7=4,($O$103)+IF($N63=$M$7+$N$7,$O$104,0),0),0))</f>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="N64" s="127"/>
       <c r="O64" s="128">
@@ -11058,7 +11058,7 @@
       <c r="P64" s="127"/>
       <c r="Q64" s="128">
         <f>(IF($Q63&lt;&gt;"",($Q$7*$O$105)+IF($Q$7=4,($O$103)+IF($Q63=$Q$7+$R$7,$O$104,0),0),0)+IF($R63&lt;&gt;"",($R$7*$O$105)+IF($R$7=4,($O$103)+IF($R63=$Q$7+$R$7,$O$104,0),0),0))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="R64" s="131"/>
       <c r="S64" s="121"/>
@@ -11079,7 +11079,7 @@
       <c r="Y64" s="59"/>
       <c r="Z64" s="126">
         <f>(IF($Z63&lt;&gt;"",($Z$7*$P$105)+IF($Z$7=4,($P$103)+IF($Z63=$Z$7+$AA$7,$P$104,0),0),0)+IF($AA63&lt;&gt;"",($AA$7*$P$105)+IF($AA$7=4,($P$103)+IF($AA63=$Z$7+$AA$7,$P$104,0),0),0))</f>
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="AA64" s="62"/>
       <c r="AB64" s="121"/>
@@ -11115,7 +11115,7 @@
         <f>IF(ISBLANK(E63),
 0,
 IF(E$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F65" s="118">
         <f>IF(ISBLANK(F63),
@@ -11157,7 +11157,7 @@
         <f>IF(ISBLANK(L63),
 0,
 IF(L$7 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M65" s="118">
         <f>IF(ISBLANK(M63),
@@ -11169,7 +11169,7 @@
         <f>IF(ISBLANK(N63),
 0,
 IF(N$7 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O65" s="118">
         <f>IF(ISBLANK(O63),
@@ -11187,7 +11187,7 @@
         <f>IF(ISBLANK(Q63),
 0,
 IF(Q$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R65" s="118">
         <f>IF(ISBLANK(R63),
@@ -11236,7 +11236,7 @@
         <f>IF(ISBLANK(Z63),
 0,
 IF(Z$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA65" s="118">
         <f>IF(ISBLANK(AA63),
@@ -11255,7 +11255,7 @@
       <c r="AJ65" s="138"/>
       <c r="AK65" s="139">
         <f>SUM(C65:AI65)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL65" s="123"/>
     </row>
@@ -11280,7 +11280,7 @@
         <f>IF(E65 = 0,
 0,
 IF(E63 = (E$7+F$7),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F66" s="118">
         <f>IF(F65 = 0,
@@ -11334,7 +11334,7 @@
         <f>IF(N65 = 0,
 0,
 IF(N63 = (M$7+N$7),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O66" s="118">
         <f>IF(O65 = 0,
@@ -11401,7 +11401,7 @@
         <f>IF(Z65 = 0,
 0,
 IF(Z63 = (Z$7+AA$7),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA66" s="118">
         <f>IF(AA65 = 0,
@@ -11420,7 +11420,7 @@
       <c r="AJ66" s="138"/>
       <c r="AK66" s="139">
         <f>SUM(C66:AI66)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL66" s="123"/>
     </row>
@@ -11430,23 +11430,23 @@
         <v>15</v>
       </c>
       <c r="B67" s="217" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C67" s="229">
         <v>5</v>
       </c>
       <c r="D67" s="230"/>
       <c r="E67" s="234">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F67" s="230"/>
       <c r="G67" s="232">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H67" s="233"/>
       <c r="I67" s="234"/>
       <c r="J67" s="233">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K67" s="235">
         <v>5</v>
@@ -11457,7 +11457,7 @@
         <v>6</v>
       </c>
       <c r="O67" s="234">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P67" s="230"/>
       <c r="Q67" s="232"/>
@@ -11476,17 +11476,17 @@
         <v>5</v>
       </c>
       <c r="W67" s="233"/>
-      <c r="X67" s="235">
-        <v>7</v>
-      </c>
-      <c r="Y67" s="230"/>
+      <c r="X67" s="235"/>
+      <c r="Y67" s="230">
+        <v>5</v>
+      </c>
       <c r="Z67" s="232">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA67" s="233"/>
       <c r="AB67" s="239">
         <f>SUM(T68:AA68)</f>
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="AC67" s="232"/>
       <c r="AD67" s="233"/>
@@ -11496,7 +11496,7 @@
         <f>SUM(AC68:AF68)</f>
         <v>0</v>
       </c>
-      <c r="AH67" s="260"/>
+      <c r="AH67" s="246"/>
       <c r="AI67" s="240"/>
       <c r="AJ67" s="239">
         <f>AH68</f>
@@ -11504,11 +11504,11 @@
       </c>
       <c r="AK67" s="241">
         <f>MAX($AL$11:$AL$98) - AL67</f>
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="AL67" s="239">
         <f>$S67+$AB67+$AG67+$AJ67</f>
-        <v>37</v>
+        <v>48</v>
       </c>
     </row>
     <row r="68" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11575,7 +11575,7 @@
       <c r="Y68" s="59"/>
       <c r="Z68" s="126">
         <f>(IF($Z67&lt;&gt;"",($Z$7*$P$105)+IF($Z$7=4,($P$103)+IF($Z67=$Z$7+$AA$7,$P$104,0),0),0)+IF($AA67&lt;&gt;"",($AA$7*$P$105)+IF($AA$7=4,($P$103)+IF($AA67=$Z$7+$AA$7,$P$104,0),0),0))</f>
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="AA68" s="62"/>
       <c r="AB68" s="121"/>
@@ -11732,7 +11732,7 @@
         <f>IF(ISBLANK(Z67),
 0,
 IF(Z$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA69" s="118">
         <f>IF(ISBLANK(AA67),
@@ -11751,7 +11751,7 @@
       <c r="AJ69" s="138"/>
       <c r="AK69" s="139">
         <f>SUM(C69:AI69)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL69" s="123"/>
     </row>
@@ -11923,66 +11923,66 @@
     <row r="71" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="117">
         <f>RANK(AL71,$AL$11:$AL$98,)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B71" s="84" t="s">
-        <v>74</v>
-      </c>
-      <c r="C71" s="46">
+        <v>68</v>
+      </c>
+      <c r="C71" s="252">
         <v>5</v>
       </c>
-      <c r="D71" s="45"/>
-      <c r="E71" s="44">
+      <c r="D71" s="253"/>
+      <c r="E71" s="254">
         <v>6</v>
       </c>
-      <c r="F71" s="45"/>
-      <c r="G71" s="48">
+      <c r="F71" s="253"/>
+      <c r="G71" s="255">
+        <v>5</v>
+      </c>
+      <c r="H71" s="256"/>
+      <c r="I71" s="254"/>
+      <c r="J71" s="256">
         <v>6</v>
       </c>
-      <c r="H71" s="47"/>
-      <c r="I71" s="44"/>
-      <c r="J71" s="47">
+      <c r="K71" s="257">
+        <v>6</v>
+      </c>
+      <c r="L71" s="256"/>
+      <c r="M71" s="254">
         <v>7</v>
       </c>
-      <c r="K71" s="49">
-        <v>5</v>
-      </c>
-      <c r="L71" s="47"/>
-      <c r="M71" s="44"/>
-      <c r="N71" s="211">
+      <c r="N71" s="253"/>
+      <c r="O71" s="254">
         <v>6</v>
       </c>
-      <c r="O71" s="44">
-        <v>7</v>
-      </c>
-      <c r="P71" s="45"/>
-      <c r="Q71" s="48"/>
-      <c r="R71" s="50">
+      <c r="P71" s="253"/>
+      <c r="Q71" s="255"/>
+      <c r="R71" s="258">
         <v>6</v>
       </c>
       <c r="S71" s="122">
         <f>SUM(C72:R72)</f>
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="T71" s="46"/>
       <c r="U71" s="47">
         <v>6</v>
       </c>
       <c r="V71" s="44">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="W71" s="47"/>
-      <c r="X71" s="49"/>
-      <c r="Y71" s="45">
-        <v>5</v>
-      </c>
+      <c r="X71" s="49">
+        <v>6</v>
+      </c>
+      <c r="Y71" s="45"/>
       <c r="Z71" s="48">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AA71" s="47"/>
       <c r="AB71" s="122">
         <f>SUM(T72:AA72)</f>
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="AC71" s="48"/>
       <c r="AD71" s="47"/>
@@ -12000,11 +12000,11 @@
       </c>
       <c r="AK71" s="111">
         <f>MAX($AL$11:$AL$98) - AL71</f>
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="AL71" s="122">
         <f>$S71+$AB71+$AG71+$AJ71</f>
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="72" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -12040,7 +12040,7 @@
       <c r="L72" s="127"/>
       <c r="M72" s="125">
         <f>(IF($M71&lt;&gt;"",($M$7*$O$105)+IF($M$7=4,($O$103)+IF($M71=$M$7+$N$7,$O$104,0),0),0)+IF($N71&lt;&gt;"",($N$7*$O$105)+IF($N$7=4,($O$103)+IF($N71=$M$7+$N$7,$O$104,0),0),0))</f>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="N72" s="127"/>
       <c r="O72" s="128">
@@ -12071,7 +12071,7 @@
       <c r="Y72" s="59"/>
       <c r="Z72" s="126">
         <f>(IF($Z71&lt;&gt;"",($Z$7*$P$105)+IF($Z$7=4,($P$103)+IF($Z71=$Z$7+$AA$7,$P$104,0),0),0)+IF($AA71&lt;&gt;"",($AA$7*$P$105)+IF($AA$7=4,($P$103)+IF($AA71=$Z$7+$AA$7,$P$104,0),0),0))</f>
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="AA72" s="62"/>
       <c r="AB72" s="121"/>
@@ -12161,7 +12161,7 @@
         <f>IF(ISBLANK(N71),
 0,
 IF(N$7 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O73" s="118">
         <f>IF(ISBLANK(O71),
@@ -12228,7 +12228,7 @@
         <f>IF(ISBLANK(Z71),
 0,
 IF(Z$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA73" s="118">
         <f>IF(ISBLANK(AA71),
@@ -12326,7 +12326,7 @@
         <f>IF(N73 = 0,
 0,
 IF(N71 = (M$7+N$7),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O74" s="118">
         <f>IF(O73 = 0,
@@ -12393,7 +12393,7 @@
         <f>IF(Z73 = 0,
 0,
 IF(Z71 = (Z$7+AA$7),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA74" s="118">
         <f>IF(AA73 = 0,
@@ -12422,63 +12422,63 @@
         <v>17</v>
       </c>
       <c r="B75" s="217" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C75" s="229">
         <v>6</v>
       </c>
       <c r="D75" s="230"/>
-      <c r="E75" s="231">
-        <v>7</v>
+      <c r="E75" s="234">
+        <v>6</v>
       </c>
       <c r="F75" s="230"/>
       <c r="G75" s="232">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H75" s="233"/>
       <c r="I75" s="234"/>
       <c r="J75" s="233">
+        <v>7</v>
+      </c>
+      <c r="K75" s="235">
         <v>5</v>
-      </c>
-      <c r="K75" s="235">
-        <v>7</v>
       </c>
       <c r="L75" s="233"/>
       <c r="M75" s="234">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N75" s="230"/>
       <c r="O75" s="234">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P75" s="230"/>
-      <c r="Q75" s="232">
-        <v>5</v>
-      </c>
-      <c r="R75" s="237"/>
+      <c r="Q75" s="232"/>
+      <c r="R75" s="237">
+        <v>6</v>
+      </c>
       <c r="S75" s="239">
         <f>SUM(C76:R76)</f>
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="T75" s="229"/>
       <c r="U75" s="233">
         <v>6</v>
       </c>
-      <c r="V75" s="234">
-        <v>5</v>
-      </c>
-      <c r="W75" s="233"/>
-      <c r="X75" s="235">
-        <v>4</v>
-      </c>
-      <c r="Y75" s="230"/>
-      <c r="Z75" s="232">
+      <c r="V75" s="234"/>
+      <c r="W75" s="233">
+        <v>6</v>
+      </c>
+      <c r="X75" s="235"/>
+      <c r="Y75" s="230">
         <v>7</v>
       </c>
-      <c r="AA75" s="233"/>
+      <c r="Z75" s="232"/>
+      <c r="AA75" s="233">
+        <v>6</v>
+      </c>
       <c r="AB75" s="239">
         <f>SUM(T76:AA76)</f>
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="AC75" s="232"/>
       <c r="AD75" s="233"/>
@@ -12496,11 +12496,11 @@
       </c>
       <c r="AK75" s="241">
         <f>MAX($AL$11:$AL$98) - AL75</f>
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="AL75" s="239">
         <f>$S75+$AB75+$AG75+$AJ75</f>
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="76" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -12516,7 +12516,7 @@
       <c r="D76" s="127"/>
       <c r="E76" s="125">
         <f>(IF($E75&lt;&gt;"",($E$7*$O$105)+IF($E$7=4,($O$103)+IF($E75=$E$7+$F$7,$O$104,0),0),0)+IF($F75&lt;&gt;"",($F$7*$O$105)+IF($F$7=4,($O$103)+IF($F75=$E$7+$F$7,$O$104,0),0),0))</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F76" s="127"/>
       <c r="G76" s="125">
@@ -12546,7 +12546,7 @@
       <c r="P76" s="127"/>
       <c r="Q76" s="128">
         <f>(IF($Q75&lt;&gt;"",($Q$7*$O$105)+IF($Q$7=4,($O$103)+IF($Q75=$Q$7+$R$7,$O$104,0),0),0)+IF($R75&lt;&gt;"",($R$7*$O$105)+IF($R$7=4,($O$103)+IF($R75=$Q$7+$R$7,$O$104,0),0),0))</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="R76" s="131"/>
       <c r="S76" s="121"/>
@@ -12557,7 +12557,7 @@
       <c r="U76" s="126"/>
       <c r="V76" s="126">
         <f>(IF($V75&lt;&gt;"",($V$7*$P$105)+IF($V$7=4,($P$103)+IF($V75=$V$7+$W$7,$P$104,0),0),0)+IF($W75&lt;&gt;"",($W$7*$P$105)+IF($W$7=4,($P$103)+IF($W75=$V$7+$W$7,$P$104,0),0),0))</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="W76" s="126"/>
       <c r="X76" s="126">
@@ -12675,7 +12675,7 @@
         <f>IF(ISBLANK(Q75),
 0,
 IF(Q$7= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R77" s="118">
         <f>IF(ISBLANK(R75),
@@ -12706,7 +12706,7 @@
         <f>IF(ISBLANK(W75),
 0,
 IF(W$7 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X77" s="118">
         <f>IF(ISBLANK(X75),
@@ -12768,7 +12768,7 @@
         <f>IF(E77 = 0,
 0,
 IF(E75 = (E$7+F$7),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F78" s="118">
         <f>IF(F77 = 0,
@@ -12908,7 +12908,7 @@
       <c r="AJ78" s="138"/>
       <c r="AK78" s="139">
         <f>SUM(C78:AI78)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL78" s="123"/>
     </row>
@@ -12918,60 +12918,60 @@
         <v>18</v>
       </c>
       <c r="B79" s="84" t="s">
-        <v>68</v>
-      </c>
-      <c r="C79" s="252">
+        <v>79</v>
+      </c>
+      <c r="C79" s="46">
+        <v>6</v>
+      </c>
+      <c r="D79" s="45"/>
+      <c r="E79" s="44"/>
+      <c r="F79" s="45">
+        <v>7</v>
+      </c>
+      <c r="G79" s="48">
+        <v>6</v>
+      </c>
+      <c r="H79" s="47"/>
+      <c r="I79" s="44"/>
+      <c r="J79" s="47">
+        <v>6</v>
+      </c>
+      <c r="K79" s="49"/>
+      <c r="L79" s="47">
+        <v>6</v>
+      </c>
+      <c r="M79" s="44"/>
+      <c r="N79" s="211">
+        <v>6</v>
+      </c>
+      <c r="O79" s="44">
         <v>5</v>
       </c>
-      <c r="D79" s="253"/>
-      <c r="E79" s="254">
-        <v>6</v>
-      </c>
-      <c r="F79" s="253"/>
-      <c r="G79" s="255">
-        <v>5</v>
-      </c>
-      <c r="H79" s="256"/>
-      <c r="I79" s="254"/>
-      <c r="J79" s="256">
-        <v>6</v>
-      </c>
-      <c r="K79" s="257">
-        <v>6</v>
-      </c>
-      <c r="L79" s="256"/>
-      <c r="M79" s="254">
-        <v>7</v>
-      </c>
-      <c r="N79" s="253"/>
-      <c r="O79" s="254">
-        <v>6</v>
-      </c>
-      <c r="P79" s="253"/>
-      <c r="Q79" s="255"/>
-      <c r="R79" s="258">
+      <c r="P79" s="45"/>
+      <c r="Q79" s="48"/>
+      <c r="R79" s="50">
         <v>6</v>
       </c>
       <c r="S79" s="122">
         <f>SUM(C80:R80)</f>
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="T79" s="46"/>
       <c r="U79" s="47">
+        <v>5</v>
+      </c>
+      <c r="V79" s="44">
         <v>6</v>
-      </c>
-      <c r="V79" s="44">
-        <v>7</v>
       </c>
       <c r="W79" s="47"/>
       <c r="X79" s="49">
         <v>6</v>
       </c>
       <c r="Y79" s="45"/>
-      <c r="Z79" s="48">
-        <v>7</v>
-      </c>
-      <c r="AA79" s="47"/>
+      <c r="Z79" s="48"/>
+      <c r="AA79" s="47">
+        <v>6</v>
+      </c>
       <c r="AB79" s="122">
         <f>SUM(T80:AA80)</f>
         <v>8</v>
@@ -12992,11 +12992,11 @@
       </c>
       <c r="AK79" s="111">
         <f>MAX($AL$11:$AL$98) - AL79</f>
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="AL79" s="122">
         <f>$S79+$AB79+$AG79+$AJ79</f>
-        <v>28</v>
+        <v>39</v>
       </c>
     </row>
     <row r="80" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -13012,7 +13012,7 @@
       <c r="D80" s="127"/>
       <c r="E80" s="125">
         <f>(IF($E79&lt;&gt;"",($E$7*$O$105)+IF($E$7=4,($O$103)+IF($E79=$E$7+$F$7,$O$104,0),0),0)+IF($F79&lt;&gt;"",($F$7*$O$105)+IF($F$7=4,($O$103)+IF($F79=$E$7+$F$7,$O$104,0),0),0))</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F80" s="127"/>
       <c r="G80" s="125">
@@ -13027,12 +13027,12 @@
       <c r="J80" s="129"/>
       <c r="K80" s="130">
         <f>(IF($K79&lt;&gt;"",($K$7*$O$105)+IF($K$7=4,($O$103)+IF($K79=$K$7+$L$7,$O$104,0),0),0)+IF($L79&lt;&gt;"",($L$7*$O$105)+IF($L$7=4,($O$103)+IF($L79=$K$7+$L$7,$O$104,0),0),0))</f>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="L80" s="127"/>
       <c r="M80" s="125">
         <f>(IF($M79&lt;&gt;"",($M$7*$O$105)+IF($M$7=4,($O$103)+IF($M79=$M$7+$N$7,$O$104,0),0),0)+IF($N79&lt;&gt;"",($N$7*$O$105)+IF($N$7=4,($O$103)+IF($N79=$M$7+$N$7,$O$104,0),0),0))</f>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="N80" s="127"/>
       <c r="O80" s="128">
@@ -13099,7 +13099,7 @@
         <f>IF(ISBLANK(E79),
 0,
 IF(E$7= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F81" s="118">
         <f>IF(ISBLANK(F79),
@@ -13141,7 +13141,7 @@
         <f>IF(ISBLANK(L79),
 0,
 IF(L$7 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M81" s="118">
         <f>IF(ISBLANK(M79),
@@ -13153,7 +13153,7 @@
         <f>IF(ISBLANK(N79),
 0,
 IF(N$7 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O81" s="118">
         <f>IF(ISBLANK(O79),
@@ -13239,7 +13239,7 @@
       <c r="AJ81" s="138"/>
       <c r="AK81" s="139">
         <f>SUM(C81:AI81)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL81" s="123"/>
     </row>
@@ -13318,7 +13318,7 @@
         <f>IF(N81 = 0,
 0,
 IF(N79 = (M$7+N$7),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O82" s="118">
         <f>IF(O81 = 0,
@@ -13404,36 +13404,36 @@
       <c r="AJ82" s="138"/>
       <c r="AK82" s="139">
         <f>SUM(C82:AI82)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL82" s="123"/>
     </row>
     <row r="83" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="216">
         <f>RANK(AL83,$AL$11:$AL$98,)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B83" s="217" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C83" s="229">
         <v>5</v>
       </c>
       <c r="D83" s="230"/>
-      <c r="E83" s="234">
-        <v>6</v>
-      </c>
-      <c r="F83" s="230"/>
+      <c r="E83" s="234"/>
+      <c r="F83" s="230">
+        <v>7</v>
+      </c>
       <c r="G83" s="232">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H83" s="233"/>
       <c r="I83" s="234"/>
       <c r="J83" s="233">
+        <v>7</v>
+      </c>
+      <c r="K83" s="235">
         <v>6</v>
-      </c>
-      <c r="K83" s="235">
-        <v>7</v>
       </c>
       <c r="L83" s="233"/>
       <c r="M83" s="234">
@@ -13441,7 +13441,7 @@
       </c>
       <c r="N83" s="230"/>
       <c r="O83" s="234">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P83" s="230"/>
       <c r="Q83" s="232"/>
@@ -13450,27 +13450,27 @@
       </c>
       <c r="S83" s="239">
         <f>SUM(C84:R84)</f>
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="T83" s="229"/>
       <c r="U83" s="233">
+        <v>7</v>
+      </c>
+      <c r="V83" s="234">
+        <v>5</v>
+      </c>
+      <c r="W83" s="233"/>
+      <c r="X83" s="235">
         <v>6</v>
       </c>
-      <c r="V83" s="234">
+      <c r="Y83" s="230"/>
+      <c r="Z83" s="232">
         <v>6</v>
       </c>
-      <c r="W83" s="233"/>
-      <c r="X83" s="235"/>
-      <c r="Y83" s="230">
-        <v>5</v>
-      </c>
-      <c r="Z83" s="232"/>
-      <c r="AA83" s="233">
-        <v>6</v>
-      </c>
+      <c r="AA83" s="233"/>
       <c r="AB83" s="239">
         <f>SUM(T84:AA84)</f>
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="AC83" s="232"/>
       <c r="AD83" s="233"/>
@@ -13488,11 +13488,11 @@
       </c>
       <c r="AK83" s="241">
         <f>MAX($AL$11:$AL$98) - AL83</f>
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="AL83" s="239">
         <f>$S83+$AB83+$AG83+$AJ83</f>
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="84" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -13508,7 +13508,7 @@
       <c r="D84" s="127"/>
       <c r="E84" s="125">
         <f>(IF($E83&lt;&gt;"",($E$7*$O$105)+IF($E$7=4,($O$103)+IF($E83=$E$7+$F$7,$O$104,0),0),0)+IF($F83&lt;&gt;"",($F$7*$O$105)+IF($F$7=4,($O$103)+IF($F83=$E$7+$F$7,$O$104,0),0),0))</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F84" s="127"/>
       <c r="G84" s="125">
@@ -13559,7 +13559,7 @@
       <c r="Y84" s="59"/>
       <c r="Z84" s="126">
         <f>(IF($Z83&lt;&gt;"",($Z$7*$P$105)+IF($Z$7=4,($P$103)+IF($Z83=$Z$7+$AA$7,$P$104,0),0),0)+IF($AA83&lt;&gt;"",($AA$7*$P$105)+IF($AA$7=4,($P$103)+IF($AA83=$Z$7+$AA$7,$P$104,0),0),0))</f>
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="AA84" s="62"/>
       <c r="AB84" s="121"/>
@@ -13595,7 +13595,7 @@
         <f>IF(ISBLANK(E83),
 0,
 IF(E$7= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F85" s="118">
         <f>IF(ISBLANK(F83),
@@ -13716,7 +13716,7 @@
         <f>IF(ISBLANK(Z83),
 0,
 IF(Z$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA85" s="118">
         <f>IF(ISBLANK(AA83),
@@ -13907,13 +13907,13 @@
     <row r="87" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="117">
         <f>RANK(AL87,$AL$11:$AL$98,)</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B87" s="84" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="C87" s="46">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D87" s="45"/>
       <c r="E87" s="44"/>
@@ -13921,23 +13921,23 @@
         <v>7</v>
       </c>
       <c r="G87" s="48">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H87" s="47"/>
       <c r="I87" s="44"/>
       <c r="J87" s="47">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K87" s="49">
         <v>6</v>
       </c>
       <c r="L87" s="47"/>
       <c r="M87" s="44">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N87" s="45"/>
       <c r="O87" s="44">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P87" s="45"/>
       <c r="Q87" s="48"/>
@@ -13953,20 +13953,20 @@
         <v>7</v>
       </c>
       <c r="V87" s="44">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="W87" s="47"/>
-      <c r="X87" s="49">
+      <c r="X87" s="49"/>
+      <c r="Y87" s="45">
         <v>6</v>
       </c>
-      <c r="Y87" s="45"/>
       <c r="Z87" s="48">
         <v>6</v>
       </c>
       <c r="AA87" s="47"/>
       <c r="AB87" s="122">
         <f>SUM(T88:AA88)</f>
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="AC87" s="48"/>
       <c r="AD87" s="47"/>
@@ -13984,11 +13984,11 @@
       </c>
       <c r="AK87" s="111">
         <f>MAX($AL$11:$AL$98) - AL87</f>
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="AL87" s="122">
         <f>$S87+$AB87+$AG87+$AJ87</f>
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="88" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -14055,7 +14055,7 @@
       <c r="Y88" s="59"/>
       <c r="Z88" s="126">
         <f>(IF($Z87&lt;&gt;"",($Z$7*$P$105)+IF($Z$7=4,($P$103)+IF($Z87=$Z$7+$AA$7,$P$104,0),0),0)+IF($AA87&lt;&gt;"",($AA$7*$P$105)+IF($AA$7=4,($P$103)+IF($AA87=$Z$7+$AA$7,$P$104,0),0),0))</f>
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="AA88" s="62"/>
       <c r="AB88" s="121"/>
@@ -14212,7 +14212,7 @@
         <f>IF(ISBLANK(Z87),
 0,
 IF(Z$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA89" s="118">
         <f>IF(ISBLANK(AA87),
@@ -14231,7 +14231,7 @@
       <c r="AJ89" s="138"/>
       <c r="AK89" s="139">
         <f>SUM(C89:AI89)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL89" s="123"/>
     </row>
@@ -14403,13 +14403,13 @@
     <row r="91" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="216">
         <f>RANK(AL91,$AL$11:$AL$98,)</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B91" s="217" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C91" s="229">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D91" s="230"/>
       <c r="E91" s="234"/>
@@ -14417,28 +14417,28 @@
         <v>7</v>
       </c>
       <c r="G91" s="232">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H91" s="233"/>
       <c r="I91" s="234"/>
       <c r="J91" s="233">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K91" s="235">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L91" s="233"/>
       <c r="M91" s="234">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N91" s="230"/>
       <c r="O91" s="234">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P91" s="230"/>
       <c r="Q91" s="232"/>
       <c r="R91" s="237">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S91" s="239">
         <f>SUM(C92:R92)</f>
@@ -14449,20 +14449,20 @@
         <v>7</v>
       </c>
       <c r="V91" s="234">
+        <v>7</v>
+      </c>
+      <c r="W91" s="233"/>
+      <c r="X91" s="235">
         <v>6</v>
       </c>
-      <c r="W91" s="233"/>
-      <c r="X91" s="235"/>
-      <c r="Y91" s="230">
-        <v>6</v>
-      </c>
+      <c r="Y91" s="230"/>
       <c r="Z91" s="232">
         <v>6</v>
       </c>
       <c r="AA91" s="233"/>
       <c r="AB91" s="239">
         <f>SUM(T92:AA92)</f>
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="AC91" s="232"/>
       <c r="AD91" s="233"/>
@@ -14480,11 +14480,11 @@
       </c>
       <c r="AK91" s="241">
         <f>MAX($AL$11:$AL$98) - AL91</f>
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="AL91" s="239">
         <f>$S91+$AB91+$AG91+$AJ91</f>
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="92" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -14551,7 +14551,7 @@
       <c r="Y92" s="59"/>
       <c r="Z92" s="126">
         <f>(IF($Z91&lt;&gt;"",($Z$7*$P$105)+IF($Z$7=4,($P$103)+IF($Z91=$Z$7+$AA$7,$P$104,0),0),0)+IF($AA91&lt;&gt;"",($AA$7*$P$105)+IF($AA$7=4,($P$103)+IF($AA91=$Z$7+$AA$7,$P$104,0),0),0))</f>
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="AA92" s="62"/>
       <c r="AB92" s="121"/>
@@ -14708,7 +14708,7 @@
         <f>IF(ISBLANK(Z91),
 0,
 IF(Z$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA93" s="118">
         <f>IF(ISBLANK(AA91),
@@ -14727,7 +14727,7 @@
       <c r="AJ93" s="138"/>
       <c r="AK93" s="139">
         <f>SUM(C93:AI93)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL93" s="123"/>
     </row>
@@ -14899,29 +14899,29 @@
     <row r="95" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A95" s="117">
         <f>RANK(AL95,$AL$11:$AL$98,)</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B95" s="84" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C95" s="187">
         <v>5</v>
       </c>
       <c r="D95" s="188"/>
-      <c r="E95" s="189"/>
-      <c r="F95" s="188">
-        <v>7</v>
-      </c>
+      <c r="E95" s="189">
+        <v>6</v>
+      </c>
+      <c r="F95" s="188"/>
       <c r="G95" s="190">
         <v>6</v>
       </c>
       <c r="H95" s="191"/>
       <c r="I95" s="189"/>
       <c r="J95" s="191">
+        <v>6</v>
+      </c>
+      <c r="K95" s="192">
         <v>7</v>
-      </c>
-      <c r="K95" s="192">
-        <v>5</v>
       </c>
       <c r="L95" s="191"/>
       <c r="M95" s="189">
@@ -14929,33 +14929,33 @@
       </c>
       <c r="N95" s="188"/>
       <c r="O95" s="189">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P95" s="188"/>
       <c r="Q95" s="190"/>
       <c r="R95" s="193">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S95" s="122">
         <f>SUM(C96:R96)</f>
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="T95" s="46"/>
       <c r="U95" s="47">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V95" s="44">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="W95" s="47"/>
-      <c r="X95" s="49">
+      <c r="X95" s="49"/>
+      <c r="Y95" s="45">
+        <v>5</v>
+      </c>
+      <c r="Z95" s="48"/>
+      <c r="AA95" s="47">
         <v>6</v>
       </c>
-      <c r="Y95" s="45"/>
-      <c r="Z95" s="48">
-        <v>6</v>
-      </c>
-      <c r="AA95" s="47"/>
       <c r="AB95" s="179">
         <f>SUM(T96:AA96)</f>
         <v>8</v>
@@ -14976,11 +14976,11 @@
       </c>
       <c r="AK95" s="111">
         <f>MAX($AL$11:$AL$98) - AL95</f>
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="AL95" s="179">
         <f>$S95+$AB95+$AG95+$AJ95</f>
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="96" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -14996,7 +14996,7 @@
       <c r="D96" s="127"/>
       <c r="E96" s="125">
         <f>(IF($E95&lt;&gt;"",($E$7*$O$105)+IF($E$7=4,($O$103)+IF($E95=$E$7+$F$7,$O$104,0),0),0)+IF($F95&lt;&gt;"",($F$7*$O$105)+IF($F$7=4,($O$103)+IF($F95=$E$7+$F$7,$O$104,0),0),0))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F96" s="127"/>
       <c r="G96" s="125">
@@ -15083,7 +15083,7 @@
         <f>IF(ISBLANK(E95),
 0,
 IF(E$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F97" s="118">
         <f>IF(ISBLANK(F95),
@@ -15223,7 +15223,7 @@
       <c r="AJ97" s="138"/>
       <c r="AK97" s="139">
         <f>SUM(C97:AI97)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL97" s="123"/>
     </row>
@@ -15525,12 +15525,12 @@
     <row r="101" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B101" s="43"/>
       <c r="N101" s="26"/>
-      <c r="O101" s="298" t="s">
+      <c r="O101" s="300" t="s">
         <v>17</v>
       </c>
-      <c r="P101" s="299"/>
-      <c r="Q101" s="299"/>
-      <c r="R101" s="300"/>
+      <c r="P101" s="301"/>
+      <c r="Q101" s="301"/>
+      <c r="R101" s="302"/>
       <c r="AG101" s="30"/>
       <c r="AH101" s="30"/>
       <c r="AI101" s="30"/>
@@ -15539,21 +15539,21 @@
     </row>
     <row r="102" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A102" s="33"/>
-      <c r="B102" s="288" t="s">
+      <c r="B102" s="290" t="s">
         <v>16</v>
       </c>
-      <c r="C102" s="289"/>
-      <c r="D102" s="289"/>
-      <c r="E102" s="289"/>
-      <c r="F102" s="289"/>
-      <c r="G102" s="289"/>
-      <c r="H102" s="289"/>
-      <c r="I102" s="289"/>
-      <c r="J102" s="289"/>
-      <c r="K102" s="289"/>
-      <c r="L102" s="289"/>
-      <c r="M102" s="289"/>
-      <c r="N102" s="290"/>
+      <c r="C102" s="291"/>
+      <c r="D102" s="291"/>
+      <c r="E102" s="291"/>
+      <c r="F102" s="291"/>
+      <c r="G102" s="291"/>
+      <c r="H102" s="291"/>
+      <c r="I102" s="291"/>
+      <c r="J102" s="291"/>
+      <c r="K102" s="291"/>
+      <c r="L102" s="291"/>
+      <c r="M102" s="291"/>
+      <c r="N102" s="292"/>
       <c r="O102" s="21">
         <v>1</v>
       </c>
@@ -15566,45 +15566,45 @@
       <c r="R102" s="22">
         <v>4</v>
       </c>
-      <c r="U102" s="301" t="s">
+      <c r="U102" s="303" t="s">
         <v>26</v>
       </c>
-      <c r="V102" s="302"/>
-      <c r="W102" s="302"/>
-      <c r="X102" s="302"/>
-      <c r="Y102" s="302"/>
-      <c r="Z102" s="302"/>
-      <c r="AA102" s="302"/>
-      <c r="AB102" s="302"/>
-      <c r="AC102" s="302"/>
-      <c r="AD102" s="303"/>
+      <c r="V102" s="304"/>
+      <c r="W102" s="304"/>
+      <c r="X102" s="304"/>
+      <c r="Y102" s="304"/>
+      <c r="Z102" s="304"/>
+      <c r="AA102" s="304"/>
+      <c r="AB102" s="304"/>
+      <c r="AC102" s="304"/>
+      <c r="AD102" s="305"/>
       <c r="AE102" s="28"/>
       <c r="AF102" s="28"/>
-      <c r="AG102" s="304" t="s">
+      <c r="AG102" s="306" t="s">
         <v>24</v>
       </c>
-      <c r="AH102" s="305"/>
-      <c r="AI102" s="305"/>
-      <c r="AJ102" s="305"/>
-      <c r="AK102" s="306"/>
+      <c r="AH102" s="307"/>
+      <c r="AI102" s="307"/>
+      <c r="AJ102" s="307"/>
+      <c r="AK102" s="308"/>
     </row>
     <row r="103" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A103" s="34"/>
-      <c r="B103" s="271" t="s">
+      <c r="B103" s="280" t="s">
         <v>6</v>
       </c>
-      <c r="C103" s="265"/>
-      <c r="D103" s="265"/>
-      <c r="E103" s="265"/>
-      <c r="F103" s="265"/>
-      <c r="G103" s="265"/>
-      <c r="H103" s="265"/>
-      <c r="I103" s="265"/>
-      <c r="J103" s="265"/>
-      <c r="K103" s="265"/>
-      <c r="L103" s="265"/>
-      <c r="M103" s="265"/>
-      <c r="N103" s="266"/>
+      <c r="C103" s="281"/>
+      <c r="D103" s="281"/>
+      <c r="E103" s="281"/>
+      <c r="F103" s="281"/>
+      <c r="G103" s="281"/>
+      <c r="H103" s="281"/>
+      <c r="I103" s="281"/>
+      <c r="J103" s="281"/>
+      <c r="K103" s="281"/>
+      <c r="L103" s="281"/>
+      <c r="M103" s="281"/>
+      <c r="N103" s="282"/>
       <c r="O103" s="20">
         <v>5</v>
       </c>
@@ -15617,49 +15617,49 @@
       <c r="R103" s="23">
         <v>20</v>
       </c>
-      <c r="U103" s="293" t="s">
+      <c r="U103" s="295" t="s">
         <v>20</v>
       </c>
-      <c r="V103" s="294"/>
-      <c r="W103" s="294"/>
-      <c r="X103" s="294"/>
-      <c r="Y103" s="294"/>
-      <c r="Z103" s="294"/>
-      <c r="AA103" s="294"/>
-      <c r="AB103" s="291">
+      <c r="V103" s="296"/>
+      <c r="W103" s="296"/>
+      <c r="X103" s="296"/>
+      <c r="Y103" s="296"/>
+      <c r="Z103" s="296"/>
+      <c r="AA103" s="296"/>
+      <c r="AB103" s="293">
         <v>22</v>
       </c>
-      <c r="AC103" s="291"/>
-      <c r="AD103" s="292"/>
+      <c r="AC103" s="293"/>
+      <c r="AD103" s="294"/>
       <c r="AE103" s="29"/>
       <c r="AF103" s="29"/>
-      <c r="AG103" s="261" t="s">
+      <c r="AG103" s="309" t="s">
         <v>21</v>
       </c>
-      <c r="AH103" s="262"/>
-      <c r="AI103" s="262"/>
-      <c r="AJ103" s="263"/>
+      <c r="AH103" s="310"/>
+      <c r="AI103" s="310"/>
+      <c r="AJ103" s="311"/>
       <c r="AK103" s="184">
         <v>230</v>
       </c>
     </row>
     <row r="104" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="34"/>
-      <c r="B104" s="271" t="s">
+      <c r="B104" s="280" t="s">
         <v>5</v>
       </c>
-      <c r="C104" s="265"/>
-      <c r="D104" s="265"/>
-      <c r="E104" s="265"/>
-      <c r="F104" s="265"/>
-      <c r="G104" s="265"/>
-      <c r="H104" s="265"/>
-      <c r="I104" s="265"/>
-      <c r="J104" s="265"/>
-      <c r="K104" s="265"/>
-      <c r="L104" s="265"/>
-      <c r="M104" s="265"/>
-      <c r="N104" s="266"/>
+      <c r="C104" s="281"/>
+      <c r="D104" s="281"/>
+      <c r="E104" s="281"/>
+      <c r="F104" s="281"/>
+      <c r="G104" s="281"/>
+      <c r="H104" s="281"/>
+      <c r="I104" s="281"/>
+      <c r="J104" s="281"/>
+      <c r="K104" s="281"/>
+      <c r="L104" s="281"/>
+      <c r="M104" s="281"/>
+      <c r="N104" s="282"/>
       <c r="O104" s="20">
         <v>2</v>
       </c>
@@ -15672,49 +15672,49 @@
       <c r="R104" s="23">
         <v>8</v>
       </c>
-      <c r="U104" s="267" t="s">
+      <c r="U104" s="285" t="s">
         <v>18</v>
       </c>
-      <c r="V104" s="268"/>
-      <c r="W104" s="268"/>
-      <c r="X104" s="268"/>
-      <c r="Y104" s="268"/>
-      <c r="Z104" s="268"/>
-      <c r="AA104" s="268"/>
-      <c r="AB104" s="269">
+      <c r="V104" s="286"/>
+      <c r="W104" s="286"/>
+      <c r="X104" s="286"/>
+      <c r="Y104" s="286"/>
+      <c r="Z104" s="286"/>
+      <c r="AA104" s="286"/>
+      <c r="AB104" s="313">
         <v>20</v>
       </c>
-      <c r="AC104" s="269"/>
-      <c r="AD104" s="270"/>
+      <c r="AC104" s="313"/>
+      <c r="AD104" s="314"/>
       <c r="AE104" s="29"/>
       <c r="AF104" s="29"/>
-      <c r="AG104" s="264" t="s">
+      <c r="AG104" s="312" t="s">
         <v>22</v>
       </c>
-      <c r="AH104" s="265"/>
-      <c r="AI104" s="265"/>
-      <c r="AJ104" s="266"/>
+      <c r="AH104" s="281"/>
+      <c r="AI104" s="281"/>
+      <c r="AJ104" s="282"/>
       <c r="AK104" s="36">
         <v>115</v>
       </c>
     </row>
     <row r="105" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A105" s="35"/>
-      <c r="B105" s="281" t="s">
+      <c r="B105" s="287" t="s">
         <v>4</v>
       </c>
-      <c r="C105" s="282"/>
-      <c r="D105" s="282"/>
-      <c r="E105" s="282"/>
-      <c r="F105" s="282"/>
-      <c r="G105" s="282"/>
-      <c r="H105" s="282"/>
-      <c r="I105" s="282"/>
-      <c r="J105" s="282"/>
-      <c r="K105" s="282"/>
-      <c r="L105" s="282"/>
-      <c r="M105" s="282"/>
-      <c r="N105" s="283"/>
+      <c r="C105" s="288"/>
+      <c r="D105" s="288"/>
+      <c r="E105" s="288"/>
+      <c r="F105" s="288"/>
+      <c r="G105" s="288"/>
+      <c r="H105" s="288"/>
+      <c r="I105" s="288"/>
+      <c r="J105" s="288"/>
+      <c r="K105" s="288"/>
+      <c r="L105" s="288"/>
+      <c r="M105" s="288"/>
+      <c r="N105" s="289"/>
       <c r="O105" s="3">
         <v>1</v>
       </c>
@@ -15727,51 +15727,51 @@
       <c r="R105" s="24">
         <v>1</v>
       </c>
-      <c r="U105" s="295" t="s">
+      <c r="U105" s="297" t="s">
         <v>19</v>
       </c>
-      <c r="V105" s="273"/>
-      <c r="W105" s="273"/>
-      <c r="X105" s="273"/>
-      <c r="Y105" s="273"/>
-      <c r="Z105" s="273"/>
-      <c r="AA105" s="273"/>
-      <c r="AB105" s="296">
+      <c r="V105" s="284"/>
+      <c r="W105" s="284"/>
+      <c r="X105" s="284"/>
+      <c r="Y105" s="284"/>
+      <c r="Z105" s="284"/>
+      <c r="AA105" s="284"/>
+      <c r="AB105" s="298">
         <f>AB103*AB104</f>
         <v>440</v>
       </c>
-      <c r="AC105" s="296"/>
-      <c r="AD105" s="297"/>
+      <c r="AC105" s="298"/>
+      <c r="AD105" s="299"/>
       <c r="AE105" s="29"/>
       <c r="AF105" s="29"/>
-      <c r="AG105" s="264" t="s">
+      <c r="AG105" s="312" t="s">
         <v>25</v>
       </c>
-      <c r="AH105" s="265"/>
-      <c r="AI105" s="265"/>
-      <c r="AJ105" s="266"/>
+      <c r="AH105" s="281"/>
+      <c r="AI105" s="281"/>
+      <c r="AJ105" s="282"/>
       <c r="AK105" s="36">
         <v>65</v>
       </c>
     </row>
     <row r="106" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG106" s="267" t="s">
+      <c r="AG106" s="285" t="s">
         <v>23</v>
       </c>
-      <c r="AH106" s="268"/>
-      <c r="AI106" s="268"/>
-      <c r="AJ106" s="268"/>
+      <c r="AH106" s="286"/>
+      <c r="AI106" s="286"/>
+      <c r="AJ106" s="286"/>
       <c r="AK106" s="186">
         <v>30</v>
       </c>
     </row>
     <row r="107" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG107" s="272" t="s">
+      <c r="AG107" s="283" t="s">
         <v>19</v>
       </c>
-      <c r="AH107" s="273"/>
-      <c r="AI107" s="273"/>
-      <c r="AJ107" s="273"/>
+      <c r="AH107" s="284"/>
+      <c r="AI107" s="284"/>
+      <c r="AJ107" s="284"/>
       <c r="AK107" s="185">
         <f>SUM(AK103:AK106)</f>
         <v>440</v>
@@ -15783,25 +15783,11 @@
     <sortCondition ref="B11:B95"/>
   </sortState>
   <mergeCells count="40">
-    <mergeCell ref="C5:S5"/>
-    <mergeCell ref="T5:AB5"/>
-    <mergeCell ref="AC5:AG5"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="AH5:AJ5"/>
-    <mergeCell ref="AG6:AG10"/>
-    <mergeCell ref="AJ6:AJ10"/>
-    <mergeCell ref="X6:AA6"/>
-    <mergeCell ref="AB6:AB10"/>
-    <mergeCell ref="AC6:AD6"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="C1:O1"/>
-    <mergeCell ref="P1:AJ1"/>
-    <mergeCell ref="C4:O4"/>
-    <mergeCell ref="P4:AJ4"/>
-    <mergeCell ref="C3:P3"/>
-    <mergeCell ref="Q3:AJ3"/>
-    <mergeCell ref="C2:P2"/>
-    <mergeCell ref="Q2:AJ2"/>
+    <mergeCell ref="AG103:AJ103"/>
+    <mergeCell ref="AG105:AJ105"/>
+    <mergeCell ref="AG104:AJ104"/>
+    <mergeCell ref="U104:AA104"/>
+    <mergeCell ref="AB104:AD104"/>
     <mergeCell ref="B104:N104"/>
     <mergeCell ref="AG107:AJ107"/>
     <mergeCell ref="AG106:AJ106"/>
@@ -15818,11 +15804,25 @@
     <mergeCell ref="O101:R101"/>
     <mergeCell ref="U102:AD102"/>
     <mergeCell ref="AG102:AK102"/>
-    <mergeCell ref="AG103:AJ103"/>
-    <mergeCell ref="AG105:AJ105"/>
-    <mergeCell ref="AG104:AJ104"/>
-    <mergeCell ref="U104:AA104"/>
-    <mergeCell ref="AB104:AD104"/>
+    <mergeCell ref="C1:O1"/>
+    <mergeCell ref="P1:AJ1"/>
+    <mergeCell ref="C4:O4"/>
+    <mergeCell ref="P4:AJ4"/>
+    <mergeCell ref="C3:P3"/>
+    <mergeCell ref="Q3:AJ3"/>
+    <mergeCell ref="C2:P2"/>
+    <mergeCell ref="Q2:AJ2"/>
+    <mergeCell ref="C5:S5"/>
+    <mergeCell ref="T5:AB5"/>
+    <mergeCell ref="AC5:AG5"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="AH5:AJ5"/>
+    <mergeCell ref="AG6:AG10"/>
+    <mergeCell ref="AJ6:AJ10"/>
+    <mergeCell ref="X6:AA6"/>
+    <mergeCell ref="AB6:AB10"/>
+    <mergeCell ref="AC6:AD6"/>
+    <mergeCell ref="AE6:AF6"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <conditionalFormatting sqref="S11:S16 AB11:AB16 AG11:AG16 AJ11:AJ16 AJ27:AJ28 AG27:AG28 AB27:AB28 S27:S28 AJ23:AJ24 AG23:AG24 AB23:AB24 S23:S24 AJ19:AJ20 AG19:AG20 AB19:AB20 S19:S20 S39:S40 AB39:AB40 AG39:AG40 AJ39:AJ40 S31:S32 AB31:AB32 AG31:AG32 AJ31:AJ32 AJ43:AJ44 AG43:AG44 AB43:AB44 S43:S44 S47:S48 AB47:AB48 AG47:AG48 AJ47:AJ48 AJ51 AG51 AB51 S51 S59 AB59 AG59 AJ59 S55 AB55 AG55 AJ55 AJ63 AG63 AB63 S63 S67 AB67 AG67 AJ67 AJ71 AG71 AB71 S71 S75 AB75 AG75 AJ75 AJ79 AG79 AB79 S79 AJ35:AJ36 AG35:AG36 AB35:AB36 S35:S36">
@@ -16465,7 +16465,7 @@
   <dimension ref="A1:AJ31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+      <selection activeCell="U26" sqref="U26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17661,10 +17661,12 @@
       <c r="T24" s="82">
         <v>4</v>
       </c>
-      <c r="U24" s="81"/>
+      <c r="U24" s="81">
+        <v>2</v>
+      </c>
       <c r="V24" s="73">
         <f>IF(O24&gt;O25,1,0)+IF(P24&gt;P25,1,0)+IF(Q24&gt;Q25,1,0)+IF(R24&gt;R25,1,0)+IF(S24&gt;S25,1,0)+IF(T24&gt;T25,1,0)+IF(U24&gt;U25,1,0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W24" s="16"/>
       <c r="X24" s="4"/>
@@ -17734,7 +17736,9 @@
       <c r="T25" s="82">
         <v>1</v>
       </c>
-      <c r="U25" s="81"/>
+      <c r="U25" s="81">
+        <v>1</v>
+      </c>
       <c r="V25" s="73">
         <f>IF(O25&gt;O24,1,0)+IF(P25&gt;P24,1,0)+IF(Q25&gt;Q24,1,0)+IF(R25&gt;R24,1,0)+IF(S25&gt;S24,1,0)+IF(T25&gt;T24,1,0)+IF(U25&gt;U24,1,0)</f>
         <v>3</v>

</xml_diff>

<commit_message>
Updated games of 2019-05-09
</commit_message>
<xml_diff>
--- a/laval.xlsx
+++ b/laval.xlsx
@@ -2526,6 +2526,147 @@
     <xf numFmtId="0" fontId="14" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="90" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="79" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="80" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="82" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="83" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="29" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="81" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="107" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="108" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="90" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2538,154 +2679,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="82" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="81" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="107" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="108" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="90" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="79" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="80" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="83" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="29" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2698,32 +2698,9 @@
   </cellStyles>
   <dxfs count="80">
     <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor indexed="13"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2861,9 +2838,32 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor indexed="13"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3772,258 +3772,258 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="C1" s="273"/>
-      <c r="D1" s="273"/>
-      <c r="E1" s="273"/>
-      <c r="F1" s="273"/>
-      <c r="G1" s="273"/>
-      <c r="H1" s="273"/>
-      <c r="I1" s="273"/>
-      <c r="J1" s="273"/>
-      <c r="K1" s="273"/>
-      <c r="L1" s="273"/>
-      <c r="M1" s="273"/>
-      <c r="N1" s="273"/>
-      <c r="O1" s="273"/>
-      <c r="P1" s="274"/>
-      <c r="Q1" s="274"/>
-      <c r="R1" s="274"/>
-      <c r="S1" s="274"/>
-      <c r="T1" s="274"/>
-      <c r="U1" s="274"/>
-      <c r="V1" s="274"/>
-      <c r="W1" s="274"/>
-      <c r="X1" s="274"/>
-      <c r="Y1" s="274"/>
-      <c r="Z1" s="274"/>
-      <c r="AA1" s="274"/>
-      <c r="AB1" s="274"/>
-      <c r="AC1" s="274"/>
-      <c r="AD1" s="274"/>
-      <c r="AE1" s="274"/>
-      <c r="AF1" s="274"/>
-      <c r="AG1" s="274"/>
-      <c r="AH1" s="274"/>
-      <c r="AI1" s="274"/>
-      <c r="AJ1" s="274"/>
+      <c r="C1" s="303"/>
+      <c r="D1" s="303"/>
+      <c r="E1" s="303"/>
+      <c r="F1" s="303"/>
+      <c r="G1" s="303"/>
+      <c r="H1" s="303"/>
+      <c r="I1" s="303"/>
+      <c r="J1" s="303"/>
+      <c r="K1" s="303"/>
+      <c r="L1" s="303"/>
+      <c r="M1" s="303"/>
+      <c r="N1" s="303"/>
+      <c r="O1" s="303"/>
+      <c r="P1" s="304"/>
+      <c r="Q1" s="304"/>
+      <c r="R1" s="304"/>
+      <c r="S1" s="304"/>
+      <c r="T1" s="304"/>
+      <c r="U1" s="304"/>
+      <c r="V1" s="304"/>
+      <c r="W1" s="304"/>
+      <c r="X1" s="304"/>
+      <c r="Y1" s="304"/>
+      <c r="Z1" s="304"/>
+      <c r="AA1" s="304"/>
+      <c r="AB1" s="304"/>
+      <c r="AC1" s="304"/>
+      <c r="AD1" s="304"/>
+      <c r="AE1" s="304"/>
+      <c r="AF1" s="304"/>
+      <c r="AG1" s="304"/>
+      <c r="AH1" s="304"/>
+      <c r="AI1" s="304"/>
+      <c r="AJ1" s="304"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="41"/>
-      <c r="C2" s="275" t="s">
+      <c r="C2" s="305" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="275"/>
-      <c r="E2" s="275"/>
-      <c r="F2" s="275"/>
-      <c r="G2" s="275"/>
-      <c r="H2" s="275"/>
-      <c r="I2" s="275"/>
-      <c r="J2" s="275"/>
-      <c r="K2" s="275"/>
-      <c r="L2" s="275"/>
-      <c r="M2" s="275"/>
-      <c r="N2" s="275"/>
-      <c r="O2" s="275"/>
-      <c r="P2" s="275"/>
-      <c r="Q2" s="276" t="s">
+      <c r="D2" s="305"/>
+      <c r="E2" s="305"/>
+      <c r="F2" s="305"/>
+      <c r="G2" s="305"/>
+      <c r="H2" s="305"/>
+      <c r="I2" s="305"/>
+      <c r="J2" s="305"/>
+      <c r="K2" s="305"/>
+      <c r="L2" s="305"/>
+      <c r="M2" s="305"/>
+      <c r="N2" s="305"/>
+      <c r="O2" s="305"/>
+      <c r="P2" s="305"/>
+      <c r="Q2" s="306" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="274"/>
-      <c r="S2" s="274"/>
-      <c r="T2" s="274"/>
-      <c r="U2" s="274"/>
-      <c r="V2" s="274"/>
-      <c r="W2" s="274"/>
-      <c r="X2" s="274"/>
-      <c r="Y2" s="274"/>
-      <c r="Z2" s="274"/>
-      <c r="AA2" s="274"/>
-      <c r="AB2" s="274"/>
-      <c r="AC2" s="274"/>
-      <c r="AD2" s="274"/>
-      <c r="AE2" s="274"/>
-      <c r="AF2" s="274"/>
-      <c r="AG2" s="274"/>
-      <c r="AH2" s="274"/>
-      <c r="AI2" s="274"/>
-      <c r="AJ2" s="274"/>
+      <c r="R2" s="304"/>
+      <c r="S2" s="304"/>
+      <c r="T2" s="304"/>
+      <c r="U2" s="304"/>
+      <c r="V2" s="304"/>
+      <c r="W2" s="304"/>
+      <c r="X2" s="304"/>
+      <c r="Y2" s="304"/>
+      <c r="Z2" s="304"/>
+      <c r="AA2" s="304"/>
+      <c r="AB2" s="304"/>
+      <c r="AC2" s="304"/>
+      <c r="AD2" s="304"/>
+      <c r="AE2" s="304"/>
+      <c r="AF2" s="304"/>
+      <c r="AG2" s="304"/>
+      <c r="AH2" s="304"/>
+      <c r="AI2" s="304"/>
+      <c r="AJ2" s="304"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A3" s="41"/>
-      <c r="C3" s="275" t="s">
+      <c r="C3" s="305" t="s">
         <v>85</v>
       </c>
-      <c r="D3" s="275"/>
-      <c r="E3" s="275"/>
-      <c r="F3" s="275"/>
-      <c r="G3" s="275"/>
-      <c r="H3" s="275"/>
-      <c r="I3" s="275"/>
-      <c r="J3" s="275"/>
-      <c r="K3" s="275"/>
-      <c r="L3" s="275"/>
-      <c r="M3" s="275"/>
-      <c r="N3" s="275"/>
-      <c r="O3" s="275"/>
-      <c r="P3" s="275"/>
-      <c r="Q3" s="276" t="s">
+      <c r="D3" s="305"/>
+      <c r="E3" s="305"/>
+      <c r="F3" s="305"/>
+      <c r="G3" s="305"/>
+      <c r="H3" s="305"/>
+      <c r="I3" s="305"/>
+      <c r="J3" s="305"/>
+      <c r="K3" s="305"/>
+      <c r="L3" s="305"/>
+      <c r="M3" s="305"/>
+      <c r="N3" s="305"/>
+      <c r="O3" s="305"/>
+      <c r="P3" s="305"/>
+      <c r="Q3" s="306" t="s">
         <v>86</v>
       </c>
-      <c r="R3" s="274"/>
-      <c r="S3" s="274"/>
-      <c r="T3" s="274"/>
-      <c r="U3" s="274"/>
-      <c r="V3" s="274"/>
-      <c r="W3" s="274"/>
-      <c r="X3" s="274"/>
-      <c r="Y3" s="274"/>
-      <c r="Z3" s="274"/>
-      <c r="AA3" s="274"/>
-      <c r="AB3" s="274"/>
-      <c r="AC3" s="274"/>
-      <c r="AD3" s="274"/>
-      <c r="AE3" s="274"/>
-      <c r="AF3" s="274"/>
-      <c r="AG3" s="274"/>
-      <c r="AH3" s="274"/>
-      <c r="AI3" s="274"/>
-      <c r="AJ3" s="274"/>
+      <c r="R3" s="304"/>
+      <c r="S3" s="304"/>
+      <c r="T3" s="304"/>
+      <c r="U3" s="304"/>
+      <c r="V3" s="304"/>
+      <c r="W3" s="304"/>
+      <c r="X3" s="304"/>
+      <c r="Y3" s="304"/>
+      <c r="Z3" s="304"/>
+      <c r="AA3" s="304"/>
+      <c r="AB3" s="304"/>
+      <c r="AC3" s="304"/>
+      <c r="AD3" s="304"/>
+      <c r="AE3" s="304"/>
+      <c r="AF3" s="304"/>
+      <c r="AG3" s="304"/>
+      <c r="AH3" s="304"/>
+      <c r="AI3" s="304"/>
+      <c r="AJ3" s="304"/>
     </row>
     <row r="4" spans="1:38" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="273"/>
-      <c r="D4" s="273"/>
-      <c r="E4" s="273"/>
-      <c r="F4" s="273"/>
-      <c r="G4" s="273"/>
-      <c r="H4" s="273"/>
-      <c r="I4" s="273"/>
-      <c r="J4" s="273"/>
-      <c r="K4" s="273"/>
-      <c r="L4" s="273"/>
-      <c r="M4" s="273"/>
-      <c r="N4" s="273"/>
-      <c r="O4" s="273"/>
-      <c r="P4" s="274"/>
-      <c r="Q4" s="274"/>
-      <c r="R4" s="274"/>
-      <c r="S4" s="274"/>
-      <c r="T4" s="274"/>
-      <c r="U4" s="274"/>
-      <c r="V4" s="274"/>
-      <c r="W4" s="274"/>
-      <c r="X4" s="274"/>
-      <c r="Y4" s="274"/>
-      <c r="Z4" s="274"/>
-      <c r="AA4" s="274"/>
-      <c r="AB4" s="274"/>
-      <c r="AC4" s="274"/>
-      <c r="AD4" s="274"/>
-      <c r="AE4" s="274"/>
-      <c r="AF4" s="274"/>
-      <c r="AG4" s="274"/>
-      <c r="AH4" s="274"/>
-      <c r="AI4" s="274"/>
-      <c r="AJ4" s="274"/>
+      <c r="C4" s="303"/>
+      <c r="D4" s="303"/>
+      <c r="E4" s="303"/>
+      <c r="F4" s="303"/>
+      <c r="G4" s="303"/>
+      <c r="H4" s="303"/>
+      <c r="I4" s="303"/>
+      <c r="J4" s="303"/>
+      <c r="K4" s="303"/>
+      <c r="L4" s="303"/>
+      <c r="M4" s="303"/>
+      <c r="N4" s="303"/>
+      <c r="O4" s="303"/>
+      <c r="P4" s="304"/>
+      <c r="Q4" s="304"/>
+      <c r="R4" s="304"/>
+      <c r="S4" s="304"/>
+      <c r="T4" s="304"/>
+      <c r="U4" s="304"/>
+      <c r="V4" s="304"/>
+      <c r="W4" s="304"/>
+      <c r="X4" s="304"/>
+      <c r="Y4" s="304"/>
+      <c r="Z4" s="304"/>
+      <c r="AA4" s="304"/>
+      <c r="AB4" s="304"/>
+      <c r="AC4" s="304"/>
+      <c r="AD4" s="304"/>
+      <c r="AE4" s="304"/>
+      <c r="AF4" s="304"/>
+      <c r="AG4" s="304"/>
+      <c r="AH4" s="304"/>
+      <c r="AI4" s="304"/>
+      <c r="AJ4" s="304"/>
     </row>
     <row r="5" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="260" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="261"/>
-      <c r="E5" s="261"/>
-      <c r="F5" s="261"/>
-      <c r="G5" s="261"/>
-      <c r="H5" s="261"/>
-      <c r="I5" s="261"/>
-      <c r="J5" s="261"/>
-      <c r="K5" s="261"/>
-      <c r="L5" s="261"/>
-      <c r="M5" s="261"/>
-      <c r="N5" s="261"/>
-      <c r="O5" s="261"/>
-      <c r="P5" s="261"/>
-      <c r="Q5" s="261"/>
-      <c r="R5" s="261"/>
-      <c r="S5" s="262"/>
-      <c r="T5" s="260" t="s">
-        <v>1</v>
-      </c>
-      <c r="U5" s="261"/>
-      <c r="V5" s="261"/>
-      <c r="W5" s="261"/>
-      <c r="X5" s="261"/>
-      <c r="Y5" s="261"/>
-      <c r="Z5" s="261"/>
-      <c r="AA5" s="261"/>
-      <c r="AB5" s="262"/>
-      <c r="AC5" s="260" t="s">
+      <c r="C5" s="307" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="308"/>
+      <c r="E5" s="308"/>
+      <c r="F5" s="308"/>
+      <c r="G5" s="308"/>
+      <c r="H5" s="308"/>
+      <c r="I5" s="308"/>
+      <c r="J5" s="308"/>
+      <c r="K5" s="308"/>
+      <c r="L5" s="308"/>
+      <c r="M5" s="308"/>
+      <c r="N5" s="308"/>
+      <c r="O5" s="308"/>
+      <c r="P5" s="308"/>
+      <c r="Q5" s="308"/>
+      <c r="R5" s="308"/>
+      <c r="S5" s="309"/>
+      <c r="T5" s="307" t="s">
+        <v>1</v>
+      </c>
+      <c r="U5" s="308"/>
+      <c r="V5" s="308"/>
+      <c r="W5" s="308"/>
+      <c r="X5" s="308"/>
+      <c r="Y5" s="308"/>
+      <c r="Z5" s="308"/>
+      <c r="AA5" s="308"/>
+      <c r="AB5" s="309"/>
+      <c r="AC5" s="307" t="s">
         <v>2</v>
       </c>
-      <c r="AD5" s="261"/>
-      <c r="AE5" s="261"/>
-      <c r="AF5" s="261"/>
-      <c r="AG5" s="263"/>
-      <c r="AH5" s="260" t="s">
+      <c r="AD5" s="308"/>
+      <c r="AE5" s="308"/>
+      <c r="AF5" s="308"/>
+      <c r="AG5" s="310"/>
+      <c r="AH5" s="307" t="s">
         <v>10</v>
       </c>
-      <c r="AI5" s="261"/>
-      <c r="AJ5" s="262"/>
+      <c r="AI5" s="308"/>
+      <c r="AJ5" s="309"/>
     </row>
     <row r="6" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="32"/>
       <c r="B6" s="4"/>
-      <c r="C6" s="264" t="s">
+      <c r="C6" s="280" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="265"/>
-      <c r="E6" s="265"/>
-      <c r="F6" s="265"/>
-      <c r="G6" s="265"/>
-      <c r="H6" s="265"/>
-      <c r="I6" s="265"/>
-      <c r="J6" s="266"/>
-      <c r="K6" s="271" t="s">
+      <c r="D6" s="275"/>
+      <c r="E6" s="275"/>
+      <c r="F6" s="275"/>
+      <c r="G6" s="275"/>
+      <c r="H6" s="275"/>
+      <c r="I6" s="275"/>
+      <c r="J6" s="276"/>
+      <c r="K6" s="274" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="265"/>
-      <c r="M6" s="265"/>
-      <c r="N6" s="265"/>
-      <c r="O6" s="265"/>
-      <c r="P6" s="265"/>
-      <c r="Q6" s="265"/>
-      <c r="R6" s="266"/>
-      <c r="S6" s="267" t="s">
+      <c r="L6" s="275"/>
+      <c r="M6" s="275"/>
+      <c r="N6" s="275"/>
+      <c r="O6" s="275"/>
+      <c r="P6" s="275"/>
+      <c r="Q6" s="275"/>
+      <c r="R6" s="276"/>
+      <c r="S6" s="277" t="s">
         <v>12</v>
       </c>
-      <c r="T6" s="264" t="s">
+      <c r="T6" s="280" t="s">
         <v>9</v>
       </c>
-      <c r="U6" s="265"/>
-      <c r="V6" s="265"/>
-      <c r="W6" s="266"/>
-      <c r="X6" s="271" t="s">
+      <c r="U6" s="275"/>
+      <c r="V6" s="275"/>
+      <c r="W6" s="276"/>
+      <c r="X6" s="274" t="s">
         <v>8</v>
       </c>
-      <c r="Y6" s="265"/>
-      <c r="Z6" s="265"/>
-      <c r="AA6" s="266"/>
-      <c r="AB6" s="267" t="s">
+      <c r="Y6" s="275"/>
+      <c r="Z6" s="275"/>
+      <c r="AA6" s="276"/>
+      <c r="AB6" s="277" t="s">
         <v>13</v>
       </c>
-      <c r="AC6" s="272" t="s">
+      <c r="AC6" s="312" t="s">
         <v>9</v>
       </c>
-      <c r="AD6" s="266"/>
-      <c r="AE6" s="271" t="s">
+      <c r="AD6" s="276"/>
+      <c r="AE6" s="274" t="s">
         <v>8</v>
       </c>
-      <c r="AF6" s="266"/>
-      <c r="AG6" s="267" t="s">
+      <c r="AF6" s="276"/>
+      <c r="AG6" s="277" t="s">
         <v>14</v>
       </c>
       <c r="AH6" s="56"/>
       <c r="AI6" s="25"/>
-      <c r="AJ6" s="267" t="s">
+      <c r="AJ6" s="277" t="s">
         <v>15</v>
       </c>
       <c r="AK6" s="4"/>
@@ -4095,7 +4095,7 @@
         <f>Résultats!$J$28</f>
         <v>3</v>
       </c>
-      <c r="S7" s="268"/>
+      <c r="S7" s="278"/>
       <c r="T7" s="237">
         <f>Résultats!$V$6</f>
         <v>4</v>
@@ -4128,10 +4128,10 @@
         <f>Résultats!$V$25</f>
         <v>3</v>
       </c>
-      <c r="AB7" s="268"/>
+      <c r="AB7" s="278"/>
       <c r="AC7" s="104">
         <f>Résultats!$AH$8</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD7" s="101">
         <f>Résultats!$AH$9</f>
@@ -4145,7 +4145,7 @@
         <f>Résultats!$AH$23</f>
         <v>0</v>
       </c>
-      <c r="AG7" s="268"/>
+      <c r="AG7" s="278"/>
       <c r="AH7" s="162">
         <f>Résultats!$AH$15</f>
         <v>0</v>
@@ -4154,7 +4154,7 @@
         <f>Résultats!$AH$16</f>
         <v>0</v>
       </c>
-      <c r="AJ7" s="268"/>
+      <c r="AJ7" s="278"/>
       <c r="AK7" s="37"/>
     </row>
     <row r="8" spans="1:38" s="39" customFormat="1" ht="58.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -4180,7 +4180,7 @@
       <c r="P8" s="192"/>
       <c r="Q8" s="196"/>
       <c r="R8" s="110"/>
-      <c r="S8" s="268"/>
+      <c r="S8" s="278"/>
       <c r="T8" s="238"/>
       <c r="U8" s="110"/>
       <c r="V8" s="149"/>
@@ -4189,15 +4189,15 @@
       <c r="Y8" s="111"/>
       <c r="Z8" s="196"/>
       <c r="AA8" s="110"/>
-      <c r="AB8" s="268"/>
+      <c r="AB8" s="278"/>
       <c r="AC8" s="112"/>
       <c r="AD8" s="110"/>
       <c r="AE8" s="113"/>
       <c r="AF8" s="110"/>
-      <c r="AG8" s="268"/>
+      <c r="AG8" s="278"/>
       <c r="AH8" s="162"/>
       <c r="AI8" s="105"/>
-      <c r="AJ8" s="268"/>
+      <c r="AJ8" s="278"/>
       <c r="AK8" s="37"/>
     </row>
     <row r="9" spans="1:38" s="39" customFormat="1" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4267,7 +4267,7 @@
         <f>Résultats!$B$28</f>
         <v>VEGAS</v>
       </c>
-      <c r="S9" s="268"/>
+      <c r="S9" s="278"/>
       <c r="T9" s="239" t="str">
         <f>Résultats!$N$6</f>
         <v>BOSTON</v>
@@ -4300,7 +4300,7 @@
         <f>Résultats!$N$25</f>
         <v>DALLAS</v>
       </c>
-      <c r="AB9" s="268"/>
+      <c r="AB9" s="278"/>
       <c r="AC9" s="153" t="str">
         <f>Résultats!$Z$8</f>
         <v>BOSTON</v>
@@ -4317,7 +4317,7 @@
         <f>Résultats!$Z$23</f>
         <v>ST-LOUIS</v>
       </c>
-      <c r="AG9" s="268"/>
+      <c r="AG9" s="278"/>
       <c r="AH9" s="163" t="str">
         <f>Résultats!$Z$15</f>
         <v xml:space="preserve"> </v>
@@ -4326,7 +4326,7 @@
         <f>Résultats!$Z$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ9" s="268"/>
+      <c r="AJ9" s="278"/>
       <c r="AK9" s="37"/>
     </row>
     <row r="10" spans="1:38" s="39" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4400,7 +4400,7 @@
         <f>Résultats!$A$28</f>
         <v>P3</v>
       </c>
-      <c r="S10" s="270"/>
+      <c r="S10" s="279"/>
       <c r="T10" s="240" t="str">
         <f>Résultats!$M$6</f>
         <v>A2</v>
@@ -4433,7 +4433,7 @@
         <f>Résultats!$M$25</f>
         <v>WC1</v>
       </c>
-      <c r="AB10" s="269"/>
+      <c r="AB10" s="311"/>
       <c r="AC10" s="159" t="str">
         <f>Résultats!$Y$8</f>
         <v>A2</v>
@@ -4450,7 +4450,7 @@
         <f>Résultats!$Y$23</f>
         <v>C3</v>
       </c>
-      <c r="AG10" s="269"/>
+      <c r="AG10" s="311"/>
       <c r="AH10" s="165" t="str">
         <f>Résultats!$Y$15</f>
         <v xml:space="preserve"> </v>
@@ -4459,7 +4459,7 @@
         <f>Résultats!$Y$16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ10" s="270"/>
+      <c r="AJ10" s="279"/>
       <c r="AK10" s="107" t="s">
         <v>51</v>
       </c>
@@ -5110,7 +5110,7 @@
       </c>
       <c r="AG15" s="120">
         <f>SUM(AC16:AF16)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH15" s="72"/>
       <c r="AI15" s="58"/>
@@ -5120,11 +5120,11 @@
       </c>
       <c r="AK15" s="109">
         <f>MAX($AL$11:$AL$98) - AL15</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AL15" s="120">
         <f>$S15+$AB15+$AG15+$AJ15</f>
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5197,7 +5197,7 @@
       <c r="AB16" s="138"/>
       <c r="AC16" s="124">
         <f>(IF($AC15&lt;&gt;"",($AC$7*$Q$105)+IF($AC$7=4,($Q$103)+IF($AC15=$AC$7+$AD$7,$Q$104,0),0),0)+IF($AD15&lt;&gt;"",($AD$7*$Q$105)+IF($AD$7=4,($Q$103)+IF($AD15=$AC$7+$AD$7,$Q$104,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD16" s="124"/>
       <c r="AE16" s="124">
@@ -5682,7 +5682,7 @@
       </c>
       <c r="AG19" s="227">
         <f>SUM(AC20:AF20)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH19" s="236"/>
       <c r="AI19" s="228"/>
@@ -5692,11 +5692,11 @@
       </c>
       <c r="AK19" s="229">
         <f>MAX($AL$11:$AL$98) - AL19</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AL19" s="227">
         <f>$S19+$AB19+$AG19+$AJ19</f>
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5769,7 +5769,7 @@
       <c r="AB20" s="138"/>
       <c r="AC20" s="124">
         <f>(IF($AC19&lt;&gt;"",($AC$7*$Q$105)+IF($AC$7=4,($Q$103)+IF($AC19=$AC$7+$AD$7,$Q$104,0),0),0)+IF($AD19&lt;&gt;"",($AD$7*$Q$105)+IF($AD$7=4,($Q$103)+IF($AD19=$AC$7+$AD$7,$Q$104,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD20" s="124"/>
       <c r="AE20" s="124">
@@ -6826,7 +6826,7 @@
       <c r="AF27" s="221"/>
       <c r="AG27" s="227">
         <f>SUM(AC28:AF28)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH27" s="214"/>
       <c r="AI27" s="215"/>
@@ -6836,11 +6836,11 @@
       </c>
       <c r="AK27" s="229">
         <f>MAX($AL$11:$AL$98) - AL27</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AL27" s="227">
         <f>$S27+$AB27+$AG27+$AJ27</f>
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6913,7 +6913,7 @@
       <c r="AB28" s="144"/>
       <c r="AC28" s="124">
         <f>(IF($AC27&lt;&gt;"",($AC$7*$Q$105)+IF($AC$7=4,($Q$103)+IF($AC27=$AC$7+$AD$7,$Q$104,0),0),0)+IF($AD27&lt;&gt;"",($AD$7*$Q$105)+IF($AD$7=4,($Q$103)+IF($AD27=$AC$7+$AD$7,$Q$104,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD28" s="124"/>
       <c r="AE28" s="124">
@@ -7398,7 +7398,7 @@
       </c>
       <c r="AG31" s="120">
         <f>SUM(AC32:AF32)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH31" s="241"/>
       <c r="AI31" s="57"/>
@@ -7408,11 +7408,11 @@
       </c>
       <c r="AK31" s="109">
         <f>MAX($AL$11:$AL$98) - AL31</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AL31" s="120">
         <f>$S31+$AB31+$AG31+$AJ31</f>
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7485,7 +7485,7 @@
       <c r="AB32" s="119"/>
       <c r="AC32" s="124">
         <f>(IF($AC31&lt;&gt;"",($AC$7*$Q$105)+IF($AC$7=4,($Q$103)+IF($AC31=$AC$7+$AD$7,$Q$104,0),0),0)+IF($AD31&lt;&gt;"",($AD$7*$Q$105)+IF($AD$7=4,($Q$103)+IF($AD31=$AC$7+$AD$7,$Q$104,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD32" s="124"/>
       <c r="AE32" s="124">
@@ -7970,7 +7970,7 @@
       </c>
       <c r="AG35" s="227">
         <f>SUM(AC36:AF36)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH35" s="230"/>
       <c r="AI35" s="215"/>
@@ -7980,11 +7980,11 @@
       </c>
       <c r="AK35" s="229">
         <f>MAX($AL$11:$AL$98) - AL35</f>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AL35" s="227">
         <f>$S35+$AB35+$AG35+$AJ35</f>
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -8057,7 +8057,7 @@
       <c r="AB36" s="119"/>
       <c r="AC36" s="124">
         <f>(IF($AC35&lt;&gt;"",($AC$7*$Q$105)+IF($AC$7=4,($Q$103)+IF($AC35=$AC$7+$AD$7,$Q$104,0),0),0)+IF($AD35&lt;&gt;"",($AD$7*$Q$105)+IF($AD$7=4,($Q$103)+IF($AD35=$AC$7+$AD$7,$Q$104,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD36" s="124"/>
       <c r="AE36" s="124">
@@ -8474,43 +8474,43 @@
         <v>8</v>
       </c>
       <c r="B39" s="82" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C39" s="46">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D39" s="45"/>
       <c r="E39" s="44">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F39" s="45"/>
-      <c r="G39" s="48">
+      <c r="G39" s="48"/>
+      <c r="H39" s="313">
+        <v>7</v>
+      </c>
+      <c r="I39" s="44"/>
+      <c r="J39" s="47">
         <v>6</v>
       </c>
-      <c r="H39" s="47"/>
-      <c r="I39" s="44">
-        <v>7</v>
-      </c>
-      <c r="J39" s="47"/>
       <c r="K39" s="49">
         <v>5</v>
       </c>
       <c r="L39" s="47"/>
       <c r="M39" s="44"/>
-      <c r="N39" s="45">
-        <v>7</v>
+      <c r="N39" s="200">
+        <v>6</v>
       </c>
       <c r="O39" s="44">
         <v>6</v>
       </c>
       <c r="P39" s="45"/>
-      <c r="Q39" s="202">
-        <v>7</v>
+      <c r="Q39" s="48">
+        <v>6</v>
       </c>
       <c r="R39" s="50"/>
       <c r="S39" s="120">
         <f>SUM(C40:R40)</f>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T39" s="46"/>
       <c r="U39" s="47">
@@ -8520,29 +8520,29 @@
         <v>6</v>
       </c>
       <c r="W39" s="47"/>
-      <c r="X39" s="49"/>
-      <c r="Y39" s="45">
-        <v>6</v>
-      </c>
-      <c r="Z39" s="48">
-        <v>6</v>
-      </c>
-      <c r="AA39" s="47"/>
+      <c r="X39" s="49">
+        <v>5</v>
+      </c>
+      <c r="Y39" s="45"/>
+      <c r="Z39" s="48"/>
+      <c r="AA39" s="47">
+        <v>7</v>
+      </c>
       <c r="AB39" s="120">
         <f>SUM(T40:AA40)</f>
         <v>19</v>
       </c>
-      <c r="AC39" s="48"/>
-      <c r="AD39" s="47">
-        <v>7</v>
-      </c>
+      <c r="AC39" s="48">
+        <v>6</v>
+      </c>
+      <c r="AD39" s="47"/>
       <c r="AE39" s="49">
         <v>6</v>
       </c>
       <c r="AF39" s="47"/>
       <c r="AG39" s="120">
         <f>SUM(AC40:AF40)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH39" s="100"/>
       <c r="AI39" s="57"/>
@@ -8577,12 +8577,12 @@
       <c r="F40" s="74"/>
       <c r="G40" s="117">
         <f>(IF($G39&lt;&gt;"",($G$7*$O$105)+IF($G$7=4,($O$103)+IF($G39=$G$7+$H$7,$O$104,0),0),0)+IF($H39&lt;&gt;"",($H$7*$O$105)+IF($H$7=4,($O$103)+IF($H39=$G$7+$H$7,$O$104,0),0),0))</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="H40" s="74"/>
       <c r="I40" s="114">
         <f>(IF($I39&lt;&gt;"",($I$7*$O$105)+IF($I$7=4,($O$103)+IF($I39=$I$7+$J$7,$O$104,0),0),0)+IF($J39&lt;&gt;"",($J$7*$O$105)+IF($J$7=4,($O$103)+IF($J39=$I$7+$J$7,$O$104,0),0),0))</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J40" s="76"/>
       <c r="K40" s="77">
@@ -8592,7 +8592,7 @@
       <c r="L40" s="74"/>
       <c r="M40" s="75">
         <f>(IF($M39&lt;&gt;"",($M$7*$O$105)+IF($M$7=4,($O$103)+IF($M39=$M$7+$N$7,$O$104,0),0),0)+IF($N39&lt;&gt;"",($N$7*$O$105)+IF($N$7=4,($O$103)+IF($N39=$M$7+$N$7,$O$104,0),0),0))</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="N40" s="74"/>
       <c r="O40" s="75">
@@ -8602,7 +8602,7 @@
       <c r="P40" s="74"/>
       <c r="Q40" s="75">
         <f>(IF($Q39&lt;&gt;"",($Q$7*$O$105)+IF($Q$7=4,($O$103)+IF($Q39=$Q$7+$R$7,$O$104,0),0),0)+IF($R39&lt;&gt;"",($R$7*$O$105)+IF($R$7=4,($O$103)+IF($R39=$Q$7+$R$7,$O$104,0),0),0))</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="R40" s="78"/>
       <c r="S40" s="119"/>
@@ -8618,18 +8618,18 @@
       <c r="W40" s="124"/>
       <c r="X40" s="124">
         <f>(IF($X39&lt;&gt;"",($X$7*$P$105)+IF($X$7=4,($P$103)+IF($X39=$X$7+$Y$7,$P$104,0),0),0)+IF($Y39&lt;&gt;"",($Y$7*$P$105)+IF($Y$7=4,($P$103)+IF($Y39=$X$7+$Y$7,$P$104,0),0),0))</f>
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="Y40" s="59"/>
       <c r="Z40" s="124">
         <f>(IF($Z39&lt;&gt;"",($Z$7*$P$105)+IF($Z$7=4,($P$103)+IF($Z39=$Z$7+$AA$7,$P$104,0),0),0)+IF($AA39&lt;&gt;"",($AA$7*$P$105)+IF($AA$7=4,($P$103)+IF($AA39=$Z$7+$AA$7,$P$104,0),0),0))</f>
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="AA40" s="60"/>
       <c r="AB40" s="119"/>
       <c r="AC40" s="124">
         <f>(IF($AC39&lt;&gt;"",($AC$7*$Q$105)+IF($AC$7=4,($Q$103)+IF($AC39=$AC$7+$AD$7,$Q$104,0),0),0)+IF($AD39&lt;&gt;"",($AD$7*$Q$105)+IF($AD$7=4,($Q$103)+IF($AD39=$AC$7+$AD$7,$Q$104,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD40" s="124"/>
       <c r="AE40" s="124">
@@ -8689,13 +8689,13 @@
         <f>IF(ISBLANK(H39),
 0,
 IF(H$7 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I41" s="116">
         <f>IF(ISBLANK(I39),
 0,
 IF(I$7= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J41" s="116">
         <f>IF(ISBLANK(J39),
@@ -8780,7 +8780,7 @@
         <f>IF(ISBLANK(X39),
 0,
 IF(X$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y41" s="116">
         <f>IF(ISBLANK(Y39),
@@ -8792,7 +8792,7 @@
         <f>IF(ISBLANK(Z39),
 0,
 IF(Z$7= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA41" s="116">
         <f>IF(ISBLANK(AA39),
@@ -8884,7 +8884,7 @@
         <f>IF(H41 = 0,
 0,
 IF(H39 = (G$7+H$7),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I42" s="116">
         <f>IF(I41 = 0,
@@ -8920,7 +8920,7 @@
         <f>IF(N41 = 0,
 0,
 IF(N39 = (M$7+N$7),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O42" s="116">
         <f>IF(O41 = 0,
@@ -8938,7 +8938,7 @@
         <f>IF(Q41 = 0,
 0,
 IF(Q39 = (Q$7+R$7),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R42" s="116">
         <f>IF(R41 = 0,
@@ -9036,53 +9036,53 @@
       <c r="AJ42" s="132"/>
       <c r="AK42" s="133">
         <f>SUM(C42:AI42)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL42" s="121"/>
     </row>
     <row r="43" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="204">
         <f>RANK(AL43,$AL$11:$AL$98,)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B43" s="205" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C43" s="217">
         <v>5</v>
       </c>
       <c r="D43" s="218"/>
-      <c r="E43" s="222">
+      <c r="E43" s="219">
+        <v>7</v>
+      </c>
+      <c r="F43" s="218"/>
+      <c r="G43" s="220">
+        <v>5</v>
+      </c>
+      <c r="H43" s="221"/>
+      <c r="I43" s="222">
         <v>6</v>
       </c>
-      <c r="F43" s="218"/>
-      <c r="G43" s="220"/>
-      <c r="H43" s="242">
-        <v>7</v>
-      </c>
-      <c r="I43" s="222"/>
-      <c r="J43" s="221">
-        <v>6</v>
-      </c>
+      <c r="J43" s="221"/>
       <c r="K43" s="223">
         <v>5</v>
       </c>
       <c r="L43" s="221"/>
-      <c r="M43" s="222"/>
-      <c r="N43" s="224">
+      <c r="M43" s="222">
         <v>6</v>
       </c>
+      <c r="N43" s="218"/>
       <c r="O43" s="222">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P43" s="218"/>
-      <c r="Q43" s="220">
-        <v>6</v>
+      <c r="Q43" s="234">
+        <v>7</v>
       </c>
       <c r="R43" s="225"/>
       <c r="S43" s="227">
         <f>SUM(C44:R44)</f>
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="T43" s="217"/>
       <c r="U43" s="221">
@@ -9092,20 +9092,20 @@
         <v>6</v>
       </c>
       <c r="W43" s="221"/>
-      <c r="X43" s="223">
-        <v>5</v>
-      </c>
-      <c r="Y43" s="218"/>
-      <c r="Z43" s="220"/>
-      <c r="AA43" s="221">
+      <c r="X43" s="223"/>
+      <c r="Y43" s="218">
+        <v>6</v>
+      </c>
+      <c r="Z43" s="234">
         <v>7</v>
       </c>
+      <c r="AA43" s="221"/>
       <c r="AB43" s="227">
         <f>SUM(T44:AA44)</f>
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="AC43" s="220">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AD43" s="221"/>
       <c r="AE43" s="223">
@@ -9114,7 +9114,7 @@
       <c r="AF43" s="221"/>
       <c r="AG43" s="227">
         <f>SUM(AC44:AF44)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH43" s="230"/>
       <c r="AI43" s="215"/>
@@ -9124,11 +9124,11 @@
       </c>
       <c r="AK43" s="229">
         <f>MAX($AL$11:$AL$98) - AL43</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AL43" s="227">
         <f>$S43+$AB43+$AG43+$AJ43</f>
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="44" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -9144,17 +9144,17 @@
       <c r="D44" s="74"/>
       <c r="E44" s="114">
         <f>(IF($E43&lt;&gt;"",($E$7*$O$105)+IF($E$7=4,($O$103)+IF($E43=$E$7+$F$7,$O$104,0),0),0)+IF($F43&lt;&gt;"",($F$7*$O$105)+IF($F$7=4,($O$103)+IF($F43=$E$7+$F$7,$O$104,0),0),0))</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F44" s="74"/>
       <c r="G44" s="75">
         <f>(IF($G43&lt;&gt;"",($G$7*$O$105)+IF($G$7=4,($O$103)+IF($G43=$G$7+$H$7,$O$104,0),0),0)+IF($H43&lt;&gt;"",($H$7*$O$105)+IF($H$7=4,($O$103)+IF($H43=$G$7+$H$7,$O$104,0),0),0))</f>
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="H44" s="74"/>
       <c r="I44" s="114">
         <f>(IF($I43&lt;&gt;"",($I$7*$O$105)+IF($I$7=4,($O$103)+IF($I43=$I$7+$J$7,$O$104,0),0),0)+IF($J43&lt;&gt;"",($J$7*$O$105)+IF($J$7=4,($O$103)+IF($J43=$I$7+$J$7,$O$104,0),0),0))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J44" s="76"/>
       <c r="K44" s="77">
@@ -9164,7 +9164,7 @@
       <c r="L44" s="74"/>
       <c r="M44" s="75">
         <f>(IF($M43&lt;&gt;"",($M$7*$O$105)+IF($M$7=4,($O$103)+IF($M43=$M$7+$N$7,$O$104,0),0),0)+IF($N43&lt;&gt;"",($N$7*$O$105)+IF($N$7=4,($O$103)+IF($N43=$M$7+$N$7,$O$104,0),0),0))</f>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="N44" s="140"/>
       <c r="O44" s="75">
@@ -9174,7 +9174,7 @@
       <c r="P44" s="74"/>
       <c r="Q44" s="75">
         <f>(IF($Q43&lt;&gt;"",($Q$7*$O$105)+IF($Q$7=4,($O$103)+IF($Q43=$Q$7+$R$7,$O$104,0),0),0)+IF($R43&lt;&gt;"",($R$7*$O$105)+IF($R$7=4,($O$103)+IF($R43=$Q$7+$R$7,$O$104,0),0),0))</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="R44" s="78"/>
       <c r="S44" s="119"/>
@@ -9190,18 +9190,18 @@
       <c r="W44" s="124"/>
       <c r="X44" s="124">
         <f>(IF($X43&lt;&gt;"",($X$7*$P$105)+IF($X$7=4,($P$103)+IF($X43=$X$7+$Y$7,$P$104,0),0),0)+IF($Y43&lt;&gt;"",($Y$7*$P$105)+IF($Y$7=4,($P$103)+IF($Y43=$X$7+$Y$7,$P$104,0),0),0))</f>
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="Y44" s="59"/>
       <c r="Z44" s="124">
         <f>(IF($Z43&lt;&gt;"",($Z$7*$P$105)+IF($Z$7=4,($P$103)+IF($Z43=$Z$7+$AA$7,$P$104,0),0),0)+IF($AA43&lt;&gt;"",($AA$7*$P$105)+IF($AA$7=4,($P$103)+IF($AA43=$Z$7+$AA$7,$P$104,0),0),0))</f>
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="AA44" s="60"/>
       <c r="AB44" s="119"/>
       <c r="AC44" s="124">
         <f>(IF($AC43&lt;&gt;"",($AC$7*$Q$105)+IF($AC$7=4,($Q$103)+IF($AC43=$AC$7+$AD$7,$Q$104,0),0),0)+IF($AD43&lt;&gt;"",($AD$7*$Q$105)+IF($AD$7=4,($Q$103)+IF($AD43=$AC$7+$AD$7,$Q$104,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD44" s="124"/>
       <c r="AE44" s="124">
@@ -9261,13 +9261,13 @@
         <f>IF(ISBLANK(H43),
 0,
 IF(H$7 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45" s="116">
         <f>IF(ISBLANK(I43),
 0,
 IF(I$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J45" s="116">
         <f>IF(ISBLANK(J43),
@@ -9297,7 +9297,7 @@
         <f>IF(ISBLANK(N43),
 0,
 IF(N$7 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O45" s="116">
         <f>IF(ISBLANK(O43),
@@ -9352,7 +9352,7 @@
         <f>IF(ISBLANK(X43),
 0,
 IF(X$7= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y45" s="116">
         <f>IF(ISBLANK(Y43),
@@ -9364,7 +9364,7 @@
         <f>IF(ISBLANK(Z43),
 0,
 IF(Z$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA45" s="116">
         <f>IF(ISBLANK(AA43),
@@ -9413,7 +9413,7 @@
       <c r="AJ45" s="132"/>
       <c r="AK45" s="133">
         <f>SUM(C45:AI45)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AL45" s="121"/>
     </row>
@@ -9438,7 +9438,7 @@
         <f>IF(E45 = 0,
 0,
 IF(E43 = (E$7+F$7),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46" s="116">
         <f>IF(F45 = 0,
@@ -9456,7 +9456,7 @@
         <f>IF(H45 = 0,
 0,
 IF(H43 = (G$7+H$7),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I46" s="116">
         <f>IF(I45 = 0,
@@ -9492,7 +9492,7 @@
         <f>IF(N45 = 0,
 0,
 IF(N43 = (M$7+N$7),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O46" s="116">
         <f>IF(O45 = 0,
@@ -9510,7 +9510,7 @@
         <f>IF(Q45 = 0,
 0,
 IF(Q43 = (Q$7+R$7),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R46" s="116">
         <f>IF(R45 = 0,
@@ -9559,7 +9559,7 @@
         <f>IF(Z45 = 0,
 0,
 IF(Z43 = (Z$7+AA$7),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA46" s="116">
         <f>IF(AA45 = 0,
@@ -9608,44 +9608,44 @@
       <c r="AJ46" s="132"/>
       <c r="AK46" s="133">
         <f>SUM(C46:AI46)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL46" s="121"/>
     </row>
     <row r="47" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="115">
         <f>RANK(AL47,$AL$11:$AL$98,)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B47" s="82" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C47" s="46">
+        <v>4</v>
+      </c>
+      <c r="D47" s="45"/>
+      <c r="E47" s="44">
         <v>5</v>
-      </c>
-      <c r="D47" s="45"/>
-      <c r="E47" s="199">
-        <v>7</v>
       </c>
       <c r="F47" s="45"/>
       <c r="G47" s="48">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H47" s="47"/>
       <c r="I47" s="44">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J47" s="47"/>
       <c r="K47" s="49">
         <v>5</v>
       </c>
       <c r="L47" s="47"/>
-      <c r="M47" s="44">
+      <c r="M47" s="44"/>
+      <c r="N47" s="45">
+        <v>7</v>
+      </c>
+      <c r="O47" s="44">
         <v>6</v>
-      </c>
-      <c r="N47" s="45"/>
-      <c r="O47" s="44">
-        <v>5</v>
       </c>
       <c r="P47" s="45"/>
       <c r="Q47" s="202">
@@ -9654,7 +9654,7 @@
       <c r="R47" s="50"/>
       <c r="S47" s="120">
         <f>SUM(C48:R48)</f>
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="T47" s="46"/>
       <c r="U47" s="47">
@@ -9668,18 +9668,18 @@
       <c r="Y47" s="45">
         <v>6</v>
       </c>
-      <c r="Z47" s="202">
-        <v>7</v>
+      <c r="Z47" s="48">
+        <v>6</v>
       </c>
       <c r="AA47" s="47"/>
       <c r="AB47" s="120">
         <f>SUM(T48:AA48)</f>
-        <v>23</v>
-      </c>
-      <c r="AC47" s="48">
-        <v>5</v>
-      </c>
-      <c r="AD47" s="47"/>
+        <v>19</v>
+      </c>
+      <c r="AC47" s="48"/>
+      <c r="AD47" s="47">
+        <v>7</v>
+      </c>
       <c r="AE47" s="49">
         <v>6</v>
       </c>
@@ -9696,11 +9696,11 @@
       </c>
       <c r="AK47" s="109">
         <f>MAX($AL$11:$AL$98) - AL47</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AL47" s="120">
         <f>$S47+$AB47+$AG47+$AJ47</f>
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:38" s="27" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -9716,7 +9716,7 @@
       <c r="D48" s="74"/>
       <c r="E48" s="75">
         <f>(IF($E47&lt;&gt;"",($E$7*$O$105)+IF($E$7=4,($O$103)+IF($E47=$E$7+$F$7,$O$104,0),0),0)+IF($F47&lt;&gt;"",($F$7*$O$105)+IF($F$7=4,($O$103)+IF($F47=$E$7+$F$7,$O$104,0),0),0))</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F48" s="74"/>
       <c r="G48" s="75">
@@ -9736,7 +9736,7 @@
       <c r="L48" s="74"/>
       <c r="M48" s="75">
         <f>(IF($M47&lt;&gt;"",($M$7*$O$105)+IF($M$7=4,($O$103)+IF($M47=$M$7+$N$7,$O$104,0),0),0)+IF($N47&lt;&gt;"",($N$7*$O$105)+IF($N$7=4,($O$103)+IF($N47=$M$7+$N$7,$O$104,0),0),0))</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="N48" s="74"/>
       <c r="O48" s="75">
@@ -9767,7 +9767,7 @@
       <c r="Y48" s="59"/>
       <c r="Z48" s="124">
         <f>(IF($Z47&lt;&gt;"",($Z$7*$P$105)+IF($Z$7=4,($P$103)+IF($Z47=$Z$7+$AA$7,$P$104,0),0),0)+IF($AA47&lt;&gt;"",($AA$7*$P$105)+IF($AA$7=4,($P$103)+IF($AA47=$Z$7+$AA$7,$P$104,0),0),0))</f>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AA48" s="60"/>
       <c r="AB48" s="119"/>
@@ -9869,7 +9869,7 @@
         <f>IF(ISBLANK(N47),
 0,
 IF(N$7 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O49" s="116">
         <f>IF(ISBLANK(O47),
@@ -9985,7 +9985,7 @@
       <c r="AJ49" s="132"/>
       <c r="AK49" s="133">
         <f>SUM(C49:AI49)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AL49" s="121"/>
     </row>
@@ -10010,7 +10010,7 @@
         <f>IF(E49 = 0,
 0,
 IF(E47 = (E$7+F$7),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F50" s="116">
         <f>IF(F49 = 0,
@@ -10131,7 +10131,7 @@
         <f>IF(Z49 = 0,
 0,
 IF(Z47 = (Z$7+AA$7),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA50" s="116">
         <f>IF(AA49 = 0,
@@ -10180,14 +10180,14 @@
       <c r="AJ50" s="132"/>
       <c r="AK50" s="133">
         <f>SUM(C50:AI50)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AL50" s="121"/>
     </row>
     <row r="51" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="204">
         <f>RANK(AL51,$AL$11:$AL$98,)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B51" s="205" t="s">
         <v>82</v>
@@ -10258,7 +10258,7 @@
       <c r="AF51" s="221"/>
       <c r="AG51" s="227">
         <f>SUM(AC52:AF52)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH51" s="230"/>
       <c r="AI51" s="215"/>
@@ -10268,11 +10268,11 @@
       </c>
       <c r="AK51" s="229">
         <f>MAX($AL$11:$AL$98) - AL51</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AL51" s="227">
         <f>$S51+$AB51+$AG51+$AJ51</f>
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="52" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -10345,7 +10345,7 @@
       <c r="AB52" s="119"/>
       <c r="AC52" s="124">
         <f>(IF($AC51&lt;&gt;"",($AC$7*$Q$105)+IF($AC$7=4,($Q$103)+IF($AC51=$AC$7+$AD$7,$Q$104,0),0),0)+IF($AD51&lt;&gt;"",($AD$7*$Q$105)+IF($AD$7=4,($Q$103)+IF($AD51=$AC$7+$AD$7,$Q$104,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD52" s="124"/>
       <c r="AE52" s="124">
@@ -10818,7 +10818,7 @@
         <v>23</v>
       </c>
       <c r="AC55" s="48"/>
-      <c r="AD55" s="312">
+      <c r="AD55" s="260">
         <v>5</v>
       </c>
       <c r="AE55" s="49">
@@ -11396,7 +11396,7 @@
       <c r="AF59" s="221"/>
       <c r="AG59" s="227">
         <f>SUM(AC60:AF60)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH59" s="230"/>
       <c r="AI59" s="215"/>
@@ -11406,11 +11406,11 @@
       </c>
       <c r="AK59" s="229">
         <f>MAX($AL$11:$AL$98) - AL59</f>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AL59" s="227">
         <f>$S59+$AB59+$AG59+$AJ59</f>
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="60" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11483,7 +11483,7 @@
       <c r="AB60" s="119"/>
       <c r="AC60" s="124">
         <f>(IF($AC59&lt;&gt;"",($AC$7*$Q$105)+IF($AC$7=4,($Q$103)+IF($AC59=$AC$7+$AD$7,$Q$104,0),0),0)+IF($AD59&lt;&gt;"",($AD$7*$Q$105)+IF($AD$7=4,($Q$103)+IF($AD59=$AC$7+$AD$7,$Q$104,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD60" s="124"/>
       <c r="AE60" s="124">
@@ -11894,21 +11894,21 @@
     <row r="63" spans="1:38" s="27" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="115">
         <f>RANK(AL63,$AL$11:$AL$98,)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B63" s="82" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C63" s="46">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D63" s="45"/>
       <c r="E63" s="44">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F63" s="45"/>
       <c r="G63" s="48">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H63" s="47"/>
       <c r="I63" s="44"/>
@@ -11919,30 +11919,30 @@
         <v>6</v>
       </c>
       <c r="L63" s="47"/>
-      <c r="M63" s="44"/>
-      <c r="N63" s="45">
-        <v>7</v>
-      </c>
+      <c r="M63" s="44">
+        <v>5</v>
+      </c>
+      <c r="N63" s="45"/>
       <c r="O63" s="44">
         <v>6</v>
       </c>
       <c r="P63" s="45"/>
-      <c r="Q63" s="202">
-        <v>7</v>
-      </c>
-      <c r="R63" s="50"/>
+      <c r="Q63" s="48"/>
+      <c r="R63" s="50">
+        <v>6</v>
+      </c>
       <c r="S63" s="120">
         <f>SUM(C64:R64)</f>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="T63" s="46"/>
       <c r="U63" s="47">
+        <v>6</v>
+      </c>
+      <c r="V63" s="44"/>
+      <c r="W63" s="47">
         <v>7</v>
       </c>
-      <c r="V63" s="44">
-        <v>6</v>
-      </c>
-      <c r="W63" s="47"/>
       <c r="X63" s="49"/>
       <c r="Y63" s="45">
         <v>7</v>
@@ -11953,19 +11953,19 @@
       <c r="AA63" s="47"/>
       <c r="AB63" s="120">
         <f>SUM(T64:AA64)</f>
-        <v>19</v>
-      </c>
-      <c r="AC63" s="48"/>
-      <c r="AD63" s="47">
+        <v>33</v>
+      </c>
+      <c r="AC63" s="48">
         <v>7</v>
       </c>
+      <c r="AD63" s="260"/>
       <c r="AE63" s="49"/>
       <c r="AF63" s="47">
         <v>7</v>
       </c>
       <c r="AG63" s="120">
         <f>SUM(AC64:AF64)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH63" s="100"/>
       <c r="AI63" s="57"/>
@@ -12015,7 +12015,7 @@
       <c r="L64" s="125"/>
       <c r="M64" s="123">
         <f>(IF($M63&lt;&gt;"",($M$7*$O$105)+IF($M$7=4,($O$103)+IF($M63=$M$7+$N$7,$O$104,0),0),0)+IF($N63&lt;&gt;"",($N$7*$O$105)+IF($N$7=4,($O$103)+IF($N63=$M$7+$N$7,$O$104,0),0),0))</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="N64" s="125"/>
       <c r="O64" s="126">
@@ -12025,7 +12025,7 @@
       <c r="P64" s="125"/>
       <c r="Q64" s="126">
         <f>(IF($Q63&lt;&gt;"",($Q$7*$O$105)+IF($Q$7=4,($O$103)+IF($Q63=$Q$7+$R$7,$O$104,0),0),0)+IF($R63&lt;&gt;"",($R$7*$O$105)+IF($R$7=4,($O$103)+IF($R63=$Q$7+$R$7,$O$104,0),0),0))</f>
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="R64" s="129"/>
       <c r="S64" s="119"/>
@@ -12036,7 +12036,7 @@
       <c r="U64" s="124"/>
       <c r="V64" s="124">
         <f>(IF($V63&lt;&gt;"",($V$7*$P$105)+IF($V$7=4,($P$103)+IF($V63=$V$7+$W$7,$P$104,0),0),0)+IF($W63&lt;&gt;"",($W$7*$P$105)+IF($W$7=4,($P$103)+IF($W63=$V$7+$W$7,$P$104,0),0),0))</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="W64" s="124"/>
       <c r="X64" s="124">
@@ -12052,7 +12052,7 @@
       <c r="AB64" s="119"/>
       <c r="AC64" s="124">
         <f>(IF($AC63&lt;&gt;"",($AC$7*$Q$105)+IF($AC$7=4,($Q$103)+IF($AC63=$AC$7+$AD$7,$Q$104,0),0),0)+IF($AD63&lt;&gt;"",($AD$7*$Q$105)+IF($AD$7=4,($Q$103)+IF($AD63=$AC$7+$AD$7,$Q$104,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD64" s="124"/>
       <c r="AE64" s="124">
@@ -12145,7 +12145,7 @@
         <f>IF(ISBLANK(N63),
 0,
 IF(N$7 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O65" s="116">
         <f>IF(ISBLANK(O63),
@@ -12163,7 +12163,7 @@
         <f>IF(ISBLANK(Q63),
 0,
 IF(Q$7= 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R65" s="116">
         <f>IF(ISBLANK(R63),
@@ -12194,7 +12194,7 @@
         <f>IF(ISBLANK(W63),
 0,
 IF(W$7 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X65" s="116">
         <f>IF(ISBLANK(X63),
@@ -12261,7 +12261,7 @@
       <c r="AJ65" s="132"/>
       <c r="AK65" s="133">
         <f>SUM(C65:AI65)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AL65" s="121"/>
     </row>
@@ -12358,7 +12358,7 @@
         <f>IF(Q65 = 0,
 0,
 IF(Q63 = (Q$7+R$7),1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R66" s="116">
         <f>IF(R65 = 0,
@@ -12456,28 +12456,28 @@
       <c r="AJ66" s="132"/>
       <c r="AK66" s="133">
         <f>SUM(C66:AI66)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL66" s="121"/>
     </row>
     <row r="67" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="204">
         <f>RANK(AL67,$AL$11:$AL$98,)</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B67" s="205" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="C67" s="217">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D67" s="218"/>
       <c r="E67" s="222">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F67" s="218"/>
       <c r="G67" s="220">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H67" s="221"/>
       <c r="I67" s="222"/>
@@ -12488,30 +12488,30 @@
         <v>6</v>
       </c>
       <c r="L67" s="221"/>
-      <c r="M67" s="222">
-        <v>5</v>
-      </c>
-      <c r="N67" s="218"/>
+      <c r="M67" s="222"/>
+      <c r="N67" s="218">
+        <v>7</v>
+      </c>
       <c r="O67" s="222">
         <v>6</v>
       </c>
       <c r="P67" s="218"/>
-      <c r="Q67" s="220"/>
-      <c r="R67" s="225">
-        <v>6</v>
-      </c>
+      <c r="Q67" s="234">
+        <v>7</v>
+      </c>
+      <c r="R67" s="225"/>
       <c r="S67" s="227">
         <f>SUM(C68:R68)</f>
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="T67" s="217"/>
       <c r="U67" s="221">
+        <v>7</v>
+      </c>
+      <c r="V67" s="222">
         <v>6</v>
       </c>
-      <c r="V67" s="222"/>
-      <c r="W67" s="221">
-        <v>7</v>
-      </c>
+      <c r="W67" s="221"/>
       <c r="X67" s="223"/>
       <c r="Y67" s="218">
         <v>7</v>
@@ -12522,12 +12522,12 @@
       <c r="AA67" s="221"/>
       <c r="AB67" s="227">
         <f>SUM(T68:AA68)</f>
-        <v>33</v>
-      </c>
-      <c r="AC67" s="220">
+        <v>19</v>
+      </c>
+      <c r="AC67" s="220"/>
+      <c r="AD67" s="221">
         <v>7</v>
       </c>
-      <c r="AD67" s="313"/>
       <c r="AE67" s="223"/>
       <c r="AF67" s="221">
         <v>7</v>
@@ -12544,11 +12544,11 @@
       </c>
       <c r="AK67" s="229">
         <f>MAX($AL$11:$AL$98) - AL67</f>
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AL67" s="227">
         <f>$S67+$AB67+$AG67+$AJ67</f>
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="68" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -12584,7 +12584,7 @@
       <c r="L68" s="125"/>
       <c r="M68" s="123">
         <f>(IF($M67&lt;&gt;"",($M$7*$O$105)+IF($M$7=4,($O$103)+IF($M67=$M$7+$N$7,$O$104,0),0),0)+IF($N67&lt;&gt;"",($N$7*$O$105)+IF($N$7=4,($O$103)+IF($N67=$M$7+$N$7,$O$104,0),0),0))</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="N68" s="125"/>
       <c r="O68" s="126">
@@ -12594,7 +12594,7 @@
       <c r="P68" s="125"/>
       <c r="Q68" s="126">
         <f>(IF($Q67&lt;&gt;"",($Q$7*$O$105)+IF($Q$7=4,($O$103)+IF($Q67=$Q$7+$R$7,$O$104,0),0),0)+IF($R67&lt;&gt;"",($R$7*$O$105)+IF($R$7=4,($O$103)+IF($R67=$Q$7+$R$7,$O$104,0),0),0))</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="R68" s="129"/>
       <c r="S68" s="119"/>
@@ -12605,7 +12605,7 @@
       <c r="U68" s="124"/>
       <c r="V68" s="124">
         <f>(IF($V67&lt;&gt;"",($V$7*$P$105)+IF($V$7=4,($P$103)+IF($V67=$V$7+$W$7,$P$104,0),0),0)+IF($W67&lt;&gt;"",($W$7*$P$105)+IF($W$7=4,($P$103)+IF($W67=$V$7+$W$7,$P$104,0),0),0))</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="W68" s="124"/>
       <c r="X68" s="124">
@@ -12714,7 +12714,7 @@
         <f>IF(ISBLANK(N67),
 0,
 IF(N$7 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O69" s="116">
         <f>IF(ISBLANK(O67),
@@ -12732,7 +12732,7 @@
         <f>IF(ISBLANK(Q67),
 0,
 IF(Q$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R69" s="116">
         <f>IF(ISBLANK(R67),
@@ -12763,7 +12763,7 @@
         <f>IF(ISBLANK(W67),
 0,
 IF(W$7 = 4, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X69" s="116">
         <f>IF(ISBLANK(X67),
@@ -12830,7 +12830,7 @@
       <c r="AJ69" s="132"/>
       <c r="AK69" s="133">
         <f>SUM(C69:AI69)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AL69" s="121"/>
     </row>
@@ -12927,7 +12927,7 @@
         <f>IF(Q69 = 0,
 0,
 IF(Q67 = (Q$7+R$7),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R70" s="116">
         <f>IF(R69 = 0,
@@ -13025,7 +13025,7 @@
       <c r="AJ70" s="132"/>
       <c r="AK70" s="133">
         <f>SUM(C70:AI70)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL70" s="121"/>
     </row>
@@ -13093,13 +13093,17 @@
         <f>SUM(T72:AA72)</f>
         <v>19</v>
       </c>
-      <c r="AC71" s="48"/>
+      <c r="AC71" s="48">
+        <v>6</v>
+      </c>
       <c r="AD71" s="47"/>
-      <c r="AE71" s="49"/>
+      <c r="AE71" s="49">
+        <v>5</v>
+      </c>
       <c r="AF71" s="47"/>
       <c r="AG71" s="120">
         <f>SUM(AC72:AF72)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH71" s="98"/>
       <c r="AI71" s="58"/>
@@ -13109,11 +13113,11 @@
       </c>
       <c r="AK71" s="109">
         <f>MAX($AL$11:$AL$98) - AL71</f>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AL71" s="120">
         <f>$S71+$AB71+$AG71+$AJ71</f>
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="72" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -13186,7 +13190,7 @@
       <c r="AB72" s="119"/>
       <c r="AC72" s="124">
         <f>(IF($AC71&lt;&gt;"",($AC$7*$Q$105)+IF($AC$7=4,($Q$103)+IF($AC71=$AC$7+$AD$7,$Q$104,0),0),0)+IF($AD71&lt;&gt;"",($AD$7*$Q$105)+IF($AD$7=4,($Q$103)+IF($AD71=$AC$7+$AD$7,$Q$104,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD72" s="124"/>
       <c r="AE72" s="124">
@@ -13668,7 +13672,7 @@
       </c>
       <c r="AG75" s="227">
         <f>SUM(AC76:AF76)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH75" s="231"/>
       <c r="AI75" s="228"/>
@@ -13678,11 +13682,11 @@
       </c>
       <c r="AK75" s="229">
         <f>MAX($AL$11:$AL$98) - AL75</f>
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AL75" s="227">
         <f>$S75+$AB75+$AG75+$AJ75</f>
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="76" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -13755,7 +13759,7 @@
       <c r="AB76" s="119"/>
       <c r="AC76" s="124">
         <f>(IF($AC75&lt;&gt;"",($AC$7*$Q$105)+IF($AC$7=4,($Q$103)+IF($AC75=$AC$7+$AD$7,$Q$104,0),0),0)+IF($AD75&lt;&gt;"",($AD$7*$Q$105)+IF($AD$7=4,($Q$103)+IF($AD75=$AC$7+$AD$7,$Q$104,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD76" s="124"/>
       <c r="AE76" s="124">
@@ -14169,7 +14173,7 @@
         <v>18</v>
       </c>
       <c r="B79" s="82" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="C79" s="46">
         <v>5</v>
@@ -14180,7 +14184,7 @@
         <v>7</v>
       </c>
       <c r="G79" s="48">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H79" s="47"/>
       <c r="I79" s="44"/>
@@ -14188,7 +14192,7 @@
         <v>7</v>
       </c>
       <c r="K79" s="49">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L79" s="47"/>
       <c r="M79" s="44">
@@ -14201,7 +14205,7 @@
       <c r="P79" s="45"/>
       <c r="Q79" s="48"/>
       <c r="R79" s="50">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S79" s="120">
         <f>SUM(C80:R80)</f>
@@ -14212,7 +14216,7 @@
         <v>7</v>
       </c>
       <c r="V79" s="44">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="W79" s="47"/>
       <c r="X79" s="49">
@@ -14227,17 +14231,17 @@
         <f>SUM(T80:AA80)</f>
         <v>30</v>
       </c>
-      <c r="AC79" s="48"/>
-      <c r="AD79" s="47">
+      <c r="AC79" s="48">
         <v>7</v>
       </c>
-      <c r="AE79" s="49">
+      <c r="AD79" s="47"/>
+      <c r="AE79" s="49"/>
+      <c r="AF79" s="47">
         <v>7</v>
       </c>
-      <c r="AF79" s="47"/>
       <c r="AG79" s="120">
         <f>SUM(AC80:AF80)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH79" s="98"/>
       <c r="AI79" s="58"/>
@@ -14247,11 +14251,11 @@
       </c>
       <c r="AK79" s="109">
         <f>MAX($AL$11:$AL$98) - AL79</f>
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AL79" s="120">
         <f>$S79+$AB79+$AG79+$AJ79</f>
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="80" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -14324,7 +14328,7 @@
       <c r="AB80" s="119"/>
       <c r="AC80" s="124">
         <f>(IF($AC79&lt;&gt;"",($AC$7*$Q$105)+IF($AC$7=4,($Q$103)+IF($AC79=$AC$7+$AD$7,$Q$104,0),0),0)+IF($AD79&lt;&gt;"",($AD$7*$Q$105)+IF($AD$7=4,($Q$103)+IF($AD79=$AC$7+$AD$7,$Q$104,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD80" s="124"/>
       <c r="AE80" s="124">
@@ -14735,10 +14739,10 @@
     <row r="83" spans="1:38" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="204">
         <f>RANK(AL83,$AL$11:$AL$98,)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B83" s="205" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C83" s="217">
         <v>5</v>
@@ -14749,7 +14753,7 @@
         <v>7</v>
       </c>
       <c r="G83" s="220">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H83" s="221"/>
       <c r="I83" s="222"/>
@@ -14757,7 +14761,7 @@
         <v>7</v>
       </c>
       <c r="K83" s="223">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L83" s="221"/>
       <c r="M83" s="222">
@@ -14770,7 +14774,7 @@
       <c r="P83" s="218"/>
       <c r="Q83" s="220"/>
       <c r="R83" s="225">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S83" s="227">
         <f>SUM(C84:R84)</f>
@@ -14781,7 +14785,7 @@
         <v>7</v>
       </c>
       <c r="V83" s="222">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="W83" s="221"/>
       <c r="X83" s="223">
@@ -14796,14 +14800,14 @@
         <f>SUM(T84:AA84)</f>
         <v>30</v>
       </c>
-      <c r="AC83" s="220">
+      <c r="AC83" s="220"/>
+      <c r="AD83" s="221">
         <v>7</v>
       </c>
-      <c r="AD83" s="221"/>
-      <c r="AE83" s="223"/>
-      <c r="AF83" s="221">
+      <c r="AE83" s="223">
         <v>7</v>
       </c>
+      <c r="AF83" s="221"/>
       <c r="AG83" s="227">
         <f>SUM(AC84:AF84)</f>
         <v>0</v>
@@ -15375,7 +15379,7 @@
       <c r="AF87" s="47"/>
       <c r="AG87" s="120">
         <f>SUM(AC88:AF88)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH87" s="98"/>
       <c r="AI87" s="58"/>
@@ -15385,11 +15389,11 @@
       </c>
       <c r="AK87" s="109">
         <f>MAX($AL$11:$AL$98) - AL87</f>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AL87" s="120">
         <f>$S87+$AB87+$AG87+$AJ87</f>
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="88" spans="1:38" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -15462,7 +15466,7 @@
       <c r="AB88" s="119"/>
       <c r="AC88" s="124">
         <f>(IF($AC87&lt;&gt;"",($AC$7*$Q$105)+IF($AC$7=4,($Q$103)+IF($AC87=$AC$7+$AD$7,$Q$104,0),0),0)+IF($AD87&lt;&gt;"",($AD$7*$Q$105)+IF($AD$7=4,($Q$103)+IF($AD87=$AC$7+$AD$7,$Q$104,0),0),0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD88" s="124"/>
       <c r="AE88" s="124">
@@ -17111,11 +17115,11 @@
       <c r="AB99" s="99"/>
       <c r="AC99" s="62">
         <f>COUNT(AC11,AC15,AC19,AC23,AC27,AC31,AC35, AC39, AC43,AC47,AC51,AC55,AC59,AC63,AC67,AC71,AC75,AC79,#REF!)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="AD99" s="63">
         <f>COUNT(AD11,AD15,AD19,AD23,AD27,AD31,AD35, AD39, AD43,AD47,AD51,AD55,AD59,AD63,AD67,AD71,AD75,AD79,#REF!)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AE99" s="64">
         <f>COUNT(AE11,AE15,AE19,AE23,AE27,AE31,AE35, AE39, AE43,AE47,AE51,AE55,AE59,AE63,AE67,AE71,AE75,AE79,#REF!)</f>
@@ -17123,7 +17127,7 @@
       </c>
       <c r="AF99" s="65">
         <f>COUNT(AF11,AF15,AF19,AF23,AF27,AF31,AF35, AF39, AF43,AF47,AF51,AF55,AF59,AF63,AF67,AF71,AF75,AF79,#REF!)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AG99" s="99"/>
       <c r="AH99" s="67">
@@ -17141,12 +17145,12 @@
     <row r="101" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B101" s="43"/>
       <c r="N101" s="26"/>
-      <c r="O101" s="297" t="s">
+      <c r="O101" s="294" t="s">
         <v>17</v>
       </c>
-      <c r="P101" s="298"/>
-      <c r="Q101" s="298"/>
-      <c r="R101" s="299"/>
+      <c r="P101" s="295"/>
+      <c r="Q101" s="295"/>
+      <c r="R101" s="296"/>
       <c r="AG101" s="30"/>
       <c r="AH101" s="30"/>
       <c r="AI101" s="30"/>
@@ -17155,21 +17159,21 @@
     </row>
     <row r="102" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A102" s="33"/>
-      <c r="B102" s="287" t="s">
+      <c r="B102" s="284" t="s">
         <v>16</v>
       </c>
-      <c r="C102" s="288"/>
-      <c r="D102" s="288"/>
-      <c r="E102" s="288"/>
-      <c r="F102" s="288"/>
-      <c r="G102" s="288"/>
-      <c r="H102" s="288"/>
-      <c r="I102" s="288"/>
-      <c r="J102" s="288"/>
-      <c r="K102" s="288"/>
-      <c r="L102" s="288"/>
-      <c r="M102" s="288"/>
-      <c r="N102" s="289"/>
+      <c r="C102" s="285"/>
+      <c r="D102" s="285"/>
+      <c r="E102" s="285"/>
+      <c r="F102" s="285"/>
+      <c r="G102" s="285"/>
+      <c r="H102" s="285"/>
+      <c r="I102" s="285"/>
+      <c r="J102" s="285"/>
+      <c r="K102" s="285"/>
+      <c r="L102" s="285"/>
+      <c r="M102" s="285"/>
+      <c r="N102" s="286"/>
       <c r="O102" s="21">
         <v>1</v>
       </c>
@@ -17182,45 +17186,45 @@
       <c r="R102" s="22">
         <v>4</v>
       </c>
-      <c r="U102" s="300" t="s">
+      <c r="U102" s="297" t="s">
         <v>26</v>
       </c>
-      <c r="V102" s="301"/>
-      <c r="W102" s="301"/>
-      <c r="X102" s="301"/>
-      <c r="Y102" s="301"/>
-      <c r="Z102" s="301"/>
-      <c r="AA102" s="301"/>
-      <c r="AB102" s="301"/>
-      <c r="AC102" s="301"/>
-      <c r="AD102" s="302"/>
+      <c r="V102" s="298"/>
+      <c r="W102" s="298"/>
+      <c r="X102" s="298"/>
+      <c r="Y102" s="298"/>
+      <c r="Z102" s="298"/>
+      <c r="AA102" s="298"/>
+      <c r="AB102" s="298"/>
+      <c r="AC102" s="298"/>
+      <c r="AD102" s="299"/>
       <c r="AE102" s="28"/>
       <c r="AF102" s="28"/>
-      <c r="AG102" s="303" t="s">
+      <c r="AG102" s="300" t="s">
         <v>24</v>
       </c>
-      <c r="AH102" s="304"/>
-      <c r="AI102" s="304"/>
-      <c r="AJ102" s="304"/>
-      <c r="AK102" s="305"/>
+      <c r="AH102" s="301"/>
+      <c r="AI102" s="301"/>
+      <c r="AJ102" s="301"/>
+      <c r="AK102" s="302"/>
     </row>
     <row r="103" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A103" s="34"/>
-      <c r="B103" s="277" t="s">
+      <c r="B103" s="271" t="s">
         <v>6</v>
       </c>
-      <c r="C103" s="278"/>
-      <c r="D103" s="278"/>
-      <c r="E103" s="278"/>
-      <c r="F103" s="278"/>
-      <c r="G103" s="278"/>
-      <c r="H103" s="278"/>
-      <c r="I103" s="278"/>
-      <c r="J103" s="278"/>
-      <c r="K103" s="278"/>
-      <c r="L103" s="278"/>
-      <c r="M103" s="278"/>
-      <c r="N103" s="279"/>
+      <c r="C103" s="265"/>
+      <c r="D103" s="265"/>
+      <c r="E103" s="265"/>
+      <c r="F103" s="265"/>
+      <c r="G103" s="265"/>
+      <c r="H103" s="265"/>
+      <c r="I103" s="265"/>
+      <c r="J103" s="265"/>
+      <c r="K103" s="265"/>
+      <c r="L103" s="265"/>
+      <c r="M103" s="265"/>
+      <c r="N103" s="266"/>
       <c r="O103" s="20">
         <v>5</v>
       </c>
@@ -17233,49 +17237,49 @@
       <c r="R103" s="23">
         <v>20</v>
       </c>
-      <c r="U103" s="292" t="s">
+      <c r="U103" s="289" t="s">
         <v>20</v>
       </c>
-      <c r="V103" s="293"/>
-      <c r="W103" s="293"/>
-      <c r="X103" s="293"/>
-      <c r="Y103" s="293"/>
-      <c r="Z103" s="293"/>
-      <c r="AA103" s="293"/>
-      <c r="AB103" s="290">
+      <c r="V103" s="290"/>
+      <c r="W103" s="290"/>
+      <c r="X103" s="290"/>
+      <c r="Y103" s="290"/>
+      <c r="Z103" s="290"/>
+      <c r="AA103" s="290"/>
+      <c r="AB103" s="287">
         <v>22</v>
       </c>
-      <c r="AC103" s="290"/>
-      <c r="AD103" s="291"/>
+      <c r="AC103" s="287"/>
+      <c r="AD103" s="288"/>
       <c r="AE103" s="29"/>
       <c r="AF103" s="29"/>
-      <c r="AG103" s="306" t="s">
+      <c r="AG103" s="261" t="s">
         <v>21</v>
       </c>
-      <c r="AH103" s="307"/>
-      <c r="AI103" s="307"/>
-      <c r="AJ103" s="308"/>
+      <c r="AH103" s="262"/>
+      <c r="AI103" s="262"/>
+      <c r="AJ103" s="263"/>
       <c r="AK103" s="173">
         <v>230</v>
       </c>
     </row>
     <row r="104" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="34"/>
-      <c r="B104" s="277" t="s">
+      <c r="B104" s="271" t="s">
         <v>5</v>
       </c>
-      <c r="C104" s="278"/>
-      <c r="D104" s="278"/>
-      <c r="E104" s="278"/>
-      <c r="F104" s="278"/>
-      <c r="G104" s="278"/>
-      <c r="H104" s="278"/>
-      <c r="I104" s="278"/>
-      <c r="J104" s="278"/>
-      <c r="K104" s="278"/>
-      <c r="L104" s="278"/>
-      <c r="M104" s="278"/>
-      <c r="N104" s="279"/>
+      <c r="C104" s="265"/>
+      <c r="D104" s="265"/>
+      <c r="E104" s="265"/>
+      <c r="F104" s="265"/>
+      <c r="G104" s="265"/>
+      <c r="H104" s="265"/>
+      <c r="I104" s="265"/>
+      <c r="J104" s="265"/>
+      <c r="K104" s="265"/>
+      <c r="L104" s="265"/>
+      <c r="M104" s="265"/>
+      <c r="N104" s="266"/>
       <c r="O104" s="20">
         <v>2</v>
       </c>
@@ -17288,49 +17292,49 @@
       <c r="R104" s="23">
         <v>8</v>
       </c>
-      <c r="U104" s="282" t="s">
+      <c r="U104" s="267" t="s">
         <v>18</v>
       </c>
-      <c r="V104" s="283"/>
-      <c r="W104" s="283"/>
-      <c r="X104" s="283"/>
-      <c r="Y104" s="283"/>
-      <c r="Z104" s="283"/>
-      <c r="AA104" s="283"/>
-      <c r="AB104" s="310">
+      <c r="V104" s="268"/>
+      <c r="W104" s="268"/>
+      <c r="X104" s="268"/>
+      <c r="Y104" s="268"/>
+      <c r="Z104" s="268"/>
+      <c r="AA104" s="268"/>
+      <c r="AB104" s="269">
         <v>20</v>
       </c>
-      <c r="AC104" s="310"/>
-      <c r="AD104" s="311"/>
+      <c r="AC104" s="269"/>
+      <c r="AD104" s="270"/>
       <c r="AE104" s="29"/>
       <c r="AF104" s="29"/>
-      <c r="AG104" s="309" t="s">
+      <c r="AG104" s="264" t="s">
         <v>22</v>
       </c>
-      <c r="AH104" s="278"/>
-      <c r="AI104" s="278"/>
-      <c r="AJ104" s="279"/>
+      <c r="AH104" s="265"/>
+      <c r="AI104" s="265"/>
+      <c r="AJ104" s="266"/>
       <c r="AK104" s="36">
         <v>115</v>
       </c>
     </row>
     <row r="105" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A105" s="35"/>
-      <c r="B105" s="284" t="s">
+      <c r="B105" s="281" t="s">
         <v>4</v>
       </c>
-      <c r="C105" s="285"/>
-      <c r="D105" s="285"/>
-      <c r="E105" s="285"/>
-      <c r="F105" s="285"/>
-      <c r="G105" s="285"/>
-      <c r="H105" s="285"/>
-      <c r="I105" s="285"/>
-      <c r="J105" s="285"/>
-      <c r="K105" s="285"/>
-      <c r="L105" s="285"/>
-      <c r="M105" s="285"/>
-      <c r="N105" s="286"/>
+      <c r="C105" s="282"/>
+      <c r="D105" s="282"/>
+      <c r="E105" s="282"/>
+      <c r="F105" s="282"/>
+      <c r="G105" s="282"/>
+      <c r="H105" s="282"/>
+      <c r="I105" s="282"/>
+      <c r="J105" s="282"/>
+      <c r="K105" s="282"/>
+      <c r="L105" s="282"/>
+      <c r="M105" s="282"/>
+      <c r="N105" s="283"/>
       <c r="O105" s="3">
         <v>1</v>
       </c>
@@ -17343,51 +17347,51 @@
       <c r="R105" s="24">
         <v>1</v>
       </c>
-      <c r="U105" s="294" t="s">
+      <c r="U105" s="291" t="s">
         <v>19</v>
       </c>
-      <c r="V105" s="281"/>
-      <c r="W105" s="281"/>
-      <c r="X105" s="281"/>
-      <c r="Y105" s="281"/>
-      <c r="Z105" s="281"/>
-      <c r="AA105" s="281"/>
-      <c r="AB105" s="295">
+      <c r="V105" s="273"/>
+      <c r="W105" s="273"/>
+      <c r="X105" s="273"/>
+      <c r="Y105" s="273"/>
+      <c r="Z105" s="273"/>
+      <c r="AA105" s="273"/>
+      <c r="AB105" s="292">
         <f>AB103*AB104</f>
         <v>440</v>
       </c>
-      <c r="AC105" s="295"/>
-      <c r="AD105" s="296"/>
+      <c r="AC105" s="292"/>
+      <c r="AD105" s="293"/>
       <c r="AE105" s="29"/>
       <c r="AF105" s="29"/>
-      <c r="AG105" s="309" t="s">
+      <c r="AG105" s="264" t="s">
         <v>25</v>
       </c>
-      <c r="AH105" s="278"/>
-      <c r="AI105" s="278"/>
-      <c r="AJ105" s="279"/>
+      <c r="AH105" s="265"/>
+      <c r="AI105" s="265"/>
+      <c r="AJ105" s="266"/>
       <c r="AK105" s="36">
         <v>65</v>
       </c>
     </row>
     <row r="106" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG106" s="282" t="s">
+      <c r="AG106" s="267" t="s">
         <v>23</v>
       </c>
-      <c r="AH106" s="283"/>
-      <c r="AI106" s="283"/>
-      <c r="AJ106" s="283"/>
+      <c r="AH106" s="268"/>
+      <c r="AI106" s="268"/>
+      <c r="AJ106" s="268"/>
       <c r="AK106" s="175">
         <v>30</v>
       </c>
     </row>
     <row r="107" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG107" s="280" t="s">
+      <c r="AG107" s="272" t="s">
         <v>19</v>
       </c>
-      <c r="AH107" s="281"/>
-      <c r="AI107" s="281"/>
-      <c r="AJ107" s="281"/>
+      <c r="AH107" s="273"/>
+      <c r="AI107" s="273"/>
+      <c r="AJ107" s="273"/>
       <c r="AK107" s="174">
         <f>SUM(AK103:AK106)</f>
         <v>440</v>
@@ -17399,11 +17403,25 @@
     <sortCondition ref="B11:B95"/>
   </sortState>
   <mergeCells count="40">
-    <mergeCell ref="AG103:AJ103"/>
-    <mergeCell ref="AG105:AJ105"/>
-    <mergeCell ref="AG104:AJ104"/>
-    <mergeCell ref="U104:AA104"/>
-    <mergeCell ref="AB104:AD104"/>
+    <mergeCell ref="C5:S5"/>
+    <mergeCell ref="T5:AB5"/>
+    <mergeCell ref="AC5:AG5"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="AH5:AJ5"/>
+    <mergeCell ref="AG6:AG10"/>
+    <mergeCell ref="AJ6:AJ10"/>
+    <mergeCell ref="X6:AA6"/>
+    <mergeCell ref="AB6:AB10"/>
+    <mergeCell ref="AC6:AD6"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="C1:O1"/>
+    <mergeCell ref="P1:AJ1"/>
+    <mergeCell ref="C4:O4"/>
+    <mergeCell ref="P4:AJ4"/>
+    <mergeCell ref="C3:P3"/>
+    <mergeCell ref="Q3:AJ3"/>
+    <mergeCell ref="C2:P2"/>
+    <mergeCell ref="Q2:AJ2"/>
     <mergeCell ref="B104:N104"/>
     <mergeCell ref="AG107:AJ107"/>
     <mergeCell ref="AG106:AJ106"/>
@@ -17420,25 +17438,11 @@
     <mergeCell ref="O101:R101"/>
     <mergeCell ref="U102:AD102"/>
     <mergeCell ref="AG102:AK102"/>
-    <mergeCell ref="C1:O1"/>
-    <mergeCell ref="P1:AJ1"/>
-    <mergeCell ref="C4:O4"/>
-    <mergeCell ref="P4:AJ4"/>
-    <mergeCell ref="C3:P3"/>
-    <mergeCell ref="Q3:AJ3"/>
-    <mergeCell ref="C2:P2"/>
-    <mergeCell ref="Q2:AJ2"/>
-    <mergeCell ref="C5:S5"/>
-    <mergeCell ref="T5:AB5"/>
-    <mergeCell ref="AC5:AG5"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="AH5:AJ5"/>
-    <mergeCell ref="AG6:AG10"/>
-    <mergeCell ref="AJ6:AJ10"/>
-    <mergeCell ref="X6:AA6"/>
-    <mergeCell ref="AB6:AB10"/>
-    <mergeCell ref="AC6:AD6"/>
-    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="AG103:AJ103"/>
+    <mergeCell ref="AG105:AJ105"/>
+    <mergeCell ref="AG104:AJ104"/>
+    <mergeCell ref="U104:AA104"/>
+    <mergeCell ref="AB104:AD104"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <conditionalFormatting sqref="S11:S16 AB11:AB16 AG11:AG16 AJ11:AJ16 AJ27:AJ28 AG27:AG28 AB27:AB28 S27:S28 AJ23:AJ24 AG23:AG24 AB23:AB24 S23:S24 AJ19:AJ20 AG19:AG20 AB19:AB20 S19:S20 S39:S40 AB39:AB40 AG39:AG40 AJ39:AJ40 S31:S32 AB31:AB32 AG31:AG32 AJ31:AJ32 AJ43:AJ44 AG43:AG44 AB43:AB44 S43:S44 S47:S48 AB47:AB48 AG47:AG48 AJ47:AJ48 AJ51 AG51 AB51 S51 S59 AB59 AG59 AJ59 S55 AB55 AG55 AJ55 AJ63 AG63 AB63 S63 S67 AB67 AG67 AJ67 AJ71 AG71 AB71 S71 S75 AB75 AG75 AJ75 AJ79 AG79 AB79 S79 AJ35:AJ36 AG35:AG36 AB35:AB36 S35:S36">
@@ -17909,17 +17913,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:R95 T11:AA95 AC11:AF95 AH11:AI95">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC96:AF98">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH96:AI98">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18091,7 +18095,7 @@
   <dimension ref="A1:AJ31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+      <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18448,7 +18452,9 @@
       <c r="Z8" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="AA8" s="79"/>
+      <c r="AA8" s="79">
+        <v>5</v>
+      </c>
       <c r="AB8" s="79"/>
       <c r="AC8" s="79"/>
       <c r="AD8" s="79"/>
@@ -18457,7 +18463,7 @@
       <c r="AG8" s="79"/>
       <c r="AH8" s="71">
         <f>IF(AA8&gt;AA9,1,0)+IF(AB8&gt;AB9,1,0)+IF(AC8&gt;AC9,1,0)+IF(AD8&gt;AD9,1,0)+IF(AE8&gt;AE9,1,0)+IF(AF8&gt;AF9,1,0)+IF(AG8&gt;AG9,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI8" s="13"/>
       <c r="AJ8" s="13"/>
@@ -18492,7 +18498,9 @@
       <c r="Z9" s="81" t="s">
         <v>57</v>
       </c>
-      <c r="AA9" s="79"/>
+      <c r="AA9" s="79">
+        <v>2</v>
+      </c>
       <c r="AB9" s="79"/>
       <c r="AC9" s="79"/>
       <c r="AD9" s="79"/>
@@ -19585,102 +19593,102 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C3:I3 C6:I6 O20:U20 C13:I13 AA8:AG8 AA15:AG15 O10:U10 O6:Q6 C10:I10 C24 C20:E20 C17:I17 O24:U24 AA22:AG22 F24:I24 G20:I20 C27:I27 S6:U6">
-    <cfRule type="cellIs" dxfId="22" priority="27" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="27" stopIfTrue="1" operator="greaterThan">
       <formula>C4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:I4 C7:I7 O21:U21 C14:I14 AA9:AG9 AA16:AG16 O11:U11 O7:Q7 C11:I11 C25 C21:E21 C18:I18 O25:U25 AA23:AG23 F25:I25 G21:I21 C28:I28 S7:U7">
-    <cfRule type="cellIs" dxfId="21" priority="28" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="28" stopIfTrue="1" operator="greaterThan">
       <formula>C3</formula>
     </cfRule>
   </conditionalFormatting>
   